<commit_message>
fix the bug that come back if selected out of order and add head_ultrasound pic and format the excel form
</commit_message>
<xml_diff>
--- a/opendatakit.collect2/form-files/neonatal/neonatal.xlsx
+++ b/opendatakit.collect2/form-files/neonatal/neonatal.xlsx
@@ -1,13 +1,13 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
-  <fileVersion appName="xl" lastEdited="5" lowestEdited="5" rupBuild="21721"/>
+  <fileVersion appName="xl" lastEdited="5" lowestEdited="5" rupBuild="22905"/>
   <workbookPr autoCompressPictures="0"/>
   <bookViews>
-    <workbookView xWindow="240" yWindow="240" windowWidth="25360" windowHeight="15300" tabRatio="500"/>
+    <workbookView xWindow="0" yWindow="0" windowWidth="25600" windowHeight="15540" tabRatio="500"/>
   </bookViews>
   <sheets>
-    <sheet name="survey" sheetId="5" r:id="rId1"/>
+    <sheet name="survey" sheetId="1" r:id="rId1"/>
     <sheet name="calculates" sheetId="2" r:id="rId2"/>
     <sheet name="choices" sheetId="3" r:id="rId3"/>
     <sheet name="settings" sheetId="4" r:id="rId4"/>
@@ -22,7 +22,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="141" uniqueCount="106">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="200" uniqueCount="153">
   <si>
     <t>type</t>
   </si>
@@ -231,96 +231,93 @@
     <t>image</t>
   </si>
   <si>
+    <t>selected(data('procedures_menu'), 'intubation')</t>
+  </si>
+  <si>
+    <t>Nutrition</t>
+  </si>
+  <si>
+    <t>nutritions_menu</t>
+  </si>
+  <si>
+    <t>select_one nutritions_menu</t>
+  </si>
+  <si>
+    <t>nutritions</t>
+  </si>
+  <si>
+    <t>Nutritions</t>
+  </si>
+  <si>
+    <t>Watch Video</t>
+  </si>
+  <si>
+    <t>sample_video</t>
+  </si>
+  <si>
+    <t>video</t>
+  </si>
+  <si>
+    <t>selected(data('procedures_menu'), 'lumbar')</t>
+  </si>
+  <si>
+    <t>selected(data('menu'),'procedures')</t>
+  </si>
+  <si>
+    <t>goto diagnostics_end</t>
+  </si>
+  <si>
+    <t>not(selected(data('menu'), 'diagnostics'))</t>
+  </si>
+  <si>
+    <t>label diagnostics_end</t>
+  </si>
+  <si>
+    <t>goto procedures_end</t>
+  </si>
+  <si>
+    <t>not(selected(data('menu'), 'procedures'))</t>
+  </si>
+  <si>
     <t>intubation_link</t>
   </si>
   <si>
+    <t>&lt;a href="http://www.youtube.com/watch?v=z7sog1n4Rgo"&gt;Go to intubation video on Youtube&lt;/a&gt;</t>
+  </si>
+  <si>
+    <t>intubation_img</t>
+  </si>
+  <si>
+    <t>&lt;b&gt;INTUBATION VIDEO&lt;/b&gt;</t>
+  </si>
+  <si>
     <t>intubation_vdo</t>
   </si>
   <si>
-    <t>video</t>
-  </si>
-  <si>
-    <t>&lt;a href="http://www.youtube.com/watch?v=z7sog1n4Rgo"&gt;Go to intubation video on Youtube&lt;/a&gt;</t>
-  </si>
-  <si>
-    <t>intubation_img</t>
-  </si>
-  <si>
-    <t>&lt;b&gt;INTUBATION VIDEO&lt;/b&gt;</t>
-  </si>
-  <si>
-    <t>ballardExam</t>
+    <t>video/video.mp4</t>
+  </si>
+  <si>
+    <t>select_one ballardExam_menu</t>
+  </si>
+  <si>
+    <t>ballardExam_menu</t>
   </si>
   <si>
     <t>Ballard Exam</t>
   </si>
   <si>
-    <t>ballardExam_menu</t>
-  </si>
-  <si>
-    <t>newExam</t>
-  </si>
-  <si>
-    <t>saveExam</t>
-  </si>
-  <si>
-    <t>Start New Exam</t>
-  </si>
-  <si>
-    <t>View Last Exam</t>
-  </si>
-  <si>
-    <t>select_one ballardExam_menu</t>
+    <t>selected(data('procedures_menu'), 'ballardExam')</t>
+  </si>
+  <si>
+    <t>New Exam !!</t>
+  </si>
+  <si>
+    <t>selected(data('ballardExam_menu'), 'newExam')</t>
   </si>
   <si>
     <t>View Last Exam !!</t>
   </si>
   <si>
-    <t>New Exam !!</t>
-  </si>
-  <si>
-    <t>conversionType</t>
-  </si>
-  <si>
-    <t>lbsToKg</t>
-  </si>
-  <si>
-    <t>Imperial to metric</t>
-  </si>
-  <si>
-    <t>Metric to imperial</t>
-  </si>
-  <si>
-    <t>kgToLbs</t>
-  </si>
-  <si>
-    <t>goto diagnostics_end</t>
-  </si>
-  <si>
-    <t>not(selected(data('menu'), 'diagnostics'))</t>
-  </si>
-  <si>
-    <t>label diagnostics_end</t>
-  </si>
-  <si>
-    <t>goto procedures_end</t>
-  </si>
-  <si>
-    <t>not(selected(data('menu'), 'procedures'))</t>
-  </si>
-  <si>
-    <t>selected(data('procedures_menu'), 'intubation')</t>
-  </si>
-  <si>
-    <t>selected(data('procedures_menu'), 'lumbar')</t>
-  </si>
-  <si>
-    <t>selected(data('procedures_menu'), 'ballardExam')</t>
-  </si>
-  <si>
-    <t>selected(data('ballardExam_menu'), 'newExam')</t>
-  </si>
-  <si>
     <t>selected(data('ballardExam_menu'), 'saveExam')</t>
   </si>
   <si>
@@ -336,26 +333,172 @@
     <t>label calculators_end</t>
   </si>
   <si>
-    <t>THE END!</t>
-  </si>
-  <si>
-    <t>video/video.mp4</t>
+    <t>not(selected(data('menu'),'medications'))</t>
+  </si>
+  <si>
+    <t>select_one medications_menu</t>
+  </si>
+  <si>
+    <t>medications_menu</t>
+  </si>
+  <si>
+    <t>Medications</t>
+  </si>
+  <si>
+    <t>dropdown</t>
+  </si>
+  <si>
+    <t>label medications_end</t>
+  </si>
+  <si>
+    <t>goto medications_end</t>
+  </si>
+  <si>
+    <t>medicine_a</t>
+  </si>
+  <si>
+    <t>Medicine_A</t>
+  </si>
+  <si>
+    <t>medicine_b</t>
+  </si>
+  <si>
+    <t>Medicine_B</t>
+  </si>
+  <si>
+    <t>medicine_c</t>
+  </si>
+  <si>
+    <t>Medicine_C</t>
+  </si>
+  <si>
+    <t>medications</t>
+  </si>
+  <si>
+    <t>xray</t>
+  </si>
+  <si>
+    <t>Chest &amp; Abnormal Xray</t>
+  </si>
+  <si>
+    <t>placement</t>
+  </si>
+  <si>
+    <t>Line Placement</t>
+  </si>
+  <si>
+    <t>Head Ultrasound Reference</t>
+  </si>
+  <si>
+    <t xml:space="preserve">note </t>
+  </si>
+  <si>
+    <t>Chest &amp; Abdominal Xray</t>
+  </si>
+  <si>
+    <t>label procedures_begin</t>
+  </si>
+  <si>
+    <t>goto procedures_begin</t>
+  </si>
+  <si>
+    <t>label back_to_main</t>
+  </si>
+  <si>
+    <t>goto back_to_main</t>
+  </si>
+  <si>
+    <t>label diagnostics_begin</t>
+  </si>
+  <si>
+    <t>goto diagnostics_begin</t>
+  </si>
+  <si>
+    <t>selected(data('menu'),'diagnostics')</t>
+  </si>
+  <si>
+    <t>goto calculators_begin</t>
+  </si>
+  <si>
+    <t>selected(data('menu'),'calculators')</t>
+  </si>
+  <si>
+    <t>label calculators_begin</t>
+  </si>
+  <si>
+    <t>goto medications_begin</t>
+  </si>
+  <si>
+    <t>selected(data('menu'), 'medications')</t>
+  </si>
+  <si>
+    <t>lable  medications_begin</t>
+  </si>
+  <si>
+    <t>weight loss</t>
+  </si>
+  <si>
+    <t>Weight Loss Calculators</t>
+  </si>
+  <si>
+    <t>weight converter</t>
+  </si>
+  <si>
+    <t>glucose</t>
+  </si>
+  <si>
+    <t>Weight Convertors Calculators</t>
+  </si>
+  <si>
+    <t>Glucose Infusion Rate Calculator</t>
+  </si>
+  <si>
+    <t>goto nutritions_begin</t>
+  </si>
+  <si>
+    <t>goto nutritions_end</t>
+  </si>
+  <si>
+    <t>selected(data('menu'), 'nutritions')</t>
+  </si>
+  <si>
+    <t>not(selected(data('menu'),'nutritions'))</t>
+  </si>
+  <si>
+    <t>lable  nutritions_begin</t>
+  </si>
+  <si>
+    <t>label nutritions_end</t>
+  </si>
+  <si>
+    <t>selected(data('diagnostic_menu'),'head')</t>
+  </si>
+  <si>
+    <t>selected(data('diagnostic_menu'),'xray')</t>
+  </si>
+  <si>
+    <t>img/head_ultrasound.jpeg</t>
+  </si>
+  <si>
+    <t>selected(data('diagnostic_menu'),'placement')</t>
   </si>
 </sst>
 </file>
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
 <styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <fonts count="5" x14ac:knownFonts="1">
+  <fonts count="7" x14ac:knownFonts="1">
     <font>
       <sz val="10"/>
       <color rgb="FF000000"/>
       <name val="Arial"/>
     </font>
     <font>
-      <sz val="10"/>
-      <color rgb="FF000000"/>
-      <name val="Arial"/>
+      <sz val="12"/>
+      <color theme="1"/>
+      <name val="Calibri"/>
+      <family val="2"/>
+      <scheme val="minor"/>
     </font>
     <font>
       <sz val="10"/>
@@ -374,8 +517,22 @@
       <color theme="11"/>
       <name val="Arial"/>
     </font>
+    <font>
+      <sz val="12"/>
+      <color rgb="FF006100"/>
+      <name val="Calibri"/>
+      <family val="2"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
+      <sz val="12"/>
+      <color rgb="FF9C6500"/>
+      <name val="Calibri"/>
+      <family val="2"/>
+      <scheme val="minor"/>
+    </font>
   </fonts>
-  <fills count="6">
+  <fills count="8">
     <fill>
       <patternFill patternType="none"/>
     </fill>
@@ -384,13 +541,23 @@
     </fill>
     <fill>
       <patternFill patternType="solid">
-        <fgColor theme="6" tint="0.39997558519241921"/>
-        <bgColor indexed="64"/>
+        <fgColor rgb="FFC6EFCE"/>
       </patternFill>
     </fill>
     <fill>
       <patternFill patternType="solid">
-        <fgColor theme="5" tint="0.39997558519241921"/>
+        <fgColor rgb="FFFFEB9C"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="7" tint="0.79998168889431442"/>
+        <bgColor indexed="65"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="6" tint="0.39997558519241921"/>
         <bgColor indexed="64"/>
       </patternFill>
     </fill>
@@ -416,7 +583,7 @@
       <diagonal/>
     </border>
   </borders>
-  <cellStyleXfs count="67">
+  <cellStyleXfs count="64">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
     <xf numFmtId="0" fontId="3" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
     <xf numFmtId="0" fontId="4" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
@@ -428,12 +595,9 @@
     <xf numFmtId="0" fontId="4" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
     <xf numFmtId="0" fontId="3" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
     <xf numFmtId="0" fontId="4" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
-    <xf numFmtId="0" fontId="3" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
-    <xf numFmtId="0" fontId="4" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
-    <xf numFmtId="0" fontId="3" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
-    <xf numFmtId="0" fontId="4" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
-    <xf numFmtId="0" fontId="3" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
-    <xf numFmtId="0" fontId="4" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="5" fillId="2" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="6" fillId="3" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="1" fillId="4" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
     <xf numFmtId="0" fontId="3" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
     <xf numFmtId="0" fontId="4" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
     <xf numFmtId="0" fontId="3" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
@@ -485,34 +649,28 @@
     <xf numFmtId="0" fontId="3" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
     <xf numFmtId="0" fontId="4" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
   </cellStyleXfs>
-  <cellXfs count="14">
+  <cellXfs count="19">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
       <alignment wrapText="1"/>
     </xf>
-    <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyFont="1"/>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" xfId="0" applyFont="1"/>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
+      <alignment wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyFont="1"/>
     <xf numFmtId="0" fontId="2" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
       <alignment wrapText="1"/>
     </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="0" fillId="5" borderId="0" xfId="0" applyFill="1" applyAlignment="1">
       <alignment wrapText="1"/>
     </xf>
-    <xf numFmtId="0" fontId="0" fillId="2" borderId="0" xfId="0" applyFill="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="0" fillId="5" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1">
       <alignment wrapText="1"/>
     </xf>
-    <xf numFmtId="0" fontId="0" fillId="3" borderId="0" xfId="0" applyFill="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="0" fillId="6" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1">
       <alignment wrapText="1"/>
     </xf>
-    <xf numFmtId="0" fontId="0" fillId="2" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1">
-      <alignment wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
-      <alignment wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyFont="1"/>
-    <xf numFmtId="0" fontId="0" fillId="4" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1">
-      <alignment wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1">
       <alignment wrapText="1"/>
     </xf>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1">
@@ -521,77 +679,87 @@
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyFill="1" applyAlignment="1">
       <alignment wrapText="1"/>
     </xf>
-    <xf numFmtId="0" fontId="0" fillId="5" borderId="0" xfId="0" applyFill="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="0" fillId="7" borderId="0" xfId="0" applyFill="1" applyAlignment="1">
       <alignment wrapText="1"/>
     </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
+    <xf numFmtId="0" fontId="5" fillId="2" borderId="0" xfId="11" applyAlignment="1">
+      <alignment wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="5" fillId="2" borderId="0" xfId="11"/>
+    <xf numFmtId="0" fontId="6" fillId="3" borderId="0" xfId="12" applyAlignment="1">
+      <alignment wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="1" fillId="4" borderId="0" xfId="13"/>
+    <xf numFmtId="0" fontId="1" fillId="4" borderId="0" xfId="13" applyAlignment="1">
+      <alignment wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="6" fillId="3" borderId="0" xfId="12"/>
   </cellXfs>
-  <cellStyles count="67">
+  <cellStyles count="64">
+    <cellStyle name="20% - Accent4" xfId="13" builtinId="42"/>
     <cellStyle name="Followed Hyperlink" xfId="2" builtinId="9" hidden="1"/>
     <cellStyle name="Followed Hyperlink" xfId="4" builtinId="9" hidden="1"/>
     <cellStyle name="Followed Hyperlink" xfId="6" builtinId="9" hidden="1"/>
     <cellStyle name="Followed Hyperlink" xfId="8" builtinId="9" hidden="1"/>
     <cellStyle name="Followed Hyperlink" xfId="10" builtinId="9" hidden="1"/>
-    <cellStyle name="Followed Hyperlink" xfId="12" builtinId="9" hidden="1"/>
-    <cellStyle name="Followed Hyperlink" xfId="14" builtinId="9" hidden="1"/>
-    <cellStyle name="Followed Hyperlink" xfId="16" builtinId="9" hidden="1"/>
-    <cellStyle name="Followed Hyperlink" xfId="18" builtinId="9" hidden="1"/>
-    <cellStyle name="Followed Hyperlink" xfId="20" builtinId="9" hidden="1"/>
-    <cellStyle name="Followed Hyperlink" xfId="22" builtinId="9" hidden="1"/>
-    <cellStyle name="Followed Hyperlink" xfId="24" builtinId="9" hidden="1"/>
-    <cellStyle name="Followed Hyperlink" xfId="26" builtinId="9" hidden="1"/>
-    <cellStyle name="Followed Hyperlink" xfId="28" builtinId="9" hidden="1"/>
-    <cellStyle name="Followed Hyperlink" xfId="30" builtinId="9" hidden="1"/>
-    <cellStyle name="Followed Hyperlink" xfId="32" builtinId="9" hidden="1"/>
-    <cellStyle name="Followed Hyperlink" xfId="34" builtinId="9" hidden="1"/>
-    <cellStyle name="Followed Hyperlink" xfId="36" builtinId="9" hidden="1"/>
-    <cellStyle name="Followed Hyperlink" xfId="38" builtinId="9" hidden="1"/>
-    <cellStyle name="Followed Hyperlink" xfId="40" builtinId="9" hidden="1"/>
-    <cellStyle name="Followed Hyperlink" xfId="42" builtinId="9" hidden="1"/>
-    <cellStyle name="Followed Hyperlink" xfId="44" builtinId="9" hidden="1"/>
-    <cellStyle name="Followed Hyperlink" xfId="46" builtinId="9" hidden="1"/>
-    <cellStyle name="Followed Hyperlink" xfId="48" builtinId="9" hidden="1"/>
-    <cellStyle name="Followed Hyperlink" xfId="50" builtinId="9" hidden="1"/>
-    <cellStyle name="Followed Hyperlink" xfId="52" builtinId="9" hidden="1"/>
-    <cellStyle name="Followed Hyperlink" xfId="54" builtinId="9" hidden="1"/>
-    <cellStyle name="Followed Hyperlink" xfId="56" builtinId="9" hidden="1"/>
-    <cellStyle name="Followed Hyperlink" xfId="58" builtinId="9" hidden="1"/>
-    <cellStyle name="Followed Hyperlink" xfId="60" builtinId="9" hidden="1"/>
-    <cellStyle name="Followed Hyperlink" xfId="62" builtinId="9" hidden="1"/>
-    <cellStyle name="Followed Hyperlink" xfId="64" builtinId="9" hidden="1"/>
-    <cellStyle name="Followed Hyperlink" xfId="66" builtinId="9" hidden="1"/>
+    <cellStyle name="Followed Hyperlink" xfId="15" builtinId="9" hidden="1"/>
+    <cellStyle name="Followed Hyperlink" xfId="17" builtinId="9" hidden="1"/>
+    <cellStyle name="Followed Hyperlink" xfId="19" builtinId="9" hidden="1"/>
+    <cellStyle name="Followed Hyperlink" xfId="21" builtinId="9" hidden="1"/>
+    <cellStyle name="Followed Hyperlink" xfId="23" builtinId="9" hidden="1"/>
+    <cellStyle name="Followed Hyperlink" xfId="25" builtinId="9" hidden="1"/>
+    <cellStyle name="Followed Hyperlink" xfId="27" builtinId="9" hidden="1"/>
+    <cellStyle name="Followed Hyperlink" xfId="29" builtinId="9" hidden="1"/>
+    <cellStyle name="Followed Hyperlink" xfId="31" builtinId="9" hidden="1"/>
+    <cellStyle name="Followed Hyperlink" xfId="33" builtinId="9" hidden="1"/>
+    <cellStyle name="Followed Hyperlink" xfId="35" builtinId="9" hidden="1"/>
+    <cellStyle name="Followed Hyperlink" xfId="37" builtinId="9" hidden="1"/>
+    <cellStyle name="Followed Hyperlink" xfId="39" builtinId="9" hidden="1"/>
+    <cellStyle name="Followed Hyperlink" xfId="41" builtinId="9" hidden="1"/>
+    <cellStyle name="Followed Hyperlink" xfId="43" builtinId="9" hidden="1"/>
+    <cellStyle name="Followed Hyperlink" xfId="45" builtinId="9" hidden="1"/>
+    <cellStyle name="Followed Hyperlink" xfId="47" builtinId="9" hidden="1"/>
+    <cellStyle name="Followed Hyperlink" xfId="49" builtinId="9" hidden="1"/>
+    <cellStyle name="Followed Hyperlink" xfId="51" builtinId="9" hidden="1"/>
+    <cellStyle name="Followed Hyperlink" xfId="53" builtinId="9" hidden="1"/>
+    <cellStyle name="Followed Hyperlink" xfId="55" builtinId="9" hidden="1"/>
+    <cellStyle name="Followed Hyperlink" xfId="57" builtinId="9" hidden="1"/>
+    <cellStyle name="Followed Hyperlink" xfId="59" builtinId="9" hidden="1"/>
+    <cellStyle name="Followed Hyperlink" xfId="61" builtinId="9" hidden="1"/>
+    <cellStyle name="Followed Hyperlink" xfId="63" builtinId="9" hidden="1"/>
+    <cellStyle name="Good" xfId="11" builtinId="26"/>
     <cellStyle name="Hyperlink" xfId="1" builtinId="8" hidden="1"/>
     <cellStyle name="Hyperlink" xfId="3" builtinId="8" hidden="1"/>
     <cellStyle name="Hyperlink" xfId="5" builtinId="8" hidden="1"/>
     <cellStyle name="Hyperlink" xfId="7" builtinId="8" hidden="1"/>
     <cellStyle name="Hyperlink" xfId="9" builtinId="8" hidden="1"/>
-    <cellStyle name="Hyperlink" xfId="11" builtinId="8" hidden="1"/>
-    <cellStyle name="Hyperlink" xfId="13" builtinId="8" hidden="1"/>
-    <cellStyle name="Hyperlink" xfId="15" builtinId="8" hidden="1"/>
-    <cellStyle name="Hyperlink" xfId="17" builtinId="8" hidden="1"/>
-    <cellStyle name="Hyperlink" xfId="19" builtinId="8" hidden="1"/>
-    <cellStyle name="Hyperlink" xfId="21" builtinId="8" hidden="1"/>
-    <cellStyle name="Hyperlink" xfId="23" builtinId="8" hidden="1"/>
-    <cellStyle name="Hyperlink" xfId="25" builtinId="8" hidden="1"/>
-    <cellStyle name="Hyperlink" xfId="27" builtinId="8" hidden="1"/>
-    <cellStyle name="Hyperlink" xfId="29" builtinId="8" hidden="1"/>
-    <cellStyle name="Hyperlink" xfId="31" builtinId="8" hidden="1"/>
-    <cellStyle name="Hyperlink" xfId="33" builtinId="8" hidden="1"/>
-    <cellStyle name="Hyperlink" xfId="35" builtinId="8" hidden="1"/>
-    <cellStyle name="Hyperlink" xfId="37" builtinId="8" hidden="1"/>
-    <cellStyle name="Hyperlink" xfId="39" builtinId="8" hidden="1"/>
-    <cellStyle name="Hyperlink" xfId="41" builtinId="8" hidden="1"/>
-    <cellStyle name="Hyperlink" xfId="43" builtinId="8" hidden="1"/>
-    <cellStyle name="Hyperlink" xfId="45" builtinId="8" hidden="1"/>
-    <cellStyle name="Hyperlink" xfId="47" builtinId="8" hidden="1"/>
-    <cellStyle name="Hyperlink" xfId="49" builtinId="8" hidden="1"/>
-    <cellStyle name="Hyperlink" xfId="51" builtinId="8" hidden="1"/>
-    <cellStyle name="Hyperlink" xfId="53" builtinId="8" hidden="1"/>
-    <cellStyle name="Hyperlink" xfId="55" builtinId="8" hidden="1"/>
-    <cellStyle name="Hyperlink" xfId="57" builtinId="8" hidden="1"/>
-    <cellStyle name="Hyperlink" xfId="59" builtinId="8" hidden="1"/>
-    <cellStyle name="Hyperlink" xfId="61" builtinId="8" hidden="1"/>
-    <cellStyle name="Hyperlink" xfId="63" builtinId="8" hidden="1"/>
-    <cellStyle name="Hyperlink" xfId="65" builtinId="8" hidden="1"/>
+    <cellStyle name="Hyperlink" xfId="14" builtinId="8" hidden="1"/>
+    <cellStyle name="Hyperlink" xfId="16" builtinId="8" hidden="1"/>
+    <cellStyle name="Hyperlink" xfId="18" builtinId="8" hidden="1"/>
+    <cellStyle name="Hyperlink" xfId="20" builtinId="8" hidden="1"/>
+    <cellStyle name="Hyperlink" xfId="22" builtinId="8" hidden="1"/>
+    <cellStyle name="Hyperlink" xfId="24" builtinId="8" hidden="1"/>
+    <cellStyle name="Hyperlink" xfId="26" builtinId="8" hidden="1"/>
+    <cellStyle name="Hyperlink" xfId="28" builtinId="8" hidden="1"/>
+    <cellStyle name="Hyperlink" xfId="30" builtinId="8" hidden="1"/>
+    <cellStyle name="Hyperlink" xfId="32" builtinId="8" hidden="1"/>
+    <cellStyle name="Hyperlink" xfId="34" builtinId="8" hidden="1"/>
+    <cellStyle name="Hyperlink" xfId="36" builtinId="8" hidden="1"/>
+    <cellStyle name="Hyperlink" xfId="38" builtinId="8" hidden="1"/>
+    <cellStyle name="Hyperlink" xfId="40" builtinId="8" hidden="1"/>
+    <cellStyle name="Hyperlink" xfId="42" builtinId="8" hidden="1"/>
+    <cellStyle name="Hyperlink" xfId="44" builtinId="8" hidden="1"/>
+    <cellStyle name="Hyperlink" xfId="46" builtinId="8" hidden="1"/>
+    <cellStyle name="Hyperlink" xfId="48" builtinId="8" hidden="1"/>
+    <cellStyle name="Hyperlink" xfId="50" builtinId="8" hidden="1"/>
+    <cellStyle name="Hyperlink" xfId="52" builtinId="8" hidden="1"/>
+    <cellStyle name="Hyperlink" xfId="54" builtinId="8" hidden="1"/>
+    <cellStyle name="Hyperlink" xfId="56" builtinId="8" hidden="1"/>
+    <cellStyle name="Hyperlink" xfId="58" builtinId="8" hidden="1"/>
+    <cellStyle name="Hyperlink" xfId="60" builtinId="8" hidden="1"/>
+    <cellStyle name="Hyperlink" xfId="62" builtinId="8" hidden="1"/>
+    <cellStyle name="Neutral" xfId="12" builtinId="28"/>
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
   </cellStyles>
   <dxfs count="0"/>
@@ -921,22 +1089,22 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <dimension ref="A1:G31"/>
+  <dimension ref="A1:I57"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A8" zoomScale="150" zoomScaleNormal="150" zoomScalePageLayoutView="150" workbookViewId="0">
-      <selection activeCell="C25" sqref="C25"/>
+    <sheetView tabSelected="1" zoomScale="125" zoomScaleNormal="125" zoomScalePageLayoutView="125" workbookViewId="0">
+      <selection activeCell="D10" sqref="D10"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr baseColWidth="10" defaultRowHeight="12" x14ac:dyDescent="0"/>
+  <sheetFormatPr baseColWidth="10" defaultColWidth="11.5" defaultRowHeight="12.75" customHeight="1" x14ac:dyDescent="0"/>
   <cols>
-    <col min="1" max="1" width="19.1640625" customWidth="1"/>
-    <col min="2" max="2" width="10.6640625" bestFit="1" customWidth="1"/>
-    <col min="3" max="3" width="37.5" customWidth="1"/>
-    <col min="4" max="4" width="35.6640625" customWidth="1"/>
-    <col min="5" max="5" width="10.1640625" bestFit="1" customWidth="1"/>
+    <col min="1" max="1" width="27.1640625" customWidth="1"/>
+    <col min="2" max="2" width="18.6640625" customWidth="1"/>
+    <col min="3" max="3" width="25.1640625" customWidth="1"/>
+    <col min="4" max="4" width="32.1640625" customWidth="1"/>
+    <col min="5" max="5" width="15.33203125" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:7">
+    <row r="1" spans="1:9" ht="12">
       <c r="A1" s="1" t="s">
         <v>0</v>
       </c>
@@ -946,164 +1114,157 @@
       <c r="C1" s="1" t="s">
         <v>2</v>
       </c>
-      <c r="D1" s="7" t="s">
+      <c r="D1" s="4" t="s">
         <v>3</v>
       </c>
-      <c r="E1" s="3" t="s">
+      <c r="E1" s="2" t="s">
         <v>67</v>
       </c>
       <c r="F1" t="s">
         <v>68</v>
       </c>
       <c r="G1" t="s">
-        <v>71</v>
-      </c>
-    </row>
-    <row r="2" spans="1:7">
-      <c r="A2" s="8" t="s">
+        <v>77</v>
+      </c>
+    </row>
+    <row r="2" spans="1:9" ht="15">
+      <c r="A2" s="16" t="s">
+        <v>126</v>
+      </c>
+      <c r="B2" s="1"/>
+      <c r="C2" s="3"/>
+      <c r="D2" s="4"/>
+      <c r="E2" s="2"/>
+    </row>
+    <row r="3" spans="1:9" ht="12">
+      <c r="A3" s="3" t="s">
         <v>4</v>
       </c>
-      <c r="B2" s="7" t="s">
+      <c r="B3" s="4" t="s">
         <v>5</v>
       </c>
-      <c r="C2" s="7" t="s">
+      <c r="C3" s="4" t="s">
         <v>6</v>
       </c>
-      <c r="D2" s="7"/>
-      <c r="E2" s="3" t="s">
+      <c r="D3" s="4"/>
+      <c r="E3" s="2" t="s">
         <v>7</v>
       </c>
     </row>
-    <row r="3" spans="1:7">
-      <c r="A3" s="4" t="s">
-        <v>90</v>
-      </c>
-      <c r="B3" s="4"/>
-      <c r="C3" s="4"/>
-      <c r="D3" s="6" t="s">
-        <v>91</v>
-      </c>
-      <c r="E3" s="4"/>
-      <c r="F3" s="4"/>
-      <c r="G3" s="4"/>
-    </row>
-    <row r="4" spans="1:7" ht="24">
-      <c r="A4" s="7" t="s">
-        <v>8</v>
-      </c>
-      <c r="B4" s="7" t="s">
-        <v>9</v>
-      </c>
-      <c r="C4" s="7" t="s">
-        <v>10</v>
-      </c>
-      <c r="D4" s="7"/>
-      <c r="E4" s="3" t="s">
-        <v>7</v>
-      </c>
-    </row>
-    <row r="5" spans="1:7">
+    <row r="4" spans="1:9" ht="12">
+      <c r="A4" s="3"/>
+      <c r="B4" s="4"/>
+      <c r="C4" s="4"/>
+      <c r="D4" s="4"/>
+      <c r="E4" s="2"/>
+    </row>
+    <row r="5" spans="1:9" ht="18" customHeight="1">
       <c r="A5" s="5" t="s">
-        <v>92</v>
+        <v>80</v>
       </c>
       <c r="B5" s="5"/>
       <c r="C5" s="5"/>
-      <c r="D5" s="5"/>
+      <c r="D5" s="6" t="s">
+        <v>81</v>
+      </c>
       <c r="E5" s="5"/>
       <c r="F5" s="5"/>
       <c r="G5" s="5"/>
     </row>
-    <row r="6" spans="1:7">
-      <c r="A6" s="4" t="s">
-        <v>93</v>
-      </c>
-      <c r="B6" s="4"/>
-      <c r="C6" s="4"/>
+    <row r="6" spans="1:9" ht="18" customHeight="1">
+      <c r="A6" s="5" t="s">
+        <v>129</v>
+      </c>
+      <c r="B6" s="5"/>
+      <c r="C6" s="5"/>
       <c r="D6" s="6" t="s">
-        <v>94</v>
-      </c>
-      <c r="E6" s="4"/>
-      <c r="F6" s="4"/>
-      <c r="G6" s="4"/>
-    </row>
-    <row r="7" spans="1:7" ht="24">
-      <c r="A7" t="s">
-        <v>11</v>
-      </c>
-      <c r="B7" t="s">
-        <v>12</v>
-      </c>
-      <c r="C7" t="s">
-        <v>13</v>
-      </c>
-      <c r="D7" s="7"/>
-      <c r="E7" s="3" t="s">
+        <v>130</v>
+      </c>
+      <c r="E6" s="5"/>
+      <c r="F6" s="5"/>
+      <c r="G6" s="5"/>
+    </row>
+    <row r="7" spans="1:9" s="12" customFormat="1" ht="18" customHeight="1">
+      <c r="A7" s="18" t="s">
+        <v>128</v>
+      </c>
+      <c r="B7" s="18"/>
+      <c r="C7" s="18"/>
+      <c r="D7" s="18"/>
+      <c r="E7" s="18"/>
+      <c r="F7" s="18"/>
+      <c r="G7" s="18"/>
+    </row>
+    <row r="8" spans="1:9" s="12" customFormat="1" ht="18" customHeight="1">
+      <c r="A8" t="s">
+        <v>8</v>
+      </c>
+      <c r="B8" t="s">
+        <v>9</v>
+      </c>
+      <c r="C8" t="s">
+        <v>10</v>
+      </c>
+      <c r="D8"/>
+      <c r="E8" t="s">
         <v>7</v>
       </c>
     </row>
-    <row r="8" spans="1:7" ht="24">
-      <c r="A8" s="9" t="s">
-        <v>21</v>
-      </c>
-      <c r="B8" s="10"/>
-      <c r="C8" s="10"/>
-      <c r="D8" s="11" t="s">
-        <v>95</v>
-      </c>
-      <c r="E8" s="10"/>
-      <c r="F8" s="12"/>
-      <c r="G8" s="12"/>
-    </row>
-    <row r="9" spans="1:7" ht="36">
-      <c r="A9" s="7" t="s">
+    <row r="9" spans="1:9" ht="18" customHeight="1">
+      <c r="A9" s="2" t="s">
         <v>17</v>
       </c>
-      <c r="B9" s="3" t="s">
-        <v>69</v>
-      </c>
-      <c r="C9" s="3" t="s">
-        <v>72</v>
-      </c>
-      <c r="D9" s="3"/>
-      <c r="E9" s="7"/>
-    </row>
-    <row r="10" spans="1:7" ht="24">
-      <c r="A10" s="7" t="s">
-        <v>17</v>
-      </c>
-      <c r="B10" s="3" t="s">
-        <v>73</v>
-      </c>
-      <c r="C10" s="3"/>
-      <c r="D10" s="3"/>
-      <c r="E10" s="7"/>
-      <c r="F10" t="s">
-        <v>18</v>
-      </c>
-    </row>
-    <row r="11" spans="1:7">
-      <c r="A11" t="s">
-        <v>17</v>
-      </c>
-      <c r="C11" t="s">
-        <v>74</v>
-      </c>
-    </row>
-    <row r="12" spans="1:7" ht="24">
-      <c r="A12" t="s">
-        <v>17</v>
-      </c>
-      <c r="B12" t="s">
-        <v>70</v>
-      </c>
-      <c r="G12" t="s">
-        <v>105</v>
-      </c>
-    </row>
-    <row r="13" spans="1:7">
-      <c r="A13" s="13" t="s">
-        <v>31</v>
-      </c>
+      <c r="B9" s="2"/>
+      <c r="C9" s="2" t="s">
+        <v>121</v>
+      </c>
+      <c r="D9" s="2" t="s">
+        <v>149</v>
+      </c>
+      <c r="E9" s="2"/>
+      <c r="F9" t="s">
+        <v>151</v>
+      </c>
+    </row>
+    <row r="10" spans="1:9" ht="18" customHeight="1">
+      <c r="A10" s="2" t="s">
+        <v>122</v>
+      </c>
+      <c r="B10" s="4"/>
+      <c r="C10" s="2" t="s">
+        <v>120</v>
+      </c>
+      <c r="D10" s="2" t="s">
+        <v>152</v>
+      </c>
+      <c r="E10" s="2"/>
+    </row>
+    <row r="11" spans="1:9" ht="18" customHeight="1">
+      <c r="A11" s="2" t="s">
+        <v>122</v>
+      </c>
+      <c r="B11" s="4"/>
+      <c r="C11" s="2" t="s">
+        <v>123</v>
+      </c>
+      <c r="D11" s="2" t="s">
+        <v>150</v>
+      </c>
+      <c r="E11" s="2"/>
+    </row>
+    <row r="12" spans="1:9" ht="15">
+      <c r="A12" s="15" t="s">
+        <v>82</v>
+      </c>
+      <c r="B12" s="15"/>
+      <c r="C12" s="15"/>
+      <c r="D12" s="15"/>
+      <c r="E12" s="15"/>
+      <c r="F12" s="15"/>
+      <c r="G12" s="15"/>
+    </row>
+    <row r="13" spans="1:9" ht="15">
+      <c r="A13" s="16"/>
       <c r="B13" s="12"/>
       <c r="C13" s="12"/>
       <c r="D13" s="12"/>
@@ -1111,187 +1272,498 @@
       <c r="F13" s="12"/>
       <c r="G13" s="12"/>
     </row>
-    <row r="15" spans="1:7" ht="24">
-      <c r="A15" s="7" t="s">
+    <row r="14" spans="1:9" s="15" customFormat="1" ht="15">
+      <c r="A14" s="13" t="s">
+        <v>125</v>
+      </c>
+      <c r="B14" s="13"/>
+      <c r="C14" s="13"/>
+      <c r="D14" s="13" t="s">
+        <v>79</v>
+      </c>
+      <c r="E14" s="13"/>
+      <c r="F14" s="13"/>
+      <c r="G14" s="13"/>
+      <c r="H14" s="12"/>
+      <c r="I14" s="12"/>
+    </row>
+    <row r="15" spans="1:9" ht="12">
+      <c r="A15" s="5" t="s">
+        <v>83</v>
+      </c>
+      <c r="B15" s="5"/>
+      <c r="C15" s="5"/>
+      <c r="D15" s="6" t="s">
+        <v>84</v>
+      </c>
+      <c r="E15" s="5"/>
+      <c r="F15" s="5"/>
+      <c r="G15" s="5"/>
+    </row>
+    <row r="16" spans="1:9" ht="15">
+      <c r="A16" s="15" t="s">
+        <v>124</v>
+      </c>
+      <c r="B16" s="15"/>
+      <c r="C16" s="15"/>
+      <c r="D16" s="15"/>
+      <c r="E16" s="15"/>
+      <c r="F16" s="15"/>
+      <c r="G16" s="15"/>
+    </row>
+    <row r="17" spans="1:8" ht="12">
+      <c r="A17" s="12" t="s">
+        <v>11</v>
+      </c>
+      <c r="B17" s="12" t="s">
+        <v>12</v>
+      </c>
+      <c r="C17" s="12" t="s">
+        <v>13</v>
+      </c>
+      <c r="D17" s="12"/>
+      <c r="E17" s="12" t="s">
+        <v>7</v>
+      </c>
+      <c r="F17" s="12"/>
+      <c r="G17" s="12"/>
+    </row>
+    <row r="18" spans="1:8" ht="24">
+      <c r="A18" s="7" t="s">
+        <v>21</v>
+      </c>
+      <c r="B18" s="8"/>
+      <c r="C18" s="8"/>
+      <c r="D18" s="9" t="s">
+        <v>69</v>
+      </c>
+      <c r="E18" s="8"/>
+      <c r="F18" s="10"/>
+      <c r="G18" s="10"/>
+    </row>
+    <row r="19" spans="1:8" ht="12.75" customHeight="1">
+      <c r="A19" s="4" t="s">
         <v>17</v>
       </c>
-      <c r="B15" s="7"/>
-      <c r="C15" s="7" t="s">
+      <c r="B19" s="2" t="s">
+        <v>85</v>
+      </c>
+      <c r="C19" s="2" t="s">
+        <v>86</v>
+      </c>
+      <c r="D19" s="2"/>
+      <c r="E19" s="4"/>
+    </row>
+    <row r="20" spans="1:8" ht="12.75" customHeight="1">
+      <c r="A20" s="4" t="s">
+        <v>17</v>
+      </c>
+      <c r="B20" s="2" t="s">
+        <v>87</v>
+      </c>
+      <c r="C20" s="2"/>
+      <c r="D20" s="2"/>
+      <c r="E20" s="4"/>
+      <c r="F20" t="s">
+        <v>18</v>
+      </c>
+    </row>
+    <row r="21" spans="1:8" ht="12.75" customHeight="1">
+      <c r="A21" t="s">
+        <v>17</v>
+      </c>
+      <c r="C21" t="s">
+        <v>88</v>
+      </c>
+      <c r="D21" s="13"/>
+    </row>
+    <row r="22" spans="1:8" ht="12.75" customHeight="1">
+      <c r="A22" t="s">
+        <v>17</v>
+      </c>
+      <c r="B22" t="s">
+        <v>89</v>
+      </c>
+      <c r="G22" t="s">
+        <v>90</v>
+      </c>
+    </row>
+    <row r="23" spans="1:8" ht="12">
+      <c r="A23" s="11" t="s">
+        <v>31</v>
+      </c>
+      <c r="B23" s="10"/>
+      <c r="C23" s="10"/>
+      <c r="D23" s="10"/>
+      <c r="E23" s="10"/>
+      <c r="F23" s="10"/>
+      <c r="G23" s="10"/>
+    </row>
+    <row r="24" spans="1:8" ht="24">
+      <c r="A24" s="4" t="s">
+        <v>17</v>
+      </c>
+      <c r="B24" s="4"/>
+      <c r="C24" s="4" t="s">
         <v>19</v>
       </c>
-      <c r="D15" s="3" t="s">
+      <c r="D24" s="2" t="s">
+        <v>78</v>
+      </c>
+      <c r="E24" s="4"/>
+      <c r="F24" t="s">
+        <v>20</v>
+      </c>
+    </row>
+    <row r="25" spans="1:8" ht="12"/>
+    <row r="26" spans="1:8" ht="24">
+      <c r="A26" t="s">
+        <v>91</v>
+      </c>
+      <c r="B26" t="s">
+        <v>92</v>
+      </c>
+      <c r="C26" t="s">
+        <v>93</v>
+      </c>
+      <c r="D26" s="2" t="s">
+        <v>94</v>
+      </c>
+      <c r="E26" t="s">
+        <v>7</v>
+      </c>
+    </row>
+    <row r="27" spans="1:8" ht="24">
+      <c r="A27" t="s">
+        <v>17</v>
+      </c>
+      <c r="C27" t="s">
+        <v>95</v>
+      </c>
+      <c r="D27" s="2" t="s">
         <v>96</v>
       </c>
-      <c r="E15" s="7"/>
-      <c r="F15" t="s">
-        <v>20</v>
-      </c>
-    </row>
-    <row r="17" spans="1:7" ht="24">
-      <c r="A17" t="s">
-        <v>82</v>
-      </c>
-      <c r="B17" t="s">
-        <v>77</v>
-      </c>
-      <c r="C17" t="s">
-        <v>76</v>
-      </c>
-      <c r="D17" s="3" t="s">
+    </row>
+    <row r="28" spans="1:8" ht="24">
+      <c r="A28" t="s">
+        <v>17</v>
+      </c>
+      <c r="C28" t="s">
         <v>97</v>
       </c>
-      <c r="E17" t="s">
+      <c r="D28" s="2" t="s">
+        <v>98</v>
+      </c>
+    </row>
+    <row r="29" spans="1:8" ht="15">
+      <c r="A29" s="15" t="s">
+        <v>99</v>
+      </c>
+      <c r="B29" s="15"/>
+      <c r="C29" s="15"/>
+      <c r="D29" s="15"/>
+      <c r="E29" s="15"/>
+      <c r="F29" s="15"/>
+      <c r="G29" s="15"/>
+      <c r="H29" s="12"/>
+    </row>
+    <row r="30" spans="1:8" ht="12">
+      <c r="A30" s="12"/>
+      <c r="B30" s="12"/>
+      <c r="C30" s="12"/>
+      <c r="D30" s="12"/>
+      <c r="E30" s="12"/>
+      <c r="F30" s="12"/>
+      <c r="G30" s="12"/>
+      <c r="H30" s="12"/>
+    </row>
+    <row r="31" spans="1:8" ht="15">
+      <c r="A31" s="14" t="s">
+        <v>131</v>
+      </c>
+      <c r="B31" s="14"/>
+      <c r="C31" s="14"/>
+      <c r="D31" s="13" t="s">
+        <v>132</v>
+      </c>
+      <c r="E31" s="14"/>
+      <c r="F31" s="14"/>
+      <c r="G31" s="14"/>
+      <c r="H31" s="12"/>
+    </row>
+    <row r="32" spans="1:8" ht="12">
+      <c r="A32" s="5" t="s">
+        <v>100</v>
+      </c>
+      <c r="B32" s="5"/>
+      <c r="C32" s="5"/>
+      <c r="D32" s="6" t="s">
+        <v>101</v>
+      </c>
+      <c r="E32" s="5"/>
+      <c r="F32" s="5"/>
+      <c r="G32" s="5"/>
+    </row>
+    <row r="33" spans="1:9" ht="15">
+      <c r="A33" s="15" t="s">
+        <v>133</v>
+      </c>
+      <c r="B33" s="15"/>
+      <c r="C33" s="15"/>
+      <c r="D33" s="15"/>
+      <c r="E33" s="15"/>
+      <c r="F33" s="15"/>
+      <c r="G33" s="15"/>
+    </row>
+    <row r="34" spans="1:9" ht="12">
+      <c r="A34" t="s">
+        <v>14</v>
+      </c>
+      <c r="B34" t="s">
+        <v>15</v>
+      </c>
+      <c r="C34" t="s">
+        <v>16</v>
+      </c>
+      <c r="E34" t="s">
         <v>7</v>
       </c>
-    </row>
-    <row r="18" spans="1:7" ht="24">
-      <c r="A18" t="s">
+      <c r="F34" s="12"/>
+      <c r="G34" s="12"/>
+    </row>
+    <row r="35" spans="1:9" ht="12">
+      <c r="A35" s="4" t="s">
+        <v>21</v>
+      </c>
+      <c r="B35" s="4"/>
+      <c r="C35" s="4"/>
+      <c r="D35" s="4"/>
+      <c r="E35" s="4"/>
+    </row>
+    <row r="36" spans="1:9" ht="12">
+      <c r="A36" s="4" t="s">
+        <v>22</v>
+      </c>
+      <c r="B36" s="4" t="s">
+        <v>23</v>
+      </c>
+      <c r="C36" s="4" t="s">
+        <v>24</v>
+      </c>
+      <c r="D36" s="4"/>
+      <c r="E36" s="4"/>
+    </row>
+    <row r="37" spans="1:9" ht="36">
+      <c r="A37" s="4" t="s">
         <v>17</v>
       </c>
-      <c r="C18" t="s">
-        <v>84</v>
-      </c>
-      <c r="D18" s="3" t="s">
-        <v>98</v>
-      </c>
-    </row>
-    <row r="19" spans="1:7" ht="24">
-      <c r="A19" t="s">
+      <c r="B37" s="4"/>
+      <c r="C37" s="4" t="s">
+        <v>25</v>
+      </c>
+      <c r="D37" s="4" t="s">
+        <v>26</v>
+      </c>
+      <c r="E37" s="4"/>
+    </row>
+    <row r="38" spans="1:9" ht="12">
+      <c r="A38" s="4" t="s">
+        <v>22</v>
+      </c>
+      <c r="B38" s="4" t="s">
+        <v>27</v>
+      </c>
+      <c r="C38" s="4" t="s">
+        <v>28</v>
+      </c>
+      <c r="D38" s="4"/>
+      <c r="E38" s="4"/>
+    </row>
+    <row r="39" spans="1:9" ht="36">
+      <c r="A39" s="4" t="s">
         <v>17</v>
       </c>
-      <c r="C19" t="s">
-        <v>83</v>
-      </c>
-      <c r="D19" s="3" t="s">
-        <v>99</v>
-      </c>
-    </row>
-    <row r="20" spans="1:7">
-      <c r="A20" s="5" t="s">
-        <v>100</v>
-      </c>
-      <c r="B20" s="5"/>
-      <c r="C20" s="5"/>
-      <c r="D20" s="5"/>
-      <c r="E20" s="5"/>
-      <c r="F20" s="5"/>
-      <c r="G20" s="5"/>
-    </row>
-    <row r="21" spans="1:7">
-      <c r="A21" s="4" t="s">
-        <v>101</v>
-      </c>
-      <c r="B21" s="4"/>
-      <c r="C21" s="4"/>
-      <c r="D21" s="6" t="s">
+      <c r="B39" s="4"/>
+      <c r="C39" s="4" t="s">
+        <v>29</v>
+      </c>
+      <c r="D39" s="4" t="s">
+        <v>30</v>
+      </c>
+      <c r="E39" s="4"/>
+      <c r="H39" s="12"/>
+    </row>
+    <row r="40" spans="1:9" ht="12.75" customHeight="1">
+      <c r="A40" s="4" t="s">
+        <v>31</v>
+      </c>
+      <c r="B40" s="4"/>
+      <c r="C40" s="4"/>
+      <c r="D40" s="4"/>
+      <c r="E40" s="4"/>
+    </row>
+    <row r="41" spans="1:9" ht="12.75" customHeight="1">
+      <c r="A41" s="15" t="s">
         <v>102</v>
       </c>
-      <c r="E21" s="4"/>
-      <c r="F21" s="4"/>
-      <c r="G21" s="4"/>
-    </row>
-    <row r="22" spans="1:7" ht="24">
-      <c r="A22" s="7" t="s">
-        <v>14</v>
-      </c>
-      <c r="B22" s="7" t="s">
-        <v>15</v>
-      </c>
-      <c r="C22" s="7" t="s">
-        <v>16</v>
-      </c>
-      <c r="D22" s="7"/>
-      <c r="E22" s="3" t="s">
+      <c r="B41" s="15"/>
+      <c r="C41" s="15"/>
+      <c r="D41" s="15"/>
+      <c r="E41" s="15"/>
+      <c r="F41" s="15"/>
+      <c r="G41" s="15"/>
+    </row>
+    <row r="42" spans="1:9" s="12" customFormat="1" ht="12.75" customHeight="1"/>
+    <row r="43" spans="1:9" s="14" customFormat="1" ht="12.75" customHeight="1">
+      <c r="A43" s="13" t="s">
+        <v>134</v>
+      </c>
+      <c r="D43" s="14" t="s">
+        <v>135</v>
+      </c>
+      <c r="H43" s="12"/>
+      <c r="I43" s="12"/>
+    </row>
+    <row r="44" spans="1:9" ht="12.75" customHeight="1">
+      <c r="A44" s="13" t="s">
+        <v>109</v>
+      </c>
+      <c r="B44" s="14"/>
+      <c r="C44" s="14"/>
+      <c r="D44" s="14" t="s">
+        <v>103</v>
+      </c>
+      <c r="E44" s="14"/>
+      <c r="F44" s="14"/>
+      <c r="G44" s="14"/>
+    </row>
+    <row r="45" spans="1:9" ht="12.75" customHeight="1">
+      <c r="A45" s="15" t="s">
+        <v>136</v>
+      </c>
+      <c r="B45" s="18"/>
+      <c r="C45" s="18"/>
+      <c r="D45" s="18"/>
+      <c r="E45" s="18"/>
+      <c r="F45" s="18"/>
+      <c r="G45" s="18"/>
+    </row>
+    <row r="46" spans="1:9" ht="12.75" customHeight="1">
+      <c r="A46" s="2" t="s">
+        <v>104</v>
+      </c>
+      <c r="B46" s="12" t="s">
+        <v>105</v>
+      </c>
+      <c r="C46" s="12" t="s">
+        <v>106</v>
+      </c>
+      <c r="D46" s="12"/>
+      <c r="E46" s="12" t="s">
+        <v>107</v>
+      </c>
+      <c r="F46" s="12"/>
+      <c r="G46" s="12"/>
+    </row>
+    <row r="47" spans="1:9" ht="12.75" customHeight="1">
+      <c r="A47" s="15" t="s">
+        <v>108</v>
+      </c>
+      <c r="B47" s="18"/>
+      <c r="C47" s="18"/>
+      <c r="D47" s="18"/>
+      <c r="E47" s="18"/>
+      <c r="F47" s="18"/>
+      <c r="G47" s="18"/>
+    </row>
+    <row r="48" spans="1:9" ht="12.75" customHeight="1">
+      <c r="B48" s="12"/>
+      <c r="C48" s="12"/>
+      <c r="D48" s="12"/>
+      <c r="E48" s="12"/>
+      <c r="F48" s="12"/>
+      <c r="G48" s="12"/>
+    </row>
+    <row r="49" spans="1:7" ht="12.75" customHeight="1">
+      <c r="A49" s="13" t="s">
+        <v>143</v>
+      </c>
+      <c r="B49" s="14"/>
+      <c r="C49" s="14"/>
+      <c r="D49" s="14" t="s">
+        <v>145</v>
+      </c>
+      <c r="E49" s="14"/>
+      <c r="F49" s="14"/>
+      <c r="G49" s="14"/>
+    </row>
+    <row r="50" spans="1:7" ht="12.75" customHeight="1">
+      <c r="A50" s="13" t="s">
+        <v>144</v>
+      </c>
+      <c r="B50" s="14"/>
+      <c r="C50" s="14"/>
+      <c r="D50" s="14" t="s">
+        <v>146</v>
+      </c>
+      <c r="E50" s="14"/>
+      <c r="F50" s="14"/>
+      <c r="G50" s="14"/>
+    </row>
+    <row r="51" spans="1:7" ht="12.75" customHeight="1">
+      <c r="A51" s="15" t="s">
+        <v>147</v>
+      </c>
+      <c r="B51" s="18"/>
+      <c r="C51" s="18"/>
+      <c r="D51" s="18"/>
+      <c r="E51" s="18"/>
+      <c r="F51" s="18"/>
+      <c r="G51" s="18"/>
+    </row>
+    <row r="52" spans="1:7" ht="12.75" customHeight="1">
+      <c r="A52" t="s">
+        <v>72</v>
+      </c>
+      <c r="B52" t="s">
+        <v>71</v>
+      </c>
+      <c r="C52" t="s">
+        <v>74</v>
+      </c>
+      <c r="E52" t="s">
         <v>7</v>
       </c>
-    </row>
-    <row r="23" spans="1:7">
-      <c r="A23" s="2" t="s">
-        <v>21</v>
-      </c>
-      <c r="B23" s="2"/>
-      <c r="C23" s="2"/>
-      <c r="D23" s="2"/>
-      <c r="E23" s="2"/>
-    </row>
-    <row r="24" spans="1:7" ht="24">
-      <c r="A24" s="2" t="s">
-        <v>22</v>
-      </c>
-      <c r="B24" s="2" t="s">
-        <v>23</v>
-      </c>
-      <c r="C24" s="2" t="s">
-        <v>24</v>
-      </c>
-      <c r="D24" s="2"/>
-      <c r="E24" s="2"/>
-    </row>
-    <row r="25" spans="1:7" ht="24">
-      <c r="A25" s="2" t="s">
+      <c r="F52" s="12"/>
+      <c r="G52" s="12"/>
+    </row>
+    <row r="53" spans="1:7" ht="12.75" customHeight="1">
+      <c r="A53" s="2" t="s">
         <v>17</v>
       </c>
-      <c r="B25" s="2"/>
-      <c r="C25" s="2" t="s">
-        <v>25</v>
-      </c>
-      <c r="D25" s="2" t="s">
-        <v>26</v>
-      </c>
-      <c r="E25" s="2"/>
-    </row>
-    <row r="26" spans="1:7">
-      <c r="A26" s="2" t="s">
-        <v>22</v>
-      </c>
-      <c r="B26" s="2" t="s">
-        <v>27</v>
-      </c>
-      <c r="C26" s="2" t="s">
-        <v>28</v>
-      </c>
-      <c r="D26" s="2"/>
-      <c r="E26" s="2"/>
-    </row>
-    <row r="27" spans="1:7" ht="24">
-      <c r="A27" s="2" t="s">
-        <v>17</v>
-      </c>
-      <c r="B27" s="2"/>
-      <c r="C27" s="2" t="s">
-        <v>29</v>
-      </c>
-      <c r="D27" s="2" t="s">
-        <v>30</v>
-      </c>
-      <c r="E27" s="2"/>
-    </row>
-    <row r="28" spans="1:7">
-      <c r="A28" s="2" t="s">
-        <v>31</v>
-      </c>
-      <c r="B28" s="2"/>
-      <c r="C28" s="2"/>
-      <c r="D28" s="2"/>
-      <c r="E28" s="2"/>
-    </row>
-    <row r="29" spans="1:7">
-      <c r="A29" s="5" t="s">
-        <v>103</v>
-      </c>
-      <c r="B29" s="5"/>
-      <c r="C29" s="5"/>
-      <c r="D29" s="5"/>
-      <c r="E29" s="5"/>
-      <c r="F29" s="5"/>
-      <c r="G29" s="5"/>
-    </row>
-    <row r="31" spans="1:7">
-      <c r="A31" t="s">
-        <v>17</v>
-      </c>
-      <c r="C31" t="s">
-        <v>104</v>
+      <c r="B53" s="12"/>
+      <c r="C53" s="12" t="s">
+        <v>70</v>
+      </c>
+      <c r="D53" s="12"/>
+      <c r="E53" s="12"/>
+      <c r="F53" s="12"/>
+      <c r="G53" s="12"/>
+    </row>
+    <row r="54" spans="1:7" ht="12.75" customHeight="1">
+      <c r="A54" s="15" t="s">
+        <v>148</v>
+      </c>
+      <c r="B54" s="18"/>
+      <c r="C54" s="18"/>
+      <c r="D54" s="18"/>
+      <c r="E54" s="18"/>
+      <c r="F54" s="18"/>
+      <c r="G54" s="18"/>
+    </row>
+    <row r="57" spans="1:7" ht="12.75" customHeight="1">
+      <c r="A57" s="17" t="s">
+        <v>127</v>
       </c>
     </row>
   </sheetData>
@@ -1368,13 +1840,16 @@
 
 <file path=xl/worksheets/sheet3.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <dimension ref="A1:C17"/>
+  <dimension ref="A1:C28"/>
   <sheetViews>
     <sheetView workbookViewId="0">
-      <selection activeCell="C17" sqref="C17"/>
+      <selection activeCell="C7" sqref="C7"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultColWidth="17.1640625" defaultRowHeight="12.75" customHeight="1" x14ac:dyDescent="0"/>
+  <cols>
+    <col min="3" max="3" width="27.1640625" customWidth="1"/>
+  </cols>
   <sheetData>
     <row r="1" spans="1:3" ht="12.75" customHeight="1">
       <c r="A1" t="s">
@@ -1422,134 +1897,200 @@
     </row>
     <row r="5" spans="1:3" ht="12.75" customHeight="1">
       <c r="A5" t="s">
-        <v>12</v>
+        <v>5</v>
       </c>
       <c r="B5" t="s">
-        <v>46</v>
+        <v>73</v>
       </c>
       <c r="C5" t="s">
-        <v>47</v>
+        <v>74</v>
       </c>
     </row>
     <row r="6" spans="1:3" ht="12.75" customHeight="1">
       <c r="A6" t="s">
-        <v>12</v>
+        <v>5</v>
       </c>
       <c r="B6" t="s">
-        <v>48</v>
+        <v>116</v>
       </c>
       <c r="C6" t="s">
-        <v>49</v>
-      </c>
-    </row>
-    <row r="7" spans="1:3" ht="12.75" customHeight="1">
-      <c r="A7" t="s">
-        <v>12</v>
-      </c>
-      <c r="B7" t="s">
-        <v>75</v>
-      </c>
-      <c r="C7" t="s">
-        <v>76</v>
-      </c>
-    </row>
-    <row r="8" spans="1:3" ht="12.75" customHeight="1">
-      <c r="A8" t="s">
-        <v>77</v>
-      </c>
-      <c r="B8" t="s">
-        <v>78</v>
-      </c>
-      <c r="C8" t="s">
-        <v>80</v>
+        <v>106</v>
       </c>
     </row>
     <row r="9" spans="1:3" ht="12.75" customHeight="1">
       <c r="A9" t="s">
-        <v>77</v>
+        <v>12</v>
       </c>
       <c r="B9" t="s">
-        <v>79</v>
+        <v>46</v>
       </c>
       <c r="C9" t="s">
-        <v>81</v>
+        <v>47</v>
       </c>
     </row>
     <row r="10" spans="1:3" ht="12.75" customHeight="1">
       <c r="A10" t="s">
-        <v>9</v>
+        <v>12</v>
       </c>
       <c r="B10" t="s">
-        <v>50</v>
+        <v>48</v>
       </c>
       <c r="C10" t="s">
-        <v>51</v>
+        <v>49</v>
       </c>
     </row>
     <row r="11" spans="1:3" ht="12.75" customHeight="1">
       <c r="A11" t="s">
-        <v>15</v>
+        <v>12</v>
       </c>
       <c r="B11" t="s">
-        <v>52</v>
+        <v>76</v>
       </c>
       <c r="C11" t="s">
-        <v>53</v>
-      </c>
-    </row>
-    <row r="12" spans="1:3" ht="12.75" customHeight="1">
-      <c r="A12" t="s">
-        <v>15</v>
-      </c>
-      <c r="B12" t="s">
-        <v>54</v>
-      </c>
-      <c r="C12" t="s">
-        <v>55</v>
+        <v>75</v>
+      </c>
+    </row>
+    <row r="13" spans="1:3" ht="12.75" customHeight="1">
+      <c r="A13" t="s">
+        <v>9</v>
+      </c>
+      <c r="B13" t="s">
+        <v>50</v>
+      </c>
+      <c r="C13" t="s">
+        <v>51</v>
       </c>
     </row>
     <row r="14" spans="1:3" ht="12.75" customHeight="1">
       <c r="A14" t="s">
-        <v>56</v>
+        <v>9</v>
       </c>
       <c r="B14" t="s">
-        <v>57</v>
+        <v>119</v>
       </c>
       <c r="C14" t="s">
-        <v>58</v>
+        <v>120</v>
       </c>
     </row>
     <row r="15" spans="1:3" ht="12.75" customHeight="1">
       <c r="A15" t="s">
-        <v>56</v>
+        <v>9</v>
       </c>
       <c r="B15" t="s">
-        <v>59</v>
+        <v>117</v>
       </c>
       <c r="C15" t="s">
-        <v>60</v>
+        <v>118</v>
       </c>
     </row>
     <row r="16" spans="1:3" ht="12.75" customHeight="1">
       <c r="A16" t="s">
-        <v>85</v>
+        <v>15</v>
       </c>
       <c r="B16" t="s">
-        <v>86</v>
+        <v>52</v>
       </c>
       <c r="C16" t="s">
-        <v>87</v>
+        <v>53</v>
       </c>
     </row>
     <row r="17" spans="1:3" ht="12.75" customHeight="1">
       <c r="A17" t="s">
-        <v>85</v>
+        <v>15</v>
       </c>
       <c r="B17" t="s">
-        <v>89</v>
+        <v>54</v>
       </c>
       <c r="C17" t="s">
-        <v>88</v>
+        <v>55</v>
+      </c>
+    </row>
+    <row r="19" spans="1:3" ht="12.75" customHeight="1">
+      <c r="A19" t="s">
+        <v>105</v>
+      </c>
+      <c r="B19" t="s">
+        <v>110</v>
+      </c>
+      <c r="C19" t="s">
+        <v>111</v>
+      </c>
+    </row>
+    <row r="20" spans="1:3" ht="12.75" customHeight="1">
+      <c r="A20" t="s">
+        <v>105</v>
+      </c>
+      <c r="B20" t="s">
+        <v>112</v>
+      </c>
+      <c r="C20" t="s">
+        <v>113</v>
+      </c>
+    </row>
+    <row r="21" spans="1:3" ht="12.75" customHeight="1">
+      <c r="A21" t="s">
+        <v>105</v>
+      </c>
+      <c r="B21" t="s">
+        <v>114</v>
+      </c>
+      <c r="C21" t="s">
+        <v>115</v>
+      </c>
+    </row>
+    <row r="23" spans="1:3" ht="12.75" customHeight="1">
+      <c r="A23" t="s">
+        <v>71</v>
+      </c>
+      <c r="B23" t="s">
+        <v>137</v>
+      </c>
+      <c r="C23" t="s">
+        <v>138</v>
+      </c>
+    </row>
+    <row r="24" spans="1:3" ht="12.75" customHeight="1">
+      <c r="A24" t="s">
+        <v>71</v>
+      </c>
+      <c r="B24" t="s">
+        <v>139</v>
+      </c>
+      <c r="C24" t="s">
+        <v>141</v>
+      </c>
+    </row>
+    <row r="25" spans="1:3" ht="12.75" customHeight="1">
+      <c r="A25" t="s">
+        <v>71</v>
+      </c>
+      <c r="B25" t="s">
+        <v>140</v>
+      </c>
+      <c r="C25" t="s">
+        <v>142</v>
+      </c>
+    </row>
+    <row r="27" spans="1:3" ht="12.75" customHeight="1">
+      <c r="A27" t="s">
+        <v>56</v>
+      </c>
+      <c r="B27" t="s">
+        <v>57</v>
+      </c>
+      <c r="C27" t="s">
+        <v>58</v>
+      </c>
+    </row>
+    <row r="28" spans="1:3" ht="12.75" customHeight="1">
+      <c r="A28" t="s">
+        <v>56</v>
+      </c>
+      <c r="B28" t="s">
+        <v>59</v>
+      </c>
+      <c r="C28" t="s">
+        <v>60</v>
       </c>
     </row>
   </sheetData>

</xml_diff>

<commit_message>
Fix bug of "labe"
</commit_message>
<xml_diff>
--- a/opendatakit.collect2/form-files/neonatal/neonatal.xlsx
+++ b/opendatakit.collect2/form-files/neonatal/neonatal.xlsx
@@ -1,7 +1,7 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
-  <fileVersion appName="xl" lastEdited="5" lowestEdited="5" rupBuild="22905"/>
+  <fileVersion appName="xl" lastEdited="5" lowestEdited="5" rupBuild="21721"/>
   <workbookPr autoCompressPictures="0"/>
   <bookViews>
     <workbookView xWindow="0" yWindow="0" windowWidth="25600" windowHeight="15540" tabRatio="500"/>
@@ -432,9 +432,6 @@
     <t>selected(data('menu'), 'medications')</t>
   </si>
   <si>
-    <t>lable  medications_begin</t>
-  </si>
-  <si>
     <t>weight loss</t>
   </si>
   <si>
@@ -465,9 +462,6 @@
     <t>not(selected(data('menu'),'nutritions'))</t>
   </si>
   <si>
-    <t>lable  nutritions_begin</t>
-  </si>
-  <si>
     <t>label nutritions_end</t>
   </si>
   <si>
@@ -481,6 +475,12 @@
   </si>
   <si>
     <t>selected(data('diagnostic_menu'),'placement')</t>
+  </si>
+  <si>
+    <t>label  medications_begin</t>
+  </si>
+  <si>
+    <t>label nutritions_begin</t>
   </si>
 </sst>
 </file>
@@ -1091,8 +1091,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:I57"/>
   <sheetViews>
-    <sheetView tabSelected="1" zoomScale="125" zoomScaleNormal="125" zoomScalePageLayoutView="125" workbookViewId="0">
-      <selection activeCell="D10" sqref="D10"/>
+    <sheetView tabSelected="1" topLeftCell="A27" zoomScale="125" zoomScaleNormal="125" zoomScalePageLayoutView="125" workbookViewId="0">
+      <selection activeCell="A51" sqref="A51"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultColWidth="11.5" defaultRowHeight="12.75" customHeight="1" x14ac:dyDescent="0"/>
@@ -1219,11 +1219,11 @@
         <v>121</v>
       </c>
       <c r="D9" s="2" t="s">
-        <v>149</v>
+        <v>147</v>
       </c>
       <c r="E9" s="2"/>
       <c r="F9" t="s">
-        <v>151</v>
+        <v>149</v>
       </c>
     </row>
     <row r="10" spans="1:9" ht="18" customHeight="1">
@@ -1235,7 +1235,7 @@
         <v>120</v>
       </c>
       <c r="D10" s="2" t="s">
-        <v>152</v>
+        <v>150</v>
       </c>
       <c r="E10" s="2"/>
     </row>
@@ -1248,7 +1248,7 @@
         <v>123</v>
       </c>
       <c r="D11" s="2" t="s">
-        <v>150</v>
+        <v>148</v>
       </c>
       <c r="E11" s="2"/>
     </row>
@@ -1639,7 +1639,7 @@
     </row>
     <row r="45" spans="1:9" ht="12.75" customHeight="1">
       <c r="A45" s="15" t="s">
-        <v>136</v>
+        <v>151</v>
       </c>
       <c r="B45" s="18"/>
       <c r="C45" s="18"/>
@@ -1686,12 +1686,12 @@
     </row>
     <row r="49" spans="1:7" ht="12.75" customHeight="1">
       <c r="A49" s="13" t="s">
-        <v>143</v>
+        <v>142</v>
       </c>
       <c r="B49" s="14"/>
       <c r="C49" s="14"/>
       <c r="D49" s="14" t="s">
-        <v>145</v>
+        <v>144</v>
       </c>
       <c r="E49" s="14"/>
       <c r="F49" s="14"/>
@@ -1699,12 +1699,12 @@
     </row>
     <row r="50" spans="1:7" ht="12.75" customHeight="1">
       <c r="A50" s="13" t="s">
-        <v>144</v>
+        <v>143</v>
       </c>
       <c r="B50" s="14"/>
       <c r="C50" s="14"/>
       <c r="D50" s="14" t="s">
-        <v>146</v>
+        <v>145</v>
       </c>
       <c r="E50" s="14"/>
       <c r="F50" s="14"/>
@@ -1712,7 +1712,7 @@
     </row>
     <row r="51" spans="1:7" ht="12.75" customHeight="1">
       <c r="A51" s="15" t="s">
-        <v>147</v>
+        <v>152</v>
       </c>
       <c r="B51" s="18"/>
       <c r="C51" s="18"/>
@@ -1752,7 +1752,7 @@
     </row>
     <row r="54" spans="1:7" ht="12.75" customHeight="1">
       <c r="A54" s="15" t="s">
-        <v>148</v>
+        <v>146</v>
       </c>
       <c r="B54" s="18"/>
       <c r="C54" s="18"/>
@@ -2043,10 +2043,10 @@
         <v>71</v>
       </c>
       <c r="B23" t="s">
+        <v>136</v>
+      </c>
+      <c r="C23" t="s">
         <v>137</v>
-      </c>
-      <c r="C23" t="s">
-        <v>138</v>
       </c>
     </row>
     <row r="24" spans="1:3" ht="12.75" customHeight="1">
@@ -2054,10 +2054,10 @@
         <v>71</v>
       </c>
       <c r="B24" t="s">
-        <v>139</v>
+        <v>138</v>
       </c>
       <c r="C24" t="s">
-        <v>141</v>
+        <v>140</v>
       </c>
     </row>
     <row r="25" spans="1:3" ht="12.75" customHeight="1">
@@ -2065,10 +2065,10 @@
         <v>71</v>
       </c>
       <c r="B25" t="s">
-        <v>140</v>
+        <v>139</v>
       </c>
       <c r="C25" t="s">
-        <v>142</v>
+        <v>141</v>
       </c>
     </row>
     <row r="27" spans="1:3" ht="12.75" customHeight="1">

</xml_diff>

<commit_message>
Added a category to ballard exam. removed excel lock files
</commit_message>
<xml_diff>
--- a/opendatakit.collect2/form-files/neonatal/neonatal.xlsx
+++ b/opendatakit.collect2/form-files/neonatal/neonatal.xlsx
@@ -1,16 +1,17 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
-  <fileVersion appName="xl" lastEdited="5" lowestEdited="5" rupBuild="21721"/>
+  <fileVersion appName="xl" lastEdited="5" lowestEdited="5" rupBuild="20910"/>
   <workbookPr autoCompressPictures="0"/>
   <bookViews>
-    <workbookView xWindow="0" yWindow="0" windowWidth="25600" windowHeight="15540" tabRatio="500"/>
+    <workbookView xWindow="2800" yWindow="500" windowWidth="22120" windowHeight="17440" tabRatio="500" activeTab="4"/>
   </bookViews>
   <sheets>
     <sheet name="survey" sheetId="1" r:id="rId1"/>
     <sheet name="calculates" sheetId="2" r:id="rId2"/>
     <sheet name="choices" sheetId="3" r:id="rId3"/>
     <sheet name="settings" sheetId="4" r:id="rId4"/>
+    <sheet name="prompt_types" sheetId="5" r:id="rId5"/>
   </sheets>
   <calcPr calcId="140001" concurrentCalc="0"/>
   <extLst>
@@ -22,7 +23,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="200" uniqueCount="153">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="242" uniqueCount="183">
   <si>
     <t>type</t>
   </si>
@@ -297,30 +298,9 @@
     <t>video/video.mp4</t>
   </si>
   <si>
-    <t>select_one ballardExam_menu</t>
-  </si>
-  <si>
-    <t>ballardExam_menu</t>
-  </si>
-  <si>
     <t>Ballard Exam</t>
   </si>
   <si>
-    <t>selected(data('procedures_menu'), 'ballardExam')</t>
-  </si>
-  <si>
-    <t>New Exam !!</t>
-  </si>
-  <si>
-    <t>selected(data('ballardExam_menu'), 'newExam')</t>
-  </si>
-  <si>
-    <t>View Last Exam !!</t>
-  </si>
-  <si>
-    <t>selected(data('ballardExam_menu'), 'saveExam')</t>
-  </si>
-  <si>
     <t>label procedures_end</t>
   </si>
   <si>
@@ -481,6 +461,117 @@
   </si>
   <si>
     <t>label nutritions_begin</t>
+  </si>
+  <si>
+    <t>ballardExam</t>
+  </si>
+  <si>
+    <t>selected(data('diagnostic_menu'), 'ballardExam')</t>
+  </si>
+  <si>
+    <t>select_one ballard_menu1</t>
+  </si>
+  <si>
+    <t>ballard_menu1</t>
+  </si>
+  <si>
+    <t>posture</t>
+  </si>
+  <si>
+    <t>square</t>
+  </si>
+  <si>
+    <t>arm</t>
+  </si>
+  <si>
+    <t>popliteal</t>
+  </si>
+  <si>
+    <t>scarf</t>
+  </si>
+  <si>
+    <t>heel</t>
+  </si>
+  <si>
+    <t>Posture</t>
+  </si>
+  <si>
+    <t>Square Window</t>
+  </si>
+  <si>
+    <t>Arm Recoil</t>
+  </si>
+  <si>
+    <t>Popliteal Angle</t>
+  </si>
+  <si>
+    <t>Scarf Sign</t>
+  </si>
+  <si>
+    <t>Heel to Ear</t>
+  </si>
+  <si>
+    <t>image_slider posture_slider</t>
+  </si>
+  <si>
+    <t>posture_slider</t>
+  </si>
+  <si>
+    <t>Choose Posture</t>
+  </si>
+  <si>
+    <t>selected(data('ballard_menu1'), 'posture')</t>
+  </si>
+  <si>
+    <t>image_slider square_slider</t>
+  </si>
+  <si>
+    <t>square_slider</t>
+  </si>
+  <si>
+    <t>Choose Square Window</t>
+  </si>
+  <si>
+    <t>selected(data('ballard_menu1'), 'square')</t>
+  </si>
+  <si>
+    <t>posture0</t>
+  </si>
+  <si>
+    <t>img/ballard/posture0.png</t>
+  </si>
+  <si>
+    <t>posture1</t>
+  </si>
+  <si>
+    <t>posture2</t>
+  </si>
+  <si>
+    <t>posture3</t>
+  </si>
+  <si>
+    <t>posture4</t>
+  </si>
+  <si>
+    <t>img/ballard/posture1.png</t>
+  </si>
+  <si>
+    <t>img/ballard/posture2.png</t>
+  </si>
+  <si>
+    <t>img/ballard/posture3.png</t>
+  </si>
+  <si>
+    <t>img/ballard/posture4.png</t>
+  </si>
+  <si>
+    <t>schema.type</t>
+  </si>
+  <si>
+    <t>image_slider</t>
+  </si>
+  <si>
+    <t>string</t>
   </si>
 </sst>
 </file>
@@ -583,7 +674,7 @@
       <diagonal/>
     </border>
   </borders>
-  <cellStyleXfs count="64">
+  <cellStyleXfs count="94">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
     <xf numFmtId="0" fontId="3" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
     <xf numFmtId="0" fontId="4" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
@@ -598,6 +689,36 @@
     <xf numFmtId="0" fontId="5" fillId="2" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
     <xf numFmtId="0" fontId="6" fillId="3" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
     <xf numFmtId="0" fontId="1" fillId="4" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="4" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="4" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="4" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="4" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="4" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="4" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="4" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="4" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="4" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="4" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="4" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="4" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="4" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="4" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="4" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
     <xf numFmtId="0" fontId="3" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
     <xf numFmtId="0" fontId="4" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
     <xf numFmtId="0" fontId="3" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
@@ -696,7 +817,7 @@
     </xf>
     <xf numFmtId="0" fontId="6" fillId="3" borderId="0" xfId="12"/>
   </cellXfs>
-  <cellStyles count="64">
+  <cellStyles count="94">
     <cellStyle name="20% - Accent4" xfId="13" builtinId="42"/>
     <cellStyle name="Followed Hyperlink" xfId="2" builtinId="9" hidden="1"/>
     <cellStyle name="Followed Hyperlink" xfId="4" builtinId="9" hidden="1"/>
@@ -728,6 +849,21 @@
     <cellStyle name="Followed Hyperlink" xfId="59" builtinId="9" hidden="1"/>
     <cellStyle name="Followed Hyperlink" xfId="61" builtinId="9" hidden="1"/>
     <cellStyle name="Followed Hyperlink" xfId="63" builtinId="9" hidden="1"/>
+    <cellStyle name="Followed Hyperlink" xfId="65" builtinId="9" hidden="1"/>
+    <cellStyle name="Followed Hyperlink" xfId="67" builtinId="9" hidden="1"/>
+    <cellStyle name="Followed Hyperlink" xfId="69" builtinId="9" hidden="1"/>
+    <cellStyle name="Followed Hyperlink" xfId="71" builtinId="9" hidden="1"/>
+    <cellStyle name="Followed Hyperlink" xfId="73" builtinId="9" hidden="1"/>
+    <cellStyle name="Followed Hyperlink" xfId="75" builtinId="9" hidden="1"/>
+    <cellStyle name="Followed Hyperlink" xfId="77" builtinId="9" hidden="1"/>
+    <cellStyle name="Followed Hyperlink" xfId="79" builtinId="9" hidden="1"/>
+    <cellStyle name="Followed Hyperlink" xfId="81" builtinId="9" hidden="1"/>
+    <cellStyle name="Followed Hyperlink" xfId="83" builtinId="9" hidden="1"/>
+    <cellStyle name="Followed Hyperlink" xfId="85" builtinId="9" hidden="1"/>
+    <cellStyle name="Followed Hyperlink" xfId="87" builtinId="9" hidden="1"/>
+    <cellStyle name="Followed Hyperlink" xfId="89" builtinId="9" hidden="1"/>
+    <cellStyle name="Followed Hyperlink" xfId="91" builtinId="9" hidden="1"/>
+    <cellStyle name="Followed Hyperlink" xfId="93" builtinId="9" hidden="1"/>
     <cellStyle name="Good" xfId="11" builtinId="26"/>
     <cellStyle name="Hyperlink" xfId="1" builtinId="8" hidden="1"/>
     <cellStyle name="Hyperlink" xfId="3" builtinId="8" hidden="1"/>
@@ -759,6 +895,21 @@
     <cellStyle name="Hyperlink" xfId="58" builtinId="8" hidden="1"/>
     <cellStyle name="Hyperlink" xfId="60" builtinId="8" hidden="1"/>
     <cellStyle name="Hyperlink" xfId="62" builtinId="8" hidden="1"/>
+    <cellStyle name="Hyperlink" xfId="64" builtinId="8" hidden="1"/>
+    <cellStyle name="Hyperlink" xfId="66" builtinId="8" hidden="1"/>
+    <cellStyle name="Hyperlink" xfId="68" builtinId="8" hidden="1"/>
+    <cellStyle name="Hyperlink" xfId="70" builtinId="8" hidden="1"/>
+    <cellStyle name="Hyperlink" xfId="72" builtinId="8" hidden="1"/>
+    <cellStyle name="Hyperlink" xfId="74" builtinId="8" hidden="1"/>
+    <cellStyle name="Hyperlink" xfId="76" builtinId="8" hidden="1"/>
+    <cellStyle name="Hyperlink" xfId="78" builtinId="8" hidden="1"/>
+    <cellStyle name="Hyperlink" xfId="80" builtinId="8" hidden="1"/>
+    <cellStyle name="Hyperlink" xfId="82" builtinId="8" hidden="1"/>
+    <cellStyle name="Hyperlink" xfId="84" builtinId="8" hidden="1"/>
+    <cellStyle name="Hyperlink" xfId="86" builtinId="8" hidden="1"/>
+    <cellStyle name="Hyperlink" xfId="88" builtinId="8" hidden="1"/>
+    <cellStyle name="Hyperlink" xfId="90" builtinId="8" hidden="1"/>
+    <cellStyle name="Hyperlink" xfId="92" builtinId="8" hidden="1"/>
     <cellStyle name="Neutral" xfId="12" builtinId="28"/>
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
   </cellStyles>
@@ -1089,10 +1240,10 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <dimension ref="A1:I57"/>
+  <dimension ref="A1:I60"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A27" zoomScale="125" zoomScaleNormal="125" zoomScalePageLayoutView="125" workbookViewId="0">
-      <selection activeCell="A51" sqref="A51"/>
+    <sheetView zoomScale="150" zoomScaleNormal="150" zoomScalePageLayoutView="150" workbookViewId="0">
+      <selection activeCell="D15" sqref="D15"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultColWidth="11.5" defaultRowHeight="12.75" customHeight="1" x14ac:dyDescent="0"/>
@@ -1104,7 +1255,7 @@
     <col min="5" max="5" width="15.33203125" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:9" ht="12">
+    <row r="1" spans="1:7" ht="12">
       <c r="A1" s="1" t="s">
         <v>0</v>
       </c>
@@ -1127,16 +1278,16 @@
         <v>77</v>
       </c>
     </row>
-    <row r="2" spans="1:9" ht="15">
+    <row r="2" spans="1:7" ht="15">
       <c r="A2" s="16" t="s">
-        <v>126</v>
+        <v>119</v>
       </c>
       <c r="B2" s="1"/>
       <c r="C2" s="3"/>
       <c r="D2" s="4"/>
       <c r="E2" s="2"/>
     </row>
-    <row r="3" spans="1:9" ht="12">
+    <row r="3" spans="1:7" ht="12">
       <c r="A3" s="3" t="s">
         <v>4</v>
       </c>
@@ -1151,14 +1302,14 @@
         <v>7</v>
       </c>
     </row>
-    <row r="4" spans="1:9" ht="12">
+    <row r="4" spans="1:7" ht="12">
       <c r="A4" s="3"/>
       <c r="B4" s="4"/>
       <c r="C4" s="4"/>
       <c r="D4" s="4"/>
       <c r="E4" s="2"/>
     </row>
-    <row r="5" spans="1:9" ht="18" customHeight="1">
+    <row r="5" spans="1:7" ht="18" customHeight="1">
       <c r="A5" s="5" t="s">
         <v>80</v>
       </c>
@@ -1171,22 +1322,22 @@
       <c r="F5" s="5"/>
       <c r="G5" s="5"/>
     </row>
-    <row r="6" spans="1:9" ht="18" customHeight="1">
+    <row r="6" spans="1:7" ht="18" customHeight="1">
       <c r="A6" s="5" t="s">
-        <v>129</v>
+        <v>122</v>
       </c>
       <c r="B6" s="5"/>
       <c r="C6" s="5"/>
       <c r="D6" s="6" t="s">
-        <v>130</v>
+        <v>123</v>
       </c>
       <c r="E6" s="5"/>
       <c r="F6" s="5"/>
       <c r="G6" s="5"/>
     </row>
-    <row r="7" spans="1:9" s="12" customFormat="1" ht="18" customHeight="1">
+    <row r="7" spans="1:7" s="12" customFormat="1" ht="18" customHeight="1">
       <c r="A7" s="18" t="s">
-        <v>128</v>
+        <v>121</v>
       </c>
       <c r="B7" s="18"/>
       <c r="C7" s="18"/>
@@ -1195,7 +1346,7 @@
       <c r="F7" s="18"/>
       <c r="G7" s="18"/>
     </row>
-    <row r="8" spans="1:9" s="12" customFormat="1" ht="18" customHeight="1">
+    <row r="8" spans="1:7" s="12" customFormat="1" ht="18" customHeight="1">
       <c r="A8" t="s">
         <v>8</v>
       </c>
@@ -1210,549 +1361,523 @@
         <v>7</v>
       </c>
     </row>
-    <row r="9" spans="1:9" ht="18" customHeight="1">
+    <row r="9" spans="1:7" ht="18" customHeight="1">
       <c r="A9" s="2" t="s">
         <v>17</v>
       </c>
       <c r="B9" s="2"/>
       <c r="C9" s="2" t="s">
-        <v>121</v>
+        <v>114</v>
       </c>
       <c r="D9" s="2" t="s">
-        <v>147</v>
+        <v>140</v>
       </c>
       <c r="E9" s="2"/>
       <c r="F9" t="s">
-        <v>149</v>
-      </c>
-    </row>
-    <row r="10" spans="1:9" ht="18" customHeight="1">
+        <v>142</v>
+      </c>
+    </row>
+    <row r="10" spans="1:7" ht="18" customHeight="1">
       <c r="A10" s="2" t="s">
-        <v>122</v>
+        <v>115</v>
       </c>
       <c r="B10" s="4"/>
       <c r="C10" s="2" t="s">
-        <v>120</v>
+        <v>113</v>
       </c>
       <c r="D10" s="2" t="s">
-        <v>150</v>
+        <v>143</v>
       </c>
       <c r="E10" s="2"/>
     </row>
-    <row r="11" spans="1:9" ht="18" customHeight="1">
+    <row r="11" spans="1:7" ht="18" customHeight="1">
       <c r="A11" s="2" t="s">
-        <v>122</v>
+        <v>115</v>
       </c>
       <c r="B11" s="4"/>
       <c r="C11" s="2" t="s">
-        <v>123</v>
+        <v>116</v>
       </c>
       <c r="D11" s="2" t="s">
+        <v>141</v>
+      </c>
+      <c r="E11" s="2"/>
+    </row>
+    <row r="12" spans="1:7" ht="24">
+      <c r="A12" t="s">
         <v>148</v>
       </c>
-      <c r="E11" s="2"/>
-    </row>
-    <row r="12" spans="1:9" ht="15">
-      <c r="A12" s="15" t="s">
+      <c r="B12" t="s">
+        <v>149</v>
+      </c>
+      <c r="C12" t="s">
+        <v>91</v>
+      </c>
+      <c r="D12" s="2" t="s">
+        <v>147</v>
+      </c>
+    </row>
+    <row r="13" spans="1:7" ht="11" customHeight="1">
+      <c r="A13" t="s">
+        <v>162</v>
+      </c>
+      <c r="B13" t="s">
+        <v>163</v>
+      </c>
+      <c r="C13" t="s">
+        <v>164</v>
+      </c>
+      <c r="D13" s="2" t="s">
+        <v>165</v>
+      </c>
+    </row>
+    <row r="14" spans="1:7" ht="11" customHeight="1">
+      <c r="A14" t="s">
+        <v>166</v>
+      </c>
+      <c r="B14" t="s">
+        <v>167</v>
+      </c>
+      <c r="C14" t="s">
+        <v>168</v>
+      </c>
+      <c r="D14" s="2" t="s">
+        <v>169</v>
+      </c>
+    </row>
+    <row r="15" spans="1:7" ht="12">
+      <c r="D15" s="2"/>
+    </row>
+    <row r="16" spans="1:7" ht="12">
+      <c r="D16" s="2"/>
+    </row>
+    <row r="17" spans="1:9" ht="12">
+      <c r="D17" s="2"/>
+    </row>
+    <row r="18" spans="1:9" ht="12">
+      <c r="D18" s="2"/>
+    </row>
+    <row r="19" spans="1:9" ht="15">
+      <c r="A19" s="15" t="s">
         <v>82</v>
       </c>
-      <c r="B12" s="15"/>
-      <c r="C12" s="15"/>
-      <c r="D12" s="15"/>
-      <c r="E12" s="15"/>
-      <c r="F12" s="15"/>
-      <c r="G12" s="15"/>
-    </row>
-    <row r="13" spans="1:9" ht="15">
-      <c r="A13" s="16"/>
-      <c r="B13" s="12"/>
-      <c r="C13" s="12"/>
-      <c r="D13" s="12"/>
-      <c r="E13" s="12"/>
-      <c r="F13" s="12"/>
-      <c r="G13" s="12"/>
-    </row>
-    <row r="14" spans="1:9" s="15" customFormat="1" ht="15">
-      <c r="A14" s="13" t="s">
-        <v>125</v>
-      </c>
-      <c r="B14" s="13"/>
-      <c r="C14" s="13"/>
-      <c r="D14" s="13" t="s">
+      <c r="B19" s="15"/>
+      <c r="C19" s="15"/>
+      <c r="D19" s="15"/>
+      <c r="E19" s="15"/>
+      <c r="F19" s="15"/>
+      <c r="G19" s="15"/>
+    </row>
+    <row r="20" spans="1:9" ht="15">
+      <c r="A20" s="16"/>
+      <c r="B20" s="12"/>
+      <c r="C20" s="12"/>
+      <c r="D20" s="12"/>
+      <c r="E20" s="12"/>
+      <c r="F20" s="12"/>
+      <c r="G20" s="12"/>
+    </row>
+    <row r="21" spans="1:9" s="15" customFormat="1" ht="15">
+      <c r="A21" s="13" t="s">
+        <v>118</v>
+      </c>
+      <c r="B21" s="13"/>
+      <c r="C21" s="13"/>
+      <c r="D21" s="13" t="s">
         <v>79</v>
       </c>
-      <c r="E14" s="13"/>
-      <c r="F14" s="13"/>
-      <c r="G14" s="13"/>
-      <c r="H14" s="12"/>
-      <c r="I14" s="12"/>
-    </row>
-    <row r="15" spans="1:9" ht="12">
-      <c r="A15" s="5" t="s">
+      <c r="E21" s="13"/>
+      <c r="F21" s="13"/>
+      <c r="G21" s="13"/>
+      <c r="H21" s="12"/>
+      <c r="I21" s="12"/>
+    </row>
+    <row r="22" spans="1:9" ht="12">
+      <c r="A22" s="5" t="s">
         <v>83</v>
       </c>
-      <c r="B15" s="5"/>
-      <c r="C15" s="5"/>
-      <c r="D15" s="6" t="s">
+      <c r="B22" s="5"/>
+      <c r="C22" s="5"/>
+      <c r="D22" s="6" t="s">
         <v>84</v>
       </c>
-      <c r="E15" s="5"/>
-      <c r="F15" s="5"/>
-      <c r="G15" s="5"/>
-    </row>
-    <row r="16" spans="1:9" ht="15">
-      <c r="A16" s="15" t="s">
-        <v>124</v>
-      </c>
-      <c r="B16" s="15"/>
-      <c r="C16" s="15"/>
-      <c r="D16" s="15"/>
-      <c r="E16" s="15"/>
-      <c r="F16" s="15"/>
-      <c r="G16" s="15"/>
-    </row>
-    <row r="17" spans="1:8" ht="12">
-      <c r="A17" s="12" t="s">
+      <c r="E22" s="5"/>
+      <c r="F22" s="5"/>
+      <c r="G22" s="5"/>
+    </row>
+    <row r="23" spans="1:9" ht="15">
+      <c r="A23" s="15" t="s">
+        <v>117</v>
+      </c>
+      <c r="B23" s="15"/>
+      <c r="C23" s="15"/>
+      <c r="D23" s="15"/>
+      <c r="E23" s="15"/>
+      <c r="F23" s="15"/>
+      <c r="G23" s="15"/>
+    </row>
+    <row r="24" spans="1:9" ht="12">
+      <c r="A24" s="12" t="s">
         <v>11</v>
       </c>
-      <c r="B17" s="12" t="s">
+      <c r="B24" s="12" t="s">
         <v>12</v>
       </c>
-      <c r="C17" s="12" t="s">
+      <c r="C24" s="12" t="s">
         <v>13</v>
       </c>
-      <c r="D17" s="12"/>
-      <c r="E17" s="12" t="s">
+      <c r="D24" s="12"/>
+      <c r="E24" s="12" t="s">
         <v>7</v>
       </c>
-      <c r="F17" s="12"/>
-      <c r="G17" s="12"/>
-    </row>
-    <row r="18" spans="1:8" ht="24">
-      <c r="A18" s="7" t="s">
+      <c r="F24" s="12"/>
+      <c r="G24" s="12"/>
+    </row>
+    <row r="25" spans="1:9" ht="24">
+      <c r="A25" s="7" t="s">
         <v>21</v>
       </c>
-      <c r="B18" s="8"/>
-      <c r="C18" s="8"/>
-      <c r="D18" s="9" t="s">
+      <c r="B25" s="8"/>
+      <c r="C25" s="8"/>
+      <c r="D25" s="9" t="s">
         <v>69</v>
       </c>
-      <c r="E18" s="8"/>
-      <c r="F18" s="10"/>
-      <c r="G18" s="10"/>
-    </row>
-    <row r="19" spans="1:8" ht="12.75" customHeight="1">
-      <c r="A19" s="4" t="s">
+      <c r="E25" s="8"/>
+      <c r="F25" s="10"/>
+      <c r="G25" s="10"/>
+    </row>
+    <row r="26" spans="1:9" ht="12.75" customHeight="1">
+      <c r="A26" s="4" t="s">
         <v>17</v>
       </c>
-      <c r="B19" s="2" t="s">
+      <c r="B26" s="2" t="s">
         <v>85</v>
       </c>
-      <c r="C19" s="2" t="s">
+      <c r="C26" s="2" t="s">
         <v>86</v>
       </c>
-      <c r="D19" s="2"/>
-      <c r="E19" s="4"/>
-    </row>
-    <row r="20" spans="1:8" ht="12.75" customHeight="1">
-      <c r="A20" s="4" t="s">
+      <c r="D26" s="2"/>
+      <c r="E26" s="4"/>
+    </row>
+    <row r="27" spans="1:9" ht="12.75" customHeight="1">
+      <c r="A27" s="4" t="s">
         <v>17</v>
       </c>
-      <c r="B20" s="2" t="s">
+      <c r="B27" s="2" t="s">
         <v>87</v>
       </c>
-      <c r="C20" s="2"/>
-      <c r="D20" s="2"/>
-      <c r="E20" s="4"/>
-      <c r="F20" t="s">
+      <c r="C27" s="2"/>
+      <c r="D27" s="2"/>
+      <c r="E27" s="4"/>
+      <c r="F27" t="s">
         <v>18</v>
       </c>
     </row>
-    <row r="21" spans="1:8" ht="12.75" customHeight="1">
-      <c r="A21" t="s">
-        <v>17</v>
-      </c>
-      <c r="C21" t="s">
-        <v>88</v>
-      </c>
-      <c r="D21" s="13"/>
-    </row>
-    <row r="22" spans="1:8" ht="12.75" customHeight="1">
-      <c r="A22" t="s">
-        <v>17</v>
-      </c>
-      <c r="B22" t="s">
-        <v>89</v>
-      </c>
-      <c r="G22" t="s">
-        <v>90</v>
-      </c>
-    </row>
-    <row r="23" spans="1:8" ht="12">
-      <c r="A23" s="11" t="s">
-        <v>31</v>
-      </c>
-      <c r="B23" s="10"/>
-      <c r="C23" s="10"/>
-      <c r="D23" s="10"/>
-      <c r="E23" s="10"/>
-      <c r="F23" s="10"/>
-      <c r="G23" s="10"/>
-    </row>
-    <row r="24" spans="1:8" ht="24">
-      <c r="A24" s="4" t="s">
-        <v>17</v>
-      </c>
-      <c r="B24" s="4"/>
-      <c r="C24" s="4" t="s">
-        <v>19</v>
-      </c>
-      <c r="D24" s="2" t="s">
-        <v>78</v>
-      </c>
-      <c r="E24" s="4"/>
-      <c r="F24" t="s">
-        <v>20</v>
-      </c>
-    </row>
-    <row r="25" spans="1:8" ht="12"/>
-    <row r="26" spans="1:8" ht="24">
-      <c r="A26" t="s">
-        <v>91</v>
-      </c>
-      <c r="B26" t="s">
-        <v>92</v>
-      </c>
-      <c r="C26" t="s">
-        <v>93</v>
-      </c>
-      <c r="D26" s="2" t="s">
-        <v>94</v>
-      </c>
-      <c r="E26" t="s">
-        <v>7</v>
-      </c>
-    </row>
-    <row r="27" spans="1:8" ht="24">
-      <c r="A27" t="s">
-        <v>17</v>
-      </c>
-      <c r="C27" t="s">
-        <v>95</v>
-      </c>
-      <c r="D27" s="2" t="s">
-        <v>96</v>
-      </c>
-    </row>
-    <row r="28" spans="1:8" ht="24">
+    <row r="28" spans="1:9" ht="12.75" customHeight="1">
       <c r="A28" t="s">
         <v>17</v>
       </c>
       <c r="C28" t="s">
-        <v>97</v>
-      </c>
-      <c r="D28" s="2" t="s">
-        <v>98</v>
-      </c>
-    </row>
-    <row r="29" spans="1:8" ht="15">
-      <c r="A29" s="15" t="s">
-        <v>99</v>
-      </c>
-      <c r="B29" s="15"/>
-      <c r="C29" s="15"/>
-      <c r="D29" s="15"/>
-      <c r="E29" s="15"/>
-      <c r="F29" s="15"/>
-      <c r="G29" s="15"/>
-      <c r="H29" s="12"/>
-    </row>
-    <row r="30" spans="1:8" ht="12">
-      <c r="A30" s="12"/>
-      <c r="B30" s="12"/>
-      <c r="C30" s="12"/>
-      <c r="D30" s="12"/>
-      <c r="E30" s="12"/>
-      <c r="F30" s="12"/>
-      <c r="G30" s="12"/>
-      <c r="H30" s="12"/>
-    </row>
-    <row r="31" spans="1:8" ht="15">
-      <c r="A31" s="14" t="s">
-        <v>131</v>
-      </c>
-      <c r="B31" s="14"/>
-      <c r="C31" s="14"/>
-      <c r="D31" s="13" t="s">
-        <v>132</v>
-      </c>
-      <c r="E31" s="14"/>
-      <c r="F31" s="14"/>
-      <c r="G31" s="14"/>
-      <c r="H31" s="12"/>
-    </row>
-    <row r="32" spans="1:8" ht="12">
-      <c r="A32" s="5" t="s">
-        <v>100</v>
-      </c>
-      <c r="B32" s="5"/>
-      <c r="C32" s="5"/>
-      <c r="D32" s="6" t="s">
-        <v>101</v>
-      </c>
-      <c r="E32" s="5"/>
-      <c r="F32" s="5"/>
-      <c r="G32" s="5"/>
-    </row>
-    <row r="33" spans="1:9" ht="15">
-      <c r="A33" s="15" t="s">
-        <v>133</v>
-      </c>
-      <c r="B33" s="15"/>
-      <c r="C33" s="15"/>
-      <c r="D33" s="15"/>
-      <c r="E33" s="15"/>
-      <c r="F33" s="15"/>
-      <c r="G33" s="15"/>
-    </row>
-    <row r="34" spans="1:9" ht="12">
-      <c r="A34" t="s">
+        <v>88</v>
+      </c>
+      <c r="D28" s="13"/>
+    </row>
+    <row r="29" spans="1:9" ht="12.75" customHeight="1">
+      <c r="A29" t="s">
+        <v>17</v>
+      </c>
+      <c r="B29" t="s">
+        <v>89</v>
+      </c>
+      <c r="G29" t="s">
+        <v>90</v>
+      </c>
+    </row>
+    <row r="30" spans="1:9" ht="12">
+      <c r="A30" s="11" t="s">
+        <v>31</v>
+      </c>
+      <c r="B30" s="10"/>
+      <c r="C30" s="10"/>
+      <c r="D30" s="10"/>
+      <c r="E30" s="10"/>
+      <c r="F30" s="10"/>
+      <c r="G30" s="10"/>
+    </row>
+    <row r="31" spans="1:9" ht="24">
+      <c r="A31" s="4" t="s">
+        <v>17</v>
+      </c>
+      <c r="B31" s="4"/>
+      <c r="C31" s="4" t="s">
+        <v>19</v>
+      </c>
+      <c r="D31" s="2" t="s">
+        <v>78</v>
+      </c>
+      <c r="E31" s="4"/>
+      <c r="F31" t="s">
+        <v>20</v>
+      </c>
+    </row>
+    <row r="32" spans="1:9" ht="15">
+      <c r="A32" s="15" t="s">
+        <v>92</v>
+      </c>
+      <c r="B32" s="15"/>
+      <c r="C32" s="15"/>
+      <c r="D32" s="15"/>
+      <c r="E32" s="15"/>
+      <c r="F32" s="15"/>
+      <c r="G32" s="15"/>
+      <c r="H32" s="12"/>
+    </row>
+    <row r="33" spans="1:9" ht="12">
+      <c r="A33" s="12"/>
+      <c r="B33" s="12"/>
+      <c r="C33" s="12"/>
+      <c r="D33" s="12"/>
+      <c r="E33" s="12"/>
+      <c r="F33" s="12"/>
+      <c r="G33" s="12"/>
+      <c r="H33" s="12"/>
+    </row>
+    <row r="34" spans="1:9" ht="15">
+      <c r="A34" s="14" t="s">
+        <v>124</v>
+      </c>
+      <c r="B34" s="14"/>
+      <c r="C34" s="14"/>
+      <c r="D34" s="13" t="s">
+        <v>125</v>
+      </c>
+      <c r="E34" s="14"/>
+      <c r="F34" s="14"/>
+      <c r="G34" s="14"/>
+      <c r="H34" s="12"/>
+    </row>
+    <row r="35" spans="1:9" ht="12">
+      <c r="A35" s="5" t="s">
+        <v>93</v>
+      </c>
+      <c r="B35" s="5"/>
+      <c r="C35" s="5"/>
+      <c r="D35" s="6" t="s">
+        <v>94</v>
+      </c>
+      <c r="E35" s="5"/>
+      <c r="F35" s="5"/>
+      <c r="G35" s="5"/>
+    </row>
+    <row r="36" spans="1:9" ht="15">
+      <c r="A36" s="15" t="s">
+        <v>126</v>
+      </c>
+      <c r="B36" s="15"/>
+      <c r="C36" s="15"/>
+      <c r="D36" s="15"/>
+      <c r="E36" s="15"/>
+      <c r="F36" s="15"/>
+      <c r="G36" s="15"/>
+    </row>
+    <row r="37" spans="1:9" ht="12">
+      <c r="A37" t="s">
         <v>14</v>
       </c>
-      <c r="B34" t="s">
+      <c r="B37" t="s">
         <v>15</v>
       </c>
-      <c r="C34" t="s">
+      <c r="C37" t="s">
         <v>16</v>
       </c>
-      <c r="E34" t="s">
+      <c r="E37" t="s">
         <v>7</v>
       </c>
-      <c r="F34" s="12"/>
-      <c r="G34" s="12"/>
-    </row>
-    <row r="35" spans="1:9" ht="12">
-      <c r="A35" s="4" t="s">
-        <v>21</v>
-      </c>
-      <c r="B35" s="4"/>
-      <c r="C35" s="4"/>
-      <c r="D35" s="4"/>
-      <c r="E35" s="4"/>
-    </row>
-    <row r="36" spans="1:9" ht="12">
-      <c r="A36" s="4" t="s">
-        <v>22</v>
-      </c>
-      <c r="B36" s="4" t="s">
-        <v>23</v>
-      </c>
-      <c r="C36" s="4" t="s">
-        <v>24</v>
-      </c>
-      <c r="D36" s="4"/>
-      <c r="E36" s="4"/>
-    </row>
-    <row r="37" spans="1:9" ht="36">
-      <c r="A37" s="4" t="s">
-        <v>17</v>
-      </c>
-      <c r="B37" s="4"/>
-      <c r="C37" s="4" t="s">
-        <v>25</v>
-      </c>
-      <c r="D37" s="4" t="s">
-        <v>26</v>
-      </c>
-      <c r="E37" s="4"/>
+      <c r="F37" s="12"/>
+      <c r="G37" s="12"/>
     </row>
     <row r="38" spans="1:9" ht="12">
       <c r="A38" s="4" t="s">
-        <v>22</v>
-      </c>
-      <c r="B38" s="4" t="s">
-        <v>27</v>
-      </c>
-      <c r="C38" s="4" t="s">
-        <v>28</v>
-      </c>
+        <v>21</v>
+      </c>
+      <c r="B38" s="4"/>
+      <c r="C38" s="4"/>
       <c r="D38" s="4"/>
       <c r="E38" s="4"/>
     </row>
-    <row r="39" spans="1:9" ht="36">
+    <row r="39" spans="1:9" ht="12">
       <c r="A39" s="4" t="s">
+        <v>22</v>
+      </c>
+      <c r="B39" s="4" t="s">
+        <v>23</v>
+      </c>
+      <c r="C39" s="4" t="s">
+        <v>24</v>
+      </c>
+      <c r="D39" s="4"/>
+      <c r="E39" s="4"/>
+    </row>
+    <row r="40" spans="1:9" ht="36">
+      <c r="A40" s="4" t="s">
         <v>17</v>
       </c>
-      <c r="B39" s="4"/>
-      <c r="C39" s="4" t="s">
+      <c r="B40" s="4"/>
+      <c r="C40" s="4" t="s">
+        <v>25</v>
+      </c>
+      <c r="D40" s="4" t="s">
+        <v>26</v>
+      </c>
+      <c r="E40" s="4"/>
+    </row>
+    <row r="41" spans="1:9" ht="12">
+      <c r="A41" s="4" t="s">
+        <v>22</v>
+      </c>
+      <c r="B41" s="4" t="s">
+        <v>27</v>
+      </c>
+      <c r="C41" s="4" t="s">
+        <v>28</v>
+      </c>
+      <c r="D41" s="4"/>
+      <c r="E41" s="4"/>
+    </row>
+    <row r="42" spans="1:9" ht="36">
+      <c r="A42" s="4" t="s">
+        <v>17</v>
+      </c>
+      <c r="B42" s="4"/>
+      <c r="C42" s="4" t="s">
         <v>29</v>
       </c>
-      <c r="D39" s="4" t="s">
+      <c r="D42" s="4" t="s">
         <v>30</v>
       </c>
-      <c r="E39" s="4"/>
-      <c r="H39" s="12"/>
-    </row>
-    <row r="40" spans="1:9" ht="12.75" customHeight="1">
-      <c r="A40" s="4" t="s">
+      <c r="E42" s="4"/>
+      <c r="H42" s="12"/>
+    </row>
+    <row r="43" spans="1:9" ht="12.75" customHeight="1">
+      <c r="A43" s="4" t="s">
         <v>31</v>
       </c>
-      <c r="B40" s="4"/>
-      <c r="C40" s="4"/>
-      <c r="D40" s="4"/>
-      <c r="E40" s="4"/>
-    </row>
-    <row r="41" spans="1:9" ht="12.75" customHeight="1">
-      <c r="A41" s="15" t="s">
+      <c r="B43" s="4"/>
+      <c r="C43" s="4"/>
+      <c r="D43" s="4"/>
+      <c r="E43" s="4"/>
+    </row>
+    <row r="44" spans="1:9" ht="12.75" customHeight="1">
+      <c r="A44" s="15" t="s">
+        <v>95</v>
+      </c>
+      <c r="B44" s="15"/>
+      <c r="C44" s="15"/>
+      <c r="D44" s="15"/>
+      <c r="E44" s="15"/>
+      <c r="F44" s="15"/>
+      <c r="G44" s="15"/>
+    </row>
+    <row r="45" spans="1:9" s="12" customFormat="1" ht="12.75" customHeight="1"/>
+    <row r="46" spans="1:9" s="14" customFormat="1" ht="12.75" customHeight="1">
+      <c r="A46" s="13" t="s">
+        <v>127</v>
+      </c>
+      <c r="D46" s="14" t="s">
+        <v>128</v>
+      </c>
+      <c r="H46" s="12"/>
+      <c r="I46" s="12"/>
+    </row>
+    <row r="47" spans="1:9" ht="12.75" customHeight="1">
+      <c r="A47" s="13" t="s">
         <v>102</v>
       </c>
-      <c r="B41" s="15"/>
-      <c r="C41" s="15"/>
-      <c r="D41" s="15"/>
-      <c r="E41" s="15"/>
-      <c r="F41" s="15"/>
-      <c r="G41" s="15"/>
-    </row>
-    <row r="42" spans="1:9" s="12" customFormat="1" ht="12.75" customHeight="1"/>
-    <row r="43" spans="1:9" s="14" customFormat="1" ht="12.75" customHeight="1">
-      <c r="A43" s="13" t="s">
-        <v>134</v>
-      </c>
-      <c r="D43" s="14" t="s">
+      <c r="B47" s="14"/>
+      <c r="C47" s="14"/>
+      <c r="D47" s="14" t="s">
+        <v>96</v>
+      </c>
+      <c r="E47" s="14"/>
+      <c r="F47" s="14"/>
+      <c r="G47" s="14"/>
+    </row>
+    <row r="48" spans="1:9" ht="12.75" customHeight="1">
+      <c r="A48" s="15" t="s">
+        <v>144</v>
+      </c>
+      <c r="B48" s="18"/>
+      <c r="C48" s="18"/>
+      <c r="D48" s="18"/>
+      <c r="E48" s="18"/>
+      <c r="F48" s="18"/>
+      <c r="G48" s="18"/>
+    </row>
+    <row r="49" spans="1:7" ht="12.75" customHeight="1">
+      <c r="A49" s="2" t="s">
+        <v>97</v>
+      </c>
+      <c r="B49" s="12" t="s">
+        <v>98</v>
+      </c>
+      <c r="C49" s="12" t="s">
+        <v>99</v>
+      </c>
+      <c r="D49" s="12"/>
+      <c r="E49" s="12" t="s">
+        <v>100</v>
+      </c>
+      <c r="F49" s="12"/>
+      <c r="G49" s="12"/>
+    </row>
+    <row r="50" spans="1:7" ht="12.75" customHeight="1">
+      <c r="A50" s="15" t="s">
+        <v>101</v>
+      </c>
+      <c r="B50" s="18"/>
+      <c r="C50" s="18"/>
+      <c r="D50" s="18"/>
+      <c r="E50" s="18"/>
+      <c r="F50" s="18"/>
+      <c r="G50" s="18"/>
+    </row>
+    <row r="51" spans="1:7" ht="12.75" customHeight="1">
+      <c r="B51" s="12"/>
+      <c r="C51" s="12"/>
+      <c r="D51" s="12"/>
+      <c r="E51" s="12"/>
+      <c r="F51" s="12"/>
+      <c r="G51" s="12"/>
+    </row>
+    <row r="52" spans="1:7" ht="12.75" customHeight="1">
+      <c r="A52" s="13" t="s">
         <v>135</v>
       </c>
-      <c r="H43" s="12"/>
-      <c r="I43" s="12"/>
-    </row>
-    <row r="44" spans="1:9" ht="12.75" customHeight="1">
-      <c r="A44" s="13" t="s">
-        <v>109</v>
-      </c>
-      <c r="B44" s="14"/>
-      <c r="C44" s="14"/>
-      <c r="D44" s="14" t="s">
-        <v>103</v>
-      </c>
-      <c r="E44" s="14"/>
-      <c r="F44" s="14"/>
-      <c r="G44" s="14"/>
-    </row>
-    <row r="45" spans="1:9" ht="12.75" customHeight="1">
-      <c r="A45" s="15" t="s">
-        <v>151</v>
-      </c>
-      <c r="B45" s="18"/>
-      <c r="C45" s="18"/>
-      <c r="D45" s="18"/>
-      <c r="E45" s="18"/>
-      <c r="F45" s="18"/>
-      <c r="G45" s="18"/>
-    </row>
-    <row r="46" spans="1:9" ht="12.75" customHeight="1">
-      <c r="A46" s="2" t="s">
-        <v>104</v>
-      </c>
-      <c r="B46" s="12" t="s">
-        <v>105</v>
-      </c>
-      <c r="C46" s="12" t="s">
-        <v>106</v>
-      </c>
-      <c r="D46" s="12"/>
-      <c r="E46" s="12" t="s">
-        <v>107</v>
-      </c>
-      <c r="F46" s="12"/>
-      <c r="G46" s="12"/>
-    </row>
-    <row r="47" spans="1:9" ht="12.75" customHeight="1">
-      <c r="A47" s="15" t="s">
-        <v>108</v>
-      </c>
-      <c r="B47" s="18"/>
-      <c r="C47" s="18"/>
-      <c r="D47" s="18"/>
-      <c r="E47" s="18"/>
-      <c r="F47" s="18"/>
-      <c r="G47" s="18"/>
-    </row>
-    <row r="48" spans="1:9" ht="12.75" customHeight="1">
-      <c r="B48" s="12"/>
-      <c r="C48" s="12"/>
-      <c r="D48" s="12"/>
-      <c r="E48" s="12"/>
-      <c r="F48" s="12"/>
-      <c r="G48" s="12"/>
-    </row>
-    <row r="49" spans="1:7" ht="12.75" customHeight="1">
-      <c r="A49" s="13" t="s">
-        <v>142</v>
-      </c>
-      <c r="B49" s="14"/>
-      <c r="C49" s="14"/>
-      <c r="D49" s="14" t="s">
-        <v>144</v>
-      </c>
-      <c r="E49" s="14"/>
-      <c r="F49" s="14"/>
-      <c r="G49" s="14"/>
-    </row>
-    <row r="50" spans="1:7" ht="12.75" customHeight="1">
-      <c r="A50" s="13" t="s">
-        <v>143</v>
-      </c>
-      <c r="B50" s="14"/>
-      <c r="C50" s="14"/>
-      <c r="D50" s="14" t="s">
-        <v>145</v>
-      </c>
-      <c r="E50" s="14"/>
-      <c r="F50" s="14"/>
-      <c r="G50" s="14"/>
-    </row>
-    <row r="51" spans="1:7" ht="12.75" customHeight="1">
-      <c r="A51" s="15" t="s">
-        <v>152</v>
-      </c>
-      <c r="B51" s="18"/>
-      <c r="C51" s="18"/>
-      <c r="D51" s="18"/>
-      <c r="E51" s="18"/>
-      <c r="F51" s="18"/>
-      <c r="G51" s="18"/>
-    </row>
-    <row r="52" spans="1:7" ht="12.75" customHeight="1">
-      <c r="A52" t="s">
-        <v>72</v>
-      </c>
-      <c r="B52" t="s">
-        <v>71</v>
-      </c>
-      <c r="C52" t="s">
-        <v>74</v>
-      </c>
-      <c r="E52" t="s">
-        <v>7</v>
-      </c>
-      <c r="F52" s="12"/>
-      <c r="G52" s="12"/>
+      <c r="B52" s="14"/>
+      <c r="C52" s="14"/>
+      <c r="D52" s="14" t="s">
+        <v>137</v>
+      </c>
+      <c r="E52" s="14"/>
+      <c r="F52" s="14"/>
+      <c r="G52" s="14"/>
     </row>
     <row r="53" spans="1:7" ht="12.75" customHeight="1">
-      <c r="A53" s="2" t="s">
-        <v>17</v>
-      </c>
-      <c r="B53" s="12"/>
-      <c r="C53" s="12" t="s">
-        <v>70</v>
-      </c>
-      <c r="D53" s="12"/>
-      <c r="E53" s="12"/>
-      <c r="F53" s="12"/>
-      <c r="G53" s="12"/>
+      <c r="A53" s="13" t="s">
+        <v>136</v>
+      </c>
+      <c r="B53" s="14"/>
+      <c r="C53" s="14"/>
+      <c r="D53" s="14" t="s">
+        <v>138</v>
+      </c>
+      <c r="E53" s="14"/>
+      <c r="F53" s="14"/>
+      <c r="G53" s="14"/>
     </row>
     <row r="54" spans="1:7" ht="12.75" customHeight="1">
       <c r="A54" s="15" t="s">
-        <v>146</v>
+        <v>145</v>
       </c>
       <c r="B54" s="18"/>
       <c r="C54" s="18"/>
@@ -1761,9 +1886,49 @@
       <c r="F54" s="18"/>
       <c r="G54" s="18"/>
     </row>
+    <row r="55" spans="1:7" ht="12.75" customHeight="1">
+      <c r="A55" t="s">
+        <v>72</v>
+      </c>
+      <c r="B55" t="s">
+        <v>71</v>
+      </c>
+      <c r="C55" t="s">
+        <v>74</v>
+      </c>
+      <c r="E55" t="s">
+        <v>7</v>
+      </c>
+      <c r="F55" s="12"/>
+      <c r="G55" s="12"/>
+    </row>
+    <row r="56" spans="1:7" ht="12.75" customHeight="1">
+      <c r="A56" s="2" t="s">
+        <v>17</v>
+      </c>
+      <c r="B56" s="12"/>
+      <c r="C56" s="12" t="s">
+        <v>70</v>
+      </c>
+      <c r="D56" s="12"/>
+      <c r="E56" s="12"/>
+      <c r="F56" s="12"/>
+      <c r="G56" s="12"/>
+    </row>
     <row r="57" spans="1:7" ht="12.75" customHeight="1">
-      <c r="A57" s="17" t="s">
-        <v>127</v>
+      <c r="A57" s="15" t="s">
+        <v>139</v>
+      </c>
+      <c r="B57" s="18"/>
+      <c r="C57" s="18"/>
+      <c r="D57" s="18"/>
+      <c r="E57" s="18"/>
+      <c r="F57" s="18"/>
+      <c r="G57" s="18"/>
+    </row>
+    <row r="60" spans="1:7" ht="12.75" customHeight="1">
+      <c r="A60" s="17" t="s">
+        <v>120</v>
       </c>
     </row>
   </sheetData>
@@ -1781,7 +1946,9 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:B5"/>
   <sheetViews>
-    <sheetView workbookViewId="0"/>
+    <sheetView workbookViewId="0">
+      <selection activeCell="B65" sqref="B65"/>
+    </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultColWidth="17.1640625" defaultRowHeight="12.75" customHeight="1" x14ac:dyDescent="0"/>
   <cols>
@@ -1840,18 +2007,19 @@
 
 <file path=xl/worksheets/sheet3.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <dimension ref="A1:C28"/>
+  <dimension ref="A1:D43"/>
   <sheetViews>
     <sheetView workbookViewId="0">
-      <selection activeCell="C7" sqref="C7"/>
+      <selection activeCell="A39" sqref="A39:D42"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultColWidth="17.1640625" defaultRowHeight="12.75" customHeight="1" x14ac:dyDescent="0"/>
   <cols>
     <col min="3" max="3" width="27.1640625" customWidth="1"/>
+    <col min="4" max="4" width="26.1640625" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:3" ht="12.75" customHeight="1">
+    <row r="1" spans="1:4" ht="12.75" customHeight="1">
       <c r="A1" t="s">
         <v>41</v>
       </c>
@@ -1861,8 +2029,11 @@
       <c r="C1" t="s">
         <v>2</v>
       </c>
-    </row>
-    <row r="2" spans="1:3" ht="12.75" customHeight="1">
+      <c r="D1" t="s">
+        <v>68</v>
+      </c>
+    </row>
+    <row r="2" spans="1:4" ht="12.75" customHeight="1">
       <c r="A2" t="s">
         <v>5</v>
       </c>
@@ -1873,7 +2044,7 @@
         <v>10</v>
       </c>
     </row>
-    <row r="3" spans="1:3" ht="12.75" customHeight="1">
+    <row r="3" spans="1:4" ht="12.75" customHeight="1">
       <c r="A3" t="s">
         <v>5</v>
       </c>
@@ -1884,7 +2055,7 @@
         <v>13</v>
       </c>
     </row>
-    <row r="4" spans="1:3" ht="12.75" customHeight="1">
+    <row r="4" spans="1:4" ht="12.75" customHeight="1">
       <c r="A4" t="s">
         <v>5</v>
       </c>
@@ -1895,7 +2066,7 @@
         <v>45</v>
       </c>
     </row>
-    <row r="5" spans="1:3" ht="12.75" customHeight="1">
+    <row r="5" spans="1:4" ht="12.75" customHeight="1">
       <c r="A5" t="s">
         <v>5</v>
       </c>
@@ -1906,18 +2077,18 @@
         <v>74</v>
       </c>
     </row>
-    <row r="6" spans="1:3" ht="12.75" customHeight="1">
+    <row r="6" spans="1:4" ht="12.75" customHeight="1">
       <c r="A6" t="s">
         <v>5</v>
       </c>
       <c r="B6" t="s">
-        <v>116</v>
+        <v>109</v>
       </c>
       <c r="C6" t="s">
-        <v>106</v>
-      </c>
-    </row>
-    <row r="9" spans="1:3" ht="12.75" customHeight="1">
+        <v>99</v>
+      </c>
+    </row>
+    <row r="9" spans="1:4" ht="12.75" customHeight="1">
       <c r="A9" t="s">
         <v>12</v>
       </c>
@@ -1928,7 +2099,7 @@
         <v>47</v>
       </c>
     </row>
-    <row r="10" spans="1:3" ht="12.75" customHeight="1">
+    <row r="10" spans="1:4" ht="12.75" customHeight="1">
       <c r="A10" t="s">
         <v>12</v>
       </c>
@@ -1939,7 +2110,7 @@
         <v>49</v>
       </c>
     </row>
-    <row r="11" spans="1:3" ht="12.75" customHeight="1">
+    <row r="11" spans="1:4" ht="12.75" customHeight="1">
       <c r="A11" t="s">
         <v>12</v>
       </c>
@@ -1950,7 +2121,7 @@
         <v>75</v>
       </c>
     </row>
-    <row r="13" spans="1:3" ht="12.75" customHeight="1">
+    <row r="13" spans="1:4" ht="12.75" customHeight="1">
       <c r="A13" t="s">
         <v>9</v>
       </c>
@@ -1961,103 +2132,92 @@
         <v>51</v>
       </c>
     </row>
-    <row r="14" spans="1:3" ht="12.75" customHeight="1">
+    <row r="14" spans="1:4" ht="12.75" customHeight="1">
       <c r="A14" t="s">
         <v>9</v>
       </c>
       <c r="B14" t="s">
-        <v>119</v>
+        <v>112</v>
       </c>
       <c r="C14" t="s">
-        <v>120</v>
-      </c>
-    </row>
-    <row r="15" spans="1:3" ht="12.75" customHeight="1">
+        <v>113</v>
+      </c>
+    </row>
+    <row r="15" spans="1:4" ht="12.75" customHeight="1">
       <c r="A15" t="s">
         <v>9</v>
       </c>
       <c r="B15" t="s">
-        <v>117</v>
+        <v>110</v>
       </c>
       <c r="C15" t="s">
-        <v>118</v>
-      </c>
-    </row>
-    <row r="16" spans="1:3" ht="12.75" customHeight="1">
+        <v>111</v>
+      </c>
+    </row>
+    <row r="16" spans="1:4" ht="12.75" customHeight="1">
       <c r="A16" t="s">
+        <v>9</v>
+      </c>
+      <c r="B16" t="s">
+        <v>146</v>
+      </c>
+      <c r="C16" t="s">
+        <v>91</v>
+      </c>
+    </row>
+    <row r="18" spans="1:3" ht="12.75" customHeight="1">
+      <c r="A18" t="s">
         <v>15</v>
       </c>
-      <c r="B16" t="s">
+      <c r="B18" t="s">
         <v>52</v>
       </c>
-      <c r="C16" t="s">
+      <c r="C18" t="s">
         <v>53</v>
-      </c>
-    </row>
-    <row r="17" spans="1:3" ht="12.75" customHeight="1">
-      <c r="A17" t="s">
-        <v>15</v>
-      </c>
-      <c r="B17" t="s">
-        <v>54</v>
-      </c>
-      <c r="C17" t="s">
-        <v>55</v>
       </c>
     </row>
     <row r="19" spans="1:3" ht="12.75" customHeight="1">
       <c r="A19" t="s">
-        <v>105</v>
+        <v>15</v>
       </c>
       <c r="B19" t="s">
-        <v>110</v>
+        <v>54</v>
       </c>
       <c r="C19" t="s">
-        <v>111</v>
-      </c>
-    </row>
-    <row r="20" spans="1:3" ht="12.75" customHeight="1">
-      <c r="A20" t="s">
-        <v>105</v>
-      </c>
-      <c r="B20" t="s">
-        <v>112</v>
-      </c>
-      <c r="C20" t="s">
-        <v>113</v>
+        <v>55</v>
       </c>
     </row>
     <row r="21" spans="1:3" ht="12.75" customHeight="1">
       <c r="A21" t="s">
+        <v>98</v>
+      </c>
+      <c r="B21" t="s">
+        <v>103</v>
+      </c>
+      <c r="C21" t="s">
+        <v>104</v>
+      </c>
+    </row>
+    <row r="22" spans="1:3" ht="12.75" customHeight="1">
+      <c r="A22" t="s">
+        <v>98</v>
+      </c>
+      <c r="B22" t="s">
         <v>105</v>
       </c>
-      <c r="B21" t="s">
-        <v>114</v>
-      </c>
-      <c r="C21" t="s">
-        <v>115</v>
+      <c r="C22" t="s">
+        <v>106</v>
       </c>
     </row>
     <row r="23" spans="1:3" ht="12.75" customHeight="1">
       <c r="A23" t="s">
-        <v>71</v>
+        <v>98</v>
       </c>
       <c r="B23" t="s">
-        <v>136</v>
+        <v>107</v>
       </c>
       <c r="C23" t="s">
-        <v>137</v>
-      </c>
-    </row>
-    <row r="24" spans="1:3" ht="12.75" customHeight="1">
-      <c r="A24" t="s">
-        <v>71</v>
-      </c>
-      <c r="B24" t="s">
-        <v>138</v>
-      </c>
-      <c r="C24" t="s">
-        <v>140</v>
+        <v>108</v>
       </c>
     </row>
     <row r="25" spans="1:3" ht="12.75" customHeight="1">
@@ -2065,32 +2225,175 @@
         <v>71</v>
       </c>
       <c r="B25" t="s">
-        <v>139</v>
+        <v>129</v>
       </c>
       <c r="C25" t="s">
-        <v>141</v>
+        <v>130</v>
+      </c>
+    </row>
+    <row r="26" spans="1:3" ht="12.75" customHeight="1">
+      <c r="A26" t="s">
+        <v>71</v>
+      </c>
+      <c r="B26" t="s">
+        <v>131</v>
+      </c>
+      <c r="C26" t="s">
+        <v>133</v>
       </c>
     </row>
     <row r="27" spans="1:3" ht="12.75" customHeight="1">
       <c r="A27" t="s">
+        <v>71</v>
+      </c>
+      <c r="B27" t="s">
+        <v>132</v>
+      </c>
+      <c r="C27" t="s">
+        <v>134</v>
+      </c>
+    </row>
+    <row r="29" spans="1:3" ht="12.75" customHeight="1">
+      <c r="A29" t="s">
         <v>56</v>
       </c>
-      <c r="B27" t="s">
+      <c r="B29" t="s">
         <v>57</v>
       </c>
-      <c r="C27" t="s">
+      <c r="C29" t="s">
         <v>58</v>
       </c>
     </row>
-    <row r="28" spans="1:3" ht="12.75" customHeight="1">
-      <c r="A28" t="s">
+    <row r="30" spans="1:3" ht="12.75" customHeight="1">
+      <c r="A30" t="s">
         <v>56</v>
       </c>
-      <c r="B28" t="s">
+      <c r="B30" t="s">
         <v>59</v>
       </c>
-      <c r="C28" t="s">
+      <c r="C30" t="s">
         <v>60</v>
+      </c>
+    </row>
+    <row r="32" spans="1:3" ht="12.75" customHeight="1">
+      <c r="A32" t="s">
+        <v>149</v>
+      </c>
+      <c r="B32" t="s">
+        <v>150</v>
+      </c>
+      <c r="C32" t="s">
+        <v>156</v>
+      </c>
+    </row>
+    <row r="33" spans="1:4" ht="12.75" customHeight="1">
+      <c r="A33" t="s">
+        <v>149</v>
+      </c>
+      <c r="B33" t="s">
+        <v>151</v>
+      </c>
+      <c r="C33" t="s">
+        <v>157</v>
+      </c>
+    </row>
+    <row r="34" spans="1:4" ht="12.75" customHeight="1">
+      <c r="A34" t="s">
+        <v>149</v>
+      </c>
+      <c r="B34" t="s">
+        <v>152</v>
+      </c>
+      <c r="C34" t="s">
+        <v>158</v>
+      </c>
+    </row>
+    <row r="35" spans="1:4" ht="12.75" customHeight="1">
+      <c r="A35" t="s">
+        <v>149</v>
+      </c>
+      <c r="B35" t="s">
+        <v>153</v>
+      </c>
+      <c r="C35" t="s">
+        <v>159</v>
+      </c>
+    </row>
+    <row r="36" spans="1:4" ht="12.75" customHeight="1">
+      <c r="A36" t="s">
+        <v>149</v>
+      </c>
+      <c r="B36" t="s">
+        <v>154</v>
+      </c>
+      <c r="C36" t="s">
+        <v>160</v>
+      </c>
+    </row>
+    <row r="37" spans="1:4" ht="12.75" customHeight="1">
+      <c r="A37" t="s">
+        <v>149</v>
+      </c>
+      <c r="B37" t="s">
+        <v>155</v>
+      </c>
+      <c r="C37" t="s">
+        <v>161</v>
+      </c>
+    </row>
+    <row r="39" spans="1:4" ht="12.75" customHeight="1">
+      <c r="A39" t="s">
+        <v>163</v>
+      </c>
+      <c r="B39" t="s">
+        <v>170</v>
+      </c>
+      <c r="D39" t="s">
+        <v>171</v>
+      </c>
+    </row>
+    <row r="40" spans="1:4" ht="12.75" customHeight="1">
+      <c r="A40" t="s">
+        <v>163</v>
+      </c>
+      <c r="B40" t="s">
+        <v>172</v>
+      </c>
+      <c r="D40" t="s">
+        <v>176</v>
+      </c>
+    </row>
+    <row r="41" spans="1:4" ht="12.75" customHeight="1">
+      <c r="A41" t="s">
+        <v>163</v>
+      </c>
+      <c r="B41" t="s">
+        <v>173</v>
+      </c>
+      <c r="D41" t="s">
+        <v>177</v>
+      </c>
+    </row>
+    <row r="42" spans="1:4" ht="12.75" customHeight="1">
+      <c r="A42" t="s">
+        <v>163</v>
+      </c>
+      <c r="B42" t="s">
+        <v>174</v>
+      </c>
+      <c r="D42" t="s">
+        <v>178</v>
+      </c>
+    </row>
+    <row r="43" spans="1:4" ht="12.75" customHeight="1">
+      <c r="A43" t="s">
+        <v>163</v>
+      </c>
+      <c r="B43" t="s">
+        <v>175</v>
+      </c>
+      <c r="D43" t="s">
+        <v>179</v>
       </c>
     </row>
   </sheetData>
@@ -2144,4 +2447,40 @@
     </ext>
   </extLst>
 </worksheet>
+</file>
+
+<file path=xl/worksheets/sheet5.xml><?xml version="1.0" encoding="utf-8"?>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
+  <dimension ref="A1:B2"/>
+  <sheetViews>
+    <sheetView tabSelected="1" workbookViewId="0">
+      <selection activeCell="B2" sqref="B2"/>
+    </sheetView>
+  </sheetViews>
+  <sheetFormatPr baseColWidth="10" defaultRowHeight="12" x14ac:dyDescent="0"/>
+  <sheetData>
+    <row r="1" spans="1:2">
+      <c r="A1" t="s">
+        <v>1</v>
+      </c>
+      <c r="B1" t="s">
+        <v>180</v>
+      </c>
+    </row>
+    <row r="2" spans="1:2">
+      <c r="A2" t="s">
+        <v>181</v>
+      </c>
+      <c r="B2" t="s">
+        <v>182</v>
+      </c>
+    </row>
+  </sheetData>
+  <pageMargins left="0.75" right="0.75" top="1" bottom="1" header="0.5" footer="0.5"/>
+  <extLst>
+    <ext xmlns:mx="http://schemas.microsoft.com/office/mac/excel/2008/main" uri="{64002731-A6B0-56B0-2670-7721B7C09600}">
+      <mx:PLV Mode="0" OnePage="0" WScale="0"/>
+    </ext>
+  </extLst>
+</worksheet>
 </file>
</xml_diff>

<commit_message>
Added neuromuscular ballard test
</commit_message>
<xml_diff>
--- a/opendatakit.collect2/form-files/neonatal/neonatal.xlsx
+++ b/opendatakit.collect2/form-files/neonatal/neonatal.xlsx
@@ -4,7 +4,7 @@
   <fileVersion appName="xl" lastEdited="5" lowestEdited="5" rupBuild="20910"/>
   <workbookPr autoCompressPictures="0"/>
   <bookViews>
-    <workbookView xWindow="2800" yWindow="500" windowWidth="22120" windowHeight="17440" tabRatio="500" activeTab="4"/>
+    <workbookView xWindow="1680" yWindow="0" windowWidth="25600" windowHeight="16060" tabRatio="500" activeTab="2"/>
   </bookViews>
   <sheets>
     <sheet name="survey" sheetId="1" r:id="rId1"/>
@@ -23,7 +23,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="242" uniqueCount="183">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="348" uniqueCount="259">
   <si>
     <t>type</t>
   </si>
@@ -484,9 +484,6 @@
     <t>arm</t>
   </si>
   <si>
-    <t>popliteal</t>
-  </si>
-  <si>
     <t>scarf</t>
   </si>
   <si>
@@ -572,6 +569,237 @@
   </si>
   <si>
     <t>string</t>
+  </si>
+  <si>
+    <t>image_slider arm_slider</t>
+  </si>
+  <si>
+    <t>arm_slider</t>
+  </si>
+  <si>
+    <t>Choose Arm Recoil</t>
+  </si>
+  <si>
+    <t>selected(data('ballard_menu1'), 'arm')</t>
+  </si>
+  <si>
+    <t>image_slider propliteal_slider</t>
+  </si>
+  <si>
+    <t>propliteal_slider</t>
+  </si>
+  <si>
+    <t>Choose Propliteal Angle</t>
+  </si>
+  <si>
+    <t>image_slider scarf_slider</t>
+  </si>
+  <si>
+    <t>scarf_slider</t>
+  </si>
+  <si>
+    <t>Choose Scarf Sign</t>
+  </si>
+  <si>
+    <t>image_slider heel_slider</t>
+  </si>
+  <si>
+    <t>heel_slider</t>
+  </si>
+  <si>
+    <t>Choose Heel to Ear</t>
+  </si>
+  <si>
+    <t>square_window0</t>
+  </si>
+  <si>
+    <t>img/ballard/square_window0.png</t>
+  </si>
+  <si>
+    <t>square_window1</t>
+  </si>
+  <si>
+    <t>img/ballard/square_window1.png</t>
+  </si>
+  <si>
+    <t>square_window2</t>
+  </si>
+  <si>
+    <t>img/ballard/square_window2.png</t>
+  </si>
+  <si>
+    <t>square_window3</t>
+  </si>
+  <si>
+    <t>img/ballard/square_window3.png</t>
+  </si>
+  <si>
+    <t>square_window4</t>
+  </si>
+  <si>
+    <t>img/ballard/square_window4.png</t>
+  </si>
+  <si>
+    <t>square_window-1</t>
+  </si>
+  <si>
+    <t>img/ballard/square_window-1.png</t>
+  </si>
+  <si>
+    <t>arm_recoil0</t>
+  </si>
+  <si>
+    <t>img/ballard/arm_recoil0.png</t>
+  </si>
+  <si>
+    <t>arm_recoil1</t>
+  </si>
+  <si>
+    <t>img/ballard/arm_recoil1.png</t>
+  </si>
+  <si>
+    <t>arm_recoil2</t>
+  </si>
+  <si>
+    <t>img/ballard/arm_recoil2.png</t>
+  </si>
+  <si>
+    <t>arm_recoil3</t>
+  </si>
+  <si>
+    <t>img/ballard/arm_recoil3.png</t>
+  </si>
+  <si>
+    <t>arm_recoil4</t>
+  </si>
+  <si>
+    <t>img/ballard/arm_recoil4.png</t>
+  </si>
+  <si>
+    <t>propliteal-1</t>
+  </si>
+  <si>
+    <t>img/ballard/propliteal-1.png</t>
+  </si>
+  <si>
+    <t>propliteal0</t>
+  </si>
+  <si>
+    <t>img/ballard/propliteal0.png</t>
+  </si>
+  <si>
+    <t>propliteal1</t>
+  </si>
+  <si>
+    <t>img/ballard/propliteal1.png</t>
+  </si>
+  <si>
+    <t>propliteal2</t>
+  </si>
+  <si>
+    <t>img/ballard/propliteal2.png</t>
+  </si>
+  <si>
+    <t>propliteal3</t>
+  </si>
+  <si>
+    <t>img/ballard/propliteal3.png</t>
+  </si>
+  <si>
+    <t>propliteal4</t>
+  </si>
+  <si>
+    <t>img/ballard/propliteal4.png</t>
+  </si>
+  <si>
+    <t>propliteal5</t>
+  </si>
+  <si>
+    <t>img/ballard/propliteal5.png</t>
+  </si>
+  <si>
+    <t>scarf_sign-1</t>
+  </si>
+  <si>
+    <t>img/ballard/scarf_sign-1.png</t>
+  </si>
+  <si>
+    <t>scarf_sign0</t>
+  </si>
+  <si>
+    <t>img/ballard/scarf_sign0.png</t>
+  </si>
+  <si>
+    <t>scarf_sign1</t>
+  </si>
+  <si>
+    <t>img/ballard/scarf_sign1.png</t>
+  </si>
+  <si>
+    <t>scarf_sign2</t>
+  </si>
+  <si>
+    <t>img/ballard/scarf_sign2.png</t>
+  </si>
+  <si>
+    <t>scarf_sign3</t>
+  </si>
+  <si>
+    <t>img/ballard/scarf_sign3.png</t>
+  </si>
+  <si>
+    <t>scarf_sign4</t>
+  </si>
+  <si>
+    <t>img/ballard/scarf_sign4.png</t>
+  </si>
+  <si>
+    <t>heel_to_ear-1</t>
+  </si>
+  <si>
+    <t>img/ballard/heel_to_ear-1.png</t>
+  </si>
+  <si>
+    <t>heel_to_ear0</t>
+  </si>
+  <si>
+    <t>img/ballard/heel_to_ear0.png</t>
+  </si>
+  <si>
+    <t>heel_to_ear1</t>
+  </si>
+  <si>
+    <t>img/ballard/heel_to_ear1.png</t>
+  </si>
+  <si>
+    <t>heel_to_ear2</t>
+  </si>
+  <si>
+    <t>img/ballard/heel_to_ear2.png</t>
+  </si>
+  <si>
+    <t>heel_to_ear3</t>
+  </si>
+  <si>
+    <t>img/ballard/heel_to_ear3.png</t>
+  </si>
+  <si>
+    <t>heel_to_ear4</t>
+  </si>
+  <si>
+    <t>img/ballard/heel_to_ear4.png</t>
+  </si>
+  <si>
+    <t>selected(data('ballard_menu1'), 'propliteal')</t>
+  </si>
+  <si>
+    <t>selected(data('ballard_menu1'), 'scarf')</t>
+  </si>
+  <si>
+    <t>selected(data('ballard_menu1'), 'heel')</t>
+  </si>
+  <si>
+    <t>propliteal</t>
   </si>
 </sst>
 </file>
@@ -674,7 +902,7 @@
       <diagonal/>
     </border>
   </borders>
-  <cellStyleXfs count="94">
+  <cellStyleXfs count="154">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
     <xf numFmtId="0" fontId="3" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
     <xf numFmtId="0" fontId="4" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
@@ -689,6 +917,66 @@
     <xf numFmtId="0" fontId="5" fillId="2" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
     <xf numFmtId="0" fontId="6" fillId="3" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
     <xf numFmtId="0" fontId="1" fillId="4" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="4" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="4" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="4" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="4" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="4" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="4" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="4" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="4" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="4" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="4" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="4" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="4" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="4" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="4" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="4" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="4" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="4" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="4" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="4" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="4" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="4" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="4" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="4" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="4" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="4" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="4" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="4" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="4" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="4" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="4" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
     <xf numFmtId="0" fontId="3" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
     <xf numFmtId="0" fontId="4" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
     <xf numFmtId="0" fontId="3" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
@@ -817,7 +1105,7 @@
     </xf>
     <xf numFmtId="0" fontId="6" fillId="3" borderId="0" xfId="12"/>
   </cellXfs>
-  <cellStyles count="94">
+  <cellStyles count="154">
     <cellStyle name="20% - Accent4" xfId="13" builtinId="42"/>
     <cellStyle name="Followed Hyperlink" xfId="2" builtinId="9" hidden="1"/>
     <cellStyle name="Followed Hyperlink" xfId="4" builtinId="9" hidden="1"/>
@@ -864,6 +1152,36 @@
     <cellStyle name="Followed Hyperlink" xfId="89" builtinId="9" hidden="1"/>
     <cellStyle name="Followed Hyperlink" xfId="91" builtinId="9" hidden="1"/>
     <cellStyle name="Followed Hyperlink" xfId="93" builtinId="9" hidden="1"/>
+    <cellStyle name="Followed Hyperlink" xfId="95" builtinId="9" hidden="1"/>
+    <cellStyle name="Followed Hyperlink" xfId="97" builtinId="9" hidden="1"/>
+    <cellStyle name="Followed Hyperlink" xfId="99" builtinId="9" hidden="1"/>
+    <cellStyle name="Followed Hyperlink" xfId="101" builtinId="9" hidden="1"/>
+    <cellStyle name="Followed Hyperlink" xfId="103" builtinId="9" hidden="1"/>
+    <cellStyle name="Followed Hyperlink" xfId="105" builtinId="9" hidden="1"/>
+    <cellStyle name="Followed Hyperlink" xfId="107" builtinId="9" hidden="1"/>
+    <cellStyle name="Followed Hyperlink" xfId="109" builtinId="9" hidden="1"/>
+    <cellStyle name="Followed Hyperlink" xfId="111" builtinId="9" hidden="1"/>
+    <cellStyle name="Followed Hyperlink" xfId="113" builtinId="9" hidden="1"/>
+    <cellStyle name="Followed Hyperlink" xfId="115" builtinId="9" hidden="1"/>
+    <cellStyle name="Followed Hyperlink" xfId="117" builtinId="9" hidden="1"/>
+    <cellStyle name="Followed Hyperlink" xfId="119" builtinId="9" hidden="1"/>
+    <cellStyle name="Followed Hyperlink" xfId="121" builtinId="9" hidden="1"/>
+    <cellStyle name="Followed Hyperlink" xfId="123" builtinId="9" hidden="1"/>
+    <cellStyle name="Followed Hyperlink" xfId="125" builtinId="9" hidden="1"/>
+    <cellStyle name="Followed Hyperlink" xfId="127" builtinId="9" hidden="1"/>
+    <cellStyle name="Followed Hyperlink" xfId="129" builtinId="9" hidden="1"/>
+    <cellStyle name="Followed Hyperlink" xfId="131" builtinId="9" hidden="1"/>
+    <cellStyle name="Followed Hyperlink" xfId="133" builtinId="9" hidden="1"/>
+    <cellStyle name="Followed Hyperlink" xfId="135" builtinId="9" hidden="1"/>
+    <cellStyle name="Followed Hyperlink" xfId="137" builtinId="9" hidden="1"/>
+    <cellStyle name="Followed Hyperlink" xfId="139" builtinId="9" hidden="1"/>
+    <cellStyle name="Followed Hyperlink" xfId="141" builtinId="9" hidden="1"/>
+    <cellStyle name="Followed Hyperlink" xfId="143" builtinId="9" hidden="1"/>
+    <cellStyle name="Followed Hyperlink" xfId="145" builtinId="9" hidden="1"/>
+    <cellStyle name="Followed Hyperlink" xfId="147" builtinId="9" hidden="1"/>
+    <cellStyle name="Followed Hyperlink" xfId="149" builtinId="9" hidden="1"/>
+    <cellStyle name="Followed Hyperlink" xfId="151" builtinId="9" hidden="1"/>
+    <cellStyle name="Followed Hyperlink" xfId="153" builtinId="9" hidden="1"/>
     <cellStyle name="Good" xfId="11" builtinId="26"/>
     <cellStyle name="Hyperlink" xfId="1" builtinId="8" hidden="1"/>
     <cellStyle name="Hyperlink" xfId="3" builtinId="8" hidden="1"/>
@@ -910,6 +1228,36 @@
     <cellStyle name="Hyperlink" xfId="88" builtinId="8" hidden="1"/>
     <cellStyle name="Hyperlink" xfId="90" builtinId="8" hidden="1"/>
     <cellStyle name="Hyperlink" xfId="92" builtinId="8" hidden="1"/>
+    <cellStyle name="Hyperlink" xfId="94" builtinId="8" hidden="1"/>
+    <cellStyle name="Hyperlink" xfId="96" builtinId="8" hidden="1"/>
+    <cellStyle name="Hyperlink" xfId="98" builtinId="8" hidden="1"/>
+    <cellStyle name="Hyperlink" xfId="100" builtinId="8" hidden="1"/>
+    <cellStyle name="Hyperlink" xfId="102" builtinId="8" hidden="1"/>
+    <cellStyle name="Hyperlink" xfId="104" builtinId="8" hidden="1"/>
+    <cellStyle name="Hyperlink" xfId="106" builtinId="8" hidden="1"/>
+    <cellStyle name="Hyperlink" xfId="108" builtinId="8" hidden="1"/>
+    <cellStyle name="Hyperlink" xfId="110" builtinId="8" hidden="1"/>
+    <cellStyle name="Hyperlink" xfId="112" builtinId="8" hidden="1"/>
+    <cellStyle name="Hyperlink" xfId="114" builtinId="8" hidden="1"/>
+    <cellStyle name="Hyperlink" xfId="116" builtinId="8" hidden="1"/>
+    <cellStyle name="Hyperlink" xfId="118" builtinId="8" hidden="1"/>
+    <cellStyle name="Hyperlink" xfId="120" builtinId="8" hidden="1"/>
+    <cellStyle name="Hyperlink" xfId="122" builtinId="8" hidden="1"/>
+    <cellStyle name="Hyperlink" xfId="124" builtinId="8" hidden="1"/>
+    <cellStyle name="Hyperlink" xfId="126" builtinId="8" hidden="1"/>
+    <cellStyle name="Hyperlink" xfId="128" builtinId="8" hidden="1"/>
+    <cellStyle name="Hyperlink" xfId="130" builtinId="8" hidden="1"/>
+    <cellStyle name="Hyperlink" xfId="132" builtinId="8" hidden="1"/>
+    <cellStyle name="Hyperlink" xfId="134" builtinId="8" hidden="1"/>
+    <cellStyle name="Hyperlink" xfId="136" builtinId="8" hidden="1"/>
+    <cellStyle name="Hyperlink" xfId="138" builtinId="8" hidden="1"/>
+    <cellStyle name="Hyperlink" xfId="140" builtinId="8" hidden="1"/>
+    <cellStyle name="Hyperlink" xfId="142" builtinId="8" hidden="1"/>
+    <cellStyle name="Hyperlink" xfId="144" builtinId="8" hidden="1"/>
+    <cellStyle name="Hyperlink" xfId="146" builtinId="8" hidden="1"/>
+    <cellStyle name="Hyperlink" xfId="148" builtinId="8" hidden="1"/>
+    <cellStyle name="Hyperlink" xfId="150" builtinId="8" hidden="1"/>
+    <cellStyle name="Hyperlink" xfId="152" builtinId="8" hidden="1"/>
     <cellStyle name="Neutral" xfId="12" builtinId="28"/>
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
   </cellStyles>
@@ -1243,7 +1591,7 @@
   <dimension ref="A1:I60"/>
   <sheetViews>
     <sheetView zoomScale="150" zoomScaleNormal="150" zoomScalePageLayoutView="150" workbookViewId="0">
-      <selection activeCell="D15" sqref="D15"/>
+      <selection activeCell="D16" sqref="D16"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultColWidth="11.5" defaultRowHeight="12.75" customHeight="1" x14ac:dyDescent="0"/>
@@ -1251,7 +1599,7 @@
     <col min="1" max="1" width="27.1640625" customWidth="1"/>
     <col min="2" max="2" width="18.6640625" customWidth="1"/>
     <col min="3" max="3" width="25.1640625" customWidth="1"/>
-    <col min="4" max="4" width="32.1640625" customWidth="1"/>
+    <col min="4" max="4" width="42.1640625" customWidth="1"/>
     <col min="5" max="5" width="15.33203125" customWidth="1"/>
   </cols>
   <sheetData>
@@ -1403,7 +1751,7 @@
       </c>
       <c r="E11" s="2"/>
     </row>
-    <row r="12" spans="1:7" ht="24">
+    <row r="12" spans="1:7" ht="12">
       <c r="A12" t="s">
         <v>148</v>
       </c>
@@ -1419,43 +1767,87 @@
     </row>
     <row r="13" spans="1:7" ht="11" customHeight="1">
       <c r="A13" t="s">
+        <v>161</v>
+      </c>
+      <c r="B13" t="s">
         <v>162</v>
       </c>
-      <c r="B13" t="s">
+      <c r="C13" t="s">
         <v>163</v>
       </c>
-      <c r="C13" t="s">
+      <c r="D13" s="2" t="s">
         <v>164</v>
-      </c>
-      <c r="D13" s="2" t="s">
-        <v>165</v>
       </c>
     </row>
     <row r="14" spans="1:7" ht="11" customHeight="1">
       <c r="A14" t="s">
+        <v>165</v>
+      </c>
+      <c r="B14" t="s">
         <v>166</v>
       </c>
-      <c r="B14" t="s">
+      <c r="C14" t="s">
         <v>167</v>
       </c>
-      <c r="C14" t="s">
+      <c r="D14" s="2" t="s">
         <v>168</v>
       </c>
-      <c r="D14" s="2" t="s">
-        <v>169</v>
-      </c>
-    </row>
-    <row r="15" spans="1:7" ht="12">
-      <c r="D15" s="2"/>
-    </row>
-    <row r="16" spans="1:7" ht="12">
-      <c r="D16" s="2"/>
-    </row>
-    <row r="17" spans="1:9" ht="12">
-      <c r="D17" s="2"/>
-    </row>
-    <row r="18" spans="1:9" ht="12">
-      <c r="D18" s="2"/>
+    </row>
+    <row r="15" spans="1:7" ht="11" customHeight="1">
+      <c r="A15" t="s">
+        <v>182</v>
+      </c>
+      <c r="B15" t="s">
+        <v>183</v>
+      </c>
+      <c r="C15" t="s">
+        <v>184</v>
+      </c>
+      <c r="D15" s="2" t="s">
+        <v>185</v>
+      </c>
+    </row>
+    <row r="16" spans="1:7" ht="11" customHeight="1">
+      <c r="A16" t="s">
+        <v>186</v>
+      </c>
+      <c r="B16" t="s">
+        <v>187</v>
+      </c>
+      <c r="C16" t="s">
+        <v>188</v>
+      </c>
+      <c r="D16" s="2" t="s">
+        <v>255</v>
+      </c>
+    </row>
+    <row r="17" spans="1:9" ht="11" customHeight="1">
+      <c r="A17" t="s">
+        <v>189</v>
+      </c>
+      <c r="B17" t="s">
+        <v>190</v>
+      </c>
+      <c r="C17" t="s">
+        <v>191</v>
+      </c>
+      <c r="D17" s="2" t="s">
+        <v>256</v>
+      </c>
+    </row>
+    <row r="18" spans="1:9" ht="11" customHeight="1">
+      <c r="A18" t="s">
+        <v>192</v>
+      </c>
+      <c r="B18" t="s">
+        <v>193</v>
+      </c>
+      <c r="C18" t="s">
+        <v>194</v>
+      </c>
+      <c r="D18" s="2" t="s">
+        <v>257</v>
+      </c>
     </row>
     <row r="19" spans="1:9" ht="15">
       <c r="A19" s="15" t="s">
@@ -1533,7 +1925,7 @@
       <c r="F24" s="12"/>
       <c r="G24" s="12"/>
     </row>
-    <row r="25" spans="1:9" ht="24">
+    <row r="25" spans="1:9" ht="12">
       <c r="A25" s="7" t="s">
         <v>21</v>
       </c>
@@ -2007,10 +2399,10 @@
 
 <file path=xl/worksheets/sheet3.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <dimension ref="A1:D43"/>
+  <dimension ref="A1:D78"/>
   <sheetViews>
-    <sheetView workbookViewId="0">
-      <selection activeCell="A39" sqref="A39:D42"/>
+    <sheetView tabSelected="1" topLeftCell="A26" workbookViewId="0">
+      <selection activeCell="B35" sqref="B35"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultColWidth="17.1640625" defaultRowHeight="12.75" customHeight="1" x14ac:dyDescent="0"/>
@@ -2283,7 +2675,7 @@
         <v>150</v>
       </c>
       <c r="C32" t="s">
-        <v>156</v>
+        <v>155</v>
       </c>
     </row>
     <row r="33" spans="1:4" ht="12.75" customHeight="1">
@@ -2294,7 +2686,7 @@
         <v>151</v>
       </c>
       <c r="C33" t="s">
-        <v>157</v>
+        <v>156</v>
       </c>
     </row>
     <row r="34" spans="1:4" ht="12.75" customHeight="1">
@@ -2305,7 +2697,7 @@
         <v>152</v>
       </c>
       <c r="C34" t="s">
-        <v>158</v>
+        <v>157</v>
       </c>
     </row>
     <row r="35" spans="1:4" ht="12.75" customHeight="1">
@@ -2313,10 +2705,10 @@
         <v>149</v>
       </c>
       <c r="B35" t="s">
-        <v>153</v>
+        <v>258</v>
       </c>
       <c r="C35" t="s">
-        <v>159</v>
+        <v>158</v>
       </c>
     </row>
     <row r="36" spans="1:4" ht="12.75" customHeight="1">
@@ -2324,10 +2716,10 @@
         <v>149</v>
       </c>
       <c r="B36" t="s">
-        <v>154</v>
+        <v>153</v>
       </c>
       <c r="C36" t="s">
-        <v>160</v>
+        <v>159</v>
       </c>
     </row>
     <row r="37" spans="1:4" ht="12.75" customHeight="1">
@@ -2335,65 +2727,399 @@
         <v>149</v>
       </c>
       <c r="B37" t="s">
-        <v>155</v>
+        <v>154</v>
       </c>
       <c r="C37" t="s">
-        <v>161</v>
+        <v>160</v>
       </c>
     </row>
     <row r="39" spans="1:4" ht="12.75" customHeight="1">
       <c r="A39" t="s">
-        <v>163</v>
+        <v>162</v>
       </c>
       <c r="B39" t="s">
+        <v>169</v>
+      </c>
+      <c r="D39" t="s">
         <v>170</v>
-      </c>
-      <c r="D39" t="s">
-        <v>171</v>
       </c>
     </row>
     <row r="40" spans="1:4" ht="12.75" customHeight="1">
       <c r="A40" t="s">
-        <v>163</v>
+        <v>162</v>
       </c>
       <c r="B40" t="s">
-        <v>172</v>
+        <v>171</v>
       </c>
       <c r="D40" t="s">
-        <v>176</v>
+        <v>175</v>
       </c>
     </row>
     <row r="41" spans="1:4" ht="12.75" customHeight="1">
       <c r="A41" t="s">
-        <v>163</v>
+        <v>162</v>
       </c>
       <c r="B41" t="s">
-        <v>173</v>
+        <v>172</v>
       </c>
       <c r="D41" t="s">
-        <v>177</v>
+        <v>176</v>
       </c>
     </row>
     <row r="42" spans="1:4" ht="12.75" customHeight="1">
       <c r="A42" t="s">
-        <v>163</v>
+        <v>162</v>
       </c>
       <c r="B42" t="s">
-        <v>174</v>
+        <v>173</v>
       </c>
       <c r="D42" t="s">
-        <v>178</v>
+        <v>177</v>
       </c>
     </row>
     <row r="43" spans="1:4" ht="12.75" customHeight="1">
       <c r="A43" t="s">
-        <v>163</v>
+        <v>162</v>
       </c>
       <c r="B43" t="s">
-        <v>175</v>
+        <v>174</v>
       </c>
       <c r="D43" t="s">
-        <v>179</v>
+        <v>178</v>
+      </c>
+    </row>
+    <row r="45" spans="1:4" ht="12.75" customHeight="1">
+      <c r="A45" t="s">
+        <v>166</v>
+      </c>
+      <c r="B45" t="s">
+        <v>205</v>
+      </c>
+      <c r="D45" t="s">
+        <v>206</v>
+      </c>
+    </row>
+    <row r="46" spans="1:4" s="2" customFormat="1" ht="12.75" customHeight="1">
+      <c r="A46" t="s">
+        <v>166</v>
+      </c>
+      <c r="B46" t="s">
+        <v>195</v>
+      </c>
+      <c r="D46" t="s">
+        <v>196</v>
+      </c>
+    </row>
+    <row r="47" spans="1:4" ht="12.75" customHeight="1">
+      <c r="A47" t="s">
+        <v>166</v>
+      </c>
+      <c r="B47" t="s">
+        <v>197</v>
+      </c>
+      <c r="D47" t="s">
+        <v>198</v>
+      </c>
+    </row>
+    <row r="48" spans="1:4" ht="12.75" customHeight="1">
+      <c r="A48" t="s">
+        <v>166</v>
+      </c>
+      <c r="B48" t="s">
+        <v>199</v>
+      </c>
+      <c r="D48" t="s">
+        <v>200</v>
+      </c>
+    </row>
+    <row r="49" spans="1:4" ht="12.75" customHeight="1">
+      <c r="A49" t="s">
+        <v>166</v>
+      </c>
+      <c r="B49" t="s">
+        <v>201</v>
+      </c>
+      <c r="D49" t="s">
+        <v>202</v>
+      </c>
+    </row>
+    <row r="50" spans="1:4" ht="12.75" customHeight="1">
+      <c r="A50" t="s">
+        <v>166</v>
+      </c>
+      <c r="B50" t="s">
+        <v>203</v>
+      </c>
+      <c r="D50" t="s">
+        <v>204</v>
+      </c>
+    </row>
+    <row r="52" spans="1:4" ht="12.75" customHeight="1">
+      <c r="A52" t="s">
+        <v>183</v>
+      </c>
+      <c r="B52" t="s">
+        <v>207</v>
+      </c>
+      <c r="C52" s="2"/>
+      <c r="D52" t="s">
+        <v>208</v>
+      </c>
+    </row>
+    <row r="53" spans="1:4" ht="12.75" customHeight="1">
+      <c r="A53" t="s">
+        <v>183</v>
+      </c>
+      <c r="B53" t="s">
+        <v>209</v>
+      </c>
+      <c r="D53" t="s">
+        <v>210</v>
+      </c>
+    </row>
+    <row r="54" spans="1:4" ht="12.75" customHeight="1">
+      <c r="A54" t="s">
+        <v>183</v>
+      </c>
+      <c r="B54" t="s">
+        <v>211</v>
+      </c>
+      <c r="D54" t="s">
+        <v>212</v>
+      </c>
+    </row>
+    <row r="55" spans="1:4" ht="12.75" customHeight="1">
+      <c r="A55" t="s">
+        <v>183</v>
+      </c>
+      <c r="B55" t="s">
+        <v>213</v>
+      </c>
+      <c r="D55" t="s">
+        <v>214</v>
+      </c>
+    </row>
+    <row r="56" spans="1:4" ht="12.75" customHeight="1">
+      <c r="A56" t="s">
+        <v>183</v>
+      </c>
+      <c r="B56" t="s">
+        <v>215</v>
+      </c>
+      <c r="D56" t="s">
+        <v>216</v>
+      </c>
+    </row>
+    <row r="58" spans="1:4" ht="12.75" customHeight="1">
+      <c r="A58" t="s">
+        <v>187</v>
+      </c>
+      <c r="B58" t="s">
+        <v>217</v>
+      </c>
+      <c r="D58" t="s">
+        <v>218</v>
+      </c>
+    </row>
+    <row r="59" spans="1:4" ht="12.75" customHeight="1">
+      <c r="A59" t="s">
+        <v>187</v>
+      </c>
+      <c r="B59" t="s">
+        <v>219</v>
+      </c>
+      <c r="C59" s="2"/>
+      <c r="D59" t="s">
+        <v>220</v>
+      </c>
+    </row>
+    <row r="60" spans="1:4" ht="12.75" customHeight="1">
+      <c r="A60" t="s">
+        <v>187</v>
+      </c>
+      <c r="B60" t="s">
+        <v>221</v>
+      </c>
+      <c r="D60" t="s">
+        <v>222</v>
+      </c>
+    </row>
+    <row r="61" spans="1:4" ht="12.75" customHeight="1">
+      <c r="A61" t="s">
+        <v>187</v>
+      </c>
+      <c r="B61" t="s">
+        <v>223</v>
+      </c>
+      <c r="D61" t="s">
+        <v>224</v>
+      </c>
+    </row>
+    <row r="62" spans="1:4" ht="12.75" customHeight="1">
+      <c r="A62" t="s">
+        <v>187</v>
+      </c>
+      <c r="B62" t="s">
+        <v>225</v>
+      </c>
+      <c r="D62" t="s">
+        <v>226</v>
+      </c>
+    </row>
+    <row r="63" spans="1:4" ht="12.75" customHeight="1">
+      <c r="A63" t="s">
+        <v>187</v>
+      </c>
+      <c r="B63" t="s">
+        <v>227</v>
+      </c>
+      <c r="D63" t="s">
+        <v>228</v>
+      </c>
+    </row>
+    <row r="64" spans="1:4" ht="12.75" customHeight="1">
+      <c r="A64" t="s">
+        <v>187</v>
+      </c>
+      <c r="B64" t="s">
+        <v>229</v>
+      </c>
+      <c r="D64" t="s">
+        <v>230</v>
+      </c>
+    </row>
+    <row r="66" spans="1:4" ht="12.75" customHeight="1">
+      <c r="A66" t="s">
+        <v>190</v>
+      </c>
+      <c r="B66" t="s">
+        <v>231</v>
+      </c>
+      <c r="D66" t="s">
+        <v>232</v>
+      </c>
+    </row>
+    <row r="67" spans="1:4" ht="12.75" customHeight="1">
+      <c r="A67" t="s">
+        <v>190</v>
+      </c>
+      <c r="B67" t="s">
+        <v>233</v>
+      </c>
+      <c r="C67" s="2"/>
+      <c r="D67" t="s">
+        <v>234</v>
+      </c>
+    </row>
+    <row r="68" spans="1:4" ht="12.75" customHeight="1">
+      <c r="A68" t="s">
+        <v>190</v>
+      </c>
+      <c r="B68" t="s">
+        <v>235</v>
+      </c>
+      <c r="D68" t="s">
+        <v>236</v>
+      </c>
+    </row>
+    <row r="69" spans="1:4" ht="12.75" customHeight="1">
+      <c r="A69" t="s">
+        <v>190</v>
+      </c>
+      <c r="B69" t="s">
+        <v>237</v>
+      </c>
+      <c r="D69" t="s">
+        <v>238</v>
+      </c>
+    </row>
+    <row r="70" spans="1:4" ht="12.75" customHeight="1">
+      <c r="A70" t="s">
+        <v>190</v>
+      </c>
+      <c r="B70" t="s">
+        <v>239</v>
+      </c>
+      <c r="D70" t="s">
+        <v>240</v>
+      </c>
+    </row>
+    <row r="71" spans="1:4" ht="12.75" customHeight="1">
+      <c r="A71" t="s">
+        <v>190</v>
+      </c>
+      <c r="B71" t="s">
+        <v>241</v>
+      </c>
+      <c r="D71" t="s">
+        <v>242</v>
+      </c>
+    </row>
+    <row r="73" spans="1:4" ht="12.75" customHeight="1">
+      <c r="A73" t="s">
+        <v>193</v>
+      </c>
+      <c r="B73" t="s">
+        <v>243</v>
+      </c>
+      <c r="D73" t="s">
+        <v>244</v>
+      </c>
+    </row>
+    <row r="74" spans="1:4" ht="12.75" customHeight="1">
+      <c r="A74" t="s">
+        <v>193</v>
+      </c>
+      <c r="B74" t="s">
+        <v>245</v>
+      </c>
+      <c r="C74" s="2"/>
+      <c r="D74" t="s">
+        <v>246</v>
+      </c>
+    </row>
+    <row r="75" spans="1:4" ht="12.75" customHeight="1">
+      <c r="A75" t="s">
+        <v>193</v>
+      </c>
+      <c r="B75" t="s">
+        <v>247</v>
+      </c>
+      <c r="D75" t="s">
+        <v>248</v>
+      </c>
+    </row>
+    <row r="76" spans="1:4" ht="12.75" customHeight="1">
+      <c r="A76" t="s">
+        <v>193</v>
+      </c>
+      <c r="B76" t="s">
+        <v>249</v>
+      </c>
+      <c r="D76" t="s">
+        <v>250</v>
+      </c>
+    </row>
+    <row r="77" spans="1:4" ht="12.75" customHeight="1">
+      <c r="A77" t="s">
+        <v>193</v>
+      </c>
+      <c r="B77" t="s">
+        <v>251</v>
+      </c>
+      <c r="D77" t="s">
+        <v>252</v>
+      </c>
+    </row>
+    <row r="78" spans="1:4" ht="12.75" customHeight="1">
+      <c r="A78" t="s">
+        <v>193</v>
+      </c>
+      <c r="B78" t="s">
+        <v>253</v>
+      </c>
+      <c r="D78" t="s">
+        <v>254</v>
       </c>
     </row>
   </sheetData>
@@ -2453,7 +3179,7 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:B2"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
+    <sheetView workbookViewId="0">
       <selection activeCell="B2" sqref="B2"/>
     </sheetView>
   </sheetViews>
@@ -2464,15 +3190,15 @@
         <v>1</v>
       </c>
       <c r="B1" t="s">
-        <v>180</v>
+        <v>179</v>
       </c>
     </row>
     <row r="2" spans="1:2">
       <c r="A2" t="s">
+        <v>180</v>
+      </c>
+      <c r="B2" t="s">
         <v>181</v>
-      </c>
-      <c r="B2" t="s">
-        <v>182</v>
       </c>
     </row>
   </sheetData>

</xml_diff>

<commit_message>
disabled next button all together
</commit_message>
<xml_diff>
--- a/opendatakit.collect2/form-files/neonatal/neonatal.xlsx
+++ b/opendatakit.collect2/form-files/neonatal/neonatal.xlsx
@@ -4,7 +4,7 @@
   <fileVersion appName="xl" lastEdited="5" lowestEdited="5" rupBuild="20910"/>
   <workbookPr autoCompressPictures="0"/>
   <bookViews>
-    <workbookView xWindow="1680" yWindow="0" windowWidth="25600" windowHeight="16060" tabRatio="500" activeTab="2"/>
+    <workbookView xWindow="1680" yWindow="0" windowWidth="25600" windowHeight="16060" tabRatio="500"/>
   </bookViews>
   <sheets>
     <sheet name="survey" sheetId="1" r:id="rId1"/>
@@ -23,7 +23,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="348" uniqueCount="259">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="350" uniqueCount="259">
   <si>
     <t>type</t>
   </si>
@@ -37,9 +37,6 @@
     <t>condition</t>
   </si>
   <si>
-    <t>select_one menu</t>
-  </si>
-  <si>
     <t>menu</t>
   </si>
   <si>
@@ -49,27 +46,18 @@
     <t>grid</t>
   </si>
   <si>
-    <t>select_one diagnostic_menu</t>
-  </si>
-  <si>
     <t>diagnostic_menu</t>
   </si>
   <si>
     <t>Diagnostics</t>
   </si>
   <si>
-    <t>select_one procedures_menu</t>
-  </si>
-  <si>
     <t>procedures_menu</t>
   </si>
   <si>
     <t>Procedures</t>
   </si>
   <si>
-    <t>select_one calculators_menu</t>
-  </si>
-  <si>
     <t>calculators_menu</t>
   </si>
   <si>
@@ -241,9 +229,6 @@
     <t>nutritions_menu</t>
   </si>
   <si>
-    <t>select_one nutritions_menu</t>
-  </si>
-  <si>
     <t>nutritions</t>
   </si>
   <si>
@@ -316,9 +301,6 @@
     <t>not(selected(data('menu'),'medications'))</t>
   </si>
   <si>
-    <t>select_one medications_menu</t>
-  </si>
-  <si>
     <t>medications_menu</t>
   </si>
   <si>
@@ -469,9 +451,6 @@
     <t>selected(data('diagnostic_menu'), 'ballardExam')</t>
   </si>
   <si>
-    <t>select_one ballard_menu1</t>
-  </si>
-  <si>
     <t>ballard_menu1</t>
   </si>
   <si>
@@ -800,6 +779,27 @@
   </si>
   <si>
     <t>propliteal</t>
+  </si>
+  <si>
+    <t>menu menu</t>
+  </si>
+  <si>
+    <t>menu diagnostic_menu</t>
+  </si>
+  <si>
+    <t>menu ballard_menu1</t>
+  </si>
+  <si>
+    <t>menu procedures_menu</t>
+  </si>
+  <si>
+    <t>menu calculators_menu</t>
+  </si>
+  <si>
+    <t>menu nutritions_menu</t>
+  </si>
+  <si>
+    <t>menu medications_menu</t>
   </si>
 </sst>
 </file>
@@ -1590,8 +1590,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:I60"/>
   <sheetViews>
-    <sheetView zoomScale="150" zoomScaleNormal="150" zoomScalePageLayoutView="150" workbookViewId="0">
-      <selection activeCell="D16" sqref="D16"/>
+    <sheetView tabSelected="1" topLeftCell="A40" zoomScale="150" zoomScaleNormal="150" zoomScalePageLayoutView="150" workbookViewId="0">
+      <selection activeCell="A50" sqref="A50"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultColWidth="11.5" defaultRowHeight="12.75" customHeight="1" x14ac:dyDescent="0"/>
@@ -1617,18 +1617,18 @@
         <v>3</v>
       </c>
       <c r="E1" s="2" t="s">
-        <v>67</v>
+        <v>63</v>
       </c>
       <c r="F1" t="s">
-        <v>68</v>
+        <v>64</v>
       </c>
       <c r="G1" t="s">
-        <v>77</v>
+        <v>72</v>
       </c>
     </row>
     <row r="2" spans="1:7" ht="15">
       <c r="A2" s="16" t="s">
-        <v>119</v>
+        <v>113</v>
       </c>
       <c r="B2" s="1"/>
       <c r="C2" s="3"/>
@@ -1637,17 +1637,17 @@
     </row>
     <row r="3" spans="1:7" ht="12">
       <c r="A3" s="3" t="s">
+        <v>252</v>
+      </c>
+      <c r="B3" s="4" t="s">
         <v>4</v>
       </c>
-      <c r="B3" s="4" t="s">
+      <c r="C3" s="4" t="s">
         <v>5</v>
-      </c>
-      <c r="C3" s="4" t="s">
-        <v>6</v>
       </c>
       <c r="D3" s="4"/>
       <c r="E3" s="2" t="s">
-        <v>7</v>
+        <v>6</v>
       </c>
     </row>
     <row r="4" spans="1:7" ht="12">
@@ -1659,12 +1659,12 @@
     </row>
     <row r="5" spans="1:7" ht="18" customHeight="1">
       <c r="A5" s="5" t="s">
-        <v>80</v>
+        <v>75</v>
       </c>
       <c r="B5" s="5"/>
       <c r="C5" s="5"/>
       <c r="D5" s="6" t="s">
-        <v>81</v>
+        <v>76</v>
       </c>
       <c r="E5" s="5"/>
       <c r="F5" s="5"/>
@@ -1672,12 +1672,12 @@
     </row>
     <row r="6" spans="1:7" ht="18" customHeight="1">
       <c r="A6" s="5" t="s">
-        <v>122</v>
+        <v>116</v>
       </c>
       <c r="B6" s="5"/>
       <c r="C6" s="5"/>
       <c r="D6" s="6" t="s">
-        <v>123</v>
+        <v>117</v>
       </c>
       <c r="E6" s="5"/>
       <c r="F6" s="5"/>
@@ -1685,7 +1685,7 @@
     </row>
     <row r="7" spans="1:7" s="12" customFormat="1" ht="18" customHeight="1">
       <c r="A7" s="18" t="s">
-        <v>121</v>
+        <v>115</v>
       </c>
       <c r="B7" s="18"/>
       <c r="C7" s="18"/>
@@ -1696,162 +1696,162 @@
     </row>
     <row r="8" spans="1:7" s="12" customFormat="1" ht="18" customHeight="1">
       <c r="A8" t="s">
+        <v>253</v>
+      </c>
+      <c r="B8" t="s">
+        <v>7</v>
+      </c>
+      <c r="C8" t="s">
         <v>8</v>
-      </c>
-      <c r="B8" t="s">
-        <v>9</v>
-      </c>
-      <c r="C8" t="s">
-        <v>10</v>
       </c>
       <c r="D8"/>
       <c r="E8" t="s">
-        <v>7</v>
+        <v>6</v>
       </c>
     </row>
     <row r="9" spans="1:7" ht="18" customHeight="1">
       <c r="A9" s="2" t="s">
-        <v>17</v>
+        <v>13</v>
       </c>
       <c r="B9" s="2"/>
       <c r="C9" s="2" t="s">
-        <v>114</v>
+        <v>108</v>
       </c>
       <c r="D9" s="2" t="s">
-        <v>140</v>
+        <v>134</v>
       </c>
       <c r="E9" s="2"/>
       <c r="F9" t="s">
-        <v>142</v>
+        <v>136</v>
       </c>
     </row>
     <row r="10" spans="1:7" ht="18" customHeight="1">
       <c r="A10" s="2" t="s">
-        <v>115</v>
+        <v>109</v>
       </c>
       <c r="B10" s="4"/>
       <c r="C10" s="2" t="s">
-        <v>113</v>
+        <v>107</v>
       </c>
       <c r="D10" s="2" t="s">
-        <v>143</v>
+        <v>137</v>
       </c>
       <c r="E10" s="2"/>
     </row>
     <row r="11" spans="1:7" ht="18" customHeight="1">
       <c r="A11" s="2" t="s">
-        <v>115</v>
+        <v>109</v>
       </c>
       <c r="B11" s="4"/>
       <c r="C11" s="2" t="s">
-        <v>116</v>
+        <v>110</v>
       </c>
       <c r="D11" s="2" t="s">
-        <v>141</v>
+        <v>135</v>
       </c>
       <c r="E11" s="2"/>
     </row>
     <row r="12" spans="1:7" ht="12">
       <c r="A12" t="s">
-        <v>148</v>
+        <v>254</v>
       </c>
       <c r="B12" t="s">
-        <v>149</v>
+        <v>142</v>
       </c>
       <c r="C12" t="s">
-        <v>91</v>
+        <v>86</v>
       </c>
       <c r="D12" s="2" t="s">
-        <v>147</v>
+        <v>141</v>
       </c>
     </row>
     <row r="13" spans="1:7" ht="11" customHeight="1">
       <c r="A13" t="s">
-        <v>161</v>
+        <v>154</v>
       </c>
       <c r="B13" t="s">
-        <v>162</v>
+        <v>155</v>
       </c>
       <c r="C13" t="s">
-        <v>163</v>
+        <v>156</v>
       </c>
       <c r="D13" s="2" t="s">
-        <v>164</v>
+        <v>157</v>
       </c>
     </row>
     <row r="14" spans="1:7" ht="11" customHeight="1">
       <c r="A14" t="s">
-        <v>165</v>
+        <v>158</v>
       </c>
       <c r="B14" t="s">
-        <v>166</v>
+        <v>159</v>
       </c>
       <c r="C14" t="s">
-        <v>167</v>
+        <v>160</v>
       </c>
       <c r="D14" s="2" t="s">
-        <v>168</v>
+        <v>161</v>
       </c>
     </row>
     <row r="15" spans="1:7" ht="11" customHeight="1">
       <c r="A15" t="s">
-        <v>182</v>
+        <v>175</v>
       </c>
       <c r="B15" t="s">
-        <v>183</v>
+        <v>176</v>
       </c>
       <c r="C15" t="s">
-        <v>184</v>
+        <v>177</v>
       </c>
       <c r="D15" s="2" t="s">
-        <v>185</v>
+        <v>178</v>
       </c>
     </row>
     <row r="16" spans="1:7" ht="11" customHeight="1">
       <c r="A16" t="s">
-        <v>186</v>
+        <v>179</v>
       </c>
       <c r="B16" t="s">
-        <v>187</v>
+        <v>180</v>
       </c>
       <c r="C16" t="s">
-        <v>188</v>
+        <v>181</v>
       </c>
       <c r="D16" s="2" t="s">
-        <v>255</v>
+        <v>248</v>
       </c>
     </row>
     <row r="17" spans="1:9" ht="11" customHeight="1">
       <c r="A17" t="s">
-        <v>189</v>
+        <v>182</v>
       </c>
       <c r="B17" t="s">
-        <v>190</v>
+        <v>183</v>
       </c>
       <c r="C17" t="s">
-        <v>191</v>
+        <v>184</v>
       </c>
       <c r="D17" s="2" t="s">
-        <v>256</v>
+        <v>249</v>
       </c>
     </row>
     <row r="18" spans="1:9" ht="11" customHeight="1">
       <c r="A18" t="s">
-        <v>192</v>
+        <v>185</v>
       </c>
       <c r="B18" t="s">
-        <v>193</v>
+        <v>186</v>
       </c>
       <c r="C18" t="s">
-        <v>194</v>
+        <v>187</v>
       </c>
       <c r="D18" s="2" t="s">
-        <v>257</v>
+        <v>250</v>
       </c>
     </row>
     <row r="19" spans="1:9" ht="15">
       <c r="A19" s="15" t="s">
-        <v>82</v>
+        <v>77</v>
       </c>
       <c r="B19" s="15"/>
       <c r="C19" s="15"/>
@@ -1871,12 +1871,12 @@
     </row>
     <row r="21" spans="1:9" s="15" customFormat="1" ht="15">
       <c r="A21" s="13" t="s">
-        <v>118</v>
+        <v>112</v>
       </c>
       <c r="B21" s="13"/>
       <c r="C21" s="13"/>
       <c r="D21" s="13" t="s">
-        <v>79</v>
+        <v>74</v>
       </c>
       <c r="E21" s="13"/>
       <c r="F21" s="13"/>
@@ -1886,12 +1886,12 @@
     </row>
     <row r="22" spans="1:9" ht="12">
       <c r="A22" s="5" t="s">
-        <v>83</v>
+        <v>78</v>
       </c>
       <c r="B22" s="5"/>
       <c r="C22" s="5"/>
       <c r="D22" s="6" t="s">
-        <v>84</v>
+        <v>79</v>
       </c>
       <c r="E22" s="5"/>
       <c r="F22" s="5"/>
@@ -1899,7 +1899,7 @@
     </row>
     <row r="23" spans="1:9" ht="15">
       <c r="A23" s="15" t="s">
-        <v>117</v>
+        <v>111</v>
       </c>
       <c r="B23" s="15"/>
       <c r="C23" s="15"/>
@@ -1910,29 +1910,29 @@
     </row>
     <row r="24" spans="1:9" ht="12">
       <c r="A24" s="12" t="s">
-        <v>11</v>
+        <v>255</v>
       </c>
       <c r="B24" s="12" t="s">
-        <v>12</v>
+        <v>9</v>
       </c>
       <c r="C24" s="12" t="s">
-        <v>13</v>
+        <v>10</v>
       </c>
       <c r="D24" s="12"/>
       <c r="E24" s="12" t="s">
-        <v>7</v>
+        <v>6</v>
       </c>
       <c r="F24" s="12"/>
       <c r="G24" s="12"/>
     </row>
     <row r="25" spans="1:9" ht="12">
       <c r="A25" s="7" t="s">
-        <v>21</v>
+        <v>17</v>
       </c>
       <c r="B25" s="8"/>
       <c r="C25" s="8"/>
       <c r="D25" s="9" t="s">
-        <v>69</v>
+        <v>65</v>
       </c>
       <c r="E25" s="8"/>
       <c r="F25" s="10"/>
@@ -1940,54 +1940,54 @@
     </row>
     <row r="26" spans="1:9" ht="12.75" customHeight="1">
       <c r="A26" s="4" t="s">
-        <v>17</v>
+        <v>13</v>
       </c>
       <c r="B26" s="2" t="s">
-        <v>85</v>
+        <v>80</v>
       </c>
       <c r="C26" s="2" t="s">
-        <v>86</v>
+        <v>81</v>
       </c>
       <c r="D26" s="2"/>
       <c r="E26" s="4"/>
     </row>
     <row r="27" spans="1:9" ht="12.75" customHeight="1">
       <c r="A27" s="4" t="s">
-        <v>17</v>
+        <v>13</v>
       </c>
       <c r="B27" s="2" t="s">
-        <v>87</v>
+        <v>82</v>
       </c>
       <c r="C27" s="2"/>
       <c r="D27" s="2"/>
       <c r="E27" s="4"/>
       <c r="F27" t="s">
-        <v>18</v>
+        <v>14</v>
       </c>
     </row>
     <row r="28" spans="1:9" ht="12.75" customHeight="1">
       <c r="A28" t="s">
-        <v>17</v>
+        <v>13</v>
       </c>
       <c r="C28" t="s">
-        <v>88</v>
+        <v>83</v>
       </c>
       <c r="D28" s="13"/>
     </row>
     <row r="29" spans="1:9" ht="12.75" customHeight="1">
       <c r="A29" t="s">
-        <v>17</v>
+        <v>13</v>
       </c>
       <c r="B29" t="s">
-        <v>89</v>
+        <v>84</v>
       </c>
       <c r="G29" t="s">
-        <v>90</v>
+        <v>85</v>
       </c>
     </row>
     <row r="30" spans="1:9" ht="12">
       <c r="A30" s="11" t="s">
-        <v>31</v>
+        <v>27</v>
       </c>
       <c r="B30" s="10"/>
       <c r="C30" s="10"/>
@@ -1998,23 +1998,23 @@
     </row>
     <row r="31" spans="1:9" ht="24">
       <c r="A31" s="4" t="s">
-        <v>17</v>
+        <v>13</v>
       </c>
       <c r="B31" s="4"/>
       <c r="C31" s="4" t="s">
-        <v>19</v>
+        <v>15</v>
       </c>
       <c r="D31" s="2" t="s">
-        <v>78</v>
+        <v>73</v>
       </c>
       <c r="E31" s="4"/>
       <c r="F31" t="s">
-        <v>20</v>
+        <v>16</v>
       </c>
     </row>
     <row r="32" spans="1:9" ht="15">
       <c r="A32" s="15" t="s">
-        <v>92</v>
+        <v>87</v>
       </c>
       <c r="B32" s="15"/>
       <c r="C32" s="15"/>
@@ -2036,12 +2036,12 @@
     </row>
     <row r="34" spans="1:9" ht="15">
       <c r="A34" s="14" t="s">
-        <v>124</v>
+        <v>118</v>
       </c>
       <c r="B34" s="14"/>
       <c r="C34" s="14"/>
       <c r="D34" s="13" t="s">
-        <v>125</v>
+        <v>119</v>
       </c>
       <c r="E34" s="14"/>
       <c r="F34" s="14"/>
@@ -2050,12 +2050,12 @@
     </row>
     <row r="35" spans="1:9" ht="12">
       <c r="A35" s="5" t="s">
-        <v>93</v>
+        <v>88</v>
       </c>
       <c r="B35" s="5"/>
       <c r="C35" s="5"/>
       <c r="D35" s="6" t="s">
-        <v>94</v>
+        <v>89</v>
       </c>
       <c r="E35" s="5"/>
       <c r="F35" s="5"/>
@@ -2063,7 +2063,7 @@
     </row>
     <row r="36" spans="1:9" ht="15">
       <c r="A36" s="15" t="s">
-        <v>126</v>
+        <v>120</v>
       </c>
       <c r="B36" s="15"/>
       <c r="C36" s="15"/>
@@ -2074,23 +2074,23 @@
     </row>
     <row r="37" spans="1:9" ht="12">
       <c r="A37" t="s">
-        <v>14</v>
+        <v>256</v>
       </c>
       <c r="B37" t="s">
-        <v>15</v>
+        <v>11</v>
       </c>
       <c r="C37" t="s">
-        <v>16</v>
+        <v>12</v>
       </c>
       <c r="E37" t="s">
-        <v>7</v>
+        <v>6</v>
       </c>
       <c r="F37" s="12"/>
       <c r="G37" s="12"/>
     </row>
     <row r="38" spans="1:9" ht="12">
       <c r="A38" s="4" t="s">
-        <v>21</v>
+        <v>17</v>
       </c>
       <c r="B38" s="4"/>
       <c r="C38" s="4"/>
@@ -2099,60 +2099,60 @@
     </row>
     <row r="39" spans="1:9" ht="12">
       <c r="A39" s="4" t="s">
-        <v>22</v>
+        <v>18</v>
       </c>
       <c r="B39" s="4" t="s">
-        <v>23</v>
+        <v>19</v>
       </c>
       <c r="C39" s="4" t="s">
-        <v>24</v>
+        <v>20</v>
       </c>
       <c r="D39" s="4"/>
       <c r="E39" s="4"/>
     </row>
     <row r="40" spans="1:9" ht="36">
       <c r="A40" s="4" t="s">
-        <v>17</v>
+        <v>13</v>
       </c>
       <c r="B40" s="4"/>
       <c r="C40" s="4" t="s">
-        <v>25</v>
+        <v>21</v>
       </c>
       <c r="D40" s="4" t="s">
-        <v>26</v>
+        <v>22</v>
       </c>
       <c r="E40" s="4"/>
     </row>
     <row r="41" spans="1:9" ht="12">
       <c r="A41" s="4" t="s">
-        <v>22</v>
+        <v>18</v>
       </c>
       <c r="B41" s="4" t="s">
-        <v>27</v>
+        <v>23</v>
       </c>
       <c r="C41" s="4" t="s">
-        <v>28</v>
+        <v>24</v>
       </c>
       <c r="D41" s="4"/>
       <c r="E41" s="4"/>
     </row>
     <row r="42" spans="1:9" ht="36">
       <c r="A42" s="4" t="s">
-        <v>17</v>
+        <v>13</v>
       </c>
       <c r="B42" s="4"/>
       <c r="C42" s="4" t="s">
-        <v>29</v>
+        <v>25</v>
       </c>
       <c r="D42" s="4" t="s">
-        <v>30</v>
+        <v>26</v>
       </c>
       <c r="E42" s="4"/>
       <c r="H42" s="12"/>
     </row>
     <row r="43" spans="1:9" ht="12.75" customHeight="1">
       <c r="A43" s="4" t="s">
-        <v>31</v>
+        <v>27</v>
       </c>
       <c r="B43" s="4"/>
       <c r="C43" s="4"/>
@@ -2161,7 +2161,7 @@
     </row>
     <row r="44" spans="1:9" ht="12.75" customHeight="1">
       <c r="A44" s="15" t="s">
-        <v>95</v>
+        <v>90</v>
       </c>
       <c r="B44" s="15"/>
       <c r="C44" s="15"/>
@@ -2173,22 +2173,22 @@
     <row r="45" spans="1:9" s="12" customFormat="1" ht="12.75" customHeight="1"/>
     <row r="46" spans="1:9" s="14" customFormat="1" ht="12.75" customHeight="1">
       <c r="A46" s="13" t="s">
-        <v>127</v>
+        <v>121</v>
       </c>
       <c r="D46" s="14" t="s">
-        <v>128</v>
+        <v>122</v>
       </c>
       <c r="H46" s="12"/>
       <c r="I46" s="12"/>
     </row>
     <row r="47" spans="1:9" ht="12.75" customHeight="1">
       <c r="A47" s="13" t="s">
-        <v>102</v>
+        <v>96</v>
       </c>
       <c r="B47" s="14"/>
       <c r="C47" s="14"/>
       <c r="D47" s="14" t="s">
-        <v>96</v>
+        <v>91</v>
       </c>
       <c r="E47" s="14"/>
       <c r="F47" s="14"/>
@@ -2196,7 +2196,7 @@
     </row>
     <row r="48" spans="1:9" ht="12.75" customHeight="1">
       <c r="A48" s="15" t="s">
-        <v>144</v>
+        <v>138</v>
       </c>
       <c r="B48" s="18"/>
       <c r="C48" s="18"/>
@@ -2207,24 +2207,24 @@
     </row>
     <row r="49" spans="1:7" ht="12.75" customHeight="1">
       <c r="A49" s="2" t="s">
-        <v>97</v>
+        <v>258</v>
       </c>
       <c r="B49" s="12" t="s">
-        <v>98</v>
+        <v>92</v>
       </c>
       <c r="C49" s="12" t="s">
-        <v>99</v>
+        <v>93</v>
       </c>
       <c r="D49" s="12"/>
       <c r="E49" s="12" t="s">
-        <v>100</v>
+        <v>94</v>
       </c>
       <c r="F49" s="12"/>
       <c r="G49" s="12"/>
     </row>
     <row r="50" spans="1:7" ht="12.75" customHeight="1">
       <c r="A50" s="15" t="s">
-        <v>101</v>
+        <v>95</v>
       </c>
       <c r="B50" s="18"/>
       <c r="C50" s="18"/>
@@ -2243,12 +2243,12 @@
     </row>
     <row r="52" spans="1:7" ht="12.75" customHeight="1">
       <c r="A52" s="13" t="s">
-        <v>135</v>
+        <v>129</v>
       </c>
       <c r="B52" s="14"/>
       <c r="C52" s="14"/>
       <c r="D52" s="14" t="s">
-        <v>137</v>
+        <v>131</v>
       </c>
       <c r="E52" s="14"/>
       <c r="F52" s="14"/>
@@ -2256,12 +2256,12 @@
     </row>
     <row r="53" spans="1:7" ht="12.75" customHeight="1">
       <c r="A53" s="13" t="s">
-        <v>136</v>
+        <v>130</v>
       </c>
       <c r="B53" s="14"/>
       <c r="C53" s="14"/>
       <c r="D53" s="14" t="s">
-        <v>138</v>
+        <v>132</v>
       </c>
       <c r="E53" s="14"/>
       <c r="F53" s="14"/>
@@ -2269,7 +2269,7 @@
     </row>
     <row r="54" spans="1:7" ht="12.75" customHeight="1">
       <c r="A54" s="15" t="s">
-        <v>145</v>
+        <v>139</v>
       </c>
       <c r="B54" s="18"/>
       <c r="C54" s="18"/>
@@ -2280,27 +2280,27 @@
     </row>
     <row r="55" spans="1:7" ht="12.75" customHeight="1">
       <c r="A55" t="s">
-        <v>72</v>
+        <v>257</v>
       </c>
       <c r="B55" t="s">
-        <v>71</v>
+        <v>67</v>
       </c>
       <c r="C55" t="s">
-        <v>74</v>
+        <v>69</v>
       </c>
       <c r="E55" t="s">
-        <v>7</v>
+        <v>6</v>
       </c>
       <c r="F55" s="12"/>
       <c r="G55" s="12"/>
     </row>
     <row r="56" spans="1:7" ht="12.75" customHeight="1">
       <c r="A56" s="2" t="s">
-        <v>17</v>
+        <v>13</v>
       </c>
       <c r="B56" s="12"/>
       <c r="C56" s="12" t="s">
-        <v>70</v>
+        <v>66</v>
       </c>
       <c r="D56" s="12"/>
       <c r="E56" s="12"/>
@@ -2309,7 +2309,7 @@
     </row>
     <row r="57" spans="1:7" ht="12.75" customHeight="1">
       <c r="A57" s="15" t="s">
-        <v>139</v>
+        <v>133</v>
       </c>
       <c r="B57" s="18"/>
       <c r="C57" s="18"/>
@@ -2320,7 +2320,7 @@
     </row>
     <row r="60" spans="1:7" ht="12.75" customHeight="1">
       <c r="A60" s="17" t="s">
-        <v>120</v>
+        <v>114</v>
       </c>
     </row>
   </sheetData>
@@ -2352,39 +2352,39 @@
         <v>1</v>
       </c>
       <c r="B1" t="s">
-        <v>32</v>
+        <v>28</v>
       </c>
     </row>
     <row r="2" spans="1:2" ht="12.75" customHeight="1">
       <c r="A2" t="s">
-        <v>33</v>
+        <v>29</v>
       </c>
       <c r="B2" t="s">
-        <v>34</v>
+        <v>30</v>
       </c>
     </row>
     <row r="3" spans="1:2" ht="12.75" customHeight="1">
       <c r="A3" t="s">
-        <v>35</v>
+        <v>31</v>
       </c>
       <c r="B3" t="s">
-        <v>36</v>
+        <v>32</v>
       </c>
     </row>
     <row r="4" spans="1:2" ht="12.75" customHeight="1">
       <c r="A4" t="s">
-        <v>37</v>
+        <v>33</v>
       </c>
       <c r="B4" t="s">
-        <v>38</v>
+        <v>34</v>
       </c>
     </row>
     <row r="5" spans="1:2" ht="12.75" customHeight="1">
       <c r="A5" t="s">
-        <v>39</v>
+        <v>35</v>
       </c>
       <c r="B5" t="s">
-        <v>40</v>
+        <v>36</v>
       </c>
     </row>
   </sheetData>
@@ -2401,7 +2401,7 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:D78"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A26" workbookViewId="0">
+    <sheetView topLeftCell="A26" workbookViewId="0">
       <selection activeCell="B35" sqref="B35"/>
     </sheetView>
   </sheetViews>
@@ -2413,7 +2413,7 @@
   <sheetData>
     <row r="1" spans="1:4" ht="12.75" customHeight="1">
       <c r="A1" t="s">
-        <v>41</v>
+        <v>37</v>
       </c>
       <c r="B1" t="s">
         <v>1</v>
@@ -2422,704 +2422,704 @@
         <v>2</v>
       </c>
       <c r="D1" t="s">
-        <v>68</v>
+        <v>64</v>
       </c>
     </row>
     <row r="2" spans="1:4" ht="12.75" customHeight="1">
       <c r="A2" t="s">
-        <v>5</v>
+        <v>4</v>
       </c>
       <c r="B2" t="s">
-        <v>42</v>
+        <v>38</v>
       </c>
       <c r="C2" t="s">
-        <v>10</v>
+        <v>8</v>
       </c>
     </row>
     <row r="3" spans="1:4" ht="12.75" customHeight="1">
       <c r="A3" t="s">
-        <v>5</v>
+        <v>4</v>
       </c>
       <c r="B3" t="s">
-        <v>43</v>
+        <v>39</v>
       </c>
       <c r="C3" t="s">
-        <v>13</v>
+        <v>10</v>
       </c>
     </row>
     <row r="4" spans="1:4" ht="12.75" customHeight="1">
       <c r="A4" t="s">
-        <v>5</v>
+        <v>4</v>
       </c>
       <c r="B4" t="s">
-        <v>44</v>
+        <v>40</v>
       </c>
       <c r="C4" t="s">
-        <v>45</v>
+        <v>41</v>
       </c>
     </row>
     <row r="5" spans="1:4" ht="12.75" customHeight="1">
       <c r="A5" t="s">
-        <v>5</v>
+        <v>4</v>
       </c>
       <c r="B5" t="s">
-        <v>73</v>
+        <v>68</v>
       </c>
       <c r="C5" t="s">
-        <v>74</v>
+        <v>69</v>
       </c>
     </row>
     <row r="6" spans="1:4" ht="12.75" customHeight="1">
       <c r="A6" t="s">
-        <v>5</v>
+        <v>4</v>
       </c>
       <c r="B6" t="s">
-        <v>109</v>
+        <v>103</v>
       </c>
       <c r="C6" t="s">
-        <v>99</v>
+        <v>93</v>
       </c>
     </row>
     <row r="9" spans="1:4" ht="12.75" customHeight="1">
       <c r="A9" t="s">
-        <v>12</v>
+        <v>9</v>
       </c>
       <c r="B9" t="s">
-        <v>46</v>
+        <v>42</v>
       </c>
       <c r="C9" t="s">
-        <v>47</v>
+        <v>43</v>
       </c>
     </row>
     <row r="10" spans="1:4" ht="12.75" customHeight="1">
       <c r="A10" t="s">
-        <v>12</v>
+        <v>9</v>
       </c>
       <c r="B10" t="s">
-        <v>48</v>
+        <v>44</v>
       </c>
       <c r="C10" t="s">
-        <v>49</v>
+        <v>45</v>
       </c>
     </row>
     <row r="11" spans="1:4" ht="12.75" customHeight="1">
       <c r="A11" t="s">
-        <v>12</v>
+        <v>9</v>
       </c>
       <c r="B11" t="s">
-        <v>76</v>
+        <v>71</v>
       </c>
       <c r="C11" t="s">
-        <v>75</v>
+        <v>70</v>
       </c>
     </row>
     <row r="13" spans="1:4" ht="12.75" customHeight="1">
       <c r="A13" t="s">
-        <v>9</v>
+        <v>7</v>
       </c>
       <c r="B13" t="s">
-        <v>50</v>
+        <v>46</v>
       </c>
       <c r="C13" t="s">
-        <v>51</v>
+        <v>47</v>
       </c>
     </row>
     <row r="14" spans="1:4" ht="12.75" customHeight="1">
       <c r="A14" t="s">
-        <v>9</v>
+        <v>7</v>
       </c>
       <c r="B14" t="s">
-        <v>112</v>
+        <v>106</v>
       </c>
       <c r="C14" t="s">
-        <v>113</v>
+        <v>107</v>
       </c>
     </row>
     <row r="15" spans="1:4" ht="12.75" customHeight="1">
       <c r="A15" t="s">
-        <v>9</v>
+        <v>7</v>
       </c>
       <c r="B15" t="s">
-        <v>110</v>
+        <v>104</v>
       </c>
       <c r="C15" t="s">
-        <v>111</v>
+        <v>105</v>
       </c>
     </row>
     <row r="16" spans="1:4" ht="12.75" customHeight="1">
       <c r="A16" t="s">
-        <v>9</v>
+        <v>7</v>
       </c>
       <c r="B16" t="s">
-        <v>146</v>
+        <v>140</v>
       </c>
       <c r="C16" t="s">
-        <v>91</v>
+        <v>86</v>
       </c>
     </row>
     <row r="18" spans="1:3" ht="12.75" customHeight="1">
       <c r="A18" t="s">
-        <v>15</v>
+        <v>11</v>
       </c>
       <c r="B18" t="s">
-        <v>52</v>
+        <v>48</v>
       </c>
       <c r="C18" t="s">
-        <v>53</v>
+        <v>49</v>
       </c>
     </row>
     <row r="19" spans="1:3" ht="12.75" customHeight="1">
       <c r="A19" t="s">
-        <v>15</v>
+        <v>11</v>
       </c>
       <c r="B19" t="s">
-        <v>54</v>
+        <v>50</v>
       </c>
       <c r="C19" t="s">
-        <v>55</v>
+        <v>51</v>
       </c>
     </row>
     <row r="21" spans="1:3" ht="12.75" customHeight="1">
       <c r="A21" t="s">
+        <v>92</v>
+      </c>
+      <c r="B21" t="s">
+        <v>97</v>
+      </c>
+      <c r="C21" t="s">
         <v>98</v>
-      </c>
-      <c r="B21" t="s">
-        <v>103</v>
-      </c>
-      <c r="C21" t="s">
-        <v>104</v>
       </c>
     </row>
     <row r="22" spans="1:3" ht="12.75" customHeight="1">
       <c r="A22" t="s">
-        <v>98</v>
+        <v>92</v>
       </c>
       <c r="B22" t="s">
-        <v>105</v>
+        <v>99</v>
       </c>
       <c r="C22" t="s">
-        <v>106</v>
+        <v>100</v>
       </c>
     </row>
     <row r="23" spans="1:3" ht="12.75" customHeight="1">
       <c r="A23" t="s">
-        <v>98</v>
+        <v>92</v>
       </c>
       <c r="B23" t="s">
-        <v>107</v>
+        <v>101</v>
       </c>
       <c r="C23" t="s">
-        <v>108</v>
+        <v>102</v>
       </c>
     </row>
     <row r="25" spans="1:3" ht="12.75" customHeight="1">
       <c r="A25" t="s">
-        <v>71</v>
+        <v>67</v>
       </c>
       <c r="B25" t="s">
-        <v>129</v>
+        <v>123</v>
       </c>
       <c r="C25" t="s">
-        <v>130</v>
+        <v>124</v>
       </c>
     </row>
     <row r="26" spans="1:3" ht="12.75" customHeight="1">
       <c r="A26" t="s">
-        <v>71</v>
+        <v>67</v>
       </c>
       <c r="B26" t="s">
-        <v>131</v>
+        <v>125</v>
       </c>
       <c r="C26" t="s">
-        <v>133</v>
+        <v>127</v>
       </c>
     </row>
     <row r="27" spans="1:3" ht="12.75" customHeight="1">
       <c r="A27" t="s">
-        <v>71</v>
+        <v>67</v>
       </c>
       <c r="B27" t="s">
-        <v>132</v>
+        <v>126</v>
       </c>
       <c r="C27" t="s">
-        <v>134</v>
+        <v>128</v>
       </c>
     </row>
     <row r="29" spans="1:3" ht="12.75" customHeight="1">
       <c r="A29" t="s">
-        <v>56</v>
+        <v>52</v>
       </c>
       <c r="B29" t="s">
-        <v>57</v>
+        <v>53</v>
       </c>
       <c r="C29" t="s">
-        <v>58</v>
+        <v>54</v>
       </c>
     </row>
     <row r="30" spans="1:3" ht="12.75" customHeight="1">
       <c r="A30" t="s">
+        <v>52</v>
+      </c>
+      <c r="B30" t="s">
+        <v>55</v>
+      </c>
+      <c r="C30" t="s">
         <v>56</v>
-      </c>
-      <c r="B30" t="s">
-        <v>59</v>
-      </c>
-      <c r="C30" t="s">
-        <v>60</v>
       </c>
     </row>
     <row r="32" spans="1:3" ht="12.75" customHeight="1">
       <c r="A32" t="s">
-        <v>149</v>
+        <v>142</v>
       </c>
       <c r="B32" t="s">
-        <v>150</v>
+        <v>143</v>
       </c>
       <c r="C32" t="s">
-        <v>155</v>
+        <v>148</v>
       </c>
     </row>
     <row r="33" spans="1:4" ht="12.75" customHeight="1">
       <c r="A33" t="s">
+        <v>142</v>
+      </c>
+      <c r="B33" t="s">
+        <v>144</v>
+      </c>
+      <c r="C33" t="s">
         <v>149</v>
-      </c>
-      <c r="B33" t="s">
-        <v>151</v>
-      </c>
-      <c r="C33" t="s">
-        <v>156</v>
       </c>
     </row>
     <row r="34" spans="1:4" ht="12.75" customHeight="1">
       <c r="A34" t="s">
-        <v>149</v>
+        <v>142</v>
       </c>
       <c r="B34" t="s">
-        <v>152</v>
+        <v>145</v>
       </c>
       <c r="C34" t="s">
-        <v>157</v>
+        <v>150</v>
       </c>
     </row>
     <row r="35" spans="1:4" ht="12.75" customHeight="1">
       <c r="A35" t="s">
-        <v>149</v>
+        <v>142</v>
       </c>
       <c r="B35" t="s">
-        <v>258</v>
+        <v>251</v>
       </c>
       <c r="C35" t="s">
-        <v>158</v>
+        <v>151</v>
       </c>
     </row>
     <row r="36" spans="1:4" ht="12.75" customHeight="1">
       <c r="A36" t="s">
-        <v>149</v>
+        <v>142</v>
       </c>
       <c r="B36" t="s">
-        <v>153</v>
+        <v>146</v>
       </c>
       <c r="C36" t="s">
-        <v>159</v>
+        <v>152</v>
       </c>
     </row>
     <row r="37" spans="1:4" ht="12.75" customHeight="1">
       <c r="A37" t="s">
-        <v>149</v>
+        <v>142</v>
       </c>
       <c r="B37" t="s">
-        <v>154</v>
+        <v>147</v>
       </c>
       <c r="C37" t="s">
-        <v>160</v>
+        <v>153</v>
       </c>
     </row>
     <row r="39" spans="1:4" ht="12.75" customHeight="1">
       <c r="A39" t="s">
+        <v>155</v>
+      </c>
+      <c r="B39" t="s">
         <v>162</v>
       </c>
-      <c r="B39" t="s">
-        <v>169</v>
-      </c>
       <c r="D39" t="s">
-        <v>170</v>
+        <v>163</v>
       </c>
     </row>
     <row r="40" spans="1:4" ht="12.75" customHeight="1">
       <c r="A40" t="s">
-        <v>162</v>
+        <v>155</v>
       </c>
       <c r="B40" t="s">
-        <v>171</v>
+        <v>164</v>
       </c>
       <c r="D40" t="s">
-        <v>175</v>
+        <v>168</v>
       </c>
     </row>
     <row r="41" spans="1:4" ht="12.75" customHeight="1">
       <c r="A41" t="s">
-        <v>162</v>
+        <v>155</v>
       </c>
       <c r="B41" t="s">
-        <v>172</v>
+        <v>165</v>
       </c>
       <c r="D41" t="s">
-        <v>176</v>
+        <v>169</v>
       </c>
     </row>
     <row r="42" spans="1:4" ht="12.75" customHeight="1">
       <c r="A42" t="s">
-        <v>162</v>
+        <v>155</v>
       </c>
       <c r="B42" t="s">
-        <v>173</v>
+        <v>166</v>
       </c>
       <c r="D42" t="s">
-        <v>177</v>
+        <v>170</v>
       </c>
     </row>
     <row r="43" spans="1:4" ht="12.75" customHeight="1">
       <c r="A43" t="s">
-        <v>162</v>
+        <v>155</v>
       </c>
       <c r="B43" t="s">
-        <v>174</v>
+        <v>167</v>
       </c>
       <c r="D43" t="s">
-        <v>178</v>
+        <v>171</v>
       </c>
     </row>
     <row r="45" spans="1:4" ht="12.75" customHeight="1">
       <c r="A45" t="s">
-        <v>166</v>
+        <v>159</v>
       </c>
       <c r="B45" t="s">
-        <v>205</v>
+        <v>198</v>
       </c>
       <c r="D45" t="s">
-        <v>206</v>
+        <v>199</v>
       </c>
     </row>
     <row r="46" spans="1:4" s="2" customFormat="1" ht="12.75" customHeight="1">
       <c r="A46" t="s">
-        <v>166</v>
+        <v>159</v>
       </c>
       <c r="B46" t="s">
-        <v>195</v>
+        <v>188</v>
       </c>
       <c r="D46" t="s">
-        <v>196</v>
+        <v>189</v>
       </c>
     </row>
     <row r="47" spans="1:4" ht="12.75" customHeight="1">
       <c r="A47" t="s">
-        <v>166</v>
+        <v>159</v>
       </c>
       <c r="B47" t="s">
-        <v>197</v>
+        <v>190</v>
       </c>
       <c r="D47" t="s">
-        <v>198</v>
+        <v>191</v>
       </c>
     </row>
     <row r="48" spans="1:4" ht="12.75" customHeight="1">
       <c r="A48" t="s">
-        <v>166</v>
+        <v>159</v>
       </c>
       <c r="B48" t="s">
-        <v>199</v>
+        <v>192</v>
       </c>
       <c r="D48" t="s">
-        <v>200</v>
+        <v>193</v>
       </c>
     </row>
     <row r="49" spans="1:4" ht="12.75" customHeight="1">
       <c r="A49" t="s">
-        <v>166</v>
+        <v>159</v>
       </c>
       <c r="B49" t="s">
-        <v>201</v>
+        <v>194</v>
       </c>
       <c r="D49" t="s">
-        <v>202</v>
+        <v>195</v>
       </c>
     </row>
     <row r="50" spans="1:4" ht="12.75" customHeight="1">
       <c r="A50" t="s">
-        <v>166</v>
+        <v>159</v>
       </c>
       <c r="B50" t="s">
-        <v>203</v>
+        <v>196</v>
       </c>
       <c r="D50" t="s">
-        <v>204</v>
+        <v>197</v>
       </c>
     </row>
     <row r="52" spans="1:4" ht="12.75" customHeight="1">
       <c r="A52" t="s">
-        <v>183</v>
+        <v>176</v>
       </c>
       <c r="B52" t="s">
-        <v>207</v>
+        <v>200</v>
       </c>
       <c r="C52" s="2"/>
       <c r="D52" t="s">
-        <v>208</v>
+        <v>201</v>
       </c>
     </row>
     <row r="53" spans="1:4" ht="12.75" customHeight="1">
       <c r="A53" t="s">
-        <v>183</v>
+        <v>176</v>
       </c>
       <c r="B53" t="s">
-        <v>209</v>
+        <v>202</v>
       </c>
       <c r="D53" t="s">
-        <v>210</v>
+        <v>203</v>
       </c>
     </row>
     <row r="54" spans="1:4" ht="12.75" customHeight="1">
       <c r="A54" t="s">
-        <v>183</v>
+        <v>176</v>
       </c>
       <c r="B54" t="s">
-        <v>211</v>
+        <v>204</v>
       </c>
       <c r="D54" t="s">
-        <v>212</v>
+        <v>205</v>
       </c>
     </row>
     <row r="55" spans="1:4" ht="12.75" customHeight="1">
       <c r="A55" t="s">
-        <v>183</v>
+        <v>176</v>
       </c>
       <c r="B55" t="s">
-        <v>213</v>
+        <v>206</v>
       </c>
       <c r="D55" t="s">
-        <v>214</v>
+        <v>207</v>
       </c>
     </row>
     <row r="56" spans="1:4" ht="12.75" customHeight="1">
       <c r="A56" t="s">
-        <v>183</v>
+        <v>176</v>
       </c>
       <c r="B56" t="s">
-        <v>215</v>
+        <v>208</v>
       </c>
       <c r="D56" t="s">
-        <v>216</v>
+        <v>209</v>
       </c>
     </row>
     <row r="58" spans="1:4" ht="12.75" customHeight="1">
       <c r="A58" t="s">
-        <v>187</v>
+        <v>180</v>
       </c>
       <c r="B58" t="s">
-        <v>217</v>
+        <v>210</v>
       </c>
       <c r="D58" t="s">
-        <v>218</v>
+        <v>211</v>
       </c>
     </row>
     <row r="59" spans="1:4" ht="12.75" customHeight="1">
       <c r="A59" t="s">
-        <v>187</v>
+        <v>180</v>
       </c>
       <c r="B59" t="s">
-        <v>219</v>
+        <v>212</v>
       </c>
       <c r="C59" s="2"/>
       <c r="D59" t="s">
-        <v>220</v>
+        <v>213</v>
       </c>
     </row>
     <row r="60" spans="1:4" ht="12.75" customHeight="1">
       <c r="A60" t="s">
-        <v>187</v>
+        <v>180</v>
       </c>
       <c r="B60" t="s">
-        <v>221</v>
+        <v>214</v>
       </c>
       <c r="D60" t="s">
-        <v>222</v>
+        <v>215</v>
       </c>
     </row>
     <row r="61" spans="1:4" ht="12.75" customHeight="1">
       <c r="A61" t="s">
-        <v>187</v>
+        <v>180</v>
       </c>
       <c r="B61" t="s">
-        <v>223</v>
+        <v>216</v>
       </c>
       <c r="D61" t="s">
-        <v>224</v>
+        <v>217</v>
       </c>
     </row>
     <row r="62" spans="1:4" ht="12.75" customHeight="1">
       <c r="A62" t="s">
-        <v>187</v>
+        <v>180</v>
       </c>
       <c r="B62" t="s">
-        <v>225</v>
+        <v>218</v>
       </c>
       <c r="D62" t="s">
-        <v>226</v>
+        <v>219</v>
       </c>
     </row>
     <row r="63" spans="1:4" ht="12.75" customHeight="1">
       <c r="A63" t="s">
-        <v>187</v>
+        <v>180</v>
       </c>
       <c r="B63" t="s">
-        <v>227</v>
+        <v>220</v>
       </c>
       <c r="D63" t="s">
-        <v>228</v>
+        <v>221</v>
       </c>
     </row>
     <row r="64" spans="1:4" ht="12.75" customHeight="1">
       <c r="A64" t="s">
-        <v>187</v>
+        <v>180</v>
       </c>
       <c r="B64" t="s">
-        <v>229</v>
+        <v>222</v>
       </c>
       <c r="D64" t="s">
-        <v>230</v>
+        <v>223</v>
       </c>
     </row>
     <row r="66" spans="1:4" ht="12.75" customHeight="1">
       <c r="A66" t="s">
-        <v>190</v>
+        <v>183</v>
       </c>
       <c r="B66" t="s">
-        <v>231</v>
+        <v>224</v>
       </c>
       <c r="D66" t="s">
-        <v>232</v>
+        <v>225</v>
       </c>
     </row>
     <row r="67" spans="1:4" ht="12.75" customHeight="1">
       <c r="A67" t="s">
-        <v>190</v>
+        <v>183</v>
       </c>
       <c r="B67" t="s">
-        <v>233</v>
+        <v>226</v>
       </c>
       <c r="C67" s="2"/>
       <c r="D67" t="s">
-        <v>234</v>
+        <v>227</v>
       </c>
     </row>
     <row r="68" spans="1:4" ht="12.75" customHeight="1">
       <c r="A68" t="s">
-        <v>190</v>
+        <v>183</v>
       </c>
       <c r="B68" t="s">
-        <v>235</v>
+        <v>228</v>
       </c>
       <c r="D68" t="s">
-        <v>236</v>
+        <v>229</v>
       </c>
     </row>
     <row r="69" spans="1:4" ht="12.75" customHeight="1">
       <c r="A69" t="s">
-        <v>190</v>
+        <v>183</v>
       </c>
       <c r="B69" t="s">
-        <v>237</v>
+        <v>230</v>
       </c>
       <c r="D69" t="s">
-        <v>238</v>
+        <v>231</v>
       </c>
     </row>
     <row r="70" spans="1:4" ht="12.75" customHeight="1">
       <c r="A70" t="s">
-        <v>190</v>
+        <v>183</v>
       </c>
       <c r="B70" t="s">
-        <v>239</v>
+        <v>232</v>
       </c>
       <c r="D70" t="s">
-        <v>240</v>
+        <v>233</v>
       </c>
     </row>
     <row r="71" spans="1:4" ht="12.75" customHeight="1">
       <c r="A71" t="s">
-        <v>190</v>
+        <v>183</v>
       </c>
       <c r="B71" t="s">
-        <v>241</v>
+        <v>234</v>
       </c>
       <c r="D71" t="s">
-        <v>242</v>
+        <v>235</v>
       </c>
     </row>
     <row r="73" spans="1:4" ht="12.75" customHeight="1">
       <c r="A73" t="s">
-        <v>193</v>
+        <v>186</v>
       </c>
       <c r="B73" t="s">
-        <v>243</v>
+        <v>236</v>
       </c>
       <c r="D73" t="s">
-        <v>244</v>
+        <v>237</v>
       </c>
     </row>
     <row r="74" spans="1:4" ht="12.75" customHeight="1">
       <c r="A74" t="s">
-        <v>193</v>
+        <v>186</v>
       </c>
       <c r="B74" t="s">
-        <v>245</v>
+        <v>238</v>
       </c>
       <c r="C74" s="2"/>
       <c r="D74" t="s">
-        <v>246</v>
+        <v>239</v>
       </c>
     </row>
     <row r="75" spans="1:4" ht="12.75" customHeight="1">
       <c r="A75" t="s">
-        <v>193</v>
+        <v>186</v>
       </c>
       <c r="B75" t="s">
-        <v>247</v>
+        <v>240</v>
       </c>
       <c r="D75" t="s">
-        <v>248</v>
+        <v>241</v>
       </c>
     </row>
     <row r="76" spans="1:4" ht="12.75" customHeight="1">
       <c r="A76" t="s">
-        <v>193</v>
+        <v>186</v>
       </c>
       <c r="B76" t="s">
-        <v>249</v>
+        <v>242</v>
       </c>
       <c r="D76" t="s">
-        <v>250</v>
+        <v>243</v>
       </c>
     </row>
     <row r="77" spans="1:4" ht="12.75" customHeight="1">
       <c r="A77" t="s">
-        <v>193</v>
+        <v>186</v>
       </c>
       <c r="B77" t="s">
-        <v>251</v>
+        <v>244</v>
       </c>
       <c r="D77" t="s">
-        <v>252</v>
+        <v>245</v>
       </c>
     </row>
     <row r="78" spans="1:4" ht="12.75" customHeight="1">
       <c r="A78" t="s">
-        <v>193</v>
+        <v>186</v>
       </c>
       <c r="B78" t="s">
-        <v>253</v>
+        <v>246</v>
       </c>
       <c r="D78" t="s">
-        <v>254</v>
+        <v>247</v>
       </c>
     </row>
   </sheetData>
@@ -3143,26 +3143,26 @@
   <sheetData>
     <row r="1" spans="1:2" ht="12.75" customHeight="1">
       <c r="A1" t="s">
-        <v>61</v>
+        <v>57</v>
       </c>
       <c r="B1" t="s">
-        <v>62</v>
+        <v>58</v>
       </c>
     </row>
     <row r="2" spans="1:2" ht="12.75" customHeight="1">
       <c r="A2" t="s">
-        <v>63</v>
+        <v>59</v>
       </c>
       <c r="B2" t="s">
-        <v>64</v>
+        <v>60</v>
       </c>
     </row>
     <row r="3" spans="1:2" ht="12.75" customHeight="1">
       <c r="A3" t="s">
-        <v>65</v>
+        <v>61</v>
       </c>
       <c r="B3" t="s">
-        <v>66</v>
+        <v>62</v>
       </c>
     </row>
   </sheetData>
@@ -3177,10 +3177,10 @@
 
 <file path=xl/worksheets/sheet5.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <dimension ref="A1:B2"/>
+  <dimension ref="A1:B3"/>
   <sheetViews>
     <sheetView workbookViewId="0">
-      <selection activeCell="B2" sqref="B2"/>
+      <selection activeCell="A4" sqref="A4"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="12" x14ac:dyDescent="0"/>
@@ -3190,15 +3190,23 @@
         <v>1</v>
       </c>
       <c r="B1" t="s">
-        <v>179</v>
+        <v>172</v>
       </c>
     </row>
     <row r="2" spans="1:2">
       <c r="A2" t="s">
-        <v>180</v>
+        <v>173</v>
       </c>
       <c r="B2" t="s">
-        <v>181</v>
+        <v>174</v>
+      </c>
+    </row>
+    <row r="3" spans="1:2">
+      <c r="A3" t="s">
+        <v>4</v>
+      </c>
+      <c r="B3" t="s">
+        <v>174</v>
       </c>
     </row>
   </sheetData>

</xml_diff>

<commit_message>
added calculators and notes to displa ballard exam
</commit_message>
<xml_diff>
--- a/opendatakit.collect2/form-files/neonatal/neonatal.xlsx
+++ b/opendatakit.collect2/form-files/neonatal/neonatal.xlsx
@@ -4,7 +4,7 @@
   <fileVersion appName="xl" lastEdited="5" lowestEdited="5" rupBuild="20910"/>
   <workbookPr autoCompressPictures="0"/>
   <bookViews>
-    <workbookView xWindow="1680" yWindow="0" windowWidth="25600" windowHeight="16060" tabRatio="500"/>
+    <workbookView xWindow="0" yWindow="0" windowWidth="28800" windowHeight="17480" tabRatio="500"/>
   </bookViews>
   <sheets>
     <sheet name="survey" sheetId="1" r:id="rId1"/>
@@ -23,7 +23,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="350" uniqueCount="259">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="380" uniqueCount="280">
   <si>
     <t>type</t>
   </si>
@@ -463,6 +463,9 @@
     <t>arm</t>
   </si>
   <si>
+    <t>popliteal</t>
+  </si>
+  <si>
     <t>scarf</t>
   </si>
   <si>
@@ -562,15 +565,6 @@
     <t>selected(data('ballard_menu1'), 'arm')</t>
   </si>
   <si>
-    <t>image_slider propliteal_slider</t>
-  </si>
-  <si>
-    <t>propliteal_slider</t>
-  </si>
-  <si>
-    <t>Choose Propliteal Angle</t>
-  </si>
-  <si>
     <t>image_slider scarf_slider</t>
   </si>
   <si>
@@ -655,48 +649,6 @@
     <t>img/ballard/arm_recoil4.png</t>
   </si>
   <si>
-    <t>propliteal-1</t>
-  </si>
-  <si>
-    <t>img/ballard/propliteal-1.png</t>
-  </si>
-  <si>
-    <t>propliteal0</t>
-  </si>
-  <si>
-    <t>img/ballard/propliteal0.png</t>
-  </si>
-  <si>
-    <t>propliteal1</t>
-  </si>
-  <si>
-    <t>img/ballard/propliteal1.png</t>
-  </si>
-  <si>
-    <t>propliteal2</t>
-  </si>
-  <si>
-    <t>img/ballard/propliteal2.png</t>
-  </si>
-  <si>
-    <t>propliteal3</t>
-  </si>
-  <si>
-    <t>img/ballard/propliteal3.png</t>
-  </si>
-  <si>
-    <t>propliteal4</t>
-  </si>
-  <si>
-    <t>img/ballard/propliteal4.png</t>
-  </si>
-  <si>
-    <t>propliteal5</t>
-  </si>
-  <si>
-    <t>img/ballard/propliteal5.png</t>
-  </si>
-  <si>
     <t>scarf_sign-1</t>
   </si>
   <si>
@@ -769,18 +721,12 @@
     <t>img/ballard/heel_to_ear4.png</t>
   </si>
   <si>
-    <t>selected(data('ballard_menu1'), 'propliteal')</t>
-  </si>
-  <si>
     <t>selected(data('ballard_menu1'), 'scarf')</t>
   </si>
   <si>
     <t>selected(data('ballard_menu1'), 'heel')</t>
   </si>
   <si>
-    <t>propliteal</t>
-  </si>
-  <si>
     <t>menu menu</t>
   </si>
   <si>
@@ -800,6 +746,217 @@
   </si>
   <si>
     <t>menu medications_menu</t>
+  </si>
+  <si>
+    <t>postureScore</t>
+  </si>
+  <si>
+    <t>Posture Score: {{calculates.postureScore}}</t>
+  </si>
+  <si>
+    <t xml:space="preserve">(function() {
+  switch (data('posture_slider')) { 
+    case('posture0'):
+      return 0;
+    case('posture1'):
+      return 1;
+    case('posture2'):
+      return 2;
+    case('posture3'):
+      return 3;
+   case('posture4'):
+      return 4;  
+  }
+}())
+        </t>
+  </si>
+  <si>
+    <t>squareScore</t>
+  </si>
+  <si>
+    <t>armScore</t>
+  </si>
+  <si>
+    <t>scarfScore</t>
+  </si>
+  <si>
+    <t>heelScore</t>
+  </si>
+  <si>
+    <t>image_slider popliteal_slider</t>
+  </si>
+  <si>
+    <t>popliteal_slider</t>
+  </si>
+  <si>
+    <t>Choose Popliteal Angle</t>
+  </si>
+  <si>
+    <t>selected(data('ballard_menu1'), 'popliteal')</t>
+  </si>
+  <si>
+    <t xml:space="preserve">(function() {
+  switch (data('arm_slider')) { 
+    case('arm_recoil0'):
+      return 0;
+    case('arm_recoil1'):
+      return 1;
+    case('arm_recoil2'):
+      return 2;
+    case('arm_recoil3'):
+      return 3;
+   case('arm_recoil4'):
+      return 4;  
+  }
+}())
+        </t>
+  </si>
+  <si>
+    <t xml:space="preserve">(function() {
+  switch (data('scarf_slider')) { 
+    case('scarf_sign-1'):
+      return -1;
+    case('scarf_sign0'):
+      return 0;
+    case('scarf_sign1'):
+      return 1;
+    case('scarf_sign2'):
+      return 2;
+    case('scarf_sign3'):
+      return 3;
+   case('scarf_sign4'):
+      return 4;  
+  }
+}())
+        </t>
+  </si>
+  <si>
+    <t xml:space="preserve">(function() {
+  switch (data('heel_slider')) { 
+    case('heel_to_ear-1'):
+      return -1;
+    case('heel_to_ear0'):
+      return 0;
+    case('heel_to_ear1'):
+      return 1;
+    case('heel_to_ear2'):
+      return 2;
+    case('heel_to_ear3'):
+      return 3;
+   case('heel_to_ear4'):
+      return 4;  
+  }
+}())
+        </t>
+  </si>
+  <si>
+    <t>Square Window Score: {{calculates.squareScore}}</t>
+  </si>
+  <si>
+    <t>Arm Recoil Score: {{calculates.armScore}}</t>
+  </si>
+  <si>
+    <t>Scarf Sign Score: {{calculates.scarfScore}}</t>
+  </si>
+  <si>
+    <t>Heel to Ear Score: {{calculates.heelScore}}</t>
+  </si>
+  <si>
+    <t xml:space="preserve">(function() {
+  switch (data('square_slider')) { 
+    case('square_window-1'):
+      return -1;
+    case('square_window0'):
+      return 0;
+    case('square_window1'):
+      return 1;
+    case('square_window2'):
+      return 2;
+    case('square_window3'):
+      return 3;
+   case('square_window4'):
+      return 4;  
+  }
+}())
+        </t>
+  </si>
+  <si>
+    <t>img/ballard/popliteal-1.png</t>
+  </si>
+  <si>
+    <t>img/ballard/popliteal0.png</t>
+  </si>
+  <si>
+    <t>img/ballard/popliteal1.png</t>
+  </si>
+  <si>
+    <t>img/ballard/popliteal2.png</t>
+  </si>
+  <si>
+    <t>img/ballard/popliteal3.png</t>
+  </si>
+  <si>
+    <t>img/ballard/popliteal4.png</t>
+  </si>
+  <si>
+    <t>img/ballard/popliteal5.png</t>
+  </si>
+  <si>
+    <t>popliteal-1</t>
+  </si>
+  <si>
+    <t>popliteal0</t>
+  </si>
+  <si>
+    <t>popliteal1</t>
+  </si>
+  <si>
+    <t>popliteal2</t>
+  </si>
+  <si>
+    <t>popliteal3</t>
+  </si>
+  <si>
+    <t>popliteal4</t>
+  </si>
+  <si>
+    <t>popliteal5</t>
+  </si>
+  <si>
+    <t xml:space="preserve">(function() {
+  switch (data('popliteal_slider')) { 
+    case('popliteal-1'):
+      return -1;
+    case('popliteal0'):
+      return 0;
+    case('popliteal1'):
+      return 1;
+    case('popliteal2'):
+      return 2;
+    case('popliteal3'):
+      return 3;
+   case('popliteal4'):
+      return 4;  
+   case('popliteal5'):
+      return 5;  
+  }
+}())
+        </t>
+  </si>
+  <si>
+    <t>totalNMScore</t>
+  </si>
+  <si>
+    <t>calculates.postureScore() + calculates.squareScore() + calculates.armScore() + calculates.poplitealScore() + calculates.scarfScore() + calculates.heelScore()</t>
+  </si>
+  <si>
+    <t>poplitealScore</t>
+  </si>
+  <si>
+    <t>Popiteal Angle Score: {{calculates.poplitealScore}}</t>
+  </si>
+  <si>
+    <t>Total NM Score: {{calculates.totalNMScore}}</t>
   </si>
 </sst>
 </file>
@@ -902,7 +1059,7 @@
       <diagonal/>
     </border>
   </borders>
-  <cellStyleXfs count="154">
+  <cellStyleXfs count="184">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
     <xf numFmtId="0" fontId="3" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
     <xf numFmtId="0" fontId="4" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
@@ -917,6 +1074,36 @@
     <xf numFmtId="0" fontId="5" fillId="2" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
     <xf numFmtId="0" fontId="6" fillId="3" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
     <xf numFmtId="0" fontId="1" fillId="4" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="4" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="4" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="4" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="4" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="4" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="4" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="4" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="4" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="4" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="4" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="4" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="4" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="4" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="4" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="4" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
     <xf numFmtId="0" fontId="3" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
     <xf numFmtId="0" fontId="4" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
     <xf numFmtId="0" fontId="3" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
@@ -1105,7 +1292,7 @@
     </xf>
     <xf numFmtId="0" fontId="6" fillId="3" borderId="0" xfId="12"/>
   </cellXfs>
-  <cellStyles count="154">
+  <cellStyles count="184">
     <cellStyle name="20% - Accent4" xfId="13" builtinId="42"/>
     <cellStyle name="Followed Hyperlink" xfId="2" builtinId="9" hidden="1"/>
     <cellStyle name="Followed Hyperlink" xfId="4" builtinId="9" hidden="1"/>
@@ -1182,6 +1369,21 @@
     <cellStyle name="Followed Hyperlink" xfId="149" builtinId="9" hidden="1"/>
     <cellStyle name="Followed Hyperlink" xfId="151" builtinId="9" hidden="1"/>
     <cellStyle name="Followed Hyperlink" xfId="153" builtinId="9" hidden="1"/>
+    <cellStyle name="Followed Hyperlink" xfId="155" builtinId="9" hidden="1"/>
+    <cellStyle name="Followed Hyperlink" xfId="157" builtinId="9" hidden="1"/>
+    <cellStyle name="Followed Hyperlink" xfId="159" builtinId="9" hidden="1"/>
+    <cellStyle name="Followed Hyperlink" xfId="161" builtinId="9" hidden="1"/>
+    <cellStyle name="Followed Hyperlink" xfId="163" builtinId="9" hidden="1"/>
+    <cellStyle name="Followed Hyperlink" xfId="165" builtinId="9" hidden="1"/>
+    <cellStyle name="Followed Hyperlink" xfId="167" builtinId="9" hidden="1"/>
+    <cellStyle name="Followed Hyperlink" xfId="169" builtinId="9" hidden="1"/>
+    <cellStyle name="Followed Hyperlink" xfId="171" builtinId="9" hidden="1"/>
+    <cellStyle name="Followed Hyperlink" xfId="173" builtinId="9" hidden="1"/>
+    <cellStyle name="Followed Hyperlink" xfId="175" builtinId="9" hidden="1"/>
+    <cellStyle name="Followed Hyperlink" xfId="177" builtinId="9" hidden="1"/>
+    <cellStyle name="Followed Hyperlink" xfId="179" builtinId="9" hidden="1"/>
+    <cellStyle name="Followed Hyperlink" xfId="181" builtinId="9" hidden="1"/>
+    <cellStyle name="Followed Hyperlink" xfId="183" builtinId="9" hidden="1"/>
     <cellStyle name="Good" xfId="11" builtinId="26"/>
     <cellStyle name="Hyperlink" xfId="1" builtinId="8" hidden="1"/>
     <cellStyle name="Hyperlink" xfId="3" builtinId="8" hidden="1"/>
@@ -1258,6 +1460,21 @@
     <cellStyle name="Hyperlink" xfId="148" builtinId="8" hidden="1"/>
     <cellStyle name="Hyperlink" xfId="150" builtinId="8" hidden="1"/>
     <cellStyle name="Hyperlink" xfId="152" builtinId="8" hidden="1"/>
+    <cellStyle name="Hyperlink" xfId="154" builtinId="8" hidden="1"/>
+    <cellStyle name="Hyperlink" xfId="156" builtinId="8" hidden="1"/>
+    <cellStyle name="Hyperlink" xfId="158" builtinId="8" hidden="1"/>
+    <cellStyle name="Hyperlink" xfId="160" builtinId="8" hidden="1"/>
+    <cellStyle name="Hyperlink" xfId="162" builtinId="8" hidden="1"/>
+    <cellStyle name="Hyperlink" xfId="164" builtinId="8" hidden="1"/>
+    <cellStyle name="Hyperlink" xfId="166" builtinId="8" hidden="1"/>
+    <cellStyle name="Hyperlink" xfId="168" builtinId="8" hidden="1"/>
+    <cellStyle name="Hyperlink" xfId="170" builtinId="8" hidden="1"/>
+    <cellStyle name="Hyperlink" xfId="172" builtinId="8" hidden="1"/>
+    <cellStyle name="Hyperlink" xfId="174" builtinId="8" hidden="1"/>
+    <cellStyle name="Hyperlink" xfId="176" builtinId="8" hidden="1"/>
+    <cellStyle name="Hyperlink" xfId="178" builtinId="8" hidden="1"/>
+    <cellStyle name="Hyperlink" xfId="180" builtinId="8" hidden="1"/>
+    <cellStyle name="Hyperlink" xfId="182" builtinId="8" hidden="1"/>
     <cellStyle name="Neutral" xfId="12" builtinId="28"/>
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
   </cellStyles>
@@ -1588,10 +1805,10 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <dimension ref="A1:I60"/>
+  <dimension ref="A1:I69"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A40" zoomScale="150" zoomScaleNormal="150" zoomScalePageLayoutView="150" workbookViewId="0">
-      <selection activeCell="A50" sqref="A50"/>
+    <sheetView tabSelected="1" topLeftCell="A8" zoomScale="150" zoomScaleNormal="150" zoomScalePageLayoutView="150" workbookViewId="0">
+      <selection activeCell="C21" sqref="C21"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultColWidth="11.5" defaultRowHeight="12.75" customHeight="1" x14ac:dyDescent="0"/>
@@ -1637,7 +1854,7 @@
     </row>
     <row r="3" spans="1:7" ht="12">
       <c r="A3" s="3" t="s">
-        <v>252</v>
+        <v>234</v>
       </c>
       <c r="B3" s="4" t="s">
         <v>4</v>
@@ -1696,7 +1913,7 @@
     </row>
     <row r="8" spans="1:7" s="12" customFormat="1" ht="18" customHeight="1">
       <c r="A8" t="s">
-        <v>253</v>
+        <v>235</v>
       </c>
       <c r="B8" t="s">
         <v>7</v>
@@ -1751,270 +1968,224 @@
       </c>
       <c r="E11" s="2"/>
     </row>
-    <row r="12" spans="1:7" ht="12">
-      <c r="A12" t="s">
-        <v>254</v>
-      </c>
-      <c r="B12" t="s">
-        <v>142</v>
-      </c>
-      <c r="C12" t="s">
-        <v>86</v>
-      </c>
+    <row r="12" spans="1:7" ht="18" customHeight="1">
+      <c r="A12" s="7" t="s">
+        <v>17</v>
+      </c>
+      <c r="B12" s="4"/>
+      <c r="C12" s="2"/>
       <c r="D12" s="2" t="s">
         <v>141</v>
       </c>
-    </row>
-    <row r="13" spans="1:7" ht="11" customHeight="1">
+      <c r="E12" s="2"/>
+    </row>
+    <row r="13" spans="1:7" ht="12">
       <c r="A13" t="s">
-        <v>154</v>
+        <v>236</v>
       </c>
       <c r="B13" t="s">
+        <v>142</v>
+      </c>
+      <c r="C13" t="s">
+        <v>86</v>
+      </c>
+    </row>
+    <row r="14" spans="1:7" ht="25" customHeight="1">
+      <c r="A14" t="s">
+        <v>13</v>
+      </c>
+      <c r="C14" t="s">
+        <v>242</v>
+      </c>
+    </row>
+    <row r="15" spans="1:7" ht="25" customHeight="1">
+      <c r="A15" t="s">
+        <v>13</v>
+      </c>
+      <c r="C15" t="s">
+        <v>255</v>
+      </c>
+    </row>
+    <row r="16" spans="1:7" ht="25" customHeight="1">
+      <c r="A16" t="s">
+        <v>13</v>
+      </c>
+      <c r="C16" t="s">
+        <v>256</v>
+      </c>
+    </row>
+    <row r="17" spans="1:9" ht="25" customHeight="1">
+      <c r="A17" t="s">
+        <v>13</v>
+      </c>
+      <c r="C17" t="s">
+        <v>278</v>
+      </c>
+    </row>
+    <row r="18" spans="1:9" ht="25" customHeight="1">
+      <c r="A18" t="s">
+        <v>13</v>
+      </c>
+      <c r="C18" t="s">
+        <v>257</v>
+      </c>
+    </row>
+    <row r="19" spans="1:9" ht="25" customHeight="1">
+      <c r="A19" t="s">
+        <v>13</v>
+      </c>
+      <c r="C19" t="s">
+        <v>258</v>
+      </c>
+    </row>
+    <row r="20" spans="1:9" ht="25" customHeight="1">
+      <c r="A20" t="s">
+        <v>13</v>
+      </c>
+      <c r="C20" t="s">
+        <v>279</v>
+      </c>
+    </row>
+    <row r="21" spans="1:9" ht="25" customHeight="1">
+      <c r="A21" s="11" t="s">
+        <v>27</v>
+      </c>
+    </row>
+    <row r="22" spans="1:9" ht="11" customHeight="1">
+      <c r="A22" t="s">
         <v>155</v>
       </c>
-      <c r="C13" t="s">
+      <c r="B22" t="s">
         <v>156</v>
       </c>
-      <c r="D13" s="2" t="s">
+      <c r="C22" t="s">
         <v>157</v>
       </c>
-    </row>
-    <row r="14" spans="1:7" ht="11" customHeight="1">
-      <c r="A14" t="s">
+      <c r="D22" s="2" t="s">
         <v>158</v>
       </c>
-      <c r="B14" t="s">
+    </row>
+    <row r="23" spans="1:9" ht="11" customHeight="1">
+      <c r="A23" t="s">
         <v>159</v>
       </c>
-      <c r="C14" t="s">
+      <c r="B23" t="s">
         <v>160</v>
       </c>
-      <c r="D14" s="2" t="s">
+      <c r="C23" t="s">
         <v>161</v>
       </c>
-    </row>
-    <row r="15" spans="1:7" ht="11" customHeight="1">
-      <c r="A15" t="s">
-        <v>175</v>
-      </c>
-      <c r="B15" t="s">
+      <c r="D23" s="2" t="s">
+        <v>162</v>
+      </c>
+    </row>
+    <row r="24" spans="1:9" ht="11" customHeight="1">
+      <c r="A24" t="s">
         <v>176</v>
       </c>
-      <c r="C15" t="s">
+      <c r="B24" t="s">
         <v>177</v>
       </c>
-      <c r="D15" s="2" t="s">
+      <c r="C24" t="s">
         <v>178</v>
       </c>
-    </row>
-    <row r="16" spans="1:7" ht="11" customHeight="1">
-      <c r="A16" t="s">
+      <c r="D24" s="2" t="s">
         <v>179</v>
       </c>
-      <c r="B16" t="s">
+    </row>
+    <row r="25" spans="1:9" ht="11" customHeight="1">
+      <c r="A25" t="s">
+        <v>248</v>
+      </c>
+      <c r="B25" t="s">
+        <v>249</v>
+      </c>
+      <c r="C25" t="s">
+        <v>250</v>
+      </c>
+      <c r="D25" s="2" t="s">
+        <v>251</v>
+      </c>
+    </row>
+    <row r="26" spans="1:9" ht="11" customHeight="1">
+      <c r="A26" t="s">
         <v>180</v>
       </c>
-      <c r="C16" t="s">
+      <c r="B26" t="s">
         <v>181</v>
       </c>
-      <c r="D16" s="2" t="s">
-        <v>248</v>
-      </c>
-    </row>
-    <row r="17" spans="1:9" ht="11" customHeight="1">
-      <c r="A17" t="s">
+      <c r="C26" t="s">
         <v>182</v>
       </c>
-      <c r="B17" t="s">
+      <c r="D26" s="2" t="s">
+        <v>232</v>
+      </c>
+    </row>
+    <row r="27" spans="1:9" ht="11" customHeight="1">
+      <c r="A27" t="s">
         <v>183</v>
       </c>
-      <c r="C17" t="s">
+      <c r="B27" t="s">
         <v>184</v>
       </c>
-      <c r="D17" s="2" t="s">
-        <v>249</v>
-      </c>
-    </row>
-    <row r="18" spans="1:9" ht="11" customHeight="1">
-      <c r="A18" t="s">
+      <c r="C27" t="s">
         <v>185</v>
       </c>
-      <c r="B18" t="s">
-        <v>186</v>
-      </c>
-      <c r="C18" t="s">
-        <v>187</v>
-      </c>
-      <c r="D18" s="2" t="s">
-        <v>250</v>
-      </c>
-    </row>
-    <row r="19" spans="1:9" ht="15">
-      <c r="A19" s="15" t="s">
+      <c r="D27" s="2" t="s">
+        <v>233</v>
+      </c>
+    </row>
+    <row r="28" spans="1:9" ht="15">
+      <c r="A28" s="15" t="s">
         <v>77</v>
       </c>
-      <c r="B19" s="15"/>
-      <c r="C19" s="15"/>
-      <c r="D19" s="15"/>
-      <c r="E19" s="15"/>
-      <c r="F19" s="15"/>
-      <c r="G19" s="15"/>
-    </row>
-    <row r="20" spans="1:9" ht="15">
-      <c r="A20" s="16"/>
-      <c r="B20" s="12"/>
-      <c r="C20" s="12"/>
-      <c r="D20" s="12"/>
-      <c r="E20" s="12"/>
-      <c r="F20" s="12"/>
-      <c r="G20" s="12"/>
-    </row>
-    <row r="21" spans="1:9" s="15" customFormat="1" ht="15">
-      <c r="A21" s="13" t="s">
+      <c r="B28" s="15"/>
+      <c r="C28" s="15"/>
+      <c r="D28" s="15"/>
+      <c r="E28" s="15"/>
+      <c r="F28" s="15"/>
+      <c r="G28" s="15"/>
+    </row>
+    <row r="29" spans="1:9" ht="15">
+      <c r="A29" s="16"/>
+      <c r="B29" s="12"/>
+      <c r="C29" s="12"/>
+      <c r="D29" s="12"/>
+      <c r="E29" s="12"/>
+      <c r="F29" s="12"/>
+      <c r="G29" s="12"/>
+    </row>
+    <row r="30" spans="1:9" s="15" customFormat="1" ht="15">
+      <c r="A30" s="13" t="s">
         <v>112</v>
       </c>
-      <c r="B21" s="13"/>
-      <c r="C21" s="13"/>
-      <c r="D21" s="13" t="s">
+      <c r="B30" s="13"/>
+      <c r="C30" s="13"/>
+      <c r="D30" s="13" t="s">
         <v>74</v>
       </c>
-      <c r="E21" s="13"/>
-      <c r="F21" s="13"/>
-      <c r="G21" s="13"/>
-      <c r="H21" s="12"/>
-      <c r="I21" s="12"/>
-    </row>
-    <row r="22" spans="1:9" ht="12">
-      <c r="A22" s="5" t="s">
+      <c r="E30" s="13"/>
+      <c r="F30" s="13"/>
+      <c r="G30" s="13"/>
+      <c r="H30" s="12"/>
+      <c r="I30" s="12"/>
+    </row>
+    <row r="31" spans="1:9" ht="12">
+      <c r="A31" s="5" t="s">
         <v>78</v>
       </c>
-      <c r="B22" s="5"/>
-      <c r="C22" s="5"/>
-      <c r="D22" s="6" t="s">
+      <c r="B31" s="5"/>
+      <c r="C31" s="5"/>
+      <c r="D31" s="6" t="s">
         <v>79</v>
       </c>
-      <c r="E22" s="5"/>
-      <c r="F22" s="5"/>
-      <c r="G22" s="5"/>
-    </row>
-    <row r="23" spans="1:9" ht="15">
-      <c r="A23" s="15" t="s">
-        <v>111</v>
-      </c>
-      <c r="B23" s="15"/>
-      <c r="C23" s="15"/>
-      <c r="D23" s="15"/>
-      <c r="E23" s="15"/>
-      <c r="F23" s="15"/>
-      <c r="G23" s="15"/>
-    </row>
-    <row r="24" spans="1:9" ht="12">
-      <c r="A24" s="12" t="s">
-        <v>255</v>
-      </c>
-      <c r="B24" s="12" t="s">
-        <v>9</v>
-      </c>
-      <c r="C24" s="12" t="s">
-        <v>10</v>
-      </c>
-      <c r="D24" s="12"/>
-      <c r="E24" s="12" t="s">
-        <v>6</v>
-      </c>
-      <c r="F24" s="12"/>
-      <c r="G24" s="12"/>
-    </row>
-    <row r="25" spans="1:9" ht="12">
-      <c r="A25" s="7" t="s">
-        <v>17</v>
-      </c>
-      <c r="B25" s="8"/>
-      <c r="C25" s="8"/>
-      <c r="D25" s="9" t="s">
-        <v>65</v>
-      </c>
-      <c r="E25" s="8"/>
-      <c r="F25" s="10"/>
-      <c r="G25" s="10"/>
-    </row>
-    <row r="26" spans="1:9" ht="12.75" customHeight="1">
-      <c r="A26" s="4" t="s">
-        <v>13</v>
-      </c>
-      <c r="B26" s="2" t="s">
-        <v>80</v>
-      </c>
-      <c r="C26" s="2" t="s">
-        <v>81</v>
-      </c>
-      <c r="D26" s="2"/>
-      <c r="E26" s="4"/>
-    </row>
-    <row r="27" spans="1:9" ht="12.75" customHeight="1">
-      <c r="A27" s="4" t="s">
-        <v>13</v>
-      </c>
-      <c r="B27" s="2" t="s">
-        <v>82</v>
-      </c>
-      <c r="C27" s="2"/>
-      <c r="D27" s="2"/>
-      <c r="E27" s="4"/>
-      <c r="F27" t="s">
-        <v>14</v>
-      </c>
-    </row>
-    <row r="28" spans="1:9" ht="12.75" customHeight="1">
-      <c r="A28" t="s">
-        <v>13</v>
-      </c>
-      <c r="C28" t="s">
-        <v>83</v>
-      </c>
-      <c r="D28" s="13"/>
-    </row>
-    <row r="29" spans="1:9" ht="12.75" customHeight="1">
-      <c r="A29" t="s">
-        <v>13</v>
-      </c>
-      <c r="B29" t="s">
-        <v>84</v>
-      </c>
-      <c r="G29" t="s">
-        <v>85</v>
-      </c>
-    </row>
-    <row r="30" spans="1:9" ht="12">
-      <c r="A30" s="11" t="s">
-        <v>27</v>
-      </c>
-      <c r="B30" s="10"/>
-      <c r="C30" s="10"/>
-      <c r="D30" s="10"/>
-      <c r="E30" s="10"/>
-      <c r="F30" s="10"/>
-      <c r="G30" s="10"/>
-    </row>
-    <row r="31" spans="1:9" ht="24">
-      <c r="A31" s="4" t="s">
-        <v>13</v>
-      </c>
-      <c r="B31" s="4"/>
-      <c r="C31" s="4" t="s">
-        <v>15</v>
-      </c>
-      <c r="D31" s="2" t="s">
-        <v>73</v>
-      </c>
-      <c r="E31" s="4"/>
-      <c r="F31" t="s">
-        <v>16</v>
-      </c>
+      <c r="E31" s="5"/>
+      <c r="F31" s="5"/>
+      <c r="G31" s="5"/>
     </row>
     <row r="32" spans="1:9" ht="15">
       <c r="A32" s="15" t="s">
-        <v>87</v>
+        <v>111</v>
       </c>
       <c r="B32" s="15"/>
       <c r="C32" s="15"/>
@@ -2022,294 +2193,296 @@
       <c r="E32" s="15"/>
       <c r="F32" s="15"/>
       <c r="G32" s="15"/>
-      <c r="H32" s="12"/>
-    </row>
-    <row r="33" spans="1:9" ht="12">
-      <c r="A33" s="12"/>
-      <c r="B33" s="12"/>
-      <c r="C33" s="12"/>
+    </row>
+    <row r="33" spans="1:8" ht="12">
+      <c r="A33" s="12" t="s">
+        <v>237</v>
+      </c>
+      <c r="B33" s="12" t="s">
+        <v>9</v>
+      </c>
+      <c r="C33" s="12" t="s">
+        <v>10</v>
+      </c>
       <c r="D33" s="12"/>
-      <c r="E33" s="12"/>
+      <c r="E33" s="12" t="s">
+        <v>6</v>
+      </c>
       <c r="F33" s="12"/>
       <c r="G33" s="12"/>
-      <c r="H33" s="12"/>
-    </row>
-    <row r="34" spans="1:9" ht="15">
-      <c r="A34" s="14" t="s">
-        <v>118</v>
-      </c>
-      <c r="B34" s="14"/>
-      <c r="C34" s="14"/>
-      <c r="D34" s="13" t="s">
-        <v>119</v>
-      </c>
-      <c r="E34" s="14"/>
-      <c r="F34" s="14"/>
-      <c r="G34" s="14"/>
-      <c r="H34" s="12"/>
-    </row>
-    <row r="35" spans="1:9" ht="12">
-      <c r="A35" s="5" t="s">
-        <v>88</v>
-      </c>
-      <c r="B35" s="5"/>
-      <c r="C35" s="5"/>
-      <c r="D35" s="6" t="s">
-        <v>89</v>
-      </c>
-      <c r="E35" s="5"/>
-      <c r="F35" s="5"/>
-      <c r="G35" s="5"/>
-    </row>
-    <row r="36" spans="1:9" ht="15">
-      <c r="A36" s="15" t="s">
-        <v>120</v>
-      </c>
-      <c r="B36" s="15"/>
-      <c r="C36" s="15"/>
-      <c r="D36" s="15"/>
-      <c r="E36" s="15"/>
-      <c r="F36" s="15"/>
-      <c r="G36" s="15"/>
-    </row>
-    <row r="37" spans="1:9" ht="12">
+    </row>
+    <row r="34" spans="1:8" ht="12">
+      <c r="A34" s="7" t="s">
+        <v>17</v>
+      </c>
+      <c r="B34" s="8"/>
+      <c r="C34" s="8"/>
+      <c r="D34" s="9" t="s">
+        <v>65</v>
+      </c>
+      <c r="E34" s="8"/>
+      <c r="F34" s="10"/>
+      <c r="G34" s="10"/>
+    </row>
+    <row r="35" spans="1:8" ht="12.75" customHeight="1">
+      <c r="A35" s="4" t="s">
+        <v>13</v>
+      </c>
+      <c r="B35" s="2" t="s">
+        <v>80</v>
+      </c>
+      <c r="C35" s="2" t="s">
+        <v>81</v>
+      </c>
+      <c r="D35" s="2"/>
+      <c r="E35" s="4"/>
+    </row>
+    <row r="36" spans="1:8" ht="12.75" customHeight="1">
+      <c r="A36" s="4" t="s">
+        <v>13</v>
+      </c>
+      <c r="B36" s="2" t="s">
+        <v>82</v>
+      </c>
+      <c r="C36" s="2"/>
+      <c r="D36" s="2"/>
+      <c r="E36" s="4"/>
+      <c r="F36" t="s">
+        <v>14</v>
+      </c>
+    </row>
+    <row r="37" spans="1:8" ht="12.75" customHeight="1">
       <c r="A37" t="s">
-        <v>256</v>
-      </c>
-      <c r="B37" t="s">
-        <v>11</v>
+        <v>13</v>
       </c>
       <c r="C37" t="s">
-        <v>12</v>
-      </c>
-      <c r="E37" t="s">
-        <v>6</v>
-      </c>
-      <c r="F37" s="12"/>
-      <c r="G37" s="12"/>
-    </row>
-    <row r="38" spans="1:9" ht="12">
-      <c r="A38" s="4" t="s">
-        <v>17</v>
-      </c>
-      <c r="B38" s="4"/>
-      <c r="C38" s="4"/>
-      <c r="D38" s="4"/>
-      <c r="E38" s="4"/>
-    </row>
-    <row r="39" spans="1:9" ht="12">
-      <c r="A39" s="4" t="s">
-        <v>18</v>
-      </c>
-      <c r="B39" s="4" t="s">
-        <v>19</v>
-      </c>
-      <c r="C39" s="4" t="s">
-        <v>20</v>
-      </c>
-      <c r="D39" s="4"/>
-      <c r="E39" s="4"/>
-    </row>
-    <row r="40" spans="1:9" ht="36">
+        <v>83</v>
+      </c>
+      <c r="D37" s="13"/>
+    </row>
+    <row r="38" spans="1:8" ht="12.75" customHeight="1">
+      <c r="A38" t="s">
+        <v>13</v>
+      </c>
+      <c r="B38" t="s">
+        <v>84</v>
+      </c>
+      <c r="G38" t="s">
+        <v>85</v>
+      </c>
+    </row>
+    <row r="39" spans="1:8" ht="12">
+      <c r="A39" s="11" t="s">
+        <v>27</v>
+      </c>
+      <c r="B39" s="10"/>
+      <c r="C39" s="10"/>
+      <c r="D39" s="10"/>
+      <c r="E39" s="10"/>
+      <c r="F39" s="10"/>
+      <c r="G39" s="10"/>
+    </row>
+    <row r="40" spans="1:8" ht="24">
       <c r="A40" s="4" t="s">
         <v>13</v>
       </c>
       <c r="B40" s="4"/>
       <c r="C40" s="4" t="s">
+        <v>15</v>
+      </c>
+      <c r="D40" s="2" t="s">
+        <v>73</v>
+      </c>
+      <c r="E40" s="4"/>
+      <c r="F40" t="s">
+        <v>16</v>
+      </c>
+    </row>
+    <row r="41" spans="1:8" ht="15">
+      <c r="A41" s="15" t="s">
+        <v>87</v>
+      </c>
+      <c r="B41" s="15"/>
+      <c r="C41" s="15"/>
+      <c r="D41" s="15"/>
+      <c r="E41" s="15"/>
+      <c r="F41" s="15"/>
+      <c r="G41" s="15"/>
+      <c r="H41" s="12"/>
+    </row>
+    <row r="42" spans="1:8" ht="12">
+      <c r="A42" s="12"/>
+      <c r="B42" s="12"/>
+      <c r="C42" s="12"/>
+      <c r="D42" s="12"/>
+      <c r="E42" s="12"/>
+      <c r="F42" s="12"/>
+      <c r="G42" s="12"/>
+      <c r="H42" s="12"/>
+    </row>
+    <row r="43" spans="1:8" ht="15">
+      <c r="A43" s="14" t="s">
+        <v>118</v>
+      </c>
+      <c r="B43" s="14"/>
+      <c r="C43" s="14"/>
+      <c r="D43" s="13" t="s">
+        <v>119</v>
+      </c>
+      <c r="E43" s="14"/>
+      <c r="F43" s="14"/>
+      <c r="G43" s="14"/>
+      <c r="H43" s="12"/>
+    </row>
+    <row r="44" spans="1:8" ht="12">
+      <c r="A44" s="5" t="s">
+        <v>88</v>
+      </c>
+      <c r="B44" s="5"/>
+      <c r="C44" s="5"/>
+      <c r="D44" s="6" t="s">
+        <v>89</v>
+      </c>
+      <c r="E44" s="5"/>
+      <c r="F44" s="5"/>
+      <c r="G44" s="5"/>
+    </row>
+    <row r="45" spans="1:8" ht="15">
+      <c r="A45" s="15" t="s">
+        <v>120</v>
+      </c>
+      <c r="B45" s="15"/>
+      <c r="C45" s="15"/>
+      <c r="D45" s="15"/>
+      <c r="E45" s="15"/>
+      <c r="F45" s="15"/>
+      <c r="G45" s="15"/>
+    </row>
+    <row r="46" spans="1:8" ht="12">
+      <c r="A46" t="s">
+        <v>238</v>
+      </c>
+      <c r="B46" t="s">
+        <v>11</v>
+      </c>
+      <c r="C46" t="s">
+        <v>12</v>
+      </c>
+      <c r="E46" t="s">
+        <v>6</v>
+      </c>
+      <c r="F46" s="12"/>
+      <c r="G46" s="12"/>
+    </row>
+    <row r="47" spans="1:8" ht="12">
+      <c r="A47" s="4" t="s">
+        <v>17</v>
+      </c>
+      <c r="B47" s="4"/>
+      <c r="C47" s="4"/>
+      <c r="D47" s="4"/>
+      <c r="E47" s="4"/>
+    </row>
+    <row r="48" spans="1:8" ht="12">
+      <c r="A48" s="4" t="s">
+        <v>18</v>
+      </c>
+      <c r="B48" s="4" t="s">
+        <v>19</v>
+      </c>
+      <c r="C48" s="4" t="s">
+        <v>20</v>
+      </c>
+      <c r="D48" s="4"/>
+      <c r="E48" s="4"/>
+    </row>
+    <row r="49" spans="1:9" ht="36">
+      <c r="A49" s="4" t="s">
+        <v>13</v>
+      </c>
+      <c r="B49" s="4"/>
+      <c r="C49" s="4" t="s">
         <v>21</v>
       </c>
-      <c r="D40" s="4" t="s">
+      <c r="D49" s="4" t="s">
         <v>22</v>
       </c>
-      <c r="E40" s="4"/>
-    </row>
-    <row r="41" spans="1:9" ht="12">
-      <c r="A41" s="4" t="s">
+      <c r="E49" s="4"/>
+    </row>
+    <row r="50" spans="1:9" ht="12">
+      <c r="A50" s="4" t="s">
         <v>18</v>
       </c>
-      <c r="B41" s="4" t="s">
+      <c r="B50" s="4" t="s">
         <v>23</v>
       </c>
-      <c r="C41" s="4" t="s">
+      <c r="C50" s="4" t="s">
         <v>24</v>
       </c>
-      <c r="D41" s="4"/>
-      <c r="E41" s="4"/>
-    </row>
-    <row r="42" spans="1:9" ht="36">
-      <c r="A42" s="4" t="s">
+      <c r="D50" s="4"/>
+      <c r="E50" s="4"/>
+    </row>
+    <row r="51" spans="1:9" ht="36">
+      <c r="A51" s="4" t="s">
         <v>13</v>
       </c>
-      <c r="B42" s="4"/>
-      <c r="C42" s="4" t="s">
+      <c r="B51" s="4"/>
+      <c r="C51" s="4" t="s">
         <v>25</v>
       </c>
-      <c r="D42" s="4" t="s">
+      <c r="D51" s="4" t="s">
         <v>26</v>
       </c>
-      <c r="E42" s="4"/>
-      <c r="H42" s="12"/>
-    </row>
-    <row r="43" spans="1:9" ht="12.75" customHeight="1">
-      <c r="A43" s="4" t="s">
+      <c r="E51" s="4"/>
+      <c r="H51" s="12"/>
+    </row>
+    <row r="52" spans="1:9" ht="12.75" customHeight="1">
+      <c r="A52" s="4" t="s">
         <v>27</v>
       </c>
-      <c r="B43" s="4"/>
-      <c r="C43" s="4"/>
-      <c r="D43" s="4"/>
-      <c r="E43" s="4"/>
-    </row>
-    <row r="44" spans="1:9" ht="12.75" customHeight="1">
-      <c r="A44" s="15" t="s">
+      <c r="B52" s="4"/>
+      <c r="C52" s="4"/>
+      <c r="D52" s="4"/>
+      <c r="E52" s="4"/>
+    </row>
+    <row r="53" spans="1:9" ht="12.75" customHeight="1">
+      <c r="A53" s="15" t="s">
         <v>90</v>
       </c>
-      <c r="B44" s="15"/>
-      <c r="C44" s="15"/>
-      <c r="D44" s="15"/>
-      <c r="E44" s="15"/>
-      <c r="F44" s="15"/>
-      <c r="G44" s="15"/>
-    </row>
-    <row r="45" spans="1:9" s="12" customFormat="1" ht="12.75" customHeight="1"/>
-    <row r="46" spans="1:9" s="14" customFormat="1" ht="12.75" customHeight="1">
-      <c r="A46" s="13" t="s">
+      <c r="B53" s="15"/>
+      <c r="C53" s="15"/>
+      <c r="D53" s="15"/>
+      <c r="E53" s="15"/>
+      <c r="F53" s="15"/>
+      <c r="G53" s="15"/>
+    </row>
+    <row r="54" spans="1:9" s="12" customFormat="1" ht="12.75" customHeight="1"/>
+    <row r="55" spans="1:9" s="14" customFormat="1" ht="12.75" customHeight="1">
+      <c r="A55" s="13" t="s">
         <v>121</v>
       </c>
-      <c r="D46" s="14" t="s">
+      <c r="D55" s="14" t="s">
         <v>122</v>
       </c>
-      <c r="H46" s="12"/>
-      <c r="I46" s="12"/>
-    </row>
-    <row r="47" spans="1:9" ht="12.75" customHeight="1">
-      <c r="A47" s="13" t="s">
+      <c r="H55" s="12"/>
+      <c r="I55" s="12"/>
+    </row>
+    <row r="56" spans="1:9" ht="12.75" customHeight="1">
+      <c r="A56" s="13" t="s">
         <v>96</v>
       </c>
-      <c r="B47" s="14"/>
-      <c r="C47" s="14"/>
-      <c r="D47" s="14" t="s">
+      <c r="B56" s="14"/>
+      <c r="C56" s="14"/>
+      <c r="D56" s="14" t="s">
         <v>91</v>
       </c>
-      <c r="E47" s="14"/>
-      <c r="F47" s="14"/>
-      <c r="G47" s="14"/>
-    </row>
-    <row r="48" spans="1:9" ht="12.75" customHeight="1">
-      <c r="A48" s="15" t="s">
+      <c r="E56" s="14"/>
+      <c r="F56" s="14"/>
+      <c r="G56" s="14"/>
+    </row>
+    <row r="57" spans="1:9" ht="12.75" customHeight="1">
+      <c r="A57" s="15" t="s">
         <v>138</v>
-      </c>
-      <c r="B48" s="18"/>
-      <c r="C48" s="18"/>
-      <c r="D48" s="18"/>
-      <c r="E48" s="18"/>
-      <c r="F48" s="18"/>
-      <c r="G48" s="18"/>
-    </row>
-    <row r="49" spans="1:7" ht="12.75" customHeight="1">
-      <c r="A49" s="2" t="s">
-        <v>258</v>
-      </c>
-      <c r="B49" s="12" t="s">
-        <v>92</v>
-      </c>
-      <c r="C49" s="12" t="s">
-        <v>93</v>
-      </c>
-      <c r="D49" s="12"/>
-      <c r="E49" s="12" t="s">
-        <v>94</v>
-      </c>
-      <c r="F49" s="12"/>
-      <c r="G49" s="12"/>
-    </row>
-    <row r="50" spans="1:7" ht="12.75" customHeight="1">
-      <c r="A50" s="15" t="s">
-        <v>95</v>
-      </c>
-      <c r="B50" s="18"/>
-      <c r="C50" s="18"/>
-      <c r="D50" s="18"/>
-      <c r="E50" s="18"/>
-      <c r="F50" s="18"/>
-      <c r="G50" s="18"/>
-    </row>
-    <row r="51" spans="1:7" ht="12.75" customHeight="1">
-      <c r="B51" s="12"/>
-      <c r="C51" s="12"/>
-      <c r="D51" s="12"/>
-      <c r="E51" s="12"/>
-      <c r="F51" s="12"/>
-      <c r="G51" s="12"/>
-    </row>
-    <row r="52" spans="1:7" ht="12.75" customHeight="1">
-      <c r="A52" s="13" t="s">
-        <v>129</v>
-      </c>
-      <c r="B52" s="14"/>
-      <c r="C52" s="14"/>
-      <c r="D52" s="14" t="s">
-        <v>131</v>
-      </c>
-      <c r="E52" s="14"/>
-      <c r="F52" s="14"/>
-      <c r="G52" s="14"/>
-    </row>
-    <row r="53" spans="1:7" ht="12.75" customHeight="1">
-      <c r="A53" s="13" t="s">
-        <v>130</v>
-      </c>
-      <c r="B53" s="14"/>
-      <c r="C53" s="14"/>
-      <c r="D53" s="14" t="s">
-        <v>132</v>
-      </c>
-      <c r="E53" s="14"/>
-      <c r="F53" s="14"/>
-      <c r="G53" s="14"/>
-    </row>
-    <row r="54" spans="1:7" ht="12.75" customHeight="1">
-      <c r="A54" s="15" t="s">
-        <v>139</v>
-      </c>
-      <c r="B54" s="18"/>
-      <c r="C54" s="18"/>
-      <c r="D54" s="18"/>
-      <c r="E54" s="18"/>
-      <c r="F54" s="18"/>
-      <c r="G54" s="18"/>
-    </row>
-    <row r="55" spans="1:7" ht="12.75" customHeight="1">
-      <c r="A55" t="s">
-        <v>257</v>
-      </c>
-      <c r="B55" t="s">
-        <v>67</v>
-      </c>
-      <c r="C55" t="s">
-        <v>69</v>
-      </c>
-      <c r="E55" t="s">
-        <v>6</v>
-      </c>
-      <c r="F55" s="12"/>
-      <c r="G55" s="12"/>
-    </row>
-    <row r="56" spans="1:7" ht="12.75" customHeight="1">
-      <c r="A56" s="2" t="s">
-        <v>13</v>
-      </c>
-      <c r="B56" s="12"/>
-      <c r="C56" s="12" t="s">
-        <v>66</v>
-      </c>
-      <c r="D56" s="12"/>
-      <c r="E56" s="12"/>
-      <c r="F56" s="12"/>
-      <c r="G56" s="12"/>
-    </row>
-    <row r="57" spans="1:7" ht="12.75" customHeight="1">
-      <c r="A57" s="15" t="s">
-        <v>133</v>
       </c>
       <c r="B57" s="18"/>
       <c r="C57" s="18"/>
@@ -2318,8 +2491,121 @@
       <c r="F57" s="18"/>
       <c r="G57" s="18"/>
     </row>
-    <row r="60" spans="1:7" ht="12.75" customHeight="1">
-      <c r="A60" s="17" t="s">
+    <row r="58" spans="1:9" ht="12.75" customHeight="1">
+      <c r="A58" s="2" t="s">
+        <v>240</v>
+      </c>
+      <c r="B58" s="12" t="s">
+        <v>92</v>
+      </c>
+      <c r="C58" s="12" t="s">
+        <v>93</v>
+      </c>
+      <c r="D58" s="12"/>
+      <c r="E58" s="12" t="s">
+        <v>94</v>
+      </c>
+      <c r="F58" s="12"/>
+      <c r="G58" s="12"/>
+    </row>
+    <row r="59" spans="1:9" ht="12.75" customHeight="1">
+      <c r="A59" s="15" t="s">
+        <v>95</v>
+      </c>
+      <c r="B59" s="18"/>
+      <c r="C59" s="18"/>
+      <c r="D59" s="18"/>
+      <c r="E59" s="18"/>
+      <c r="F59" s="18"/>
+      <c r="G59" s="18"/>
+    </row>
+    <row r="60" spans="1:9" ht="12.75" customHeight="1">
+      <c r="B60" s="12"/>
+      <c r="C60" s="12"/>
+      <c r="D60" s="12"/>
+      <c r="E60" s="12"/>
+      <c r="F60" s="12"/>
+      <c r="G60" s="12"/>
+    </row>
+    <row r="61" spans="1:9" ht="12.75" customHeight="1">
+      <c r="A61" s="13" t="s">
+        <v>129</v>
+      </c>
+      <c r="B61" s="14"/>
+      <c r="C61" s="14"/>
+      <c r="D61" s="14" t="s">
+        <v>131</v>
+      </c>
+      <c r="E61" s="14"/>
+      <c r="F61" s="14"/>
+      <c r="G61" s="14"/>
+    </row>
+    <row r="62" spans="1:9" ht="12.75" customHeight="1">
+      <c r="A62" s="13" t="s">
+        <v>130</v>
+      </c>
+      <c r="B62" s="14"/>
+      <c r="C62" s="14"/>
+      <c r="D62" s="14" t="s">
+        <v>132</v>
+      </c>
+      <c r="E62" s="14"/>
+      <c r="F62" s="14"/>
+      <c r="G62" s="14"/>
+    </row>
+    <row r="63" spans="1:9" ht="12.75" customHeight="1">
+      <c r="A63" s="15" t="s">
+        <v>139</v>
+      </c>
+      <c r="B63" s="18"/>
+      <c r="C63" s="18"/>
+      <c r="D63" s="18"/>
+      <c r="E63" s="18"/>
+      <c r="F63" s="18"/>
+      <c r="G63" s="18"/>
+    </row>
+    <row r="64" spans="1:9" ht="12.75" customHeight="1">
+      <c r="A64" t="s">
+        <v>239</v>
+      </c>
+      <c r="B64" t="s">
+        <v>67</v>
+      </c>
+      <c r="C64" t="s">
+        <v>69</v>
+      </c>
+      <c r="E64" t="s">
+        <v>6</v>
+      </c>
+      <c r="F64" s="12"/>
+      <c r="G64" s="12"/>
+    </row>
+    <row r="65" spans="1:7" ht="12.75" customHeight="1">
+      <c r="A65" s="2" t="s">
+        <v>13</v>
+      </c>
+      <c r="B65" s="12"/>
+      <c r="C65" s="12" t="s">
+        <v>66</v>
+      </c>
+      <c r="D65" s="12"/>
+      <c r="E65" s="12"/>
+      <c r="F65" s="12"/>
+      <c r="G65" s="12"/>
+    </row>
+    <row r="66" spans="1:7" ht="12.75" customHeight="1">
+      <c r="A66" s="15" t="s">
+        <v>133</v>
+      </c>
+      <c r="B66" s="18"/>
+      <c r="C66" s="18"/>
+      <c r="D66" s="18"/>
+      <c r="E66" s="18"/>
+      <c r="F66" s="18"/>
+      <c r="G66" s="18"/>
+    </row>
+    <row r="69" spans="1:7" ht="12.75" customHeight="1">
+      <c r="A69" s="17" t="s">
         <v>114</v>
       </c>
     </row>
@@ -2336,10 +2622,10 @@
 
 <file path=xl/worksheets/sheet2.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <dimension ref="A1:B5"/>
+  <dimension ref="A1:B12"/>
   <sheetViews>
-    <sheetView workbookViewId="0">
-      <selection activeCell="B65" sqref="B65"/>
+    <sheetView zoomScale="150" zoomScaleNormal="150" zoomScalePageLayoutView="150" workbookViewId="0">
+      <selection activeCell="A10" sqref="A10"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultColWidth="17.1640625" defaultRowHeight="12.75" customHeight="1" x14ac:dyDescent="0"/>
@@ -2387,8 +2673,65 @@
         <v>36</v>
       </c>
     </row>
+    <row r="6" spans="1:2" ht="12" customHeight="1">
+      <c r="A6" t="s">
+        <v>241</v>
+      </c>
+      <c r="B6" t="s">
+        <v>243</v>
+      </c>
+    </row>
+    <row r="7" spans="1:2" ht="12" customHeight="1">
+      <c r="A7" t="s">
+        <v>244</v>
+      </c>
+      <c r="B7" t="s">
+        <v>259</v>
+      </c>
+    </row>
+    <row r="8" spans="1:2" ht="12" customHeight="1">
+      <c r="A8" t="s">
+        <v>245</v>
+      </c>
+      <c r="B8" t="s">
+        <v>252</v>
+      </c>
+    </row>
+    <row r="9" spans="1:2" ht="12" customHeight="1">
+      <c r="A9" t="s">
+        <v>277</v>
+      </c>
+      <c r="B9" t="s">
+        <v>274</v>
+      </c>
+    </row>
+    <row r="10" spans="1:2" ht="12" customHeight="1">
+      <c r="A10" t="s">
+        <v>246</v>
+      </c>
+      <c r="B10" t="s">
+        <v>253</v>
+      </c>
+    </row>
+    <row r="11" spans="1:2" ht="12" customHeight="1">
+      <c r="A11" t="s">
+        <v>247</v>
+      </c>
+      <c r="B11" t="s">
+        <v>254</v>
+      </c>
+    </row>
+    <row r="12" spans="1:2" ht="42" customHeight="1">
+      <c r="A12" t="s">
+        <v>275</v>
+      </c>
+      <c r="B12" t="s">
+        <v>276</v>
+      </c>
+    </row>
   </sheetData>
   <pageMargins left="0.75" right="0.75" top="1" bottom="1" header="0.5" footer="0.5"/>
+  <pageSetup orientation="portrait" horizontalDpi="4294967292" verticalDpi="4294967292"/>
   <extLst>
     <ext xmlns:mx="http://schemas.microsoft.com/office/mac/excel/2008/main" uri="{64002731-A6B0-56B0-2670-7721B7C09600}">
       <mx:PLV Mode="0" OnePage="0" WScale="0"/>
@@ -2401,8 +2744,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:D78"/>
   <sheetViews>
-    <sheetView topLeftCell="A26" workbookViewId="0">
-      <selection activeCell="B35" sqref="B35"/>
+    <sheetView workbookViewId="0">
+      <selection activeCell="A63" sqref="A63"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultColWidth="17.1640625" defaultRowHeight="12.75" customHeight="1" x14ac:dyDescent="0"/>
@@ -2675,7 +3018,7 @@
         <v>143</v>
       </c>
       <c r="C32" t="s">
-        <v>148</v>
+        <v>149</v>
       </c>
     </row>
     <row r="33" spans="1:4" ht="12.75" customHeight="1">
@@ -2686,7 +3029,7 @@
         <v>144</v>
       </c>
       <c r="C33" t="s">
-        <v>149</v>
+        <v>150</v>
       </c>
     </row>
     <row r="34" spans="1:4" ht="12.75" customHeight="1">
@@ -2697,7 +3040,7 @@
         <v>145</v>
       </c>
       <c r="C34" t="s">
-        <v>150</v>
+        <v>151</v>
       </c>
     </row>
     <row r="35" spans="1:4" ht="12.75" customHeight="1">
@@ -2705,10 +3048,10 @@
         <v>142</v>
       </c>
       <c r="B35" t="s">
-        <v>251</v>
+        <v>146</v>
       </c>
       <c r="C35" t="s">
-        <v>151</v>
+        <v>152</v>
       </c>
     </row>
     <row r="36" spans="1:4" ht="12.75" customHeight="1">
@@ -2716,10 +3059,10 @@
         <v>142</v>
       </c>
       <c r="B36" t="s">
-        <v>146</v>
+        <v>147</v>
       </c>
       <c r="C36" t="s">
-        <v>152</v>
+        <v>153</v>
       </c>
     </row>
     <row r="37" spans="1:4" ht="12.75" customHeight="1">
@@ -2727,399 +3070,399 @@
         <v>142</v>
       </c>
       <c r="B37" t="s">
-        <v>147</v>
+        <v>148</v>
       </c>
       <c r="C37" t="s">
-        <v>153</v>
+        <v>154</v>
       </c>
     </row>
     <row r="39" spans="1:4" ht="12.75" customHeight="1">
       <c r="A39" t="s">
-        <v>155</v>
+        <v>156</v>
       </c>
       <c r="B39" t="s">
-        <v>162</v>
+        <v>163</v>
       </c>
       <c r="D39" t="s">
-        <v>163</v>
+        <v>164</v>
       </c>
     </row>
     <row r="40" spans="1:4" ht="12.75" customHeight="1">
       <c r="A40" t="s">
-        <v>155</v>
+        <v>156</v>
       </c>
       <c r="B40" t="s">
-        <v>164</v>
+        <v>165</v>
       </c>
       <c r="D40" t="s">
-        <v>168</v>
+        <v>169</v>
       </c>
     </row>
     <row r="41" spans="1:4" ht="12.75" customHeight="1">
       <c r="A41" t="s">
-        <v>155</v>
+        <v>156</v>
       </c>
       <c r="B41" t="s">
-        <v>165</v>
+        <v>166</v>
       </c>
       <c r="D41" t="s">
-        <v>169</v>
+        <v>170</v>
       </c>
     </row>
     <row r="42" spans="1:4" ht="12.75" customHeight="1">
       <c r="A42" t="s">
-        <v>155</v>
+        <v>156</v>
       </c>
       <c r="B42" t="s">
-        <v>166</v>
+        <v>167</v>
       </c>
       <c r="D42" t="s">
-        <v>170</v>
+        <v>171</v>
       </c>
     </row>
     <row r="43" spans="1:4" ht="12.75" customHeight="1">
       <c r="A43" t="s">
-        <v>155</v>
+        <v>156</v>
       </c>
       <c r="B43" t="s">
-        <v>167</v>
+        <v>168</v>
       </c>
       <c r="D43" t="s">
-        <v>171</v>
+        <v>172</v>
       </c>
     </row>
     <row r="45" spans="1:4" ht="12.75" customHeight="1">
       <c r="A45" t="s">
-        <v>159</v>
+        <v>160</v>
       </c>
       <c r="B45" t="s">
-        <v>198</v>
+        <v>196</v>
       </c>
       <c r="D45" t="s">
-        <v>199</v>
+        <v>197</v>
       </c>
     </row>
     <row r="46" spans="1:4" s="2" customFormat="1" ht="12.75" customHeight="1">
       <c r="A46" t="s">
-        <v>159</v>
+        <v>160</v>
       </c>
       <c r="B46" t="s">
-        <v>188</v>
+        <v>186</v>
       </c>
       <c r="D46" t="s">
-        <v>189</v>
+        <v>187</v>
       </c>
     </row>
     <row r="47" spans="1:4" ht="12.75" customHeight="1">
       <c r="A47" t="s">
-        <v>159</v>
+        <v>160</v>
       </c>
       <c r="B47" t="s">
-        <v>190</v>
+        <v>188</v>
       </c>
       <c r="D47" t="s">
-        <v>191</v>
+        <v>189</v>
       </c>
     </row>
     <row r="48" spans="1:4" ht="12.75" customHeight="1">
       <c r="A48" t="s">
-        <v>159</v>
+        <v>160</v>
       </c>
       <c r="B48" t="s">
-        <v>192</v>
+        <v>190</v>
       </c>
       <c r="D48" t="s">
-        <v>193</v>
+        <v>191</v>
       </c>
     </row>
     <row r="49" spans="1:4" ht="12.75" customHeight="1">
       <c r="A49" t="s">
-        <v>159</v>
+        <v>160</v>
       </c>
       <c r="B49" t="s">
-        <v>194</v>
+        <v>192</v>
       </c>
       <c r="D49" t="s">
-        <v>195</v>
+        <v>193</v>
       </c>
     </row>
     <row r="50" spans="1:4" ht="12.75" customHeight="1">
       <c r="A50" t="s">
-        <v>159</v>
+        <v>160</v>
       </c>
       <c r="B50" t="s">
-        <v>196</v>
+        <v>194</v>
       </c>
       <c r="D50" t="s">
-        <v>197</v>
+        <v>195</v>
       </c>
     </row>
     <row r="52" spans="1:4" ht="12.75" customHeight="1">
       <c r="A52" t="s">
-        <v>176</v>
+        <v>177</v>
       </c>
       <c r="B52" t="s">
-        <v>200</v>
+        <v>198</v>
       </c>
       <c r="C52" s="2"/>
       <c r="D52" t="s">
-        <v>201</v>
+        <v>199</v>
       </c>
     </row>
     <row r="53" spans="1:4" ht="12.75" customHeight="1">
       <c r="A53" t="s">
-        <v>176</v>
+        <v>177</v>
       </c>
       <c r="B53" t="s">
-        <v>202</v>
+        <v>200</v>
       </c>
       <c r="D53" t="s">
-        <v>203</v>
+        <v>201</v>
       </c>
     </row>
     <row r="54" spans="1:4" ht="12.75" customHeight="1">
       <c r="A54" t="s">
-        <v>176</v>
+        <v>177</v>
       </c>
       <c r="B54" t="s">
-        <v>204</v>
+        <v>202</v>
       </c>
       <c r="D54" t="s">
-        <v>205</v>
+        <v>203</v>
       </c>
     </row>
     <row r="55" spans="1:4" ht="12.75" customHeight="1">
       <c r="A55" t="s">
-        <v>176</v>
+        <v>177</v>
       </c>
       <c r="B55" t="s">
-        <v>206</v>
+        <v>204</v>
       </c>
       <c r="D55" t="s">
-        <v>207</v>
+        <v>205</v>
       </c>
     </row>
     <row r="56" spans="1:4" ht="12.75" customHeight="1">
       <c r="A56" t="s">
-        <v>176</v>
+        <v>177</v>
       </c>
       <c r="B56" t="s">
-        <v>208</v>
+        <v>206</v>
       </c>
       <c r="D56" t="s">
-        <v>209</v>
+        <v>207</v>
       </c>
     </row>
     <row r="58" spans="1:4" ht="12.75" customHeight="1">
       <c r="A58" t="s">
-        <v>180</v>
+        <v>249</v>
       </c>
       <c r="B58" t="s">
-        <v>210</v>
+        <v>267</v>
       </c>
       <c r="D58" t="s">
-        <v>211</v>
+        <v>260</v>
       </c>
     </row>
     <row r="59" spans="1:4" ht="12.75" customHeight="1">
       <c r="A59" t="s">
-        <v>180</v>
+        <v>249</v>
       </c>
       <c r="B59" t="s">
-        <v>212</v>
+        <v>268</v>
       </c>
       <c r="C59" s="2"/>
       <c r="D59" t="s">
-        <v>213</v>
+        <v>261</v>
       </c>
     </row>
     <row r="60" spans="1:4" ht="12.75" customHeight="1">
       <c r="A60" t="s">
-        <v>180</v>
+        <v>249</v>
       </c>
       <c r="B60" t="s">
-        <v>214</v>
+        <v>269</v>
       </c>
       <c r="D60" t="s">
-        <v>215</v>
+        <v>262</v>
       </c>
     </row>
     <row r="61" spans="1:4" ht="12.75" customHeight="1">
       <c r="A61" t="s">
-        <v>180</v>
+        <v>249</v>
       </c>
       <c r="B61" t="s">
-        <v>216</v>
+        <v>270</v>
       </c>
       <c r="D61" t="s">
-        <v>217</v>
+        <v>263</v>
       </c>
     </row>
     <row r="62" spans="1:4" ht="12.75" customHeight="1">
       <c r="A62" t="s">
-        <v>180</v>
+        <v>249</v>
       </c>
       <c r="B62" t="s">
-        <v>218</v>
+        <v>271</v>
       </c>
       <c r="D62" t="s">
-        <v>219</v>
+        <v>264</v>
       </c>
     </row>
     <row r="63" spans="1:4" ht="12.75" customHeight="1">
       <c r="A63" t="s">
-        <v>180</v>
+        <v>249</v>
       </c>
       <c r="B63" t="s">
-        <v>220</v>
+        <v>272</v>
       </c>
       <c r="D63" t="s">
-        <v>221</v>
+        <v>265</v>
       </c>
     </row>
     <row r="64" spans="1:4" ht="12.75" customHeight="1">
       <c r="A64" t="s">
-        <v>180</v>
+        <v>249</v>
       </c>
       <c r="B64" t="s">
-        <v>222</v>
+        <v>273</v>
       </c>
       <c r="D64" t="s">
-        <v>223</v>
+        <v>266</v>
       </c>
     </row>
     <row r="66" spans="1:4" ht="12.75" customHeight="1">
       <c r="A66" t="s">
-        <v>183</v>
+        <v>181</v>
       </c>
       <c r="B66" t="s">
-        <v>224</v>
+        <v>208</v>
       </c>
       <c r="D66" t="s">
-        <v>225</v>
+        <v>209</v>
       </c>
     </row>
     <row r="67" spans="1:4" ht="12.75" customHeight="1">
       <c r="A67" t="s">
-        <v>183</v>
+        <v>181</v>
       </c>
       <c r="B67" t="s">
-        <v>226</v>
+        <v>210</v>
       </c>
       <c r="C67" s="2"/>
       <c r="D67" t="s">
-        <v>227</v>
+        <v>211</v>
       </c>
     </row>
     <row r="68" spans="1:4" ht="12.75" customHeight="1">
       <c r="A68" t="s">
-        <v>183</v>
+        <v>181</v>
       </c>
       <c r="B68" t="s">
-        <v>228</v>
+        <v>212</v>
       </c>
       <c r="D68" t="s">
-        <v>229</v>
+        <v>213</v>
       </c>
     </row>
     <row r="69" spans="1:4" ht="12.75" customHeight="1">
       <c r="A69" t="s">
-        <v>183</v>
+        <v>181</v>
       </c>
       <c r="B69" t="s">
-        <v>230</v>
+        <v>214</v>
       </c>
       <c r="D69" t="s">
-        <v>231</v>
+        <v>215</v>
       </c>
     </row>
     <row r="70" spans="1:4" ht="12.75" customHeight="1">
       <c r="A70" t="s">
-        <v>183</v>
+        <v>181</v>
       </c>
       <c r="B70" t="s">
-        <v>232</v>
+        <v>216</v>
       </c>
       <c r="D70" t="s">
-        <v>233</v>
+        <v>217</v>
       </c>
     </row>
     <row r="71" spans="1:4" ht="12.75" customHeight="1">
       <c r="A71" t="s">
-        <v>183</v>
+        <v>181</v>
       </c>
       <c r="B71" t="s">
-        <v>234</v>
+        <v>218</v>
       </c>
       <c r="D71" t="s">
-        <v>235</v>
+        <v>219</v>
       </c>
     </row>
     <row r="73" spans="1:4" ht="12.75" customHeight="1">
       <c r="A73" t="s">
-        <v>186</v>
+        <v>184</v>
       </c>
       <c r="B73" t="s">
-        <v>236</v>
+        <v>220</v>
       </c>
       <c r="D73" t="s">
-        <v>237</v>
+        <v>221</v>
       </c>
     </row>
     <row r="74" spans="1:4" ht="12.75" customHeight="1">
       <c r="A74" t="s">
-        <v>186</v>
+        <v>184</v>
       </c>
       <c r="B74" t="s">
-        <v>238</v>
+        <v>222</v>
       </c>
       <c r="C74" s="2"/>
       <c r="D74" t="s">
-        <v>239</v>
+        <v>223</v>
       </c>
     </row>
     <row r="75" spans="1:4" ht="12.75" customHeight="1">
       <c r="A75" t="s">
-        <v>186</v>
+        <v>184</v>
       </c>
       <c r="B75" t="s">
-        <v>240</v>
+        <v>224</v>
       </c>
       <c r="D75" t="s">
-        <v>241</v>
+        <v>225</v>
       </c>
     </row>
     <row r="76" spans="1:4" ht="12.75" customHeight="1">
       <c r="A76" t="s">
-        <v>186</v>
+        <v>184</v>
       </c>
       <c r="B76" t="s">
-        <v>242</v>
+        <v>226</v>
       </c>
       <c r="D76" t="s">
-        <v>243</v>
+        <v>227</v>
       </c>
     </row>
     <row r="77" spans="1:4" ht="12.75" customHeight="1">
       <c r="A77" t="s">
-        <v>186</v>
+        <v>184</v>
       </c>
       <c r="B77" t="s">
-        <v>244</v>
+        <v>228</v>
       </c>
       <c r="D77" t="s">
-        <v>245</v>
+        <v>229</v>
       </c>
     </row>
     <row r="78" spans="1:4" ht="12.75" customHeight="1">
       <c r="A78" t="s">
-        <v>186</v>
+        <v>184</v>
       </c>
       <c r="B78" t="s">
-        <v>246</v>
+        <v>230</v>
       </c>
       <c r="D78" t="s">
-        <v>247</v>
+        <v>231</v>
       </c>
     </row>
   </sheetData>
@@ -3190,15 +3533,15 @@
         <v>1</v>
       </c>
       <c r="B1" t="s">
-        <v>172</v>
+        <v>173</v>
       </c>
     </row>
     <row r="2" spans="1:2">
       <c r="A2" t="s">
-        <v>173</v>
+        <v>174</v>
       </c>
       <c r="B2" t="s">
-        <v>174</v>
+        <v>175</v>
       </c>
     </row>
     <row r="3" spans="1:2">
@@ -3206,7 +3549,7 @@
         <v>4</v>
       </c>
       <c r="B3" t="s">
-        <v>174</v>
+        <v>175</v>
       </c>
     </row>
   </sheetData>

</xml_diff>

<commit_message>
Finished physical ballard exam
</commit_message>
<xml_diff>
--- a/opendatakit.collect2/form-files/neonatal/neonatal.xlsx
+++ b/opendatakit.collect2/form-files/neonatal/neonatal.xlsx
@@ -4,7 +4,7 @@
   <fileVersion appName="xl" lastEdited="5" lowestEdited="5" rupBuild="20910"/>
   <workbookPr autoCompressPictures="0"/>
   <bookViews>
-    <workbookView xWindow="0" yWindow="0" windowWidth="28800" windowHeight="17480" tabRatio="500"/>
+    <workbookView xWindow="0" yWindow="0" windowWidth="23900" windowHeight="17400" tabRatio="500" activeTab="2"/>
   </bookViews>
   <sheets>
     <sheet name="survey" sheetId="1" r:id="rId1"/>
@@ -23,7 +23,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="380" uniqueCount="280">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="589" uniqueCount="431">
   <si>
     <t>type</t>
   </si>
@@ -250,12 +250,6 @@
     <t>selected(data('menu'),'procedures')</t>
   </si>
   <si>
-    <t>goto diagnostics_end</t>
-  </si>
-  <si>
-    <t>not(selected(data('menu'), 'diagnostics'))</t>
-  </si>
-  <si>
     <t>label diagnostics_end</t>
   </si>
   <si>
@@ -371,12 +365,6 @@
   </si>
   <si>
     <t>label diagnostics_begin</t>
-  </si>
-  <si>
-    <t>goto diagnostics_begin</t>
-  </si>
-  <si>
-    <t>selected(data('menu'),'diagnostics')</t>
   </si>
   <si>
     <t>goto calculators_begin</t>
@@ -957,6 +945,579 @@
   </si>
   <si>
     <t>Total NM Score: {{calculates.totalNMScore}}</t>
+  </si>
+  <si>
+    <t>menu ballard_menu0</t>
+  </si>
+  <si>
+    <t>ballard_menu0</t>
+  </si>
+  <si>
+    <t>Ballard Exam - Neuromuscular</t>
+  </si>
+  <si>
+    <t>selected(data('ballard_menu0'), 'neuromuscular')</t>
+  </si>
+  <si>
+    <t>menu ballard_menu2</t>
+  </si>
+  <si>
+    <t>ballard_menu2</t>
+  </si>
+  <si>
+    <t>Ballard Exam - Physical</t>
+  </si>
+  <si>
+    <t>selected(data('ballard_menu0'), 'physical')</t>
+  </si>
+  <si>
+    <t>neuromuscular</t>
+  </si>
+  <si>
+    <t>Neuromuscular</t>
+  </si>
+  <si>
+    <t>physical</t>
+  </si>
+  <si>
+    <t>Physical</t>
+  </si>
+  <si>
+    <t>skin</t>
+  </si>
+  <si>
+    <t>Choose Skin Score</t>
+  </si>
+  <si>
+    <t>selected(data('ballard_menu2'), 'skin')</t>
+  </si>
+  <si>
+    <t>lanugo</t>
+  </si>
+  <si>
+    <t>selected(data('ballard_menu2'), 'lanugo')</t>
+  </si>
+  <si>
+    <t>selected(data('ballard_menu2'), 'plantar')</t>
+  </si>
+  <si>
+    <t>plantar</t>
+  </si>
+  <si>
+    <t>breast</t>
+  </si>
+  <si>
+    <t>selected(data('ballard_menu2'), 'breast')</t>
+  </si>
+  <si>
+    <t>eye_ear</t>
+  </si>
+  <si>
+    <t>selected(data('ballard_menu2'), 'eye_ear')</t>
+  </si>
+  <si>
+    <t>genitals</t>
+  </si>
+  <si>
+    <t>selected(data('ballard_menu2'), 'genitals')</t>
+  </si>
+  <si>
+    <t>Choose Lanugo Score</t>
+  </si>
+  <si>
+    <t>Choose Breast Score</t>
+  </si>
+  <si>
+    <t>Choose Eye/Ear Score</t>
+  </si>
+  <si>
+    <t>Choose Plantar Surface Score</t>
+  </si>
+  <si>
+    <t>Choose Genitals Score</t>
+  </si>
+  <si>
+    <t>Skin</t>
+  </si>
+  <si>
+    <t>Lanugo</t>
+  </si>
+  <si>
+    <t>Plantar Surface</t>
+  </si>
+  <si>
+    <t>Eye/Ear</t>
+  </si>
+  <si>
+    <t>Genitals</t>
+  </si>
+  <si>
+    <t>skin_menu</t>
+  </si>
+  <si>
+    <t>lanugo_menu</t>
+  </si>
+  <si>
+    <t>plantar_menu</t>
+  </si>
+  <si>
+    <t>breast_menu</t>
+  </si>
+  <si>
+    <t>eye_ear_menu</t>
+  </si>
+  <si>
+    <t>genitals_menu</t>
+  </si>
+  <si>
+    <t>skin-1</t>
+  </si>
+  <si>
+    <t>skin0</t>
+  </si>
+  <si>
+    <t>skin1</t>
+  </si>
+  <si>
+    <t>skin2</t>
+  </si>
+  <si>
+    <t>skin3</t>
+  </si>
+  <si>
+    <t>skin4</t>
+  </si>
+  <si>
+    <t>skin5</t>
+  </si>
+  <si>
+    <t>sticky, friable, transparent</t>
+  </si>
+  <si>
+    <t>gelatinour, red, translucent</t>
+  </si>
+  <si>
+    <t>smooth, pink, visible veins</t>
+  </si>
+  <si>
+    <t>superficial peeling &amp;/or rash, few veins</t>
+  </si>
+  <si>
+    <t>cracking, pale areas, rare veins</t>
+  </si>
+  <si>
+    <t>parchment, deep cracking, no vessels</t>
+  </si>
+  <si>
+    <t>leathery, cracked, wrinkled</t>
+  </si>
+  <si>
+    <t>select_one skin_menu</t>
+  </si>
+  <si>
+    <t>select_one lanugo_menu</t>
+  </si>
+  <si>
+    <t>select_one plantar_menu</t>
+  </si>
+  <si>
+    <t>select_one breast_menu</t>
+  </si>
+  <si>
+    <t>select_one eye_ear_menu</t>
+  </si>
+  <si>
+    <t>select_one genitals_menu</t>
+  </si>
+  <si>
+    <t>lanugo-1</t>
+  </si>
+  <si>
+    <t>lanugo0</t>
+  </si>
+  <si>
+    <t>lanugo1</t>
+  </si>
+  <si>
+    <t>lanugo2</t>
+  </si>
+  <si>
+    <t>lanugo3</t>
+  </si>
+  <si>
+    <t>lanugo4</t>
+  </si>
+  <si>
+    <t>none</t>
+  </si>
+  <si>
+    <t>sparse</t>
+  </si>
+  <si>
+    <t>abundant</t>
+  </si>
+  <si>
+    <t>thinning</t>
+  </si>
+  <si>
+    <t>bald areas</t>
+  </si>
+  <si>
+    <t>mostly bald</t>
+  </si>
+  <si>
+    <t>plantar-1</t>
+  </si>
+  <si>
+    <t>plantar0</t>
+  </si>
+  <si>
+    <t>plantar1</t>
+  </si>
+  <si>
+    <t>plantar2</t>
+  </si>
+  <si>
+    <t>plantar3</t>
+  </si>
+  <si>
+    <t>plantar4</t>
+  </si>
+  <si>
+    <t>plantar-2</t>
+  </si>
+  <si>
+    <t>heel-toe &lt; 40 mm</t>
+  </si>
+  <si>
+    <t>heel-toe 40-50 mm</t>
+  </si>
+  <si>
+    <t>&gt; 50 mm, no crease</t>
+  </si>
+  <si>
+    <t>faint red marks</t>
+  </si>
+  <si>
+    <t>anterior transverse crease only</t>
+  </si>
+  <si>
+    <t>creases ant. 2/3</t>
+  </si>
+  <si>
+    <t>creases over entire sole</t>
+  </si>
+  <si>
+    <t>breast-1</t>
+  </si>
+  <si>
+    <t>breast0</t>
+  </si>
+  <si>
+    <t>breast1</t>
+  </si>
+  <si>
+    <t>breast2</t>
+  </si>
+  <si>
+    <t>breast3</t>
+  </si>
+  <si>
+    <t>breast4</t>
+  </si>
+  <si>
+    <t>imperceptible</t>
+  </si>
+  <si>
+    <t>barely perceptible</t>
+  </si>
+  <si>
+    <t>flat areola, no bud</t>
+  </si>
+  <si>
+    <t>stippled areola, 1-2 mm bud</t>
+  </si>
+  <si>
+    <t>raised areola, 3-4 mm bud</t>
+  </si>
+  <si>
+    <t>full areola, 5-10 mm bud</t>
+  </si>
+  <si>
+    <t>eye_ear-1</t>
+  </si>
+  <si>
+    <t>eye_ear0</t>
+  </si>
+  <si>
+    <t>eye_ear2</t>
+  </si>
+  <si>
+    <t>eye_ear1</t>
+  </si>
+  <si>
+    <t>eye_ear3</t>
+  </si>
+  <si>
+    <t>eye_ear4</t>
+  </si>
+  <si>
+    <t>eye_ear-2</t>
+  </si>
+  <si>
+    <t>lids fused tightly</t>
+  </si>
+  <si>
+    <t>lids fused loosely</t>
+  </si>
+  <si>
+    <t>lids open, pinna flat, stays folded</t>
+  </si>
+  <si>
+    <t>sl. curved pinna, soft, slow recoil</t>
+  </si>
+  <si>
+    <t>well-curved pinna, soft but ready recoil</t>
+  </si>
+  <si>
+    <t>formed &amp; firm, instant recoil</t>
+  </si>
+  <si>
+    <t>thick cartilage, ear stiff</t>
+  </si>
+  <si>
+    <t>genitals-1</t>
+  </si>
+  <si>
+    <t>genitals0</t>
+  </si>
+  <si>
+    <t>genitals1</t>
+  </si>
+  <si>
+    <t>genitals2</t>
+  </si>
+  <si>
+    <t>genitals3</t>
+  </si>
+  <si>
+    <t>genitals4</t>
+  </si>
+  <si>
+    <t>male: scrotum flat, smooth
+female: clitoris prominent &amp; labia flat</t>
+  </si>
+  <si>
+    <t>male: scrotum empty, faint rugae
+female: prominent clitoris &amp; small labia minora</t>
+  </si>
+  <si>
+    <t>male: testes in upper canal rare rugae
+female: prominent clitoris &amp; enlarging minor</t>
+  </si>
+  <si>
+    <t>male: testes descending, few rugae
+female: majora &amp; minora equally prominent</t>
+  </si>
+  <si>
+    <t>male: testes down, good rugae
+female: majora large, minora small</t>
+  </si>
+  <si>
+    <t>male: testes pendulous, deep rugae
+female: majora cover clitoris &amp; minora</t>
+  </si>
+  <si>
+    <t>Breast</t>
+  </si>
+  <si>
+    <t>Final Score</t>
+  </si>
+  <si>
+    <t>&lt;h2&gt;Physical Score&lt;/h2&gt;</t>
+  </si>
+  <si>
+    <t>&lt;h2&gt;Neuromuscular Score&lt;/h2&gt;</t>
+  </si>
+  <si>
+    <t>Skin Score: {{calculates.skinScore}}</t>
+  </si>
+  <si>
+    <t>Lanugo Score: {{calculates.lanugoScore}}</t>
+  </si>
+  <si>
+    <t>Plantar Surface Score: {{calculates.surfaceScore}}</t>
+  </si>
+  <si>
+    <t>Breast Score: {{calculates.breastScore}}</t>
+  </si>
+  <si>
+    <t>Eye/Ear Score: {{calculates.earEyeScore}}</t>
+  </si>
+  <si>
+    <t>Genitals Score: {{calculates.genitalsScore}}</t>
+  </si>
+  <si>
+    <t>Total Physical Score: {{calculates.totalPhysicalScore}}</t>
+  </si>
+  <si>
+    <t>skinScore</t>
+  </si>
+  <si>
+    <t>lanugoScore</t>
+  </si>
+  <si>
+    <t>plantarScore</t>
+  </si>
+  <si>
+    <t>breastScore</t>
+  </si>
+  <si>
+    <t>earEyeScore</t>
+  </si>
+  <si>
+    <t>genitalsScore</t>
+  </si>
+  <si>
+    <t>totalPhysicalScore</t>
+  </si>
+  <si>
+    <t>calculates.skinScore() + calculates.lanugoScore() + calculates.plantarScore() + calculates.breastScore() + calculates.earEyeScore() + calculates.genitalsScore()</t>
+  </si>
+  <si>
+    <t xml:space="preserve">(function() {
+  switch (data('skin_menu')) { 
+    case('skin-1'):
+      return -1;
+    case('skin0'):
+      return 0;
+    case('skin1'):
+      return 1;
+    case('skin2'):
+      return 2;
+    case('skin3'):
+      return 3;
+   case('skin4'):
+      return 4;  
+   case('skin5'):
+      return 5;  
+  }
+}())
+        </t>
+  </si>
+  <si>
+    <t xml:space="preserve">(function() {
+  switch (data('lanugo_menu')) { 
+    case('lanugo-1'):
+      return -1;
+    case('lanugo0'):
+      return 0;
+    case('lanugo1'):
+      return 1;
+    case('lanugo2'):
+      return 2;
+    case('lanugo3'):
+      return 3;
+   case('lanugo4'):
+      return 4;  
+  }
+}())
+        </t>
+  </si>
+  <si>
+    <t xml:space="preserve">(function() {
+  switch (data('plantar_menu')) { 
+    case('plantar-2'):
+      return -2;
+    case('plantar-1'):
+      return -1;
+    case('plantar0'):
+      return 0;
+    case('plantar1'):
+      return 1;
+    case('plantar2'):
+      return 2;
+    case('plantar3'):
+      return 3;
+   case('plantar4'):
+      return 4;  
+  }
+}())
+        </t>
+  </si>
+  <si>
+    <t xml:space="preserve">(function() {
+  switch (data('breast_menu')) { 
+    case('breast-1'):
+      return -1;
+    case('breast0'):
+      return 0;
+    case('breast1'):
+      return 1;
+    case('breast2'):
+      return 2;
+    case('breast3'):
+      return 3;
+   case('breast4'):
+      return 4;  
+  }
+}())
+        </t>
+  </si>
+  <si>
+    <t xml:space="preserve">(function() {
+  switch (data('ear_eye_menu')) { 
+   case('ear_eye-2'):
+      return -2;  
+    case('ear_eye-1'):
+      return -1;
+    case('ear_eye0'):
+      return 0;
+    case('ear_eye1'):
+      return 1;
+    case('ear_eye2'):
+      return 2;
+    case('ear_eye3'):
+      return 3;
+   case('ear_eye4'):
+      return 4;  
+  }
+}())
+        </t>
+  </si>
+  <si>
+    <t xml:space="preserve">(function() {
+  switch (data('genitals_menu')) { 
+    case('genitals-1'):
+      return -1;
+    case('genitals0'):
+      return 0;
+    case('genitals1'):
+      return 1;
+    case('genitals2'):
+      return 2;
+    case('genitals3'):
+      return 3;
+   case('genitals4'):
+      return 4;  
+  }
+}())
+        </t>
+  </si>
+  <si>
+    <t>final_ballard_score</t>
+  </si>
+  <si>
+    <t>selected(data('ballard_menu0'), 'final_ballard_score')</t>
+  </si>
+  <si>
+    <t>&lt;h2&gt;Total Score {{calculates.totalBallardScore}}&lt;/h2&gt;</t>
+  </si>
+  <si>
+    <t>totalBallardScore</t>
+  </si>
+  <si>
+    <t>calculates.totalNMScore() + calculates.totalPhysicalScore()</t>
   </si>
 </sst>
 </file>
@@ -1059,7 +1620,7 @@
       <diagonal/>
     </border>
   </borders>
-  <cellStyleXfs count="184">
+  <cellStyleXfs count="274">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
     <xf numFmtId="0" fontId="3" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
     <xf numFmtId="0" fontId="4" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
@@ -1074,6 +1635,96 @@
     <xf numFmtId="0" fontId="5" fillId="2" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
     <xf numFmtId="0" fontId="6" fillId="3" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
     <xf numFmtId="0" fontId="1" fillId="4" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="4" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="4" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="4" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="4" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="4" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="4" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="4" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="4" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="4" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="4" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="4" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="4" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="4" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="4" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="4" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="4" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="4" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="4" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="4" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="4" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="4" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="4" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="4" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="4" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="4" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="4" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="4" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="4" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="4" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="4" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="4" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="4" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="4" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="4" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="4" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="4" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="4" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="4" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="4" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="4" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="4" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="4" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="4" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="4" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="4" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
     <xf numFmtId="0" fontId="3" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
     <xf numFmtId="0" fontId="4" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
     <xf numFmtId="0" fontId="3" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
@@ -1292,7 +1943,7 @@
     </xf>
     <xf numFmtId="0" fontId="6" fillId="3" borderId="0" xfId="12"/>
   </cellXfs>
-  <cellStyles count="184">
+  <cellStyles count="274">
     <cellStyle name="20% - Accent4" xfId="13" builtinId="42"/>
     <cellStyle name="Followed Hyperlink" xfId="2" builtinId="9" hidden="1"/>
     <cellStyle name="Followed Hyperlink" xfId="4" builtinId="9" hidden="1"/>
@@ -1384,6 +2035,51 @@
     <cellStyle name="Followed Hyperlink" xfId="179" builtinId="9" hidden="1"/>
     <cellStyle name="Followed Hyperlink" xfId="181" builtinId="9" hidden="1"/>
     <cellStyle name="Followed Hyperlink" xfId="183" builtinId="9" hidden="1"/>
+    <cellStyle name="Followed Hyperlink" xfId="185" builtinId="9" hidden="1"/>
+    <cellStyle name="Followed Hyperlink" xfId="187" builtinId="9" hidden="1"/>
+    <cellStyle name="Followed Hyperlink" xfId="189" builtinId="9" hidden="1"/>
+    <cellStyle name="Followed Hyperlink" xfId="191" builtinId="9" hidden="1"/>
+    <cellStyle name="Followed Hyperlink" xfId="193" builtinId="9" hidden="1"/>
+    <cellStyle name="Followed Hyperlink" xfId="195" builtinId="9" hidden="1"/>
+    <cellStyle name="Followed Hyperlink" xfId="197" builtinId="9" hidden="1"/>
+    <cellStyle name="Followed Hyperlink" xfId="199" builtinId="9" hidden="1"/>
+    <cellStyle name="Followed Hyperlink" xfId="201" builtinId="9" hidden="1"/>
+    <cellStyle name="Followed Hyperlink" xfId="203" builtinId="9" hidden="1"/>
+    <cellStyle name="Followed Hyperlink" xfId="205" builtinId="9" hidden="1"/>
+    <cellStyle name="Followed Hyperlink" xfId="207" builtinId="9" hidden="1"/>
+    <cellStyle name="Followed Hyperlink" xfId="209" builtinId="9" hidden="1"/>
+    <cellStyle name="Followed Hyperlink" xfId="211" builtinId="9" hidden="1"/>
+    <cellStyle name="Followed Hyperlink" xfId="213" builtinId="9" hidden="1"/>
+    <cellStyle name="Followed Hyperlink" xfId="215" builtinId="9" hidden="1"/>
+    <cellStyle name="Followed Hyperlink" xfId="217" builtinId="9" hidden="1"/>
+    <cellStyle name="Followed Hyperlink" xfId="219" builtinId="9" hidden="1"/>
+    <cellStyle name="Followed Hyperlink" xfId="221" builtinId="9" hidden="1"/>
+    <cellStyle name="Followed Hyperlink" xfId="223" builtinId="9" hidden="1"/>
+    <cellStyle name="Followed Hyperlink" xfId="225" builtinId="9" hidden="1"/>
+    <cellStyle name="Followed Hyperlink" xfId="227" builtinId="9" hidden="1"/>
+    <cellStyle name="Followed Hyperlink" xfId="229" builtinId="9" hidden="1"/>
+    <cellStyle name="Followed Hyperlink" xfId="231" builtinId="9" hidden="1"/>
+    <cellStyle name="Followed Hyperlink" xfId="233" builtinId="9" hidden="1"/>
+    <cellStyle name="Followed Hyperlink" xfId="235" builtinId="9" hidden="1"/>
+    <cellStyle name="Followed Hyperlink" xfId="237" builtinId="9" hidden="1"/>
+    <cellStyle name="Followed Hyperlink" xfId="239" builtinId="9" hidden="1"/>
+    <cellStyle name="Followed Hyperlink" xfId="241" builtinId="9" hidden="1"/>
+    <cellStyle name="Followed Hyperlink" xfId="243" builtinId="9" hidden="1"/>
+    <cellStyle name="Followed Hyperlink" xfId="245" builtinId="9" hidden="1"/>
+    <cellStyle name="Followed Hyperlink" xfId="247" builtinId="9" hidden="1"/>
+    <cellStyle name="Followed Hyperlink" xfId="249" builtinId="9" hidden="1"/>
+    <cellStyle name="Followed Hyperlink" xfId="251" builtinId="9" hidden="1"/>
+    <cellStyle name="Followed Hyperlink" xfId="253" builtinId="9" hidden="1"/>
+    <cellStyle name="Followed Hyperlink" xfId="255" builtinId="9" hidden="1"/>
+    <cellStyle name="Followed Hyperlink" xfId="257" builtinId="9" hidden="1"/>
+    <cellStyle name="Followed Hyperlink" xfId="259" builtinId="9" hidden="1"/>
+    <cellStyle name="Followed Hyperlink" xfId="261" builtinId="9" hidden="1"/>
+    <cellStyle name="Followed Hyperlink" xfId="263" builtinId="9" hidden="1"/>
+    <cellStyle name="Followed Hyperlink" xfId="265" builtinId="9" hidden="1"/>
+    <cellStyle name="Followed Hyperlink" xfId="267" builtinId="9" hidden="1"/>
+    <cellStyle name="Followed Hyperlink" xfId="269" builtinId="9" hidden="1"/>
+    <cellStyle name="Followed Hyperlink" xfId="271" builtinId="9" hidden="1"/>
+    <cellStyle name="Followed Hyperlink" xfId="273" builtinId="9" hidden="1"/>
     <cellStyle name="Good" xfId="11" builtinId="26"/>
     <cellStyle name="Hyperlink" xfId="1" builtinId="8" hidden="1"/>
     <cellStyle name="Hyperlink" xfId="3" builtinId="8" hidden="1"/>
@@ -1475,6 +2171,51 @@
     <cellStyle name="Hyperlink" xfId="178" builtinId="8" hidden="1"/>
     <cellStyle name="Hyperlink" xfId="180" builtinId="8" hidden="1"/>
     <cellStyle name="Hyperlink" xfId="182" builtinId="8" hidden="1"/>
+    <cellStyle name="Hyperlink" xfId="184" builtinId="8" hidden="1"/>
+    <cellStyle name="Hyperlink" xfId="186" builtinId="8" hidden="1"/>
+    <cellStyle name="Hyperlink" xfId="188" builtinId="8" hidden="1"/>
+    <cellStyle name="Hyperlink" xfId="190" builtinId="8" hidden="1"/>
+    <cellStyle name="Hyperlink" xfId="192" builtinId="8" hidden="1"/>
+    <cellStyle name="Hyperlink" xfId="194" builtinId="8" hidden="1"/>
+    <cellStyle name="Hyperlink" xfId="196" builtinId="8" hidden="1"/>
+    <cellStyle name="Hyperlink" xfId="198" builtinId="8" hidden="1"/>
+    <cellStyle name="Hyperlink" xfId="200" builtinId="8" hidden="1"/>
+    <cellStyle name="Hyperlink" xfId="202" builtinId="8" hidden="1"/>
+    <cellStyle name="Hyperlink" xfId="204" builtinId="8" hidden="1"/>
+    <cellStyle name="Hyperlink" xfId="206" builtinId="8" hidden="1"/>
+    <cellStyle name="Hyperlink" xfId="208" builtinId="8" hidden="1"/>
+    <cellStyle name="Hyperlink" xfId="210" builtinId="8" hidden="1"/>
+    <cellStyle name="Hyperlink" xfId="212" builtinId="8" hidden="1"/>
+    <cellStyle name="Hyperlink" xfId="214" builtinId="8" hidden="1"/>
+    <cellStyle name="Hyperlink" xfId="216" builtinId="8" hidden="1"/>
+    <cellStyle name="Hyperlink" xfId="218" builtinId="8" hidden="1"/>
+    <cellStyle name="Hyperlink" xfId="220" builtinId="8" hidden="1"/>
+    <cellStyle name="Hyperlink" xfId="222" builtinId="8" hidden="1"/>
+    <cellStyle name="Hyperlink" xfId="224" builtinId="8" hidden="1"/>
+    <cellStyle name="Hyperlink" xfId="226" builtinId="8" hidden="1"/>
+    <cellStyle name="Hyperlink" xfId="228" builtinId="8" hidden="1"/>
+    <cellStyle name="Hyperlink" xfId="230" builtinId="8" hidden="1"/>
+    <cellStyle name="Hyperlink" xfId="232" builtinId="8" hidden="1"/>
+    <cellStyle name="Hyperlink" xfId="234" builtinId="8" hidden="1"/>
+    <cellStyle name="Hyperlink" xfId="236" builtinId="8" hidden="1"/>
+    <cellStyle name="Hyperlink" xfId="238" builtinId="8" hidden="1"/>
+    <cellStyle name="Hyperlink" xfId="240" builtinId="8" hidden="1"/>
+    <cellStyle name="Hyperlink" xfId="242" builtinId="8" hidden="1"/>
+    <cellStyle name="Hyperlink" xfId="244" builtinId="8" hidden="1"/>
+    <cellStyle name="Hyperlink" xfId="246" builtinId="8" hidden="1"/>
+    <cellStyle name="Hyperlink" xfId="248" builtinId="8" hidden="1"/>
+    <cellStyle name="Hyperlink" xfId="250" builtinId="8" hidden="1"/>
+    <cellStyle name="Hyperlink" xfId="252" builtinId="8" hidden="1"/>
+    <cellStyle name="Hyperlink" xfId="254" builtinId="8" hidden="1"/>
+    <cellStyle name="Hyperlink" xfId="256" builtinId="8" hidden="1"/>
+    <cellStyle name="Hyperlink" xfId="258" builtinId="8" hidden="1"/>
+    <cellStyle name="Hyperlink" xfId="260" builtinId="8" hidden="1"/>
+    <cellStyle name="Hyperlink" xfId="262" builtinId="8" hidden="1"/>
+    <cellStyle name="Hyperlink" xfId="264" builtinId="8" hidden="1"/>
+    <cellStyle name="Hyperlink" xfId="266" builtinId="8" hidden="1"/>
+    <cellStyle name="Hyperlink" xfId="268" builtinId="8" hidden="1"/>
+    <cellStyle name="Hyperlink" xfId="270" builtinId="8" hidden="1"/>
+    <cellStyle name="Hyperlink" xfId="272" builtinId="8" hidden="1"/>
     <cellStyle name="Neutral" xfId="12" builtinId="28"/>
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
   </cellStyles>
@@ -1805,10 +2546,10 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <dimension ref="A1:I69"/>
+  <dimension ref="A1:I87"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A8" zoomScale="150" zoomScaleNormal="150" zoomScalePageLayoutView="150" workbookViewId="0">
-      <selection activeCell="C21" sqref="C21"/>
+    <sheetView zoomScale="150" zoomScaleNormal="150" zoomScalePageLayoutView="150" workbookViewId="0">
+      <selection activeCell="A20" sqref="A20"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultColWidth="11.5" defaultRowHeight="12.75" customHeight="1" x14ac:dyDescent="0"/>
@@ -1845,7 +2586,7 @@
     </row>
     <row r="2" spans="1:7" ht="15">
       <c r="A2" s="16" t="s">
-        <v>113</v>
+        <v>111</v>
       </c>
       <c r="B2" s="1"/>
       <c r="C2" s="3"/>
@@ -1854,7 +2595,7 @@
     </row>
     <row r="3" spans="1:7" ht="12">
       <c r="A3" s="3" t="s">
-        <v>234</v>
+        <v>230</v>
       </c>
       <c r="B3" s="4" t="s">
         <v>4</v>
@@ -1874,35 +2615,9 @@
       <c r="D4" s="4"/>
       <c r="E4" s="2"/>
     </row>
-    <row r="5" spans="1:7" ht="18" customHeight="1">
-      <c r="A5" s="5" t="s">
-        <v>75</v>
-      </c>
-      <c r="B5" s="5"/>
-      <c r="C5" s="5"/>
-      <c r="D5" s="6" t="s">
-        <v>76</v>
-      </c>
-      <c r="E5" s="5"/>
-      <c r="F5" s="5"/>
-      <c r="G5" s="5"/>
-    </row>
-    <row r="6" spans="1:7" ht="18" customHeight="1">
-      <c r="A6" s="5" t="s">
-        <v>116</v>
-      </c>
-      <c r="B6" s="5"/>
-      <c r="C6" s="5"/>
-      <c r="D6" s="6" t="s">
-        <v>117</v>
-      </c>
-      <c r="E6" s="5"/>
-      <c r="F6" s="5"/>
-      <c r="G6" s="5"/>
-    </row>
     <row r="7" spans="1:7" s="12" customFormat="1" ht="18" customHeight="1">
       <c r="A7" s="18" t="s">
-        <v>115</v>
+        <v>113</v>
       </c>
       <c r="B7" s="18"/>
       <c r="C7" s="18"/>
@@ -1913,7 +2628,7 @@
     </row>
     <row r="8" spans="1:7" s="12" customFormat="1" ht="18" customHeight="1">
       <c r="A8" t="s">
-        <v>235</v>
+        <v>231</v>
       </c>
       <c r="B8" t="s">
         <v>7</v>
@@ -1932,647 +2647,640 @@
       </c>
       <c r="B9" s="2"/>
       <c r="C9" s="2" t="s">
-        <v>108</v>
+        <v>106</v>
       </c>
       <c r="D9" s="2" t="s">
-        <v>134</v>
+        <v>130</v>
       </c>
       <c r="E9" s="2"/>
       <c r="F9" t="s">
-        <v>136</v>
+        <v>132</v>
       </c>
     </row>
     <row r="10" spans="1:7" ht="18" customHeight="1">
       <c r="A10" s="2" t="s">
-        <v>109</v>
+        <v>107</v>
       </c>
       <c r="B10" s="4"/>
       <c r="C10" s="2" t="s">
-        <v>107</v>
+        <v>105</v>
       </c>
       <c r="D10" s="2" t="s">
-        <v>137</v>
+        <v>133</v>
       </c>
       <c r="E10" s="2"/>
     </row>
     <row r="11" spans="1:7" ht="18" customHeight="1">
       <c r="A11" s="2" t="s">
-        <v>109</v>
+        <v>107</v>
       </c>
       <c r="B11" s="4"/>
       <c r="C11" s="2" t="s">
-        <v>110</v>
+        <v>108</v>
       </c>
       <c r="D11" s="2" t="s">
-        <v>135</v>
+        <v>131</v>
       </c>
       <c r="E11" s="2"/>
     </row>
     <row r="12" spans="1:7" ht="18" customHeight="1">
-      <c r="A12" s="7" t="s">
-        <v>17</v>
-      </c>
-      <c r="B12" s="4"/>
-      <c r="C12" s="2"/>
+      <c r="A12" s="2" t="s">
+        <v>276</v>
+      </c>
+      <c r="B12" s="2" t="s">
+        <v>277</v>
+      </c>
+      <c r="C12" s="2" t="s">
+        <v>84</v>
+      </c>
       <c r="D12" s="2" t="s">
-        <v>141</v>
+        <v>137</v>
       </c>
       <c r="E12" s="2"/>
     </row>
     <row r="13" spans="1:7" ht="12">
       <c r="A13" t="s">
-        <v>236</v>
+        <v>232</v>
       </c>
       <c r="B13" t="s">
-        <v>142</v>
+        <v>138</v>
       </c>
       <c r="C13" t="s">
-        <v>86</v>
-      </c>
-    </row>
-    <row r="14" spans="1:7" ht="25" customHeight="1">
+        <v>278</v>
+      </c>
+      <c r="D13" s="2" t="s">
+        <v>279</v>
+      </c>
+    </row>
+    <row r="14" spans="1:7" ht="11" customHeight="1">
       <c r="A14" t="s">
+        <v>151</v>
+      </c>
+      <c r="B14" t="s">
+        <v>152</v>
+      </c>
+      <c r="C14" t="s">
+        <v>153</v>
+      </c>
+      <c r="D14" s="2" t="s">
+        <v>154</v>
+      </c>
+    </row>
+    <row r="15" spans="1:7" ht="11" customHeight="1">
+      <c r="A15" t="s">
+        <v>155</v>
+      </c>
+      <c r="B15" t="s">
+        <v>156</v>
+      </c>
+      <c r="C15" t="s">
+        <v>157</v>
+      </c>
+      <c r="D15" s="2" t="s">
+        <v>158</v>
+      </c>
+    </row>
+    <row r="16" spans="1:7" ht="11" customHeight="1">
+      <c r="A16" t="s">
+        <v>172</v>
+      </c>
+      <c r="B16" t="s">
+        <v>173</v>
+      </c>
+      <c r="C16" t="s">
+        <v>174</v>
+      </c>
+      <c r="D16" s="2" t="s">
+        <v>175</v>
+      </c>
+    </row>
+    <row r="17" spans="1:5" ht="11" customHeight="1">
+      <c r="A17" t="s">
+        <v>244</v>
+      </c>
+      <c r="B17" t="s">
+        <v>245</v>
+      </c>
+      <c r="C17" t="s">
+        <v>246</v>
+      </c>
+      <c r="D17" s="2" t="s">
+        <v>247</v>
+      </c>
+    </row>
+    <row r="18" spans="1:5" ht="11" customHeight="1">
+      <c r="A18" t="s">
+        <v>176</v>
+      </c>
+      <c r="B18" t="s">
+        <v>177</v>
+      </c>
+      <c r="C18" t="s">
+        <v>178</v>
+      </c>
+      <c r="D18" s="2" t="s">
+        <v>228</v>
+      </c>
+    </row>
+    <row r="19" spans="1:5" ht="11" customHeight="1">
+      <c r="A19" t="s">
+        <v>179</v>
+      </c>
+      <c r="B19" t="s">
+        <v>180</v>
+      </c>
+      <c r="C19" t="s">
+        <v>181</v>
+      </c>
+      <c r="D19" s="2" t="s">
+        <v>229</v>
+      </c>
+    </row>
+    <row r="20" spans="1:5" ht="11" customHeight="1">
+      <c r="A20" t="s">
+        <v>280</v>
+      </c>
+      <c r="B20" t="s">
+        <v>281</v>
+      </c>
+      <c r="C20" t="s">
+        <v>282</v>
+      </c>
+      <c r="D20" s="2" t="s">
+        <v>283</v>
+      </c>
+    </row>
+    <row r="21" spans="1:5" ht="11" customHeight="1">
+      <c r="A21" t="s">
+        <v>331</v>
+      </c>
+      <c r="B21" t="s">
+        <v>311</v>
+      </c>
+      <c r="C21" t="s">
+        <v>289</v>
+      </c>
+      <c r="D21" s="2" t="s">
+        <v>290</v>
+      </c>
+    </row>
+    <row r="22" spans="1:5" ht="11" customHeight="1">
+      <c r="A22" t="s">
+        <v>332</v>
+      </c>
+      <c r="B22" t="s">
+        <v>312</v>
+      </c>
+      <c r="C22" t="s">
+        <v>301</v>
+      </c>
+      <c r="D22" s="2" t="s">
+        <v>292</v>
+      </c>
+    </row>
+    <row r="23" spans="1:5" ht="11" customHeight="1">
+      <c r="A23" t="s">
+        <v>333</v>
+      </c>
+      <c r="B23" t="s">
+        <v>313</v>
+      </c>
+      <c r="C23" t="s">
+        <v>304</v>
+      </c>
+      <c r="D23" s="2" t="s">
+        <v>293</v>
+      </c>
+    </row>
+    <row r="24" spans="1:5" ht="11" customHeight="1">
+      <c r="A24" t="s">
+        <v>334</v>
+      </c>
+      <c r="B24" t="s">
+        <v>314</v>
+      </c>
+      <c r="C24" t="s">
+        <v>302</v>
+      </c>
+      <c r="D24" s="2" t="s">
+        <v>296</v>
+      </c>
+    </row>
+    <row r="25" spans="1:5" ht="11" customHeight="1">
+      <c r="A25" t="s">
+        <v>335</v>
+      </c>
+      <c r="B25" t="s">
+        <v>315</v>
+      </c>
+      <c r="C25" t="s">
+        <v>303</v>
+      </c>
+      <c r="D25" s="2" t="s">
+        <v>298</v>
+      </c>
+    </row>
+    <row r="26" spans="1:5" ht="12" customHeight="1">
+      <c r="A26" t="s">
+        <v>336</v>
+      </c>
+      <c r="B26" t="s">
+        <v>316</v>
+      </c>
+      <c r="C26" t="s">
+        <v>305</v>
+      </c>
+      <c r="D26" s="2" t="s">
+        <v>300</v>
+      </c>
+    </row>
+    <row r="27" spans="1:5" ht="18" customHeight="1">
+      <c r="A27" s="7" t="s">
+        <v>17</v>
+      </c>
+      <c r="B27" s="4"/>
+      <c r="C27" s="2"/>
+      <c r="D27" s="2" t="s">
+        <v>427</v>
+      </c>
+      <c r="E27" s="2"/>
+    </row>
+    <row r="28" spans="1:5" ht="18" customHeight="1">
+      <c r="A28" s="9" t="s">
         <v>13</v>
       </c>
-      <c r="C14" t="s">
-        <v>242</v>
-      </c>
-    </row>
-    <row r="15" spans="1:7" ht="25" customHeight="1">
-      <c r="A15" t="s">
+      <c r="B28" s="4"/>
+      <c r="C28" s="2" t="s">
+        <v>404</v>
+      </c>
+      <c r="D28" s="2"/>
+      <c r="E28" s="2"/>
+    </row>
+    <row r="29" spans="1:5" ht="25" customHeight="1">
+      <c r="A29" t="s">
         <v>13</v>
       </c>
-      <c r="C15" t="s">
-        <v>255</v>
-      </c>
-    </row>
-    <row r="16" spans="1:7" ht="25" customHeight="1">
-      <c r="A16" t="s">
+      <c r="C29" t="s">
+        <v>238</v>
+      </c>
+    </row>
+    <row r="30" spans="1:5" ht="25" customHeight="1">
+      <c r="A30" t="s">
         <v>13</v>
       </c>
-      <c r="C16" t="s">
-        <v>256</v>
-      </c>
-    </row>
-    <row r="17" spans="1:9" ht="25" customHeight="1">
-      <c r="A17" t="s">
+      <c r="C30" t="s">
+        <v>251</v>
+      </c>
+    </row>
+    <row r="31" spans="1:5" ht="25" customHeight="1">
+      <c r="A31" t="s">
         <v>13</v>
       </c>
-      <c r="C17" t="s">
-        <v>278</v>
-      </c>
-    </row>
-    <row r="18" spans="1:9" ht="25" customHeight="1">
-      <c r="A18" t="s">
+      <c r="C31" t="s">
+        <v>252</v>
+      </c>
+    </row>
+    <row r="32" spans="1:5" ht="25" customHeight="1">
+      <c r="A32" t="s">
         <v>13</v>
       </c>
-      <c r="C18" t="s">
-        <v>257</v>
-      </c>
-    </row>
-    <row r="19" spans="1:9" ht="25" customHeight="1">
-      <c r="A19" t="s">
+      <c r="C32" t="s">
+        <v>274</v>
+      </c>
+    </row>
+    <row r="33" spans="1:9" ht="25" customHeight="1">
+      <c r="A33" t="s">
         <v>13</v>
       </c>
-      <c r="C19" t="s">
-        <v>258</v>
-      </c>
-    </row>
-    <row r="20" spans="1:9" ht="25" customHeight="1">
-      <c r="A20" t="s">
+      <c r="C33" t="s">
+        <v>253</v>
+      </c>
+    </row>
+    <row r="34" spans="1:9" ht="25" customHeight="1">
+      <c r="A34" t="s">
         <v>13</v>
       </c>
-      <c r="C20" t="s">
-        <v>279</v>
-      </c>
-    </row>
-    <row r="21" spans="1:9" ht="25" customHeight="1">
-      <c r="A21" s="11" t="s">
-        <v>27</v>
-      </c>
-    </row>
-    <row r="22" spans="1:9" ht="11" customHeight="1">
-      <c r="A22" t="s">
-        <v>155</v>
-      </c>
-      <c r="B22" t="s">
-        <v>156</v>
-      </c>
-      <c r="C22" t="s">
-        <v>157</v>
-      </c>
-      <c r="D22" s="2" t="s">
-        <v>158</v>
-      </c>
-    </row>
-    <row r="23" spans="1:9" ht="11" customHeight="1">
-      <c r="A23" t="s">
-        <v>159</v>
-      </c>
-      <c r="B23" t="s">
-        <v>160</v>
-      </c>
-      <c r="C23" t="s">
-        <v>161</v>
-      </c>
-      <c r="D23" s="2" t="s">
-        <v>162</v>
-      </c>
-    </row>
-    <row r="24" spans="1:9" ht="11" customHeight="1">
-      <c r="A24" t="s">
-        <v>176</v>
-      </c>
-      <c r="B24" t="s">
-        <v>177</v>
-      </c>
-      <c r="C24" t="s">
-        <v>178</v>
-      </c>
-      <c r="D24" s="2" t="s">
-        <v>179</v>
-      </c>
-    </row>
-    <row r="25" spans="1:9" ht="11" customHeight="1">
-      <c r="A25" t="s">
-        <v>248</v>
-      </c>
-      <c r="B25" t="s">
-        <v>249</v>
-      </c>
-      <c r="C25" t="s">
-        <v>250</v>
-      </c>
-      <c r="D25" s="2" t="s">
-        <v>251</v>
-      </c>
-    </row>
-    <row r="26" spans="1:9" ht="11" customHeight="1">
-      <c r="A26" t="s">
-        <v>180</v>
-      </c>
-      <c r="B26" t="s">
-        <v>181</v>
-      </c>
-      <c r="C26" t="s">
-        <v>182</v>
-      </c>
-      <c r="D26" s="2" t="s">
-        <v>232</v>
-      </c>
-    </row>
-    <row r="27" spans="1:9" ht="11" customHeight="1">
-      <c r="A27" t="s">
-        <v>183</v>
-      </c>
-      <c r="B27" t="s">
-        <v>184</v>
-      </c>
-      <c r="C27" t="s">
-        <v>185</v>
-      </c>
-      <c r="D27" s="2" t="s">
-        <v>233</v>
-      </c>
-    </row>
-    <row r="28" spans="1:9" ht="15">
-      <c r="A28" s="15" t="s">
-        <v>77</v>
-      </c>
-      <c r="B28" s="15"/>
-      <c r="C28" s="15"/>
-      <c r="D28" s="15"/>
-      <c r="E28" s="15"/>
-      <c r="F28" s="15"/>
-      <c r="G28" s="15"/>
-    </row>
-    <row r="29" spans="1:9" ht="15">
-      <c r="A29" s="16"/>
-      <c r="B29" s="12"/>
-      <c r="C29" s="12"/>
-      <c r="D29" s="12"/>
-      <c r="E29" s="12"/>
-      <c r="F29" s="12"/>
-      <c r="G29" s="12"/>
-    </row>
-    <row r="30" spans="1:9" s="15" customFormat="1" ht="15">
-      <c r="A30" s="13" t="s">
-        <v>112</v>
-      </c>
-      <c r="B30" s="13"/>
-      <c r="C30" s="13"/>
-      <c r="D30" s="13" t="s">
-        <v>74</v>
-      </c>
-      <c r="E30" s="13"/>
-      <c r="F30" s="13"/>
-      <c r="G30" s="13"/>
-      <c r="H30" s="12"/>
-      <c r="I30" s="12"/>
-    </row>
-    <row r="31" spans="1:9" ht="12">
-      <c r="A31" s="5" t="s">
-        <v>78</v>
-      </c>
-      <c r="B31" s="5"/>
-      <c r="C31" s="5"/>
-      <c r="D31" s="6" t="s">
-        <v>79</v>
-      </c>
-      <c r="E31" s="5"/>
-      <c r="F31" s="5"/>
-      <c r="G31" s="5"/>
-    </row>
-    <row r="32" spans="1:9" ht="15">
-      <c r="A32" s="15" t="s">
-        <v>111</v>
-      </c>
-      <c r="B32" s="15"/>
-      <c r="C32" s="15"/>
-      <c r="D32" s="15"/>
-      <c r="E32" s="15"/>
-      <c r="F32" s="15"/>
-      <c r="G32" s="15"/>
-    </row>
-    <row r="33" spans="1:8" ht="12">
-      <c r="A33" s="12" t="s">
-        <v>237</v>
-      </c>
-      <c r="B33" s="12" t="s">
-        <v>9</v>
-      </c>
-      <c r="C33" s="12" t="s">
-        <v>10</v>
-      </c>
-      <c r="D33" s="12"/>
-      <c r="E33" s="12" t="s">
-        <v>6</v>
-      </c>
-      <c r="F33" s="12"/>
-      <c r="G33" s="12"/>
-    </row>
-    <row r="34" spans="1:8" ht="12">
-      <c r="A34" s="7" t="s">
-        <v>17</v>
-      </c>
-      <c r="B34" s="8"/>
-      <c r="C34" s="8"/>
-      <c r="D34" s="9" t="s">
-        <v>65</v>
-      </c>
-      <c r="E34" s="8"/>
-      <c r="F34" s="10"/>
-      <c r="G34" s="10"/>
-    </row>
-    <row r="35" spans="1:8" ht="12.75" customHeight="1">
-      <c r="A35" s="4" t="s">
+      <c r="C34" t="s">
+        <v>254</v>
+      </c>
+    </row>
+    <row r="35" spans="1:9" ht="25" customHeight="1">
+      <c r="A35" t="s">
         <v>13</v>
       </c>
-      <c r="B35" s="2" t="s">
-        <v>80</v>
-      </c>
-      <c r="C35" s="2" t="s">
-        <v>81</v>
-      </c>
-      <c r="D35" s="2"/>
-      <c r="E35" s="4"/>
-    </row>
-    <row r="36" spans="1:8" ht="12.75" customHeight="1">
-      <c r="A36" s="4" t="s">
+      <c r="C35" t="s">
+        <v>275</v>
+      </c>
+    </row>
+    <row r="36" spans="1:9" ht="25" customHeight="1">
+      <c r="A36" t="s">
         <v>13</v>
       </c>
-      <c r="B36" s="2" t="s">
-        <v>82</v>
-      </c>
-      <c r="C36" s="2"/>
-      <c r="D36" s="2"/>
-      <c r="E36" s="4"/>
-      <c r="F36" t="s">
-        <v>14</v>
-      </c>
-    </row>
-    <row r="37" spans="1:8" ht="12.75" customHeight="1">
+      <c r="C36" t="s">
+        <v>403</v>
+      </c>
+    </row>
+    <row r="37" spans="1:9" ht="25" customHeight="1">
       <c r="A37" t="s">
         <v>13</v>
       </c>
       <c r="C37" t="s">
-        <v>83</v>
-      </c>
-      <c r="D37" s="13"/>
-    </row>
-    <row r="38" spans="1:8" ht="12.75" customHeight="1">
+        <v>405</v>
+      </c>
+    </row>
+    <row r="38" spans="1:9" ht="25" customHeight="1">
       <c r="A38" t="s">
         <v>13</v>
       </c>
-      <c r="B38" t="s">
-        <v>84</v>
-      </c>
-      <c r="G38" t="s">
+      <c r="C38" t="s">
+        <v>406</v>
+      </c>
+    </row>
+    <row r="39" spans="1:9" ht="25" customHeight="1">
+      <c r="A39" t="s">
+        <v>13</v>
+      </c>
+      <c r="C39" t="s">
+        <v>407</v>
+      </c>
+    </row>
+    <row r="40" spans="1:9" ht="25" customHeight="1">
+      <c r="A40" t="s">
+        <v>13</v>
+      </c>
+      <c r="C40" t="s">
+        <v>408</v>
+      </c>
+    </row>
+    <row r="41" spans="1:9" ht="25" customHeight="1">
+      <c r="A41" t="s">
+        <v>13</v>
+      </c>
+      <c r="C41" t="s">
+        <v>409</v>
+      </c>
+    </row>
+    <row r="42" spans="1:9" ht="25" customHeight="1">
+      <c r="A42" t="s">
+        <v>13</v>
+      </c>
+      <c r="C42" t="s">
+        <v>410</v>
+      </c>
+    </row>
+    <row r="43" spans="1:9" ht="25" customHeight="1">
+      <c r="A43" t="s">
+        <v>13</v>
+      </c>
+      <c r="C43" t="s">
+        <v>411</v>
+      </c>
+    </row>
+    <row r="44" spans="1:9" ht="25" customHeight="1">
+      <c r="A44" t="s">
+        <v>13</v>
+      </c>
+      <c r="C44" t="s">
+        <v>428</v>
+      </c>
+    </row>
+    <row r="45" spans="1:9" ht="25" customHeight="1">
+      <c r="A45" s="11" t="s">
+        <v>27</v>
+      </c>
+    </row>
+    <row r="46" spans="1:9" ht="15">
+      <c r="A46" s="15" t="s">
+        <v>75</v>
+      </c>
+      <c r="B46" s="15"/>
+      <c r="C46" s="15"/>
+      <c r="D46" s="15"/>
+      <c r="E46" s="15"/>
+      <c r="F46" s="15"/>
+      <c r="G46" s="15"/>
+    </row>
+    <row r="47" spans="1:9" ht="15">
+      <c r="A47" s="16"/>
+      <c r="B47" s="12"/>
+      <c r="C47" s="12"/>
+      <c r="D47" s="12"/>
+      <c r="E47" s="12"/>
+      <c r="F47" s="12"/>
+      <c r="G47" s="12"/>
+    </row>
+    <row r="48" spans="1:9" s="15" customFormat="1" ht="15">
+      <c r="A48" s="13" t="s">
+        <v>110</v>
+      </c>
+      <c r="B48" s="13"/>
+      <c r="C48" s="13"/>
+      <c r="D48" s="13" t="s">
+        <v>74</v>
+      </c>
+      <c r="E48" s="13"/>
+      <c r="F48" s="13"/>
+      <c r="G48" s="13"/>
+      <c r="H48" s="12"/>
+      <c r="I48" s="12"/>
+    </row>
+    <row r="49" spans="1:8" ht="12">
+      <c r="A49" s="5" t="s">
+        <v>76</v>
+      </c>
+      <c r="B49" s="5"/>
+      <c r="C49" s="5"/>
+      <c r="D49" s="6" t="s">
+        <v>77</v>
+      </c>
+      <c r="E49" s="5"/>
+      <c r="F49" s="5"/>
+      <c r="G49" s="5"/>
+    </row>
+    <row r="50" spans="1:8" ht="15">
+      <c r="A50" s="15" t="s">
+        <v>109</v>
+      </c>
+      <c r="B50" s="15"/>
+      <c r="C50" s="15"/>
+      <c r="D50" s="15"/>
+      <c r="E50" s="15"/>
+      <c r="F50" s="15"/>
+      <c r="G50" s="15"/>
+    </row>
+    <row r="51" spans="1:8" ht="12">
+      <c r="A51" s="12" t="s">
+        <v>233</v>
+      </c>
+      <c r="B51" s="12" t="s">
+        <v>9</v>
+      </c>
+      <c r="C51" s="12" t="s">
+        <v>10</v>
+      </c>
+      <c r="D51" s="12"/>
+      <c r="E51" s="12" t="s">
+        <v>6</v>
+      </c>
+      <c r="F51" s="12"/>
+      <c r="G51" s="12"/>
+    </row>
+    <row r="52" spans="1:8" ht="12">
+      <c r="A52" s="7" t="s">
+        <v>17</v>
+      </c>
+      <c r="B52" s="8"/>
+      <c r="C52" s="8"/>
+      <c r="D52" s="9" t="s">
+        <v>65</v>
+      </c>
+      <c r="E52" s="8"/>
+      <c r="F52" s="10"/>
+      <c r="G52" s="10"/>
+    </row>
+    <row r="53" spans="1:8" ht="12.75" customHeight="1">
+      <c r="A53" s="4" t="s">
+        <v>13</v>
+      </c>
+      <c r="B53" s="2" t="s">
+        <v>78</v>
+      </c>
+      <c r="C53" s="2" t="s">
+        <v>79</v>
+      </c>
+      <c r="D53" s="2"/>
+      <c r="E53" s="4"/>
+    </row>
+    <row r="54" spans="1:8" ht="12.75" customHeight="1">
+      <c r="A54" s="4" t="s">
+        <v>13</v>
+      </c>
+      <c r="B54" s="2" t="s">
+        <v>80</v>
+      </c>
+      <c r="C54" s="2"/>
+      <c r="D54" s="2"/>
+      <c r="E54" s="4"/>
+      <c r="F54" t="s">
+        <v>14</v>
+      </c>
+    </row>
+    <row r="55" spans="1:8" ht="12.75" customHeight="1">
+      <c r="A55" t="s">
+        <v>13</v>
+      </c>
+      <c r="C55" t="s">
+        <v>81</v>
+      </c>
+      <c r="D55" s="13"/>
+    </row>
+    <row r="56" spans="1:8" ht="12.75" customHeight="1">
+      <c r="A56" t="s">
+        <v>13</v>
+      </c>
+      <c r="B56" t="s">
+        <v>82</v>
+      </c>
+      <c r="G56" t="s">
+        <v>83</v>
+      </c>
+    </row>
+    <row r="57" spans="1:8" ht="12">
+      <c r="A57" s="11" t="s">
+        <v>27</v>
+      </c>
+      <c r="B57" s="10"/>
+      <c r="C57" s="10"/>
+      <c r="D57" s="10"/>
+      <c r="E57" s="10"/>
+      <c r="F57" s="10"/>
+      <c r="G57" s="10"/>
+    </row>
+    <row r="58" spans="1:8" ht="24">
+      <c r="A58" s="4" t="s">
+        <v>13</v>
+      </c>
+      <c r="B58" s="4"/>
+      <c r="C58" s="4" t="s">
+        <v>15</v>
+      </c>
+      <c r="D58" s="2" t="s">
+        <v>73</v>
+      </c>
+      <c r="E58" s="4"/>
+      <c r="F58" t="s">
+        <v>16</v>
+      </c>
+    </row>
+    <row r="59" spans="1:8" ht="15">
+      <c r="A59" s="15" t="s">
         <v>85</v>
       </c>
-    </row>
-    <row r="39" spans="1:8" ht="12">
-      <c r="A39" s="11" t="s">
-        <v>27</v>
-      </c>
-      <c r="B39" s="10"/>
-      <c r="C39" s="10"/>
-      <c r="D39" s="10"/>
-      <c r="E39" s="10"/>
-      <c r="F39" s="10"/>
-      <c r="G39" s="10"/>
-    </row>
-    <row r="40" spans="1:8" ht="24">
-      <c r="A40" s="4" t="s">
-        <v>13</v>
-      </c>
-      <c r="B40" s="4"/>
-      <c r="C40" s="4" t="s">
-        <v>15</v>
-      </c>
-      <c r="D40" s="2" t="s">
-        <v>73</v>
-      </c>
-      <c r="E40" s="4"/>
-      <c r="F40" t="s">
-        <v>16</v>
-      </c>
-    </row>
-    <row r="41" spans="1:8" ht="15">
-      <c r="A41" s="15" t="s">
-        <v>87</v>
-      </c>
-      <c r="B41" s="15"/>
-      <c r="C41" s="15"/>
-      <c r="D41" s="15"/>
-      <c r="E41" s="15"/>
-      <c r="F41" s="15"/>
-      <c r="G41" s="15"/>
-      <c r="H41" s="12"/>
-    </row>
-    <row r="42" spans="1:8" ht="12">
-      <c r="A42" s="12"/>
-      <c r="B42" s="12"/>
-      <c r="C42" s="12"/>
-      <c r="D42" s="12"/>
-      <c r="E42" s="12"/>
-      <c r="F42" s="12"/>
-      <c r="G42" s="12"/>
-      <c r="H42" s="12"/>
-    </row>
-    <row r="43" spans="1:8" ht="15">
-      <c r="A43" s="14" t="s">
-        <v>118</v>
-      </c>
-      <c r="B43" s="14"/>
-      <c r="C43" s="14"/>
-      <c r="D43" s="13" t="s">
-        <v>119</v>
-      </c>
-      <c r="E43" s="14"/>
-      <c r="F43" s="14"/>
-      <c r="G43" s="14"/>
-      <c r="H43" s="12"/>
-    </row>
-    <row r="44" spans="1:8" ht="12">
-      <c r="A44" s="5" t="s">
-        <v>88</v>
-      </c>
-      <c r="B44" s="5"/>
-      <c r="C44" s="5"/>
-      <c r="D44" s="6" t="s">
-        <v>89</v>
-      </c>
-      <c r="E44" s="5"/>
-      <c r="F44" s="5"/>
-      <c r="G44" s="5"/>
-    </row>
-    <row r="45" spans="1:8" ht="15">
-      <c r="A45" s="15" t="s">
-        <v>120</v>
-      </c>
-      <c r="B45" s="15"/>
-      <c r="C45" s="15"/>
-      <c r="D45" s="15"/>
-      <c r="E45" s="15"/>
-      <c r="F45" s="15"/>
-      <c r="G45" s="15"/>
-    </row>
-    <row r="46" spans="1:8" ht="12">
-      <c r="A46" t="s">
-        <v>238</v>
-      </c>
-      <c r="B46" t="s">
-        <v>11</v>
-      </c>
-      <c r="C46" t="s">
-        <v>12</v>
-      </c>
-      <c r="E46" t="s">
-        <v>6</v>
-      </c>
-      <c r="F46" s="12"/>
-      <c r="G46" s="12"/>
-    </row>
-    <row r="47" spans="1:8" ht="12">
-      <c r="A47" s="4" t="s">
-        <v>17</v>
-      </c>
-      <c r="B47" s="4"/>
-      <c r="C47" s="4"/>
-      <c r="D47" s="4"/>
-      <c r="E47" s="4"/>
-    </row>
-    <row r="48" spans="1:8" ht="12">
-      <c r="A48" s="4" t="s">
-        <v>18</v>
-      </c>
-      <c r="B48" s="4" t="s">
-        <v>19</v>
-      </c>
-      <c r="C48" s="4" t="s">
-        <v>20</v>
-      </c>
-      <c r="D48" s="4"/>
-      <c r="E48" s="4"/>
-    </row>
-    <row r="49" spans="1:9" ht="36">
-      <c r="A49" s="4" t="s">
-        <v>13</v>
-      </c>
-      <c r="B49" s="4"/>
-      <c r="C49" s="4" t="s">
-        <v>21</v>
-      </c>
-      <c r="D49" s="4" t="s">
-        <v>22</v>
-      </c>
-      <c r="E49" s="4"/>
-    </row>
-    <row r="50" spans="1:9" ht="12">
-      <c r="A50" s="4" t="s">
-        <v>18</v>
-      </c>
-      <c r="B50" s="4" t="s">
-        <v>23</v>
-      </c>
-      <c r="C50" s="4" t="s">
-        <v>24</v>
-      </c>
-      <c r="D50" s="4"/>
-      <c r="E50" s="4"/>
-    </row>
-    <row r="51" spans="1:9" ht="36">
-      <c r="A51" s="4" t="s">
-        <v>13</v>
-      </c>
-      <c r="B51" s="4"/>
-      <c r="C51" s="4" t="s">
-        <v>25</v>
-      </c>
-      <c r="D51" s="4" t="s">
-        <v>26</v>
-      </c>
-      <c r="E51" s="4"/>
-      <c r="H51" s="12"/>
-    </row>
-    <row r="52" spans="1:9" ht="12.75" customHeight="1">
-      <c r="A52" s="4" t="s">
-        <v>27</v>
-      </c>
-      <c r="B52" s="4"/>
-      <c r="C52" s="4"/>
-      <c r="D52" s="4"/>
-      <c r="E52" s="4"/>
-    </row>
-    <row r="53" spans="1:9" ht="12.75" customHeight="1">
-      <c r="A53" s="15" t="s">
-        <v>90</v>
-      </c>
-      <c r="B53" s="15"/>
-      <c r="C53" s="15"/>
-      <c r="D53" s="15"/>
-      <c r="E53" s="15"/>
-      <c r="F53" s="15"/>
-      <c r="G53" s="15"/>
-    </row>
-    <row r="54" spans="1:9" s="12" customFormat="1" ht="12.75" customHeight="1"/>
-    <row r="55" spans="1:9" s="14" customFormat="1" ht="12.75" customHeight="1">
-      <c r="A55" s="13" t="s">
-        <v>121</v>
-      </c>
-      <c r="D55" s="14" t="s">
-        <v>122</v>
-      </c>
-      <c r="H55" s="12"/>
-      <c r="I55" s="12"/>
-    </row>
-    <row r="56" spans="1:9" ht="12.75" customHeight="1">
-      <c r="A56" s="13" t="s">
-        <v>96</v>
-      </c>
-      <c r="B56" s="14"/>
-      <c r="C56" s="14"/>
-      <c r="D56" s="14" t="s">
-        <v>91</v>
-      </c>
-      <c r="E56" s="14"/>
-      <c r="F56" s="14"/>
-      <c r="G56" s="14"/>
-    </row>
-    <row r="57" spans="1:9" ht="12.75" customHeight="1">
-      <c r="A57" s="15" t="s">
-        <v>138</v>
-      </c>
-      <c r="B57" s="18"/>
-      <c r="C57" s="18"/>
-      <c r="D57" s="18"/>
-      <c r="E57" s="18"/>
-      <c r="F57" s="18"/>
-      <c r="G57" s="18"/>
-    </row>
-    <row r="58" spans="1:9" ht="12.75" customHeight="1">
-      <c r="A58" s="2" t="s">
-        <v>240</v>
-      </c>
-      <c r="B58" s="12" t="s">
-        <v>92</v>
-      </c>
-      <c r="C58" s="12" t="s">
-        <v>93</v>
-      </c>
-      <c r="D58" s="12"/>
-      <c r="E58" s="12" t="s">
-        <v>94</v>
-      </c>
-      <c r="F58" s="12"/>
-      <c r="G58" s="12"/>
-    </row>
-    <row r="59" spans="1:9" ht="12.75" customHeight="1">
-      <c r="A59" s="15" t="s">
-        <v>95</v>
-      </c>
-      <c r="B59" s="18"/>
-      <c r="C59" s="18"/>
-      <c r="D59" s="18"/>
-      <c r="E59" s="18"/>
-      <c r="F59" s="18"/>
-      <c r="G59" s="18"/>
-    </row>
-    <row r="60" spans="1:9" ht="12.75" customHeight="1">
+      <c r="B59" s="15"/>
+      <c r="C59" s="15"/>
+      <c r="D59" s="15"/>
+      <c r="E59" s="15"/>
+      <c r="F59" s="15"/>
+      <c r="G59" s="15"/>
+      <c r="H59" s="12"/>
+    </row>
+    <row r="60" spans="1:8" ht="12">
+      <c r="A60" s="12"/>
       <c r="B60" s="12"/>
       <c r="C60" s="12"/>
       <c r="D60" s="12"/>
       <c r="E60" s="12"/>
       <c r="F60" s="12"/>
       <c r="G60" s="12"/>
-    </row>
-    <row r="61" spans="1:9" ht="12.75" customHeight="1">
-      <c r="A61" s="13" t="s">
-        <v>129</v>
+      <c r="H60" s="12"/>
+    </row>
+    <row r="61" spans="1:8" ht="15">
+      <c r="A61" s="14" t="s">
+        <v>114</v>
       </c>
       <c r="B61" s="14"/>
       <c r="C61" s="14"/>
-      <c r="D61" s="14" t="s">
-        <v>131</v>
+      <c r="D61" s="13" t="s">
+        <v>115</v>
       </c>
       <c r="E61" s="14"/>
       <c r="F61" s="14"/>
       <c r="G61" s="14"/>
-    </row>
-    <row r="62" spans="1:9" ht="12.75" customHeight="1">
-      <c r="A62" s="13" t="s">
-        <v>130</v>
-      </c>
-      <c r="B62" s="14"/>
-      <c r="C62" s="14"/>
-      <c r="D62" s="14" t="s">
-        <v>132</v>
-      </c>
-      <c r="E62" s="14"/>
-      <c r="F62" s="14"/>
-      <c r="G62" s="14"/>
-    </row>
-    <row r="63" spans="1:9" ht="12.75" customHeight="1">
+      <c r="H61" s="12"/>
+    </row>
+    <row r="62" spans="1:8" ht="12">
+      <c r="A62" s="5" t="s">
+        <v>86</v>
+      </c>
+      <c r="B62" s="5"/>
+      <c r="C62" s="5"/>
+      <c r="D62" s="6" t="s">
+        <v>87</v>
+      </c>
+      <c r="E62" s="5"/>
+      <c r="F62" s="5"/>
+      <c r="G62" s="5"/>
+    </row>
+    <row r="63" spans="1:8" ht="15">
       <c r="A63" s="15" t="s">
-        <v>139</v>
-      </c>
-      <c r="B63" s="18"/>
-      <c r="C63" s="18"/>
-      <c r="D63" s="18"/>
-      <c r="E63" s="18"/>
-      <c r="F63" s="18"/>
-      <c r="G63" s="18"/>
-    </row>
-    <row r="64" spans="1:9" ht="12.75" customHeight="1">
+        <v>116</v>
+      </c>
+      <c r="B63" s="15"/>
+      <c r="C63" s="15"/>
+      <c r="D63" s="15"/>
+      <c r="E63" s="15"/>
+      <c r="F63" s="15"/>
+      <c r="G63" s="15"/>
+    </row>
+    <row r="64" spans="1:8" ht="12">
       <c r="A64" t="s">
-        <v>239</v>
+        <v>234</v>
       </c>
       <c r="B64" t="s">
-        <v>67</v>
+        <v>11</v>
       </c>
       <c r="C64" t="s">
-        <v>69</v>
+        <v>12</v>
       </c>
       <c r="E64" t="s">
         <v>6</v>
@@ -2580,33 +3288,239 @@
       <c r="F64" s="12"/>
       <c r="G64" s="12"/>
     </row>
-    <row r="65" spans="1:7" ht="12.75" customHeight="1">
-      <c r="A65" s="2" t="s">
+    <row r="65" spans="1:9" ht="12">
+      <c r="A65" s="4" t="s">
+        <v>17</v>
+      </c>
+      <c r="B65" s="4"/>
+      <c r="C65" s="4"/>
+      <c r="D65" s="4"/>
+      <c r="E65" s="4"/>
+    </row>
+    <row r="66" spans="1:9" ht="12">
+      <c r="A66" s="4" t="s">
+        <v>18</v>
+      </c>
+      <c r="B66" s="4" t="s">
+        <v>19</v>
+      </c>
+      <c r="C66" s="4" t="s">
+        <v>20</v>
+      </c>
+      <c r="D66" s="4"/>
+      <c r="E66" s="4"/>
+    </row>
+    <row r="67" spans="1:9" ht="36">
+      <c r="A67" s="4" t="s">
         <v>13</v>
       </c>
-      <c r="B65" s="12"/>
-      <c r="C65" s="12" t="s">
+      <c r="B67" s="4"/>
+      <c r="C67" s="4" t="s">
+        <v>21</v>
+      </c>
+      <c r="D67" s="4" t="s">
+        <v>22</v>
+      </c>
+      <c r="E67" s="4"/>
+    </row>
+    <row r="68" spans="1:9" ht="12">
+      <c r="A68" s="4" t="s">
+        <v>18</v>
+      </c>
+      <c r="B68" s="4" t="s">
+        <v>23</v>
+      </c>
+      <c r="C68" s="4" t="s">
+        <v>24</v>
+      </c>
+      <c r="D68" s="4"/>
+      <c r="E68" s="4"/>
+    </row>
+    <row r="69" spans="1:9" ht="36">
+      <c r="A69" s="4" t="s">
+        <v>13</v>
+      </c>
+      <c r="B69" s="4"/>
+      <c r="C69" s="4" t="s">
+        <v>25</v>
+      </c>
+      <c r="D69" s="4" t="s">
+        <v>26</v>
+      </c>
+      <c r="E69" s="4"/>
+      <c r="H69" s="12"/>
+    </row>
+    <row r="70" spans="1:9" ht="12.75" customHeight="1">
+      <c r="A70" s="4" t="s">
+        <v>27</v>
+      </c>
+      <c r="B70" s="4"/>
+      <c r="C70" s="4"/>
+      <c r="D70" s="4"/>
+      <c r="E70" s="4"/>
+    </row>
+    <row r="71" spans="1:9" ht="12.75" customHeight="1">
+      <c r="A71" s="15" t="s">
+        <v>88</v>
+      </c>
+      <c r="B71" s="15"/>
+      <c r="C71" s="15"/>
+      <c r="D71" s="15"/>
+      <c r="E71" s="15"/>
+      <c r="F71" s="15"/>
+      <c r="G71" s="15"/>
+    </row>
+    <row r="72" spans="1:9" s="12" customFormat="1" ht="12.75" customHeight="1"/>
+    <row r="73" spans="1:9" s="14" customFormat="1" ht="12.75" customHeight="1">
+      <c r="A73" s="13" t="s">
+        <v>117</v>
+      </c>
+      <c r="D73" s="14" t="s">
+        <v>118</v>
+      </c>
+      <c r="H73" s="12"/>
+      <c r="I73" s="12"/>
+    </row>
+    <row r="74" spans="1:9" ht="12.75" customHeight="1">
+      <c r="A74" s="13" t="s">
+        <v>94</v>
+      </c>
+      <c r="B74" s="14"/>
+      <c r="C74" s="14"/>
+      <c r="D74" s="14" t="s">
+        <v>89</v>
+      </c>
+      <c r="E74" s="14"/>
+      <c r="F74" s="14"/>
+      <c r="G74" s="14"/>
+    </row>
+    <row r="75" spans="1:9" ht="12.75" customHeight="1">
+      <c r="A75" s="15" t="s">
+        <v>134</v>
+      </c>
+      <c r="B75" s="18"/>
+      <c r="C75" s="18"/>
+      <c r="D75" s="18"/>
+      <c r="E75" s="18"/>
+      <c r="F75" s="18"/>
+      <c r="G75" s="18"/>
+    </row>
+    <row r="76" spans="1:9" ht="12.75" customHeight="1">
+      <c r="A76" s="2" t="s">
+        <v>236</v>
+      </c>
+      <c r="B76" s="12" t="s">
+        <v>90</v>
+      </c>
+      <c r="C76" s="12" t="s">
+        <v>91</v>
+      </c>
+      <c r="D76" s="12"/>
+      <c r="E76" s="12" t="s">
+        <v>92</v>
+      </c>
+      <c r="F76" s="12"/>
+      <c r="G76" s="12"/>
+    </row>
+    <row r="77" spans="1:9" ht="12.75" customHeight="1">
+      <c r="A77" s="15" t="s">
+        <v>93</v>
+      </c>
+      <c r="B77" s="18"/>
+      <c r="C77" s="18"/>
+      <c r="D77" s="18"/>
+      <c r="E77" s="18"/>
+      <c r="F77" s="18"/>
+      <c r="G77" s="18"/>
+    </row>
+    <row r="78" spans="1:9" ht="12.75" customHeight="1">
+      <c r="B78" s="12"/>
+      <c r="C78" s="12"/>
+      <c r="D78" s="12"/>
+      <c r="E78" s="12"/>
+      <c r="F78" s="12"/>
+      <c r="G78" s="12"/>
+    </row>
+    <row r="79" spans="1:9" ht="12.75" customHeight="1">
+      <c r="A79" s="13" t="s">
+        <v>125</v>
+      </c>
+      <c r="B79" s="14"/>
+      <c r="C79" s="14"/>
+      <c r="D79" s="14" t="s">
+        <v>127</v>
+      </c>
+      <c r="E79" s="14"/>
+      <c r="F79" s="14"/>
+      <c r="G79" s="14"/>
+    </row>
+    <row r="80" spans="1:9" ht="12.75" customHeight="1">
+      <c r="A80" s="13" t="s">
+        <v>126</v>
+      </c>
+      <c r="B80" s="14"/>
+      <c r="C80" s="14"/>
+      <c r="D80" s="14" t="s">
+        <v>128</v>
+      </c>
+      <c r="E80" s="14"/>
+      <c r="F80" s="14"/>
+      <c r="G80" s="14"/>
+    </row>
+    <row r="81" spans="1:7" ht="12.75" customHeight="1">
+      <c r="A81" s="15" t="s">
+        <v>135</v>
+      </c>
+      <c r="B81" s="18"/>
+      <c r="C81" s="18"/>
+      <c r="D81" s="18"/>
+      <c r="E81" s="18"/>
+      <c r="F81" s="18"/>
+      <c r="G81" s="18"/>
+    </row>
+    <row r="82" spans="1:7" ht="12.75" customHeight="1">
+      <c r="A82" t="s">
+        <v>235</v>
+      </c>
+      <c r="B82" t="s">
+        <v>67</v>
+      </c>
+      <c r="C82" t="s">
+        <v>69</v>
+      </c>
+      <c r="E82" t="s">
+        <v>6</v>
+      </c>
+      <c r="F82" s="12"/>
+      <c r="G82" s="12"/>
+    </row>
+    <row r="83" spans="1:7" ht="12.75" customHeight="1">
+      <c r="A83" s="2" t="s">
+        <v>13</v>
+      </c>
+      <c r="B83" s="12"/>
+      <c r="C83" s="12" t="s">
         <v>66</v>
       </c>
-      <c r="D65" s="12"/>
-      <c r="E65" s="12"/>
-      <c r="F65" s="12"/>
-      <c r="G65" s="12"/>
-    </row>
-    <row r="66" spans="1:7" ht="12.75" customHeight="1">
-      <c r="A66" s="15" t="s">
-        <v>133</v>
-      </c>
-      <c r="B66" s="18"/>
-      <c r="C66" s="18"/>
-      <c r="D66" s="18"/>
-      <c r="E66" s="18"/>
-      <c r="F66" s="18"/>
-      <c r="G66" s="18"/>
-    </row>
-    <row r="69" spans="1:7" ht="12.75" customHeight="1">
-      <c r="A69" s="17" t="s">
-        <v>114</v>
+      <c r="D83" s="12"/>
+      <c r="E83" s="12"/>
+      <c r="F83" s="12"/>
+      <c r="G83" s="12"/>
+    </row>
+    <row r="84" spans="1:7" ht="12.75" customHeight="1">
+      <c r="A84" s="15" t="s">
+        <v>129</v>
+      </c>
+      <c r="B84" s="18"/>
+      <c r="C84" s="18"/>
+      <c r="D84" s="18"/>
+      <c r="E84" s="18"/>
+      <c r="F84" s="18"/>
+      <c r="G84" s="18"/>
+    </row>
+    <row r="87" spans="1:7" ht="12.75" customHeight="1">
+      <c r="A87" s="17" t="s">
+        <v>112</v>
       </c>
     </row>
   </sheetData>
@@ -2622,10 +3536,10 @@
 
 <file path=xl/worksheets/sheet2.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <dimension ref="A1:B12"/>
+  <dimension ref="A1:B20"/>
   <sheetViews>
     <sheetView zoomScale="150" zoomScaleNormal="150" zoomScalePageLayoutView="150" workbookViewId="0">
-      <selection activeCell="A10" sqref="A10"/>
+      <selection activeCell="B22" sqref="B22"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultColWidth="17.1640625" defaultRowHeight="12.75" customHeight="1" x14ac:dyDescent="0"/>
@@ -2675,58 +3589,122 @@
     </row>
     <row r="6" spans="1:2" ht="12" customHeight="1">
       <c r="A6" t="s">
-        <v>241</v>
+        <v>237</v>
       </c>
       <c r="B6" t="s">
-        <v>243</v>
+        <v>239</v>
       </c>
     </row>
     <row r="7" spans="1:2" ht="12" customHeight="1">
       <c r="A7" t="s">
-        <v>244</v>
+        <v>240</v>
       </c>
       <c r="B7" t="s">
-        <v>259</v>
+        <v>255</v>
       </c>
     </row>
     <row r="8" spans="1:2" ht="12" customHeight="1">
       <c r="A8" t="s">
-        <v>245</v>
+        <v>241</v>
       </c>
       <c r="B8" t="s">
-        <v>252</v>
+        <v>248</v>
       </c>
     </row>
     <row r="9" spans="1:2" ht="12" customHeight="1">
       <c r="A9" t="s">
-        <v>277</v>
+        <v>273</v>
       </c>
       <c r="B9" t="s">
-        <v>274</v>
+        <v>270</v>
       </c>
     </row>
     <row r="10" spans="1:2" ht="12" customHeight="1">
       <c r="A10" t="s">
-        <v>246</v>
+        <v>242</v>
       </c>
       <c r="B10" t="s">
-        <v>253</v>
+        <v>249</v>
       </c>
     </row>
     <row r="11" spans="1:2" ht="12" customHeight="1">
       <c r="A11" t="s">
-        <v>247</v>
+        <v>243</v>
       </c>
       <c r="B11" t="s">
-        <v>254</v>
+        <v>250</v>
       </c>
     </row>
     <row r="12" spans="1:2" ht="42" customHeight="1">
       <c r="A12" t="s">
-        <v>275</v>
+        <v>271</v>
       </c>
       <c r="B12" t="s">
-        <v>276</v>
+        <v>272</v>
+      </c>
+    </row>
+    <row r="13" spans="1:2" ht="12.75" customHeight="1">
+      <c r="A13" t="s">
+        <v>412</v>
+      </c>
+      <c r="B13" t="s">
+        <v>420</v>
+      </c>
+    </row>
+    <row r="14" spans="1:2" ht="12.75" customHeight="1">
+      <c r="A14" t="s">
+        <v>413</v>
+      </c>
+      <c r="B14" t="s">
+        <v>421</v>
+      </c>
+    </row>
+    <row r="15" spans="1:2" ht="12.75" customHeight="1">
+      <c r="A15" t="s">
+        <v>414</v>
+      </c>
+      <c r="B15" t="s">
+        <v>422</v>
+      </c>
+    </row>
+    <row r="16" spans="1:2" ht="12.75" customHeight="1">
+      <c r="A16" t="s">
+        <v>415</v>
+      </c>
+      <c r="B16" t="s">
+        <v>423</v>
+      </c>
+    </row>
+    <row r="17" spans="1:2" ht="12.75" customHeight="1">
+      <c r="A17" t="s">
+        <v>416</v>
+      </c>
+      <c r="B17" t="s">
+        <v>424</v>
+      </c>
+    </row>
+    <row r="18" spans="1:2" ht="12.75" customHeight="1">
+      <c r="A18" t="s">
+        <v>417</v>
+      </c>
+      <c r="B18" t="s">
+        <v>425</v>
+      </c>
+    </row>
+    <row r="19" spans="1:2" ht="12.75" customHeight="1">
+      <c r="A19" t="s">
+        <v>418</v>
+      </c>
+      <c r="B19" t="s">
+        <v>419</v>
+      </c>
+    </row>
+    <row r="20" spans="1:2" ht="12.75" customHeight="1">
+      <c r="A20" t="s">
+        <v>429</v>
+      </c>
+      <c r="B20" t="s">
+        <v>430</v>
       </c>
     </row>
   </sheetData>
@@ -2742,10 +3720,10 @@
 
 <file path=xl/worksheets/sheet3.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <dimension ref="A1:D78"/>
+  <dimension ref="A1:D134"/>
   <sheetViews>
-    <sheetView workbookViewId="0">
-      <selection activeCell="A63" sqref="A63"/>
+    <sheetView tabSelected="1" topLeftCell="A31" workbookViewId="0">
+      <selection activeCell="A42" sqref="A42:XFD42"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultColWidth="17.1640625" defaultRowHeight="12.75" customHeight="1" x14ac:dyDescent="0"/>
@@ -2817,10 +3795,10 @@
         <v>4</v>
       </c>
       <c r="B6" t="s">
-        <v>103</v>
+        <v>101</v>
       </c>
       <c r="C6" t="s">
-        <v>93</v>
+        <v>91</v>
       </c>
     </row>
     <row r="9" spans="1:4" ht="12.75" customHeight="1">
@@ -2872,10 +3850,10 @@
         <v>7</v>
       </c>
       <c r="B14" t="s">
-        <v>106</v>
+        <v>104</v>
       </c>
       <c r="C14" t="s">
-        <v>107</v>
+        <v>105</v>
       </c>
     </row>
     <row r="15" spans="1:4" ht="12.75" customHeight="1">
@@ -2883,10 +3861,10 @@
         <v>7</v>
       </c>
       <c r="B15" t="s">
-        <v>104</v>
+        <v>102</v>
       </c>
       <c r="C15" t="s">
-        <v>105</v>
+        <v>103</v>
       </c>
     </row>
     <row r="16" spans="1:4" ht="12.75" customHeight="1">
@@ -2894,10 +3872,10 @@
         <v>7</v>
       </c>
       <c r="B16" t="s">
-        <v>140</v>
+        <v>136</v>
       </c>
       <c r="C16" t="s">
-        <v>86</v>
+        <v>84</v>
       </c>
     </row>
     <row r="18" spans="1:3" ht="12.75" customHeight="1">
@@ -2924,35 +3902,35 @@
     </row>
     <row r="21" spans="1:3" ht="12.75" customHeight="1">
       <c r="A21" t="s">
-        <v>92</v>
+        <v>90</v>
       </c>
       <c r="B21" t="s">
-        <v>97</v>
+        <v>95</v>
       </c>
       <c r="C21" t="s">
-        <v>98</v>
+        <v>96</v>
       </c>
     </row>
     <row r="22" spans="1:3" ht="12.75" customHeight="1">
       <c r="A22" t="s">
-        <v>92</v>
+        <v>90</v>
       </c>
       <c r="B22" t="s">
-        <v>99</v>
+        <v>97</v>
       </c>
       <c r="C22" t="s">
-        <v>100</v>
+        <v>98</v>
       </c>
     </row>
     <row r="23" spans="1:3" ht="12.75" customHeight="1">
       <c r="A23" t="s">
-        <v>92</v>
+        <v>90</v>
       </c>
       <c r="B23" t="s">
-        <v>101</v>
+        <v>99</v>
       </c>
       <c r="C23" t="s">
-        <v>102</v>
+        <v>100</v>
       </c>
     </row>
     <row r="25" spans="1:3" ht="12.75" customHeight="1">
@@ -2960,10 +3938,10 @@
         <v>67</v>
       </c>
       <c r="B25" t="s">
-        <v>123</v>
+        <v>119</v>
       </c>
       <c r="C25" t="s">
-        <v>124</v>
+        <v>120</v>
       </c>
     </row>
     <row r="26" spans="1:3" ht="12.75" customHeight="1">
@@ -2971,10 +3949,10 @@
         <v>67</v>
       </c>
       <c r="B26" t="s">
-        <v>125</v>
+        <v>121</v>
       </c>
       <c r="C26" t="s">
-        <v>127</v>
+        <v>123</v>
       </c>
     </row>
     <row r="27" spans="1:3" ht="12.75" customHeight="1">
@@ -2982,10 +3960,10 @@
         <v>67</v>
       </c>
       <c r="B27" t="s">
-        <v>126</v>
+        <v>122</v>
       </c>
       <c r="C27" t="s">
-        <v>128</v>
+        <v>124</v>
       </c>
     </row>
     <row r="29" spans="1:3" ht="12.75" customHeight="1">
@@ -3012,172 +3990,161 @@
     </row>
     <row r="32" spans="1:3" ht="12.75" customHeight="1">
       <c r="A32" t="s">
-        <v>142</v>
+        <v>277</v>
       </c>
       <c r="B32" t="s">
-        <v>143</v>
+        <v>284</v>
       </c>
       <c r="C32" t="s">
-        <v>149</v>
+        <v>285</v>
       </c>
     </row>
     <row r="33" spans="1:4" ht="12.75" customHeight="1">
       <c r="A33" t="s">
-        <v>142</v>
+        <v>277</v>
       </c>
       <c r="B33" t="s">
-        <v>144</v>
+        <v>286</v>
       </c>
       <c r="C33" t="s">
-        <v>150</v>
+        <v>287</v>
       </c>
     </row>
     <row r="34" spans="1:4" ht="12.75" customHeight="1">
       <c r="A34" t="s">
-        <v>142</v>
+        <v>277</v>
       </c>
       <c r="B34" t="s">
-        <v>145</v>
+        <v>426</v>
       </c>
       <c r="C34" t="s">
-        <v>151</v>
-      </c>
-    </row>
-    <row r="35" spans="1:4" ht="12.75" customHeight="1">
-      <c r="A35" t="s">
-        <v>142</v>
-      </c>
-      <c r="B35" t="s">
-        <v>146</v>
-      </c>
-      <c r="C35" t="s">
-        <v>152</v>
+        <v>402</v>
       </c>
     </row>
     <row r="36" spans="1:4" ht="12.75" customHeight="1">
       <c r="A36" t="s">
-        <v>142</v>
+        <v>138</v>
       </c>
       <c r="B36" t="s">
-        <v>147</v>
+        <v>139</v>
       </c>
       <c r="C36" t="s">
-        <v>153</v>
+        <v>145</v>
       </c>
     </row>
     <row r="37" spans="1:4" ht="12.75" customHeight="1">
       <c r="A37" t="s">
-        <v>142</v>
+        <v>138</v>
       </c>
       <c r="B37" t="s">
-        <v>148</v>
+        <v>140</v>
       </c>
       <c r="C37" t="s">
-        <v>154</v>
+        <v>146</v>
+      </c>
+    </row>
+    <row r="38" spans="1:4" ht="12.75" customHeight="1">
+      <c r="A38" t="s">
+        <v>138</v>
+      </c>
+      <c r="B38" t="s">
+        <v>141</v>
+      </c>
+      <c r="C38" t="s">
+        <v>147</v>
       </c>
     </row>
     <row r="39" spans="1:4" ht="12.75" customHeight="1">
       <c r="A39" t="s">
-        <v>156</v>
+        <v>138</v>
       </c>
       <c r="B39" t="s">
-        <v>163</v>
-      </c>
-      <c r="D39" t="s">
-        <v>164</v>
+        <v>142</v>
+      </c>
+      <c r="C39" t="s">
+        <v>148</v>
       </c>
     </row>
     <row r="40" spans="1:4" ht="12.75" customHeight="1">
       <c r="A40" t="s">
-        <v>156</v>
+        <v>138</v>
       </c>
       <c r="B40" t="s">
-        <v>165</v>
-      </c>
-      <c r="D40" t="s">
-        <v>169</v>
+        <v>143</v>
+      </c>
+      <c r="C40" t="s">
+        <v>149</v>
       </c>
     </row>
     <row r="41" spans="1:4" ht="12.75" customHeight="1">
       <c r="A41" t="s">
-        <v>156</v>
+        <v>138</v>
       </c>
       <c r="B41" t="s">
-        <v>166</v>
-      </c>
-      <c r="D41" t="s">
-        <v>170</v>
-      </c>
-    </row>
-    <row r="42" spans="1:4" ht="12.75" customHeight="1">
-      <c r="A42" t="s">
-        <v>156</v>
-      </c>
-      <c r="B42" t="s">
-        <v>167</v>
-      </c>
-      <c r="D42" t="s">
-        <v>171</v>
+        <v>144</v>
+      </c>
+      <c r="C41" t="s">
+        <v>150</v>
       </c>
     </row>
     <row r="43" spans="1:4" ht="12.75" customHeight="1">
       <c r="A43" t="s">
-        <v>156</v>
+        <v>152</v>
       </c>
       <c r="B43" t="s">
-        <v>168</v>
+        <v>159</v>
       </c>
       <c r="D43" t="s">
-        <v>172</v>
+        <v>160</v>
+      </c>
+    </row>
+    <row r="44" spans="1:4" ht="12.75" customHeight="1">
+      <c r="A44" t="s">
+        <v>152</v>
+      </c>
+      <c r="B44" t="s">
+        <v>161</v>
+      </c>
+      <c r="D44" t="s">
+        <v>165</v>
       </c>
     </row>
     <row r="45" spans="1:4" ht="12.75" customHeight="1">
       <c r="A45" t="s">
-        <v>160</v>
+        <v>152</v>
       </c>
       <c r="B45" t="s">
-        <v>196</v>
+        <v>162</v>
       </c>
       <c r="D45" t="s">
-        <v>197</v>
-      </c>
-    </row>
-    <row r="46" spans="1:4" s="2" customFormat="1" ht="12.75" customHeight="1">
+        <v>166</v>
+      </c>
+    </row>
+    <row r="46" spans="1:4" ht="12.75" customHeight="1">
       <c r="A46" t="s">
-        <v>160</v>
+        <v>152</v>
       </c>
       <c r="B46" t="s">
-        <v>186</v>
+        <v>163</v>
       </c>
       <c r="D46" t="s">
-        <v>187</v>
+        <v>167</v>
       </c>
     </row>
     <row r="47" spans="1:4" ht="12.75" customHeight="1">
       <c r="A47" t="s">
-        <v>160</v>
+        <v>152</v>
       </c>
       <c r="B47" t="s">
-        <v>188</v>
+        <v>164</v>
       </c>
       <c r="D47" t="s">
-        <v>189</v>
-      </c>
-    </row>
-    <row r="48" spans="1:4" ht="12.75" customHeight="1">
-      <c r="A48" t="s">
-        <v>160</v>
-      </c>
-      <c r="B48" t="s">
-        <v>190</v>
-      </c>
-      <c r="D48" t="s">
-        <v>191</v>
+        <v>168</v>
       </c>
     </row>
     <row r="49" spans="1:4" ht="12.75" customHeight="1">
       <c r="A49" t="s">
-        <v>160</v>
+        <v>156</v>
       </c>
       <c r="B49" t="s">
         <v>192</v>
@@ -3186,283 +4153,822 @@
         <v>193</v>
       </c>
     </row>
-    <row r="50" spans="1:4" ht="12.75" customHeight="1">
+    <row r="50" spans="1:4" s="2" customFormat="1" ht="12.75" customHeight="1">
       <c r="A50" t="s">
-        <v>160</v>
+        <v>156</v>
       </c>
       <c r="B50" t="s">
-        <v>194</v>
+        <v>182</v>
       </c>
       <c r="D50" t="s">
-        <v>195</v>
+        <v>183</v>
+      </c>
+    </row>
+    <row r="51" spans="1:4" ht="12.75" customHeight="1">
+      <c r="A51" t="s">
+        <v>156</v>
+      </c>
+      <c r="B51" t="s">
+        <v>184</v>
+      </c>
+      <c r="D51" t="s">
+        <v>185</v>
       </c>
     </row>
     <row r="52" spans="1:4" ht="12.75" customHeight="1">
       <c r="A52" t="s">
-        <v>177</v>
+        <v>156</v>
       </c>
       <c r="B52" t="s">
-        <v>198</v>
-      </c>
-      <c r="C52" s="2"/>
+        <v>186</v>
+      </c>
       <c r="D52" t="s">
-        <v>199</v>
+        <v>187</v>
       </c>
     </row>
     <row r="53" spans="1:4" ht="12.75" customHeight="1">
       <c r="A53" t="s">
-        <v>177</v>
+        <v>156</v>
       </c>
       <c r="B53" t="s">
-        <v>200</v>
+        <v>188</v>
       </c>
       <c r="D53" t="s">
-        <v>201</v>
+        <v>189</v>
       </c>
     </row>
     <row r="54" spans="1:4" ht="12.75" customHeight="1">
       <c r="A54" t="s">
-        <v>177</v>
+        <v>156</v>
       </c>
       <c r="B54" t="s">
-        <v>202</v>
+        <v>190</v>
       </c>
       <c r="D54" t="s">
-        <v>203</v>
-      </c>
-    </row>
-    <row r="55" spans="1:4" ht="12.75" customHeight="1">
-      <c r="A55" t="s">
-        <v>177</v>
-      </c>
-      <c r="B55" t="s">
-        <v>204</v>
-      </c>
-      <c r="D55" t="s">
-        <v>205</v>
+        <v>191</v>
       </c>
     </row>
     <row r="56" spans="1:4" ht="12.75" customHeight="1">
       <c r="A56" t="s">
-        <v>177</v>
+        <v>173</v>
       </c>
       <c r="B56" t="s">
-        <v>206</v>
-      </c>
+        <v>194</v>
+      </c>
+      <c r="C56" s="2"/>
       <c r="D56" t="s">
-        <v>207</v>
+        <v>195</v>
+      </c>
+    </row>
+    <row r="57" spans="1:4" ht="12.75" customHeight="1">
+      <c r="A57" t="s">
+        <v>173</v>
+      </c>
+      <c r="B57" t="s">
+        <v>196</v>
+      </c>
+      <c r="D57" t="s">
+        <v>197</v>
       </c>
     </row>
     <row r="58" spans="1:4" ht="12.75" customHeight="1">
       <c r="A58" t="s">
-        <v>249</v>
+        <v>173</v>
       </c>
       <c r="B58" t="s">
-        <v>267</v>
+        <v>198</v>
       </c>
       <c r="D58" t="s">
-        <v>260</v>
+        <v>199</v>
       </c>
     </row>
     <row r="59" spans="1:4" ht="12.75" customHeight="1">
       <c r="A59" t="s">
-        <v>249</v>
+        <v>173</v>
       </c>
       <c r="B59" t="s">
-        <v>268</v>
-      </c>
-      <c r="C59" s="2"/>
+        <v>200</v>
+      </c>
       <c r="D59" t="s">
-        <v>261</v>
+        <v>201</v>
       </c>
     </row>
     <row r="60" spans="1:4" ht="12.75" customHeight="1">
       <c r="A60" t="s">
-        <v>249</v>
+        <v>173</v>
       </c>
       <c r="B60" t="s">
-        <v>269</v>
+        <v>202</v>
       </c>
       <c r="D60" t="s">
-        <v>262</v>
-      </c>
-    </row>
-    <row r="61" spans="1:4" ht="12.75" customHeight="1">
-      <c r="A61" t="s">
-        <v>249</v>
-      </c>
-      <c r="B61" t="s">
-        <v>270</v>
-      </c>
-      <c r="D61" t="s">
-        <v>263</v>
+        <v>203</v>
       </c>
     </row>
     <row r="62" spans="1:4" ht="12.75" customHeight="1">
       <c r="A62" t="s">
-        <v>249</v>
+        <v>245</v>
       </c>
       <c r="B62" t="s">
-        <v>271</v>
+        <v>263</v>
       </c>
       <c r="D62" t="s">
-        <v>264</v>
+        <v>256</v>
       </c>
     </row>
     <row r="63" spans="1:4" ht="12.75" customHeight="1">
       <c r="A63" t="s">
-        <v>249</v>
+        <v>245</v>
       </c>
       <c r="B63" t="s">
-        <v>272</v>
-      </c>
+        <v>264</v>
+      </c>
+      <c r="C63" s="2"/>
       <c r="D63" t="s">
-        <v>265</v>
+        <v>257</v>
       </c>
     </row>
     <row r="64" spans="1:4" ht="12.75" customHeight="1">
       <c r="A64" t="s">
-        <v>249</v>
+        <v>245</v>
       </c>
       <c r="B64" t="s">
-        <v>273</v>
+        <v>265</v>
       </c>
       <c r="D64" t="s">
+        <v>258</v>
+      </c>
+    </row>
+    <row r="65" spans="1:4" ht="12.75" customHeight="1">
+      <c r="A65" t="s">
+        <v>245</v>
+      </c>
+      <c r="B65" t="s">
         <v>266</v>
+      </c>
+      <c r="D65" t="s">
+        <v>259</v>
       </c>
     </row>
     <row r="66" spans="1:4" ht="12.75" customHeight="1">
       <c r="A66" t="s">
-        <v>181</v>
+        <v>245</v>
       </c>
       <c r="B66" t="s">
-        <v>208</v>
+        <v>267</v>
       </c>
       <c r="D66" t="s">
-        <v>209</v>
+        <v>260</v>
       </c>
     </row>
     <row r="67" spans="1:4" ht="12.75" customHeight="1">
       <c r="A67" t="s">
-        <v>181</v>
+        <v>245</v>
       </c>
       <c r="B67" t="s">
-        <v>210</v>
-      </c>
-      <c r="C67" s="2"/>
+        <v>268</v>
+      </c>
       <c r="D67" t="s">
-        <v>211</v>
+        <v>261</v>
       </c>
     </row>
     <row r="68" spans="1:4" ht="12.75" customHeight="1">
       <c r="A68" t="s">
-        <v>181</v>
+        <v>245</v>
       </c>
       <c r="B68" t="s">
-        <v>212</v>
+        <v>269</v>
       </c>
       <c r="D68" t="s">
-        <v>213</v>
-      </c>
-    </row>
-    <row r="69" spans="1:4" ht="12.75" customHeight="1">
-      <c r="A69" t="s">
-        <v>181</v>
-      </c>
-      <c r="B69" t="s">
-        <v>214</v>
-      </c>
-      <c r="D69" t="s">
-        <v>215</v>
+        <v>262</v>
       </c>
     </row>
     <row r="70" spans="1:4" ht="12.75" customHeight="1">
       <c r="A70" t="s">
-        <v>181</v>
+        <v>177</v>
       </c>
       <c r="B70" t="s">
-        <v>216</v>
+        <v>204</v>
       </c>
       <c r="D70" t="s">
-        <v>217</v>
+        <v>205</v>
       </c>
     </row>
     <row r="71" spans="1:4" ht="12.75" customHeight="1">
       <c r="A71" t="s">
-        <v>181</v>
+        <v>177</v>
       </c>
       <c r="B71" t="s">
-        <v>218</v>
-      </c>
+        <v>206</v>
+      </c>
+      <c r="C71" s="2"/>
       <c r="D71" t="s">
-        <v>219</v>
+        <v>207</v>
+      </c>
+    </row>
+    <row r="72" spans="1:4" ht="12.75" customHeight="1">
+      <c r="A72" t="s">
+        <v>177</v>
+      </c>
+      <c r="B72" t="s">
+        <v>208</v>
+      </c>
+      <c r="D72" t="s">
+        <v>209</v>
       </c>
     </row>
     <row r="73" spans="1:4" ht="12.75" customHeight="1">
       <c r="A73" t="s">
-        <v>184</v>
+        <v>177</v>
       </c>
       <c r="B73" t="s">
-        <v>220</v>
+        <v>210</v>
       </c>
       <c r="D73" t="s">
-        <v>221</v>
+        <v>211</v>
       </c>
     </row>
     <row r="74" spans="1:4" ht="12.75" customHeight="1">
       <c r="A74" t="s">
-        <v>184</v>
+        <v>177</v>
       </c>
       <c r="B74" t="s">
-        <v>222</v>
-      </c>
-      <c r="C74" s="2"/>
+        <v>212</v>
+      </c>
       <c r="D74" t="s">
-        <v>223</v>
+        <v>213</v>
       </c>
     </row>
     <row r="75" spans="1:4" ht="12.75" customHeight="1">
       <c r="A75" t="s">
-        <v>184</v>
+        <v>177</v>
       </c>
       <c r="B75" t="s">
-        <v>224</v>
+        <v>214</v>
       </c>
       <c r="D75" t="s">
-        <v>225</v>
-      </c>
-    </row>
-    <row r="76" spans="1:4" ht="12.75" customHeight="1">
-      <c r="A76" t="s">
-        <v>184</v>
-      </c>
-      <c r="B76" t="s">
-        <v>226</v>
-      </c>
-      <c r="D76" t="s">
-        <v>227</v>
+        <v>215</v>
       </c>
     </row>
     <row r="77" spans="1:4" ht="12.75" customHeight="1">
       <c r="A77" t="s">
-        <v>184</v>
+        <v>180</v>
       </c>
       <c r="B77" t="s">
-        <v>228</v>
+        <v>216</v>
       </c>
       <c r="D77" t="s">
-        <v>229</v>
+        <v>217</v>
       </c>
     </row>
     <row r="78" spans="1:4" ht="12.75" customHeight="1">
       <c r="A78" t="s">
-        <v>184</v>
+        <v>180</v>
       </c>
       <c r="B78" t="s">
-        <v>230</v>
-      </c>
+        <v>218</v>
+      </c>
+      <c r="C78" s="2"/>
       <c r="D78" t="s">
-        <v>231</v>
+        <v>219</v>
+      </c>
+    </row>
+    <row r="79" spans="1:4" ht="12.75" customHeight="1">
+      <c r="A79" t="s">
+        <v>180</v>
+      </c>
+      <c r="B79" t="s">
+        <v>220</v>
+      </c>
+      <c r="D79" t="s">
+        <v>221</v>
+      </c>
+    </row>
+    <row r="80" spans="1:4" ht="12.75" customHeight="1">
+      <c r="A80" t="s">
+        <v>180</v>
+      </c>
+      <c r="B80" t="s">
+        <v>222</v>
+      </c>
+      <c r="D80" t="s">
+        <v>223</v>
+      </c>
+    </row>
+    <row r="81" spans="1:4" ht="12.75" customHeight="1">
+      <c r="A81" t="s">
+        <v>180</v>
+      </c>
+      <c r="B81" t="s">
+        <v>224</v>
+      </c>
+      <c r="D81" t="s">
+        <v>225</v>
+      </c>
+    </row>
+    <row r="82" spans="1:4" ht="12.75" customHeight="1">
+      <c r="A82" t="s">
+        <v>180</v>
+      </c>
+      <c r="B82" t="s">
+        <v>226</v>
+      </c>
+      <c r="D82" t="s">
+        <v>227</v>
+      </c>
+    </row>
+    <row r="84" spans="1:4" ht="12.75" customHeight="1">
+      <c r="A84" t="s">
+        <v>281</v>
+      </c>
+      <c r="B84" t="s">
+        <v>288</v>
+      </c>
+      <c r="C84" t="s">
+        <v>306</v>
+      </c>
+    </row>
+    <row r="85" spans="1:4" ht="12.75" customHeight="1">
+      <c r="A85" t="s">
+        <v>281</v>
+      </c>
+      <c r="B85" t="s">
+        <v>291</v>
+      </c>
+      <c r="C85" t="s">
+        <v>307</v>
+      </c>
+    </row>
+    <row r="86" spans="1:4" ht="12.75" customHeight="1">
+      <c r="A86" t="s">
+        <v>281</v>
+      </c>
+      <c r="B86" t="s">
+        <v>294</v>
+      </c>
+      <c r="C86" t="s">
+        <v>308</v>
+      </c>
+    </row>
+    <row r="87" spans="1:4" ht="12.75" customHeight="1">
+      <c r="A87" t="s">
+        <v>281</v>
+      </c>
+      <c r="B87" t="s">
+        <v>295</v>
+      </c>
+      <c r="C87" t="s">
+        <v>401</v>
+      </c>
+    </row>
+    <row r="88" spans="1:4" ht="12.75" customHeight="1">
+      <c r="A88" t="s">
+        <v>281</v>
+      </c>
+      <c r="B88" t="s">
+        <v>297</v>
+      </c>
+      <c r="C88" t="s">
+        <v>309</v>
+      </c>
+    </row>
+    <row r="89" spans="1:4" ht="12.75" customHeight="1">
+      <c r="A89" t="s">
+        <v>281</v>
+      </c>
+      <c r="B89" t="s">
+        <v>299</v>
+      </c>
+      <c r="C89" t="s">
+        <v>310</v>
+      </c>
+    </row>
+    <row r="91" spans="1:4" ht="12.75" customHeight="1">
+      <c r="A91" t="s">
+        <v>311</v>
+      </c>
+      <c r="B91" t="s">
+        <v>317</v>
+      </c>
+      <c r="C91" t="s">
+        <v>324</v>
+      </c>
+    </row>
+    <row r="92" spans="1:4" ht="12.75" customHeight="1">
+      <c r="A92" t="s">
+        <v>311</v>
+      </c>
+      <c r="B92" t="s">
+        <v>318</v>
+      </c>
+      <c r="C92" t="s">
+        <v>325</v>
+      </c>
+    </row>
+    <row r="93" spans="1:4" ht="12.75" customHeight="1">
+      <c r="A93" t="s">
+        <v>311</v>
+      </c>
+      <c r="B93" t="s">
+        <v>319</v>
+      </c>
+      <c r="C93" t="s">
+        <v>326</v>
+      </c>
+    </row>
+    <row r="94" spans="1:4" ht="12.75" customHeight="1">
+      <c r="A94" t="s">
+        <v>311</v>
+      </c>
+      <c r="B94" t="s">
+        <v>320</v>
+      </c>
+      <c r="C94" t="s">
+        <v>327</v>
+      </c>
+    </row>
+    <row r="95" spans="1:4" ht="12.75" customHeight="1">
+      <c r="A95" t="s">
+        <v>311</v>
+      </c>
+      <c r="B95" t="s">
+        <v>321</v>
+      </c>
+      <c r="C95" t="s">
+        <v>328</v>
+      </c>
+    </row>
+    <row r="96" spans="1:4" ht="12.75" customHeight="1">
+      <c r="A96" t="s">
+        <v>311</v>
+      </c>
+      <c r="B96" t="s">
+        <v>322</v>
+      </c>
+      <c r="C96" t="s">
+        <v>329</v>
+      </c>
+    </row>
+    <row r="97" spans="1:3" ht="12.75" customHeight="1">
+      <c r="A97" t="s">
+        <v>311</v>
+      </c>
+      <c r="B97" t="s">
+        <v>323</v>
+      </c>
+      <c r="C97" t="s">
+        <v>330</v>
+      </c>
+    </row>
+    <row r="99" spans="1:3" ht="12.75" customHeight="1">
+      <c r="A99" t="s">
+        <v>312</v>
+      </c>
+      <c r="B99" t="s">
+        <v>337</v>
+      </c>
+      <c r="C99" t="s">
+        <v>343</v>
+      </c>
+    </row>
+    <row r="100" spans="1:3" ht="12.75" customHeight="1">
+      <c r="A100" t="s">
+        <v>312</v>
+      </c>
+      <c r="B100" t="s">
+        <v>338</v>
+      </c>
+      <c r="C100" t="s">
+        <v>344</v>
+      </c>
+    </row>
+    <row r="101" spans="1:3" ht="12.75" customHeight="1">
+      <c r="A101" t="s">
+        <v>312</v>
+      </c>
+      <c r="B101" t="s">
+        <v>339</v>
+      </c>
+      <c r="C101" t="s">
+        <v>345</v>
+      </c>
+    </row>
+    <row r="102" spans="1:3" ht="12.75" customHeight="1">
+      <c r="A102" t="s">
+        <v>312</v>
+      </c>
+      <c r="B102" t="s">
+        <v>340</v>
+      </c>
+      <c r="C102" t="s">
+        <v>346</v>
+      </c>
+    </row>
+    <row r="103" spans="1:3" ht="12.75" customHeight="1">
+      <c r="A103" t="s">
+        <v>312</v>
+      </c>
+      <c r="B103" t="s">
+        <v>341</v>
+      </c>
+      <c r="C103" t="s">
+        <v>347</v>
+      </c>
+    </row>
+    <row r="104" spans="1:3" ht="12.75" customHeight="1">
+      <c r="A104" t="s">
+        <v>312</v>
+      </c>
+      <c r="B104" t="s">
+        <v>342</v>
+      </c>
+      <c r="C104" t="s">
+        <v>348</v>
+      </c>
+    </row>
+    <row r="106" spans="1:3" ht="12.75" customHeight="1">
+      <c r="A106" t="s">
+        <v>313</v>
+      </c>
+      <c r="B106" t="s">
+        <v>355</v>
+      </c>
+      <c r="C106" t="s">
+        <v>356</v>
+      </c>
+    </row>
+    <row r="107" spans="1:3" ht="12.75" customHeight="1">
+      <c r="A107" t="s">
+        <v>313</v>
+      </c>
+      <c r="B107" t="s">
+        <v>349</v>
+      </c>
+      <c r="C107" t="s">
+        <v>357</v>
+      </c>
+    </row>
+    <row r="108" spans="1:3" ht="12.75" customHeight="1">
+      <c r="A108" t="s">
+        <v>313</v>
+      </c>
+      <c r="B108" t="s">
+        <v>350</v>
+      </c>
+      <c r="C108" t="s">
+        <v>358</v>
+      </c>
+    </row>
+    <row r="109" spans="1:3" ht="12.75" customHeight="1">
+      <c r="A109" t="s">
+        <v>313</v>
+      </c>
+      <c r="B109" t="s">
+        <v>351</v>
+      </c>
+      <c r="C109" t="s">
+        <v>359</v>
+      </c>
+    </row>
+    <row r="110" spans="1:3" ht="12.75" customHeight="1">
+      <c r="A110" t="s">
+        <v>313</v>
+      </c>
+      <c r="B110" t="s">
+        <v>352</v>
+      </c>
+      <c r="C110" t="s">
+        <v>360</v>
+      </c>
+    </row>
+    <row r="111" spans="1:3" ht="12.75" customHeight="1">
+      <c r="A111" t="s">
+        <v>313</v>
+      </c>
+      <c r="B111" t="s">
+        <v>353</v>
+      </c>
+      <c r="C111" t="s">
+        <v>361</v>
+      </c>
+    </row>
+    <row r="112" spans="1:3" ht="12.75" customHeight="1">
+      <c r="A112" t="s">
+        <v>313</v>
+      </c>
+      <c r="B112" t="s">
+        <v>354</v>
+      </c>
+      <c r="C112" t="s">
+        <v>362</v>
+      </c>
+    </row>
+    <row r="114" spans="1:3" ht="12.75" customHeight="1">
+      <c r="A114" t="s">
+        <v>314</v>
+      </c>
+      <c r="B114" t="s">
+        <v>363</v>
+      </c>
+      <c r="C114" t="s">
+        <v>369</v>
+      </c>
+    </row>
+    <row r="115" spans="1:3" ht="12.75" customHeight="1">
+      <c r="A115" t="s">
+        <v>314</v>
+      </c>
+      <c r="B115" t="s">
+        <v>364</v>
+      </c>
+      <c r="C115" t="s">
+        <v>370</v>
+      </c>
+    </row>
+    <row r="116" spans="1:3" ht="12.75" customHeight="1">
+      <c r="A116" t="s">
+        <v>314</v>
+      </c>
+      <c r="B116" t="s">
+        <v>365</v>
+      </c>
+      <c r="C116" t="s">
+        <v>371</v>
+      </c>
+    </row>
+    <row r="117" spans="1:3" ht="12.75" customHeight="1">
+      <c r="A117" t="s">
+        <v>314</v>
+      </c>
+      <c r="B117" t="s">
+        <v>366</v>
+      </c>
+      <c r="C117" t="s">
+        <v>372</v>
+      </c>
+    </row>
+    <row r="118" spans="1:3" ht="12.75" customHeight="1">
+      <c r="A118" t="s">
+        <v>314</v>
+      </c>
+      <c r="B118" t="s">
+        <v>367</v>
+      </c>
+      <c r="C118" t="s">
+        <v>373</v>
+      </c>
+    </row>
+    <row r="119" spans="1:3" ht="12.75" customHeight="1">
+      <c r="A119" t="s">
+        <v>314</v>
+      </c>
+      <c r="B119" t="s">
+        <v>368</v>
+      </c>
+      <c r="C119" t="s">
+        <v>374</v>
+      </c>
+    </row>
+    <row r="121" spans="1:3" ht="12.75" customHeight="1">
+      <c r="A121" t="s">
+        <v>315</v>
+      </c>
+      <c r="B121" t="s">
+        <v>381</v>
+      </c>
+      <c r="C121" t="s">
+        <v>382</v>
+      </c>
+    </row>
+    <row r="122" spans="1:3" ht="12.75" customHeight="1">
+      <c r="A122" t="s">
+        <v>315</v>
+      </c>
+      <c r="B122" t="s">
+        <v>375</v>
+      </c>
+      <c r="C122" t="s">
+        <v>383</v>
+      </c>
+    </row>
+    <row r="123" spans="1:3" ht="12.75" customHeight="1">
+      <c r="A123" t="s">
+        <v>315</v>
+      </c>
+      <c r="B123" t="s">
+        <v>376</v>
+      </c>
+      <c r="C123" t="s">
+        <v>384</v>
+      </c>
+    </row>
+    <row r="124" spans="1:3" ht="12.75" customHeight="1">
+      <c r="A124" t="s">
+        <v>315</v>
+      </c>
+      <c r="B124" t="s">
+        <v>378</v>
+      </c>
+      <c r="C124" t="s">
+        <v>385</v>
+      </c>
+    </row>
+    <row r="125" spans="1:3" ht="12.75" customHeight="1">
+      <c r="A125" t="s">
+        <v>315</v>
+      </c>
+      <c r="B125" t="s">
+        <v>377</v>
+      </c>
+      <c r="C125" t="s">
+        <v>386</v>
+      </c>
+    </row>
+    <row r="126" spans="1:3" ht="12.75" customHeight="1">
+      <c r="A126" t="s">
+        <v>315</v>
+      </c>
+      <c r="B126" t="s">
+        <v>379</v>
+      </c>
+      <c r="C126" t="s">
+        <v>387</v>
+      </c>
+    </row>
+    <row r="127" spans="1:3" ht="12.75" customHeight="1">
+      <c r="A127" t="s">
+        <v>315</v>
+      </c>
+      <c r="B127" t="s">
+        <v>380</v>
+      </c>
+      <c r="C127" t="s">
+        <v>388</v>
+      </c>
+    </row>
+    <row r="129" spans="1:3" ht="12.75" customHeight="1">
+      <c r="A129" t="s">
+        <v>316</v>
+      </c>
+      <c r="B129" t="s">
+        <v>389</v>
+      </c>
+      <c r="C129" t="s">
+        <v>395</v>
+      </c>
+    </row>
+    <row r="130" spans="1:3" ht="12.75" customHeight="1">
+      <c r="A130" t="s">
+        <v>316</v>
+      </c>
+      <c r="B130" t="s">
+        <v>390</v>
+      </c>
+      <c r="C130" t="s">
+        <v>396</v>
+      </c>
+    </row>
+    <row r="131" spans="1:3" ht="12.75" customHeight="1">
+      <c r="A131" t="s">
+        <v>316</v>
+      </c>
+      <c r="B131" t="s">
+        <v>391</v>
+      </c>
+      <c r="C131" t="s">
+        <v>397</v>
+      </c>
+    </row>
+    <row r="132" spans="1:3" ht="12.75" customHeight="1">
+      <c r="A132" t="s">
+        <v>316</v>
+      </c>
+      <c r="B132" t="s">
+        <v>392</v>
+      </c>
+      <c r="C132" t="s">
+        <v>398</v>
+      </c>
+    </row>
+    <row r="133" spans="1:3" ht="12.75" customHeight="1">
+      <c r="A133" t="s">
+        <v>316</v>
+      </c>
+      <c r="B133" t="s">
+        <v>393</v>
+      </c>
+      <c r="C133" t="s">
+        <v>399</v>
+      </c>
+    </row>
+    <row r="134" spans="1:3" ht="12.75" customHeight="1">
+      <c r="A134" t="s">
+        <v>316</v>
+      </c>
+      <c r="B134" t="s">
+        <v>394</v>
+      </c>
+      <c r="C134" t="s">
+        <v>400</v>
       </c>
     </row>
   </sheetData>
@@ -3533,15 +5039,15 @@
         <v>1</v>
       </c>
       <c r="B1" t="s">
-        <v>173</v>
+        <v>169</v>
       </c>
     </row>
     <row r="2" spans="1:2">
       <c r="A2" t="s">
-        <v>174</v>
+        <v>170</v>
       </c>
       <c r="B2" t="s">
-        <v>175</v>
+        <v>171</v>
       </c>
     </row>
     <row r="3" spans="1:2">
@@ -3549,7 +5055,7 @@
         <v>4</v>
       </c>
       <c r="B3" t="s">
-        <v>175</v>
+        <v>171</v>
       </c>
     </row>
   </sheetData>

</xml_diff>

<commit_message>
fixed some bugs in ballard exam
</commit_message>
<xml_diff>
--- a/opendatakit.collect2/form-files/neonatal/neonatal.xlsx
+++ b/opendatakit.collect2/form-files/neonatal/neonatal.xlsx
@@ -4,7 +4,7 @@
   <fileVersion appName="xl" lastEdited="5" lowestEdited="5" rupBuild="20910"/>
   <workbookPr autoCompressPictures="0"/>
   <bookViews>
-    <workbookView xWindow="0" yWindow="0" windowWidth="23900" windowHeight="17400" tabRatio="500" activeTab="2"/>
+    <workbookView xWindow="0" yWindow="0" windowWidth="23900" windowHeight="17400" tabRatio="500" activeTab="1"/>
   </bookViews>
   <sheets>
     <sheet name="survey" sheetId="1" r:id="rId1"/>
@@ -23,7 +23,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="589" uniqueCount="431">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="603" uniqueCount="445">
   <si>
     <t>type</t>
   </si>
@@ -1346,9 +1346,6 @@
     <t>Lanugo Score: {{calculates.lanugoScore}}</t>
   </si>
   <si>
-    <t>Plantar Surface Score: {{calculates.surfaceScore}}</t>
-  </si>
-  <si>
     <t>Breast Score: {{calculates.breastScore}}</t>
   </si>
   <si>
@@ -1519,12 +1516,57 @@
   <si>
     <t>calculates.totalNMScore() + calculates.totalPhysicalScore()</t>
   </si>
+  <si>
+    <t>goto diagnostics_end</t>
+  </si>
+  <si>
+    <t>not(selected(data('menu'), 'diagnostics'))</t>
+  </si>
+  <si>
+    <t>goto diagnostics_begin</t>
+  </si>
+  <si>
+    <t>selected(data('menu'),'diagnostics')</t>
+  </si>
+  <si>
+    <t>label neuromuscular_begin</t>
+  </si>
+  <si>
+    <t>label neuromuscular_end</t>
+  </si>
+  <si>
+    <t>goto neuromuscular_end</t>
+  </si>
+  <si>
+    <t>goto neuromuscular_begin</t>
+  </si>
+  <si>
+    <t>goto physical_end</t>
+  </si>
+  <si>
+    <t>goto physical_begin</t>
+  </si>
+  <si>
+    <t>label physical_begin</t>
+  </si>
+  <si>
+    <t>label physical_end</t>
+  </si>
+  <si>
+    <t>not(selected(data('ballard_menu0'), 'neuromuscular'))</t>
+  </si>
+  <si>
+    <t>not(selected(data('ballard_menu0'), 'physical'))</t>
+  </si>
+  <si>
+    <t>Plantar Surface Score: {{calculates.plantarScore}}</t>
+  </si>
 </sst>
 </file>
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
 <styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <fonts count="7" x14ac:knownFonts="1">
+  <fonts count="8" x14ac:knownFonts="1">
     <font>
       <sz val="10"/>
       <color rgb="FF000000"/>
@@ -1568,8 +1610,14 @@
       <family val="2"/>
       <scheme val="minor"/>
     </font>
+    <font>
+      <sz val="12"/>
+      <color rgb="FF9C6500"/>
+      <name val="Calibri"/>
+      <family val="2"/>
+    </font>
   </fonts>
-  <fills count="8">
+  <fills count="10">
     <fill>
       <patternFill patternType="none"/>
     </fill>
@@ -1610,6 +1658,18 @@
         <bgColor indexed="64"/>
       </patternFill>
     </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor rgb="FFC4D79B"/>
+        <bgColor rgb="FF000000"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor rgb="FFFFEB9C"/>
+        <bgColor rgb="FF000000"/>
+      </patternFill>
+    </fill>
   </fills>
   <borders count="1">
     <border>
@@ -1620,7 +1680,7 @@
       <diagonal/>
     </border>
   </borders>
-  <cellStyleXfs count="274">
+  <cellStyleXfs count="286">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
     <xf numFmtId="0" fontId="3" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
     <xf numFmtId="0" fontId="4" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
@@ -1895,8 +1955,20 @@
     <xf numFmtId="0" fontId="4" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
     <xf numFmtId="0" fontId="3" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
     <xf numFmtId="0" fontId="4" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="4" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="4" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="4" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="4" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="4" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="4" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
   </cellStyleXfs>
-  <cellXfs count="19">
+  <cellXfs count="22">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
       <alignment wrapText="1"/>
     </xf>
@@ -1942,8 +2014,13 @@
       <alignment wrapText="1"/>
     </xf>
     <xf numFmtId="0" fontId="6" fillId="3" borderId="0" xfId="12"/>
+    <xf numFmtId="0" fontId="0" fillId="8" borderId="0" xfId="0" applyFill="1" applyAlignment="1">
+      <alignment wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="7" fillId="9" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1"/>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1"/>
   </cellXfs>
-  <cellStyles count="274">
+  <cellStyles count="286">
     <cellStyle name="20% - Accent4" xfId="13" builtinId="42"/>
     <cellStyle name="Followed Hyperlink" xfId="2" builtinId="9" hidden="1"/>
     <cellStyle name="Followed Hyperlink" xfId="4" builtinId="9" hidden="1"/>
@@ -2080,6 +2157,12 @@
     <cellStyle name="Followed Hyperlink" xfId="269" builtinId="9" hidden="1"/>
     <cellStyle name="Followed Hyperlink" xfId="271" builtinId="9" hidden="1"/>
     <cellStyle name="Followed Hyperlink" xfId="273" builtinId="9" hidden="1"/>
+    <cellStyle name="Followed Hyperlink" xfId="275" builtinId="9" hidden="1"/>
+    <cellStyle name="Followed Hyperlink" xfId="277" builtinId="9" hidden="1"/>
+    <cellStyle name="Followed Hyperlink" xfId="279" builtinId="9" hidden="1"/>
+    <cellStyle name="Followed Hyperlink" xfId="281" builtinId="9" hidden="1"/>
+    <cellStyle name="Followed Hyperlink" xfId="283" builtinId="9" hidden="1"/>
+    <cellStyle name="Followed Hyperlink" xfId="285" builtinId="9" hidden="1"/>
     <cellStyle name="Good" xfId="11" builtinId="26"/>
     <cellStyle name="Hyperlink" xfId="1" builtinId="8" hidden="1"/>
     <cellStyle name="Hyperlink" xfId="3" builtinId="8" hidden="1"/>
@@ -2216,6 +2299,12 @@
     <cellStyle name="Hyperlink" xfId="268" builtinId="8" hidden="1"/>
     <cellStyle name="Hyperlink" xfId="270" builtinId="8" hidden="1"/>
     <cellStyle name="Hyperlink" xfId="272" builtinId="8" hidden="1"/>
+    <cellStyle name="Hyperlink" xfId="274" builtinId="8" hidden="1"/>
+    <cellStyle name="Hyperlink" xfId="276" builtinId="8" hidden="1"/>
+    <cellStyle name="Hyperlink" xfId="278" builtinId="8" hidden="1"/>
+    <cellStyle name="Hyperlink" xfId="280" builtinId="8" hidden="1"/>
+    <cellStyle name="Hyperlink" xfId="282" builtinId="8" hidden="1"/>
+    <cellStyle name="Hyperlink" xfId="284" builtinId="8" hidden="1"/>
     <cellStyle name="Neutral" xfId="12" builtinId="28"/>
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
   </cellStyles>
@@ -2546,10 +2635,10 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <dimension ref="A1:I87"/>
+  <dimension ref="A1:I95"/>
   <sheetViews>
-    <sheetView zoomScale="150" zoomScaleNormal="150" zoomScalePageLayoutView="150" workbookViewId="0">
-      <selection activeCell="A20" sqref="A20"/>
+    <sheetView topLeftCell="A36" zoomScale="150" zoomScaleNormal="150" zoomScalePageLayoutView="150" workbookViewId="0">
+      <selection activeCell="C48" sqref="C48"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultColWidth="11.5" defaultRowHeight="12.75" customHeight="1" x14ac:dyDescent="0"/>
@@ -2615,6 +2704,32 @@
       <c r="D4" s="4"/>
       <c r="E4" s="2"/>
     </row>
+    <row r="5" spans="1:7" ht="12.75" customHeight="1">
+      <c r="A5" s="19" t="s">
+        <v>430</v>
+      </c>
+      <c r="B5" s="19"/>
+      <c r="C5" s="19"/>
+      <c r="D5" s="19" t="s">
+        <v>431</v>
+      </c>
+      <c r="E5" s="19"/>
+      <c r="F5" s="19"/>
+      <c r="G5" s="19"/>
+    </row>
+    <row r="6" spans="1:7" ht="12.75" customHeight="1">
+      <c r="A6" s="19" t="s">
+        <v>432</v>
+      </c>
+      <c r="B6" s="19"/>
+      <c r="C6" s="19"/>
+      <c r="D6" s="19" t="s">
+        <v>433</v>
+      </c>
+      <c r="E6" s="19"/>
+      <c r="F6" s="19"/>
+      <c r="G6" s="19"/>
+    </row>
     <row r="7" spans="1:7" s="12" customFormat="1" ht="18" customHeight="1">
       <c r="A7" s="18" t="s">
         <v>113</v>
@@ -2698,294 +2813,326 @@
       </c>
       <c r="E12" s="2"/>
     </row>
-    <row r="13" spans="1:7" ht="12">
-      <c r="A13" t="s">
+    <row r="13" spans="1:7" ht="12.75" customHeight="1">
+      <c r="A13" s="19" t="s">
+        <v>436</v>
+      </c>
+      <c r="B13" s="19"/>
+      <c r="C13" s="19"/>
+      <c r="D13" s="19" t="s">
+        <v>442</v>
+      </c>
+      <c r="E13" s="19"/>
+      <c r="F13" s="19"/>
+      <c r="G13" s="19"/>
+    </row>
+    <row r="14" spans="1:7" ht="12.75" customHeight="1">
+      <c r="A14" s="19" t="s">
+        <v>437</v>
+      </c>
+      <c r="B14" s="19"/>
+      <c r="C14" s="19"/>
+      <c r="D14" s="19" t="s">
+        <v>279</v>
+      </c>
+      <c r="E14" s="19"/>
+      <c r="F14" s="19"/>
+      <c r="G14" s="19"/>
+    </row>
+    <row r="15" spans="1:7" s="12" customFormat="1" ht="18" customHeight="1">
+      <c r="A15" s="18" t="s">
+        <v>434</v>
+      </c>
+      <c r="B15" s="18"/>
+      <c r="C15" s="18"/>
+      <c r="D15" s="18"/>
+      <c r="E15" s="18"/>
+      <c r="F15" s="18"/>
+      <c r="G15" s="18"/>
+    </row>
+    <row r="16" spans="1:7" ht="12">
+      <c r="A16" t="s">
         <v>232</v>
       </c>
-      <c r="B13" t="s">
+      <c r="B16" t="s">
         <v>138</v>
       </c>
-      <c r="C13" t="s">
+      <c r="C16" t="s">
         <v>278</v>
       </c>
-      <c r="D13" s="2" t="s">
-        <v>279</v>
-      </c>
-    </row>
-    <row r="14" spans="1:7" ht="11" customHeight="1">
-      <c r="A14" t="s">
+      <c r="D16" s="2"/>
+    </row>
+    <row r="17" spans="1:9" ht="11" customHeight="1">
+      <c r="A17" t="s">
         <v>151</v>
       </c>
-      <c r="B14" t="s">
+      <c r="B17" t="s">
         <v>152</v>
       </c>
-      <c r="C14" t="s">
+      <c r="C17" t="s">
         <v>153</v>
       </c>
-      <c r="D14" s="2" t="s">
+      <c r="D17" s="2" t="s">
         <v>154</v>
       </c>
     </row>
-    <row r="15" spans="1:7" ht="11" customHeight="1">
-      <c r="A15" t="s">
+    <row r="18" spans="1:9" ht="11" customHeight="1">
+      <c r="A18" t="s">
         <v>155</v>
       </c>
-      <c r="B15" t="s">
+      <c r="B18" t="s">
         <v>156</v>
       </c>
-      <c r="C15" t="s">
+      <c r="C18" t="s">
         <v>157</v>
       </c>
-      <c r="D15" s="2" t="s">
+      <c r="D18" s="2" t="s">
         <v>158</v>
       </c>
     </row>
-    <row r="16" spans="1:7" ht="11" customHeight="1">
-      <c r="A16" t="s">
+    <row r="19" spans="1:9" ht="11" customHeight="1">
+      <c r="A19" t="s">
         <v>172</v>
       </c>
-      <c r="B16" t="s">
+      <c r="B19" t="s">
         <v>173</v>
       </c>
-      <c r="C16" t="s">
+      <c r="C19" t="s">
         <v>174</v>
       </c>
-      <c r="D16" s="2" t="s">
+      <c r="D19" s="2" t="s">
         <v>175</v>
       </c>
     </row>
-    <row r="17" spans="1:5" ht="11" customHeight="1">
-      <c r="A17" t="s">
+    <row r="20" spans="1:9" ht="11" customHeight="1">
+      <c r="A20" t="s">
         <v>244</v>
       </c>
-      <c r="B17" t="s">
+      <c r="B20" t="s">
         <v>245</v>
       </c>
-      <c r="C17" t="s">
+      <c r="C20" t="s">
         <v>246</v>
       </c>
-      <c r="D17" s="2" t="s">
+      <c r="D20" s="2" t="s">
         <v>247</v>
       </c>
     </row>
-    <row r="18" spans="1:5" ht="11" customHeight="1">
-      <c r="A18" t="s">
+    <row r="21" spans="1:9" ht="11" customHeight="1">
+      <c r="A21" t="s">
         <v>176</v>
       </c>
-      <c r="B18" t="s">
+      <c r="B21" t="s">
         <v>177</v>
       </c>
-      <c r="C18" t="s">
+      <c r="C21" t="s">
         <v>178</v>
       </c>
-      <c r="D18" s="2" t="s">
+      <c r="D21" s="2" t="s">
         <v>228</v>
       </c>
     </row>
-    <row r="19" spans="1:5" ht="11" customHeight="1">
-      <c r="A19" t="s">
+    <row r="22" spans="1:9" ht="11" customHeight="1">
+      <c r="A22" t="s">
         <v>179</v>
       </c>
-      <c r="B19" t="s">
+      <c r="B22" t="s">
         <v>180</v>
       </c>
-      <c r="C19" t="s">
+      <c r="C22" t="s">
         <v>181</v>
       </c>
-      <c r="D19" s="2" t="s">
+      <c r="D22" s="2" t="s">
         <v>229</v>
       </c>
     </row>
-    <row r="20" spans="1:5" ht="11" customHeight="1">
-      <c r="A20" t="s">
+    <row r="23" spans="1:9" ht="11" customHeight="1">
+      <c r="A23" s="20" t="s">
+        <v>435</v>
+      </c>
+      <c r="B23" s="20"/>
+      <c r="C23" s="20"/>
+      <c r="D23" s="20"/>
+      <c r="E23" s="20"/>
+      <c r="F23" s="20"/>
+      <c r="G23" s="20"/>
+      <c r="H23" s="21"/>
+      <c r="I23" s="21"/>
+    </row>
+    <row r="24" spans="1:9" ht="12.75" customHeight="1">
+      <c r="A24" s="19" t="s">
+        <v>438</v>
+      </c>
+      <c r="B24" s="19"/>
+      <c r="C24" s="19"/>
+      <c r="D24" s="19" t="s">
+        <v>443</v>
+      </c>
+      <c r="E24" s="19"/>
+      <c r="F24" s="19"/>
+      <c r="G24" s="19"/>
+    </row>
+    <row r="25" spans="1:9" ht="12.75" customHeight="1">
+      <c r="A25" s="19" t="s">
+        <v>439</v>
+      </c>
+      <c r="B25" s="19"/>
+      <c r="C25" s="19"/>
+      <c r="D25" s="19" t="s">
+        <v>283</v>
+      </c>
+      <c r="E25" s="19"/>
+      <c r="F25" s="19"/>
+      <c r="G25" s="19"/>
+    </row>
+    <row r="26" spans="1:9" s="12" customFormat="1" ht="18" customHeight="1">
+      <c r="A26" s="18" t="s">
+        <v>440</v>
+      </c>
+      <c r="B26" s="18"/>
+      <c r="C26" s="18"/>
+      <c r="D26" s="18"/>
+      <c r="E26" s="18"/>
+      <c r="F26" s="18"/>
+      <c r="G26" s="18"/>
+    </row>
+    <row r="27" spans="1:9" ht="11" customHeight="1">
+      <c r="A27" t="s">
         <v>280</v>
       </c>
-      <c r="B20" t="s">
+      <c r="B27" t="s">
         <v>281</v>
       </c>
-      <c r="C20" t="s">
+      <c r="C27" t="s">
         <v>282</v>
       </c>
-      <c r="D20" s="2" t="s">
-        <v>283</v>
-      </c>
-    </row>
-    <row r="21" spans="1:5" ht="11" customHeight="1">
-      <c r="A21" t="s">
+      <c r="D27" s="2"/>
+    </row>
+    <row r="28" spans="1:9" ht="11" customHeight="1">
+      <c r="A28" t="s">
         <v>331</v>
       </c>
-      <c r="B21" t="s">
+      <c r="B28" t="s">
         <v>311</v>
       </c>
-      <c r="C21" t="s">
+      <c r="C28" t="s">
         <v>289</v>
       </c>
-      <c r="D21" s="2" t="s">
+      <c r="D28" s="2" t="s">
         <v>290</v>
       </c>
     </row>
-    <row r="22" spans="1:5" ht="11" customHeight="1">
-      <c r="A22" t="s">
+    <row r="29" spans="1:9" ht="11" customHeight="1">
+      <c r="A29" t="s">
         <v>332</v>
       </c>
-      <c r="B22" t="s">
+      <c r="B29" t="s">
         <v>312</v>
       </c>
-      <c r="C22" t="s">
+      <c r="C29" t="s">
         <v>301</v>
       </c>
-      <c r="D22" s="2" t="s">
+      <c r="D29" s="2" t="s">
         <v>292</v>
       </c>
     </row>
-    <row r="23" spans="1:5" ht="11" customHeight="1">
-      <c r="A23" t="s">
+    <row r="30" spans="1:9" ht="11" customHeight="1">
+      <c r="A30" t="s">
         <v>333</v>
       </c>
-      <c r="B23" t="s">
+      <c r="B30" t="s">
         <v>313</v>
       </c>
-      <c r="C23" t="s">
+      <c r="C30" t="s">
         <v>304</v>
       </c>
-      <c r="D23" s="2" t="s">
+      <c r="D30" s="2" t="s">
         <v>293</v>
       </c>
     </row>
-    <row r="24" spans="1:5" ht="11" customHeight="1">
-      <c r="A24" t="s">
+    <row r="31" spans="1:9" ht="11" customHeight="1">
+      <c r="A31" t="s">
         <v>334</v>
       </c>
-      <c r="B24" t="s">
+      <c r="B31" t="s">
         <v>314</v>
       </c>
-      <c r="C24" t="s">
+      <c r="C31" t="s">
         <v>302</v>
       </c>
-      <c r="D24" s="2" t="s">
+      <c r="D31" s="2" t="s">
         <v>296</v>
       </c>
     </row>
-    <row r="25" spans="1:5" ht="11" customHeight="1">
-      <c r="A25" t="s">
+    <row r="32" spans="1:9" ht="11" customHeight="1">
+      <c r="A32" t="s">
         <v>335</v>
       </c>
-      <c r="B25" t="s">
+      <c r="B32" t="s">
         <v>315</v>
       </c>
-      <c r="C25" t="s">
+      <c r="C32" t="s">
         <v>303</v>
       </c>
-      <c r="D25" s="2" t="s">
+      <c r="D32" s="2" t="s">
         <v>298</v>
       </c>
     </row>
-    <row r="26" spans="1:5" ht="12" customHeight="1">
-      <c r="A26" t="s">
+    <row r="33" spans="1:9" ht="12" customHeight="1">
+      <c r="A33" t="s">
         <v>336</v>
       </c>
-      <c r="B26" t="s">
+      <c r="B33" t="s">
         <v>316</v>
       </c>
-      <c r="C26" t="s">
+      <c r="C33" t="s">
         <v>305</v>
       </c>
-      <c r="D26" s="2" t="s">
+      <c r="D33" s="2" t="s">
         <v>300</v>
       </c>
     </row>
-    <row r="27" spans="1:5" ht="18" customHeight="1">
-      <c r="A27" s="7" t="s">
+    <row r="34" spans="1:9" ht="12" customHeight="1">
+      <c r="A34" s="20" t="s">
+        <v>441</v>
+      </c>
+      <c r="B34" s="20"/>
+      <c r="C34" s="20"/>
+      <c r="D34" s="20"/>
+      <c r="E34" s="20"/>
+      <c r="F34" s="20"/>
+      <c r="G34" s="20"/>
+      <c r="H34" s="21"/>
+      <c r="I34" s="21"/>
+    </row>
+    <row r="35" spans="1:9" ht="18" customHeight="1">
+      <c r="A35" s="7" t="s">
         <v>17</v>
       </c>
-      <c r="B27" s="4"/>
-      <c r="C27" s="2"/>
-      <c r="D27" s="2" t="s">
-        <v>427</v>
-      </c>
-      <c r="E27" s="2"/>
-    </row>
-    <row r="28" spans="1:5" ht="18" customHeight="1">
-      <c r="A28" s="9" t="s">
+      <c r="B35" s="4"/>
+      <c r="C35" s="2"/>
+      <c r="D35" s="2" t="s">
+        <v>426</v>
+      </c>
+      <c r="E35" s="2"/>
+    </row>
+    <row r="36" spans="1:9" ht="18" customHeight="1">
+      <c r="A36" s="9" t="s">
         <v>13</v>
       </c>
-      <c r="B28" s="4"/>
-      <c r="C28" s="2" t="s">
+      <c r="B36" s="4"/>
+      <c r="C36" s="2" t="s">
         <v>404</v>
       </c>
-      <c r="D28" s="2"/>
-      <c r="E28" s="2"/>
-    </row>
-    <row r="29" spans="1:5" ht="25" customHeight="1">
-      <c r="A29" t="s">
-        <v>13</v>
-      </c>
-      <c r="C29" t="s">
-        <v>238</v>
-      </c>
-    </row>
-    <row r="30" spans="1:5" ht="25" customHeight="1">
-      <c r="A30" t="s">
-        <v>13</v>
-      </c>
-      <c r="C30" t="s">
-        <v>251</v>
-      </c>
-    </row>
-    <row r="31" spans="1:5" ht="25" customHeight="1">
-      <c r="A31" t="s">
-        <v>13</v>
-      </c>
-      <c r="C31" t="s">
-        <v>252</v>
-      </c>
-    </row>
-    <row r="32" spans="1:5" ht="25" customHeight="1">
-      <c r="A32" t="s">
-        <v>13</v>
-      </c>
-      <c r="C32" t="s">
-        <v>274</v>
-      </c>
-    </row>
-    <row r="33" spans="1:9" ht="25" customHeight="1">
-      <c r="A33" t="s">
-        <v>13</v>
-      </c>
-      <c r="C33" t="s">
-        <v>253</v>
-      </c>
-    </row>
-    <row r="34" spans="1:9" ht="25" customHeight="1">
-      <c r="A34" t="s">
-        <v>13</v>
-      </c>
-      <c r="C34" t="s">
-        <v>254</v>
-      </c>
-    </row>
-    <row r="35" spans="1:9" ht="25" customHeight="1">
-      <c r="A35" t="s">
-        <v>13</v>
-      </c>
-      <c r="C35" t="s">
-        <v>275</v>
-      </c>
-    </row>
-    <row r="36" spans="1:9" ht="25" customHeight="1">
-      <c r="A36" t="s">
-        <v>13</v>
-      </c>
-      <c r="C36" t="s">
-        <v>403</v>
-      </c>
+      <c r="D36" s="2"/>
+      <c r="E36" s="2"/>
     </row>
     <row r="37" spans="1:9" ht="25" customHeight="1">
       <c r="A37" t="s">
         <v>13</v>
       </c>
       <c r="C37" t="s">
-        <v>405</v>
+        <v>238</v>
       </c>
     </row>
     <row r="38" spans="1:9" ht="25" customHeight="1">
@@ -2993,7 +3140,7 @@
         <v>13</v>
       </c>
       <c r="C38" t="s">
-        <v>406</v>
+        <v>251</v>
       </c>
     </row>
     <row r="39" spans="1:9" ht="25" customHeight="1">
@@ -3001,7 +3148,7 @@
         <v>13</v>
       </c>
       <c r="C39" t="s">
-        <v>407</v>
+        <v>252</v>
       </c>
     </row>
     <row r="40" spans="1:9" ht="25" customHeight="1">
@@ -3009,7 +3156,7 @@
         <v>13</v>
       </c>
       <c r="C40" t="s">
-        <v>408</v>
+        <v>274</v>
       </c>
     </row>
     <row r="41" spans="1:9" ht="25" customHeight="1">
@@ -3017,7 +3164,7 @@
         <v>13</v>
       </c>
       <c r="C41" t="s">
-        <v>409</v>
+        <v>253</v>
       </c>
     </row>
     <row r="42" spans="1:9" ht="25" customHeight="1">
@@ -3025,7 +3172,7 @@
         <v>13</v>
       </c>
       <c r="C42" t="s">
-        <v>410</v>
+        <v>254</v>
       </c>
     </row>
     <row r="43" spans="1:9" ht="25" customHeight="1">
@@ -3033,7 +3180,7 @@
         <v>13</v>
       </c>
       <c r="C43" t="s">
-        <v>411</v>
+        <v>275</v>
       </c>
     </row>
     <row r="44" spans="1:9" ht="25" customHeight="1">
@@ -3041,327 +3188,293 @@
         <v>13</v>
       </c>
       <c r="C44" t="s">
-        <v>428</v>
+        <v>403</v>
       </c>
     </row>
     <row r="45" spans="1:9" ht="25" customHeight="1">
-      <c r="A45" s="11" t="s">
+      <c r="A45" t="s">
+        <v>13</v>
+      </c>
+      <c r="C45" t="s">
+        <v>405</v>
+      </c>
+    </row>
+    <row r="46" spans="1:9" ht="25" customHeight="1">
+      <c r="A46" t="s">
+        <v>13</v>
+      </c>
+      <c r="C46" t="s">
+        <v>406</v>
+      </c>
+    </row>
+    <row r="47" spans="1:9" ht="25" customHeight="1">
+      <c r="A47" t="s">
+        <v>13</v>
+      </c>
+      <c r="C47" t="s">
+        <v>444</v>
+      </c>
+    </row>
+    <row r="48" spans="1:9" ht="25" customHeight="1">
+      <c r="A48" t="s">
+        <v>13</v>
+      </c>
+      <c r="C48" t="s">
+        <v>407</v>
+      </c>
+    </row>
+    <row r="49" spans="1:9" ht="25" customHeight="1">
+      <c r="A49" t="s">
+        <v>13</v>
+      </c>
+      <c r="C49" t="s">
+        <v>408</v>
+      </c>
+    </row>
+    <row r="50" spans="1:9" ht="25" customHeight="1">
+      <c r="A50" t="s">
+        <v>13</v>
+      </c>
+      <c r="C50" t="s">
+        <v>409</v>
+      </c>
+    </row>
+    <row r="51" spans="1:9" ht="25" customHeight="1">
+      <c r="A51" t="s">
+        <v>13</v>
+      </c>
+      <c r="C51" t="s">
+        <v>410</v>
+      </c>
+    </row>
+    <row r="52" spans="1:9" ht="25" customHeight="1">
+      <c r="A52" t="s">
+        <v>13</v>
+      </c>
+      <c r="C52" t="s">
+        <v>427</v>
+      </c>
+    </row>
+    <row r="53" spans="1:9" ht="25" customHeight="1">
+      <c r="A53" s="11" t="s">
         <v>27</v>
       </c>
     </row>
-    <row r="46" spans="1:9" ht="15">
-      <c r="A46" s="15" t="s">
+    <row r="54" spans="1:9" ht="15">
+      <c r="A54" s="15" t="s">
         <v>75</v>
       </c>
-      <c r="B46" s="15"/>
-      <c r="C46" s="15"/>
-      <c r="D46" s="15"/>
-      <c r="E46" s="15"/>
-      <c r="F46" s="15"/>
-      <c r="G46" s="15"/>
-    </row>
-    <row r="47" spans="1:9" ht="15">
-      <c r="A47" s="16"/>
-      <c r="B47" s="12"/>
-      <c r="C47" s="12"/>
-      <c r="D47" s="12"/>
-      <c r="E47" s="12"/>
-      <c r="F47" s="12"/>
-      <c r="G47" s="12"/>
-    </row>
-    <row r="48" spans="1:9" s="15" customFormat="1" ht="15">
-      <c r="A48" s="13" t="s">
+      <c r="B54" s="15"/>
+      <c r="C54" s="15"/>
+      <c r="D54" s="15"/>
+      <c r="E54" s="15"/>
+      <c r="F54" s="15"/>
+      <c r="G54" s="15"/>
+    </row>
+    <row r="55" spans="1:9" ht="15">
+      <c r="A55" s="16"/>
+      <c r="B55" s="12"/>
+      <c r="C55" s="12"/>
+      <c r="D55" s="12"/>
+      <c r="E55" s="12"/>
+      <c r="F55" s="12"/>
+      <c r="G55" s="12"/>
+    </row>
+    <row r="56" spans="1:9" s="15" customFormat="1" ht="15">
+      <c r="A56" s="13" t="s">
         <v>110</v>
       </c>
-      <c r="B48" s="13"/>
-      <c r="C48" s="13"/>
-      <c r="D48" s="13" t="s">
+      <c r="B56" s="13"/>
+      <c r="C56" s="13"/>
+      <c r="D56" s="13" t="s">
         <v>74</v>
       </c>
-      <c r="E48" s="13"/>
-      <c r="F48" s="13"/>
-      <c r="G48" s="13"/>
-      <c r="H48" s="12"/>
-      <c r="I48" s="12"/>
-    </row>
-    <row r="49" spans="1:8" ht="12">
-      <c r="A49" s="5" t="s">
+      <c r="E56" s="13"/>
+      <c r="F56" s="13"/>
+      <c r="G56" s="13"/>
+      <c r="H56" s="12"/>
+      <c r="I56" s="12"/>
+    </row>
+    <row r="57" spans="1:9" ht="12">
+      <c r="A57" s="5" t="s">
         <v>76</v>
       </c>
-      <c r="B49" s="5"/>
-      <c r="C49" s="5"/>
-      <c r="D49" s="6" t="s">
+      <c r="B57" s="5"/>
+      <c r="C57" s="5"/>
+      <c r="D57" s="6" t="s">
         <v>77</v>
       </c>
-      <c r="E49" s="5"/>
-      <c r="F49" s="5"/>
-      <c r="G49" s="5"/>
-    </row>
-    <row r="50" spans="1:8" ht="15">
-      <c r="A50" s="15" t="s">
+      <c r="E57" s="5"/>
+      <c r="F57" s="5"/>
+      <c r="G57" s="5"/>
+    </row>
+    <row r="58" spans="1:9" ht="15">
+      <c r="A58" s="15" t="s">
         <v>109</v>
       </c>
-      <c r="B50" s="15"/>
-      <c r="C50" s="15"/>
-      <c r="D50" s="15"/>
-      <c r="E50" s="15"/>
-      <c r="F50" s="15"/>
-      <c r="G50" s="15"/>
-    </row>
-    <row r="51" spans="1:8" ht="12">
-      <c r="A51" s="12" t="s">
+      <c r="B58" s="15"/>
+      <c r="C58" s="15"/>
+      <c r="D58" s="15"/>
+      <c r="E58" s="15"/>
+      <c r="F58" s="15"/>
+      <c r="G58" s="15"/>
+    </row>
+    <row r="59" spans="1:9" ht="12">
+      <c r="A59" s="12" t="s">
         <v>233</v>
       </c>
-      <c r="B51" s="12" t="s">
+      <c r="B59" s="12" t="s">
         <v>9</v>
       </c>
-      <c r="C51" s="12" t="s">
+      <c r="C59" s="12" t="s">
         <v>10</v>
       </c>
-      <c r="D51" s="12"/>
-      <c r="E51" s="12" t="s">
+      <c r="D59" s="12"/>
+      <c r="E59" s="12" t="s">
         <v>6</v>
       </c>
-      <c r="F51" s="12"/>
-      <c r="G51" s="12"/>
-    </row>
-    <row r="52" spans="1:8" ht="12">
-      <c r="A52" s="7" t="s">
+      <c r="F59" s="12"/>
+      <c r="G59" s="12"/>
+    </row>
+    <row r="60" spans="1:9" ht="12">
+      <c r="A60" s="7" t="s">
         <v>17</v>
       </c>
-      <c r="B52" s="8"/>
-      <c r="C52" s="8"/>
-      <c r="D52" s="9" t="s">
+      <c r="B60" s="8"/>
+      <c r="C60" s="8"/>
+      <c r="D60" s="9" t="s">
         <v>65</v>
       </c>
-      <c r="E52" s="8"/>
-      <c r="F52" s="10"/>
-      <c r="G52" s="10"/>
-    </row>
-    <row r="53" spans="1:8" ht="12.75" customHeight="1">
-      <c r="A53" s="4" t="s">
+      <c r="E60" s="8"/>
+      <c r="F60" s="10"/>
+      <c r="G60" s="10"/>
+    </row>
+    <row r="61" spans="1:9" ht="12.75" customHeight="1">
+      <c r="A61" s="4" t="s">
         <v>13</v>
       </c>
-      <c r="B53" s="2" t="s">
+      <c r="B61" s="2" t="s">
         <v>78</v>
       </c>
-      <c r="C53" s="2" t="s">
+      <c r="C61" s="2" t="s">
         <v>79</v>
       </c>
-      <c r="D53" s="2"/>
-      <c r="E53" s="4"/>
-    </row>
-    <row r="54" spans="1:8" ht="12.75" customHeight="1">
-      <c r="A54" s="4" t="s">
+      <c r="D61" s="2"/>
+      <c r="E61" s="4"/>
+    </row>
+    <row r="62" spans="1:9" ht="12.75" customHeight="1">
+      <c r="A62" s="4" t="s">
         <v>13</v>
       </c>
-      <c r="B54" s="2" t="s">
+      <c r="B62" s="2" t="s">
         <v>80</v>
       </c>
-      <c r="C54" s="2"/>
-      <c r="D54" s="2"/>
-      <c r="E54" s="4"/>
-      <c r="F54" t="s">
+      <c r="C62" s="2"/>
+      <c r="D62" s="2"/>
+      <c r="E62" s="4"/>
+      <c r="F62" t="s">
         <v>14</v>
       </c>
     </row>
-    <row r="55" spans="1:8" ht="12.75" customHeight="1">
-      <c r="A55" t="s">
+    <row r="63" spans="1:9" ht="12.75" customHeight="1">
+      <c r="A63" t="s">
         <v>13</v>
       </c>
-      <c r="C55" t="s">
+      <c r="C63" t="s">
         <v>81</v>
       </c>
-      <c r="D55" s="13"/>
-    </row>
-    <row r="56" spans="1:8" ht="12.75" customHeight="1">
-      <c r="A56" t="s">
+      <c r="D63" s="13"/>
+    </row>
+    <row r="64" spans="1:9" ht="12.75" customHeight="1">
+      <c r="A64" t="s">
         <v>13</v>
       </c>
-      <c r="B56" t="s">
+      <c r="B64" t="s">
         <v>82</v>
       </c>
-      <c r="G56" t="s">
+      <c r="G64" t="s">
         <v>83</v>
       </c>
     </row>
-    <row r="57" spans="1:8" ht="12">
-      <c r="A57" s="11" t="s">
+    <row r="65" spans="1:8" ht="12">
+      <c r="A65" s="11" t="s">
         <v>27</v>
       </c>
-      <c r="B57" s="10"/>
-      <c r="C57" s="10"/>
-      <c r="D57" s="10"/>
-      <c r="E57" s="10"/>
-      <c r="F57" s="10"/>
-      <c r="G57" s="10"/>
-    </row>
-    <row r="58" spans="1:8" ht="24">
-      <c r="A58" s="4" t="s">
+      <c r="B65" s="10"/>
+      <c r="C65" s="10"/>
+      <c r="D65" s="10"/>
+      <c r="E65" s="10"/>
+      <c r="F65" s="10"/>
+      <c r="G65" s="10"/>
+    </row>
+    <row r="66" spans="1:8" ht="24">
+      <c r="A66" s="4" t="s">
         <v>13</v>
       </c>
-      <c r="B58" s="4"/>
-      <c r="C58" s="4" t="s">
+      <c r="B66" s="4"/>
+      <c r="C66" s="4" t="s">
         <v>15</v>
       </c>
-      <c r="D58" s="2" t="s">
+      <c r="D66" s="2" t="s">
         <v>73</v>
       </c>
-      <c r="E58" s="4"/>
-      <c r="F58" t="s">
+      <c r="E66" s="4"/>
+      <c r="F66" t="s">
         <v>16</v>
       </c>
     </row>
-    <row r="59" spans="1:8" ht="15">
-      <c r="A59" s="15" t="s">
+    <row r="67" spans="1:8" ht="15">
+      <c r="A67" s="15" t="s">
         <v>85</v>
       </c>
-      <c r="B59" s="15"/>
-      <c r="C59" s="15"/>
-      <c r="D59" s="15"/>
-      <c r="E59" s="15"/>
-      <c r="F59" s="15"/>
-      <c r="G59" s="15"/>
-      <c r="H59" s="12"/>
-    </row>
-    <row r="60" spans="1:8" ht="12">
-      <c r="A60" s="12"/>
-      <c r="B60" s="12"/>
-      <c r="C60" s="12"/>
-      <c r="D60" s="12"/>
-      <c r="E60" s="12"/>
-      <c r="F60" s="12"/>
-      <c r="G60" s="12"/>
-      <c r="H60" s="12"/>
-    </row>
-    <row r="61" spans="1:8" ht="15">
-      <c r="A61" s="14" t="s">
+      <c r="B67" s="15"/>
+      <c r="C67" s="15"/>
+      <c r="D67" s="15"/>
+      <c r="E67" s="15"/>
+      <c r="F67" s="15"/>
+      <c r="G67" s="15"/>
+      <c r="H67" s="12"/>
+    </row>
+    <row r="68" spans="1:8" ht="12">
+      <c r="A68" s="12"/>
+      <c r="B68" s="12"/>
+      <c r="C68" s="12"/>
+      <c r="D68" s="12"/>
+      <c r="E68" s="12"/>
+      <c r="F68" s="12"/>
+      <c r="G68" s="12"/>
+      <c r="H68" s="12"/>
+    </row>
+    <row r="69" spans="1:8" ht="15">
+      <c r="A69" s="14" t="s">
         <v>114</v>
       </c>
-      <c r="B61" s="14"/>
-      <c r="C61" s="14"/>
-      <c r="D61" s="13" t="s">
+      <c r="B69" s="14"/>
+      <c r="C69" s="14"/>
+      <c r="D69" s="13" t="s">
         <v>115</v>
       </c>
-      <c r="E61" s="14"/>
-      <c r="F61" s="14"/>
-      <c r="G61" s="14"/>
-      <c r="H61" s="12"/>
-    </row>
-    <row r="62" spans="1:8" ht="12">
-      <c r="A62" s="5" t="s">
+      <c r="E69" s="14"/>
+      <c r="F69" s="14"/>
+      <c r="G69" s="14"/>
+      <c r="H69" s="12"/>
+    </row>
+    <row r="70" spans="1:8" ht="12">
+      <c r="A70" s="5" t="s">
         <v>86</v>
       </c>
-      <c r="B62" s="5"/>
-      <c r="C62" s="5"/>
-      <c r="D62" s="6" t="s">
+      <c r="B70" s="5"/>
+      <c r="C70" s="5"/>
+      <c r="D70" s="6" t="s">
         <v>87</v>
       </c>
-      <c r="E62" s="5"/>
-      <c r="F62" s="5"/>
-      <c r="G62" s="5"/>
-    </row>
-    <row r="63" spans="1:8" ht="15">
-      <c r="A63" s="15" t="s">
+      <c r="E70" s="5"/>
+      <c r="F70" s="5"/>
+      <c r="G70" s="5"/>
+    </row>
+    <row r="71" spans="1:8" ht="15">
+      <c r="A71" s="15" t="s">
         <v>116</v>
-      </c>
-      <c r="B63" s="15"/>
-      <c r="C63" s="15"/>
-      <c r="D63" s="15"/>
-      <c r="E63" s="15"/>
-      <c r="F63" s="15"/>
-      <c r="G63" s="15"/>
-    </row>
-    <row r="64" spans="1:8" ht="12">
-      <c r="A64" t="s">
-        <v>234</v>
-      </c>
-      <c r="B64" t="s">
-        <v>11</v>
-      </c>
-      <c r="C64" t="s">
-        <v>12</v>
-      </c>
-      <c r="E64" t="s">
-        <v>6</v>
-      </c>
-      <c r="F64" s="12"/>
-      <c r="G64" s="12"/>
-    </row>
-    <row r="65" spans="1:9" ht="12">
-      <c r="A65" s="4" t="s">
-        <v>17</v>
-      </c>
-      <c r="B65" s="4"/>
-      <c r="C65" s="4"/>
-      <c r="D65" s="4"/>
-      <c r="E65" s="4"/>
-    </row>
-    <row r="66" spans="1:9" ht="12">
-      <c r="A66" s="4" t="s">
-        <v>18</v>
-      </c>
-      <c r="B66" s="4" t="s">
-        <v>19</v>
-      </c>
-      <c r="C66" s="4" t="s">
-        <v>20</v>
-      </c>
-      <c r="D66" s="4"/>
-      <c r="E66" s="4"/>
-    </row>
-    <row r="67" spans="1:9" ht="36">
-      <c r="A67" s="4" t="s">
-        <v>13</v>
-      </c>
-      <c r="B67" s="4"/>
-      <c r="C67" s="4" t="s">
-        <v>21</v>
-      </c>
-      <c r="D67" s="4" t="s">
-        <v>22</v>
-      </c>
-      <c r="E67" s="4"/>
-    </row>
-    <row r="68" spans="1:9" ht="12">
-      <c r="A68" s="4" t="s">
-        <v>18</v>
-      </c>
-      <c r="B68" s="4" t="s">
-        <v>23</v>
-      </c>
-      <c r="C68" s="4" t="s">
-        <v>24</v>
-      </c>
-      <c r="D68" s="4"/>
-      <c r="E68" s="4"/>
-    </row>
-    <row r="69" spans="1:9" ht="36">
-      <c r="A69" s="4" t="s">
-        <v>13</v>
-      </c>
-      <c r="B69" s="4"/>
-      <c r="C69" s="4" t="s">
-        <v>25</v>
-      </c>
-      <c r="D69" s="4" t="s">
-        <v>26</v>
-      </c>
-      <c r="E69" s="4"/>
-      <c r="H69" s="12"/>
-    </row>
-    <row r="70" spans="1:9" ht="12.75" customHeight="1">
-      <c r="A70" s="4" t="s">
-        <v>27</v>
-      </c>
-      <c r="B70" s="4"/>
-      <c r="C70" s="4"/>
-      <c r="D70" s="4"/>
-      <c r="E70" s="4"/>
-    </row>
-    <row r="71" spans="1:9" ht="12.75" customHeight="1">
-      <c r="A71" s="15" t="s">
-        <v>88</v>
       </c>
       <c r="B71" s="15"/>
       <c r="C71" s="15"/>
@@ -3370,156 +3483,254 @@
       <c r="F71" s="15"/>
       <c r="G71" s="15"/>
     </row>
-    <row r="72" spans="1:9" s="12" customFormat="1" ht="12.75" customHeight="1"/>
-    <row r="73" spans="1:9" s="14" customFormat="1" ht="12.75" customHeight="1">
-      <c r="A73" s="13" t="s">
+    <row r="72" spans="1:8" ht="12">
+      <c r="A72" t="s">
+        <v>234</v>
+      </c>
+      <c r="B72" t="s">
+        <v>11</v>
+      </c>
+      <c r="C72" t="s">
+        <v>12</v>
+      </c>
+      <c r="E72" t="s">
+        <v>6</v>
+      </c>
+      <c r="F72" s="12"/>
+      <c r="G72" s="12"/>
+    </row>
+    <row r="73" spans="1:8" ht="12">
+      <c r="A73" s="4" t="s">
+        <v>17</v>
+      </c>
+      <c r="B73" s="4"/>
+      <c r="C73" s="4"/>
+      <c r="D73" s="4"/>
+      <c r="E73" s="4"/>
+    </row>
+    <row r="74" spans="1:8" ht="12">
+      <c r="A74" s="4" t="s">
+        <v>18</v>
+      </c>
+      <c r="B74" s="4" t="s">
+        <v>19</v>
+      </c>
+      <c r="C74" s="4" t="s">
+        <v>20</v>
+      </c>
+      <c r="D74" s="4"/>
+      <c r="E74" s="4"/>
+    </row>
+    <row r="75" spans="1:8" ht="36">
+      <c r="A75" s="4" t="s">
+        <v>13</v>
+      </c>
+      <c r="B75" s="4"/>
+      <c r="C75" s="4" t="s">
+        <v>21</v>
+      </c>
+      <c r="D75" s="4" t="s">
+        <v>22</v>
+      </c>
+      <c r="E75" s="4"/>
+    </row>
+    <row r="76" spans="1:8" ht="12">
+      <c r="A76" s="4" t="s">
+        <v>18</v>
+      </c>
+      <c r="B76" s="4" t="s">
+        <v>23</v>
+      </c>
+      <c r="C76" s="4" t="s">
+        <v>24</v>
+      </c>
+      <c r="D76" s="4"/>
+      <c r="E76" s="4"/>
+    </row>
+    <row r="77" spans="1:8" ht="36">
+      <c r="A77" s="4" t="s">
+        <v>13</v>
+      </c>
+      <c r="B77" s="4"/>
+      <c r="C77" s="4" t="s">
+        <v>25</v>
+      </c>
+      <c r="D77" s="4" t="s">
+        <v>26</v>
+      </c>
+      <c r="E77" s="4"/>
+      <c r="H77" s="12"/>
+    </row>
+    <row r="78" spans="1:8" ht="12.75" customHeight="1">
+      <c r="A78" s="4" t="s">
+        <v>27</v>
+      </c>
+      <c r="B78" s="4"/>
+      <c r="C78" s="4"/>
+      <c r="D78" s="4"/>
+      <c r="E78" s="4"/>
+    </row>
+    <row r="79" spans="1:8" ht="12.75" customHeight="1">
+      <c r="A79" s="15" t="s">
+        <v>88</v>
+      </c>
+      <c r="B79" s="15"/>
+      <c r="C79" s="15"/>
+      <c r="D79" s="15"/>
+      <c r="E79" s="15"/>
+      <c r="F79" s="15"/>
+      <c r="G79" s="15"/>
+    </row>
+    <row r="80" spans="1:8" s="12" customFormat="1" ht="12.75" customHeight="1"/>
+    <row r="81" spans="1:9" s="14" customFormat="1" ht="12.75" customHeight="1">
+      <c r="A81" s="13" t="s">
         <v>117</v>
       </c>
-      <c r="D73" s="14" t="s">
+      <c r="D81" s="14" t="s">
         <v>118</v>
       </c>
-      <c r="H73" s="12"/>
-      <c r="I73" s="12"/>
-    </row>
-    <row r="74" spans="1:9" ht="12.75" customHeight="1">
-      <c r="A74" s="13" t="s">
+      <c r="H81" s="12"/>
+      <c r="I81" s="12"/>
+    </row>
+    <row r="82" spans="1:9" ht="12.75" customHeight="1">
+      <c r="A82" s="13" t="s">
         <v>94</v>
       </c>
-      <c r="B74" s="14"/>
-      <c r="C74" s="14"/>
-      <c r="D74" s="14" t="s">
+      <c r="B82" s="14"/>
+      <c r="C82" s="14"/>
+      <c r="D82" s="14" t="s">
         <v>89</v>
       </c>
-      <c r="E74" s="14"/>
-      <c r="F74" s="14"/>
-      <c r="G74" s="14"/>
-    </row>
-    <row r="75" spans="1:9" ht="12.75" customHeight="1">
-      <c r="A75" s="15" t="s">
+      <c r="E82" s="14"/>
+      <c r="F82" s="14"/>
+      <c r="G82" s="14"/>
+    </row>
+    <row r="83" spans="1:9" ht="12.75" customHeight="1">
+      <c r="A83" s="15" t="s">
         <v>134</v>
       </c>
-      <c r="B75" s="18"/>
-      <c r="C75" s="18"/>
-      <c r="D75" s="18"/>
-      <c r="E75" s="18"/>
-      <c r="F75" s="18"/>
-      <c r="G75" s="18"/>
-    </row>
-    <row r="76" spans="1:9" ht="12.75" customHeight="1">
-      <c r="A76" s="2" t="s">
+      <c r="B83" s="18"/>
+      <c r="C83" s="18"/>
+      <c r="D83" s="18"/>
+      <c r="E83" s="18"/>
+      <c r="F83" s="18"/>
+      <c r="G83" s="18"/>
+    </row>
+    <row r="84" spans="1:9" ht="12.75" customHeight="1">
+      <c r="A84" s="2" t="s">
         <v>236</v>
       </c>
-      <c r="B76" s="12" t="s">
+      <c r="B84" s="12" t="s">
         <v>90</v>
       </c>
-      <c r="C76" s="12" t="s">
+      <c r="C84" s="12" t="s">
         <v>91</v>
       </c>
-      <c r="D76" s="12"/>
-      <c r="E76" s="12" t="s">
+      <c r="D84" s="12"/>
+      <c r="E84" s="12" t="s">
         <v>92</v>
       </c>
-      <c r="F76" s="12"/>
-      <c r="G76" s="12"/>
-    </row>
-    <row r="77" spans="1:9" ht="12.75" customHeight="1">
-      <c r="A77" s="15" t="s">
+      <c r="F84" s="12"/>
+      <c r="G84" s="12"/>
+    </row>
+    <row r="85" spans="1:9" ht="12.75" customHeight="1">
+      <c r="A85" s="15" t="s">
         <v>93</v>
       </c>
-      <c r="B77" s="18"/>
-      <c r="C77" s="18"/>
-      <c r="D77" s="18"/>
-      <c r="E77" s="18"/>
-      <c r="F77" s="18"/>
-      <c r="G77" s="18"/>
-    </row>
-    <row r="78" spans="1:9" ht="12.75" customHeight="1">
-      <c r="B78" s="12"/>
-      <c r="C78" s="12"/>
-      <c r="D78" s="12"/>
-      <c r="E78" s="12"/>
-      <c r="F78" s="12"/>
-      <c r="G78" s="12"/>
-    </row>
-    <row r="79" spans="1:9" ht="12.75" customHeight="1">
-      <c r="A79" s="13" t="s">
+      <c r="B85" s="18"/>
+      <c r="C85" s="18"/>
+      <c r="D85" s="18"/>
+      <c r="E85" s="18"/>
+      <c r="F85" s="18"/>
+      <c r="G85" s="18"/>
+    </row>
+    <row r="86" spans="1:9" ht="12.75" customHeight="1">
+      <c r="B86" s="12"/>
+      <c r="C86" s="12"/>
+      <c r="D86" s="12"/>
+      <c r="E86" s="12"/>
+      <c r="F86" s="12"/>
+      <c r="G86" s="12"/>
+    </row>
+    <row r="87" spans="1:9" ht="12.75" customHeight="1">
+      <c r="A87" s="13" t="s">
         <v>125</v>
       </c>
-      <c r="B79" s="14"/>
-      <c r="C79" s="14"/>
-      <c r="D79" s="14" t="s">
+      <c r="B87" s="14"/>
+      <c r="C87" s="14"/>
+      <c r="D87" s="14" t="s">
         <v>127</v>
       </c>
-      <c r="E79" s="14"/>
-      <c r="F79" s="14"/>
-      <c r="G79" s="14"/>
-    </row>
-    <row r="80" spans="1:9" ht="12.75" customHeight="1">
-      <c r="A80" s="13" t="s">
+      <c r="E87" s="14"/>
+      <c r="F87" s="14"/>
+      <c r="G87" s="14"/>
+    </row>
+    <row r="88" spans="1:9" ht="12.75" customHeight="1">
+      <c r="A88" s="13" t="s">
         <v>126</v>
       </c>
-      <c r="B80" s="14"/>
-      <c r="C80" s="14"/>
-      <c r="D80" s="14" t="s">
+      <c r="B88" s="14"/>
+      <c r="C88" s="14"/>
+      <c r="D88" s="14" t="s">
         <v>128</v>
       </c>
-      <c r="E80" s="14"/>
-      <c r="F80" s="14"/>
-      <c r="G80" s="14"/>
-    </row>
-    <row r="81" spans="1:7" ht="12.75" customHeight="1">
-      <c r="A81" s="15" t="s">
+      <c r="E88" s="14"/>
+      <c r="F88" s="14"/>
+      <c r="G88" s="14"/>
+    </row>
+    <row r="89" spans="1:9" ht="12.75" customHeight="1">
+      <c r="A89" s="15" t="s">
         <v>135</v>
       </c>
-      <c r="B81" s="18"/>
-      <c r="C81" s="18"/>
-      <c r="D81" s="18"/>
-      <c r="E81" s="18"/>
-      <c r="F81" s="18"/>
-      <c r="G81" s="18"/>
-    </row>
-    <row r="82" spans="1:7" ht="12.75" customHeight="1">
-      <c r="A82" t="s">
+      <c r="B89" s="18"/>
+      <c r="C89" s="18"/>
+      <c r="D89" s="18"/>
+      <c r="E89" s="18"/>
+      <c r="F89" s="18"/>
+      <c r="G89" s="18"/>
+    </row>
+    <row r="90" spans="1:9" ht="12.75" customHeight="1">
+      <c r="A90" t="s">
         <v>235</v>
       </c>
-      <c r="B82" t="s">
+      <c r="B90" t="s">
         <v>67</v>
       </c>
-      <c r="C82" t="s">
+      <c r="C90" t="s">
         <v>69</v>
       </c>
-      <c r="E82" t="s">
+      <c r="E90" t="s">
         <v>6</v>
       </c>
-      <c r="F82" s="12"/>
-      <c r="G82" s="12"/>
-    </row>
-    <row r="83" spans="1:7" ht="12.75" customHeight="1">
-      <c r="A83" s="2" t="s">
+      <c r="F90" s="12"/>
+      <c r="G90" s="12"/>
+    </row>
+    <row r="91" spans="1:9" ht="12.75" customHeight="1">
+      <c r="A91" s="2" t="s">
         <v>13</v>
       </c>
-      <c r="B83" s="12"/>
-      <c r="C83" s="12" t="s">
+      <c r="B91" s="12"/>
+      <c r="C91" s="12" t="s">
         <v>66</v>
       </c>
-      <c r="D83" s="12"/>
-      <c r="E83" s="12"/>
-      <c r="F83" s="12"/>
-      <c r="G83" s="12"/>
-    </row>
-    <row r="84" spans="1:7" ht="12.75" customHeight="1">
-      <c r="A84" s="15" t="s">
+      <c r="D91" s="12"/>
+      <c r="E91" s="12"/>
+      <c r="F91" s="12"/>
+      <c r="G91" s="12"/>
+    </row>
+    <row r="92" spans="1:9" ht="12.75" customHeight="1">
+      <c r="A92" s="15" t="s">
         <v>129</v>
       </c>
-      <c r="B84" s="18"/>
-      <c r="C84" s="18"/>
-      <c r="D84" s="18"/>
-      <c r="E84" s="18"/>
-      <c r="F84" s="18"/>
-      <c r="G84" s="18"/>
-    </row>
-    <row r="87" spans="1:7" ht="12.75" customHeight="1">
-      <c r="A87" s="17" t="s">
+      <c r="B92" s="18"/>
+      <c r="C92" s="18"/>
+      <c r="D92" s="18"/>
+      <c r="E92" s="18"/>
+      <c r="F92" s="18"/>
+      <c r="G92" s="18"/>
+    </row>
+    <row r="95" spans="1:9" ht="12.75" customHeight="1">
+      <c r="A95" s="17" t="s">
         <v>112</v>
       </c>
     </row>
@@ -3538,8 +3749,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:B20"/>
   <sheetViews>
-    <sheetView zoomScale="150" zoomScaleNormal="150" zoomScalePageLayoutView="150" workbookViewId="0">
-      <selection activeCell="B22" sqref="B22"/>
+    <sheetView tabSelected="1" zoomScale="150" zoomScaleNormal="150" zoomScalePageLayoutView="150" workbookViewId="0">
+      <selection activeCell="A22" sqref="A22"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultColWidth="17.1640625" defaultRowHeight="12.75" customHeight="1" x14ac:dyDescent="0"/>
@@ -3645,66 +3856,66 @@
     </row>
     <row r="13" spans="1:2" ht="12.75" customHeight="1">
       <c r="A13" t="s">
-        <v>412</v>
+        <v>411</v>
       </c>
       <c r="B13" t="s">
-        <v>420</v>
+        <v>419</v>
       </c>
     </row>
     <row r="14" spans="1:2" ht="12.75" customHeight="1">
       <c r="A14" t="s">
-        <v>413</v>
+        <v>412</v>
       </c>
       <c r="B14" t="s">
-        <v>421</v>
+        <v>420</v>
       </c>
     </row>
     <row r="15" spans="1:2" ht="12.75" customHeight="1">
       <c r="A15" t="s">
-        <v>414</v>
+        <v>413</v>
       </c>
       <c r="B15" t="s">
-        <v>422</v>
+        <v>421</v>
       </c>
     </row>
     <row r="16" spans="1:2" ht="12.75" customHeight="1">
       <c r="A16" t="s">
-        <v>415</v>
+        <v>414</v>
       </c>
       <c r="B16" t="s">
-        <v>423</v>
+        <v>422</v>
       </c>
     </row>
     <row r="17" spans="1:2" ht="12.75" customHeight="1">
       <c r="A17" t="s">
-        <v>416</v>
+        <v>415</v>
       </c>
       <c r="B17" t="s">
-        <v>424</v>
+        <v>423</v>
       </c>
     </row>
     <row r="18" spans="1:2" ht="12.75" customHeight="1">
       <c r="A18" t="s">
-        <v>417</v>
+        <v>416</v>
       </c>
       <c r="B18" t="s">
-        <v>425</v>
+        <v>424</v>
       </c>
     </row>
     <row r="19" spans="1:2" ht="12.75" customHeight="1">
       <c r="A19" t="s">
+        <v>417</v>
+      </c>
+      <c r="B19" t="s">
         <v>418</v>
-      </c>
-      <c r="B19" t="s">
-        <v>419</v>
       </c>
     </row>
     <row r="20" spans="1:2" ht="12.75" customHeight="1">
       <c r="A20" t="s">
+        <v>428</v>
+      </c>
+      <c r="B20" t="s">
         <v>429</v>
-      </c>
-      <c r="B20" t="s">
-        <v>430</v>
       </c>
     </row>
   </sheetData>
@@ -3722,7 +3933,7 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:D134"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A31" workbookViewId="0">
+    <sheetView topLeftCell="A71" workbookViewId="0">
       <selection activeCell="A42" sqref="A42:XFD42"/>
     </sheetView>
   </sheetViews>
@@ -4015,7 +4226,7 @@
         <v>277</v>
       </c>
       <c r="B34" t="s">
-        <v>426</v>
+        <v>425</v>
       </c>
       <c r="C34" t="s">
         <v>402</v>

</xml_diff>

<commit_message>
Add calculators to Calculator and Nutrition Section
</commit_message>
<xml_diff>
--- a/opendatakit.collect2/form-files/neonatal/neonatal.xlsx
+++ b/opendatakit.collect2/form-files/neonatal/neonatal.xlsx
@@ -1,10 +1,10 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
-  <fileVersion appName="xl" lastEdited="5" lowestEdited="5" rupBuild="22905"/>
+  <fileVersion appName="xl" lastEdited="5" lowestEdited="5" rupBuild="21721"/>
   <workbookPr autoCompressPictures="0"/>
   <bookViews>
-    <workbookView xWindow="320" yWindow="0" windowWidth="24680" windowHeight="15340" tabRatio="500"/>
+    <workbookView xWindow="320" yWindow="0" windowWidth="20220" windowHeight="15340" tabRatio="500"/>
   </bookViews>
   <sheets>
     <sheet name="survey" sheetId="1" r:id="rId1"/>
@@ -23,7 +23,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="690" uniqueCount="498">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="830" uniqueCount="529">
   <si>
     <t>type</t>
   </si>
@@ -79,9 +79,6 @@
     <t>weightPound</t>
   </si>
   <si>
-    <t>Enter weight in pounds:</t>
-  </si>
-  <si>
     <t>&lt;p&gt;Baby weight is: {{calculates.convertToKilo}} kilograms&lt;/p&gt;</t>
   </si>
   <si>
@@ -91,9 +88,6 @@
     <t>weightKilo</t>
   </si>
   <si>
-    <t>Enter weight in kilograms:</t>
-  </si>
-  <si>
     <t>&lt;p&gt;Baby weight is: {{calculates.convertToPound}} pounds&lt;/p&gt;</t>
   </si>
   <si>
@@ -118,18 +112,6 @@
     <t>(data('weightKilo')*2.20462).toFixed(2)</t>
   </si>
   <si>
-    <t>weightLossKg</t>
-  </si>
-  <si>
-    <t>data('currentWeightKg') - data('birthWeightKg')</t>
-  </si>
-  <si>
-    <t>weightLossKgPerc</t>
-  </si>
-  <si>
-    <t>(calculates.weightLossKg() * 100.0 / data('birthWeightKg')).toFixed(2)</t>
-  </si>
-  <si>
     <t>list_name</t>
   </si>
   <si>
@@ -364,21 +346,6 @@
     <t>selected(data('menu'), 'medications')</t>
   </si>
   <si>
-    <t>weight loss</t>
-  </si>
-  <si>
-    <t>Weight Loss Calculators</t>
-  </si>
-  <si>
-    <t>weight converter</t>
-  </si>
-  <si>
-    <t>glucose</t>
-  </si>
-  <si>
-    <t>Weight Convertors Calculators</t>
-  </si>
-  <si>
     <t>Glucose Infusion Rate Calculator</t>
   </si>
   <si>
@@ -710,9 +677,6 @@
   </si>
   <si>
     <t>menu calculators_menu</t>
-  </si>
-  <si>
-    <t>menu nutritions_menu</t>
   </si>
   <si>
     <t>menu medications_menu</t>
@@ -1719,6 +1683,135 @@
   </si>
   <si>
     <t>&lt;b&gt;116&lt;/b&gt;</t>
+  </si>
+  <si>
+    <t>templatePath</t>
+  </si>
+  <si>
+    <t>selected(data('calculators_menu'),'weight_converter')</t>
+  </si>
+  <si>
+    <t>select_one conversion_type</t>
+  </si>
+  <si>
+    <t>conversion_type</t>
+  </si>
+  <si>
+    <t>Conversion type</t>
+  </si>
+  <si>
+    <t>selected(data('conversion_type'),'kgToLb')</t>
+  </si>
+  <si>
+    <t>Enter weight (kg):</t>
+  </si>
+  <si>
+    <t>selected(data('conversion_type'),'lbToKg')</t>
+  </si>
+  <si>
+    <t>Enter weight (lbs):</t>
+  </si>
+  <si>
+    <t>selected(data('calculators_menu'),'weight_loss')</t>
+  </si>
+  <si>
+    <t>birthW</t>
+  </si>
+  <si>
+    <t>Enter birth weigh (g):</t>
+  </si>
+  <si>
+    <t>currW</t>
+  </si>
+  <si>
+    <t>Enter current weight (g):</t>
+  </si>
+  <si>
+    <t>&lt;p&gt;Baby Weight Lost:&lt;/p&gt;</t>
+  </si>
+  <si>
+    <t>data('birthW') &amp;&amp; data('currW')</t>
+  </si>
+  <si>
+    <t>&lt;p&gt;{{calculates.weightLoss}} g&lt;/p&gt;</t>
+  </si>
+  <si>
+    <t>&lt;p&gt;{{calculates.weightLossPerc}} %&lt;/p&gt;</t>
+  </si>
+  <si>
+    <t>selected(data('calculators_menu'),'glucose_cal')</t>
+  </si>
+  <si>
+    <t>totalFluid</t>
+  </si>
+  <si>
+    <t>Total fluids (mL)</t>
+  </si>
+  <si>
+    <t>dextrosePerc</t>
+  </si>
+  <si>
+    <t>Dextrose percentage (%)</t>
+  </si>
+  <si>
+    <t>&lt;p&gt;Glucose Infusion Rate: {{calculates.glucoseCal}} g/kg/min&lt;/p&gt;</t>
+  </si>
+  <si>
+    <t>data('totalFluid') &amp;&amp; data('dextrosePerc')</t>
+  </si>
+  <si>
+    <t>kgToLb</t>
+  </si>
+  <si>
+    <t>Metric to imperial</t>
+  </si>
+  <si>
+    <t>lbToKg</t>
+  </si>
+  <si>
+    <t>Imperial to metric</t>
+  </si>
+  <si>
+    <t>weightLoss</t>
+  </si>
+  <si>
+    <t>weightLossPerc</t>
+  </si>
+  <si>
+    <t>data('birthW') - data('currW')</t>
+  </si>
+  <si>
+    <t>(calculates.weightLoss()*100.0/data('birthW')).toFixed(2)</t>
+  </si>
+  <si>
+    <t>glucoseCal</t>
+  </si>
+  <si>
+    <t>glucose_cal</t>
+  </si>
+  <si>
+    <t>(data('totalFluid')*(data('dextrosePerc')/100)/144).toFixed(2)</t>
+  </si>
+  <si>
+    <t>defaultConversionType</t>
+  </si>
+  <si>
+    <t>not(selected(data('conversion_type'),'kgToLb')) &amp;&amp; not(selected(data('conversion_type'),'lbToKg'))</t>
+  </si>
+  <si>
+    <t>default_weightKilo</t>
+  </si>
+  <si>
+    <t>data('default_weightKilo')</t>
+  </si>
+  <si>
+    <t>default_convertToPound</t>
+  </si>
+  <si>
+    <t>(data('default_weightKilo')*2.20462).toFixed(2)</t>
+  </si>
+  <si>
+    <t>&lt;p&gt;Baby weight is: {{calculates.default_convertToPound}} pounds&lt;/p&gt;</t>
   </si>
 </sst>
 </file>
@@ -1782,7 +1875,7 @@
       <family val="2"/>
     </font>
   </fonts>
-  <fills count="13">
+  <fills count="17">
     <fill>
       <patternFill patternType="none"/>
     </fill>
@@ -1853,6 +1946,30 @@
         <bgColor rgb="FF000000"/>
       </patternFill>
     </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor rgb="FFEBF1DE"/>
+        <bgColor rgb="FF000000"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor rgb="FFF2DCDB"/>
+        <bgColor rgb="FF000000"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor rgb="FFD8E4BC"/>
+        <bgColor rgb="FF000000"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor rgb="FFE6B8B7"/>
+        <bgColor rgb="FF000000"/>
+      </patternFill>
+    </fill>
   </fills>
   <borders count="1">
     <border>
@@ -1863,7 +1980,7 @@
       <diagonal/>
     </border>
   </borders>
-  <cellStyleXfs count="364">
+  <cellStyleXfs count="398">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
     <xf numFmtId="0" fontId="3" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
     <xf numFmtId="0" fontId="4" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
@@ -2228,8 +2345,42 @@
     <xf numFmtId="0" fontId="4" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
     <xf numFmtId="0" fontId="3" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
     <xf numFmtId="0" fontId="4" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="4" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="4" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="4" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="4" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="4" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="4" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="4" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="4" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="4" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="4" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="4" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="4" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="4" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="4" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="4" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="4" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="4" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
   </cellStyleXfs>
-  <cellXfs count="39">
+  <cellXfs count="43">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
       <alignment wrapText="1"/>
     </xf>
@@ -2307,8 +2458,20 @@
     <xf numFmtId="0" fontId="8" fillId="12" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1">
       <alignment wrapText="1"/>
     </xf>
+    <xf numFmtId="0" fontId="0" fillId="13" borderId="0" xfId="0" applyFill="1" applyAlignment="1">
+      <alignment wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="14" borderId="0" xfId="0" applyFill="1" applyAlignment="1">
+      <alignment wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="15" borderId="0" xfId="0" applyFill="1" applyAlignment="1">
+      <alignment wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="16" borderId="0" xfId="0" applyFill="1" applyAlignment="1">
+      <alignment wrapText="1"/>
+    </xf>
   </cellXfs>
-  <cellStyles count="364">
+  <cellStyles count="398">
     <cellStyle name="20% - Accent4" xfId="13" builtinId="42"/>
     <cellStyle name="Followed Hyperlink" xfId="2" builtinId="9" hidden="1"/>
     <cellStyle name="Followed Hyperlink" xfId="4" builtinId="9" hidden="1"/>
@@ -2490,6 +2653,23 @@
     <cellStyle name="Followed Hyperlink" xfId="359" builtinId="9" hidden="1"/>
     <cellStyle name="Followed Hyperlink" xfId="361" builtinId="9" hidden="1"/>
     <cellStyle name="Followed Hyperlink" xfId="363" builtinId="9" hidden="1"/>
+    <cellStyle name="Followed Hyperlink" xfId="365" builtinId="9" hidden="1"/>
+    <cellStyle name="Followed Hyperlink" xfId="367" builtinId="9" hidden="1"/>
+    <cellStyle name="Followed Hyperlink" xfId="369" builtinId="9" hidden="1"/>
+    <cellStyle name="Followed Hyperlink" xfId="371" builtinId="9" hidden="1"/>
+    <cellStyle name="Followed Hyperlink" xfId="373" builtinId="9" hidden="1"/>
+    <cellStyle name="Followed Hyperlink" xfId="375" builtinId="9" hidden="1"/>
+    <cellStyle name="Followed Hyperlink" xfId="377" builtinId="9" hidden="1"/>
+    <cellStyle name="Followed Hyperlink" xfId="379" builtinId="9" hidden="1"/>
+    <cellStyle name="Followed Hyperlink" xfId="381" builtinId="9" hidden="1"/>
+    <cellStyle name="Followed Hyperlink" xfId="383" builtinId="9" hidden="1"/>
+    <cellStyle name="Followed Hyperlink" xfId="385" builtinId="9" hidden="1"/>
+    <cellStyle name="Followed Hyperlink" xfId="387" builtinId="9" hidden="1"/>
+    <cellStyle name="Followed Hyperlink" xfId="389" builtinId="9" hidden="1"/>
+    <cellStyle name="Followed Hyperlink" xfId="391" builtinId="9" hidden="1"/>
+    <cellStyle name="Followed Hyperlink" xfId="393" builtinId="9" hidden="1"/>
+    <cellStyle name="Followed Hyperlink" xfId="395" builtinId="9" hidden="1"/>
+    <cellStyle name="Followed Hyperlink" xfId="397" builtinId="9" hidden="1"/>
     <cellStyle name="Good" xfId="11" builtinId="26"/>
     <cellStyle name="Hyperlink" xfId="1" builtinId="8" hidden="1"/>
     <cellStyle name="Hyperlink" xfId="3" builtinId="8" hidden="1"/>
@@ -2671,6 +2851,23 @@
     <cellStyle name="Hyperlink" xfId="358" builtinId="8" hidden="1"/>
     <cellStyle name="Hyperlink" xfId="360" builtinId="8" hidden="1"/>
     <cellStyle name="Hyperlink" xfId="362" builtinId="8" hidden="1"/>
+    <cellStyle name="Hyperlink" xfId="364" builtinId="8" hidden="1"/>
+    <cellStyle name="Hyperlink" xfId="366" builtinId="8" hidden="1"/>
+    <cellStyle name="Hyperlink" xfId="368" builtinId="8" hidden="1"/>
+    <cellStyle name="Hyperlink" xfId="370" builtinId="8" hidden="1"/>
+    <cellStyle name="Hyperlink" xfId="372" builtinId="8" hidden="1"/>
+    <cellStyle name="Hyperlink" xfId="374" builtinId="8" hidden="1"/>
+    <cellStyle name="Hyperlink" xfId="376" builtinId="8" hidden="1"/>
+    <cellStyle name="Hyperlink" xfId="378" builtinId="8" hidden="1"/>
+    <cellStyle name="Hyperlink" xfId="380" builtinId="8" hidden="1"/>
+    <cellStyle name="Hyperlink" xfId="382" builtinId="8" hidden="1"/>
+    <cellStyle name="Hyperlink" xfId="384" builtinId="8" hidden="1"/>
+    <cellStyle name="Hyperlink" xfId="386" builtinId="8" hidden="1"/>
+    <cellStyle name="Hyperlink" xfId="388" builtinId="8" hidden="1"/>
+    <cellStyle name="Hyperlink" xfId="390" builtinId="8" hidden="1"/>
+    <cellStyle name="Hyperlink" xfId="392" builtinId="8" hidden="1"/>
+    <cellStyle name="Hyperlink" xfId="394" builtinId="8" hidden="1"/>
+    <cellStyle name="Hyperlink" xfId="396" builtinId="8" hidden="1"/>
     <cellStyle name="Neutral" xfId="12" builtinId="28"/>
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
   </cellStyles>
@@ -3001,10 +3198,10 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <dimension ref="A1:J145"/>
+  <dimension ref="A1:J198"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A99" zoomScale="150" zoomScaleNormal="150" zoomScalePageLayoutView="150" workbookViewId="0">
-      <selection activeCell="E119" sqref="E119"/>
+    <sheetView tabSelected="1" topLeftCell="A118" zoomScale="150" zoomScaleNormal="150" zoomScalePageLayoutView="150" workbookViewId="0">
+      <selection activeCell="A130" sqref="A130:XFD130"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultColWidth="11.5" defaultRowHeight="12.75" customHeight="1" x14ac:dyDescent="0"/>
@@ -3016,9 +3213,9 @@
     <col min="6" max="6" width="15.33203125" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:8" ht="12">
+    <row r="1" spans="1:9" ht="12">
       <c r="A1" t="s">
-        <v>439</v>
+        <v>427</v>
       </c>
       <c r="B1" s="1" t="s">
         <v>0</v>
@@ -3033,27 +3230,30 @@
         <v>3</v>
       </c>
       <c r="F1" s="2" t="s">
-        <v>61</v>
+        <v>55</v>
       </c>
       <c r="G1" t="s">
-        <v>62</v>
+        <v>56</v>
       </c>
       <c r="H1" t="s">
-        <v>70</v>
-      </c>
-    </row>
-    <row r="2" spans="1:8" ht="15">
+        <v>64</v>
+      </c>
+      <c r="I1" t="s">
+        <v>486</v>
+      </c>
+    </row>
+    <row r="2" spans="1:9" ht="15">
       <c r="B2" s="16" t="s">
-        <v>106</v>
+        <v>100</v>
       </c>
       <c r="C2" s="1"/>
       <c r="D2" s="3"/>
       <c r="E2" s="4"/>
       <c r="F2" s="2"/>
     </row>
-    <row r="3" spans="1:8" ht="12">
+    <row r="3" spans="1:9" ht="12">
       <c r="B3" s="3" t="s">
-        <v>224</v>
+        <v>213</v>
       </c>
       <c r="C3" s="4" t="s">
         <v>4</v>
@@ -3066,47 +3266,47 @@
         <v>6</v>
       </c>
     </row>
-    <row r="4" spans="1:8" ht="12">
+    <row r="4" spans="1:9" ht="12">
       <c r="B4" s="3"/>
       <c r="C4" s="4"/>
       <c r="D4" s="4"/>
       <c r="E4" s="4"/>
       <c r="F4" s="2"/>
     </row>
-    <row r="5" spans="1:8" ht="12.75" customHeight="1">
+    <row r="5" spans="1:9" ht="12.75" customHeight="1">
       <c r="A5" s="22" t="s">
         <v>8</v>
       </c>
       <c r="B5" s="19" t="s">
-        <v>424</v>
+        <v>412</v>
       </c>
       <c r="C5" s="19"/>
       <c r="D5" s="19"/>
       <c r="E5" s="19" t="s">
-        <v>425</v>
+        <v>413</v>
       </c>
       <c r="F5" s="19"/>
       <c r="G5" s="19"/>
       <c r="H5" s="19"/>
     </row>
-    <row r="6" spans="1:8" ht="12.75" customHeight="1">
+    <row r="6" spans="1:9" ht="12.75" customHeight="1">
       <c r="A6" s="22"/>
       <c r="B6" s="19" t="s">
-        <v>426</v>
+        <v>414</v>
       </c>
       <c r="C6" s="19"/>
       <c r="D6" s="19"/>
       <c r="E6" s="19" t="s">
-        <v>427</v>
+        <v>415</v>
       </c>
       <c r="F6" s="19"/>
       <c r="G6" s="19"/>
       <c r="H6" s="19"/>
     </row>
-    <row r="7" spans="1:8" s="12" customFormat="1" ht="18" customHeight="1">
+    <row r="7" spans="1:9" s="12" customFormat="1" ht="18" customHeight="1">
       <c r="A7" s="23"/>
       <c r="B7" s="18" t="s">
-        <v>108</v>
+        <v>102</v>
       </c>
       <c r="C7" s="18"/>
       <c r="D7" s="18"/>
@@ -3115,10 +3315,10 @@
       <c r="G7" s="18"/>
       <c r="H7" s="18"/>
     </row>
-    <row r="8" spans="1:8" s="12" customFormat="1" ht="18" customHeight="1">
+    <row r="8" spans="1:9" s="12" customFormat="1" ht="18" customHeight="1">
       <c r="A8" s="23"/>
       <c r="B8" t="s">
-        <v>225</v>
+        <v>214</v>
       </c>
       <c r="C8" t="s">
         <v>7</v>
@@ -3131,99 +3331,99 @@
         <v>6</v>
       </c>
     </row>
-    <row r="9" spans="1:8" ht="18" customHeight="1">
+    <row r="9" spans="1:9" ht="18" customHeight="1">
       <c r="A9" s="22"/>
       <c r="B9" s="2" t="s">
         <v>13</v>
       </c>
       <c r="C9" s="2"/>
       <c r="D9" s="2" t="s">
-        <v>101</v>
+        <v>95</v>
       </c>
       <c r="E9" s="2" t="s">
-        <v>124</v>
+        <v>113</v>
       </c>
       <c r="F9" s="2"/>
       <c r="G9" t="s">
-        <v>126</v>
-      </c>
-    </row>
-    <row r="10" spans="1:8" ht="18" customHeight="1">
+        <v>115</v>
+      </c>
+    </row>
+    <row r="10" spans="1:9" ht="18" customHeight="1">
       <c r="A10" s="22"/>
       <c r="B10" s="2" t="s">
-        <v>102</v>
+        <v>96</v>
       </c>
       <c r="C10" s="4"/>
       <c r="D10" s="2" t="s">
-        <v>100</v>
+        <v>94</v>
       </c>
       <c r="E10" s="2" t="s">
-        <v>127</v>
+        <v>116</v>
       </c>
       <c r="F10" s="2"/>
     </row>
-    <row r="11" spans="1:8" ht="18" customHeight="1">
+    <row r="11" spans="1:9" ht="18" customHeight="1">
       <c r="A11" s="22"/>
       <c r="B11" s="2" t="s">
-        <v>102</v>
+        <v>96</v>
       </c>
       <c r="C11" s="4"/>
       <c r="D11" s="2" t="s">
-        <v>103</v>
+        <v>97</v>
       </c>
       <c r="E11" s="2" t="s">
-        <v>125</v>
+        <v>114</v>
       </c>
       <c r="F11" s="2"/>
     </row>
-    <row r="12" spans="1:8" ht="18" customHeight="1">
+    <row r="12" spans="1:9" ht="18" customHeight="1">
       <c r="A12" s="22"/>
       <c r="B12" s="2" t="s">
-        <v>270</v>
+        <v>258</v>
       </c>
       <c r="C12" s="2" t="s">
-        <v>271</v>
+        <v>259</v>
       </c>
       <c r="D12" s="2" t="s">
-        <v>79</v>
+        <v>73</v>
       </c>
       <c r="E12" s="2" t="s">
-        <v>131</v>
+        <v>120</v>
       </c>
       <c r="F12" s="2"/>
     </row>
-    <row r="13" spans="1:8" ht="12.75" customHeight="1">
+    <row r="13" spans="1:9" ht="12.75" customHeight="1">
       <c r="A13" s="22"/>
       <c r="B13" s="19" t="s">
-        <v>430</v>
+        <v>418</v>
       </c>
       <c r="C13" s="19"/>
       <c r="D13" s="19"/>
       <c r="E13" s="19" t="s">
-        <v>436</v>
+        <v>424</v>
       </c>
       <c r="F13" s="19"/>
       <c r="G13" s="19"/>
       <c r="H13" s="19"/>
     </row>
-    <row r="14" spans="1:8" ht="12.75" customHeight="1">
+    <row r="14" spans="1:9" ht="12.75" customHeight="1">
       <c r="A14" s="22"/>
       <c r="B14" s="19" t="s">
-        <v>431</v>
+        <v>419</v>
       </c>
       <c r="C14" s="19"/>
       <c r="D14" s="19"/>
       <c r="E14" s="19" t="s">
-        <v>273</v>
+        <v>261</v>
       </c>
       <c r="F14" s="19"/>
       <c r="G14" s="19"/>
       <c r="H14" s="19"/>
     </row>
-    <row r="15" spans="1:8" s="12" customFormat="1" ht="18" customHeight="1">
+    <row r="15" spans="1:9" s="12" customFormat="1" ht="18" customHeight="1">
       <c r="A15" s="23"/>
       <c r="B15" s="18" t="s">
-        <v>428</v>
+        <v>416</v>
       </c>
       <c r="C15" s="18"/>
       <c r="D15" s="18"/>
@@ -3232,113 +3432,113 @@
       <c r="G15" s="18"/>
       <c r="H15" s="18"/>
     </row>
-    <row r="16" spans="1:8" ht="12">
+    <row r="16" spans="1:9" ht="12">
       <c r="A16" s="22"/>
       <c r="B16" t="s">
-        <v>226</v>
+        <v>215</v>
       </c>
       <c r="C16" t="s">
-        <v>132</v>
+        <v>121</v>
       </c>
       <c r="D16" t="s">
-        <v>272</v>
+        <v>260</v>
       </c>
       <c r="E16" s="2"/>
     </row>
     <row r="17" spans="1:10" ht="11" customHeight="1">
       <c r="A17" s="22"/>
       <c r="B17" t="s">
-        <v>145</v>
+        <v>134</v>
       </c>
       <c r="C17" t="s">
-        <v>146</v>
+        <v>135</v>
       </c>
       <c r="D17" t="s">
-        <v>147</v>
+        <v>136</v>
       </c>
       <c r="E17" s="2" t="s">
-        <v>148</v>
+        <v>137</v>
       </c>
     </row>
     <row r="18" spans="1:10" ht="11" customHeight="1">
       <c r="A18" s="22"/>
       <c r="B18" t="s">
-        <v>149</v>
+        <v>138</v>
       </c>
       <c r="C18" t="s">
-        <v>150</v>
+        <v>139</v>
       </c>
       <c r="D18" t="s">
-        <v>151</v>
+        <v>140</v>
       </c>
       <c r="E18" s="2" t="s">
-        <v>152</v>
+        <v>141</v>
       </c>
     </row>
     <row r="19" spans="1:10" ht="11" customHeight="1">
       <c r="A19" s="22"/>
       <c r="B19" t="s">
-        <v>166</v>
+        <v>155</v>
       </c>
       <c r="C19" t="s">
-        <v>167</v>
+        <v>156</v>
       </c>
       <c r="D19" t="s">
-        <v>168</v>
+        <v>157</v>
       </c>
       <c r="E19" s="2" t="s">
-        <v>169</v>
+        <v>158</v>
       </c>
     </row>
     <row r="20" spans="1:10" ht="11" customHeight="1">
       <c r="A20" s="22"/>
       <c r="B20" t="s">
-        <v>238</v>
+        <v>226</v>
       </c>
       <c r="C20" t="s">
-        <v>239</v>
+        <v>227</v>
       </c>
       <c r="D20" t="s">
-        <v>240</v>
+        <v>228</v>
       </c>
       <c r="E20" s="2" t="s">
-        <v>241</v>
+        <v>229</v>
       </c>
     </row>
     <row r="21" spans="1:10" ht="11" customHeight="1">
       <c r="A21" s="22"/>
       <c r="B21" t="s">
-        <v>170</v>
+        <v>159</v>
       </c>
       <c r="C21" t="s">
-        <v>171</v>
+        <v>160</v>
       </c>
       <c r="D21" t="s">
-        <v>172</v>
+        <v>161</v>
       </c>
       <c r="E21" s="2" t="s">
-        <v>222</v>
+        <v>211</v>
       </c>
     </row>
     <row r="22" spans="1:10" ht="11" customHeight="1">
       <c r="A22" s="22"/>
       <c r="B22" t="s">
-        <v>173</v>
+        <v>162</v>
       </c>
       <c r="C22" t="s">
-        <v>174</v>
+        <v>163</v>
       </c>
       <c r="D22" t="s">
-        <v>175</v>
+        <v>164</v>
       </c>
       <c r="E22" s="2" t="s">
-        <v>223</v>
+        <v>212</v>
       </c>
     </row>
     <row r="23" spans="1:10" ht="11" customHeight="1">
       <c r="A23" s="22"/>
       <c r="B23" s="20" t="s">
-        <v>429</v>
+        <v>417</v>
       </c>
       <c r="C23" s="20"/>
       <c r="D23" s="20"/>
@@ -3352,12 +3552,12 @@
     <row r="24" spans="1:10" ht="12.75" customHeight="1">
       <c r="A24" s="22"/>
       <c r="B24" s="19" t="s">
-        <v>432</v>
+        <v>420</v>
       </c>
       <c r="C24" s="19"/>
       <c r="D24" s="19"/>
       <c r="E24" s="19" t="s">
-        <v>437</v>
+        <v>425</v>
       </c>
       <c r="F24" s="19"/>
       <c r="G24" s="19"/>
@@ -3366,12 +3566,12 @@
     <row r="25" spans="1:10" ht="12.75" customHeight="1">
       <c r="A25" s="22"/>
       <c r="B25" s="19" t="s">
-        <v>433</v>
+        <v>421</v>
       </c>
       <c r="C25" s="19"/>
       <c r="D25" s="19"/>
       <c r="E25" s="19" t="s">
-        <v>277</v>
+        <v>265</v>
       </c>
       <c r="F25" s="19"/>
       <c r="G25" s="19"/>
@@ -3380,7 +3580,7 @@
     <row r="26" spans="1:10" s="12" customFormat="1" ht="18" customHeight="1">
       <c r="A26" s="23"/>
       <c r="B26" s="18" t="s">
-        <v>434</v>
+        <v>422</v>
       </c>
       <c r="C26" s="18"/>
       <c r="D26" s="18"/>
@@ -3392,110 +3592,110 @@
     <row r="27" spans="1:10" ht="11" customHeight="1">
       <c r="A27" s="22"/>
       <c r="B27" t="s">
-        <v>274</v>
+        <v>262</v>
       </c>
       <c r="C27" t="s">
-        <v>275</v>
+        <v>263</v>
       </c>
       <c r="D27" t="s">
-        <v>276</v>
+        <v>264</v>
       </c>
       <c r="E27" s="2"/>
     </row>
     <row r="28" spans="1:10" ht="11" customHeight="1">
       <c r="A28" s="22"/>
       <c r="B28" t="s">
-        <v>325</v>
+        <v>313</v>
       </c>
       <c r="C28" t="s">
-        <v>305</v>
+        <v>293</v>
       </c>
       <c r="D28" t="s">
-        <v>283</v>
+        <v>271</v>
       </c>
       <c r="E28" s="2" t="s">
-        <v>284</v>
+        <v>272</v>
       </c>
     </row>
     <row r="29" spans="1:10" ht="11" customHeight="1">
       <c r="A29" s="22"/>
       <c r="B29" t="s">
-        <v>326</v>
+        <v>314</v>
       </c>
       <c r="C29" t="s">
-        <v>306</v>
+        <v>294</v>
       </c>
       <c r="D29" t="s">
-        <v>295</v>
+        <v>283</v>
       </c>
       <c r="E29" s="2" t="s">
-        <v>286</v>
+        <v>274</v>
       </c>
     </row>
     <row r="30" spans="1:10" ht="11" customHeight="1">
       <c r="A30" s="22"/>
       <c r="B30" t="s">
-        <v>327</v>
+        <v>315</v>
       </c>
       <c r="C30" t="s">
-        <v>307</v>
+        <v>295</v>
       </c>
       <c r="D30" t="s">
-        <v>298</v>
+        <v>286</v>
       </c>
       <c r="E30" s="2" t="s">
-        <v>287</v>
+        <v>275</v>
       </c>
     </row>
     <row r="31" spans="1:10" ht="11" customHeight="1">
       <c r="A31" s="22"/>
       <c r="B31" t="s">
-        <v>328</v>
+        <v>316</v>
       </c>
       <c r="C31" t="s">
-        <v>308</v>
+        <v>296</v>
       </c>
       <c r="D31" t="s">
-        <v>296</v>
+        <v>284</v>
       </c>
       <c r="E31" s="2" t="s">
-        <v>290</v>
+        <v>278</v>
       </c>
     </row>
     <row r="32" spans="1:10" ht="11" customHeight="1">
       <c r="A32" s="22"/>
       <c r="B32" t="s">
-        <v>329</v>
+        <v>317</v>
       </c>
       <c r="C32" t="s">
-        <v>309</v>
+        <v>297</v>
       </c>
       <c r="D32" t="s">
-        <v>297</v>
+        <v>285</v>
       </c>
       <c r="E32" s="2" t="s">
-        <v>292</v>
+        <v>280</v>
       </c>
     </row>
     <row r="33" spans="1:10" ht="12" customHeight="1">
       <c r="A33" s="22"/>
       <c r="B33" t="s">
-        <v>330</v>
+        <v>318</v>
       </c>
       <c r="C33" t="s">
-        <v>310</v>
+        <v>298</v>
       </c>
       <c r="D33" t="s">
-        <v>299</v>
+        <v>287</v>
       </c>
       <c r="E33" s="2" t="s">
-        <v>294</v>
+        <v>282</v>
       </c>
     </row>
     <row r="34" spans="1:10" ht="12" customHeight="1">
       <c r="A34" s="22"/>
       <c r="B34" s="20" t="s">
-        <v>435</v>
+        <v>423</v>
       </c>
       <c r="C34" s="20"/>
       <c r="D34" s="20"/>
@@ -3514,7 +3714,7 @@
       <c r="C35" s="4"/>
       <c r="D35" s="2"/>
       <c r="E35" s="2" t="s">
-        <v>420</v>
+        <v>408</v>
       </c>
       <c r="F35" s="2"/>
     </row>
@@ -3525,7 +3725,7 @@
       </c>
       <c r="C36" s="4"/>
       <c r="D36" s="2" t="s">
-        <v>398</v>
+        <v>386</v>
       </c>
       <c r="E36" s="2"/>
       <c r="F36" s="2"/>
@@ -3536,7 +3736,7 @@
         <v>13</v>
       </c>
       <c r="D37" t="s">
-        <v>232</v>
+        <v>220</v>
       </c>
     </row>
     <row r="38" spans="1:10" ht="25" customHeight="1">
@@ -3545,7 +3745,7 @@
         <v>13</v>
       </c>
       <c r="D38" t="s">
-        <v>245</v>
+        <v>233</v>
       </c>
     </row>
     <row r="39" spans="1:10" ht="25" customHeight="1">
@@ -3554,7 +3754,7 @@
         <v>13</v>
       </c>
       <c r="D39" t="s">
-        <v>246</v>
+        <v>234</v>
       </c>
     </row>
     <row r="40" spans="1:10" ht="25" customHeight="1">
@@ -3563,7 +3763,7 @@
         <v>13</v>
       </c>
       <c r="D40" t="s">
-        <v>268</v>
+        <v>256</v>
       </c>
     </row>
     <row r="41" spans="1:10" ht="25" customHeight="1">
@@ -3572,7 +3772,7 @@
         <v>13</v>
       </c>
       <c r="D41" t="s">
-        <v>247</v>
+        <v>235</v>
       </c>
     </row>
     <row r="42" spans="1:10" ht="25" customHeight="1">
@@ -3581,7 +3781,7 @@
         <v>13</v>
       </c>
       <c r="D42" t="s">
-        <v>248</v>
+        <v>236</v>
       </c>
     </row>
     <row r="43" spans="1:10" ht="25" customHeight="1">
@@ -3590,7 +3790,7 @@
         <v>13</v>
       </c>
       <c r="D43" t="s">
-        <v>269</v>
+        <v>257</v>
       </c>
     </row>
     <row r="44" spans="1:10" ht="25" customHeight="1">
@@ -3599,7 +3799,7 @@
         <v>13</v>
       </c>
       <c r="D44" t="s">
-        <v>397</v>
+        <v>385</v>
       </c>
     </row>
     <row r="45" spans="1:10" ht="25" customHeight="1">
@@ -3608,7 +3808,7 @@
         <v>13</v>
       </c>
       <c r="D45" t="s">
-        <v>399</v>
+        <v>387</v>
       </c>
     </row>
     <row r="46" spans="1:10" ht="25" customHeight="1">
@@ -3617,7 +3817,7 @@
         <v>13</v>
       </c>
       <c r="D46" t="s">
-        <v>400</v>
+        <v>388</v>
       </c>
     </row>
     <row r="47" spans="1:10" ht="25" customHeight="1">
@@ -3626,7 +3826,7 @@
         <v>13</v>
       </c>
       <c r="D47" t="s">
-        <v>438</v>
+        <v>426</v>
       </c>
     </row>
     <row r="48" spans="1:10" ht="25" customHeight="1">
@@ -3635,7 +3835,7 @@
         <v>13</v>
       </c>
       <c r="D48" t="s">
-        <v>401</v>
+        <v>389</v>
       </c>
     </row>
     <row r="49" spans="1:10" ht="25" customHeight="1">
@@ -3644,7 +3844,7 @@
         <v>13</v>
       </c>
       <c r="D49" t="s">
-        <v>402</v>
+        <v>390</v>
       </c>
     </row>
     <row r="50" spans="1:10" ht="25" customHeight="1">
@@ -3653,7 +3853,7 @@
         <v>13</v>
       </c>
       <c r="D50" t="s">
-        <v>403</v>
+        <v>391</v>
       </c>
     </row>
     <row r="51" spans="1:10" ht="25" customHeight="1">
@@ -3662,7 +3862,7 @@
         <v>13</v>
       </c>
       <c r="D51" t="s">
-        <v>404</v>
+        <v>392</v>
       </c>
     </row>
     <row r="52" spans="1:10" ht="25" customHeight="1">
@@ -3671,19 +3871,19 @@
         <v>13</v>
       </c>
       <c r="D52" t="s">
-        <v>421</v>
+        <v>409</v>
       </c>
     </row>
     <row r="53" spans="1:10" ht="25" customHeight="1">
       <c r="A53" s="22"/>
       <c r="B53" s="11" t="s">
-        <v>25</v>
+        <v>23</v>
       </c>
     </row>
     <row r="54" spans="1:10" ht="15">
       <c r="A54" s="22"/>
       <c r="B54" s="15" t="s">
-        <v>72</v>
+        <v>66</v>
       </c>
       <c r="C54" s="15"/>
       <c r="D54" s="15"/>
@@ -3703,15 +3903,15 @@
     </row>
     <row r="56" spans="1:10" s="15" customFormat="1" ht="15">
       <c r="A56" s="22" t="s">
-        <v>459</v>
+        <v>447</v>
       </c>
       <c r="B56" s="13" t="s">
-        <v>105</v>
+        <v>99</v>
       </c>
       <c r="C56" s="13"/>
       <c r="D56" s="13"/>
       <c r="E56" s="13" t="s">
-        <v>71</v>
+        <v>65</v>
       </c>
       <c r="F56" s="13"/>
       <c r="G56" s="13"/>
@@ -3722,12 +3922,12 @@
     <row r="57" spans="1:10" ht="12">
       <c r="A57" s="22"/>
       <c r="B57" s="5" t="s">
-        <v>73</v>
+        <v>67</v>
       </c>
       <c r="C57" s="5"/>
       <c r="D57" s="5"/>
       <c r="E57" s="6" t="s">
-        <v>74</v>
+        <v>68</v>
       </c>
       <c r="F57" s="5"/>
       <c r="G57" s="5"/>
@@ -3736,7 +3936,7 @@
     <row r="58" spans="1:10" ht="15">
       <c r="A58" s="22"/>
       <c r="B58" s="15" t="s">
-        <v>104</v>
+        <v>98</v>
       </c>
       <c r="C58" s="15"/>
       <c r="D58" s="15"/>
@@ -3748,7 +3948,7 @@
     <row r="59" spans="1:10" ht="12">
       <c r="A59" s="22"/>
       <c r="B59" s="12" t="s">
-        <v>227</v>
+        <v>216</v>
       </c>
       <c r="C59" s="12" t="s">
         <v>9</v>
@@ -3771,7 +3971,7 @@
       <c r="C60" s="8"/>
       <c r="D60" s="8"/>
       <c r="E60" s="9" t="s">
-        <v>63</v>
+        <v>57</v>
       </c>
       <c r="F60" s="8"/>
       <c r="G60" s="10"/>
@@ -3783,10 +3983,10 @@
         <v>13</v>
       </c>
       <c r="C61" s="2" t="s">
-        <v>75</v>
+        <v>69</v>
       </c>
       <c r="D61" s="2" t="s">
-        <v>440</v>
+        <v>428</v>
       </c>
       <c r="E61" s="2"/>
       <c r="F61" s="4"/>
@@ -3797,7 +3997,7 @@
         <v>13</v>
       </c>
       <c r="D62" t="s">
-        <v>441</v>
+        <v>429</v>
       </c>
       <c r="E62" s="2"/>
       <c r="F62" s="4"/>
@@ -3809,7 +4009,7 @@
       </c>
       <c r="C63" s="2"/>
       <c r="D63" s="2" t="s">
-        <v>442</v>
+        <v>430</v>
       </c>
       <c r="E63" s="2"/>
       <c r="F63" s="4"/>
@@ -3821,7 +4021,7 @@
       </c>
       <c r="C64" s="2"/>
       <c r="D64" s="2" t="s">
-        <v>443</v>
+        <v>431</v>
       </c>
       <c r="E64" s="2"/>
       <c r="F64" s="4"/>
@@ -3833,7 +4033,7 @@
       </c>
       <c r="C65" s="2"/>
       <c r="D65" s="2" t="s">
-        <v>444</v>
+        <v>432</v>
       </c>
       <c r="E65" s="2"/>
       <c r="F65" s="4"/>
@@ -3845,7 +4045,7 @@
       </c>
       <c r="C66" s="2"/>
       <c r="D66" s="2" t="s">
-        <v>445</v>
+        <v>433</v>
       </c>
       <c r="E66" s="2"/>
       <c r="F66" s="4"/>
@@ -3857,7 +4057,7 @@
       </c>
       <c r="C67" s="2"/>
       <c r="D67" s="2" t="s">
-        <v>446</v>
+        <v>434</v>
       </c>
       <c r="E67" s="2"/>
       <c r="F67" s="4"/>
@@ -3869,7 +4069,7 @@
       </c>
       <c r="C68" s="2"/>
       <c r="D68" s="2" t="s">
-        <v>447</v>
+        <v>435</v>
       </c>
       <c r="E68" s="2"/>
       <c r="F68" s="4"/>
@@ -3881,7 +4081,7 @@
       </c>
       <c r="C69" s="2"/>
       <c r="D69" s="2" t="s">
-        <v>455</v>
+        <v>443</v>
       </c>
       <c r="E69" s="2"/>
       <c r="F69" s="4"/>
@@ -3893,7 +4093,7 @@
       </c>
       <c r="C70" s="2"/>
       <c r="D70" s="2" t="s">
-        <v>454</v>
+        <v>442</v>
       </c>
       <c r="E70" s="2"/>
       <c r="F70" s="4"/>
@@ -3905,7 +4105,7 @@
       </c>
       <c r="C71" s="2"/>
       <c r="D71" s="2" t="s">
-        <v>456</v>
+        <v>444</v>
       </c>
       <c r="E71" s="2"/>
       <c r="F71" s="4"/>
@@ -3917,7 +4117,7 @@
       </c>
       <c r="C72" s="2"/>
       <c r="D72" s="2" t="s">
-        <v>457</v>
+        <v>445</v>
       </c>
       <c r="E72" s="2"/>
       <c r="F72" s="4"/>
@@ -3929,7 +4129,7 @@
       </c>
       <c r="C73" s="2"/>
       <c r="D73" s="2" t="s">
-        <v>448</v>
+        <v>436</v>
       </c>
       <c r="E73" s="2"/>
       <c r="F73" s="4"/>
@@ -3941,7 +4141,7 @@
       </c>
       <c r="C74" s="2"/>
       <c r="D74" s="2" t="s">
-        <v>451</v>
+        <v>439</v>
       </c>
       <c r="E74" s="2"/>
       <c r="F74" s="4"/>
@@ -3953,7 +4153,7 @@
       </c>
       <c r="C75" s="2"/>
       <c r="D75" s="2" t="s">
-        <v>452</v>
+        <v>440</v>
       </c>
       <c r="E75" s="2"/>
       <c r="F75" s="4"/>
@@ -3965,7 +4165,7 @@
       </c>
       <c r="C76" s="2"/>
       <c r="D76" s="2" t="s">
-        <v>453</v>
+        <v>441</v>
       </c>
       <c r="E76" s="2"/>
       <c r="F76" s="4"/>
@@ -3977,7 +4177,7 @@
       </c>
       <c r="C77" s="2"/>
       <c r="D77" s="2" t="s">
-        <v>449</v>
+        <v>437</v>
       </c>
       <c r="E77" s="2"/>
       <c r="F77" s="4"/>
@@ -3989,7 +4189,7 @@
       </c>
       <c r="C78" s="2"/>
       <c r="D78" s="2" t="s">
-        <v>450</v>
+        <v>438</v>
       </c>
       <c r="E78" s="2"/>
       <c r="F78" s="4"/>
@@ -4001,7 +4201,7 @@
       </c>
       <c r="C79" s="2"/>
       <c r="D79" s="2" t="s">
-        <v>458</v>
+        <v>446</v>
       </c>
       <c r="E79" s="2"/>
       <c r="F79" s="4"/>
@@ -4030,7 +4230,7 @@
         <v>13</v>
       </c>
       <c r="C82" s="2" t="s">
-        <v>76</v>
+        <v>70</v>
       </c>
       <c r="D82" s="2"/>
       <c r="E82" s="2"/>
@@ -4045,7 +4245,7 @@
         <v>13</v>
       </c>
       <c r="D83" t="s">
-        <v>77</v>
+        <v>71</v>
       </c>
       <c r="E83" s="13"/>
     </row>
@@ -4055,13 +4255,13 @@
         <v>13</v>
       </c>
       <c r="H84" t="s">
-        <v>78</v>
+        <v>72</v>
       </c>
     </row>
     <row r="85" spans="1:8" ht="12">
       <c r="A85" s="22"/>
       <c r="B85" s="11" t="s">
-        <v>25</v>
+        <v>23</v>
       </c>
       <c r="C85" s="10"/>
       <c r="D85" s="10"/>
@@ -4073,23 +4273,23 @@
     <row r="86" spans="1:8" s="10" customFormat="1" ht="12"/>
     <row r="87" spans="1:8" s="10" customFormat="1" ht="15">
       <c r="B87" s="10" t="s">
-        <v>489</v>
+        <v>477</v>
       </c>
       <c r="E87" s="13" t="s">
-        <v>494</v>
+        <v>482</v>
       </c>
     </row>
     <row r="88" spans="1:8" s="10" customFormat="1" ht="15">
       <c r="B88" s="10" t="s">
-        <v>490</v>
+        <v>478</v>
       </c>
       <c r="E88" s="38" t="s">
-        <v>493</v>
+        <v>481</v>
       </c>
     </row>
     <row r="89" spans="1:8" s="10" customFormat="1" ht="12">
       <c r="B89" s="10" t="s">
-        <v>491</v>
+        <v>479</v>
       </c>
     </row>
     <row r="90" spans="1:8" s="10" customFormat="1" ht="12">
@@ -4097,24 +4297,24 @@
         <v>13</v>
       </c>
       <c r="D90" s="10" t="s">
-        <v>42</v>
+        <v>36</v>
       </c>
     </row>
     <row r="91" spans="1:8" s="10" customFormat="1" ht="12">
       <c r="B91" s="10" t="s">
-        <v>492</v>
+        <v>480</v>
       </c>
     </row>
     <row r="92" spans="1:8" s="10" customFormat="1" ht="12"/>
     <row r="93" spans="1:8" ht="30">
       <c r="A93" s="22"/>
       <c r="B93" s="13" t="s">
-        <v>464</v>
+        <v>452</v>
       </c>
       <c r="C93" s="13"/>
       <c r="D93" s="13"/>
       <c r="E93" s="13" t="s">
-        <v>460</v>
+        <v>448</v>
       </c>
       <c r="F93" s="13"/>
       <c r="G93" s="13"/>
@@ -4123,12 +4323,12 @@
     <row r="94" spans="1:8" ht="30">
       <c r="A94" s="22"/>
       <c r="B94" s="13" t="s">
-        <v>465</v>
+        <v>453</v>
       </c>
       <c r="C94" s="13"/>
       <c r="D94" s="13"/>
       <c r="E94" s="13" t="s">
-        <v>466</v>
+        <v>454</v>
       </c>
       <c r="F94" s="13"/>
       <c r="G94" s="13"/>
@@ -4137,7 +4337,7 @@
     <row r="95" spans="1:8" ht="15">
       <c r="A95" s="22"/>
       <c r="B95" s="15" t="s">
-        <v>462</v>
+        <v>450</v>
       </c>
       <c r="C95" s="15"/>
       <c r="D95" s="15"/>
@@ -4159,10 +4359,10 @@
     <row r="97" spans="1:8" ht="24">
       <c r="A97" s="22"/>
       <c r="B97" t="s">
-        <v>473</v>
+        <v>461</v>
       </c>
       <c r="C97" t="s">
-        <v>472</v>
+        <v>460</v>
       </c>
       <c r="F97" t="s">
         <v>6</v>
@@ -4173,12 +4373,12 @@
     <row r="98" spans="1:8" ht="30">
       <c r="A98" s="22"/>
       <c r="B98" s="13" t="s">
-        <v>478</v>
+        <v>466</v>
       </c>
       <c r="C98" s="13"/>
       <c r="D98" s="13"/>
       <c r="E98" s="13" t="s">
-        <v>475</v>
+        <v>463</v>
       </c>
       <c r="F98" s="13"/>
       <c r="G98" s="10"/>
@@ -4187,12 +4387,12 @@
     <row r="99" spans="1:8" ht="30">
       <c r="A99" s="22"/>
       <c r="B99" s="13" t="s">
-        <v>479</v>
+        <v>467</v>
       </c>
       <c r="C99" s="13"/>
       <c r="D99" s="13"/>
       <c r="E99" s="13" t="s">
-        <v>480</v>
+        <v>468</v>
       </c>
       <c r="F99" s="13"/>
       <c r="G99" s="10"/>
@@ -4201,7 +4401,7 @@
     <row r="100" spans="1:8" ht="15">
       <c r="A100" s="22"/>
       <c r="B100" s="15" t="s">
-        <v>476</v>
+        <v>464</v>
       </c>
       <c r="C100" s="15"/>
       <c r="D100" s="15"/>
@@ -4224,7 +4424,7 @@
       </c>
       <c r="C102" s="12"/>
       <c r="D102" s="26" t="s">
-        <v>487</v>
+        <v>475</v>
       </c>
       <c r="E102" s="12"/>
       <c r="F102" s="12"/>
@@ -4234,7 +4434,7 @@
     <row r="103" spans="1:8" ht="12">
       <c r="A103" s="22"/>
       <c r="B103" s="2" t="s">
-        <v>25</v>
+        <v>23</v>
       </c>
       <c r="C103" s="12"/>
       <c r="D103" s="26"/>
@@ -4246,7 +4446,7 @@
     <row r="104" spans="1:8" ht="15">
       <c r="A104" s="22"/>
       <c r="B104" s="15" t="s">
-        <v>477</v>
+        <v>465</v>
       </c>
       <c r="C104" s="18"/>
       <c r="D104" s="32"/>
@@ -4258,24 +4458,24 @@
     <row r="105" spans="1:8" ht="30">
       <c r="A105" s="28"/>
       <c r="B105" s="13" t="s">
-        <v>482</v>
+        <v>470</v>
       </c>
       <c r="C105" s="13"/>
       <c r="D105" s="13"/>
       <c r="E105" s="13" t="s">
-        <v>474</v>
+        <v>462</v>
       </c>
       <c r="F105" s="13"/>
     </row>
     <row r="106" spans="1:8" ht="30">
       <c r="A106" s="28"/>
       <c r="B106" s="13" t="s">
-        <v>483</v>
+        <v>471</v>
       </c>
       <c r="C106" s="13"/>
       <c r="D106" s="13"/>
       <c r="E106" s="13" t="s">
-        <v>484</v>
+        <v>472</v>
       </c>
       <c r="F106" s="13"/>
     </row>
@@ -4285,7 +4485,7 @@
       </c>
       <c r="C107" s="27"/>
       <c r="D107" s="27" t="s">
-        <v>496</v>
+        <v>484</v>
       </c>
       <c r="E107" s="27"/>
       <c r="F107" s="27"/>
@@ -4293,7 +4493,7 @@
     <row r="108" spans="1:8" ht="15">
       <c r="A108" s="28"/>
       <c r="B108" s="15" t="s">
-        <v>485</v>
+        <v>473</v>
       </c>
       <c r="C108" s="15"/>
       <c r="D108" s="15"/>
@@ -4313,7 +4513,7 @@
       </c>
       <c r="C110" s="21"/>
       <c r="D110" s="29" t="s">
-        <v>481</v>
+        <v>469</v>
       </c>
       <c r="E110" s="29"/>
       <c r="F110" s="21"/>
@@ -4321,7 +4521,7 @@
     <row r="111" spans="1:8" ht="12">
       <c r="A111" s="28"/>
       <c r="B111" t="s">
-        <v>25</v>
+        <v>23</v>
       </c>
       <c r="C111" s="21"/>
       <c r="D111" s="29"/>
@@ -4338,7 +4538,7 @@
     <row r="113" spans="1:9" ht="15">
       <c r="A113" s="28"/>
       <c r="B113" s="15" t="s">
-        <v>486</v>
+        <v>474</v>
       </c>
       <c r="C113" s="30"/>
       <c r="D113" s="31"/>
@@ -4351,7 +4551,7 @@
       </c>
       <c r="C114" s="34"/>
       <c r="D114" s="35" t="s">
-        <v>495</v>
+        <v>483</v>
       </c>
       <c r="E114" s="34"/>
       <c r="F114" s="34"/>
@@ -4359,7 +4559,7 @@
     <row r="115" spans="1:9" ht="15">
       <c r="A115" s="28"/>
       <c r="B115" s="15" t="s">
-        <v>463</v>
+        <v>451</v>
       </c>
       <c r="C115" s="30"/>
       <c r="D115" s="31"/>
@@ -4372,7 +4572,7 @@
       </c>
       <c r="C116" s="34"/>
       <c r="D116" s="35" t="s">
-        <v>497</v>
+        <v>485</v>
       </c>
       <c r="E116" s="34"/>
       <c r="F116" s="34"/>
@@ -4380,7 +4580,7 @@
     <row r="117" spans="1:9" ht="15">
       <c r="A117" s="28"/>
       <c r="B117" s="15" t="s">
-        <v>80</v>
+        <v>74</v>
       </c>
       <c r="C117" s="30"/>
       <c r="D117" s="31"/>
@@ -4398,33 +4598,33 @@
     <row r="119" spans="1:9" s="13" customFormat="1" ht="15">
       <c r="A119" s="27"/>
       <c r="B119" s="13" t="s">
-        <v>109</v>
+        <v>103</v>
       </c>
       <c r="C119" s="36"/>
       <c r="D119" s="37"/>
       <c r="E119" s="14" t="s">
-        <v>488</v>
+        <v>476</v>
       </c>
       <c r="F119" s="36"/>
     </row>
     <row r="120" spans="1:9" s="13" customFormat="1" ht="15">
       <c r="A120" s="27"/>
       <c r="B120" s="13" t="s">
-        <v>81</v>
+        <v>75</v>
       </c>
       <c r="C120" s="36"/>
       <c r="D120" s="37"/>
       <c r="E120" s="14" t="s">
-        <v>82</v>
+        <v>76</v>
       </c>
       <c r="F120" s="36"/>
     </row>
     <row r="121" spans="1:9" ht="15">
       <c r="A121" s="22" t="s">
-        <v>470</v>
+        <v>458</v>
       </c>
       <c r="B121" s="15" t="s">
-        <v>110</v>
+        <v>104</v>
       </c>
       <c r="C121" s="15"/>
       <c r="D121" s="15"/>
@@ -4436,7 +4636,7 @@
     <row r="122" spans="1:9" ht="12">
       <c r="A122" s="22"/>
       <c r="B122" t="s">
-        <v>228</v>
+        <v>217</v>
       </c>
       <c r="C122" t="s">
         <v>11</v>
@@ -4447,261 +4647,772 @@
       <c r="F122" t="s">
         <v>6</v>
       </c>
-      <c r="G122" s="12"/>
-      <c r="H122" s="12"/>
+      <c r="G122" s="21"/>
+      <c r="H122" s="21"/>
     </row>
     <row r="123" spans="1:9" ht="12">
       <c r="A123" s="22"/>
-      <c r="B123" s="4" t="s">
+      <c r="B123" s="39" t="s">
         <v>15</v>
       </c>
-      <c r="C123" s="4"/>
-      <c r="D123" s="4"/>
-      <c r="E123" s="4"/>
-      <c r="F123" s="4"/>
+      <c r="E123" t="s">
+        <v>487</v>
+      </c>
     </row>
     <row r="124" spans="1:9" ht="12">
       <c r="A124" s="22"/>
-      <c r="B124" s="4" t="s">
+      <c r="B124" t="s">
+        <v>13</v>
+      </c>
+      <c r="D124" t="s">
+        <v>41</v>
+      </c>
+    </row>
+    <row r="125" spans="1:9" ht="12">
+      <c r="A125" s="22"/>
+      <c r="B125" t="s">
+        <v>488</v>
+      </c>
+      <c r="C125" t="s">
+        <v>489</v>
+      </c>
+      <c r="D125" t="s">
+        <v>490</v>
+      </c>
+      <c r="F125" t="s">
+        <v>81</v>
+      </c>
+    </row>
+    <row r="126" spans="1:9" ht="12.75" customHeight="1">
+      <c r="A126" s="28"/>
+      <c r="B126" s="39" t="s">
+        <v>15</v>
+      </c>
+      <c r="C126" t="s">
+        <v>522</v>
+      </c>
+      <c r="E126" t="s">
+        <v>523</v>
+      </c>
+    </row>
+    <row r="127" spans="1:9" ht="12.75" customHeight="1">
+      <c r="A127" s="28"/>
+      <c r="B127" t="s">
         <v>16</v>
       </c>
-      <c r="C124" s="4" t="s">
+      <c r="C127" t="s">
+        <v>524</v>
+      </c>
+      <c r="D127" t="s">
+        <v>492</v>
+      </c>
+    </row>
+    <row r="128" spans="1:9" ht="12.75" customHeight="1">
+      <c r="A128" s="28"/>
+      <c r="B128" t="s">
+        <v>13</v>
+      </c>
+      <c r="D128" t="s">
+        <v>528</v>
+      </c>
+      <c r="E128" t="s">
+        <v>525</v>
+      </c>
+      <c r="I128" s="21"/>
+    </row>
+    <row r="129" spans="1:9" ht="12.75" customHeight="1">
+      <c r="A129" s="28"/>
+      <c r="B129" s="40" t="s">
+        <v>23</v>
+      </c>
+    </row>
+    <row r="130" spans="1:9" ht="12">
+      <c r="A130" s="22"/>
+      <c r="B130" s="39" t="s">
+        <v>15</v>
+      </c>
+      <c r="E130" t="s">
+        <v>491</v>
+      </c>
+    </row>
+    <row r="131" spans="1:9" ht="12">
+      <c r="A131" s="22"/>
+      <c r="B131" t="s">
+        <v>16</v>
+      </c>
+      <c r="C131" t="s">
+        <v>20</v>
+      </c>
+      <c r="D131" t="s">
+        <v>492</v>
+      </c>
+    </row>
+    <row r="132" spans="1:9" ht="12.75" customHeight="1">
+      <c r="A132" s="22"/>
+      <c r="B132" t="s">
+        <v>13</v>
+      </c>
+      <c r="D132" t="s">
+        <v>21</v>
+      </c>
+      <c r="E132" t="s">
+        <v>22</v>
+      </c>
+      <c r="I132" s="21"/>
+    </row>
+    <row r="133" spans="1:9" ht="12.75" customHeight="1">
+      <c r="A133" s="22"/>
+      <c r="B133" s="40" t="s">
+        <v>23</v>
+      </c>
+    </row>
+    <row r="134" spans="1:9" ht="12.75" customHeight="1">
+      <c r="A134" s="22"/>
+      <c r="B134" s="39" t="s">
+        <v>15</v>
+      </c>
+      <c r="E134" t="s">
+        <v>493</v>
+      </c>
+    </row>
+    <row r="135" spans="1:9" ht="12.75" customHeight="1">
+      <c r="A135" s="22"/>
+      <c r="B135" t="s">
+        <v>16</v>
+      </c>
+      <c r="C135" t="s">
         <v>17</v>
       </c>
-      <c r="D124" s="4" t="s">
+      <c r="D135" t="s">
+        <v>494</v>
+      </c>
+    </row>
+    <row r="136" spans="1:9" ht="12.75" customHeight="1">
+      <c r="A136" s="22"/>
+      <c r="B136" t="s">
+        <v>13</v>
+      </c>
+      <c r="D136" t="s">
         <v>18</v>
       </c>
-      <c r="E124" s="4"/>
-      <c r="F124" s="4"/>
-    </row>
-    <row r="125" spans="1:9" ht="36">
-      <c r="A125" s="22"/>
-      <c r="B125" s="4" t="s">
-        <v>13</v>
-      </c>
-      <c r="C125" s="4"/>
-      <c r="D125" s="4" t="s">
+      <c r="E136" t="s">
         <v>19</v>
       </c>
-      <c r="E125" s="4" t="s">
-        <v>20</v>
-      </c>
-      <c r="F125" s="4"/>
-    </row>
-    <row r="126" spans="1:9" ht="12">
-      <c r="A126" s="22"/>
-      <c r="B126" s="4" t="s">
-        <v>16</v>
-      </c>
-      <c r="C126" s="4" t="s">
-        <v>21</v>
-      </c>
-      <c r="D126" s="4" t="s">
-        <v>22</v>
-      </c>
-      <c r="E126" s="4"/>
-      <c r="F126" s="4"/>
-    </row>
-    <row r="127" spans="1:9" ht="36">
-      <c r="A127" s="22"/>
-      <c r="B127" s="4" t="s">
-        <v>13</v>
-      </c>
-      <c r="C127" s="4"/>
-      <c r="D127" s="4" t="s">
+    </row>
+    <row r="137" spans="1:9" ht="12.75" customHeight="1">
+      <c r="A137" s="22"/>
+      <c r="B137" s="40" t="s">
         <v>23</v>
       </c>
-      <c r="E127" s="4" t="s">
-        <v>24</v>
-      </c>
-      <c r="F127" s="4"/>
-      <c r="I127" s="12"/>
-    </row>
-    <row r="128" spans="1:9" ht="12.75" customHeight="1">
-      <c r="A128" s="22"/>
-      <c r="B128" s="4" t="s">
-        <v>25</v>
-      </c>
-      <c r="C128" s="4"/>
-      <c r="D128" s="4"/>
-      <c r="E128" s="4"/>
-      <c r="F128" s="4"/>
-    </row>
-    <row r="129" spans="1:10" ht="12.75" customHeight="1">
-      <c r="A129" s="22"/>
-      <c r="B129" s="15" t="s">
-        <v>83</v>
-      </c>
-      <c r="C129" s="15"/>
-      <c r="D129" s="15"/>
-      <c r="E129" s="15"/>
-      <c r="F129" s="15"/>
-      <c r="G129" s="15"/>
-      <c r="H129" s="15"/>
-    </row>
-    <row r="130" spans="1:10" s="12" customFormat="1" ht="12.75" customHeight="1"/>
-    <row r="131" spans="1:10" s="14" customFormat="1" ht="12.75" customHeight="1">
-      <c r="A131" s="25"/>
-      <c r="B131" s="13" t="s">
-        <v>111</v>
-      </c>
-      <c r="E131" s="14" t="s">
-        <v>112</v>
-      </c>
-      <c r="I131" s="12"/>
-      <c r="J131" s="12"/>
-    </row>
-    <row r="132" spans="1:10" ht="12.75" customHeight="1">
-      <c r="B132" s="13" t="s">
-        <v>89</v>
-      </c>
-      <c r="C132" s="14"/>
-      <c r="D132" s="14"/>
-      <c r="E132" s="14" t="s">
-        <v>84</v>
-      </c>
-      <c r="F132" s="14"/>
-      <c r="G132" s="14"/>
-      <c r="H132" s="14"/>
-    </row>
-    <row r="133" spans="1:10" ht="12.75" customHeight="1">
-      <c r="A133" s="22" t="s">
-        <v>471</v>
-      </c>
-      <c r="B133" s="15" t="s">
-        <v>128</v>
-      </c>
-      <c r="C133" s="18"/>
-      <c r="D133" s="18"/>
-      <c r="E133" s="18"/>
-      <c r="F133" s="18"/>
-      <c r="G133" s="18"/>
-      <c r="H133" s="18"/>
-    </row>
-    <row r="134" spans="1:10" ht="12.75" customHeight="1">
-      <c r="A134" s="22"/>
-      <c r="B134" s="2" t="s">
-        <v>230</v>
-      </c>
-      <c r="C134" s="12" t="s">
-        <v>85</v>
-      </c>
-      <c r="D134" s="12" t="s">
-        <v>86</v>
-      </c>
-      <c r="E134" s="12"/>
-      <c r="F134" s="12" t="s">
-        <v>87</v>
-      </c>
-      <c r="G134" s="12"/>
-      <c r="H134" s="12"/>
-    </row>
-    <row r="135" spans="1:10" ht="12.75" customHeight="1">
-      <c r="A135" s="22"/>
-      <c r="B135" s="15" t="s">
-        <v>88</v>
-      </c>
-      <c r="C135" s="18"/>
-      <c r="D135" s="18"/>
-      <c r="E135" s="18"/>
-      <c r="F135" s="18"/>
-      <c r="G135" s="18"/>
-      <c r="H135" s="18"/>
-    </row>
-    <row r="136" spans="1:10" ht="12.75" customHeight="1">
-      <c r="C136" s="12"/>
-      <c r="D136" s="12"/>
-      <c r="E136" s="12"/>
-      <c r="F136" s="12"/>
-      <c r="G136" s="12"/>
-      <c r="H136" s="12"/>
-    </row>
-    <row r="137" spans="1:10" ht="12.75" customHeight="1">
-      <c r="B137" s="13" t="s">
-        <v>119</v>
-      </c>
-      <c r="C137" s="14"/>
-      <c r="D137" s="14"/>
-      <c r="E137" s="14" t="s">
-        <v>121</v>
-      </c>
-      <c r="F137" s="14"/>
-      <c r="G137" s="14"/>
-      <c r="H137" s="14"/>
-    </row>
-    <row r="138" spans="1:10" ht="12.75" customHeight="1">
-      <c r="B138" s="13" t="s">
-        <v>120</v>
-      </c>
-      <c r="C138" s="14"/>
-      <c r="D138" s="14"/>
-      <c r="E138" s="14" t="s">
-        <v>122</v>
-      </c>
-      <c r="F138" s="14"/>
-      <c r="G138" s="14"/>
-      <c r="H138" s="14"/>
-    </row>
-    <row r="139" spans="1:10" ht="12.75" customHeight="1">
-      <c r="A139" s="22" t="s">
-        <v>64</v>
-      </c>
-      <c r="B139" s="15" t="s">
-        <v>129</v>
-      </c>
-      <c r="C139" s="18"/>
-      <c r="D139" s="18"/>
-      <c r="E139" s="18"/>
-      <c r="F139" s="18"/>
-      <c r="G139" s="18"/>
-      <c r="H139" s="18"/>
-    </row>
-    <row r="140" spans="1:10" ht="12.75" customHeight="1">
+    </row>
+    <row r="138" spans="1:9" ht="12.75" customHeight="1">
+      <c r="A138" s="22"/>
+      <c r="B138" s="40" t="s">
+        <v>23</v>
+      </c>
+    </row>
+    <row r="139" spans="1:9" ht="12.75" customHeight="1">
+      <c r="A139" s="22"/>
+      <c r="B139" s="41" t="s">
+        <v>15</v>
+      </c>
+      <c r="E139" t="s">
+        <v>495</v>
+      </c>
+    </row>
+    <row r="140" spans="1:9" ht="12.75" customHeight="1">
       <c r="A140" s="22"/>
       <c r="B140" t="s">
-        <v>229</v>
-      </c>
-      <c r="C140" t="s">
-        <v>65</v>
+        <v>13</v>
       </c>
       <c r="D140" t="s">
-        <v>67</v>
-      </c>
-      <c r="F140" t="s">
+        <v>43</v>
+      </c>
+    </row>
+    <row r="141" spans="1:9" ht="12.75" customHeight="1">
+      <c r="A141" s="22"/>
+      <c r="B141" t="s">
+        <v>16</v>
+      </c>
+      <c r="C141" t="s">
+        <v>496</v>
+      </c>
+      <c r="D141" t="s">
+        <v>497</v>
+      </c>
+    </row>
+    <row r="142" spans="1:9" ht="12.75" customHeight="1">
+      <c r="A142" s="22"/>
+      <c r="B142" t="s">
+        <v>16</v>
+      </c>
+      <c r="C142" t="s">
+        <v>498</v>
+      </c>
+      <c r="D142" t="s">
+        <v>499</v>
+      </c>
+    </row>
+    <row r="143" spans="1:9" ht="12.75" customHeight="1">
+      <c r="A143" s="22"/>
+      <c r="B143" t="s">
+        <v>13</v>
+      </c>
+      <c r="D143" t="s">
+        <v>500</v>
+      </c>
+      <c r="E143" t="s">
+        <v>501</v>
+      </c>
+    </row>
+    <row r="144" spans="1:9" ht="12.75" customHeight="1">
+      <c r="A144" s="22"/>
+      <c r="B144" t="s">
+        <v>13</v>
+      </c>
+      <c r="D144" t="s">
+        <v>502</v>
+      </c>
+      <c r="E144" t="s">
+        <v>501</v>
+      </c>
+    </row>
+    <row r="145" spans="1:10" ht="12.75" customHeight="1">
+      <c r="A145" s="22"/>
+      <c r="B145" t="s">
+        <v>13</v>
+      </c>
+      <c r="D145" t="s">
+        <v>503</v>
+      </c>
+      <c r="E145" t="s">
+        <v>501</v>
+      </c>
+    </row>
+    <row r="146" spans="1:10" ht="12.75" customHeight="1">
+      <c r="A146" s="22"/>
+      <c r="B146" s="42" t="s">
+        <v>23</v>
+      </c>
+    </row>
+    <row r="147" spans="1:10" ht="12.75" customHeight="1">
+      <c r="A147" s="22"/>
+      <c r="B147" s="41" t="s">
+        <v>15</v>
+      </c>
+      <c r="E147" t="s">
+        <v>504</v>
+      </c>
+    </row>
+    <row r="148" spans="1:10" ht="12.75" customHeight="1">
+      <c r="A148" s="22"/>
+      <c r="B148" t="s">
+        <v>13</v>
+      </c>
+      <c r="D148" t="s">
+        <v>107</v>
+      </c>
+    </row>
+    <row r="149" spans="1:10" ht="12.75" customHeight="1">
+      <c r="A149" s="22"/>
+      <c r="B149" t="s">
+        <v>16</v>
+      </c>
+      <c r="C149" t="s">
+        <v>505</v>
+      </c>
+      <c r="D149" t="s">
+        <v>506</v>
+      </c>
+    </row>
+    <row r="150" spans="1:10" ht="12.75" customHeight="1">
+      <c r="A150" s="22"/>
+      <c r="B150" t="s">
+        <v>16</v>
+      </c>
+      <c r="C150" t="s">
+        <v>507</v>
+      </c>
+      <c r="D150" t="s">
+        <v>508</v>
+      </c>
+    </row>
+    <row r="151" spans="1:10" ht="12.75" customHeight="1">
+      <c r="A151" s="22"/>
+      <c r="B151" t="s">
+        <v>13</v>
+      </c>
+      <c r="D151" t="s">
+        <v>509</v>
+      </c>
+      <c r="E151" t="s">
+        <v>510</v>
+      </c>
+    </row>
+    <row r="152" spans="1:10" ht="12.75" customHeight="1">
+      <c r="A152" s="22"/>
+      <c r="B152" s="42" t="s">
+        <v>23</v>
+      </c>
+    </row>
+    <row r="153" spans="1:10" ht="12.75" customHeight="1">
+      <c r="A153" s="22"/>
+      <c r="B153" s="15" t="s">
+        <v>77</v>
+      </c>
+      <c r="C153" s="15"/>
+      <c r="D153" s="15"/>
+      <c r="E153" s="15"/>
+      <c r="F153" s="15"/>
+      <c r="G153" s="15"/>
+      <c r="H153" s="15"/>
+    </row>
+    <row r="154" spans="1:10" s="12" customFormat="1" ht="12.75" customHeight="1"/>
+    <row r="155" spans="1:10" s="14" customFormat="1" ht="12.75" customHeight="1">
+      <c r="A155" s="25"/>
+      <c r="B155" s="13" t="s">
+        <v>105</v>
+      </c>
+      <c r="E155" s="14" t="s">
+        <v>106</v>
+      </c>
+      <c r="I155" s="12"/>
+      <c r="J155" s="12"/>
+    </row>
+    <row r="156" spans="1:10" ht="12.75" customHeight="1">
+      <c r="B156" s="13" t="s">
+        <v>83</v>
+      </c>
+      <c r="C156" s="14"/>
+      <c r="D156" s="14"/>
+      <c r="E156" s="14" t="s">
+        <v>78</v>
+      </c>
+      <c r="F156" s="14"/>
+      <c r="G156" s="14"/>
+      <c r="H156" s="14"/>
+    </row>
+    <row r="157" spans="1:10" ht="12.75" customHeight="1">
+      <c r="A157" s="22" t="s">
+        <v>459</v>
+      </c>
+      <c r="B157" s="15" t="s">
+        <v>117</v>
+      </c>
+      <c r="C157" s="18"/>
+      <c r="D157" s="18"/>
+      <c r="E157" s="18"/>
+      <c r="F157" s="18"/>
+      <c r="G157" s="18"/>
+      <c r="H157" s="18"/>
+    </row>
+    <row r="158" spans="1:10" ht="12.75" customHeight="1">
+      <c r="A158" s="22"/>
+      <c r="B158" s="2" t="s">
+        <v>218</v>
+      </c>
+      <c r="C158" s="12" t="s">
+        <v>79</v>
+      </c>
+      <c r="D158" s="12" t="s">
+        <v>80</v>
+      </c>
+      <c r="E158" s="12"/>
+      <c r="F158" s="12" t="s">
+        <v>81</v>
+      </c>
+      <c r="G158" s="12"/>
+      <c r="H158" s="12"/>
+    </row>
+    <row r="159" spans="1:10" ht="12.75" customHeight="1">
+      <c r="A159" s="22"/>
+      <c r="B159" s="15" t="s">
+        <v>82</v>
+      </c>
+      <c r="C159" s="18"/>
+      <c r="D159" s="18"/>
+      <c r="E159" s="18"/>
+      <c r="F159" s="18"/>
+      <c r="G159" s="18"/>
+      <c r="H159" s="18"/>
+    </row>
+    <row r="161" spans="1:9" ht="12.75" customHeight="1">
+      <c r="B161" s="13" t="s">
+        <v>108</v>
+      </c>
+      <c r="C161" s="14"/>
+      <c r="D161" s="14"/>
+      <c r="E161" s="14" t="s">
+        <v>110</v>
+      </c>
+      <c r="F161" s="14"/>
+      <c r="G161" s="14"/>
+      <c r="H161" s="14"/>
+    </row>
+    <row r="162" spans="1:9" ht="12.75" customHeight="1">
+      <c r="B162" s="13" t="s">
+        <v>109</v>
+      </c>
+      <c r="C162" s="14"/>
+      <c r="D162" s="14"/>
+      <c r="E162" s="14" t="s">
+        <v>111</v>
+      </c>
+      <c r="F162" s="14"/>
+      <c r="G162" s="14"/>
+      <c r="H162" s="14"/>
+    </row>
+    <row r="163" spans="1:9" ht="12.75" customHeight="1">
+      <c r="A163" s="22" t="s">
+        <v>58</v>
+      </c>
+      <c r="B163" s="15" t="s">
+        <v>118</v>
+      </c>
+      <c r="C163" s="18"/>
+      <c r="D163" s="18"/>
+      <c r="E163" s="18"/>
+      <c r="F163" s="18"/>
+      <c r="G163" s="18"/>
+      <c r="H163" s="18"/>
+    </row>
+    <row r="164" spans="1:9" ht="12.75" customHeight="1">
+      <c r="A164" s="28"/>
+      <c r="B164" t="s">
+        <v>217</v>
+      </c>
+      <c r="C164" t="s">
+        <v>11</v>
+      </c>
+      <c r="D164" t="s">
+        <v>61</v>
+      </c>
+      <c r="F164" t="s">
         <v>6</v>
       </c>
-      <c r="G140" s="12"/>
-      <c r="H140" s="12"/>
-    </row>
-    <row r="141" spans="1:10" ht="12.75" customHeight="1">
-      <c r="A141" s="22"/>
-      <c r="B141" s="2" t="s">
+      <c r="G164" s="21"/>
+      <c r="H164" s="21"/>
+    </row>
+    <row r="165" spans="1:9" ht="12.75" customHeight="1">
+      <c r="A165" s="28"/>
+      <c r="B165" s="39" t="s">
+        <v>15</v>
+      </c>
+      <c r="E165" t="s">
+        <v>487</v>
+      </c>
+    </row>
+    <row r="166" spans="1:9" ht="12.75" customHeight="1">
+      <c r="A166" s="28"/>
+      <c r="B166" t="s">
         <v>13</v>
       </c>
-      <c r="C141" s="12"/>
-      <c r="D141" s="12" t="s">
-        <v>64</v>
-      </c>
-      <c r="E141" s="12"/>
-      <c r="F141" s="12"/>
-      <c r="G141" s="12"/>
-      <c r="H141" s="12"/>
-    </row>
-    <row r="142" spans="1:10" ht="12.75" customHeight="1">
-      <c r="A142" s="22"/>
-      <c r="B142" s="15" t="s">
-        <v>123</v>
-      </c>
-      <c r="C142" s="18"/>
-      <c r="D142" s="18"/>
-      <c r="E142" s="18"/>
-      <c r="F142" s="18"/>
-      <c r="G142" s="18"/>
-      <c r="H142" s="18"/>
-    </row>
-    <row r="145" spans="2:2" ht="12.75" customHeight="1">
-      <c r="B145" s="17" t="s">
+      <c r="D166" t="s">
+        <v>41</v>
+      </c>
+    </row>
+    <row r="167" spans="1:9" ht="12.75" customHeight="1">
+      <c r="A167" s="28"/>
+      <c r="B167" t="s">
+        <v>488</v>
+      </c>
+      <c r="C167" t="s">
+        <v>489</v>
+      </c>
+      <c r="D167" t="s">
+        <v>490</v>
+      </c>
+      <c r="F167" t="s">
+        <v>81</v>
+      </c>
+    </row>
+    <row r="168" spans="1:9" ht="12.75" customHeight="1">
+      <c r="A168" s="28"/>
+      <c r="B168" s="39" t="s">
+        <v>15</v>
+      </c>
+      <c r="C168" t="s">
+        <v>522</v>
+      </c>
+      <c r="E168" t="s">
+        <v>523</v>
+      </c>
+    </row>
+    <row r="169" spans="1:9" ht="12.75" customHeight="1">
+      <c r="A169" s="28"/>
+      <c r="B169" t="s">
+        <v>16</v>
+      </c>
+      <c r="C169" t="s">
+        <v>524</v>
+      </c>
+      <c r="D169" t="s">
+        <v>492</v>
+      </c>
+    </row>
+    <row r="170" spans="1:9" ht="12.75" customHeight="1">
+      <c r="A170" s="28"/>
+      <c r="B170" t="s">
+        <v>13</v>
+      </c>
+      <c r="D170" t="s">
+        <v>528</v>
+      </c>
+      <c r="E170" t="s">
+        <v>525</v>
+      </c>
+      <c r="I170" s="21"/>
+    </row>
+    <row r="171" spans="1:9" ht="12.75" customHeight="1">
+      <c r="A171" s="28"/>
+      <c r="B171" s="40" t="s">
+        <v>23</v>
+      </c>
+    </row>
+    <row r="172" spans="1:9" ht="12.75" customHeight="1">
+      <c r="A172" s="28"/>
+      <c r="B172" s="39" t="s">
+        <v>15</v>
+      </c>
+      <c r="E172" t="s">
+        <v>491</v>
+      </c>
+    </row>
+    <row r="173" spans="1:9" ht="12.75" customHeight="1">
+      <c r="A173" s="28"/>
+      <c r="B173" t="s">
+        <v>16</v>
+      </c>
+      <c r="C173" t="s">
+        <v>20</v>
+      </c>
+      <c r="D173" t="s">
+        <v>492</v>
+      </c>
+    </row>
+    <row r="174" spans="1:9" ht="12.75" customHeight="1">
+      <c r="A174" s="28"/>
+      <c r="B174" t="s">
+        <v>13</v>
+      </c>
+      <c r="D174" t="s">
+        <v>21</v>
+      </c>
+      <c r="E174" t="s">
+        <v>22</v>
+      </c>
+      <c r="I174" s="21"/>
+    </row>
+    <row r="175" spans="1:9" ht="12.75" customHeight="1">
+      <c r="A175" s="28"/>
+      <c r="B175" s="40" t="s">
+        <v>23</v>
+      </c>
+    </row>
+    <row r="176" spans="1:9" ht="12.75" customHeight="1">
+      <c r="A176" s="28"/>
+      <c r="B176" s="39" t="s">
+        <v>15</v>
+      </c>
+      <c r="E176" t="s">
+        <v>493</v>
+      </c>
+    </row>
+    <row r="177" spans="1:5" ht="12.75" customHeight="1">
+      <c r="A177" s="28"/>
+      <c r="B177" t="s">
+        <v>16</v>
+      </c>
+      <c r="C177" t="s">
+        <v>17</v>
+      </c>
+      <c r="D177" t="s">
+        <v>494</v>
+      </c>
+    </row>
+    <row r="178" spans="1:5" ht="12.75" customHeight="1">
+      <c r="A178" s="28"/>
+      <c r="B178" t="s">
+        <v>13</v>
+      </c>
+      <c r="D178" t="s">
+        <v>18</v>
+      </c>
+      <c r="E178" t="s">
+        <v>19</v>
+      </c>
+    </row>
+    <row r="179" spans="1:5" ht="12.75" customHeight="1">
+      <c r="A179" s="28"/>
+      <c r="B179" s="40" t="s">
+        <v>23</v>
+      </c>
+    </row>
+    <row r="180" spans="1:5" ht="12.75" customHeight="1">
+      <c r="A180" s="28"/>
+      <c r="B180" s="40" t="s">
+        <v>23</v>
+      </c>
+    </row>
+    <row r="181" spans="1:5" ht="12.75" customHeight="1">
+      <c r="A181" s="28"/>
+      <c r="B181" s="41" t="s">
+        <v>15</v>
+      </c>
+      <c r="E181" t="s">
+        <v>495</v>
+      </c>
+    </row>
+    <row r="182" spans="1:5" ht="12.75" customHeight="1">
+      <c r="A182" s="28"/>
+      <c r="B182" t="s">
+        <v>13</v>
+      </c>
+      <c r="D182" t="s">
+        <v>43</v>
+      </c>
+    </row>
+    <row r="183" spans="1:5" ht="12.75" customHeight="1">
+      <c r="A183" s="28"/>
+      <c r="B183" t="s">
+        <v>16</v>
+      </c>
+      <c r="C183" t="s">
+        <v>496</v>
+      </c>
+      <c r="D183" t="s">
+        <v>497</v>
+      </c>
+    </row>
+    <row r="184" spans="1:5" ht="12.75" customHeight="1">
+      <c r="A184" s="28"/>
+      <c r="B184" t="s">
+        <v>16</v>
+      </c>
+      <c r="C184" t="s">
+        <v>498</v>
+      </c>
+      <c r="D184" t="s">
+        <v>499</v>
+      </c>
+    </row>
+    <row r="185" spans="1:5" ht="12.75" customHeight="1">
+      <c r="A185" s="28"/>
+      <c r="B185" t="s">
+        <v>13</v>
+      </c>
+      <c r="D185" t="s">
+        <v>500</v>
+      </c>
+      <c r="E185" t="s">
+        <v>501</v>
+      </c>
+    </row>
+    <row r="186" spans="1:5" ht="12.75" customHeight="1">
+      <c r="A186" s="28"/>
+      <c r="B186" t="s">
+        <v>13</v>
+      </c>
+      <c r="D186" t="s">
+        <v>502</v>
+      </c>
+      <c r="E186" t="s">
+        <v>501</v>
+      </c>
+    </row>
+    <row r="187" spans="1:5" ht="12.75" customHeight="1">
+      <c r="A187" s="28"/>
+      <c r="B187" t="s">
+        <v>13</v>
+      </c>
+      <c r="D187" t="s">
+        <v>503</v>
+      </c>
+      <c r="E187" t="s">
+        <v>501</v>
+      </c>
+    </row>
+    <row r="188" spans="1:5" ht="12.75" customHeight="1">
+      <c r="A188" s="28"/>
+      <c r="B188" s="42" t="s">
+        <v>23</v>
+      </c>
+    </row>
+    <row r="189" spans="1:5" ht="12.75" customHeight="1">
+      <c r="A189" s="28"/>
+      <c r="B189" s="41" t="s">
+        <v>15</v>
+      </c>
+      <c r="E189" t="s">
+        <v>504</v>
+      </c>
+    </row>
+    <row r="190" spans="1:5" ht="12.75" customHeight="1">
+      <c r="A190" s="28"/>
+      <c r="B190" t="s">
+        <v>13</v>
+      </c>
+      <c r="D190" t="s">
         <v>107</v>
+      </c>
+    </row>
+    <row r="191" spans="1:5" ht="12.75" customHeight="1">
+      <c r="A191" s="28"/>
+      <c r="B191" t="s">
+        <v>16</v>
+      </c>
+      <c r="C191" t="s">
+        <v>505</v>
+      </c>
+      <c r="D191" t="s">
+        <v>506</v>
+      </c>
+    </row>
+    <row r="192" spans="1:5" ht="12.75" customHeight="1">
+      <c r="A192" s="28"/>
+      <c r="B192" t="s">
+        <v>16</v>
+      </c>
+      <c r="C192" t="s">
+        <v>507</v>
+      </c>
+      <c r="D192" t="s">
+        <v>508</v>
+      </c>
+    </row>
+    <row r="193" spans="1:8" ht="12.75" customHeight="1">
+      <c r="A193" s="28"/>
+      <c r="B193" t="s">
+        <v>13</v>
+      </c>
+      <c r="D193" t="s">
+        <v>509</v>
+      </c>
+      <c r="E193" t="s">
+        <v>510</v>
+      </c>
+    </row>
+    <row r="194" spans="1:8" ht="12.75" customHeight="1">
+      <c r="A194" s="28"/>
+      <c r="B194" s="42" t="s">
+        <v>23</v>
+      </c>
+    </row>
+    <row r="195" spans="1:8" ht="12.75" customHeight="1">
+      <c r="A195" s="22"/>
+      <c r="B195" s="15" t="s">
+        <v>112</v>
+      </c>
+      <c r="C195" s="18"/>
+      <c r="D195" s="18"/>
+      <c r="E195" s="18"/>
+      <c r="F195" s="18"/>
+      <c r="G195" s="18"/>
+      <c r="H195" s="18"/>
+    </row>
+    <row r="198" spans="1:8" ht="12.75" customHeight="1">
+      <c r="B198" s="17" t="s">
+        <v>101</v>
       </c>
     </row>
   </sheetData>
@@ -4717,10 +5428,10 @@
 
 <file path=xl/worksheets/sheet2.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <dimension ref="A1:B20"/>
+  <dimension ref="A1:B23"/>
   <sheetViews>
     <sheetView zoomScale="150" zoomScaleNormal="150" zoomScalePageLayoutView="150" workbookViewId="0">
-      <selection activeCell="A22" sqref="A22"/>
+      <selection activeCell="B4" sqref="B4"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultColWidth="17.1640625" defaultRowHeight="12.75" customHeight="1" x14ac:dyDescent="0"/>
@@ -4733,159 +5444,175 @@
         <v>1</v>
       </c>
       <c r="B1" t="s">
-        <v>26</v>
+        <v>24</v>
       </c>
     </row>
     <row r="2" spans="1:2" ht="12.75" customHeight="1">
       <c r="A2" t="s">
-        <v>27</v>
+        <v>25</v>
       </c>
       <c r="B2" t="s">
-        <v>28</v>
+        <v>26</v>
       </c>
     </row>
     <row r="3" spans="1:2" ht="12.75" customHeight="1">
       <c r="A3" t="s">
-        <v>29</v>
+        <v>27</v>
       </c>
       <c r="B3" t="s">
-        <v>30</v>
+        <v>28</v>
       </c>
     </row>
     <row r="4" spans="1:2" ht="12.75" customHeight="1">
       <c r="A4" t="s">
-        <v>31</v>
+        <v>526</v>
       </c>
       <c r="B4" t="s">
-        <v>32</v>
+        <v>527</v>
       </c>
     </row>
     <row r="5" spans="1:2" ht="12.75" customHeight="1">
       <c r="A5" t="s">
-        <v>33</v>
+        <v>515</v>
       </c>
       <c r="B5" t="s">
-        <v>34</v>
-      </c>
-    </row>
-    <row r="6" spans="1:2" ht="12" customHeight="1">
+        <v>517</v>
+      </c>
+    </row>
+    <row r="6" spans="1:2" ht="12.75" customHeight="1">
       <c r="A6" t="s">
-        <v>231</v>
+        <v>516</v>
       </c>
       <c r="B6" t="s">
-        <v>233</v>
-      </c>
-    </row>
-    <row r="7" spans="1:2" ht="12" customHeight="1">
+        <v>518</v>
+      </c>
+    </row>
+    <row r="7" spans="1:2" ht="12.75" customHeight="1">
       <c r="A7" t="s">
-        <v>234</v>
+        <v>519</v>
       </c>
       <c r="B7" t="s">
-        <v>249</v>
-      </c>
-    </row>
-    <row r="8" spans="1:2" ht="12" customHeight="1">
-      <c r="A8" t="s">
-        <v>235</v>
-      </c>
-      <c r="B8" t="s">
-        <v>242</v>
+        <v>521</v>
       </c>
     </row>
     <row r="9" spans="1:2" ht="12" customHeight="1">
       <c r="A9" t="s">
-        <v>267</v>
+        <v>219</v>
       </c>
       <c r="B9" t="s">
-        <v>264</v>
+        <v>221</v>
       </c>
     </row>
     <row r="10" spans="1:2" ht="12" customHeight="1">
       <c r="A10" t="s">
-        <v>236</v>
+        <v>222</v>
       </c>
       <c r="B10" t="s">
-        <v>243</v>
+        <v>237</v>
       </c>
     </row>
     <row r="11" spans="1:2" ht="12" customHeight="1">
       <c r="A11" t="s">
-        <v>237</v>
+        <v>223</v>
       </c>
       <c r="B11" t="s">
-        <v>244</v>
-      </c>
-    </row>
-    <row r="12" spans="1:2" ht="42" customHeight="1">
+        <v>230</v>
+      </c>
+    </row>
+    <row r="12" spans="1:2" ht="12" customHeight="1">
       <c r="A12" t="s">
-        <v>265</v>
+        <v>255</v>
       </c>
       <c r="B12" t="s">
-        <v>266</v>
-      </c>
-    </row>
-    <row r="13" spans="1:2" ht="12.75" customHeight="1">
+        <v>252</v>
+      </c>
+    </row>
+    <row r="13" spans="1:2" ht="12" customHeight="1">
       <c r="A13" t="s">
-        <v>405</v>
+        <v>224</v>
       </c>
       <c r="B13" t="s">
-        <v>413</v>
-      </c>
-    </row>
-    <row r="14" spans="1:2" ht="12.75" customHeight="1">
+        <v>231</v>
+      </c>
+    </row>
+    <row r="14" spans="1:2" ht="12" customHeight="1">
       <c r="A14" t="s">
-        <v>406</v>
+        <v>225</v>
       </c>
       <c r="B14" t="s">
-        <v>414</v>
-      </c>
-    </row>
-    <row r="15" spans="1:2" ht="12.75" customHeight="1">
+        <v>232</v>
+      </c>
+    </row>
+    <row r="15" spans="1:2" ht="42" customHeight="1">
       <c r="A15" t="s">
-        <v>407</v>
+        <v>253</v>
       </c>
       <c r="B15" t="s">
-        <v>415</v>
+        <v>254</v>
       </c>
     </row>
     <row r="16" spans="1:2" ht="12.75" customHeight="1">
       <c r="A16" t="s">
-        <v>408</v>
+        <v>393</v>
       </c>
       <c r="B16" t="s">
-        <v>416</v>
+        <v>401</v>
       </c>
     </row>
     <row r="17" spans="1:2" ht="12.75" customHeight="1">
       <c r="A17" t="s">
-        <v>409</v>
+        <v>394</v>
       </c>
       <c r="B17" t="s">
-        <v>417</v>
+        <v>402</v>
       </c>
     </row>
     <row r="18" spans="1:2" ht="12.75" customHeight="1">
       <c r="A18" t="s">
-        <v>410</v>
+        <v>395</v>
       </c>
       <c r="B18" t="s">
-        <v>418</v>
+        <v>403</v>
       </c>
     </row>
     <row r="19" spans="1:2" ht="12.75" customHeight="1">
       <c r="A19" t="s">
-        <v>411</v>
+        <v>396</v>
       </c>
       <c r="B19" t="s">
-        <v>412</v>
+        <v>404</v>
       </c>
     </row>
     <row r="20" spans="1:2" ht="12.75" customHeight="1">
       <c r="A20" t="s">
-        <v>422</v>
+        <v>397</v>
       </c>
       <c r="B20" t="s">
-        <v>423</v>
+        <v>405</v>
+      </c>
+    </row>
+    <row r="21" spans="1:2" ht="12.75" customHeight="1">
+      <c r="A21" t="s">
+        <v>398</v>
+      </c>
+      <c r="B21" t="s">
+        <v>406</v>
+      </c>
+    </row>
+    <row r="22" spans="1:2" ht="12.75" customHeight="1">
+      <c r="A22" t="s">
+        <v>399</v>
+      </c>
+      <c r="B22" t="s">
+        <v>400</v>
+      </c>
+    </row>
+    <row r="23" spans="1:2" ht="12.75" customHeight="1">
+      <c r="A23" t="s">
+        <v>410</v>
+      </c>
+      <c r="B23" t="s">
+        <v>411</v>
       </c>
     </row>
   </sheetData>
@@ -4901,10 +5628,10 @@
 
 <file path=xl/worksheets/sheet3.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <dimension ref="A1:D137"/>
+  <dimension ref="A1:D140"/>
   <sheetViews>
-    <sheetView topLeftCell="A125" workbookViewId="0">
-      <selection activeCell="A136" sqref="A136"/>
+    <sheetView workbookViewId="0">
+      <selection activeCell="B21" sqref="B21"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultColWidth="17.1640625" defaultRowHeight="12.75" customHeight="1" x14ac:dyDescent="0"/>
@@ -4915,7 +5642,7 @@
   <sheetData>
     <row r="1" spans="1:4" ht="12.75" customHeight="1">
       <c r="A1" t="s">
-        <v>35</v>
+        <v>29</v>
       </c>
       <c r="B1" t="s">
         <v>1</v>
@@ -4924,7 +5651,7 @@
         <v>2</v>
       </c>
       <c r="D1" t="s">
-        <v>62</v>
+        <v>56</v>
       </c>
     </row>
     <row r="2" spans="1:4" ht="12.75" customHeight="1">
@@ -4932,7 +5659,7 @@
         <v>4</v>
       </c>
       <c r="B2" t="s">
-        <v>36</v>
+        <v>30</v>
       </c>
       <c r="C2" t="s">
         <v>8</v>
@@ -4943,7 +5670,7 @@
         <v>4</v>
       </c>
       <c r="B3" t="s">
-        <v>37</v>
+        <v>31</v>
       </c>
       <c r="C3" t="s">
         <v>10</v>
@@ -4954,10 +5681,10 @@
         <v>4</v>
       </c>
       <c r="B4" t="s">
-        <v>38</v>
+        <v>32</v>
       </c>
       <c r="C4" t="s">
-        <v>39</v>
+        <v>33</v>
       </c>
     </row>
     <row r="5" spans="1:4" ht="12.75" customHeight="1">
@@ -4965,10 +5692,10 @@
         <v>4</v>
       </c>
       <c r="B5" t="s">
-        <v>66</v>
+        <v>60</v>
       </c>
       <c r="C5" t="s">
-        <v>67</v>
+        <v>61</v>
       </c>
     </row>
     <row r="6" spans="1:4" ht="12.75" customHeight="1">
@@ -4976,10 +5703,10 @@
         <v>4</v>
       </c>
       <c r="B6" t="s">
-        <v>96</v>
+        <v>90</v>
       </c>
       <c r="C6" t="s">
-        <v>86</v>
+        <v>80</v>
       </c>
     </row>
     <row r="9" spans="1:4" ht="12.75" customHeight="1">
@@ -4987,10 +5714,10 @@
         <v>9</v>
       </c>
       <c r="B9" t="s">
-        <v>40</v>
+        <v>34</v>
       </c>
       <c r="C9" t="s">
-        <v>41</v>
+        <v>35</v>
       </c>
     </row>
     <row r="10" spans="1:4" ht="12.75" customHeight="1">
@@ -4998,10 +5725,10 @@
         <v>9</v>
       </c>
       <c r="B10" t="s">
-        <v>42</v>
+        <v>36</v>
       </c>
       <c r="C10" t="s">
-        <v>43</v>
+        <v>37</v>
       </c>
     </row>
     <row r="11" spans="1:4" ht="12.75" customHeight="1">
@@ -5009,10 +5736,10 @@
         <v>9</v>
       </c>
       <c r="B11" t="s">
-        <v>69</v>
+        <v>63</v>
       </c>
       <c r="C11" t="s">
-        <v>68</v>
+        <v>62</v>
       </c>
     </row>
     <row r="13" spans="1:4" ht="12.75" customHeight="1">
@@ -5020,10 +5747,10 @@
         <v>7</v>
       </c>
       <c r="B13" t="s">
-        <v>44</v>
+        <v>38</v>
       </c>
       <c r="C13" t="s">
-        <v>45</v>
+        <v>39</v>
       </c>
     </row>
     <row r="14" spans="1:4" ht="12.75" customHeight="1">
@@ -5031,10 +5758,10 @@
         <v>7</v>
       </c>
       <c r="B14" t="s">
-        <v>99</v>
+        <v>93</v>
       </c>
       <c r="C14" t="s">
-        <v>100</v>
+        <v>94</v>
       </c>
     </row>
     <row r="15" spans="1:4" ht="12.75" customHeight="1">
@@ -5042,10 +5769,10 @@
         <v>7</v>
       </c>
       <c r="B15" t="s">
-        <v>97</v>
+        <v>91</v>
       </c>
       <c r="C15" t="s">
-        <v>98</v>
+        <v>92</v>
       </c>
     </row>
     <row r="16" spans="1:4" ht="12.75" customHeight="1">
@@ -5053,10 +5780,10 @@
         <v>7</v>
       </c>
       <c r="B16" t="s">
-        <v>130</v>
+        <v>119</v>
       </c>
       <c r="C16" t="s">
-        <v>79</v>
+        <v>73</v>
       </c>
     </row>
     <row r="18" spans="1:3" ht="12.75" customHeight="1">
@@ -5064,10 +5791,10 @@
         <v>11</v>
       </c>
       <c r="B18" t="s">
-        <v>46</v>
+        <v>40</v>
       </c>
       <c r="C18" t="s">
-        <v>47</v>
+        <v>41</v>
       </c>
     </row>
     <row r="19" spans="1:3" ht="12.75" customHeight="1">
@@ -5075,1103 +5802,1136 @@
         <v>11</v>
       </c>
       <c r="B19" t="s">
-        <v>48</v>
+        <v>42</v>
       </c>
       <c r="C19" t="s">
-        <v>49</v>
+        <v>43</v>
+      </c>
+    </row>
+    <row r="20" spans="1:3" ht="12.75" customHeight="1">
+      <c r="A20" t="s">
+        <v>11</v>
+      </c>
+      <c r="B20" t="s">
+        <v>520</v>
+      </c>
+      <c r="C20" t="s">
+        <v>107</v>
       </c>
     </row>
     <row r="21" spans="1:3" ht="12.75" customHeight="1">
       <c r="A21" t="s">
-        <v>85</v>
+        <v>489</v>
       </c>
       <c r="B21" t="s">
-        <v>90</v>
+        <v>511</v>
       </c>
       <c r="C21" t="s">
-        <v>91</v>
+        <v>512</v>
       </c>
     </row>
     <row r="22" spans="1:3" ht="12.75" customHeight="1">
       <c r="A22" t="s">
+        <v>489</v>
+      </c>
+      <c r="B22" t="s">
+        <v>513</v>
+      </c>
+      <c r="C22" t="s">
+        <v>514</v>
+      </c>
+    </row>
+    <row r="24" spans="1:3" ht="12.75" customHeight="1">
+      <c r="A24" t="s">
+        <v>79</v>
+      </c>
+      <c r="B24" t="s">
+        <v>84</v>
+      </c>
+      <c r="C24" t="s">
         <v>85</v>
-      </c>
-      <c r="B22" t="s">
-        <v>92</v>
-      </c>
-      <c r="C22" t="s">
-        <v>93</v>
-      </c>
-    </row>
-    <row r="23" spans="1:3" ht="12.75" customHeight="1">
-      <c r="A23" t="s">
-        <v>85</v>
-      </c>
-      <c r="B23" t="s">
-        <v>94</v>
-      </c>
-      <c r="C23" t="s">
-        <v>95</v>
       </c>
     </row>
     <row r="25" spans="1:3" ht="12.75" customHeight="1">
       <c r="A25" t="s">
-        <v>65</v>
+        <v>79</v>
       </c>
       <c r="B25" t="s">
-        <v>113</v>
+        <v>86</v>
       </c>
       <c r="C25" t="s">
-        <v>114</v>
+        <v>87</v>
       </c>
     </row>
     <row r="26" spans="1:3" ht="12.75" customHeight="1">
       <c r="A26" t="s">
-        <v>65</v>
+        <v>79</v>
       </c>
       <c r="B26" t="s">
-        <v>115</v>
+        <v>88</v>
       </c>
       <c r="C26" t="s">
-        <v>117</v>
-      </c>
-    </row>
-    <row r="27" spans="1:3" ht="12.75" customHeight="1">
-      <c r="A27" t="s">
-        <v>65</v>
-      </c>
-      <c r="B27" t="s">
-        <v>116</v>
-      </c>
-      <c r="C27" t="s">
-        <v>118</v>
+        <v>89</v>
+      </c>
+    </row>
+    <row r="28" spans="1:3" ht="12.75" customHeight="1">
+      <c r="A28" t="s">
+        <v>59</v>
+      </c>
+      <c r="B28" t="s">
+        <v>40</v>
+      </c>
+      <c r="C28" t="s">
+        <v>41</v>
       </c>
     </row>
     <row r="29" spans="1:3" ht="12.75" customHeight="1">
       <c r="A29" t="s">
-        <v>50</v>
+        <v>59</v>
       </c>
       <c r="B29" t="s">
-        <v>51</v>
+        <v>42</v>
       </c>
       <c r="C29" t="s">
-        <v>52</v>
+        <v>43</v>
       </c>
     </row>
     <row r="30" spans="1:3" ht="12.75" customHeight="1">
       <c r="A30" t="s">
-        <v>50</v>
+        <v>59</v>
       </c>
       <c r="B30" t="s">
-        <v>53</v>
+        <v>520</v>
       </c>
       <c r="C30" t="s">
-        <v>54</v>
+        <v>107</v>
       </c>
     </row>
     <row r="32" spans="1:3" ht="12.75" customHeight="1">
       <c r="A32" t="s">
-        <v>271</v>
+        <v>44</v>
       </c>
       <c r="B32" t="s">
-        <v>278</v>
+        <v>45</v>
       </c>
       <c r="C32" t="s">
-        <v>279</v>
+        <v>46</v>
       </c>
     </row>
     <row r="33" spans="1:4" ht="12.75" customHeight="1">
       <c r="A33" t="s">
-        <v>271</v>
+        <v>44</v>
       </c>
       <c r="B33" t="s">
-        <v>280</v>
+        <v>47</v>
       </c>
       <c r="C33" t="s">
-        <v>281</v>
-      </c>
-    </row>
-    <row r="34" spans="1:4" ht="12.75" customHeight="1">
-      <c r="A34" t="s">
-        <v>271</v>
-      </c>
-      <c r="B34" t="s">
-        <v>419</v>
-      </c>
-      <c r="C34" t="s">
-        <v>396</v>
+        <v>48</v>
+      </c>
+    </row>
+    <row r="35" spans="1:4" ht="12.75" customHeight="1">
+      <c r="A35" t="s">
+        <v>259</v>
+      </c>
+      <c r="B35" t="s">
+        <v>266</v>
+      </c>
+      <c r="C35" t="s">
+        <v>267</v>
       </c>
     </row>
     <row r="36" spans="1:4" ht="12.75" customHeight="1">
       <c r="A36" t="s">
-        <v>132</v>
+        <v>259</v>
       </c>
       <c r="B36" t="s">
-        <v>133</v>
+        <v>268</v>
       </c>
       <c r="C36" t="s">
-        <v>139</v>
+        <v>269</v>
       </c>
     </row>
     <row r="37" spans="1:4" ht="12.75" customHeight="1">
       <c r="A37" t="s">
-        <v>132</v>
+        <v>259</v>
       </c>
       <c r="B37" t="s">
-        <v>134</v>
+        <v>407</v>
       </c>
       <c r="C37" t="s">
-        <v>140</v>
-      </c>
-    </row>
-    <row r="38" spans="1:4" ht="12.75" customHeight="1">
-      <c r="A38" t="s">
-        <v>132</v>
-      </c>
-      <c r="B38" t="s">
-        <v>135</v>
-      </c>
-      <c r="C38" t="s">
-        <v>141</v>
+        <v>384</v>
       </c>
     </row>
     <row r="39" spans="1:4" ht="12.75" customHeight="1">
       <c r="A39" t="s">
-        <v>132</v>
+        <v>121</v>
       </c>
       <c r="B39" t="s">
-        <v>136</v>
+        <v>122</v>
       </c>
       <c r="C39" t="s">
-        <v>142</v>
+        <v>128</v>
       </c>
     </row>
     <row r="40" spans="1:4" ht="12.75" customHeight="1">
       <c r="A40" t="s">
-        <v>132</v>
+        <v>121</v>
       </c>
       <c r="B40" t="s">
-        <v>137</v>
+        <v>123</v>
       </c>
       <c r="C40" t="s">
-        <v>143</v>
+        <v>129</v>
       </c>
     </row>
     <row r="41" spans="1:4" ht="12.75" customHeight="1">
       <c r="A41" t="s">
-        <v>132</v>
+        <v>121</v>
       </c>
       <c r="B41" t="s">
-        <v>138</v>
+        <v>124</v>
       </c>
       <c r="C41" t="s">
-        <v>144</v>
+        <v>130</v>
+      </c>
+    </row>
+    <row r="42" spans="1:4" ht="12.75" customHeight="1">
+      <c r="A42" t="s">
+        <v>121</v>
+      </c>
+      <c r="B42" t="s">
+        <v>125</v>
+      </c>
+      <c r="C42" t="s">
+        <v>131</v>
       </c>
     </row>
     <row r="43" spans="1:4" ht="12.75" customHeight="1">
       <c r="A43" t="s">
-        <v>146</v>
+        <v>121</v>
       </c>
       <c r="B43" t="s">
-        <v>153</v>
-      </c>
-      <c r="D43" t="s">
-        <v>154</v>
+        <v>126</v>
+      </c>
+      <c r="C43" t="s">
+        <v>132</v>
       </c>
     </row>
     <row r="44" spans="1:4" ht="12.75" customHeight="1">
       <c r="A44" t="s">
-        <v>146</v>
+        <v>121</v>
       </c>
       <c r="B44" t="s">
-        <v>155</v>
-      </c>
-      <c r="D44" t="s">
-        <v>159</v>
-      </c>
-    </row>
-    <row r="45" spans="1:4" ht="12.75" customHeight="1">
-      <c r="A45" t="s">
-        <v>146</v>
-      </c>
-      <c r="B45" t="s">
-        <v>156</v>
-      </c>
-      <c r="D45" t="s">
-        <v>160</v>
+        <v>127</v>
+      </c>
+      <c r="C44" t="s">
+        <v>133</v>
       </c>
     </row>
     <row r="46" spans="1:4" ht="12.75" customHeight="1">
       <c r="A46" t="s">
-        <v>146</v>
+        <v>135</v>
       </c>
       <c r="B46" t="s">
-        <v>157</v>
+        <v>142</v>
       </c>
       <c r="D46" t="s">
-        <v>161</v>
+        <v>143</v>
       </c>
     </row>
     <row r="47" spans="1:4" ht="12.75" customHeight="1">
       <c r="A47" t="s">
-        <v>146</v>
+        <v>135</v>
       </c>
       <c r="B47" t="s">
-        <v>158</v>
+        <v>144</v>
       </c>
       <c r="D47" t="s">
-        <v>162</v>
+        <v>148</v>
+      </c>
+    </row>
+    <row r="48" spans="1:4" ht="12.75" customHeight="1">
+      <c r="A48" t="s">
+        <v>135</v>
+      </c>
+      <c r="B48" t="s">
+        <v>145</v>
+      </c>
+      <c r="D48" t="s">
+        <v>149</v>
       </c>
     </row>
     <row r="49" spans="1:4" ht="12.75" customHeight="1">
       <c r="A49" t="s">
+        <v>135</v>
+      </c>
+      <c r="B49" t="s">
+        <v>146</v>
+      </c>
+      <c r="D49" t="s">
         <v>150</v>
       </c>
-      <c r="B49" t="s">
-        <v>186</v>
-      </c>
-      <c r="D49" t="s">
-        <v>187</v>
-      </c>
-    </row>
-    <row r="50" spans="1:4" s="2" customFormat="1" ht="12.75" customHeight="1">
+    </row>
+    <row r="50" spans="1:4" ht="12.75" customHeight="1">
       <c r="A50" t="s">
-        <v>150</v>
+        <v>135</v>
       </c>
       <c r="B50" t="s">
-        <v>176</v>
+        <v>147</v>
       </c>
       <c r="D50" t="s">
-        <v>177</v>
-      </c>
-    </row>
-    <row r="51" spans="1:4" ht="12.75" customHeight="1">
-      <c r="A51" t="s">
-        <v>150</v>
-      </c>
-      <c r="B51" t="s">
-        <v>178</v>
-      </c>
-      <c r="D51" t="s">
-        <v>179</v>
+        <v>151</v>
       </c>
     </row>
     <row r="52" spans="1:4" ht="12.75" customHeight="1">
       <c r="A52" t="s">
-        <v>150</v>
+        <v>139</v>
       </c>
       <c r="B52" t="s">
-        <v>180</v>
+        <v>175</v>
       </c>
       <c r="D52" t="s">
-        <v>181</v>
-      </c>
-    </row>
-    <row r="53" spans="1:4" ht="12.75" customHeight="1">
+        <v>176</v>
+      </c>
+    </row>
+    <row r="53" spans="1:4" s="2" customFormat="1" ht="12.75" customHeight="1">
       <c r="A53" t="s">
-        <v>150</v>
+        <v>139</v>
       </c>
       <c r="B53" t="s">
-        <v>182</v>
+        <v>165</v>
       </c>
       <c r="D53" t="s">
-        <v>183</v>
+        <v>166</v>
       </c>
     </row>
     <row r="54" spans="1:4" ht="12.75" customHeight="1">
       <c r="A54" t="s">
-        <v>150</v>
+        <v>139</v>
       </c>
       <c r="B54" t="s">
-        <v>184</v>
+        <v>167</v>
       </c>
       <c r="D54" t="s">
-        <v>185</v>
+        <v>168</v>
+      </c>
+    </row>
+    <row r="55" spans="1:4" ht="12.75" customHeight="1">
+      <c r="A55" t="s">
+        <v>139</v>
+      </c>
+      <c r="B55" t="s">
+        <v>169</v>
+      </c>
+      <c r="D55" t="s">
+        <v>170</v>
       </c>
     </row>
     <row r="56" spans="1:4" ht="12.75" customHeight="1">
       <c r="A56" t="s">
-        <v>167</v>
+        <v>139</v>
       </c>
       <c r="B56" t="s">
-        <v>188</v>
-      </c>
-      <c r="C56" s="2"/>
+        <v>171</v>
+      </c>
       <c r="D56" t="s">
-        <v>189</v>
+        <v>172</v>
       </c>
     </row>
     <row r="57" spans="1:4" ht="12.75" customHeight="1">
       <c r="A57" t="s">
-        <v>167</v>
+        <v>139</v>
       </c>
       <c r="B57" t="s">
-        <v>190</v>
+        <v>173</v>
       </c>
       <c r="D57" t="s">
-        <v>191</v>
-      </c>
-    </row>
-    <row r="58" spans="1:4" ht="12.75" customHeight="1">
-      <c r="A58" t="s">
-        <v>167</v>
-      </c>
-      <c r="B58" t="s">
-        <v>192</v>
-      </c>
-      <c r="D58" t="s">
-        <v>193</v>
+        <v>174</v>
       </c>
     </row>
     <row r="59" spans="1:4" ht="12.75" customHeight="1">
       <c r="A59" t="s">
-        <v>167</v>
+        <v>156</v>
       </c>
       <c r="B59" t="s">
-        <v>194</v>
-      </c>
+        <v>177</v>
+      </c>
+      <c r="C59" s="2"/>
       <c r="D59" t="s">
-        <v>195</v>
+        <v>178</v>
       </c>
     </row>
     <row r="60" spans="1:4" ht="12.75" customHeight="1">
       <c r="A60" t="s">
-        <v>167</v>
+        <v>156</v>
       </c>
       <c r="B60" t="s">
-        <v>196</v>
+        <v>179</v>
       </c>
       <c r="D60" t="s">
-        <v>197</v>
+        <v>180</v>
+      </c>
+    </row>
+    <row r="61" spans="1:4" ht="12.75" customHeight="1">
+      <c r="A61" t="s">
+        <v>156</v>
+      </c>
+      <c r="B61" t="s">
+        <v>181</v>
+      </c>
+      <c r="D61" t="s">
+        <v>182</v>
       </c>
     </row>
     <row r="62" spans="1:4" ht="12.75" customHeight="1">
       <c r="A62" t="s">
-        <v>239</v>
+        <v>156</v>
       </c>
       <c r="B62" t="s">
-        <v>257</v>
+        <v>183</v>
       </c>
       <c r="D62" t="s">
-        <v>250</v>
+        <v>184</v>
       </c>
     </row>
     <row r="63" spans="1:4" ht="12.75" customHeight="1">
       <c r="A63" t="s">
-        <v>239</v>
+        <v>156</v>
       </c>
       <c r="B63" t="s">
-        <v>258</v>
-      </c>
-      <c r="C63" s="2"/>
+        <v>185</v>
+      </c>
       <c r="D63" t="s">
-        <v>251</v>
-      </c>
-    </row>
-    <row r="64" spans="1:4" ht="12.75" customHeight="1">
-      <c r="A64" t="s">
-        <v>239</v>
-      </c>
-      <c r="B64" t="s">
-        <v>259</v>
-      </c>
-      <c r="D64" t="s">
-        <v>252</v>
+        <v>186</v>
       </c>
     </row>
     <row r="65" spans="1:4" ht="12.75" customHeight="1">
       <c r="A65" t="s">
-        <v>239</v>
+        <v>227</v>
       </c>
       <c r="B65" t="s">
-        <v>260</v>
+        <v>245</v>
       </c>
       <c r="D65" t="s">
-        <v>253</v>
+        <v>238</v>
       </c>
     </row>
     <row r="66" spans="1:4" ht="12.75" customHeight="1">
       <c r="A66" t="s">
+        <v>227</v>
+      </c>
+      <c r="B66" t="s">
+        <v>246</v>
+      </c>
+      <c r="C66" s="2"/>
+      <c r="D66" t="s">
         <v>239</v>
-      </c>
-      <c r="B66" t="s">
-        <v>261</v>
-      </c>
-      <c r="D66" t="s">
-        <v>254</v>
       </c>
     </row>
     <row r="67" spans="1:4" ht="12.75" customHeight="1">
       <c r="A67" t="s">
-        <v>239</v>
+        <v>227</v>
       </c>
       <c r="B67" t="s">
-        <v>262</v>
+        <v>247</v>
       </c>
       <c r="D67" t="s">
-        <v>255</v>
+        <v>240</v>
       </c>
     </row>
     <row r="68" spans="1:4" ht="12.75" customHeight="1">
       <c r="A68" t="s">
-        <v>239</v>
+        <v>227</v>
       </c>
       <c r="B68" t="s">
-        <v>263</v>
+        <v>248</v>
       </c>
       <c r="D68" t="s">
-        <v>256</v>
+        <v>241</v>
+      </c>
+    </row>
+    <row r="69" spans="1:4" ht="12.75" customHeight="1">
+      <c r="A69" t="s">
+        <v>227</v>
+      </c>
+      <c r="B69" t="s">
+        <v>249</v>
+      </c>
+      <c r="D69" t="s">
+        <v>242</v>
       </c>
     </row>
     <row r="70" spans="1:4" ht="12.75" customHeight="1">
       <c r="A70" t="s">
-        <v>171</v>
+        <v>227</v>
       </c>
       <c r="B70" t="s">
-        <v>198</v>
+        <v>250</v>
       </c>
       <c r="D70" t="s">
-        <v>199</v>
+        <v>243</v>
       </c>
     </row>
     <row r="71" spans="1:4" ht="12.75" customHeight="1">
       <c r="A71" t="s">
-        <v>171</v>
+        <v>227</v>
       </c>
       <c r="B71" t="s">
-        <v>200</v>
-      </c>
-      <c r="C71" s="2"/>
+        <v>251</v>
+      </c>
       <c r="D71" t="s">
-        <v>201</v>
-      </c>
-    </row>
-    <row r="72" spans="1:4" ht="12.75" customHeight="1">
-      <c r="A72" t="s">
-        <v>171</v>
-      </c>
-      <c r="B72" t="s">
-        <v>202</v>
-      </c>
-      <c r="D72" t="s">
-        <v>203</v>
+        <v>244</v>
       </c>
     </row>
     <row r="73" spans="1:4" ht="12.75" customHeight="1">
       <c r="A73" t="s">
-        <v>171</v>
+        <v>160</v>
       </c>
       <c r="B73" t="s">
-        <v>204</v>
+        <v>187</v>
       </c>
       <c r="D73" t="s">
-        <v>205</v>
+        <v>188</v>
       </c>
     </row>
     <row r="74" spans="1:4" ht="12.75" customHeight="1">
       <c r="A74" t="s">
-        <v>171</v>
+        <v>160</v>
       </c>
       <c r="B74" t="s">
-        <v>206</v>
-      </c>
+        <v>189</v>
+      </c>
+      <c r="C74" s="2"/>
       <c r="D74" t="s">
-        <v>207</v>
+        <v>190</v>
       </c>
     </row>
     <row r="75" spans="1:4" ht="12.75" customHeight="1">
       <c r="A75" t="s">
-        <v>171</v>
+        <v>160</v>
       </c>
       <c r="B75" t="s">
-        <v>208</v>
+        <v>191</v>
       </c>
       <c r="D75" t="s">
-        <v>209</v>
+        <v>192</v>
+      </c>
+    </row>
+    <row r="76" spans="1:4" ht="12.75" customHeight="1">
+      <c r="A76" t="s">
+        <v>160</v>
+      </c>
+      <c r="B76" t="s">
+        <v>193</v>
+      </c>
+      <c r="D76" t="s">
+        <v>194</v>
       </c>
     </row>
     <row r="77" spans="1:4" ht="12.75" customHeight="1">
       <c r="A77" t="s">
-        <v>174</v>
+        <v>160</v>
       </c>
       <c r="B77" t="s">
-        <v>210</v>
+        <v>195</v>
       </c>
       <c r="D77" t="s">
-        <v>211</v>
+        <v>196</v>
       </c>
     </row>
     <row r="78" spans="1:4" ht="12.75" customHeight="1">
       <c r="A78" t="s">
-        <v>174</v>
+        <v>160</v>
       </c>
       <c r="B78" t="s">
-        <v>212</v>
-      </c>
-      <c r="C78" s="2"/>
+        <v>197</v>
+      </c>
       <c r="D78" t="s">
-        <v>213</v>
-      </c>
-    </row>
-    <row r="79" spans="1:4" ht="12.75" customHeight="1">
-      <c r="A79" t="s">
-        <v>174</v>
-      </c>
-      <c r="B79" t="s">
-        <v>214</v>
-      </c>
-      <c r="D79" t="s">
-        <v>215</v>
+        <v>198</v>
       </c>
     </row>
     <row r="80" spans="1:4" ht="12.75" customHeight="1">
       <c r="A80" t="s">
-        <v>174</v>
+        <v>163</v>
       </c>
       <c r="B80" t="s">
-        <v>216</v>
+        <v>199</v>
       </c>
       <c r="D80" t="s">
-        <v>217</v>
+        <v>200</v>
       </c>
     </row>
     <row r="81" spans="1:4" ht="12.75" customHeight="1">
       <c r="A81" t="s">
-        <v>174</v>
+        <v>163</v>
       </c>
       <c r="B81" t="s">
-        <v>218</v>
-      </c>
+        <v>201</v>
+      </c>
+      <c r="C81" s="2"/>
       <c r="D81" t="s">
-        <v>219</v>
+        <v>202</v>
       </c>
     </row>
     <row r="82" spans="1:4" ht="12.75" customHeight="1">
       <c r="A82" t="s">
-        <v>174</v>
+        <v>163</v>
       </c>
       <c r="B82" t="s">
-        <v>220</v>
+        <v>203</v>
       </c>
       <c r="D82" t="s">
-        <v>221</v>
+        <v>204</v>
+      </c>
+    </row>
+    <row r="83" spans="1:4" ht="12.75" customHeight="1">
+      <c r="A83" t="s">
+        <v>163</v>
+      </c>
+      <c r="B83" t="s">
+        <v>205</v>
+      </c>
+      <c r="D83" t="s">
+        <v>206</v>
       </c>
     </row>
     <row r="84" spans="1:4" ht="12.75" customHeight="1">
       <c r="A84" t="s">
-        <v>275</v>
+        <v>163</v>
       </c>
       <c r="B84" t="s">
-        <v>282</v>
-      </c>
-      <c r="C84" t="s">
-        <v>300</v>
+        <v>207</v>
+      </c>
+      <c r="D84" t="s">
+        <v>208</v>
       </c>
     </row>
     <row r="85" spans="1:4" ht="12.75" customHeight="1">
       <c r="A85" t="s">
-        <v>275</v>
+        <v>163</v>
       </c>
       <c r="B85" t="s">
-        <v>285</v>
-      </c>
-      <c r="C85" t="s">
-        <v>301</v>
-      </c>
-    </row>
-    <row r="86" spans="1:4" ht="12.75" customHeight="1">
-      <c r="A86" t="s">
-        <v>275</v>
-      </c>
-      <c r="B86" t="s">
-        <v>288</v>
-      </c>
-      <c r="C86" t="s">
-        <v>302</v>
+        <v>209</v>
+      </c>
+      <c r="D85" t="s">
+        <v>210</v>
       </c>
     </row>
     <row r="87" spans="1:4" ht="12.75" customHeight="1">
       <c r="A87" t="s">
-        <v>275</v>
+        <v>263</v>
       </c>
       <c r="B87" t="s">
-        <v>289</v>
+        <v>270</v>
       </c>
       <c r="C87" t="s">
-        <v>395</v>
+        <v>288</v>
       </c>
     </row>
     <row r="88" spans="1:4" ht="12.75" customHeight="1">
       <c r="A88" t="s">
-        <v>275</v>
+        <v>263</v>
       </c>
       <c r="B88" t="s">
-        <v>291</v>
+        <v>273</v>
       </c>
       <c r="C88" t="s">
-        <v>303</v>
+        <v>289</v>
       </c>
     </row>
     <row r="89" spans="1:4" ht="12.75" customHeight="1">
       <c r="A89" t="s">
-        <v>275</v>
+        <v>263</v>
       </c>
       <c r="B89" t="s">
-        <v>293</v>
+        <v>276</v>
       </c>
       <c r="C89" t="s">
-        <v>304</v>
+        <v>290</v>
+      </c>
+    </row>
+    <row r="90" spans="1:4" ht="12.75" customHeight="1">
+      <c r="A90" t="s">
+        <v>263</v>
+      </c>
+      <c r="B90" t="s">
+        <v>277</v>
+      </c>
+      <c r="C90" t="s">
+        <v>383</v>
       </c>
     </row>
     <row r="91" spans="1:4" ht="12.75" customHeight="1">
       <c r="A91" t="s">
-        <v>305</v>
+        <v>263</v>
       </c>
       <c r="B91" t="s">
-        <v>311</v>
+        <v>279</v>
       </c>
       <c r="C91" t="s">
-        <v>318</v>
+        <v>291</v>
       </c>
     </row>
     <row r="92" spans="1:4" ht="12.75" customHeight="1">
       <c r="A92" t="s">
-        <v>305</v>
+        <v>263</v>
       </c>
       <c r="B92" t="s">
-        <v>312</v>
+        <v>281</v>
       </c>
       <c r="C92" t="s">
-        <v>319</v>
-      </c>
-    </row>
-    <row r="93" spans="1:4" ht="12.75" customHeight="1">
-      <c r="A93" t="s">
-        <v>305</v>
-      </c>
-      <c r="B93" t="s">
-        <v>313</v>
-      </c>
-      <c r="C93" t="s">
-        <v>320</v>
+        <v>292</v>
       </c>
     </row>
     <row r="94" spans="1:4" ht="12.75" customHeight="1">
       <c r="A94" t="s">
-        <v>305</v>
+        <v>293</v>
       </c>
       <c r="B94" t="s">
-        <v>314</v>
+        <v>299</v>
       </c>
       <c r="C94" t="s">
-        <v>321</v>
+        <v>306</v>
       </c>
     </row>
     <row r="95" spans="1:4" ht="12.75" customHeight="1">
       <c r="A95" t="s">
-        <v>305</v>
+        <v>293</v>
       </c>
       <c r="B95" t="s">
-        <v>315</v>
+        <v>300</v>
       </c>
       <c r="C95" t="s">
-        <v>322</v>
+        <v>307</v>
       </c>
     </row>
     <row r="96" spans="1:4" ht="12.75" customHeight="1">
       <c r="A96" t="s">
-        <v>305</v>
+        <v>293</v>
       </c>
       <c r="B96" t="s">
-        <v>316</v>
+        <v>301</v>
       </c>
       <c r="C96" t="s">
-        <v>323</v>
+        <v>308</v>
       </c>
     </row>
     <row r="97" spans="1:3" ht="12.75" customHeight="1">
       <c r="A97" t="s">
-        <v>305</v>
+        <v>293</v>
       </c>
       <c r="B97" t="s">
-        <v>317</v>
+        <v>302</v>
       </c>
       <c r="C97" t="s">
-        <v>324</v>
+        <v>309</v>
+      </c>
+    </row>
+    <row r="98" spans="1:3" ht="12.75" customHeight="1">
+      <c r="A98" t="s">
+        <v>293</v>
+      </c>
+      <c r="B98" t="s">
+        <v>303</v>
+      </c>
+      <c r="C98" t="s">
+        <v>310</v>
       </c>
     </row>
     <row r="99" spans="1:3" ht="12.75" customHeight="1">
       <c r="A99" t="s">
-        <v>306</v>
+        <v>293</v>
       </c>
       <c r="B99" t="s">
-        <v>331</v>
+        <v>304</v>
       </c>
       <c r="C99" t="s">
-        <v>337</v>
+        <v>311</v>
       </c>
     </row>
     <row r="100" spans="1:3" ht="12.75" customHeight="1">
       <c r="A100" t="s">
-        <v>306</v>
+        <v>293</v>
       </c>
       <c r="B100" t="s">
-        <v>332</v>
+        <v>305</v>
       </c>
       <c r="C100" t="s">
-        <v>338</v>
-      </c>
-    </row>
-    <row r="101" spans="1:3" ht="12.75" customHeight="1">
-      <c r="A101" t="s">
-        <v>306</v>
-      </c>
-      <c r="B101" t="s">
-        <v>333</v>
-      </c>
-      <c r="C101" t="s">
-        <v>339</v>
+        <v>312</v>
       </c>
     </row>
     <row r="102" spans="1:3" ht="12.75" customHeight="1">
       <c r="A102" t="s">
-        <v>306</v>
+        <v>294</v>
       </c>
       <c r="B102" t="s">
-        <v>334</v>
+        <v>319</v>
       </c>
       <c r="C102" t="s">
-        <v>340</v>
+        <v>325</v>
       </c>
     </row>
     <row r="103" spans="1:3" ht="12.75" customHeight="1">
       <c r="A103" t="s">
-        <v>306</v>
+        <v>294</v>
       </c>
       <c r="B103" t="s">
-        <v>335</v>
+        <v>320</v>
       </c>
       <c r="C103" t="s">
-        <v>341</v>
+        <v>326</v>
       </c>
     </row>
     <row r="104" spans="1:3" ht="12.75" customHeight="1">
       <c r="A104" t="s">
-        <v>306</v>
+        <v>294</v>
       </c>
       <c r="B104" t="s">
-        <v>336</v>
+        <v>321</v>
       </c>
       <c r="C104" t="s">
-        <v>342</v>
+        <v>327</v>
+      </c>
+    </row>
+    <row r="105" spans="1:3" ht="12.75" customHeight="1">
+      <c r="A105" t="s">
+        <v>294</v>
+      </c>
+      <c r="B105" t="s">
+        <v>322</v>
+      </c>
+      <c r="C105" t="s">
+        <v>328</v>
       </c>
     </row>
     <row r="106" spans="1:3" ht="12.75" customHeight="1">
       <c r="A106" t="s">
-        <v>307</v>
+        <v>294</v>
       </c>
       <c r="B106" t="s">
-        <v>349</v>
+        <v>323</v>
       </c>
       <c r="C106" t="s">
-        <v>350</v>
+        <v>329</v>
       </c>
     </row>
     <row r="107" spans="1:3" ht="12.75" customHeight="1">
       <c r="A107" t="s">
-        <v>307</v>
+        <v>294</v>
       </c>
       <c r="B107" t="s">
-        <v>343</v>
+        <v>324</v>
       </c>
       <c r="C107" t="s">
-        <v>351</v>
-      </c>
-    </row>
-    <row r="108" spans="1:3" ht="12.75" customHeight="1">
-      <c r="A108" t="s">
-        <v>307</v>
-      </c>
-      <c r="B108" t="s">
-        <v>344</v>
-      </c>
-      <c r="C108" t="s">
-        <v>352</v>
+        <v>330</v>
       </c>
     </row>
     <row r="109" spans="1:3" ht="12.75" customHeight="1">
       <c r="A109" t="s">
-        <v>307</v>
+        <v>295</v>
       </c>
       <c r="B109" t="s">
-        <v>345</v>
+        <v>337</v>
       </c>
       <c r="C109" t="s">
-        <v>353</v>
+        <v>338</v>
       </c>
     </row>
     <row r="110" spans="1:3" ht="12.75" customHeight="1">
       <c r="A110" t="s">
-        <v>307</v>
+        <v>295</v>
       </c>
       <c r="B110" t="s">
-        <v>346</v>
+        <v>331</v>
       </c>
       <c r="C110" t="s">
-        <v>354</v>
+        <v>339</v>
       </c>
     </row>
     <row r="111" spans="1:3" ht="12.75" customHeight="1">
       <c r="A111" t="s">
-        <v>307</v>
+        <v>295</v>
       </c>
       <c r="B111" t="s">
-        <v>347</v>
+        <v>332</v>
       </c>
       <c r="C111" t="s">
-        <v>355</v>
+        <v>340</v>
       </c>
     </row>
     <row r="112" spans="1:3" ht="12.75" customHeight="1">
       <c r="A112" t="s">
-        <v>307</v>
+        <v>295</v>
       </c>
       <c r="B112" t="s">
-        <v>348</v>
+        <v>333</v>
       </c>
       <c r="C112" t="s">
-        <v>356</v>
+        <v>341</v>
+      </c>
+    </row>
+    <row r="113" spans="1:3" ht="12.75" customHeight="1">
+      <c r="A113" t="s">
+        <v>295</v>
+      </c>
+      <c r="B113" t="s">
+        <v>334</v>
+      </c>
+      <c r="C113" t="s">
+        <v>342</v>
       </c>
     </row>
     <row r="114" spans="1:3" ht="12.75" customHeight="1">
       <c r="A114" t="s">
-        <v>308</v>
+        <v>295</v>
       </c>
       <c r="B114" t="s">
-        <v>357</v>
+        <v>335</v>
       </c>
       <c r="C114" t="s">
-        <v>363</v>
+        <v>343</v>
       </c>
     </row>
     <row r="115" spans="1:3" ht="12.75" customHeight="1">
       <c r="A115" t="s">
-        <v>308</v>
+        <v>295</v>
       </c>
       <c r="B115" t="s">
-        <v>358</v>
+        <v>336</v>
       </c>
       <c r="C115" t="s">
-        <v>364</v>
-      </c>
-    </row>
-    <row r="116" spans="1:3" ht="12.75" customHeight="1">
-      <c r="A116" t="s">
-        <v>308</v>
-      </c>
-      <c r="B116" t="s">
-        <v>359</v>
-      </c>
-      <c r="C116" t="s">
-        <v>365</v>
+        <v>344</v>
       </c>
     </row>
     <row r="117" spans="1:3" ht="12.75" customHeight="1">
       <c r="A117" t="s">
-        <v>308</v>
+        <v>296</v>
       </c>
       <c r="B117" t="s">
-        <v>360</v>
+        <v>345</v>
       </c>
       <c r="C117" t="s">
-        <v>366</v>
+        <v>351</v>
       </c>
     </row>
     <row r="118" spans="1:3" ht="12.75" customHeight="1">
       <c r="A118" t="s">
-        <v>308</v>
+        <v>296</v>
       </c>
       <c r="B118" t="s">
-        <v>361</v>
+        <v>346</v>
       </c>
       <c r="C118" t="s">
-        <v>367</v>
+        <v>352</v>
       </c>
     </row>
     <row r="119" spans="1:3" ht="12.75" customHeight="1">
       <c r="A119" t="s">
-        <v>308</v>
+        <v>296</v>
       </c>
       <c r="B119" t="s">
-        <v>362</v>
+        <v>347</v>
       </c>
       <c r="C119" t="s">
-        <v>368</v>
+        <v>353</v>
+      </c>
+    </row>
+    <row r="120" spans="1:3" ht="12.75" customHeight="1">
+      <c r="A120" t="s">
+        <v>296</v>
+      </c>
+      <c r="B120" t="s">
+        <v>348</v>
+      </c>
+      <c r="C120" t="s">
+        <v>354</v>
       </c>
     </row>
     <row r="121" spans="1:3" ht="12.75" customHeight="1">
       <c r="A121" t="s">
-        <v>309</v>
+        <v>296</v>
       </c>
       <c r="B121" t="s">
-        <v>375</v>
+        <v>349</v>
       </c>
       <c r="C121" t="s">
-        <v>376</v>
+        <v>355</v>
       </c>
     </row>
     <row r="122" spans="1:3" ht="12.75" customHeight="1">
       <c r="A122" t="s">
-        <v>309</v>
+        <v>296</v>
       </c>
       <c r="B122" t="s">
-        <v>369</v>
+        <v>350</v>
       </c>
       <c r="C122" t="s">
-        <v>377</v>
-      </c>
-    </row>
-    <row r="123" spans="1:3" ht="12.75" customHeight="1">
-      <c r="A123" t="s">
-        <v>309</v>
-      </c>
-      <c r="B123" t="s">
-        <v>370</v>
-      </c>
-      <c r="C123" t="s">
-        <v>378</v>
+        <v>356</v>
       </c>
     </row>
     <row r="124" spans="1:3" ht="12.75" customHeight="1">
       <c r="A124" t="s">
-        <v>309</v>
+        <v>297</v>
       </c>
       <c r="B124" t="s">
-        <v>372</v>
+        <v>363</v>
       </c>
       <c r="C124" t="s">
-        <v>379</v>
+        <v>364</v>
       </c>
     </row>
     <row r="125" spans="1:3" ht="12.75" customHeight="1">
       <c r="A125" t="s">
-        <v>309</v>
+        <v>297</v>
       </c>
       <c r="B125" t="s">
-        <v>371</v>
+        <v>357</v>
       </c>
       <c r="C125" t="s">
-        <v>380</v>
+        <v>365</v>
       </c>
     </row>
     <row r="126" spans="1:3" ht="12.75" customHeight="1">
       <c r="A126" t="s">
-        <v>309</v>
+        <v>297</v>
       </c>
       <c r="B126" t="s">
-        <v>373</v>
+        <v>358</v>
       </c>
       <c r="C126" t="s">
-        <v>381</v>
+        <v>366</v>
       </c>
     </row>
     <row r="127" spans="1:3" ht="12.75" customHeight="1">
       <c r="A127" t="s">
-        <v>309</v>
+        <v>297</v>
       </c>
       <c r="B127" t="s">
-        <v>374</v>
+        <v>360</v>
       </c>
       <c r="C127" t="s">
-        <v>382</v>
+        <v>367</v>
+      </c>
+    </row>
+    <row r="128" spans="1:3" ht="12.75" customHeight="1">
+      <c r="A128" t="s">
+        <v>297</v>
+      </c>
+      <c r="B128" t="s">
+        <v>359</v>
+      </c>
+      <c r="C128" t="s">
+        <v>368</v>
       </c>
     </row>
     <row r="129" spans="1:3" ht="12.75" customHeight="1">
       <c r="A129" t="s">
-        <v>310</v>
+        <v>297</v>
       </c>
       <c r="B129" t="s">
-        <v>383</v>
+        <v>361</v>
       </c>
       <c r="C129" t="s">
-        <v>389</v>
+        <v>369</v>
       </c>
     </row>
     <row r="130" spans="1:3" ht="12.75" customHeight="1">
       <c r="A130" t="s">
-        <v>310</v>
+        <v>297</v>
       </c>
       <c r="B130" t="s">
-        <v>384</v>
+        <v>362</v>
       </c>
       <c r="C130" t="s">
-        <v>390</v>
-      </c>
-    </row>
-    <row r="131" spans="1:3" ht="12.75" customHeight="1">
-      <c r="A131" t="s">
-        <v>310</v>
-      </c>
-      <c r="B131" t="s">
-        <v>385</v>
-      </c>
-      <c r="C131" t="s">
-        <v>391</v>
+        <v>370</v>
       </c>
     </row>
     <row r="132" spans="1:3" ht="12.75" customHeight="1">
       <c r="A132" t="s">
-        <v>310</v>
+        <v>298</v>
       </c>
       <c r="B132" t="s">
-        <v>386</v>
+        <v>371</v>
       </c>
       <c r="C132" t="s">
-        <v>392</v>
+        <v>377</v>
       </c>
     </row>
     <row r="133" spans="1:3" ht="12.75" customHeight="1">
       <c r="A133" t="s">
-        <v>310</v>
+        <v>298</v>
       </c>
       <c r="B133" t="s">
-        <v>387</v>
+        <v>372</v>
       </c>
       <c r="C133" t="s">
-        <v>393</v>
+        <v>378</v>
       </c>
     </row>
     <row r="134" spans="1:3" ht="12.75" customHeight="1">
       <c r="A134" t="s">
-        <v>310</v>
+        <v>298</v>
       </c>
       <c r="B134" t="s">
-        <v>388</v>
+        <v>373</v>
       </c>
       <c r="C134" t="s">
-        <v>394</v>
+        <v>379</v>
+      </c>
+    </row>
+    <row r="135" spans="1:3" ht="12.75" customHeight="1">
+      <c r="A135" t="s">
+        <v>298</v>
+      </c>
+      <c r="B135" t="s">
+        <v>374</v>
+      </c>
+      <c r="C135" t="s">
+        <v>380</v>
       </c>
     </row>
     <row r="136" spans="1:3" ht="12.75" customHeight="1">
       <c r="A136" t="s">
-        <v>472</v>
+        <v>298</v>
       </c>
       <c r="B136" t="s">
-        <v>467</v>
+        <v>375</v>
       </c>
       <c r="C136" t="s">
-        <v>461</v>
+        <v>381</v>
       </c>
     </row>
     <row r="137" spans="1:3" ht="12.75" customHeight="1">
       <c r="A137" t="s">
-        <v>472</v>
+        <v>298</v>
       </c>
       <c r="B137" t="s">
-        <v>468</v>
+        <v>376</v>
       </c>
       <c r="C137" t="s">
-        <v>469</v>
+        <v>382</v>
+      </c>
+    </row>
+    <row r="139" spans="1:3" ht="12.75" customHeight="1">
+      <c r="A139" t="s">
+        <v>460</v>
+      </c>
+      <c r="B139" t="s">
+        <v>455</v>
+      </c>
+      <c r="C139" t="s">
+        <v>449</v>
+      </c>
+    </row>
+    <row r="140" spans="1:3" ht="12.75" customHeight="1">
+      <c r="A140" t="s">
+        <v>460</v>
+      </c>
+      <c r="B140" t="s">
+        <v>456</v>
+      </c>
+      <c r="C140" t="s">
+        <v>457</v>
       </c>
     </row>
   </sheetData>
@@ -6195,26 +6955,26 @@
   <sheetData>
     <row r="1" spans="1:2" ht="12.75" customHeight="1">
       <c r="A1" t="s">
-        <v>55</v>
+        <v>49</v>
       </c>
       <c r="B1" t="s">
-        <v>56</v>
+        <v>50</v>
       </c>
     </row>
     <row r="2" spans="1:2" ht="12.75" customHeight="1">
       <c r="A2" t="s">
-        <v>57</v>
+        <v>51</v>
       </c>
       <c r="B2" t="s">
-        <v>58</v>
+        <v>52</v>
       </c>
     </row>
     <row r="3" spans="1:2" ht="12.75" customHeight="1">
       <c r="A3" t="s">
-        <v>59</v>
+        <v>53</v>
       </c>
       <c r="B3" t="s">
-        <v>60</v>
+        <v>54</v>
       </c>
     </row>
   </sheetData>
@@ -6242,15 +7002,15 @@
         <v>1</v>
       </c>
       <c r="B1" t="s">
-        <v>163</v>
+        <v>152</v>
       </c>
     </row>
     <row r="2" spans="1:2">
       <c r="A2" t="s">
-        <v>164</v>
+        <v>153</v>
       </c>
       <c r="B2" t="s">
-        <v>165</v>
+        <v>154</v>
       </c>
     </row>
     <row r="3" spans="1:2">
@@ -6258,7 +7018,7 @@
         <v>4</v>
       </c>
       <c r="B3" t="s">
-        <v>165</v>
+        <v>154</v>
       </c>
     </row>
   </sheetData>

</xml_diff>

<commit_message>
added shell for clear ballard
</commit_message>
<xml_diff>
--- a/opendatakit.collect2/form-files/neonatal/neonatal.xlsx
+++ b/opendatakit.collect2/form-files/neonatal/neonatal.xlsx
@@ -1,10 +1,10 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
-  <fileVersion appName="xl" lastEdited="5" lowestEdited="5" rupBuild="22905"/>
+  <fileVersion appName="xl" lastEdited="5" lowestEdited="5" rupBuild="20910"/>
   <workbookPr autoCompressPictures="0"/>
   <bookViews>
-    <workbookView xWindow="320" yWindow="0" windowWidth="24680" windowHeight="15340" tabRatio="500"/>
+    <workbookView xWindow="320" yWindow="0" windowWidth="28480" windowHeight="17560" tabRatio="500" activeTab="1"/>
   </bookViews>
   <sheets>
     <sheet name="survey" sheetId="1" r:id="rId1"/>
@@ -23,7 +23,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="690" uniqueCount="498">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="643" uniqueCount="469">
   <si>
     <t>type</t>
   </si>
@@ -418,9 +418,6 @@
     <t>ballardExam</t>
   </si>
   <si>
-    <t>selected(data('diagnostic_menu'), 'ballardExam')</t>
-  </si>
-  <si>
     <t>ballard_menu1</t>
   </si>
   <si>
@@ -719,9 +716,6 @@
   </si>
   <si>
     <t>postureScore</t>
-  </si>
-  <si>
-    <t>Posture Score: {{calculates.postureScore}}</t>
   </si>
   <si>
     <t xml:space="preserve">(function() {
@@ -818,18 +812,6 @@
   }
 }())
         </t>
-  </si>
-  <si>
-    <t>Square Window Score: {{calculates.squareScore}}</t>
-  </si>
-  <si>
-    <t>Arm Recoil Score: {{calculates.armScore}}</t>
-  </si>
-  <si>
-    <t>Scarf Sign Score: {{calculates.scarfScore}}</t>
-  </si>
-  <si>
-    <t>Heel to Ear Score: {{calculates.heelScore}}</t>
   </si>
   <si>
     <t xml:space="preserve">(function() {
@@ -923,24 +905,12 @@
     <t>poplitealScore</t>
   </si>
   <si>
-    <t>Popiteal Angle Score: {{calculates.poplitealScore}}</t>
-  </si>
-  <si>
-    <t>Total NM Score: {{calculates.totalNMScore}}</t>
-  </si>
-  <si>
-    <t>menu ballard_menu0</t>
-  </si>
-  <si>
     <t>ballard_menu0</t>
   </si>
   <si>
     <t>Ballard Exam - Neuromuscular</t>
   </si>
   <si>
-    <t>selected(data('ballard_menu0'), 'neuromuscular')</t>
-  </si>
-  <si>
     <t>menu ballard_menu2</t>
   </si>
   <si>
@@ -948,9 +918,6 @@
   </si>
   <si>
     <t>Ballard Exam - Physical</t>
-  </si>
-  <si>
-    <t>selected(data('ballard_menu0'), 'physical')</t>
   </si>
   <si>
     <t>neuromuscular</t>
@@ -1316,30 +1283,6 @@
     <t>Final Score</t>
   </si>
   <si>
-    <t>&lt;h2&gt;Physical Score&lt;/h2&gt;</t>
-  </si>
-  <si>
-    <t>&lt;h2&gt;Neuromuscular Score&lt;/h2&gt;</t>
-  </si>
-  <si>
-    <t>Skin Score: {{calculates.skinScore}}</t>
-  </si>
-  <si>
-    <t>Lanugo Score: {{calculates.lanugoScore}}</t>
-  </si>
-  <si>
-    <t>Breast Score: {{calculates.breastScore}}</t>
-  </si>
-  <si>
-    <t>Eye/Ear Score: {{calculates.earEyeScore}}</t>
-  </si>
-  <si>
-    <t>Genitals Score: {{calculates.genitalsScore}}</t>
-  </si>
-  <si>
-    <t>Total Physical Score: {{calculates.totalPhysicalScore}}</t>
-  </si>
-  <si>
     <t>skinScore</t>
   </si>
   <si>
@@ -1352,16 +1295,10 @@
     <t>breastScore</t>
   </si>
   <si>
-    <t>earEyeScore</t>
-  </si>
-  <si>
     <t>genitalsScore</t>
   </si>
   <si>
     <t>totalPhysicalScore</t>
-  </si>
-  <si>
-    <t>calculates.skinScore() + calculates.lanugoScore() + calculates.plantarScore() + calculates.breastScore() + calculates.earEyeScore() + calculates.genitalsScore()</t>
   </si>
   <si>
     <t xml:space="preserve">(function() {
@@ -1445,27 +1382,6 @@
   </si>
   <si>
     <t xml:space="preserve">(function() {
-  switch (data('ear_eye_menu')) { 
-   case('ear_eye-2'):
-      return -2;  
-    case('ear_eye-1'):
-      return -1;
-    case('ear_eye0'):
-      return 0;
-    case('ear_eye1'):
-      return 1;
-    case('ear_eye2'):
-      return 2;
-    case('ear_eye3'):
-      return 3;
-   case('ear_eye4'):
-      return 4;  
-  }
-}())
-        </t>
-  </si>
-  <si>
-    <t xml:space="preserve">(function() {
   switch (data('genitals_menu')) { 
     case('genitals-1'):
       return -1;
@@ -1487,12 +1403,6 @@
     <t>final_ballard_score</t>
   </si>
   <si>
-    <t>selected(data('ballard_menu0'), 'final_ballard_score')</t>
-  </si>
-  <si>
-    <t>&lt;h2&gt;Total Score {{calculates.totalBallardScore}}&lt;/h2&gt;</t>
-  </si>
-  <si>
     <t>totalBallardScore</t>
   </si>
   <si>
@@ -1511,39 +1421,6 @@
     <t>selected(data('menu'),'diagnostics')</t>
   </si>
   <si>
-    <t>label neuromuscular_begin</t>
-  </si>
-  <si>
-    <t>label neuromuscular_end</t>
-  </si>
-  <si>
-    <t>goto neuromuscular_end</t>
-  </si>
-  <si>
-    <t>goto neuromuscular_begin</t>
-  </si>
-  <si>
-    <t>goto physical_end</t>
-  </si>
-  <si>
-    <t>goto physical_begin</t>
-  </si>
-  <si>
-    <t>label physical_begin</t>
-  </si>
-  <si>
-    <t>label physical_end</t>
-  </si>
-  <si>
-    <t>not(selected(data('ballard_menu0'), 'neuromuscular'))</t>
-  </si>
-  <si>
-    <t>not(selected(data('ballard_menu0'), 'physical'))</t>
-  </si>
-  <si>
-    <t>Plantar Surface Score: {{calculates.plantarScore}}</t>
-  </si>
-  <si>
     <t>comments</t>
   </si>
   <si>
@@ -1719,13 +1596,79 @@
   </si>
   <si>
     <t>&lt;b&gt;116&lt;/b&gt;</t>
+  </si>
+  <si>
+    <t>Total Score</t>
+  </si>
+  <si>
+    <t>selected(data('diagnostic_menu'),'ballardExam')</t>
+  </si>
+  <si>
+    <t>eyeEarScore</t>
+  </si>
+  <si>
+    <t>calculates.skinScore() + calculates.lanugoScore() + calculates.plantarScore() + calculates.breastScore() + calculates.eyeEarScore() + calculates.genitalsScore()</t>
+  </si>
+  <si>
+    <r>
+      <t>&lt;h2&gt;Neuromuscular Score&lt;/h2&gt;
+&lt;ul&gt;
+&lt;li&gt;Posture Score: {{calculates.postureScore}}&lt;/li&gt;
+&lt;li&gt;Square Window Score: {{calculates.squareScore}}&lt;/li&gt;
+&lt;li&gt;Arm Recoil Score: {{calculates.armScore}}&lt;/li&gt;
+&lt;li&gt;Popiteal Angle Score: {{calculates.poplitealScore}}&lt;/li&gt;
+&lt;li&gt;Scarf Sign Score: {{calculates.scarfScore}}&lt;/li&gt;
+&lt;li&gt;</t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="10"/>
+        <color rgb="FF000000"/>
+        <rFont val="Arial"/>
+      </rPr>
+      <t>Heel to Ear Score: {{calculates.heelScore}}&lt;/li&gt;
+&lt;li&gt;Total NM Score: {{calculates.totalNMScore}}&lt;/li&gt;
+&lt;/ul&gt;
+&lt;h2&gt;Physical Score&lt;/h2&gt;
+&lt;ul&gt;
+&lt;li&gt;Skin Score: {{calculates.skinScore}}&lt;/li&gt;
+&lt;li&gt;Lanugo Score: {{calculates.lanugoScore}}&lt;/li&gt;
+&lt;li&gt;Plantar Surface Score: {{calculates.plantarScore}}&lt;/li&gt;
+&lt;li&gt;Breast Score: {{calculates.breastScore}}&lt;/li&gt;
+&lt;li&gt;Eye/Ear Score: {{calculates.eyeEarScore}}&lt;/li&gt;
+&lt;li&gt;Genitals Score: {{calculates.genitalsScore}}&lt;/li&gt;
+&lt;li&gt;Total Physical Score: {{calculates.totalPhysicalScore}}&lt;/li&gt;
+&lt;/ul&gt;
+&lt;h2&gt;Total Score {{calculates.totalBallardScore}}&lt;/h2&gt;</t>
+    </r>
+  </si>
+  <si>
+    <t xml:space="preserve">(function() {
+  switch (data('eye_ear_menu')) { 
+   case('eye_ear-2'):
+      return -2;  
+    case('eye_ear-1'):
+      return -1;
+    case('eye_ear0'):
+      return 0;
+    case('eye_ear1'):
+      return 1;
+    case('eye_ear2'):
+      return 2;
+    case('eye_ear3'):
+      return 3;
+   case('eye_ear4'):
+      return 4;  
+  }
+}())
+        </t>
   </si>
 </sst>
 </file>
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
 <styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <fonts count="9" x14ac:knownFonts="1">
+  <fonts count="8" x14ac:knownFonts="1">
     <font>
       <sz val="10"/>
       <color rgb="FF000000"/>
@@ -1771,18 +1714,12 @@
     </font>
     <font>
       <sz val="12"/>
-      <color rgb="FF9C6500"/>
-      <name val="Calibri"/>
-      <family val="2"/>
-    </font>
-    <font>
-      <sz val="12"/>
       <color rgb="FF006100"/>
       <name val="Calibri"/>
       <family val="2"/>
     </font>
   </fonts>
-  <fills count="13">
+  <fills count="12">
     <fill>
       <patternFill patternType="none"/>
     </fill>
@@ -1831,12 +1768,6 @@
     </fill>
     <fill>
       <patternFill patternType="solid">
-        <fgColor rgb="FFFFEB9C"/>
-        <bgColor rgb="FF000000"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
         <fgColor rgb="FFCCFFCC"/>
         <bgColor indexed="64"/>
       </patternFill>
@@ -1863,7 +1794,7 @@
       <diagonal/>
     </border>
   </borders>
-  <cellStyleXfs count="364">
+  <cellStyleXfs count="390">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
     <xf numFmtId="0" fontId="3" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
     <xf numFmtId="0" fontId="4" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
@@ -2228,8 +2159,34 @@
     <xf numFmtId="0" fontId="4" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
     <xf numFmtId="0" fontId="3" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
     <xf numFmtId="0" fontId="4" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="4" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="4" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="4" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="4" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="4" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="4" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="4" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="4" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="4" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="4" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="4" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="4" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="4" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
   </cellStyleXfs>
-  <cellXfs count="39">
+  <cellXfs count="38">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
       <alignment wrapText="1"/>
     </xf>
@@ -2278,19 +2235,18 @@
     <xf numFmtId="0" fontId="0" fillId="8" borderId="0" xfId="0" applyFill="1" applyAlignment="1">
       <alignment wrapText="1"/>
     </xf>
-    <xf numFmtId="0" fontId="7" fillId="9" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1"/>
-    <xf numFmtId="0" fontId="0" fillId="10" borderId="0" xfId="0" applyFill="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="0" fillId="9" borderId="0" xfId="0" applyFill="1" applyAlignment="1">
       <alignment wrapText="1"/>
     </xf>
-    <xf numFmtId="0" fontId="0" fillId="10" borderId="0" xfId="0" applyFill="1"/>
+    <xf numFmtId="0" fontId="0" fillId="9" borderId="0" xfId="0" applyFill="1"/>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="13" applyFill="1"/>
     <xf numFmtId="0" fontId="5" fillId="0" borderId="0" xfId="11" applyFill="1"/>
     <xf numFmtId="20" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1"/>
     <xf numFmtId="0" fontId="5" fillId="0" borderId="0" xfId="11" applyFill="1" applyAlignment="1">
       <alignment wrapText="1"/>
     </xf>
-    <xf numFmtId="0" fontId="0" fillId="11" borderId="0" xfId="0" applyFill="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="0" fillId="10" borderId="0" xfId="0" applyFill="1" applyAlignment="1">
       <alignment wrapText="1"/>
     </xf>
     <xf numFmtId="20" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyAlignment="1"/>
@@ -2304,11 +2260,11 @@
     <xf numFmtId="20" fontId="6" fillId="0" borderId="0" xfId="12" applyNumberFormat="1" applyFill="1" applyAlignment="1"/>
     <xf numFmtId="0" fontId="5" fillId="2" borderId="0" xfId="11" applyAlignment="1"/>
     <xf numFmtId="20" fontId="5" fillId="2" borderId="0" xfId="11" applyNumberFormat="1" applyAlignment="1"/>
-    <xf numFmtId="0" fontId="8" fillId="12" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="7" fillId="11" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1">
       <alignment wrapText="1"/>
     </xf>
   </cellXfs>
-  <cellStyles count="364">
+  <cellStyles count="390">
     <cellStyle name="20% - Accent4" xfId="13" builtinId="42"/>
     <cellStyle name="Followed Hyperlink" xfId="2" builtinId="9" hidden="1"/>
     <cellStyle name="Followed Hyperlink" xfId="4" builtinId="9" hidden="1"/>
@@ -2490,6 +2446,19 @@
     <cellStyle name="Followed Hyperlink" xfId="359" builtinId="9" hidden="1"/>
     <cellStyle name="Followed Hyperlink" xfId="361" builtinId="9" hidden="1"/>
     <cellStyle name="Followed Hyperlink" xfId="363" builtinId="9" hidden="1"/>
+    <cellStyle name="Followed Hyperlink" xfId="365" builtinId="9" hidden="1"/>
+    <cellStyle name="Followed Hyperlink" xfId="367" builtinId="9" hidden="1"/>
+    <cellStyle name="Followed Hyperlink" xfId="369" builtinId="9" hidden="1"/>
+    <cellStyle name="Followed Hyperlink" xfId="371" builtinId="9" hidden="1"/>
+    <cellStyle name="Followed Hyperlink" xfId="373" builtinId="9" hidden="1"/>
+    <cellStyle name="Followed Hyperlink" xfId="375" builtinId="9" hidden="1"/>
+    <cellStyle name="Followed Hyperlink" xfId="377" builtinId="9" hidden="1"/>
+    <cellStyle name="Followed Hyperlink" xfId="379" builtinId="9" hidden="1"/>
+    <cellStyle name="Followed Hyperlink" xfId="381" builtinId="9" hidden="1"/>
+    <cellStyle name="Followed Hyperlink" xfId="383" builtinId="9" hidden="1"/>
+    <cellStyle name="Followed Hyperlink" xfId="385" builtinId="9" hidden="1"/>
+    <cellStyle name="Followed Hyperlink" xfId="387" builtinId="9" hidden="1"/>
+    <cellStyle name="Followed Hyperlink" xfId="389" builtinId="9" hidden="1"/>
     <cellStyle name="Good" xfId="11" builtinId="26"/>
     <cellStyle name="Hyperlink" xfId="1" builtinId="8" hidden="1"/>
     <cellStyle name="Hyperlink" xfId="3" builtinId="8" hidden="1"/>
@@ -2671,6 +2640,19 @@
     <cellStyle name="Hyperlink" xfId="358" builtinId="8" hidden="1"/>
     <cellStyle name="Hyperlink" xfId="360" builtinId="8" hidden="1"/>
     <cellStyle name="Hyperlink" xfId="362" builtinId="8" hidden="1"/>
+    <cellStyle name="Hyperlink" xfId="364" builtinId="8" hidden="1"/>
+    <cellStyle name="Hyperlink" xfId="366" builtinId="8" hidden="1"/>
+    <cellStyle name="Hyperlink" xfId="368" builtinId="8" hidden="1"/>
+    <cellStyle name="Hyperlink" xfId="370" builtinId="8" hidden="1"/>
+    <cellStyle name="Hyperlink" xfId="372" builtinId="8" hidden="1"/>
+    <cellStyle name="Hyperlink" xfId="374" builtinId="8" hidden="1"/>
+    <cellStyle name="Hyperlink" xfId="376" builtinId="8" hidden="1"/>
+    <cellStyle name="Hyperlink" xfId="378" builtinId="8" hidden="1"/>
+    <cellStyle name="Hyperlink" xfId="380" builtinId="8" hidden="1"/>
+    <cellStyle name="Hyperlink" xfId="382" builtinId="8" hidden="1"/>
+    <cellStyle name="Hyperlink" xfId="384" builtinId="8" hidden="1"/>
+    <cellStyle name="Hyperlink" xfId="386" builtinId="8" hidden="1"/>
+    <cellStyle name="Hyperlink" xfId="388" builtinId="8" hidden="1"/>
     <cellStyle name="Neutral" xfId="12" builtinId="28"/>
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
   </cellStyles>
@@ -3001,10 +2983,10 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <dimension ref="A1:J145"/>
+  <dimension ref="A1:J120"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A99" zoomScale="150" zoomScaleNormal="150" zoomScalePageLayoutView="150" workbookViewId="0">
-      <selection activeCell="E119" sqref="E119"/>
+    <sheetView topLeftCell="A6" zoomScale="150" zoomScaleNormal="150" zoomScalePageLayoutView="150" workbookViewId="0">
+      <selection activeCell="D16" sqref="D16"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultColWidth="11.5" defaultRowHeight="12.75" customHeight="1" x14ac:dyDescent="0"/>
@@ -3018,7 +3000,7 @@
   <sheetData>
     <row r="1" spans="1:8" ht="12">
       <c r="A1" t="s">
-        <v>439</v>
+        <v>404</v>
       </c>
       <c r="B1" s="1" t="s">
         <v>0</v>
@@ -3053,7 +3035,7 @@
     </row>
     <row r="3" spans="1:8" ht="12">
       <c r="B3" s="3" t="s">
-        <v>224</v>
+        <v>223</v>
       </c>
       <c r="C3" s="4" t="s">
         <v>4</v>
@@ -3074,37 +3056,37 @@
       <c r="F4" s="2"/>
     </row>
     <row r="5" spans="1:8" ht="12.75" customHeight="1">
-      <c r="A5" s="22" t="s">
+      <c r="A5" s="21" t="s">
         <v>8</v>
       </c>
       <c r="B5" s="19" t="s">
-        <v>424</v>
+        <v>400</v>
       </c>
       <c r="C5" s="19"/>
       <c r="D5" s="19"/>
       <c r="E5" s="19" t="s">
-        <v>425</v>
+        <v>401</v>
       </c>
       <c r="F5" s="19"/>
       <c r="G5" s="19"/>
       <c r="H5" s="19"/>
     </row>
     <row r="6" spans="1:8" ht="12.75" customHeight="1">
-      <c r="A6" s="22"/>
+      <c r="A6" s="21"/>
       <c r="B6" s="19" t="s">
-        <v>426</v>
+        <v>402</v>
       </c>
       <c r="C6" s="19"/>
       <c r="D6" s="19"/>
       <c r="E6" s="19" t="s">
-        <v>427</v>
+        <v>403</v>
       </c>
       <c r="F6" s="19"/>
       <c r="G6" s="19"/>
       <c r="H6" s="19"/>
     </row>
     <row r="7" spans="1:8" s="12" customFormat="1" ht="18" customHeight="1">
-      <c r="A7" s="23"/>
+      <c r="A7" s="22"/>
       <c r="B7" s="18" t="s">
         <v>108</v>
       </c>
@@ -3116,9 +3098,9 @@
       <c r="H7" s="18"/>
     </row>
     <row r="8" spans="1:8" s="12" customFormat="1" ht="18" customHeight="1">
-      <c r="A8" s="23"/>
+      <c r="A8" s="22"/>
       <c r="B8" t="s">
-        <v>225</v>
+        <v>224</v>
       </c>
       <c r="C8" t="s">
         <v>7</v>
@@ -3132,7 +3114,7 @@
       </c>
     </row>
     <row r="9" spans="1:8" ht="18" customHeight="1">
-      <c r="A9" s="22"/>
+      <c r="A9" s="21"/>
       <c r="B9" s="2" t="s">
         <v>13</v>
       </c>
@@ -3149,7 +3131,7 @@
       </c>
     </row>
     <row r="10" spans="1:8" ht="18" customHeight="1">
-      <c r="A10" s="22"/>
+      <c r="A10" s="21"/>
       <c r="B10" s="2" t="s">
         <v>102</v>
       </c>
@@ -3163,7 +3145,7 @@
       <c r="F10" s="2"/>
     </row>
     <row r="11" spans="1:8" ht="18" customHeight="1">
-      <c r="A11" s="22"/>
+      <c r="A11" s="21"/>
       <c r="B11" s="2" t="s">
         <v>102</v>
       </c>
@@ -3176,1531 +3158,1263 @@
       </c>
       <c r="F11" s="2"/>
     </row>
-    <row r="12" spans="1:8" ht="18" customHeight="1">
-      <c r="A12" s="22"/>
-      <c r="B12" s="2" t="s">
-        <v>270</v>
-      </c>
-      <c r="C12" s="2" t="s">
-        <v>271</v>
-      </c>
-      <c r="D12" s="2" t="s">
-        <v>79</v>
-      </c>
-      <c r="E12" s="2" t="s">
+    <row r="12" spans="1:8" s="13" customFormat="1" ht="18" customHeight="1">
+      <c r="B12" s="7" t="s">
+        <v>15</v>
+      </c>
+      <c r="E12" s="13" t="s">
+        <v>464</v>
+      </c>
+    </row>
+    <row r="13" spans="1:8" ht="12">
+      <c r="A13" s="21"/>
+      <c r="B13" t="s">
+        <v>225</v>
+      </c>
+      <c r="C13" t="s">
         <v>131</v>
       </c>
-      <c r="F12" s="2"/>
-    </row>
-    <row r="13" spans="1:8" ht="12.75" customHeight="1">
-      <c r="A13" s="22"/>
-      <c r="B13" s="19" t="s">
-        <v>430</v>
-      </c>
-      <c r="C13" s="19"/>
-      <c r="D13" s="19"/>
-      <c r="E13" s="19" t="s">
-        <v>436</v>
-      </c>
-      <c r="F13" s="19"/>
-      <c r="G13" s="19"/>
-      <c r="H13" s="19"/>
-    </row>
-    <row r="14" spans="1:8" ht="12.75" customHeight="1">
-      <c r="A14" s="22"/>
-      <c r="B14" s="19" t="s">
-        <v>431</v>
-      </c>
-      <c r="C14" s="19"/>
-      <c r="D14" s="19"/>
-      <c r="E14" s="19" t="s">
+      <c r="D13" t="s">
+        <v>263</v>
+      </c>
+      <c r="E13" s="2"/>
+    </row>
+    <row r="14" spans="1:8" ht="12">
+      <c r="A14" s="27"/>
+      <c r="B14" t="s">
+        <v>264</v>
+      </c>
+      <c r="C14" t="s">
+        <v>265</v>
+      </c>
+      <c r="D14" t="s">
+        <v>266</v>
+      </c>
+    </row>
+    <row r="15" spans="1:8" ht="14" customHeight="1">
+      <c r="A15" s="21" t="s">
+        <v>463</v>
+      </c>
+      <c r="B15" t="s">
+        <v>13</v>
+      </c>
+      <c r="D15" t="s">
+        <v>467</v>
+      </c>
+    </row>
+    <row r="16" spans="1:8" ht="12">
+      <c r="A16" s="27"/>
+      <c r="B16" s="11" t="s">
+        <v>25</v>
+      </c>
+      <c r="C16" s="11"/>
+      <c r="D16" s="11"/>
+      <c r="E16" s="11"/>
+      <c r="F16" s="11"/>
+      <c r="G16" s="11"/>
+      <c r="H16" s="11"/>
+    </row>
+    <row r="17" spans="1:10" ht="11" customHeight="1">
+      <c r="A17" s="21"/>
+      <c r="B17" t="s">
+        <v>144</v>
+      </c>
+      <c r="C17" t="s">
+        <v>145</v>
+      </c>
+      <c r="D17" t="s">
+        <v>146</v>
+      </c>
+      <c r="E17" s="2" t="s">
+        <v>147</v>
+      </c>
+    </row>
+    <row r="18" spans="1:10" ht="11" customHeight="1">
+      <c r="A18" s="21"/>
+      <c r="B18" t="s">
+        <v>148</v>
+      </c>
+      <c r="C18" t="s">
+        <v>149</v>
+      </c>
+      <c r="D18" t="s">
+        <v>150</v>
+      </c>
+      <c r="E18" s="2" t="s">
+        <v>151</v>
+      </c>
+    </row>
+    <row r="19" spans="1:10" ht="11" customHeight="1">
+      <c r="A19" s="21"/>
+      <c r="B19" t="s">
+        <v>165</v>
+      </c>
+      <c r="C19" t="s">
+        <v>166</v>
+      </c>
+      <c r="D19" t="s">
+        <v>167</v>
+      </c>
+      <c r="E19" s="2" t="s">
+        <v>168</v>
+      </c>
+    </row>
+    <row r="20" spans="1:10" ht="11" customHeight="1">
+      <c r="A20" s="21"/>
+      <c r="B20" t="s">
+        <v>236</v>
+      </c>
+      <c r="C20" t="s">
+        <v>237</v>
+      </c>
+      <c r="D20" t="s">
+        <v>238</v>
+      </c>
+      <c r="E20" s="2" t="s">
+        <v>239</v>
+      </c>
+    </row>
+    <row r="21" spans="1:10" ht="11" customHeight="1">
+      <c r="A21" s="21"/>
+      <c r="B21" t="s">
+        <v>169</v>
+      </c>
+      <c r="C21" t="s">
+        <v>170</v>
+      </c>
+      <c r="D21" t="s">
+        <v>171</v>
+      </c>
+      <c r="E21" s="2" t="s">
+        <v>221</v>
+      </c>
+    </row>
+    <row r="22" spans="1:10" ht="11" customHeight="1">
+      <c r="A22" s="21"/>
+      <c r="B22" t="s">
+        <v>172</v>
+      </c>
+      <c r="C22" t="s">
+        <v>173</v>
+      </c>
+      <c r="D22" t="s">
+        <v>174</v>
+      </c>
+      <c r="E22" s="2" t="s">
+        <v>222</v>
+      </c>
+    </row>
+    <row r="23" spans="1:10" ht="11" customHeight="1">
+      <c r="A23" s="21"/>
+      <c r="B23" t="s">
+        <v>314</v>
+      </c>
+      <c r="C23" t="s">
+        <v>294</v>
+      </c>
+      <c r="D23" t="s">
+        <v>272</v>
+      </c>
+      <c r="E23" s="2" t="s">
         <v>273</v>
       </c>
-      <c r="F14" s="19"/>
-      <c r="G14" s="19"/>
-      <c r="H14" s="19"/>
-    </row>
-    <row r="15" spans="1:8" s="12" customFormat="1" ht="18" customHeight="1">
-      <c r="A15" s="23"/>
-      <c r="B15" s="18" t="s">
-        <v>428</v>
-      </c>
-      <c r="C15" s="18"/>
-      <c r="D15" s="18"/>
-      <c r="E15" s="18"/>
-      <c r="F15" s="18"/>
-      <c r="G15" s="18"/>
-      <c r="H15" s="18"/>
-    </row>
-    <row r="16" spans="1:8" ht="12">
-      <c r="A16" s="22"/>
-      <c r="B16" t="s">
+    </row>
+    <row r="24" spans="1:10" ht="11" customHeight="1">
+      <c r="A24" s="21"/>
+      <c r="B24" t="s">
+        <v>315</v>
+      </c>
+      <c r="C24" t="s">
+        <v>295</v>
+      </c>
+      <c r="D24" t="s">
+        <v>284</v>
+      </c>
+      <c r="E24" s="2" t="s">
+        <v>275</v>
+      </c>
+    </row>
+    <row r="25" spans="1:10" ht="11" customHeight="1">
+      <c r="A25" s="21"/>
+      <c r="B25" t="s">
+        <v>316</v>
+      </c>
+      <c r="C25" t="s">
+        <v>296</v>
+      </c>
+      <c r="D25" t="s">
+        <v>287</v>
+      </c>
+      <c r="E25" s="2" t="s">
+        <v>276</v>
+      </c>
+    </row>
+    <row r="26" spans="1:10" ht="11" customHeight="1">
+      <c r="A26" s="21"/>
+      <c r="B26" t="s">
+        <v>317</v>
+      </c>
+      <c r="C26" t="s">
+        <v>297</v>
+      </c>
+      <c r="D26" t="s">
+        <v>285</v>
+      </c>
+      <c r="E26" s="2" t="s">
+        <v>279</v>
+      </c>
+    </row>
+    <row r="27" spans="1:10" ht="11" customHeight="1">
+      <c r="A27" s="21"/>
+      <c r="B27" t="s">
+        <v>318</v>
+      </c>
+      <c r="C27" t="s">
+        <v>298</v>
+      </c>
+      <c r="D27" t="s">
+        <v>286</v>
+      </c>
+      <c r="E27" s="2" t="s">
+        <v>281</v>
+      </c>
+    </row>
+    <row r="28" spans="1:10" ht="12" customHeight="1">
+      <c r="A28" s="21"/>
+      <c r="B28" t="s">
+        <v>319</v>
+      </c>
+      <c r="C28" t="s">
+        <v>299</v>
+      </c>
+      <c r="D28" t="s">
+        <v>288</v>
+      </c>
+      <c r="E28" s="2" t="s">
+        <v>283</v>
+      </c>
+    </row>
+    <row r="29" spans="1:10" ht="15">
+      <c r="A29" s="21"/>
+      <c r="B29" s="15" t="s">
+        <v>72</v>
+      </c>
+      <c r="C29" s="15"/>
+      <c r="D29" s="15"/>
+      <c r="E29" s="15"/>
+      <c r="F29" s="15"/>
+      <c r="G29" s="15"/>
+      <c r="H29" s="15"/>
+    </row>
+    <row r="30" spans="1:10" ht="15">
+      <c r="B30" s="23"/>
+      <c r="C30" s="12"/>
+      <c r="D30" s="12"/>
+      <c r="E30" s="12"/>
+      <c r="F30" s="12"/>
+      <c r="G30" s="12"/>
+      <c r="H30" s="12"/>
+    </row>
+    <row r="31" spans="1:10" s="15" customFormat="1" ht="15">
+      <c r="A31" s="21" t="s">
+        <v>424</v>
+      </c>
+      <c r="B31" s="13" t="s">
+        <v>105</v>
+      </c>
+      <c r="C31" s="13"/>
+      <c r="D31" s="13"/>
+      <c r="E31" s="13" t="s">
+        <v>71</v>
+      </c>
+      <c r="F31" s="13"/>
+      <c r="G31" s="13"/>
+      <c r="H31" s="13"/>
+      <c r="I31" s="12"/>
+      <c r="J31" s="12"/>
+    </row>
+    <row r="32" spans="1:10" ht="12">
+      <c r="A32" s="21"/>
+      <c r="B32" s="5" t="s">
+        <v>73</v>
+      </c>
+      <c r="C32" s="5"/>
+      <c r="D32" s="5"/>
+      <c r="E32" s="6" t="s">
+        <v>74</v>
+      </c>
+      <c r="F32" s="5"/>
+      <c r="G32" s="5"/>
+      <c r="H32" s="5"/>
+    </row>
+    <row r="33" spans="1:8" ht="15">
+      <c r="A33" s="21"/>
+      <c r="B33" s="15" t="s">
+        <v>104</v>
+      </c>
+      <c r="C33" s="15"/>
+      <c r="D33" s="15"/>
+      <c r="E33" s="15"/>
+      <c r="F33" s="15"/>
+      <c r="G33" s="15"/>
+      <c r="H33" s="15"/>
+    </row>
+    <row r="34" spans="1:8" ht="12">
+      <c r="A34" s="21"/>
+      <c r="B34" s="12" t="s">
         <v>226</v>
       </c>
-      <c r="C16" t="s">
-        <v>132</v>
-      </c>
-      <c r="D16" t="s">
-        <v>272</v>
-      </c>
-      <c r="E16" s="2"/>
-    </row>
-    <row r="17" spans="1:10" ht="11" customHeight="1">
-      <c r="A17" s="22"/>
-      <c r="B17" t="s">
-        <v>145</v>
-      </c>
-      <c r="C17" t="s">
-        <v>146</v>
-      </c>
-      <c r="D17" t="s">
-        <v>147</v>
-      </c>
-      <c r="E17" s="2" t="s">
-        <v>148</v>
-      </c>
-    </row>
-    <row r="18" spans="1:10" ht="11" customHeight="1">
-      <c r="A18" s="22"/>
-      <c r="B18" t="s">
-        <v>149</v>
-      </c>
-      <c r="C18" t="s">
-        <v>150</v>
-      </c>
-      <c r="D18" t="s">
-        <v>151</v>
-      </c>
-      <c r="E18" s="2" t="s">
-        <v>152</v>
-      </c>
-    </row>
-    <row r="19" spans="1:10" ht="11" customHeight="1">
-      <c r="A19" s="22"/>
-      <c r="B19" t="s">
-        <v>166</v>
-      </c>
-      <c r="C19" t="s">
-        <v>167</v>
-      </c>
-      <c r="D19" t="s">
-        <v>168</v>
-      </c>
-      <c r="E19" s="2" t="s">
-        <v>169</v>
-      </c>
-    </row>
-    <row r="20" spans="1:10" ht="11" customHeight="1">
-      <c r="A20" s="22"/>
-      <c r="B20" t="s">
-        <v>238</v>
-      </c>
-      <c r="C20" t="s">
-        <v>239</v>
-      </c>
-      <c r="D20" t="s">
-        <v>240</v>
-      </c>
-      <c r="E20" s="2" t="s">
-        <v>241</v>
-      </c>
-    </row>
-    <row r="21" spans="1:10" ht="11" customHeight="1">
-      <c r="A21" s="22"/>
-      <c r="B21" t="s">
-        <v>170</v>
-      </c>
-      <c r="C21" t="s">
-        <v>171</v>
-      </c>
-      <c r="D21" t="s">
-        <v>172</v>
-      </c>
-      <c r="E21" s="2" t="s">
-        <v>222</v>
-      </c>
-    </row>
-    <row r="22" spans="1:10" ht="11" customHeight="1">
-      <c r="A22" s="22"/>
-      <c r="B22" t="s">
-        <v>173</v>
-      </c>
-      <c r="C22" t="s">
-        <v>174</v>
-      </c>
-      <c r="D22" t="s">
-        <v>175</v>
-      </c>
-      <c r="E22" s="2" t="s">
-        <v>223</v>
-      </c>
-    </row>
-    <row r="23" spans="1:10" ht="11" customHeight="1">
-      <c r="A23" s="22"/>
-      <c r="B23" s="20" t="s">
-        <v>429</v>
-      </c>
-      <c r="C23" s="20"/>
-      <c r="D23" s="20"/>
-      <c r="E23" s="20"/>
-      <c r="F23" s="20"/>
-      <c r="G23" s="20"/>
-      <c r="H23" s="20"/>
-      <c r="I23" s="21"/>
-      <c r="J23" s="21"/>
-    </row>
-    <row r="24" spans="1:10" ht="12.75" customHeight="1">
-      <c r="A24" s="22"/>
-      <c r="B24" s="19" t="s">
-        <v>432</v>
-      </c>
-      <c r="C24" s="19"/>
-      <c r="D24" s="19"/>
-      <c r="E24" s="19" t="s">
-        <v>437</v>
-      </c>
-      <c r="F24" s="19"/>
-      <c r="G24" s="19"/>
-      <c r="H24" s="19"/>
-    </row>
-    <row r="25" spans="1:10" ht="12.75" customHeight="1">
-      <c r="A25" s="22"/>
-      <c r="B25" s="19" t="s">
-        <v>433</v>
-      </c>
-      <c r="C25" s="19"/>
-      <c r="D25" s="19"/>
-      <c r="E25" s="19" t="s">
-        <v>277</v>
-      </c>
-      <c r="F25" s="19"/>
-      <c r="G25" s="19"/>
-      <c r="H25" s="19"/>
-    </row>
-    <row r="26" spans="1:10" s="12" customFormat="1" ht="18" customHeight="1">
-      <c r="A26" s="23"/>
-      <c r="B26" s="18" t="s">
-        <v>434</v>
-      </c>
-      <c r="C26" s="18"/>
-      <c r="D26" s="18"/>
-      <c r="E26" s="18"/>
-      <c r="F26" s="18"/>
-      <c r="G26" s="18"/>
-      <c r="H26" s="18"/>
-    </row>
-    <row r="27" spans="1:10" ht="11" customHeight="1">
-      <c r="A27" s="22"/>
-      <c r="B27" t="s">
-        <v>274</v>
-      </c>
-      <c r="C27" t="s">
-        <v>275</v>
-      </c>
-      <c r="D27" t="s">
-        <v>276</v>
-      </c>
-      <c r="E27" s="2"/>
-    </row>
-    <row r="28" spans="1:10" ht="11" customHeight="1">
-      <c r="A28" s="22"/>
-      <c r="B28" t="s">
-        <v>325</v>
-      </c>
-      <c r="C28" t="s">
-        <v>305</v>
-      </c>
-      <c r="D28" t="s">
-        <v>283</v>
-      </c>
-      <c r="E28" s="2" t="s">
-        <v>284</v>
-      </c>
-    </row>
-    <row r="29" spans="1:10" ht="11" customHeight="1">
-      <c r="A29" s="22"/>
-      <c r="B29" t="s">
-        <v>326</v>
-      </c>
-      <c r="C29" t="s">
-        <v>306</v>
-      </c>
-      <c r="D29" t="s">
-        <v>295</v>
-      </c>
-      <c r="E29" s="2" t="s">
-        <v>286</v>
-      </c>
-    </row>
-    <row r="30" spans="1:10" ht="11" customHeight="1">
-      <c r="A30" s="22"/>
-      <c r="B30" t="s">
-        <v>327</v>
-      </c>
-      <c r="C30" t="s">
-        <v>307</v>
-      </c>
-      <c r="D30" t="s">
-        <v>298</v>
-      </c>
-      <c r="E30" s="2" t="s">
-        <v>287</v>
-      </c>
-    </row>
-    <row r="31" spans="1:10" ht="11" customHeight="1">
-      <c r="A31" s="22"/>
-      <c r="B31" t="s">
-        <v>328</v>
-      </c>
-      <c r="C31" t="s">
-        <v>308</v>
-      </c>
-      <c r="D31" t="s">
-        <v>296</v>
-      </c>
-      <c r="E31" s="2" t="s">
-        <v>290</v>
-      </c>
-    </row>
-    <row r="32" spans="1:10" ht="11" customHeight="1">
-      <c r="A32" s="22"/>
-      <c r="B32" t="s">
-        <v>329</v>
-      </c>
-      <c r="C32" t="s">
-        <v>309</v>
-      </c>
-      <c r="D32" t="s">
-        <v>297</v>
-      </c>
-      <c r="E32" s="2" t="s">
-        <v>292</v>
-      </c>
-    </row>
-    <row r="33" spans="1:10" ht="12" customHeight="1">
-      <c r="A33" s="22"/>
-      <c r="B33" t="s">
-        <v>330</v>
-      </c>
-      <c r="C33" t="s">
-        <v>310</v>
-      </c>
-      <c r="D33" t="s">
-        <v>299</v>
-      </c>
-      <c r="E33" s="2" t="s">
-        <v>294</v>
-      </c>
-    </row>
-    <row r="34" spans="1:10" ht="12" customHeight="1">
-      <c r="A34" s="22"/>
-      <c r="B34" s="20" t="s">
-        <v>435</v>
-      </c>
-      <c r="C34" s="20"/>
-      <c r="D34" s="20"/>
-      <c r="E34" s="20"/>
-      <c r="F34" s="20"/>
-      <c r="G34" s="20"/>
-      <c r="H34" s="20"/>
-      <c r="I34" s="21"/>
-      <c r="J34" s="21"/>
-    </row>
-    <row r="35" spans="1:10" ht="18" customHeight="1">
-      <c r="A35" s="22"/>
+      <c r="C34" s="12" t="s">
+        <v>9</v>
+      </c>
+      <c r="D34" s="12" t="s">
+        <v>10</v>
+      </c>
+      <c r="E34" s="12"/>
+      <c r="F34" s="12" t="s">
+        <v>6</v>
+      </c>
+      <c r="G34" s="12"/>
+      <c r="H34" s="12"/>
+    </row>
+    <row r="35" spans="1:8" ht="12">
+      <c r="A35" s="21"/>
       <c r="B35" s="7" t="s">
         <v>15</v>
       </c>
-      <c r="C35" s="4"/>
-      <c r="D35" s="2"/>
-      <c r="E35" s="2" t="s">
-        <v>420</v>
-      </c>
-      <c r="F35" s="2"/>
-    </row>
-    <row r="36" spans="1:10" ht="18" customHeight="1">
-      <c r="A36" s="22"/>
-      <c r="B36" s="9" t="s">
+      <c r="C35" s="8"/>
+      <c r="D35" s="8"/>
+      <c r="E35" s="9" t="s">
+        <v>63</v>
+      </c>
+      <c r="F35" s="8"/>
+      <c r="G35" s="10"/>
+      <c r="H35" s="10"/>
+    </row>
+    <row r="36" spans="1:8" ht="12.75" customHeight="1">
+      <c r="A36" s="21"/>
+      <c r="B36" s="4" t="s">
         <v>13</v>
       </c>
-      <c r="C36" s="4"/>
+      <c r="C36" s="2" t="s">
+        <v>75</v>
+      </c>
       <c r="D36" s="2" t="s">
-        <v>398</v>
+        <v>405</v>
       </c>
       <c r="E36" s="2"/>
-      <c r="F36" s="2"/>
-    </row>
-    <row r="37" spans="1:10" ht="25" customHeight="1">
-      <c r="A37" s="22"/>
-      <c r="B37" t="s">
+      <c r="F36" s="4"/>
+    </row>
+    <row r="37" spans="1:8" ht="12.75" customHeight="1">
+      <c r="A37" s="21"/>
+      <c r="B37" s="4" t="s">
         <v>13</v>
       </c>
       <c r="D37" t="s">
-        <v>232</v>
-      </c>
-    </row>
-    <row r="38" spans="1:10" ht="25" customHeight="1">
-      <c r="A38" s="22"/>
+        <v>406</v>
+      </c>
+      <c r="E37" s="2"/>
+      <c r="F37" s="4"/>
+    </row>
+    <row r="38" spans="1:8" ht="12.75" customHeight="1">
+      <c r="A38" s="21"/>
       <c r="B38" t="s">
         <v>13</v>
       </c>
-      <c r="D38" t="s">
-        <v>245</v>
-      </c>
-    </row>
-    <row r="39" spans="1:10" ht="25" customHeight="1">
-      <c r="A39" s="22"/>
-      <c r="B39" t="s">
+      <c r="C38" s="2"/>
+      <c r="D38" s="2" t="s">
+        <v>407</v>
+      </c>
+      <c r="E38" s="2"/>
+      <c r="F38" s="4"/>
+    </row>
+    <row r="39" spans="1:8" ht="12.75" customHeight="1">
+      <c r="A39" s="21"/>
+      <c r="B39" s="2" t="s">
         <v>13</v>
       </c>
-      <c r="D39" t="s">
-        <v>246</v>
-      </c>
-    </row>
-    <row r="40" spans="1:10" ht="25" customHeight="1">
-      <c r="A40" s="22"/>
-      <c r="B40" t="s">
+      <c r="C39" s="2"/>
+      <c r="D39" s="2" t="s">
+        <v>408</v>
+      </c>
+      <c r="E39" s="2"/>
+      <c r="F39" s="4"/>
+    </row>
+    <row r="40" spans="1:8" ht="12.75" customHeight="1">
+      <c r="A40" s="21"/>
+      <c r="B40" s="2" t="s">
         <v>13</v>
       </c>
-      <c r="D40" t="s">
-        <v>268</v>
-      </c>
-    </row>
-    <row r="41" spans="1:10" ht="25" customHeight="1">
-      <c r="A41" s="22"/>
-      <c r="B41" t="s">
+      <c r="C40" s="2"/>
+      <c r="D40" s="2" t="s">
+        <v>409</v>
+      </c>
+      <c r="E40" s="2"/>
+      <c r="F40" s="4"/>
+    </row>
+    <row r="41" spans="1:8" ht="12.75" customHeight="1">
+      <c r="A41" s="21"/>
+      <c r="B41" s="2" t="s">
         <v>13</v>
       </c>
-      <c r="D41" t="s">
-        <v>247</v>
-      </c>
-    </row>
-    <row r="42" spans="1:10" ht="25" customHeight="1">
-      <c r="A42" s="22"/>
-      <c r="B42" t="s">
+      <c r="C41" s="2"/>
+      <c r="D41" s="2" t="s">
+        <v>410</v>
+      </c>
+      <c r="E41" s="2"/>
+      <c r="F41" s="4"/>
+    </row>
+    <row r="42" spans="1:8" ht="12.75" customHeight="1">
+      <c r="A42" s="21"/>
+      <c r="B42" s="2" t="s">
         <v>13</v>
       </c>
-      <c r="D42" t="s">
-        <v>248</v>
-      </c>
-    </row>
-    <row r="43" spans="1:10" ht="25" customHeight="1">
-      <c r="A43" s="22"/>
-      <c r="B43" t="s">
+      <c r="C42" s="2"/>
+      <c r="D42" s="2" t="s">
+        <v>411</v>
+      </c>
+      <c r="E42" s="2"/>
+      <c r="F42" s="4"/>
+    </row>
+    <row r="43" spans="1:8" ht="12.75" customHeight="1">
+      <c r="A43" s="21"/>
+      <c r="B43" s="2" t="s">
         <v>13</v>
       </c>
-      <c r="D43" t="s">
-        <v>269</v>
-      </c>
-    </row>
-    <row r="44" spans="1:10" ht="25" customHeight="1">
-      <c r="A44" s="22"/>
-      <c r="B44" t="s">
+      <c r="C43" s="2"/>
+      <c r="D43" s="2" t="s">
+        <v>412</v>
+      </c>
+      <c r="E43" s="2"/>
+      <c r="F43" s="4"/>
+    </row>
+    <row r="44" spans="1:8" ht="12.75" customHeight="1">
+      <c r="A44" s="21"/>
+      <c r="B44" s="2" t="s">
         <v>13</v>
       </c>
-      <c r="D44" t="s">
-        <v>397</v>
-      </c>
-    </row>
-    <row r="45" spans="1:10" ht="25" customHeight="1">
-      <c r="A45" s="22"/>
-      <c r="B45" t="s">
+      <c r="C44" s="2"/>
+      <c r="D44" s="2" t="s">
+        <v>420</v>
+      </c>
+      <c r="E44" s="2"/>
+      <c r="F44" s="4"/>
+    </row>
+    <row r="45" spans="1:8" ht="12.75" customHeight="1">
+      <c r="A45" s="21"/>
+      <c r="B45" s="2" t="s">
         <v>13</v>
       </c>
-      <c r="D45" t="s">
-        <v>399</v>
-      </c>
-    </row>
-    <row r="46" spans="1:10" ht="25" customHeight="1">
-      <c r="A46" s="22"/>
-      <c r="B46" t="s">
+      <c r="C45" s="2"/>
+      <c r="D45" s="2" t="s">
+        <v>419</v>
+      </c>
+      <c r="E45" s="2"/>
+      <c r="F45" s="4"/>
+    </row>
+    <row r="46" spans="1:8" ht="12.75" customHeight="1">
+      <c r="A46" s="21"/>
+      <c r="B46" s="2" t="s">
         <v>13</v>
       </c>
-      <c r="D46" t="s">
-        <v>400</v>
-      </c>
-    </row>
-    <row r="47" spans="1:10" ht="25" customHeight="1">
-      <c r="A47" s="22"/>
-      <c r="B47" t="s">
+      <c r="C46" s="2"/>
+      <c r="D46" s="2" t="s">
+        <v>421</v>
+      </c>
+      <c r="E46" s="2"/>
+      <c r="F46" s="4"/>
+    </row>
+    <row r="47" spans="1:8" ht="12.75" customHeight="1">
+      <c r="A47" s="21"/>
+      <c r="B47" s="2" t="s">
         <v>13</v>
       </c>
-      <c r="D47" t="s">
-        <v>438</v>
-      </c>
-    </row>
-    <row r="48" spans="1:10" ht="25" customHeight="1">
-      <c r="A48" s="22"/>
-      <c r="B48" t="s">
+      <c r="C47" s="2"/>
+      <c r="D47" s="2" t="s">
+        <v>422</v>
+      </c>
+      <c r="E47" s="2"/>
+      <c r="F47" s="4"/>
+    </row>
+    <row r="48" spans="1:8" ht="12.75" customHeight="1">
+      <c r="A48" s="21"/>
+      <c r="B48" s="2" t="s">
         <v>13</v>
       </c>
-      <c r="D48" t="s">
-        <v>401</v>
-      </c>
-    </row>
-    <row r="49" spans="1:10" ht="25" customHeight="1">
-      <c r="A49" s="22"/>
-      <c r="B49" t="s">
+      <c r="C48" s="2"/>
+      <c r="D48" s="2" t="s">
+        <v>413</v>
+      </c>
+      <c r="E48" s="2"/>
+      <c r="F48" s="4"/>
+    </row>
+    <row r="49" spans="1:8" ht="12.75" customHeight="1">
+      <c r="A49" s="21"/>
+      <c r="B49" s="2" t="s">
         <v>13</v>
       </c>
-      <c r="D49" t="s">
-        <v>402</v>
-      </c>
-    </row>
-    <row r="50" spans="1:10" ht="25" customHeight="1">
-      <c r="A50" s="22"/>
-      <c r="B50" t="s">
+      <c r="C49" s="2"/>
+      <c r="D49" s="2" t="s">
+        <v>416</v>
+      </c>
+      <c r="E49" s="2"/>
+      <c r="F49" s="4"/>
+    </row>
+    <row r="50" spans="1:8" ht="12.75" customHeight="1">
+      <c r="A50" s="21"/>
+      <c r="B50" s="2" t="s">
         <v>13</v>
       </c>
-      <c r="D50" t="s">
-        <v>403</v>
-      </c>
-    </row>
-    <row r="51" spans="1:10" ht="25" customHeight="1">
-      <c r="A51" s="22"/>
-      <c r="B51" t="s">
+      <c r="C50" s="2"/>
+      <c r="D50" s="2" t="s">
+        <v>417</v>
+      </c>
+      <c r="E50" s="2"/>
+      <c r="F50" s="4"/>
+    </row>
+    <row r="51" spans="1:8" ht="12.75" customHeight="1">
+      <c r="A51" s="21"/>
+      <c r="B51" s="2" t="s">
         <v>13</v>
       </c>
-      <c r="D51" t="s">
-        <v>404</v>
-      </c>
-    </row>
-    <row r="52" spans="1:10" ht="25" customHeight="1">
-      <c r="A52" s="22"/>
-      <c r="B52" t="s">
+      <c r="C51" s="2"/>
+      <c r="D51" s="2" t="s">
+        <v>418</v>
+      </c>
+      <c r="E51" s="2"/>
+      <c r="F51" s="4"/>
+    </row>
+    <row r="52" spans="1:8" ht="12.75" customHeight="1">
+      <c r="A52" s="21"/>
+      <c r="B52" s="2" t="s">
         <v>13</v>
       </c>
-      <c r="D52" t="s">
-        <v>421</v>
-      </c>
-    </row>
-    <row r="53" spans="1:10" ht="25" customHeight="1">
-      <c r="A53" s="22"/>
-      <c r="B53" s="11" t="s">
+      <c r="C52" s="2"/>
+      <c r="D52" s="2" t="s">
+        <v>414</v>
+      </c>
+      <c r="E52" s="2"/>
+      <c r="F52" s="4"/>
+    </row>
+    <row r="53" spans="1:8" ht="12.75" customHeight="1">
+      <c r="A53" s="21"/>
+      <c r="B53" s="2" t="s">
+        <v>13</v>
+      </c>
+      <c r="C53" s="2"/>
+      <c r="D53" s="2" t="s">
+        <v>415</v>
+      </c>
+      <c r="E53" s="2"/>
+      <c r="F53" s="4"/>
+    </row>
+    <row r="54" spans="1:8" ht="17" customHeight="1">
+      <c r="A54" s="21"/>
+      <c r="B54" s="2" t="s">
+        <v>13</v>
+      </c>
+      <c r="C54" s="2"/>
+      <c r="D54" s="2" t="s">
+        <v>423</v>
+      </c>
+      <c r="E54" s="2"/>
+      <c r="F54" s="4"/>
+    </row>
+    <row r="55" spans="1:8" ht="12.75" customHeight="1">
+      <c r="A55" s="21"/>
+      <c r="B55" s="2" t="s">
+        <v>13</v>
+      </c>
+      <c r="C55" s="2"/>
+      <c r="D55" s="2"/>
+      <c r="E55" s="2"/>
+      <c r="F55" s="4"/>
+    </row>
+    <row r="56" spans="1:8" ht="12.75" customHeight="1">
+      <c r="A56" s="21"/>
+      <c r="B56" s="4"/>
+      <c r="C56" s="2"/>
+      <c r="D56" s="2"/>
+      <c r="E56" s="2"/>
+      <c r="F56" s="4"/>
+    </row>
+    <row r="57" spans="1:8" ht="12.75" customHeight="1">
+      <c r="A57" s="21"/>
+      <c r="B57" s="2" t="s">
+        <v>13</v>
+      </c>
+      <c r="C57" s="2" t="s">
+        <v>76</v>
+      </c>
+      <c r="D57" s="2"/>
+      <c r="E57" s="2"/>
+      <c r="F57" s="4"/>
+      <c r="G57" t="s">
+        <v>14</v>
+      </c>
+    </row>
+    <row r="58" spans="1:8" ht="12.75" customHeight="1">
+      <c r="A58" s="21"/>
+      <c r="B58" t="s">
+        <v>13</v>
+      </c>
+      <c r="D58" t="s">
+        <v>77</v>
+      </c>
+      <c r="E58" s="13"/>
+    </row>
+    <row r="59" spans="1:8" ht="12.75" customHeight="1">
+      <c r="A59" s="21"/>
+      <c r="B59" t="s">
+        <v>13</v>
+      </c>
+      <c r="H59" t="s">
+        <v>78</v>
+      </c>
+    </row>
+    <row r="60" spans="1:8" ht="12">
+      <c r="A60" s="21"/>
+      <c r="B60" s="11" t="s">
         <v>25</v>
       </c>
-    </row>
-    <row r="54" spans="1:10" ht="15">
-      <c r="A54" s="22"/>
-      <c r="B54" s="15" t="s">
-        <v>72</v>
-      </c>
-      <c r="C54" s="15"/>
-      <c r="D54" s="15"/>
-      <c r="E54" s="15"/>
-      <c r="F54" s="15"/>
-      <c r="G54" s="15"/>
-      <c r="H54" s="15"/>
-    </row>
-    <row r="55" spans="1:10" ht="15">
-      <c r="B55" s="24"/>
-      <c r="C55" s="12"/>
-      <c r="D55" s="12"/>
-      <c r="E55" s="12"/>
-      <c r="F55" s="12"/>
-      <c r="G55" s="12"/>
-      <c r="H55" s="12"/>
-    </row>
-    <row r="56" spans="1:10" s="15" customFormat="1" ht="15">
-      <c r="A56" s="22" t="s">
-        <v>459</v>
-      </c>
-      <c r="B56" s="13" t="s">
-        <v>105</v>
-      </c>
-      <c r="C56" s="13"/>
-      <c r="D56" s="13"/>
-      <c r="E56" s="13" t="s">
-        <v>71</v>
-      </c>
-      <c r="F56" s="13"/>
-      <c r="G56" s="13"/>
-      <c r="H56" s="13"/>
-      <c r="I56" s="12"/>
-      <c r="J56" s="12"/>
-    </row>
-    <row r="57" spans="1:10" ht="12">
-      <c r="A57" s="22"/>
-      <c r="B57" s="5" t="s">
-        <v>73</v>
-      </c>
-      <c r="C57" s="5"/>
-      <c r="D57" s="5"/>
-      <c r="E57" s="6" t="s">
-        <v>74</v>
-      </c>
-      <c r="F57" s="5"/>
-      <c r="G57" s="5"/>
-      <c r="H57" s="5"/>
-    </row>
-    <row r="58" spans="1:10" ht="15">
-      <c r="A58" s="22"/>
-      <c r="B58" s="15" t="s">
-        <v>104</v>
-      </c>
-      <c r="C58" s="15"/>
-      <c r="D58" s="15"/>
-      <c r="E58" s="15"/>
-      <c r="F58" s="15"/>
-      <c r="G58" s="15"/>
-      <c r="H58" s="15"/>
-    </row>
-    <row r="59" spans="1:10" ht="12">
-      <c r="A59" s="22"/>
-      <c r="B59" s="12" t="s">
-        <v>227</v>
-      </c>
-      <c r="C59" s="12" t="s">
-        <v>9</v>
-      </c>
-      <c r="D59" s="12" t="s">
-        <v>10</v>
-      </c>
-      <c r="E59" s="12"/>
-      <c r="F59" s="12" t="s">
-        <v>6</v>
-      </c>
-      <c r="G59" s="12"/>
-      <c r="H59" s="12"/>
-    </row>
-    <row r="60" spans="1:10" ht="12">
-      <c r="A60" s="22"/>
-      <c r="B60" s="7" t="s">
-        <v>15</v>
-      </c>
-      <c r="C60" s="8"/>
-      <c r="D60" s="8"/>
-      <c r="E60" s="9" t="s">
-        <v>63</v>
-      </c>
-      <c r="F60" s="8"/>
+      <c r="C60" s="10"/>
+      <c r="D60" s="10"/>
+      <c r="E60" s="10"/>
+      <c r="F60" s="10"/>
       <c r="G60" s="10"/>
       <c r="H60" s="10"/>
     </row>
-    <row r="61" spans="1:10" ht="12.75" customHeight="1">
-      <c r="A61" s="22"/>
-      <c r="B61" s="4" t="s">
+    <row r="61" spans="1:8" s="10" customFormat="1" ht="12"/>
+    <row r="62" spans="1:8" s="10" customFormat="1" ht="15">
+      <c r="B62" s="10" t="s">
+        <v>454</v>
+      </c>
+      <c r="E62" s="13" t="s">
+        <v>459</v>
+      </c>
+    </row>
+    <row r="63" spans="1:8" s="10" customFormat="1" ht="15">
+      <c r="B63" s="10" t="s">
+        <v>455</v>
+      </c>
+      <c r="E63" s="37" t="s">
+        <v>458</v>
+      </c>
+    </row>
+    <row r="64" spans="1:8" s="10" customFormat="1" ht="12">
+      <c r="B64" s="10" t="s">
+        <v>456</v>
+      </c>
+    </row>
+    <row r="65" spans="1:8" s="10" customFormat="1" ht="12">
+      <c r="B65" s="10" t="s">
         <v>13</v>
       </c>
-      <c r="C61" s="2" t="s">
-        <v>75</v>
-      </c>
-      <c r="D61" s="2" t="s">
+      <c r="D65" s="10" t="s">
+        <v>42</v>
+      </c>
+    </row>
+    <row r="66" spans="1:8" s="10" customFormat="1" ht="12">
+      <c r="B66" s="10" t="s">
+        <v>457</v>
+      </c>
+    </row>
+    <row r="67" spans="1:8" s="10" customFormat="1" ht="12"/>
+    <row r="68" spans="1:8" ht="30">
+      <c r="A68" s="21"/>
+      <c r="B68" s="13" t="s">
+        <v>429</v>
+      </c>
+      <c r="C68" s="13"/>
+      <c r="D68" s="13"/>
+      <c r="E68" s="13" t="s">
+        <v>425</v>
+      </c>
+      <c r="F68" s="13"/>
+      <c r="G68" s="13"/>
+      <c r="H68" s="13"/>
+    </row>
+    <row r="69" spans="1:8" ht="30">
+      <c r="A69" s="21"/>
+      <c r="B69" s="13" t="s">
+        <v>430</v>
+      </c>
+      <c r="C69" s="13"/>
+      <c r="D69" s="13"/>
+      <c r="E69" s="13" t="s">
+        <v>431</v>
+      </c>
+      <c r="F69" s="13"/>
+      <c r="G69" s="13"/>
+      <c r="H69" s="13"/>
+    </row>
+    <row r="70" spans="1:8" ht="15">
+      <c r="A70" s="21"/>
+      <c r="B70" s="15" t="s">
+        <v>427</v>
+      </c>
+      <c r="C70" s="15"/>
+      <c r="D70" s="15"/>
+      <c r="E70" s="15"/>
+      <c r="F70" s="15"/>
+      <c r="G70" s="15"/>
+      <c r="H70" s="15"/>
+    </row>
+    <row r="71" spans="1:8" ht="12">
+      <c r="A71" s="21"/>
+      <c r="B71" s="10"/>
+      <c r="C71" s="10"/>
+      <c r="D71" s="10"/>
+      <c r="E71" s="10"/>
+      <c r="F71" s="10"/>
+      <c r="G71" s="10"/>
+      <c r="H71" s="10"/>
+    </row>
+    <row r="72" spans="1:8" ht="24">
+      <c r="A72" s="21"/>
+      <c r="B72" t="s">
+        <v>438</v>
+      </c>
+      <c r="C72" t="s">
+        <v>437</v>
+      </c>
+      <c r="F72" t="s">
+        <v>6</v>
+      </c>
+      <c r="G72" s="10"/>
+      <c r="H72" s="10"/>
+    </row>
+    <row r="73" spans="1:8" ht="30">
+      <c r="A73" s="21"/>
+      <c r="B73" s="13" t="s">
+        <v>443</v>
+      </c>
+      <c r="C73" s="13"/>
+      <c r="D73" s="13"/>
+      <c r="E73" s="13" t="s">
         <v>440</v>
       </c>
-      <c r="E61" s="2"/>
-      <c r="F61" s="4"/>
-    </row>
-    <row r="62" spans="1:10" ht="12.75" customHeight="1">
-      <c r="A62" s="22"/>
-      <c r="B62" s="4" t="s">
-        <v>13</v>
-      </c>
-      <c r="D62" t="s">
+      <c r="F73" s="13"/>
+      <c r="G73" s="10"/>
+      <c r="H73" s="10"/>
+    </row>
+    <row r="74" spans="1:8" ht="30">
+      <c r="A74" s="21"/>
+      <c r="B74" s="13" t="s">
+        <v>444</v>
+      </c>
+      <c r="C74" s="13"/>
+      <c r="D74" s="13"/>
+      <c r="E74" s="13" t="s">
+        <v>445</v>
+      </c>
+      <c r="F74" s="13"/>
+      <c r="G74" s="10"/>
+      <c r="H74" s="10"/>
+    </row>
+    <row r="75" spans="1:8" ht="15">
+      <c r="A75" s="21"/>
+      <c r="B75" s="15" t="s">
         <v>441</v>
       </c>
-      <c r="E62" s="2"/>
-      <c r="F62" s="4"/>
-    </row>
-    <row r="63" spans="1:10" ht="12.75" customHeight="1">
-      <c r="A63" s="22"/>
-      <c r="B63" t="s">
-        <v>13</v>
-      </c>
-      <c r="C63" s="2"/>
-      <c r="D63" s="2" t="s">
-        <v>442</v>
-      </c>
-      <c r="E63" s="2"/>
-      <c r="F63" s="4"/>
-    </row>
-    <row r="64" spans="1:10" ht="12.75" customHeight="1">
-      <c r="A64" s="22"/>
-      <c r="B64" s="2" t="s">
-        <v>13</v>
-      </c>
-      <c r="C64" s="2"/>
-      <c r="D64" s="2" t="s">
-        <v>443</v>
-      </c>
-      <c r="E64" s="2"/>
-      <c r="F64" s="4"/>
-    </row>
-    <row r="65" spans="1:6" ht="12.75" customHeight="1">
-      <c r="A65" s="22"/>
-      <c r="B65" s="2" t="s">
-        <v>13</v>
-      </c>
-      <c r="C65" s="2"/>
-      <c r="D65" s="2" t="s">
-        <v>444</v>
-      </c>
-      <c r="E65" s="2"/>
-      <c r="F65" s="4"/>
-    </row>
-    <row r="66" spans="1:6" ht="12.75" customHeight="1">
-      <c r="A66" s="22"/>
-      <c r="B66" s="2" t="s">
-        <v>13</v>
-      </c>
-      <c r="C66" s="2"/>
-      <c r="D66" s="2" t="s">
-        <v>445</v>
-      </c>
-      <c r="E66" s="2"/>
-      <c r="F66" s="4"/>
-    </row>
-    <row r="67" spans="1:6" ht="12.75" customHeight="1">
-      <c r="A67" s="22"/>
-      <c r="B67" s="2" t="s">
-        <v>13</v>
-      </c>
-      <c r="C67" s="2"/>
-      <c r="D67" s="2" t="s">
-        <v>446</v>
-      </c>
-      <c r="E67" s="2"/>
-      <c r="F67" s="4"/>
-    </row>
-    <row r="68" spans="1:6" ht="12.75" customHeight="1">
-      <c r="A68" s="22"/>
-      <c r="B68" s="2" t="s">
-        <v>13</v>
-      </c>
-      <c r="C68" s="2"/>
-      <c r="D68" s="2" t="s">
-        <v>447</v>
-      </c>
-      <c r="E68" s="2"/>
-      <c r="F68" s="4"/>
-    </row>
-    <row r="69" spans="1:6" ht="12.75" customHeight="1">
-      <c r="A69" s="22"/>
-      <c r="B69" s="2" t="s">
-        <v>13</v>
-      </c>
-      <c r="C69" s="2"/>
-      <c r="D69" s="2" t="s">
-        <v>455</v>
-      </c>
-      <c r="E69" s="2"/>
-      <c r="F69" s="4"/>
-    </row>
-    <row r="70" spans="1:6" ht="12.75" customHeight="1">
-      <c r="A70" s="22"/>
-      <c r="B70" s="2" t="s">
-        <v>13</v>
-      </c>
-      <c r="C70" s="2"/>
-      <c r="D70" s="2" t="s">
-        <v>454</v>
-      </c>
-      <c r="E70" s="2"/>
-      <c r="F70" s="4"/>
-    </row>
-    <row r="71" spans="1:6" ht="12.75" customHeight="1">
-      <c r="A71" s="22"/>
-      <c r="B71" s="2" t="s">
-        <v>13</v>
-      </c>
-      <c r="C71" s="2"/>
-      <c r="D71" s="2" t="s">
-        <v>456</v>
-      </c>
-      <c r="E71" s="2"/>
-      <c r="F71" s="4"/>
-    </row>
-    <row r="72" spans="1:6" ht="12.75" customHeight="1">
-      <c r="A72" s="22"/>
-      <c r="B72" s="2" t="s">
-        <v>13</v>
-      </c>
-      <c r="C72" s="2"/>
-      <c r="D72" s="2" t="s">
-        <v>457</v>
-      </c>
-      <c r="E72" s="2"/>
-      <c r="F72" s="4"/>
-    </row>
-    <row r="73" spans="1:6" ht="12.75" customHeight="1">
-      <c r="A73" s="22"/>
-      <c r="B73" s="2" t="s">
-        <v>13</v>
-      </c>
-      <c r="C73" s="2"/>
-      <c r="D73" s="2" t="s">
-        <v>448</v>
-      </c>
-      <c r="E73" s="2"/>
-      <c r="F73" s="4"/>
-    </row>
-    <row r="74" spans="1:6" ht="12.75" customHeight="1">
-      <c r="A74" s="22"/>
-      <c r="B74" s="2" t="s">
-        <v>13</v>
-      </c>
-      <c r="C74" s="2"/>
-      <c r="D74" s="2" t="s">
-        <v>451</v>
-      </c>
-      <c r="E74" s="2"/>
-      <c r="F74" s="4"/>
-    </row>
-    <row r="75" spans="1:6" ht="12.75" customHeight="1">
-      <c r="A75" s="22"/>
-      <c r="B75" s="2" t="s">
-        <v>13</v>
-      </c>
-      <c r="C75" s="2"/>
-      <c r="D75" s="2" t="s">
-        <v>452</v>
-      </c>
-      <c r="E75" s="2"/>
-      <c r="F75" s="4"/>
-    </row>
-    <row r="76" spans="1:6" ht="12.75" customHeight="1">
-      <c r="A76" s="22"/>
-      <c r="B76" s="2" t="s">
-        <v>13</v>
-      </c>
-      <c r="C76" s="2"/>
-      <c r="D76" s="2" t="s">
-        <v>453</v>
-      </c>
-      <c r="E76" s="2"/>
-      <c r="F76" s="4"/>
-    </row>
-    <row r="77" spans="1:6" ht="12.75" customHeight="1">
-      <c r="A77" s="22"/>
+      <c r="C75" s="15"/>
+      <c r="D75" s="15"/>
+      <c r="E75" s="15"/>
+      <c r="G75" s="10"/>
+      <c r="H75" s="10"/>
+    </row>
+    <row r="76" spans="1:8" ht="12">
+      <c r="A76" s="21"/>
+      <c r="B76" t="s">
+        <v>15</v>
+      </c>
+      <c r="G76" s="10"/>
+      <c r="H76" s="10"/>
+    </row>
+    <row r="77" spans="1:8" ht="12">
+      <c r="A77" s="21"/>
       <c r="B77" s="2" t="s">
         <v>13</v>
       </c>
-      <c r="C77" s="2"/>
-      <c r="D77" s="2" t="s">
+      <c r="C77" s="12"/>
+      <c r="D77" s="25" t="s">
+        <v>452</v>
+      </c>
+      <c r="E77" s="12"/>
+      <c r="F77" s="12"/>
+      <c r="G77" s="10"/>
+      <c r="H77" s="10"/>
+    </row>
+    <row r="78" spans="1:8" ht="12">
+      <c r="A78" s="21"/>
+      <c r="B78" s="2" t="s">
+        <v>25</v>
+      </c>
+      <c r="C78" s="12"/>
+      <c r="D78" s="25"/>
+      <c r="E78" s="12"/>
+      <c r="F78" s="12"/>
+      <c r="G78" s="10"/>
+      <c r="H78" s="10"/>
+    </row>
+    <row r="79" spans="1:8" ht="15">
+      <c r="A79" s="21"/>
+      <c r="B79" s="15" t="s">
+        <v>442</v>
+      </c>
+      <c r="C79" s="18"/>
+      <c r="D79" s="31"/>
+      <c r="E79" s="18"/>
+      <c r="F79" s="12"/>
+      <c r="G79" s="10"/>
+      <c r="H79" s="10"/>
+    </row>
+    <row r="80" spans="1:8" ht="30">
+      <c r="A80" s="27"/>
+      <c r="B80" s="13" t="s">
+        <v>447</v>
+      </c>
+      <c r="C80" s="13"/>
+      <c r="D80" s="13"/>
+      <c r="E80" s="13" t="s">
+        <v>439</v>
+      </c>
+      <c r="F80" s="13"/>
+    </row>
+    <row r="81" spans="1:8" ht="30">
+      <c r="A81" s="27"/>
+      <c r="B81" s="13" t="s">
+        <v>448</v>
+      </c>
+      <c r="C81" s="13"/>
+      <c r="D81" s="13"/>
+      <c r="E81" s="13" t="s">
         <v>449</v>
       </c>
-      <c r="E77" s="2"/>
-      <c r="F77" s="4"/>
-    </row>
-    <row r="78" spans="1:6" ht="12.75" customHeight="1">
-      <c r="A78" s="22"/>
-      <c r="B78" s="2" t="s">
+      <c r="F81" s="13"/>
+    </row>
+    <row r="82" spans="1:8" s="10" customFormat="1" ht="15">
+      <c r="B82" s="26" t="s">
         <v>13</v>
       </c>
-      <c r="C78" s="2"/>
-      <c r="D78" s="2" t="s">
+      <c r="C82" s="26"/>
+      <c r="D82" s="26" t="s">
+        <v>461</v>
+      </c>
+      <c r="E82" s="26"/>
+      <c r="F82" s="26"/>
+    </row>
+    <row r="83" spans="1:8" ht="15">
+      <c r="A83" s="27"/>
+      <c r="B83" s="15" t="s">
         <v>450</v>
       </c>
-      <c r="E78" s="2"/>
-      <c r="F78" s="4"/>
-    </row>
-    <row r="79" spans="1:6" ht="17" customHeight="1">
-      <c r="A79" s="22"/>
-      <c r="B79" s="2" t="s">
+      <c r="C83" s="15"/>
+      <c r="D83" s="15"/>
+      <c r="E83" s="15"/>
+      <c r="F83" s="15"/>
+    </row>
+    <row r="84" spans="1:8" ht="12">
+      <c r="A84" s="27"/>
+      <c r="B84" t="s">
+        <v>15</v>
+      </c>
+    </row>
+    <row r="85" spans="1:8" ht="12">
+      <c r="A85" s="27"/>
+      <c r="B85" t="s">
         <v>13</v>
       </c>
-      <c r="C79" s="2"/>
-      <c r="D79" s="2" t="s">
-        <v>458</v>
-      </c>
-      <c r="E79" s="2"/>
-      <c r="F79" s="4"/>
-    </row>
-    <row r="80" spans="1:6" ht="12.75" customHeight="1">
-      <c r="A80" s="22"/>
-      <c r="B80" s="2" t="s">
+      <c r="C85" s="20"/>
+      <c r="D85" s="28" t="s">
+        <v>446</v>
+      </c>
+      <c r="E85" s="28"/>
+      <c r="F85" s="20"/>
+    </row>
+    <row r="86" spans="1:8" ht="12">
+      <c r="A86" s="27"/>
+      <c r="B86" t="s">
+        <v>25</v>
+      </c>
+      <c r="C86" s="20"/>
+      <c r="D86" s="28"/>
+      <c r="E86" s="20"/>
+      <c r="F86" s="20"/>
+    </row>
+    <row r="87" spans="1:8" ht="12">
+      <c r="A87" s="27"/>
+      <c r="C87" s="20"/>
+      <c r="D87" s="28"/>
+      <c r="E87" s="20"/>
+      <c r="F87" s="20"/>
+    </row>
+    <row r="88" spans="1:8" ht="15">
+      <c r="A88" s="27"/>
+      <c r="B88" s="15" t="s">
+        <v>451</v>
+      </c>
+      <c r="C88" s="29"/>
+      <c r="D88" s="30"/>
+      <c r="E88" s="29"/>
+      <c r="F88" s="29"/>
+    </row>
+    <row r="89" spans="1:8" s="10" customFormat="1" ht="15">
+      <c r="B89" s="32" t="s">
         <v>13</v>
       </c>
-      <c r="C80" s="2"/>
-      <c r="D80" s="2"/>
-      <c r="E80" s="2"/>
-      <c r="F80" s="4"/>
-    </row>
-    <row r="81" spans="1:8" ht="12.75" customHeight="1">
-      <c r="A81" s="22"/>
-      <c r="B81" s="4"/>
-      <c r="C81" s="2"/>
-      <c r="D81" s="2"/>
-      <c r="E81" s="2"/>
-      <c r="F81" s="4"/>
-    </row>
-    <row r="82" spans="1:8" ht="12.75" customHeight="1">
-      <c r="A82" s="22"/>
-      <c r="B82" s="2" t="s">
+      <c r="C89" s="33"/>
+      <c r="D89" s="34" t="s">
+        <v>460</v>
+      </c>
+      <c r="E89" s="33"/>
+      <c r="F89" s="33"/>
+    </row>
+    <row r="90" spans="1:8" ht="15">
+      <c r="A90" s="27"/>
+      <c r="B90" s="15" t="s">
+        <v>428</v>
+      </c>
+      <c r="C90" s="29"/>
+      <c r="D90" s="30"/>
+      <c r="E90" s="29"/>
+      <c r="F90" s="29"/>
+    </row>
+    <row r="91" spans="1:8" s="10" customFormat="1" ht="15">
+      <c r="B91" s="32" t="s">
         <v>13</v>
       </c>
-      <c r="C82" s="2" t="s">
-        <v>76</v>
-      </c>
-      <c r="D82" s="2"/>
-      <c r="E82" s="2"/>
-      <c r="F82" s="4"/>
-      <c r="G82" t="s">
-        <v>14</v>
-      </c>
-    </row>
-    <row r="83" spans="1:8" ht="12.75" customHeight="1">
-      <c r="A83" s="22"/>
-      <c r="B83" t="s">
-        <v>13</v>
-      </c>
-      <c r="D83" t="s">
-        <v>77</v>
-      </c>
-      <c r="E83" s="13"/>
-    </row>
-    <row r="84" spans="1:8" ht="12.75" customHeight="1">
-      <c r="A84" s="22"/>
-      <c r="B84" t="s">
-        <v>13</v>
-      </c>
-      <c r="H84" t="s">
-        <v>78</v>
-      </c>
-    </row>
-    <row r="85" spans="1:8" ht="12">
-      <c r="A85" s="22"/>
-      <c r="B85" s="11" t="s">
-        <v>25</v>
-      </c>
-      <c r="C85" s="10"/>
-      <c r="D85" s="10"/>
-      <c r="E85" s="10"/>
-      <c r="F85" s="10"/>
-      <c r="G85" s="10"/>
-      <c r="H85" s="10"/>
-    </row>
-    <row r="86" spans="1:8" s="10" customFormat="1" ht="12"/>
-    <row r="87" spans="1:8" s="10" customFormat="1" ht="15">
-      <c r="B87" s="10" t="s">
-        <v>489</v>
-      </c>
-      <c r="E87" s="13" t="s">
-        <v>494</v>
-      </c>
-    </row>
-    <row r="88" spans="1:8" s="10" customFormat="1" ht="15">
-      <c r="B88" s="10" t="s">
-        <v>490</v>
-      </c>
-      <c r="E88" s="38" t="s">
-        <v>493</v>
-      </c>
-    </row>
-    <row r="89" spans="1:8" s="10" customFormat="1" ht="12">
-      <c r="B89" s="10" t="s">
-        <v>491</v>
-      </c>
-    </row>
-    <row r="90" spans="1:8" s="10" customFormat="1" ht="12">
-      <c r="B90" s="10" t="s">
-        <v>13</v>
-      </c>
-      <c r="D90" s="10" t="s">
-        <v>42</v>
-      </c>
-    </row>
-    <row r="91" spans="1:8" s="10" customFormat="1" ht="12">
-      <c r="B91" s="10" t="s">
-        <v>492</v>
-      </c>
-    </row>
-    <row r="92" spans="1:8" s="10" customFormat="1" ht="12"/>
-    <row r="93" spans="1:8" ht="30">
-      <c r="A93" s="22"/>
-      <c r="B93" s="13" t="s">
-        <v>464</v>
-      </c>
-      <c r="C93" s="13"/>
-      <c r="D93" s="13"/>
-      <c r="E93" s="13" t="s">
-        <v>460</v>
-      </c>
-      <c r="F93" s="13"/>
-      <c r="G93" s="13"/>
-      <c r="H93" s="13"/>
-    </row>
-    <row r="94" spans="1:8" ht="30">
-      <c r="A94" s="22"/>
+      <c r="C91" s="33"/>
+      <c r="D91" s="34" t="s">
+        <v>462</v>
+      </c>
+      <c r="E91" s="33"/>
+      <c r="F91" s="33"/>
+    </row>
+    <row r="92" spans="1:8" ht="15">
+      <c r="A92" s="27"/>
+      <c r="B92" s="15" t="s">
+        <v>80</v>
+      </c>
+      <c r="C92" s="29"/>
+      <c r="D92" s="30"/>
+      <c r="E92" s="29"/>
+      <c r="F92" s="29"/>
+    </row>
+    <row r="93" spans="1:8" ht="15">
+      <c r="A93" s="10"/>
+      <c r="B93" s="32"/>
+      <c r="C93" s="33"/>
+      <c r="D93" s="34"/>
+      <c r="E93" s="33"/>
+      <c r="F93" s="33"/>
+    </row>
+    <row r="94" spans="1:8" s="13" customFormat="1" ht="15">
+      <c r="A94" s="26"/>
       <c r="B94" s="13" t="s">
-        <v>465</v>
-      </c>
-      <c r="C94" s="13"/>
-      <c r="D94" s="13"/>
-      <c r="E94" s="13" t="s">
-        <v>466</v>
-      </c>
-      <c r="F94" s="13"/>
-      <c r="G94" s="13"/>
-      <c r="H94" s="13"/>
-    </row>
-    <row r="95" spans="1:8" ht="15">
-      <c r="A95" s="22"/>
-      <c r="B95" s="15" t="s">
-        <v>462</v>
-      </c>
-      <c r="C95" s="15"/>
-      <c r="D95" s="15"/>
-      <c r="E95" s="15"/>
-      <c r="F95" s="15"/>
-      <c r="G95" s="15"/>
-      <c r="H95" s="15"/>
-    </row>
-    <row r="96" spans="1:8" ht="12">
-      <c r="A96" s="22"/>
-      <c r="B96" s="10"/>
-      <c r="C96" s="10"/>
-      <c r="D96" s="10"/>
-      <c r="E96" s="10"/>
-      <c r="F96" s="10"/>
-      <c r="G96" s="10"/>
-      <c r="H96" s="10"/>
-    </row>
-    <row r="97" spans="1:8" ht="24">
-      <c r="A97" s="22"/>
+        <v>109</v>
+      </c>
+      <c r="C94" s="35"/>
+      <c r="D94" s="36"/>
+      <c r="E94" s="14" t="s">
+        <v>453</v>
+      </c>
+      <c r="F94" s="35"/>
+    </row>
+    <row r="95" spans="1:8" s="13" customFormat="1" ht="15">
+      <c r="A95" s="26"/>
+      <c r="B95" s="13" t="s">
+        <v>81</v>
+      </c>
+      <c r="C95" s="35"/>
+      <c r="D95" s="36"/>
+      <c r="E95" s="14" t="s">
+        <v>82</v>
+      </c>
+      <c r="F95" s="35"/>
+    </row>
+    <row r="96" spans="1:8" ht="15">
+      <c r="A96" s="21" t="s">
+        <v>435</v>
+      </c>
+      <c r="B96" s="15" t="s">
+        <v>110</v>
+      </c>
+      <c r="C96" s="15"/>
+      <c r="D96" s="15"/>
+      <c r="E96" s="15"/>
+      <c r="F96" s="15"/>
+      <c r="G96" s="15"/>
+      <c r="H96" s="15"/>
+    </row>
+    <row r="97" spans="1:10" ht="12">
+      <c r="A97" s="21"/>
       <c r="B97" t="s">
-        <v>473</v>
+        <v>227</v>
       </c>
       <c r="C97" t="s">
-        <v>472</v>
+        <v>11</v>
+      </c>
+      <c r="D97" t="s">
+        <v>12</v>
       </c>
       <c r="F97" t="s">
         <v>6</v>
       </c>
-      <c r="G97" s="10"/>
-      <c r="H97" s="10"/>
-    </row>
-    <row r="98" spans="1:8" ht="30">
-      <c r="A98" s="22"/>
-      <c r="B98" s="13" t="s">
-        <v>478</v>
-      </c>
-      <c r="C98" s="13"/>
-      <c r="D98" s="13"/>
-      <c r="E98" s="13" t="s">
-        <v>475</v>
-      </c>
-      <c r="F98" s="13"/>
-      <c r="G98" s="10"/>
-      <c r="H98" s="10"/>
-    </row>
-    <row r="99" spans="1:8" ht="30">
-      <c r="A99" s="22"/>
-      <c r="B99" s="13" t="s">
-        <v>479</v>
-      </c>
-      <c r="C99" s="13"/>
-      <c r="D99" s="13"/>
-      <c r="E99" s="13" t="s">
-        <v>480</v>
-      </c>
-      <c r="F99" s="13"/>
-      <c r="G99" s="10"/>
-      <c r="H99" s="10"/>
-    </row>
-    <row r="100" spans="1:8" ht="15">
-      <c r="A100" s="22"/>
-      <c r="B100" s="15" t="s">
-        <v>476</v>
-      </c>
-      <c r="C100" s="15"/>
-      <c r="D100" s="15"/>
-      <c r="E100" s="15"/>
-      <c r="G100" s="10"/>
-      <c r="H100" s="10"/>
-    </row>
-    <row r="101" spans="1:8" ht="12">
-      <c r="A101" s="22"/>
-      <c r="B101" t="s">
+      <c r="G97" s="12"/>
+      <c r="H97" s="12"/>
+    </row>
+    <row r="98" spans="1:10" ht="12">
+      <c r="A98" s="21"/>
+      <c r="B98" s="4" t="s">
         <v>15</v>
       </c>
-      <c r="G101" s="10"/>
-      <c r="H101" s="10"/>
-    </row>
-    <row r="102" spans="1:8" ht="12">
-      <c r="A102" s="22"/>
-      <c r="B102" s="2" t="s">
+      <c r="C98" s="4"/>
+      <c r="D98" s="4"/>
+      <c r="E98" s="4"/>
+      <c r="F98" s="4"/>
+    </row>
+    <row r="99" spans="1:10" ht="12">
+      <c r="A99" s="21"/>
+      <c r="B99" s="4" t="s">
+        <v>16</v>
+      </c>
+      <c r="C99" s="4" t="s">
+        <v>17</v>
+      </c>
+      <c r="D99" s="4" t="s">
+        <v>18</v>
+      </c>
+      <c r="E99" s="4"/>
+      <c r="F99" s="4"/>
+    </row>
+    <row r="100" spans="1:10" ht="36">
+      <c r="A100" s="21"/>
+      <c r="B100" s="4" t="s">
         <v>13</v>
       </c>
-      <c r="C102" s="12"/>
-      <c r="D102" s="26" t="s">
-        <v>487</v>
-      </c>
-      <c r="E102" s="12"/>
-      <c r="F102" s="12"/>
-      <c r="G102" s="10"/>
-      <c r="H102" s="10"/>
-    </row>
-    <row r="103" spans="1:8" ht="12">
-      <c r="A103" s="22"/>
-      <c r="B103" s="2" t="s">
+      <c r="C100" s="4"/>
+      <c r="D100" s="4" t="s">
+        <v>19</v>
+      </c>
+      <c r="E100" s="4" t="s">
+        <v>20</v>
+      </c>
+      <c r="F100" s="4"/>
+    </row>
+    <row r="101" spans="1:10" ht="12">
+      <c r="A101" s="21"/>
+      <c r="B101" s="4" t="s">
+        <v>16</v>
+      </c>
+      <c r="C101" s="4" t="s">
+        <v>21</v>
+      </c>
+      <c r="D101" s="4" t="s">
+        <v>22</v>
+      </c>
+      <c r="E101" s="4"/>
+      <c r="F101" s="4"/>
+    </row>
+    <row r="102" spans="1:10" ht="36">
+      <c r="A102" s="21"/>
+      <c r="B102" s="4" t="s">
+        <v>13</v>
+      </c>
+      <c r="C102" s="4"/>
+      <c r="D102" s="4" t="s">
+        <v>23</v>
+      </c>
+      <c r="E102" s="4" t="s">
+        <v>24</v>
+      </c>
+      <c r="F102" s="4"/>
+      <c r="I102" s="12"/>
+    </row>
+    <row r="103" spans="1:10" ht="12.75" customHeight="1">
+      <c r="A103" s="21"/>
+      <c r="B103" s="4" t="s">
         <v>25</v>
       </c>
-      <c r="C103" s="12"/>
-      <c r="D103" s="26"/>
-      <c r="E103" s="12"/>
-      <c r="F103" s="12"/>
-      <c r="G103" s="10"/>
-      <c r="H103" s="10"/>
-    </row>
-    <row r="104" spans="1:8" ht="15">
-      <c r="A104" s="22"/>
+      <c r="C103" s="4"/>
+      <c r="D103" s="4"/>
+      <c r="E103" s="4"/>
+      <c r="F103" s="4"/>
+    </row>
+    <row r="104" spans="1:10" ht="12.75" customHeight="1">
+      <c r="A104" s="21"/>
       <c r="B104" s="15" t="s">
-        <v>477</v>
-      </c>
-      <c r="C104" s="18"/>
-      <c r="D104" s="32"/>
-      <c r="E104" s="18"/>
-      <c r="F104" s="12"/>
-      <c r="G104" s="10"/>
-      <c r="H104" s="10"/>
-    </row>
-    <row r="105" spans="1:8" ht="30">
-      <c r="A105" s="28"/>
-      <c r="B105" s="13" t="s">
-        <v>482</v>
-      </c>
-      <c r="C105" s="13"/>
-      <c r="D105" s="13"/>
-      <c r="E105" s="13" t="s">
-        <v>474</v>
-      </c>
-      <c r="F105" s="13"/>
-    </row>
-    <row r="106" spans="1:8" ht="30">
-      <c r="A106" s="28"/>
+        <v>83</v>
+      </c>
+      <c r="C104" s="15"/>
+      <c r="D104" s="15"/>
+      <c r="E104" s="15"/>
+      <c r="F104" s="15"/>
+      <c r="G104" s="15"/>
+      <c r="H104" s="15"/>
+    </row>
+    <row r="105" spans="1:10" s="12" customFormat="1" ht="12.75" customHeight="1"/>
+    <row r="106" spans="1:10" s="14" customFormat="1" ht="12.75" customHeight="1">
+      <c r="A106" s="24"/>
       <c r="B106" s="13" t="s">
-        <v>483</v>
-      </c>
-      <c r="C106" s="13"/>
-      <c r="D106" s="13"/>
-      <c r="E106" s="13" t="s">
-        <v>484</v>
-      </c>
-      <c r="F106" s="13"/>
-    </row>
-    <row r="107" spans="1:8" s="10" customFormat="1" ht="15">
-      <c r="B107" s="27" t="s">
+        <v>111</v>
+      </c>
+      <c r="E106" s="14" t="s">
+        <v>112</v>
+      </c>
+      <c r="I106" s="12"/>
+      <c r="J106" s="12"/>
+    </row>
+    <row r="107" spans="1:10" ht="12.75" customHeight="1">
+      <c r="B107" s="13" t="s">
+        <v>89</v>
+      </c>
+      <c r="C107" s="14"/>
+      <c r="D107" s="14"/>
+      <c r="E107" s="14" t="s">
+        <v>84</v>
+      </c>
+      <c r="F107" s="14"/>
+      <c r="G107" s="14"/>
+      <c r="H107" s="14"/>
+    </row>
+    <row r="108" spans="1:10" ht="12.75" customHeight="1">
+      <c r="A108" s="21" t="s">
+        <v>436</v>
+      </c>
+      <c r="B108" s="15" t="s">
+        <v>128</v>
+      </c>
+      <c r="C108" s="18"/>
+      <c r="D108" s="18"/>
+      <c r="E108" s="18"/>
+      <c r="F108" s="18"/>
+      <c r="G108" s="18"/>
+      <c r="H108" s="18"/>
+    </row>
+    <row r="109" spans="1:10" ht="12.75" customHeight="1">
+      <c r="A109" s="21"/>
+      <c r="B109" s="2" t="s">
+        <v>229</v>
+      </c>
+      <c r="C109" s="12" t="s">
+        <v>85</v>
+      </c>
+      <c r="D109" s="12" t="s">
+        <v>86</v>
+      </c>
+      <c r="E109" s="12"/>
+      <c r="F109" s="12" t="s">
+        <v>87</v>
+      </c>
+      <c r="G109" s="12"/>
+      <c r="H109" s="12"/>
+    </row>
+    <row r="110" spans="1:10" ht="12.75" customHeight="1">
+      <c r="A110" s="21"/>
+      <c r="B110" s="15" t="s">
+        <v>88</v>
+      </c>
+      <c r="C110" s="18"/>
+      <c r="D110" s="18"/>
+      <c r="E110" s="18"/>
+      <c r="F110" s="18"/>
+      <c r="G110" s="18"/>
+      <c r="H110" s="18"/>
+    </row>
+    <row r="111" spans="1:10" ht="12.75" customHeight="1">
+      <c r="C111" s="12"/>
+      <c r="D111" s="12"/>
+      <c r="E111" s="12"/>
+      <c r="F111" s="12"/>
+      <c r="G111" s="12"/>
+      <c r="H111" s="12"/>
+    </row>
+    <row r="112" spans="1:10" ht="12.75" customHeight="1">
+      <c r="B112" s="13" t="s">
+        <v>119</v>
+      </c>
+      <c r="C112" s="14"/>
+      <c r="D112" s="14"/>
+      <c r="E112" s="14" t="s">
+        <v>121</v>
+      </c>
+      <c r="F112" s="14"/>
+      <c r="G112" s="14"/>
+      <c r="H112" s="14"/>
+    </row>
+    <row r="113" spans="1:8" ht="12.75" customHeight="1">
+      <c r="B113" s="13" t="s">
+        <v>120</v>
+      </c>
+      <c r="C113" s="14"/>
+      <c r="D113" s="14"/>
+      <c r="E113" s="14" t="s">
+        <v>122</v>
+      </c>
+      <c r="F113" s="14"/>
+      <c r="G113" s="14"/>
+      <c r="H113" s="14"/>
+    </row>
+    <row r="114" spans="1:8" ht="12.75" customHeight="1">
+      <c r="A114" s="21" t="s">
+        <v>64</v>
+      </c>
+      <c r="B114" s="15" t="s">
+        <v>129</v>
+      </c>
+      <c r="C114" s="18"/>
+      <c r="D114" s="18"/>
+      <c r="E114" s="18"/>
+      <c r="F114" s="18"/>
+      <c r="G114" s="18"/>
+      <c r="H114" s="18"/>
+    </row>
+    <row r="115" spans="1:8" ht="12.75" customHeight="1">
+      <c r="A115" s="21"/>
+      <c r="B115" t="s">
+        <v>228</v>
+      </c>
+      <c r="C115" t="s">
+        <v>65</v>
+      </c>
+      <c r="D115" t="s">
+        <v>67</v>
+      </c>
+      <c r="F115" t="s">
+        <v>6</v>
+      </c>
+      <c r="G115" s="12"/>
+      <c r="H115" s="12"/>
+    </row>
+    <row r="116" spans="1:8" ht="12.75" customHeight="1">
+      <c r="A116" s="21"/>
+      <c r="B116" s="2" t="s">
         <v>13</v>
       </c>
-      <c r="C107" s="27"/>
-      <c r="D107" s="27" t="s">
-        <v>496</v>
-      </c>
-      <c r="E107" s="27"/>
-      <c r="F107" s="27"/>
-    </row>
-    <row r="108" spans="1:8" ht="15">
-      <c r="A108" s="28"/>
-      <c r="B108" s="15" t="s">
-        <v>485</v>
-      </c>
-      <c r="C108" s="15"/>
-      <c r="D108" s="15"/>
-      <c r="E108" s="15"/>
-      <c r="F108" s="15"/>
-    </row>
-    <row r="109" spans="1:8" ht="12">
-      <c r="A109" s="28"/>
-      <c r="B109" t="s">
-        <v>15</v>
-      </c>
-    </row>
-    <row r="110" spans="1:8" ht="12">
-      <c r="A110" s="28"/>
-      <c r="B110" t="s">
-        <v>13</v>
-      </c>
-      <c r="C110" s="21"/>
-      <c r="D110" s="29" t="s">
-        <v>481</v>
-      </c>
-      <c r="E110" s="29"/>
-      <c r="F110" s="21"/>
-    </row>
-    <row r="111" spans="1:8" ht="12">
-      <c r="A111" s="28"/>
-      <c r="B111" t="s">
-        <v>25</v>
-      </c>
-      <c r="C111" s="21"/>
-      <c r="D111" s="29"/>
-      <c r="E111" s="21"/>
-      <c r="F111" s="21"/>
-    </row>
-    <row r="112" spans="1:8" ht="12">
-      <c r="A112" s="28"/>
-      <c r="C112" s="21"/>
-      <c r="D112" s="29"/>
-      <c r="E112" s="21"/>
-      <c r="F112" s="21"/>
-    </row>
-    <row r="113" spans="1:9" ht="15">
-      <c r="A113" s="28"/>
-      <c r="B113" s="15" t="s">
-        <v>486</v>
-      </c>
-      <c r="C113" s="30"/>
-      <c r="D113" s="31"/>
-      <c r="E113" s="30"/>
-      <c r="F113" s="30"/>
-    </row>
-    <row r="114" spans="1:9" s="10" customFormat="1" ht="15">
-      <c r="B114" s="33" t="s">
-        <v>13</v>
-      </c>
-      <c r="C114" s="34"/>
-      <c r="D114" s="35" t="s">
-        <v>495</v>
-      </c>
-      <c r="E114" s="34"/>
-      <c r="F114" s="34"/>
-    </row>
-    <row r="115" spans="1:9" ht="15">
-      <c r="A115" s="28"/>
-      <c r="B115" s="15" t="s">
-        <v>463</v>
-      </c>
-      <c r="C115" s="30"/>
-      <c r="D115" s="31"/>
-      <c r="E115" s="30"/>
-      <c r="F115" s="30"/>
-    </row>
-    <row r="116" spans="1:9" s="10" customFormat="1" ht="15">
-      <c r="B116" s="33" t="s">
-        <v>13</v>
-      </c>
-      <c r="C116" s="34"/>
-      <c r="D116" s="35" t="s">
-        <v>497</v>
-      </c>
-      <c r="E116" s="34"/>
-      <c r="F116" s="34"/>
-    </row>
-    <row r="117" spans="1:9" ht="15">
-      <c r="A117" s="28"/>
+      <c r="C116" s="12"/>
+      <c r="D116" s="12" t="s">
+        <v>64</v>
+      </c>
+      <c r="E116" s="12"/>
+      <c r="F116" s="12"/>
+      <c r="G116" s="12"/>
+      <c r="H116" s="12"/>
+    </row>
+    <row r="117" spans="1:8" ht="12.75" customHeight="1">
+      <c r="A117" s="21"/>
       <c r="B117" s="15" t="s">
-        <v>80</v>
-      </c>
-      <c r="C117" s="30"/>
-      <c r="D117" s="31"/>
-      <c r="E117" s="30"/>
-      <c r="F117" s="30"/>
-    </row>
-    <row r="118" spans="1:9" ht="15">
-      <c r="A118" s="10"/>
-      <c r="B118" s="33"/>
-      <c r="C118" s="34"/>
-      <c r="D118" s="35"/>
-      <c r="E118" s="34"/>
-      <c r="F118" s="34"/>
-    </row>
-    <row r="119" spans="1:9" s="13" customFormat="1" ht="15">
-      <c r="A119" s="27"/>
-      <c r="B119" s="13" t="s">
-        <v>109</v>
-      </c>
-      <c r="C119" s="36"/>
-      <c r="D119" s="37"/>
-      <c r="E119" s="14" t="s">
-        <v>488</v>
-      </c>
-      <c r="F119" s="36"/>
-    </row>
-    <row r="120" spans="1:9" s="13" customFormat="1" ht="15">
-      <c r="A120" s="27"/>
-      <c r="B120" s="13" t="s">
-        <v>81</v>
-      </c>
-      <c r="C120" s="36"/>
-      <c r="D120" s="37"/>
-      <c r="E120" s="14" t="s">
-        <v>82</v>
-      </c>
-      <c r="F120" s="36"/>
-    </row>
-    <row r="121" spans="1:9" ht="15">
-      <c r="A121" s="22" t="s">
-        <v>470</v>
-      </c>
-      <c r="B121" s="15" t="s">
-        <v>110</v>
-      </c>
-      <c r="C121" s="15"/>
-      <c r="D121" s="15"/>
-      <c r="E121" s="15"/>
-      <c r="F121" s="15"/>
-      <c r="G121" s="15"/>
-      <c r="H121" s="15"/>
-    </row>
-    <row r="122" spans="1:9" ht="12">
-      <c r="A122" s="22"/>
-      <c r="B122" t="s">
-        <v>228</v>
-      </c>
-      <c r="C122" t="s">
-        <v>11</v>
-      </c>
-      <c r="D122" t="s">
-        <v>12</v>
-      </c>
-      <c r="F122" t="s">
-        <v>6</v>
-      </c>
-      <c r="G122" s="12"/>
-      <c r="H122" s="12"/>
-    </row>
-    <row r="123" spans="1:9" ht="12">
-      <c r="A123" s="22"/>
-      <c r="B123" s="4" t="s">
-        <v>15</v>
-      </c>
-      <c r="C123" s="4"/>
-      <c r="D123" s="4"/>
-      <c r="E123" s="4"/>
-      <c r="F123" s="4"/>
-    </row>
-    <row r="124" spans="1:9" ht="12">
-      <c r="A124" s="22"/>
-      <c r="B124" s="4" t="s">
-        <v>16</v>
-      </c>
-      <c r="C124" s="4" t="s">
-        <v>17</v>
-      </c>
-      <c r="D124" s="4" t="s">
-        <v>18</v>
-      </c>
-      <c r="E124" s="4"/>
-      <c r="F124" s="4"/>
-    </row>
-    <row r="125" spans="1:9" ht="36">
-      <c r="A125" s="22"/>
-      <c r="B125" s="4" t="s">
-        <v>13</v>
-      </c>
-      <c r="C125" s="4"/>
-      <c r="D125" s="4" t="s">
-        <v>19</v>
-      </c>
-      <c r="E125" s="4" t="s">
-        <v>20</v>
-      </c>
-      <c r="F125" s="4"/>
-    </row>
-    <row r="126" spans="1:9" ht="12">
-      <c r="A126" s="22"/>
-      <c r="B126" s="4" t="s">
-        <v>16</v>
-      </c>
-      <c r="C126" s="4" t="s">
-        <v>21</v>
-      </c>
-      <c r="D126" s="4" t="s">
-        <v>22</v>
-      </c>
-      <c r="E126" s="4"/>
-      <c r="F126" s="4"/>
-    </row>
-    <row r="127" spans="1:9" ht="36">
-      <c r="A127" s="22"/>
-      <c r="B127" s="4" t="s">
-        <v>13</v>
-      </c>
-      <c r="C127" s="4"/>
-      <c r="D127" s="4" t="s">
-        <v>23</v>
-      </c>
-      <c r="E127" s="4" t="s">
-        <v>24</v>
-      </c>
-      <c r="F127" s="4"/>
-      <c r="I127" s="12"/>
-    </row>
-    <row r="128" spans="1:9" ht="12.75" customHeight="1">
-      <c r="A128" s="22"/>
-      <c r="B128" s="4" t="s">
-        <v>25</v>
-      </c>
-      <c r="C128" s="4"/>
-      <c r="D128" s="4"/>
-      <c r="E128" s="4"/>
-      <c r="F128" s="4"/>
-    </row>
-    <row r="129" spans="1:10" ht="12.75" customHeight="1">
-      <c r="A129" s="22"/>
-      <c r="B129" s="15" t="s">
-        <v>83</v>
-      </c>
-      <c r="C129" s="15"/>
-      <c r="D129" s="15"/>
-      <c r="E129" s="15"/>
-      <c r="F129" s="15"/>
-      <c r="G129" s="15"/>
-      <c r="H129" s="15"/>
-    </row>
-    <row r="130" spans="1:10" s="12" customFormat="1" ht="12.75" customHeight="1"/>
-    <row r="131" spans="1:10" s="14" customFormat="1" ht="12.75" customHeight="1">
-      <c r="A131" s="25"/>
-      <c r="B131" s="13" t="s">
-        <v>111</v>
-      </c>
-      <c r="E131" s="14" t="s">
-        <v>112</v>
-      </c>
-      <c r="I131" s="12"/>
-      <c r="J131" s="12"/>
-    </row>
-    <row r="132" spans="1:10" ht="12.75" customHeight="1">
-      <c r="B132" s="13" t="s">
-        <v>89</v>
-      </c>
-      <c r="C132" s="14"/>
-      <c r="D132" s="14"/>
-      <c r="E132" s="14" t="s">
-        <v>84</v>
-      </c>
-      <c r="F132" s="14"/>
-      <c r="G132" s="14"/>
-      <c r="H132" s="14"/>
-    </row>
-    <row r="133" spans="1:10" ht="12.75" customHeight="1">
-      <c r="A133" s="22" t="s">
-        <v>471</v>
-      </c>
-      <c r="B133" s="15" t="s">
-        <v>128</v>
-      </c>
-      <c r="C133" s="18"/>
-      <c r="D133" s="18"/>
-      <c r="E133" s="18"/>
-      <c r="F133" s="18"/>
-      <c r="G133" s="18"/>
-      <c r="H133" s="18"/>
-    </row>
-    <row r="134" spans="1:10" ht="12.75" customHeight="1">
-      <c r="A134" s="22"/>
-      <c r="B134" s="2" t="s">
-        <v>230</v>
-      </c>
-      <c r="C134" s="12" t="s">
-        <v>85</v>
-      </c>
-      <c r="D134" s="12" t="s">
-        <v>86</v>
-      </c>
-      <c r="E134" s="12"/>
-      <c r="F134" s="12" t="s">
-        <v>87</v>
-      </c>
-      <c r="G134" s="12"/>
-      <c r="H134" s="12"/>
-    </row>
-    <row r="135" spans="1:10" ht="12.75" customHeight="1">
-      <c r="A135" s="22"/>
-      <c r="B135" s="15" t="s">
-        <v>88</v>
-      </c>
-      <c r="C135" s="18"/>
-      <c r="D135" s="18"/>
-      <c r="E135" s="18"/>
-      <c r="F135" s="18"/>
-      <c r="G135" s="18"/>
-      <c r="H135" s="18"/>
-    </row>
-    <row r="136" spans="1:10" ht="12.75" customHeight="1">
-      <c r="C136" s="12"/>
-      <c r="D136" s="12"/>
-      <c r="E136" s="12"/>
-      <c r="F136" s="12"/>
-      <c r="G136" s="12"/>
-      <c r="H136" s="12"/>
-    </row>
-    <row r="137" spans="1:10" ht="12.75" customHeight="1">
-      <c r="B137" s="13" t="s">
-        <v>119</v>
-      </c>
-      <c r="C137" s="14"/>
-      <c r="D137" s="14"/>
-      <c r="E137" s="14" t="s">
-        <v>121</v>
-      </c>
-      <c r="F137" s="14"/>
-      <c r="G137" s="14"/>
-      <c r="H137" s="14"/>
-    </row>
-    <row r="138" spans="1:10" ht="12.75" customHeight="1">
-      <c r="B138" s="13" t="s">
-        <v>120</v>
-      </c>
-      <c r="C138" s="14"/>
-      <c r="D138" s="14"/>
-      <c r="E138" s="14" t="s">
-        <v>122</v>
-      </c>
-      <c r="F138" s="14"/>
-      <c r="G138" s="14"/>
-      <c r="H138" s="14"/>
-    </row>
-    <row r="139" spans="1:10" ht="12.75" customHeight="1">
-      <c r="A139" s="22" t="s">
-        <v>64</v>
-      </c>
-      <c r="B139" s="15" t="s">
-        <v>129</v>
-      </c>
-      <c r="C139" s="18"/>
-      <c r="D139" s="18"/>
-      <c r="E139" s="18"/>
-      <c r="F139" s="18"/>
-      <c r="G139" s="18"/>
-      <c r="H139" s="18"/>
-    </row>
-    <row r="140" spans="1:10" ht="12.75" customHeight="1">
-      <c r="A140" s="22"/>
-      <c r="B140" t="s">
-        <v>229</v>
-      </c>
-      <c r="C140" t="s">
-        <v>65</v>
-      </c>
-      <c r="D140" t="s">
-        <v>67</v>
-      </c>
-      <c r="F140" t="s">
-        <v>6</v>
-      </c>
-      <c r="G140" s="12"/>
-      <c r="H140" s="12"/>
-    </row>
-    <row r="141" spans="1:10" ht="12.75" customHeight="1">
-      <c r="A141" s="22"/>
-      <c r="B141" s="2" t="s">
-        <v>13</v>
-      </c>
-      <c r="C141" s="12"/>
-      <c r="D141" s="12" t="s">
-        <v>64</v>
-      </c>
-      <c r="E141" s="12"/>
-      <c r="F141" s="12"/>
-      <c r="G141" s="12"/>
-      <c r="H141" s="12"/>
-    </row>
-    <row r="142" spans="1:10" ht="12.75" customHeight="1">
-      <c r="A142" s="22"/>
-      <c r="B142" s="15" t="s">
         <v>123</v>
       </c>
-      <c r="C142" s="18"/>
-      <c r="D142" s="18"/>
-      <c r="E142" s="18"/>
-      <c r="F142" s="18"/>
-      <c r="G142" s="18"/>
-      <c r="H142" s="18"/>
-    </row>
-    <row r="145" spans="2:2" ht="12.75" customHeight="1">
-      <c r="B145" s="17" t="s">
+      <c r="C117" s="18"/>
+      <c r="D117" s="18"/>
+      <c r="E117" s="18"/>
+      <c r="F117" s="18"/>
+      <c r="G117" s="18"/>
+      <c r="H117" s="18"/>
+    </row>
+    <row r="120" spans="1:8" ht="12.75" customHeight="1">
+      <c r="B120" s="17" t="s">
         <v>107</v>
       </c>
     </row>
@@ -4719,8 +4433,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:B20"/>
   <sheetViews>
-    <sheetView zoomScale="150" zoomScaleNormal="150" zoomScalePageLayoutView="150" workbookViewId="0">
-      <selection activeCell="A22" sqref="A22"/>
+    <sheetView tabSelected="1" zoomScale="150" zoomScaleNormal="150" zoomScalePageLayoutView="150" workbookViewId="0">
+      <selection activeCell="B18" sqref="B18"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultColWidth="17.1640625" defaultRowHeight="12.75" customHeight="1" x14ac:dyDescent="0"/>
@@ -4770,122 +4484,122 @@
     </row>
     <row r="6" spans="1:2" ht="12" customHeight="1">
       <c r="A6" t="s">
+        <v>230</v>
+      </c>
+      <c r="B6" t="s">
         <v>231</v>
-      </c>
-      <c r="B6" t="s">
-        <v>233</v>
       </c>
     </row>
     <row r="7" spans="1:2" ht="12" customHeight="1">
       <c r="A7" t="s">
-        <v>234</v>
+        <v>232</v>
       </c>
       <c r="B7" t="s">
-        <v>249</v>
+        <v>243</v>
       </c>
     </row>
     <row r="8" spans="1:2" ht="12" customHeight="1">
       <c r="A8" t="s">
-        <v>235</v>
+        <v>233</v>
       </c>
       <c r="B8" t="s">
-        <v>242</v>
+        <v>240</v>
       </c>
     </row>
     <row r="9" spans="1:2" ht="12" customHeight="1">
       <c r="A9" t="s">
-        <v>267</v>
+        <v>261</v>
       </c>
       <c r="B9" t="s">
-        <v>264</v>
+        <v>258</v>
       </c>
     </row>
     <row r="10" spans="1:2" ht="12" customHeight="1">
       <c r="A10" t="s">
-        <v>236</v>
+        <v>234</v>
       </c>
       <c r="B10" t="s">
-        <v>243</v>
+        <v>241</v>
       </c>
     </row>
     <row r="11" spans="1:2" ht="12" customHeight="1">
       <c r="A11" t="s">
-        <v>237</v>
+        <v>235</v>
       </c>
       <c r="B11" t="s">
-        <v>244</v>
+        <v>242</v>
       </c>
     </row>
     <row r="12" spans="1:2" ht="42" customHeight="1">
       <c r="A12" t="s">
-        <v>265</v>
+        <v>259</v>
       </c>
       <c r="B12" t="s">
-        <v>266</v>
+        <v>260</v>
       </c>
     </row>
     <row r="13" spans="1:2" ht="12.75" customHeight="1">
       <c r="A13" t="s">
-        <v>405</v>
+        <v>386</v>
       </c>
       <c r="B13" t="s">
-        <v>413</v>
+        <v>392</v>
       </c>
     </row>
     <row r="14" spans="1:2" ht="12.75" customHeight="1">
       <c r="A14" t="s">
-        <v>406</v>
+        <v>387</v>
       </c>
       <c r="B14" t="s">
-        <v>414</v>
+        <v>393</v>
       </c>
     </row>
     <row r="15" spans="1:2" ht="12.75" customHeight="1">
       <c r="A15" t="s">
-        <v>407</v>
+        <v>388</v>
       </c>
       <c r="B15" t="s">
-        <v>415</v>
+        <v>394</v>
       </c>
     </row>
     <row r="16" spans="1:2" ht="12.75" customHeight="1">
       <c r="A16" t="s">
-        <v>408</v>
+        <v>389</v>
       </c>
       <c r="B16" t="s">
-        <v>416</v>
+        <v>395</v>
       </c>
     </row>
     <row r="17" spans="1:2" ht="12.75" customHeight="1">
       <c r="A17" t="s">
-        <v>409</v>
+        <v>465</v>
       </c>
       <c r="B17" t="s">
-        <v>417</v>
+        <v>468</v>
       </c>
     </row>
     <row r="18" spans="1:2" ht="12.75" customHeight="1">
       <c r="A18" t="s">
-        <v>410</v>
+        <v>390</v>
       </c>
       <c r="B18" t="s">
-        <v>418</v>
+        <v>396</v>
       </c>
     </row>
     <row r="19" spans="1:2" ht="12.75" customHeight="1">
       <c r="A19" t="s">
-        <v>411</v>
+        <v>391</v>
       </c>
       <c r="B19" t="s">
-        <v>412</v>
+        <v>466</v>
       </c>
     </row>
     <row r="20" spans="1:2" ht="12.75" customHeight="1">
       <c r="A20" t="s">
-        <v>422</v>
+        <v>398</v>
       </c>
       <c r="B20" t="s">
-        <v>423</v>
+        <v>399</v>
       </c>
     </row>
   </sheetData>
@@ -4903,8 +4617,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:D137"/>
   <sheetViews>
-    <sheetView topLeftCell="A125" workbookViewId="0">
-      <selection activeCell="A136" sqref="A136"/>
+    <sheetView topLeftCell="A86" workbookViewId="0">
+      <selection activeCell="A91" sqref="A91:XFD97"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultColWidth="17.1640625" defaultRowHeight="12.75" customHeight="1" x14ac:dyDescent="0"/>
@@ -5171,1007 +4885,1007 @@
     </row>
     <row r="32" spans="1:3" ht="12.75" customHeight="1">
       <c r="A32" t="s">
+        <v>262</v>
+      </c>
+      <c r="B32" t="s">
+        <v>267</v>
+      </c>
+      <c r="C32" t="s">
+        <v>268</v>
+      </c>
+    </row>
+    <row r="33" spans="1:3" ht="12.75" customHeight="1">
+      <c r="A33" t="s">
+        <v>262</v>
+      </c>
+      <c r="B33" t="s">
+        <v>269</v>
+      </c>
+      <c r="C33" t="s">
+        <v>270</v>
+      </c>
+    </row>
+    <row r="34" spans="1:3" ht="12.75" customHeight="1">
+      <c r="A34" t="s">
+        <v>262</v>
+      </c>
+      <c r="B34" t="s">
+        <v>397</v>
+      </c>
+      <c r="C34" t="s">
+        <v>385</v>
+      </c>
+    </row>
+    <row r="36" spans="1:3" ht="12.75" customHeight="1">
+      <c r="A36" t="s">
+        <v>131</v>
+      </c>
+      <c r="B36" t="s">
+        <v>132</v>
+      </c>
+      <c r="C36" t="s">
+        <v>138</v>
+      </c>
+    </row>
+    <row r="37" spans="1:3" ht="12.75" customHeight="1">
+      <c r="A37" t="s">
+        <v>131</v>
+      </c>
+      <c r="B37" t="s">
+        <v>133</v>
+      </c>
+      <c r="C37" t="s">
+        <v>139</v>
+      </c>
+    </row>
+    <row r="38" spans="1:3" ht="12.75" customHeight="1">
+      <c r="A38" t="s">
+        <v>131</v>
+      </c>
+      <c r="B38" t="s">
+        <v>134</v>
+      </c>
+      <c r="C38" t="s">
+        <v>140</v>
+      </c>
+    </row>
+    <row r="39" spans="1:3" ht="12.75" customHeight="1">
+      <c r="A39" t="s">
+        <v>131</v>
+      </c>
+      <c r="B39" t="s">
+        <v>135</v>
+      </c>
+      <c r="C39" t="s">
+        <v>141</v>
+      </c>
+    </row>
+    <row r="40" spans="1:3" ht="12.75" customHeight="1">
+      <c r="A40" t="s">
+        <v>131</v>
+      </c>
+      <c r="B40" t="s">
+        <v>136</v>
+      </c>
+      <c r="C40" t="s">
+        <v>142</v>
+      </c>
+    </row>
+    <row r="41" spans="1:3" ht="12.75" customHeight="1">
+      <c r="A41" t="s">
+        <v>131</v>
+      </c>
+      <c r="B41" t="s">
+        <v>137</v>
+      </c>
+      <c r="C41" t="s">
+        <v>143</v>
+      </c>
+    </row>
+    <row r="43" spans="1:3" ht="12.75" customHeight="1">
+      <c r="A43" t="s">
+        <v>265</v>
+      </c>
+      <c r="B43" t="s">
         <v>271</v>
       </c>
-      <c r="B32" t="s">
+      <c r="C43" t="s">
+        <v>289</v>
+      </c>
+    </row>
+    <row r="44" spans="1:3" ht="12.75" customHeight="1">
+      <c r="A44" t="s">
+        <v>265</v>
+      </c>
+      <c r="B44" t="s">
+        <v>274</v>
+      </c>
+      <c r="C44" t="s">
+        <v>290</v>
+      </c>
+    </row>
+    <row r="45" spans="1:3" ht="12.75" customHeight="1">
+      <c r="A45" t="s">
+        <v>265</v>
+      </c>
+      <c r="B45" t="s">
+        <v>277</v>
+      </c>
+      <c r="C45" t="s">
+        <v>291</v>
+      </c>
+    </row>
+    <row r="46" spans="1:3" ht="12.75" customHeight="1">
+      <c r="A46" t="s">
+        <v>265</v>
+      </c>
+      <c r="B46" t="s">
         <v>278</v>
       </c>
-      <c r="C32" t="s">
-        <v>279</v>
-      </c>
-    </row>
-    <row r="33" spans="1:4" ht="12.75" customHeight="1">
-      <c r="A33" t="s">
-        <v>271</v>
-      </c>
-      <c r="B33" t="s">
+      <c r="C46" t="s">
+        <v>384</v>
+      </c>
+    </row>
+    <row r="47" spans="1:3" ht="12.75" customHeight="1">
+      <c r="A47" t="s">
+        <v>265</v>
+      </c>
+      <c r="B47" t="s">
         <v>280</v>
       </c>
-      <c r="C33" t="s">
-        <v>281</v>
-      </c>
-    </row>
-    <row r="34" spans="1:4" ht="12.75" customHeight="1">
-      <c r="A34" t="s">
-        <v>271</v>
-      </c>
-      <c r="B34" t="s">
-        <v>419</v>
-      </c>
-      <c r="C34" t="s">
-        <v>396</v>
-      </c>
-    </row>
-    <row r="36" spans="1:4" ht="12.75" customHeight="1">
-      <c r="A36" t="s">
-        <v>132</v>
-      </c>
-      <c r="B36" t="s">
-        <v>133</v>
-      </c>
-      <c r="C36" t="s">
-        <v>139</v>
-      </c>
-    </row>
-    <row r="37" spans="1:4" ht="12.75" customHeight="1">
-      <c r="A37" t="s">
-        <v>132</v>
-      </c>
-      <c r="B37" t="s">
-        <v>134</v>
-      </c>
-      <c r="C37" t="s">
-        <v>140</v>
-      </c>
-    </row>
-    <row r="38" spans="1:4" ht="12.75" customHeight="1">
-      <c r="A38" t="s">
-        <v>132</v>
-      </c>
-      <c r="B38" t="s">
-        <v>135</v>
-      </c>
-      <c r="C38" t="s">
-        <v>141</v>
-      </c>
-    </row>
-    <row r="39" spans="1:4" ht="12.75" customHeight="1">
-      <c r="A39" t="s">
-        <v>132</v>
-      </c>
-      <c r="B39" t="s">
-        <v>136</v>
-      </c>
-      <c r="C39" t="s">
-        <v>142</v>
-      </c>
-    </row>
-    <row r="40" spans="1:4" ht="12.75" customHeight="1">
-      <c r="A40" t="s">
-        <v>132</v>
-      </c>
-      <c r="B40" t="s">
-        <v>137</v>
-      </c>
-      <c r="C40" t="s">
-        <v>143</v>
-      </c>
-    </row>
-    <row r="41" spans="1:4" ht="12.75" customHeight="1">
-      <c r="A41" t="s">
-        <v>132</v>
-      </c>
-      <c r="B41" t="s">
-        <v>138</v>
-      </c>
-      <c r="C41" t="s">
-        <v>144</v>
-      </c>
-    </row>
-    <row r="43" spans="1:4" ht="12.75" customHeight="1">
-      <c r="A43" t="s">
-        <v>146</v>
-      </c>
-      <c r="B43" t="s">
+      <c r="C47" t="s">
+        <v>292</v>
+      </c>
+    </row>
+    <row r="48" spans="1:3" ht="12.75" customHeight="1">
+      <c r="A48" t="s">
+        <v>265</v>
+      </c>
+      <c r="B48" t="s">
+        <v>282</v>
+      </c>
+      <c r="C48" t="s">
+        <v>293</v>
+      </c>
+    </row>
+    <row r="50" spans="1:4" ht="12.75" customHeight="1">
+      <c r="A50" t="s">
+        <v>145</v>
+      </c>
+      <c r="B50" t="s">
+        <v>152</v>
+      </c>
+      <c r="D50" t="s">
         <v>153</v>
-      </c>
-      <c r="D43" t="s">
-        <v>154</v>
-      </c>
-    </row>
-    <row r="44" spans="1:4" ht="12.75" customHeight="1">
-      <c r="A44" t="s">
-        <v>146</v>
-      </c>
-      <c r="B44" t="s">
-        <v>155</v>
-      </c>
-      <c r="D44" t="s">
-        <v>159</v>
-      </c>
-    </row>
-    <row r="45" spans="1:4" ht="12.75" customHeight="1">
-      <c r="A45" t="s">
-        <v>146</v>
-      </c>
-      <c r="B45" t="s">
-        <v>156</v>
-      </c>
-      <c r="D45" t="s">
-        <v>160</v>
-      </c>
-    </row>
-    <row r="46" spans="1:4" ht="12.75" customHeight="1">
-      <c r="A46" t="s">
-        <v>146</v>
-      </c>
-      <c r="B46" t="s">
-        <v>157</v>
-      </c>
-      <c r="D46" t="s">
-        <v>161</v>
-      </c>
-    </row>
-    <row r="47" spans="1:4" ht="12.75" customHeight="1">
-      <c r="A47" t="s">
-        <v>146</v>
-      </c>
-      <c r="B47" t="s">
-        <v>158</v>
-      </c>
-      <c r="D47" t="s">
-        <v>162</v>
-      </c>
-    </row>
-    <row r="49" spans="1:4" ht="12.75" customHeight="1">
-      <c r="A49" t="s">
-        <v>150</v>
-      </c>
-      <c r="B49" t="s">
-        <v>186</v>
-      </c>
-      <c r="D49" t="s">
-        <v>187</v>
-      </c>
-    </row>
-    <row r="50" spans="1:4" s="2" customFormat="1" ht="12.75" customHeight="1">
-      <c r="A50" t="s">
-        <v>150</v>
-      </c>
-      <c r="B50" t="s">
-        <v>176</v>
-      </c>
-      <c r="D50" t="s">
-        <v>177</v>
       </c>
     </row>
     <row r="51" spans="1:4" ht="12.75" customHeight="1">
       <c r="A51" t="s">
-        <v>150</v>
+        <v>145</v>
       </c>
       <c r="B51" t="s">
-        <v>178</v>
+        <v>154</v>
       </c>
       <c r="D51" t="s">
-        <v>179</v>
+        <v>158</v>
       </c>
     </row>
     <row r="52" spans="1:4" ht="12.75" customHeight="1">
       <c r="A52" t="s">
-        <v>150</v>
+        <v>145</v>
       </c>
       <c r="B52" t="s">
-        <v>180</v>
+        <v>155</v>
       </c>
       <c r="D52" t="s">
-        <v>181</v>
+        <v>159</v>
       </c>
     </row>
     <row r="53" spans="1:4" ht="12.75" customHeight="1">
       <c r="A53" t="s">
-        <v>150</v>
+        <v>145</v>
       </c>
       <c r="B53" t="s">
-        <v>182</v>
+        <v>156</v>
       </c>
       <c r="D53" t="s">
-        <v>183</v>
+        <v>160</v>
       </c>
     </row>
     <row r="54" spans="1:4" ht="12.75" customHeight="1">
       <c r="A54" t="s">
-        <v>150</v>
+        <v>145</v>
       </c>
       <c r="B54" t="s">
-        <v>184</v>
+        <v>157</v>
       </c>
       <c r="D54" t="s">
-        <v>185</v>
+        <v>161</v>
       </c>
     </row>
     <row r="56" spans="1:4" ht="12.75" customHeight="1">
       <c r="A56" t="s">
-        <v>167</v>
+        <v>149</v>
       </c>
       <c r="B56" t="s">
-        <v>188</v>
-      </c>
-      <c r="C56" s="2"/>
+        <v>185</v>
+      </c>
       <c r="D56" t="s">
-        <v>189</v>
-      </c>
-    </row>
-    <row r="57" spans="1:4" ht="12.75" customHeight="1">
+        <v>186</v>
+      </c>
+    </row>
+    <row r="57" spans="1:4" s="2" customFormat="1" ht="12.75" customHeight="1">
       <c r="A57" t="s">
-        <v>167</v>
+        <v>149</v>
       </c>
       <c r="B57" t="s">
-        <v>190</v>
+        <v>175</v>
       </c>
       <c r="D57" t="s">
-        <v>191</v>
+        <v>176</v>
       </c>
     </row>
     <row r="58" spans="1:4" ht="12.75" customHeight="1">
       <c r="A58" t="s">
-        <v>167</v>
+        <v>149</v>
       </c>
       <c r="B58" t="s">
-        <v>192</v>
+        <v>177</v>
       </c>
       <c r="D58" t="s">
-        <v>193</v>
+        <v>178</v>
       </c>
     </row>
     <row r="59" spans="1:4" ht="12.75" customHeight="1">
       <c r="A59" t="s">
-        <v>167</v>
+        <v>149</v>
       </c>
       <c r="B59" t="s">
-        <v>194</v>
+        <v>179</v>
       </c>
       <c r="D59" t="s">
-        <v>195</v>
+        <v>180</v>
       </c>
     </row>
     <row r="60" spans="1:4" ht="12.75" customHeight="1">
       <c r="A60" t="s">
-        <v>167</v>
+        <v>149</v>
       </c>
       <c r="B60" t="s">
-        <v>196</v>
+        <v>181</v>
       </c>
       <c r="D60" t="s">
-        <v>197</v>
-      </c>
-    </row>
-    <row r="62" spans="1:4" ht="12.75" customHeight="1">
-      <c r="A62" t="s">
-        <v>239</v>
-      </c>
-      <c r="B62" t="s">
-        <v>257</v>
-      </c>
-      <c r="D62" t="s">
-        <v>250</v>
+        <v>182</v>
+      </c>
+    </row>
+    <row r="61" spans="1:4" ht="12.75" customHeight="1">
+      <c r="A61" t="s">
+        <v>149</v>
+      </c>
+      <c r="B61" t="s">
+        <v>183</v>
+      </c>
+      <c r="D61" t="s">
+        <v>184</v>
       </c>
     </row>
     <row r="63" spans="1:4" ht="12.75" customHeight="1">
       <c r="A63" t="s">
-        <v>239</v>
+        <v>166</v>
       </c>
       <c r="B63" t="s">
-        <v>258</v>
+        <v>187</v>
       </c>
       <c r="C63" s="2"/>
       <c r="D63" t="s">
-        <v>251</v>
+        <v>188</v>
       </c>
     </row>
     <row r="64" spans="1:4" ht="12.75" customHeight="1">
       <c r="A64" t="s">
-        <v>239</v>
+        <v>166</v>
       </c>
       <c r="B64" t="s">
-        <v>259</v>
+        <v>189</v>
       </c>
       <c r="D64" t="s">
-        <v>252</v>
+        <v>190</v>
       </c>
     </row>
     <row r="65" spans="1:4" ht="12.75" customHeight="1">
       <c r="A65" t="s">
-        <v>239</v>
+        <v>166</v>
       </c>
       <c r="B65" t="s">
-        <v>260</v>
+        <v>191</v>
       </c>
       <c r="D65" t="s">
-        <v>253</v>
+        <v>192</v>
       </c>
     </row>
     <row r="66" spans="1:4" ht="12.75" customHeight="1">
       <c r="A66" t="s">
-        <v>239</v>
+        <v>166</v>
       </c>
       <c r="B66" t="s">
-        <v>261</v>
+        <v>193</v>
       </c>
       <c r="D66" t="s">
-        <v>254</v>
+        <v>194</v>
       </c>
     </row>
     <row r="67" spans="1:4" ht="12.75" customHeight="1">
       <c r="A67" t="s">
-        <v>239</v>
+        <v>166</v>
       </c>
       <c r="B67" t="s">
-        <v>262</v>
+        <v>195</v>
       </c>
       <c r="D67" t="s">
-        <v>255</v>
-      </c>
-    </row>
-    <row r="68" spans="1:4" ht="12.75" customHeight="1">
-      <c r="A68" t="s">
-        <v>239</v>
-      </c>
-      <c r="B68" t="s">
-        <v>263</v>
-      </c>
-      <c r="D68" t="s">
-        <v>256</v>
+        <v>196</v>
+      </c>
+    </row>
+    <row r="69" spans="1:4" ht="12.75" customHeight="1">
+      <c r="A69" t="s">
+        <v>237</v>
+      </c>
+      <c r="B69" t="s">
+        <v>251</v>
+      </c>
+      <c r="D69" t="s">
+        <v>244</v>
       </c>
     </row>
     <row r="70" spans="1:4" ht="12.75" customHeight="1">
       <c r="A70" t="s">
-        <v>171</v>
+        <v>237</v>
       </c>
       <c r="B70" t="s">
-        <v>198</v>
-      </c>
+        <v>252</v>
+      </c>
+      <c r="C70" s="2"/>
       <c r="D70" t="s">
-        <v>199</v>
+        <v>245</v>
       </c>
     </row>
     <row r="71" spans="1:4" ht="12.75" customHeight="1">
       <c r="A71" t="s">
-        <v>171</v>
+        <v>237</v>
       </c>
       <c r="B71" t="s">
-        <v>200</v>
-      </c>
-      <c r="C71" s="2"/>
+        <v>253</v>
+      </c>
       <c r="D71" t="s">
-        <v>201</v>
+        <v>246</v>
       </c>
     </row>
     <row r="72" spans="1:4" ht="12.75" customHeight="1">
       <c r="A72" t="s">
-        <v>171</v>
+        <v>237</v>
       </c>
       <c r="B72" t="s">
-        <v>202</v>
+        <v>254</v>
       </c>
       <c r="D72" t="s">
-        <v>203</v>
+        <v>247</v>
       </c>
     </row>
     <row r="73" spans="1:4" ht="12.75" customHeight="1">
       <c r="A73" t="s">
-        <v>171</v>
+        <v>237</v>
       </c>
       <c r="B73" t="s">
-        <v>204</v>
+        <v>255</v>
       </c>
       <c r="D73" t="s">
-        <v>205</v>
+        <v>248</v>
       </c>
     </row>
     <row r="74" spans="1:4" ht="12.75" customHeight="1">
       <c r="A74" t="s">
-        <v>171</v>
+        <v>237</v>
       </c>
       <c r="B74" t="s">
-        <v>206</v>
+        <v>256</v>
       </c>
       <c r="D74" t="s">
-        <v>207</v>
+        <v>249</v>
       </c>
     </row>
     <row r="75" spans="1:4" ht="12.75" customHeight="1">
       <c r="A75" t="s">
-        <v>171</v>
+        <v>237</v>
       </c>
       <c r="B75" t="s">
-        <v>208</v>
+        <v>257</v>
       </c>
       <c r="D75" t="s">
-        <v>209</v>
+        <v>250</v>
       </c>
     </row>
     <row r="77" spans="1:4" ht="12.75" customHeight="1">
       <c r="A77" t="s">
-        <v>174</v>
+        <v>170</v>
       </c>
       <c r="B77" t="s">
-        <v>210</v>
+        <v>197</v>
       </c>
       <c r="D77" t="s">
-        <v>211</v>
+        <v>198</v>
       </c>
     </row>
     <row r="78" spans="1:4" ht="12.75" customHeight="1">
       <c r="A78" t="s">
-        <v>174</v>
+        <v>170</v>
       </c>
       <c r="B78" t="s">
-        <v>212</v>
+        <v>199</v>
       </c>
       <c r="C78" s="2"/>
       <c r="D78" t="s">
-        <v>213</v>
+        <v>200</v>
       </c>
     </row>
     <row r="79" spans="1:4" ht="12.75" customHeight="1">
       <c r="A79" t="s">
-        <v>174</v>
+        <v>170</v>
       </c>
       <c r="B79" t="s">
-        <v>214</v>
+        <v>201</v>
       </c>
       <c r="D79" t="s">
-        <v>215</v>
+        <v>202</v>
       </c>
     </row>
     <row r="80" spans="1:4" ht="12.75" customHeight="1">
       <c r="A80" t="s">
-        <v>174</v>
+        <v>170</v>
       </c>
       <c r="B80" t="s">
-        <v>216</v>
+        <v>203</v>
       </c>
       <c r="D80" t="s">
-        <v>217</v>
+        <v>204</v>
       </c>
     </row>
     <row r="81" spans="1:4" ht="12.75" customHeight="1">
       <c r="A81" t="s">
-        <v>174</v>
+        <v>170</v>
       </c>
       <c r="B81" t="s">
-        <v>218</v>
+        <v>205</v>
       </c>
       <c r="D81" t="s">
-        <v>219</v>
+        <v>206</v>
       </c>
     </row>
     <row r="82" spans="1:4" ht="12.75" customHeight="1">
       <c r="A82" t="s">
-        <v>174</v>
+        <v>170</v>
       </c>
       <c r="B82" t="s">
-        <v>220</v>
+        <v>207</v>
       </c>
       <c r="D82" t="s">
-        <v>221</v>
+        <v>208</v>
       </c>
     </row>
     <row r="84" spans="1:4" ht="12.75" customHeight="1">
       <c r="A84" t="s">
-        <v>275</v>
+        <v>173</v>
       </c>
       <c r="B84" t="s">
-        <v>282</v>
-      </c>
-      <c r="C84" t="s">
-        <v>300</v>
+        <v>209</v>
+      </c>
+      <c r="D84" t="s">
+        <v>210</v>
       </c>
     </row>
     <row r="85" spans="1:4" ht="12.75" customHeight="1">
       <c r="A85" t="s">
-        <v>275</v>
+        <v>173</v>
       </c>
       <c r="B85" t="s">
-        <v>285</v>
-      </c>
-      <c r="C85" t="s">
-        <v>301</v>
+        <v>211</v>
+      </c>
+      <c r="C85" s="2"/>
+      <c r="D85" t="s">
+        <v>212</v>
       </c>
     </row>
     <row r="86" spans="1:4" ht="12.75" customHeight="1">
       <c r="A86" t="s">
-        <v>275</v>
+        <v>173</v>
       </c>
       <c r="B86" t="s">
-        <v>288</v>
-      </c>
-      <c r="C86" t="s">
-        <v>302</v>
+        <v>213</v>
+      </c>
+      <c r="D86" t="s">
+        <v>214</v>
       </c>
     </row>
     <row r="87" spans="1:4" ht="12.75" customHeight="1">
       <c r="A87" t="s">
-        <v>275</v>
+        <v>173</v>
       </c>
       <c r="B87" t="s">
-        <v>289</v>
-      </c>
-      <c r="C87" t="s">
-        <v>395</v>
+        <v>215</v>
+      </c>
+      <c r="D87" t="s">
+        <v>216</v>
       </c>
     </row>
     <row r="88" spans="1:4" ht="12.75" customHeight="1">
       <c r="A88" t="s">
-        <v>275</v>
+        <v>173</v>
       </c>
       <c r="B88" t="s">
-        <v>291</v>
-      </c>
-      <c r="C88" t="s">
-        <v>303</v>
+        <v>217</v>
+      </c>
+      <c r="D88" t="s">
+        <v>218</v>
       </c>
     </row>
     <row r="89" spans="1:4" ht="12.75" customHeight="1">
       <c r="A89" t="s">
-        <v>275</v>
+        <v>173</v>
       </c>
       <c r="B89" t="s">
-        <v>293</v>
-      </c>
-      <c r="C89" t="s">
-        <v>304</v>
+        <v>219</v>
+      </c>
+      <c r="D89" t="s">
+        <v>220</v>
       </c>
     </row>
     <row r="91" spans="1:4" ht="12.75" customHeight="1">
       <c r="A91" t="s">
-        <v>305</v>
+        <v>294</v>
       </c>
       <c r="B91" t="s">
-        <v>311</v>
+        <v>300</v>
       </c>
       <c r="C91" t="s">
-        <v>318</v>
+        <v>307</v>
       </c>
     </row>
     <row r="92" spans="1:4" ht="12.75" customHeight="1">
       <c r="A92" t="s">
-        <v>305</v>
+        <v>294</v>
       </c>
       <c r="B92" t="s">
-        <v>312</v>
+        <v>301</v>
       </c>
       <c r="C92" t="s">
-        <v>319</v>
+        <v>308</v>
       </c>
     </row>
     <row r="93" spans="1:4" ht="12.75" customHeight="1">
       <c r="A93" t="s">
-        <v>305</v>
+        <v>294</v>
       </c>
       <c r="B93" t="s">
-        <v>313</v>
+        <v>302</v>
       </c>
       <c r="C93" t="s">
-        <v>320</v>
+        <v>309</v>
       </c>
     </row>
     <row r="94" spans="1:4" ht="12.75" customHeight="1">
       <c r="A94" t="s">
-        <v>305</v>
+        <v>294</v>
       </c>
       <c r="B94" t="s">
-        <v>314</v>
+        <v>303</v>
       </c>
       <c r="C94" t="s">
-        <v>321</v>
+        <v>310</v>
       </c>
     </row>
     <row r="95" spans="1:4" ht="12.75" customHeight="1">
       <c r="A95" t="s">
-        <v>305</v>
+        <v>294</v>
       </c>
       <c r="B95" t="s">
-        <v>315</v>
+        <v>304</v>
       </c>
       <c r="C95" t="s">
-        <v>322</v>
+        <v>311</v>
       </c>
     </row>
     <row r="96" spans="1:4" ht="12.75" customHeight="1">
       <c r="A96" t="s">
+        <v>294</v>
+      </c>
+      <c r="B96" t="s">
         <v>305</v>
       </c>
-      <c r="B96" t="s">
-        <v>316</v>
-      </c>
       <c r="C96" t="s">
-        <v>323</v>
+        <v>312</v>
       </c>
     </row>
     <row r="97" spans="1:3" ht="12.75" customHeight="1">
       <c r="A97" t="s">
-        <v>305</v>
+        <v>294</v>
       </c>
       <c r="B97" t="s">
-        <v>317</v>
+        <v>306</v>
       </c>
       <c r="C97" t="s">
-        <v>324</v>
+        <v>313</v>
       </c>
     </row>
     <row r="99" spans="1:3" ht="12.75" customHeight="1">
       <c r="A99" t="s">
-        <v>306</v>
+        <v>295</v>
       </c>
       <c r="B99" t="s">
-        <v>331</v>
+        <v>320</v>
       </c>
       <c r="C99" t="s">
-        <v>337</v>
+        <v>326</v>
       </c>
     </row>
     <row r="100" spans="1:3" ht="12.75" customHeight="1">
       <c r="A100" t="s">
-        <v>306</v>
+        <v>295</v>
       </c>
       <c r="B100" t="s">
-        <v>332</v>
+        <v>321</v>
       </c>
       <c r="C100" t="s">
-        <v>338</v>
+        <v>327</v>
       </c>
     </row>
     <row r="101" spans="1:3" ht="12.75" customHeight="1">
       <c r="A101" t="s">
-        <v>306</v>
+        <v>295</v>
       </c>
       <c r="B101" t="s">
-        <v>333</v>
+        <v>322</v>
       </c>
       <c r="C101" t="s">
-        <v>339</v>
+        <v>328</v>
       </c>
     </row>
     <row r="102" spans="1:3" ht="12.75" customHeight="1">
       <c r="A102" t="s">
-        <v>306</v>
+        <v>295</v>
       </c>
       <c r="B102" t="s">
-        <v>334</v>
+        <v>323</v>
       </c>
       <c r="C102" t="s">
-        <v>340</v>
+        <v>329</v>
       </c>
     </row>
     <row r="103" spans="1:3" ht="12.75" customHeight="1">
       <c r="A103" t="s">
-        <v>306</v>
+        <v>295</v>
       </c>
       <c r="B103" t="s">
-        <v>335</v>
+        <v>324</v>
       </c>
       <c r="C103" t="s">
-        <v>341</v>
+        <v>330</v>
       </c>
     </row>
     <row r="104" spans="1:3" ht="12.75" customHeight="1">
       <c r="A104" t="s">
-        <v>306</v>
+        <v>295</v>
       </c>
       <c r="B104" t="s">
-        <v>336</v>
+        <v>325</v>
       </c>
       <c r="C104" t="s">
-        <v>342</v>
+        <v>331</v>
       </c>
     </row>
     <row r="106" spans="1:3" ht="12.75" customHeight="1">
       <c r="A106" t="s">
-        <v>307</v>
+        <v>296</v>
       </c>
       <c r="B106" t="s">
-        <v>349</v>
+        <v>338</v>
       </c>
       <c r="C106" t="s">
-        <v>350</v>
+        <v>339</v>
       </c>
     </row>
     <row r="107" spans="1:3" ht="12.75" customHeight="1">
       <c r="A107" t="s">
-        <v>307</v>
+        <v>296</v>
       </c>
       <c r="B107" t="s">
-        <v>343</v>
+        <v>332</v>
       </c>
       <c r="C107" t="s">
-        <v>351</v>
+        <v>340</v>
       </c>
     </row>
     <row r="108" spans="1:3" ht="12.75" customHeight="1">
       <c r="A108" t="s">
-        <v>307</v>
+        <v>296</v>
       </c>
       <c r="B108" t="s">
-        <v>344</v>
+        <v>333</v>
       </c>
       <c r="C108" t="s">
-        <v>352</v>
+        <v>341</v>
       </c>
     </row>
     <row r="109" spans="1:3" ht="12.75" customHeight="1">
       <c r="A109" t="s">
-        <v>307</v>
+        <v>296</v>
       </c>
       <c r="B109" t="s">
-        <v>345</v>
+        <v>334</v>
       </c>
       <c r="C109" t="s">
-        <v>353</v>
+        <v>342</v>
       </c>
     </row>
     <row r="110" spans="1:3" ht="12.75" customHeight="1">
       <c r="A110" t="s">
-        <v>307</v>
+        <v>296</v>
       </c>
       <c r="B110" t="s">
-        <v>346</v>
+        <v>335</v>
       </c>
       <c r="C110" t="s">
-        <v>354</v>
+        <v>343</v>
       </c>
     </row>
     <row r="111" spans="1:3" ht="12.75" customHeight="1">
       <c r="A111" t="s">
-        <v>307</v>
+        <v>296</v>
       </c>
       <c r="B111" t="s">
-        <v>347</v>
+        <v>336</v>
       </c>
       <c r="C111" t="s">
-        <v>355</v>
+        <v>344</v>
       </c>
     </row>
     <row r="112" spans="1:3" ht="12.75" customHeight="1">
       <c r="A112" t="s">
-        <v>307</v>
+        <v>296</v>
       </c>
       <c r="B112" t="s">
-        <v>348</v>
+        <v>337</v>
       </c>
       <c r="C112" t="s">
-        <v>356</v>
+        <v>345</v>
       </c>
     </row>
     <row r="114" spans="1:3" ht="12.75" customHeight="1">
       <c r="A114" t="s">
-        <v>308</v>
+        <v>297</v>
       </c>
       <c r="B114" t="s">
-        <v>357</v>
+        <v>346</v>
       </c>
       <c r="C114" t="s">
-        <v>363</v>
+        <v>352</v>
       </c>
     </row>
     <row r="115" spans="1:3" ht="12.75" customHeight="1">
       <c r="A115" t="s">
-        <v>308</v>
+        <v>297</v>
       </c>
       <c r="B115" t="s">
-        <v>358</v>
+        <v>347</v>
       </c>
       <c r="C115" t="s">
-        <v>364</v>
+        <v>353</v>
       </c>
     </row>
     <row r="116" spans="1:3" ht="12.75" customHeight="1">
       <c r="A116" t="s">
-        <v>308</v>
+        <v>297</v>
       </c>
       <c r="B116" t="s">
-        <v>359</v>
+        <v>348</v>
       </c>
       <c r="C116" t="s">
-        <v>365</v>
+        <v>354</v>
       </c>
     </row>
     <row r="117" spans="1:3" ht="12.75" customHeight="1">
       <c r="A117" t="s">
-        <v>308</v>
+        <v>297</v>
       </c>
       <c r="B117" t="s">
-        <v>360</v>
+        <v>349</v>
       </c>
       <c r="C117" t="s">
-        <v>366</v>
+        <v>355</v>
       </c>
     </row>
     <row r="118" spans="1:3" ht="12.75" customHeight="1">
       <c r="A118" t="s">
-        <v>308</v>
+        <v>297</v>
       </c>
       <c r="B118" t="s">
-        <v>361</v>
+        <v>350</v>
       </c>
       <c r="C118" t="s">
-        <v>367</v>
+        <v>356</v>
       </c>
     </row>
     <row r="119" spans="1:3" ht="12.75" customHeight="1">
       <c r="A119" t="s">
-        <v>308</v>
+        <v>297</v>
       </c>
       <c r="B119" t="s">
-        <v>362</v>
+        <v>351</v>
       </c>
       <c r="C119" t="s">
-        <v>368</v>
+        <v>357</v>
       </c>
     </row>
     <row r="121" spans="1:3" ht="12.75" customHeight="1">
       <c r="A121" t="s">
-        <v>309</v>
+        <v>298</v>
       </c>
       <c r="B121" t="s">
-        <v>375</v>
+        <v>364</v>
       </c>
       <c r="C121" t="s">
-        <v>376</v>
+        <v>365</v>
       </c>
     </row>
     <row r="122" spans="1:3" ht="12.75" customHeight="1">
       <c r="A122" t="s">
-        <v>309</v>
+        <v>298</v>
       </c>
       <c r="B122" t="s">
-        <v>369</v>
+        <v>358</v>
       </c>
       <c r="C122" t="s">
-        <v>377</v>
+        <v>366</v>
       </c>
     </row>
     <row r="123" spans="1:3" ht="12.75" customHeight="1">
       <c r="A123" t="s">
-        <v>309</v>
+        <v>298</v>
       </c>
       <c r="B123" t="s">
-        <v>370</v>
+        <v>359</v>
       </c>
       <c r="C123" t="s">
-        <v>378</v>
+        <v>367</v>
       </c>
     </row>
     <row r="124" spans="1:3" ht="12.75" customHeight="1">
       <c r="A124" t="s">
-        <v>309</v>
+        <v>298</v>
       </c>
       <c r="B124" t="s">
-        <v>372</v>
+        <v>361</v>
       </c>
       <c r="C124" t="s">
-        <v>379</v>
+        <v>368</v>
       </c>
     </row>
     <row r="125" spans="1:3" ht="12.75" customHeight="1">
       <c r="A125" t="s">
-        <v>309</v>
+        <v>298</v>
       </c>
       <c r="B125" t="s">
-        <v>371</v>
+        <v>360</v>
       </c>
       <c r="C125" t="s">
-        <v>380</v>
+        <v>369</v>
       </c>
     </row>
     <row r="126" spans="1:3" ht="12.75" customHeight="1">
       <c r="A126" t="s">
-        <v>309</v>
+        <v>298</v>
       </c>
       <c r="B126" t="s">
-        <v>373</v>
+        <v>362</v>
       </c>
       <c r="C126" t="s">
-        <v>381</v>
+        <v>370</v>
       </c>
     </row>
     <row r="127" spans="1:3" ht="12.75" customHeight="1">
       <c r="A127" t="s">
-        <v>309</v>
+        <v>298</v>
       </c>
       <c r="B127" t="s">
-        <v>374</v>
+        <v>363</v>
       </c>
       <c r="C127" t="s">
-        <v>382</v>
+        <v>371</v>
       </c>
     </row>
     <row r="129" spans="1:3" ht="12.75" customHeight="1">
       <c r="A129" t="s">
-        <v>310</v>
+        <v>299</v>
       </c>
       <c r="B129" t="s">
-        <v>383</v>
+        <v>372</v>
       </c>
       <c r="C129" t="s">
-        <v>389</v>
+        <v>378</v>
       </c>
     </row>
     <row r="130" spans="1:3" ht="12.75" customHeight="1">
       <c r="A130" t="s">
-        <v>310</v>
+        <v>299</v>
       </c>
       <c r="B130" t="s">
-        <v>384</v>
+        <v>373</v>
       </c>
       <c r="C130" t="s">
-        <v>390</v>
+        <v>379</v>
       </c>
     </row>
     <row r="131" spans="1:3" ht="12.75" customHeight="1">
       <c r="A131" t="s">
-        <v>310</v>
+        <v>299</v>
       </c>
       <c r="B131" t="s">
-        <v>385</v>
+        <v>374</v>
       </c>
       <c r="C131" t="s">
-        <v>391</v>
+        <v>380</v>
       </c>
     </row>
     <row r="132" spans="1:3" ht="12.75" customHeight="1">
       <c r="A132" t="s">
-        <v>310</v>
+        <v>299</v>
       </c>
       <c r="B132" t="s">
-        <v>386</v>
+        <v>375</v>
       </c>
       <c r="C132" t="s">
-        <v>392</v>
+        <v>381</v>
       </c>
     </row>
     <row r="133" spans="1:3" ht="12.75" customHeight="1">
       <c r="A133" t="s">
-        <v>310</v>
+        <v>299</v>
       </c>
       <c r="B133" t="s">
-        <v>387</v>
+        <v>376</v>
       </c>
       <c r="C133" t="s">
-        <v>393</v>
+        <v>382</v>
       </c>
     </row>
     <row r="134" spans="1:3" ht="12.75" customHeight="1">
       <c r="A134" t="s">
-        <v>310</v>
+        <v>299</v>
       </c>
       <c r="B134" t="s">
-        <v>388</v>
+        <v>377</v>
       </c>
       <c r="C134" t="s">
-        <v>394</v>
+        <v>383</v>
       </c>
     </row>
     <row r="136" spans="1:3" ht="12.75" customHeight="1">
       <c r="A136" t="s">
-        <v>472</v>
+        <v>437</v>
       </c>
       <c r="B136" t="s">
-        <v>467</v>
+        <v>432</v>
       </c>
       <c r="C136" t="s">
-        <v>461</v>
+        <v>426</v>
       </c>
     </row>
     <row r="137" spans="1:3" ht="12.75" customHeight="1">
       <c r="A137" t="s">
-        <v>472</v>
+        <v>437</v>
       </c>
       <c r="B137" t="s">
-        <v>468</v>
+        <v>433</v>
       </c>
       <c r="C137" t="s">
-        <v>469</v>
+        <v>434</v>
       </c>
     </row>
   </sheetData>
@@ -6242,15 +5956,15 @@
         <v>1</v>
       </c>
       <c r="B1" t="s">
-        <v>163</v>
+        <v>162</v>
       </c>
     </row>
     <row r="2" spans="1:2">
       <c r="A2" t="s">
+        <v>163</v>
+      </c>
+      <c r="B2" t="s">
         <v>164</v>
-      </c>
-      <c r="B2" t="s">
-        <v>165</v>
       </c>
     </row>
     <row r="3" spans="1:2">
@@ -6258,7 +5972,7 @@
         <v>4</v>
       </c>
       <c r="B3" t="s">
-        <v>165</v>
+        <v>164</v>
       </c>
     </row>
   </sheetData>

</xml_diff>

<commit_message>
added template for ballard_exam
</commit_message>
<xml_diff>
--- a/opendatakit.collect2/form-files/neonatal/neonatal.xlsx
+++ b/opendatakit.collect2/form-files/neonatal/neonatal.xlsx
@@ -4,7 +4,7 @@
   <fileVersion appName="xl" lastEdited="5" lowestEdited="5" rupBuild="20910"/>
   <workbookPr autoCompressPictures="0"/>
   <bookViews>
-    <workbookView xWindow="320" yWindow="0" windowWidth="28480" windowHeight="17560" tabRatio="500" activeTab="1"/>
+    <workbookView xWindow="0" yWindow="0" windowWidth="28800" windowHeight="17560" tabRatio="500"/>
   </bookViews>
   <sheets>
     <sheet name="survey" sheetId="1" r:id="rId1"/>
@@ -23,7 +23,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="643" uniqueCount="469">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="637" uniqueCount="465">
   <si>
     <t>type</t>
   </si>
@@ -698,9 +698,6 @@
   </si>
   <si>
     <t>menu diagnostic_menu</t>
-  </si>
-  <si>
-    <t>menu ballard_menu1</t>
   </si>
   <si>
     <t>menu procedures_menu</t>
@@ -908,16 +905,7 @@
     <t>ballard_menu0</t>
   </si>
   <si>
-    <t>Ballard Exam - Neuromuscular</t>
-  </si>
-  <si>
-    <t>menu ballard_menu2</t>
-  </si>
-  <si>
     <t>ballard_menu2</t>
-  </si>
-  <si>
-    <t>Ballard Exam - Physical</t>
   </si>
   <si>
     <t>neuromuscular</t>
@@ -1598,9 +1586,6 @@
     <t>&lt;b&gt;116&lt;/b&gt;</t>
   </si>
   <si>
-    <t>Total Score</t>
-  </si>
-  <si>
     <t>selected(data('diagnostic_menu'),'ballardExam')</t>
   </si>
   <si>
@@ -1608,39 +1593,6 @@
   </si>
   <si>
     <t>calculates.skinScore() + calculates.lanugoScore() + calculates.plantarScore() + calculates.breastScore() + calculates.eyeEarScore() + calculates.genitalsScore()</t>
-  </si>
-  <si>
-    <r>
-      <t>&lt;h2&gt;Neuromuscular Score&lt;/h2&gt;
-&lt;ul&gt;
-&lt;li&gt;Posture Score: {{calculates.postureScore}}&lt;/li&gt;
-&lt;li&gt;Square Window Score: {{calculates.squareScore}}&lt;/li&gt;
-&lt;li&gt;Arm Recoil Score: {{calculates.armScore}}&lt;/li&gt;
-&lt;li&gt;Popiteal Angle Score: {{calculates.poplitealScore}}&lt;/li&gt;
-&lt;li&gt;Scarf Sign Score: {{calculates.scarfScore}}&lt;/li&gt;
-&lt;li&gt;</t>
-    </r>
-    <r>
-      <rPr>
-        <sz val="10"/>
-        <color rgb="FF000000"/>
-        <rFont val="Arial"/>
-      </rPr>
-      <t>Heel to Ear Score: {{calculates.heelScore}}&lt;/li&gt;
-&lt;li&gt;Total NM Score: {{calculates.totalNMScore}}&lt;/li&gt;
-&lt;/ul&gt;
-&lt;h2&gt;Physical Score&lt;/h2&gt;
-&lt;ul&gt;
-&lt;li&gt;Skin Score: {{calculates.skinScore}}&lt;/li&gt;
-&lt;li&gt;Lanugo Score: {{calculates.lanugoScore}}&lt;/li&gt;
-&lt;li&gt;Plantar Surface Score: {{calculates.plantarScore}}&lt;/li&gt;
-&lt;li&gt;Breast Score: {{calculates.breastScore}}&lt;/li&gt;
-&lt;li&gt;Eye/Ear Score: {{calculates.eyeEarScore}}&lt;/li&gt;
-&lt;li&gt;Genitals Score: {{calculates.genitalsScore}}&lt;/li&gt;
-&lt;li&gt;Total Physical Score: {{calculates.totalPhysicalScore}}&lt;/li&gt;
-&lt;/ul&gt;
-&lt;h2&gt;Total Score {{calculates.totalBallardScore}}&lt;/h2&gt;</t>
-    </r>
   </si>
   <si>
     <t xml:space="preserve">(function() {
@@ -1662,6 +1614,12 @@
   }
 }())
         </t>
+  </si>
+  <si>
+    <t>templatePath</t>
+  </si>
+  <si>
+    <t>templates/ballard_exam.handlebar</t>
   </si>
 </sst>
 </file>
@@ -1794,7 +1752,7 @@
       <diagonal/>
     </border>
   </borders>
-  <cellStyleXfs count="390">
+  <cellStyleXfs count="392">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
     <xf numFmtId="0" fontId="3" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
     <xf numFmtId="0" fontId="4" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
@@ -1809,6 +1767,8 @@
     <xf numFmtId="0" fontId="5" fillId="2" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
     <xf numFmtId="0" fontId="6" fillId="3" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
     <xf numFmtId="0" fontId="1" fillId="4" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="4" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
     <xf numFmtId="0" fontId="3" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
     <xf numFmtId="0" fontId="4" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
     <xf numFmtId="0" fontId="3" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
@@ -2264,7 +2224,7 @@
       <alignment wrapText="1"/>
     </xf>
   </cellXfs>
-  <cellStyles count="390">
+  <cellStyles count="392">
     <cellStyle name="20% - Accent4" xfId="13" builtinId="42"/>
     <cellStyle name="Followed Hyperlink" xfId="2" builtinId="9" hidden="1"/>
     <cellStyle name="Followed Hyperlink" xfId="4" builtinId="9" hidden="1"/>
@@ -2459,6 +2419,7 @@
     <cellStyle name="Followed Hyperlink" xfId="385" builtinId="9" hidden="1"/>
     <cellStyle name="Followed Hyperlink" xfId="387" builtinId="9" hidden="1"/>
     <cellStyle name="Followed Hyperlink" xfId="389" builtinId="9" hidden="1"/>
+    <cellStyle name="Followed Hyperlink" xfId="391" builtinId="9" hidden="1"/>
     <cellStyle name="Good" xfId="11" builtinId="26"/>
     <cellStyle name="Hyperlink" xfId="1" builtinId="8" hidden="1"/>
     <cellStyle name="Hyperlink" xfId="3" builtinId="8" hidden="1"/>
@@ -2653,6 +2614,7 @@
     <cellStyle name="Hyperlink" xfId="384" builtinId="8" hidden="1"/>
     <cellStyle name="Hyperlink" xfId="386" builtinId="8" hidden="1"/>
     <cellStyle name="Hyperlink" xfId="388" builtinId="8" hidden="1"/>
+    <cellStyle name="Hyperlink" xfId="390" builtinId="8" hidden="1"/>
     <cellStyle name="Neutral" xfId="12" builtinId="28"/>
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
   </cellStyles>
@@ -2983,10 +2945,10 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <dimension ref="A1:J120"/>
+  <dimension ref="A1:J118"/>
   <sheetViews>
-    <sheetView topLeftCell="A6" zoomScale="150" zoomScaleNormal="150" zoomScalePageLayoutView="150" workbookViewId="0">
-      <selection activeCell="D16" sqref="D16"/>
+    <sheetView tabSelected="1" topLeftCell="G6" zoomScale="150" zoomScaleNormal="150" zoomScalePageLayoutView="150" workbookViewId="0">
+      <selection activeCell="I14" sqref="I14"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultColWidth="11.5" defaultRowHeight="12.75" customHeight="1" x14ac:dyDescent="0"/>
@@ -2996,11 +2958,12 @@
     <col min="4" max="4" width="25.1640625" customWidth="1"/>
     <col min="5" max="5" width="42.1640625" customWidth="1"/>
     <col min="6" max="6" width="15.33203125" customWidth="1"/>
+    <col min="9" max="9" width="19.6640625" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:8" ht="12">
+    <row r="1" spans="1:9" ht="12">
       <c r="A1" t="s">
-        <v>404</v>
+        <v>400</v>
       </c>
       <c r="B1" s="1" t="s">
         <v>0</v>
@@ -3023,8 +2986,11 @@
       <c r="H1" t="s">
         <v>70</v>
       </c>
-    </row>
-    <row r="2" spans="1:8" ht="15">
+      <c r="I1" t="s">
+        <v>463</v>
+      </c>
+    </row>
+    <row r="2" spans="1:9" ht="15">
       <c r="B2" s="16" t="s">
         <v>106</v>
       </c>
@@ -3033,7 +2999,7 @@
       <c r="E2" s="4"/>
       <c r="F2" s="2"/>
     </row>
-    <row r="3" spans="1:8" ht="12">
+    <row r="3" spans="1:9" ht="12">
       <c r="B3" s="3" t="s">
         <v>223</v>
       </c>
@@ -3048,44 +3014,44 @@
         <v>6</v>
       </c>
     </row>
-    <row r="4" spans="1:8" ht="12">
+    <row r="4" spans="1:9" ht="12">
       <c r="B4" s="3"/>
       <c r="C4" s="4"/>
       <c r="D4" s="4"/>
       <c r="E4" s="4"/>
       <c r="F4" s="2"/>
     </row>
-    <row r="5" spans="1:8" ht="12.75" customHeight="1">
+    <row r="5" spans="1:9" ht="12.75" customHeight="1">
       <c r="A5" s="21" t="s">
         <v>8</v>
       </c>
       <c r="B5" s="19" t="s">
-        <v>400</v>
+        <v>396</v>
       </c>
       <c r="C5" s="19"/>
       <c r="D5" s="19"/>
       <c r="E5" s="19" t="s">
-        <v>401</v>
+        <v>397</v>
       </c>
       <c r="F5" s="19"/>
       <c r="G5" s="19"/>
       <c r="H5" s="19"/>
     </row>
-    <row r="6" spans="1:8" ht="12.75" customHeight="1">
+    <row r="6" spans="1:9" ht="12.75" customHeight="1">
       <c r="A6" s="21"/>
       <c r="B6" s="19" t="s">
-        <v>402</v>
+        <v>398</v>
       </c>
       <c r="C6" s="19"/>
       <c r="D6" s="19"/>
       <c r="E6" s="19" t="s">
-        <v>403</v>
+        <v>399</v>
       </c>
       <c r="F6" s="19"/>
       <c r="G6" s="19"/>
       <c r="H6" s="19"/>
     </row>
-    <row r="7" spans="1:8" s="12" customFormat="1" ht="18" customHeight="1">
+    <row r="7" spans="1:9" s="12" customFormat="1" ht="18" customHeight="1">
       <c r="A7" s="22"/>
       <c r="B7" s="18" t="s">
         <v>108</v>
@@ -3097,7 +3063,7 @@
       <c r="G7" s="18"/>
       <c r="H7" s="18"/>
     </row>
-    <row r="8" spans="1:8" s="12" customFormat="1" ht="18" customHeight="1">
+    <row r="8" spans="1:9" s="12" customFormat="1" ht="18" customHeight="1">
       <c r="A8" s="22"/>
       <c r="B8" t="s">
         <v>224</v>
@@ -3113,7 +3079,7 @@
         <v>6</v>
       </c>
     </row>
-    <row r="9" spans="1:8" ht="18" customHeight="1">
+    <row r="9" spans="1:9" ht="18" customHeight="1">
       <c r="A9" s="21"/>
       <c r="B9" s="2" t="s">
         <v>13</v>
@@ -3130,7 +3096,7 @@
         <v>126</v>
       </c>
     </row>
-    <row r="10" spans="1:8" ht="18" customHeight="1">
+    <row r="10" spans="1:9" ht="18" customHeight="1">
       <c r="A10" s="21"/>
       <c r="B10" s="2" t="s">
         <v>102</v>
@@ -3144,7 +3110,7 @@
       </c>
       <c r="F10" s="2"/>
     </row>
-    <row r="11" spans="1:8" ht="18" customHeight="1">
+    <row r="11" spans="1:9" ht="18" customHeight="1">
       <c r="A11" s="21"/>
       <c r="B11" s="2" t="s">
         <v>102</v>
@@ -3158,177 +3124,181 @@
       </c>
       <c r="F11" s="2"/>
     </row>
-    <row r="12" spans="1:8" s="13" customFormat="1" ht="18" customHeight="1">
+    <row r="12" spans="1:9" s="13" customFormat="1" ht="18" customHeight="1">
       <c r="B12" s="7" t="s">
         <v>15</v>
       </c>
       <c r="E12" s="13" t="s">
-        <v>464</v>
-      </c>
-    </row>
-    <row r="13" spans="1:8" ht="12">
+        <v>459</v>
+      </c>
+    </row>
+    <row r="13" spans="1:9" ht="24">
       <c r="A13" s="21"/>
       <c r="B13" t="s">
-        <v>225</v>
-      </c>
-      <c r="C13" t="s">
-        <v>131</v>
-      </c>
-      <c r="D13" t="s">
-        <v>263</v>
+        <v>13</v>
       </c>
       <c r="E13" s="2"/>
-    </row>
-    <row r="14" spans="1:8" ht="12">
+      <c r="I13" t="s">
+        <v>464</v>
+      </c>
+    </row>
+    <row r="14" spans="1:9" ht="12">
       <c r="A14" s="27"/>
-      <c r="B14" t="s">
-        <v>264</v>
-      </c>
-      <c r="C14" t="s">
-        <v>265</v>
-      </c>
-      <c r="D14" t="s">
-        <v>266</v>
-      </c>
-    </row>
-    <row r="15" spans="1:8" ht="14" customHeight="1">
-      <c r="A15" s="21" t="s">
-        <v>463</v>
-      </c>
+      <c r="B14" s="11" t="s">
+        <v>25</v>
+      </c>
+      <c r="C14" s="11"/>
+      <c r="D14" s="11"/>
+      <c r="E14" s="11"/>
+      <c r="F14" s="11"/>
+      <c r="G14" s="11"/>
+      <c r="H14" s="11"/>
+    </row>
+    <row r="15" spans="1:9" ht="11" customHeight="1">
+      <c r="A15" s="21"/>
       <c r="B15" t="s">
-        <v>13</v>
+        <v>144</v>
+      </c>
+      <c r="C15" t="s">
+        <v>145</v>
       </c>
       <c r="D15" t="s">
-        <v>467</v>
-      </c>
-    </row>
-    <row r="16" spans="1:8" ht="12">
-      <c r="A16" s="27"/>
-      <c r="B16" s="11" t="s">
-        <v>25</v>
-      </c>
-      <c r="C16" s="11"/>
-      <c r="D16" s="11"/>
-      <c r="E16" s="11"/>
-      <c r="F16" s="11"/>
-      <c r="G16" s="11"/>
-      <c r="H16" s="11"/>
+        <v>146</v>
+      </c>
+      <c r="E15" s="2" t="s">
+        <v>147</v>
+      </c>
+    </row>
+    <row r="16" spans="1:9" ht="11" customHeight="1">
+      <c r="A16" s="21"/>
+      <c r="B16" t="s">
+        <v>148</v>
+      </c>
+      <c r="C16" t="s">
+        <v>149</v>
+      </c>
+      <c r="D16" t="s">
+        <v>150</v>
+      </c>
+      <c r="E16" s="2" t="s">
+        <v>151</v>
+      </c>
     </row>
     <row r="17" spans="1:10" ht="11" customHeight="1">
       <c r="A17" s="21"/>
       <c r="B17" t="s">
-        <v>144</v>
+        <v>165</v>
       </c>
       <c r="C17" t="s">
-        <v>145</v>
+        <v>166</v>
       </c>
       <c r="D17" t="s">
-        <v>146</v>
+        <v>167</v>
       </c>
       <c r="E17" s="2" t="s">
-        <v>147</v>
+        <v>168</v>
       </c>
     </row>
     <row r="18" spans="1:10" ht="11" customHeight="1">
       <c r="A18" s="21"/>
       <c r="B18" t="s">
-        <v>148</v>
+        <v>235</v>
       </c>
       <c r="C18" t="s">
-        <v>149</v>
+        <v>236</v>
       </c>
       <c r="D18" t="s">
-        <v>150</v>
+        <v>237</v>
       </c>
       <c r="E18" s="2" t="s">
-        <v>151</v>
+        <v>238</v>
       </c>
     </row>
     <row r="19" spans="1:10" ht="11" customHeight="1">
       <c r="A19" s="21"/>
       <c r="B19" t="s">
-        <v>165</v>
+        <v>169</v>
       </c>
       <c r="C19" t="s">
-        <v>166</v>
+        <v>170</v>
       </c>
       <c r="D19" t="s">
-        <v>167</v>
+        <v>171</v>
       </c>
       <c r="E19" s="2" t="s">
-        <v>168</v>
+        <v>221</v>
       </c>
     </row>
     <row r="20" spans="1:10" ht="11" customHeight="1">
       <c r="A20" s="21"/>
       <c r="B20" t="s">
-        <v>236</v>
+        <v>172</v>
       </c>
       <c r="C20" t="s">
-        <v>237</v>
+        <v>173</v>
       </c>
       <c r="D20" t="s">
-        <v>238</v>
+        <v>174</v>
       </c>
       <c r="E20" s="2" t="s">
-        <v>239</v>
+        <v>222</v>
       </c>
     </row>
     <row r="21" spans="1:10" ht="11" customHeight="1">
       <c r="A21" s="21"/>
       <c r="B21" t="s">
-        <v>169</v>
+        <v>310</v>
       </c>
       <c r="C21" t="s">
-        <v>170</v>
+        <v>290</v>
       </c>
       <c r="D21" t="s">
-        <v>171</v>
+        <v>268</v>
       </c>
       <c r="E21" s="2" t="s">
-        <v>221</v>
+        <v>269</v>
       </c>
     </row>
     <row r="22" spans="1:10" ht="11" customHeight="1">
       <c r="A22" s="21"/>
       <c r="B22" t="s">
-        <v>172</v>
+        <v>311</v>
       </c>
       <c r="C22" t="s">
-        <v>173</v>
+        <v>291</v>
       </c>
       <c r="D22" t="s">
-        <v>174</v>
+        <v>280</v>
       </c>
       <c r="E22" s="2" t="s">
-        <v>222</v>
+        <v>271</v>
       </c>
     </row>
     <row r="23" spans="1:10" ht="11" customHeight="1">
       <c r="A23" s="21"/>
       <c r="B23" t="s">
-        <v>314</v>
+        <v>312</v>
       </c>
       <c r="C23" t="s">
-        <v>294</v>
+        <v>292</v>
       </c>
       <c r="D23" t="s">
+        <v>283</v>
+      </c>
+      <c r="E23" s="2" t="s">
         <v>272</v>
-      </c>
-      <c r="E23" s="2" t="s">
-        <v>273</v>
       </c>
     </row>
     <row r="24" spans="1:10" ht="11" customHeight="1">
       <c r="A24" s="21"/>
       <c r="B24" t="s">
-        <v>315</v>
+        <v>313</v>
       </c>
       <c r="C24" t="s">
-        <v>295</v>
+        <v>293</v>
       </c>
       <c r="D24" t="s">
-        <v>284</v>
+        <v>281</v>
       </c>
       <c r="E24" s="2" t="s">
         <v>275</v>
@@ -3337,193 +3307,187 @@
     <row r="25" spans="1:10" ht="11" customHeight="1">
       <c r="A25" s="21"/>
       <c r="B25" t="s">
-        <v>316</v>
+        <v>314</v>
       </c>
       <c r="C25" t="s">
-        <v>296</v>
+        <v>294</v>
       </c>
       <c r="D25" t="s">
-        <v>287</v>
+        <v>282</v>
       </c>
       <c r="E25" s="2" t="s">
-        <v>276</v>
-      </c>
-    </row>
-    <row r="26" spans="1:10" ht="11" customHeight="1">
+        <v>277</v>
+      </c>
+    </row>
+    <row r="26" spans="1:10" ht="12" customHeight="1">
       <c r="A26" s="21"/>
       <c r="B26" t="s">
-        <v>317</v>
+        <v>315</v>
       </c>
       <c r="C26" t="s">
-        <v>297</v>
+        <v>295</v>
       </c>
       <c r="D26" t="s">
-        <v>285</v>
+        <v>284</v>
       </c>
       <c r="E26" s="2" t="s">
         <v>279</v>
       </c>
     </row>
-    <row r="27" spans="1:10" ht="11" customHeight="1">
+    <row r="27" spans="1:10" ht="15">
       <c r="A27" s="21"/>
-      <c r="B27" t="s">
-        <v>318</v>
-      </c>
-      <c r="C27" t="s">
-        <v>298</v>
-      </c>
-      <c r="D27" t="s">
-        <v>286</v>
-      </c>
-      <c r="E27" s="2" t="s">
-        <v>281</v>
-      </c>
-    </row>
-    <row r="28" spans="1:10" ht="12" customHeight="1">
-      <c r="A28" s="21"/>
-      <c r="B28" t="s">
-        <v>319</v>
-      </c>
-      <c r="C28" t="s">
-        <v>299</v>
-      </c>
-      <c r="D28" t="s">
-        <v>288</v>
-      </c>
-      <c r="E28" s="2" t="s">
-        <v>283</v>
-      </c>
-    </row>
-    <row r="29" spans="1:10" ht="15">
-      <c r="A29" s="21"/>
-      <c r="B29" s="15" t="s">
+      <c r="B27" s="15" t="s">
         <v>72</v>
       </c>
-      <c r="C29" s="15"/>
-      <c r="D29" s="15"/>
-      <c r="E29" s="15"/>
-      <c r="F29" s="15"/>
-      <c r="G29" s="15"/>
-      <c r="H29" s="15"/>
-    </row>
-    <row r="30" spans="1:10" ht="15">
-      <c r="B30" s="23"/>
-      <c r="C30" s="12"/>
-      <c r="D30" s="12"/>
-      <c r="E30" s="12"/>
-      <c r="F30" s="12"/>
-      <c r="G30" s="12"/>
-      <c r="H30" s="12"/>
-    </row>
-    <row r="31" spans="1:10" s="15" customFormat="1" ht="15">
-      <c r="A31" s="21" t="s">
-        <v>424</v>
-      </c>
-      <c r="B31" s="13" t="s">
+      <c r="C27" s="15"/>
+      <c r="D27" s="15"/>
+      <c r="E27" s="15"/>
+      <c r="F27" s="15"/>
+      <c r="G27" s="15"/>
+      <c r="H27" s="15"/>
+    </row>
+    <row r="28" spans="1:10" ht="15">
+      <c r="B28" s="23"/>
+      <c r="C28" s="12"/>
+      <c r="D28" s="12"/>
+      <c r="E28" s="12"/>
+      <c r="F28" s="12"/>
+      <c r="G28" s="12"/>
+      <c r="H28" s="12"/>
+    </row>
+    <row r="29" spans="1:10" s="15" customFormat="1" ht="15">
+      <c r="A29" s="21" t="s">
+        <v>420</v>
+      </c>
+      <c r="B29" s="13" t="s">
         <v>105</v>
       </c>
-      <c r="C31" s="13"/>
-      <c r="D31" s="13"/>
-      <c r="E31" s="13" t="s">
+      <c r="C29" s="13"/>
+      <c r="D29" s="13"/>
+      <c r="E29" s="13" t="s">
         <v>71</v>
       </c>
-      <c r="F31" s="13"/>
-      <c r="G31" s="13"/>
-      <c r="H31" s="13"/>
-      <c r="I31" s="12"/>
-      <c r="J31" s="12"/>
+      <c r="F29" s="13"/>
+      <c r="G29" s="13"/>
+      <c r="H29" s="13"/>
+      <c r="I29" s="12"/>
+      <c r="J29" s="12"/>
+    </row>
+    <row r="30" spans="1:10" ht="12">
+      <c r="A30" s="21"/>
+      <c r="B30" s="5" t="s">
+        <v>73</v>
+      </c>
+      <c r="C30" s="5"/>
+      <c r="D30" s="5"/>
+      <c r="E30" s="6" t="s">
+        <v>74</v>
+      </c>
+      <c r="F30" s="5"/>
+      <c r="G30" s="5"/>
+      <c r="H30" s="5"/>
+    </row>
+    <row r="31" spans="1:10" ht="15">
+      <c r="A31" s="21"/>
+      <c r="B31" s="15" t="s">
+        <v>104</v>
+      </c>
+      <c r="C31" s="15"/>
+      <c r="D31" s="15"/>
+      <c r="E31" s="15"/>
+      <c r="F31" s="15"/>
+      <c r="G31" s="15"/>
+      <c r="H31" s="15"/>
     </row>
     <row r="32" spans="1:10" ht="12">
       <c r="A32" s="21"/>
-      <c r="B32" s="5" t="s">
-        <v>73</v>
-      </c>
-      <c r="C32" s="5"/>
-      <c r="D32" s="5"/>
-      <c r="E32" s="6" t="s">
-        <v>74</v>
-      </c>
-      <c r="F32" s="5"/>
-      <c r="G32" s="5"/>
-      <c r="H32" s="5"/>
-    </row>
-    <row r="33" spans="1:8" ht="15">
+      <c r="B32" s="12" t="s">
+        <v>225</v>
+      </c>
+      <c r="C32" s="12" t="s">
+        <v>9</v>
+      </c>
+      <c r="D32" s="12" t="s">
+        <v>10</v>
+      </c>
+      <c r="E32" s="12"/>
+      <c r="F32" s="12" t="s">
+        <v>6</v>
+      </c>
+      <c r="G32" s="12"/>
+      <c r="H32" s="12"/>
+    </row>
+    <row r="33" spans="1:8" ht="12">
       <c r="A33" s="21"/>
-      <c r="B33" s="15" t="s">
-        <v>104</v>
-      </c>
-      <c r="C33" s="15"/>
-      <c r="D33" s="15"/>
-      <c r="E33" s="15"/>
-      <c r="F33" s="15"/>
-      <c r="G33" s="15"/>
-      <c r="H33" s="15"/>
-    </row>
-    <row r="34" spans="1:8" ht="12">
+      <c r="B33" s="7" t="s">
+        <v>15</v>
+      </c>
+      <c r="C33" s="8"/>
+      <c r="D33" s="8"/>
+      <c r="E33" s="9" t="s">
+        <v>63</v>
+      </c>
+      <c r="F33" s="8"/>
+      <c r="G33" s="10"/>
+      <c r="H33" s="10"/>
+    </row>
+    <row r="34" spans="1:8" ht="12.75" customHeight="1">
       <c r="A34" s="21"/>
-      <c r="B34" s="12" t="s">
-        <v>226</v>
-      </c>
-      <c r="C34" s="12" t="s">
-        <v>9</v>
-      </c>
-      <c r="D34" s="12" t="s">
-        <v>10</v>
-      </c>
-      <c r="E34" s="12"/>
-      <c r="F34" s="12" t="s">
-        <v>6</v>
-      </c>
-      <c r="G34" s="12"/>
-      <c r="H34" s="12"/>
-    </row>
-    <row r="35" spans="1:8" ht="12">
+      <c r="B34" s="4" t="s">
+        <v>13</v>
+      </c>
+      <c r="C34" s="2" t="s">
+        <v>75</v>
+      </c>
+      <c r="D34" s="2" t="s">
+        <v>401</v>
+      </c>
+      <c r="E34" s="2"/>
+      <c r="F34" s="4"/>
+    </row>
+    <row r="35" spans="1:8" ht="12.75" customHeight="1">
       <c r="A35" s="21"/>
-      <c r="B35" s="7" t="s">
-        <v>15</v>
-      </c>
-      <c r="C35" s="8"/>
-      <c r="D35" s="8"/>
-      <c r="E35" s="9" t="s">
-        <v>63</v>
-      </c>
-      <c r="F35" s="8"/>
-      <c r="G35" s="10"/>
-      <c r="H35" s="10"/>
+      <c r="B35" s="4" t="s">
+        <v>13</v>
+      </c>
+      <c r="D35" t="s">
+        <v>402</v>
+      </c>
+      <c r="E35" s="2"/>
+      <c r="F35" s="4"/>
     </row>
     <row r="36" spans="1:8" ht="12.75" customHeight="1">
       <c r="A36" s="21"/>
-      <c r="B36" s="4" t="s">
+      <c r="B36" t="s">
         <v>13</v>
       </c>
-      <c r="C36" s="2" t="s">
-        <v>75</v>
-      </c>
+      <c r="C36" s="2"/>
       <c r="D36" s="2" t="s">
-        <v>405</v>
+        <v>403</v>
       </c>
       <c r="E36" s="2"/>
       <c r="F36" s="4"/>
     </row>
     <row r="37" spans="1:8" ht="12.75" customHeight="1">
       <c r="A37" s="21"/>
-      <c r="B37" s="4" t="s">
+      <c r="B37" s="2" t="s">
         <v>13</v>
       </c>
-      <c r="D37" t="s">
-        <v>406</v>
+      <c r="C37" s="2"/>
+      <c r="D37" s="2" t="s">
+        <v>404</v>
       </c>
       <c r="E37" s="2"/>
       <c r="F37" s="4"/>
     </row>
     <row r="38" spans="1:8" ht="12.75" customHeight="1">
       <c r="A38" s="21"/>
-      <c r="B38" t="s">
+      <c r="B38" s="2" t="s">
         <v>13</v>
       </c>
       <c r="C38" s="2"/>
       <c r="D38" s="2" t="s">
-        <v>407</v>
+        <v>405</v>
       </c>
       <c r="E38" s="2"/>
       <c r="F38" s="4"/>
@@ -3535,7 +3499,7 @@
       </c>
       <c r="C39" s="2"/>
       <c r="D39" s="2" t="s">
-        <v>408</v>
+        <v>406</v>
       </c>
       <c r="E39" s="2"/>
       <c r="F39" s="4"/>
@@ -3547,7 +3511,7 @@
       </c>
       <c r="C40" s="2"/>
       <c r="D40" s="2" t="s">
-        <v>409</v>
+        <v>407</v>
       </c>
       <c r="E40" s="2"/>
       <c r="F40" s="4"/>
@@ -3559,7 +3523,7 @@
       </c>
       <c r="C41" s="2"/>
       <c r="D41" s="2" t="s">
-        <v>410</v>
+        <v>408</v>
       </c>
       <c r="E41" s="2"/>
       <c r="F41" s="4"/>
@@ -3571,7 +3535,7 @@
       </c>
       <c r="C42" s="2"/>
       <c r="D42" s="2" t="s">
-        <v>411</v>
+        <v>416</v>
       </c>
       <c r="E42" s="2"/>
       <c r="F42" s="4"/>
@@ -3583,7 +3547,7 @@
       </c>
       <c r="C43" s="2"/>
       <c r="D43" s="2" t="s">
-        <v>412</v>
+        <v>415</v>
       </c>
       <c r="E43" s="2"/>
       <c r="F43" s="4"/>
@@ -3595,7 +3559,7 @@
       </c>
       <c r="C44" s="2"/>
       <c r="D44" s="2" t="s">
-        <v>420</v>
+        <v>417</v>
       </c>
       <c r="E44" s="2"/>
       <c r="F44" s="4"/>
@@ -3607,7 +3571,7 @@
       </c>
       <c r="C45" s="2"/>
       <c r="D45" s="2" t="s">
-        <v>419</v>
+        <v>418</v>
       </c>
       <c r="E45" s="2"/>
       <c r="F45" s="4"/>
@@ -3619,7 +3583,7 @@
       </c>
       <c r="C46" s="2"/>
       <c r="D46" s="2" t="s">
-        <v>421</v>
+        <v>409</v>
       </c>
       <c r="E46" s="2"/>
       <c r="F46" s="4"/>
@@ -3631,7 +3595,7 @@
       </c>
       <c r="C47" s="2"/>
       <c r="D47" s="2" t="s">
-        <v>422</v>
+        <v>412</v>
       </c>
       <c r="E47" s="2"/>
       <c r="F47" s="4"/>
@@ -3655,7 +3619,7 @@
       </c>
       <c r="C49" s="2"/>
       <c r="D49" s="2" t="s">
-        <v>416</v>
+        <v>414</v>
       </c>
       <c r="E49" s="2"/>
       <c r="F49" s="4"/>
@@ -3667,7 +3631,7 @@
       </c>
       <c r="C50" s="2"/>
       <c r="D50" s="2" t="s">
-        <v>417</v>
+        <v>410</v>
       </c>
       <c r="E50" s="2"/>
       <c r="F50" s="4"/>
@@ -3679,19 +3643,19 @@
       </c>
       <c r="C51" s="2"/>
       <c r="D51" s="2" t="s">
-        <v>418</v>
+        <v>411</v>
       </c>
       <c r="E51" s="2"/>
       <c r="F51" s="4"/>
     </row>
-    <row r="52" spans="1:8" ht="12.75" customHeight="1">
+    <row r="52" spans="1:8" ht="17" customHeight="1">
       <c r="A52" s="21"/>
       <c r="B52" s="2" t="s">
         <v>13</v>
       </c>
       <c r="C52" s="2"/>
       <c r="D52" s="2" t="s">
-        <v>414</v>
+        <v>419</v>
       </c>
       <c r="E52" s="2"/>
       <c r="F52" s="4"/>
@@ -3702,21 +3666,15 @@
         <v>13</v>
       </c>
       <c r="C53" s="2"/>
-      <c r="D53" s="2" t="s">
-        <v>415</v>
-      </c>
+      <c r="D53" s="2"/>
       <c r="E53" s="2"/>
       <c r="F53" s="4"/>
     </row>
-    <row r="54" spans="1:8" ht="17" customHeight="1">
+    <row r="54" spans="1:8" ht="12.75" customHeight="1">
       <c r="A54" s="21"/>
-      <c r="B54" s="2" t="s">
-        <v>13</v>
-      </c>
+      <c r="B54" s="4"/>
       <c r="C54" s="2"/>
-      <c r="D54" s="2" t="s">
-        <v>423</v>
-      </c>
+      <c r="D54" s="2"/>
       <c r="E54" s="2"/>
       <c r="F54" s="4"/>
     </row>
@@ -3725,334 +3683,337 @@
       <c r="B55" s="2" t="s">
         <v>13</v>
       </c>
-      <c r="C55" s="2"/>
+      <c r="C55" s="2" t="s">
+        <v>76</v>
+      </c>
       <c r="D55" s="2"/>
       <c r="E55" s="2"/>
       <c r="F55" s="4"/>
+      <c r="G55" t="s">
+        <v>14</v>
+      </c>
     </row>
     <row r="56" spans="1:8" ht="12.75" customHeight="1">
       <c r="A56" s="21"/>
-      <c r="B56" s="4"/>
-      <c r="C56" s="2"/>
-      <c r="D56" s="2"/>
-      <c r="E56" s="2"/>
-      <c r="F56" s="4"/>
+      <c r="B56" t="s">
+        <v>13</v>
+      </c>
+      <c r="D56" t="s">
+        <v>77</v>
+      </c>
+      <c r="E56" s="13"/>
     </row>
     <row r="57" spans="1:8" ht="12.75" customHeight="1">
       <c r="A57" s="21"/>
-      <c r="B57" s="2" t="s">
+      <c r="B57" t="s">
         <v>13</v>
       </c>
-      <c r="C57" s="2" t="s">
-        <v>76</v>
-      </c>
-      <c r="D57" s="2"/>
-      <c r="E57" s="2"/>
-      <c r="F57" s="4"/>
-      <c r="G57" t="s">
-        <v>14</v>
-      </c>
-    </row>
-    <row r="58" spans="1:8" ht="12.75" customHeight="1">
+      <c r="H57" t="s">
+        <v>78</v>
+      </c>
+    </row>
+    <row r="58" spans="1:8" ht="12">
       <c r="A58" s="21"/>
-      <c r="B58" t="s">
+      <c r="B58" s="11" t="s">
+        <v>25</v>
+      </c>
+      <c r="C58" s="10"/>
+      <c r="D58" s="10"/>
+      <c r="E58" s="10"/>
+      <c r="F58" s="10"/>
+      <c r="G58" s="10"/>
+      <c r="H58" s="10"/>
+    </row>
+    <row r="59" spans="1:8" s="10" customFormat="1" ht="12"/>
+    <row r="60" spans="1:8" s="10" customFormat="1" ht="15">
+      <c r="B60" s="10" t="s">
+        <v>450</v>
+      </c>
+      <c r="E60" s="13" t="s">
+        <v>455</v>
+      </c>
+    </row>
+    <row r="61" spans="1:8" s="10" customFormat="1" ht="15">
+      <c r="B61" s="10" t="s">
+        <v>451</v>
+      </c>
+      <c r="E61" s="37" t="s">
+        <v>454</v>
+      </c>
+    </row>
+    <row r="62" spans="1:8" s="10" customFormat="1" ht="12">
+      <c r="B62" s="10" t="s">
+        <v>452</v>
+      </c>
+    </row>
+    <row r="63" spans="1:8" s="10" customFormat="1" ht="12">
+      <c r="B63" s="10" t="s">
         <v>13</v>
       </c>
-      <c r="D58" t="s">
-        <v>77</v>
-      </c>
-      <c r="E58" s="13"/>
-    </row>
-    <row r="59" spans="1:8" ht="12.75" customHeight="1">
-      <c r="A59" s="21"/>
-      <c r="B59" t="s">
-        <v>13</v>
-      </c>
-      <c r="H59" t="s">
-        <v>78</v>
-      </c>
-    </row>
-    <row r="60" spans="1:8" ht="12">
-      <c r="A60" s="21"/>
-      <c r="B60" s="11" t="s">
-        <v>25</v>
-      </c>
-      <c r="C60" s="10"/>
-      <c r="D60" s="10"/>
-      <c r="E60" s="10"/>
-      <c r="F60" s="10"/>
-      <c r="G60" s="10"/>
-      <c r="H60" s="10"/>
-    </row>
-    <row r="61" spans="1:8" s="10" customFormat="1" ht="12"/>
-    <row r="62" spans="1:8" s="10" customFormat="1" ht="15">
-      <c r="B62" s="10" t="s">
-        <v>454</v>
-      </c>
-      <c r="E62" s="13" t="s">
-        <v>459</v>
-      </c>
-    </row>
-    <row r="63" spans="1:8" s="10" customFormat="1" ht="15">
-      <c r="B63" s="10" t="s">
-        <v>455</v>
-      </c>
-      <c r="E63" s="37" t="s">
-        <v>458</v>
+      <c r="D63" s="10" t="s">
+        <v>42</v>
       </c>
     </row>
     <row r="64" spans="1:8" s="10" customFormat="1" ht="12">
       <c r="B64" s="10" t="s">
-        <v>456</v>
-      </c>
-    </row>
-    <row r="65" spans="1:8" s="10" customFormat="1" ht="12">
-      <c r="B65" s="10" t="s">
-        <v>13</v>
-      </c>
-      <c r="D65" s="10" t="s">
-        <v>42</v>
-      </c>
-    </row>
-    <row r="66" spans="1:8" s="10" customFormat="1" ht="12">
-      <c r="B66" s="10" t="s">
-        <v>457</v>
-      </c>
-    </row>
-    <row r="67" spans="1:8" s="10" customFormat="1" ht="12"/>
-    <row r="68" spans="1:8" ht="30">
+        <v>453</v>
+      </c>
+    </row>
+    <row r="65" spans="1:8" s="10" customFormat="1" ht="12"/>
+    <row r="66" spans="1:8" ht="30">
+      <c r="A66" s="21"/>
+      <c r="B66" s="13" t="s">
+        <v>425</v>
+      </c>
+      <c r="C66" s="13"/>
+      <c r="D66" s="13"/>
+      <c r="E66" s="13" t="s">
+        <v>421</v>
+      </c>
+      <c r="F66" s="13"/>
+      <c r="G66" s="13"/>
+      <c r="H66" s="13"/>
+    </row>
+    <row r="67" spans="1:8" ht="30">
+      <c r="A67" s="21"/>
+      <c r="B67" s="13" t="s">
+        <v>426</v>
+      </c>
+      <c r="C67" s="13"/>
+      <c r="D67" s="13"/>
+      <c r="E67" s="13" t="s">
+        <v>427</v>
+      </c>
+      <c r="F67" s="13"/>
+      <c r="G67" s="13"/>
+      <c r="H67" s="13"/>
+    </row>
+    <row r="68" spans="1:8" ht="15">
       <c r="A68" s="21"/>
-      <c r="B68" s="13" t="s">
-        <v>429</v>
-      </c>
-      <c r="C68" s="13"/>
-      <c r="D68" s="13"/>
-      <c r="E68" s="13" t="s">
-        <v>425</v>
-      </c>
-      <c r="F68" s="13"/>
-      <c r="G68" s="13"/>
-      <c r="H68" s="13"/>
-    </row>
-    <row r="69" spans="1:8" ht="30">
+      <c r="B68" s="15" t="s">
+        <v>423</v>
+      </c>
+      <c r="C68" s="15"/>
+      <c r="D68" s="15"/>
+      <c r="E68" s="15"/>
+      <c r="F68" s="15"/>
+      <c r="G68" s="15"/>
+      <c r="H68" s="15"/>
+    </row>
+    <row r="69" spans="1:8" ht="12">
       <c r="A69" s="21"/>
-      <c r="B69" s="13" t="s">
-        <v>430</v>
-      </c>
-      <c r="C69" s="13"/>
-      <c r="D69" s="13"/>
-      <c r="E69" s="13" t="s">
-        <v>431</v>
-      </c>
-      <c r="F69" s="13"/>
-      <c r="G69" s="13"/>
-      <c r="H69" s="13"/>
-    </row>
-    <row r="70" spans="1:8" ht="15">
+      <c r="B69" s="10"/>
+      <c r="C69" s="10"/>
+      <c r="D69" s="10"/>
+      <c r="E69" s="10"/>
+      <c r="F69" s="10"/>
+      <c r="G69" s="10"/>
+      <c r="H69" s="10"/>
+    </row>
+    <row r="70" spans="1:8" ht="24">
       <c r="A70" s="21"/>
-      <c r="B70" s="15" t="s">
-        <v>427</v>
-      </c>
-      <c r="C70" s="15"/>
-      <c r="D70" s="15"/>
-      <c r="E70" s="15"/>
-      <c r="F70" s="15"/>
-      <c r="G70" s="15"/>
-      <c r="H70" s="15"/>
-    </row>
-    <row r="71" spans="1:8" ht="12">
+      <c r="B70" t="s">
+        <v>434</v>
+      </c>
+      <c r="C70" t="s">
+        <v>433</v>
+      </c>
+      <c r="F70" t="s">
+        <v>6</v>
+      </c>
+      <c r="G70" s="10"/>
+      <c r="H70" s="10"/>
+    </row>
+    <row r="71" spans="1:8" ht="30">
       <c r="A71" s="21"/>
-      <c r="B71" s="10"/>
-      <c r="C71" s="10"/>
-      <c r="D71" s="10"/>
-      <c r="E71" s="10"/>
-      <c r="F71" s="10"/>
+      <c r="B71" s="13" t="s">
+        <v>439</v>
+      </c>
+      <c r="C71" s="13"/>
+      <c r="D71" s="13"/>
+      <c r="E71" s="13" t="s">
+        <v>436</v>
+      </c>
+      <c r="F71" s="13"/>
       <c r="G71" s="10"/>
       <c r="H71" s="10"/>
     </row>
-    <row r="72" spans="1:8" ht="24">
+    <row r="72" spans="1:8" ht="30">
       <c r="A72" s="21"/>
-      <c r="B72" t="s">
-        <v>438</v>
-      </c>
-      <c r="C72" t="s">
-        <v>437</v>
-      </c>
-      <c r="F72" t="s">
-        <v>6</v>
-      </c>
+      <c r="B72" s="13" t="s">
+        <v>440</v>
+      </c>
+      <c r="C72" s="13"/>
+      <c r="D72" s="13"/>
+      <c r="E72" s="13" t="s">
+        <v>441</v>
+      </c>
+      <c r="F72" s="13"/>
       <c r="G72" s="10"/>
       <c r="H72" s="10"/>
     </row>
-    <row r="73" spans="1:8" ht="30">
+    <row r="73" spans="1:8" ht="15">
       <c r="A73" s="21"/>
-      <c r="B73" s="13" t="s">
-        <v>443</v>
-      </c>
-      <c r="C73" s="13"/>
-      <c r="D73" s="13"/>
-      <c r="E73" s="13" t="s">
-        <v>440</v>
-      </c>
-      <c r="F73" s="13"/>
+      <c r="B73" s="15" t="s">
+        <v>437</v>
+      </c>
+      <c r="C73" s="15"/>
+      <c r="D73" s="15"/>
+      <c r="E73" s="15"/>
       <c r="G73" s="10"/>
       <c r="H73" s="10"/>
     </row>
-    <row r="74" spans="1:8" ht="30">
+    <row r="74" spans="1:8" ht="12">
       <c r="A74" s="21"/>
-      <c r="B74" s="13" t="s">
-        <v>444</v>
-      </c>
-      <c r="C74" s="13"/>
-      <c r="D74" s="13"/>
-      <c r="E74" s="13" t="s">
-        <v>445</v>
-      </c>
-      <c r="F74" s="13"/>
+      <c r="B74" t="s">
+        <v>15</v>
+      </c>
       <c r="G74" s="10"/>
       <c r="H74" s="10"/>
     </row>
-    <row r="75" spans="1:8" ht="15">
+    <row r="75" spans="1:8" ht="12">
       <c r="A75" s="21"/>
-      <c r="B75" s="15" t="s">
-        <v>441</v>
-      </c>
-      <c r="C75" s="15"/>
-      <c r="D75" s="15"/>
-      <c r="E75" s="15"/>
+      <c r="B75" s="2" t="s">
+        <v>13</v>
+      </c>
+      <c r="C75" s="12"/>
+      <c r="D75" s="25" t="s">
+        <v>448</v>
+      </c>
+      <c r="E75" s="12"/>
+      <c r="F75" s="12"/>
       <c r="G75" s="10"/>
       <c r="H75" s="10"/>
     </row>
     <row r="76" spans="1:8" ht="12">
       <c r="A76" s="21"/>
-      <c r="B76" t="s">
-        <v>15</v>
-      </c>
+      <c r="B76" s="2" t="s">
+        <v>25</v>
+      </c>
+      <c r="C76" s="12"/>
+      <c r="D76" s="25"/>
+      <c r="E76" s="12"/>
+      <c r="F76" s="12"/>
       <c r="G76" s="10"/>
       <c r="H76" s="10"/>
     </row>
-    <row r="77" spans="1:8" ht="12">
+    <row r="77" spans="1:8" ht="15">
       <c r="A77" s="21"/>
-      <c r="B77" s="2" t="s">
-        <v>13</v>
-      </c>
-      <c r="C77" s="12"/>
-      <c r="D77" s="25" t="s">
-        <v>452</v>
-      </c>
-      <c r="E77" s="12"/>
+      <c r="B77" s="15" t="s">
+        <v>438</v>
+      </c>
+      <c r="C77" s="18"/>
+      <c r="D77" s="31"/>
+      <c r="E77" s="18"/>
       <c r="F77" s="12"/>
       <c r="G77" s="10"/>
       <c r="H77" s="10"/>
     </row>
-    <row r="78" spans="1:8" ht="12">
-      <c r="A78" s="21"/>
-      <c r="B78" s="2" t="s">
-        <v>25</v>
-      </c>
-      <c r="C78" s="12"/>
-      <c r="D78" s="25"/>
-      <c r="E78" s="12"/>
-      <c r="F78" s="12"/>
-      <c r="G78" s="10"/>
-      <c r="H78" s="10"/>
-    </row>
-    <row r="79" spans="1:8" ht="15">
-      <c r="A79" s="21"/>
-      <c r="B79" s="15" t="s">
+    <row r="78" spans="1:8" ht="30">
+      <c r="A78" s="27"/>
+      <c r="B78" s="13" t="s">
+        <v>443</v>
+      </c>
+      <c r="C78" s="13"/>
+      <c r="D78" s="13"/>
+      <c r="E78" s="13" t="s">
+        <v>435</v>
+      </c>
+      <c r="F78" s="13"/>
+    </row>
+    <row r="79" spans="1:8" ht="30">
+      <c r="A79" s="27"/>
+      <c r="B79" s="13" t="s">
+        <v>444</v>
+      </c>
+      <c r="C79" s="13"/>
+      <c r="D79" s="13"/>
+      <c r="E79" s="13" t="s">
+        <v>445</v>
+      </c>
+      <c r="F79" s="13"/>
+    </row>
+    <row r="80" spans="1:8" s="10" customFormat="1" ht="15">
+      <c r="B80" s="26" t="s">
+        <v>13</v>
+      </c>
+      <c r="C80" s="26"/>
+      <c r="D80" s="26" t="s">
+        <v>457</v>
+      </c>
+      <c r="E80" s="26"/>
+      <c r="F80" s="26"/>
+    </row>
+    <row r="81" spans="1:8" ht="15">
+      <c r="A81" s="27"/>
+      <c r="B81" s="15" t="s">
+        <v>446</v>
+      </c>
+      <c r="C81" s="15"/>
+      <c r="D81" s="15"/>
+      <c r="E81" s="15"/>
+      <c r="F81" s="15"/>
+    </row>
+    <row r="82" spans="1:8" ht="12">
+      <c r="A82" s="27"/>
+      <c r="B82" t="s">
+        <v>15</v>
+      </c>
+    </row>
+    <row r="83" spans="1:8" ht="12">
+      <c r="A83" s="27"/>
+      <c r="B83" t="s">
+        <v>13</v>
+      </c>
+      <c r="C83" s="20"/>
+      <c r="D83" s="28" t="s">
         <v>442</v>
       </c>
-      <c r="C79" s="18"/>
-      <c r="D79" s="31"/>
-      <c r="E79" s="18"/>
-      <c r="F79" s="12"/>
-      <c r="G79" s="10"/>
-      <c r="H79" s="10"/>
-    </row>
-    <row r="80" spans="1:8" ht="30">
-      <c r="A80" s="27"/>
-      <c r="B80" s="13" t="s">
-        <v>447</v>
-      </c>
-      <c r="C80" s="13"/>
-      <c r="D80" s="13"/>
-      <c r="E80" s="13" t="s">
-        <v>439</v>
-      </c>
-      <c r="F80" s="13"/>
-    </row>
-    <row r="81" spans="1:8" ht="30">
-      <c r="A81" s="27"/>
-      <c r="B81" s="13" t="s">
-        <v>448</v>
-      </c>
-      <c r="C81" s="13"/>
-      <c r="D81" s="13"/>
-      <c r="E81" s="13" t="s">
-        <v>449</v>
-      </c>
-      <c r="F81" s="13"/>
-    </row>
-    <row r="82" spans="1:8" s="10" customFormat="1" ht="15">
-      <c r="B82" s="26" t="s">
-        <v>13</v>
-      </c>
-      <c r="C82" s="26"/>
-      <c r="D82" s="26" t="s">
-        <v>461</v>
-      </c>
-      <c r="E82" s="26"/>
-      <c r="F82" s="26"/>
-    </row>
-    <row r="83" spans="1:8" ht="15">
-      <c r="A83" s="27"/>
-      <c r="B83" s="15" t="s">
-        <v>450</v>
-      </c>
-      <c r="C83" s="15"/>
-      <c r="D83" s="15"/>
-      <c r="E83" s="15"/>
-      <c r="F83" s="15"/>
+      <c r="E83" s="28"/>
+      <c r="F83" s="20"/>
     </row>
     <row r="84" spans="1:8" ht="12">
       <c r="A84" s="27"/>
       <c r="B84" t="s">
-        <v>15</v>
-      </c>
+        <v>25</v>
+      </c>
+      <c r="C84" s="20"/>
+      <c r="D84" s="28"/>
+      <c r="E84" s="20"/>
+      <c r="F84" s="20"/>
     </row>
     <row r="85" spans="1:8" ht="12">
       <c r="A85" s="27"/>
-      <c r="B85" t="s">
+      <c r="C85" s="20"/>
+      <c r="D85" s="28"/>
+      <c r="E85" s="20"/>
+      <c r="F85" s="20"/>
+    </row>
+    <row r="86" spans="1:8" ht="15">
+      <c r="A86" s="27"/>
+      <c r="B86" s="15" t="s">
+        <v>447</v>
+      </c>
+      <c r="C86" s="29"/>
+      <c r="D86" s="30"/>
+      <c r="E86" s="29"/>
+      <c r="F86" s="29"/>
+    </row>
+    <row r="87" spans="1:8" s="10" customFormat="1" ht="15">
+      <c r="B87" s="32" t="s">
         <v>13</v>
       </c>
-      <c r="C85" s="20"/>
-      <c r="D85" s="28" t="s">
-        <v>446</v>
-      </c>
-      <c r="E85" s="28"/>
-      <c r="F85" s="20"/>
-    </row>
-    <row r="86" spans="1:8" ht="12">
-      <c r="A86" s="27"/>
-      <c r="B86" t="s">
-        <v>25</v>
-      </c>
-      <c r="C86" s="20"/>
-      <c r="D86" s="28"/>
-      <c r="E86" s="20"/>
-      <c r="F86" s="20"/>
-    </row>
-    <row r="87" spans="1:8" ht="12">
-      <c r="A87" s="27"/>
-      <c r="C87" s="20"/>
-      <c r="D87" s="28"/>
-      <c r="E87" s="20"/>
-      <c r="F87" s="20"/>
+      <c r="C87" s="33"/>
+      <c r="D87" s="34" t="s">
+        <v>456</v>
+      </c>
+      <c r="E87" s="33"/>
+      <c r="F87" s="33"/>
     </row>
     <row r="88" spans="1:8" ht="15">
       <c r="A88" s="27"/>
       <c r="B88" s="15" t="s">
-        <v>451</v>
+        <v>424</v>
       </c>
       <c r="C88" s="29"/>
       <c r="D88" s="30"/>
@@ -4065,7 +4026,7 @@
       </c>
       <c r="C89" s="33"/>
       <c r="D89" s="34" t="s">
-        <v>460</v>
+        <v>458</v>
       </c>
       <c r="E89" s="33"/>
       <c r="F89" s="33"/>
@@ -4073,105 +4034,112 @@
     <row r="90" spans="1:8" ht="15">
       <c r="A90" s="27"/>
       <c r="B90" s="15" t="s">
-        <v>428</v>
+        <v>80</v>
       </c>
       <c r="C90" s="29"/>
       <c r="D90" s="30"/>
       <c r="E90" s="29"/>
       <c r="F90" s="29"/>
     </row>
-    <row r="91" spans="1:8" s="10" customFormat="1" ht="15">
-      <c r="B91" s="32" t="s">
-        <v>13</v>
-      </c>
+    <row r="91" spans="1:8" ht="15">
+      <c r="A91" s="10"/>
+      <c r="B91" s="32"/>
       <c r="C91" s="33"/>
-      <c r="D91" s="34" t="s">
-        <v>462</v>
-      </c>
+      <c r="D91" s="34"/>
       <c r="E91" s="33"/>
       <c r="F91" s="33"/>
     </row>
-    <row r="92" spans="1:8" ht="15">
-      <c r="A92" s="27"/>
-      <c r="B92" s="15" t="s">
-        <v>80</v>
-      </c>
-      <c r="C92" s="29"/>
-      <c r="D92" s="30"/>
-      <c r="E92" s="29"/>
-      <c r="F92" s="29"/>
-    </row>
-    <row r="93" spans="1:8" ht="15">
-      <c r="A93" s="10"/>
-      <c r="B93" s="32"/>
-      <c r="C93" s="33"/>
-      <c r="D93" s="34"/>
-      <c r="E93" s="33"/>
-      <c r="F93" s="33"/>
-    </row>
-    <row r="94" spans="1:8" s="13" customFormat="1" ht="15">
-      <c r="A94" s="26"/>
-      <c r="B94" s="13" t="s">
+    <row r="92" spans="1:8" s="13" customFormat="1" ht="15">
+      <c r="A92" s="26"/>
+      <c r="B92" s="13" t="s">
         <v>109</v>
       </c>
-      <c r="C94" s="35"/>
-      <c r="D94" s="36"/>
-      <c r="E94" s="14" t="s">
-        <v>453</v>
-      </c>
-      <c r="F94" s="35"/>
-    </row>
-    <row r="95" spans="1:8" s="13" customFormat="1" ht="15">
-      <c r="A95" s="26"/>
-      <c r="B95" s="13" t="s">
+      <c r="C92" s="35"/>
+      <c r="D92" s="36"/>
+      <c r="E92" s="14" t="s">
+        <v>449</v>
+      </c>
+      <c r="F92" s="35"/>
+    </row>
+    <row r="93" spans="1:8" s="13" customFormat="1" ht="15">
+      <c r="A93" s="26"/>
+      <c r="B93" s="13" t="s">
         <v>81</v>
       </c>
-      <c r="C95" s="35"/>
-      <c r="D95" s="36"/>
-      <c r="E95" s="14" t="s">
+      <c r="C93" s="35"/>
+      <c r="D93" s="36"/>
+      <c r="E93" s="14" t="s">
         <v>82</v>
       </c>
-      <c r="F95" s="35"/>
-    </row>
-    <row r="96" spans="1:8" ht="15">
-      <c r="A96" s="21" t="s">
-        <v>435</v>
-      </c>
-      <c r="B96" s="15" t="s">
+      <c r="F93" s="35"/>
+    </row>
+    <row r="94" spans="1:8" ht="15">
+      <c r="A94" s="21" t="s">
+        <v>431</v>
+      </c>
+      <c r="B94" s="15" t="s">
         <v>110</v>
       </c>
-      <c r="C96" s="15"/>
-      <c r="D96" s="15"/>
-      <c r="E96" s="15"/>
-      <c r="F96" s="15"/>
-      <c r="G96" s="15"/>
-      <c r="H96" s="15"/>
+      <c r="C94" s="15"/>
+      <c r="D94" s="15"/>
+      <c r="E94" s="15"/>
+      <c r="F94" s="15"/>
+      <c r="G94" s="15"/>
+      <c r="H94" s="15"/>
+    </row>
+    <row r="95" spans="1:8" ht="12">
+      <c r="A95" s="21"/>
+      <c r="B95" t="s">
+        <v>226</v>
+      </c>
+      <c r="C95" t="s">
+        <v>11</v>
+      </c>
+      <c r="D95" t="s">
+        <v>12</v>
+      </c>
+      <c r="F95" t="s">
+        <v>6</v>
+      </c>
+      <c r="G95" s="12"/>
+      <c r="H95" s="12"/>
+    </row>
+    <row r="96" spans="1:8" ht="12">
+      <c r="A96" s="21"/>
+      <c r="B96" s="4" t="s">
+        <v>15</v>
+      </c>
+      <c r="C96" s="4"/>
+      <c r="D96" s="4"/>
+      <c r="E96" s="4"/>
+      <c r="F96" s="4"/>
     </row>
     <row r="97" spans="1:10" ht="12">
       <c r="A97" s="21"/>
-      <c r="B97" t="s">
-        <v>227</v>
-      </c>
-      <c r="C97" t="s">
-        <v>11</v>
-      </c>
-      <c r="D97" t="s">
-        <v>12</v>
-      </c>
-      <c r="F97" t="s">
-        <v>6</v>
-      </c>
-      <c r="G97" s="12"/>
-      <c r="H97" s="12"/>
-    </row>
-    <row r="98" spans="1:10" ht="12">
+      <c r="B97" s="4" t="s">
+        <v>16</v>
+      </c>
+      <c r="C97" s="4" t="s">
+        <v>17</v>
+      </c>
+      <c r="D97" s="4" t="s">
+        <v>18</v>
+      </c>
+      <c r="E97" s="4"/>
+      <c r="F97" s="4"/>
+    </row>
+    <row r="98" spans="1:10" ht="36">
       <c r="A98" s="21"/>
       <c r="B98" s="4" t="s">
-        <v>15</v>
+        <v>13</v>
       </c>
       <c r="C98" s="4"/>
-      <c r="D98" s="4"/>
-      <c r="E98" s="4"/>
+      <c r="D98" s="4" t="s">
+        <v>19</v>
+      </c>
+      <c r="E98" s="4" t="s">
+        <v>20</v>
+      </c>
       <c r="F98" s="4"/>
     </row>
     <row r="99" spans="1:10" ht="12">
@@ -4180,10 +4148,10 @@
         <v>16</v>
       </c>
       <c r="C99" s="4" t="s">
-        <v>17</v>
+        <v>21</v>
       </c>
       <c r="D99" s="4" t="s">
-        <v>18</v>
+        <v>22</v>
       </c>
       <c r="E99" s="4"/>
       <c r="F99" s="4"/>
@@ -4195,95 +4163,97 @@
       </c>
       <c r="C100" s="4"/>
       <c r="D100" s="4" t="s">
-        <v>19</v>
+        <v>23</v>
       </c>
       <c r="E100" s="4" t="s">
-        <v>20</v>
+        <v>24</v>
       </c>
       <c r="F100" s="4"/>
-    </row>
-    <row r="101" spans="1:10" ht="12">
+      <c r="I100" s="12"/>
+    </row>
+    <row r="101" spans="1:10" ht="12.75" customHeight="1">
       <c r="A101" s="21"/>
       <c r="B101" s="4" t="s">
-        <v>16</v>
-      </c>
-      <c r="C101" s="4" t="s">
-        <v>21</v>
-      </c>
-      <c r="D101" s="4" t="s">
-        <v>22</v>
-      </c>
+        <v>25</v>
+      </c>
+      <c r="C101" s="4"/>
+      <c r="D101" s="4"/>
       <c r="E101" s="4"/>
       <c r="F101" s="4"/>
     </row>
-    <row r="102" spans="1:10" ht="36">
+    <row r="102" spans="1:10" ht="12.75" customHeight="1">
       <c r="A102" s="21"/>
-      <c r="B102" s="4" t="s">
-        <v>13</v>
-      </c>
-      <c r="C102" s="4"/>
-      <c r="D102" s="4" t="s">
-        <v>23</v>
-      </c>
-      <c r="E102" s="4" t="s">
-        <v>24</v>
-      </c>
-      <c r="F102" s="4"/>
-      <c r="I102" s="12"/>
-    </row>
-    <row r="103" spans="1:10" ht="12.75" customHeight="1">
-      <c r="A103" s="21"/>
-      <c r="B103" s="4" t="s">
-        <v>25</v>
-      </c>
-      <c r="C103" s="4"/>
-      <c r="D103" s="4"/>
-      <c r="E103" s="4"/>
-      <c r="F103" s="4"/>
-    </row>
-    <row r="104" spans="1:10" ht="12.75" customHeight="1">
-      <c r="A104" s="21"/>
-      <c r="B104" s="15" t="s">
+      <c r="B102" s="15" t="s">
         <v>83</v>
       </c>
-      <c r="C104" s="15"/>
-      <c r="D104" s="15"/>
-      <c r="E104" s="15"/>
-      <c r="F104" s="15"/>
-      <c r="G104" s="15"/>
-      <c r="H104" s="15"/>
-    </row>
-    <row r="105" spans="1:10" s="12" customFormat="1" ht="12.75" customHeight="1"/>
-    <row r="106" spans="1:10" s="14" customFormat="1" ht="12.75" customHeight="1">
-      <c r="A106" s="24"/>
-      <c r="B106" s="13" t="s">
+      <c r="C102" s="15"/>
+      <c r="D102" s="15"/>
+      <c r="E102" s="15"/>
+      <c r="F102" s="15"/>
+      <c r="G102" s="15"/>
+      <c r="H102" s="15"/>
+    </row>
+    <row r="103" spans="1:10" s="12" customFormat="1" ht="12.75" customHeight="1"/>
+    <row r="104" spans="1:10" s="14" customFormat="1" ht="12.75" customHeight="1">
+      <c r="A104" s="24"/>
+      <c r="B104" s="13" t="s">
         <v>111</v>
       </c>
-      <c r="E106" s="14" t="s">
+      <c r="E104" s="14" t="s">
         <v>112</v>
       </c>
-      <c r="I106" s="12"/>
-      <c r="J106" s="12"/>
+      <c r="I104" s="12"/>
+      <c r="J104" s="12"/>
+    </row>
+    <row r="105" spans="1:10" ht="12.75" customHeight="1">
+      <c r="B105" s="13" t="s">
+        <v>89</v>
+      </c>
+      <c r="C105" s="14"/>
+      <c r="D105" s="14"/>
+      <c r="E105" s="14" t="s">
+        <v>84</v>
+      </c>
+      <c r="F105" s="14"/>
+      <c r="G105" s="14"/>
+      <c r="H105" s="14"/>
+    </row>
+    <row r="106" spans="1:10" ht="12.75" customHeight="1">
+      <c r="A106" s="21" t="s">
+        <v>432</v>
+      </c>
+      <c r="B106" s="15" t="s">
+        <v>128</v>
+      </c>
+      <c r="C106" s="18"/>
+      <c r="D106" s="18"/>
+      <c r="E106" s="18"/>
+      <c r="F106" s="18"/>
+      <c r="G106" s="18"/>
+      <c r="H106" s="18"/>
     </row>
     <row r="107" spans="1:10" ht="12.75" customHeight="1">
-      <c r="B107" s="13" t="s">
-        <v>89</v>
-      </c>
-      <c r="C107" s="14"/>
-      <c r="D107" s="14"/>
-      <c r="E107" s="14" t="s">
-        <v>84</v>
-      </c>
-      <c r="F107" s="14"/>
-      <c r="G107" s="14"/>
-      <c r="H107" s="14"/>
+      <c r="A107" s="21"/>
+      <c r="B107" s="2" t="s">
+        <v>228</v>
+      </c>
+      <c r="C107" s="12" t="s">
+        <v>85</v>
+      </c>
+      <c r="D107" s="12" t="s">
+        <v>86</v>
+      </c>
+      <c r="E107" s="12"/>
+      <c r="F107" s="12" t="s">
+        <v>87</v>
+      </c>
+      <c r="G107" s="12"/>
+      <c r="H107" s="12"/>
     </row>
     <row r="108" spans="1:10" ht="12.75" customHeight="1">
-      <c r="A108" s="21" t="s">
-        <v>436</v>
-      </c>
+      <c r="A108" s="21"/>
       <c r="B108" s="15" t="s">
-        <v>128</v>
+        <v>88</v>
       </c>
       <c r="C108" s="18"/>
       <c r="D108" s="18"/>
@@ -4293,128 +4263,98 @@
       <c r="H108" s="18"/>
     </row>
     <row r="109" spans="1:10" ht="12.75" customHeight="1">
-      <c r="A109" s="21"/>
-      <c r="B109" s="2" t="s">
-        <v>229</v>
-      </c>
-      <c r="C109" s="12" t="s">
-        <v>85</v>
-      </c>
-      <c r="D109" s="12" t="s">
-        <v>86</v>
-      </c>
+      <c r="C109" s="12"/>
+      <c r="D109" s="12"/>
       <c r="E109" s="12"/>
-      <c r="F109" s="12" t="s">
-        <v>87</v>
-      </c>
+      <c r="F109" s="12"/>
       <c r="G109" s="12"/>
       <c r="H109" s="12"/>
     </row>
     <row r="110" spans="1:10" ht="12.75" customHeight="1">
-      <c r="A110" s="21"/>
-      <c r="B110" s="15" t="s">
-        <v>88</v>
-      </c>
-      <c r="C110" s="18"/>
-      <c r="D110" s="18"/>
-      <c r="E110" s="18"/>
-      <c r="F110" s="18"/>
-      <c r="G110" s="18"/>
-      <c r="H110" s="18"/>
+      <c r="B110" s="13" t="s">
+        <v>119</v>
+      </c>
+      <c r="C110" s="14"/>
+      <c r="D110" s="14"/>
+      <c r="E110" s="14" t="s">
+        <v>121</v>
+      </c>
+      <c r="F110" s="14"/>
+      <c r="G110" s="14"/>
+      <c r="H110" s="14"/>
     </row>
     <row r="111" spans="1:10" ht="12.75" customHeight="1">
-      <c r="C111" s="12"/>
-      <c r="D111" s="12"/>
-      <c r="E111" s="12"/>
-      <c r="F111" s="12"/>
-      <c r="G111" s="12"/>
-      <c r="H111" s="12"/>
+      <c r="B111" s="13" t="s">
+        <v>120</v>
+      </c>
+      <c r="C111" s="14"/>
+      <c r="D111" s="14"/>
+      <c r="E111" s="14" t="s">
+        <v>122</v>
+      </c>
+      <c r="F111" s="14"/>
+      <c r="G111" s="14"/>
+      <c r="H111" s="14"/>
     </row>
     <row r="112" spans="1:10" ht="12.75" customHeight="1">
-      <c r="B112" s="13" t="s">
-        <v>119</v>
-      </c>
-      <c r="C112" s="14"/>
-      <c r="D112" s="14"/>
-      <c r="E112" s="14" t="s">
-        <v>121</v>
-      </c>
-      <c r="F112" s="14"/>
-      <c r="G112" s="14"/>
-      <c r="H112" s="14"/>
+      <c r="A112" s="21" t="s">
+        <v>64</v>
+      </c>
+      <c r="B112" s="15" t="s">
+        <v>129</v>
+      </c>
+      <c r="C112" s="18"/>
+      <c r="D112" s="18"/>
+      <c r="E112" s="18"/>
+      <c r="F112" s="18"/>
+      <c r="G112" s="18"/>
+      <c r="H112" s="18"/>
     </row>
     <row r="113" spans="1:8" ht="12.75" customHeight="1">
-      <c r="B113" s="13" t="s">
-        <v>120</v>
-      </c>
-      <c r="C113" s="14"/>
-      <c r="D113" s="14"/>
-      <c r="E113" s="14" t="s">
-        <v>122</v>
-      </c>
-      <c r="F113" s="14"/>
-      <c r="G113" s="14"/>
-      <c r="H113" s="14"/>
+      <c r="A113" s="21"/>
+      <c r="B113" t="s">
+        <v>227</v>
+      </c>
+      <c r="C113" t="s">
+        <v>65</v>
+      </c>
+      <c r="D113" t="s">
+        <v>67</v>
+      </c>
+      <c r="F113" t="s">
+        <v>6</v>
+      </c>
+      <c r="G113" s="12"/>
+      <c r="H113" s="12"/>
     </row>
     <row r="114" spans="1:8" ht="12.75" customHeight="1">
-      <c r="A114" s="21" t="s">
+      <c r="A114" s="21"/>
+      <c r="B114" s="2" t="s">
+        <v>13</v>
+      </c>
+      <c r="C114" s="12"/>
+      <c r="D114" s="12" t="s">
         <v>64</v>
       </c>
-      <c r="B114" s="15" t="s">
-        <v>129</v>
-      </c>
-      <c r="C114" s="18"/>
-      <c r="D114" s="18"/>
-      <c r="E114" s="18"/>
-      <c r="F114" s="18"/>
-      <c r="G114" s="18"/>
-      <c r="H114" s="18"/>
+      <c r="E114" s="12"/>
+      <c r="F114" s="12"/>
+      <c r="G114" s="12"/>
+      <c r="H114" s="12"/>
     </row>
     <row r="115" spans="1:8" ht="12.75" customHeight="1">
       <c r="A115" s="21"/>
-      <c r="B115" t="s">
-        <v>228</v>
-      </c>
-      <c r="C115" t="s">
-        <v>65</v>
-      </c>
-      <c r="D115" t="s">
-        <v>67</v>
-      </c>
-      <c r="F115" t="s">
-        <v>6</v>
-      </c>
-      <c r="G115" s="12"/>
-      <c r="H115" s="12"/>
-    </row>
-    <row r="116" spans="1:8" ht="12.75" customHeight="1">
-      <c r="A116" s="21"/>
-      <c r="B116" s="2" t="s">
-        <v>13</v>
-      </c>
-      <c r="C116" s="12"/>
-      <c r="D116" s="12" t="s">
-        <v>64</v>
-      </c>
-      <c r="E116" s="12"/>
-      <c r="F116" s="12"/>
-      <c r="G116" s="12"/>
-      <c r="H116" s="12"/>
-    </row>
-    <row r="117" spans="1:8" ht="12.75" customHeight="1">
-      <c r="A117" s="21"/>
-      <c r="B117" s="15" t="s">
+      <c r="B115" s="15" t="s">
         <v>123</v>
       </c>
-      <c r="C117" s="18"/>
-      <c r="D117" s="18"/>
-      <c r="E117" s="18"/>
-      <c r="F117" s="18"/>
-      <c r="G117" s="18"/>
-      <c r="H117" s="18"/>
-    </row>
-    <row r="120" spans="1:8" ht="12.75" customHeight="1">
-      <c r="B120" s="17" t="s">
+      <c r="C115" s="18"/>
+      <c r="D115" s="18"/>
+      <c r="E115" s="18"/>
+      <c r="F115" s="18"/>
+      <c r="G115" s="18"/>
+      <c r="H115" s="18"/>
+    </row>
+    <row r="118" spans="1:8" ht="12.75" customHeight="1">
+      <c r="B118" s="17" t="s">
         <v>107</v>
       </c>
     </row>
@@ -4433,7 +4373,7 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:B20"/>
   <sheetViews>
-    <sheetView tabSelected="1" zoomScale="150" zoomScaleNormal="150" zoomScalePageLayoutView="150" workbookViewId="0">
+    <sheetView zoomScale="150" zoomScaleNormal="150" zoomScalePageLayoutView="150" workbookViewId="0">
       <selection activeCell="B18" sqref="B18"/>
     </sheetView>
   </sheetViews>
@@ -4484,122 +4424,122 @@
     </row>
     <row r="6" spans="1:2" ht="12" customHeight="1">
       <c r="A6" t="s">
+        <v>229</v>
+      </c>
+      <c r="B6" t="s">
         <v>230</v>
-      </c>
-      <c r="B6" t="s">
-        <v>231</v>
       </c>
     </row>
     <row r="7" spans="1:2" ht="12" customHeight="1">
       <c r="A7" t="s">
-        <v>232</v>
+        <v>231</v>
       </c>
       <c r="B7" t="s">
-        <v>243</v>
+        <v>242</v>
       </c>
     </row>
     <row r="8" spans="1:2" ht="12" customHeight="1">
       <c r="A8" t="s">
-        <v>233</v>
+        <v>232</v>
       </c>
       <c r="B8" t="s">
-        <v>240</v>
+        <v>239</v>
       </c>
     </row>
     <row r="9" spans="1:2" ht="12" customHeight="1">
       <c r="A9" t="s">
-        <v>261</v>
+        <v>260</v>
       </c>
       <c r="B9" t="s">
-        <v>258</v>
+        <v>257</v>
       </c>
     </row>
     <row r="10" spans="1:2" ht="12" customHeight="1">
       <c r="A10" t="s">
-        <v>234</v>
+        <v>233</v>
       </c>
       <c r="B10" t="s">
-        <v>241</v>
+        <v>240</v>
       </c>
     </row>
     <row r="11" spans="1:2" ht="12" customHeight="1">
       <c r="A11" t="s">
-        <v>235</v>
+        <v>234</v>
       </c>
       <c r="B11" t="s">
-        <v>242</v>
+        <v>241</v>
       </c>
     </row>
     <row r="12" spans="1:2" ht="42" customHeight="1">
       <c r="A12" t="s">
+        <v>258</v>
+      </c>
+      <c r="B12" t="s">
         <v>259</v>
-      </c>
-      <c r="B12" t="s">
-        <v>260</v>
       </c>
     </row>
     <row r="13" spans="1:2" ht="12.75" customHeight="1">
       <c r="A13" t="s">
-        <v>386</v>
+        <v>382</v>
       </c>
       <c r="B13" t="s">
-        <v>392</v>
+        <v>388</v>
       </c>
     </row>
     <row r="14" spans="1:2" ht="12.75" customHeight="1">
       <c r="A14" t="s">
-        <v>387</v>
+        <v>383</v>
       </c>
       <c r="B14" t="s">
-        <v>393</v>
+        <v>389</v>
       </c>
     </row>
     <row r="15" spans="1:2" ht="12.75" customHeight="1">
       <c r="A15" t="s">
-        <v>388</v>
+        <v>384</v>
       </c>
       <c r="B15" t="s">
-        <v>394</v>
+        <v>390</v>
       </c>
     </row>
     <row r="16" spans="1:2" ht="12.75" customHeight="1">
       <c r="A16" t="s">
-        <v>389</v>
+        <v>385</v>
       </c>
       <c r="B16" t="s">
-        <v>395</v>
+        <v>391</v>
       </c>
     </row>
     <row r="17" spans="1:2" ht="12.75" customHeight="1">
       <c r="A17" t="s">
-        <v>465</v>
+        <v>460</v>
       </c>
       <c r="B17" t="s">
-        <v>468</v>
+        <v>462</v>
       </c>
     </row>
     <row r="18" spans="1:2" ht="12.75" customHeight="1">
       <c r="A18" t="s">
-        <v>390</v>
+        <v>386</v>
       </c>
       <c r="B18" t="s">
-        <v>396</v>
+        <v>392</v>
       </c>
     </row>
     <row r="19" spans="1:2" ht="12.75" customHeight="1">
       <c r="A19" t="s">
-        <v>391</v>
+        <v>387</v>
       </c>
       <c r="B19" t="s">
-        <v>466</v>
+        <v>461</v>
       </c>
     </row>
     <row r="20" spans="1:2" ht="12.75" customHeight="1">
       <c r="A20" t="s">
-        <v>398</v>
+        <v>394</v>
       </c>
       <c r="B20" t="s">
-        <v>399</v>
+        <v>395</v>
       </c>
     </row>
   </sheetData>
@@ -4885,35 +4825,35 @@
     </row>
     <row r="32" spans="1:3" ht="12.75" customHeight="1">
       <c r="A32" t="s">
-        <v>262</v>
+        <v>261</v>
       </c>
       <c r="B32" t="s">
-        <v>267</v>
+        <v>263</v>
       </c>
       <c r="C32" t="s">
-        <v>268</v>
+        <v>264</v>
       </c>
     </row>
     <row r="33" spans="1:3" ht="12.75" customHeight="1">
       <c r="A33" t="s">
-        <v>262</v>
+        <v>261</v>
       </c>
       <c r="B33" t="s">
-        <v>269</v>
+        <v>265</v>
       </c>
       <c r="C33" t="s">
-        <v>270</v>
+        <v>266</v>
       </c>
     </row>
     <row r="34" spans="1:3" ht="12.75" customHeight="1">
       <c r="A34" t="s">
-        <v>262</v>
+        <v>261</v>
       </c>
       <c r="B34" t="s">
-        <v>397</v>
+        <v>393</v>
       </c>
       <c r="C34" t="s">
-        <v>385</v>
+        <v>381</v>
       </c>
     </row>
     <row r="36" spans="1:3" ht="12.75" customHeight="1">
@@ -4984,68 +4924,68 @@
     </row>
     <row r="43" spans="1:3" ht="12.75" customHeight="1">
       <c r="A43" t="s">
-        <v>265</v>
+        <v>262</v>
       </c>
       <c r="B43" t="s">
-        <v>271</v>
+        <v>267</v>
       </c>
       <c r="C43" t="s">
-        <v>289</v>
+        <v>285</v>
       </c>
     </row>
     <row r="44" spans="1:3" ht="12.75" customHeight="1">
       <c r="A44" t="s">
-        <v>265</v>
+        <v>262</v>
       </c>
       <c r="B44" t="s">
-        <v>274</v>
+        <v>270</v>
       </c>
       <c r="C44" t="s">
-        <v>290</v>
+        <v>286</v>
       </c>
     </row>
     <row r="45" spans="1:3" ht="12.75" customHeight="1">
       <c r="A45" t="s">
-        <v>265</v>
+        <v>262</v>
       </c>
       <c r="B45" t="s">
-        <v>277</v>
+        <v>273</v>
       </c>
       <c r="C45" t="s">
-        <v>291</v>
+        <v>287</v>
       </c>
     </row>
     <row r="46" spans="1:3" ht="12.75" customHeight="1">
       <c r="A46" t="s">
-        <v>265</v>
+        <v>262</v>
       </c>
       <c r="B46" t="s">
-        <v>278</v>
+        <v>274</v>
       </c>
       <c r="C46" t="s">
-        <v>384</v>
+        <v>380</v>
       </c>
     </row>
     <row r="47" spans="1:3" ht="12.75" customHeight="1">
       <c r="A47" t="s">
-        <v>265</v>
+        <v>262</v>
       </c>
       <c r="B47" t="s">
-        <v>280</v>
+        <v>276</v>
       </c>
       <c r="C47" t="s">
-        <v>292</v>
+        <v>288</v>
       </c>
     </row>
     <row r="48" spans="1:3" ht="12.75" customHeight="1">
       <c r="A48" t="s">
-        <v>265</v>
+        <v>262</v>
       </c>
       <c r="B48" t="s">
-        <v>282</v>
+        <v>278</v>
       </c>
       <c r="C48" t="s">
-        <v>293</v>
+        <v>289</v>
       </c>
     </row>
     <row r="50" spans="1:4" ht="12.75" customHeight="1">
@@ -5227,80 +5167,80 @@
     </row>
     <row r="69" spans="1:4" ht="12.75" customHeight="1">
       <c r="A69" t="s">
-        <v>237</v>
+        <v>236</v>
       </c>
       <c r="B69" t="s">
-        <v>251</v>
+        <v>250</v>
       </c>
       <c r="D69" t="s">
-        <v>244</v>
+        <v>243</v>
       </c>
     </row>
     <row r="70" spans="1:4" ht="12.75" customHeight="1">
       <c r="A70" t="s">
-        <v>237</v>
+        <v>236</v>
       </c>
       <c r="B70" t="s">
-        <v>252</v>
+        <v>251</v>
       </c>
       <c r="C70" s="2"/>
       <c r="D70" t="s">
-        <v>245</v>
+        <v>244</v>
       </c>
     </row>
     <row r="71" spans="1:4" ht="12.75" customHeight="1">
       <c r="A71" t="s">
-        <v>237</v>
+        <v>236</v>
       </c>
       <c r="B71" t="s">
-        <v>253</v>
+        <v>252</v>
       </c>
       <c r="D71" t="s">
-        <v>246</v>
+        <v>245</v>
       </c>
     </row>
     <row r="72" spans="1:4" ht="12.75" customHeight="1">
       <c r="A72" t="s">
-        <v>237</v>
+        <v>236</v>
       </c>
       <c r="B72" t="s">
-        <v>254</v>
+        <v>253</v>
       </c>
       <c r="D72" t="s">
-        <v>247</v>
+        <v>246</v>
       </c>
     </row>
     <row r="73" spans="1:4" ht="12.75" customHeight="1">
       <c r="A73" t="s">
-        <v>237</v>
+        <v>236</v>
       </c>
       <c r="B73" t="s">
-        <v>255</v>
+        <v>254</v>
       </c>
       <c r="D73" t="s">
-        <v>248</v>
+        <v>247</v>
       </c>
     </row>
     <row r="74" spans="1:4" ht="12.75" customHeight="1">
       <c r="A74" t="s">
-        <v>237</v>
+        <v>236</v>
       </c>
       <c r="B74" t="s">
-        <v>256</v>
+        <v>255</v>
       </c>
       <c r="D74" t="s">
-        <v>249</v>
+        <v>248</v>
       </c>
     </row>
     <row r="75" spans="1:4" ht="12.75" customHeight="1">
       <c r="A75" t="s">
-        <v>237</v>
+        <v>236</v>
       </c>
       <c r="B75" t="s">
-        <v>257</v>
+        <v>256</v>
       </c>
       <c r="D75" t="s">
-        <v>250</v>
+        <v>249</v>
       </c>
     </row>
     <row r="77" spans="1:4" ht="12.75" customHeight="1">
@@ -5439,453 +5379,453 @@
     </row>
     <row r="91" spans="1:4" ht="12.75" customHeight="1">
       <c r="A91" t="s">
-        <v>294</v>
+        <v>290</v>
       </c>
       <c r="B91" t="s">
-        <v>300</v>
+        <v>296</v>
       </c>
       <c r="C91" t="s">
-        <v>307</v>
+        <v>303</v>
       </c>
     </row>
     <row r="92" spans="1:4" ht="12.75" customHeight="1">
       <c r="A92" t="s">
-        <v>294</v>
+        <v>290</v>
       </c>
       <c r="B92" t="s">
-        <v>301</v>
+        <v>297</v>
       </c>
       <c r="C92" t="s">
-        <v>308</v>
+        <v>304</v>
       </c>
     </row>
     <row r="93" spans="1:4" ht="12.75" customHeight="1">
       <c r="A93" t="s">
-        <v>294</v>
+        <v>290</v>
       </c>
       <c r="B93" t="s">
-        <v>302</v>
+        <v>298</v>
       </c>
       <c r="C93" t="s">
-        <v>309</v>
+        <v>305</v>
       </c>
     </row>
     <row r="94" spans="1:4" ht="12.75" customHeight="1">
       <c r="A94" t="s">
-        <v>294</v>
+        <v>290</v>
       </c>
       <c r="B94" t="s">
-        <v>303</v>
+        <v>299</v>
       </c>
       <c r="C94" t="s">
-        <v>310</v>
+        <v>306</v>
       </c>
     </row>
     <row r="95" spans="1:4" ht="12.75" customHeight="1">
       <c r="A95" t="s">
-        <v>294</v>
+        <v>290</v>
       </c>
       <c r="B95" t="s">
-        <v>304</v>
+        <v>300</v>
       </c>
       <c r="C95" t="s">
-        <v>311</v>
+        <v>307</v>
       </c>
     </row>
     <row r="96" spans="1:4" ht="12.75" customHeight="1">
       <c r="A96" t="s">
-        <v>294</v>
+        <v>290</v>
       </c>
       <c r="B96" t="s">
-        <v>305</v>
+        <v>301</v>
       </c>
       <c r="C96" t="s">
-        <v>312</v>
+        <v>308</v>
       </c>
     </row>
     <row r="97" spans="1:3" ht="12.75" customHeight="1">
       <c r="A97" t="s">
-        <v>294</v>
+        <v>290</v>
       </c>
       <c r="B97" t="s">
-        <v>306</v>
+        <v>302</v>
       </c>
       <c r="C97" t="s">
-        <v>313</v>
+        <v>309</v>
       </c>
     </row>
     <row r="99" spans="1:3" ht="12.75" customHeight="1">
       <c r="A99" t="s">
-        <v>295</v>
+        <v>291</v>
       </c>
       <c r="B99" t="s">
-        <v>320</v>
+        <v>316</v>
       </c>
       <c r="C99" t="s">
-        <v>326</v>
+        <v>322</v>
       </c>
     </row>
     <row r="100" spans="1:3" ht="12.75" customHeight="1">
       <c r="A100" t="s">
-        <v>295</v>
+        <v>291</v>
       </c>
       <c r="B100" t="s">
-        <v>321</v>
+        <v>317</v>
       </c>
       <c r="C100" t="s">
-        <v>327</v>
+        <v>323</v>
       </c>
     </row>
     <row r="101" spans="1:3" ht="12.75" customHeight="1">
       <c r="A101" t="s">
-        <v>295</v>
+        <v>291</v>
       </c>
       <c r="B101" t="s">
-        <v>322</v>
+        <v>318</v>
       </c>
       <c r="C101" t="s">
-        <v>328</v>
+        <v>324</v>
       </c>
     </row>
     <row r="102" spans="1:3" ht="12.75" customHeight="1">
       <c r="A102" t="s">
-        <v>295</v>
+        <v>291</v>
       </c>
       <c r="B102" t="s">
-        <v>323</v>
+        <v>319</v>
       </c>
       <c r="C102" t="s">
-        <v>329</v>
+        <v>325</v>
       </c>
     </row>
     <row r="103" spans="1:3" ht="12.75" customHeight="1">
       <c r="A103" t="s">
-        <v>295</v>
+        <v>291</v>
       </c>
       <c r="B103" t="s">
-        <v>324</v>
+        <v>320</v>
       </c>
       <c r="C103" t="s">
-        <v>330</v>
+        <v>326</v>
       </c>
     </row>
     <row r="104" spans="1:3" ht="12.75" customHeight="1">
       <c r="A104" t="s">
-        <v>295</v>
+        <v>291</v>
       </c>
       <c r="B104" t="s">
-        <v>325</v>
+        <v>321</v>
       </c>
       <c r="C104" t="s">
-        <v>331</v>
+        <v>327</v>
       </c>
     </row>
     <row r="106" spans="1:3" ht="12.75" customHeight="1">
       <c r="A106" t="s">
-        <v>296</v>
+        <v>292</v>
       </c>
       <c r="B106" t="s">
-        <v>338</v>
+        <v>334</v>
       </c>
       <c r="C106" t="s">
-        <v>339</v>
+        <v>335</v>
       </c>
     </row>
     <row r="107" spans="1:3" ht="12.75" customHeight="1">
       <c r="A107" t="s">
-        <v>296</v>
+        <v>292</v>
       </c>
       <c r="B107" t="s">
-        <v>332</v>
+        <v>328</v>
       </c>
       <c r="C107" t="s">
-        <v>340</v>
+        <v>336</v>
       </c>
     </row>
     <row r="108" spans="1:3" ht="12.75" customHeight="1">
       <c r="A108" t="s">
-        <v>296</v>
+        <v>292</v>
       </c>
       <c r="B108" t="s">
-        <v>333</v>
+        <v>329</v>
       </c>
       <c r="C108" t="s">
-        <v>341</v>
+        <v>337</v>
       </c>
     </row>
     <row r="109" spans="1:3" ht="12.75" customHeight="1">
       <c r="A109" t="s">
-        <v>296</v>
+        <v>292</v>
       </c>
       <c r="B109" t="s">
-        <v>334</v>
+        <v>330</v>
       </c>
       <c r="C109" t="s">
-        <v>342</v>
+        <v>338</v>
       </c>
     </row>
     <row r="110" spans="1:3" ht="12.75" customHeight="1">
       <c r="A110" t="s">
-        <v>296</v>
+        <v>292</v>
       </c>
       <c r="B110" t="s">
-        <v>335</v>
+        <v>331</v>
       </c>
       <c r="C110" t="s">
-        <v>343</v>
+        <v>339</v>
       </c>
     </row>
     <row r="111" spans="1:3" ht="12.75" customHeight="1">
       <c r="A111" t="s">
-        <v>296</v>
+        <v>292</v>
       </c>
       <c r="B111" t="s">
-        <v>336</v>
+        <v>332</v>
       </c>
       <c r="C111" t="s">
-        <v>344</v>
+        <v>340</v>
       </c>
     </row>
     <row r="112" spans="1:3" ht="12.75" customHeight="1">
       <c r="A112" t="s">
-        <v>296</v>
+        <v>292</v>
       </c>
       <c r="B112" t="s">
-        <v>337</v>
+        <v>333</v>
       </c>
       <c r="C112" t="s">
-        <v>345</v>
+        <v>341</v>
       </c>
     </row>
     <row r="114" spans="1:3" ht="12.75" customHeight="1">
       <c r="A114" t="s">
-        <v>297</v>
+        <v>293</v>
       </c>
       <c r="B114" t="s">
-        <v>346</v>
+        <v>342</v>
       </c>
       <c r="C114" t="s">
-        <v>352</v>
+        <v>348</v>
       </c>
     </row>
     <row r="115" spans="1:3" ht="12.75" customHeight="1">
       <c r="A115" t="s">
-        <v>297</v>
+        <v>293</v>
       </c>
       <c r="B115" t="s">
-        <v>347</v>
+        <v>343</v>
       </c>
       <c r="C115" t="s">
-        <v>353</v>
+        <v>349</v>
       </c>
     </row>
     <row r="116" spans="1:3" ht="12.75" customHeight="1">
       <c r="A116" t="s">
-        <v>297</v>
+        <v>293</v>
       </c>
       <c r="B116" t="s">
-        <v>348</v>
+        <v>344</v>
       </c>
       <c r="C116" t="s">
-        <v>354</v>
+        <v>350</v>
       </c>
     </row>
     <row r="117" spans="1:3" ht="12.75" customHeight="1">
       <c r="A117" t="s">
-        <v>297</v>
+        <v>293</v>
       </c>
       <c r="B117" t="s">
-        <v>349</v>
+        <v>345</v>
       </c>
       <c r="C117" t="s">
-        <v>355</v>
+        <v>351</v>
       </c>
     </row>
     <row r="118" spans="1:3" ht="12.75" customHeight="1">
       <c r="A118" t="s">
-        <v>297</v>
+        <v>293</v>
       </c>
       <c r="B118" t="s">
-        <v>350</v>
+        <v>346</v>
       </c>
       <c r="C118" t="s">
-        <v>356</v>
+        <v>352</v>
       </c>
     </row>
     <row r="119" spans="1:3" ht="12.75" customHeight="1">
       <c r="A119" t="s">
-        <v>297</v>
+        <v>293</v>
       </c>
       <c r="B119" t="s">
-        <v>351</v>
+        <v>347</v>
       </c>
       <c r="C119" t="s">
-        <v>357</v>
+        <v>353</v>
       </c>
     </row>
     <row r="121" spans="1:3" ht="12.75" customHeight="1">
       <c r="A121" t="s">
-        <v>298</v>
+        <v>294</v>
       </c>
       <c r="B121" t="s">
-        <v>364</v>
+        <v>360</v>
       </c>
       <c r="C121" t="s">
-        <v>365</v>
+        <v>361</v>
       </c>
     </row>
     <row r="122" spans="1:3" ht="12.75" customHeight="1">
       <c r="A122" t="s">
-        <v>298</v>
+        <v>294</v>
       </c>
       <c r="B122" t="s">
-        <v>358</v>
+        <v>354</v>
       </c>
       <c r="C122" t="s">
-        <v>366</v>
+        <v>362</v>
       </c>
     </row>
     <row r="123" spans="1:3" ht="12.75" customHeight="1">
       <c r="A123" t="s">
-        <v>298</v>
+        <v>294</v>
       </c>
       <c r="B123" t="s">
-        <v>359</v>
+        <v>355</v>
       </c>
       <c r="C123" t="s">
-        <v>367</v>
+        <v>363</v>
       </c>
     </row>
     <row r="124" spans="1:3" ht="12.75" customHeight="1">
       <c r="A124" t="s">
-        <v>298</v>
+        <v>294</v>
       </c>
       <c r="B124" t="s">
-        <v>361</v>
+        <v>357</v>
       </c>
       <c r="C124" t="s">
-        <v>368</v>
+        <v>364</v>
       </c>
     </row>
     <row r="125" spans="1:3" ht="12.75" customHeight="1">
       <c r="A125" t="s">
-        <v>298</v>
+        <v>294</v>
       </c>
       <c r="B125" t="s">
-        <v>360</v>
+        <v>356</v>
       </c>
       <c r="C125" t="s">
-        <v>369</v>
+        <v>365</v>
       </c>
     </row>
     <row r="126" spans="1:3" ht="12.75" customHeight="1">
       <c r="A126" t="s">
-        <v>298</v>
+        <v>294</v>
       </c>
       <c r="B126" t="s">
-        <v>362</v>
+        <v>358</v>
       </c>
       <c r="C126" t="s">
-        <v>370</v>
+        <v>366</v>
       </c>
     </row>
     <row r="127" spans="1:3" ht="12.75" customHeight="1">
       <c r="A127" t="s">
-        <v>298</v>
+        <v>294</v>
       </c>
       <c r="B127" t="s">
-        <v>363</v>
+        <v>359</v>
       </c>
       <c r="C127" t="s">
-        <v>371</v>
+        <v>367</v>
       </c>
     </row>
     <row r="129" spans="1:3" ht="12.75" customHeight="1">
       <c r="A129" t="s">
-        <v>299</v>
+        <v>295</v>
       </c>
       <c r="B129" t="s">
-        <v>372</v>
+        <v>368</v>
       </c>
       <c r="C129" t="s">
-        <v>378</v>
+        <v>374</v>
       </c>
     </row>
     <row r="130" spans="1:3" ht="12.75" customHeight="1">
       <c r="A130" t="s">
-        <v>299</v>
+        <v>295</v>
       </c>
       <c r="B130" t="s">
-        <v>373</v>
+        <v>369</v>
       </c>
       <c r="C130" t="s">
-        <v>379</v>
+        <v>375</v>
       </c>
     </row>
     <row r="131" spans="1:3" ht="12.75" customHeight="1">
       <c r="A131" t="s">
-        <v>299</v>
+        <v>295</v>
       </c>
       <c r="B131" t="s">
-        <v>374</v>
+        <v>370</v>
       </c>
       <c r="C131" t="s">
-        <v>380</v>
+        <v>376</v>
       </c>
     </row>
     <row r="132" spans="1:3" ht="12.75" customHeight="1">
       <c r="A132" t="s">
-        <v>299</v>
+        <v>295</v>
       </c>
       <c r="B132" t="s">
-        <v>375</v>
+        <v>371</v>
       </c>
       <c r="C132" t="s">
-        <v>381</v>
+        <v>377</v>
       </c>
     </row>
     <row r="133" spans="1:3" ht="12.75" customHeight="1">
       <c r="A133" t="s">
-        <v>299</v>
+        <v>295</v>
       </c>
       <c r="B133" t="s">
-        <v>376</v>
+        <v>372</v>
       </c>
       <c r="C133" t="s">
-        <v>382</v>
+        <v>378</v>
       </c>
     </row>
     <row r="134" spans="1:3" ht="12.75" customHeight="1">
       <c r="A134" t="s">
-        <v>299</v>
+        <v>295</v>
       </c>
       <c r="B134" t="s">
-        <v>377</v>
+        <v>373</v>
       </c>
       <c r="C134" t="s">
-        <v>383</v>
+        <v>379</v>
       </c>
     </row>
     <row r="136" spans="1:3" ht="12.75" customHeight="1">
       <c r="A136" t="s">
-        <v>437</v>
+        <v>433</v>
       </c>
       <c r="B136" t="s">
-        <v>432</v>
+        <v>428</v>
       </c>
       <c r="C136" t="s">
-        <v>426</v>
+        <v>422</v>
       </c>
     </row>
     <row r="137" spans="1:3" ht="12.75" customHeight="1">
       <c r="A137" t="s">
-        <v>437</v>
+        <v>433</v>
       </c>
       <c r="B137" t="s">
-        <v>433</v>
+        <v>429</v>
       </c>
       <c r="C137" t="s">
-        <v>434</v>
+        <v>430</v>
       </c>
     </row>
   </sheetData>

</xml_diff>

<commit_message>
Added template of medication with Caffeine information
</commit_message>
<xml_diff>
--- a/opendatakit.collect2/form-files/neonatal/neonatal.xlsx
+++ b/opendatakit.collect2/form-files/neonatal/neonatal.xlsx
@@ -4,7 +4,7 @@
   <fileVersion appName="xl" lastEdited="5" lowestEdited="5" rupBuild="21721"/>
   <workbookPr autoCompressPictures="0"/>
   <bookViews>
-    <workbookView xWindow="320" yWindow="0" windowWidth="20220" windowHeight="15340" tabRatio="500"/>
+    <workbookView xWindow="320" yWindow="0" windowWidth="23140" windowHeight="15340" tabRatio="500" activeTab="2"/>
   </bookViews>
   <sheets>
     <sheet name="survey" sheetId="1" r:id="rId1"/>
@@ -23,7 +23,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="830" uniqueCount="529">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="842" uniqueCount="534">
   <si>
     <t>type</t>
   </si>
@@ -277,24 +277,6 @@
     <t>goto medications_end</t>
   </si>
   <si>
-    <t>medicine_a</t>
-  </si>
-  <si>
-    <t>Medicine_A</t>
-  </si>
-  <si>
-    <t>medicine_b</t>
-  </si>
-  <si>
-    <t>Medicine_B</t>
-  </si>
-  <si>
-    <t>medicine_c</t>
-  </si>
-  <si>
-    <t>Medicine_C</t>
-  </si>
-  <si>
     <t>medications</t>
   </si>
   <si>
@@ -677,9 +659,6 @@
   </si>
   <si>
     <t>menu calculators_menu</t>
-  </si>
-  <si>
-    <t>menu medications_menu</t>
   </si>
   <si>
     <t>postureScore</t>
@@ -1812,6 +1791,42 @@
   </si>
   <si>
     <t>&lt;p&gt;Baby weight is: {{calculates.default_convertToPound}} pounds&lt;/p&gt;</t>
+  </si>
+  <si>
+    <t>Please select medication:</t>
+  </si>
+  <si>
+    <t>caffeine</t>
+  </si>
+  <si>
+    <t>templates/caffeine.handlebars</t>
+  </si>
+  <si>
+    <t>Medication B selected</t>
+  </si>
+  <si>
+    <t>Medication C selected</t>
+  </si>
+  <si>
+    <t>select_one medications_menu</t>
+  </si>
+  <si>
+    <t>selected(data('medications_menu'),'caffeine')</t>
+  </si>
+  <si>
+    <t>selected(data('medications_menu'),'medB')</t>
+  </si>
+  <si>
+    <t>selected(data('medications_menu'),'medC')</t>
+  </si>
+  <si>
+    <t>medB</t>
+  </si>
+  <si>
+    <t>medC</t>
+  </si>
+  <si>
+    <t>Caffeine</t>
   </si>
 </sst>
 </file>
@@ -1875,7 +1890,7 @@
       <family val="2"/>
     </font>
   </fonts>
-  <fills count="17">
+  <fills count="19">
     <fill>
       <patternFill patternType="none"/>
     </fill>
@@ -1970,6 +1985,18 @@
         <bgColor rgb="FF000000"/>
       </patternFill>
     </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="6" tint="0.79998168889431442"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="5" tint="0.79998168889431442"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
   </fills>
   <borders count="1">
     <border>
@@ -1980,7 +2007,7 @@
       <diagonal/>
     </border>
   </borders>
-  <cellStyleXfs count="398">
+  <cellStyleXfs count="402">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
     <xf numFmtId="0" fontId="3" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
     <xf numFmtId="0" fontId="4" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
@@ -2379,8 +2406,12 @@
     <xf numFmtId="0" fontId="4" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
     <xf numFmtId="0" fontId="3" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
     <xf numFmtId="0" fontId="4" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="4" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="4" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
   </cellStyleXfs>
-  <cellXfs count="43">
+  <cellXfs count="45">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
       <alignment wrapText="1"/>
     </xf>
@@ -2470,8 +2501,14 @@
     <xf numFmtId="0" fontId="0" fillId="16" borderId="0" xfId="0" applyFill="1" applyAlignment="1">
       <alignment wrapText="1"/>
     </xf>
+    <xf numFmtId="0" fontId="0" fillId="17" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1">
+      <alignment wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="18" borderId="0" xfId="0" applyFill="1" applyAlignment="1">
+      <alignment wrapText="1"/>
+    </xf>
   </cellXfs>
-  <cellStyles count="398">
+  <cellStyles count="402">
     <cellStyle name="20% - Accent4" xfId="13" builtinId="42"/>
     <cellStyle name="Followed Hyperlink" xfId="2" builtinId="9" hidden="1"/>
     <cellStyle name="Followed Hyperlink" xfId="4" builtinId="9" hidden="1"/>
@@ -2670,6 +2707,8 @@
     <cellStyle name="Followed Hyperlink" xfId="393" builtinId="9" hidden="1"/>
     <cellStyle name="Followed Hyperlink" xfId="395" builtinId="9" hidden="1"/>
     <cellStyle name="Followed Hyperlink" xfId="397" builtinId="9" hidden="1"/>
+    <cellStyle name="Followed Hyperlink" xfId="399" builtinId="9" hidden="1"/>
+    <cellStyle name="Followed Hyperlink" xfId="401" builtinId="9" hidden="1"/>
     <cellStyle name="Good" xfId="11" builtinId="26"/>
     <cellStyle name="Hyperlink" xfId="1" builtinId="8" hidden="1"/>
     <cellStyle name="Hyperlink" xfId="3" builtinId="8" hidden="1"/>
@@ -2868,6 +2907,8 @@
     <cellStyle name="Hyperlink" xfId="392" builtinId="8" hidden="1"/>
     <cellStyle name="Hyperlink" xfId="394" builtinId="8" hidden="1"/>
     <cellStyle name="Hyperlink" xfId="396" builtinId="8" hidden="1"/>
+    <cellStyle name="Hyperlink" xfId="398" builtinId="8" hidden="1"/>
+    <cellStyle name="Hyperlink" xfId="400" builtinId="8" hidden="1"/>
     <cellStyle name="Neutral" xfId="12" builtinId="28"/>
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
   </cellStyles>
@@ -3198,10 +3239,10 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <dimension ref="A1:J198"/>
+  <dimension ref="A1:J203"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A118" zoomScale="150" zoomScaleNormal="150" zoomScalePageLayoutView="150" workbookViewId="0">
-      <selection activeCell="A130" sqref="A130:XFD130"/>
+    <sheetView topLeftCell="A148" zoomScale="150" zoomScaleNormal="150" zoomScalePageLayoutView="150" workbookViewId="0">
+      <selection activeCell="C161" sqref="C161"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultColWidth="11.5" defaultRowHeight="12.75" customHeight="1" x14ac:dyDescent="0"/>
@@ -3215,7 +3256,7 @@
   <sheetData>
     <row r="1" spans="1:9" ht="12">
       <c r="A1" t="s">
-        <v>427</v>
+        <v>420</v>
       </c>
       <c r="B1" s="1" t="s">
         <v>0</v>
@@ -3239,12 +3280,12 @@
         <v>64</v>
       </c>
       <c r="I1" t="s">
-        <v>486</v>
+        <v>479</v>
       </c>
     </row>
     <row r="2" spans="1:9" ht="15">
       <c r="B2" s="16" t="s">
-        <v>100</v>
+        <v>94</v>
       </c>
       <c r="C2" s="1"/>
       <c r="D2" s="3"/>
@@ -3253,7 +3294,7 @@
     </row>
     <row r="3" spans="1:9" ht="12">
       <c r="B3" s="3" t="s">
-        <v>213</v>
+        <v>207</v>
       </c>
       <c r="C3" s="4" t="s">
         <v>4</v>
@@ -3278,12 +3319,12 @@
         <v>8</v>
       </c>
       <c r="B5" s="19" t="s">
-        <v>412</v>
+        <v>405</v>
       </c>
       <c r="C5" s="19"/>
       <c r="D5" s="19"/>
       <c r="E5" s="19" t="s">
-        <v>413</v>
+        <v>406</v>
       </c>
       <c r="F5" s="19"/>
       <c r="G5" s="19"/>
@@ -3292,12 +3333,12 @@
     <row r="6" spans="1:9" ht="12.75" customHeight="1">
       <c r="A6" s="22"/>
       <c r="B6" s="19" t="s">
-        <v>414</v>
+        <v>407</v>
       </c>
       <c r="C6" s="19"/>
       <c r="D6" s="19"/>
       <c r="E6" s="19" t="s">
-        <v>415</v>
+        <v>408</v>
       </c>
       <c r="F6" s="19"/>
       <c r="G6" s="19"/>
@@ -3306,7 +3347,7 @@
     <row r="7" spans="1:9" s="12" customFormat="1" ht="18" customHeight="1">
       <c r="A7" s="23"/>
       <c r="B7" s="18" t="s">
-        <v>102</v>
+        <v>96</v>
       </c>
       <c r="C7" s="18"/>
       <c r="D7" s="18"/>
@@ -3318,7 +3359,7 @@
     <row r="8" spans="1:9" s="12" customFormat="1" ht="18" customHeight="1">
       <c r="A8" s="23"/>
       <c r="B8" t="s">
-        <v>214</v>
+        <v>208</v>
       </c>
       <c r="C8" t="s">
         <v>7</v>
@@ -3338,69 +3379,69 @@
       </c>
       <c r="C9" s="2"/>
       <c r="D9" s="2" t="s">
-        <v>95</v>
+        <v>89</v>
       </c>
       <c r="E9" s="2" t="s">
-        <v>113</v>
+        <v>107</v>
       </c>
       <c r="F9" s="2"/>
       <c r="G9" t="s">
-        <v>115</v>
+        <v>109</v>
       </c>
     </row>
     <row r="10" spans="1:9" ht="18" customHeight="1">
       <c r="A10" s="22"/>
       <c r="B10" s="2" t="s">
-        <v>96</v>
+        <v>90</v>
       </c>
       <c r="C10" s="4"/>
       <c r="D10" s="2" t="s">
-        <v>94</v>
+        <v>88</v>
       </c>
       <c r="E10" s="2" t="s">
-        <v>116</v>
+        <v>110</v>
       </c>
       <c r="F10" s="2"/>
     </row>
     <row r="11" spans="1:9" ht="18" customHeight="1">
       <c r="A11" s="22"/>
       <c r="B11" s="2" t="s">
-        <v>96</v>
+        <v>90</v>
       </c>
       <c r="C11" s="4"/>
       <c r="D11" s="2" t="s">
-        <v>97</v>
+        <v>91</v>
       </c>
       <c r="E11" s="2" t="s">
-        <v>114</v>
+        <v>108</v>
       </c>
       <c r="F11" s="2"/>
     </row>
     <row r="12" spans="1:9" ht="18" customHeight="1">
       <c r="A12" s="22"/>
       <c r="B12" s="2" t="s">
-        <v>258</v>
+        <v>251</v>
       </c>
       <c r="C12" s="2" t="s">
-        <v>259</v>
+        <v>252</v>
       </c>
       <c r="D12" s="2" t="s">
         <v>73</v>
       </c>
       <c r="E12" s="2" t="s">
-        <v>120</v>
+        <v>114</v>
       </c>
       <c r="F12" s="2"/>
     </row>
     <row r="13" spans="1:9" ht="12.75" customHeight="1">
       <c r="A13" s="22"/>
       <c r="B13" s="19" t="s">
-        <v>418</v>
+        <v>411</v>
       </c>
       <c r="C13" s="19"/>
       <c r="D13" s="19"/>
       <c r="E13" s="19" t="s">
-        <v>424</v>
+        <v>417</v>
       </c>
       <c r="F13" s="19"/>
       <c r="G13" s="19"/>
@@ -3409,12 +3450,12 @@
     <row r="14" spans="1:9" ht="12.75" customHeight="1">
       <c r="A14" s="22"/>
       <c r="B14" s="19" t="s">
-        <v>419</v>
+        <v>412</v>
       </c>
       <c r="C14" s="19"/>
       <c r="D14" s="19"/>
       <c r="E14" s="19" t="s">
-        <v>261</v>
+        <v>254</v>
       </c>
       <c r="F14" s="19"/>
       <c r="G14" s="19"/>
@@ -3423,7 +3464,7 @@
     <row r="15" spans="1:9" s="12" customFormat="1" ht="18" customHeight="1">
       <c r="A15" s="23"/>
       <c r="B15" s="18" t="s">
-        <v>416</v>
+        <v>409</v>
       </c>
       <c r="C15" s="18"/>
       <c r="D15" s="18"/>
@@ -3435,110 +3476,110 @@
     <row r="16" spans="1:9" ht="12">
       <c r="A16" s="22"/>
       <c r="B16" t="s">
-        <v>215</v>
+        <v>209</v>
       </c>
       <c r="C16" t="s">
-        <v>121</v>
+        <v>115</v>
       </c>
       <c r="D16" t="s">
-        <v>260</v>
+        <v>253</v>
       </c>
       <c r="E16" s="2"/>
     </row>
     <row r="17" spans="1:10" ht="11" customHeight="1">
       <c r="A17" s="22"/>
       <c r="B17" t="s">
-        <v>134</v>
+        <v>128</v>
       </c>
       <c r="C17" t="s">
-        <v>135</v>
+        <v>129</v>
       </c>
       <c r="D17" t="s">
-        <v>136</v>
+        <v>130</v>
       </c>
       <c r="E17" s="2" t="s">
-        <v>137</v>
+        <v>131</v>
       </c>
     </row>
     <row r="18" spans="1:10" ht="11" customHeight="1">
       <c r="A18" s="22"/>
       <c r="B18" t="s">
-        <v>138</v>
+        <v>132</v>
       </c>
       <c r="C18" t="s">
-        <v>139</v>
+        <v>133</v>
       </c>
       <c r="D18" t="s">
-        <v>140</v>
+        <v>134</v>
       </c>
       <c r="E18" s="2" t="s">
-        <v>141</v>
+        <v>135</v>
       </c>
     </row>
     <row r="19" spans="1:10" ht="11" customHeight="1">
       <c r="A19" s="22"/>
       <c r="B19" t="s">
-        <v>155</v>
+        <v>149</v>
       </c>
       <c r="C19" t="s">
-        <v>156</v>
+        <v>150</v>
       </c>
       <c r="D19" t="s">
-        <v>157</v>
+        <v>151</v>
       </c>
       <c r="E19" s="2" t="s">
-        <v>158</v>
+        <v>152</v>
       </c>
     </row>
     <row r="20" spans="1:10" ht="11" customHeight="1">
       <c r="A20" s="22"/>
       <c r="B20" t="s">
-        <v>226</v>
+        <v>219</v>
       </c>
       <c r="C20" t="s">
-        <v>227</v>
+        <v>220</v>
       </c>
       <c r="D20" t="s">
-        <v>228</v>
+        <v>221</v>
       </c>
       <c r="E20" s="2" t="s">
-        <v>229</v>
+        <v>222</v>
       </c>
     </row>
     <row r="21" spans="1:10" ht="11" customHeight="1">
       <c r="A21" s="22"/>
       <c r="B21" t="s">
-        <v>159</v>
+        <v>153</v>
       </c>
       <c r="C21" t="s">
-        <v>160</v>
+        <v>154</v>
       </c>
       <c r="D21" t="s">
-        <v>161</v>
+        <v>155</v>
       </c>
       <c r="E21" s="2" t="s">
-        <v>211</v>
+        <v>205</v>
       </c>
     </row>
     <row r="22" spans="1:10" ht="11" customHeight="1">
       <c r="A22" s="22"/>
       <c r="B22" t="s">
-        <v>162</v>
+        <v>156</v>
       </c>
       <c r="C22" t="s">
-        <v>163</v>
+        <v>157</v>
       </c>
       <c r="D22" t="s">
-        <v>164</v>
+        <v>158</v>
       </c>
       <c r="E22" s="2" t="s">
-        <v>212</v>
+        <v>206</v>
       </c>
     </row>
     <row r="23" spans="1:10" ht="11" customHeight="1">
       <c r="A23" s="22"/>
       <c r="B23" s="20" t="s">
-        <v>417</v>
+        <v>410</v>
       </c>
       <c r="C23" s="20"/>
       <c r="D23" s="20"/>
@@ -3552,12 +3593,12 @@
     <row r="24" spans="1:10" ht="12.75" customHeight="1">
       <c r="A24" s="22"/>
       <c r="B24" s="19" t="s">
-        <v>420</v>
+        <v>413</v>
       </c>
       <c r="C24" s="19"/>
       <c r="D24" s="19"/>
       <c r="E24" s="19" t="s">
-        <v>425</v>
+        <v>418</v>
       </c>
       <c r="F24" s="19"/>
       <c r="G24" s="19"/>
@@ -3566,12 +3607,12 @@
     <row r="25" spans="1:10" ht="12.75" customHeight="1">
       <c r="A25" s="22"/>
       <c r="B25" s="19" t="s">
-        <v>421</v>
+        <v>414</v>
       </c>
       <c r="C25" s="19"/>
       <c r="D25" s="19"/>
       <c r="E25" s="19" t="s">
-        <v>265</v>
+        <v>258</v>
       </c>
       <c r="F25" s="19"/>
       <c r="G25" s="19"/>
@@ -3580,7 +3621,7 @@
     <row r="26" spans="1:10" s="12" customFormat="1" ht="18" customHeight="1">
       <c r="A26" s="23"/>
       <c r="B26" s="18" t="s">
-        <v>422</v>
+        <v>415</v>
       </c>
       <c r="C26" s="18"/>
       <c r="D26" s="18"/>
@@ -3592,110 +3633,110 @@
     <row r="27" spans="1:10" ht="11" customHeight="1">
       <c r="A27" s="22"/>
       <c r="B27" t="s">
-        <v>262</v>
+        <v>255</v>
       </c>
       <c r="C27" t="s">
-        <v>263</v>
+        <v>256</v>
       </c>
       <c r="D27" t="s">
-        <v>264</v>
+        <v>257</v>
       </c>
       <c r="E27" s="2"/>
     </row>
     <row r="28" spans="1:10" ht="11" customHeight="1">
       <c r="A28" s="22"/>
       <c r="B28" t="s">
-        <v>313</v>
+        <v>306</v>
       </c>
       <c r="C28" t="s">
-        <v>293</v>
+        <v>286</v>
       </c>
       <c r="D28" t="s">
-        <v>271</v>
+        <v>264</v>
       </c>
       <c r="E28" s="2" t="s">
-        <v>272</v>
+        <v>265</v>
       </c>
     </row>
     <row r="29" spans="1:10" ht="11" customHeight="1">
       <c r="A29" s="22"/>
       <c r="B29" t="s">
-        <v>314</v>
+        <v>307</v>
       </c>
       <c r="C29" t="s">
-        <v>294</v>
+        <v>287</v>
       </c>
       <c r="D29" t="s">
-        <v>283</v>
+        <v>276</v>
       </c>
       <c r="E29" s="2" t="s">
-        <v>274</v>
+        <v>267</v>
       </c>
     </row>
     <row r="30" spans="1:10" ht="11" customHeight="1">
       <c r="A30" s="22"/>
       <c r="B30" t="s">
-        <v>315</v>
+        <v>308</v>
       </c>
       <c r="C30" t="s">
-        <v>295</v>
+        <v>288</v>
       </c>
       <c r="D30" t="s">
-        <v>286</v>
+        <v>279</v>
       </c>
       <c r="E30" s="2" t="s">
-        <v>275</v>
+        <v>268</v>
       </c>
     </row>
     <row r="31" spans="1:10" ht="11" customHeight="1">
       <c r="A31" s="22"/>
       <c r="B31" t="s">
-        <v>316</v>
+        <v>309</v>
       </c>
       <c r="C31" t="s">
-        <v>296</v>
+        <v>289</v>
       </c>
       <c r="D31" t="s">
-        <v>284</v>
+        <v>277</v>
       </c>
       <c r="E31" s="2" t="s">
-        <v>278</v>
+        <v>271</v>
       </c>
     </row>
     <row r="32" spans="1:10" ht="11" customHeight="1">
       <c r="A32" s="22"/>
       <c r="B32" t="s">
-        <v>317</v>
+        <v>310</v>
       </c>
       <c r="C32" t="s">
-        <v>297</v>
+        <v>290</v>
       </c>
       <c r="D32" t="s">
-        <v>285</v>
+        <v>278</v>
       </c>
       <c r="E32" s="2" t="s">
-        <v>280</v>
+        <v>273</v>
       </c>
     </row>
     <row r="33" spans="1:10" ht="12" customHeight="1">
       <c r="A33" s="22"/>
       <c r="B33" t="s">
-        <v>318</v>
+        <v>311</v>
       </c>
       <c r="C33" t="s">
-        <v>298</v>
+        <v>291</v>
       </c>
       <c r="D33" t="s">
-        <v>287</v>
+        <v>280</v>
       </c>
       <c r="E33" s="2" t="s">
-        <v>282</v>
+        <v>275</v>
       </c>
     </row>
     <row r="34" spans="1:10" ht="12" customHeight="1">
       <c r="A34" s="22"/>
       <c r="B34" s="20" t="s">
-        <v>423</v>
+        <v>416</v>
       </c>
       <c r="C34" s="20"/>
       <c r="D34" s="20"/>
@@ -3714,7 +3755,7 @@
       <c r="C35" s="4"/>
       <c r="D35" s="2"/>
       <c r="E35" s="2" t="s">
-        <v>408</v>
+        <v>401</v>
       </c>
       <c r="F35" s="2"/>
     </row>
@@ -3725,7 +3766,7 @@
       </c>
       <c r="C36" s="4"/>
       <c r="D36" s="2" t="s">
-        <v>386</v>
+        <v>379</v>
       </c>
       <c r="E36" s="2"/>
       <c r="F36" s="2"/>
@@ -3736,7 +3777,7 @@
         <v>13</v>
       </c>
       <c r="D37" t="s">
-        <v>220</v>
+        <v>213</v>
       </c>
     </row>
     <row r="38" spans="1:10" ht="25" customHeight="1">
@@ -3745,7 +3786,7 @@
         <v>13</v>
       </c>
       <c r="D38" t="s">
-        <v>233</v>
+        <v>226</v>
       </c>
     </row>
     <row r="39" spans="1:10" ht="25" customHeight="1">
@@ -3754,7 +3795,7 @@
         <v>13</v>
       </c>
       <c r="D39" t="s">
-        <v>234</v>
+        <v>227</v>
       </c>
     </row>
     <row r="40" spans="1:10" ht="25" customHeight="1">
@@ -3763,7 +3804,7 @@
         <v>13</v>
       </c>
       <c r="D40" t="s">
-        <v>256</v>
+        <v>249</v>
       </c>
     </row>
     <row r="41" spans="1:10" ht="25" customHeight="1">
@@ -3772,7 +3813,7 @@
         <v>13</v>
       </c>
       <c r="D41" t="s">
-        <v>235</v>
+        <v>228</v>
       </c>
     </row>
     <row r="42" spans="1:10" ht="25" customHeight="1">
@@ -3781,7 +3822,7 @@
         <v>13</v>
       </c>
       <c r="D42" t="s">
-        <v>236</v>
+        <v>229</v>
       </c>
     </row>
     <row r="43" spans="1:10" ht="25" customHeight="1">
@@ -3790,7 +3831,7 @@
         <v>13</v>
       </c>
       <c r="D43" t="s">
-        <v>257</v>
+        <v>250</v>
       </c>
     </row>
     <row r="44" spans="1:10" ht="25" customHeight="1">
@@ -3799,7 +3840,7 @@
         <v>13</v>
       </c>
       <c r="D44" t="s">
-        <v>385</v>
+        <v>378</v>
       </c>
     </row>
     <row r="45" spans="1:10" ht="25" customHeight="1">
@@ -3808,7 +3849,7 @@
         <v>13</v>
       </c>
       <c r="D45" t="s">
-        <v>387</v>
+        <v>380</v>
       </c>
     </row>
     <row r="46" spans="1:10" ht="25" customHeight="1">
@@ -3817,7 +3858,7 @@
         <v>13</v>
       </c>
       <c r="D46" t="s">
-        <v>388</v>
+        <v>381</v>
       </c>
     </row>
     <row r="47" spans="1:10" ht="25" customHeight="1">
@@ -3826,7 +3867,7 @@
         <v>13</v>
       </c>
       <c r="D47" t="s">
-        <v>426</v>
+        <v>419</v>
       </c>
     </row>
     <row r="48" spans="1:10" ht="25" customHeight="1">
@@ -3835,7 +3876,7 @@
         <v>13</v>
       </c>
       <c r="D48" t="s">
-        <v>389</v>
+        <v>382</v>
       </c>
     </row>
     <row r="49" spans="1:10" ht="25" customHeight="1">
@@ -3844,7 +3885,7 @@
         <v>13</v>
       </c>
       <c r="D49" t="s">
-        <v>390</v>
+        <v>383</v>
       </c>
     </row>
     <row r="50" spans="1:10" ht="25" customHeight="1">
@@ -3853,7 +3894,7 @@
         <v>13</v>
       </c>
       <c r="D50" t="s">
-        <v>391</v>
+        <v>384</v>
       </c>
     </row>
     <row r="51" spans="1:10" ht="25" customHeight="1">
@@ -3862,7 +3903,7 @@
         <v>13</v>
       </c>
       <c r="D51" t="s">
-        <v>392</v>
+        <v>385</v>
       </c>
     </row>
     <row r="52" spans="1:10" ht="25" customHeight="1">
@@ -3871,7 +3912,7 @@
         <v>13</v>
       </c>
       <c r="D52" t="s">
-        <v>409</v>
+        <v>402</v>
       </c>
     </row>
     <row r="53" spans="1:10" ht="25" customHeight="1">
@@ -3903,10 +3944,10 @@
     </row>
     <row r="56" spans="1:10" s="15" customFormat="1" ht="15">
       <c r="A56" s="22" t="s">
-        <v>447</v>
+        <v>440</v>
       </c>
       <c r="B56" s="13" t="s">
-        <v>99</v>
+        <v>93</v>
       </c>
       <c r="C56" s="13"/>
       <c r="D56" s="13"/>
@@ -3936,7 +3977,7 @@
     <row r="58" spans="1:10" ht="15">
       <c r="A58" s="22"/>
       <c r="B58" s="15" t="s">
-        <v>98</v>
+        <v>92</v>
       </c>
       <c r="C58" s="15"/>
       <c r="D58" s="15"/>
@@ -3948,7 +3989,7 @@
     <row r="59" spans="1:10" ht="12">
       <c r="A59" s="22"/>
       <c r="B59" s="12" t="s">
-        <v>216</v>
+        <v>210</v>
       </c>
       <c r="C59" s="12" t="s">
         <v>9</v>
@@ -3986,7 +4027,7 @@
         <v>69</v>
       </c>
       <c r="D61" s="2" t="s">
-        <v>428</v>
+        <v>421</v>
       </c>
       <c r="E61" s="2"/>
       <c r="F61" s="4"/>
@@ -3997,7 +4038,7 @@
         <v>13</v>
       </c>
       <c r="D62" t="s">
-        <v>429</v>
+        <v>422</v>
       </c>
       <c r="E62" s="2"/>
       <c r="F62" s="4"/>
@@ -4009,7 +4050,7 @@
       </c>
       <c r="C63" s="2"/>
       <c r="D63" s="2" t="s">
-        <v>430</v>
+        <v>423</v>
       </c>
       <c r="E63" s="2"/>
       <c r="F63" s="4"/>
@@ -4021,7 +4062,7 @@
       </c>
       <c r="C64" s="2"/>
       <c r="D64" s="2" t="s">
-        <v>431</v>
+        <v>424</v>
       </c>
       <c r="E64" s="2"/>
       <c r="F64" s="4"/>
@@ -4033,7 +4074,7 @@
       </c>
       <c r="C65" s="2"/>
       <c r="D65" s="2" t="s">
-        <v>432</v>
+        <v>425</v>
       </c>
       <c r="E65" s="2"/>
       <c r="F65" s="4"/>
@@ -4045,7 +4086,7 @@
       </c>
       <c r="C66" s="2"/>
       <c r="D66" s="2" t="s">
-        <v>433</v>
+        <v>426</v>
       </c>
       <c r="E66" s="2"/>
       <c r="F66" s="4"/>
@@ -4057,7 +4098,7 @@
       </c>
       <c r="C67" s="2"/>
       <c r="D67" s="2" t="s">
-        <v>434</v>
+        <v>427</v>
       </c>
       <c r="E67" s="2"/>
       <c r="F67" s="4"/>
@@ -4069,7 +4110,7 @@
       </c>
       <c r="C68" s="2"/>
       <c r="D68" s="2" t="s">
-        <v>435</v>
+        <v>428</v>
       </c>
       <c r="E68" s="2"/>
       <c r="F68" s="4"/>
@@ -4081,7 +4122,7 @@
       </c>
       <c r="C69" s="2"/>
       <c r="D69" s="2" t="s">
-        <v>443</v>
+        <v>436</v>
       </c>
       <c r="E69" s="2"/>
       <c r="F69" s="4"/>
@@ -4093,7 +4134,7 @@
       </c>
       <c r="C70" s="2"/>
       <c r="D70" s="2" t="s">
-        <v>442</v>
+        <v>435</v>
       </c>
       <c r="E70" s="2"/>
       <c r="F70" s="4"/>
@@ -4105,7 +4146,7 @@
       </c>
       <c r="C71" s="2"/>
       <c r="D71" s="2" t="s">
-        <v>444</v>
+        <v>437</v>
       </c>
       <c r="E71" s="2"/>
       <c r="F71" s="4"/>
@@ -4117,7 +4158,7 @@
       </c>
       <c r="C72" s="2"/>
       <c r="D72" s="2" t="s">
-        <v>445</v>
+        <v>438</v>
       </c>
       <c r="E72" s="2"/>
       <c r="F72" s="4"/>
@@ -4129,7 +4170,7 @@
       </c>
       <c r="C73" s="2"/>
       <c r="D73" s="2" t="s">
-        <v>436</v>
+        <v>429</v>
       </c>
       <c r="E73" s="2"/>
       <c r="F73" s="4"/>
@@ -4141,7 +4182,7 @@
       </c>
       <c r="C74" s="2"/>
       <c r="D74" s="2" t="s">
-        <v>439</v>
+        <v>432</v>
       </c>
       <c r="E74" s="2"/>
       <c r="F74" s="4"/>
@@ -4153,7 +4194,7 @@
       </c>
       <c r="C75" s="2"/>
       <c r="D75" s="2" t="s">
-        <v>440</v>
+        <v>433</v>
       </c>
       <c r="E75" s="2"/>
       <c r="F75" s="4"/>
@@ -4165,7 +4206,7 @@
       </c>
       <c r="C76" s="2"/>
       <c r="D76" s="2" t="s">
-        <v>441</v>
+        <v>434</v>
       </c>
       <c r="E76" s="2"/>
       <c r="F76" s="4"/>
@@ -4177,7 +4218,7 @@
       </c>
       <c r="C77" s="2"/>
       <c r="D77" s="2" t="s">
-        <v>437</v>
+        <v>430</v>
       </c>
       <c r="E77" s="2"/>
       <c r="F77" s="4"/>
@@ -4189,7 +4230,7 @@
       </c>
       <c r="C78" s="2"/>
       <c r="D78" s="2" t="s">
-        <v>438</v>
+        <v>431</v>
       </c>
       <c r="E78" s="2"/>
       <c r="F78" s="4"/>
@@ -4201,7 +4242,7 @@
       </c>
       <c r="C79" s="2"/>
       <c r="D79" s="2" t="s">
-        <v>446</v>
+        <v>439</v>
       </c>
       <c r="E79" s="2"/>
       <c r="F79" s="4"/>
@@ -4273,23 +4314,23 @@
     <row r="86" spans="1:8" s="10" customFormat="1" ht="12"/>
     <row r="87" spans="1:8" s="10" customFormat="1" ht="15">
       <c r="B87" s="10" t="s">
-        <v>477</v>
+        <v>470</v>
       </c>
       <c r="E87" s="13" t="s">
-        <v>482</v>
+        <v>475</v>
       </c>
     </row>
     <row r="88" spans="1:8" s="10" customFormat="1" ht="15">
       <c r="B88" s="10" t="s">
-        <v>478</v>
+        <v>471</v>
       </c>
       <c r="E88" s="38" t="s">
-        <v>481</v>
+        <v>474</v>
       </c>
     </row>
     <row r="89" spans="1:8" s="10" customFormat="1" ht="12">
       <c r="B89" s="10" t="s">
-        <v>479</v>
+        <v>472</v>
       </c>
     </row>
     <row r="90" spans="1:8" s="10" customFormat="1" ht="12">
@@ -4302,19 +4343,19 @@
     </row>
     <row r="91" spans="1:8" s="10" customFormat="1" ht="12">
       <c r="B91" s="10" t="s">
-        <v>480</v>
+        <v>473</v>
       </c>
     </row>
     <row r="92" spans="1:8" s="10" customFormat="1" ht="12"/>
     <row r="93" spans="1:8" ht="30">
       <c r="A93" s="22"/>
       <c r="B93" s="13" t="s">
-        <v>452</v>
+        <v>445</v>
       </c>
       <c r="C93" s="13"/>
       <c r="D93" s="13"/>
       <c r="E93" s="13" t="s">
-        <v>448</v>
+        <v>441</v>
       </c>
       <c r="F93" s="13"/>
       <c r="G93" s="13"/>
@@ -4323,12 +4364,12 @@
     <row r="94" spans="1:8" ht="30">
       <c r="A94" s="22"/>
       <c r="B94" s="13" t="s">
-        <v>453</v>
+        <v>446</v>
       </c>
       <c r="C94" s="13"/>
       <c r="D94" s="13"/>
       <c r="E94" s="13" t="s">
-        <v>454</v>
+        <v>447</v>
       </c>
       <c r="F94" s="13"/>
       <c r="G94" s="13"/>
@@ -4337,7 +4378,7 @@
     <row r="95" spans="1:8" ht="15">
       <c r="A95" s="22"/>
       <c r="B95" s="15" t="s">
-        <v>450</v>
+        <v>443</v>
       </c>
       <c r="C95" s="15"/>
       <c r="D95" s="15"/>
@@ -4359,10 +4400,10 @@
     <row r="97" spans="1:8" ht="24">
       <c r="A97" s="22"/>
       <c r="B97" t="s">
-        <v>461</v>
+        <v>454</v>
       </c>
       <c r="C97" t="s">
-        <v>460</v>
+        <v>453</v>
       </c>
       <c r="F97" t="s">
         <v>6</v>
@@ -4373,12 +4414,12 @@
     <row r="98" spans="1:8" ht="30">
       <c r="A98" s="22"/>
       <c r="B98" s="13" t="s">
-        <v>466</v>
+        <v>459</v>
       </c>
       <c r="C98" s="13"/>
       <c r="D98" s="13"/>
       <c r="E98" s="13" t="s">
-        <v>463</v>
+        <v>456</v>
       </c>
       <c r="F98" s="13"/>
       <c r="G98" s="10"/>
@@ -4387,12 +4428,12 @@
     <row r="99" spans="1:8" ht="30">
       <c r="A99" s="22"/>
       <c r="B99" s="13" t="s">
-        <v>467</v>
+        <v>460</v>
       </c>
       <c r="C99" s="13"/>
       <c r="D99" s="13"/>
       <c r="E99" s="13" t="s">
-        <v>468</v>
+        <v>461</v>
       </c>
       <c r="F99" s="13"/>
       <c r="G99" s="10"/>
@@ -4401,7 +4442,7 @@
     <row r="100" spans="1:8" ht="15">
       <c r="A100" s="22"/>
       <c r="B100" s="15" t="s">
-        <v>464</v>
+        <v>457</v>
       </c>
       <c r="C100" s="15"/>
       <c r="D100" s="15"/>
@@ -4424,7 +4465,7 @@
       </c>
       <c r="C102" s="12"/>
       <c r="D102" s="26" t="s">
-        <v>475</v>
+        <v>468</v>
       </c>
       <c r="E102" s="12"/>
       <c r="F102" s="12"/>
@@ -4446,7 +4487,7 @@
     <row r="104" spans="1:8" ht="15">
       <c r="A104" s="22"/>
       <c r="B104" s="15" t="s">
-        <v>465</v>
+        <v>458</v>
       </c>
       <c r="C104" s="18"/>
       <c r="D104" s="32"/>
@@ -4458,24 +4499,24 @@
     <row r="105" spans="1:8" ht="30">
       <c r="A105" s="28"/>
       <c r="B105" s="13" t="s">
-        <v>470</v>
+        <v>463</v>
       </c>
       <c r="C105" s="13"/>
       <c r="D105" s="13"/>
       <c r="E105" s="13" t="s">
-        <v>462</v>
+        <v>455</v>
       </c>
       <c r="F105" s="13"/>
     </row>
     <row r="106" spans="1:8" ht="30">
       <c r="A106" s="28"/>
       <c r="B106" s="13" t="s">
-        <v>471</v>
+        <v>464</v>
       </c>
       <c r="C106" s="13"/>
       <c r="D106" s="13"/>
       <c r="E106" s="13" t="s">
-        <v>472</v>
+        <v>465</v>
       </c>
       <c r="F106" s="13"/>
     </row>
@@ -4485,7 +4526,7 @@
       </c>
       <c r="C107" s="27"/>
       <c r="D107" s="27" t="s">
-        <v>484</v>
+        <v>477</v>
       </c>
       <c r="E107" s="27"/>
       <c r="F107" s="27"/>
@@ -4493,7 +4534,7 @@
     <row r="108" spans="1:8" ht="15">
       <c r="A108" s="28"/>
       <c r="B108" s="15" t="s">
-        <v>473</v>
+        <v>466</v>
       </c>
       <c r="C108" s="15"/>
       <c r="D108" s="15"/>
@@ -4513,7 +4554,7 @@
       </c>
       <c r="C110" s="21"/>
       <c r="D110" s="29" t="s">
-        <v>469</v>
+        <v>462</v>
       </c>
       <c r="E110" s="29"/>
       <c r="F110" s="21"/>
@@ -4538,7 +4579,7 @@
     <row r="113" spans="1:9" ht="15">
       <c r="A113" s="28"/>
       <c r="B113" s="15" t="s">
-        <v>474</v>
+        <v>467</v>
       </c>
       <c r="C113" s="30"/>
       <c r="D113" s="31"/>
@@ -4551,7 +4592,7 @@
       </c>
       <c r="C114" s="34"/>
       <c r="D114" s="35" t="s">
-        <v>483</v>
+        <v>476</v>
       </c>
       <c r="E114" s="34"/>
       <c r="F114" s="34"/>
@@ -4559,7 +4600,7 @@
     <row r="115" spans="1:9" ht="15">
       <c r="A115" s="28"/>
       <c r="B115" s="15" t="s">
-        <v>451</v>
+        <v>444</v>
       </c>
       <c r="C115" s="30"/>
       <c r="D115" s="31"/>
@@ -4572,7 +4613,7 @@
       </c>
       <c r="C116" s="34"/>
       <c r="D116" s="35" t="s">
-        <v>485</v>
+        <v>478</v>
       </c>
       <c r="E116" s="34"/>
       <c r="F116" s="34"/>
@@ -4598,12 +4639,12 @@
     <row r="119" spans="1:9" s="13" customFormat="1" ht="15">
       <c r="A119" s="27"/>
       <c r="B119" s="13" t="s">
-        <v>103</v>
+        <v>97</v>
       </c>
       <c r="C119" s="36"/>
       <c r="D119" s="37"/>
       <c r="E119" s="14" t="s">
-        <v>476</v>
+        <v>469</v>
       </c>
       <c r="F119" s="36"/>
     </row>
@@ -4621,10 +4662,10 @@
     </row>
     <row r="121" spans="1:9" ht="15">
       <c r="A121" s="22" t="s">
-        <v>458</v>
+        <v>451</v>
       </c>
       <c r="B121" s="15" t="s">
-        <v>104</v>
+        <v>98</v>
       </c>
       <c r="C121" s="15"/>
       <c r="D121" s="15"/>
@@ -4636,7 +4677,7 @@
     <row r="122" spans="1:9" ht="12">
       <c r="A122" s="22"/>
       <c r="B122" t="s">
-        <v>217</v>
+        <v>211</v>
       </c>
       <c r="C122" t="s">
         <v>11</v>
@@ -4656,7 +4697,7 @@
         <v>15</v>
       </c>
       <c r="E123" t="s">
-        <v>487</v>
+        <v>480</v>
       </c>
     </row>
     <row r="124" spans="1:9" ht="12">
@@ -4671,13 +4712,13 @@
     <row r="125" spans="1:9" ht="12">
       <c r="A125" s="22"/>
       <c r="B125" t="s">
-        <v>488</v>
+        <v>481</v>
       </c>
       <c r="C125" t="s">
-        <v>489</v>
+        <v>482</v>
       </c>
       <c r="D125" t="s">
-        <v>490</v>
+        <v>483</v>
       </c>
       <c r="F125" t="s">
         <v>81</v>
@@ -4689,10 +4730,10 @@
         <v>15</v>
       </c>
       <c r="C126" t="s">
-        <v>522</v>
+        <v>515</v>
       </c>
       <c r="E126" t="s">
-        <v>523</v>
+        <v>516</v>
       </c>
     </row>
     <row r="127" spans="1:9" ht="12.75" customHeight="1">
@@ -4701,10 +4742,10 @@
         <v>16</v>
       </c>
       <c r="C127" t="s">
-        <v>524</v>
+        <v>517</v>
       </c>
       <c r="D127" t="s">
-        <v>492</v>
+        <v>485</v>
       </c>
     </row>
     <row r="128" spans="1:9" ht="12.75" customHeight="1">
@@ -4713,10 +4754,10 @@
         <v>13</v>
       </c>
       <c r="D128" t="s">
-        <v>528</v>
+        <v>521</v>
       </c>
       <c r="E128" t="s">
-        <v>525</v>
+        <v>518</v>
       </c>
       <c r="I128" s="21"/>
     </row>
@@ -4732,7 +4773,7 @@
         <v>15</v>
       </c>
       <c r="E130" t="s">
-        <v>491</v>
+        <v>484</v>
       </c>
     </row>
     <row r="131" spans="1:9" ht="12">
@@ -4744,7 +4785,7 @@
         <v>20</v>
       </c>
       <c r="D131" t="s">
-        <v>492</v>
+        <v>485</v>
       </c>
     </row>
     <row r="132" spans="1:9" ht="12.75" customHeight="1">
@@ -4772,7 +4813,7 @@
         <v>15</v>
       </c>
       <c r="E134" t="s">
-        <v>493</v>
+        <v>486</v>
       </c>
     </row>
     <row r="135" spans="1:9" ht="12.75" customHeight="1">
@@ -4784,7 +4825,7 @@
         <v>17</v>
       </c>
       <c r="D135" t="s">
-        <v>494</v>
+        <v>487</v>
       </c>
     </row>
     <row r="136" spans="1:9" ht="12.75" customHeight="1">
@@ -4817,7 +4858,7 @@
         <v>15</v>
       </c>
       <c r="E139" t="s">
-        <v>495</v>
+        <v>488</v>
       </c>
     </row>
     <row r="140" spans="1:9" ht="12.75" customHeight="1">
@@ -4835,10 +4876,10 @@
         <v>16</v>
       </c>
       <c r="C141" t="s">
-        <v>496</v>
+        <v>489</v>
       </c>
       <c r="D141" t="s">
-        <v>497</v>
+        <v>490</v>
       </c>
     </row>
     <row r="142" spans="1:9" ht="12.75" customHeight="1">
@@ -4847,10 +4888,10 @@
         <v>16</v>
       </c>
       <c r="C142" t="s">
-        <v>498</v>
+        <v>491</v>
       </c>
       <c r="D142" t="s">
-        <v>499</v>
+        <v>492</v>
       </c>
     </row>
     <row r="143" spans="1:9" ht="12.75" customHeight="1">
@@ -4859,10 +4900,10 @@
         <v>13</v>
       </c>
       <c r="D143" t="s">
-        <v>500</v>
+        <v>493</v>
       </c>
       <c r="E143" t="s">
-        <v>501</v>
+        <v>494</v>
       </c>
     </row>
     <row r="144" spans="1:9" ht="12.75" customHeight="1">
@@ -4871,10 +4912,10 @@
         <v>13</v>
       </c>
       <c r="D144" t="s">
-        <v>502</v>
+        <v>495</v>
       </c>
       <c r="E144" t="s">
-        <v>501</v>
+        <v>494</v>
       </c>
     </row>
     <row r="145" spans="1:10" ht="12.75" customHeight="1">
@@ -4883,10 +4924,10 @@
         <v>13</v>
       </c>
       <c r="D145" t="s">
-        <v>503</v>
+        <v>496</v>
       </c>
       <c r="E145" t="s">
-        <v>501</v>
+        <v>494</v>
       </c>
     </row>
     <row r="146" spans="1:10" ht="12.75" customHeight="1">
@@ -4901,7 +4942,7 @@
         <v>15</v>
       </c>
       <c r="E147" t="s">
-        <v>504</v>
+        <v>497</v>
       </c>
     </row>
     <row r="148" spans="1:10" ht="12.75" customHeight="1">
@@ -4910,7 +4951,7 @@
         <v>13</v>
       </c>
       <c r="D148" t="s">
-        <v>107</v>
+        <v>101</v>
       </c>
     </row>
     <row r="149" spans="1:10" ht="12.75" customHeight="1">
@@ -4919,10 +4960,10 @@
         <v>16</v>
       </c>
       <c r="C149" t="s">
-        <v>505</v>
+        <v>498</v>
       </c>
       <c r="D149" t="s">
-        <v>506</v>
+        <v>499</v>
       </c>
     </row>
     <row r="150" spans="1:10" ht="12.75" customHeight="1">
@@ -4931,10 +4972,10 @@
         <v>16</v>
       </c>
       <c r="C150" t="s">
-        <v>507</v>
+        <v>500</v>
       </c>
       <c r="D150" t="s">
-        <v>508</v>
+        <v>501</v>
       </c>
     </row>
     <row r="151" spans="1:10" ht="12.75" customHeight="1">
@@ -4943,10 +4984,10 @@
         <v>13</v>
       </c>
       <c r="D151" t="s">
-        <v>509</v>
+        <v>502</v>
       </c>
       <c r="E151" t="s">
-        <v>510</v>
+        <v>503</v>
       </c>
     </row>
     <row r="152" spans="1:10" ht="12.75" customHeight="1">
@@ -4971,10 +5012,10 @@
     <row r="155" spans="1:10" s="14" customFormat="1" ht="12.75" customHeight="1">
       <c r="A155" s="25"/>
       <c r="B155" s="13" t="s">
-        <v>105</v>
+        <v>99</v>
       </c>
       <c r="E155" s="14" t="s">
-        <v>106</v>
+        <v>100</v>
       </c>
       <c r="I155" s="12"/>
       <c r="J155" s="12"/>
@@ -4994,10 +5035,10 @@
     </row>
     <row r="157" spans="1:10" ht="12.75" customHeight="1">
       <c r="A157" s="22" t="s">
-        <v>459</v>
+        <v>452</v>
       </c>
       <c r="B157" s="15" t="s">
-        <v>117</v>
+        <v>111</v>
       </c>
       <c r="C157" s="18"/>
       <c r="D157" s="18"/>
@@ -5008,411 +5049,460 @@
     </row>
     <row r="158" spans="1:10" ht="12.75" customHeight="1">
       <c r="A158" s="22"/>
-      <c r="B158" s="2" t="s">
-        <v>218</v>
-      </c>
-      <c r="C158" s="12" t="s">
-        <v>79</v>
-      </c>
-      <c r="D158" s="12" t="s">
-        <v>80</v>
-      </c>
-      <c r="E158" s="12"/>
-      <c r="F158" s="12" t="s">
-        <v>81</v>
-      </c>
-      <c r="G158" s="12"/>
+      <c r="B158" s="43" t="s">
+        <v>15</v>
+      </c>
       <c r="H158" s="12"/>
     </row>
     <row r="159" spans="1:10" ht="12.75" customHeight="1">
       <c r="A159" s="22"/>
-      <c r="B159" s="15" t="s">
+      <c r="B159" t="s">
+        <v>527</v>
+      </c>
+      <c r="C159" t="s">
+        <v>79</v>
+      </c>
+      <c r="D159" t="s">
+        <v>522</v>
+      </c>
+      <c r="F159" t="s">
+        <v>81</v>
+      </c>
+    </row>
+    <row r="160" spans="1:10" ht="12.75" customHeight="1">
+      <c r="A160" s="22"/>
+      <c r="B160" t="s">
+        <v>13</v>
+      </c>
+      <c r="C160" t="s">
+        <v>523</v>
+      </c>
+      <c r="E160" t="s">
+        <v>528</v>
+      </c>
+      <c r="I160" t="s">
+        <v>524</v>
+      </c>
+    </row>
+    <row r="161" spans="1:9" ht="12.75" customHeight="1">
+      <c r="A161" s="22"/>
+      <c r="B161" t="s">
+        <v>13</v>
+      </c>
+      <c r="D161" t="s">
+        <v>525</v>
+      </c>
+      <c r="E161" t="s">
+        <v>529</v>
+      </c>
+    </row>
+    <row r="162" spans="1:9" ht="12.75" customHeight="1">
+      <c r="A162" s="22"/>
+      <c r="B162" t="s">
+        <v>13</v>
+      </c>
+      <c r="D162" t="s">
+        <v>526</v>
+      </c>
+      <c r="E162" t="s">
+        <v>530</v>
+      </c>
+    </row>
+    <row r="163" spans="1:9" ht="12.75" customHeight="1">
+      <c r="A163" s="22"/>
+      <c r="B163" s="44" t="s">
+        <v>23</v>
+      </c>
+    </row>
+    <row r="164" spans="1:9" ht="12.75" customHeight="1">
+      <c r="A164" s="22"/>
+      <c r="B164" s="15" t="s">
         <v>82</v>
       </c>
-      <c r="C159" s="18"/>
-      <c r="D159" s="18"/>
-      <c r="E159" s="18"/>
-      <c r="F159" s="18"/>
-      <c r="G159" s="18"/>
-      <c r="H159" s="18"/>
-    </row>
-    <row r="161" spans="1:9" ht="12.75" customHeight="1">
-      <c r="B161" s="13" t="s">
-        <v>108</v>
-      </c>
-      <c r="C161" s="14"/>
-      <c r="D161" s="14"/>
-      <c r="E161" s="14" t="s">
-        <v>110</v>
-      </c>
-      <c r="F161" s="14"/>
-      <c r="G161" s="14"/>
-      <c r="H161" s="14"/>
-    </row>
-    <row r="162" spans="1:9" ht="12.75" customHeight="1">
-      <c r="B162" s="13" t="s">
-        <v>109</v>
-      </c>
-      <c r="C162" s="14"/>
-      <c r="D162" s="14"/>
-      <c r="E162" s="14" t="s">
-        <v>111</v>
-      </c>
-      <c r="F162" s="14"/>
-      <c r="G162" s="14"/>
-      <c r="H162" s="14"/>
-    </row>
-    <row r="163" spans="1:9" ht="12.75" customHeight="1">
-      <c r="A163" s="22" t="s">
+      <c r="C164" s="18"/>
+      <c r="D164" s="18"/>
+      <c r="E164" s="18"/>
+      <c r="F164" s="18"/>
+      <c r="G164" s="18"/>
+      <c r="H164" s="18"/>
+    </row>
+    <row r="166" spans="1:9" ht="12.75" customHeight="1">
+      <c r="B166" s="13" t="s">
+        <v>102</v>
+      </c>
+      <c r="C166" s="14"/>
+      <c r="D166" s="14"/>
+      <c r="E166" s="14" t="s">
+        <v>104</v>
+      </c>
+      <c r="F166" s="14"/>
+      <c r="G166" s="14"/>
+      <c r="H166" s="14"/>
+    </row>
+    <row r="167" spans="1:9" ht="12.75" customHeight="1">
+      <c r="B167" s="13" t="s">
+        <v>103</v>
+      </c>
+      <c r="C167" s="14"/>
+      <c r="D167" s="14"/>
+      <c r="E167" s="14" t="s">
+        <v>105</v>
+      </c>
+      <c r="F167" s="14"/>
+      <c r="G167" s="14"/>
+      <c r="H167" s="14"/>
+    </row>
+    <row r="168" spans="1:9" ht="12.75" customHeight="1">
+      <c r="A168" s="22" t="s">
         <v>58</v>
       </c>
-      <c r="B163" s="15" t="s">
-        <v>118</v>
-      </c>
-      <c r="C163" s="18"/>
-      <c r="D163" s="18"/>
-      <c r="E163" s="18"/>
-      <c r="F163" s="18"/>
-      <c r="G163" s="18"/>
-      <c r="H163" s="18"/>
-    </row>
-    <row r="164" spans="1:9" ht="12.75" customHeight="1">
-      <c r="A164" s="28"/>
-      <c r="B164" t="s">
-        <v>217</v>
-      </c>
-      <c r="C164" t="s">
-        <v>11</v>
-      </c>
-      <c r="D164" t="s">
-        <v>61</v>
-      </c>
-      <c r="F164" t="s">
-        <v>6</v>
-      </c>
-      <c r="G164" s="21"/>
-      <c r="H164" s="21"/>
-    </row>
-    <row r="165" spans="1:9" ht="12.75" customHeight="1">
-      <c r="A165" s="28"/>
-      <c r="B165" s="39" t="s">
-        <v>15</v>
-      </c>
-      <c r="E165" t="s">
-        <v>487</v>
-      </c>
-    </row>
-    <row r="166" spans="1:9" ht="12.75" customHeight="1">
-      <c r="A166" s="28"/>
-      <c r="B166" t="s">
-        <v>13</v>
-      </c>
-      <c r="D166" t="s">
-        <v>41</v>
-      </c>
-    </row>
-    <row r="167" spans="1:9" ht="12.75" customHeight="1">
-      <c r="A167" s="28"/>
-      <c r="B167" t="s">
-        <v>488</v>
-      </c>
-      <c r="C167" t="s">
-        <v>489</v>
-      </c>
-      <c r="D167" t="s">
-        <v>490</v>
-      </c>
-      <c r="F167" t="s">
-        <v>81</v>
-      </c>
-    </row>
-    <row r="168" spans="1:9" ht="12.75" customHeight="1">
-      <c r="A168" s="28"/>
-      <c r="B168" s="39" t="s">
-        <v>15</v>
-      </c>
-      <c r="C168" t="s">
-        <v>522</v>
-      </c>
-      <c r="E168" t="s">
-        <v>523</v>
-      </c>
+      <c r="B168" s="15" t="s">
+        <v>112</v>
+      </c>
+      <c r="C168" s="18"/>
+      <c r="D168" s="18"/>
+      <c r="E168" s="18"/>
+      <c r="F168" s="18"/>
+      <c r="G168" s="18"/>
+      <c r="H168" s="18"/>
     </row>
     <row r="169" spans="1:9" ht="12.75" customHeight="1">
       <c r="A169" s="28"/>
       <c r="B169" t="s">
-        <v>16</v>
+        <v>211</v>
       </c>
       <c r="C169" t="s">
-        <v>524</v>
+        <v>11</v>
       </c>
       <c r="D169" t="s">
-        <v>492</v>
-      </c>
+        <v>61</v>
+      </c>
+      <c r="F169" t="s">
+        <v>6</v>
+      </c>
+      <c r="G169" s="21"/>
+      <c r="H169" s="21"/>
     </row>
     <row r="170" spans="1:9" ht="12.75" customHeight="1">
       <c r="A170" s="28"/>
-      <c r="B170" t="s">
-        <v>13</v>
-      </c>
-      <c r="D170" t="s">
-        <v>528</v>
+      <c r="B170" s="39" t="s">
+        <v>15</v>
       </c>
       <c r="E170" t="s">
-        <v>525</v>
-      </c>
-      <c r="I170" s="21"/>
+        <v>480</v>
+      </c>
     </row>
     <row r="171" spans="1:9" ht="12.75" customHeight="1">
       <c r="A171" s="28"/>
-      <c r="B171" s="40" t="s">
-        <v>23</v>
+      <c r="B171" t="s">
+        <v>13</v>
+      </c>
+      <c r="D171" t="s">
+        <v>41</v>
       </c>
     </row>
     <row r="172" spans="1:9" ht="12.75" customHeight="1">
       <c r="A172" s="28"/>
-      <c r="B172" s="39" t="s">
-        <v>15</v>
-      </c>
-      <c r="E172" t="s">
-        <v>491</v>
+      <c r="B172" t="s">
+        <v>481</v>
+      </c>
+      <c r="C172" t="s">
+        <v>482</v>
+      </c>
+      <c r="D172" t="s">
+        <v>483</v>
+      </c>
+      <c r="F172" t="s">
+        <v>81</v>
       </c>
     </row>
     <row r="173" spans="1:9" ht="12.75" customHeight="1">
       <c r="A173" s="28"/>
-      <c r="B173" t="s">
-        <v>16</v>
+      <c r="B173" s="39" t="s">
+        <v>15</v>
       </c>
       <c r="C173" t="s">
-        <v>20</v>
-      </c>
-      <c r="D173" t="s">
-        <v>492</v>
+        <v>515</v>
+      </c>
+      <c r="E173" t="s">
+        <v>516</v>
       </c>
     </row>
     <row r="174" spans="1:9" ht="12.75" customHeight="1">
       <c r="A174" s="28"/>
       <c r="B174" t="s">
-        <v>13</v>
+        <v>16</v>
+      </c>
+      <c r="C174" t="s">
+        <v>517</v>
       </c>
       <c r="D174" t="s">
-        <v>21</v>
-      </c>
-      <c r="E174" t="s">
-        <v>22</v>
-      </c>
-      <c r="I174" s="21"/>
+        <v>485</v>
+      </c>
     </row>
     <row r="175" spans="1:9" ht="12.75" customHeight="1">
       <c r="A175" s="28"/>
-      <c r="B175" s="40" t="s">
-        <v>23</v>
-      </c>
+      <c r="B175" t="s">
+        <v>13</v>
+      </c>
+      <c r="D175" t="s">
+        <v>521</v>
+      </c>
+      <c r="E175" t="s">
+        <v>518</v>
+      </c>
+      <c r="I175" s="21"/>
     </row>
     <row r="176" spans="1:9" ht="12.75" customHeight="1">
       <c r="A176" s="28"/>
-      <c r="B176" s="39" t="s">
+      <c r="B176" s="40" t="s">
+        <v>23</v>
+      </c>
+    </row>
+    <row r="177" spans="1:9" ht="12.75" customHeight="1">
+      <c r="A177" s="28"/>
+      <c r="B177" s="39" t="s">
         <v>15</v>
       </c>
-      <c r="E176" t="s">
-        <v>493</v>
-      </c>
-    </row>
-    <row r="177" spans="1:5" ht="12.75" customHeight="1">
-      <c r="A177" s="28"/>
-      <c r="B177" t="s">
-        <v>16</v>
-      </c>
-      <c r="C177" t="s">
-        <v>17</v>
-      </c>
-      <c r="D177" t="s">
-        <v>494</v>
-      </c>
-    </row>
-    <row r="178" spans="1:5" ht="12.75" customHeight="1">
+      <c r="E177" t="s">
+        <v>484</v>
+      </c>
+    </row>
+    <row r="178" spans="1:9" ht="12.75" customHeight="1">
       <c r="A178" s="28"/>
       <c r="B178" t="s">
+        <v>16</v>
+      </c>
+      <c r="C178" t="s">
+        <v>20</v>
+      </c>
+      <c r="D178" t="s">
+        <v>485</v>
+      </c>
+    </row>
+    <row r="179" spans="1:9" ht="12.75" customHeight="1">
+      <c r="A179" s="28"/>
+      <c r="B179" t="s">
         <v>13</v>
       </c>
-      <c r="D178" t="s">
-        <v>18</v>
-      </c>
-      <c r="E178" t="s">
-        <v>19</v>
-      </c>
-    </row>
-    <row r="179" spans="1:5" ht="12.75" customHeight="1">
-      <c r="A179" s="28"/>
-      <c r="B179" s="40" t="s">
-        <v>23</v>
-      </c>
-    </row>
-    <row r="180" spans="1:5" ht="12.75" customHeight="1">
+      <c r="D179" t="s">
+        <v>21</v>
+      </c>
+      <c r="E179" t="s">
+        <v>22</v>
+      </c>
+      <c r="I179" s="21"/>
+    </row>
+    <row r="180" spans="1:9" ht="12.75" customHeight="1">
       <c r="A180" s="28"/>
       <c r="B180" s="40" t="s">
         <v>23</v>
       </c>
     </row>
-    <row r="181" spans="1:5" ht="12.75" customHeight="1">
+    <row r="181" spans="1:9" ht="12.75" customHeight="1">
       <c r="A181" s="28"/>
-      <c r="B181" s="41" t="s">
+      <c r="B181" s="39" t="s">
         <v>15</v>
       </c>
       <c r="E181" t="s">
-        <v>495</v>
-      </c>
-    </row>
-    <row r="182" spans="1:5" ht="12.75" customHeight="1">
+        <v>486</v>
+      </c>
+    </row>
+    <row r="182" spans="1:9" ht="12.75" customHeight="1">
       <c r="A182" s="28"/>
       <c r="B182" t="s">
-        <v>13</v>
+        <v>16</v>
+      </c>
+      <c r="C182" t="s">
+        <v>17</v>
       </c>
       <c r="D182" t="s">
-        <v>43</v>
-      </c>
-    </row>
-    <row r="183" spans="1:5" ht="12.75" customHeight="1">
+        <v>487</v>
+      </c>
+    </row>
+    <row r="183" spans="1:9" ht="12.75" customHeight="1">
       <c r="A183" s="28"/>
       <c r="B183" t="s">
-        <v>16</v>
-      </c>
-      <c r="C183" t="s">
-        <v>496</v>
+        <v>13</v>
       </c>
       <c r="D183" t="s">
-        <v>497</v>
-      </c>
-    </row>
-    <row r="184" spans="1:5" ht="12.75" customHeight="1">
+        <v>18</v>
+      </c>
+      <c r="E183" t="s">
+        <v>19</v>
+      </c>
+    </row>
+    <row r="184" spans="1:9" ht="12.75" customHeight="1">
       <c r="A184" s="28"/>
-      <c r="B184" t="s">
-        <v>16</v>
-      </c>
-      <c r="C184" t="s">
-        <v>498</v>
-      </c>
-      <c r="D184" t="s">
-        <v>499</v>
-      </c>
-    </row>
-    <row r="185" spans="1:5" ht="12.75" customHeight="1">
+      <c r="B184" s="40" t="s">
+        <v>23</v>
+      </c>
+    </row>
+    <row r="185" spans="1:9" ht="12.75" customHeight="1">
       <c r="A185" s="28"/>
-      <c r="B185" t="s">
-        <v>13</v>
-      </c>
-      <c r="D185" t="s">
-        <v>500</v>
-      </c>
-      <c r="E185" t="s">
-        <v>501</v>
-      </c>
-    </row>
-    <row r="186" spans="1:5" ht="12.75" customHeight="1">
+      <c r="B185" s="40" t="s">
+        <v>23</v>
+      </c>
+    </row>
+    <row r="186" spans="1:9" ht="12.75" customHeight="1">
       <c r="A186" s="28"/>
-      <c r="B186" t="s">
-        <v>13</v>
-      </c>
-      <c r="D186" t="s">
-        <v>502</v>
+      <c r="B186" s="41" t="s">
+        <v>15</v>
       </c>
       <c r="E186" t="s">
-        <v>501</v>
-      </c>
-    </row>
-    <row r="187" spans="1:5" ht="12.75" customHeight="1">
+        <v>488</v>
+      </c>
+    </row>
+    <row r="187" spans="1:9" ht="12.75" customHeight="1">
       <c r="A187" s="28"/>
       <c r="B187" t="s">
         <v>13</v>
       </c>
       <c r="D187" t="s">
-        <v>503</v>
-      </c>
-      <c r="E187" t="s">
-        <v>501</v>
-      </c>
-    </row>
-    <row r="188" spans="1:5" ht="12.75" customHeight="1">
+        <v>43</v>
+      </c>
+    </row>
+    <row r="188" spans="1:9" ht="12.75" customHeight="1">
       <c r="A188" s="28"/>
-      <c r="B188" s="42" t="s">
-        <v>23</v>
-      </c>
-    </row>
-    <row r="189" spans="1:5" ht="12.75" customHeight="1">
+      <c r="B188" t="s">
+        <v>16</v>
+      </c>
+      <c r="C188" t="s">
+        <v>489</v>
+      </c>
+      <c r="D188" t="s">
+        <v>490</v>
+      </c>
+    </row>
+    <row r="189" spans="1:9" ht="12.75" customHeight="1">
       <c r="A189" s="28"/>
-      <c r="B189" s="41" t="s">
-        <v>15</v>
-      </c>
-      <c r="E189" t="s">
-        <v>504</v>
-      </c>
-    </row>
-    <row r="190" spans="1:5" ht="12.75" customHeight="1">
+      <c r="B189" t="s">
+        <v>16</v>
+      </c>
+      <c r="C189" t="s">
+        <v>491</v>
+      </c>
+      <c r="D189" t="s">
+        <v>492</v>
+      </c>
+    </row>
+    <row r="190" spans="1:9" ht="12.75" customHeight="1">
       <c r="A190" s="28"/>
       <c r="B190" t="s">
         <v>13</v>
       </c>
       <c r="D190" t="s">
-        <v>107</v>
-      </c>
-    </row>
-    <row r="191" spans="1:5" ht="12.75" customHeight="1">
+        <v>493</v>
+      </c>
+      <c r="E190" t="s">
+        <v>494</v>
+      </c>
+    </row>
+    <row r="191" spans="1:9" ht="12.75" customHeight="1">
       <c r="A191" s="28"/>
       <c r="B191" t="s">
-        <v>16</v>
-      </c>
-      <c r="C191" t="s">
-        <v>505</v>
+        <v>13</v>
       </c>
       <c r="D191" t="s">
-        <v>506</v>
-      </c>
-    </row>
-    <row r="192" spans="1:5" ht="12.75" customHeight="1">
+        <v>495</v>
+      </c>
+      <c r="E191" t="s">
+        <v>494</v>
+      </c>
+    </row>
+    <row r="192" spans="1:9" ht="12.75" customHeight="1">
       <c r="A192" s="28"/>
       <c r="B192" t="s">
-        <v>16</v>
-      </c>
-      <c r="C192" t="s">
-        <v>507</v>
+        <v>13</v>
       </c>
       <c r="D192" t="s">
-        <v>508</v>
+        <v>496</v>
+      </c>
+      <c r="E192" t="s">
+        <v>494</v>
       </c>
     </row>
     <row r="193" spans="1:8" ht="12.75" customHeight="1">
       <c r="A193" s="28"/>
-      <c r="B193" t="s">
-        <v>13</v>
-      </c>
-      <c r="D193" t="s">
-        <v>509</v>
-      </c>
-      <c r="E193" t="s">
-        <v>510</v>
+      <c r="B193" s="42" t="s">
+        <v>23</v>
       </c>
     </row>
     <row r="194" spans="1:8" ht="12.75" customHeight="1">
       <c r="A194" s="28"/>
-      <c r="B194" s="42" t="s">
+      <c r="B194" s="41" t="s">
+        <v>15</v>
+      </c>
+      <c r="E194" t="s">
+        <v>497</v>
+      </c>
+    </row>
+    <row r="195" spans="1:8" ht="12.75" customHeight="1">
+      <c r="A195" s="28"/>
+      <c r="B195" t="s">
+        <v>13</v>
+      </c>
+      <c r="D195" t="s">
+        <v>101</v>
+      </c>
+    </row>
+    <row r="196" spans="1:8" ht="12.75" customHeight="1">
+      <c r="A196" s="28"/>
+      <c r="B196" t="s">
+        <v>16</v>
+      </c>
+      <c r="C196" t="s">
+        <v>498</v>
+      </c>
+      <c r="D196" t="s">
+        <v>499</v>
+      </c>
+    </row>
+    <row r="197" spans="1:8" ht="12.75" customHeight="1">
+      <c r="A197" s="28"/>
+      <c r="B197" t="s">
+        <v>16</v>
+      </c>
+      <c r="C197" t="s">
+        <v>500</v>
+      </c>
+      <c r="D197" t="s">
+        <v>501</v>
+      </c>
+    </row>
+    <row r="198" spans="1:8" ht="12.75" customHeight="1">
+      <c r="A198" s="28"/>
+      <c r="B198" t="s">
+        <v>13</v>
+      </c>
+      <c r="D198" t="s">
+        <v>502</v>
+      </c>
+      <c r="E198" t="s">
+        <v>503</v>
+      </c>
+    </row>
+    <row r="199" spans="1:8" ht="12.75" customHeight="1">
+      <c r="A199" s="28"/>
+      <c r="B199" s="42" t="s">
         <v>23</v>
       </c>
     </row>
-    <row r="195" spans="1:8" ht="12.75" customHeight="1">
-      <c r="A195" s="22"/>
-      <c r="B195" s="15" t="s">
-        <v>112</v>
-      </c>
-      <c r="C195" s="18"/>
-      <c r="D195" s="18"/>
-      <c r="E195" s="18"/>
-      <c r="F195" s="18"/>
-      <c r="G195" s="18"/>
-      <c r="H195" s="18"/>
-    </row>
-    <row r="198" spans="1:8" ht="12.75" customHeight="1">
-      <c r="B198" s="17" t="s">
-        <v>101</v>
+    <row r="200" spans="1:8" ht="12.75" customHeight="1">
+      <c r="A200" s="22"/>
+      <c r="B200" s="15" t="s">
+        <v>106</v>
+      </c>
+      <c r="C200" s="18"/>
+      <c r="D200" s="18"/>
+      <c r="E200" s="18"/>
+      <c r="F200" s="18"/>
+      <c r="G200" s="18"/>
+      <c r="H200" s="18"/>
+    </row>
+    <row r="203" spans="1:8" ht="12.75" customHeight="1">
+      <c r="B203" s="17" t="s">
+        <v>95</v>
       </c>
     </row>
   </sheetData>
@@ -5465,154 +5555,154 @@
     </row>
     <row r="4" spans="1:2" ht="12.75" customHeight="1">
       <c r="A4" t="s">
-        <v>526</v>
+        <v>519</v>
       </c>
       <c r="B4" t="s">
-        <v>527</v>
+        <v>520</v>
       </c>
     </row>
     <row r="5" spans="1:2" ht="12.75" customHeight="1">
       <c r="A5" t="s">
-        <v>515</v>
+        <v>508</v>
       </c>
       <c r="B5" t="s">
-        <v>517</v>
+        <v>510</v>
       </c>
     </row>
     <row r="6" spans="1:2" ht="12.75" customHeight="1">
       <c r="A6" t="s">
-        <v>516</v>
+        <v>509</v>
       </c>
       <c r="B6" t="s">
-        <v>518</v>
+        <v>511</v>
       </c>
     </row>
     <row r="7" spans="1:2" ht="12.75" customHeight="1">
       <c r="A7" t="s">
-        <v>519</v>
+        <v>512</v>
       </c>
       <c r="B7" t="s">
-        <v>521</v>
+        <v>514</v>
       </c>
     </row>
     <row r="9" spans="1:2" ht="12" customHeight="1">
       <c r="A9" t="s">
-        <v>219</v>
+        <v>212</v>
       </c>
       <c r="B9" t="s">
-        <v>221</v>
+        <v>214</v>
       </c>
     </row>
     <row r="10" spans="1:2" ht="12" customHeight="1">
       <c r="A10" t="s">
-        <v>222</v>
+        <v>215</v>
       </c>
       <c r="B10" t="s">
-        <v>237</v>
+        <v>230</v>
       </c>
     </row>
     <row r="11" spans="1:2" ht="12" customHeight="1">
       <c r="A11" t="s">
+        <v>216</v>
+      </c>
+      <c r="B11" t="s">
         <v>223</v>
-      </c>
-      <c r="B11" t="s">
-        <v>230</v>
       </c>
     </row>
     <row r="12" spans="1:2" ht="12" customHeight="1">
       <c r="A12" t="s">
-        <v>255</v>
+        <v>248</v>
       </c>
       <c r="B12" t="s">
-        <v>252</v>
+        <v>245</v>
       </c>
     </row>
     <row r="13" spans="1:2" ht="12" customHeight="1">
       <c r="A13" t="s">
+        <v>217</v>
+      </c>
+      <c r="B13" t="s">
         <v>224</v>
-      </c>
-      <c r="B13" t="s">
-        <v>231</v>
       </c>
     </row>
     <row r="14" spans="1:2" ht="12" customHeight="1">
       <c r="A14" t="s">
+        <v>218</v>
+      </c>
+      <c r="B14" t="s">
         <v>225</v>
-      </c>
-      <c r="B14" t="s">
-        <v>232</v>
       </c>
     </row>
     <row r="15" spans="1:2" ht="42" customHeight="1">
       <c r="A15" t="s">
-        <v>253</v>
+        <v>246</v>
       </c>
       <c r="B15" t="s">
-        <v>254</v>
+        <v>247</v>
       </c>
     </row>
     <row r="16" spans="1:2" ht="12.75" customHeight="1">
       <c r="A16" t="s">
-        <v>393</v>
+        <v>386</v>
       </c>
       <c r="B16" t="s">
-        <v>401</v>
+        <v>394</v>
       </c>
     </row>
     <row r="17" spans="1:2" ht="12.75" customHeight="1">
       <c r="A17" t="s">
-        <v>394</v>
+        <v>387</v>
       </c>
       <c r="B17" t="s">
-        <v>402</v>
+        <v>395</v>
       </c>
     </row>
     <row r="18" spans="1:2" ht="12.75" customHeight="1">
       <c r="A18" t="s">
-        <v>395</v>
+        <v>388</v>
       </c>
       <c r="B18" t="s">
-        <v>403</v>
+        <v>396</v>
       </c>
     </row>
     <row r="19" spans="1:2" ht="12.75" customHeight="1">
       <c r="A19" t="s">
-        <v>396</v>
+        <v>389</v>
       </c>
       <c r="B19" t="s">
-        <v>404</v>
+        <v>397</v>
       </c>
     </row>
     <row r="20" spans="1:2" ht="12.75" customHeight="1">
       <c r="A20" t="s">
-        <v>397</v>
+        <v>390</v>
       </c>
       <c r="B20" t="s">
-        <v>405</v>
+        <v>398</v>
       </c>
     </row>
     <row r="21" spans="1:2" ht="12.75" customHeight="1">
       <c r="A21" t="s">
-        <v>398</v>
+        <v>391</v>
       </c>
       <c r="B21" t="s">
-        <v>406</v>
+        <v>399</v>
       </c>
     </row>
     <row r="22" spans="1:2" ht="12.75" customHeight="1">
       <c r="A22" t="s">
-        <v>399</v>
+        <v>392</v>
       </c>
       <c r="B22" t="s">
-        <v>400</v>
+        <v>393</v>
       </c>
     </row>
     <row r="23" spans="1:2" ht="12.75" customHeight="1">
       <c r="A23" t="s">
-        <v>410</v>
+        <v>403</v>
       </c>
       <c r="B23" t="s">
-        <v>411</v>
+        <v>404</v>
       </c>
     </row>
   </sheetData>
@@ -5630,8 +5720,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:D140"/>
   <sheetViews>
-    <sheetView workbookViewId="0">
-      <selection activeCell="B21" sqref="B21"/>
+    <sheetView tabSelected="1" workbookViewId="0">
+      <selection activeCell="C25" sqref="C25"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultColWidth="17.1640625" defaultRowHeight="12.75" customHeight="1" x14ac:dyDescent="0"/>
@@ -5703,7 +5793,7 @@
         <v>4</v>
       </c>
       <c r="B6" t="s">
-        <v>90</v>
+        <v>84</v>
       </c>
       <c r="C6" t="s">
         <v>80</v>
@@ -5758,10 +5848,10 @@
         <v>7</v>
       </c>
       <c r="B14" t="s">
-        <v>93</v>
+        <v>87</v>
       </c>
       <c r="C14" t="s">
-        <v>94</v>
+        <v>88</v>
       </c>
     </row>
     <row r="15" spans="1:4" ht="12.75" customHeight="1">
@@ -5769,10 +5859,10 @@
         <v>7</v>
       </c>
       <c r="B15" t="s">
-        <v>91</v>
+        <v>85</v>
       </c>
       <c r="C15" t="s">
-        <v>92</v>
+        <v>86</v>
       </c>
     </row>
     <row r="16" spans="1:4" ht="12.75" customHeight="1">
@@ -5780,7 +5870,7 @@
         <v>7</v>
       </c>
       <c r="B16" t="s">
-        <v>119</v>
+        <v>113</v>
       </c>
       <c r="C16" t="s">
         <v>73</v>
@@ -5813,32 +5903,32 @@
         <v>11</v>
       </c>
       <c r="B20" t="s">
-        <v>520</v>
+        <v>513</v>
       </c>
       <c r="C20" t="s">
-        <v>107</v>
+        <v>101</v>
       </c>
     </row>
     <row r="21" spans="1:3" ht="12.75" customHeight="1">
       <c r="A21" t="s">
-        <v>489</v>
+        <v>482</v>
       </c>
       <c r="B21" t="s">
-        <v>511</v>
+        <v>504</v>
       </c>
       <c r="C21" t="s">
-        <v>512</v>
+        <v>505</v>
       </c>
     </row>
     <row r="22" spans="1:3" ht="12.75" customHeight="1">
       <c r="A22" t="s">
-        <v>489</v>
+        <v>482</v>
       </c>
       <c r="B22" t="s">
-        <v>513</v>
+        <v>506</v>
       </c>
       <c r="C22" t="s">
-        <v>514</v>
+        <v>507</v>
       </c>
     </row>
     <row r="24" spans="1:3" ht="12.75" customHeight="1">
@@ -5846,10 +5936,10 @@
         <v>79</v>
       </c>
       <c r="B24" t="s">
-        <v>84</v>
+        <v>523</v>
       </c>
       <c r="C24" t="s">
-        <v>85</v>
+        <v>533</v>
       </c>
     </row>
     <row r="25" spans="1:3" ht="12.75" customHeight="1">
@@ -5857,10 +5947,10 @@
         <v>79</v>
       </c>
       <c r="B25" t="s">
-        <v>86</v>
+        <v>531</v>
       </c>
       <c r="C25" t="s">
-        <v>87</v>
+        <v>531</v>
       </c>
     </row>
     <row r="26" spans="1:3" ht="12.75" customHeight="1">
@@ -5868,10 +5958,10 @@
         <v>79</v>
       </c>
       <c r="B26" t="s">
-        <v>88</v>
+        <v>532</v>
       </c>
       <c r="C26" t="s">
-        <v>89</v>
+        <v>532</v>
       </c>
     </row>
     <row r="28" spans="1:3" ht="12.75" customHeight="1">
@@ -5901,10 +5991,10 @@
         <v>59</v>
       </c>
       <c r="B30" t="s">
-        <v>520</v>
+        <v>513</v>
       </c>
       <c r="C30" t="s">
-        <v>107</v>
+        <v>101</v>
       </c>
     </row>
     <row r="32" spans="1:3" ht="12.75" customHeight="1">
@@ -5931,1007 +6021,1007 @@
     </row>
     <row r="35" spans="1:4" ht="12.75" customHeight="1">
       <c r="A35" t="s">
+        <v>252</v>
+      </c>
+      <c r="B35" t="s">
         <v>259</v>
       </c>
-      <c r="B35" t="s">
-        <v>266</v>
-      </c>
       <c r="C35" t="s">
-        <v>267</v>
+        <v>260</v>
       </c>
     </row>
     <row r="36" spans="1:4" ht="12.75" customHeight="1">
       <c r="A36" t="s">
-        <v>259</v>
+        <v>252</v>
       </c>
       <c r="B36" t="s">
-        <v>268</v>
+        <v>261</v>
       </c>
       <c r="C36" t="s">
-        <v>269</v>
+        <v>262</v>
       </c>
     </row>
     <row r="37" spans="1:4" ht="12.75" customHeight="1">
       <c r="A37" t="s">
-        <v>259</v>
+        <v>252</v>
       </c>
       <c r="B37" t="s">
-        <v>407</v>
+        <v>400</v>
       </c>
       <c r="C37" t="s">
-        <v>384</v>
+        <v>377</v>
       </c>
     </row>
     <row r="39" spans="1:4" ht="12.75" customHeight="1">
       <c r="A39" t="s">
-        <v>121</v>
+        <v>115</v>
       </c>
       <c r="B39" t="s">
+        <v>116</v>
+      </c>
+      <c r="C39" t="s">
         <v>122</v>
-      </c>
-      <c r="C39" t="s">
-        <v>128</v>
       </c>
     </row>
     <row r="40" spans="1:4" ht="12.75" customHeight="1">
       <c r="A40" t="s">
-        <v>121</v>
+        <v>115</v>
       </c>
       <c r="B40" t="s">
+        <v>117</v>
+      </c>
+      <c r="C40" t="s">
         <v>123</v>
-      </c>
-      <c r="C40" t="s">
-        <v>129</v>
       </c>
     </row>
     <row r="41" spans="1:4" ht="12.75" customHeight="1">
       <c r="A41" t="s">
-        <v>121</v>
+        <v>115</v>
       </c>
       <c r="B41" t="s">
+        <v>118</v>
+      </c>
+      <c r="C41" t="s">
         <v>124</v>
-      </c>
-      <c r="C41" t="s">
-        <v>130</v>
       </c>
     </row>
     <row r="42" spans="1:4" ht="12.75" customHeight="1">
       <c r="A42" t="s">
-        <v>121</v>
+        <v>115</v>
       </c>
       <c r="B42" t="s">
+        <v>119</v>
+      </c>
+      <c r="C42" t="s">
         <v>125</v>
-      </c>
-      <c r="C42" t="s">
-        <v>131</v>
       </c>
     </row>
     <row r="43" spans="1:4" ht="12.75" customHeight="1">
       <c r="A43" t="s">
-        <v>121</v>
+        <v>115</v>
       </c>
       <c r="B43" t="s">
+        <v>120</v>
+      </c>
+      <c r="C43" t="s">
         <v>126</v>
-      </c>
-      <c r="C43" t="s">
-        <v>132</v>
       </c>
     </row>
     <row r="44" spans="1:4" ht="12.75" customHeight="1">
       <c r="A44" t="s">
+        <v>115</v>
+      </c>
+      <c r="B44" t="s">
         <v>121</v>
       </c>
-      <c r="B44" t="s">
+      <c r="C44" t="s">
         <v>127</v>
-      </c>
-      <c r="C44" t="s">
-        <v>133</v>
       </c>
     </row>
     <row r="46" spans="1:4" ht="12.75" customHeight="1">
       <c r="A46" t="s">
-        <v>135</v>
+        <v>129</v>
       </c>
       <c r="B46" t="s">
-        <v>142</v>
+        <v>136</v>
       </c>
       <c r="D46" t="s">
-        <v>143</v>
+        <v>137</v>
       </c>
     </row>
     <row r="47" spans="1:4" ht="12.75" customHeight="1">
       <c r="A47" t="s">
-        <v>135</v>
+        <v>129</v>
       </c>
       <c r="B47" t="s">
-        <v>144</v>
+        <v>138</v>
       </c>
       <c r="D47" t="s">
-        <v>148</v>
+        <v>142</v>
       </c>
     </row>
     <row r="48" spans="1:4" ht="12.75" customHeight="1">
       <c r="A48" t="s">
-        <v>135</v>
+        <v>129</v>
       </c>
       <c r="B48" t="s">
-        <v>145</v>
+        <v>139</v>
       </c>
       <c r="D48" t="s">
-        <v>149</v>
+        <v>143</v>
       </c>
     </row>
     <row r="49" spans="1:4" ht="12.75" customHeight="1">
       <c r="A49" t="s">
-        <v>135</v>
+        <v>129</v>
       </c>
       <c r="B49" t="s">
-        <v>146</v>
+        <v>140</v>
       </c>
       <c r="D49" t="s">
-        <v>150</v>
+        <v>144</v>
       </c>
     </row>
     <row r="50" spans="1:4" ht="12.75" customHeight="1">
       <c r="A50" t="s">
-        <v>135</v>
+        <v>129</v>
       </c>
       <c r="B50" t="s">
-        <v>147</v>
+        <v>141</v>
       </c>
       <c r="D50" t="s">
-        <v>151</v>
+        <v>145</v>
       </c>
     </row>
     <row r="52" spans="1:4" ht="12.75" customHeight="1">
       <c r="A52" t="s">
-        <v>139</v>
+        <v>133</v>
       </c>
       <c r="B52" t="s">
-        <v>175</v>
+        <v>169</v>
       </c>
       <c r="D52" t="s">
-        <v>176</v>
+        <v>170</v>
       </c>
     </row>
     <row r="53" spans="1:4" s="2" customFormat="1" ht="12.75" customHeight="1">
       <c r="A53" t="s">
-        <v>139</v>
+        <v>133</v>
       </c>
       <c r="B53" t="s">
-        <v>165</v>
+        <v>159</v>
       </c>
       <c r="D53" t="s">
-        <v>166</v>
+        <v>160</v>
       </c>
     </row>
     <row r="54" spans="1:4" ht="12.75" customHeight="1">
       <c r="A54" t="s">
-        <v>139</v>
+        <v>133</v>
       </c>
       <c r="B54" t="s">
-        <v>167</v>
+        <v>161</v>
       </c>
       <c r="D54" t="s">
-        <v>168</v>
+        <v>162</v>
       </c>
     </row>
     <row r="55" spans="1:4" ht="12.75" customHeight="1">
       <c r="A55" t="s">
-        <v>139</v>
+        <v>133</v>
       </c>
       <c r="B55" t="s">
-        <v>169</v>
+        <v>163</v>
       </c>
       <c r="D55" t="s">
-        <v>170</v>
+        <v>164</v>
       </c>
     </row>
     <row r="56" spans="1:4" ht="12.75" customHeight="1">
       <c r="A56" t="s">
-        <v>139</v>
+        <v>133</v>
       </c>
       <c r="B56" t="s">
-        <v>171</v>
+        <v>165</v>
       </c>
       <c r="D56" t="s">
-        <v>172</v>
+        <v>166</v>
       </c>
     </row>
     <row r="57" spans="1:4" ht="12.75" customHeight="1">
       <c r="A57" t="s">
-        <v>139</v>
+        <v>133</v>
       </c>
       <c r="B57" t="s">
-        <v>173</v>
+        <v>167</v>
       </c>
       <c r="D57" t="s">
-        <v>174</v>
+        <v>168</v>
       </c>
     </row>
     <row r="59" spans="1:4" ht="12.75" customHeight="1">
       <c r="A59" t="s">
-        <v>156</v>
+        <v>150</v>
       </c>
       <c r="B59" t="s">
-        <v>177</v>
+        <v>171</v>
       </c>
       <c r="C59" s="2"/>
       <c r="D59" t="s">
-        <v>178</v>
+        <v>172</v>
       </c>
     </row>
     <row r="60" spans="1:4" ht="12.75" customHeight="1">
       <c r="A60" t="s">
-        <v>156</v>
+        <v>150</v>
       </c>
       <c r="B60" t="s">
-        <v>179</v>
+        <v>173</v>
       </c>
       <c r="D60" t="s">
-        <v>180</v>
+        <v>174</v>
       </c>
     </row>
     <row r="61" spans="1:4" ht="12.75" customHeight="1">
       <c r="A61" t="s">
-        <v>156</v>
+        <v>150</v>
       </c>
       <c r="B61" t="s">
-        <v>181</v>
+        <v>175</v>
       </c>
       <c r="D61" t="s">
-        <v>182</v>
+        <v>176</v>
       </c>
     </row>
     <row r="62" spans="1:4" ht="12.75" customHeight="1">
       <c r="A62" t="s">
-        <v>156</v>
+        <v>150</v>
       </c>
       <c r="B62" t="s">
-        <v>183</v>
+        <v>177</v>
       </c>
       <c r="D62" t="s">
-        <v>184</v>
+        <v>178</v>
       </c>
     </row>
     <row r="63" spans="1:4" ht="12.75" customHeight="1">
       <c r="A63" t="s">
-        <v>156</v>
+        <v>150</v>
       </c>
       <c r="B63" t="s">
-        <v>185</v>
+        <v>179</v>
       </c>
       <c r="D63" t="s">
-        <v>186</v>
+        <v>180</v>
       </c>
     </row>
     <row r="65" spans="1:4" ht="12.75" customHeight="1">
       <c r="A65" t="s">
-        <v>227</v>
+        <v>220</v>
       </c>
       <c r="B65" t="s">
-        <v>245</v>
+        <v>238</v>
       </c>
       <c r="D65" t="s">
-        <v>238</v>
+        <v>231</v>
       </c>
     </row>
     <row r="66" spans="1:4" ht="12.75" customHeight="1">
       <c r="A66" t="s">
-        <v>227</v>
+        <v>220</v>
       </c>
       <c r="B66" t="s">
-        <v>246</v>
+        <v>239</v>
       </c>
       <c r="C66" s="2"/>
       <c r="D66" t="s">
-        <v>239</v>
+        <v>232</v>
       </c>
     </row>
     <row r="67" spans="1:4" ht="12.75" customHeight="1">
       <c r="A67" t="s">
-        <v>227</v>
+        <v>220</v>
       </c>
       <c r="B67" t="s">
-        <v>247</v>
+        <v>240</v>
       </c>
       <c r="D67" t="s">
-        <v>240</v>
+        <v>233</v>
       </c>
     </row>
     <row r="68" spans="1:4" ht="12.75" customHeight="1">
       <c r="A68" t="s">
-        <v>227</v>
+        <v>220</v>
       </c>
       <c r="B68" t="s">
-        <v>248</v>
+        <v>241</v>
       </c>
       <c r="D68" t="s">
-        <v>241</v>
+        <v>234</v>
       </c>
     </row>
     <row r="69" spans="1:4" ht="12.75" customHeight="1">
       <c r="A69" t="s">
-        <v>227</v>
+        <v>220</v>
       </c>
       <c r="B69" t="s">
-        <v>249</v>
+        <v>242</v>
       </c>
       <c r="D69" t="s">
-        <v>242</v>
+        <v>235</v>
       </c>
     </row>
     <row r="70" spans="1:4" ht="12.75" customHeight="1">
       <c r="A70" t="s">
-        <v>227</v>
+        <v>220</v>
       </c>
       <c r="B70" t="s">
-        <v>250</v>
+        <v>243</v>
       </c>
       <c r="D70" t="s">
-        <v>243</v>
+        <v>236</v>
       </c>
     </row>
     <row r="71" spans="1:4" ht="12.75" customHeight="1">
       <c r="A71" t="s">
-        <v>227</v>
+        <v>220</v>
       </c>
       <c r="B71" t="s">
-        <v>251</v>
+        <v>244</v>
       </c>
       <c r="D71" t="s">
-        <v>244</v>
+        <v>237</v>
       </c>
     </row>
     <row r="73" spans="1:4" ht="12.75" customHeight="1">
       <c r="A73" t="s">
-        <v>160</v>
+        <v>154</v>
       </c>
       <c r="B73" t="s">
-        <v>187</v>
+        <v>181</v>
       </c>
       <c r="D73" t="s">
-        <v>188</v>
+        <v>182</v>
       </c>
     </row>
     <row r="74" spans="1:4" ht="12.75" customHeight="1">
       <c r="A74" t="s">
-        <v>160</v>
+        <v>154</v>
       </c>
       <c r="B74" t="s">
-        <v>189</v>
+        <v>183</v>
       </c>
       <c r="C74" s="2"/>
       <c r="D74" t="s">
-        <v>190</v>
+        <v>184</v>
       </c>
     </row>
     <row r="75" spans="1:4" ht="12.75" customHeight="1">
       <c r="A75" t="s">
-        <v>160</v>
+        <v>154</v>
       </c>
       <c r="B75" t="s">
-        <v>191</v>
+        <v>185</v>
       </c>
       <c r="D75" t="s">
-        <v>192</v>
+        <v>186</v>
       </c>
     </row>
     <row r="76" spans="1:4" ht="12.75" customHeight="1">
       <c r="A76" t="s">
-        <v>160</v>
+        <v>154</v>
       </c>
       <c r="B76" t="s">
-        <v>193</v>
+        <v>187</v>
       </c>
       <c r="D76" t="s">
-        <v>194</v>
+        <v>188</v>
       </c>
     </row>
     <row r="77" spans="1:4" ht="12.75" customHeight="1">
       <c r="A77" t="s">
-        <v>160</v>
+        <v>154</v>
       </c>
       <c r="B77" t="s">
-        <v>195</v>
+        <v>189</v>
       </c>
       <c r="D77" t="s">
-        <v>196</v>
+        <v>190</v>
       </c>
     </row>
     <row r="78" spans="1:4" ht="12.75" customHeight="1">
       <c r="A78" t="s">
-        <v>160</v>
+        <v>154</v>
       </c>
       <c r="B78" t="s">
-        <v>197</v>
+        <v>191</v>
       </c>
       <c r="D78" t="s">
-        <v>198</v>
+        <v>192</v>
       </c>
     </row>
     <row r="80" spans="1:4" ht="12.75" customHeight="1">
       <c r="A80" t="s">
-        <v>163</v>
+        <v>157</v>
       </c>
       <c r="B80" t="s">
-        <v>199</v>
+        <v>193</v>
       </c>
       <c r="D80" t="s">
-        <v>200</v>
+        <v>194</v>
       </c>
     </row>
     <row r="81" spans="1:4" ht="12.75" customHeight="1">
       <c r="A81" t="s">
-        <v>163</v>
+        <v>157</v>
       </c>
       <c r="B81" t="s">
-        <v>201</v>
+        <v>195</v>
       </c>
       <c r="C81" s="2"/>
       <c r="D81" t="s">
-        <v>202</v>
+        <v>196</v>
       </c>
     </row>
     <row r="82" spans="1:4" ht="12.75" customHeight="1">
       <c r="A82" t="s">
-        <v>163</v>
+        <v>157</v>
       </c>
       <c r="B82" t="s">
-        <v>203</v>
+        <v>197</v>
       </c>
       <c r="D82" t="s">
-        <v>204</v>
+        <v>198</v>
       </c>
     </row>
     <row r="83" spans="1:4" ht="12.75" customHeight="1">
       <c r="A83" t="s">
-        <v>163</v>
+        <v>157</v>
       </c>
       <c r="B83" t="s">
-        <v>205</v>
+        <v>199</v>
       </c>
       <c r="D83" t="s">
-        <v>206</v>
+        <v>200</v>
       </c>
     </row>
     <row r="84" spans="1:4" ht="12.75" customHeight="1">
       <c r="A84" t="s">
-        <v>163</v>
+        <v>157</v>
       </c>
       <c r="B84" t="s">
-        <v>207</v>
+        <v>201</v>
       </c>
       <c r="D84" t="s">
-        <v>208</v>
+        <v>202</v>
       </c>
     </row>
     <row r="85" spans="1:4" ht="12.75" customHeight="1">
       <c r="A85" t="s">
-        <v>163</v>
+        <v>157</v>
       </c>
       <c r="B85" t="s">
-        <v>209</v>
+        <v>203</v>
       </c>
       <c r="D85" t="s">
-        <v>210</v>
+        <v>204</v>
       </c>
     </row>
     <row r="87" spans="1:4" ht="12.75" customHeight="1">
       <c r="A87" t="s">
+        <v>256</v>
+      </c>
+      <c r="B87" t="s">
         <v>263</v>
       </c>
-      <c r="B87" t="s">
-        <v>270</v>
-      </c>
       <c r="C87" t="s">
-        <v>288</v>
+        <v>281</v>
       </c>
     </row>
     <row r="88" spans="1:4" ht="12.75" customHeight="1">
       <c r="A88" t="s">
-        <v>263</v>
+        <v>256</v>
       </c>
       <c r="B88" t="s">
-        <v>273</v>
+        <v>266</v>
       </c>
       <c r="C88" t="s">
-        <v>289</v>
+        <v>282</v>
       </c>
     </row>
     <row r="89" spans="1:4" ht="12.75" customHeight="1">
       <c r="A89" t="s">
-        <v>263</v>
+        <v>256</v>
       </c>
       <c r="B89" t="s">
-        <v>276</v>
+        <v>269</v>
       </c>
       <c r="C89" t="s">
-        <v>290</v>
+        <v>283</v>
       </c>
     </row>
     <row r="90" spans="1:4" ht="12.75" customHeight="1">
       <c r="A90" t="s">
-        <v>263</v>
+        <v>256</v>
       </c>
       <c r="B90" t="s">
-        <v>277</v>
+        <v>270</v>
       </c>
       <c r="C90" t="s">
-        <v>383</v>
+        <v>376</v>
       </c>
     </row>
     <row r="91" spans="1:4" ht="12.75" customHeight="1">
       <c r="A91" t="s">
-        <v>263</v>
+        <v>256</v>
       </c>
       <c r="B91" t="s">
-        <v>279</v>
+        <v>272</v>
       </c>
       <c r="C91" t="s">
-        <v>291</v>
+        <v>284</v>
       </c>
     </row>
     <row r="92" spans="1:4" ht="12.75" customHeight="1">
       <c r="A92" t="s">
-        <v>263</v>
+        <v>256</v>
       </c>
       <c r="B92" t="s">
-        <v>281</v>
+        <v>274</v>
       </c>
       <c r="C92" t="s">
-        <v>292</v>
+        <v>285</v>
       </c>
     </row>
     <row r="94" spans="1:4" ht="12.75" customHeight="1">
       <c r="A94" t="s">
-        <v>293</v>
+        <v>286</v>
       </c>
       <c r="B94" t="s">
+        <v>292</v>
+      </c>
+      <c r="C94" t="s">
         <v>299</v>
-      </c>
-      <c r="C94" t="s">
-        <v>306</v>
       </c>
     </row>
     <row r="95" spans="1:4" ht="12.75" customHeight="1">
       <c r="A95" t="s">
+        <v>286</v>
+      </c>
+      <c r="B95" t="s">
         <v>293</v>
       </c>
-      <c r="B95" t="s">
+      <c r="C95" t="s">
         <v>300</v>
-      </c>
-      <c r="C95" t="s">
-        <v>307</v>
       </c>
     </row>
     <row r="96" spans="1:4" ht="12.75" customHeight="1">
       <c r="A96" t="s">
-        <v>293</v>
+        <v>286</v>
       </c>
       <c r="B96" t="s">
+        <v>294</v>
+      </c>
+      <c r="C96" t="s">
         <v>301</v>
-      </c>
-      <c r="C96" t="s">
-        <v>308</v>
       </c>
     </row>
     <row r="97" spans="1:3" ht="12.75" customHeight="1">
       <c r="A97" t="s">
-        <v>293</v>
+        <v>286</v>
       </c>
       <c r="B97" t="s">
+        <v>295</v>
+      </c>
+      <c r="C97" t="s">
         <v>302</v>
-      </c>
-      <c r="C97" t="s">
-        <v>309</v>
       </c>
     </row>
     <row r="98" spans="1:3" ht="12.75" customHeight="1">
       <c r="A98" t="s">
-        <v>293</v>
+        <v>286</v>
       </c>
       <c r="B98" t="s">
+        <v>296</v>
+      </c>
+      <c r="C98" t="s">
         <v>303</v>
-      </c>
-      <c r="C98" t="s">
-        <v>310</v>
       </c>
     </row>
     <row r="99" spans="1:3" ht="12.75" customHeight="1">
       <c r="A99" t="s">
-        <v>293</v>
+        <v>286</v>
       </c>
       <c r="B99" t="s">
+        <v>297</v>
+      </c>
+      <c r="C99" t="s">
         <v>304</v>
-      </c>
-      <c r="C99" t="s">
-        <v>311</v>
       </c>
     </row>
     <row r="100" spans="1:3" ht="12.75" customHeight="1">
       <c r="A100" t="s">
-        <v>293</v>
+        <v>286</v>
       </c>
       <c r="B100" t="s">
+        <v>298</v>
+      </c>
+      <c r="C100" t="s">
         <v>305</v>
-      </c>
-      <c r="C100" t="s">
-        <v>312</v>
       </c>
     </row>
     <row r="102" spans="1:3" ht="12.75" customHeight="1">
       <c r="A102" t="s">
-        <v>294</v>
+        <v>287</v>
       </c>
       <c r="B102" t="s">
-        <v>319</v>
+        <v>312</v>
       </c>
       <c r="C102" t="s">
-        <v>325</v>
+        <v>318</v>
       </c>
     </row>
     <row r="103" spans="1:3" ht="12.75" customHeight="1">
       <c r="A103" t="s">
-        <v>294</v>
+        <v>287</v>
       </c>
       <c r="B103" t="s">
-        <v>320</v>
+        <v>313</v>
       </c>
       <c r="C103" t="s">
-        <v>326</v>
+        <v>319</v>
       </c>
     </row>
     <row r="104" spans="1:3" ht="12.75" customHeight="1">
       <c r="A104" t="s">
-        <v>294</v>
+        <v>287</v>
       </c>
       <c r="B104" t="s">
-        <v>321</v>
+        <v>314</v>
       </c>
       <c r="C104" t="s">
-        <v>327</v>
+        <v>320</v>
       </c>
     </row>
     <row r="105" spans="1:3" ht="12.75" customHeight="1">
       <c r="A105" t="s">
-        <v>294</v>
+        <v>287</v>
       </c>
       <c r="B105" t="s">
-        <v>322</v>
+        <v>315</v>
       </c>
       <c r="C105" t="s">
-        <v>328</v>
+        <v>321</v>
       </c>
     </row>
     <row r="106" spans="1:3" ht="12.75" customHeight="1">
       <c r="A106" t="s">
-        <v>294</v>
+        <v>287</v>
       </c>
       <c r="B106" t="s">
-        <v>323</v>
+        <v>316</v>
       </c>
       <c r="C106" t="s">
-        <v>329</v>
+        <v>322</v>
       </c>
     </row>
     <row r="107" spans="1:3" ht="12.75" customHeight="1">
       <c r="A107" t="s">
-        <v>294</v>
+        <v>287</v>
       </c>
       <c r="B107" t="s">
-        <v>324</v>
+        <v>317</v>
       </c>
       <c r="C107" t="s">
-        <v>330</v>
+        <v>323</v>
       </c>
     </row>
     <row r="109" spans="1:3" ht="12.75" customHeight="1">
       <c r="A109" t="s">
-        <v>295</v>
+        <v>288</v>
       </c>
       <c r="B109" t="s">
-        <v>337</v>
+        <v>330</v>
       </c>
       <c r="C109" t="s">
-        <v>338</v>
+        <v>331</v>
       </c>
     </row>
     <row r="110" spans="1:3" ht="12.75" customHeight="1">
       <c r="A110" t="s">
-        <v>295</v>
+        <v>288</v>
       </c>
       <c r="B110" t="s">
-        <v>331</v>
+        <v>324</v>
       </c>
       <c r="C110" t="s">
-        <v>339</v>
+        <v>332</v>
       </c>
     </row>
     <row r="111" spans="1:3" ht="12.75" customHeight="1">
       <c r="A111" t="s">
-        <v>295</v>
+        <v>288</v>
       </c>
       <c r="B111" t="s">
-        <v>332</v>
+        <v>325</v>
       </c>
       <c r="C111" t="s">
-        <v>340</v>
+        <v>333</v>
       </c>
     </row>
     <row r="112" spans="1:3" ht="12.75" customHeight="1">
       <c r="A112" t="s">
-        <v>295</v>
+        <v>288</v>
       </c>
       <c r="B112" t="s">
-        <v>333</v>
+        <v>326</v>
       </c>
       <c r="C112" t="s">
-        <v>341</v>
+        <v>334</v>
       </c>
     </row>
     <row r="113" spans="1:3" ht="12.75" customHeight="1">
       <c r="A113" t="s">
-        <v>295</v>
+        <v>288</v>
       </c>
       <c r="B113" t="s">
-        <v>334</v>
+        <v>327</v>
       </c>
       <c r="C113" t="s">
-        <v>342</v>
+        <v>335</v>
       </c>
     </row>
     <row r="114" spans="1:3" ht="12.75" customHeight="1">
       <c r="A114" t="s">
-        <v>295</v>
+        <v>288</v>
       </c>
       <c r="B114" t="s">
-        <v>335</v>
+        <v>328</v>
       </c>
       <c r="C114" t="s">
-        <v>343</v>
+        <v>336</v>
       </c>
     </row>
     <row r="115" spans="1:3" ht="12.75" customHeight="1">
       <c r="A115" t="s">
-        <v>295</v>
+        <v>288</v>
       </c>
       <c r="B115" t="s">
-        <v>336</v>
+        <v>329</v>
       </c>
       <c r="C115" t="s">
-        <v>344</v>
+        <v>337</v>
       </c>
     </row>
     <row r="117" spans="1:3" ht="12.75" customHeight="1">
       <c r="A117" t="s">
-        <v>296</v>
+        <v>289</v>
       </c>
       <c r="B117" t="s">
-        <v>345</v>
+        <v>338</v>
       </c>
       <c r="C117" t="s">
-        <v>351</v>
+        <v>344</v>
       </c>
     </row>
     <row r="118" spans="1:3" ht="12.75" customHeight="1">
       <c r="A118" t="s">
-        <v>296</v>
+        <v>289</v>
       </c>
       <c r="B118" t="s">
-        <v>346</v>
+        <v>339</v>
       </c>
       <c r="C118" t="s">
-        <v>352</v>
+        <v>345</v>
       </c>
     </row>
     <row r="119" spans="1:3" ht="12.75" customHeight="1">
       <c r="A119" t="s">
-        <v>296</v>
+        <v>289</v>
       </c>
       <c r="B119" t="s">
-        <v>347</v>
+        <v>340</v>
       </c>
       <c r="C119" t="s">
-        <v>353</v>
+        <v>346</v>
       </c>
     </row>
     <row r="120" spans="1:3" ht="12.75" customHeight="1">
       <c r="A120" t="s">
-        <v>296</v>
+        <v>289</v>
       </c>
       <c r="B120" t="s">
-        <v>348</v>
+        <v>341</v>
       </c>
       <c r="C120" t="s">
-        <v>354</v>
+        <v>347</v>
       </c>
     </row>
     <row r="121" spans="1:3" ht="12.75" customHeight="1">
       <c r="A121" t="s">
-        <v>296</v>
+        <v>289</v>
       </c>
       <c r="B121" t="s">
-        <v>349</v>
+        <v>342</v>
       </c>
       <c r="C121" t="s">
-        <v>355</v>
+        <v>348</v>
       </c>
     </row>
     <row r="122" spans="1:3" ht="12.75" customHeight="1">
       <c r="A122" t="s">
-        <v>296</v>
+        <v>289</v>
       </c>
       <c r="B122" t="s">
-        <v>350</v>
+        <v>343</v>
       </c>
       <c r="C122" t="s">
-        <v>356</v>
+        <v>349</v>
       </c>
     </row>
     <row r="124" spans="1:3" ht="12.75" customHeight="1">
       <c r="A124" t="s">
-        <v>297</v>
+        <v>290</v>
       </c>
       <c r="B124" t="s">
-        <v>363</v>
+        <v>356</v>
       </c>
       <c r="C124" t="s">
-        <v>364</v>
+        <v>357</v>
       </c>
     </row>
     <row r="125" spans="1:3" ht="12.75" customHeight="1">
       <c r="A125" t="s">
-        <v>297</v>
+        <v>290</v>
       </c>
       <c r="B125" t="s">
-        <v>357</v>
+        <v>350</v>
       </c>
       <c r="C125" t="s">
-        <v>365</v>
+        <v>358</v>
       </c>
     </row>
     <row r="126" spans="1:3" ht="12.75" customHeight="1">
       <c r="A126" t="s">
-        <v>297</v>
+        <v>290</v>
       </c>
       <c r="B126" t="s">
-        <v>358</v>
+        <v>351</v>
       </c>
       <c r="C126" t="s">
-        <v>366</v>
+        <v>359</v>
       </c>
     </row>
     <row r="127" spans="1:3" ht="12.75" customHeight="1">
       <c r="A127" t="s">
-        <v>297</v>
+        <v>290</v>
       </c>
       <c r="B127" t="s">
+        <v>353</v>
+      </c>
+      <c r="C127" t="s">
         <v>360</v>
-      </c>
-      <c r="C127" t="s">
-        <v>367</v>
       </c>
     </row>
     <row r="128" spans="1:3" ht="12.75" customHeight="1">
       <c r="A128" t="s">
-        <v>297</v>
+        <v>290</v>
       </c>
       <c r="B128" t="s">
-        <v>359</v>
+        <v>352</v>
       </c>
       <c r="C128" t="s">
-        <v>368</v>
+        <v>361</v>
       </c>
     </row>
     <row r="129" spans="1:3" ht="12.75" customHeight="1">
       <c r="A129" t="s">
-        <v>297</v>
+        <v>290</v>
       </c>
       <c r="B129" t="s">
-        <v>361</v>
+        <v>354</v>
       </c>
       <c r="C129" t="s">
-        <v>369</v>
+        <v>362</v>
       </c>
     </row>
     <row r="130" spans="1:3" ht="12.75" customHeight="1">
       <c r="A130" t="s">
-        <v>297</v>
+        <v>290</v>
       </c>
       <c r="B130" t="s">
-        <v>362</v>
+        <v>355</v>
       </c>
       <c r="C130" t="s">
-        <v>370</v>
+        <v>363</v>
       </c>
     </row>
     <row r="132" spans="1:3" ht="12.75" customHeight="1">
       <c r="A132" t="s">
-        <v>298</v>
+        <v>291</v>
       </c>
       <c r="B132" t="s">
-        <v>371</v>
+        <v>364</v>
       </c>
       <c r="C132" t="s">
-        <v>377</v>
+        <v>370</v>
       </c>
     </row>
     <row r="133" spans="1:3" ht="12.75" customHeight="1">
       <c r="A133" t="s">
-        <v>298</v>
+        <v>291</v>
       </c>
       <c r="B133" t="s">
-        <v>372</v>
+        <v>365</v>
       </c>
       <c r="C133" t="s">
-        <v>378</v>
+        <v>371</v>
       </c>
     </row>
     <row r="134" spans="1:3" ht="12.75" customHeight="1">
       <c r="A134" t="s">
-        <v>298</v>
+        <v>291</v>
       </c>
       <c r="B134" t="s">
-        <v>373</v>
+        <v>366</v>
       </c>
       <c r="C134" t="s">
-        <v>379</v>
+        <v>372</v>
       </c>
     </row>
     <row r="135" spans="1:3" ht="12.75" customHeight="1">
       <c r="A135" t="s">
-        <v>298</v>
+        <v>291</v>
       </c>
       <c r="B135" t="s">
-        <v>374</v>
+        <v>367</v>
       </c>
       <c r="C135" t="s">
-        <v>380</v>
+        <v>373</v>
       </c>
     </row>
     <row r="136" spans="1:3" ht="12.75" customHeight="1">
       <c r="A136" t="s">
-        <v>298</v>
+        <v>291</v>
       </c>
       <c r="B136" t="s">
-        <v>375</v>
+        <v>368</v>
       </c>
       <c r="C136" t="s">
-        <v>381</v>
+        <v>374</v>
       </c>
     </row>
     <row r="137" spans="1:3" ht="12.75" customHeight="1">
       <c r="A137" t="s">
-        <v>298</v>
+        <v>291</v>
       </c>
       <c r="B137" t="s">
-        <v>376</v>
+        <v>369</v>
       </c>
       <c r="C137" t="s">
-        <v>382</v>
+        <v>375</v>
       </c>
     </row>
     <row r="139" spans="1:3" ht="12.75" customHeight="1">
       <c r="A139" t="s">
-        <v>460</v>
+        <v>453</v>
       </c>
       <c r="B139" t="s">
-        <v>455</v>
+        <v>448</v>
       </c>
       <c r="C139" t="s">
-        <v>449</v>
+        <v>442</v>
       </c>
     </row>
     <row r="140" spans="1:3" ht="12.75" customHeight="1">
       <c r="A140" t="s">
-        <v>460</v>
+        <v>453</v>
       </c>
       <c r="B140" t="s">
-        <v>456</v>
+        <v>449</v>
       </c>
       <c r="C140" t="s">
-        <v>457</v>
+        <v>450</v>
       </c>
     </row>
   </sheetData>
@@ -7002,15 +7092,15 @@
         <v>1</v>
       </c>
       <c r="B1" t="s">
-        <v>152</v>
+        <v>146</v>
       </c>
     </row>
     <row r="2" spans="1:2">
       <c r="A2" t="s">
-        <v>153</v>
+        <v>147</v>
       </c>
       <c r="B2" t="s">
-        <v>154</v>
+        <v>148</v>
       </c>
     </row>
     <row r="3" spans="1:2">
@@ -7018,7 +7108,7 @@
         <v>4</v>
       </c>
       <c r="B3" t="s">
-        <v>154</v>
+        <v>148</v>
       </c>
     </row>
   </sheetData>

</xml_diff>

<commit_message>
removed logic from spread sheet since it is now in the promptType
</commit_message>
<xml_diff>
--- a/opendatakit.collect2/form-files/neonatal/neonatal.xlsx
+++ b/opendatakit.collect2/form-files/neonatal/neonatal.xlsx
@@ -4,7 +4,7 @@
   <fileVersion appName="xl" lastEdited="5" lowestEdited="5" rupBuild="20910"/>
   <workbookPr autoCompressPictures="0"/>
   <bookViews>
-    <workbookView xWindow="0" yWindow="0" windowWidth="28800" windowHeight="17560" tabRatio="500"/>
+    <workbookView xWindow="0" yWindow="0" windowWidth="24660" windowHeight="16520" tabRatio="500" activeTab="2"/>
   </bookViews>
   <sheets>
     <sheet name="survey" sheetId="1" r:id="rId1"/>
@@ -23,7 +23,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="637" uniqueCount="465">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="561" uniqueCount="403">
   <si>
     <t>type</t>
   </si>
@@ -418,69 +418,12 @@
     <t>ballardExam</t>
   </si>
   <si>
-    <t>ballard_menu1</t>
-  </si>
-  <si>
-    <t>posture</t>
-  </si>
-  <si>
-    <t>square</t>
-  </si>
-  <si>
-    <t>arm</t>
-  </si>
-  <si>
-    <t>popliteal</t>
-  </si>
-  <si>
-    <t>scarf</t>
-  </si>
-  <si>
-    <t>heel</t>
-  </si>
-  <si>
-    <t>Posture</t>
-  </si>
-  <si>
-    <t>Square Window</t>
-  </si>
-  <si>
-    <t>Arm Recoil</t>
-  </si>
-  <si>
-    <t>Popliteal Angle</t>
-  </si>
-  <si>
-    <t>Scarf Sign</t>
-  </si>
-  <si>
-    <t>Heel to Ear</t>
-  </si>
-  <si>
-    <t>image_slider posture_slider</t>
-  </si>
-  <si>
-    <t>posture_slider</t>
-  </si>
-  <si>
     <t>Choose Posture</t>
   </si>
   <si>
-    <t>selected(data('ballard_menu1'), 'posture')</t>
-  </si>
-  <si>
-    <t>image_slider square_slider</t>
-  </si>
-  <si>
-    <t>square_slider</t>
-  </si>
-  <si>
     <t>Choose Square Window</t>
   </si>
   <si>
-    <t>selected(data('ballard_menu1'), 'square')</t>
-  </si>
-  <si>
     <t>posture0</t>
   </si>
   <si>
@@ -520,180 +463,84 @@
     <t>string</t>
   </si>
   <si>
-    <t>image_slider arm_slider</t>
-  </si>
-  <si>
-    <t>arm_slider</t>
-  </si>
-  <si>
     <t>Choose Arm Recoil</t>
   </si>
   <si>
-    <t>selected(data('ballard_menu1'), 'arm')</t>
-  </si>
-  <si>
-    <t>image_slider scarf_slider</t>
-  </si>
-  <si>
-    <t>scarf_slider</t>
-  </si>
-  <si>
     <t>Choose Scarf Sign</t>
   </si>
   <si>
-    <t>image_slider heel_slider</t>
-  </si>
-  <si>
-    <t>heel_slider</t>
-  </si>
-  <si>
     <t>Choose Heel to Ear</t>
   </si>
   <si>
-    <t>square_window0</t>
-  </si>
-  <si>
     <t>img/ballard/square_window0.png</t>
   </si>
   <si>
-    <t>square_window1</t>
-  </si>
-  <si>
     <t>img/ballard/square_window1.png</t>
   </si>
   <si>
-    <t>square_window2</t>
-  </si>
-  <si>
     <t>img/ballard/square_window2.png</t>
   </si>
   <si>
-    <t>square_window3</t>
-  </si>
-  <si>
     <t>img/ballard/square_window3.png</t>
   </si>
   <si>
-    <t>square_window4</t>
-  </si>
-  <si>
     <t>img/ballard/square_window4.png</t>
   </si>
   <si>
-    <t>square_window-1</t>
-  </si>
-  <si>
     <t>img/ballard/square_window-1.png</t>
   </si>
   <si>
-    <t>arm_recoil0</t>
-  </si>
-  <si>
     <t>img/ballard/arm_recoil0.png</t>
   </si>
   <si>
-    <t>arm_recoil1</t>
-  </si>
-  <si>
     <t>img/ballard/arm_recoil1.png</t>
   </si>
   <si>
-    <t>arm_recoil2</t>
-  </si>
-  <si>
     <t>img/ballard/arm_recoil2.png</t>
   </si>
   <si>
-    <t>arm_recoil3</t>
-  </si>
-  <si>
     <t>img/ballard/arm_recoil3.png</t>
   </si>
   <si>
-    <t>arm_recoil4</t>
-  </si>
-  <si>
     <t>img/ballard/arm_recoil4.png</t>
   </si>
   <si>
-    <t>scarf_sign-1</t>
-  </si>
-  <si>
     <t>img/ballard/scarf_sign-1.png</t>
   </si>
   <si>
-    <t>scarf_sign0</t>
-  </si>
-  <si>
     <t>img/ballard/scarf_sign0.png</t>
   </si>
   <si>
-    <t>scarf_sign1</t>
-  </si>
-  <si>
     <t>img/ballard/scarf_sign1.png</t>
   </si>
   <si>
-    <t>scarf_sign2</t>
-  </si>
-  <si>
     <t>img/ballard/scarf_sign2.png</t>
   </si>
   <si>
-    <t>scarf_sign3</t>
-  </si>
-  <si>
     <t>img/ballard/scarf_sign3.png</t>
   </si>
   <si>
-    <t>scarf_sign4</t>
-  </si>
-  <si>
     <t>img/ballard/scarf_sign4.png</t>
   </si>
   <si>
-    <t>heel_to_ear-1</t>
-  </si>
-  <si>
     <t>img/ballard/heel_to_ear-1.png</t>
   </si>
   <si>
-    <t>heel_to_ear0</t>
-  </si>
-  <si>
     <t>img/ballard/heel_to_ear0.png</t>
   </si>
   <si>
-    <t>heel_to_ear1</t>
-  </si>
-  <si>
     <t>img/ballard/heel_to_ear1.png</t>
   </si>
   <si>
-    <t>heel_to_ear2</t>
-  </si>
-  <si>
     <t>img/ballard/heel_to_ear2.png</t>
   </si>
   <si>
-    <t>heel_to_ear3</t>
-  </si>
-  <si>
     <t>img/ballard/heel_to_ear3.png</t>
   </si>
   <si>
-    <t>heel_to_ear4</t>
-  </si>
-  <si>
     <t>img/ballard/heel_to_ear4.png</t>
   </si>
   <si>
-    <t>selected(data('ballard_menu1'), 'scarf')</t>
-  </si>
-  <si>
-    <t>selected(data('ballard_menu1'), 'heel')</t>
-  </si>
-  <si>
     <t>menu menu</t>
   </si>
   <si>
@@ -712,124 +559,9 @@
     <t>menu medications_menu</t>
   </si>
   <si>
-    <t>postureScore</t>
-  </si>
-  <si>
-    <t xml:space="preserve">(function() {
-  switch (data('posture_slider')) { 
-    case('posture0'):
-      return 0;
-    case('posture1'):
-      return 1;
-    case('posture2'):
-      return 2;
-    case('posture3'):
-      return 3;
-   case('posture4'):
-      return 4;  
-  }
-}())
-        </t>
-  </si>
-  <si>
-    <t>squareScore</t>
-  </si>
-  <si>
-    <t>armScore</t>
-  </si>
-  <si>
-    <t>scarfScore</t>
-  </si>
-  <si>
-    <t>heelScore</t>
-  </si>
-  <si>
-    <t>image_slider popliteal_slider</t>
-  </si>
-  <si>
-    <t>popliteal_slider</t>
-  </si>
-  <si>
     <t>Choose Popliteal Angle</t>
   </si>
   <si>
-    <t>selected(data('ballard_menu1'), 'popliteal')</t>
-  </si>
-  <si>
-    <t xml:space="preserve">(function() {
-  switch (data('arm_slider')) { 
-    case('arm_recoil0'):
-      return 0;
-    case('arm_recoil1'):
-      return 1;
-    case('arm_recoil2'):
-      return 2;
-    case('arm_recoil3'):
-      return 3;
-   case('arm_recoil4'):
-      return 4;  
-  }
-}())
-        </t>
-  </si>
-  <si>
-    <t xml:space="preserve">(function() {
-  switch (data('scarf_slider')) { 
-    case('scarf_sign-1'):
-      return -1;
-    case('scarf_sign0'):
-      return 0;
-    case('scarf_sign1'):
-      return 1;
-    case('scarf_sign2'):
-      return 2;
-    case('scarf_sign3'):
-      return 3;
-   case('scarf_sign4'):
-      return 4;  
-  }
-}())
-        </t>
-  </si>
-  <si>
-    <t xml:space="preserve">(function() {
-  switch (data('heel_slider')) { 
-    case('heel_to_ear-1'):
-      return -1;
-    case('heel_to_ear0'):
-      return 0;
-    case('heel_to_ear1'):
-      return 1;
-    case('heel_to_ear2'):
-      return 2;
-    case('heel_to_ear3'):
-      return 3;
-   case('heel_to_ear4'):
-      return 4;  
-  }
-}())
-        </t>
-  </si>
-  <si>
-    <t xml:space="preserve">(function() {
-  switch (data('square_slider')) { 
-    case('square_window-1'):
-      return -1;
-    case('square_window0'):
-      return 0;
-    case('square_window1'):
-      return 1;
-    case('square_window2'):
-      return 2;
-    case('square_window3'):
-      return 3;
-   case('square_window4'):
-      return 4;  
-  }
-}())
-        </t>
-  </si>
-  <si>
     <t>img/ballard/popliteal-1.png</t>
   </si>
   <si>
@@ -872,93 +604,9 @@
     <t>popliteal5</t>
   </si>
   <si>
-    <t xml:space="preserve">(function() {
-  switch (data('popliteal_slider')) { 
-    case('popliteal-1'):
-      return -1;
-    case('popliteal0'):
-      return 0;
-    case('popliteal1'):
-      return 1;
-    case('popliteal2'):
-      return 2;
-    case('popliteal3'):
-      return 3;
-   case('popliteal4'):
-      return 4;  
-   case('popliteal5'):
-      return 5;  
-  }
-}())
-        </t>
-  </si>
-  <si>
-    <t>totalNMScore</t>
-  </si>
-  <si>
-    <t>calculates.postureScore() + calculates.squareScore() + calculates.armScore() + calculates.poplitealScore() + calculates.scarfScore() + calculates.heelScore()</t>
-  </si>
-  <si>
-    <t>poplitealScore</t>
-  </si>
-  <si>
-    <t>ballard_menu0</t>
-  </si>
-  <si>
-    <t>ballard_menu2</t>
-  </si>
-  <si>
-    <t>neuromuscular</t>
-  </si>
-  <si>
-    <t>Neuromuscular</t>
-  </si>
-  <si>
-    <t>physical</t>
-  </si>
-  <si>
-    <t>Physical</t>
-  </si>
-  <si>
-    <t>skin</t>
-  </si>
-  <si>
     <t>Choose Skin Score</t>
   </si>
   <si>
-    <t>selected(data('ballard_menu2'), 'skin')</t>
-  </si>
-  <si>
-    <t>lanugo</t>
-  </si>
-  <si>
-    <t>selected(data('ballard_menu2'), 'lanugo')</t>
-  </si>
-  <si>
-    <t>selected(data('ballard_menu2'), 'plantar')</t>
-  </si>
-  <si>
-    <t>plantar</t>
-  </si>
-  <si>
-    <t>breast</t>
-  </si>
-  <si>
-    <t>selected(data('ballard_menu2'), 'breast')</t>
-  </si>
-  <si>
-    <t>eye_ear</t>
-  </si>
-  <si>
-    <t>selected(data('ballard_menu2'), 'eye_ear')</t>
-  </si>
-  <si>
-    <t>genitals</t>
-  </si>
-  <si>
-    <t>selected(data('ballard_menu2'), 'genitals')</t>
-  </si>
-  <si>
     <t>Choose Lanugo Score</t>
   </si>
   <si>
@@ -972,21 +620,6 @@
   </si>
   <si>
     <t>Choose Genitals Score</t>
-  </si>
-  <si>
-    <t>Skin</t>
-  </si>
-  <si>
-    <t>Lanugo</t>
-  </si>
-  <si>
-    <t>Plantar Surface</t>
-  </si>
-  <si>
-    <t>Eye/Ear</t>
-  </si>
-  <si>
-    <t>Genitals</t>
   </si>
   <si>
     <t>skin_menu</t>
@@ -1265,138 +898,6 @@
 female: majora cover clitoris &amp; minora</t>
   </si>
   <si>
-    <t>Breast</t>
-  </si>
-  <si>
-    <t>Final Score</t>
-  </si>
-  <si>
-    <t>skinScore</t>
-  </si>
-  <si>
-    <t>lanugoScore</t>
-  </si>
-  <si>
-    <t>plantarScore</t>
-  </si>
-  <si>
-    <t>breastScore</t>
-  </si>
-  <si>
-    <t>genitalsScore</t>
-  </si>
-  <si>
-    <t>totalPhysicalScore</t>
-  </si>
-  <si>
-    <t xml:space="preserve">(function() {
-  switch (data('skin_menu')) { 
-    case('skin-1'):
-      return -1;
-    case('skin0'):
-      return 0;
-    case('skin1'):
-      return 1;
-    case('skin2'):
-      return 2;
-    case('skin3'):
-      return 3;
-   case('skin4'):
-      return 4;  
-   case('skin5'):
-      return 5;  
-  }
-}())
-        </t>
-  </si>
-  <si>
-    <t xml:space="preserve">(function() {
-  switch (data('lanugo_menu')) { 
-    case('lanugo-1'):
-      return -1;
-    case('lanugo0'):
-      return 0;
-    case('lanugo1'):
-      return 1;
-    case('lanugo2'):
-      return 2;
-    case('lanugo3'):
-      return 3;
-   case('lanugo4'):
-      return 4;  
-  }
-}())
-        </t>
-  </si>
-  <si>
-    <t xml:space="preserve">(function() {
-  switch (data('plantar_menu')) { 
-    case('plantar-2'):
-      return -2;
-    case('plantar-1'):
-      return -1;
-    case('plantar0'):
-      return 0;
-    case('plantar1'):
-      return 1;
-    case('plantar2'):
-      return 2;
-    case('plantar3'):
-      return 3;
-   case('plantar4'):
-      return 4;  
-  }
-}())
-        </t>
-  </si>
-  <si>
-    <t xml:space="preserve">(function() {
-  switch (data('breast_menu')) { 
-    case('breast-1'):
-      return -1;
-    case('breast0'):
-      return 0;
-    case('breast1'):
-      return 1;
-    case('breast2'):
-      return 2;
-    case('breast3'):
-      return 3;
-   case('breast4'):
-      return 4;  
-  }
-}())
-        </t>
-  </si>
-  <si>
-    <t xml:space="preserve">(function() {
-  switch (data('genitals_menu')) { 
-    case('genitals-1'):
-      return -1;
-    case('genitals0'):
-      return 0;
-    case('genitals1'):
-      return 1;
-    case('genitals2'):
-      return 2;
-    case('genitals3'):
-      return 3;
-   case('genitals4'):
-      return 4;  
-  }
-}())
-        </t>
-  </si>
-  <si>
-    <t>final_ballard_score</t>
-  </si>
-  <si>
-    <t>totalBallardScore</t>
-  </si>
-  <si>
-    <t>calculates.totalNMScore() + calculates.totalPhysicalScore()</t>
-  </si>
-  <si>
     <t>goto diagnostics_end</t>
   </si>
   <si>
@@ -1589,37 +1090,154 @@
     <t>selected(data('diagnostic_menu'),'ballardExam')</t>
   </si>
   <si>
-    <t>eyeEarScore</t>
-  </si>
-  <si>
-    <t>calculates.skinScore() + calculates.lanugoScore() + calculates.plantarScore() + calculates.breastScore() + calculates.eyeEarScore() + calculates.genitalsScore()</t>
-  </si>
-  <si>
-    <t xml:space="preserve">(function() {
-  switch (data('eye_ear_menu')) { 
-   case('eye_ear-2'):
-      return -2;  
-    case('eye_ear-1'):
-      return -1;
-    case('eye_ear0'):
-      return 0;
-    case('eye_ear1'):
-      return 1;
-    case('eye_ear2'):
-      return 2;
-    case('eye_ear3'):
-      return 3;
-   case('eye_ear4'):
-      return 4;  
-  }
-}())
-        </t>
-  </si>
-  <si>
     <t>templatePath</t>
   </si>
   <si>
-    <t>templates/ballard_exam.handlebar</t>
+    <t>ballard</t>
+  </si>
+  <si>
+    <t>ballard_menu</t>
+  </si>
+  <si>
+    <t>selected(data('ballard_menu'), 'posture')</t>
+  </si>
+  <si>
+    <t>selected(data('ballard_menu'), 'square')</t>
+  </si>
+  <si>
+    <t>selected(data('ballard_menu'), 'skin')</t>
+  </si>
+  <si>
+    <t>selected(data('ballard_menu'), 'lanugo')</t>
+  </si>
+  <si>
+    <t>selected(data('ballard_menu'), 'plantar')</t>
+  </si>
+  <si>
+    <t>selected(data('ballard_menu'), 'breast')</t>
+  </si>
+  <si>
+    <t>selected(data('ballard_menu'), 'eye_ear')</t>
+  </si>
+  <si>
+    <t>selected(data('ballard_menu'), 'genitals')</t>
+  </si>
+  <si>
+    <t>selected(data('ballard_menu'), 'arm')</t>
+  </si>
+  <si>
+    <t>selected(data('ballard_menu'), 'popliteal')</t>
+  </si>
+  <si>
+    <t>selected(data('ballard_menu'), 'scarf')</t>
+  </si>
+  <si>
+    <t>selected(data('ballard_menu'), 'heel')</t>
+  </si>
+  <si>
+    <t>posture_menu</t>
+  </si>
+  <si>
+    <t>square_menu</t>
+  </si>
+  <si>
+    <t>arm_menu</t>
+  </si>
+  <si>
+    <t>popliteal_menu</t>
+  </si>
+  <si>
+    <t>scarf_menu</t>
+  </si>
+  <si>
+    <t>heel_menu</t>
+  </si>
+  <si>
+    <t>image_slider posture_menu</t>
+  </si>
+  <si>
+    <t>image_slider square_menu</t>
+  </si>
+  <si>
+    <t>image_slider arm_menu</t>
+  </si>
+  <si>
+    <t>image_slider popliteal_menu</t>
+  </si>
+  <si>
+    <t>image_slider scarf_menu</t>
+  </si>
+  <si>
+    <t>image_slider heel_menu</t>
+  </si>
+  <si>
+    <t>square-1</t>
+  </si>
+  <si>
+    <t>square0</t>
+  </si>
+  <si>
+    <t>square1</t>
+  </si>
+  <si>
+    <t>square2</t>
+  </si>
+  <si>
+    <t>square3</t>
+  </si>
+  <si>
+    <t>square4</t>
+  </si>
+  <si>
+    <t>arm0</t>
+  </si>
+  <si>
+    <t>arm1</t>
+  </si>
+  <si>
+    <t>arm2</t>
+  </si>
+  <si>
+    <t>arm3</t>
+  </si>
+  <si>
+    <t>arm4</t>
+  </si>
+  <si>
+    <t>scarf-1</t>
+  </si>
+  <si>
+    <t>scarf0</t>
+  </si>
+  <si>
+    <t>scarf1</t>
+  </si>
+  <si>
+    <t>scarf2</t>
+  </si>
+  <si>
+    <t>scarf3</t>
+  </si>
+  <si>
+    <t>scarf4</t>
+  </si>
+  <si>
+    <t>heel-1</t>
+  </si>
+  <si>
+    <t>heel0</t>
+  </si>
+  <si>
+    <t>heel1</t>
+  </si>
+  <si>
+    <t>heel2</t>
+  </si>
+  <si>
+    <t>heel3</t>
+  </si>
+  <si>
+    <t>heel4</t>
   </si>
 </sst>
 </file>
@@ -1752,7 +1370,7 @@
       <diagonal/>
     </border>
   </borders>
-  <cellStyleXfs count="392">
+  <cellStyleXfs count="398">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
     <xf numFmtId="0" fontId="3" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
     <xf numFmtId="0" fontId="4" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
@@ -1767,6 +1385,12 @@
     <xf numFmtId="0" fontId="5" fillId="2" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
     <xf numFmtId="0" fontId="6" fillId="3" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
     <xf numFmtId="0" fontId="1" fillId="4" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="4" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="4" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="4" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
     <xf numFmtId="0" fontId="3" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
     <xf numFmtId="0" fontId="4" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
     <xf numFmtId="0" fontId="3" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
@@ -2224,7 +1848,7 @@
       <alignment wrapText="1"/>
     </xf>
   </cellXfs>
-  <cellStyles count="392">
+  <cellStyles count="398">
     <cellStyle name="20% - Accent4" xfId="13" builtinId="42"/>
     <cellStyle name="Followed Hyperlink" xfId="2" builtinId="9" hidden="1"/>
     <cellStyle name="Followed Hyperlink" xfId="4" builtinId="9" hidden="1"/>
@@ -2420,6 +2044,9 @@
     <cellStyle name="Followed Hyperlink" xfId="387" builtinId="9" hidden="1"/>
     <cellStyle name="Followed Hyperlink" xfId="389" builtinId="9" hidden="1"/>
     <cellStyle name="Followed Hyperlink" xfId="391" builtinId="9" hidden="1"/>
+    <cellStyle name="Followed Hyperlink" xfId="393" builtinId="9" hidden="1"/>
+    <cellStyle name="Followed Hyperlink" xfId="395" builtinId="9" hidden="1"/>
+    <cellStyle name="Followed Hyperlink" xfId="397" builtinId="9" hidden="1"/>
     <cellStyle name="Good" xfId="11" builtinId="26"/>
     <cellStyle name="Hyperlink" xfId="1" builtinId="8" hidden="1"/>
     <cellStyle name="Hyperlink" xfId="3" builtinId="8" hidden="1"/>
@@ -2615,6 +2242,9 @@
     <cellStyle name="Hyperlink" xfId="386" builtinId="8" hidden="1"/>
     <cellStyle name="Hyperlink" xfId="388" builtinId="8" hidden="1"/>
     <cellStyle name="Hyperlink" xfId="390" builtinId="8" hidden="1"/>
+    <cellStyle name="Hyperlink" xfId="392" builtinId="8" hidden="1"/>
+    <cellStyle name="Hyperlink" xfId="394" builtinId="8" hidden="1"/>
+    <cellStyle name="Hyperlink" xfId="396" builtinId="8" hidden="1"/>
     <cellStyle name="Neutral" xfId="12" builtinId="28"/>
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
   </cellStyles>
@@ -2945,10 +2575,10 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <dimension ref="A1:J118"/>
+  <dimension ref="A1:J116"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="G6" zoomScale="150" zoomScaleNormal="150" zoomScalePageLayoutView="150" workbookViewId="0">
-      <selection activeCell="I14" sqref="I14"/>
+    <sheetView zoomScale="150" zoomScaleNormal="150" zoomScalePageLayoutView="150" workbookViewId="0">
+      <selection activeCell="B19" sqref="B19"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultColWidth="11.5" defaultRowHeight="12.75" customHeight="1" x14ac:dyDescent="0"/>
@@ -2963,7 +2593,7 @@
   <sheetData>
     <row r="1" spans="1:9" ht="12">
       <c r="A1" t="s">
-        <v>400</v>
+        <v>293</v>
       </c>
       <c r="B1" s="1" t="s">
         <v>0</v>
@@ -2987,7 +2617,7 @@
         <v>70</v>
       </c>
       <c r="I1" t="s">
-        <v>463</v>
+        <v>353</v>
       </c>
     </row>
     <row r="2" spans="1:9" ht="15">
@@ -3001,7 +2631,7 @@
     </row>
     <row r="3" spans="1:9" ht="12">
       <c r="B3" s="3" t="s">
-        <v>223</v>
+        <v>172</v>
       </c>
       <c r="C3" s="4" t="s">
         <v>4</v>
@@ -3026,12 +2656,12 @@
         <v>8</v>
       </c>
       <c r="B5" s="19" t="s">
-        <v>396</v>
+        <v>289</v>
       </c>
       <c r="C5" s="19"/>
       <c r="D5" s="19"/>
       <c r="E5" s="19" t="s">
-        <v>397</v>
+        <v>290</v>
       </c>
       <c r="F5" s="19"/>
       <c r="G5" s="19"/>
@@ -3040,12 +2670,12 @@
     <row r="6" spans="1:9" ht="12.75" customHeight="1">
       <c r="A6" s="21"/>
       <c r="B6" s="19" t="s">
-        <v>398</v>
+        <v>291</v>
       </c>
       <c r="C6" s="19"/>
       <c r="D6" s="19"/>
       <c r="E6" s="19" t="s">
-        <v>399</v>
+        <v>292</v>
       </c>
       <c r="F6" s="19"/>
       <c r="G6" s="19"/>
@@ -3066,7 +2696,7 @@
     <row r="8" spans="1:9" s="12" customFormat="1" ht="18" customHeight="1">
       <c r="A8" s="22"/>
       <c r="B8" t="s">
-        <v>224</v>
+        <v>173</v>
       </c>
       <c r="C8" t="s">
         <v>7</v>
@@ -3075,9 +2705,7 @@
         <v>8</v>
       </c>
       <c r="E8"/>
-      <c r="F8" t="s">
-        <v>6</v>
-      </c>
+      <c r="F8"/>
     </row>
     <row r="9" spans="1:9" ht="18" customHeight="1">
       <c r="A9" s="21"/>
@@ -3124,490 +2752,496 @@
       </c>
       <c r="F11" s="2"/>
     </row>
-    <row r="12" spans="1:9" s="13" customFormat="1" ht="18" customHeight="1">
-      <c r="B12" s="7" t="s">
-        <v>15</v>
-      </c>
-      <c r="E12" s="13" t="s">
-        <v>459</v>
-      </c>
-    </row>
-    <row r="13" spans="1:9" ht="24">
+    <row r="12" spans="1:9" ht="12">
+      <c r="A12" s="21"/>
+      <c r="B12" t="s">
+        <v>354</v>
+      </c>
+      <c r="C12" t="s">
+        <v>355</v>
+      </c>
+      <c r="E12" s="2" t="s">
+        <v>352</v>
+      </c>
+    </row>
+    <row r="13" spans="1:9" ht="11" customHeight="1">
       <c r="A13" s="21"/>
       <c r="B13" t="s">
-        <v>13</v>
-      </c>
-      <c r="E13" s="2"/>
-      <c r="I13" t="s">
-        <v>464</v>
-      </c>
-    </row>
-    <row r="14" spans="1:9" ht="12">
-      <c r="A14" s="27"/>
-      <c r="B14" s="11" t="s">
-        <v>25</v>
-      </c>
-      <c r="C14" s="11"/>
-      <c r="D14" s="11"/>
-      <c r="E14" s="11"/>
-      <c r="F14" s="11"/>
-      <c r="G14" s="11"/>
-      <c r="H14" s="11"/>
+        <v>374</v>
+      </c>
+      <c r="C13" t="s">
+        <v>368</v>
+      </c>
+      <c r="D13" t="s">
+        <v>131</v>
+      </c>
+      <c r="E13" s="2" t="s">
+        <v>356</v>
+      </c>
+    </row>
+    <row r="14" spans="1:9" ht="11" customHeight="1">
+      <c r="A14" s="21"/>
+      <c r="B14" t="s">
+        <v>375</v>
+      </c>
+      <c r="C14" t="s">
+        <v>369</v>
+      </c>
+      <c r="D14" t="s">
+        <v>132</v>
+      </c>
+      <c r="E14" s="2" t="s">
+        <v>357</v>
+      </c>
     </row>
     <row r="15" spans="1:9" ht="11" customHeight="1">
       <c r="A15" s="21"/>
       <c r="B15" t="s">
-        <v>144</v>
+        <v>376</v>
       </c>
       <c r="C15" t="s">
-        <v>145</v>
+        <v>370</v>
       </c>
       <c r="D15" t="s">
         <v>146</v>
       </c>
       <c r="E15" s="2" t="s">
-        <v>147</v>
+        <v>364</v>
       </c>
     </row>
     <row r="16" spans="1:9" ht="11" customHeight="1">
       <c r="A16" s="21"/>
       <c r="B16" t="s">
-        <v>148</v>
+        <v>377</v>
       </c>
       <c r="C16" t="s">
-        <v>149</v>
+        <v>371</v>
       </c>
       <c r="D16" t="s">
-        <v>150</v>
+        <v>178</v>
       </c>
       <c r="E16" s="2" t="s">
-        <v>151</v>
+        <v>365</v>
       </c>
     </row>
     <row r="17" spans="1:10" ht="11" customHeight="1">
       <c r="A17" s="21"/>
       <c r="B17" t="s">
-        <v>165</v>
+        <v>378</v>
       </c>
       <c r="C17" t="s">
-        <v>166</v>
+        <v>372</v>
       </c>
       <c r="D17" t="s">
-        <v>167</v>
+        <v>147</v>
       </c>
       <c r="E17" s="2" t="s">
-        <v>168</v>
+        <v>366</v>
       </c>
     </row>
     <row r="18" spans="1:10" ht="11" customHeight="1">
       <c r="A18" s="21"/>
       <c r="B18" t="s">
-        <v>235</v>
+        <v>379</v>
       </c>
       <c r="C18" t="s">
-        <v>236</v>
+        <v>373</v>
       </c>
       <c r="D18" t="s">
-        <v>237</v>
+        <v>148</v>
       </c>
       <c r="E18" s="2" t="s">
-        <v>238</v>
+        <v>367</v>
       </c>
     </row>
     <row r="19" spans="1:10" ht="11" customHeight="1">
       <c r="A19" s="21"/>
       <c r="B19" t="s">
-        <v>169</v>
+        <v>219</v>
       </c>
       <c r="C19" t="s">
-        <v>170</v>
+        <v>199</v>
       </c>
       <c r="D19" t="s">
-        <v>171</v>
+        <v>193</v>
       </c>
       <c r="E19" s="2" t="s">
-        <v>221</v>
+        <v>358</v>
       </c>
     </row>
     <row r="20" spans="1:10" ht="11" customHeight="1">
       <c r="A20" s="21"/>
       <c r="B20" t="s">
-        <v>172</v>
+        <v>220</v>
       </c>
       <c r="C20" t="s">
-        <v>173</v>
+        <v>200</v>
       </c>
       <c r="D20" t="s">
-        <v>174</v>
+        <v>194</v>
       </c>
       <c r="E20" s="2" t="s">
-        <v>222</v>
+        <v>359</v>
       </c>
     </row>
     <row r="21" spans="1:10" ht="11" customHeight="1">
       <c r="A21" s="21"/>
       <c r="B21" t="s">
-        <v>310</v>
+        <v>221</v>
       </c>
       <c r="C21" t="s">
-        <v>290</v>
+        <v>201</v>
       </c>
       <c r="D21" t="s">
-        <v>268</v>
+        <v>197</v>
       </c>
       <c r="E21" s="2" t="s">
-        <v>269</v>
+        <v>360</v>
       </c>
     </row>
     <row r="22" spans="1:10" ht="11" customHeight="1">
       <c r="A22" s="21"/>
       <c r="B22" t="s">
-        <v>311</v>
+        <v>222</v>
       </c>
       <c r="C22" t="s">
-        <v>291</v>
+        <v>202</v>
       </c>
       <c r="D22" t="s">
-        <v>280</v>
+        <v>195</v>
       </c>
       <c r="E22" s="2" t="s">
-        <v>271</v>
+        <v>361</v>
       </c>
     </row>
     <row r="23" spans="1:10" ht="11" customHeight="1">
       <c r="A23" s="21"/>
       <c r="B23" t="s">
-        <v>312</v>
+        <v>223</v>
       </c>
       <c r="C23" t="s">
-        <v>292</v>
+        <v>203</v>
       </c>
       <c r="D23" t="s">
-        <v>283</v>
+        <v>196</v>
       </c>
       <c r="E23" s="2" t="s">
-        <v>272</v>
-      </c>
-    </row>
-    <row r="24" spans="1:10" ht="11" customHeight="1">
+        <v>362</v>
+      </c>
+    </row>
+    <row r="24" spans="1:10" ht="12" customHeight="1">
       <c r="A24" s="21"/>
       <c r="B24" t="s">
+        <v>224</v>
+      </c>
+      <c r="C24" t="s">
+        <v>204</v>
+      </c>
+      <c r="D24" t="s">
+        <v>198</v>
+      </c>
+      <c r="E24" s="2" t="s">
+        <v>363</v>
+      </c>
+    </row>
+    <row r="25" spans="1:10" ht="15">
+      <c r="A25" s="21"/>
+      <c r="B25" s="15" t="s">
+        <v>72</v>
+      </c>
+      <c r="C25" s="15"/>
+      <c r="D25" s="15"/>
+      <c r="E25" s="15"/>
+      <c r="F25" s="15"/>
+      <c r="G25" s="15"/>
+      <c r="H25" s="15"/>
+    </row>
+    <row r="26" spans="1:10" ht="15">
+      <c r="B26" s="23"/>
+      <c r="C26" s="12"/>
+      <c r="D26" s="12"/>
+      <c r="E26" s="12"/>
+      <c r="F26" s="12"/>
+      <c r="G26" s="12"/>
+      <c r="H26" s="12"/>
+    </row>
+    <row r="27" spans="1:10" s="15" customFormat="1" ht="15">
+      <c r="A27" s="21" t="s">
         <v>313</v>
       </c>
-      <c r="C24" t="s">
-        <v>293</v>
-      </c>
-      <c r="D24" t="s">
-        <v>281</v>
-      </c>
-      <c r="E24" s="2" t="s">
-        <v>275</v>
-      </c>
-    </row>
-    <row r="25" spans="1:10" ht="11" customHeight="1">
-      <c r="A25" s="21"/>
-      <c r="B25" t="s">
-        <v>314</v>
-      </c>
-      <c r="C25" t="s">
-        <v>294</v>
-      </c>
-      <c r="D25" t="s">
-        <v>282</v>
-      </c>
-      <c r="E25" s="2" t="s">
-        <v>277</v>
-      </c>
-    </row>
-    <row r="26" spans="1:10" ht="12" customHeight="1">
-      <c r="A26" s="21"/>
-      <c r="B26" t="s">
-        <v>315</v>
-      </c>
-      <c r="C26" t="s">
-        <v>295</v>
-      </c>
-      <c r="D26" t="s">
-        <v>284</v>
-      </c>
-      <c r="E26" s="2" t="s">
-        <v>279</v>
-      </c>
-    </row>
-    <row r="27" spans="1:10" ht="15">
-      <c r="A27" s="21"/>
-      <c r="B27" s="15" t="s">
-        <v>72</v>
-      </c>
-      <c r="C27" s="15"/>
-      <c r="D27" s="15"/>
-      <c r="E27" s="15"/>
-      <c r="F27" s="15"/>
-      <c r="G27" s="15"/>
-      <c r="H27" s="15"/>
-    </row>
-    <row r="28" spans="1:10" ht="15">
-      <c r="B28" s="23"/>
-      <c r="C28" s="12"/>
-      <c r="D28" s="12"/>
-      <c r="E28" s="12"/>
-      <c r="F28" s="12"/>
-      <c r="G28" s="12"/>
-      <c r="H28" s="12"/>
-    </row>
-    <row r="29" spans="1:10" s="15" customFormat="1" ht="15">
-      <c r="A29" s="21" t="s">
-        <v>420</v>
-      </c>
-      <c r="B29" s="13" t="s">
+      <c r="B27" s="13" t="s">
         <v>105</v>
       </c>
-      <c r="C29" s="13"/>
-      <c r="D29" s="13"/>
-      <c r="E29" s="13" t="s">
+      <c r="C27" s="13"/>
+      <c r="D27" s="13"/>
+      <c r="E27" s="13" t="s">
         <v>71</v>
       </c>
-      <c r="F29" s="13"/>
-      <c r="G29" s="13"/>
-      <c r="H29" s="13"/>
-      <c r="I29" s="12"/>
-      <c r="J29" s="12"/>
+      <c r="F27" s="13"/>
+      <c r="G27" s="13"/>
+      <c r="H27" s="13"/>
+      <c r="I27" s="12"/>
+      <c r="J27" s="12"/>
+    </row>
+    <row r="28" spans="1:10" ht="12">
+      <c r="A28" s="21"/>
+      <c r="B28" s="5" t="s">
+        <v>73</v>
+      </c>
+      <c r="C28" s="5"/>
+      <c r="D28" s="5"/>
+      <c r="E28" s="6" t="s">
+        <v>74</v>
+      </c>
+      <c r="F28" s="5"/>
+      <c r="G28" s="5"/>
+      <c r="H28" s="5"/>
+    </row>
+    <row r="29" spans="1:10" ht="15">
+      <c r="A29" s="21"/>
+      <c r="B29" s="15" t="s">
+        <v>104</v>
+      </c>
+      <c r="C29" s="15"/>
+      <c r="D29" s="15"/>
+      <c r="E29" s="15"/>
+      <c r="F29" s="15"/>
+      <c r="G29" s="15"/>
+      <c r="H29" s="15"/>
     </row>
     <row r="30" spans="1:10" ht="12">
       <c r="A30" s="21"/>
-      <c r="B30" s="5" t="s">
-        <v>73</v>
-      </c>
-      <c r="C30" s="5"/>
-      <c r="D30" s="5"/>
-      <c r="E30" s="6" t="s">
-        <v>74</v>
-      </c>
-      <c r="F30" s="5"/>
-      <c r="G30" s="5"/>
-      <c r="H30" s="5"/>
-    </row>
-    <row r="31" spans="1:10" ht="15">
+      <c r="B30" s="12" t="s">
+        <v>174</v>
+      </c>
+      <c r="C30" s="12" t="s">
+        <v>9</v>
+      </c>
+      <c r="D30" s="12" t="s">
+        <v>10</v>
+      </c>
+      <c r="E30" s="12"/>
+      <c r="F30" s="12" t="s">
+        <v>6</v>
+      </c>
+      <c r="G30" s="12"/>
+      <c r="H30" s="12"/>
+    </row>
+    <row r="31" spans="1:10" ht="12">
       <c r="A31" s="21"/>
-      <c r="B31" s="15" t="s">
-        <v>104</v>
-      </c>
-      <c r="C31" s="15"/>
-      <c r="D31" s="15"/>
-      <c r="E31" s="15"/>
-      <c r="F31" s="15"/>
-      <c r="G31" s="15"/>
-      <c r="H31" s="15"/>
-    </row>
-    <row r="32" spans="1:10" ht="12">
+      <c r="B31" s="7" t="s">
+        <v>15</v>
+      </c>
+      <c r="C31" s="8"/>
+      <c r="D31" s="8"/>
+      <c r="E31" s="9" t="s">
+        <v>63</v>
+      </c>
+      <c r="F31" s="8"/>
+      <c r="G31" s="10"/>
+      <c r="H31" s="10"/>
+    </row>
+    <row r="32" spans="1:10" ht="12.75" customHeight="1">
       <c r="A32" s="21"/>
-      <c r="B32" s="12" t="s">
-        <v>225</v>
-      </c>
-      <c r="C32" s="12" t="s">
-        <v>9</v>
-      </c>
-      <c r="D32" s="12" t="s">
-        <v>10</v>
-      </c>
-      <c r="E32" s="12"/>
-      <c r="F32" s="12" t="s">
-        <v>6</v>
-      </c>
-      <c r="G32" s="12"/>
-      <c r="H32" s="12"/>
-    </row>
-    <row r="33" spans="1:8" ht="12">
+      <c r="B32" s="4" t="s">
+        <v>13</v>
+      </c>
+      <c r="C32" s="2" t="s">
+        <v>75</v>
+      </c>
+      <c r="D32" s="2" t="s">
+        <v>294</v>
+      </c>
+      <c r="E32" s="2"/>
+      <c r="F32" s="4"/>
+    </row>
+    <row r="33" spans="1:6" ht="12.75" customHeight="1">
       <c r="A33" s="21"/>
-      <c r="B33" s="7" t="s">
-        <v>15</v>
-      </c>
-      <c r="C33" s="8"/>
-      <c r="D33" s="8"/>
-      <c r="E33" s="9" t="s">
-        <v>63</v>
-      </c>
-      <c r="F33" s="8"/>
-      <c r="G33" s="10"/>
-      <c r="H33" s="10"/>
-    </row>
-    <row r="34" spans="1:8" ht="12.75" customHeight="1">
+      <c r="B33" s="4" t="s">
+        <v>13</v>
+      </c>
+      <c r="D33" t="s">
+        <v>295</v>
+      </c>
+      <c r="E33" s="2"/>
+      <c r="F33" s="4"/>
+    </row>
+    <row r="34" spans="1:6" ht="12.75" customHeight="1">
       <c r="A34" s="21"/>
-      <c r="B34" s="4" t="s">
+      <c r="B34" t="s">
         <v>13</v>
       </c>
-      <c r="C34" s="2" t="s">
-        <v>75</v>
-      </c>
+      <c r="C34" s="2"/>
       <c r="D34" s="2" t="s">
-        <v>401</v>
+        <v>296</v>
       </c>
       <c r="E34" s="2"/>
       <c r="F34" s="4"/>
     </row>
-    <row r="35" spans="1:8" ht="12.75" customHeight="1">
+    <row r="35" spans="1:6" ht="12.75" customHeight="1">
       <c r="A35" s="21"/>
-      <c r="B35" s="4" t="s">
+      <c r="B35" s="2" t="s">
         <v>13</v>
       </c>
-      <c r="D35" t="s">
-        <v>402</v>
+      <c r="C35" s="2"/>
+      <c r="D35" s="2" t="s">
+        <v>297</v>
       </c>
       <c r="E35" s="2"/>
       <c r="F35" s="4"/>
     </row>
-    <row r="36" spans="1:8" ht="12.75" customHeight="1">
+    <row r="36" spans="1:6" ht="12.75" customHeight="1">
       <c r="A36" s="21"/>
-      <c r="B36" t="s">
+      <c r="B36" s="2" t="s">
         <v>13</v>
       </c>
       <c r="C36" s="2"/>
       <c r="D36" s="2" t="s">
-        <v>403</v>
+        <v>298</v>
       </c>
       <c r="E36" s="2"/>
       <c r="F36" s="4"/>
     </row>
-    <row r="37" spans="1:8" ht="12.75" customHeight="1">
+    <row r="37" spans="1:6" ht="12.75" customHeight="1">
       <c r="A37" s="21"/>
       <c r="B37" s="2" t="s">
         <v>13</v>
       </c>
       <c r="C37" s="2"/>
       <c r="D37" s="2" t="s">
-        <v>404</v>
+        <v>299</v>
       </c>
       <c r="E37" s="2"/>
       <c r="F37" s="4"/>
     </row>
-    <row r="38" spans="1:8" ht="12.75" customHeight="1">
+    <row r="38" spans="1:6" ht="12.75" customHeight="1">
       <c r="A38" s="21"/>
       <c r="B38" s="2" t="s">
         <v>13</v>
       </c>
       <c r="C38" s="2"/>
       <c r="D38" s="2" t="s">
-        <v>405</v>
+        <v>300</v>
       </c>
       <c r="E38" s="2"/>
       <c r="F38" s="4"/>
     </row>
-    <row r="39" spans="1:8" ht="12.75" customHeight="1">
+    <row r="39" spans="1:6" ht="12.75" customHeight="1">
       <c r="A39" s="21"/>
       <c r="B39" s="2" t="s">
         <v>13</v>
       </c>
       <c r="C39" s="2"/>
       <c r="D39" s="2" t="s">
-        <v>406</v>
+        <v>301</v>
       </c>
       <c r="E39" s="2"/>
       <c r="F39" s="4"/>
     </row>
-    <row r="40" spans="1:8" ht="12.75" customHeight="1">
+    <row r="40" spans="1:6" ht="12.75" customHeight="1">
       <c r="A40" s="21"/>
       <c r="B40" s="2" t="s">
         <v>13</v>
       </c>
       <c r="C40" s="2"/>
       <c r="D40" s="2" t="s">
-        <v>407</v>
+        <v>309</v>
       </c>
       <c r="E40" s="2"/>
       <c r="F40" s="4"/>
     </row>
-    <row r="41" spans="1:8" ht="12.75" customHeight="1">
+    <row r="41" spans="1:6" ht="12.75" customHeight="1">
       <c r="A41" s="21"/>
       <c r="B41" s="2" t="s">
         <v>13</v>
       </c>
       <c r="C41" s="2"/>
       <c r="D41" s="2" t="s">
-        <v>408</v>
+        <v>308</v>
       </c>
       <c r="E41" s="2"/>
       <c r="F41" s="4"/>
     </row>
-    <row r="42" spans="1:8" ht="12.75" customHeight="1">
+    <row r="42" spans="1:6" ht="12.75" customHeight="1">
       <c r="A42" s="21"/>
       <c r="B42" s="2" t="s">
         <v>13</v>
       </c>
       <c r="C42" s="2"/>
       <c r="D42" s="2" t="s">
-        <v>416</v>
+        <v>310</v>
       </c>
       <c r="E42" s="2"/>
       <c r="F42" s="4"/>
     </row>
-    <row r="43" spans="1:8" ht="12.75" customHeight="1">
+    <row r="43" spans="1:6" ht="12.75" customHeight="1">
       <c r="A43" s="21"/>
       <c r="B43" s="2" t="s">
         <v>13</v>
       </c>
       <c r="C43" s="2"/>
       <c r="D43" s="2" t="s">
-        <v>415</v>
+        <v>311</v>
       </c>
       <c r="E43" s="2"/>
       <c r="F43" s="4"/>
     </row>
-    <row r="44" spans="1:8" ht="12.75" customHeight="1">
+    <row r="44" spans="1:6" ht="12.75" customHeight="1">
       <c r="A44" s="21"/>
       <c r="B44" s="2" t="s">
         <v>13</v>
       </c>
       <c r="C44" s="2"/>
       <c r="D44" s="2" t="s">
-        <v>417</v>
+        <v>302</v>
       </c>
       <c r="E44" s="2"/>
       <c r="F44" s="4"/>
     </row>
-    <row r="45" spans="1:8" ht="12.75" customHeight="1">
+    <row r="45" spans="1:6" ht="12.75" customHeight="1">
       <c r="A45" s="21"/>
       <c r="B45" s="2" t="s">
         <v>13</v>
       </c>
       <c r="C45" s="2"/>
       <c r="D45" s="2" t="s">
-        <v>418</v>
+        <v>305</v>
       </c>
       <c r="E45" s="2"/>
       <c r="F45" s="4"/>
     </row>
-    <row r="46" spans="1:8" ht="12.75" customHeight="1">
+    <row r="46" spans="1:6" ht="12.75" customHeight="1">
       <c r="A46" s="21"/>
       <c r="B46" s="2" t="s">
         <v>13</v>
       </c>
       <c r="C46" s="2"/>
       <c r="D46" s="2" t="s">
-        <v>409</v>
+        <v>306</v>
       </c>
       <c r="E46" s="2"/>
       <c r="F46" s="4"/>
     </row>
-    <row r="47" spans="1:8" ht="12.75" customHeight="1">
+    <row r="47" spans="1:6" ht="12.75" customHeight="1">
       <c r="A47" s="21"/>
       <c r="B47" s="2" t="s">
         <v>13</v>
       </c>
       <c r="C47" s="2"/>
       <c r="D47" s="2" t="s">
-        <v>412</v>
+        <v>307</v>
       </c>
       <c r="E47" s="2"/>
       <c r="F47" s="4"/>
     </row>
-    <row r="48" spans="1:8" ht="12.75" customHeight="1">
+    <row r="48" spans="1:6" ht="12.75" customHeight="1">
       <c r="A48" s="21"/>
       <c r="B48" s="2" t="s">
         <v>13</v>
       </c>
       <c r="C48" s="2"/>
       <c r="D48" s="2" t="s">
-        <v>413</v>
+        <v>303</v>
       </c>
       <c r="E48" s="2"/>
       <c r="F48" s="4"/>
@@ -3619,19 +3253,19 @@
       </c>
       <c r="C49" s="2"/>
       <c r="D49" s="2" t="s">
-        <v>414</v>
+        <v>304</v>
       </c>
       <c r="E49" s="2"/>
       <c r="F49" s="4"/>
     </row>
-    <row r="50" spans="1:8" ht="12.75" customHeight="1">
+    <row r="50" spans="1:8" ht="17" customHeight="1">
       <c r="A50" s="21"/>
       <c r="B50" s="2" t="s">
         <v>13</v>
       </c>
       <c r="C50" s="2"/>
       <c r="D50" s="2" t="s">
-        <v>410</v>
+        <v>312</v>
       </c>
       <c r="E50" s="2"/>
       <c r="F50" s="4"/>
@@ -3642,21 +3276,15 @@
         <v>13</v>
       </c>
       <c r="C51" s="2"/>
-      <c r="D51" s="2" t="s">
-        <v>411</v>
-      </c>
+      <c r="D51" s="2"/>
       <c r="E51" s="2"/>
       <c r="F51" s="4"/>
     </row>
-    <row r="52" spans="1:8" ht="17" customHeight="1">
+    <row r="52" spans="1:8" ht="12.75" customHeight="1">
       <c r="A52" s="21"/>
-      <c r="B52" s="2" t="s">
-        <v>13</v>
-      </c>
+      <c r="B52" s="4"/>
       <c r="C52" s="2"/>
-      <c r="D52" s="2" t="s">
-        <v>419</v>
-      </c>
+      <c r="D52" s="2"/>
       <c r="E52" s="2"/>
       <c r="F52" s="4"/>
     </row>
@@ -3665,334 +3293,337 @@
       <c r="B53" s="2" t="s">
         <v>13</v>
       </c>
-      <c r="C53" s="2"/>
+      <c r="C53" s="2" t="s">
+        <v>76</v>
+      </c>
       <c r="D53" s="2"/>
       <c r="E53" s="2"/>
       <c r="F53" s="4"/>
+      <c r="G53" t="s">
+        <v>14</v>
+      </c>
     </row>
     <row r="54" spans="1:8" ht="12.75" customHeight="1">
       <c r="A54" s="21"/>
-      <c r="B54" s="4"/>
-      <c r="C54" s="2"/>
-      <c r="D54" s="2"/>
-      <c r="E54" s="2"/>
-      <c r="F54" s="4"/>
+      <c r="B54" t="s">
+        <v>13</v>
+      </c>
+      <c r="D54" t="s">
+        <v>77</v>
+      </c>
+      <c r="E54" s="13"/>
     </row>
     <row r="55" spans="1:8" ht="12.75" customHeight="1">
       <c r="A55" s="21"/>
-      <c r="B55" s="2" t="s">
+      <c r="B55" t="s">
         <v>13</v>
       </c>
-      <c r="C55" s="2" t="s">
-        <v>76</v>
-      </c>
-      <c r="D55" s="2"/>
-      <c r="E55" s="2"/>
-      <c r="F55" s="4"/>
-      <c r="G55" t="s">
-        <v>14</v>
-      </c>
-    </row>
-    <row r="56" spans="1:8" ht="12.75" customHeight="1">
+      <c r="H55" t="s">
+        <v>78</v>
+      </c>
+    </row>
+    <row r="56" spans="1:8" ht="12">
       <c r="A56" s="21"/>
-      <c r="B56" t="s">
+      <c r="B56" s="11" t="s">
+        <v>25</v>
+      </c>
+      <c r="C56" s="10"/>
+      <c r="D56" s="10"/>
+      <c r="E56" s="10"/>
+      <c r="F56" s="10"/>
+      <c r="G56" s="10"/>
+      <c r="H56" s="10"/>
+    </row>
+    <row r="57" spans="1:8" s="10" customFormat="1" ht="12"/>
+    <row r="58" spans="1:8" s="10" customFormat="1" ht="15">
+      <c r="B58" s="10" t="s">
+        <v>343</v>
+      </c>
+      <c r="E58" s="13" t="s">
+        <v>348</v>
+      </c>
+    </row>
+    <row r="59" spans="1:8" s="10" customFormat="1" ht="15">
+      <c r="B59" s="10" t="s">
+        <v>344</v>
+      </c>
+      <c r="E59" s="37" t="s">
+        <v>347</v>
+      </c>
+    </row>
+    <row r="60" spans="1:8" s="10" customFormat="1" ht="12">
+      <c r="B60" s="10" t="s">
+        <v>345</v>
+      </c>
+    </row>
+    <row r="61" spans="1:8" s="10" customFormat="1" ht="12">
+      <c r="B61" s="10" t="s">
         <v>13</v>
       </c>
-      <c r="D56" t="s">
-        <v>77</v>
-      </c>
-      <c r="E56" s="13"/>
-    </row>
-    <row r="57" spans="1:8" ht="12.75" customHeight="1">
-      <c r="A57" s="21"/>
-      <c r="B57" t="s">
-        <v>13</v>
-      </c>
-      <c r="H57" t="s">
-        <v>78</v>
-      </c>
-    </row>
-    <row r="58" spans="1:8" ht="12">
-      <c r="A58" s="21"/>
-      <c r="B58" s="11" t="s">
-        <v>25</v>
-      </c>
-      <c r="C58" s="10"/>
-      <c r="D58" s="10"/>
-      <c r="E58" s="10"/>
-      <c r="F58" s="10"/>
-      <c r="G58" s="10"/>
-      <c r="H58" s="10"/>
-    </row>
-    <row r="59" spans="1:8" s="10" customFormat="1" ht="12"/>
-    <row r="60" spans="1:8" s="10" customFormat="1" ht="15">
-      <c r="B60" s="10" t="s">
-        <v>450</v>
-      </c>
-      <c r="E60" s="13" t="s">
-        <v>455</v>
-      </c>
-    </row>
-    <row r="61" spans="1:8" s="10" customFormat="1" ht="15">
-      <c r="B61" s="10" t="s">
-        <v>451</v>
-      </c>
-      <c r="E61" s="37" t="s">
-        <v>454</v>
+      <c r="D61" s="10" t="s">
+        <v>42</v>
       </c>
     </row>
     <row r="62" spans="1:8" s="10" customFormat="1" ht="12">
       <c r="B62" s="10" t="s">
-        <v>452</v>
-      </c>
-    </row>
-    <row r="63" spans="1:8" s="10" customFormat="1" ht="12">
-      <c r="B63" s="10" t="s">
-        <v>13</v>
-      </c>
-      <c r="D63" s="10" t="s">
-        <v>42</v>
-      </c>
-    </row>
-    <row r="64" spans="1:8" s="10" customFormat="1" ht="12">
-      <c r="B64" s="10" t="s">
-        <v>453</v>
-      </c>
-    </row>
-    <row r="65" spans="1:8" s="10" customFormat="1" ht="12"/>
-    <row r="66" spans="1:8" ht="30">
+        <v>346</v>
+      </c>
+    </row>
+    <row r="63" spans="1:8" s="10" customFormat="1" ht="12"/>
+    <row r="64" spans="1:8" ht="30">
+      <c r="A64" s="21"/>
+      <c r="B64" s="13" t="s">
+        <v>318</v>
+      </c>
+      <c r="C64" s="13"/>
+      <c r="D64" s="13"/>
+      <c r="E64" s="13" t="s">
+        <v>314</v>
+      </c>
+      <c r="F64" s="13"/>
+      <c r="G64" s="13"/>
+      <c r="H64" s="13"/>
+    </row>
+    <row r="65" spans="1:8" ht="30">
+      <c r="A65" s="21"/>
+      <c r="B65" s="13" t="s">
+        <v>319</v>
+      </c>
+      <c r="C65" s="13"/>
+      <c r="D65" s="13"/>
+      <c r="E65" s="13" t="s">
+        <v>320</v>
+      </c>
+      <c r="F65" s="13"/>
+      <c r="G65" s="13"/>
+      <c r="H65" s="13"/>
+    </row>
+    <row r="66" spans="1:8" ht="15">
       <c r="A66" s="21"/>
-      <c r="B66" s="13" t="s">
-        <v>425</v>
-      </c>
-      <c r="C66" s="13"/>
-      <c r="D66" s="13"/>
-      <c r="E66" s="13" t="s">
-        <v>421</v>
-      </c>
-      <c r="F66" s="13"/>
-      <c r="G66" s="13"/>
-      <c r="H66" s="13"/>
-    </row>
-    <row r="67" spans="1:8" ht="30">
+      <c r="B66" s="15" t="s">
+        <v>316</v>
+      </c>
+      <c r="C66" s="15"/>
+      <c r="D66" s="15"/>
+      <c r="E66" s="15"/>
+      <c r="F66" s="15"/>
+      <c r="G66" s="15"/>
+      <c r="H66" s="15"/>
+    </row>
+    <row r="67" spans="1:8" ht="12">
       <c r="A67" s="21"/>
-      <c r="B67" s="13" t="s">
-        <v>426</v>
-      </c>
-      <c r="C67" s="13"/>
-      <c r="D67" s="13"/>
-      <c r="E67" s="13" t="s">
-        <v>427</v>
-      </c>
-      <c r="F67" s="13"/>
-      <c r="G67" s="13"/>
-      <c r="H67" s="13"/>
-    </row>
-    <row r="68" spans="1:8" ht="15">
+      <c r="B67" s="10"/>
+      <c r="C67" s="10"/>
+      <c r="D67" s="10"/>
+      <c r="E67" s="10"/>
+      <c r="F67" s="10"/>
+      <c r="G67" s="10"/>
+      <c r="H67" s="10"/>
+    </row>
+    <row r="68" spans="1:8" ht="24">
       <c r="A68" s="21"/>
-      <c r="B68" s="15" t="s">
-        <v>423</v>
-      </c>
-      <c r="C68" s="15"/>
-      <c r="D68" s="15"/>
-      <c r="E68" s="15"/>
-      <c r="F68" s="15"/>
-      <c r="G68" s="15"/>
-      <c r="H68" s="15"/>
-    </row>
-    <row r="69" spans="1:8" ht="12">
+      <c r="B68" t="s">
+        <v>327</v>
+      </c>
+      <c r="C68" t="s">
+        <v>326</v>
+      </c>
+      <c r="F68" t="s">
+        <v>6</v>
+      </c>
+      <c r="G68" s="10"/>
+      <c r="H68" s="10"/>
+    </row>
+    <row r="69" spans="1:8" ht="30">
       <c r="A69" s="21"/>
-      <c r="B69" s="10"/>
-      <c r="C69" s="10"/>
-      <c r="D69" s="10"/>
-      <c r="E69" s="10"/>
-      <c r="F69" s="10"/>
+      <c r="B69" s="13" t="s">
+        <v>332</v>
+      </c>
+      <c r="C69" s="13"/>
+      <c r="D69" s="13"/>
+      <c r="E69" s="13" t="s">
+        <v>329</v>
+      </c>
+      <c r="F69" s="13"/>
       <c r="G69" s="10"/>
       <c r="H69" s="10"/>
     </row>
-    <row r="70" spans="1:8" ht="24">
+    <row r="70" spans="1:8" ht="30">
       <c r="A70" s="21"/>
-      <c r="B70" t="s">
-        <v>434</v>
-      </c>
-      <c r="C70" t="s">
-        <v>433</v>
-      </c>
-      <c r="F70" t="s">
-        <v>6</v>
-      </c>
+      <c r="B70" s="13" t="s">
+        <v>333</v>
+      </c>
+      <c r="C70" s="13"/>
+      <c r="D70" s="13"/>
+      <c r="E70" s="13" t="s">
+        <v>334</v>
+      </c>
+      <c r="F70" s="13"/>
       <c r="G70" s="10"/>
       <c r="H70" s="10"/>
     </row>
-    <row r="71" spans="1:8" ht="30">
+    <row r="71" spans="1:8" ht="15">
       <c r="A71" s="21"/>
-      <c r="B71" s="13" t="s">
-        <v>439</v>
-      </c>
-      <c r="C71" s="13"/>
-      <c r="D71" s="13"/>
-      <c r="E71" s="13" t="s">
-        <v>436</v>
-      </c>
-      <c r="F71" s="13"/>
+      <c r="B71" s="15" t="s">
+        <v>330</v>
+      </c>
+      <c r="C71" s="15"/>
+      <c r="D71" s="15"/>
+      <c r="E71" s="15"/>
       <c r="G71" s="10"/>
       <c r="H71" s="10"/>
     </row>
-    <row r="72" spans="1:8" ht="30">
+    <row r="72" spans="1:8" ht="12">
       <c r="A72" s="21"/>
-      <c r="B72" s="13" t="s">
-        <v>440</v>
-      </c>
-      <c r="C72" s="13"/>
-      <c r="D72" s="13"/>
-      <c r="E72" s="13" t="s">
-        <v>441</v>
-      </c>
-      <c r="F72" s="13"/>
+      <c r="B72" t="s">
+        <v>15</v>
+      </c>
       <c r="G72" s="10"/>
       <c r="H72" s="10"/>
     </row>
-    <row r="73" spans="1:8" ht="15">
+    <row r="73" spans="1:8" ht="12">
       <c r="A73" s="21"/>
-      <c r="B73" s="15" t="s">
-        <v>437</v>
-      </c>
-      <c r="C73" s="15"/>
-      <c r="D73" s="15"/>
-      <c r="E73" s="15"/>
+      <c r="B73" s="2" t="s">
+        <v>13</v>
+      </c>
+      <c r="C73" s="12"/>
+      <c r="D73" s="25" t="s">
+        <v>341</v>
+      </c>
+      <c r="E73" s="12"/>
+      <c r="F73" s="12"/>
       <c r="G73" s="10"/>
       <c r="H73" s="10"/>
     </row>
     <row r="74" spans="1:8" ht="12">
       <c r="A74" s="21"/>
-      <c r="B74" t="s">
-        <v>15</v>
-      </c>
+      <c r="B74" s="2" t="s">
+        <v>25</v>
+      </c>
+      <c r="C74" s="12"/>
+      <c r="D74" s="25"/>
+      <c r="E74" s="12"/>
+      <c r="F74" s="12"/>
       <c r="G74" s="10"/>
       <c r="H74" s="10"/>
     </row>
-    <row r="75" spans="1:8" ht="12">
+    <row r="75" spans="1:8" ht="15">
       <c r="A75" s="21"/>
-      <c r="B75" s="2" t="s">
-        <v>13</v>
-      </c>
-      <c r="C75" s="12"/>
-      <c r="D75" s="25" t="s">
-        <v>448</v>
-      </c>
-      <c r="E75" s="12"/>
+      <c r="B75" s="15" t="s">
+        <v>331</v>
+      </c>
+      <c r="C75" s="18"/>
+      <c r="D75" s="31"/>
+      <c r="E75" s="18"/>
       <c r="F75" s="12"/>
       <c r="G75" s="10"/>
       <c r="H75" s="10"/>
     </row>
-    <row r="76" spans="1:8" ht="12">
-      <c r="A76" s="21"/>
-      <c r="B76" s="2" t="s">
-        <v>25</v>
-      </c>
-      <c r="C76" s="12"/>
-      <c r="D76" s="25"/>
-      <c r="E76" s="12"/>
-      <c r="F76" s="12"/>
-      <c r="G76" s="10"/>
-      <c r="H76" s="10"/>
-    </row>
-    <row r="77" spans="1:8" ht="15">
-      <c r="A77" s="21"/>
-      <c r="B77" s="15" t="s">
-        <v>438</v>
-      </c>
-      <c r="C77" s="18"/>
-      <c r="D77" s="31"/>
-      <c r="E77" s="18"/>
-      <c r="F77" s="12"/>
-      <c r="G77" s="10"/>
-      <c r="H77" s="10"/>
-    </row>
-    <row r="78" spans="1:8" ht="30">
-      <c r="A78" s="27"/>
-      <c r="B78" s="13" t="s">
-        <v>443</v>
-      </c>
-      <c r="C78" s="13"/>
-      <c r="D78" s="13"/>
-      <c r="E78" s="13" t="s">
-        <v>435</v>
-      </c>
-      <c r="F78" s="13"/>
-    </row>
-    <row r="79" spans="1:8" ht="30">
+    <row r="76" spans="1:8" ht="30">
+      <c r="A76" s="27"/>
+      <c r="B76" s="13" t="s">
+        <v>336</v>
+      </c>
+      <c r="C76" s="13"/>
+      <c r="D76" s="13"/>
+      <c r="E76" s="13" t="s">
+        <v>328</v>
+      </c>
+      <c r="F76" s="13"/>
+    </row>
+    <row r="77" spans="1:8" ht="30">
+      <c r="A77" s="27"/>
+      <c r="B77" s="13" t="s">
+        <v>337</v>
+      </c>
+      <c r="C77" s="13"/>
+      <c r="D77" s="13"/>
+      <c r="E77" s="13" t="s">
+        <v>338</v>
+      </c>
+      <c r="F77" s="13"/>
+    </row>
+    <row r="78" spans="1:8" s="10" customFormat="1" ht="15">
+      <c r="B78" s="26" t="s">
+        <v>13</v>
+      </c>
+      <c r="C78" s="26"/>
+      <c r="D78" s="26" t="s">
+        <v>350</v>
+      </c>
+      <c r="E78" s="26"/>
+      <c r="F78" s="26"/>
+    </row>
+    <row r="79" spans="1:8" ht="15">
       <c r="A79" s="27"/>
-      <c r="B79" s="13" t="s">
-        <v>444</v>
-      </c>
-      <c r="C79" s="13"/>
-      <c r="D79" s="13"/>
-      <c r="E79" s="13" t="s">
-        <v>445</v>
-      </c>
-      <c r="F79" s="13"/>
-    </row>
-    <row r="80" spans="1:8" s="10" customFormat="1" ht="15">
-      <c r="B80" s="26" t="s">
+      <c r="B79" s="15" t="s">
+        <v>339</v>
+      </c>
+      <c r="C79" s="15"/>
+      <c r="D79" s="15"/>
+      <c r="E79" s="15"/>
+      <c r="F79" s="15"/>
+    </row>
+    <row r="80" spans="1:8" ht="12">
+      <c r="A80" s="27"/>
+      <c r="B80" t="s">
+        <v>15</v>
+      </c>
+    </row>
+    <row r="81" spans="1:8" ht="12">
+      <c r="A81" s="27"/>
+      <c r="B81" t="s">
         <v>13</v>
       </c>
-      <c r="C80" s="26"/>
-      <c r="D80" s="26" t="s">
-        <v>457</v>
-      </c>
-      <c r="E80" s="26"/>
-      <c r="F80" s="26"/>
-    </row>
-    <row r="81" spans="1:8" ht="15">
-      <c r="A81" s="27"/>
-      <c r="B81" s="15" t="s">
-        <v>446</v>
-      </c>
-      <c r="C81" s="15"/>
-      <c r="D81" s="15"/>
-      <c r="E81" s="15"/>
-      <c r="F81" s="15"/>
+      <c r="C81" s="20"/>
+      <c r="D81" s="28" t="s">
+        <v>335</v>
+      </c>
+      <c r="E81" s="28"/>
+      <c r="F81" s="20"/>
     </row>
     <row r="82" spans="1:8" ht="12">
       <c r="A82" s="27"/>
       <c r="B82" t="s">
-        <v>15</v>
-      </c>
+        <v>25</v>
+      </c>
+      <c r="C82" s="20"/>
+      <c r="D82" s="28"/>
+      <c r="E82" s="20"/>
+      <c r="F82" s="20"/>
     </row>
     <row r="83" spans="1:8" ht="12">
       <c r="A83" s="27"/>
-      <c r="B83" t="s">
+      <c r="C83" s="20"/>
+      <c r="D83" s="28"/>
+      <c r="E83" s="20"/>
+      <c r="F83" s="20"/>
+    </row>
+    <row r="84" spans="1:8" ht="15">
+      <c r="A84" s="27"/>
+      <c r="B84" s="15" t="s">
+        <v>340</v>
+      </c>
+      <c r="C84" s="29"/>
+      <c r="D84" s="30"/>
+      <c r="E84" s="29"/>
+      <c r="F84" s="29"/>
+    </row>
+    <row r="85" spans="1:8" s="10" customFormat="1" ht="15">
+      <c r="B85" s="32" t="s">
         <v>13</v>
       </c>
-      <c r="C83" s="20"/>
-      <c r="D83" s="28" t="s">
-        <v>442</v>
-      </c>
-      <c r="E83" s="28"/>
-      <c r="F83" s="20"/>
-    </row>
-    <row r="84" spans="1:8" ht="12">
-      <c r="A84" s="27"/>
-      <c r="B84" t="s">
-        <v>25</v>
-      </c>
-      <c r="C84" s="20"/>
-      <c r="D84" s="28"/>
-      <c r="E84" s="20"/>
-      <c r="F84" s="20"/>
-    </row>
-    <row r="85" spans="1:8" ht="12">
-      <c r="A85" s="27"/>
-      <c r="C85" s="20"/>
-      <c r="D85" s="28"/>
-      <c r="E85" s="20"/>
-      <c r="F85" s="20"/>
+      <c r="C85" s="33"/>
+      <c r="D85" s="34" t="s">
+        <v>349</v>
+      </c>
+      <c r="E85" s="33"/>
+      <c r="F85" s="33"/>
     </row>
     <row r="86" spans="1:8" ht="15">
       <c r="A86" s="27"/>
       <c r="B86" s="15" t="s">
-        <v>447</v>
+        <v>317</v>
       </c>
       <c r="C86" s="29"/>
       <c r="D86" s="30"/>
@@ -4005,7 +3636,7 @@
       </c>
       <c r="C87" s="33"/>
       <c r="D87" s="34" t="s">
-        <v>456</v>
+        <v>351</v>
       </c>
       <c r="E87" s="33"/>
       <c r="F87" s="33"/>
@@ -4013,105 +3644,112 @@
     <row r="88" spans="1:8" ht="15">
       <c r="A88" s="27"/>
       <c r="B88" s="15" t="s">
-        <v>424</v>
+        <v>80</v>
       </c>
       <c r="C88" s="29"/>
       <c r="D88" s="30"/>
       <c r="E88" s="29"/>
       <c r="F88" s="29"/>
     </row>
-    <row r="89" spans="1:8" s="10" customFormat="1" ht="15">
-      <c r="B89" s="32" t="s">
-        <v>13</v>
-      </c>
+    <row r="89" spans="1:8" ht="15">
+      <c r="A89" s="10"/>
+      <c r="B89" s="32"/>
       <c r="C89" s="33"/>
-      <c r="D89" s="34" t="s">
-        <v>458</v>
-      </c>
+      <c r="D89" s="34"/>
       <c r="E89" s="33"/>
       <c r="F89" s="33"/>
     </row>
-    <row r="90" spans="1:8" ht="15">
-      <c r="A90" s="27"/>
-      <c r="B90" s="15" t="s">
-        <v>80</v>
-      </c>
-      <c r="C90" s="29"/>
-      <c r="D90" s="30"/>
-      <c r="E90" s="29"/>
-      <c r="F90" s="29"/>
-    </row>
-    <row r="91" spans="1:8" ht="15">
-      <c r="A91" s="10"/>
-      <c r="B91" s="32"/>
-      <c r="C91" s="33"/>
-      <c r="D91" s="34"/>
-      <c r="E91" s="33"/>
-      <c r="F91" s="33"/>
-    </row>
-    <row r="92" spans="1:8" s="13" customFormat="1" ht="15">
-      <c r="A92" s="26"/>
-      <c r="B92" s="13" t="s">
+    <row r="90" spans="1:8" s="13" customFormat="1" ht="15">
+      <c r="A90" s="26"/>
+      <c r="B90" s="13" t="s">
         <v>109</v>
       </c>
-      <c r="C92" s="35"/>
-      <c r="D92" s="36"/>
-      <c r="E92" s="14" t="s">
-        <v>449</v>
-      </c>
-      <c r="F92" s="35"/>
-    </row>
-    <row r="93" spans="1:8" s="13" customFormat="1" ht="15">
-      <c r="A93" s="26"/>
-      <c r="B93" s="13" t="s">
+      <c r="C90" s="35"/>
+      <c r="D90" s="36"/>
+      <c r="E90" s="14" t="s">
+        <v>342</v>
+      </c>
+      <c r="F90" s="35"/>
+    </row>
+    <row r="91" spans="1:8" s="13" customFormat="1" ht="15">
+      <c r="A91" s="26"/>
+      <c r="B91" s="13" t="s">
         <v>81</v>
       </c>
-      <c r="C93" s="35"/>
-      <c r="D93" s="36"/>
-      <c r="E93" s="14" t="s">
+      <c r="C91" s="35"/>
+      <c r="D91" s="36"/>
+      <c r="E91" s="14" t="s">
         <v>82</v>
       </c>
-      <c r="F93" s="35"/>
-    </row>
-    <row r="94" spans="1:8" ht="15">
-      <c r="A94" s="21" t="s">
-        <v>431</v>
-      </c>
-      <c r="B94" s="15" t="s">
+      <c r="F91" s="35"/>
+    </row>
+    <row r="92" spans="1:8" ht="15">
+      <c r="A92" s="21" t="s">
+        <v>324</v>
+      </c>
+      <c r="B92" s="15" t="s">
         <v>110</v>
       </c>
-      <c r="C94" s="15"/>
-      <c r="D94" s="15"/>
-      <c r="E94" s="15"/>
-      <c r="F94" s="15"/>
-      <c r="G94" s="15"/>
-      <c r="H94" s="15"/>
+      <c r="C92" s="15"/>
+      <c r="D92" s="15"/>
+      <c r="E92" s="15"/>
+      <c r="F92" s="15"/>
+      <c r="G92" s="15"/>
+      <c r="H92" s="15"/>
+    </row>
+    <row r="93" spans="1:8" ht="12">
+      <c r="A93" s="21"/>
+      <c r="B93" t="s">
+        <v>175</v>
+      </c>
+      <c r="C93" t="s">
+        <v>11</v>
+      </c>
+      <c r="D93" t="s">
+        <v>12</v>
+      </c>
+      <c r="F93" t="s">
+        <v>6</v>
+      </c>
+      <c r="G93" s="12"/>
+      <c r="H93" s="12"/>
+    </row>
+    <row r="94" spans="1:8" ht="12">
+      <c r="A94" s="21"/>
+      <c r="B94" s="4" t="s">
+        <v>15</v>
+      </c>
+      <c r="C94" s="4"/>
+      <c r="D94" s="4"/>
+      <c r="E94" s="4"/>
+      <c r="F94" s="4"/>
     </row>
     <row r="95" spans="1:8" ht="12">
       <c r="A95" s="21"/>
-      <c r="B95" t="s">
-        <v>226</v>
-      </c>
-      <c r="C95" t="s">
-        <v>11</v>
-      </c>
-      <c r="D95" t="s">
-        <v>12</v>
-      </c>
-      <c r="F95" t="s">
-        <v>6</v>
-      </c>
-      <c r="G95" s="12"/>
-      <c r="H95" s="12"/>
-    </row>
-    <row r="96" spans="1:8" ht="12">
+      <c r="B95" s="4" t="s">
+        <v>16</v>
+      </c>
+      <c r="C95" s="4" t="s">
+        <v>17</v>
+      </c>
+      <c r="D95" s="4" t="s">
+        <v>18</v>
+      </c>
+      <c r="E95" s="4"/>
+      <c r="F95" s="4"/>
+    </row>
+    <row r="96" spans="1:8" ht="36">
       <c r="A96" s="21"/>
       <c r="B96" s="4" t="s">
-        <v>15</v>
+        <v>13</v>
       </c>
       <c r="C96" s="4"/>
-      <c r="D96" s="4"/>
-      <c r="E96" s="4"/>
+      <c r="D96" s="4" t="s">
+        <v>19</v>
+      </c>
+      <c r="E96" s="4" t="s">
+        <v>20</v>
+      </c>
       <c r="F96" s="4"/>
     </row>
     <row r="97" spans="1:10" ht="12">
@@ -4120,10 +3758,10 @@
         <v>16</v>
       </c>
       <c r="C97" s="4" t="s">
-        <v>17</v>
+        <v>21</v>
       </c>
       <c r="D97" s="4" t="s">
-        <v>18</v>
+        <v>22</v>
       </c>
       <c r="E97" s="4"/>
       <c r="F97" s="4"/>
@@ -4135,95 +3773,97 @@
       </c>
       <c r="C98" s="4"/>
       <c r="D98" s="4" t="s">
-        <v>19</v>
+        <v>23</v>
       </c>
       <c r="E98" s="4" t="s">
-        <v>20</v>
+        <v>24</v>
       </c>
       <c r="F98" s="4"/>
-    </row>
-    <row r="99" spans="1:10" ht="12">
+      <c r="I98" s="12"/>
+    </row>
+    <row r="99" spans="1:10" ht="12.75" customHeight="1">
       <c r="A99" s="21"/>
       <c r="B99" s="4" t="s">
-        <v>16</v>
-      </c>
-      <c r="C99" s="4" t="s">
-        <v>21</v>
-      </c>
-      <c r="D99" s="4" t="s">
-        <v>22</v>
-      </c>
+        <v>25</v>
+      </c>
+      <c r="C99" s="4"/>
+      <c r="D99" s="4"/>
       <c r="E99" s="4"/>
       <c r="F99" s="4"/>
     </row>
-    <row r="100" spans="1:10" ht="36">
+    <row r="100" spans="1:10" ht="12.75" customHeight="1">
       <c r="A100" s="21"/>
-      <c r="B100" s="4" t="s">
-        <v>13</v>
-      </c>
-      <c r="C100" s="4"/>
-      <c r="D100" s="4" t="s">
-        <v>23</v>
-      </c>
-      <c r="E100" s="4" t="s">
-        <v>24</v>
-      </c>
-      <c r="F100" s="4"/>
-      <c r="I100" s="12"/>
-    </row>
-    <row r="101" spans="1:10" ht="12.75" customHeight="1">
-      <c r="A101" s="21"/>
-      <c r="B101" s="4" t="s">
-        <v>25</v>
-      </c>
-      <c r="C101" s="4"/>
-      <c r="D101" s="4"/>
-      <c r="E101" s="4"/>
-      <c r="F101" s="4"/>
-    </row>
-    <row r="102" spans="1:10" ht="12.75" customHeight="1">
-      <c r="A102" s="21"/>
-      <c r="B102" s="15" t="s">
+      <c r="B100" s="15" t="s">
         <v>83</v>
       </c>
-      <c r="C102" s="15"/>
-      <c r="D102" s="15"/>
-      <c r="E102" s="15"/>
-      <c r="F102" s="15"/>
-      <c r="G102" s="15"/>
-      <c r="H102" s="15"/>
-    </row>
-    <row r="103" spans="1:10" s="12" customFormat="1" ht="12.75" customHeight="1"/>
-    <row r="104" spans="1:10" s="14" customFormat="1" ht="12.75" customHeight="1">
-      <c r="A104" s="24"/>
-      <c r="B104" s="13" t="s">
+      <c r="C100" s="15"/>
+      <c r="D100" s="15"/>
+      <c r="E100" s="15"/>
+      <c r="F100" s="15"/>
+      <c r="G100" s="15"/>
+      <c r="H100" s="15"/>
+    </row>
+    <row r="101" spans="1:10" s="12" customFormat="1" ht="12.75" customHeight="1"/>
+    <row r="102" spans="1:10" s="14" customFormat="1" ht="12.75" customHeight="1">
+      <c r="A102" s="24"/>
+      <c r="B102" s="13" t="s">
         <v>111</v>
       </c>
-      <c r="E104" s="14" t="s">
+      <c r="E102" s="14" t="s">
         <v>112</v>
       </c>
-      <c r="I104" s="12"/>
-      <c r="J104" s="12"/>
+      <c r="I102" s="12"/>
+      <c r="J102" s="12"/>
+    </row>
+    <row r="103" spans="1:10" ht="12.75" customHeight="1">
+      <c r="B103" s="13" t="s">
+        <v>89</v>
+      </c>
+      <c r="C103" s="14"/>
+      <c r="D103" s="14"/>
+      <c r="E103" s="14" t="s">
+        <v>84</v>
+      </c>
+      <c r="F103" s="14"/>
+      <c r="G103" s="14"/>
+      <c r="H103" s="14"/>
+    </row>
+    <row r="104" spans="1:10" ht="12.75" customHeight="1">
+      <c r="A104" s="21" t="s">
+        <v>325</v>
+      </c>
+      <c r="B104" s="15" t="s">
+        <v>128</v>
+      </c>
+      <c r="C104" s="18"/>
+      <c r="D104" s="18"/>
+      <c r="E104" s="18"/>
+      <c r="F104" s="18"/>
+      <c r="G104" s="18"/>
+      <c r="H104" s="18"/>
     </row>
     <row r="105" spans="1:10" ht="12.75" customHeight="1">
-      <c r="B105" s="13" t="s">
-        <v>89</v>
-      </c>
-      <c r="C105" s="14"/>
-      <c r="D105" s="14"/>
-      <c r="E105" s="14" t="s">
-        <v>84</v>
-      </c>
-      <c r="F105" s="14"/>
-      <c r="G105" s="14"/>
-      <c r="H105" s="14"/>
+      <c r="A105" s="21"/>
+      <c r="B105" s="2" t="s">
+        <v>177</v>
+      </c>
+      <c r="C105" s="12" t="s">
+        <v>85</v>
+      </c>
+      <c r="D105" s="12" t="s">
+        <v>86</v>
+      </c>
+      <c r="E105" s="12"/>
+      <c r="F105" s="12" t="s">
+        <v>87</v>
+      </c>
+      <c r="G105" s="12"/>
+      <c r="H105" s="12"/>
     </row>
     <row r="106" spans="1:10" ht="12.75" customHeight="1">
-      <c r="A106" s="21" t="s">
-        <v>432</v>
-      </c>
+      <c r="A106" s="21"/>
       <c r="B106" s="15" t="s">
-        <v>128</v>
+        <v>88</v>
       </c>
       <c r="C106" s="18"/>
       <c r="D106" s="18"/>
@@ -4233,128 +3873,98 @@
       <c r="H106" s="18"/>
     </row>
     <row r="107" spans="1:10" ht="12.75" customHeight="1">
-      <c r="A107" s="21"/>
-      <c r="B107" s="2" t="s">
-        <v>228</v>
-      </c>
-      <c r="C107" s="12" t="s">
-        <v>85</v>
-      </c>
-      <c r="D107" s="12" t="s">
-        <v>86</v>
-      </c>
+      <c r="C107" s="12"/>
+      <c r="D107" s="12"/>
       <c r="E107" s="12"/>
-      <c r="F107" s="12" t="s">
-        <v>87</v>
-      </c>
+      <c r="F107" s="12"/>
       <c r="G107" s="12"/>
       <c r="H107" s="12"/>
     </row>
     <row r="108" spans="1:10" ht="12.75" customHeight="1">
-      <c r="A108" s="21"/>
-      <c r="B108" s="15" t="s">
-        <v>88</v>
-      </c>
-      <c r="C108" s="18"/>
-      <c r="D108" s="18"/>
-      <c r="E108" s="18"/>
-      <c r="F108" s="18"/>
-      <c r="G108" s="18"/>
-      <c r="H108" s="18"/>
+      <c r="B108" s="13" t="s">
+        <v>119</v>
+      </c>
+      <c r="C108" s="14"/>
+      <c r="D108" s="14"/>
+      <c r="E108" s="14" t="s">
+        <v>121</v>
+      </c>
+      <c r="F108" s="14"/>
+      <c r="G108" s="14"/>
+      <c r="H108" s="14"/>
     </row>
     <row r="109" spans="1:10" ht="12.75" customHeight="1">
-      <c r="C109" s="12"/>
-      <c r="D109" s="12"/>
-      <c r="E109" s="12"/>
-      <c r="F109" s="12"/>
-      <c r="G109" s="12"/>
-      <c r="H109" s="12"/>
+      <c r="B109" s="13" t="s">
+        <v>120</v>
+      </c>
+      <c r="C109" s="14"/>
+      <c r="D109" s="14"/>
+      <c r="E109" s="14" t="s">
+        <v>122</v>
+      </c>
+      <c r="F109" s="14"/>
+      <c r="G109" s="14"/>
+      <c r="H109" s="14"/>
     </row>
     <row r="110" spans="1:10" ht="12.75" customHeight="1">
-      <c r="B110" s="13" t="s">
-        <v>119</v>
-      </c>
-      <c r="C110" s="14"/>
-      <c r="D110" s="14"/>
-      <c r="E110" s="14" t="s">
-        <v>121</v>
-      </c>
-      <c r="F110" s="14"/>
-      <c r="G110" s="14"/>
-      <c r="H110" s="14"/>
+      <c r="A110" s="21" t="s">
+        <v>64</v>
+      </c>
+      <c r="B110" s="15" t="s">
+        <v>129</v>
+      </c>
+      <c r="C110" s="18"/>
+      <c r="D110" s="18"/>
+      <c r="E110" s="18"/>
+      <c r="F110" s="18"/>
+      <c r="G110" s="18"/>
+      <c r="H110" s="18"/>
     </row>
     <row r="111" spans="1:10" ht="12.75" customHeight="1">
-      <c r="B111" s="13" t="s">
-        <v>120</v>
-      </c>
-      <c r="C111" s="14"/>
-      <c r="D111" s="14"/>
-      <c r="E111" s="14" t="s">
-        <v>122</v>
-      </c>
-      <c r="F111" s="14"/>
-      <c r="G111" s="14"/>
-      <c r="H111" s="14"/>
+      <c r="A111" s="21"/>
+      <c r="B111" t="s">
+        <v>176</v>
+      </c>
+      <c r="C111" t="s">
+        <v>65</v>
+      </c>
+      <c r="D111" t="s">
+        <v>67</v>
+      </c>
+      <c r="F111" t="s">
+        <v>6</v>
+      </c>
+      <c r="G111" s="12"/>
+      <c r="H111" s="12"/>
     </row>
     <row r="112" spans="1:10" ht="12.75" customHeight="1">
-      <c r="A112" s="21" t="s">
+      <c r="A112" s="21"/>
+      <c r="B112" s="2" t="s">
+        <v>13</v>
+      </c>
+      <c r="C112" s="12"/>
+      <c r="D112" s="12" t="s">
         <v>64</v>
       </c>
-      <c r="B112" s="15" t="s">
-        <v>129</v>
-      </c>
-      <c r="C112" s="18"/>
-      <c r="D112" s="18"/>
-      <c r="E112" s="18"/>
-      <c r="F112" s="18"/>
-      <c r="G112" s="18"/>
-      <c r="H112" s="18"/>
+      <c r="E112" s="12"/>
+      <c r="F112" s="12"/>
+      <c r="G112" s="12"/>
+      <c r="H112" s="12"/>
     </row>
     <row r="113" spans="1:8" ht="12.75" customHeight="1">
       <c r="A113" s="21"/>
-      <c r="B113" t="s">
-        <v>227</v>
-      </c>
-      <c r="C113" t="s">
-        <v>65</v>
-      </c>
-      <c r="D113" t="s">
-        <v>67</v>
-      </c>
-      <c r="F113" t="s">
-        <v>6</v>
-      </c>
-      <c r="G113" s="12"/>
-      <c r="H113" s="12"/>
-    </row>
-    <row r="114" spans="1:8" ht="12.75" customHeight="1">
-      <c r="A114" s="21"/>
-      <c r="B114" s="2" t="s">
-        <v>13</v>
-      </c>
-      <c r="C114" s="12"/>
-      <c r="D114" s="12" t="s">
-        <v>64</v>
-      </c>
-      <c r="E114" s="12"/>
-      <c r="F114" s="12"/>
-      <c r="G114" s="12"/>
-      <c r="H114" s="12"/>
-    </row>
-    <row r="115" spans="1:8" ht="12.75" customHeight="1">
-      <c r="A115" s="21"/>
-      <c r="B115" s="15" t="s">
+      <c r="B113" s="15" t="s">
         <v>123</v>
       </c>
-      <c r="C115" s="18"/>
-      <c r="D115" s="18"/>
-      <c r="E115" s="18"/>
-      <c r="F115" s="18"/>
-      <c r="G115" s="18"/>
-      <c r="H115" s="18"/>
-    </row>
-    <row r="118" spans="1:8" ht="12.75" customHeight="1">
-      <c r="B118" s="17" t="s">
+      <c r="C113" s="18"/>
+      <c r="D113" s="18"/>
+      <c r="E113" s="18"/>
+      <c r="F113" s="18"/>
+      <c r="G113" s="18"/>
+      <c r="H113" s="18"/>
+    </row>
+    <row r="116" spans="1:8" ht="12.75" customHeight="1">
+      <c r="B116" s="17" t="s">
         <v>107</v>
       </c>
     </row>
@@ -4371,10 +3981,10 @@
 
 <file path=xl/worksheets/sheet2.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <dimension ref="A1:B20"/>
+  <dimension ref="A1:B12"/>
   <sheetViews>
     <sheetView zoomScale="150" zoomScaleNormal="150" zoomScalePageLayoutView="150" workbookViewId="0">
-      <selection activeCell="B18" sqref="B18"/>
+      <selection activeCell="A6" sqref="A6:B20"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultColWidth="17.1640625" defaultRowHeight="12.75" customHeight="1" x14ac:dyDescent="0"/>
@@ -4422,126 +4032,13 @@
         <v>34</v>
       </c>
     </row>
-    <row r="6" spans="1:2" ht="12" customHeight="1">
-      <c r="A6" t="s">
-        <v>229</v>
-      </c>
-      <c r="B6" t="s">
-        <v>230</v>
-      </c>
-    </row>
-    <row r="7" spans="1:2" ht="12" customHeight="1">
-      <c r="A7" t="s">
-        <v>231</v>
-      </c>
-      <c r="B7" t="s">
-        <v>242</v>
-      </c>
-    </row>
-    <row r="8" spans="1:2" ht="12" customHeight="1">
-      <c r="A8" t="s">
-        <v>232</v>
-      </c>
-      <c r="B8" t="s">
-        <v>239</v>
-      </c>
-    </row>
-    <row r="9" spans="1:2" ht="12" customHeight="1">
-      <c r="A9" t="s">
-        <v>260</v>
-      </c>
-      <c r="B9" t="s">
-        <v>257</v>
-      </c>
-    </row>
-    <row r="10" spans="1:2" ht="12" customHeight="1">
-      <c r="A10" t="s">
-        <v>233</v>
-      </c>
-      <c r="B10" t="s">
-        <v>240</v>
-      </c>
-    </row>
-    <row r="11" spans="1:2" ht="12" customHeight="1">
-      <c r="A11" t="s">
-        <v>234</v>
-      </c>
-      <c r="B11" t="s">
-        <v>241</v>
-      </c>
-    </row>
-    <row r="12" spans="1:2" ht="42" customHeight="1">
-      <c r="A12" t="s">
-        <v>258</v>
-      </c>
-      <c r="B12" t="s">
-        <v>259</v>
-      </c>
-    </row>
-    <row r="13" spans="1:2" ht="12.75" customHeight="1">
-      <c r="A13" t="s">
-        <v>382</v>
-      </c>
-      <c r="B13" t="s">
-        <v>388</v>
-      </c>
-    </row>
-    <row r="14" spans="1:2" ht="12.75" customHeight="1">
-      <c r="A14" t="s">
-        <v>383</v>
-      </c>
-      <c r="B14" t="s">
-        <v>389</v>
-      </c>
-    </row>
-    <row r="15" spans="1:2" ht="12.75" customHeight="1">
-      <c r="A15" t="s">
-        <v>384</v>
-      </c>
-      <c r="B15" t="s">
-        <v>390</v>
-      </c>
-    </row>
-    <row r="16" spans="1:2" ht="12.75" customHeight="1">
-      <c r="A16" t="s">
-        <v>385</v>
-      </c>
-      <c r="B16" t="s">
-        <v>391</v>
-      </c>
-    </row>
-    <row r="17" spans="1:2" ht="12.75" customHeight="1">
-      <c r="A17" t="s">
-        <v>460</v>
-      </c>
-      <c r="B17" t="s">
-        <v>462</v>
-      </c>
-    </row>
-    <row r="18" spans="1:2" ht="12.75" customHeight="1">
-      <c r="A18" t="s">
-        <v>386</v>
-      </c>
-      <c r="B18" t="s">
-        <v>392</v>
-      </c>
-    </row>
-    <row r="19" spans="1:2" ht="12.75" customHeight="1">
-      <c r="A19" t="s">
-        <v>387</v>
-      </c>
-      <c r="B19" t="s">
-        <v>461</v>
-      </c>
-    </row>
-    <row r="20" spans="1:2" ht="12.75" customHeight="1">
-      <c r="A20" t="s">
-        <v>394</v>
-      </c>
-      <c r="B20" t="s">
-        <v>395</v>
-      </c>
-    </row>
+    <row r="6" spans="1:2" ht="12" customHeight="1"/>
+    <row r="7" spans="1:2" ht="12" customHeight="1"/>
+    <row r="8" spans="1:2" ht="12" customHeight="1"/>
+    <row r="9" spans="1:2" ht="12" customHeight="1"/>
+    <row r="10" spans="1:2" ht="12" customHeight="1"/>
+    <row r="11" spans="1:2" ht="12" customHeight="1"/>
+    <row r="12" spans="1:2" ht="42" customHeight="1"/>
   </sheetData>
   <pageMargins left="0.75" right="0.75" top="1" bottom="1" header="0.5" footer="0.5"/>
   <pageSetup orientation="portrait" horizontalDpi="4294967292" verticalDpi="4294967292"/>
@@ -4555,10 +4052,10 @@
 
 <file path=xl/worksheets/sheet3.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <dimension ref="A1:D137"/>
+  <dimension ref="A1:D119"/>
   <sheetViews>
-    <sheetView topLeftCell="A86" workbookViewId="0">
-      <selection activeCell="A91" sqref="A91:XFD97"/>
+    <sheetView tabSelected="1" topLeftCell="A32" workbookViewId="0">
+      <selection activeCell="B66" sqref="B66:B71"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultColWidth="17.1640625" defaultRowHeight="12.75" customHeight="1" x14ac:dyDescent="0"/>
@@ -4713,7 +4210,7 @@
         <v>79</v>
       </c>
     </row>
-    <row r="18" spans="1:3" ht="12.75" customHeight="1">
+    <row r="18" spans="1:4" ht="12.75" customHeight="1">
       <c r="A18" t="s">
         <v>11</v>
       </c>
@@ -4724,7 +4221,7 @@
         <v>47</v>
       </c>
     </row>
-    <row r="19" spans="1:3" ht="12.75" customHeight="1">
+    <row r="19" spans="1:4" ht="12.75" customHeight="1">
       <c r="A19" t="s">
         <v>11</v>
       </c>
@@ -4735,7 +4232,7 @@
         <v>49</v>
       </c>
     </row>
-    <row r="21" spans="1:3" ht="12.75" customHeight="1">
+    <row r="21" spans="1:4" ht="12.75" customHeight="1">
       <c r="A21" t="s">
         <v>85</v>
       </c>
@@ -4746,7 +4243,7 @@
         <v>91</v>
       </c>
     </row>
-    <row r="22" spans="1:3" ht="12.75" customHeight="1">
+    <row r="22" spans="1:4" ht="12.75" customHeight="1">
       <c r="A22" t="s">
         <v>85</v>
       </c>
@@ -4757,7 +4254,7 @@
         <v>93</v>
       </c>
     </row>
-    <row r="23" spans="1:3" ht="12.75" customHeight="1">
+    <row r="23" spans="1:4" ht="12.75" customHeight="1">
       <c r="A23" t="s">
         <v>85</v>
       </c>
@@ -4768,7 +4265,7 @@
         <v>95</v>
       </c>
     </row>
-    <row r="25" spans="1:3" ht="12.75" customHeight="1">
+    <row r="25" spans="1:4" ht="12.75" customHeight="1">
       <c r="A25" t="s">
         <v>65</v>
       </c>
@@ -4779,7 +4276,7 @@
         <v>114</v>
       </c>
     </row>
-    <row r="26" spans="1:3" ht="12.75" customHeight="1">
+    <row r="26" spans="1:4" ht="12.75" customHeight="1">
       <c r="A26" t="s">
         <v>65</v>
       </c>
@@ -4790,7 +4287,7 @@
         <v>117</v>
       </c>
     </row>
-    <row r="27" spans="1:3" ht="12.75" customHeight="1">
+    <row r="27" spans="1:4" ht="12.75" customHeight="1">
       <c r="A27" t="s">
         <v>65</v>
       </c>
@@ -4801,7 +4298,7 @@
         <v>118</v>
       </c>
     </row>
-    <row r="29" spans="1:3" ht="12.75" customHeight="1">
+    <row r="29" spans="1:4" ht="12.75" customHeight="1">
       <c r="A29" t="s">
         <v>50</v>
       </c>
@@ -4812,7 +4309,7 @@
         <v>52</v>
       </c>
     </row>
-    <row r="30" spans="1:3" ht="12.75" customHeight="1">
+    <row r="30" spans="1:4" ht="12.75" customHeight="1">
       <c r="A30" t="s">
         <v>50</v>
       </c>
@@ -4823,1009 +4320,844 @@
         <v>54</v>
       </c>
     </row>
-    <row r="32" spans="1:3" ht="12.75" customHeight="1">
+    <row r="32" spans="1:4" ht="12.75" customHeight="1">
       <c r="A32" t="s">
-        <v>261</v>
+        <v>368</v>
       </c>
       <c r="B32" t="s">
-        <v>263</v>
-      </c>
-      <c r="C32" t="s">
-        <v>264</v>
-      </c>
-    </row>
-    <row r="33" spans="1:3" ht="12.75" customHeight="1">
+        <v>133</v>
+      </c>
+      <c r="D32" t="s">
+        <v>134</v>
+      </c>
+    </row>
+    <row r="33" spans="1:4" ht="12.75" customHeight="1">
       <c r="A33" t="s">
-        <v>261</v>
+        <v>368</v>
       </c>
       <c r="B33" t="s">
-        <v>265</v>
-      </c>
-      <c r="C33" t="s">
-        <v>266</v>
-      </c>
-    </row>
-    <row r="34" spans="1:3" ht="12.75" customHeight="1">
+        <v>135</v>
+      </c>
+      <c r="D33" t="s">
+        <v>139</v>
+      </c>
+    </row>
+    <row r="34" spans="1:4" ht="12.75" customHeight="1">
       <c r="A34" t="s">
-        <v>261</v>
+        <v>368</v>
       </c>
       <c r="B34" t="s">
-        <v>393</v>
-      </c>
-      <c r="C34" t="s">
+        <v>136</v>
+      </c>
+      <c r="D34" t="s">
+        <v>140</v>
+      </c>
+    </row>
+    <row r="35" spans="1:4" ht="12.75" customHeight="1">
+      <c r="A35" t="s">
+        <v>368</v>
+      </c>
+      <c r="B35" t="s">
+        <v>137</v>
+      </c>
+      <c r="D35" t="s">
+        <v>141</v>
+      </c>
+    </row>
+    <row r="36" spans="1:4" ht="12.75" customHeight="1">
+      <c r="A36" t="s">
+        <v>368</v>
+      </c>
+      <c r="B36" t="s">
+        <v>138</v>
+      </c>
+      <c r="D36" t="s">
+        <v>142</v>
+      </c>
+    </row>
+    <row r="38" spans="1:4" ht="12.75" customHeight="1">
+      <c r="A38" t="s">
+        <v>369</v>
+      </c>
+      <c r="B38" t="s">
+        <v>380</v>
+      </c>
+      <c r="D38" t="s">
+        <v>154</v>
+      </c>
+    </row>
+    <row r="39" spans="1:4" s="2" customFormat="1" ht="12.75" customHeight="1">
+      <c r="A39" t="s">
+        <v>369</v>
+      </c>
+      <c r="B39" t="s">
         <v>381</v>
       </c>
-    </row>
-    <row r="36" spans="1:3" ht="12.75" customHeight="1">
-      <c r="A36" t="s">
-        <v>131</v>
-      </c>
-      <c r="B36" t="s">
-        <v>132</v>
-      </c>
-      <c r="C36" t="s">
-        <v>138</v>
-      </c>
-    </row>
-    <row r="37" spans="1:3" ht="12.75" customHeight="1">
-      <c r="A37" t="s">
-        <v>131</v>
-      </c>
-      <c r="B37" t="s">
-        <v>133</v>
-      </c>
-      <c r="C37" t="s">
-        <v>139</v>
-      </c>
-    </row>
-    <row r="38" spans="1:3" ht="12.75" customHeight="1">
-      <c r="A38" t="s">
-        <v>131</v>
-      </c>
-      <c r="B38" t="s">
-        <v>134</v>
-      </c>
-      <c r="C38" t="s">
-        <v>140</v>
-      </c>
-    </row>
-    <row r="39" spans="1:3" ht="12.75" customHeight="1">
-      <c r="A39" t="s">
-        <v>131</v>
-      </c>
-      <c r="B39" t="s">
-        <v>135</v>
-      </c>
-      <c r="C39" t="s">
-        <v>141</v>
-      </c>
-    </row>
-    <row r="40" spans="1:3" ht="12.75" customHeight="1">
+      <c r="D39" t="s">
+        <v>149</v>
+      </c>
+    </row>
+    <row r="40" spans="1:4" ht="12.75" customHeight="1">
       <c r="A40" t="s">
-        <v>131</v>
+        <v>369</v>
       </c>
       <c r="B40" t="s">
-        <v>136</v>
-      </c>
-      <c r="C40" t="s">
-        <v>142</v>
-      </c>
-    </row>
-    <row r="41" spans="1:3" ht="12.75" customHeight="1">
+        <v>382</v>
+      </c>
+      <c r="D40" t="s">
+        <v>150</v>
+      </c>
+    </row>
+    <row r="41" spans="1:4" ht="12.75" customHeight="1">
       <c r="A41" t="s">
-        <v>131</v>
+        <v>369</v>
       </c>
       <c r="B41" t="s">
-        <v>137</v>
-      </c>
-      <c r="C41" t="s">
-        <v>143</v>
-      </c>
-    </row>
-    <row r="43" spans="1:3" ht="12.75" customHeight="1">
+        <v>383</v>
+      </c>
+      <c r="D41" t="s">
+        <v>151</v>
+      </c>
+    </row>
+    <row r="42" spans="1:4" ht="12.75" customHeight="1">
+      <c r="A42" t="s">
+        <v>369</v>
+      </c>
+      <c r="B42" t="s">
+        <v>384</v>
+      </c>
+      <c r="D42" t="s">
+        <v>152</v>
+      </c>
+    </row>
+    <row r="43" spans="1:4" ht="12.75" customHeight="1">
       <c r="A43" t="s">
-        <v>262</v>
+        <v>369</v>
       </c>
       <c r="B43" t="s">
-        <v>267</v>
-      </c>
-      <c r="C43" t="s">
-        <v>285</v>
-      </c>
-    </row>
-    <row r="44" spans="1:3" ht="12.75" customHeight="1">
-      <c r="A44" t="s">
-        <v>262</v>
-      </c>
-      <c r="B44" t="s">
-        <v>270</v>
-      </c>
-      <c r="C44" t="s">
-        <v>286</v>
-      </c>
-    </row>
-    <row r="45" spans="1:3" ht="12.75" customHeight="1">
+        <v>385</v>
+      </c>
+      <c r="D43" t="s">
+        <v>153</v>
+      </c>
+    </row>
+    <row r="45" spans="1:4" ht="12.75" customHeight="1">
       <c r="A45" t="s">
-        <v>262</v>
+        <v>370</v>
       </c>
       <c r="B45" t="s">
-        <v>273</v>
-      </c>
-      <c r="C45" t="s">
-        <v>287</v>
-      </c>
-    </row>
-    <row r="46" spans="1:3" ht="12.75" customHeight="1">
+        <v>386</v>
+      </c>
+      <c r="C45" s="2"/>
+      <c r="D45" t="s">
+        <v>155</v>
+      </c>
+    </row>
+    <row r="46" spans="1:4" ht="12.75" customHeight="1">
       <c r="A46" t="s">
-        <v>262</v>
+        <v>370</v>
       </c>
       <c r="B46" t="s">
-        <v>274</v>
-      </c>
-      <c r="C46" t="s">
-        <v>380</v>
-      </c>
-    </row>
-    <row r="47" spans="1:3" ht="12.75" customHeight="1">
+        <v>387</v>
+      </c>
+      <c r="D46" t="s">
+        <v>156</v>
+      </c>
+    </row>
+    <row r="47" spans="1:4" ht="12.75" customHeight="1">
       <c r="A47" t="s">
-        <v>262</v>
+        <v>370</v>
       </c>
       <c r="B47" t="s">
-        <v>276</v>
-      </c>
-      <c r="C47" t="s">
-        <v>288</v>
-      </c>
-    </row>
-    <row r="48" spans="1:3" ht="12.75" customHeight="1">
+        <v>388</v>
+      </c>
+      <c r="D47" t="s">
+        <v>157</v>
+      </c>
+    </row>
+    <row r="48" spans="1:4" ht="12.75" customHeight="1">
       <c r="A48" t="s">
-        <v>262</v>
+        <v>370</v>
       </c>
       <c r="B48" t="s">
-        <v>278</v>
-      </c>
-      <c r="C48" t="s">
-        <v>289</v>
-      </c>
-    </row>
-    <row r="50" spans="1:4" ht="12.75" customHeight="1">
-      <c r="A50" t="s">
-        <v>145</v>
-      </c>
-      <c r="B50" t="s">
-        <v>152</v>
-      </c>
-      <c r="D50" t="s">
-        <v>153</v>
+        <v>389</v>
+      </c>
+      <c r="D48" t="s">
+        <v>158</v>
+      </c>
+    </row>
+    <row r="49" spans="1:4" ht="12.75" customHeight="1">
+      <c r="A49" t="s">
+        <v>370</v>
+      </c>
+      <c r="B49" t="s">
+        <v>390</v>
+      </c>
+      <c r="D49" t="s">
+        <v>159</v>
       </c>
     </row>
     <row r="51" spans="1:4" ht="12.75" customHeight="1">
       <c r="A51" t="s">
-        <v>145</v>
+        <v>371</v>
       </c>
       <c r="B51" t="s">
-        <v>154</v>
+        <v>186</v>
       </c>
       <c r="D51" t="s">
-        <v>158</v>
+        <v>179</v>
       </c>
     </row>
     <row r="52" spans="1:4" ht="12.75" customHeight="1">
       <c r="A52" t="s">
-        <v>145</v>
+        <v>371</v>
       </c>
       <c r="B52" t="s">
-        <v>155</v>
-      </c>
+        <v>187</v>
+      </c>
+      <c r="C52" s="2"/>
       <c r="D52" t="s">
-        <v>159</v>
+        <v>180</v>
       </c>
     </row>
     <row r="53" spans="1:4" ht="12.75" customHeight="1">
       <c r="A53" t="s">
-        <v>145</v>
+        <v>371</v>
       </c>
       <c r="B53" t="s">
-        <v>156</v>
+        <v>188</v>
       </c>
       <c r="D53" t="s">
-        <v>160</v>
+        <v>181</v>
       </c>
     </row>
     <row r="54" spans="1:4" ht="12.75" customHeight="1">
       <c r="A54" t="s">
-        <v>145</v>
+        <v>371</v>
       </c>
       <c r="B54" t="s">
-        <v>157</v>
+        <v>189</v>
       </c>
       <c r="D54" t="s">
-        <v>161</v>
+        <v>182</v>
+      </c>
+    </row>
+    <row r="55" spans="1:4" ht="12.75" customHeight="1">
+      <c r="A55" t="s">
+        <v>371</v>
+      </c>
+      <c r="B55" t="s">
+        <v>190</v>
+      </c>
+      <c r="D55" t="s">
+        <v>183</v>
       </c>
     </row>
     <row r="56" spans="1:4" ht="12.75" customHeight="1">
       <c r="A56" t="s">
-        <v>149</v>
+        <v>371</v>
       </c>
       <c r="B56" t="s">
+        <v>191</v>
+      </c>
+      <c r="D56" t="s">
+        <v>184</v>
+      </c>
+    </row>
+    <row r="57" spans="1:4" ht="12.75" customHeight="1">
+      <c r="A57" t="s">
+        <v>371</v>
+      </c>
+      <c r="B57" t="s">
+        <v>192</v>
+      </c>
+      <c r="D57" t="s">
         <v>185</v>
-      </c>
-      <c r="D56" t="s">
-        <v>186</v>
-      </c>
-    </row>
-    <row r="57" spans="1:4" s="2" customFormat="1" ht="12.75" customHeight="1">
-      <c r="A57" t="s">
-        <v>149</v>
-      </c>
-      <c r="B57" t="s">
-        <v>175</v>
-      </c>
-      <c r="D57" t="s">
-        <v>176</v>
-      </c>
-    </row>
-    <row r="58" spans="1:4" ht="12.75" customHeight="1">
-      <c r="A58" t="s">
-        <v>149</v>
-      </c>
-      <c r="B58" t="s">
-        <v>177</v>
-      </c>
-      <c r="D58" t="s">
-        <v>178</v>
       </c>
     </row>
     <row r="59" spans="1:4" ht="12.75" customHeight="1">
       <c r="A59" t="s">
-        <v>149</v>
+        <v>372</v>
       </c>
       <c r="B59" t="s">
-        <v>179</v>
+        <v>391</v>
       </c>
       <c r="D59" t="s">
-        <v>180</v>
+        <v>160</v>
       </c>
     </row>
     <row r="60" spans="1:4" ht="12.75" customHeight="1">
       <c r="A60" t="s">
-        <v>149</v>
+        <v>372</v>
       </c>
       <c r="B60" t="s">
-        <v>181</v>
-      </c>
+        <v>392</v>
+      </c>
+      <c r="C60" s="2"/>
       <c r="D60" t="s">
-        <v>182</v>
+        <v>161</v>
       </c>
     </row>
     <row r="61" spans="1:4" ht="12.75" customHeight="1">
       <c r="A61" t="s">
-        <v>149</v>
+        <v>372</v>
       </c>
       <c r="B61" t="s">
-        <v>183</v>
+        <v>393</v>
       </c>
       <c r="D61" t="s">
-        <v>184</v>
+        <v>162</v>
+      </c>
+    </row>
+    <row r="62" spans="1:4" ht="12.75" customHeight="1">
+      <c r="A62" t="s">
+        <v>372</v>
+      </c>
+      <c r="B62" t="s">
+        <v>394</v>
+      </c>
+      <c r="D62" t="s">
+        <v>163</v>
       </c>
     </row>
     <row r="63" spans="1:4" ht="12.75" customHeight="1">
       <c r="A63" t="s">
-        <v>166</v>
+        <v>372</v>
       </c>
       <c r="B63" t="s">
-        <v>187</v>
-      </c>
-      <c r="C63" s="2"/>
+        <v>395</v>
+      </c>
       <c r="D63" t="s">
-        <v>188</v>
+        <v>164</v>
       </c>
     </row>
     <row r="64" spans="1:4" ht="12.75" customHeight="1">
       <c r="A64" t="s">
-        <v>166</v>
+        <v>372</v>
       </c>
       <c r="B64" t="s">
-        <v>189</v>
+        <v>396</v>
       </c>
       <c r="D64" t="s">
-        <v>190</v>
-      </c>
-    </row>
-    <row r="65" spans="1:4" ht="12.75" customHeight="1">
-      <c r="A65" t="s">
-        <v>166</v>
-      </c>
-      <c r="B65" t="s">
-        <v>191</v>
-      </c>
-      <c r="D65" t="s">
-        <v>192</v>
+        <v>165</v>
       </c>
     </row>
     <row r="66" spans="1:4" ht="12.75" customHeight="1">
       <c r="A66" t="s">
+        <v>373</v>
+      </c>
+      <c r="B66" t="s">
+        <v>397</v>
+      </c>
+      <c r="D66" t="s">
         <v>166</v>
-      </c>
-      <c r="B66" t="s">
-        <v>193</v>
-      </c>
-      <c r="D66" t="s">
-        <v>194</v>
       </c>
     </row>
     <row r="67" spans="1:4" ht="12.75" customHeight="1">
       <c r="A67" t="s">
-        <v>166</v>
+        <v>373</v>
       </c>
       <c r="B67" t="s">
-        <v>195</v>
-      </c>
+        <v>398</v>
+      </c>
+      <c r="C67" s="2"/>
       <c r="D67" t="s">
-        <v>196</v>
+        <v>167</v>
+      </c>
+    </row>
+    <row r="68" spans="1:4" ht="12.75" customHeight="1">
+      <c r="A68" t="s">
+        <v>373</v>
+      </c>
+      <c r="B68" t="s">
+        <v>399</v>
+      </c>
+      <c r="D68" t="s">
+        <v>168</v>
       </c>
     </row>
     <row r="69" spans="1:4" ht="12.75" customHeight="1">
       <c r="A69" t="s">
-        <v>236</v>
+        <v>373</v>
       </c>
       <c r="B69" t="s">
-        <v>250</v>
+        <v>400</v>
       </c>
       <c r="D69" t="s">
-        <v>243</v>
+        <v>169</v>
       </c>
     </row>
     <row r="70" spans="1:4" ht="12.75" customHeight="1">
       <c r="A70" t="s">
-        <v>236</v>
+        <v>373</v>
       </c>
       <c r="B70" t="s">
-        <v>251</v>
-      </c>
-      <c r="C70" s="2"/>
+        <v>401</v>
+      </c>
       <c r="D70" t="s">
-        <v>244</v>
+        <v>170</v>
       </c>
     </row>
     <row r="71" spans="1:4" ht="12.75" customHeight="1">
       <c r="A71" t="s">
-        <v>236</v>
+        <v>373</v>
       </c>
       <c r="B71" t="s">
-        <v>252</v>
+        <v>402</v>
       </c>
       <c r="D71" t="s">
-        <v>245</v>
-      </c>
-    </row>
-    <row r="72" spans="1:4" ht="12.75" customHeight="1">
-      <c r="A72" t="s">
-        <v>236</v>
-      </c>
-      <c r="B72" t="s">
-        <v>253</v>
-      </c>
-      <c r="D72" t="s">
-        <v>246</v>
+        <v>171</v>
       </c>
     </row>
     <row r="73" spans="1:4" ht="12.75" customHeight="1">
       <c r="A73" t="s">
-        <v>236</v>
+        <v>199</v>
       </c>
       <c r="B73" t="s">
-        <v>254</v>
-      </c>
-      <c r="D73" t="s">
-        <v>247</v>
+        <v>205</v>
+      </c>
+      <c r="C73" t="s">
+        <v>212</v>
       </c>
     </row>
     <row r="74" spans="1:4" ht="12.75" customHeight="1">
       <c r="A74" t="s">
-        <v>236</v>
+        <v>199</v>
       </c>
       <c r="B74" t="s">
-        <v>255</v>
-      </c>
-      <c r="D74" t="s">
-        <v>248</v>
+        <v>206</v>
+      </c>
+      <c r="C74" t="s">
+        <v>213</v>
       </c>
     </row>
     <row r="75" spans="1:4" ht="12.75" customHeight="1">
       <c r="A75" t="s">
-        <v>236</v>
+        <v>199</v>
       </c>
       <c r="B75" t="s">
-        <v>256</v>
-      </c>
-      <c r="D75" t="s">
-        <v>249</v>
+        <v>207</v>
+      </c>
+      <c r="C75" t="s">
+        <v>214</v>
+      </c>
+    </row>
+    <row r="76" spans="1:4" ht="12.75" customHeight="1">
+      <c r="A76" t="s">
+        <v>199</v>
+      </c>
+      <c r="B76" t="s">
+        <v>208</v>
+      </c>
+      <c r="C76" t="s">
+        <v>215</v>
       </c>
     </row>
     <row r="77" spans="1:4" ht="12.75" customHeight="1">
       <c r="A77" t="s">
-        <v>170</v>
+        <v>199</v>
       </c>
       <c r="B77" t="s">
-        <v>197</v>
-      </c>
-      <c r="D77" t="s">
-        <v>198</v>
+        <v>209</v>
+      </c>
+      <c r="C77" t="s">
+        <v>216</v>
       </c>
     </row>
     <row r="78" spans="1:4" ht="12.75" customHeight="1">
       <c r="A78" t="s">
-        <v>170</v>
+        <v>199</v>
       </c>
       <c r="B78" t="s">
-        <v>199</v>
-      </c>
-      <c r="C78" s="2"/>
-      <c r="D78" t="s">
-        <v>200</v>
+        <v>210</v>
+      </c>
+      <c r="C78" t="s">
+        <v>217</v>
       </c>
     </row>
     <row r="79" spans="1:4" ht="12.75" customHeight="1">
       <c r="A79" t="s">
-        <v>170</v>
+        <v>199</v>
       </c>
       <c r="B79" t="s">
+        <v>211</v>
+      </c>
+      <c r="C79" t="s">
+        <v>218</v>
+      </c>
+    </row>
+    <row r="81" spans="1:3" ht="12.75" customHeight="1">
+      <c r="A81" t="s">
+        <v>200</v>
+      </c>
+      <c r="B81" t="s">
+        <v>225</v>
+      </c>
+      <c r="C81" t="s">
+        <v>231</v>
+      </c>
+    </row>
+    <row r="82" spans="1:3" ht="12.75" customHeight="1">
+      <c r="A82" t="s">
+        <v>200</v>
+      </c>
+      <c r="B82" t="s">
+        <v>226</v>
+      </c>
+      <c r="C82" t="s">
+        <v>232</v>
+      </c>
+    </row>
+    <row r="83" spans="1:3" ht="12.75" customHeight="1">
+      <c r="A83" t="s">
+        <v>200</v>
+      </c>
+      <c r="B83" t="s">
+        <v>227</v>
+      </c>
+      <c r="C83" t="s">
+        <v>233</v>
+      </c>
+    </row>
+    <row r="84" spans="1:3" ht="12.75" customHeight="1">
+      <c r="A84" t="s">
+        <v>200</v>
+      </c>
+      <c r="B84" t="s">
+        <v>228</v>
+      </c>
+      <c r="C84" t="s">
+        <v>234</v>
+      </c>
+    </row>
+    <row r="85" spans="1:3" ht="12.75" customHeight="1">
+      <c r="A85" t="s">
+        <v>200</v>
+      </c>
+      <c r="B85" t="s">
+        <v>229</v>
+      </c>
+      <c r="C85" t="s">
+        <v>235</v>
+      </c>
+    </row>
+    <row r="86" spans="1:3" ht="12.75" customHeight="1">
+      <c r="A86" t="s">
+        <v>200</v>
+      </c>
+      <c r="B86" t="s">
+        <v>230</v>
+      </c>
+      <c r="C86" t="s">
+        <v>236</v>
+      </c>
+    </row>
+    <row r="88" spans="1:3" ht="12.75" customHeight="1">
+      <c r="A88" t="s">
         <v>201</v>
       </c>
-      <c r="D79" t="s">
+      <c r="B88" t="s">
+        <v>243</v>
+      </c>
+      <c r="C88" t="s">
+        <v>244</v>
+      </c>
+    </row>
+    <row r="89" spans="1:3" ht="12.75" customHeight="1">
+      <c r="A89" t="s">
+        <v>201</v>
+      </c>
+      <c r="B89" t="s">
+        <v>237</v>
+      </c>
+      <c r="C89" t="s">
+        <v>245</v>
+      </c>
+    </row>
+    <row r="90" spans="1:3" ht="12.75" customHeight="1">
+      <c r="A90" t="s">
+        <v>201</v>
+      </c>
+      <c r="B90" t="s">
+        <v>238</v>
+      </c>
+      <c r="C90" t="s">
+        <v>246</v>
+      </c>
+    </row>
+    <row r="91" spans="1:3" ht="12.75" customHeight="1">
+      <c r="A91" t="s">
+        <v>201</v>
+      </c>
+      <c r="B91" t="s">
+        <v>239</v>
+      </c>
+      <c r="C91" t="s">
+        <v>247</v>
+      </c>
+    </row>
+    <row r="92" spans="1:3" ht="12.75" customHeight="1">
+      <c r="A92" t="s">
+        <v>201</v>
+      </c>
+      <c r="B92" t="s">
+        <v>240</v>
+      </c>
+      <c r="C92" t="s">
+        <v>248</v>
+      </c>
+    </row>
+    <row r="93" spans="1:3" ht="12.75" customHeight="1">
+      <c r="A93" t="s">
+        <v>201</v>
+      </c>
+      <c r="B93" t="s">
+        <v>241</v>
+      </c>
+      <c r="C93" t="s">
+        <v>249</v>
+      </c>
+    </row>
+    <row r="94" spans="1:3" ht="12.75" customHeight="1">
+      <c r="A94" t="s">
+        <v>201</v>
+      </c>
+      <c r="B94" t="s">
+        <v>242</v>
+      </c>
+      <c r="C94" t="s">
+        <v>250</v>
+      </c>
+    </row>
+    <row r="96" spans="1:3" ht="12.75" customHeight="1">
+      <c r="A96" t="s">
         <v>202</v>
       </c>
-    </row>
-    <row r="80" spans="1:4" ht="12.75" customHeight="1">
-      <c r="A80" t="s">
-        <v>170</v>
-      </c>
-      <c r="B80" t="s">
-        <v>203</v>
-      </c>
-      <c r="D80" t="s">
-        <v>204</v>
-      </c>
-    </row>
-    <row r="81" spans="1:4" ht="12.75" customHeight="1">
-      <c r="A81" t="s">
-        <v>170</v>
-      </c>
-      <c r="B81" t="s">
-        <v>205</v>
-      </c>
-      <c r="D81" t="s">
-        <v>206</v>
-      </c>
-    </row>
-    <row r="82" spans="1:4" ht="12.75" customHeight="1">
-      <c r="A82" t="s">
-        <v>170</v>
-      </c>
-      <c r="B82" t="s">
-        <v>207</v>
-      </c>
-      <c r="D82" t="s">
-        <v>208</v>
-      </c>
-    </row>
-    <row r="84" spans="1:4" ht="12.75" customHeight="1">
-      <c r="A84" t="s">
-        <v>173</v>
-      </c>
-      <c r="B84" t="s">
-        <v>209</v>
-      </c>
-      <c r="D84" t="s">
-        <v>210</v>
-      </c>
-    </row>
-    <row r="85" spans="1:4" ht="12.75" customHeight="1">
-      <c r="A85" t="s">
-        <v>173</v>
-      </c>
-      <c r="B85" t="s">
-        <v>211</v>
-      </c>
-      <c r="C85" s="2"/>
-      <c r="D85" t="s">
-        <v>212</v>
-      </c>
-    </row>
-    <row r="86" spans="1:4" ht="12.75" customHeight="1">
-      <c r="A86" t="s">
-        <v>173</v>
-      </c>
-      <c r="B86" t="s">
-        <v>213</v>
-      </c>
-      <c r="D86" t="s">
-        <v>214</v>
-      </c>
-    </row>
-    <row r="87" spans="1:4" ht="12.75" customHeight="1">
-      <c r="A87" t="s">
-        <v>173</v>
-      </c>
-      <c r="B87" t="s">
-        <v>215</v>
-      </c>
-      <c r="D87" t="s">
-        <v>216</v>
-      </c>
-    </row>
-    <row r="88" spans="1:4" ht="12.75" customHeight="1">
-      <c r="A88" t="s">
-        <v>173</v>
-      </c>
-      <c r="B88" t="s">
-        <v>217</v>
-      </c>
-      <c r="D88" t="s">
-        <v>218</v>
-      </c>
-    </row>
-    <row r="89" spans="1:4" ht="12.75" customHeight="1">
-      <c r="A89" t="s">
-        <v>173</v>
-      </c>
-      <c r="B89" t="s">
-        <v>219</v>
-      </c>
-      <c r="D89" t="s">
-        <v>220</v>
-      </c>
-    </row>
-    <row r="91" spans="1:4" ht="12.75" customHeight="1">
-      <c r="A91" t="s">
-        <v>290</v>
-      </c>
-      <c r="B91" t="s">
-        <v>296</v>
-      </c>
-      <c r="C91" t="s">
-        <v>303</v>
-      </c>
-    </row>
-    <row r="92" spans="1:4" ht="12.75" customHeight="1">
-      <c r="A92" t="s">
-        <v>290</v>
-      </c>
-      <c r="B92" t="s">
-        <v>297</v>
-      </c>
-      <c r="C92" t="s">
-        <v>304</v>
-      </c>
-    </row>
-    <row r="93" spans="1:4" ht="12.75" customHeight="1">
-      <c r="A93" t="s">
-        <v>290</v>
-      </c>
-      <c r="B93" t="s">
-        <v>298</v>
-      </c>
-      <c r="C93" t="s">
-        <v>305</v>
-      </c>
-    </row>
-    <row r="94" spans="1:4" ht="12.75" customHeight="1">
-      <c r="A94" t="s">
-        <v>290</v>
-      </c>
-      <c r="B94" t="s">
-        <v>299</v>
-      </c>
-      <c r="C94" t="s">
-        <v>306</v>
-      </c>
-    </row>
-    <row r="95" spans="1:4" ht="12.75" customHeight="1">
-      <c r="A95" t="s">
-        <v>290</v>
-      </c>
-      <c r="B95" t="s">
-        <v>300</v>
-      </c>
-      <c r="C95" t="s">
-        <v>307</v>
-      </c>
-    </row>
-    <row r="96" spans="1:4" ht="12.75" customHeight="1">
-      <c r="A96" t="s">
-        <v>290</v>
-      </c>
       <c r="B96" t="s">
-        <v>301</v>
+        <v>251</v>
       </c>
       <c r="C96" t="s">
-        <v>308</v>
+        <v>257</v>
       </c>
     </row>
     <row r="97" spans="1:3" ht="12.75" customHeight="1">
       <c r="A97" t="s">
-        <v>290</v>
+        <v>202</v>
       </c>
       <c r="B97" t="s">
-        <v>302</v>
+        <v>252</v>
       </c>
       <c r="C97" t="s">
-        <v>309</v>
+        <v>258</v>
+      </c>
+    </row>
+    <row r="98" spans="1:3" ht="12.75" customHeight="1">
+      <c r="A98" t="s">
+        <v>202</v>
+      </c>
+      <c r="B98" t="s">
+        <v>253</v>
+      </c>
+      <c r="C98" t="s">
+        <v>259</v>
       </c>
     </row>
     <row r="99" spans="1:3" ht="12.75" customHeight="1">
       <c r="A99" t="s">
-        <v>291</v>
+        <v>202</v>
       </c>
       <c r="B99" t="s">
-        <v>316</v>
+        <v>254</v>
       </c>
       <c r="C99" t="s">
-        <v>322</v>
+        <v>260</v>
       </c>
     </row>
     <row r="100" spans="1:3" ht="12.75" customHeight="1">
       <c r="A100" t="s">
-        <v>291</v>
+        <v>202</v>
       </c>
       <c r="B100" t="s">
-        <v>317</v>
+        <v>255</v>
       </c>
       <c r="C100" t="s">
-        <v>323</v>
+        <v>261</v>
       </c>
     </row>
     <row r="101" spans="1:3" ht="12.75" customHeight="1">
       <c r="A101" t="s">
-        <v>291</v>
+        <v>202</v>
       </c>
       <c r="B101" t="s">
-        <v>318</v>
+        <v>256</v>
       </c>
       <c r="C101" t="s">
-        <v>324</v>
-      </c>
-    </row>
-    <row r="102" spans="1:3" ht="12.75" customHeight="1">
-      <c r="A102" t="s">
-        <v>291</v>
-      </c>
-      <c r="B102" t="s">
-        <v>319</v>
-      </c>
-      <c r="C102" t="s">
-        <v>325</v>
+        <v>262</v>
       </c>
     </row>
     <row r="103" spans="1:3" ht="12.75" customHeight="1">
       <c r="A103" t="s">
-        <v>291</v>
+        <v>203</v>
       </c>
       <c r="B103" t="s">
-        <v>320</v>
+        <v>269</v>
       </c>
       <c r="C103" t="s">
-        <v>326</v>
+        <v>270</v>
       </c>
     </row>
     <row r="104" spans="1:3" ht="12.75" customHeight="1">
       <c r="A104" t="s">
-        <v>291</v>
+        <v>203</v>
       </c>
       <c r="B104" t="s">
-        <v>321</v>
+        <v>263</v>
       </c>
       <c r="C104" t="s">
-        <v>327</v>
+        <v>271</v>
+      </c>
+    </row>
+    <row r="105" spans="1:3" ht="12.75" customHeight="1">
+      <c r="A105" t="s">
+        <v>203</v>
+      </c>
+      <c r="B105" t="s">
+        <v>264</v>
+      </c>
+      <c r="C105" t="s">
+        <v>272</v>
       </c>
     </row>
     <row r="106" spans="1:3" ht="12.75" customHeight="1">
       <c r="A106" t="s">
-        <v>292</v>
+        <v>203</v>
       </c>
       <c r="B106" t="s">
-        <v>334</v>
+        <v>266</v>
       </c>
       <c r="C106" t="s">
-        <v>335</v>
+        <v>273</v>
       </c>
     </row>
     <row r="107" spans="1:3" ht="12.75" customHeight="1">
       <c r="A107" t="s">
-        <v>292</v>
+        <v>203</v>
       </c>
       <c r="B107" t="s">
-        <v>328</v>
+        <v>265</v>
       </c>
       <c r="C107" t="s">
-        <v>336</v>
+        <v>274</v>
       </c>
     </row>
     <row r="108" spans="1:3" ht="12.75" customHeight="1">
       <c r="A108" t="s">
-        <v>292</v>
+        <v>203</v>
       </c>
       <c r="B108" t="s">
-        <v>329</v>
+        <v>267</v>
       </c>
       <c r="C108" t="s">
-        <v>337</v>
+        <v>275</v>
       </c>
     </row>
     <row r="109" spans="1:3" ht="12.75" customHeight="1">
       <c r="A109" t="s">
-        <v>292</v>
+        <v>203</v>
       </c>
       <c r="B109" t="s">
-        <v>330</v>
+        <v>268</v>
       </c>
       <c r="C109" t="s">
-        <v>338</v>
-      </c>
-    </row>
-    <row r="110" spans="1:3" ht="12.75" customHeight="1">
-      <c r="A110" t="s">
-        <v>292</v>
-      </c>
-      <c r="B110" t="s">
-        <v>331</v>
-      </c>
-      <c r="C110" t="s">
-        <v>339</v>
+        <v>276</v>
       </c>
     </row>
     <row r="111" spans="1:3" ht="12.75" customHeight="1">
       <c r="A111" t="s">
-        <v>292</v>
+        <v>204</v>
       </c>
       <c r="B111" t="s">
-        <v>332</v>
+        <v>277</v>
       </c>
       <c r="C111" t="s">
-        <v>340</v>
+        <v>283</v>
       </c>
     </row>
     <row r="112" spans="1:3" ht="12.75" customHeight="1">
       <c r="A112" t="s">
-        <v>292</v>
+        <v>204</v>
       </c>
       <c r="B112" t="s">
-        <v>333</v>
+        <v>278</v>
       </c>
       <c r="C112" t="s">
-        <v>341</v>
+        <v>284</v>
+      </c>
+    </row>
+    <row r="113" spans="1:3" ht="12.75" customHeight="1">
+      <c r="A113" t="s">
+        <v>204</v>
+      </c>
+      <c r="B113" t="s">
+        <v>279</v>
+      </c>
+      <c r="C113" t="s">
+        <v>285</v>
       </c>
     </row>
     <row r="114" spans="1:3" ht="12.75" customHeight="1">
       <c r="A114" t="s">
-        <v>293</v>
+        <v>204</v>
       </c>
       <c r="B114" t="s">
-        <v>342</v>
+        <v>280</v>
       </c>
       <c r="C114" t="s">
-        <v>348</v>
+        <v>286</v>
       </c>
     </row>
     <row r="115" spans="1:3" ht="12.75" customHeight="1">
       <c r="A115" t="s">
-        <v>293</v>
+        <v>204</v>
       </c>
       <c r="B115" t="s">
-        <v>343</v>
+        <v>281</v>
       </c>
       <c r="C115" t="s">
-        <v>349</v>
+        <v>287</v>
       </c>
     </row>
     <row r="116" spans="1:3" ht="12.75" customHeight="1">
       <c r="A116" t="s">
-        <v>293</v>
+        <v>204</v>
       </c>
       <c r="B116" t="s">
-        <v>344</v>
+        <v>282</v>
       </c>
       <c r="C116" t="s">
-        <v>350</v>
-      </c>
-    </row>
-    <row r="117" spans="1:3" ht="12.75" customHeight="1">
-      <c r="A117" t="s">
-        <v>293</v>
-      </c>
-      <c r="B117" t="s">
-        <v>345</v>
-      </c>
-      <c r="C117" t="s">
-        <v>351</v>
+        <v>288</v>
       </c>
     </row>
     <row r="118" spans="1:3" ht="12.75" customHeight="1">
       <c r="A118" t="s">
-        <v>293</v>
+        <v>326</v>
       </c>
       <c r="B118" t="s">
-        <v>346</v>
+        <v>321</v>
       </c>
       <c r="C118" t="s">
-        <v>352</v>
+        <v>315</v>
       </c>
     </row>
     <row r="119" spans="1:3" ht="12.75" customHeight="1">
       <c r="A119" t="s">
-        <v>293</v>
+        <v>326</v>
       </c>
       <c r="B119" t="s">
-        <v>347</v>
+        <v>322</v>
       </c>
       <c r="C119" t="s">
-        <v>353</v>
-      </c>
-    </row>
-    <row r="121" spans="1:3" ht="12.75" customHeight="1">
-      <c r="A121" t="s">
-        <v>294</v>
-      </c>
-      <c r="B121" t="s">
-        <v>360</v>
-      </c>
-      <c r="C121" t="s">
-        <v>361</v>
-      </c>
-    </row>
-    <row r="122" spans="1:3" ht="12.75" customHeight="1">
-      <c r="A122" t="s">
-        <v>294</v>
-      </c>
-      <c r="B122" t="s">
-        <v>354</v>
-      </c>
-      <c r="C122" t="s">
-        <v>362</v>
-      </c>
-    </row>
-    <row r="123" spans="1:3" ht="12.75" customHeight="1">
-      <c r="A123" t="s">
-        <v>294</v>
-      </c>
-      <c r="B123" t="s">
-        <v>355</v>
-      </c>
-      <c r="C123" t="s">
-        <v>363</v>
-      </c>
-    </row>
-    <row r="124" spans="1:3" ht="12.75" customHeight="1">
-      <c r="A124" t="s">
-        <v>294</v>
-      </c>
-      <c r="B124" t="s">
-        <v>357</v>
-      </c>
-      <c r="C124" t="s">
-        <v>364</v>
-      </c>
-    </row>
-    <row r="125" spans="1:3" ht="12.75" customHeight="1">
-      <c r="A125" t="s">
-        <v>294</v>
-      </c>
-      <c r="B125" t="s">
-        <v>356</v>
-      </c>
-      <c r="C125" t="s">
-        <v>365</v>
-      </c>
-    </row>
-    <row r="126" spans="1:3" ht="12.75" customHeight="1">
-      <c r="A126" t="s">
-        <v>294</v>
-      </c>
-      <c r="B126" t="s">
-        <v>358</v>
-      </c>
-      <c r="C126" t="s">
-        <v>366</v>
-      </c>
-    </row>
-    <row r="127" spans="1:3" ht="12.75" customHeight="1">
-      <c r="A127" t="s">
-        <v>294</v>
-      </c>
-      <c r="B127" t="s">
-        <v>359</v>
-      </c>
-      <c r="C127" t="s">
-        <v>367</v>
-      </c>
-    </row>
-    <row r="129" spans="1:3" ht="12.75" customHeight="1">
-      <c r="A129" t="s">
-        <v>295</v>
-      </c>
-      <c r="B129" t="s">
-        <v>368</v>
-      </c>
-      <c r="C129" t="s">
-        <v>374</v>
-      </c>
-    </row>
-    <row r="130" spans="1:3" ht="12.75" customHeight="1">
-      <c r="A130" t="s">
-        <v>295</v>
-      </c>
-      <c r="B130" t="s">
-        <v>369</v>
-      </c>
-      <c r="C130" t="s">
-        <v>375</v>
-      </c>
-    </row>
-    <row r="131" spans="1:3" ht="12.75" customHeight="1">
-      <c r="A131" t="s">
-        <v>295</v>
-      </c>
-      <c r="B131" t="s">
-        <v>370</v>
-      </c>
-      <c r="C131" t="s">
-        <v>376</v>
-      </c>
-    </row>
-    <row r="132" spans="1:3" ht="12.75" customHeight="1">
-      <c r="A132" t="s">
-        <v>295</v>
-      </c>
-      <c r="B132" t="s">
-        <v>371</v>
-      </c>
-      <c r="C132" t="s">
-        <v>377</v>
-      </c>
-    </row>
-    <row r="133" spans="1:3" ht="12.75" customHeight="1">
-      <c r="A133" t="s">
-        <v>295</v>
-      </c>
-      <c r="B133" t="s">
-        <v>372</v>
-      </c>
-      <c r="C133" t="s">
-        <v>378</v>
-      </c>
-    </row>
-    <row r="134" spans="1:3" ht="12.75" customHeight="1">
-      <c r="A134" t="s">
-        <v>295</v>
-      </c>
-      <c r="B134" t="s">
-        <v>373</v>
-      </c>
-      <c r="C134" t="s">
-        <v>379</v>
-      </c>
-    </row>
-    <row r="136" spans="1:3" ht="12.75" customHeight="1">
-      <c r="A136" t="s">
-        <v>433</v>
-      </c>
-      <c r="B136" t="s">
-        <v>428</v>
-      </c>
-      <c r="C136" t="s">
-        <v>422</v>
-      </c>
-    </row>
-    <row r="137" spans="1:3" ht="12.75" customHeight="1">
-      <c r="A137" t="s">
-        <v>433</v>
-      </c>
-      <c r="B137" t="s">
-        <v>429</v>
-      </c>
-      <c r="C137" t="s">
-        <v>430</v>
+        <v>323</v>
       </c>
     </row>
   </sheetData>
@@ -5883,10 +5215,10 @@
 
 <file path=xl/worksheets/sheet5.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <dimension ref="A1:B3"/>
+  <dimension ref="A1:B4"/>
   <sheetViews>
     <sheetView workbookViewId="0">
-      <selection activeCell="A4" sqref="A4"/>
+      <selection activeCell="B5" sqref="B5"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="12" x14ac:dyDescent="0"/>
@@ -5896,15 +5228,15 @@
         <v>1</v>
       </c>
       <c r="B1" t="s">
-        <v>162</v>
+        <v>143</v>
       </c>
     </row>
     <row r="2" spans="1:2">
       <c r="A2" t="s">
-        <v>163</v>
+        <v>144</v>
       </c>
       <c r="B2" t="s">
-        <v>164</v>
+        <v>145</v>
       </c>
     </row>
     <row r="3" spans="1:2">
@@ -5912,7 +5244,15 @@
         <v>4</v>
       </c>
       <c r="B3" t="s">
-        <v>164</v>
+        <v>145</v>
+      </c>
+    </row>
+    <row r="4" spans="1:2">
+      <c r="A4" t="s">
+        <v>354</v>
+      </c>
+      <c r="B4" t="s">
+        <v>145</v>
       </c>
     </row>
   </sheetData>

</xml_diff>

<commit_message>
add image to icon2
</commit_message>
<xml_diff>
--- a/opendatakit.collect2/form-files/neonatal/neonatal.xlsx
+++ b/opendatakit.collect2/form-files/neonatal/neonatal.xlsx
@@ -1,10 +1,10 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
-  <fileVersion appName="xl" lastEdited="5" lowestEdited="5" rupBuild="21721"/>
+  <fileVersion appName="xl" lastEdited="5" lowestEdited="5" rupBuild="22905"/>
   <workbookPr autoCompressPictures="0"/>
   <bookViews>
-    <workbookView xWindow="320" yWindow="0" windowWidth="23140" windowHeight="15340" tabRatio="500" activeTab="2"/>
+    <workbookView xWindow="320" yWindow="0" windowWidth="15200" windowHeight="15480" tabRatio="500"/>
   </bookViews>
   <sheets>
     <sheet name="survey" sheetId="1" r:id="rId1"/>
@@ -23,7 +23,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="842" uniqueCount="534">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="861" uniqueCount="551">
   <si>
     <t>type</t>
   </si>
@@ -124,9 +124,6 @@
     <t>calculators</t>
   </si>
   <si>
-    <t>All Calculators</t>
-  </si>
-  <si>
     <t>intubation</t>
   </si>
   <si>
@@ -263,9 +260,6 @@
   </si>
   <si>
     <t>medications_menu</t>
-  </si>
-  <si>
-    <t>Medications</t>
   </si>
   <si>
     <t>dropdown</t>
@@ -1827,6 +1821,63 @@
   </si>
   <si>
     <t>Caffeine</t>
+  </si>
+  <si>
+    <t>img/diagnostic_icon.jpg</t>
+  </si>
+  <si>
+    <t>img/procedure_icon.jpg</t>
+  </si>
+  <si>
+    <t>img/calulators.jpg</t>
+  </si>
+  <si>
+    <t>img/nutrition_icon.jpg</t>
+  </si>
+  <si>
+    <t>img/med_icon.jpg</t>
+  </si>
+  <si>
+    <t>img/diagnostic_icons/sagittal.jpg</t>
+  </si>
+  <si>
+    <t>img/diagnostic_icons/line.jpg</t>
+  </si>
+  <si>
+    <t>img/diagnostic_icons/chest.jpg</t>
+  </si>
+  <si>
+    <t>img/diagnostic_icons/ballard.jpg</t>
+  </si>
+  <si>
+    <t>img/diagnostic_icons/coronal.jpg</t>
+  </si>
+  <si>
+    <t>head_cornal</t>
+  </si>
+  <si>
+    <t>Head Coronal</t>
+  </si>
+  <si>
+    <t>headultra_slider</t>
+  </si>
+  <si>
+    <t>img/Sagittal/1.png</t>
+  </si>
+  <si>
+    <t>img/Sagittal/2.png</t>
+  </si>
+  <si>
+    <t>img/Sagittal/3.png</t>
+  </si>
+  <si>
+    <t>img/Sagittal/4.png</t>
+  </si>
+  <si>
+    <t>img/Sagittal/5.png</t>
+  </si>
+  <si>
+    <t>image_slider headultra_slider</t>
   </si>
 </sst>
 </file>
@@ -2007,7 +2058,7 @@
       <diagonal/>
     </border>
   </borders>
-  <cellStyleXfs count="402">
+  <cellStyleXfs count="406">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
     <xf numFmtId="0" fontId="3" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
     <xf numFmtId="0" fontId="4" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
@@ -2022,6 +2073,10 @@
     <xf numFmtId="0" fontId="5" fillId="2" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
     <xf numFmtId="0" fontId="6" fillId="3" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
     <xf numFmtId="0" fontId="1" fillId="4" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="4" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="4" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
     <xf numFmtId="0" fontId="3" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
     <xf numFmtId="0" fontId="4" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
     <xf numFmtId="0" fontId="3" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
@@ -2508,7 +2563,7 @@
       <alignment wrapText="1"/>
     </xf>
   </cellXfs>
-  <cellStyles count="402">
+  <cellStyles count="406">
     <cellStyle name="20% - Accent4" xfId="13" builtinId="42"/>
     <cellStyle name="Followed Hyperlink" xfId="2" builtinId="9" hidden="1"/>
     <cellStyle name="Followed Hyperlink" xfId="4" builtinId="9" hidden="1"/>
@@ -2709,6 +2764,8 @@
     <cellStyle name="Followed Hyperlink" xfId="397" builtinId="9" hidden="1"/>
     <cellStyle name="Followed Hyperlink" xfId="399" builtinId="9" hidden="1"/>
     <cellStyle name="Followed Hyperlink" xfId="401" builtinId="9" hidden="1"/>
+    <cellStyle name="Followed Hyperlink" xfId="403" builtinId="9" hidden="1"/>
+    <cellStyle name="Followed Hyperlink" xfId="405" builtinId="9" hidden="1"/>
     <cellStyle name="Good" xfId="11" builtinId="26"/>
     <cellStyle name="Hyperlink" xfId="1" builtinId="8" hidden="1"/>
     <cellStyle name="Hyperlink" xfId="3" builtinId="8" hidden="1"/>
@@ -2909,6 +2966,8 @@
     <cellStyle name="Hyperlink" xfId="396" builtinId="8" hidden="1"/>
     <cellStyle name="Hyperlink" xfId="398" builtinId="8" hidden="1"/>
     <cellStyle name="Hyperlink" xfId="400" builtinId="8" hidden="1"/>
+    <cellStyle name="Hyperlink" xfId="402" builtinId="8" hidden="1"/>
+    <cellStyle name="Hyperlink" xfId="404" builtinId="8" hidden="1"/>
     <cellStyle name="Neutral" xfId="12" builtinId="28"/>
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
   </cellStyles>
@@ -3241,8 +3300,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:J203"/>
   <sheetViews>
-    <sheetView topLeftCell="A148" zoomScale="150" zoomScaleNormal="150" zoomScalePageLayoutView="150" workbookViewId="0">
-      <selection activeCell="C161" sqref="C161"/>
+    <sheetView tabSelected="1" topLeftCell="A5" zoomScale="150" zoomScaleNormal="150" zoomScalePageLayoutView="150" workbookViewId="0">
+      <selection activeCell="C9" sqref="C9"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultColWidth="11.5" defaultRowHeight="12.75" customHeight="1" x14ac:dyDescent="0"/>
@@ -3256,7 +3315,7 @@
   <sheetData>
     <row r="1" spans="1:9" ht="12">
       <c r="A1" t="s">
-        <v>420</v>
+        <v>418</v>
       </c>
       <c r="B1" s="1" t="s">
         <v>0</v>
@@ -3271,21 +3330,21 @@
         <v>3</v>
       </c>
       <c r="F1" s="2" t="s">
+        <v>54</v>
+      </c>
+      <c r="G1" t="s">
         <v>55</v>
       </c>
-      <c r="G1" t="s">
-        <v>56</v>
-      </c>
       <c r="H1" t="s">
-        <v>64</v>
+        <v>63</v>
       </c>
       <c r="I1" t="s">
-        <v>479</v>
+        <v>477</v>
       </c>
     </row>
     <row r="2" spans="1:9" ht="15">
       <c r="B2" s="16" t="s">
-        <v>94</v>
+        <v>92</v>
       </c>
       <c r="C2" s="1"/>
       <c r="D2" s="3"/>
@@ -3294,7 +3353,7 @@
     </row>
     <row r="3" spans="1:9" ht="12">
       <c r="B3" s="3" t="s">
-        <v>207</v>
+        <v>205</v>
       </c>
       <c r="C3" s="4" t="s">
         <v>4</v>
@@ -3319,12 +3378,12 @@
         <v>8</v>
       </c>
       <c r="B5" s="19" t="s">
-        <v>405</v>
+        <v>403</v>
       </c>
       <c r="C5" s="19"/>
       <c r="D5" s="19"/>
       <c r="E5" s="19" t="s">
-        <v>406</v>
+        <v>404</v>
       </c>
       <c r="F5" s="19"/>
       <c r="G5" s="19"/>
@@ -3333,12 +3392,12 @@
     <row r="6" spans="1:9" ht="12.75" customHeight="1">
       <c r="A6" s="22"/>
       <c r="B6" s="19" t="s">
-        <v>407</v>
+        <v>405</v>
       </c>
       <c r="C6" s="19"/>
       <c r="D6" s="19"/>
       <c r="E6" s="19" t="s">
-        <v>408</v>
+        <v>406</v>
       </c>
       <c r="F6" s="19"/>
       <c r="G6" s="19"/>
@@ -3347,7 +3406,7 @@
     <row r="7" spans="1:9" s="12" customFormat="1" ht="18" customHeight="1">
       <c r="A7" s="23"/>
       <c r="B7" s="18" t="s">
-        <v>96</v>
+        <v>94</v>
       </c>
       <c r="C7" s="18"/>
       <c r="D7" s="18"/>
@@ -3359,7 +3418,7 @@
     <row r="8" spans="1:9" s="12" customFormat="1" ht="18" customHeight="1">
       <c r="A8" s="23"/>
       <c r="B8" t="s">
-        <v>208</v>
+        <v>206</v>
       </c>
       <c r="C8" t="s">
         <v>7</v>
@@ -3375,73 +3434,75 @@
     <row r="9" spans="1:9" ht="18" customHeight="1">
       <c r="A9" s="22"/>
       <c r="B9" s="2" t="s">
-        <v>13</v>
-      </c>
-      <c r="C9" s="2"/>
+        <v>550</v>
+      </c>
+      <c r="C9" s="2" t="s">
+        <v>544</v>
+      </c>
       <c r="D9" s="2" t="s">
-        <v>89</v>
+        <v>87</v>
       </c>
       <c r="E9" s="2" t="s">
-        <v>107</v>
+        <v>105</v>
       </c>
       <c r="F9" s="2"/>
       <c r="G9" t="s">
-        <v>109</v>
+        <v>107</v>
       </c>
     </row>
     <row r="10" spans="1:9" ht="18" customHeight="1">
       <c r="A10" s="22"/>
       <c r="B10" s="2" t="s">
-        <v>90</v>
+        <v>88</v>
       </c>
       <c r="C10" s="4"/>
       <c r="D10" s="2" t="s">
-        <v>88</v>
+        <v>86</v>
       </c>
       <c r="E10" s="2" t="s">
-        <v>110</v>
+        <v>108</v>
       </c>
       <c r="F10" s="2"/>
     </row>
     <row r="11" spans="1:9" ht="18" customHeight="1">
       <c r="A11" s="22"/>
       <c r="B11" s="2" t="s">
-        <v>90</v>
+        <v>88</v>
       </c>
       <c r="C11" s="4"/>
       <c r="D11" s="2" t="s">
-        <v>91</v>
+        <v>89</v>
       </c>
       <c r="E11" s="2" t="s">
-        <v>108</v>
+        <v>106</v>
       </c>
       <c r="F11" s="2"/>
     </row>
     <row r="12" spans="1:9" ht="18" customHeight="1">
       <c r="A12" s="22"/>
       <c r="B12" s="2" t="s">
-        <v>251</v>
+        <v>249</v>
       </c>
       <c r="C12" s="2" t="s">
-        <v>252</v>
+        <v>250</v>
       </c>
       <c r="D12" s="2" t="s">
-        <v>73</v>
+        <v>72</v>
       </c>
       <c r="E12" s="2" t="s">
-        <v>114</v>
+        <v>112</v>
       </c>
       <c r="F12" s="2"/>
     </row>
     <row r="13" spans="1:9" ht="12.75" customHeight="1">
       <c r="A13" s="22"/>
       <c r="B13" s="19" t="s">
-        <v>411</v>
+        <v>409</v>
       </c>
       <c r="C13" s="19"/>
       <c r="D13" s="19"/>
       <c r="E13" s="19" t="s">
-        <v>417</v>
+        <v>415</v>
       </c>
       <c r="F13" s="19"/>
       <c r="G13" s="19"/>
@@ -3450,12 +3511,12 @@
     <row r="14" spans="1:9" ht="12.75" customHeight="1">
       <c r="A14" s="22"/>
       <c r="B14" s="19" t="s">
-        <v>412</v>
+        <v>410</v>
       </c>
       <c r="C14" s="19"/>
       <c r="D14" s="19"/>
       <c r="E14" s="19" t="s">
-        <v>254</v>
+        <v>252</v>
       </c>
       <c r="F14" s="19"/>
       <c r="G14" s="19"/>
@@ -3464,7 +3525,7 @@
     <row r="15" spans="1:9" s="12" customFormat="1" ht="18" customHeight="1">
       <c r="A15" s="23"/>
       <c r="B15" s="18" t="s">
-        <v>409</v>
+        <v>407</v>
       </c>
       <c r="C15" s="18"/>
       <c r="D15" s="18"/>
@@ -3476,110 +3537,110 @@
     <row r="16" spans="1:9" ht="12">
       <c r="A16" s="22"/>
       <c r="B16" t="s">
-        <v>209</v>
+        <v>207</v>
       </c>
       <c r="C16" t="s">
-        <v>115</v>
+        <v>113</v>
       </c>
       <c r="D16" t="s">
-        <v>253</v>
+        <v>251</v>
       </c>
       <c r="E16" s="2"/>
     </row>
     <row r="17" spans="1:10" ht="11" customHeight="1">
       <c r="A17" s="22"/>
       <c r="B17" t="s">
+        <v>126</v>
+      </c>
+      <c r="C17" t="s">
+        <v>127</v>
+      </c>
+      <c r="D17" t="s">
         <v>128</v>
       </c>
-      <c r="C17" t="s">
+      <c r="E17" s="2" t="s">
         <v>129</v>
-      </c>
-      <c r="D17" t="s">
-        <v>130</v>
-      </c>
-      <c r="E17" s="2" t="s">
-        <v>131</v>
       </c>
     </row>
     <row r="18" spans="1:10" ht="11" customHeight="1">
       <c r="A18" s="22"/>
       <c r="B18" t="s">
+        <v>130</v>
+      </c>
+      <c r="C18" t="s">
+        <v>131</v>
+      </c>
+      <c r="D18" t="s">
         <v>132</v>
       </c>
-      <c r="C18" t="s">
+      <c r="E18" s="2" t="s">
         <v>133</v>
-      </c>
-      <c r="D18" t="s">
-        <v>134</v>
-      </c>
-      <c r="E18" s="2" t="s">
-        <v>135</v>
       </c>
     </row>
     <row r="19" spans="1:10" ht="11" customHeight="1">
       <c r="A19" s="22"/>
       <c r="B19" t="s">
+        <v>147</v>
+      </c>
+      <c r="C19" t="s">
+        <v>148</v>
+      </c>
+      <c r="D19" t="s">
         <v>149</v>
       </c>
-      <c r="C19" t="s">
+      <c r="E19" s="2" t="s">
         <v>150</v>
-      </c>
-      <c r="D19" t="s">
-        <v>151</v>
-      </c>
-      <c r="E19" s="2" t="s">
-        <v>152</v>
       </c>
     </row>
     <row r="20" spans="1:10" ht="11" customHeight="1">
       <c r="A20" s="22"/>
       <c r="B20" t="s">
+        <v>217</v>
+      </c>
+      <c r="C20" t="s">
+        <v>218</v>
+      </c>
+      <c r="D20" t="s">
         <v>219</v>
       </c>
-      <c r="C20" t="s">
+      <c r="E20" s="2" t="s">
         <v>220</v>
-      </c>
-      <c r="D20" t="s">
-        <v>221</v>
-      </c>
-      <c r="E20" s="2" t="s">
-        <v>222</v>
       </c>
     </row>
     <row r="21" spans="1:10" ht="11" customHeight="1">
       <c r="A21" s="22"/>
       <c r="B21" t="s">
+        <v>151</v>
+      </c>
+      <c r="C21" t="s">
+        <v>152</v>
+      </c>
+      <c r="D21" t="s">
         <v>153</v>
       </c>
-      <c r="C21" t="s">
-        <v>154</v>
-      </c>
-      <c r="D21" t="s">
-        <v>155</v>
-      </c>
       <c r="E21" s="2" t="s">
-        <v>205</v>
+        <v>203</v>
       </c>
     </row>
     <row r="22" spans="1:10" ht="11" customHeight="1">
       <c r="A22" s="22"/>
       <c r="B22" t="s">
+        <v>154</v>
+      </c>
+      <c r="C22" t="s">
+        <v>155</v>
+      </c>
+      <c r="D22" t="s">
         <v>156</v>
       </c>
-      <c r="C22" t="s">
-        <v>157</v>
-      </c>
-      <c r="D22" t="s">
-        <v>158</v>
-      </c>
       <c r="E22" s="2" t="s">
-        <v>206</v>
+        <v>204</v>
       </c>
     </row>
     <row r="23" spans="1:10" ht="11" customHeight="1">
       <c r="A23" s="22"/>
       <c r="B23" s="20" t="s">
-        <v>410</v>
+        <v>408</v>
       </c>
       <c r="C23" s="20"/>
       <c r="D23" s="20"/>
@@ -3593,12 +3654,12 @@
     <row r="24" spans="1:10" ht="12.75" customHeight="1">
       <c r="A24" s="22"/>
       <c r="B24" s="19" t="s">
-        <v>413</v>
+        <v>411</v>
       </c>
       <c r="C24" s="19"/>
       <c r="D24" s="19"/>
       <c r="E24" s="19" t="s">
-        <v>418</v>
+        <v>416</v>
       </c>
       <c r="F24" s="19"/>
       <c r="G24" s="19"/>
@@ -3607,12 +3668,12 @@
     <row r="25" spans="1:10" ht="12.75" customHeight="1">
       <c r="A25" s="22"/>
       <c r="B25" s="19" t="s">
-        <v>414</v>
+        <v>412</v>
       </c>
       <c r="C25" s="19"/>
       <c r="D25" s="19"/>
       <c r="E25" s="19" t="s">
-        <v>258</v>
+        <v>256</v>
       </c>
       <c r="F25" s="19"/>
       <c r="G25" s="19"/>
@@ -3621,7 +3682,7 @@
     <row r="26" spans="1:10" s="12" customFormat="1" ht="18" customHeight="1">
       <c r="A26" s="23"/>
       <c r="B26" s="18" t="s">
-        <v>415</v>
+        <v>413</v>
       </c>
       <c r="C26" s="18"/>
       <c r="D26" s="18"/>
@@ -3633,110 +3694,110 @@
     <row r="27" spans="1:10" ht="11" customHeight="1">
       <c r="A27" s="22"/>
       <c r="B27" t="s">
+        <v>253</v>
+      </c>
+      <c r="C27" t="s">
+        <v>254</v>
+      </c>
+      <c r="D27" t="s">
         <v>255</v>
-      </c>
-      <c r="C27" t="s">
-        <v>256</v>
-      </c>
-      <c r="D27" t="s">
-        <v>257</v>
       </c>
       <c r="E27" s="2"/>
     </row>
     <row r="28" spans="1:10" ht="11" customHeight="1">
       <c r="A28" s="22"/>
       <c r="B28" t="s">
-        <v>306</v>
+        <v>304</v>
       </c>
       <c r="C28" t="s">
-        <v>286</v>
+        <v>284</v>
       </c>
       <c r="D28" t="s">
-        <v>264</v>
+        <v>262</v>
       </c>
       <c r="E28" s="2" t="s">
-        <v>265</v>
+        <v>263</v>
       </c>
     </row>
     <row r="29" spans="1:10" ht="11" customHeight="1">
       <c r="A29" s="22"/>
       <c r="B29" t="s">
-        <v>307</v>
+        <v>305</v>
       </c>
       <c r="C29" t="s">
-        <v>287</v>
+        <v>285</v>
       </c>
       <c r="D29" t="s">
-        <v>276</v>
+        <v>274</v>
       </c>
       <c r="E29" s="2" t="s">
-        <v>267</v>
+        <v>265</v>
       </c>
     </row>
     <row r="30" spans="1:10" ht="11" customHeight="1">
       <c r="A30" s="22"/>
       <c r="B30" t="s">
-        <v>308</v>
+        <v>306</v>
       </c>
       <c r="C30" t="s">
-        <v>288</v>
+        <v>286</v>
       </c>
       <c r="D30" t="s">
-        <v>279</v>
+        <v>277</v>
       </c>
       <c r="E30" s="2" t="s">
-        <v>268</v>
+        <v>266</v>
       </c>
     </row>
     <row r="31" spans="1:10" ht="11" customHeight="1">
       <c r="A31" s="22"/>
       <c r="B31" t="s">
-        <v>309</v>
+        <v>307</v>
       </c>
       <c r="C31" t="s">
-        <v>289</v>
+        <v>287</v>
       </c>
       <c r="D31" t="s">
-        <v>277</v>
+        <v>275</v>
       </c>
       <c r="E31" s="2" t="s">
-        <v>271</v>
+        <v>269</v>
       </c>
     </row>
     <row r="32" spans="1:10" ht="11" customHeight="1">
       <c r="A32" s="22"/>
       <c r="B32" t="s">
-        <v>310</v>
+        <v>308</v>
       </c>
       <c r="C32" t="s">
-        <v>290</v>
+        <v>288</v>
       </c>
       <c r="D32" t="s">
-        <v>278</v>
+        <v>276</v>
       </c>
       <c r="E32" s="2" t="s">
-        <v>273</v>
+        <v>271</v>
       </c>
     </row>
     <row r="33" spans="1:10" ht="12" customHeight="1">
       <c r="A33" s="22"/>
       <c r="B33" t="s">
-        <v>311</v>
+        <v>309</v>
       </c>
       <c r="C33" t="s">
-        <v>291</v>
+        <v>289</v>
       </c>
       <c r="D33" t="s">
-        <v>280</v>
+        <v>278</v>
       </c>
       <c r="E33" s="2" t="s">
-        <v>275</v>
+        <v>273</v>
       </c>
     </row>
     <row r="34" spans="1:10" ht="12" customHeight="1">
       <c r="A34" s="22"/>
       <c r="B34" s="20" t="s">
-        <v>416</v>
+        <v>414</v>
       </c>
       <c r="C34" s="20"/>
       <c r="D34" s="20"/>
@@ -3755,7 +3816,7 @@
       <c r="C35" s="4"/>
       <c r="D35" s="2"/>
       <c r="E35" s="2" t="s">
-        <v>401</v>
+        <v>399</v>
       </c>
       <c r="F35" s="2"/>
     </row>
@@ -3766,7 +3827,7 @@
       </c>
       <c r="C36" s="4"/>
       <c r="D36" s="2" t="s">
-        <v>379</v>
+        <v>377</v>
       </c>
       <c r="E36" s="2"/>
       <c r="F36" s="2"/>
@@ -3777,7 +3838,7 @@
         <v>13</v>
       </c>
       <c r="D37" t="s">
-        <v>213</v>
+        <v>211</v>
       </c>
     </row>
     <row r="38" spans="1:10" ht="25" customHeight="1">
@@ -3786,7 +3847,7 @@
         <v>13</v>
       </c>
       <c r="D38" t="s">
-        <v>226</v>
+        <v>224</v>
       </c>
     </row>
     <row r="39" spans="1:10" ht="25" customHeight="1">
@@ -3795,7 +3856,7 @@
         <v>13</v>
       </c>
       <c r="D39" t="s">
-        <v>227</v>
+        <v>225</v>
       </c>
     </row>
     <row r="40" spans="1:10" ht="25" customHeight="1">
@@ -3804,7 +3865,7 @@
         <v>13</v>
       </c>
       <c r="D40" t="s">
-        <v>249</v>
+        <v>247</v>
       </c>
     </row>
     <row r="41" spans="1:10" ht="25" customHeight="1">
@@ -3813,7 +3874,7 @@
         <v>13</v>
       </c>
       <c r="D41" t="s">
-        <v>228</v>
+        <v>226</v>
       </c>
     </row>
     <row r="42" spans="1:10" ht="25" customHeight="1">
@@ -3822,7 +3883,7 @@
         <v>13</v>
       </c>
       <c r="D42" t="s">
-        <v>229</v>
+        <v>227</v>
       </c>
     </row>
     <row r="43" spans="1:10" ht="25" customHeight="1">
@@ -3831,7 +3892,7 @@
         <v>13</v>
       </c>
       <c r="D43" t="s">
-        <v>250</v>
+        <v>248</v>
       </c>
     </row>
     <row r="44" spans="1:10" ht="25" customHeight="1">
@@ -3840,7 +3901,7 @@
         <v>13</v>
       </c>
       <c r="D44" t="s">
-        <v>378</v>
+        <v>376</v>
       </c>
     </row>
     <row r="45" spans="1:10" ht="25" customHeight="1">
@@ -3849,7 +3910,7 @@
         <v>13</v>
       </c>
       <c r="D45" t="s">
-        <v>380</v>
+        <v>378</v>
       </c>
     </row>
     <row r="46" spans="1:10" ht="25" customHeight="1">
@@ -3858,7 +3919,7 @@
         <v>13</v>
       </c>
       <c r="D46" t="s">
-        <v>381</v>
+        <v>379</v>
       </c>
     </row>
     <row r="47" spans="1:10" ht="25" customHeight="1">
@@ -3867,7 +3928,7 @@
         <v>13</v>
       </c>
       <c r="D47" t="s">
-        <v>419</v>
+        <v>417</v>
       </c>
     </row>
     <row r="48" spans="1:10" ht="25" customHeight="1">
@@ -3876,7 +3937,7 @@
         <v>13</v>
       </c>
       <c r="D48" t="s">
-        <v>382</v>
+        <v>380</v>
       </c>
     </row>
     <row r="49" spans="1:10" ht="25" customHeight="1">
@@ -3885,7 +3946,7 @@
         <v>13</v>
       </c>
       <c r="D49" t="s">
-        <v>383</v>
+        <v>381</v>
       </c>
     </row>
     <row r="50" spans="1:10" ht="25" customHeight="1">
@@ -3894,7 +3955,7 @@
         <v>13</v>
       </c>
       <c r="D50" t="s">
-        <v>384</v>
+        <v>382</v>
       </c>
     </row>
     <row r="51" spans="1:10" ht="25" customHeight="1">
@@ -3903,7 +3964,7 @@
         <v>13</v>
       </c>
       <c r="D51" t="s">
-        <v>385</v>
+        <v>383</v>
       </c>
     </row>
     <row r="52" spans="1:10" ht="25" customHeight="1">
@@ -3912,7 +3973,7 @@
         <v>13</v>
       </c>
       <c r="D52" t="s">
-        <v>402</v>
+        <v>400</v>
       </c>
     </row>
     <row r="53" spans="1:10" ht="25" customHeight="1">
@@ -3924,7 +3985,7 @@
     <row r="54" spans="1:10" ht="15">
       <c r="A54" s="22"/>
       <c r="B54" s="15" t="s">
-        <v>66</v>
+        <v>65</v>
       </c>
       <c r="C54" s="15"/>
       <c r="D54" s="15"/>
@@ -3944,15 +4005,15 @@
     </row>
     <row r="56" spans="1:10" s="15" customFormat="1" ht="15">
       <c r="A56" s="22" t="s">
-        <v>440</v>
+        <v>438</v>
       </c>
       <c r="B56" s="13" t="s">
-        <v>93</v>
+        <v>91</v>
       </c>
       <c r="C56" s="13"/>
       <c r="D56" s="13"/>
       <c r="E56" s="13" t="s">
-        <v>65</v>
+        <v>64</v>
       </c>
       <c r="F56" s="13"/>
       <c r="G56" s="13"/>
@@ -3963,12 +4024,12 @@
     <row r="57" spans="1:10" ht="12">
       <c r="A57" s="22"/>
       <c r="B57" s="5" t="s">
-        <v>67</v>
+        <v>66</v>
       </c>
       <c r="C57" s="5"/>
       <c r="D57" s="5"/>
       <c r="E57" s="6" t="s">
-        <v>68</v>
+        <v>67</v>
       </c>
       <c r="F57" s="5"/>
       <c r="G57" s="5"/>
@@ -3977,7 +4038,7 @@
     <row r="58" spans="1:10" ht="15">
       <c r="A58" s="22"/>
       <c r="B58" s="15" t="s">
-        <v>92</v>
+        <v>90</v>
       </c>
       <c r="C58" s="15"/>
       <c r="D58" s="15"/>
@@ -3989,7 +4050,7 @@
     <row r="59" spans="1:10" ht="12">
       <c r="A59" s="22"/>
       <c r="B59" s="12" t="s">
-        <v>210</v>
+        <v>208</v>
       </c>
       <c r="C59" s="12" t="s">
         <v>9</v>
@@ -4012,7 +4073,7 @@
       <c r="C60" s="8"/>
       <c r="D60" s="8"/>
       <c r="E60" s="9" t="s">
-        <v>57</v>
+        <v>56</v>
       </c>
       <c r="F60" s="8"/>
       <c r="G60" s="10"/>
@@ -4024,10 +4085,10 @@
         <v>13</v>
       </c>
       <c r="C61" s="2" t="s">
-        <v>69</v>
+        <v>68</v>
       </c>
       <c r="D61" s="2" t="s">
-        <v>421</v>
+        <v>419</v>
       </c>
       <c r="E61" s="2"/>
       <c r="F61" s="4"/>
@@ -4038,7 +4099,7 @@
         <v>13</v>
       </c>
       <c r="D62" t="s">
-        <v>422</v>
+        <v>420</v>
       </c>
       <c r="E62" s="2"/>
       <c r="F62" s="4"/>
@@ -4050,7 +4111,7 @@
       </c>
       <c r="C63" s="2"/>
       <c r="D63" s="2" t="s">
-        <v>423</v>
+        <v>421</v>
       </c>
       <c r="E63" s="2"/>
       <c r="F63" s="4"/>
@@ -4062,7 +4123,7 @@
       </c>
       <c r="C64" s="2"/>
       <c r="D64" s="2" t="s">
-        <v>424</v>
+        <v>422</v>
       </c>
       <c r="E64" s="2"/>
       <c r="F64" s="4"/>
@@ -4074,7 +4135,7 @@
       </c>
       <c r="C65" s="2"/>
       <c r="D65" s="2" t="s">
-        <v>425</v>
+        <v>423</v>
       </c>
       <c r="E65" s="2"/>
       <c r="F65" s="4"/>
@@ -4086,7 +4147,7 @@
       </c>
       <c r="C66" s="2"/>
       <c r="D66" s="2" t="s">
-        <v>426</v>
+        <v>424</v>
       </c>
       <c r="E66" s="2"/>
       <c r="F66" s="4"/>
@@ -4098,7 +4159,7 @@
       </c>
       <c r="C67" s="2"/>
       <c r="D67" s="2" t="s">
-        <v>427</v>
+        <v>425</v>
       </c>
       <c r="E67" s="2"/>
       <c r="F67" s="4"/>
@@ -4110,7 +4171,7 @@
       </c>
       <c r="C68" s="2"/>
       <c r="D68" s="2" t="s">
-        <v>428</v>
+        <v>426</v>
       </c>
       <c r="E68" s="2"/>
       <c r="F68" s="4"/>
@@ -4122,7 +4183,7 @@
       </c>
       <c r="C69" s="2"/>
       <c r="D69" s="2" t="s">
-        <v>436</v>
+        <v>434</v>
       </c>
       <c r="E69" s="2"/>
       <c r="F69" s="4"/>
@@ -4134,7 +4195,7 @@
       </c>
       <c r="C70" s="2"/>
       <c r="D70" s="2" t="s">
-        <v>435</v>
+        <v>433</v>
       </c>
       <c r="E70" s="2"/>
       <c r="F70" s="4"/>
@@ -4146,7 +4207,7 @@
       </c>
       <c r="C71" s="2"/>
       <c r="D71" s="2" t="s">
-        <v>437</v>
+        <v>435</v>
       </c>
       <c r="E71" s="2"/>
       <c r="F71" s="4"/>
@@ -4158,7 +4219,7 @@
       </c>
       <c r="C72" s="2"/>
       <c r="D72" s="2" t="s">
-        <v>438</v>
+        <v>436</v>
       </c>
       <c r="E72" s="2"/>
       <c r="F72" s="4"/>
@@ -4170,7 +4231,7 @@
       </c>
       <c r="C73" s="2"/>
       <c r="D73" s="2" t="s">
-        <v>429</v>
+        <v>427</v>
       </c>
       <c r="E73" s="2"/>
       <c r="F73" s="4"/>
@@ -4182,7 +4243,7 @@
       </c>
       <c r="C74" s="2"/>
       <c r="D74" s="2" t="s">
-        <v>432</v>
+        <v>430</v>
       </c>
       <c r="E74" s="2"/>
       <c r="F74" s="4"/>
@@ -4194,7 +4255,7 @@
       </c>
       <c r="C75" s="2"/>
       <c r="D75" s="2" t="s">
-        <v>433</v>
+        <v>431</v>
       </c>
       <c r="E75" s="2"/>
       <c r="F75" s="4"/>
@@ -4206,7 +4267,7 @@
       </c>
       <c r="C76" s="2"/>
       <c r="D76" s="2" t="s">
-        <v>434</v>
+        <v>432</v>
       </c>
       <c r="E76" s="2"/>
       <c r="F76" s="4"/>
@@ -4218,7 +4279,7 @@
       </c>
       <c r="C77" s="2"/>
       <c r="D77" s="2" t="s">
-        <v>430</v>
+        <v>428</v>
       </c>
       <c r="E77" s="2"/>
       <c r="F77" s="4"/>
@@ -4230,7 +4291,7 @@
       </c>
       <c r="C78" s="2"/>
       <c r="D78" s="2" t="s">
-        <v>431</v>
+        <v>429</v>
       </c>
       <c r="E78" s="2"/>
       <c r="F78" s="4"/>
@@ -4242,7 +4303,7 @@
       </c>
       <c r="C79" s="2"/>
       <c r="D79" s="2" t="s">
-        <v>439</v>
+        <v>437</v>
       </c>
       <c r="E79" s="2"/>
       <c r="F79" s="4"/>
@@ -4271,7 +4332,7 @@
         <v>13</v>
       </c>
       <c r="C82" s="2" t="s">
-        <v>70</v>
+        <v>69</v>
       </c>
       <c r="D82" s="2"/>
       <c r="E82" s="2"/>
@@ -4286,7 +4347,7 @@
         <v>13</v>
       </c>
       <c r="D83" t="s">
-        <v>71</v>
+        <v>70</v>
       </c>
       <c r="E83" s="13"/>
     </row>
@@ -4296,7 +4357,7 @@
         <v>13</v>
       </c>
       <c r="H84" t="s">
-        <v>72</v>
+        <v>71</v>
       </c>
     </row>
     <row r="85" spans="1:8" ht="12">
@@ -4314,23 +4375,23 @@
     <row r="86" spans="1:8" s="10" customFormat="1" ht="12"/>
     <row r="87" spans="1:8" s="10" customFormat="1" ht="15">
       <c r="B87" s="10" t="s">
-        <v>470</v>
+        <v>468</v>
       </c>
       <c r="E87" s="13" t="s">
-        <v>475</v>
+        <v>473</v>
       </c>
     </row>
     <row r="88" spans="1:8" s="10" customFormat="1" ht="15">
       <c r="B88" s="10" t="s">
-        <v>471</v>
+        <v>469</v>
       </c>
       <c r="E88" s="38" t="s">
-        <v>474</v>
+        <v>472</v>
       </c>
     </row>
     <row r="89" spans="1:8" s="10" customFormat="1" ht="12">
       <c r="B89" s="10" t="s">
-        <v>472</v>
+        <v>470</v>
       </c>
     </row>
     <row r="90" spans="1:8" s="10" customFormat="1" ht="12">
@@ -4338,24 +4399,24 @@
         <v>13</v>
       </c>
       <c r="D90" s="10" t="s">
-        <v>36</v>
+        <v>35</v>
       </c>
     </row>
     <row r="91" spans="1:8" s="10" customFormat="1" ht="12">
       <c r="B91" s="10" t="s">
-        <v>473</v>
+        <v>471</v>
       </c>
     </row>
     <row r="92" spans="1:8" s="10" customFormat="1" ht="12"/>
     <row r="93" spans="1:8" ht="30">
       <c r="A93" s="22"/>
       <c r="B93" s="13" t="s">
-        <v>445</v>
+        <v>443</v>
       </c>
       <c r="C93" s="13"/>
       <c r="D93" s="13"/>
       <c r="E93" s="13" t="s">
-        <v>441</v>
+        <v>439</v>
       </c>
       <c r="F93" s="13"/>
       <c r="G93" s="13"/>
@@ -4364,12 +4425,12 @@
     <row r="94" spans="1:8" ht="30">
       <c r="A94" s="22"/>
       <c r="B94" s="13" t="s">
-        <v>446</v>
+        <v>444</v>
       </c>
       <c r="C94" s="13"/>
       <c r="D94" s="13"/>
       <c r="E94" s="13" t="s">
-        <v>447</v>
+        <v>445</v>
       </c>
       <c r="F94" s="13"/>
       <c r="G94" s="13"/>
@@ -4378,7 +4439,7 @@
     <row r="95" spans="1:8" ht="15">
       <c r="A95" s="22"/>
       <c r="B95" s="15" t="s">
-        <v>443</v>
+        <v>441</v>
       </c>
       <c r="C95" s="15"/>
       <c r="D95" s="15"/>
@@ -4400,10 +4461,10 @@
     <row r="97" spans="1:8" ht="24">
       <c r="A97" s="22"/>
       <c r="B97" t="s">
-        <v>454</v>
+        <v>452</v>
       </c>
       <c r="C97" t="s">
-        <v>453</v>
+        <v>451</v>
       </c>
       <c r="F97" t="s">
         <v>6</v>
@@ -4414,12 +4475,12 @@
     <row r="98" spans="1:8" ht="30">
       <c r="A98" s="22"/>
       <c r="B98" s="13" t="s">
-        <v>459</v>
+        <v>457</v>
       </c>
       <c r="C98" s="13"/>
       <c r="D98" s="13"/>
       <c r="E98" s="13" t="s">
-        <v>456</v>
+        <v>454</v>
       </c>
       <c r="F98" s="13"/>
       <c r="G98" s="10"/>
@@ -4428,12 +4489,12 @@
     <row r="99" spans="1:8" ht="30">
       <c r="A99" s="22"/>
       <c r="B99" s="13" t="s">
-        <v>460</v>
+        <v>458</v>
       </c>
       <c r="C99" s="13"/>
       <c r="D99" s="13"/>
       <c r="E99" s="13" t="s">
-        <v>461</v>
+        <v>459</v>
       </c>
       <c r="F99" s="13"/>
       <c r="G99" s="10"/>
@@ -4442,7 +4503,7 @@
     <row r="100" spans="1:8" ht="15">
       <c r="A100" s="22"/>
       <c r="B100" s="15" t="s">
-        <v>457</v>
+        <v>455</v>
       </c>
       <c r="C100" s="15"/>
       <c r="D100" s="15"/>
@@ -4465,7 +4526,7 @@
       </c>
       <c r="C102" s="12"/>
       <c r="D102" s="26" t="s">
-        <v>468</v>
+        <v>466</v>
       </c>
       <c r="E102" s="12"/>
       <c r="F102" s="12"/>
@@ -4487,7 +4548,7 @@
     <row r="104" spans="1:8" ht="15">
       <c r="A104" s="22"/>
       <c r="B104" s="15" t="s">
-        <v>458</v>
+        <v>456</v>
       </c>
       <c r="C104" s="18"/>
       <c r="D104" s="32"/>
@@ -4499,24 +4560,24 @@
     <row r="105" spans="1:8" ht="30">
       <c r="A105" s="28"/>
       <c r="B105" s="13" t="s">
-        <v>463</v>
+        <v>461</v>
       </c>
       <c r="C105" s="13"/>
       <c r="D105" s="13"/>
       <c r="E105" s="13" t="s">
-        <v>455</v>
+        <v>453</v>
       </c>
       <c r="F105" s="13"/>
     </row>
     <row r="106" spans="1:8" ht="30">
       <c r="A106" s="28"/>
       <c r="B106" s="13" t="s">
-        <v>464</v>
+        <v>462</v>
       </c>
       <c r="C106" s="13"/>
       <c r="D106" s="13"/>
       <c r="E106" s="13" t="s">
-        <v>465</v>
+        <v>463</v>
       </c>
       <c r="F106" s="13"/>
     </row>
@@ -4526,7 +4587,7 @@
       </c>
       <c r="C107" s="27"/>
       <c r="D107" s="27" t="s">
-        <v>477</v>
+        <v>475</v>
       </c>
       <c r="E107" s="27"/>
       <c r="F107" s="27"/>
@@ -4534,7 +4595,7 @@
     <row r="108" spans="1:8" ht="15">
       <c r="A108" s="28"/>
       <c r="B108" s="15" t="s">
-        <v>466</v>
+        <v>464</v>
       </c>
       <c r="C108" s="15"/>
       <c r="D108" s="15"/>
@@ -4554,7 +4615,7 @@
       </c>
       <c r="C110" s="21"/>
       <c r="D110" s="29" t="s">
-        <v>462</v>
+        <v>460</v>
       </c>
       <c r="E110" s="29"/>
       <c r="F110" s="21"/>
@@ -4579,7 +4640,7 @@
     <row r="113" spans="1:9" ht="15">
       <c r="A113" s="28"/>
       <c r="B113" s="15" t="s">
-        <v>467</v>
+        <v>465</v>
       </c>
       <c r="C113" s="30"/>
       <c r="D113" s="31"/>
@@ -4592,7 +4653,7 @@
       </c>
       <c r="C114" s="34"/>
       <c r="D114" s="35" t="s">
-        <v>476</v>
+        <v>474</v>
       </c>
       <c r="E114" s="34"/>
       <c r="F114" s="34"/>
@@ -4600,7 +4661,7 @@
     <row r="115" spans="1:9" ht="15">
       <c r="A115" s="28"/>
       <c r="B115" s="15" t="s">
-        <v>444</v>
+        <v>442</v>
       </c>
       <c r="C115" s="30"/>
       <c r="D115" s="31"/>
@@ -4613,7 +4674,7 @@
       </c>
       <c r="C116" s="34"/>
       <c r="D116" s="35" t="s">
-        <v>478</v>
+        <v>476</v>
       </c>
       <c r="E116" s="34"/>
       <c r="F116" s="34"/>
@@ -4621,7 +4682,7 @@
     <row r="117" spans="1:9" ht="15">
       <c r="A117" s="28"/>
       <c r="B117" s="15" t="s">
-        <v>74</v>
+        <v>73</v>
       </c>
       <c r="C117" s="30"/>
       <c r="D117" s="31"/>
@@ -4639,33 +4700,33 @@
     <row r="119" spans="1:9" s="13" customFormat="1" ht="15">
       <c r="A119" s="27"/>
       <c r="B119" s="13" t="s">
-        <v>97</v>
+        <v>95</v>
       </c>
       <c r="C119" s="36"/>
       <c r="D119" s="37"/>
       <c r="E119" s="14" t="s">
-        <v>469</v>
+        <v>467</v>
       </c>
       <c r="F119" s="36"/>
     </row>
     <row r="120" spans="1:9" s="13" customFormat="1" ht="15">
       <c r="A120" s="27"/>
       <c r="B120" s="13" t="s">
-        <v>75</v>
+        <v>74</v>
       </c>
       <c r="C120" s="36"/>
       <c r="D120" s="37"/>
       <c r="E120" s="14" t="s">
-        <v>76</v>
+        <v>75</v>
       </c>
       <c r="F120" s="36"/>
     </row>
     <row r="121" spans="1:9" ht="15">
       <c r="A121" s="22" t="s">
-        <v>451</v>
+        <v>449</v>
       </c>
       <c r="B121" s="15" t="s">
-        <v>98</v>
+        <v>96</v>
       </c>
       <c r="C121" s="15"/>
       <c r="D121" s="15"/>
@@ -4677,7 +4738,7 @@
     <row r="122" spans="1:9" ht="12">
       <c r="A122" s="22"/>
       <c r="B122" t="s">
-        <v>211</v>
+        <v>209</v>
       </c>
       <c r="C122" t="s">
         <v>11</v>
@@ -4697,7 +4758,7 @@
         <v>15</v>
       </c>
       <c r="E123" t="s">
-        <v>480</v>
+        <v>478</v>
       </c>
     </row>
     <row r="124" spans="1:9" ht="12">
@@ -4706,22 +4767,22 @@
         <v>13</v>
       </c>
       <c r="D124" t="s">
-        <v>41</v>
+        <v>40</v>
       </c>
     </row>
     <row r="125" spans="1:9" ht="12">
       <c r="A125" s="22"/>
       <c r="B125" t="s">
+        <v>479</v>
+      </c>
+      <c r="C125" t="s">
+        <v>480</v>
+      </c>
+      <c r="D125" t="s">
         <v>481</v>
       </c>
-      <c r="C125" t="s">
-        <v>482</v>
-      </c>
-      <c r="D125" t="s">
-        <v>483</v>
-      </c>
       <c r="F125" t="s">
-        <v>81</v>
+        <v>79</v>
       </c>
     </row>
     <row r="126" spans="1:9" ht="12.75" customHeight="1">
@@ -4730,10 +4791,10 @@
         <v>15</v>
       </c>
       <c r="C126" t="s">
-        <v>515</v>
+        <v>513</v>
       </c>
       <c r="E126" t="s">
-        <v>516</v>
+        <v>514</v>
       </c>
     </row>
     <row r="127" spans="1:9" ht="12.75" customHeight="1">
@@ -4742,10 +4803,10 @@
         <v>16</v>
       </c>
       <c r="C127" t="s">
-        <v>517</v>
+        <v>515</v>
       </c>
       <c r="D127" t="s">
-        <v>485</v>
+        <v>483</v>
       </c>
     </row>
     <row r="128" spans="1:9" ht="12.75" customHeight="1">
@@ -4754,10 +4815,10 @@
         <v>13</v>
       </c>
       <c r="D128" t="s">
-        <v>521</v>
+        <v>519</v>
       </c>
       <c r="E128" t="s">
-        <v>518</v>
+        <v>516</v>
       </c>
       <c r="I128" s="21"/>
     </row>
@@ -4773,7 +4834,7 @@
         <v>15</v>
       </c>
       <c r="E130" t="s">
-        <v>484</v>
+        <v>482</v>
       </c>
     </row>
     <row r="131" spans="1:9" ht="12">
@@ -4785,7 +4846,7 @@
         <v>20</v>
       </c>
       <c r="D131" t="s">
-        <v>485</v>
+        <v>483</v>
       </c>
     </row>
     <row r="132" spans="1:9" ht="12.75" customHeight="1">
@@ -4813,7 +4874,7 @@
         <v>15</v>
       </c>
       <c r="E134" t="s">
-        <v>486</v>
+        <v>484</v>
       </c>
     </row>
     <row r="135" spans="1:9" ht="12.75" customHeight="1">
@@ -4825,7 +4886,7 @@
         <v>17</v>
       </c>
       <c r="D135" t="s">
-        <v>487</v>
+        <v>485</v>
       </c>
     </row>
     <row r="136" spans="1:9" ht="12.75" customHeight="1">
@@ -4858,7 +4919,7 @@
         <v>15</v>
       </c>
       <c r="E139" t="s">
-        <v>488</v>
+        <v>486</v>
       </c>
     </row>
     <row r="140" spans="1:9" ht="12.75" customHeight="1">
@@ -4867,7 +4928,7 @@
         <v>13</v>
       </c>
       <c r="D140" t="s">
-        <v>43</v>
+        <v>42</v>
       </c>
     </row>
     <row r="141" spans="1:9" ht="12.75" customHeight="1">
@@ -4876,10 +4937,10 @@
         <v>16</v>
       </c>
       <c r="C141" t="s">
-        <v>489</v>
+        <v>487</v>
       </c>
       <c r="D141" t="s">
-        <v>490</v>
+        <v>488</v>
       </c>
     </row>
     <row r="142" spans="1:9" ht="12.75" customHeight="1">
@@ -4888,10 +4949,10 @@
         <v>16</v>
       </c>
       <c r="C142" t="s">
-        <v>491</v>
+        <v>489</v>
       </c>
       <c r="D142" t="s">
-        <v>492</v>
+        <v>490</v>
       </c>
     </row>
     <row r="143" spans="1:9" ht="12.75" customHeight="1">
@@ -4900,10 +4961,10 @@
         <v>13</v>
       </c>
       <c r="D143" t="s">
-        <v>493</v>
+        <v>491</v>
       </c>
       <c r="E143" t="s">
-        <v>494</v>
+        <v>492</v>
       </c>
     </row>
     <row r="144" spans="1:9" ht="12.75" customHeight="1">
@@ -4912,10 +4973,10 @@
         <v>13</v>
       </c>
       <c r="D144" t="s">
-        <v>495</v>
+        <v>493</v>
       </c>
       <c r="E144" t="s">
-        <v>494</v>
+        <v>492</v>
       </c>
     </row>
     <row r="145" spans="1:10" ht="12.75" customHeight="1">
@@ -4924,10 +4985,10 @@
         <v>13</v>
       </c>
       <c r="D145" t="s">
-        <v>496</v>
+        <v>494</v>
       </c>
       <c r="E145" t="s">
-        <v>494</v>
+        <v>492</v>
       </c>
     </row>
     <row r="146" spans="1:10" ht="12.75" customHeight="1">
@@ -4942,7 +5003,7 @@
         <v>15</v>
       </c>
       <c r="E147" t="s">
-        <v>497</v>
+        <v>495</v>
       </c>
     </row>
     <row r="148" spans="1:10" ht="12.75" customHeight="1">
@@ -4951,7 +5012,7 @@
         <v>13</v>
       </c>
       <c r="D148" t="s">
-        <v>101</v>
+        <v>99</v>
       </c>
     </row>
     <row r="149" spans="1:10" ht="12.75" customHeight="1">
@@ -4960,10 +5021,10 @@
         <v>16</v>
       </c>
       <c r="C149" t="s">
-        <v>498</v>
+        <v>496</v>
       </c>
       <c r="D149" t="s">
-        <v>499</v>
+        <v>497</v>
       </c>
     </row>
     <row r="150" spans="1:10" ht="12.75" customHeight="1">
@@ -4972,10 +5033,10 @@
         <v>16</v>
       </c>
       <c r="C150" t="s">
-        <v>500</v>
+        <v>498</v>
       </c>
       <c r="D150" t="s">
-        <v>501</v>
+        <v>499</v>
       </c>
     </row>
     <row r="151" spans="1:10" ht="12.75" customHeight="1">
@@ -4984,10 +5045,10 @@
         <v>13</v>
       </c>
       <c r="D151" t="s">
-        <v>502</v>
+        <v>500</v>
       </c>
       <c r="E151" t="s">
-        <v>503</v>
+        <v>501</v>
       </c>
     </row>
     <row r="152" spans="1:10" ht="12.75" customHeight="1">
@@ -4999,7 +5060,7 @@
     <row r="153" spans="1:10" ht="12.75" customHeight="1">
       <c r="A153" s="22"/>
       <c r="B153" s="15" t="s">
-        <v>77</v>
+        <v>76</v>
       </c>
       <c r="C153" s="15"/>
       <c r="D153" s="15"/>
@@ -5012,22 +5073,22 @@
     <row r="155" spans="1:10" s="14" customFormat="1" ht="12.75" customHeight="1">
       <c r="A155" s="25"/>
       <c r="B155" s="13" t="s">
-        <v>99</v>
+        <v>97</v>
       </c>
       <c r="E155" s="14" t="s">
-        <v>100</v>
+        <v>98</v>
       </c>
       <c r="I155" s="12"/>
       <c r="J155" s="12"/>
     </row>
     <row r="156" spans="1:10" ht="12.75" customHeight="1">
       <c r="B156" s="13" t="s">
-        <v>83</v>
+        <v>81</v>
       </c>
       <c r="C156" s="14"/>
       <c r="D156" s="14"/>
       <c r="E156" s="14" t="s">
-        <v>78</v>
+        <v>77</v>
       </c>
       <c r="F156" s="14"/>
       <c r="G156" s="14"/>
@@ -5035,10 +5096,10 @@
     </row>
     <row r="157" spans="1:10" ht="12.75" customHeight="1">
       <c r="A157" s="22" t="s">
-        <v>452</v>
+        <v>450</v>
       </c>
       <c r="B157" s="15" t="s">
-        <v>111</v>
+        <v>109</v>
       </c>
       <c r="C157" s="18"/>
       <c r="D157" s="18"/>
@@ -5057,16 +5118,16 @@
     <row r="159" spans="1:10" ht="12.75" customHeight="1">
       <c r="A159" s="22"/>
       <c r="B159" t="s">
-        <v>527</v>
+        <v>525</v>
       </c>
       <c r="C159" t="s">
+        <v>78</v>
+      </c>
+      <c r="D159" t="s">
+        <v>520</v>
+      </c>
+      <c r="F159" t="s">
         <v>79</v>
-      </c>
-      <c r="D159" t="s">
-        <v>522</v>
-      </c>
-      <c r="F159" t="s">
-        <v>81</v>
       </c>
     </row>
     <row r="160" spans="1:10" ht="12.75" customHeight="1">
@@ -5075,13 +5136,13 @@
         <v>13</v>
       </c>
       <c r="C160" t="s">
-        <v>523</v>
+        <v>521</v>
       </c>
       <c r="E160" t="s">
-        <v>528</v>
+        <v>526</v>
       </c>
       <c r="I160" t="s">
-        <v>524</v>
+        <v>522</v>
       </c>
     </row>
     <row r="161" spans="1:9" ht="12.75" customHeight="1">
@@ -5090,10 +5151,10 @@
         <v>13</v>
       </c>
       <c r="D161" t="s">
-        <v>525</v>
+        <v>523</v>
       </c>
       <c r="E161" t="s">
-        <v>529</v>
+        <v>527</v>
       </c>
     </row>
     <row r="162" spans="1:9" ht="12.75" customHeight="1">
@@ -5102,10 +5163,10 @@
         <v>13</v>
       </c>
       <c r="D162" t="s">
-        <v>526</v>
+        <v>524</v>
       </c>
       <c r="E162" t="s">
-        <v>530</v>
+        <v>528</v>
       </c>
     </row>
     <row r="163" spans="1:9" ht="12.75" customHeight="1">
@@ -5117,7 +5178,7 @@
     <row r="164" spans="1:9" ht="12.75" customHeight="1">
       <c r="A164" s="22"/>
       <c r="B164" s="15" t="s">
-        <v>82</v>
+        <v>80</v>
       </c>
       <c r="C164" s="18"/>
       <c r="D164" s="18"/>
@@ -5128,12 +5189,12 @@
     </row>
     <row r="166" spans="1:9" ht="12.75" customHeight="1">
       <c r="B166" s="13" t="s">
-        <v>102</v>
+        <v>100</v>
       </c>
       <c r="C166" s="14"/>
       <c r="D166" s="14"/>
       <c r="E166" s="14" t="s">
-        <v>104</v>
+        <v>102</v>
       </c>
       <c r="F166" s="14"/>
       <c r="G166" s="14"/>
@@ -5141,12 +5202,12 @@
     </row>
     <row r="167" spans="1:9" ht="12.75" customHeight="1">
       <c r="B167" s="13" t="s">
-        <v>103</v>
+        <v>101</v>
       </c>
       <c r="C167" s="14"/>
       <c r="D167" s="14"/>
       <c r="E167" s="14" t="s">
-        <v>105</v>
+        <v>103</v>
       </c>
       <c r="F167" s="14"/>
       <c r="G167" s="14"/>
@@ -5154,10 +5215,10 @@
     </row>
     <row r="168" spans="1:9" ht="12.75" customHeight="1">
       <c r="A168" s="22" t="s">
-        <v>58</v>
+        <v>57</v>
       </c>
       <c r="B168" s="15" t="s">
-        <v>112</v>
+        <v>110</v>
       </c>
       <c r="C168" s="18"/>
       <c r="D168" s="18"/>
@@ -5169,13 +5230,13 @@
     <row r="169" spans="1:9" ht="12.75" customHeight="1">
       <c r="A169" s="28"/>
       <c r="B169" t="s">
-        <v>211</v>
+        <v>209</v>
       </c>
       <c r="C169" t="s">
         <v>11</v>
       </c>
       <c r="D169" t="s">
-        <v>61</v>
+        <v>60</v>
       </c>
       <c r="F169" t="s">
         <v>6</v>
@@ -5189,7 +5250,7 @@
         <v>15</v>
       </c>
       <c r="E170" t="s">
-        <v>480</v>
+        <v>478</v>
       </c>
     </row>
     <row r="171" spans="1:9" ht="12.75" customHeight="1">
@@ -5198,22 +5259,22 @@
         <v>13</v>
       </c>
       <c r="D171" t="s">
-        <v>41</v>
+        <v>40</v>
       </c>
     </row>
     <row r="172" spans="1:9" ht="12.75" customHeight="1">
       <c r="A172" s="28"/>
       <c r="B172" t="s">
+        <v>479</v>
+      </c>
+      <c r="C172" t="s">
+        <v>480</v>
+      </c>
+      <c r="D172" t="s">
         <v>481</v>
       </c>
-      <c r="C172" t="s">
-        <v>482</v>
-      </c>
-      <c r="D172" t="s">
-        <v>483</v>
-      </c>
       <c r="F172" t="s">
-        <v>81</v>
+        <v>79</v>
       </c>
     </row>
     <row r="173" spans="1:9" ht="12.75" customHeight="1">
@@ -5222,10 +5283,10 @@
         <v>15</v>
       </c>
       <c r="C173" t="s">
-        <v>515</v>
+        <v>513</v>
       </c>
       <c r="E173" t="s">
-        <v>516</v>
+        <v>514</v>
       </c>
     </row>
     <row r="174" spans="1:9" ht="12.75" customHeight="1">
@@ -5234,10 +5295,10 @@
         <v>16</v>
       </c>
       <c r="C174" t="s">
-        <v>517</v>
+        <v>515</v>
       </c>
       <c r="D174" t="s">
-        <v>485</v>
+        <v>483</v>
       </c>
     </row>
     <row r="175" spans="1:9" ht="12.75" customHeight="1">
@@ -5246,10 +5307,10 @@
         <v>13</v>
       </c>
       <c r="D175" t="s">
-        <v>521</v>
+        <v>519</v>
       </c>
       <c r="E175" t="s">
-        <v>518</v>
+        <v>516</v>
       </c>
       <c r="I175" s="21"/>
     </row>
@@ -5265,7 +5326,7 @@
         <v>15</v>
       </c>
       <c r="E177" t="s">
-        <v>484</v>
+        <v>482</v>
       </c>
     </row>
     <row r="178" spans="1:9" ht="12.75" customHeight="1">
@@ -5277,7 +5338,7 @@
         <v>20</v>
       </c>
       <c r="D178" t="s">
-        <v>485</v>
+        <v>483</v>
       </c>
     </row>
     <row r="179" spans="1:9" ht="12.75" customHeight="1">
@@ -5305,7 +5366,7 @@
         <v>15</v>
       </c>
       <c r="E181" t="s">
-        <v>486</v>
+        <v>484</v>
       </c>
     </row>
     <row r="182" spans="1:9" ht="12.75" customHeight="1">
@@ -5317,7 +5378,7 @@
         <v>17</v>
       </c>
       <c r="D182" t="s">
-        <v>487</v>
+        <v>485</v>
       </c>
     </row>
     <row r="183" spans="1:9" ht="12.75" customHeight="1">
@@ -5350,7 +5411,7 @@
         <v>15</v>
       </c>
       <c r="E186" t="s">
-        <v>488</v>
+        <v>486</v>
       </c>
     </row>
     <row r="187" spans="1:9" ht="12.75" customHeight="1">
@@ -5359,7 +5420,7 @@
         <v>13</v>
       </c>
       <c r="D187" t="s">
-        <v>43</v>
+        <v>42</v>
       </c>
     </row>
     <row r="188" spans="1:9" ht="12.75" customHeight="1">
@@ -5368,10 +5429,10 @@
         <v>16</v>
       </c>
       <c r="C188" t="s">
-        <v>489</v>
+        <v>487</v>
       </c>
       <c r="D188" t="s">
-        <v>490</v>
+        <v>488</v>
       </c>
     </row>
     <row r="189" spans="1:9" ht="12.75" customHeight="1">
@@ -5380,10 +5441,10 @@
         <v>16</v>
       </c>
       <c r="C189" t="s">
-        <v>491</v>
+        <v>489</v>
       </c>
       <c r="D189" t="s">
-        <v>492</v>
+        <v>490</v>
       </c>
     </row>
     <row r="190" spans="1:9" ht="12.75" customHeight="1">
@@ -5392,10 +5453,10 @@
         <v>13</v>
       </c>
       <c r="D190" t="s">
-        <v>493</v>
+        <v>491</v>
       </c>
       <c r="E190" t="s">
-        <v>494</v>
+        <v>492</v>
       </c>
     </row>
     <row r="191" spans="1:9" ht="12.75" customHeight="1">
@@ -5404,10 +5465,10 @@
         <v>13</v>
       </c>
       <c r="D191" t="s">
-        <v>495</v>
+        <v>493</v>
       </c>
       <c r="E191" t="s">
-        <v>494</v>
+        <v>492</v>
       </c>
     </row>
     <row r="192" spans="1:9" ht="12.75" customHeight="1">
@@ -5416,10 +5477,10 @@
         <v>13</v>
       </c>
       <c r="D192" t="s">
-        <v>496</v>
+        <v>494</v>
       </c>
       <c r="E192" t="s">
-        <v>494</v>
+        <v>492</v>
       </c>
     </row>
     <row r="193" spans="1:8" ht="12.75" customHeight="1">
@@ -5434,7 +5495,7 @@
         <v>15</v>
       </c>
       <c r="E194" t="s">
-        <v>497</v>
+        <v>495</v>
       </c>
     </row>
     <row r="195" spans="1:8" ht="12.75" customHeight="1">
@@ -5443,7 +5504,7 @@
         <v>13</v>
       </c>
       <c r="D195" t="s">
-        <v>101</v>
+        <v>99</v>
       </c>
     </row>
     <row r="196" spans="1:8" ht="12.75" customHeight="1">
@@ -5452,10 +5513,10 @@
         <v>16</v>
       </c>
       <c r="C196" t="s">
-        <v>498</v>
+        <v>496</v>
       </c>
       <c r="D196" t="s">
-        <v>499</v>
+        <v>497</v>
       </c>
     </row>
     <row r="197" spans="1:8" ht="12.75" customHeight="1">
@@ -5464,10 +5525,10 @@
         <v>16</v>
       </c>
       <c r="C197" t="s">
-        <v>500</v>
+        <v>498</v>
       </c>
       <c r="D197" t="s">
-        <v>501</v>
+        <v>499</v>
       </c>
     </row>
     <row r="198" spans="1:8" ht="12.75" customHeight="1">
@@ -5476,10 +5537,10 @@
         <v>13</v>
       </c>
       <c r="D198" t="s">
-        <v>502</v>
+        <v>500</v>
       </c>
       <c r="E198" t="s">
-        <v>503</v>
+        <v>501</v>
       </c>
     </row>
     <row r="199" spans="1:8" ht="12.75" customHeight="1">
@@ -5491,7 +5552,7 @@
     <row r="200" spans="1:8" ht="12.75" customHeight="1">
       <c r="A200" s="22"/>
       <c r="B200" s="15" t="s">
-        <v>106</v>
+        <v>104</v>
       </c>
       <c r="C200" s="18"/>
       <c r="D200" s="18"/>
@@ -5502,7 +5563,7 @@
     </row>
     <row r="203" spans="1:8" ht="12.75" customHeight="1">
       <c r="B203" s="17" t="s">
-        <v>95</v>
+        <v>93</v>
       </c>
     </row>
   </sheetData>
@@ -5555,154 +5616,154 @@
     </row>
     <row r="4" spans="1:2" ht="12.75" customHeight="1">
       <c r="A4" t="s">
-        <v>519</v>
+        <v>517</v>
       </c>
       <c r="B4" t="s">
-        <v>520</v>
+        <v>518</v>
       </c>
     </row>
     <row r="5" spans="1:2" ht="12.75" customHeight="1">
       <c r="A5" t="s">
+        <v>506</v>
+      </c>
+      <c r="B5" t="s">
         <v>508</v>
-      </c>
-      <c r="B5" t="s">
-        <v>510</v>
       </c>
     </row>
     <row r="6" spans="1:2" ht="12.75" customHeight="1">
       <c r="A6" t="s">
+        <v>507</v>
+      </c>
+      <c r="B6" t="s">
         <v>509</v>
-      </c>
-      <c r="B6" t="s">
-        <v>511</v>
       </c>
     </row>
     <row r="7" spans="1:2" ht="12.75" customHeight="1">
       <c r="A7" t="s">
+        <v>510</v>
+      </c>
+      <c r="B7" t="s">
         <v>512</v>
-      </c>
-      <c r="B7" t="s">
-        <v>514</v>
       </c>
     </row>
     <row r="9" spans="1:2" ht="12" customHeight="1">
       <c r="A9" t="s">
+        <v>210</v>
+      </c>
+      <c r="B9" t="s">
         <v>212</v>
-      </c>
-      <c r="B9" t="s">
-        <v>214</v>
       </c>
     </row>
     <row r="10" spans="1:2" ht="12" customHeight="1">
       <c r="A10" t="s">
-        <v>215</v>
+        <v>213</v>
       </c>
       <c r="B10" t="s">
-        <v>230</v>
+        <v>228</v>
       </c>
     </row>
     <row r="11" spans="1:2" ht="12" customHeight="1">
       <c r="A11" t="s">
-        <v>216</v>
+        <v>214</v>
       </c>
       <c r="B11" t="s">
-        <v>223</v>
+        <v>221</v>
       </c>
     </row>
     <row r="12" spans="1:2" ht="12" customHeight="1">
       <c r="A12" t="s">
-        <v>248</v>
+        <v>246</v>
       </c>
       <c r="B12" t="s">
-        <v>245</v>
+        <v>243</v>
       </c>
     </row>
     <row r="13" spans="1:2" ht="12" customHeight="1">
       <c r="A13" t="s">
-        <v>217</v>
+        <v>215</v>
       </c>
       <c r="B13" t="s">
-        <v>224</v>
+        <v>222</v>
       </c>
     </row>
     <row r="14" spans="1:2" ht="12" customHeight="1">
       <c r="A14" t="s">
-        <v>218</v>
+        <v>216</v>
       </c>
       <c r="B14" t="s">
-        <v>225</v>
+        <v>223</v>
       </c>
     </row>
     <row r="15" spans="1:2" ht="42" customHeight="1">
       <c r="A15" t="s">
-        <v>246</v>
+        <v>244</v>
       </c>
       <c r="B15" t="s">
-        <v>247</v>
+        <v>245</v>
       </c>
     </row>
     <row r="16" spans="1:2" ht="12.75" customHeight="1">
       <c r="A16" t="s">
-        <v>386</v>
+        <v>384</v>
       </c>
       <c r="B16" t="s">
-        <v>394</v>
+        <v>392</v>
       </c>
     </row>
     <row r="17" spans="1:2" ht="12.75" customHeight="1">
       <c r="A17" t="s">
-        <v>387</v>
+        <v>385</v>
       </c>
       <c r="B17" t="s">
-        <v>395</v>
+        <v>393</v>
       </c>
     </row>
     <row r="18" spans="1:2" ht="12.75" customHeight="1">
       <c r="A18" t="s">
-        <v>388</v>
+        <v>386</v>
       </c>
       <c r="B18" t="s">
-        <v>396</v>
+        <v>394</v>
       </c>
     </row>
     <row r="19" spans="1:2" ht="12.75" customHeight="1">
       <c r="A19" t="s">
-        <v>389</v>
+        <v>387</v>
       </c>
       <c r="B19" t="s">
-        <v>397</v>
+        <v>395</v>
       </c>
     </row>
     <row r="20" spans="1:2" ht="12.75" customHeight="1">
       <c r="A20" t="s">
-        <v>390</v>
+        <v>388</v>
       </c>
       <c r="B20" t="s">
-        <v>398</v>
+        <v>396</v>
       </c>
     </row>
     <row r="21" spans="1:2" ht="12.75" customHeight="1">
       <c r="A21" t="s">
-        <v>391</v>
+        <v>389</v>
       </c>
       <c r="B21" t="s">
-        <v>399</v>
+        <v>397</v>
       </c>
     </row>
     <row r="22" spans="1:2" ht="12.75" customHeight="1">
       <c r="A22" t="s">
-        <v>392</v>
+        <v>390</v>
       </c>
       <c r="B22" t="s">
-        <v>393</v>
+        <v>391</v>
       </c>
     </row>
     <row r="23" spans="1:2" ht="12.75" customHeight="1">
       <c r="A23" t="s">
-        <v>403</v>
+        <v>401</v>
       </c>
       <c r="B23" t="s">
-        <v>404</v>
+        <v>402</v>
       </c>
     </row>
   </sheetData>
@@ -5718,10 +5779,10 @@
 
 <file path=xl/worksheets/sheet3.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <dimension ref="A1:D140"/>
+  <dimension ref="A1:D147"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="C25" sqref="C25"/>
+    <sheetView topLeftCell="A127" workbookViewId="0">
+      <selection activeCell="A143" sqref="A143:D147"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultColWidth="17.1640625" defaultRowHeight="12.75" customHeight="1" x14ac:dyDescent="0"/>
@@ -5741,7 +5802,7 @@
         <v>2</v>
       </c>
       <c r="D1" t="s">
-        <v>56</v>
+        <v>55</v>
       </c>
     </row>
     <row r="2" spans="1:4" ht="12.75" customHeight="1">
@@ -5751,8 +5812,8 @@
       <c r="B2" t="s">
         <v>30</v>
       </c>
-      <c r="C2" t="s">
-        <v>8</v>
+      <c r="D2" t="s">
+        <v>532</v>
       </c>
     </row>
     <row r="3" spans="1:4" ht="12.75" customHeight="1">
@@ -5762,8 +5823,8 @@
       <c r="B3" t="s">
         <v>31</v>
       </c>
-      <c r="C3" t="s">
-        <v>10</v>
+      <c r="D3" t="s">
+        <v>533</v>
       </c>
     </row>
     <row r="4" spans="1:4" ht="12.75" customHeight="1">
@@ -5773,8 +5834,8 @@
       <c r="B4" t="s">
         <v>32</v>
       </c>
-      <c r="C4" t="s">
-        <v>33</v>
+      <c r="D4" t="s">
+        <v>534</v>
       </c>
     </row>
     <row r="5" spans="1:4" ht="12.75" customHeight="1">
@@ -5782,10 +5843,10 @@
         <v>4</v>
       </c>
       <c r="B5" t="s">
-        <v>60</v>
-      </c>
-      <c r="C5" t="s">
-        <v>61</v>
+        <v>59</v>
+      </c>
+      <c r="D5" t="s">
+        <v>535</v>
       </c>
     </row>
     <row r="6" spans="1:4" ht="12.75" customHeight="1">
@@ -5793,10 +5854,10 @@
         <v>4</v>
       </c>
       <c r="B6" t="s">
-        <v>84</v>
-      </c>
-      <c r="C6" t="s">
-        <v>80</v>
+        <v>82</v>
+      </c>
+      <c r="D6" t="s">
+        <v>536</v>
       </c>
     </row>
     <row r="9" spans="1:4" ht="12.75" customHeight="1">
@@ -5804,10 +5865,10 @@
         <v>9</v>
       </c>
       <c r="B9" t="s">
+        <v>33</v>
+      </c>
+      <c r="C9" t="s">
         <v>34</v>
-      </c>
-      <c r="C9" t="s">
-        <v>35</v>
       </c>
     </row>
     <row r="10" spans="1:4" ht="12.75" customHeight="1">
@@ -5815,10 +5876,10 @@
         <v>9</v>
       </c>
       <c r="B10" t="s">
+        <v>35</v>
+      </c>
+      <c r="C10" t="s">
         <v>36</v>
-      </c>
-      <c r="C10" t="s">
-        <v>37</v>
       </c>
     </row>
     <row r="11" spans="1:4" ht="12.75" customHeight="1">
@@ -5826,10 +5887,10 @@
         <v>9</v>
       </c>
       <c r="B11" t="s">
-        <v>63</v>
+        <v>62</v>
       </c>
       <c r="C11" t="s">
-        <v>62</v>
+        <v>61</v>
       </c>
     </row>
     <row r="13" spans="1:4" ht="12.75" customHeight="1">
@@ -5837,10 +5898,13 @@
         <v>7</v>
       </c>
       <c r="B13" t="s">
+        <v>37</v>
+      </c>
+      <c r="C13" t="s">
         <v>38</v>
       </c>
-      <c r="C13" t="s">
-        <v>39</v>
+      <c r="D13" t="s">
+        <v>537</v>
       </c>
     </row>
     <row r="14" spans="1:4" ht="12.75" customHeight="1">
@@ -5848,10 +5912,13 @@
         <v>7</v>
       </c>
       <c r="B14" t="s">
-        <v>87</v>
+        <v>85</v>
       </c>
       <c r="C14" t="s">
-        <v>88</v>
+        <v>86</v>
+      </c>
+      <c r="D14" t="s">
+        <v>538</v>
       </c>
     </row>
     <row r="15" spans="1:4" ht="12.75" customHeight="1">
@@ -5859,10 +5926,13 @@
         <v>7</v>
       </c>
       <c r="B15" t="s">
-        <v>85</v>
+        <v>83</v>
       </c>
       <c r="C15" t="s">
-        <v>86</v>
+        <v>84</v>
+      </c>
+      <c r="D15" t="s">
+        <v>539</v>
       </c>
     </row>
     <row r="16" spans="1:4" ht="12.75" customHeight="1">
@@ -5870,1158 +5940,1215 @@
         <v>7</v>
       </c>
       <c r="B16" t="s">
-        <v>113</v>
+        <v>111</v>
       </c>
       <c r="C16" t="s">
-        <v>73</v>
-      </c>
-    </row>
-    <row r="18" spans="1:3" ht="12.75" customHeight="1">
-      <c r="A18" t="s">
-        <v>11</v>
-      </c>
-      <c r="B18" t="s">
-        <v>40</v>
-      </c>
-      <c r="C18" t="s">
-        <v>41</v>
-      </c>
-    </row>
-    <row r="19" spans="1:3" ht="12.75" customHeight="1">
+        <v>72</v>
+      </c>
+      <c r="D16" t="s">
+        <v>540</v>
+      </c>
+    </row>
+    <row r="17" spans="1:4" ht="12.75" customHeight="1">
+      <c r="A17" t="s">
+        <v>7</v>
+      </c>
+      <c r="B17" t="s">
+        <v>542</v>
+      </c>
+      <c r="C17" t="s">
+        <v>543</v>
+      </c>
+      <c r="D17" t="s">
+        <v>541</v>
+      </c>
+    </row>
+    <row r="19" spans="1:4" ht="12.75" customHeight="1">
       <c r="A19" t="s">
         <v>11</v>
       </c>
       <c r="B19" t="s">
-        <v>42</v>
+        <v>39</v>
       </c>
       <c r="C19" t="s">
-        <v>43</v>
-      </c>
-    </row>
-    <row r="20" spans="1:3" ht="12.75" customHeight="1">
+        <v>40</v>
+      </c>
+    </row>
+    <row r="20" spans="1:4" ht="12.75" customHeight="1">
       <c r="A20" t="s">
         <v>11</v>
       </c>
       <c r="B20" t="s">
-        <v>513</v>
+        <v>41</v>
       </c>
       <c r="C20" t="s">
-        <v>101</v>
-      </c>
-    </row>
-    <row r="21" spans="1:3" ht="12.75" customHeight="1">
+        <v>42</v>
+      </c>
+    </row>
+    <row r="21" spans="1:4" ht="12.75" customHeight="1">
       <c r="A21" t="s">
-        <v>482</v>
+        <v>11</v>
       </c>
       <c r="B21" t="s">
+        <v>511</v>
+      </c>
+      <c r="C21" t="s">
+        <v>99</v>
+      </c>
+    </row>
+    <row r="22" spans="1:4" ht="12.75" customHeight="1">
+      <c r="A22" t="s">
+        <v>480</v>
+      </c>
+      <c r="B22" t="s">
+        <v>502</v>
+      </c>
+      <c r="C22" t="s">
+        <v>503</v>
+      </c>
+    </row>
+    <row r="23" spans="1:4" ht="12.75" customHeight="1">
+      <c r="A23" t="s">
+        <v>480</v>
+      </c>
+      <c r="B23" t="s">
         <v>504</v>
       </c>
-      <c r="C21" t="s">
+      <c r="C23" t="s">
         <v>505</v>
       </c>
     </row>
-    <row r="22" spans="1:3" ht="12.75" customHeight="1">
-      <c r="A22" t="s">
-        <v>482</v>
-      </c>
-      <c r="B22" t="s">
-        <v>506</v>
-      </c>
-      <c r="C22" t="s">
-        <v>507</v>
-      </c>
-    </row>
-    <row r="24" spans="1:3" ht="12.75" customHeight="1">
-      <c r="A24" t="s">
-        <v>79</v>
-      </c>
-      <c r="B24" t="s">
-        <v>523</v>
-      </c>
-      <c r="C24" t="s">
-        <v>533</v>
-      </c>
-    </row>
-    <row r="25" spans="1:3" ht="12.75" customHeight="1">
+    <row r="25" spans="1:4" ht="12.75" customHeight="1">
       <c r="A25" t="s">
-        <v>79</v>
+        <v>78</v>
       </c>
       <c r="B25" t="s">
-        <v>531</v>
+        <v>521</v>
       </c>
       <c r="C25" t="s">
         <v>531</v>
       </c>
     </row>
-    <row r="26" spans="1:3" ht="12.75" customHeight="1">
+    <row r="26" spans="1:4" ht="12.75" customHeight="1">
       <c r="A26" t="s">
-        <v>79</v>
+        <v>78</v>
       </c>
       <c r="B26" t="s">
-        <v>532</v>
+        <v>529</v>
       </c>
       <c r="C26" t="s">
-        <v>532</v>
-      </c>
-    </row>
-    <row r="28" spans="1:3" ht="12.75" customHeight="1">
-      <c r="A28" t="s">
-        <v>59</v>
-      </c>
-      <c r="B28" t="s">
+        <v>529</v>
+      </c>
+    </row>
+    <row r="27" spans="1:4" ht="12.75" customHeight="1">
+      <c r="A27" t="s">
+        <v>78</v>
+      </c>
+      <c r="B27" t="s">
+        <v>530</v>
+      </c>
+      <c r="C27" t="s">
+        <v>530</v>
+      </c>
+    </row>
+    <row r="29" spans="1:4" ht="12.75" customHeight="1">
+      <c r="A29" t="s">
+        <v>58</v>
+      </c>
+      <c r="B29" t="s">
+        <v>39</v>
+      </c>
+      <c r="C29" t="s">
         <v>40</v>
       </c>
-      <c r="C28" t="s">
+    </row>
+    <row r="30" spans="1:4" ht="12.75" customHeight="1">
+      <c r="A30" t="s">
+        <v>58</v>
+      </c>
+      <c r="B30" t="s">
         <v>41</v>
       </c>
-    </row>
-    <row r="29" spans="1:3" ht="12.75" customHeight="1">
-      <c r="A29" t="s">
-        <v>59</v>
-      </c>
-      <c r="B29" t="s">
+      <c r="C30" t="s">
         <v>42</v>
       </c>
-      <c r="C29" t="s">
-        <v>43</v>
-      </c>
-    </row>
-    <row r="30" spans="1:3" ht="12.75" customHeight="1">
-      <c r="A30" t="s">
-        <v>59</v>
-      </c>
-      <c r="B30" t="s">
-        <v>513</v>
-      </c>
-      <c r="C30" t="s">
-        <v>101</v>
-      </c>
-    </row>
-    <row r="32" spans="1:3" ht="12.75" customHeight="1">
-      <c r="A32" t="s">
-        <v>44</v>
-      </c>
-      <c r="B32" t="s">
-        <v>45</v>
-      </c>
-      <c r="C32" t="s">
-        <v>46</v>
+    </row>
+    <row r="31" spans="1:4" ht="12.75" customHeight="1">
+      <c r="A31" t="s">
+        <v>58</v>
+      </c>
+      <c r="B31" t="s">
+        <v>511</v>
+      </c>
+      <c r="C31" t="s">
+        <v>99</v>
       </c>
     </row>
     <row r="33" spans="1:4" ht="12.75" customHeight="1">
       <c r="A33" t="s">
+        <v>43</v>
+      </c>
+      <c r="B33" t="s">
         <v>44</v>
       </c>
-      <c r="B33" t="s">
+      <c r="C33" t="s">
+        <v>45</v>
+      </c>
+    </row>
+    <row r="34" spans="1:4" ht="12.75" customHeight="1">
+      <c r="A34" t="s">
+        <v>43</v>
+      </c>
+      <c r="B34" t="s">
+        <v>46</v>
+      </c>
+      <c r="C34" t="s">
         <v>47</v>
-      </c>
-      <c r="C33" t="s">
-        <v>48</v>
-      </c>
-    </row>
-    <row r="35" spans="1:4" ht="12.75" customHeight="1">
-      <c r="A35" t="s">
-        <v>252</v>
-      </c>
-      <c r="B35" t="s">
-        <v>259</v>
-      </c>
-      <c r="C35" t="s">
-        <v>260</v>
       </c>
     </row>
     <row r="36" spans="1:4" ht="12.75" customHeight="1">
       <c r="A36" t="s">
-        <v>252</v>
+        <v>250</v>
       </c>
       <c r="B36" t="s">
-        <v>261</v>
+        <v>257</v>
       </c>
       <c r="C36" t="s">
-        <v>262</v>
+        <v>258</v>
       </c>
     </row>
     <row r="37" spans="1:4" ht="12.75" customHeight="1">
       <c r="A37" t="s">
-        <v>252</v>
+        <v>250</v>
       </c>
       <c r="B37" t="s">
-        <v>400</v>
+        <v>259</v>
       </c>
       <c r="C37" t="s">
-        <v>377</v>
-      </c>
-    </row>
-    <row r="39" spans="1:4" ht="12.75" customHeight="1">
-      <c r="A39" t="s">
-        <v>115</v>
-      </c>
-      <c r="B39" t="s">
-        <v>116</v>
-      </c>
-      <c r="C39" t="s">
-        <v>122</v>
+        <v>260</v>
+      </c>
+    </row>
+    <row r="38" spans="1:4" ht="12.75" customHeight="1">
+      <c r="A38" t="s">
+        <v>250</v>
+      </c>
+      <c r="B38" t="s">
+        <v>398</v>
+      </c>
+      <c r="C38" t="s">
+        <v>375</v>
       </c>
     </row>
     <row r="40" spans="1:4" ht="12.75" customHeight="1">
       <c r="A40" t="s">
-        <v>115</v>
+        <v>113</v>
       </c>
       <c r="B40" t="s">
-        <v>117</v>
+        <v>114</v>
       </c>
       <c r="C40" t="s">
-        <v>123</v>
+        <v>120</v>
       </c>
     </row>
     <row r="41" spans="1:4" ht="12.75" customHeight="1">
       <c r="A41" t="s">
+        <v>113</v>
+      </c>
+      <c r="B41" t="s">
         <v>115</v>
       </c>
-      <c r="B41" t="s">
-        <v>118</v>
-      </c>
       <c r="C41" t="s">
-        <v>124</v>
+        <v>121</v>
       </c>
     </row>
     <row r="42" spans="1:4" ht="12.75" customHeight="1">
       <c r="A42" t="s">
-        <v>115</v>
+        <v>113</v>
       </c>
       <c r="B42" t="s">
-        <v>119</v>
+        <v>116</v>
       </c>
       <c r="C42" t="s">
-        <v>125</v>
+        <v>122</v>
       </c>
     </row>
     <row r="43" spans="1:4" ht="12.75" customHeight="1">
       <c r="A43" t="s">
-        <v>115</v>
+        <v>113</v>
       </c>
       <c r="B43" t="s">
-        <v>120</v>
+        <v>117</v>
       </c>
       <c r="C43" t="s">
-        <v>126</v>
+        <v>123</v>
       </c>
     </row>
     <row r="44" spans="1:4" ht="12.75" customHeight="1">
       <c r="A44" t="s">
-        <v>115</v>
+        <v>113</v>
       </c>
       <c r="B44" t="s">
-        <v>121</v>
+        <v>118</v>
       </c>
       <c r="C44" t="s">
-        <v>127</v>
-      </c>
-    </row>
-    <row r="46" spans="1:4" ht="12.75" customHeight="1">
-      <c r="A46" t="s">
-        <v>129</v>
-      </c>
-      <c r="B46" t="s">
-        <v>136</v>
-      </c>
-      <c r="D46" t="s">
-        <v>137</v>
+        <v>124</v>
+      </c>
+    </row>
+    <row r="45" spans="1:4" ht="12.75" customHeight="1">
+      <c r="A45" t="s">
+        <v>113</v>
+      </c>
+      <c r="B45" t="s">
+        <v>119</v>
+      </c>
+      <c r="C45" t="s">
+        <v>125</v>
       </c>
     </row>
     <row r="47" spans="1:4" ht="12.75" customHeight="1">
       <c r="A47" t="s">
-        <v>129</v>
+        <v>127</v>
       </c>
       <c r="B47" t="s">
-        <v>138</v>
+        <v>134</v>
       </c>
       <c r="D47" t="s">
-        <v>142</v>
+        <v>135</v>
       </c>
     </row>
     <row r="48" spans="1:4" ht="12.75" customHeight="1">
       <c r="A48" t="s">
-        <v>129</v>
+        <v>127</v>
       </c>
       <c r="B48" t="s">
-        <v>139</v>
+        <v>136</v>
       </c>
       <c r="D48" t="s">
-        <v>143</v>
+        <v>140</v>
       </c>
     </row>
     <row r="49" spans="1:4" ht="12.75" customHeight="1">
       <c r="A49" t="s">
-        <v>129</v>
+        <v>127</v>
       </c>
       <c r="B49" t="s">
-        <v>140</v>
+        <v>137</v>
       </c>
       <c r="D49" t="s">
-        <v>144</v>
+        <v>141</v>
       </c>
     </row>
     <row r="50" spans="1:4" ht="12.75" customHeight="1">
       <c r="A50" t="s">
-        <v>129</v>
+        <v>127</v>
       </c>
       <c r="B50" t="s">
-        <v>141</v>
+        <v>138</v>
       </c>
       <c r="D50" t="s">
-        <v>145</v>
-      </c>
-    </row>
-    <row r="52" spans="1:4" ht="12.75" customHeight="1">
-      <c r="A52" t="s">
-        <v>133</v>
-      </c>
-      <c r="B52" t="s">
-        <v>169</v>
-      </c>
-      <c r="D52" t="s">
-        <v>170</v>
-      </c>
-    </row>
-    <row r="53" spans="1:4" s="2" customFormat="1" ht="12.75" customHeight="1">
+        <v>142</v>
+      </c>
+    </row>
+    <row r="51" spans="1:4" ht="12.75" customHeight="1">
+      <c r="A51" t="s">
+        <v>127</v>
+      </c>
+      <c r="B51" t="s">
+        <v>139</v>
+      </c>
+      <c r="D51" t="s">
+        <v>143</v>
+      </c>
+    </row>
+    <row r="53" spans="1:4" ht="12.75" customHeight="1">
       <c r="A53" t="s">
-        <v>133</v>
+        <v>131</v>
       </c>
       <c r="B53" t="s">
-        <v>159</v>
+        <v>167</v>
       </c>
       <c r="D53" t="s">
-        <v>160</v>
-      </c>
-    </row>
-    <row r="54" spans="1:4" ht="12.75" customHeight="1">
+        <v>168</v>
+      </c>
+    </row>
+    <row r="54" spans="1:4" s="2" customFormat="1" ht="12.75" customHeight="1">
       <c r="A54" t="s">
-        <v>133</v>
+        <v>131</v>
       </c>
       <c r="B54" t="s">
-        <v>161</v>
+        <v>157</v>
       </c>
       <c r="D54" t="s">
-        <v>162</v>
+        <v>158</v>
       </c>
     </row>
     <row r="55" spans="1:4" ht="12.75" customHeight="1">
       <c r="A55" t="s">
-        <v>133</v>
+        <v>131</v>
       </c>
       <c r="B55" t="s">
-        <v>163</v>
+        <v>159</v>
       </c>
       <c r="D55" t="s">
-        <v>164</v>
+        <v>160</v>
       </c>
     </row>
     <row r="56" spans="1:4" ht="12.75" customHeight="1">
       <c r="A56" t="s">
-        <v>133</v>
+        <v>131</v>
       </c>
       <c r="B56" t="s">
-        <v>165</v>
+        <v>161</v>
       </c>
       <c r="D56" t="s">
-        <v>166</v>
+        <v>162</v>
       </c>
     </row>
     <row r="57" spans="1:4" ht="12.75" customHeight="1">
       <c r="A57" t="s">
-        <v>133</v>
+        <v>131</v>
       </c>
       <c r="B57" t="s">
-        <v>167</v>
+        <v>163</v>
       </c>
       <c r="D57" t="s">
-        <v>168</v>
-      </c>
-    </row>
-    <row r="59" spans="1:4" ht="12.75" customHeight="1">
-      <c r="A59" t="s">
-        <v>150</v>
-      </c>
-      <c r="B59" t="s">
-        <v>171</v>
-      </c>
-      <c r="C59" s="2"/>
-      <c r="D59" t="s">
-        <v>172</v>
+        <v>164</v>
+      </c>
+    </row>
+    <row r="58" spans="1:4" ht="12.75" customHeight="1">
+      <c r="A58" t="s">
+        <v>131</v>
+      </c>
+      <c r="B58" t="s">
+        <v>165</v>
+      </c>
+      <c r="D58" t="s">
+        <v>166</v>
       </c>
     </row>
     <row r="60" spans="1:4" ht="12.75" customHeight="1">
       <c r="A60" t="s">
-        <v>150</v>
+        <v>148</v>
       </c>
       <c r="B60" t="s">
-        <v>173</v>
-      </c>
+        <v>169</v>
+      </c>
+      <c r="C60" s="2"/>
       <c r="D60" t="s">
-        <v>174</v>
+        <v>170</v>
       </c>
     </row>
     <row r="61" spans="1:4" ht="12.75" customHeight="1">
       <c r="A61" t="s">
-        <v>150</v>
+        <v>148</v>
       </c>
       <c r="B61" t="s">
-        <v>175</v>
+        <v>171</v>
       </c>
       <c r="D61" t="s">
-        <v>176</v>
+        <v>172</v>
       </c>
     </row>
     <row r="62" spans="1:4" ht="12.75" customHeight="1">
       <c r="A62" t="s">
-        <v>150</v>
+        <v>148</v>
       </c>
       <c r="B62" t="s">
-        <v>177</v>
+        <v>173</v>
       </c>
       <c r="D62" t="s">
-        <v>178</v>
+        <v>174</v>
       </c>
     </row>
     <row r="63" spans="1:4" ht="12.75" customHeight="1">
       <c r="A63" t="s">
-        <v>150</v>
+        <v>148</v>
       </c>
       <c r="B63" t="s">
-        <v>179</v>
+        <v>175</v>
       </c>
       <c r="D63" t="s">
-        <v>180</v>
-      </c>
-    </row>
-    <row r="65" spans="1:4" ht="12.75" customHeight="1">
-      <c r="A65" t="s">
-        <v>220</v>
-      </c>
-      <c r="B65" t="s">
-        <v>238</v>
-      </c>
-      <c r="D65" t="s">
-        <v>231</v>
+        <v>176</v>
+      </c>
+    </row>
+    <row r="64" spans="1:4" ht="12.75" customHeight="1">
+      <c r="A64" t="s">
+        <v>148</v>
+      </c>
+      <c r="B64" t="s">
+        <v>177</v>
+      </c>
+      <c r="D64" t="s">
+        <v>178</v>
       </c>
     </row>
     <row r="66" spans="1:4" ht="12.75" customHeight="1">
       <c r="A66" t="s">
-        <v>220</v>
+        <v>218</v>
       </c>
       <c r="B66" t="s">
-        <v>239</v>
-      </c>
-      <c r="C66" s="2"/>
+        <v>236</v>
+      </c>
       <c r="D66" t="s">
-        <v>232</v>
+        <v>229</v>
       </c>
     </row>
     <row r="67" spans="1:4" ht="12.75" customHeight="1">
       <c r="A67" t="s">
-        <v>220</v>
+        <v>218</v>
       </c>
       <c r="B67" t="s">
-        <v>240</v>
-      </c>
+        <v>237</v>
+      </c>
+      <c r="C67" s="2"/>
       <c r="D67" t="s">
-        <v>233</v>
+        <v>230</v>
       </c>
     </row>
     <row r="68" spans="1:4" ht="12.75" customHeight="1">
       <c r="A68" t="s">
-        <v>220</v>
+        <v>218</v>
       </c>
       <c r="B68" t="s">
-        <v>241</v>
+        <v>238</v>
       </c>
       <c r="D68" t="s">
-        <v>234</v>
+        <v>231</v>
       </c>
     </row>
     <row r="69" spans="1:4" ht="12.75" customHeight="1">
       <c r="A69" t="s">
-        <v>220</v>
+        <v>218</v>
       </c>
       <c r="B69" t="s">
-        <v>242</v>
+        <v>239</v>
       </c>
       <c r="D69" t="s">
-        <v>235</v>
+        <v>232</v>
       </c>
     </row>
     <row r="70" spans="1:4" ht="12.75" customHeight="1">
       <c r="A70" t="s">
-        <v>220</v>
+        <v>218</v>
       </c>
       <c r="B70" t="s">
-        <v>243</v>
+        <v>240</v>
       </c>
       <c r="D70" t="s">
-        <v>236</v>
+        <v>233</v>
       </c>
     </row>
     <row r="71" spans="1:4" ht="12.75" customHeight="1">
       <c r="A71" t="s">
-        <v>220</v>
+        <v>218</v>
       </c>
       <c r="B71" t="s">
-        <v>244</v>
+        <v>241</v>
       </c>
       <c r="D71" t="s">
-        <v>237</v>
-      </c>
-    </row>
-    <row r="73" spans="1:4" ht="12.75" customHeight="1">
-      <c r="A73" t="s">
-        <v>154</v>
-      </c>
-      <c r="B73" t="s">
-        <v>181</v>
-      </c>
-      <c r="D73" t="s">
-        <v>182</v>
+        <v>234</v>
+      </c>
+    </row>
+    <row r="72" spans="1:4" ht="12.75" customHeight="1">
+      <c r="A72" t="s">
+        <v>218</v>
+      </c>
+      <c r="B72" t="s">
+        <v>242</v>
+      </c>
+      <c r="D72" t="s">
+        <v>235</v>
       </c>
     </row>
     <row r="74" spans="1:4" ht="12.75" customHeight="1">
       <c r="A74" t="s">
-        <v>154</v>
+        <v>152</v>
       </c>
       <c r="B74" t="s">
-        <v>183</v>
-      </c>
-      <c r="C74" s="2"/>
+        <v>179</v>
+      </c>
       <c r="D74" t="s">
-        <v>184</v>
+        <v>180</v>
       </c>
     </row>
     <row r="75" spans="1:4" ht="12.75" customHeight="1">
       <c r="A75" t="s">
-        <v>154</v>
+        <v>152</v>
       </c>
       <c r="B75" t="s">
-        <v>185</v>
-      </c>
+        <v>181</v>
+      </c>
+      <c r="C75" s="2"/>
       <c r="D75" t="s">
-        <v>186</v>
+        <v>182</v>
       </c>
     </row>
     <row r="76" spans="1:4" ht="12.75" customHeight="1">
       <c r="A76" t="s">
-        <v>154</v>
+        <v>152</v>
       </c>
       <c r="B76" t="s">
-        <v>187</v>
+        <v>183</v>
       </c>
       <c r="D76" t="s">
-        <v>188</v>
+        <v>184</v>
       </c>
     </row>
     <row r="77" spans="1:4" ht="12.75" customHeight="1">
       <c r="A77" t="s">
-        <v>154</v>
+        <v>152</v>
       </c>
       <c r="B77" t="s">
-        <v>189</v>
+        <v>185</v>
       </c>
       <c r="D77" t="s">
-        <v>190</v>
+        <v>186</v>
       </c>
     </row>
     <row r="78" spans="1:4" ht="12.75" customHeight="1">
       <c r="A78" t="s">
-        <v>154</v>
+        <v>152</v>
       </c>
       <c r="B78" t="s">
-        <v>191</v>
+        <v>187</v>
       </c>
       <c r="D78" t="s">
-        <v>192</v>
-      </c>
-    </row>
-    <row r="80" spans="1:4" ht="12.75" customHeight="1">
-      <c r="A80" t="s">
-        <v>157</v>
-      </c>
-      <c r="B80" t="s">
-        <v>193</v>
-      </c>
-      <c r="D80" t="s">
-        <v>194</v>
+        <v>188</v>
+      </c>
+    </row>
+    <row r="79" spans="1:4" ht="12.75" customHeight="1">
+      <c r="A79" t="s">
+        <v>152</v>
+      </c>
+      <c r="B79" t="s">
+        <v>189</v>
+      </c>
+      <c r="D79" t="s">
+        <v>190</v>
       </c>
     </row>
     <row r="81" spans="1:4" ht="12.75" customHeight="1">
       <c r="A81" t="s">
-        <v>157</v>
+        <v>155</v>
       </c>
       <c r="B81" t="s">
-        <v>195</v>
-      </c>
-      <c r="C81" s="2"/>
+        <v>191</v>
+      </c>
       <c r="D81" t="s">
-        <v>196</v>
+        <v>192</v>
       </c>
     </row>
     <row r="82" spans="1:4" ht="12.75" customHeight="1">
       <c r="A82" t="s">
-        <v>157</v>
+        <v>155</v>
       </c>
       <c r="B82" t="s">
-        <v>197</v>
-      </c>
+        <v>193</v>
+      </c>
+      <c r="C82" s="2"/>
       <c r="D82" t="s">
-        <v>198</v>
+        <v>194</v>
       </c>
     </row>
     <row r="83" spans="1:4" ht="12.75" customHeight="1">
       <c r="A83" t="s">
-        <v>157</v>
+        <v>155</v>
       </c>
       <c r="B83" t="s">
-        <v>199</v>
+        <v>195</v>
       </c>
       <c r="D83" t="s">
-        <v>200</v>
+        <v>196</v>
       </c>
     </row>
     <row r="84" spans="1:4" ht="12.75" customHeight="1">
       <c r="A84" t="s">
-        <v>157</v>
+        <v>155</v>
       </c>
       <c r="B84" t="s">
-        <v>201</v>
+        <v>197</v>
       </c>
       <c r="D84" t="s">
-        <v>202</v>
+        <v>198</v>
       </c>
     </row>
     <row r="85" spans="1:4" ht="12.75" customHeight="1">
       <c r="A85" t="s">
-        <v>157</v>
+        <v>155</v>
       </c>
       <c r="B85" t="s">
-        <v>203</v>
+        <v>199</v>
       </c>
       <c r="D85" t="s">
-        <v>204</v>
-      </c>
-    </row>
-    <row r="87" spans="1:4" ht="12.75" customHeight="1">
-      <c r="A87" t="s">
-        <v>256</v>
-      </c>
-      <c r="B87" t="s">
-        <v>263</v>
-      </c>
-      <c r="C87" t="s">
-        <v>281</v>
+        <v>200</v>
+      </c>
+    </row>
+    <row r="86" spans="1:4" ht="12.75" customHeight="1">
+      <c r="A86" t="s">
+        <v>155</v>
+      </c>
+      <c r="B86" t="s">
+        <v>201</v>
+      </c>
+      <c r="D86" t="s">
+        <v>202</v>
       </c>
     </row>
     <row r="88" spans="1:4" ht="12.75" customHeight="1">
       <c r="A88" t="s">
-        <v>256</v>
+        <v>254</v>
       </c>
       <c r="B88" t="s">
-        <v>266</v>
+        <v>261</v>
       </c>
       <c r="C88" t="s">
-        <v>282</v>
+        <v>279</v>
       </c>
     </row>
     <row r="89" spans="1:4" ht="12.75" customHeight="1">
       <c r="A89" t="s">
-        <v>256</v>
+        <v>254</v>
       </c>
       <c r="B89" t="s">
-        <v>269</v>
+        <v>264</v>
       </c>
       <c r="C89" t="s">
-        <v>283</v>
+        <v>280</v>
       </c>
     </row>
     <row r="90" spans="1:4" ht="12.75" customHeight="1">
       <c r="A90" t="s">
-        <v>256</v>
+        <v>254</v>
       </c>
       <c r="B90" t="s">
-        <v>270</v>
+        <v>267</v>
       </c>
       <c r="C90" t="s">
-        <v>376</v>
+        <v>281</v>
       </c>
     </row>
     <row r="91" spans="1:4" ht="12.75" customHeight="1">
       <c r="A91" t="s">
-        <v>256</v>
+        <v>254</v>
       </c>
       <c r="B91" t="s">
-        <v>272</v>
+        <v>268</v>
       </c>
       <c r="C91" t="s">
-        <v>284</v>
+        <v>374</v>
       </c>
     </row>
     <row r="92" spans="1:4" ht="12.75" customHeight="1">
       <c r="A92" t="s">
-        <v>256</v>
+        <v>254</v>
       </c>
       <c r="B92" t="s">
-        <v>274</v>
+        <v>270</v>
       </c>
       <c r="C92" t="s">
-        <v>285</v>
-      </c>
-    </row>
-    <row r="94" spans="1:4" ht="12.75" customHeight="1">
-      <c r="A94" t="s">
-        <v>286</v>
-      </c>
-      <c r="B94" t="s">
-        <v>292</v>
-      </c>
-      <c r="C94" t="s">
-        <v>299</v>
+        <v>282</v>
+      </c>
+    </row>
+    <row r="93" spans="1:4" ht="12.75" customHeight="1">
+      <c r="A93" t="s">
+        <v>254</v>
+      </c>
+      <c r="B93" t="s">
+        <v>272</v>
+      </c>
+      <c r="C93" t="s">
+        <v>283</v>
       </c>
     </row>
     <row r="95" spans="1:4" ht="12.75" customHeight="1">
       <c r="A95" t="s">
-        <v>286</v>
+        <v>284</v>
       </c>
       <c r="B95" t="s">
-        <v>293</v>
+        <v>290</v>
       </c>
       <c r="C95" t="s">
-        <v>300</v>
+        <v>297</v>
       </c>
     </row>
     <row r="96" spans="1:4" ht="12.75" customHeight="1">
       <c r="A96" t="s">
-        <v>286</v>
+        <v>284</v>
       </c>
       <c r="B96" t="s">
-        <v>294</v>
+        <v>291</v>
       </c>
       <c r="C96" t="s">
-        <v>301</v>
+        <v>298</v>
       </c>
     </row>
     <row r="97" spans="1:3" ht="12.75" customHeight="1">
       <c r="A97" t="s">
-        <v>286</v>
+        <v>284</v>
       </c>
       <c r="B97" t="s">
-        <v>295</v>
+        <v>292</v>
       </c>
       <c r="C97" t="s">
-        <v>302</v>
+        <v>299</v>
       </c>
     </row>
     <row r="98" spans="1:3" ht="12.75" customHeight="1">
       <c r="A98" t="s">
-        <v>286</v>
+        <v>284</v>
       </c>
       <c r="B98" t="s">
-        <v>296</v>
+        <v>293</v>
       </c>
       <c r="C98" t="s">
-        <v>303</v>
+        <v>300</v>
       </c>
     </row>
     <row r="99" spans="1:3" ht="12.75" customHeight="1">
       <c r="A99" t="s">
-        <v>286</v>
+        <v>284</v>
       </c>
       <c r="B99" t="s">
-        <v>297</v>
+        <v>294</v>
       </c>
       <c r="C99" t="s">
-        <v>304</v>
+        <v>301</v>
       </c>
     </row>
     <row r="100" spans="1:3" ht="12.75" customHeight="1">
       <c r="A100" t="s">
-        <v>286</v>
+        <v>284</v>
       </c>
       <c r="B100" t="s">
-        <v>298</v>
+        <v>295</v>
       </c>
       <c r="C100" t="s">
-        <v>305</v>
-      </c>
-    </row>
-    <row r="102" spans="1:3" ht="12.75" customHeight="1">
-      <c r="A102" t="s">
-        <v>287</v>
-      </c>
-      <c r="B102" t="s">
-        <v>312</v>
-      </c>
-      <c r="C102" t="s">
-        <v>318</v>
+        <v>302</v>
+      </c>
+    </row>
+    <row r="101" spans="1:3" ht="12.75" customHeight="1">
+      <c r="A101" t="s">
+        <v>284</v>
+      </c>
+      <c r="B101" t="s">
+        <v>296</v>
+      </c>
+      <c r="C101" t="s">
+        <v>303</v>
       </c>
     </row>
     <row r="103" spans="1:3" ht="12.75" customHeight="1">
       <c r="A103" t="s">
-        <v>287</v>
+        <v>285</v>
       </c>
       <c r="B103" t="s">
-        <v>313</v>
+        <v>310</v>
       </c>
       <c r="C103" t="s">
-        <v>319</v>
+        <v>316</v>
       </c>
     </row>
     <row r="104" spans="1:3" ht="12.75" customHeight="1">
       <c r="A104" t="s">
-        <v>287</v>
+        <v>285</v>
       </c>
       <c r="B104" t="s">
-        <v>314</v>
+        <v>311</v>
       </c>
       <c r="C104" t="s">
-        <v>320</v>
+        <v>317</v>
       </c>
     </row>
     <row r="105" spans="1:3" ht="12.75" customHeight="1">
       <c r="A105" t="s">
-        <v>287</v>
+        <v>285</v>
       </c>
       <c r="B105" t="s">
-        <v>315</v>
+        <v>312</v>
       </c>
       <c r="C105" t="s">
-        <v>321</v>
+        <v>318</v>
       </c>
     </row>
     <row r="106" spans="1:3" ht="12.75" customHeight="1">
       <c r="A106" t="s">
-        <v>287</v>
+        <v>285</v>
       </c>
       <c r="B106" t="s">
-        <v>316</v>
+        <v>313</v>
       </c>
       <c r="C106" t="s">
-        <v>322</v>
+        <v>319</v>
       </c>
     </row>
     <row r="107" spans="1:3" ht="12.75" customHeight="1">
       <c r="A107" t="s">
-        <v>287</v>
+        <v>285</v>
       </c>
       <c r="B107" t="s">
-        <v>317</v>
+        <v>314</v>
       </c>
       <c r="C107" t="s">
-        <v>323</v>
-      </c>
-    </row>
-    <row r="109" spans="1:3" ht="12.75" customHeight="1">
-      <c r="A109" t="s">
-        <v>288</v>
-      </c>
-      <c r="B109" t="s">
-        <v>330</v>
-      </c>
-      <c r="C109" t="s">
-        <v>331</v>
+        <v>320</v>
+      </c>
+    </row>
+    <row r="108" spans="1:3" ht="12.75" customHeight="1">
+      <c r="A108" t="s">
+        <v>285</v>
+      </c>
+      <c r="B108" t="s">
+        <v>315</v>
+      </c>
+      <c r="C108" t="s">
+        <v>321</v>
       </c>
     </row>
     <row r="110" spans="1:3" ht="12.75" customHeight="1">
       <c r="A110" t="s">
-        <v>288</v>
+        <v>286</v>
       </c>
       <c r="B110" t="s">
-        <v>324</v>
+        <v>328</v>
       </c>
       <c r="C110" t="s">
-        <v>332</v>
+        <v>329</v>
       </c>
     </row>
     <row r="111" spans="1:3" ht="12.75" customHeight="1">
       <c r="A111" t="s">
-        <v>288</v>
+        <v>286</v>
       </c>
       <c r="B111" t="s">
-        <v>325</v>
+        <v>322</v>
       </c>
       <c r="C111" t="s">
-        <v>333</v>
+        <v>330</v>
       </c>
     </row>
     <row r="112" spans="1:3" ht="12.75" customHeight="1">
       <c r="A112" t="s">
-        <v>288</v>
+        <v>286</v>
       </c>
       <c r="B112" t="s">
-        <v>326</v>
+        <v>323</v>
       </c>
       <c r="C112" t="s">
-        <v>334</v>
+        <v>331</v>
       </c>
     </row>
     <row r="113" spans="1:3" ht="12.75" customHeight="1">
       <c r="A113" t="s">
-        <v>288</v>
+        <v>286</v>
       </c>
       <c r="B113" t="s">
-        <v>327</v>
+        <v>324</v>
       </c>
       <c r="C113" t="s">
-        <v>335</v>
+        <v>332</v>
       </c>
     </row>
     <row r="114" spans="1:3" ht="12.75" customHeight="1">
       <c r="A114" t="s">
-        <v>288</v>
+        <v>286</v>
       </c>
       <c r="B114" t="s">
-        <v>328</v>
+        <v>325</v>
       </c>
       <c r="C114" t="s">
-        <v>336</v>
+        <v>333</v>
       </c>
     </row>
     <row r="115" spans="1:3" ht="12.75" customHeight="1">
       <c r="A115" t="s">
-        <v>288</v>
+        <v>286</v>
       </c>
       <c r="B115" t="s">
-        <v>329</v>
+        <v>326</v>
       </c>
       <c r="C115" t="s">
-        <v>337</v>
-      </c>
-    </row>
-    <row r="117" spans="1:3" ht="12.75" customHeight="1">
-      <c r="A117" t="s">
-        <v>289</v>
-      </c>
-      <c r="B117" t="s">
-        <v>338</v>
-      </c>
-      <c r="C117" t="s">
-        <v>344</v>
+        <v>334</v>
+      </c>
+    </row>
+    <row r="116" spans="1:3" ht="12.75" customHeight="1">
+      <c r="A116" t="s">
+        <v>286</v>
+      </c>
+      <c r="B116" t="s">
+        <v>327</v>
+      </c>
+      <c r="C116" t="s">
+        <v>335</v>
       </c>
     </row>
     <row r="118" spans="1:3" ht="12.75" customHeight="1">
       <c r="A118" t="s">
-        <v>289</v>
+        <v>287</v>
       </c>
       <c r="B118" t="s">
-        <v>339</v>
+        <v>336</v>
       </c>
       <c r="C118" t="s">
-        <v>345</v>
+        <v>342</v>
       </c>
     </row>
     <row r="119" spans="1:3" ht="12.75" customHeight="1">
       <c r="A119" t="s">
-        <v>289</v>
+        <v>287</v>
       </c>
       <c r="B119" t="s">
-        <v>340</v>
+        <v>337</v>
       </c>
       <c r="C119" t="s">
-        <v>346</v>
+        <v>343</v>
       </c>
     </row>
     <row r="120" spans="1:3" ht="12.75" customHeight="1">
       <c r="A120" t="s">
-        <v>289</v>
+        <v>287</v>
       </c>
       <c r="B120" t="s">
-        <v>341</v>
+        <v>338</v>
       </c>
       <c r="C120" t="s">
-        <v>347</v>
+        <v>344</v>
       </c>
     </row>
     <row r="121" spans="1:3" ht="12.75" customHeight="1">
       <c r="A121" t="s">
-        <v>289</v>
+        <v>287</v>
       </c>
       <c r="B121" t="s">
-        <v>342</v>
+        <v>339</v>
       </c>
       <c r="C121" t="s">
-        <v>348</v>
+        <v>345</v>
       </c>
     </row>
     <row r="122" spans="1:3" ht="12.75" customHeight="1">
       <c r="A122" t="s">
-        <v>289</v>
+        <v>287</v>
       </c>
       <c r="B122" t="s">
-        <v>343</v>
+        <v>340</v>
       </c>
       <c r="C122" t="s">
-        <v>349</v>
-      </c>
-    </row>
-    <row r="124" spans="1:3" ht="12.75" customHeight="1">
-      <c r="A124" t="s">
-        <v>290</v>
-      </c>
-      <c r="B124" t="s">
-        <v>356</v>
-      </c>
-      <c r="C124" t="s">
-        <v>357</v>
+        <v>346</v>
+      </c>
+    </row>
+    <row r="123" spans="1:3" ht="12.75" customHeight="1">
+      <c r="A123" t="s">
+        <v>287</v>
+      </c>
+      <c r="B123" t="s">
+        <v>341</v>
+      </c>
+      <c r="C123" t="s">
+        <v>347</v>
       </c>
     </row>
     <row r="125" spans="1:3" ht="12.75" customHeight="1">
       <c r="A125" t="s">
-        <v>290</v>
+        <v>288</v>
       </c>
       <c r="B125" t="s">
-        <v>350</v>
+        <v>354</v>
       </c>
       <c r="C125" t="s">
-        <v>358</v>
+        <v>355</v>
       </c>
     </row>
     <row r="126" spans="1:3" ht="12.75" customHeight="1">
       <c r="A126" t="s">
-        <v>290</v>
+        <v>288</v>
       </c>
       <c r="B126" t="s">
-        <v>351</v>
+        <v>348</v>
       </c>
       <c r="C126" t="s">
-        <v>359</v>
+        <v>356</v>
       </c>
     </row>
     <row r="127" spans="1:3" ht="12.75" customHeight="1">
       <c r="A127" t="s">
-        <v>290</v>
+        <v>288</v>
       </c>
       <c r="B127" t="s">
-        <v>353</v>
+        <v>349</v>
       </c>
       <c r="C127" t="s">
-        <v>360</v>
+        <v>357</v>
       </c>
     </row>
     <row r="128" spans="1:3" ht="12.75" customHeight="1">
       <c r="A128" t="s">
-        <v>290</v>
+        <v>288</v>
       </c>
       <c r="B128" t="s">
+        <v>351</v>
+      </c>
+      <c r="C128" t="s">
+        <v>358</v>
+      </c>
+    </row>
+    <row r="129" spans="1:4" ht="12.75" customHeight="1">
+      <c r="A129" t="s">
+        <v>288</v>
+      </c>
+      <c r="B129" t="s">
+        <v>350</v>
+      </c>
+      <c r="C129" t="s">
+        <v>359</v>
+      </c>
+    </row>
+    <row r="130" spans="1:4" ht="12.75" customHeight="1">
+      <c r="A130" t="s">
+        <v>288</v>
+      </c>
+      <c r="B130" t="s">
         <v>352</v>
       </c>
-      <c r="C128" t="s">
+      <c r="C130" t="s">
+        <v>360</v>
+      </c>
+    </row>
+    <row r="131" spans="1:4" ht="12.75" customHeight="1">
+      <c r="A131" t="s">
+        <v>288</v>
+      </c>
+      <c r="B131" t="s">
+        <v>353</v>
+      </c>
+      <c r="C131" t="s">
         <v>361</v>
       </c>
     </row>
-    <row r="129" spans="1:3" ht="12.75" customHeight="1">
-      <c r="A129" t="s">
-        <v>290</v>
-      </c>
-      <c r="B129" t="s">
-        <v>354</v>
-      </c>
-      <c r="C129" t="s">
+    <row r="133" spans="1:4" ht="12.75" customHeight="1">
+      <c r="A133" t="s">
+        <v>289</v>
+      </c>
+      <c r="B133" t="s">
         <v>362</v>
       </c>
-    </row>
-    <row r="130" spans="1:3" ht="12.75" customHeight="1">
-      <c r="A130" t="s">
-        <v>290</v>
-      </c>
-      <c r="B130" t="s">
-        <v>355</v>
-      </c>
-      <c r="C130" t="s">
+      <c r="C133" t="s">
+        <v>368</v>
+      </c>
+    </row>
+    <row r="134" spans="1:4" ht="12.75" customHeight="1">
+      <c r="A134" t="s">
+        <v>289</v>
+      </c>
+      <c r="B134" t="s">
         <v>363</v>
       </c>
-    </row>
-    <row r="132" spans="1:3" ht="12.75" customHeight="1">
-      <c r="A132" t="s">
-        <v>291</v>
-      </c>
-      <c r="B132" t="s">
+      <c r="C134" t="s">
+        <v>369</v>
+      </c>
+    </row>
+    <row r="135" spans="1:4" ht="12.75" customHeight="1">
+      <c r="A135" t="s">
+        <v>289</v>
+      </c>
+      <c r="B135" t="s">
         <v>364</v>
       </c>
-      <c r="C132" t="s">
+      <c r="C135" t="s">
         <v>370</v>
       </c>
     </row>
-    <row r="133" spans="1:3" ht="12.75" customHeight="1">
-      <c r="A133" t="s">
-        <v>291</v>
-      </c>
-      <c r="B133" t="s">
+    <row r="136" spans="1:4" ht="12.75" customHeight="1">
+      <c r="A136" t="s">
+        <v>289</v>
+      </c>
+      <c r="B136" t="s">
         <v>365</v>
       </c>
-      <c r="C133" t="s">
+      <c r="C136" t="s">
         <v>371</v>
       </c>
     </row>
-    <row r="134" spans="1:3" ht="12.75" customHeight="1">
-      <c r="A134" t="s">
-        <v>291</v>
-      </c>
-      <c r="B134" t="s">
+    <row r="137" spans="1:4" ht="12.75" customHeight="1">
+      <c r="A137" t="s">
+        <v>289</v>
+      </c>
+      <c r="B137" t="s">
         <v>366</v>
       </c>
-      <c r="C134" t="s">
+      <c r="C137" t="s">
         <v>372</v>
       </c>
     </row>
-    <row r="135" spans="1:3" ht="12.75" customHeight="1">
-      <c r="A135" t="s">
-        <v>291</v>
-      </c>
-      <c r="B135" t="s">
+    <row r="138" spans="1:4" ht="12.75" customHeight="1">
+      <c r="A138" t="s">
+        <v>289</v>
+      </c>
+      <c r="B138" t="s">
         <v>367</v>
       </c>
-      <c r="C135" t="s">
+      <c r="C138" t="s">
         <v>373</v>
       </c>
     </row>
-    <row r="136" spans="1:3" ht="12.75" customHeight="1">
-      <c r="A136" t="s">
-        <v>291</v>
-      </c>
-      <c r="B136" t="s">
-        <v>368</v>
-      </c>
-      <c r="C136" t="s">
-        <v>374</v>
-      </c>
-    </row>
-    <row r="137" spans="1:3" ht="12.75" customHeight="1">
-      <c r="A137" t="s">
-        <v>291</v>
-      </c>
-      <c r="B137" t="s">
-        <v>369</v>
-      </c>
-      <c r="C137" t="s">
-        <v>375</v>
-      </c>
-    </row>
-    <row r="139" spans="1:3" ht="12.75" customHeight="1">
-      <c r="A139" t="s">
-        <v>453</v>
-      </c>
-      <c r="B139" t="s">
+    <row r="140" spans="1:4" ht="12.75" customHeight="1">
+      <c r="A140" t="s">
+        <v>451</v>
+      </c>
+      <c r="B140" t="s">
+        <v>446</v>
+      </c>
+      <c r="C140" t="s">
+        <v>440</v>
+      </c>
+    </row>
+    <row r="141" spans="1:4" ht="12.75" customHeight="1">
+      <c r="A141" t="s">
+        <v>451</v>
+      </c>
+      <c r="B141" t="s">
+        <v>447</v>
+      </c>
+      <c r="C141" t="s">
         <v>448</v>
       </c>
-      <c r="C139" t="s">
-        <v>442</v>
-      </c>
-    </row>
-    <row r="140" spans="1:3" ht="12.75" customHeight="1">
-      <c r="A140" t="s">
-        <v>453</v>
-      </c>
-      <c r="B140" t="s">
-        <v>449</v>
-      </c>
-      <c r="C140" t="s">
-        <v>450</v>
+    </row>
+    <row r="143" spans="1:4" ht="12.75" customHeight="1">
+      <c r="A143" s="2" t="s">
+        <v>544</v>
+      </c>
+      <c r="D143" t="s">
+        <v>545</v>
+      </c>
+    </row>
+    <row r="144" spans="1:4" ht="12.75" customHeight="1">
+      <c r="A144" t="s">
+        <v>544</v>
+      </c>
+      <c r="D144" t="s">
+        <v>546</v>
+      </c>
+    </row>
+    <row r="145" spans="1:4" ht="12.75" customHeight="1">
+      <c r="A145" s="2" t="s">
+        <v>544</v>
+      </c>
+      <c r="D145" t="s">
+        <v>547</v>
+      </c>
+    </row>
+    <row r="146" spans="1:4" ht="12.75" customHeight="1">
+      <c r="A146" s="2" t="s">
+        <v>544</v>
+      </c>
+      <c r="D146" t="s">
+        <v>548</v>
+      </c>
+    </row>
+    <row r="147" spans="1:4" ht="12.75" customHeight="1">
+      <c r="A147" s="2" t="s">
+        <v>544</v>
+      </c>
+      <c r="D147" t="s">
+        <v>549</v>
       </c>
     </row>
   </sheetData>
@@ -7045,26 +7172,26 @@
   <sheetData>
     <row r="1" spans="1:2" ht="12.75" customHeight="1">
       <c r="A1" t="s">
+        <v>48</v>
+      </c>
+      <c r="B1" t="s">
         <v>49</v>
-      </c>
-      <c r="B1" t="s">
-        <v>50</v>
       </c>
     </row>
     <row r="2" spans="1:2" ht="12.75" customHeight="1">
       <c r="A2" t="s">
+        <v>50</v>
+      </c>
+      <c r="B2" t="s">
         <v>51</v>
-      </c>
-      <c r="B2" t="s">
-        <v>52</v>
       </c>
     </row>
     <row r="3" spans="1:2" ht="12.75" customHeight="1">
       <c r="A3" t="s">
+        <v>52</v>
+      </c>
+      <c r="B3" t="s">
         <v>53</v>
-      </c>
-      <c r="B3" t="s">
-        <v>54</v>
       </c>
     </row>
   </sheetData>
@@ -7092,15 +7219,15 @@
         <v>1</v>
       </c>
       <c r="B1" t="s">
-        <v>146</v>
+        <v>144</v>
       </c>
     </row>
     <row r="2" spans="1:2">
       <c r="A2" t="s">
-        <v>147</v>
+        <v>145</v>
       </c>
       <c r="B2" t="s">
-        <v>148</v>
+        <v>146</v>
       </c>
     </row>
     <row r="3" spans="1:2">
@@ -7108,7 +7235,7 @@
         <v>4</v>
       </c>
       <c r="B3" t="s">
-        <v>148</v>
+        <v>146</v>
       </c>
     </row>
   </sheetData>

</xml_diff>

<commit_message>
add more content to headultrasound
</commit_message>
<xml_diff>
--- a/opendatakit.collect2/form-files/neonatal/neonatal.xlsx
+++ b/opendatakit.collect2/form-files/neonatal/neonatal.xlsx
@@ -1,10 +1,10 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
-  <fileVersion appName="xl" lastEdited="5" lowestEdited="5" rupBuild="20910"/>
+  <fileVersion appName="xl" lastEdited="5" lowestEdited="5" rupBuild="22905"/>
   <workbookPr autoCompressPictures="0"/>
   <bookViews>
-    <workbookView xWindow="320" yWindow="0" windowWidth="25840" windowHeight="16180" tabRatio="500" activeTab="2"/>
+    <workbookView xWindow="0" yWindow="0" windowWidth="21640" windowHeight="15560" tabRatio="500"/>
   </bookViews>
   <sheets>
     <sheet name="survey" sheetId="1" r:id="rId1"/>
@@ -23,7 +23,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="768" uniqueCount="486">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="788" uniqueCount="497">
   <si>
     <t>type</t>
   </si>
@@ -1683,6 +1683,66 @@
   </si>
   <si>
     <t>square-1</t>
+  </si>
+  <si>
+    <t>head_ref</t>
+  </si>
+  <si>
+    <t>headultra_coronal_slider</t>
+  </si>
+  <si>
+    <t>img/coronal/1.png</t>
+  </si>
+  <si>
+    <t>img/coronal/2.png</t>
+  </si>
+  <si>
+    <t>img/coronal/3.png</t>
+  </si>
+  <si>
+    <t>img/coronal/4.png</t>
+  </si>
+  <si>
+    <t>img/coronal/5.png</t>
+  </si>
+  <si>
+    <t xml:space="preserve">&lt;h1&gt;ULTRASOUND OF THE NEONATAL HEAD PROTOCOL&lt;/h1&gt;
+&lt;hr&gt;
+&lt;h2&gt;INDICATIONS&lt;/h2&gt;
+ &lt;ul&gt;
+  &lt;li&gt;
+   &lt;div&gt;
+   &lt;ul&gt;Prematurity:
+    &lt;li&gt;Some people discriminate between the terms preterm and premature.&lt;/li&gt;
+    &lt;li&gt;&lt;b&gt;Preterm&lt;/b&gt; refers to delivering prior to 37weeks whilst a premature infant is one that has not yet reached the level of fetal development that generally allows life outside the womb.&lt;/li&gt;
+    &lt;li&gt;The fine network of vessels (the germinal matrix) on the floor of the anterior horn of the lateral ventricles (the ependyma) are extremely fragile.&lt;li&gt;
+    &lt;li&gt;If there is any hypoxic episode, the reactive increase in blood pressure can result in a haemorrhage of these vessels.&lt;li&gt;
+    &lt;li&gt;Usually assessed at day 1 and again at day 7.&lt;/li&gt;
+   &lt;/ul&gt;
+  &lt;/div&gt;
+ &lt;/li&gt;
+  &lt;li&gt;Increased head circumference&lt;/li&gt;
+ &lt;li&gt;Persisting large fontanelle&lt;/li&gt;
+ &lt;li&gt;Craniosynostosis (premature closure of sutures)&lt;/li&gt;
+    &lt;li&gt;Trauma&lt;/li&gt;
+ &lt;li&gt;Known hypoxia&lt;/li&gt;
+ &lt;li&gt;Follow up of known pathology&lt;/li&gt;
+ &lt;li&gt;Failure to thrive&lt;/li&gt;
+ &lt;li&gt;Suspected intracranial mass or infection&lt;/li&gt;
+&lt;/ul&gt;
+&lt;h2&gt;LIMITATIONS&lt;/h2&gt;
+&lt;div&gt;If the anterior fontanel is very small or closed your visibility will be reduced or completely obscured. Even with a large fontanelle, the peripheral extremes of the brain are obscured from view.&lt;/div&gt;
+&lt;hr&gt;
+</t>
+  </si>
+  <si>
+    <t>selected(data('diagnostic_menu'),'head_ref')</t>
+  </si>
+  <si>
+    <t>selected(data('diagnostic_menu'),'head_coronal')</t>
+  </si>
+  <si>
+    <t>image_slider headultra_coronal_slider</t>
   </si>
 </sst>
 </file>
@@ -3090,11 +3150,11 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <dimension ref="A1:J174"/>
+  <dimension ref="A1:J176"/>
   <sheetViews>
-    <sheetView zoomScale="150" zoomScaleNormal="150" zoomScalePageLayoutView="150" workbookViewId="0">
-      <pane ySplit="1" topLeftCell="A4" activePane="bottomLeft" state="frozen"/>
-      <selection pane="bottomLeft" activeCell="C12" sqref="C12"/>
+    <sheetView tabSelected="1" zoomScale="150" zoomScaleNormal="150" zoomScalePageLayoutView="150" workbookViewId="0">
+      <pane ySplit="1" topLeftCell="A2" activePane="bottomLeft" state="frozen"/>
+      <selection pane="bottomLeft" activeCell="D11" sqref="D11"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultColWidth="11.5" defaultRowHeight="12.75" customHeight="1" x14ac:dyDescent="0"/>
@@ -3243,95 +3303,89 @@
         <v>107</v>
       </c>
     </row>
-    <row r="10" spans="1:9" ht="18" customHeight="1">
+    <row r="10" spans="1:9" ht="29" customHeight="1">
       <c r="A10" s="21"/>
       <c r="B10" s="2" t="s">
-        <v>88</v>
-      </c>
-      <c r="C10" s="4"/>
+        <v>496</v>
+      </c>
+      <c r="C10" s="2" t="s">
+        <v>487</v>
+      </c>
       <c r="D10" s="2" t="s">
-        <v>86</v>
+        <v>87</v>
       </c>
       <c r="E10" s="2" t="s">
-        <v>108</v>
+        <v>495</v>
       </c>
       <c r="F10" s="2"/>
     </row>
     <row r="11" spans="1:9" ht="18" customHeight="1">
       <c r="A11" s="21"/>
       <c r="B11" s="2" t="s">
+        <v>13</v>
+      </c>
+      <c r="C11" s="2"/>
+      <c r="D11" s="2" t="s">
+        <v>493</v>
+      </c>
+      <c r="E11" s="2" t="s">
+        <v>494</v>
+      </c>
+      <c r="F11" s="2"/>
+    </row>
+    <row r="12" spans="1:9" ht="18" customHeight="1">
+      <c r="A12" s="21"/>
+      <c r="B12" s="2" t="s">
         <v>88</v>
       </c>
-      <c r="C11" s="4"/>
-      <c r="D11" s="2" t="s">
+      <c r="C12" s="4"/>
+      <c r="D12" s="2" t="s">
+        <v>86</v>
+      </c>
+      <c r="E12" s="2" t="s">
+        <v>108</v>
+      </c>
+      <c r="F12" s="2"/>
+    </row>
+    <row r="13" spans="1:9" ht="18" customHeight="1">
+      <c r="A13" s="21"/>
+      <c r="B13" s="2" t="s">
+        <v>88</v>
+      </c>
+      <c r="C13" s="4"/>
+      <c r="D13" s="2" t="s">
         <v>89</v>
       </c>
-      <c r="E11" s="2" t="s">
+      <c r="E13" s="2" t="s">
         <v>106</v>
       </c>
-      <c r="F11" s="2"/>
-    </row>
-    <row r="12" spans="1:9" ht="12">
-      <c r="A12" s="21"/>
-      <c r="B12" t="s">
-        <v>435</v>
-      </c>
-      <c r="C12" t="s">
-        <v>436</v>
-      </c>
-      <c r="E12" s="2" t="s">
-        <v>437</v>
-      </c>
-    </row>
-    <row r="13" spans="1:9" ht="11" customHeight="1">
-      <c r="A13" s="21"/>
-      <c r="B13" t="s">
-        <v>438</v>
-      </c>
-      <c r="C13" t="s">
-        <v>439</v>
-      </c>
-      <c r="D13" t="s">
-        <v>112</v>
-      </c>
-      <c r="E13" s="2" t="s">
-        <v>440</v>
-      </c>
-      <c r="F13" t="s">
-        <v>441</v>
-      </c>
-    </row>
-    <row r="14" spans="1:9" ht="11" customHeight="1">
+      <c r="F13" s="2"/>
+    </row>
+    <row r="14" spans="1:9" ht="12">
       <c r="A14" s="21"/>
       <c r="B14" t="s">
-        <v>442</v>
+        <v>435</v>
       </c>
       <c r="C14" t="s">
-        <v>443</v>
-      </c>
-      <c r="D14" t="s">
-        <v>113</v>
+        <v>436</v>
       </c>
       <c r="E14" s="2" t="s">
-        <v>444</v>
-      </c>
-      <c r="F14" t="s">
-        <v>441</v>
+        <v>437</v>
       </c>
     </row>
     <row r="15" spans="1:9" ht="11" customHeight="1">
       <c r="A15" s="21"/>
       <c r="B15" t="s">
-        <v>445</v>
+        <v>438</v>
       </c>
       <c r="C15" t="s">
-        <v>446</v>
+        <v>439</v>
       </c>
       <c r="D15" t="s">
-        <v>127</v>
+        <v>112</v>
       </c>
       <c r="E15" s="2" t="s">
-        <v>447</v>
+        <v>440</v>
       </c>
       <c r="F15" t="s">
         <v>441</v>
@@ -3340,16 +3394,16 @@
     <row r="16" spans="1:9" ht="11" customHeight="1">
       <c r="A16" s="21"/>
       <c r="B16" t="s">
-        <v>448</v>
+        <v>442</v>
       </c>
       <c r="C16" t="s">
-        <v>449</v>
+        <v>443</v>
       </c>
       <c r="D16" t="s">
-        <v>163</v>
+        <v>113</v>
       </c>
       <c r="E16" s="2" t="s">
-        <v>450</v>
+        <v>444</v>
       </c>
       <c r="F16" t="s">
         <v>441</v>
@@ -3358,16 +3412,16 @@
     <row r="17" spans="1:10" ht="11" customHeight="1">
       <c r="A17" s="21"/>
       <c r="B17" t="s">
-        <v>451</v>
+        <v>445</v>
       </c>
       <c r="C17" t="s">
-        <v>452</v>
+        <v>446</v>
       </c>
       <c r="D17" t="s">
-        <v>128</v>
+        <v>127</v>
       </c>
       <c r="E17" s="2" t="s">
-        <v>453</v>
+        <v>447</v>
       </c>
       <c r="F17" t="s">
         <v>441</v>
@@ -3376,16 +3430,16 @@
     <row r="18" spans="1:10" ht="11" customHeight="1">
       <c r="A18" s="21"/>
       <c r="B18" t="s">
-        <v>454</v>
+        <v>448</v>
       </c>
       <c r="C18" t="s">
-        <v>455</v>
+        <v>449</v>
       </c>
       <c r="D18" t="s">
-        <v>129</v>
+        <v>163</v>
       </c>
       <c r="E18" s="2" t="s">
-        <v>456</v>
+        <v>450</v>
       </c>
       <c r="F18" t="s">
         <v>441</v>
@@ -3394,391 +3448,403 @@
     <row r="19" spans="1:10" ht="11" customHeight="1">
       <c r="A19" s="21"/>
       <c r="B19" t="s">
-        <v>212</v>
+        <v>451</v>
       </c>
       <c r="C19" t="s">
-        <v>192</v>
+        <v>452</v>
       </c>
       <c r="D19" t="s">
-        <v>186</v>
+        <v>128</v>
       </c>
       <c r="E19" s="2" t="s">
-        <v>457</v>
+        <v>453</v>
+      </c>
+      <c r="F19" t="s">
+        <v>441</v>
       </c>
     </row>
     <row r="20" spans="1:10" ht="11" customHeight="1">
       <c r="A20" s="21"/>
       <c r="B20" t="s">
-        <v>213</v>
+        <v>454</v>
       </c>
       <c r="C20" t="s">
-        <v>193</v>
+        <v>455</v>
       </c>
       <c r="D20" t="s">
-        <v>187</v>
+        <v>129</v>
       </c>
       <c r="E20" s="2" t="s">
-        <v>458</v>
+        <v>456</v>
+      </c>
+      <c r="F20" t="s">
+        <v>441</v>
       </c>
     </row>
     <row r="21" spans="1:10" ht="11" customHeight="1">
       <c r="A21" s="21"/>
       <c r="B21" t="s">
-        <v>214</v>
+        <v>212</v>
       </c>
       <c r="C21" t="s">
-        <v>194</v>
+        <v>192</v>
       </c>
       <c r="D21" t="s">
-        <v>190</v>
+        <v>186</v>
       </c>
       <c r="E21" s="2" t="s">
-        <v>459</v>
+        <v>457</v>
       </c>
     </row>
     <row r="22" spans="1:10" ht="11" customHeight="1">
       <c r="A22" s="21"/>
       <c r="B22" t="s">
-        <v>215</v>
+        <v>213</v>
       </c>
       <c r="C22" t="s">
-        <v>195</v>
+        <v>193</v>
       </c>
       <c r="D22" t="s">
-        <v>188</v>
+        <v>187</v>
       </c>
       <c r="E22" s="2" t="s">
-        <v>460</v>
+        <v>458</v>
       </c>
     </row>
     <row r="23" spans="1:10" ht="11" customHeight="1">
       <c r="A23" s="21"/>
       <c r="B23" t="s">
-        <v>216</v>
+        <v>214</v>
       </c>
       <c r="C23" t="s">
-        <v>196</v>
+        <v>194</v>
       </c>
       <c r="D23" t="s">
-        <v>189</v>
+        <v>190</v>
       </c>
       <c r="E23" s="2" t="s">
-        <v>461</v>
-      </c>
-    </row>
-    <row r="24" spans="1:10" ht="12" customHeight="1">
+        <v>459</v>
+      </c>
+    </row>
+    <row r="24" spans="1:10" ht="11" customHeight="1">
       <c r="A24" s="21"/>
       <c r="B24" t="s">
+        <v>215</v>
+      </c>
+      <c r="C24" t="s">
+        <v>195</v>
+      </c>
+      <c r="D24" t="s">
+        <v>188</v>
+      </c>
+      <c r="E24" s="2" t="s">
+        <v>460</v>
+      </c>
+    </row>
+    <row r="25" spans="1:10" ht="11" customHeight="1">
+      <c r="A25" s="21"/>
+      <c r="B25" t="s">
+        <v>216</v>
+      </c>
+      <c r="C25" t="s">
+        <v>196</v>
+      </c>
+      <c r="D25" t="s">
+        <v>189</v>
+      </c>
+      <c r="E25" s="2" t="s">
+        <v>461</v>
+      </c>
+    </row>
+    <row r="26" spans="1:10" ht="12" customHeight="1">
+      <c r="A26" s="21"/>
+      <c r="B26" t="s">
         <v>217</v>
       </c>
-      <c r="C24" t="s">
+      <c r="C26" t="s">
         <v>197</v>
       </c>
-      <c r="D24" t="s">
+      <c r="D26" t="s">
         <v>191</v>
       </c>
-      <c r="E24" s="2" t="s">
+      <c r="E26" s="2" t="s">
         <v>462</v>
       </c>
     </row>
-    <row r="25" spans="1:10" ht="15">
-      <c r="A25" s="21"/>
-      <c r="B25" s="15" t="s">
+    <row r="27" spans="1:10" ht="15">
+      <c r="A27" s="21"/>
+      <c r="B27" s="15" t="s">
         <v>65</v>
       </c>
-      <c r="C25" s="15"/>
-      <c r="D25" s="15"/>
-      <c r="E25" s="15"/>
-      <c r="F25" s="15"/>
-      <c r="G25" s="15"/>
-      <c r="H25" s="15"/>
-    </row>
-    <row r="26" spans="1:10" ht="15">
-      <c r="B26" s="23"/>
-      <c r="C26" s="12"/>
-      <c r="D26" s="12"/>
-      <c r="E26" s="12"/>
-      <c r="F26" s="12"/>
-      <c r="G26" s="12"/>
-      <c r="H26" s="12"/>
-    </row>
-    <row r="27" spans="1:10" s="15" customFormat="1" ht="15">
-      <c r="A27" s="21" t="s">
+      <c r="C27" s="15"/>
+      <c r="D27" s="15"/>
+      <c r="E27" s="15"/>
+      <c r="F27" s="15"/>
+      <c r="G27" s="15"/>
+      <c r="H27" s="15"/>
+    </row>
+    <row r="28" spans="1:10" ht="15">
+      <c r="B28" s="23"/>
+      <c r="C28" s="12"/>
+      <c r="D28" s="12"/>
+      <c r="E28" s="12"/>
+      <c r="F28" s="12"/>
+      <c r="G28" s="12"/>
+      <c r="H28" s="12"/>
+    </row>
+    <row r="29" spans="1:10" s="15" customFormat="1" ht="15">
+      <c r="A29" s="21" t="s">
         <v>322</v>
       </c>
-      <c r="B27" s="13" t="s">
+      <c r="B29" s="13" t="s">
         <v>91</v>
       </c>
-      <c r="C27" s="13"/>
-      <c r="D27" s="13"/>
-      <c r="E27" s="13" t="s">
+      <c r="C29" s="13"/>
+      <c r="D29" s="13"/>
+      <c r="E29" s="13" t="s">
         <v>64</v>
       </c>
-      <c r="F27" s="13"/>
-      <c r="G27" s="13"/>
-      <c r="H27" s="13"/>
-      <c r="I27" s="12"/>
-      <c r="J27" s="12"/>
-    </row>
-    <row r="28" spans="1:10" ht="12">
-      <c r="A28" s="21"/>
-      <c r="B28" s="5" t="s">
-        <v>66</v>
-      </c>
-      <c r="C28" s="5"/>
-      <c r="D28" s="5"/>
-      <c r="E28" s="6" t="s">
-        <v>67</v>
-      </c>
-      <c r="F28" s="5"/>
-      <c r="G28" s="5"/>
-      <c r="H28" s="5"/>
-    </row>
-    <row r="29" spans="1:10" ht="15">
-      <c r="A29" s="21"/>
-      <c r="B29" s="15" t="s">
-        <v>90</v>
-      </c>
-      <c r="C29" s="15"/>
-      <c r="D29" s="15"/>
-      <c r="E29" s="15"/>
-      <c r="F29" s="15"/>
-      <c r="G29" s="15"/>
-      <c r="H29" s="15"/>
+      <c r="F29" s="13"/>
+      <c r="G29" s="13"/>
+      <c r="H29" s="13"/>
+      <c r="I29" s="12"/>
+      <c r="J29" s="12"/>
     </row>
     <row r="30" spans="1:10" ht="12">
       <c r="A30" s="21"/>
-      <c r="B30" s="12" t="s">
+      <c r="B30" s="5" t="s">
+        <v>66</v>
+      </c>
+      <c r="C30" s="5"/>
+      <c r="D30" s="5"/>
+      <c r="E30" s="6" t="s">
+        <v>67</v>
+      </c>
+      <c r="F30" s="5"/>
+      <c r="G30" s="5"/>
+      <c r="H30" s="5"/>
+    </row>
+    <row r="31" spans="1:10" ht="15">
+      <c r="A31" s="21"/>
+      <c r="B31" s="15" t="s">
+        <v>90</v>
+      </c>
+      <c r="C31" s="15"/>
+      <c r="D31" s="15"/>
+      <c r="E31" s="15"/>
+      <c r="F31" s="15"/>
+      <c r="G31" s="15"/>
+      <c r="H31" s="15"/>
+    </row>
+    <row r="32" spans="1:10" ht="12">
+      <c r="A32" s="21"/>
+      <c r="B32" s="12" t="s">
         <v>155</v>
       </c>
-      <c r="C30" s="12" t="s">
+      <c r="C32" s="12" t="s">
         <v>9</v>
       </c>
-      <c r="D30" s="12" t="s">
+      <c r="D32" s="12" t="s">
         <v>10</v>
       </c>
-      <c r="E30" s="12"/>
-      <c r="F30" s="12" t="s">
+      <c r="E32" s="12"/>
+      <c r="F32" s="12" t="s">
         <v>6</v>
       </c>
-      <c r="G30" s="12"/>
-      <c r="H30" s="12"/>
-    </row>
-    <row r="31" spans="1:10" ht="12">
-      <c r="A31" s="21"/>
-      <c r="B31" s="7" t="s">
+      <c r="G32" s="12"/>
+      <c r="H32" s="12"/>
+    </row>
+    <row r="33" spans="1:8" ht="12">
+      <c r="A33" s="21"/>
+      <c r="B33" s="7" t="s">
         <v>15</v>
       </c>
-      <c r="C31" s="8"/>
-      <c r="D31" s="8"/>
-      <c r="E31" s="9" t="s">
+      <c r="C33" s="8"/>
+      <c r="D33" s="8"/>
+      <c r="E33" s="9" t="s">
         <v>56</v>
       </c>
-      <c r="F31" s="8"/>
-      <c r="G31" s="10"/>
-      <c r="H31" s="10"/>
-    </row>
-    <row r="32" spans="1:10" ht="12.75" customHeight="1">
-      <c r="A32" s="21"/>
-      <c r="B32" s="4" t="s">
+      <c r="F33" s="8"/>
+      <c r="G33" s="10"/>
+      <c r="H33" s="10"/>
+    </row>
+    <row r="34" spans="1:8" ht="12.75" customHeight="1">
+      <c r="A34" s="21"/>
+      <c r="B34" s="4" t="s">
         <v>13</v>
       </c>
-      <c r="C32" s="2" t="s">
+      <c r="C34" s="2" t="s">
         <v>68</v>
       </c>
-      <c r="D32" s="2" t="s">
+      <c r="D34" s="2" t="s">
         <v>303</v>
-      </c>
-      <c r="E32" s="2"/>
-      <c r="F32" s="4"/>
-    </row>
-    <row r="33" spans="1:6" ht="12.75" customHeight="1">
-      <c r="A33" s="21"/>
-      <c r="B33" s="4" t="s">
-        <v>13</v>
-      </c>
-      <c r="D33" t="s">
-        <v>304</v>
-      </c>
-      <c r="E33" s="2"/>
-      <c r="F33" s="4"/>
-    </row>
-    <row r="34" spans="1:6" ht="12.75" customHeight="1">
-      <c r="A34" s="21"/>
-      <c r="B34" t="s">
-        <v>13</v>
-      </c>
-      <c r="C34" s="2"/>
-      <c r="D34" s="2" t="s">
-        <v>305</v>
       </c>
       <c r="E34" s="2"/>
       <c r="F34" s="4"/>
     </row>
-    <row r="35" spans="1:6" ht="12.75" customHeight="1">
+    <row r="35" spans="1:8" ht="12.75" customHeight="1">
       <c r="A35" s="21"/>
-      <c r="B35" s="2" t="s">
+      <c r="B35" s="4" t="s">
         <v>13</v>
       </c>
-      <c r="C35" s="2"/>
-      <c r="D35" s="2" t="s">
-        <v>306</v>
+      <c r="D35" t="s">
+        <v>304</v>
       </c>
       <c r="E35" s="2"/>
       <c r="F35" s="4"/>
     </row>
-    <row r="36" spans="1:6" ht="12.75" customHeight="1">
+    <row r="36" spans="1:8" ht="12.75" customHeight="1">
       <c r="A36" s="21"/>
-      <c r="B36" s="2" t="s">
+      <c r="B36" t="s">
         <v>13</v>
       </c>
       <c r="C36" s="2"/>
       <c r="D36" s="2" t="s">
-        <v>307</v>
+        <v>305</v>
       </c>
       <c r="E36" s="2"/>
       <c r="F36" s="4"/>
     </row>
-    <row r="37" spans="1:6" ht="12.75" customHeight="1">
+    <row r="37" spans="1:8" ht="12.75" customHeight="1">
       <c r="A37" s="21"/>
       <c r="B37" s="2" t="s">
         <v>13</v>
       </c>
       <c r="C37" s="2"/>
       <c r="D37" s="2" t="s">
-        <v>308</v>
+        <v>306</v>
       </c>
       <c r="E37" s="2"/>
       <c r="F37" s="4"/>
     </row>
-    <row r="38" spans="1:6" ht="12.75" customHeight="1">
+    <row r="38" spans="1:8" ht="12.75" customHeight="1">
       <c r="A38" s="21"/>
       <c r="B38" s="2" t="s">
         <v>13</v>
       </c>
       <c r="C38" s="2"/>
       <c r="D38" s="2" t="s">
-        <v>309</v>
+        <v>307</v>
       </c>
       <c r="E38" s="2"/>
       <c r="F38" s="4"/>
     </row>
-    <row r="39" spans="1:6" ht="12.75" customHeight="1">
+    <row r="39" spans="1:8" ht="12.75" customHeight="1">
       <c r="A39" s="21"/>
       <c r="B39" s="2" t="s">
         <v>13</v>
       </c>
       <c r="C39" s="2"/>
       <c r="D39" s="2" t="s">
-        <v>310</v>
+        <v>308</v>
       </c>
       <c r="E39" s="2"/>
       <c r="F39" s="4"/>
     </row>
-    <row r="40" spans="1:6" ht="12.75" customHeight="1">
+    <row r="40" spans="1:8" ht="12.75" customHeight="1">
       <c r="A40" s="21"/>
       <c r="B40" s="2" t="s">
         <v>13</v>
       </c>
       <c r="C40" s="2"/>
       <c r="D40" s="2" t="s">
-        <v>318</v>
+        <v>309</v>
       </c>
       <c r="E40" s="2"/>
       <c r="F40" s="4"/>
     </row>
-    <row r="41" spans="1:6" ht="12.75" customHeight="1">
+    <row r="41" spans="1:8" ht="12.75" customHeight="1">
       <c r="A41" s="21"/>
       <c r="B41" s="2" t="s">
         <v>13</v>
       </c>
       <c r="C41" s="2"/>
       <c r="D41" s="2" t="s">
-        <v>317</v>
+        <v>310</v>
       </c>
       <c r="E41" s="2"/>
       <c r="F41" s="4"/>
     </row>
-    <row r="42" spans="1:6" ht="12.75" customHeight="1">
+    <row r="42" spans="1:8" ht="12.75" customHeight="1">
       <c r="A42" s="21"/>
       <c r="B42" s="2" t="s">
         <v>13</v>
       </c>
       <c r="C42" s="2"/>
       <c r="D42" s="2" t="s">
-        <v>319</v>
+        <v>318</v>
       </c>
       <c r="E42" s="2"/>
       <c r="F42" s="4"/>
     </row>
-    <row r="43" spans="1:6" ht="12.75" customHeight="1">
+    <row r="43" spans="1:8" ht="12.75" customHeight="1">
       <c r="A43" s="21"/>
       <c r="B43" s="2" t="s">
         <v>13</v>
       </c>
       <c r="C43" s="2"/>
       <c r="D43" s="2" t="s">
-        <v>320</v>
+        <v>317</v>
       </c>
       <c r="E43" s="2"/>
       <c r="F43" s="4"/>
     </row>
-    <row r="44" spans="1:6" ht="12.75" customHeight="1">
+    <row r="44" spans="1:8" ht="12.75" customHeight="1">
       <c r="A44" s="21"/>
       <c r="B44" s="2" t="s">
         <v>13</v>
       </c>
       <c r="C44" s="2"/>
       <c r="D44" s="2" t="s">
-        <v>311</v>
+        <v>319</v>
       </c>
       <c r="E44" s="2"/>
       <c r="F44" s="4"/>
     </row>
-    <row r="45" spans="1:6" ht="12.75" customHeight="1">
+    <row r="45" spans="1:8" ht="12.75" customHeight="1">
       <c r="A45" s="21"/>
       <c r="B45" s="2" t="s">
         <v>13</v>
       </c>
       <c r="C45" s="2"/>
       <c r="D45" s="2" t="s">
-        <v>314</v>
+        <v>320</v>
       </c>
       <c r="E45" s="2"/>
       <c r="F45" s="4"/>
     </row>
-    <row r="46" spans="1:6" ht="12.75" customHeight="1">
+    <row r="46" spans="1:8" ht="12.75" customHeight="1">
       <c r="A46" s="21"/>
       <c r="B46" s="2" t="s">
         <v>13</v>
       </c>
       <c r="C46" s="2"/>
       <c r="D46" s="2" t="s">
-        <v>315</v>
+        <v>311</v>
       </c>
       <c r="E46" s="2"/>
       <c r="F46" s="4"/>
     </row>
-    <row r="47" spans="1:6" ht="12.75" customHeight="1">
+    <row r="47" spans="1:8" ht="12.75" customHeight="1">
       <c r="A47" s="21"/>
       <c r="B47" s="2" t="s">
         <v>13</v>
       </c>
       <c r="C47" s="2"/>
       <c r="D47" s="2" t="s">
-        <v>316</v>
+        <v>314</v>
       </c>
       <c r="E47" s="2"/>
       <c r="F47" s="4"/>
     </row>
-    <row r="48" spans="1:6" ht="12.75" customHeight="1">
+    <row r="48" spans="1:8" ht="12.75" customHeight="1">
       <c r="A48" s="21"/>
       <c r="B48" s="2" t="s">
         <v>13</v>
       </c>
       <c r="C48" s="2"/>
       <c r="D48" s="2" t="s">
-        <v>312</v>
+        <v>315</v>
       </c>
       <c r="E48" s="2"/>
       <c r="F48" s="4"/>
@@ -3790,19 +3856,19 @@
       </c>
       <c r="C49" s="2"/>
       <c r="D49" s="2" t="s">
-        <v>313</v>
+        <v>316</v>
       </c>
       <c r="E49" s="2"/>
       <c r="F49" s="4"/>
     </row>
-    <row r="50" spans="1:8" ht="17" customHeight="1">
+    <row r="50" spans="1:8" ht="12.75" customHeight="1">
       <c r="A50" s="21"/>
       <c r="B50" s="2" t="s">
         <v>13</v>
       </c>
       <c r="C50" s="2"/>
       <c r="D50" s="2" t="s">
-        <v>321</v>
+        <v>312</v>
       </c>
       <c r="E50" s="2"/>
       <c r="F50" s="4"/>
@@ -3813,15 +3879,21 @@
         <v>13</v>
       </c>
       <c r="C51" s="2"/>
-      <c r="D51" s="2"/>
+      <c r="D51" s="2" t="s">
+        <v>313</v>
+      </c>
       <c r="E51" s="2"/>
       <c r="F51" s="4"/>
     </row>
-    <row r="52" spans="1:8" ht="12.75" customHeight="1">
+    <row r="52" spans="1:8" ht="17" customHeight="1">
       <c r="A52" s="21"/>
-      <c r="B52" s="4"/>
+      <c r="B52" s="2" t="s">
+        <v>13</v>
+      </c>
       <c r="C52" s="2"/>
-      <c r="D52" s="2"/>
+      <c r="D52" s="2" t="s">
+        <v>321</v>
+      </c>
       <c r="E52" s="2"/>
       <c r="F52" s="4"/>
     </row>
@@ -3830,337 +3902,334 @@
       <c r="B53" s="2" t="s">
         <v>13</v>
       </c>
-      <c r="C53" s="2" t="s">
-        <v>69</v>
-      </c>
+      <c r="C53" s="2"/>
       <c r="D53" s="2"/>
       <c r="E53" s="2"/>
       <c r="F53" s="4"/>
-      <c r="G53" t="s">
-        <v>14</v>
-      </c>
     </row>
     <row r="54" spans="1:8" ht="12.75" customHeight="1">
       <c r="A54" s="21"/>
-      <c r="B54" t="s">
-        <v>13</v>
-      </c>
-      <c r="D54" t="s">
-        <v>70</v>
-      </c>
-      <c r="E54" s="13"/>
+      <c r="B54" s="4"/>
+      <c r="C54" s="2"/>
+      <c r="D54" s="2"/>
+      <c r="E54" s="2"/>
+      <c r="F54" s="4"/>
     </row>
     <row r="55" spans="1:8" ht="12.75" customHeight="1">
       <c r="A55" s="21"/>
-      <c r="B55" t="s">
+      <c r="B55" s="2" t="s">
         <v>13</v>
       </c>
-      <c r="H55" t="s">
+      <c r="C55" s="2" t="s">
+        <v>69</v>
+      </c>
+      <c r="D55" s="2"/>
+      <c r="E55" s="2"/>
+      <c r="F55" s="4"/>
+      <c r="G55" t="s">
+        <v>14</v>
+      </c>
+    </row>
+    <row r="56" spans="1:8" ht="12.75" customHeight="1">
+      <c r="A56" s="21"/>
+      <c r="B56" t="s">
+        <v>13</v>
+      </c>
+      <c r="D56" t="s">
+        <v>70</v>
+      </c>
+      <c r="E56" s="13"/>
+    </row>
+    <row r="57" spans="1:8" ht="12.75" customHeight="1">
+      <c r="A57" s="21"/>
+      <c r="B57" t="s">
+        <v>13</v>
+      </c>
+      <c r="H57" t="s">
         <v>71</v>
       </c>
     </row>
-    <row r="56" spans="1:8" ht="12">
-      <c r="A56" s="21"/>
-      <c r="B56" s="11" t="s">
+    <row r="58" spans="1:8" ht="12">
+      <c r="A58" s="21"/>
+      <c r="B58" s="11" t="s">
         <v>23</v>
       </c>
-      <c r="C56" s="10"/>
-      <c r="D56" s="10"/>
-      <c r="E56" s="10"/>
-      <c r="F56" s="10"/>
-      <c r="G56" s="10"/>
-      <c r="H56" s="10"/>
-    </row>
-    <row r="57" spans="1:8" s="10" customFormat="1" ht="12"/>
-    <row r="58" spans="1:8" s="10" customFormat="1" ht="15">
-      <c r="B58" s="10" t="s">
+      <c r="C58" s="10"/>
+      <c r="D58" s="10"/>
+      <c r="E58" s="10"/>
+      <c r="F58" s="10"/>
+      <c r="G58" s="10"/>
+      <c r="H58" s="10"/>
+    </row>
+    <row r="59" spans="1:8" s="10" customFormat="1" ht="12"/>
+    <row r="60" spans="1:8" s="10" customFormat="1" ht="15">
+      <c r="B60" s="10" t="s">
         <v>352</v>
       </c>
-      <c r="E58" s="13" t="s">
+      <c r="E60" s="13" t="s">
         <v>357</v>
       </c>
     </row>
-    <row r="59" spans="1:8" s="10" customFormat="1" ht="15">
-      <c r="B59" s="10" t="s">
+    <row r="61" spans="1:8" s="10" customFormat="1" ht="15">
+      <c r="B61" s="10" t="s">
         <v>353</v>
       </c>
-      <c r="E59" s="37" t="s">
+      <c r="E61" s="37" t="s">
         <v>356</v>
-      </c>
-    </row>
-    <row r="60" spans="1:8" s="10" customFormat="1" ht="12">
-      <c r="B60" s="10" t="s">
-        <v>354</v>
-      </c>
-    </row>
-    <row r="61" spans="1:8" s="10" customFormat="1" ht="12">
-      <c r="B61" s="10" t="s">
-        <v>13</v>
-      </c>
-      <c r="D61" s="10" t="s">
-        <v>35</v>
       </c>
     </row>
     <row r="62" spans="1:8" s="10" customFormat="1" ht="12">
       <c r="B62" s="10" t="s">
+        <v>354</v>
+      </c>
+    </row>
+    <row r="63" spans="1:8" s="10" customFormat="1" ht="12">
+      <c r="B63" s="10" t="s">
+        <v>13</v>
+      </c>
+      <c r="D63" s="10" t="s">
+        <v>35</v>
+      </c>
+    </row>
+    <row r="64" spans="1:8" s="10" customFormat="1" ht="12">
+      <c r="B64" s="10" t="s">
         <v>355</v>
       </c>
     </row>
-    <row r="63" spans="1:8" s="10" customFormat="1" ht="12"/>
-    <row r="64" spans="1:8" ht="30">
-      <c r="A64" s="21"/>
-      <c r="B64" s="13" t="s">
+    <row r="65" spans="1:8" s="10" customFormat="1" ht="12"/>
+    <row r="66" spans="1:8" ht="30">
+      <c r="A66" s="21"/>
+      <c r="B66" s="13" t="s">
         <v>327</v>
       </c>
-      <c r="C64" s="13"/>
-      <c r="D64" s="13"/>
-      <c r="E64" s="13" t="s">
+      <c r="C66" s="13"/>
+      <c r="D66" s="13"/>
+      <c r="E66" s="13" t="s">
         <v>323</v>
       </c>
-      <c r="F64" s="13"/>
-      <c r="G64" s="13"/>
-      <c r="H64" s="13"/>
-    </row>
-    <row r="65" spans="1:8" ht="30">
-      <c r="A65" s="21"/>
-      <c r="B65" s="13" t="s">
+      <c r="F66" s="13"/>
+      <c r="G66" s="13"/>
+      <c r="H66" s="13"/>
+    </row>
+    <row r="67" spans="1:8" ht="30">
+      <c r="A67" s="21"/>
+      <c r="B67" s="13" t="s">
         <v>328</v>
       </c>
-      <c r="C65" s="13"/>
-      <c r="D65" s="13"/>
-      <c r="E65" s="13" t="s">
+      <c r="C67" s="13"/>
+      <c r="D67" s="13"/>
+      <c r="E67" s="13" t="s">
         <v>329</v>
       </c>
-      <c r="F65" s="13"/>
-      <c r="G65" s="13"/>
-      <c r="H65" s="13"/>
-    </row>
-    <row r="66" spans="1:8" ht="15">
-      <c r="A66" s="21"/>
-      <c r="B66" s="15" t="s">
+      <c r="F67" s="13"/>
+      <c r="G67" s="13"/>
+      <c r="H67" s="13"/>
+    </row>
+    <row r="68" spans="1:8" ht="15">
+      <c r="A68" s="21"/>
+      <c r="B68" s="15" t="s">
         <v>325</v>
       </c>
-      <c r="C66" s="15"/>
-      <c r="D66" s="15"/>
-      <c r="E66" s="15"/>
-      <c r="F66" s="15"/>
-      <c r="G66" s="15"/>
-      <c r="H66" s="15"/>
-    </row>
-    <row r="67" spans="1:8" ht="12">
-      <c r="A67" s="21"/>
-      <c r="B67" s="10"/>
-      <c r="C67" s="10"/>
-      <c r="D67" s="10"/>
-      <c r="E67" s="10"/>
-      <c r="F67" s="10"/>
-      <c r="G67" s="10"/>
-      <c r="H67" s="10"/>
-    </row>
-    <row r="68" spans="1:8" ht="24">
-      <c r="A68" s="21"/>
-      <c r="B68" t="s">
-        <v>336</v>
-      </c>
-      <c r="C68" t="s">
-        <v>335</v>
-      </c>
-      <c r="F68" t="s">
-        <v>6</v>
-      </c>
-      <c r="G68" s="10"/>
-      <c r="H68" s="10"/>
-    </row>
-    <row r="69" spans="1:8" ht="30">
+      <c r="C68" s="15"/>
+      <c r="D68" s="15"/>
+      <c r="E68" s="15"/>
+      <c r="F68" s="15"/>
+      <c r="G68" s="15"/>
+      <c r="H68" s="15"/>
+    </row>
+    <row r="69" spans="1:8" ht="12">
       <c r="A69" s="21"/>
-      <c r="B69" s="13" t="s">
-        <v>341</v>
-      </c>
-      <c r="C69" s="13"/>
-      <c r="D69" s="13"/>
-      <c r="E69" s="13" t="s">
-        <v>338</v>
-      </c>
-      <c r="F69" s="13"/>
+      <c r="B69" s="10"/>
+      <c r="C69" s="10"/>
+      <c r="D69" s="10"/>
+      <c r="E69" s="10"/>
+      <c r="F69" s="10"/>
       <c r="G69" s="10"/>
       <c r="H69" s="10"/>
     </row>
-    <row r="70" spans="1:8" ht="30">
+    <row r="70" spans="1:8" ht="24">
       <c r="A70" s="21"/>
-      <c r="B70" s="13" t="s">
-        <v>342</v>
-      </c>
-      <c r="C70" s="13"/>
-      <c r="D70" s="13"/>
-      <c r="E70" s="13" t="s">
-        <v>343</v>
-      </c>
-      <c r="F70" s="13"/>
+      <c r="B70" t="s">
+        <v>336</v>
+      </c>
+      <c r="C70" t="s">
+        <v>335</v>
+      </c>
+      <c r="F70" t="s">
+        <v>6</v>
+      </c>
       <c r="G70" s="10"/>
       <c r="H70" s="10"/>
     </row>
-    <row r="71" spans="1:8" ht="15">
+    <row r="71" spans="1:8" ht="30">
       <c r="A71" s="21"/>
-      <c r="B71" s="15" t="s">
-        <v>339</v>
-      </c>
-      <c r="C71" s="15"/>
-      <c r="D71" s="15"/>
-      <c r="E71" s="15"/>
+      <c r="B71" s="13" t="s">
+        <v>341</v>
+      </c>
+      <c r="C71" s="13"/>
+      <c r="D71" s="13"/>
+      <c r="E71" s="13" t="s">
+        <v>338</v>
+      </c>
+      <c r="F71" s="13"/>
       <c r="G71" s="10"/>
       <c r="H71" s="10"/>
     </row>
-    <row r="72" spans="1:8" ht="12">
+    <row r="72" spans="1:8" ht="30">
       <c r="A72" s="21"/>
-      <c r="B72" t="s">
-        <v>15</v>
-      </c>
+      <c r="B72" s="13" t="s">
+        <v>342</v>
+      </c>
+      <c r="C72" s="13"/>
+      <c r="D72" s="13"/>
+      <c r="E72" s="13" t="s">
+        <v>343</v>
+      </c>
+      <c r="F72" s="13"/>
       <c r="G72" s="10"/>
       <c r="H72" s="10"/>
     </row>
-    <row r="73" spans="1:8" ht="12">
+    <row r="73" spans="1:8" ht="15">
       <c r="A73" s="21"/>
-      <c r="B73" s="2" t="s">
-        <v>13</v>
-      </c>
-      <c r="C73" s="12"/>
-      <c r="D73" s="25" t="s">
-        <v>350</v>
-      </c>
-      <c r="E73" s="12"/>
-      <c r="F73" s="12"/>
+      <c r="B73" s="15" t="s">
+        <v>339</v>
+      </c>
+      <c r="C73" s="15"/>
+      <c r="D73" s="15"/>
+      <c r="E73" s="15"/>
       <c r="G73" s="10"/>
       <c r="H73" s="10"/>
     </row>
     <row r="74" spans="1:8" ht="12">
       <c r="A74" s="21"/>
-      <c r="B74" s="2" t="s">
-        <v>23</v>
-      </c>
-      <c r="C74" s="12"/>
-      <c r="D74" s="25"/>
-      <c r="E74" s="12"/>
-      <c r="F74" s="12"/>
+      <c r="B74" t="s">
+        <v>15</v>
+      </c>
       <c r="G74" s="10"/>
       <c r="H74" s="10"/>
     </row>
-    <row r="75" spans="1:8" ht="15">
+    <row r="75" spans="1:8" ht="12">
       <c r="A75" s="21"/>
-      <c r="B75" s="15" t="s">
-        <v>340</v>
-      </c>
-      <c r="C75" s="18"/>
-      <c r="D75" s="31"/>
-      <c r="E75" s="18"/>
+      <c r="B75" s="2" t="s">
+        <v>13</v>
+      </c>
+      <c r="C75" s="12"/>
+      <c r="D75" s="25" t="s">
+        <v>350</v>
+      </c>
+      <c r="E75" s="12"/>
       <c r="F75" s="12"/>
       <c r="G75" s="10"/>
       <c r="H75" s="10"/>
     </row>
-    <row r="76" spans="1:8" ht="30">
-      <c r="A76" s="27"/>
-      <c r="B76" s="13" t="s">
+    <row r="76" spans="1:8" ht="12">
+      <c r="A76" s="21"/>
+      <c r="B76" s="2" t="s">
+        <v>23</v>
+      </c>
+      <c r="C76" s="12"/>
+      <c r="D76" s="25"/>
+      <c r="E76" s="12"/>
+      <c r="F76" s="12"/>
+      <c r="G76" s="10"/>
+      <c r="H76" s="10"/>
+    </row>
+    <row r="77" spans="1:8" ht="15">
+      <c r="A77" s="21"/>
+      <c r="B77" s="15" t="s">
+        <v>340</v>
+      </c>
+      <c r="C77" s="18"/>
+      <c r="D77" s="31"/>
+      <c r="E77" s="18"/>
+      <c r="F77" s="12"/>
+      <c r="G77" s="10"/>
+      <c r="H77" s="10"/>
+    </row>
+    <row r="78" spans="1:8" ht="30">
+      <c r="A78" s="27"/>
+      <c r="B78" s="13" t="s">
         <v>345</v>
       </c>
-      <c r="C76" s="13"/>
-      <c r="D76" s="13"/>
-      <c r="E76" s="13" t="s">
+      <c r="C78" s="13"/>
+      <c r="D78" s="13"/>
+      <c r="E78" s="13" t="s">
         <v>337</v>
       </c>
-      <c r="F76" s="13"/>
-    </row>
-    <row r="77" spans="1:8" ht="30">
-      <c r="A77" s="27"/>
-      <c r="B77" s="13" t="s">
+      <c r="F78" s="13"/>
+    </row>
+    <row r="79" spans="1:8" ht="30">
+      <c r="A79" s="27"/>
+      <c r="B79" s="13" t="s">
         <v>346</v>
       </c>
-      <c r="C77" s="13"/>
-      <c r="D77" s="13"/>
-      <c r="E77" s="13" t="s">
+      <c r="C79" s="13"/>
+      <c r="D79" s="13"/>
+      <c r="E79" s="13" t="s">
         <v>347</v>
       </c>
-      <c r="F77" s="13"/>
-    </row>
-    <row r="78" spans="1:8" s="10" customFormat="1" ht="15">
-      <c r="B78" s="26" t="s">
+      <c r="F79" s="13"/>
+    </row>
+    <row r="80" spans="1:8" s="10" customFormat="1" ht="15">
+      <c r="B80" s="26" t="s">
         <v>13</v>
       </c>
-      <c r="C78" s="26"/>
-      <c r="D78" s="26" t="s">
+      <c r="C80" s="26"/>
+      <c r="D80" s="26" t="s">
         <v>359</v>
       </c>
-      <c r="E78" s="26"/>
-      <c r="F78" s="26"/>
-    </row>
-    <row r="79" spans="1:8" ht="15">
-      <c r="A79" s="27"/>
-      <c r="B79" s="15" t="s">
+      <c r="E80" s="26"/>
+      <c r="F80" s="26"/>
+    </row>
+    <row r="81" spans="1:8" ht="15">
+      <c r="A81" s="27"/>
+      <c r="B81" s="15" t="s">
         <v>348</v>
       </c>
-      <c r="C79" s="15"/>
-      <c r="D79" s="15"/>
-      <c r="E79" s="15"/>
-      <c r="F79" s="15"/>
-    </row>
-    <row r="80" spans="1:8" ht="12">
-      <c r="A80" s="27"/>
-      <c r="B80" t="s">
-        <v>15</v>
-      </c>
-    </row>
-    <row r="81" spans="1:8" ht="12">
-      <c r="A81" s="27"/>
-      <c r="B81" t="s">
-        <v>13</v>
-      </c>
-      <c r="C81" s="20"/>
-      <c r="D81" s="28" t="s">
-        <v>344</v>
-      </c>
-      <c r="E81" s="28"/>
-      <c r="F81" s="20"/>
+      <c r="C81" s="15"/>
+      <c r="D81" s="15"/>
+      <c r="E81" s="15"/>
+      <c r="F81" s="15"/>
     </row>
     <row r="82" spans="1:8" ht="12">
       <c r="A82" s="27"/>
       <c r="B82" t="s">
-        <v>23</v>
-      </c>
-      <c r="C82" s="20"/>
-      <c r="D82" s="28"/>
-      <c r="E82" s="20"/>
-      <c r="F82" s="20"/>
+        <v>15</v>
+      </c>
     </row>
     <row r="83" spans="1:8" ht="12">
       <c r="A83" s="27"/>
+      <c r="B83" t="s">
+        <v>13</v>
+      </c>
       <c r="C83" s="20"/>
-      <c r="D83" s="28"/>
-      <c r="E83" s="20"/>
+      <c r="D83" s="28" t="s">
+        <v>344</v>
+      </c>
+      <c r="E83" s="28"/>
       <c r="F83" s="20"/>
     </row>
-    <row r="84" spans="1:8" ht="15">
+    <row r="84" spans="1:8" ht="12">
       <c r="A84" s="27"/>
-      <c r="B84" s="15" t="s">
-        <v>349</v>
-      </c>
-      <c r="C84" s="29"/>
-      <c r="D84" s="30"/>
-      <c r="E84" s="29"/>
-      <c r="F84" s="29"/>
-    </row>
-    <row r="85" spans="1:8" s="10" customFormat="1" ht="15">
-      <c r="B85" s="32" t="s">
-        <v>13</v>
-      </c>
-      <c r="C85" s="33"/>
-      <c r="D85" s="34" t="s">
-        <v>358</v>
-      </c>
-      <c r="E85" s="33"/>
-      <c r="F85" s="33"/>
+      <c r="B84" t="s">
+        <v>23</v>
+      </c>
+      <c r="C84" s="20"/>
+      <c r="D84" s="28"/>
+      <c r="E84" s="20"/>
+      <c r="F84" s="20"/>
+    </row>
+    <row r="85" spans="1:8" ht="12">
+      <c r="A85" s="27"/>
+      <c r="C85" s="20"/>
+      <c r="D85" s="28"/>
+      <c r="E85" s="20"/>
+      <c r="F85" s="20"/>
     </row>
     <row r="86" spans="1:8" ht="15">
       <c r="A86" s="27"/>
       <c r="B86" s="15" t="s">
-        <v>326</v>
+        <v>349</v>
       </c>
       <c r="C86" s="29"/>
       <c r="D86" s="30"/>
@@ -4173,7 +4242,7 @@
       </c>
       <c r="C87" s="33"/>
       <c r="D87" s="34" t="s">
-        <v>360</v>
+        <v>358</v>
       </c>
       <c r="E87" s="33"/>
       <c r="F87" s="33"/>
@@ -4181,301 +4250,298 @@
     <row r="88" spans="1:8" ht="15">
       <c r="A88" s="27"/>
       <c r="B88" s="15" t="s">
-        <v>73</v>
+        <v>326</v>
       </c>
       <c r="C88" s="29"/>
       <c r="D88" s="30"/>
       <c r="E88" s="29"/>
       <c r="F88" s="29"/>
     </row>
-    <row r="89" spans="1:8" ht="15">
-      <c r="A89" s="10"/>
-      <c r="B89" s="32"/>
+    <row r="89" spans="1:8" s="10" customFormat="1" ht="15">
+      <c r="B89" s="32" t="s">
+        <v>13</v>
+      </c>
       <c r="C89" s="33"/>
-      <c r="D89" s="34"/>
+      <c r="D89" s="34" t="s">
+        <v>360</v>
+      </c>
       <c r="E89" s="33"/>
       <c r="F89" s="33"/>
     </row>
-    <row r="90" spans="1:8" s="13" customFormat="1" ht="15">
-      <c r="A90" s="26"/>
-      <c r="B90" s="13" t="s">
+    <row r="90" spans="1:8" ht="15">
+      <c r="A90" s="27"/>
+      <c r="B90" s="15" t="s">
+        <v>73</v>
+      </c>
+      <c r="C90" s="29"/>
+      <c r="D90" s="30"/>
+      <c r="E90" s="29"/>
+      <c r="F90" s="29"/>
+    </row>
+    <row r="91" spans="1:8" ht="15">
+      <c r="A91" s="10"/>
+      <c r="B91" s="32"/>
+      <c r="C91" s="33"/>
+      <c r="D91" s="34"/>
+      <c r="E91" s="33"/>
+      <c r="F91" s="33"/>
+    </row>
+    <row r="92" spans="1:8" s="13" customFormat="1" ht="15">
+      <c r="A92" s="26"/>
+      <c r="B92" s="13" t="s">
         <v>95</v>
       </c>
-      <c r="C90" s="35"/>
-      <c r="D90" s="36"/>
-      <c r="E90" s="14" t="s">
+      <c r="C92" s="35"/>
+      <c r="D92" s="36"/>
+      <c r="E92" s="14" t="s">
         <v>351</v>
       </c>
-      <c r="F90" s="35"/>
-    </row>
-    <row r="91" spans="1:8" s="13" customFormat="1" ht="15">
-      <c r="A91" s="26"/>
-      <c r="B91" s="13" t="s">
+      <c r="F92" s="35"/>
+    </row>
+    <row r="93" spans="1:8" s="13" customFormat="1" ht="15">
+      <c r="A93" s="26"/>
+      <c r="B93" s="13" t="s">
         <v>74</v>
       </c>
-      <c r="C91" s="35"/>
-      <c r="D91" s="36"/>
-      <c r="E91" s="14" t="s">
+      <c r="C93" s="35"/>
+      <c r="D93" s="36"/>
+      <c r="E93" s="14" t="s">
         <v>75</v>
       </c>
-      <c r="F91" s="35"/>
-    </row>
-    <row r="92" spans="1:8" ht="15">
-      <c r="A92" s="21" t="s">
+      <c r="F93" s="35"/>
+    </row>
+    <row r="94" spans="1:8" ht="15">
+      <c r="A94" s="21" t="s">
         <v>333</v>
       </c>
-      <c r="B92" s="15" t="s">
+      <c r="B94" s="15" t="s">
         <v>96</v>
       </c>
-      <c r="C92" s="15"/>
-      <c r="D92" s="15"/>
-      <c r="E92" s="15"/>
-      <c r="F92" s="15"/>
-      <c r="G92" s="15"/>
-      <c r="H92" s="15"/>
-    </row>
-    <row r="93" spans="1:8" ht="12">
-      <c r="A93" s="21"/>
-      <c r="B93" t="s">
-        <v>156</v>
-      </c>
-      <c r="C93" t="s">
-        <v>11</v>
-      </c>
-      <c r="D93" t="s">
-        <v>12</v>
-      </c>
-      <c r="F93" t="s">
-        <v>6</v>
-      </c>
-      <c r="G93" s="20"/>
-      <c r="H93" s="20"/>
-    </row>
-    <row r="94" spans="1:8" ht="12">
-      <c r="A94" s="21"/>
-      <c r="B94" s="38" t="s">
-        <v>15</v>
-      </c>
-      <c r="E94" t="s">
-        <v>362</v>
-      </c>
+      <c r="C94" s="15"/>
+      <c r="D94" s="15"/>
+      <c r="E94" s="15"/>
+      <c r="F94" s="15"/>
+      <c r="G94" s="15"/>
+      <c r="H94" s="15"/>
     </row>
     <row r="95" spans="1:8" ht="12">
       <c r="A95" s="21"/>
       <c r="B95" t="s">
-        <v>13</v>
+        <v>156</v>
+      </c>
+      <c r="C95" t="s">
+        <v>11</v>
       </c>
       <c r="D95" t="s">
-        <v>40</v>
-      </c>
+        <v>12</v>
+      </c>
+      <c r="F95" t="s">
+        <v>6</v>
+      </c>
+      <c r="G95" s="20"/>
+      <c r="H95" s="20"/>
     </row>
     <row r="96" spans="1:8" ht="12">
       <c r="A96" s="21"/>
-      <c r="B96" t="s">
+      <c r="B96" s="38" t="s">
+        <v>15</v>
+      </c>
+      <c r="E96" t="s">
+        <v>362</v>
+      </c>
+    </row>
+    <row r="97" spans="1:9" ht="12">
+      <c r="A97" s="21"/>
+      <c r="B97" t="s">
+        <v>13</v>
+      </c>
+      <c r="D97" t="s">
+        <v>40</v>
+      </c>
+    </row>
+    <row r="98" spans="1:9" ht="12">
+      <c r="A98" s="21"/>
+      <c r="B98" t="s">
         <v>363</v>
       </c>
-      <c r="C96" t="s">
+      <c r="C98" t="s">
         <v>364</v>
       </c>
-      <c r="D96" t="s">
+      <c r="D98" t="s">
         <v>365</v>
       </c>
-      <c r="F96" t="s">
+      <c r="F98" t="s">
         <v>79</v>
-      </c>
-    </row>
-    <row r="97" spans="1:9" ht="12.75" customHeight="1">
-      <c r="A97" s="27"/>
-      <c r="B97" s="38" t="s">
-        <v>15</v>
-      </c>
-      <c r="C97" t="s">
-        <v>397</v>
-      </c>
-      <c r="E97" t="s">
-        <v>398</v>
-      </c>
-    </row>
-    <row r="98" spans="1:9" ht="12.75" customHeight="1">
-      <c r="A98" s="27"/>
-      <c r="B98" t="s">
-        <v>16</v>
-      </c>
-      <c r="C98" t="s">
-        <v>399</v>
-      </c>
-      <c r="D98" t="s">
-        <v>367</v>
       </c>
     </row>
     <row r="99" spans="1:9" ht="12.75" customHeight="1">
       <c r="A99" s="27"/>
-      <c r="B99" t="s">
-        <v>13</v>
-      </c>
-      <c r="D99" t="s">
-        <v>403</v>
+      <c r="B99" s="38" t="s">
+        <v>15</v>
+      </c>
+      <c r="C99" t="s">
+        <v>397</v>
       </c>
       <c r="E99" t="s">
-        <v>400</v>
-      </c>
-      <c r="I99" s="20"/>
+        <v>398</v>
+      </c>
     </row>
     <row r="100" spans="1:9" ht="12.75" customHeight="1">
       <c r="A100" s="27"/>
-      <c r="B100" s="39" t="s">
+      <c r="B100" t="s">
+        <v>16</v>
+      </c>
+      <c r="C100" t="s">
+        <v>399</v>
+      </c>
+      <c r="D100" t="s">
+        <v>367</v>
+      </c>
+    </row>
+    <row r="101" spans="1:9" ht="12.75" customHeight="1">
+      <c r="A101" s="27"/>
+      <c r="B101" t="s">
+        <v>13</v>
+      </c>
+      <c r="D101" t="s">
+        <v>403</v>
+      </c>
+      <c r="E101" t="s">
+        <v>400</v>
+      </c>
+      <c r="I101" s="20"/>
+    </row>
+    <row r="102" spans="1:9" ht="12.75" customHeight="1">
+      <c r="A102" s="27"/>
+      <c r="B102" s="39" t="s">
         <v>23</v>
       </c>
     </row>
-    <row r="101" spans="1:9" ht="12">
-      <c r="A101" s="21"/>
-      <c r="B101" s="38" t="s">
+    <row r="103" spans="1:9" ht="12">
+      <c r="A103" s="21"/>
+      <c r="B103" s="38" t="s">
         <v>15</v>
       </c>
-      <c r="E101" t="s">
+      <c r="E103" t="s">
         <v>366</v>
       </c>
     </row>
-    <row r="102" spans="1:9" ht="12">
-      <c r="A102" s="21"/>
-      <c r="B102" t="s">
+    <row r="104" spans="1:9" ht="12">
+      <c r="A104" s="21"/>
+      <c r="B104" t="s">
         <v>16</v>
       </c>
-      <c r="C102" t="s">
+      <c r="C104" t="s">
         <v>20</v>
       </c>
-      <c r="D102" t="s">
+      <c r="D104" t="s">
         <v>367</v>
-      </c>
-    </row>
-    <row r="103" spans="1:9" ht="12.75" customHeight="1">
-      <c r="A103" s="21"/>
-      <c r="B103" t="s">
-        <v>13</v>
-      </c>
-      <c r="D103" t="s">
-        <v>21</v>
-      </c>
-      <c r="E103" t="s">
-        <v>22</v>
-      </c>
-      <c r="I103" s="20"/>
-    </row>
-    <row r="104" spans="1:9" ht="12.75" customHeight="1">
-      <c r="A104" s="21"/>
-      <c r="B104" s="39" t="s">
-        <v>23</v>
       </c>
     </row>
     <row r="105" spans="1:9" ht="12.75" customHeight="1">
       <c r="A105" s="21"/>
-      <c r="B105" s="38" t="s">
-        <v>15</v>
+      <c r="B105" t="s">
+        <v>13</v>
+      </c>
+      <c r="D105" t="s">
+        <v>21</v>
       </c>
       <c r="E105" t="s">
-        <v>368</v>
-      </c>
+        <v>22</v>
+      </c>
+      <c r="I105" s="20"/>
     </row>
     <row r="106" spans="1:9" ht="12.75" customHeight="1">
       <c r="A106" s="21"/>
-      <c r="B106" t="s">
-        <v>16</v>
-      </c>
-      <c r="C106" t="s">
-        <v>17</v>
-      </c>
-      <c r="D106" t="s">
-        <v>369</v>
+      <c r="B106" s="39" t="s">
+        <v>23</v>
       </c>
     </row>
     <row r="107" spans="1:9" ht="12.75" customHeight="1">
       <c r="A107" s="21"/>
-      <c r="B107" t="s">
-        <v>13</v>
-      </c>
-      <c r="D107" t="s">
-        <v>18</v>
+      <c r="B107" s="38" t="s">
+        <v>15</v>
       </c>
       <c r="E107" t="s">
-        <v>19</v>
+        <v>368</v>
       </c>
     </row>
     <row r="108" spans="1:9" ht="12.75" customHeight="1">
       <c r="A108" s="21"/>
-      <c r="B108" s="39" t="s">
-        <v>23</v>
+      <c r="B108" t="s">
+        <v>16</v>
+      </c>
+      <c r="C108" t="s">
+        <v>17</v>
+      </c>
+      <c r="D108" t="s">
+        <v>369</v>
       </c>
     </row>
     <row r="109" spans="1:9" ht="12.75" customHeight="1">
       <c r="A109" s="21"/>
-      <c r="B109" s="39" t="s">
-        <v>23</v>
+      <c r="B109" t="s">
+        <v>13</v>
+      </c>
+      <c r="D109" t="s">
+        <v>18</v>
+      </c>
+      <c r="E109" t="s">
+        <v>19</v>
       </c>
     </row>
     <row r="110" spans="1:9" ht="12.75" customHeight="1">
       <c r="A110" s="21"/>
-      <c r="B110" s="40" t="s">
-        <v>15</v>
-      </c>
-      <c r="E110" t="s">
-        <v>370</v>
+      <c r="B110" s="39" t="s">
+        <v>23</v>
       </c>
     </row>
     <row r="111" spans="1:9" ht="12.75" customHeight="1">
       <c r="A111" s="21"/>
-      <c r="B111" t="s">
-        <v>13</v>
-      </c>
-      <c r="D111" t="s">
-        <v>42</v>
+      <c r="B111" s="39" t="s">
+        <v>23</v>
       </c>
     </row>
     <row r="112" spans="1:9" ht="12.75" customHeight="1">
       <c r="A112" s="21"/>
-      <c r="B112" t="s">
-        <v>16</v>
-      </c>
-      <c r="C112" t="s">
-        <v>371</v>
-      </c>
-      <c r="D112" t="s">
-        <v>372</v>
+      <c r="B112" s="40" t="s">
+        <v>15</v>
+      </c>
+      <c r="E112" t="s">
+        <v>370</v>
       </c>
     </row>
     <row r="113" spans="1:10" ht="12.75" customHeight="1">
       <c r="A113" s="21"/>
       <c r="B113" t="s">
-        <v>16</v>
-      </c>
-      <c r="C113" t="s">
-        <v>373</v>
+        <v>13</v>
       </c>
       <c r="D113" t="s">
-        <v>374</v>
+        <v>42</v>
       </c>
     </row>
     <row r="114" spans="1:10" ht="12.75" customHeight="1">
       <c r="A114" s="21"/>
       <c r="B114" t="s">
-        <v>13</v>
+        <v>16</v>
+      </c>
+      <c r="C114" t="s">
+        <v>371</v>
       </c>
       <c r="D114" t="s">
-        <v>375</v>
-      </c>
-      <c r="E114" t="s">
-        <v>376</v>
+        <v>372</v>
       </c>
     </row>
     <row r="115" spans="1:10" ht="12.75" customHeight="1">
       <c r="A115" s="21"/>
       <c r="B115" t="s">
-        <v>13</v>
+        <v>16</v>
+      </c>
+      <c r="C115" t="s">
+        <v>373</v>
       </c>
       <c r="D115" t="s">
-        <v>377</v>
-      </c>
-      <c r="E115" t="s">
-        <v>376</v>
+        <v>374</v>
       </c>
     </row>
     <row r="116" spans="1:10" ht="12.75" customHeight="1">
@@ -4484,7 +4550,7 @@
         <v>13</v>
       </c>
       <c r="D116" t="s">
-        <v>378</v>
+        <v>375</v>
       </c>
       <c r="E116" t="s">
         <v>376</v>
@@ -4492,168 +4558,165 @@
     </row>
     <row r="117" spans="1:10" ht="12.75" customHeight="1">
       <c r="A117" s="21"/>
-      <c r="B117" s="41" t="s">
-        <v>23</v>
+      <c r="B117" t="s">
+        <v>13</v>
+      </c>
+      <c r="D117" t="s">
+        <v>377</v>
+      </c>
+      <c r="E117" t="s">
+        <v>376</v>
       </c>
     </row>
     <row r="118" spans="1:10" ht="12.75" customHeight="1">
       <c r="A118" s="21"/>
-      <c r="B118" s="40" t="s">
-        <v>15</v>
+      <c r="B118" t="s">
+        <v>13</v>
+      </c>
+      <c r="D118" t="s">
+        <v>378</v>
       </c>
       <c r="E118" t="s">
-        <v>379</v>
+        <v>376</v>
       </c>
     </row>
     <row r="119" spans="1:10" ht="12.75" customHeight="1">
       <c r="A119" s="21"/>
-      <c r="B119" t="s">
-        <v>13</v>
-      </c>
-      <c r="D119" t="s">
-        <v>99</v>
+      <c r="B119" s="41" t="s">
+        <v>23</v>
       </c>
     </row>
     <row r="120" spans="1:10" ht="12.75" customHeight="1">
       <c r="A120" s="21"/>
-      <c r="B120" t="s">
-        <v>16</v>
-      </c>
-      <c r="C120" t="s">
-        <v>380</v>
-      </c>
-      <c r="D120" t="s">
-        <v>381</v>
+      <c r="B120" s="40" t="s">
+        <v>15</v>
+      </c>
+      <c r="E120" t="s">
+        <v>379</v>
       </c>
     </row>
     <row r="121" spans="1:10" ht="12.75" customHeight="1">
       <c r="A121" s="21"/>
       <c r="B121" t="s">
-        <v>16</v>
-      </c>
-      <c r="C121" t="s">
-        <v>382</v>
+        <v>13</v>
       </c>
       <c r="D121" t="s">
-        <v>383</v>
+        <v>99</v>
       </c>
     </row>
     <row r="122" spans="1:10" ht="12.75" customHeight="1">
       <c r="A122" s="21"/>
       <c r="B122" t="s">
-        <v>13</v>
+        <v>16</v>
+      </c>
+      <c r="C122" t="s">
+        <v>380</v>
       </c>
       <c r="D122" t="s">
-        <v>384</v>
-      </c>
-      <c r="E122" t="s">
-        <v>385</v>
+        <v>381</v>
       </c>
     </row>
     <row r="123" spans="1:10" ht="12.75" customHeight="1">
       <c r="A123" s="21"/>
-      <c r="B123" s="41" t="s">
-        <v>23</v>
+      <c r="B123" t="s">
+        <v>16</v>
+      </c>
+      <c r="C123" t="s">
+        <v>382</v>
+      </c>
+      <c r="D123" t="s">
+        <v>383</v>
       </c>
     </row>
     <row r="124" spans="1:10" ht="12.75" customHeight="1">
       <c r="A124" s="21"/>
-      <c r="B124" s="15" t="s">
+      <c r="B124" t="s">
+        <v>13</v>
+      </c>
+      <c r="D124" t="s">
+        <v>384</v>
+      </c>
+      <c r="E124" t="s">
+        <v>385</v>
+      </c>
+    </row>
+    <row r="125" spans="1:10" ht="12.75" customHeight="1">
+      <c r="A125" s="21"/>
+      <c r="B125" s="41" t="s">
+        <v>23</v>
+      </c>
+    </row>
+    <row r="126" spans="1:10" ht="12.75" customHeight="1">
+      <c r="A126" s="21"/>
+      <c r="B126" s="15" t="s">
         <v>76</v>
       </c>
-      <c r="C124" s="15"/>
-      <c r="D124" s="15"/>
-      <c r="E124" s="15"/>
-      <c r="F124" s="15"/>
-      <c r="G124" s="15"/>
-      <c r="H124" s="15"/>
-    </row>
-    <row r="125" spans="1:10" s="12" customFormat="1" ht="12.75" customHeight="1"/>
-    <row r="126" spans="1:10" s="14" customFormat="1" ht="12.75" customHeight="1">
-      <c r="A126" s="24"/>
-      <c r="B126" s="13" t="s">
+      <c r="C126" s="15"/>
+      <c r="D126" s="15"/>
+      <c r="E126" s="15"/>
+      <c r="F126" s="15"/>
+      <c r="G126" s="15"/>
+      <c r="H126" s="15"/>
+    </row>
+    <row r="127" spans="1:10" s="12" customFormat="1" ht="12.75" customHeight="1"/>
+    <row r="128" spans="1:10" s="14" customFormat="1" ht="12.75" customHeight="1">
+      <c r="A128" s="24"/>
+      <c r="B128" s="13" t="s">
         <v>97</v>
       </c>
-      <c r="E126" s="14" t="s">
+      <c r="E128" s="14" t="s">
         <v>98</v>
       </c>
-      <c r="I126" s="12"/>
-      <c r="J126" s="12"/>
-    </row>
-    <row r="127" spans="1:10" ht="12.75" customHeight="1">
-      <c r="B127" s="13" t="s">
+      <c r="I128" s="12"/>
+      <c r="J128" s="12"/>
+    </row>
+    <row r="129" spans="1:9" ht="12.75" customHeight="1">
+      <c r="B129" s="13" t="s">
         <v>81</v>
       </c>
-      <c r="C127" s="14"/>
-      <c r="D127" s="14"/>
-      <c r="E127" s="14" t="s">
+      <c r="C129" s="14"/>
+      <c r="D129" s="14"/>
+      <c r="E129" s="14" t="s">
         <v>77</v>
       </c>
-      <c r="F127" s="14"/>
-      <c r="G127" s="14"/>
-      <c r="H127" s="14"/>
-    </row>
-    <row r="128" spans="1:10" ht="12.75" customHeight="1">
-      <c r="A128" s="21" t="s">
+      <c r="F129" s="14"/>
+      <c r="G129" s="14"/>
+      <c r="H129" s="14"/>
+    </row>
+    <row r="130" spans="1:9" ht="12.75" customHeight="1">
+      <c r="A130" s="21" t="s">
         <v>334</v>
       </c>
-      <c r="B128" s="15" t="s">
+      <c r="B130" s="15" t="s">
         <v>109</v>
       </c>
-      <c r="C128" s="18"/>
-      <c r="D128" s="18"/>
-      <c r="E128" s="18"/>
-      <c r="F128" s="18"/>
-      <c r="G128" s="18"/>
-      <c r="H128" s="18"/>
-    </row>
-    <row r="129" spans="1:9" ht="12.75" customHeight="1">
-      <c r="A129" s="21"/>
-      <c r="B129" s="42" t="s">
-        <v>15</v>
-      </c>
-      <c r="H129" s="12"/>
-    </row>
-    <row r="130" spans="1:9" ht="12.75" customHeight="1">
-      <c r="A130" s="21"/>
-      <c r="B130" t="s">
-        <v>409</v>
-      </c>
-      <c r="C130" t="s">
-        <v>78</v>
-      </c>
-      <c r="D130" t="s">
-        <v>404</v>
-      </c>
-      <c r="F130" t="s">
-        <v>79</v>
-      </c>
+      <c r="C130" s="18"/>
+      <c r="D130" s="18"/>
+      <c r="E130" s="18"/>
+      <c r="F130" s="18"/>
+      <c r="G130" s="18"/>
+      <c r="H130" s="18"/>
     </row>
     <row r="131" spans="1:9" ht="12.75" customHeight="1">
       <c r="A131" s="21"/>
-      <c r="B131" t="s">
-        <v>13</v>
-      </c>
-      <c r="C131" t="s">
-        <v>405</v>
-      </c>
-      <c r="E131" t="s">
-        <v>410</v>
-      </c>
-      <c r="I131" t="s">
-        <v>406</v>
-      </c>
+      <c r="B131" s="42" t="s">
+        <v>15</v>
+      </c>
+      <c r="H131" s="12"/>
     </row>
     <row r="132" spans="1:9" ht="12.75" customHeight="1">
       <c r="A132" s="21"/>
       <c r="B132" t="s">
-        <v>13</v>
+        <v>409</v>
+      </c>
+      <c r="C132" t="s">
+        <v>78</v>
       </c>
       <c r="D132" t="s">
-        <v>407</v>
-      </c>
-      <c r="E132" t="s">
-        <v>411</v>
+        <v>404</v>
+      </c>
+      <c r="F132" t="s">
+        <v>79</v>
       </c>
     </row>
     <row r="133" spans="1:9" ht="12.75" customHeight="1">
@@ -4661,313 +4724,316 @@
       <c r="B133" t="s">
         <v>13</v>
       </c>
-      <c r="D133" t="s">
-        <v>408</v>
+      <c r="C133" t="s">
+        <v>405</v>
       </c>
       <c r="E133" t="s">
-        <v>412</v>
+        <v>410</v>
+      </c>
+      <c r="I133" t="s">
+        <v>406</v>
       </c>
     </row>
     <row r="134" spans="1:9" ht="12.75" customHeight="1">
       <c r="A134" s="21"/>
-      <c r="B134" s="43" t="s">
-        <v>23</v>
+      <c r="B134" t="s">
+        <v>13</v>
+      </c>
+      <c r="D134" t="s">
+        <v>407</v>
+      </c>
+      <c r="E134" t="s">
+        <v>411</v>
       </c>
     </row>
     <row r="135" spans="1:9" ht="12.75" customHeight="1">
       <c r="A135" s="21"/>
-      <c r="B135" s="15" t="s">
+      <c r="B135" t="s">
+        <v>13</v>
+      </c>
+      <c r="D135" t="s">
+        <v>408</v>
+      </c>
+      <c r="E135" t="s">
+        <v>412</v>
+      </c>
+    </row>
+    <row r="136" spans="1:9" ht="12.75" customHeight="1">
+      <c r="A136" s="21"/>
+      <c r="B136" s="43" t="s">
+        <v>23</v>
+      </c>
+    </row>
+    <row r="137" spans="1:9" ht="12.75" customHeight="1">
+      <c r="A137" s="21"/>
+      <c r="B137" s="15" t="s">
         <v>80</v>
       </c>
-      <c r="C135" s="18"/>
-      <c r="D135" s="18"/>
-      <c r="E135" s="18"/>
-      <c r="F135" s="18"/>
-      <c r="G135" s="18"/>
-      <c r="H135" s="18"/>
-    </row>
-    <row r="137" spans="1:9" ht="12.75" customHeight="1">
-      <c r="B137" s="13" t="s">
+      <c r="C137" s="18"/>
+      <c r="D137" s="18"/>
+      <c r="E137" s="18"/>
+      <c r="F137" s="18"/>
+      <c r="G137" s="18"/>
+      <c r="H137" s="18"/>
+    </row>
+    <row r="139" spans="1:9" ht="12.75" customHeight="1">
+      <c r="B139" s="13" t="s">
         <v>100</v>
       </c>
-      <c r="C137" s="14"/>
-      <c r="D137" s="14"/>
-      <c r="E137" s="14" t="s">
+      <c r="C139" s="14"/>
+      <c r="D139" s="14"/>
+      <c r="E139" s="14" t="s">
         <v>102</v>
       </c>
-      <c r="F137" s="14"/>
-      <c r="G137" s="14"/>
-      <c r="H137" s="14"/>
-    </row>
-    <row r="138" spans="1:9" ht="12.75" customHeight="1">
-      <c r="B138" s="13" t="s">
+      <c r="F139" s="14"/>
+      <c r="G139" s="14"/>
+      <c r="H139" s="14"/>
+    </row>
+    <row r="140" spans="1:9" ht="12.75" customHeight="1">
+      <c r="B140" s="13" t="s">
         <v>101</v>
       </c>
-      <c r="C138" s="14"/>
-      <c r="D138" s="14"/>
-      <c r="E138" s="14" t="s">
+      <c r="C140" s="14"/>
+      <c r="D140" s="14"/>
+      <c r="E140" s="14" t="s">
         <v>103</v>
       </c>
-      <c r="F138" s="14"/>
-      <c r="G138" s="14"/>
-      <c r="H138" s="14"/>
-    </row>
-    <row r="139" spans="1:9" ht="12.75" customHeight="1">
-      <c r="A139" s="21" t="s">
+      <c r="F140" s="14"/>
+      <c r="G140" s="14"/>
+      <c r="H140" s="14"/>
+    </row>
+    <row r="141" spans="1:9" ht="12.75" customHeight="1">
+      <c r="A141" s="21" t="s">
         <v>57</v>
       </c>
-      <c r="B139" s="15" t="s">
+      <c r="B141" s="15" t="s">
         <v>110</v>
       </c>
-      <c r="C139" s="18"/>
-      <c r="D139" s="18"/>
-      <c r="E139" s="18"/>
-      <c r="F139" s="18"/>
-      <c r="G139" s="18"/>
-      <c r="H139" s="18"/>
-    </row>
-    <row r="140" spans="1:9" ht="12.75" customHeight="1">
-      <c r="A140" s="27"/>
-      <c r="B140" t="s">
-        <v>156</v>
-      </c>
-      <c r="C140" t="s">
-        <v>11</v>
-      </c>
-      <c r="D140" t="s">
-        <v>60</v>
-      </c>
-      <c r="F140" t="s">
-        <v>6</v>
-      </c>
-      <c r="G140" s="20"/>
-      <c r="H140" s="20"/>
-    </row>
-    <row r="141" spans="1:9" ht="12.75" customHeight="1">
-      <c r="A141" s="27"/>
-      <c r="B141" s="38" t="s">
-        <v>15</v>
-      </c>
-      <c r="E141" t="s">
-        <v>362</v>
-      </c>
+      <c r="C141" s="18"/>
+      <c r="D141" s="18"/>
+      <c r="E141" s="18"/>
+      <c r="F141" s="18"/>
+      <c r="G141" s="18"/>
+      <c r="H141" s="18"/>
     </row>
     <row r="142" spans="1:9" ht="12.75" customHeight="1">
       <c r="A142" s="27"/>
       <c r="B142" t="s">
-        <v>13</v>
+        <v>156</v>
+      </c>
+      <c r="C142" t="s">
+        <v>11</v>
       </c>
       <c r="D142" t="s">
-        <v>40</v>
-      </c>
+        <v>60</v>
+      </c>
+      <c r="F142" t="s">
+        <v>6</v>
+      </c>
+      <c r="G142" s="20"/>
+      <c r="H142" s="20"/>
     </row>
     <row r="143" spans="1:9" ht="12.75" customHeight="1">
       <c r="A143" s="27"/>
-      <c r="B143" t="s">
-        <v>363</v>
-      </c>
-      <c r="C143" t="s">
-        <v>364</v>
-      </c>
-      <c r="D143" t="s">
-        <v>365</v>
-      </c>
-      <c r="F143" t="s">
-        <v>79</v>
+      <c r="B143" s="38" t="s">
+        <v>15</v>
+      </c>
+      <c r="E143" t="s">
+        <v>362</v>
       </c>
     </row>
     <row r="144" spans="1:9" ht="12.75" customHeight="1">
       <c r="A144" s="27"/>
-      <c r="B144" s="38" t="s">
-        <v>15</v>
-      </c>
-      <c r="C144" t="s">
-        <v>397</v>
-      </c>
-      <c r="E144" t="s">
-        <v>398</v>
+      <c r="B144" t="s">
+        <v>13</v>
+      </c>
+      <c r="D144" t="s">
+        <v>40</v>
       </c>
     </row>
     <row r="145" spans="1:9" ht="12.75" customHeight="1">
       <c r="A145" s="27"/>
       <c r="B145" t="s">
-        <v>16</v>
+        <v>363</v>
       </c>
       <c r="C145" t="s">
-        <v>399</v>
+        <v>364</v>
       </c>
       <c r="D145" t="s">
-        <v>367</v>
+        <v>365</v>
+      </c>
+      <c r="F145" t="s">
+        <v>79</v>
       </c>
     </row>
     <row r="146" spans="1:9" ht="12.75" customHeight="1">
       <c r="A146" s="27"/>
-      <c r="B146" t="s">
-        <v>13</v>
-      </c>
-      <c r="D146" t="s">
-        <v>403</v>
+      <c r="B146" s="38" t="s">
+        <v>15</v>
+      </c>
+      <c r="C146" t="s">
+        <v>397</v>
       </c>
       <c r="E146" t="s">
-        <v>400</v>
-      </c>
-      <c r="I146" s="20"/>
+        <v>398</v>
+      </c>
     </row>
     <row r="147" spans="1:9" ht="12.75" customHeight="1">
       <c r="A147" s="27"/>
-      <c r="B147" s="39" t="s">
-        <v>23</v>
+      <c r="B147" t="s">
+        <v>16</v>
+      </c>
+      <c r="C147" t="s">
+        <v>399</v>
+      </c>
+      <c r="D147" t="s">
+        <v>367</v>
       </c>
     </row>
     <row r="148" spans="1:9" ht="12.75" customHeight="1">
       <c r="A148" s="27"/>
-      <c r="B148" s="38" t="s">
-        <v>15</v>
+      <c r="B148" t="s">
+        <v>13</v>
+      </c>
+      <c r="D148" t="s">
+        <v>403</v>
       </c>
       <c r="E148" t="s">
-        <v>366</v>
-      </c>
+        <v>400</v>
+      </c>
+      <c r="I148" s="20"/>
     </row>
     <row r="149" spans="1:9" ht="12.75" customHeight="1">
       <c r="A149" s="27"/>
-      <c r="B149" t="s">
-        <v>16</v>
-      </c>
-      <c r="C149" t="s">
-        <v>20</v>
-      </c>
-      <c r="D149" t="s">
-        <v>367</v>
+      <c r="B149" s="39" t="s">
+        <v>23</v>
       </c>
     </row>
     <row r="150" spans="1:9" ht="12.75" customHeight="1">
       <c r="A150" s="27"/>
-      <c r="B150" t="s">
-        <v>13</v>
-      </c>
-      <c r="D150" t="s">
-        <v>21</v>
+      <c r="B150" s="38" t="s">
+        <v>15</v>
       </c>
       <c r="E150" t="s">
-        <v>22</v>
-      </c>
-      <c r="I150" s="20"/>
+        <v>366</v>
+      </c>
     </row>
     <row r="151" spans="1:9" ht="12.75" customHeight="1">
       <c r="A151" s="27"/>
-      <c r="B151" s="39" t="s">
-        <v>23</v>
+      <c r="B151" t="s">
+        <v>16</v>
+      </c>
+      <c r="C151" t="s">
+        <v>20</v>
+      </c>
+      <c r="D151" t="s">
+        <v>367</v>
       </c>
     </row>
     <row r="152" spans="1:9" ht="12.75" customHeight="1">
       <c r="A152" s="27"/>
-      <c r="B152" s="38" t="s">
-        <v>15</v>
+      <c r="B152" t="s">
+        <v>13</v>
+      </c>
+      <c r="D152" t="s">
+        <v>21</v>
       </c>
       <c r="E152" t="s">
-        <v>368</v>
-      </c>
+        <v>22</v>
+      </c>
+      <c r="I152" s="20"/>
     </row>
     <row r="153" spans="1:9" ht="12.75" customHeight="1">
       <c r="A153" s="27"/>
-      <c r="B153" t="s">
-        <v>16</v>
-      </c>
-      <c r="C153" t="s">
-        <v>17</v>
-      </c>
-      <c r="D153" t="s">
-        <v>369</v>
+      <c r="B153" s="39" t="s">
+        <v>23</v>
       </c>
     </row>
     <row r="154" spans="1:9" ht="12.75" customHeight="1">
       <c r="A154" s="27"/>
-      <c r="B154" t="s">
-        <v>13</v>
-      </c>
-      <c r="D154" t="s">
-        <v>18</v>
+      <c r="B154" s="38" t="s">
+        <v>15</v>
       </c>
       <c r="E154" t="s">
-        <v>19</v>
+        <v>368</v>
       </c>
     </row>
     <row r="155" spans="1:9" ht="12.75" customHeight="1">
       <c r="A155" s="27"/>
-      <c r="B155" s="39" t="s">
-        <v>23</v>
+      <c r="B155" t="s">
+        <v>16</v>
+      </c>
+      <c r="C155" t="s">
+        <v>17</v>
+      </c>
+      <c r="D155" t="s">
+        <v>369</v>
       </c>
     </row>
     <row r="156" spans="1:9" ht="12.75" customHeight="1">
       <c r="A156" s="27"/>
-      <c r="B156" s="39" t="s">
-        <v>23</v>
+      <c r="B156" t="s">
+        <v>13</v>
+      </c>
+      <c r="D156" t="s">
+        <v>18</v>
+      </c>
+      <c r="E156" t="s">
+        <v>19</v>
       </c>
     </row>
     <row r="157" spans="1:9" ht="12.75" customHeight="1">
       <c r="A157" s="27"/>
-      <c r="B157" s="40" t="s">
-        <v>15</v>
-      </c>
-      <c r="E157" t="s">
-        <v>370</v>
+      <c r="B157" s="39" t="s">
+        <v>23</v>
       </c>
     </row>
     <row r="158" spans="1:9" ht="12.75" customHeight="1">
       <c r="A158" s="27"/>
-      <c r="B158" t="s">
-        <v>13</v>
-      </c>
-      <c r="D158" t="s">
-        <v>42</v>
+      <c r="B158" s="39" t="s">
+        <v>23</v>
       </c>
     </row>
     <row r="159" spans="1:9" ht="12.75" customHeight="1">
       <c r="A159" s="27"/>
-      <c r="B159" t="s">
-        <v>16</v>
-      </c>
-      <c r="C159" t="s">
-        <v>371</v>
-      </c>
-      <c r="D159" t="s">
-        <v>372</v>
+      <c r="B159" s="40" t="s">
+        <v>15</v>
+      </c>
+      <c r="E159" t="s">
+        <v>370</v>
       </c>
     </row>
     <row r="160" spans="1:9" ht="12.75" customHeight="1">
       <c r="A160" s="27"/>
       <c r="B160" t="s">
-        <v>16</v>
-      </c>
-      <c r="C160" t="s">
-        <v>373</v>
+        <v>13</v>
       </c>
       <c r="D160" t="s">
-        <v>374</v>
+        <v>42</v>
       </c>
     </row>
     <row r="161" spans="1:8" ht="12.75" customHeight="1">
       <c r="A161" s="27"/>
       <c r="B161" t="s">
-        <v>13</v>
+        <v>16</v>
+      </c>
+      <c r="C161" t="s">
+        <v>371</v>
       </c>
       <c r="D161" t="s">
-        <v>375</v>
-      </c>
-      <c r="E161" t="s">
-        <v>376</v>
+        <v>372</v>
       </c>
     </row>
     <row r="162" spans="1:8" ht="12.75" customHeight="1">
       <c r="A162" s="27"/>
       <c r="B162" t="s">
-        <v>13</v>
+        <v>16</v>
+      </c>
+      <c r="C162" t="s">
+        <v>373</v>
       </c>
       <c r="D162" t="s">
-        <v>377</v>
-      </c>
-      <c r="E162" t="s">
-        <v>376</v>
+        <v>374</v>
       </c>
     </row>
     <row r="163" spans="1:8" ht="12.75" customHeight="1">
@@ -4976,7 +5042,7 @@
         <v>13</v>
       </c>
       <c r="D163" t="s">
-        <v>378</v>
+        <v>375</v>
       </c>
       <c r="E163" t="s">
         <v>376</v>
@@ -4984,84 +5050,108 @@
     </row>
     <row r="164" spans="1:8" ht="12.75" customHeight="1">
       <c r="A164" s="27"/>
-      <c r="B164" s="41" t="s">
-        <v>23</v>
+      <c r="B164" t="s">
+        <v>13</v>
+      </c>
+      <c r="D164" t="s">
+        <v>377</v>
+      </c>
+      <c r="E164" t="s">
+        <v>376</v>
       </c>
     </row>
     <row r="165" spans="1:8" ht="12.75" customHeight="1">
       <c r="A165" s="27"/>
-      <c r="B165" s="40" t="s">
-        <v>15</v>
+      <c r="B165" t="s">
+        <v>13</v>
+      </c>
+      <c r="D165" t="s">
+        <v>378</v>
       </c>
       <c r="E165" t="s">
-        <v>379</v>
+        <v>376</v>
       </c>
     </row>
     <row r="166" spans="1:8" ht="12.75" customHeight="1">
       <c r="A166" s="27"/>
-      <c r="B166" t="s">
-        <v>13</v>
-      </c>
-      <c r="D166" t="s">
-        <v>99</v>
+      <c r="B166" s="41" t="s">
+        <v>23</v>
       </c>
     </row>
     <row r="167" spans="1:8" ht="12.75" customHeight="1">
       <c r="A167" s="27"/>
-      <c r="B167" t="s">
-        <v>16</v>
-      </c>
-      <c r="C167" t="s">
-        <v>380</v>
-      </c>
-      <c r="D167" t="s">
-        <v>381</v>
+      <c r="B167" s="40" t="s">
+        <v>15</v>
+      </c>
+      <c r="E167" t="s">
+        <v>379</v>
       </c>
     </row>
     <row r="168" spans="1:8" ht="12.75" customHeight="1">
       <c r="A168" s="27"/>
       <c r="B168" t="s">
-        <v>16</v>
-      </c>
-      <c r="C168" t="s">
-        <v>382</v>
+        <v>13</v>
       </c>
       <c r="D168" t="s">
-        <v>383</v>
+        <v>99</v>
       </c>
     </row>
     <row r="169" spans="1:8" ht="12.75" customHeight="1">
       <c r="A169" s="27"/>
       <c r="B169" t="s">
-        <v>13</v>
+        <v>16</v>
+      </c>
+      <c r="C169" t="s">
+        <v>380</v>
       </c>
       <c r="D169" t="s">
-        <v>384</v>
-      </c>
-      <c r="E169" t="s">
-        <v>385</v>
+        <v>381</v>
       </c>
     </row>
     <row r="170" spans="1:8" ht="12.75" customHeight="1">
       <c r="A170" s="27"/>
-      <c r="B170" s="41" t="s">
+      <c r="B170" t="s">
+        <v>16</v>
+      </c>
+      <c r="C170" t="s">
+        <v>382</v>
+      </c>
+      <c r="D170" t="s">
+        <v>383</v>
+      </c>
+    </row>
+    <row r="171" spans="1:8" ht="12.75" customHeight="1">
+      <c r="A171" s="27"/>
+      <c r="B171" t="s">
+        <v>13</v>
+      </c>
+      <c r="D171" t="s">
+        <v>384</v>
+      </c>
+      <c r="E171" t="s">
+        <v>385</v>
+      </c>
+    </row>
+    <row r="172" spans="1:8" ht="12.75" customHeight="1">
+      <c r="A172" s="27"/>
+      <c r="B172" s="41" t="s">
         <v>23</v>
       </c>
     </row>
-    <row r="171" spans="1:8" ht="12.75" customHeight="1">
-      <c r="A171" s="21"/>
-      <c r="B171" s="15" t="s">
+    <row r="173" spans="1:8" ht="12.75" customHeight="1">
+      <c r="A173" s="21"/>
+      <c r="B173" s="15" t="s">
         <v>104</v>
       </c>
-      <c r="C171" s="18"/>
-      <c r="D171" s="18"/>
-      <c r="E171" s="18"/>
-      <c r="F171" s="18"/>
-      <c r="G171" s="18"/>
-      <c r="H171" s="18"/>
-    </row>
-    <row r="174" spans="1:8" ht="12.75" customHeight="1">
-      <c r="B174" s="17" t="s">
+      <c r="C173" s="18"/>
+      <c r="D173" s="18"/>
+      <c r="E173" s="18"/>
+      <c r="F173" s="18"/>
+      <c r="G173" s="18"/>
+      <c r="H173" s="18"/>
+    </row>
+    <row r="176" spans="1:8" ht="12.75" customHeight="1">
+      <c r="B176" s="17" t="s">
         <v>93</v>
       </c>
     </row>
@@ -5278,10 +5368,10 @@
 
 <file path=xl/worksheets/sheet3.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <dimension ref="A1:D129"/>
+  <dimension ref="A1:D136"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A101" workbookViewId="0">
-      <selection activeCell="A122" sqref="A122:XFD128"/>
+    <sheetView topLeftCell="A112" workbookViewId="0">
+      <selection activeCell="C147" sqref="C147"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultColWidth="17.1640625" defaultRowHeight="12.75" customHeight="1" x14ac:dyDescent="0"/>
@@ -5462,15 +5552,15 @@
         <v>425</v>
       </c>
     </row>
-    <row r="19" spans="1:4" ht="12.75" customHeight="1">
-      <c r="A19" t="s">
-        <v>11</v>
-      </c>
-      <c r="B19" t="s">
-        <v>39</v>
-      </c>
-      <c r="C19" t="s">
-        <v>40</v>
+    <row r="18" spans="1:4" ht="12.75" customHeight="1">
+      <c r="A18" t="s">
+        <v>7</v>
+      </c>
+      <c r="B18" t="s">
+        <v>486</v>
+      </c>
+      <c r="C18" t="s">
+        <v>87</v>
       </c>
     </row>
     <row r="20" spans="1:4" ht="12.75" customHeight="1">
@@ -5478,10 +5568,10 @@
         <v>11</v>
       </c>
       <c r="B20" t="s">
-        <v>41</v>
+        <v>39</v>
       </c>
       <c r="C20" t="s">
-        <v>42</v>
+        <v>40</v>
       </c>
     </row>
     <row r="21" spans="1:4" ht="12.75" customHeight="1">
@@ -5489,21 +5579,21 @@
         <v>11</v>
       </c>
       <c r="B21" t="s">
-        <v>395</v>
+        <v>41</v>
       </c>
       <c r="C21" t="s">
-        <v>99</v>
+        <v>42</v>
       </c>
     </row>
     <row r="22" spans="1:4" ht="12.75" customHeight="1">
       <c r="A22" t="s">
-        <v>364</v>
+        <v>11</v>
       </c>
       <c r="B22" t="s">
-        <v>386</v>
+        <v>395</v>
       </c>
       <c r="C22" t="s">
-        <v>387</v>
+        <v>99</v>
       </c>
     </row>
     <row r="23" spans="1:4" ht="12.75" customHeight="1">
@@ -5511,21 +5601,21 @@
         <v>364</v>
       </c>
       <c r="B23" t="s">
+        <v>386</v>
+      </c>
+      <c r="C23" t="s">
+        <v>387</v>
+      </c>
+    </row>
+    <row r="24" spans="1:4" ht="12.75" customHeight="1">
+      <c r="A24" t="s">
+        <v>364</v>
+      </c>
+      <c r="B24" t="s">
         <v>388</v>
       </c>
-      <c r="C23" t="s">
+      <c r="C24" t="s">
         <v>389</v>
-      </c>
-    </row>
-    <row r="25" spans="1:4" ht="12.75" customHeight="1">
-      <c r="A25" t="s">
-        <v>78</v>
-      </c>
-      <c r="B25" t="s">
-        <v>405</v>
-      </c>
-      <c r="C25" t="s">
-        <v>415</v>
       </c>
     </row>
     <row r="26" spans="1:4" ht="12.75" customHeight="1">
@@ -5533,10 +5623,10 @@
         <v>78</v>
       </c>
       <c r="B26" t="s">
-        <v>413</v>
+        <v>405</v>
       </c>
       <c r="C26" t="s">
-        <v>413</v>
+        <v>415</v>
       </c>
     </row>
     <row r="27" spans="1:4" ht="12.75" customHeight="1">
@@ -5544,21 +5634,21 @@
         <v>78</v>
       </c>
       <c r="B27" t="s">
+        <v>413</v>
+      </c>
+      <c r="C27" t="s">
+        <v>413</v>
+      </c>
+    </row>
+    <row r="28" spans="1:4" ht="12.75" customHeight="1">
+      <c r="A28" t="s">
+        <v>78</v>
+      </c>
+      <c r="B28" t="s">
         <v>414</v>
       </c>
-      <c r="C27" t="s">
+      <c r="C28" t="s">
         <v>414</v>
-      </c>
-    </row>
-    <row r="29" spans="1:4" ht="12.75" customHeight="1">
-      <c r="A29" t="s">
-        <v>58</v>
-      </c>
-      <c r="B29" t="s">
-        <v>39</v>
-      </c>
-      <c r="C29" t="s">
-        <v>40</v>
       </c>
     </row>
     <row r="30" spans="1:4" ht="12.75" customHeight="1">
@@ -5566,10 +5656,10 @@
         <v>58</v>
       </c>
       <c r="B30" t="s">
-        <v>41</v>
+        <v>39</v>
       </c>
       <c r="C30" t="s">
-        <v>42</v>
+        <v>40</v>
       </c>
     </row>
     <row r="31" spans="1:4" ht="12.75" customHeight="1">
@@ -5577,21 +5667,21 @@
         <v>58</v>
       </c>
       <c r="B31" t="s">
+        <v>41</v>
+      </c>
+      <c r="C31" t="s">
+        <v>42</v>
+      </c>
+    </row>
+    <row r="32" spans="1:4" ht="12.75" customHeight="1">
+      <c r="A32" t="s">
+        <v>58</v>
+      </c>
+      <c r="B32" t="s">
         <v>395</v>
       </c>
-      <c r="C31" t="s">
+      <c r="C32" t="s">
         <v>99</v>
-      </c>
-    </row>
-    <row r="33" spans="1:4" ht="12.75" customHeight="1">
-      <c r="A33" t="s">
-        <v>43</v>
-      </c>
-      <c r="B33" t="s">
-        <v>44</v>
-      </c>
-      <c r="C33" t="s">
-        <v>45</v>
       </c>
     </row>
     <row r="34" spans="1:4" ht="12.75" customHeight="1">
@@ -5599,21 +5689,21 @@
         <v>43</v>
       </c>
       <c r="B34" t="s">
+        <v>44</v>
+      </c>
+      <c r="C34" t="s">
+        <v>45</v>
+      </c>
+    </row>
+    <row r="35" spans="1:4" ht="12.75" customHeight="1">
+      <c r="A35" t="s">
+        <v>43</v>
+      </c>
+      <c r="B35" t="s">
         <v>46</v>
       </c>
-      <c r="C34" t="s">
+      <c r="C35" t="s">
         <v>47</v>
-      </c>
-    </row>
-    <row r="36" spans="1:4" ht="12.75" customHeight="1">
-      <c r="A36" t="s">
-        <v>439</v>
-      </c>
-      <c r="B36" t="s">
-        <v>114</v>
-      </c>
-      <c r="D36" t="s">
-        <v>115</v>
       </c>
     </row>
     <row r="37" spans="1:4" ht="12.75" customHeight="1">
@@ -5621,10 +5711,10 @@
         <v>439</v>
       </c>
       <c r="B37" t="s">
-        <v>116</v>
+        <v>114</v>
       </c>
       <c r="D37" t="s">
-        <v>120</v>
+        <v>115</v>
       </c>
     </row>
     <row r="38" spans="1:4" ht="12.75" customHeight="1">
@@ -5632,10 +5722,10 @@
         <v>439</v>
       </c>
       <c r="B38" t="s">
-        <v>117</v>
+        <v>116</v>
       </c>
       <c r="D38" t="s">
-        <v>121</v>
+        <v>120</v>
       </c>
     </row>
     <row r="39" spans="1:4" ht="12.75" customHeight="1">
@@ -5643,10 +5733,10 @@
         <v>439</v>
       </c>
       <c r="B39" t="s">
-        <v>118</v>
+        <v>117</v>
       </c>
       <c r="D39" t="s">
-        <v>122</v>
+        <v>121</v>
       </c>
     </row>
     <row r="40" spans="1:4" ht="12.75" customHeight="1">
@@ -5654,43 +5744,43 @@
         <v>439</v>
       </c>
       <c r="B40" t="s">
+        <v>118</v>
+      </c>
+      <c r="D40" t="s">
+        <v>122</v>
+      </c>
+    </row>
+    <row r="41" spans="1:4" ht="12.75" customHeight="1">
+      <c r="A41" t="s">
+        <v>439</v>
+      </c>
+      <c r="B41" t="s">
         <v>119</v>
       </c>
-      <c r="D40" t="s">
+      <c r="D41" t="s">
         <v>123</v>
       </c>
     </row>
-    <row r="42" spans="1:4" ht="12.75" customHeight="1">
-      <c r="A42" t="s">
-        <v>443</v>
-      </c>
-      <c r="B42" t="s">
-        <v>485</v>
-      </c>
-      <c r="D42" t="s">
-        <v>135</v>
-      </c>
-    </row>
-    <row r="43" spans="1:4" s="2" customFormat="1" ht="12.75" customHeight="1">
+    <row r="43" spans="1:4" ht="12.75" customHeight="1">
       <c r="A43" t="s">
         <v>443</v>
       </c>
       <c r="B43" t="s">
-        <v>484</v>
+        <v>485</v>
       </c>
       <c r="D43" t="s">
-        <v>130</v>
-      </c>
-    </row>
-    <row r="44" spans="1:4" ht="12.75" customHeight="1">
+        <v>135</v>
+      </c>
+    </row>
+    <row r="44" spans="1:4" s="2" customFormat="1" ht="12.75" customHeight="1">
       <c r="A44" t="s">
         <v>443</v>
       </c>
       <c r="B44" t="s">
-        <v>483</v>
+        <v>484</v>
       </c>
       <c r="D44" t="s">
-        <v>131</v>
+        <v>130</v>
       </c>
     </row>
     <row r="45" spans="1:4" ht="12.75" customHeight="1">
@@ -5698,10 +5788,10 @@
         <v>443</v>
       </c>
       <c r="B45" t="s">
-        <v>482</v>
+        <v>483</v>
       </c>
       <c r="D45" t="s">
-        <v>132</v>
+        <v>131</v>
       </c>
     </row>
     <row r="46" spans="1:4" ht="12.75" customHeight="1">
@@ -5709,10 +5799,10 @@
         <v>443</v>
       </c>
       <c r="B46" t="s">
-        <v>481</v>
+        <v>482</v>
       </c>
       <c r="D46" t="s">
-        <v>133</v>
+        <v>132</v>
       </c>
     </row>
     <row r="47" spans="1:4" ht="12.75" customHeight="1">
@@ -5720,22 +5810,21 @@
         <v>443</v>
       </c>
       <c r="B47" t="s">
+        <v>481</v>
+      </c>
+      <c r="D47" t="s">
+        <v>133</v>
+      </c>
+    </row>
+    <row r="48" spans="1:4" ht="12.75" customHeight="1">
+      <c r="A48" t="s">
+        <v>443</v>
+      </c>
+      <c r="B48" t="s">
         <v>480</v>
       </c>
-      <c r="D47" t="s">
+      <c r="D48" t="s">
         <v>134</v>
-      </c>
-    </row>
-    <row r="49" spans="1:4" ht="12.75" customHeight="1">
-      <c r="A49" t="s">
-        <v>446</v>
-      </c>
-      <c r="B49" t="s">
-        <v>479</v>
-      </c>
-      <c r="C49" s="2"/>
-      <c r="D49" t="s">
-        <v>136</v>
       </c>
     </row>
     <row r="50" spans="1:4" ht="12.75" customHeight="1">
@@ -5743,10 +5832,11 @@
         <v>446</v>
       </c>
       <c r="B50" t="s">
-        <v>478</v>
-      </c>
+        <v>479</v>
+      </c>
+      <c r="C50" s="2"/>
       <c r="D50" t="s">
-        <v>137</v>
+        <v>136</v>
       </c>
     </row>
     <row r="51" spans="1:4" ht="12.75" customHeight="1">
@@ -5754,10 +5844,10 @@
         <v>446</v>
       </c>
       <c r="B51" t="s">
-        <v>477</v>
+        <v>478</v>
       </c>
       <c r="D51" t="s">
-        <v>138</v>
+        <v>137</v>
       </c>
     </row>
     <row r="52" spans="1:4" ht="12.75" customHeight="1">
@@ -5765,10 +5855,10 @@
         <v>446</v>
       </c>
       <c r="B52" t="s">
-        <v>476</v>
+        <v>477</v>
       </c>
       <c r="D52" t="s">
-        <v>139</v>
+        <v>138</v>
       </c>
     </row>
     <row r="53" spans="1:4" ht="12.75" customHeight="1">
@@ -5776,21 +5866,21 @@
         <v>446</v>
       </c>
       <c r="B53" t="s">
+        <v>476</v>
+      </c>
+      <c r="D53" t="s">
+        <v>139</v>
+      </c>
+    </row>
+    <row r="54" spans="1:4" ht="12.75" customHeight="1">
+      <c r="A54" t="s">
+        <v>446</v>
+      </c>
+      <c r="B54" t="s">
         <v>475</v>
       </c>
-      <c r="D53" t="s">
+      <c r="D54" t="s">
         <v>140</v>
-      </c>
-    </row>
-    <row r="55" spans="1:4" ht="12.75" customHeight="1">
-      <c r="A55" t="s">
-        <v>449</v>
-      </c>
-      <c r="B55" t="s">
-        <v>175</v>
-      </c>
-      <c r="D55" t="s">
-        <v>168</v>
       </c>
     </row>
     <row r="56" spans="1:4" ht="12.75" customHeight="1">
@@ -5798,11 +5888,10 @@
         <v>449</v>
       </c>
       <c r="B56" t="s">
-        <v>176</v>
-      </c>
-      <c r="C56" s="2"/>
+        <v>175</v>
+      </c>
       <c r="D56" t="s">
-        <v>169</v>
+        <v>168</v>
       </c>
     </row>
     <row r="57" spans="1:4" ht="12.75" customHeight="1">
@@ -5810,10 +5899,11 @@
         <v>449</v>
       </c>
       <c r="B57" t="s">
-        <v>177</v>
-      </c>
+        <v>176</v>
+      </c>
+      <c r="C57" s="2"/>
       <c r="D57" t="s">
-        <v>170</v>
+        <v>169</v>
       </c>
     </row>
     <row r="58" spans="1:4" ht="12.75" customHeight="1">
@@ -5821,10 +5911,10 @@
         <v>449</v>
       </c>
       <c r="B58" t="s">
-        <v>178</v>
+        <v>177</v>
       </c>
       <c r="D58" t="s">
-        <v>171</v>
+        <v>170</v>
       </c>
     </row>
     <row r="59" spans="1:4" ht="12.75" customHeight="1">
@@ -5832,10 +5922,10 @@
         <v>449</v>
       </c>
       <c r="B59" t="s">
-        <v>179</v>
+        <v>178</v>
       </c>
       <c r="D59" t="s">
-        <v>172</v>
+        <v>171</v>
       </c>
     </row>
     <row r="60" spans="1:4" ht="12.75" customHeight="1">
@@ -5843,10 +5933,10 @@
         <v>449</v>
       </c>
       <c r="B60" t="s">
-        <v>180</v>
+        <v>179</v>
       </c>
       <c r="D60" t="s">
-        <v>173</v>
+        <v>172</v>
       </c>
     </row>
     <row r="61" spans="1:4" ht="12.75" customHeight="1">
@@ -5854,21 +5944,21 @@
         <v>449</v>
       </c>
       <c r="B61" t="s">
+        <v>180</v>
+      </c>
+      <c r="D61" t="s">
+        <v>173</v>
+      </c>
+    </row>
+    <row r="62" spans="1:4" ht="12.75" customHeight="1">
+      <c r="A62" t="s">
+        <v>449</v>
+      </c>
+      <c r="B62" t="s">
         <v>181</v>
       </c>
-      <c r="D61" t="s">
+      <c r="D62" t="s">
         <v>174</v>
-      </c>
-    </row>
-    <row r="63" spans="1:4" ht="12.75" customHeight="1">
-      <c r="A63" t="s">
-        <v>452</v>
-      </c>
-      <c r="B63" t="s">
-        <v>474</v>
-      </c>
-      <c r="D63" t="s">
-        <v>141</v>
       </c>
     </row>
     <row r="64" spans="1:4" ht="12.75" customHeight="1">
@@ -5876,11 +5966,10 @@
         <v>452</v>
       </c>
       <c r="B64" t="s">
-        <v>473</v>
-      </c>
-      <c r="C64" s="2"/>
+        <v>474</v>
+      </c>
       <c r="D64" t="s">
-        <v>142</v>
+        <v>141</v>
       </c>
     </row>
     <row r="65" spans="1:4" ht="12.75" customHeight="1">
@@ -5888,10 +5977,11 @@
         <v>452</v>
       </c>
       <c r="B65" t="s">
-        <v>472</v>
-      </c>
+        <v>473</v>
+      </c>
+      <c r="C65" s="2"/>
       <c r="D65" t="s">
-        <v>143</v>
+        <v>142</v>
       </c>
     </row>
     <row r="66" spans="1:4" ht="12.75" customHeight="1">
@@ -5899,10 +5989,10 @@
         <v>452</v>
       </c>
       <c r="B66" t="s">
-        <v>471</v>
+        <v>472</v>
       </c>
       <c r="D66" t="s">
-        <v>144</v>
+        <v>143</v>
       </c>
     </row>
     <row r="67" spans="1:4" ht="12.75" customHeight="1">
@@ -5910,10 +6000,10 @@
         <v>452</v>
       </c>
       <c r="B67" t="s">
-        <v>470</v>
+        <v>471</v>
       </c>
       <c r="D67" t="s">
-        <v>145</v>
+        <v>144</v>
       </c>
     </row>
     <row r="68" spans="1:4" ht="12.75" customHeight="1">
@@ -5921,21 +6011,21 @@
         <v>452</v>
       </c>
       <c r="B68" t="s">
+        <v>470</v>
+      </c>
+      <c r="D68" t="s">
+        <v>145</v>
+      </c>
+    </row>
+    <row r="69" spans="1:4" ht="12.75" customHeight="1">
+      <c r="A69" t="s">
+        <v>452</v>
+      </c>
+      <c r="B69" t="s">
         <v>469</v>
       </c>
-      <c r="D68" t="s">
+      <c r="D69" t="s">
         <v>146</v>
-      </c>
-    </row>
-    <row r="70" spans="1:4" ht="12.75" customHeight="1">
-      <c r="A70" t="s">
-        <v>455</v>
-      </c>
-      <c r="B70" t="s">
-        <v>468</v>
-      </c>
-      <c r="D70" t="s">
-        <v>147</v>
       </c>
     </row>
     <row r="71" spans="1:4" ht="12.75" customHeight="1">
@@ -5943,11 +6033,10 @@
         <v>455</v>
       </c>
       <c r="B71" t="s">
-        <v>467</v>
-      </c>
-      <c r="C71" s="2"/>
+        <v>468</v>
+      </c>
       <c r="D71" t="s">
-        <v>148</v>
+        <v>147</v>
       </c>
     </row>
     <row r="72" spans="1:4" ht="12.75" customHeight="1">
@@ -5955,10 +6044,11 @@
         <v>455</v>
       </c>
       <c r="B72" t="s">
-        <v>466</v>
-      </c>
+        <v>467</v>
+      </c>
+      <c r="C72" s="2"/>
       <c r="D72" t="s">
-        <v>149</v>
+        <v>148</v>
       </c>
     </row>
     <row r="73" spans="1:4" ht="12.75" customHeight="1">
@@ -5966,10 +6056,10 @@
         <v>455</v>
       </c>
       <c r="B73" t="s">
-        <v>465</v>
+        <v>466</v>
       </c>
       <c r="D73" t="s">
-        <v>150</v>
+        <v>149</v>
       </c>
     </row>
     <row r="74" spans="1:4" ht="12.75" customHeight="1">
@@ -5977,10 +6067,10 @@
         <v>455</v>
       </c>
       <c r="B74" t="s">
-        <v>464</v>
+        <v>465</v>
       </c>
       <c r="D74" t="s">
-        <v>151</v>
+        <v>150</v>
       </c>
     </row>
     <row r="75" spans="1:4" ht="12.75" customHeight="1">
@@ -5988,21 +6078,21 @@
         <v>455</v>
       </c>
       <c r="B75" t="s">
+        <v>464</v>
+      </c>
+      <c r="D75" t="s">
+        <v>151</v>
+      </c>
+    </row>
+    <row r="76" spans="1:4" ht="12.75" customHeight="1">
+      <c r="A76" t="s">
+        <v>455</v>
+      </c>
+      <c r="B76" t="s">
         <v>463</v>
       </c>
-      <c r="D75" t="s">
+      <c r="D76" t="s">
         <v>152</v>
-      </c>
-    </row>
-    <row r="77" spans="1:4" ht="12.75" customHeight="1">
-      <c r="A77" t="s">
-        <v>192</v>
-      </c>
-      <c r="B77" t="s">
-        <v>198</v>
-      </c>
-      <c r="C77" t="s">
-        <v>205</v>
       </c>
     </row>
     <row r="78" spans="1:4" ht="12.75" customHeight="1">
@@ -6010,10 +6100,10 @@
         <v>192</v>
       </c>
       <c r="B78" t="s">
-        <v>199</v>
+        <v>198</v>
       </c>
       <c r="C78" t="s">
-        <v>206</v>
+        <v>205</v>
       </c>
     </row>
     <row r="79" spans="1:4" ht="12.75" customHeight="1">
@@ -6021,10 +6111,10 @@
         <v>192</v>
       </c>
       <c r="B79" t="s">
-        <v>200</v>
+        <v>199</v>
       </c>
       <c r="C79" t="s">
-        <v>207</v>
+        <v>206</v>
       </c>
     </row>
     <row r="80" spans="1:4" ht="12.75" customHeight="1">
@@ -6032,10 +6122,10 @@
         <v>192</v>
       </c>
       <c r="B80" t="s">
-        <v>201</v>
+        <v>200</v>
       </c>
       <c r="C80" t="s">
-        <v>208</v>
+        <v>207</v>
       </c>
     </row>
     <row r="81" spans="1:3" ht="12.75" customHeight="1">
@@ -6043,10 +6133,10 @@
         <v>192</v>
       </c>
       <c r="B81" t="s">
-        <v>202</v>
+        <v>201</v>
       </c>
       <c r="C81" t="s">
-        <v>209</v>
+        <v>208</v>
       </c>
     </row>
     <row r="82" spans="1:3" ht="12.75" customHeight="1">
@@ -6054,10 +6144,10 @@
         <v>192</v>
       </c>
       <c r="B82" t="s">
-        <v>203</v>
+        <v>202</v>
       </c>
       <c r="C82" t="s">
-        <v>210</v>
+        <v>209</v>
       </c>
     </row>
     <row r="83" spans="1:3" ht="12.75" customHeight="1">
@@ -6065,21 +6155,21 @@
         <v>192</v>
       </c>
       <c r="B83" t="s">
+        <v>203</v>
+      </c>
+      <c r="C83" t="s">
+        <v>210</v>
+      </c>
+    </row>
+    <row r="84" spans="1:3" ht="12.75" customHeight="1">
+      <c r="A84" t="s">
+        <v>192</v>
+      </c>
+      <c r="B84" t="s">
         <v>204</v>
       </c>
-      <c r="C83" t="s">
+      <c r="C84" t="s">
         <v>211</v>
-      </c>
-    </row>
-    <row r="85" spans="1:3" ht="12.75" customHeight="1">
-      <c r="A85" t="s">
-        <v>193</v>
-      </c>
-      <c r="B85" t="s">
-        <v>218</v>
-      </c>
-      <c r="C85" t="s">
-        <v>224</v>
       </c>
     </row>
     <row r="86" spans="1:3" ht="12.75" customHeight="1">
@@ -6087,10 +6177,10 @@
         <v>193</v>
       </c>
       <c r="B86" t="s">
-        <v>219</v>
+        <v>218</v>
       </c>
       <c r="C86" t="s">
-        <v>225</v>
+        <v>224</v>
       </c>
     </row>
     <row r="87" spans="1:3" ht="12.75" customHeight="1">
@@ -6098,10 +6188,10 @@
         <v>193</v>
       </c>
       <c r="B87" t="s">
-        <v>220</v>
+        <v>219</v>
       </c>
       <c r="C87" t="s">
-        <v>226</v>
+        <v>225</v>
       </c>
     </row>
     <row r="88" spans="1:3" ht="12.75" customHeight="1">
@@ -6109,10 +6199,10 @@
         <v>193</v>
       </c>
       <c r="B88" t="s">
-        <v>221</v>
+        <v>220</v>
       </c>
       <c r="C88" t="s">
-        <v>227</v>
+        <v>226</v>
       </c>
     </row>
     <row r="89" spans="1:3" ht="12.75" customHeight="1">
@@ -6120,10 +6210,10 @@
         <v>193</v>
       </c>
       <c r="B89" t="s">
-        <v>222</v>
+        <v>221</v>
       </c>
       <c r="C89" t="s">
-        <v>228</v>
+        <v>227</v>
       </c>
     </row>
     <row r="90" spans="1:3" ht="12.75" customHeight="1">
@@ -6131,21 +6221,21 @@
         <v>193</v>
       </c>
       <c r="B90" t="s">
+        <v>222</v>
+      </c>
+      <c r="C90" t="s">
+        <v>228</v>
+      </c>
+    </row>
+    <row r="91" spans="1:3" ht="12.75" customHeight="1">
+      <c r="A91" t="s">
+        <v>193</v>
+      </c>
+      <c r="B91" t="s">
         <v>223</v>
       </c>
-      <c r="C90" t="s">
+      <c r="C91" t="s">
         <v>229</v>
-      </c>
-    </row>
-    <row r="92" spans="1:3" ht="12.75" customHeight="1">
-      <c r="A92" t="s">
-        <v>194</v>
-      </c>
-      <c r="B92" t="s">
-        <v>236</v>
-      </c>
-      <c r="C92" t="s">
-        <v>237</v>
       </c>
     </row>
     <row r="93" spans="1:3" ht="12.75" customHeight="1">
@@ -6153,10 +6243,10 @@
         <v>194</v>
       </c>
       <c r="B93" t="s">
-        <v>230</v>
+        <v>236</v>
       </c>
       <c r="C93" t="s">
-        <v>238</v>
+        <v>237</v>
       </c>
     </row>
     <row r="94" spans="1:3" ht="12.75" customHeight="1">
@@ -6164,10 +6254,10 @@
         <v>194</v>
       </c>
       <c r="B94" t="s">
-        <v>231</v>
+        <v>230</v>
       </c>
       <c r="C94" t="s">
-        <v>239</v>
+        <v>238</v>
       </c>
     </row>
     <row r="95" spans="1:3" ht="12.75" customHeight="1">
@@ -6175,10 +6265,10 @@
         <v>194</v>
       </c>
       <c r="B95" t="s">
-        <v>232</v>
+        <v>231</v>
       </c>
       <c r="C95" t="s">
-        <v>240</v>
+        <v>239</v>
       </c>
     </row>
     <row r="96" spans="1:3" ht="12.75" customHeight="1">
@@ -6186,10 +6276,10 @@
         <v>194</v>
       </c>
       <c r="B96" t="s">
-        <v>233</v>
+        <v>232</v>
       </c>
       <c r="C96" t="s">
-        <v>241</v>
+        <v>240</v>
       </c>
     </row>
     <row r="97" spans="1:3" ht="12.75" customHeight="1">
@@ -6197,10 +6287,10 @@
         <v>194</v>
       </c>
       <c r="B97" t="s">
-        <v>234</v>
+        <v>233</v>
       </c>
       <c r="C97" t="s">
-        <v>242</v>
+        <v>241</v>
       </c>
     </row>
     <row r="98" spans="1:3" ht="12.75" customHeight="1">
@@ -6208,21 +6298,21 @@
         <v>194</v>
       </c>
       <c r="B98" t="s">
+        <v>234</v>
+      </c>
+      <c r="C98" t="s">
+        <v>242</v>
+      </c>
+    </row>
+    <row r="99" spans="1:3" ht="12.75" customHeight="1">
+      <c r="A99" t="s">
+        <v>194</v>
+      </c>
+      <c r="B99" t="s">
         <v>235</v>
       </c>
-      <c r="C98" t="s">
+      <c r="C99" t="s">
         <v>243</v>
-      </c>
-    </row>
-    <row r="100" spans="1:3" ht="12.75" customHeight="1">
-      <c r="A100" t="s">
-        <v>195</v>
-      </c>
-      <c r="B100" t="s">
-        <v>244</v>
-      </c>
-      <c r="C100" t="s">
-        <v>250</v>
       </c>
     </row>
     <row r="101" spans="1:3" ht="12.75" customHeight="1">
@@ -6230,10 +6320,10 @@
         <v>195</v>
       </c>
       <c r="B101" t="s">
-        <v>245</v>
+        <v>244</v>
       </c>
       <c r="C101" t="s">
-        <v>251</v>
+        <v>250</v>
       </c>
     </row>
     <row r="102" spans="1:3" ht="12.75" customHeight="1">
@@ -6241,10 +6331,10 @@
         <v>195</v>
       </c>
       <c r="B102" t="s">
-        <v>246</v>
+        <v>245</v>
       </c>
       <c r="C102" t="s">
-        <v>252</v>
+        <v>251</v>
       </c>
     </row>
     <row r="103" spans="1:3" ht="12.75" customHeight="1">
@@ -6252,10 +6342,10 @@
         <v>195</v>
       </c>
       <c r="B103" t="s">
-        <v>247</v>
+        <v>246</v>
       </c>
       <c r="C103" t="s">
-        <v>253</v>
+        <v>252</v>
       </c>
     </row>
     <row r="104" spans="1:3" ht="12.75" customHeight="1">
@@ -6263,10 +6353,10 @@
         <v>195</v>
       </c>
       <c r="B104" t="s">
-        <v>248</v>
+        <v>247</v>
       </c>
       <c r="C104" t="s">
-        <v>254</v>
+        <v>253</v>
       </c>
     </row>
     <row r="105" spans="1:3" ht="12.75" customHeight="1">
@@ -6274,21 +6364,21 @@
         <v>195</v>
       </c>
       <c r="B105" t="s">
+        <v>248</v>
+      </c>
+      <c r="C105" t="s">
+        <v>254</v>
+      </c>
+    </row>
+    <row r="106" spans="1:3" ht="12.75" customHeight="1">
+      <c r="A106" t="s">
+        <v>195</v>
+      </c>
+      <c r="B106" t="s">
         <v>249</v>
       </c>
-      <c r="C105" t="s">
+      <c r="C106" t="s">
         <v>255</v>
-      </c>
-    </row>
-    <row r="107" spans="1:3" ht="12.75" customHeight="1">
-      <c r="A107" t="s">
-        <v>196</v>
-      </c>
-      <c r="B107" t="s">
-        <v>262</v>
-      </c>
-      <c r="C107" t="s">
-        <v>263</v>
       </c>
     </row>
     <row r="108" spans="1:3" ht="12.75" customHeight="1">
@@ -6296,10 +6386,10 @@
         <v>196</v>
       </c>
       <c r="B108" t="s">
-        <v>256</v>
+        <v>262</v>
       </c>
       <c r="C108" t="s">
-        <v>264</v>
+        <v>263</v>
       </c>
     </row>
     <row r="109" spans="1:3" ht="12.75" customHeight="1">
@@ -6307,10 +6397,10 @@
         <v>196</v>
       </c>
       <c r="B109" t="s">
-        <v>257</v>
+        <v>256</v>
       </c>
       <c r="C109" t="s">
-        <v>265</v>
+        <v>264</v>
       </c>
     </row>
     <row r="110" spans="1:3" ht="12.75" customHeight="1">
@@ -6318,10 +6408,10 @@
         <v>196</v>
       </c>
       <c r="B110" t="s">
-        <v>259</v>
+        <v>257</v>
       </c>
       <c r="C110" t="s">
-        <v>266</v>
+        <v>265</v>
       </c>
     </row>
     <row r="111" spans="1:3" ht="12.75" customHeight="1">
@@ -6329,10 +6419,10 @@
         <v>196</v>
       </c>
       <c r="B111" t="s">
-        <v>258</v>
+        <v>259</v>
       </c>
       <c r="C111" t="s">
-        <v>267</v>
+        <v>266</v>
       </c>
     </row>
     <row r="112" spans="1:3" ht="12.75" customHeight="1">
@@ -6340,10 +6430,10 @@
         <v>196</v>
       </c>
       <c r="B112" t="s">
-        <v>260</v>
+        <v>258</v>
       </c>
       <c r="C112" t="s">
-        <v>268</v>
+        <v>267</v>
       </c>
     </row>
     <row r="113" spans="1:4" ht="12.75" customHeight="1">
@@ -6351,21 +6441,21 @@
         <v>196</v>
       </c>
       <c r="B113" t="s">
+        <v>260</v>
+      </c>
+      <c r="C113" t="s">
+        <v>268</v>
+      </c>
+    </row>
+    <row r="114" spans="1:4" ht="12.75" customHeight="1">
+      <c r="A114" t="s">
+        <v>196</v>
+      </c>
+      <c r="B114" t="s">
         <v>261</v>
       </c>
-      <c r="C113" t="s">
+      <c r="C114" t="s">
         <v>269</v>
-      </c>
-    </row>
-    <row r="115" spans="1:4" ht="12.75" customHeight="1">
-      <c r="A115" t="s">
-        <v>197</v>
-      </c>
-      <c r="B115" t="s">
-        <v>270</v>
-      </c>
-      <c r="C115" t="s">
-        <v>276</v>
       </c>
     </row>
     <row r="116" spans="1:4" ht="12.75" customHeight="1">
@@ -6373,10 +6463,10 @@
         <v>197</v>
       </c>
       <c r="B116" t="s">
-        <v>271</v>
+        <v>270</v>
       </c>
       <c r="C116" t="s">
-        <v>277</v>
+        <v>276</v>
       </c>
     </row>
     <row r="117" spans="1:4" ht="12.75" customHeight="1">
@@ -6384,10 +6474,10 @@
         <v>197</v>
       </c>
       <c r="B117" t="s">
-        <v>272</v>
+        <v>271</v>
       </c>
       <c r="C117" t="s">
-        <v>278</v>
+        <v>277</v>
       </c>
     </row>
     <row r="118" spans="1:4" ht="12.75" customHeight="1">
@@ -6395,10 +6485,10 @@
         <v>197</v>
       </c>
       <c r="B118" t="s">
-        <v>273</v>
+        <v>272</v>
       </c>
       <c r="C118" t="s">
-        <v>279</v>
+        <v>278</v>
       </c>
     </row>
     <row r="119" spans="1:4" ht="12.75" customHeight="1">
@@ -6406,10 +6496,10 @@
         <v>197</v>
       </c>
       <c r="B119" t="s">
-        <v>274</v>
+        <v>273</v>
       </c>
       <c r="C119" t="s">
-        <v>280</v>
+        <v>279</v>
       </c>
     </row>
     <row r="120" spans="1:4" ht="12.75" customHeight="1">
@@ -6417,21 +6507,21 @@
         <v>197</v>
       </c>
       <c r="B120" t="s">
+        <v>274</v>
+      </c>
+      <c r="C120" t="s">
+        <v>280</v>
+      </c>
+    </row>
+    <row r="121" spans="1:4" ht="12.75" customHeight="1">
+      <c r="A121" t="s">
+        <v>197</v>
+      </c>
+      <c r="B121" t="s">
         <v>275</v>
       </c>
-      <c r="C120" t="s">
+      <c r="C121" t="s">
         <v>281</v>
-      </c>
-    </row>
-    <row r="122" spans="1:4" ht="12.75" customHeight="1">
-      <c r="A122" t="s">
-        <v>335</v>
-      </c>
-      <c r="B122" t="s">
-        <v>330</v>
-      </c>
-      <c r="C122" t="s">
-        <v>324</v>
       </c>
     </row>
     <row r="123" spans="1:4" ht="12.75" customHeight="1">
@@ -6439,34 +6529,37 @@
         <v>335</v>
       </c>
       <c r="B123" t="s">
+        <v>330</v>
+      </c>
+      <c r="C123" t="s">
+        <v>324</v>
+      </c>
+    </row>
+    <row r="124" spans="1:4" ht="12.75" customHeight="1">
+      <c r="A124" t="s">
+        <v>335</v>
+      </c>
+      <c r="B124" t="s">
         <v>331</v>
       </c>
-      <c r="C123" t="s">
+      <c r="C124" t="s">
         <v>332</v>
       </c>
     </row>
-    <row r="125" spans="1:4" ht="12.75" customHeight="1">
-      <c r="A125" s="2" t="s">
+    <row r="126" spans="1:4" ht="12.75" customHeight="1">
+      <c r="A126" s="2" t="s">
         <v>428</v>
       </c>
-      <c r="D125" t="s">
+      <c r="D126" t="s">
         <v>429</v>
       </c>
     </row>
-    <row r="126" spans="1:4" ht="12.75" customHeight="1">
-      <c r="A126" t="s">
+    <row r="127" spans="1:4" ht="12.75" customHeight="1">
+      <c r="A127" t="s">
         <v>428</v>
       </c>
-      <c r="D126" t="s">
+      <c r="D127" t="s">
         <v>430</v>
-      </c>
-    </row>
-    <row r="127" spans="1:4" ht="12.75" customHeight="1">
-      <c r="A127" s="2" t="s">
-        <v>428</v>
-      </c>
-      <c r="D127" t="s">
-        <v>431</v>
       </c>
     </row>
     <row r="128" spans="1:4" ht="12.75" customHeight="1">
@@ -6474,7 +6567,7 @@
         <v>428</v>
       </c>
       <c r="D128" t="s">
-        <v>432</v>
+        <v>431</v>
       </c>
     </row>
     <row r="129" spans="1:4" ht="12.75" customHeight="1">
@@ -6482,7 +6575,55 @@
         <v>428</v>
       </c>
       <c r="D129" t="s">
+        <v>432</v>
+      </c>
+    </row>
+    <row r="130" spans="1:4" ht="12.75" customHeight="1">
+      <c r="A130" s="2" t="s">
+        <v>428</v>
+      </c>
+      <c r="D130" t="s">
         <v>433</v>
+      </c>
+    </row>
+    <row r="132" spans="1:4" ht="12.75" customHeight="1">
+      <c r="A132" t="s">
+        <v>487</v>
+      </c>
+      <c r="D132" t="s">
+        <v>488</v>
+      </c>
+    </row>
+    <row r="133" spans="1:4" ht="12.75" customHeight="1">
+      <c r="A133" t="s">
+        <v>487</v>
+      </c>
+      <c r="D133" t="s">
+        <v>489</v>
+      </c>
+    </row>
+    <row r="134" spans="1:4" ht="12.75" customHeight="1">
+      <c r="A134" t="s">
+        <v>487</v>
+      </c>
+      <c r="D134" t="s">
+        <v>490</v>
+      </c>
+    </row>
+    <row r="135" spans="1:4" ht="12.75" customHeight="1">
+      <c r="A135" t="s">
+        <v>487</v>
+      </c>
+      <c r="D135" t="s">
+        <v>491</v>
+      </c>
+    </row>
+    <row r="136" spans="1:4" ht="12.75" customHeight="1">
+      <c r="A136" t="s">
+        <v>487</v>
+      </c>
+      <c r="D136" t="s">
+        <v>492</v>
       </c>
     </row>
   </sheetData>

</xml_diff>

<commit_message>
remove label in diagnostics
</commit_message>
<xml_diff>
--- a/opendatakit.collect2/form-files/neonatal/neonatal.xlsx
+++ b/opendatakit.collect2/form-files/neonatal/neonatal.xlsx
@@ -4,7 +4,7 @@
   <fileVersion appName="xl" lastEdited="5" lowestEdited="5" rupBuild="22905"/>
   <workbookPr autoCompressPictures="0"/>
   <bookViews>
-    <workbookView xWindow="0" yWindow="0" windowWidth="21640" windowHeight="15560" tabRatio="500"/>
+    <workbookView xWindow="0" yWindow="0" windowWidth="21640" windowHeight="15560" tabRatio="500" activeTab="2"/>
   </bookViews>
   <sheets>
     <sheet name="survey" sheetId="1" r:id="rId1"/>
@@ -23,7 +23,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="788" uniqueCount="497">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="783" uniqueCount="493">
   <si>
     <t>type</t>
   </si>
@@ -139,9 +139,6 @@
     <t>head</t>
   </si>
   <si>
-    <t>Head UltraSound</t>
-  </si>
-  <si>
     <t>weight_converter</t>
   </si>
   <si>
@@ -241,9 +238,6 @@
     <t>video/video.mp4</t>
   </si>
   <si>
-    <t>Ballard Exam</t>
-  </si>
-  <si>
     <t>label procedures_end</t>
   </si>
   <si>
@@ -275,9 +269,6 @@
   </si>
   <si>
     <t>xray</t>
-  </si>
-  <si>
-    <t>Chest &amp; Abnormal Xray</t>
   </si>
   <si>
     <t>placement</t>
@@ -1506,9 +1497,6 @@
   </si>
   <si>
     <t>head_cornal</t>
-  </si>
-  <si>
-    <t>Head Coronal</t>
   </si>
   <si>
     <t>headultra_slider</t>
@@ -3152,7 +3140,7 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:J176"/>
   <sheetViews>
-    <sheetView tabSelected="1" zoomScale="150" zoomScaleNormal="150" zoomScalePageLayoutView="150" workbookViewId="0">
+    <sheetView zoomScale="150" zoomScaleNormal="150" zoomScalePageLayoutView="150" workbookViewId="0">
       <pane ySplit="1" topLeftCell="A2" activePane="bottomLeft" state="frozen"/>
       <selection pane="bottomLeft" activeCell="D11" sqref="D11"/>
     </sheetView>
@@ -3168,7 +3156,7 @@
   <sheetData>
     <row r="1" spans="1:9" ht="12">
       <c r="A1" t="s">
-        <v>302</v>
+        <v>299</v>
       </c>
       <c r="B1" s="1" t="s">
         <v>0</v>
@@ -3183,21 +3171,21 @@
         <v>3</v>
       </c>
       <c r="F1" s="2" t="s">
+        <v>53</v>
+      </c>
+      <c r="G1" t="s">
         <v>54</v>
       </c>
-      <c r="G1" t="s">
-        <v>55</v>
-      </c>
       <c r="H1" t="s">
-        <v>63</v>
+        <v>62</v>
       </c>
       <c r="I1" t="s">
-        <v>361</v>
+        <v>358</v>
       </c>
     </row>
     <row r="2" spans="1:9" ht="15">
       <c r="B2" s="16" t="s">
-        <v>92</v>
+        <v>89</v>
       </c>
       <c r="C2" s="1"/>
       <c r="D2" s="3"/>
@@ -3206,7 +3194,7 @@
     </row>
     <row r="3" spans="1:9" ht="12">
       <c r="B3" s="3" t="s">
-        <v>153</v>
+        <v>150</v>
       </c>
       <c r="C3" s="4" t="s">
         <v>4</v>
@@ -3231,12 +3219,12 @@
         <v>8</v>
       </c>
       <c r="B5" s="19" t="s">
-        <v>298</v>
+        <v>295</v>
       </c>
       <c r="C5" s="19"/>
       <c r="D5" s="19"/>
       <c r="E5" s="19" t="s">
-        <v>299</v>
+        <v>296</v>
       </c>
       <c r="F5" s="19"/>
       <c r="G5" s="19"/>
@@ -3245,12 +3233,12 @@
     <row r="6" spans="1:9" ht="12.75" customHeight="1">
       <c r="A6" s="21"/>
       <c r="B6" s="19" t="s">
-        <v>300</v>
+        <v>297</v>
       </c>
       <c r="C6" s="19"/>
       <c r="D6" s="19"/>
       <c r="E6" s="19" t="s">
-        <v>301</v>
+        <v>298</v>
       </c>
       <c r="F6" s="19"/>
       <c r="G6" s="19"/>
@@ -3259,7 +3247,7 @@
     <row r="7" spans="1:9" s="12" customFormat="1" ht="18" customHeight="1">
       <c r="A7" s="22"/>
       <c r="B7" s="18" t="s">
-        <v>94</v>
+        <v>91</v>
       </c>
       <c r="C7" s="18"/>
       <c r="D7" s="18"/>
@@ -3271,7 +3259,7 @@
     <row r="8" spans="1:9" s="12" customFormat="1" ht="18" customHeight="1">
       <c r="A8" s="22"/>
       <c r="B8" t="s">
-        <v>154</v>
+        <v>151</v>
       </c>
       <c r="C8" t="s">
         <v>7</v>
@@ -3287,35 +3275,35 @@
     <row r="9" spans="1:9" ht="18" customHeight="1">
       <c r="A9" s="21"/>
       <c r="B9" s="2" t="s">
-        <v>434</v>
+        <v>430</v>
       </c>
       <c r="C9" s="2" t="s">
-        <v>428</v>
+        <v>424</v>
       </c>
       <c r="D9" s="2" t="s">
-        <v>87</v>
+        <v>84</v>
       </c>
       <c r="E9" s="2" t="s">
-        <v>105</v>
+        <v>102</v>
       </c>
       <c r="F9" s="2"/>
       <c r="G9" t="s">
-        <v>107</v>
+        <v>104</v>
       </c>
     </row>
     <row r="10" spans="1:9" ht="29" customHeight="1">
       <c r="A10" s="21"/>
       <c r="B10" s="2" t="s">
-        <v>496</v>
+        <v>492</v>
       </c>
       <c r="C10" s="2" t="s">
-        <v>487</v>
+        <v>483</v>
       </c>
       <c r="D10" s="2" t="s">
-        <v>87</v>
+        <v>84</v>
       </c>
       <c r="E10" s="2" t="s">
-        <v>495</v>
+        <v>491</v>
       </c>
       <c r="F10" s="2"/>
     </row>
@@ -3326,255 +3314,255 @@
       </c>
       <c r="C11" s="2"/>
       <c r="D11" s="2" t="s">
-        <v>493</v>
+        <v>489</v>
       </c>
       <c r="E11" s="2" t="s">
-        <v>494</v>
+        <v>490</v>
       </c>
       <c r="F11" s="2"/>
     </row>
     <row r="12" spans="1:9" ht="18" customHeight="1">
       <c r="A12" s="21"/>
       <c r="B12" s="2" t="s">
-        <v>88</v>
+        <v>85</v>
       </c>
       <c r="C12" s="4"/>
       <c r="D12" s="2" t="s">
-        <v>86</v>
+        <v>83</v>
       </c>
       <c r="E12" s="2" t="s">
-        <v>108</v>
+        <v>105</v>
       </c>
       <c r="F12" s="2"/>
     </row>
     <row r="13" spans="1:9" ht="18" customHeight="1">
       <c r="A13" s="21"/>
       <c r="B13" s="2" t="s">
-        <v>88</v>
+        <v>85</v>
       </c>
       <c r="C13" s="4"/>
       <c r="D13" s="2" t="s">
-        <v>89</v>
+        <v>86</v>
       </c>
       <c r="E13" s="2" t="s">
-        <v>106</v>
+        <v>103</v>
       </c>
       <c r="F13" s="2"/>
     </row>
     <row r="14" spans="1:9" ht="12">
       <c r="A14" s="21"/>
       <c r="B14" t="s">
-        <v>435</v>
+        <v>431</v>
       </c>
       <c r="C14" t="s">
-        <v>436</v>
+        <v>432</v>
       </c>
       <c r="E14" s="2" t="s">
-        <v>437</v>
+        <v>433</v>
       </c>
     </row>
     <row r="15" spans="1:9" ht="11" customHeight="1">
       <c r="A15" s="21"/>
       <c r="B15" t="s">
-        <v>438</v>
+        <v>434</v>
       </c>
       <c r="C15" t="s">
-        <v>439</v>
+        <v>435</v>
       </c>
       <c r="D15" t="s">
-        <v>112</v>
+        <v>109</v>
       </c>
       <c r="E15" s="2" t="s">
-        <v>440</v>
+        <v>436</v>
       </c>
       <c r="F15" t="s">
-        <v>441</v>
+        <v>437</v>
       </c>
     </row>
     <row r="16" spans="1:9" ht="11" customHeight="1">
       <c r="A16" s="21"/>
       <c r="B16" t="s">
-        <v>442</v>
+        <v>438</v>
       </c>
       <c r="C16" t="s">
-        <v>443</v>
+        <v>439</v>
       </c>
       <c r="D16" t="s">
-        <v>113</v>
+        <v>110</v>
       </c>
       <c r="E16" s="2" t="s">
-        <v>444</v>
+        <v>440</v>
       </c>
       <c r="F16" t="s">
-        <v>441</v>
+        <v>437</v>
       </c>
     </row>
     <row r="17" spans="1:10" ht="11" customHeight="1">
       <c r="A17" s="21"/>
       <c r="B17" t="s">
-        <v>445</v>
+        <v>441</v>
       </c>
       <c r="C17" t="s">
-        <v>446</v>
+        <v>442</v>
       </c>
       <c r="D17" t="s">
-        <v>127</v>
+        <v>124</v>
       </c>
       <c r="E17" s="2" t="s">
-        <v>447</v>
+        <v>443</v>
       </c>
       <c r="F17" t="s">
-        <v>441</v>
+        <v>437</v>
       </c>
     </row>
     <row r="18" spans="1:10" ht="11" customHeight="1">
       <c r="A18" s="21"/>
       <c r="B18" t="s">
-        <v>448</v>
+        <v>444</v>
       </c>
       <c r="C18" t="s">
-        <v>449</v>
+        <v>445</v>
       </c>
       <c r="D18" t="s">
-        <v>163</v>
+        <v>160</v>
       </c>
       <c r="E18" s="2" t="s">
-        <v>450</v>
+        <v>446</v>
       </c>
       <c r="F18" t="s">
-        <v>441</v>
+        <v>437</v>
       </c>
     </row>
     <row r="19" spans="1:10" ht="11" customHeight="1">
       <c r="A19" s="21"/>
       <c r="B19" t="s">
-        <v>451</v>
+        <v>447</v>
       </c>
       <c r="C19" t="s">
-        <v>452</v>
+        <v>448</v>
       </c>
       <c r="D19" t="s">
-        <v>128</v>
+        <v>125</v>
       </c>
       <c r="E19" s="2" t="s">
-        <v>453</v>
+        <v>449</v>
       </c>
       <c r="F19" t="s">
-        <v>441</v>
+        <v>437</v>
       </c>
     </row>
     <row r="20" spans="1:10" ht="11" customHeight="1">
       <c r="A20" s="21"/>
       <c r="B20" t="s">
-        <v>454</v>
+        <v>450</v>
       </c>
       <c r="C20" t="s">
-        <v>455</v>
+        <v>451</v>
       </c>
       <c r="D20" t="s">
-        <v>129</v>
+        <v>126</v>
       </c>
       <c r="E20" s="2" t="s">
-        <v>456</v>
+        <v>452</v>
       </c>
       <c r="F20" t="s">
-        <v>441</v>
+        <v>437</v>
       </c>
     </row>
     <row r="21" spans="1:10" ht="11" customHeight="1">
       <c r="A21" s="21"/>
       <c r="B21" t="s">
-        <v>212</v>
+        <v>209</v>
       </c>
       <c r="C21" t="s">
-        <v>192</v>
+        <v>189</v>
       </c>
       <c r="D21" t="s">
-        <v>186</v>
+        <v>183</v>
       </c>
       <c r="E21" s="2" t="s">
-        <v>457</v>
+        <v>453</v>
       </c>
     </row>
     <row r="22" spans="1:10" ht="11" customHeight="1">
       <c r="A22" s="21"/>
       <c r="B22" t="s">
-        <v>213</v>
+        <v>210</v>
       </c>
       <c r="C22" t="s">
-        <v>193</v>
+        <v>190</v>
       </c>
       <c r="D22" t="s">
-        <v>187</v>
+        <v>184</v>
       </c>
       <c r="E22" s="2" t="s">
-        <v>458</v>
+        <v>454</v>
       </c>
     </row>
     <row r="23" spans="1:10" ht="11" customHeight="1">
       <c r="A23" s="21"/>
       <c r="B23" t="s">
-        <v>214</v>
+        <v>211</v>
       </c>
       <c r="C23" t="s">
-        <v>194</v>
+        <v>191</v>
       </c>
       <c r="D23" t="s">
-        <v>190</v>
+        <v>187</v>
       </c>
       <c r="E23" s="2" t="s">
-        <v>459</v>
+        <v>455</v>
       </c>
     </row>
     <row r="24" spans="1:10" ht="11" customHeight="1">
       <c r="A24" s="21"/>
       <c r="B24" t="s">
-        <v>215</v>
+        <v>212</v>
       </c>
       <c r="C24" t="s">
-        <v>195</v>
+        <v>192</v>
       </c>
       <c r="D24" t="s">
-        <v>188</v>
+        <v>185</v>
       </c>
       <c r="E24" s="2" t="s">
-        <v>460</v>
+        <v>456</v>
       </c>
     </row>
     <row r="25" spans="1:10" ht="11" customHeight="1">
       <c r="A25" s="21"/>
       <c r="B25" t="s">
-        <v>216</v>
+        <v>213</v>
       </c>
       <c r="C25" t="s">
-        <v>196</v>
+        <v>193</v>
       </c>
       <c r="D25" t="s">
-        <v>189</v>
+        <v>186</v>
       </c>
       <c r="E25" s="2" t="s">
-        <v>461</v>
+        <v>457</v>
       </c>
     </row>
     <row r="26" spans="1:10" ht="12" customHeight="1">
       <c r="A26" s="21"/>
       <c r="B26" t="s">
-        <v>217</v>
+        <v>214</v>
       </c>
       <c r="C26" t="s">
-        <v>197</v>
+        <v>194</v>
       </c>
       <c r="D26" t="s">
-        <v>191</v>
+        <v>188</v>
       </c>
       <c r="E26" s="2" t="s">
-        <v>462</v>
+        <v>458</v>
       </c>
     </row>
     <row r="27" spans="1:10" ht="15">
       <c r="A27" s="21"/>
       <c r="B27" s="15" t="s">
-        <v>65</v>
+        <v>64</v>
       </c>
       <c r="C27" s="15"/>
       <c r="D27" s="15"/>
@@ -3594,15 +3582,15 @@
     </row>
     <row r="29" spans="1:10" s="15" customFormat="1" ht="15">
       <c r="A29" s="21" t="s">
-        <v>322</v>
+        <v>319</v>
       </c>
       <c r="B29" s="13" t="s">
-        <v>91</v>
+        <v>88</v>
       </c>
       <c r="C29" s="13"/>
       <c r="D29" s="13"/>
       <c r="E29" s="13" t="s">
-        <v>64</v>
+        <v>63</v>
       </c>
       <c r="F29" s="13"/>
       <c r="G29" s="13"/>
@@ -3613,12 +3601,12 @@
     <row r="30" spans="1:10" ht="12">
       <c r="A30" s="21"/>
       <c r="B30" s="5" t="s">
-        <v>66</v>
+        <v>65</v>
       </c>
       <c r="C30" s="5"/>
       <c r="D30" s="5"/>
       <c r="E30" s="6" t="s">
-        <v>67</v>
+        <v>66</v>
       </c>
       <c r="F30" s="5"/>
       <c r="G30" s="5"/>
@@ -3627,7 +3615,7 @@
     <row r="31" spans="1:10" ht="15">
       <c r="A31" s="21"/>
       <c r="B31" s="15" t="s">
-        <v>90</v>
+        <v>87</v>
       </c>
       <c r="C31" s="15"/>
       <c r="D31" s="15"/>
@@ -3639,7 +3627,7 @@
     <row r="32" spans="1:10" ht="12">
       <c r="A32" s="21"/>
       <c r="B32" s="12" t="s">
-        <v>155</v>
+        <v>152</v>
       </c>
       <c r="C32" s="12" t="s">
         <v>9</v>
@@ -3662,7 +3650,7 @@
       <c r="C33" s="8"/>
       <c r="D33" s="8"/>
       <c r="E33" s="9" t="s">
-        <v>56</v>
+        <v>55</v>
       </c>
       <c r="F33" s="8"/>
       <c r="G33" s="10"/>
@@ -3674,10 +3662,10 @@
         <v>13</v>
       </c>
       <c r="C34" s="2" t="s">
-        <v>68</v>
+        <v>67</v>
       </c>
       <c r="D34" s="2" t="s">
-        <v>303</v>
+        <v>300</v>
       </c>
       <c r="E34" s="2"/>
       <c r="F34" s="4"/>
@@ -3688,7 +3676,7 @@
         <v>13</v>
       </c>
       <c r="D35" t="s">
-        <v>304</v>
+        <v>301</v>
       </c>
       <c r="E35" s="2"/>
       <c r="F35" s="4"/>
@@ -3700,7 +3688,7 @@
       </c>
       <c r="C36" s="2"/>
       <c r="D36" s="2" t="s">
-        <v>305</v>
+        <v>302</v>
       </c>
       <c r="E36" s="2"/>
       <c r="F36" s="4"/>
@@ -3712,7 +3700,7 @@
       </c>
       <c r="C37" s="2"/>
       <c r="D37" s="2" t="s">
-        <v>306</v>
+        <v>303</v>
       </c>
       <c r="E37" s="2"/>
       <c r="F37" s="4"/>
@@ -3724,7 +3712,7 @@
       </c>
       <c r="C38" s="2"/>
       <c r="D38" s="2" t="s">
-        <v>307</v>
+        <v>304</v>
       </c>
       <c r="E38" s="2"/>
       <c r="F38" s="4"/>
@@ -3736,7 +3724,7 @@
       </c>
       <c r="C39" s="2"/>
       <c r="D39" s="2" t="s">
-        <v>308</v>
+        <v>305</v>
       </c>
       <c r="E39" s="2"/>
       <c r="F39" s="4"/>
@@ -3748,7 +3736,7 @@
       </c>
       <c r="C40" s="2"/>
       <c r="D40" s="2" t="s">
-        <v>309</v>
+        <v>306</v>
       </c>
       <c r="E40" s="2"/>
       <c r="F40" s="4"/>
@@ -3760,7 +3748,7 @@
       </c>
       <c r="C41" s="2"/>
       <c r="D41" s="2" t="s">
-        <v>310</v>
+        <v>307</v>
       </c>
       <c r="E41" s="2"/>
       <c r="F41" s="4"/>
@@ -3772,7 +3760,7 @@
       </c>
       <c r="C42" s="2"/>
       <c r="D42" s="2" t="s">
-        <v>318</v>
+        <v>315</v>
       </c>
       <c r="E42" s="2"/>
       <c r="F42" s="4"/>
@@ -3784,7 +3772,7 @@
       </c>
       <c r="C43" s="2"/>
       <c r="D43" s="2" t="s">
-        <v>317</v>
+        <v>314</v>
       </c>
       <c r="E43" s="2"/>
       <c r="F43" s="4"/>
@@ -3796,7 +3784,7 @@
       </c>
       <c r="C44" s="2"/>
       <c r="D44" s="2" t="s">
-        <v>319</v>
+        <v>316</v>
       </c>
       <c r="E44" s="2"/>
       <c r="F44" s="4"/>
@@ -3808,7 +3796,7 @@
       </c>
       <c r="C45" s="2"/>
       <c r="D45" s="2" t="s">
-        <v>320</v>
+        <v>317</v>
       </c>
       <c r="E45" s="2"/>
       <c r="F45" s="4"/>
@@ -3820,7 +3808,7 @@
       </c>
       <c r="C46" s="2"/>
       <c r="D46" s="2" t="s">
-        <v>311</v>
+        <v>308</v>
       </c>
       <c r="E46" s="2"/>
       <c r="F46" s="4"/>
@@ -3832,7 +3820,7 @@
       </c>
       <c r="C47" s="2"/>
       <c r="D47" s="2" t="s">
-        <v>314</v>
+        <v>311</v>
       </c>
       <c r="E47" s="2"/>
       <c r="F47" s="4"/>
@@ -3844,7 +3832,7 @@
       </c>
       <c r="C48" s="2"/>
       <c r="D48" s="2" t="s">
-        <v>315</v>
+        <v>312</v>
       </c>
       <c r="E48" s="2"/>
       <c r="F48" s="4"/>
@@ -3856,7 +3844,7 @@
       </c>
       <c r="C49" s="2"/>
       <c r="D49" s="2" t="s">
-        <v>316</v>
+        <v>313</v>
       </c>
       <c r="E49" s="2"/>
       <c r="F49" s="4"/>
@@ -3868,7 +3856,7 @@
       </c>
       <c r="C50" s="2"/>
       <c r="D50" s="2" t="s">
-        <v>312</v>
+        <v>309</v>
       </c>
       <c r="E50" s="2"/>
       <c r="F50" s="4"/>
@@ -3880,7 +3868,7 @@
       </c>
       <c r="C51" s="2"/>
       <c r="D51" s="2" t="s">
-        <v>313</v>
+        <v>310</v>
       </c>
       <c r="E51" s="2"/>
       <c r="F51" s="4"/>
@@ -3892,7 +3880,7 @@
       </c>
       <c r="C52" s="2"/>
       <c r="D52" s="2" t="s">
-        <v>321</v>
+        <v>318</v>
       </c>
       <c r="E52" s="2"/>
       <c r="F52" s="4"/>
@@ -3921,7 +3909,7 @@
         <v>13</v>
       </c>
       <c r="C55" s="2" t="s">
-        <v>69</v>
+        <v>68</v>
       </c>
       <c r="D55" s="2"/>
       <c r="E55" s="2"/>
@@ -3936,7 +3924,7 @@
         <v>13</v>
       </c>
       <c r="D56" t="s">
-        <v>70</v>
+        <v>69</v>
       </c>
       <c r="E56" s="13"/>
     </row>
@@ -3946,7 +3934,7 @@
         <v>13</v>
       </c>
       <c r="H57" t="s">
-        <v>71</v>
+        <v>70</v>
       </c>
     </row>
     <row r="58" spans="1:8" ht="12">
@@ -3964,23 +3952,23 @@
     <row r="59" spans="1:8" s="10" customFormat="1" ht="12"/>
     <row r="60" spans="1:8" s="10" customFormat="1" ht="15">
       <c r="B60" s="10" t="s">
-        <v>352</v>
+        <v>349</v>
       </c>
       <c r="E60" s="13" t="s">
-        <v>357</v>
+        <v>354</v>
       </c>
     </row>
     <row r="61" spans="1:8" s="10" customFormat="1" ht="15">
       <c r="B61" s="10" t="s">
+        <v>350</v>
+      </c>
+      <c r="E61" s="37" t="s">
         <v>353</v>
-      </c>
-      <c r="E61" s="37" t="s">
-        <v>356</v>
       </c>
     </row>
     <row r="62" spans="1:8" s="10" customFormat="1" ht="12">
       <c r="B62" s="10" t="s">
-        <v>354</v>
+        <v>351</v>
       </c>
     </row>
     <row r="63" spans="1:8" s="10" customFormat="1" ht="12">
@@ -3993,19 +3981,19 @@
     </row>
     <row r="64" spans="1:8" s="10" customFormat="1" ht="12">
       <c r="B64" s="10" t="s">
-        <v>355</v>
+        <v>352</v>
       </c>
     </row>
     <row r="65" spans="1:8" s="10" customFormat="1" ht="12"/>
     <row r="66" spans="1:8" ht="30">
       <c r="A66" s="21"/>
       <c r="B66" s="13" t="s">
-        <v>327</v>
+        <v>324</v>
       </c>
       <c r="C66" s="13"/>
       <c r="D66" s="13"/>
       <c r="E66" s="13" t="s">
-        <v>323</v>
+        <v>320</v>
       </c>
       <c r="F66" s="13"/>
       <c r="G66" s="13"/>
@@ -4014,12 +4002,12 @@
     <row r="67" spans="1:8" ht="30">
       <c r="A67" s="21"/>
       <c r="B67" s="13" t="s">
-        <v>328</v>
+        <v>325</v>
       </c>
       <c r="C67" s="13"/>
       <c r="D67" s="13"/>
       <c r="E67" s="13" t="s">
-        <v>329</v>
+        <v>326</v>
       </c>
       <c r="F67" s="13"/>
       <c r="G67" s="13"/>
@@ -4028,7 +4016,7 @@
     <row r="68" spans="1:8" ht="15">
       <c r="A68" s="21"/>
       <c r="B68" s="15" t="s">
-        <v>325</v>
+        <v>322</v>
       </c>
       <c r="C68" s="15"/>
       <c r="D68" s="15"/>
@@ -4050,10 +4038,10 @@
     <row r="70" spans="1:8" ht="24">
       <c r="A70" s="21"/>
       <c r="B70" t="s">
-        <v>336</v>
+        <v>333</v>
       </c>
       <c r="C70" t="s">
-        <v>335</v>
+        <v>332</v>
       </c>
       <c r="F70" t="s">
         <v>6</v>
@@ -4064,12 +4052,12 @@
     <row r="71" spans="1:8" ht="30">
       <c r="A71" s="21"/>
       <c r="B71" s="13" t="s">
-        <v>341</v>
+        <v>338</v>
       </c>
       <c r="C71" s="13"/>
       <c r="D71" s="13"/>
       <c r="E71" s="13" t="s">
-        <v>338</v>
+        <v>335</v>
       </c>
       <c r="F71" s="13"/>
       <c r="G71" s="10"/>
@@ -4078,12 +4066,12 @@
     <row r="72" spans="1:8" ht="30">
       <c r="A72" s="21"/>
       <c r="B72" s="13" t="s">
-        <v>342</v>
+        <v>339</v>
       </c>
       <c r="C72" s="13"/>
       <c r="D72" s="13"/>
       <c r="E72" s="13" t="s">
-        <v>343</v>
+        <v>340</v>
       </c>
       <c r="F72" s="13"/>
       <c r="G72" s="10"/>
@@ -4092,7 +4080,7 @@
     <row r="73" spans="1:8" ht="15">
       <c r="A73" s="21"/>
       <c r="B73" s="15" t="s">
-        <v>339</v>
+        <v>336</v>
       </c>
       <c r="C73" s="15"/>
       <c r="D73" s="15"/>
@@ -4115,7 +4103,7 @@
       </c>
       <c r="C75" s="12"/>
       <c r="D75" s="25" t="s">
-        <v>350</v>
+        <v>347</v>
       </c>
       <c r="E75" s="12"/>
       <c r="F75" s="12"/>
@@ -4137,7 +4125,7 @@
     <row r="77" spans="1:8" ht="15">
       <c r="A77" s="21"/>
       <c r="B77" s="15" t="s">
-        <v>340</v>
+        <v>337</v>
       </c>
       <c r="C77" s="18"/>
       <c r="D77" s="31"/>
@@ -4149,24 +4137,24 @@
     <row r="78" spans="1:8" ht="30">
       <c r="A78" s="27"/>
       <c r="B78" s="13" t="s">
-        <v>345</v>
+        <v>342</v>
       </c>
       <c r="C78" s="13"/>
       <c r="D78" s="13"/>
       <c r="E78" s="13" t="s">
-        <v>337</v>
+        <v>334</v>
       </c>
       <c r="F78" s="13"/>
     </row>
     <row r="79" spans="1:8" ht="30">
       <c r="A79" s="27"/>
       <c r="B79" s="13" t="s">
-        <v>346</v>
+        <v>343</v>
       </c>
       <c r="C79" s="13"/>
       <c r="D79" s="13"/>
       <c r="E79" s="13" t="s">
-        <v>347</v>
+        <v>344</v>
       </c>
       <c r="F79" s="13"/>
     </row>
@@ -4176,7 +4164,7 @@
       </c>
       <c r="C80" s="26"/>
       <c r="D80" s="26" t="s">
-        <v>359</v>
+        <v>356</v>
       </c>
       <c r="E80" s="26"/>
       <c r="F80" s="26"/>
@@ -4184,7 +4172,7 @@
     <row r="81" spans="1:8" ht="15">
       <c r="A81" s="27"/>
       <c r="B81" s="15" t="s">
-        <v>348</v>
+        <v>345</v>
       </c>
       <c r="C81" s="15"/>
       <c r="D81" s="15"/>
@@ -4204,7 +4192,7 @@
       </c>
       <c r="C83" s="20"/>
       <c r="D83" s="28" t="s">
-        <v>344</v>
+        <v>341</v>
       </c>
       <c r="E83" s="28"/>
       <c r="F83" s="20"/>
@@ -4229,7 +4217,7 @@
     <row r="86" spans="1:8" ht="15">
       <c r="A86" s="27"/>
       <c r="B86" s="15" t="s">
-        <v>349</v>
+        <v>346</v>
       </c>
       <c r="C86" s="29"/>
       <c r="D86" s="30"/>
@@ -4242,7 +4230,7 @@
       </c>
       <c r="C87" s="33"/>
       <c r="D87" s="34" t="s">
-        <v>358</v>
+        <v>355</v>
       </c>
       <c r="E87" s="33"/>
       <c r="F87" s="33"/>
@@ -4250,7 +4238,7 @@
     <row r="88" spans="1:8" ht="15">
       <c r="A88" s="27"/>
       <c r="B88" s="15" t="s">
-        <v>326</v>
+        <v>323</v>
       </c>
       <c r="C88" s="29"/>
       <c r="D88" s="30"/>
@@ -4263,7 +4251,7 @@
       </c>
       <c r="C89" s="33"/>
       <c r="D89" s="34" t="s">
-        <v>360</v>
+        <v>357</v>
       </c>
       <c r="E89" s="33"/>
       <c r="F89" s="33"/>
@@ -4271,7 +4259,7 @@
     <row r="90" spans="1:8" ht="15">
       <c r="A90" s="27"/>
       <c r="B90" s="15" t="s">
-        <v>73</v>
+        <v>71</v>
       </c>
       <c r="C90" s="29"/>
       <c r="D90" s="30"/>
@@ -4289,33 +4277,33 @@
     <row r="92" spans="1:8" s="13" customFormat="1" ht="15">
       <c r="A92" s="26"/>
       <c r="B92" s="13" t="s">
-        <v>95</v>
+        <v>92</v>
       </c>
       <c r="C92" s="35"/>
       <c r="D92" s="36"/>
       <c r="E92" s="14" t="s">
-        <v>351</v>
+        <v>348</v>
       </c>
       <c r="F92" s="35"/>
     </row>
     <row r="93" spans="1:8" s="13" customFormat="1" ht="15">
       <c r="A93" s="26"/>
       <c r="B93" s="13" t="s">
-        <v>74</v>
+        <v>72</v>
       </c>
       <c r="C93" s="35"/>
       <c r="D93" s="36"/>
       <c r="E93" s="14" t="s">
-        <v>75</v>
+        <v>73</v>
       </c>
       <c r="F93" s="35"/>
     </row>
     <row r="94" spans="1:8" ht="15">
       <c r="A94" s="21" t="s">
-        <v>333</v>
+        <v>330</v>
       </c>
       <c r="B94" s="15" t="s">
-        <v>96</v>
+        <v>93</v>
       </c>
       <c r="C94" s="15"/>
       <c r="D94" s="15"/>
@@ -4327,7 +4315,7 @@
     <row r="95" spans="1:8" ht="12">
       <c r="A95" s="21"/>
       <c r="B95" t="s">
-        <v>156</v>
+        <v>153</v>
       </c>
       <c r="C95" t="s">
         <v>11</v>
@@ -4347,7 +4335,7 @@
         <v>15</v>
       </c>
       <c r="E96" t="s">
-        <v>362</v>
+        <v>359</v>
       </c>
     </row>
     <row r="97" spans="1:9" ht="12">
@@ -4356,22 +4344,22 @@
         <v>13</v>
       </c>
       <c r="D97" t="s">
-        <v>40</v>
+        <v>39</v>
       </c>
     </row>
     <row r="98" spans="1:9" ht="12">
       <c r="A98" s="21"/>
       <c r="B98" t="s">
-        <v>363</v>
+        <v>360</v>
       </c>
       <c r="C98" t="s">
-        <v>364</v>
+        <v>361</v>
       </c>
       <c r="D98" t="s">
-        <v>365</v>
+        <v>362</v>
       </c>
       <c r="F98" t="s">
-        <v>79</v>
+        <v>77</v>
       </c>
     </row>
     <row r="99" spans="1:9" ht="12.75" customHeight="1">
@@ -4380,10 +4368,10 @@
         <v>15</v>
       </c>
       <c r="C99" t="s">
-        <v>397</v>
+        <v>394</v>
       </c>
       <c r="E99" t="s">
-        <v>398</v>
+        <v>395</v>
       </c>
     </row>
     <row r="100" spans="1:9" ht="12.75" customHeight="1">
@@ -4392,10 +4380,10 @@
         <v>16</v>
       </c>
       <c r="C100" t="s">
-        <v>399</v>
+        <v>396</v>
       </c>
       <c r="D100" t="s">
-        <v>367</v>
+        <v>364</v>
       </c>
     </row>
     <row r="101" spans="1:9" ht="12.75" customHeight="1">
@@ -4404,10 +4392,10 @@
         <v>13</v>
       </c>
       <c r="D101" t="s">
-        <v>403</v>
+        <v>400</v>
       </c>
       <c r="E101" t="s">
-        <v>400</v>
+        <v>397</v>
       </c>
       <c r="I101" s="20"/>
     </row>
@@ -4423,7 +4411,7 @@
         <v>15</v>
       </c>
       <c r="E103" t="s">
-        <v>366</v>
+        <v>363</v>
       </c>
     </row>
     <row r="104" spans="1:9" ht="12">
@@ -4435,7 +4423,7 @@
         <v>20</v>
       </c>
       <c r="D104" t="s">
-        <v>367</v>
+        <v>364</v>
       </c>
     </row>
     <row r="105" spans="1:9" ht="12.75" customHeight="1">
@@ -4463,7 +4451,7 @@
         <v>15</v>
       </c>
       <c r="E107" t="s">
-        <v>368</v>
+        <v>365</v>
       </c>
     </row>
     <row r="108" spans="1:9" ht="12.75" customHeight="1">
@@ -4475,7 +4463,7 @@
         <v>17</v>
       </c>
       <c r="D108" t="s">
-        <v>369</v>
+        <v>366</v>
       </c>
     </row>
     <row r="109" spans="1:9" ht="12.75" customHeight="1">
@@ -4508,7 +4496,7 @@
         <v>15</v>
       </c>
       <c r="E112" t="s">
-        <v>370</v>
+        <v>367</v>
       </c>
     </row>
     <row r="113" spans="1:10" ht="12.75" customHeight="1">
@@ -4517,7 +4505,7 @@
         <v>13</v>
       </c>
       <c r="D113" t="s">
-        <v>42</v>
+        <v>41</v>
       </c>
     </row>
     <row r="114" spans="1:10" ht="12.75" customHeight="1">
@@ -4526,10 +4514,10 @@
         <v>16</v>
       </c>
       <c r="C114" t="s">
-        <v>371</v>
+        <v>368</v>
       </c>
       <c r="D114" t="s">
-        <v>372</v>
+        <v>369</v>
       </c>
     </row>
     <row r="115" spans="1:10" ht="12.75" customHeight="1">
@@ -4538,10 +4526,10 @@
         <v>16</v>
       </c>
       <c r="C115" t="s">
-        <v>373</v>
+        <v>370</v>
       </c>
       <c r="D115" t="s">
-        <v>374</v>
+        <v>371</v>
       </c>
     </row>
     <row r="116" spans="1:10" ht="12.75" customHeight="1">
@@ -4550,10 +4538,10 @@
         <v>13</v>
       </c>
       <c r="D116" t="s">
-        <v>375</v>
+        <v>372</v>
       </c>
       <c r="E116" t="s">
-        <v>376</v>
+        <v>373</v>
       </c>
     </row>
     <row r="117" spans="1:10" ht="12.75" customHeight="1">
@@ -4562,10 +4550,10 @@
         <v>13</v>
       </c>
       <c r="D117" t="s">
-        <v>377</v>
+        <v>374</v>
       </c>
       <c r="E117" t="s">
-        <v>376</v>
+        <v>373</v>
       </c>
     </row>
     <row r="118" spans="1:10" ht="12.75" customHeight="1">
@@ -4574,10 +4562,10 @@
         <v>13</v>
       </c>
       <c r="D118" t="s">
-        <v>378</v>
+        <v>375</v>
       </c>
       <c r="E118" t="s">
-        <v>376</v>
+        <v>373</v>
       </c>
     </row>
     <row r="119" spans="1:10" ht="12.75" customHeight="1">
@@ -4592,7 +4580,7 @@
         <v>15</v>
       </c>
       <c r="E120" t="s">
-        <v>379</v>
+        <v>376</v>
       </c>
     </row>
     <row r="121" spans="1:10" ht="12.75" customHeight="1">
@@ -4601,7 +4589,7 @@
         <v>13</v>
       </c>
       <c r="D121" t="s">
-        <v>99</v>
+        <v>96</v>
       </c>
     </row>
     <row r="122" spans="1:10" ht="12.75" customHeight="1">
@@ -4610,10 +4598,10 @@
         <v>16</v>
       </c>
       <c r="C122" t="s">
-        <v>380</v>
+        <v>377</v>
       </c>
       <c r="D122" t="s">
-        <v>381</v>
+        <v>378</v>
       </c>
     </row>
     <row r="123" spans="1:10" ht="12.75" customHeight="1">
@@ -4622,10 +4610,10 @@
         <v>16</v>
       </c>
       <c r="C123" t="s">
-        <v>382</v>
+        <v>379</v>
       </c>
       <c r="D123" t="s">
-        <v>383</v>
+        <v>380</v>
       </c>
     </row>
     <row r="124" spans="1:10" ht="12.75" customHeight="1">
@@ -4634,10 +4622,10 @@
         <v>13</v>
       </c>
       <c r="D124" t="s">
-        <v>384</v>
+        <v>381</v>
       </c>
       <c r="E124" t="s">
-        <v>385</v>
+        <v>382</v>
       </c>
     </row>
     <row r="125" spans="1:10" ht="12.75" customHeight="1">
@@ -4649,7 +4637,7 @@
     <row r="126" spans="1:10" ht="12.75" customHeight="1">
       <c r="A126" s="21"/>
       <c r="B126" s="15" t="s">
-        <v>76</v>
+        <v>74</v>
       </c>
       <c r="C126" s="15"/>
       <c r="D126" s="15"/>
@@ -4662,22 +4650,22 @@
     <row r="128" spans="1:10" s="14" customFormat="1" ht="12.75" customHeight="1">
       <c r="A128" s="24"/>
       <c r="B128" s="13" t="s">
-        <v>97</v>
+        <v>94</v>
       </c>
       <c r="E128" s="14" t="s">
-        <v>98</v>
+        <v>95</v>
       </c>
       <c r="I128" s="12"/>
       <c r="J128" s="12"/>
     </row>
     <row r="129" spans="1:9" ht="12.75" customHeight="1">
       <c r="B129" s="13" t="s">
-        <v>81</v>
+        <v>79</v>
       </c>
       <c r="C129" s="14"/>
       <c r="D129" s="14"/>
       <c r="E129" s="14" t="s">
-        <v>77</v>
+        <v>75</v>
       </c>
       <c r="F129" s="14"/>
       <c r="G129" s="14"/>
@@ -4685,10 +4673,10 @@
     </row>
     <row r="130" spans="1:9" ht="12.75" customHeight="1">
       <c r="A130" s="21" t="s">
-        <v>334</v>
+        <v>331</v>
       </c>
       <c r="B130" s="15" t="s">
-        <v>109</v>
+        <v>106</v>
       </c>
       <c r="C130" s="18"/>
       <c r="D130" s="18"/>
@@ -4707,16 +4695,16 @@
     <row r="132" spans="1:9" ht="12.75" customHeight="1">
       <c r="A132" s="21"/>
       <c r="B132" t="s">
-        <v>409</v>
+        <v>406</v>
       </c>
       <c r="C132" t="s">
-        <v>78</v>
+        <v>76</v>
       </c>
       <c r="D132" t="s">
-        <v>404</v>
+        <v>401</v>
       </c>
       <c r="F132" t="s">
-        <v>79</v>
+        <v>77</v>
       </c>
     </row>
     <row r="133" spans="1:9" ht="12.75" customHeight="1">
@@ -4725,13 +4713,13 @@
         <v>13</v>
       </c>
       <c r="C133" t="s">
-        <v>405</v>
+        <v>402</v>
       </c>
       <c r="E133" t="s">
-        <v>410</v>
+        <v>407</v>
       </c>
       <c r="I133" t="s">
-        <v>406</v>
+        <v>403</v>
       </c>
     </row>
     <row r="134" spans="1:9" ht="12.75" customHeight="1">
@@ -4740,10 +4728,10 @@
         <v>13</v>
       </c>
       <c r="D134" t="s">
-        <v>407</v>
+        <v>404</v>
       </c>
       <c r="E134" t="s">
-        <v>411</v>
+        <v>408</v>
       </c>
     </row>
     <row r="135" spans="1:9" ht="12.75" customHeight="1">
@@ -4752,10 +4740,10 @@
         <v>13</v>
       </c>
       <c r="D135" t="s">
-        <v>408</v>
+        <v>405</v>
       </c>
       <c r="E135" t="s">
-        <v>412</v>
+        <v>409</v>
       </c>
     </row>
     <row r="136" spans="1:9" ht="12.75" customHeight="1">
@@ -4767,7 +4755,7 @@
     <row r="137" spans="1:9" ht="12.75" customHeight="1">
       <c r="A137" s="21"/>
       <c r="B137" s="15" t="s">
-        <v>80</v>
+        <v>78</v>
       </c>
       <c r="C137" s="18"/>
       <c r="D137" s="18"/>
@@ -4778,12 +4766,12 @@
     </row>
     <row r="139" spans="1:9" ht="12.75" customHeight="1">
       <c r="B139" s="13" t="s">
-        <v>100</v>
+        <v>97</v>
       </c>
       <c r="C139" s="14"/>
       <c r="D139" s="14"/>
       <c r="E139" s="14" t="s">
-        <v>102</v>
+        <v>99</v>
       </c>
       <c r="F139" s="14"/>
       <c r="G139" s="14"/>
@@ -4791,12 +4779,12 @@
     </row>
     <row r="140" spans="1:9" ht="12.75" customHeight="1">
       <c r="B140" s="13" t="s">
-        <v>101</v>
+        <v>98</v>
       </c>
       <c r="C140" s="14"/>
       <c r="D140" s="14"/>
       <c r="E140" s="14" t="s">
-        <v>103</v>
+        <v>100</v>
       </c>
       <c r="F140" s="14"/>
       <c r="G140" s="14"/>
@@ -4804,10 +4792,10 @@
     </row>
     <row r="141" spans="1:9" ht="12.75" customHeight="1">
       <c r="A141" s="21" t="s">
-        <v>57</v>
+        <v>56</v>
       </c>
       <c r="B141" s="15" t="s">
-        <v>110</v>
+        <v>107</v>
       </c>
       <c r="C141" s="18"/>
       <c r="D141" s="18"/>
@@ -4819,13 +4807,13 @@
     <row r="142" spans="1:9" ht="12.75" customHeight="1">
       <c r="A142" s="27"/>
       <c r="B142" t="s">
-        <v>156</v>
+        <v>153</v>
       </c>
       <c r="C142" t="s">
         <v>11</v>
       </c>
       <c r="D142" t="s">
-        <v>60</v>
+        <v>59</v>
       </c>
       <c r="F142" t="s">
         <v>6</v>
@@ -4839,7 +4827,7 @@
         <v>15</v>
       </c>
       <c r="E143" t="s">
-        <v>362</v>
+        <v>359</v>
       </c>
     </row>
     <row r="144" spans="1:9" ht="12.75" customHeight="1">
@@ -4848,22 +4836,22 @@
         <v>13</v>
       </c>
       <c r="D144" t="s">
-        <v>40</v>
+        <v>39</v>
       </c>
     </row>
     <row r="145" spans="1:9" ht="12.75" customHeight="1">
       <c r="A145" s="27"/>
       <c r="B145" t="s">
-        <v>363</v>
+        <v>360</v>
       </c>
       <c r="C145" t="s">
-        <v>364</v>
+        <v>361</v>
       </c>
       <c r="D145" t="s">
-        <v>365</v>
+        <v>362</v>
       </c>
       <c r="F145" t="s">
-        <v>79</v>
+        <v>77</v>
       </c>
     </row>
     <row r="146" spans="1:9" ht="12.75" customHeight="1">
@@ -4872,10 +4860,10 @@
         <v>15</v>
       </c>
       <c r="C146" t="s">
-        <v>397</v>
+        <v>394</v>
       </c>
       <c r="E146" t="s">
-        <v>398</v>
+        <v>395</v>
       </c>
     </row>
     <row r="147" spans="1:9" ht="12.75" customHeight="1">
@@ -4884,10 +4872,10 @@
         <v>16</v>
       </c>
       <c r="C147" t="s">
-        <v>399</v>
+        <v>396</v>
       </c>
       <c r="D147" t="s">
-        <v>367</v>
+        <v>364</v>
       </c>
     </row>
     <row r="148" spans="1:9" ht="12.75" customHeight="1">
@@ -4896,10 +4884,10 @@
         <v>13</v>
       </c>
       <c r="D148" t="s">
-        <v>403</v>
+        <v>400</v>
       </c>
       <c r="E148" t="s">
-        <v>400</v>
+        <v>397</v>
       </c>
       <c r="I148" s="20"/>
     </row>
@@ -4915,7 +4903,7 @@
         <v>15</v>
       </c>
       <c r="E150" t="s">
-        <v>366</v>
+        <v>363</v>
       </c>
     </row>
     <row r="151" spans="1:9" ht="12.75" customHeight="1">
@@ -4927,7 +4915,7 @@
         <v>20</v>
       </c>
       <c r="D151" t="s">
-        <v>367</v>
+        <v>364</v>
       </c>
     </row>
     <row r="152" spans="1:9" ht="12.75" customHeight="1">
@@ -4955,7 +4943,7 @@
         <v>15</v>
       </c>
       <c r="E154" t="s">
-        <v>368</v>
+        <v>365</v>
       </c>
     </row>
     <row r="155" spans="1:9" ht="12.75" customHeight="1">
@@ -4967,7 +4955,7 @@
         <v>17</v>
       </c>
       <c r="D155" t="s">
-        <v>369</v>
+        <v>366</v>
       </c>
     </row>
     <row r="156" spans="1:9" ht="12.75" customHeight="1">
@@ -5000,7 +4988,7 @@
         <v>15</v>
       </c>
       <c r="E159" t="s">
-        <v>370</v>
+        <v>367</v>
       </c>
     </row>
     <row r="160" spans="1:9" ht="12.75" customHeight="1">
@@ -5009,7 +4997,7 @@
         <v>13</v>
       </c>
       <c r="D160" t="s">
-        <v>42</v>
+        <v>41</v>
       </c>
     </row>
     <row r="161" spans="1:8" ht="12.75" customHeight="1">
@@ -5018,10 +5006,10 @@
         <v>16</v>
       </c>
       <c r="C161" t="s">
-        <v>371</v>
+        <v>368</v>
       </c>
       <c r="D161" t="s">
-        <v>372</v>
+        <v>369</v>
       </c>
     </row>
     <row r="162" spans="1:8" ht="12.75" customHeight="1">
@@ -5030,10 +5018,10 @@
         <v>16</v>
       </c>
       <c r="C162" t="s">
-        <v>373</v>
+        <v>370</v>
       </c>
       <c r="D162" t="s">
-        <v>374</v>
+        <v>371</v>
       </c>
     </row>
     <row r="163" spans="1:8" ht="12.75" customHeight="1">
@@ -5042,10 +5030,10 @@
         <v>13</v>
       </c>
       <c r="D163" t="s">
-        <v>375</v>
+        <v>372</v>
       </c>
       <c r="E163" t="s">
-        <v>376</v>
+        <v>373</v>
       </c>
     </row>
     <row r="164" spans="1:8" ht="12.75" customHeight="1">
@@ -5054,10 +5042,10 @@
         <v>13</v>
       </c>
       <c r="D164" t="s">
-        <v>377</v>
+        <v>374</v>
       </c>
       <c r="E164" t="s">
-        <v>376</v>
+        <v>373</v>
       </c>
     </row>
     <row r="165" spans="1:8" ht="12.75" customHeight="1">
@@ -5066,10 +5054,10 @@
         <v>13</v>
       </c>
       <c r="D165" t="s">
-        <v>378</v>
+        <v>375</v>
       </c>
       <c r="E165" t="s">
-        <v>376</v>
+        <v>373</v>
       </c>
     </row>
     <row r="166" spans="1:8" ht="12.75" customHeight="1">
@@ -5084,7 +5072,7 @@
         <v>15</v>
       </c>
       <c r="E167" t="s">
-        <v>379</v>
+        <v>376</v>
       </c>
     </row>
     <row r="168" spans="1:8" ht="12.75" customHeight="1">
@@ -5093,7 +5081,7 @@
         <v>13</v>
       </c>
       <c r="D168" t="s">
-        <v>99</v>
+        <v>96</v>
       </c>
     </row>
     <row r="169" spans="1:8" ht="12.75" customHeight="1">
@@ -5102,10 +5090,10 @@
         <v>16</v>
       </c>
       <c r="C169" t="s">
-        <v>380</v>
+        <v>377</v>
       </c>
       <c r="D169" t="s">
-        <v>381</v>
+        <v>378</v>
       </c>
     </row>
     <row r="170" spans="1:8" ht="12.75" customHeight="1">
@@ -5114,10 +5102,10 @@
         <v>16</v>
       </c>
       <c r="C170" t="s">
-        <v>382</v>
+        <v>379</v>
       </c>
       <c r="D170" t="s">
-        <v>383</v>
+        <v>380</v>
       </c>
     </row>
     <row r="171" spans="1:8" ht="12.75" customHeight="1">
@@ -5126,10 +5114,10 @@
         <v>13</v>
       </c>
       <c r="D171" t="s">
-        <v>384</v>
+        <v>381</v>
       </c>
       <c r="E171" t="s">
-        <v>385</v>
+        <v>382</v>
       </c>
     </row>
     <row r="172" spans="1:8" ht="12.75" customHeight="1">
@@ -5141,7 +5129,7 @@
     <row r="173" spans="1:8" ht="12.75" customHeight="1">
       <c r="A173" s="21"/>
       <c r="B173" s="15" t="s">
-        <v>104</v>
+        <v>101</v>
       </c>
       <c r="C173" s="18"/>
       <c r="D173" s="18"/>
@@ -5152,7 +5140,7 @@
     </row>
     <row r="176" spans="1:8" ht="12.75" customHeight="1">
       <c r="B176" s="17" t="s">
-        <v>93</v>
+        <v>90</v>
       </c>
     </row>
   </sheetData>
@@ -5205,154 +5193,154 @@
     </row>
     <row r="4" spans="1:2" ht="12.75" customHeight="1">
       <c r="A4" t="s">
-        <v>401</v>
+        <v>398</v>
       </c>
       <c r="B4" t="s">
-        <v>402</v>
+        <v>399</v>
       </c>
     </row>
     <row r="5" spans="1:2" ht="12.75" customHeight="1">
       <c r="A5" t="s">
-        <v>390</v>
+        <v>387</v>
       </c>
       <c r="B5" t="s">
-        <v>392</v>
+        <v>389</v>
       </c>
     </row>
     <row r="6" spans="1:2" ht="12.75" customHeight="1">
       <c r="A6" t="s">
-        <v>391</v>
+        <v>388</v>
       </c>
       <c r="B6" t="s">
-        <v>393</v>
+        <v>390</v>
       </c>
     </row>
     <row r="7" spans="1:2" ht="12.75" customHeight="1">
       <c r="A7" t="s">
-        <v>394</v>
+        <v>391</v>
       </c>
       <c r="B7" t="s">
-        <v>396</v>
+        <v>393</v>
       </c>
     </row>
     <row r="9" spans="1:2" ht="12" customHeight="1">
       <c r="A9" t="s">
-        <v>157</v>
+        <v>154</v>
       </c>
       <c r="B9" t="s">
-        <v>158</v>
+        <v>155</v>
       </c>
     </row>
     <row r="10" spans="1:2" ht="12" customHeight="1">
       <c r="A10" t="s">
-        <v>159</v>
+        <v>156</v>
       </c>
       <c r="B10" t="s">
-        <v>167</v>
+        <v>164</v>
       </c>
     </row>
     <row r="11" spans="1:2" ht="12" customHeight="1">
       <c r="A11" t="s">
-        <v>160</v>
+        <v>157</v>
       </c>
       <c r="B11" t="s">
-        <v>164</v>
+        <v>161</v>
       </c>
     </row>
     <row r="12" spans="1:2" ht="12" customHeight="1">
       <c r="A12" t="s">
-        <v>185</v>
+        <v>182</v>
       </c>
       <c r="B12" t="s">
-        <v>182</v>
+        <v>179</v>
       </c>
     </row>
     <row r="13" spans="1:2" ht="12" customHeight="1">
       <c r="A13" t="s">
-        <v>161</v>
+        <v>158</v>
       </c>
       <c r="B13" t="s">
-        <v>165</v>
+        <v>162</v>
       </c>
     </row>
     <row r="14" spans="1:2" ht="12" customHeight="1">
       <c r="A14" t="s">
-        <v>162</v>
+        <v>159</v>
       </c>
       <c r="B14" t="s">
-        <v>166</v>
+        <v>163</v>
       </c>
     </row>
     <row r="15" spans="1:2" ht="42" customHeight="1">
       <c r="A15" t="s">
-        <v>183</v>
+        <v>180</v>
       </c>
       <c r="B15" t="s">
-        <v>184</v>
+        <v>181</v>
       </c>
     </row>
     <row r="16" spans="1:2" ht="12.75" customHeight="1">
       <c r="A16" t="s">
-        <v>282</v>
+        <v>279</v>
       </c>
       <c r="B16" t="s">
-        <v>290</v>
+        <v>287</v>
       </c>
     </row>
     <row r="17" spans="1:2" ht="12.75" customHeight="1">
       <c r="A17" t="s">
-        <v>283</v>
+        <v>280</v>
       </c>
       <c r="B17" t="s">
-        <v>291</v>
+        <v>288</v>
       </c>
     </row>
     <row r="18" spans="1:2" ht="12.75" customHeight="1">
       <c r="A18" t="s">
-        <v>284</v>
+        <v>281</v>
       </c>
       <c r="B18" t="s">
-        <v>292</v>
+        <v>289</v>
       </c>
     </row>
     <row r="19" spans="1:2" ht="12.75" customHeight="1">
       <c r="A19" t="s">
-        <v>285</v>
+        <v>282</v>
       </c>
       <c r="B19" t="s">
-        <v>293</v>
+        <v>290</v>
       </c>
     </row>
     <row r="20" spans="1:2" ht="12.75" customHeight="1">
       <c r="A20" t="s">
-        <v>286</v>
+        <v>283</v>
       </c>
       <c r="B20" t="s">
-        <v>294</v>
+        <v>291</v>
       </c>
     </row>
     <row r="21" spans="1:2" ht="12.75" customHeight="1">
       <c r="A21" t="s">
-        <v>287</v>
+        <v>284</v>
       </c>
       <c r="B21" t="s">
-        <v>295</v>
+        <v>292</v>
       </c>
     </row>
     <row r="22" spans="1:2" ht="12.75" customHeight="1">
       <c r="A22" t="s">
-        <v>288</v>
+        <v>285</v>
       </c>
       <c r="B22" t="s">
-        <v>289</v>
+        <v>286</v>
       </c>
     </row>
     <row r="23" spans="1:2" ht="12.75" customHeight="1">
       <c r="A23" t="s">
-        <v>296</v>
+        <v>293</v>
       </c>
       <c r="B23" t="s">
-        <v>297</v>
+        <v>294</v>
       </c>
     </row>
   </sheetData>
@@ -5370,8 +5358,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:D136"/>
   <sheetViews>
-    <sheetView topLeftCell="A112" workbookViewId="0">
-      <selection activeCell="C147" sqref="C147"/>
+    <sheetView tabSelected="1" workbookViewId="0">
+      <selection activeCell="C17" sqref="C17"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultColWidth="17.1640625" defaultRowHeight="12.75" customHeight="1" x14ac:dyDescent="0"/>
@@ -5391,7 +5379,7 @@
         <v>2</v>
       </c>
       <c r="D1" t="s">
-        <v>55</v>
+        <v>54</v>
       </c>
     </row>
     <row r="2" spans="1:4" ht="12.75" customHeight="1">
@@ -5402,7 +5390,7 @@
         <v>30</v>
       </c>
       <c r="D2" t="s">
-        <v>416</v>
+        <v>413</v>
       </c>
     </row>
     <row r="3" spans="1:4" ht="12.75" customHeight="1">
@@ -5413,7 +5401,7 @@
         <v>31</v>
       </c>
       <c r="D3" t="s">
-        <v>417</v>
+        <v>414</v>
       </c>
     </row>
     <row r="4" spans="1:4" ht="12.75" customHeight="1">
@@ -5424,7 +5412,7 @@
         <v>32</v>
       </c>
       <c r="D4" t="s">
-        <v>418</v>
+        <v>415</v>
       </c>
     </row>
     <row r="5" spans="1:4" ht="12.75" customHeight="1">
@@ -5432,10 +5420,10 @@
         <v>4</v>
       </c>
       <c r="B5" t="s">
-        <v>59</v>
+        <v>58</v>
       </c>
       <c r="D5" t="s">
-        <v>419</v>
+        <v>416</v>
       </c>
     </row>
     <row r="6" spans="1:4" ht="12.75" customHeight="1">
@@ -5443,10 +5431,10 @@
         <v>4</v>
       </c>
       <c r="B6" t="s">
-        <v>82</v>
+        <v>80</v>
       </c>
       <c r="D6" t="s">
-        <v>420</v>
+        <v>417</v>
       </c>
     </row>
     <row r="9" spans="1:4" ht="12.75" customHeight="1">
@@ -5476,10 +5464,10 @@
         <v>9</v>
       </c>
       <c r="B11" t="s">
-        <v>62</v>
+        <v>61</v>
       </c>
       <c r="C11" t="s">
-        <v>61</v>
+        <v>60</v>
       </c>
     </row>
     <row r="13" spans="1:4" ht="12.75" customHeight="1">
@@ -5489,11 +5477,8 @@
       <c r="B13" t="s">
         <v>37</v>
       </c>
-      <c r="C13" t="s">
-        <v>38</v>
-      </c>
       <c r="D13" t="s">
-        <v>421</v>
+        <v>418</v>
       </c>
     </row>
     <row r="14" spans="1:4" ht="12.75" customHeight="1">
@@ -5501,13 +5486,10 @@
         <v>7</v>
       </c>
       <c r="B14" t="s">
-        <v>85</v>
-      </c>
-      <c r="C14" t="s">
-        <v>86</v>
+        <v>82</v>
       </c>
       <c r="D14" t="s">
-        <v>422</v>
+        <v>419</v>
       </c>
     </row>
     <row r="15" spans="1:4" ht="12.75" customHeight="1">
@@ -5515,13 +5497,10 @@
         <v>7</v>
       </c>
       <c r="B15" t="s">
-        <v>83</v>
-      </c>
-      <c r="C15" t="s">
-        <v>84</v>
+        <v>81</v>
       </c>
       <c r="D15" t="s">
-        <v>423</v>
+        <v>420</v>
       </c>
     </row>
     <row r="16" spans="1:4" ht="12.75" customHeight="1">
@@ -5529,13 +5508,10 @@
         <v>7</v>
       </c>
       <c r="B16" t="s">
-        <v>111</v>
-      </c>
-      <c r="C16" t="s">
-        <v>72</v>
+        <v>108</v>
       </c>
       <c r="D16" t="s">
-        <v>424</v>
+        <v>421</v>
       </c>
     </row>
     <row r="17" spans="1:4" ht="12.75" customHeight="1">
@@ -5543,13 +5519,10 @@
         <v>7</v>
       </c>
       <c r="B17" t="s">
-        <v>426</v>
-      </c>
-      <c r="C17" t="s">
-        <v>427</v>
+        <v>423</v>
       </c>
       <c r="D17" t="s">
-        <v>425</v>
+        <v>422</v>
       </c>
     </row>
     <row r="18" spans="1:4" ht="12.75" customHeight="1">
@@ -5557,10 +5530,10 @@
         <v>7</v>
       </c>
       <c r="B18" t="s">
-        <v>486</v>
+        <v>482</v>
       </c>
       <c r="C18" t="s">
-        <v>87</v>
+        <v>84</v>
       </c>
     </row>
     <row r="20" spans="1:4" ht="12.75" customHeight="1">
@@ -5568,10 +5541,10 @@
         <v>11</v>
       </c>
       <c r="B20" t="s">
+        <v>38</v>
+      </c>
+      <c r="C20" t="s">
         <v>39</v>
-      </c>
-      <c r="C20" t="s">
-        <v>40</v>
       </c>
     </row>
     <row r="21" spans="1:4" ht="12.75" customHeight="1">
@@ -5579,10 +5552,10 @@
         <v>11</v>
       </c>
       <c r="B21" t="s">
+        <v>40</v>
+      </c>
+      <c r="C21" t="s">
         <v>41</v>
-      </c>
-      <c r="C21" t="s">
-        <v>42</v>
       </c>
     </row>
     <row r="22" spans="1:4" ht="12.75" customHeight="1">
@@ -5590,1040 +5563,1040 @@
         <v>11</v>
       </c>
       <c r="B22" t="s">
-        <v>395</v>
+        <v>392</v>
       </c>
       <c r="C22" t="s">
-        <v>99</v>
+        <v>96</v>
       </c>
     </row>
     <row r="23" spans="1:4" ht="12.75" customHeight="1">
       <c r="A23" t="s">
-        <v>364</v>
+        <v>361</v>
       </c>
       <c r="B23" t="s">
-        <v>386</v>
+        <v>383</v>
       </c>
       <c r="C23" t="s">
-        <v>387</v>
+        <v>384</v>
       </c>
     </row>
     <row r="24" spans="1:4" ht="12.75" customHeight="1">
       <c r="A24" t="s">
-        <v>364</v>
+        <v>361</v>
       </c>
       <c r="B24" t="s">
-        <v>388</v>
+        <v>385</v>
       </c>
       <c r="C24" t="s">
-        <v>389</v>
+        <v>386</v>
       </c>
     </row>
     <row r="26" spans="1:4" ht="12.75" customHeight="1">
       <c r="A26" t="s">
-        <v>78</v>
+        <v>76</v>
       </c>
       <c r="B26" t="s">
-        <v>405</v>
+        <v>402</v>
       </c>
       <c r="C26" t="s">
-        <v>415</v>
+        <v>412</v>
       </c>
     </row>
     <row r="27" spans="1:4" ht="12.75" customHeight="1">
       <c r="A27" t="s">
-        <v>78</v>
+        <v>76</v>
       </c>
       <c r="B27" t="s">
-        <v>413</v>
+        <v>410</v>
       </c>
       <c r="C27" t="s">
-        <v>413</v>
+        <v>410</v>
       </c>
     </row>
     <row r="28" spans="1:4" ht="12.75" customHeight="1">
       <c r="A28" t="s">
-        <v>78</v>
+        <v>76</v>
       </c>
       <c r="B28" t="s">
-        <v>414</v>
+        <v>411</v>
       </c>
       <c r="C28" t="s">
-        <v>414</v>
+        <v>411</v>
       </c>
     </row>
     <row r="30" spans="1:4" ht="12.75" customHeight="1">
       <c r="A30" t="s">
-        <v>58</v>
+        <v>57</v>
       </c>
       <c r="B30" t="s">
+        <v>38</v>
+      </c>
+      <c r="C30" t="s">
         <v>39</v>
-      </c>
-      <c r="C30" t="s">
-        <v>40</v>
       </c>
     </row>
     <row r="31" spans="1:4" ht="12.75" customHeight="1">
       <c r="A31" t="s">
-        <v>58</v>
+        <v>57</v>
       </c>
       <c r="B31" t="s">
+        <v>40</v>
+      </c>
+      <c r="C31" t="s">
         <v>41</v>
-      </c>
-      <c r="C31" t="s">
-        <v>42</v>
       </c>
     </row>
     <row r="32" spans="1:4" ht="12.75" customHeight="1">
       <c r="A32" t="s">
-        <v>58</v>
+        <v>57</v>
       </c>
       <c r="B32" t="s">
-        <v>395</v>
+        <v>392</v>
       </c>
       <c r="C32" t="s">
-        <v>99</v>
+        <v>96</v>
       </c>
     </row>
     <row r="34" spans="1:4" ht="12.75" customHeight="1">
       <c r="A34" t="s">
+        <v>42</v>
+      </c>
+      <c r="B34" t="s">
         <v>43</v>
       </c>
-      <c r="B34" t="s">
+      <c r="C34" t="s">
         <v>44</v>
-      </c>
-      <c r="C34" t="s">
-        <v>45</v>
       </c>
     </row>
     <row r="35" spans="1:4" ht="12.75" customHeight="1">
       <c r="A35" t="s">
-        <v>43</v>
+        <v>42</v>
       </c>
       <c r="B35" t="s">
+        <v>45</v>
+      </c>
+      <c r="C35" t="s">
         <v>46</v>
-      </c>
-      <c r="C35" t="s">
-        <v>47</v>
       </c>
     </row>
     <row r="37" spans="1:4" ht="12.75" customHeight="1">
       <c r="A37" t="s">
-        <v>439</v>
+        <v>435</v>
       </c>
       <c r="B37" t="s">
-        <v>114</v>
+        <v>111</v>
       </c>
       <c r="D37" t="s">
-        <v>115</v>
+        <v>112</v>
       </c>
     </row>
     <row r="38" spans="1:4" ht="12.75" customHeight="1">
       <c r="A38" t="s">
-        <v>439</v>
+        <v>435</v>
       </c>
       <c r="B38" t="s">
-        <v>116</v>
+        <v>113</v>
       </c>
       <c r="D38" t="s">
-        <v>120</v>
+        <v>117</v>
       </c>
     </row>
     <row r="39" spans="1:4" ht="12.75" customHeight="1">
       <c r="A39" t="s">
-        <v>439</v>
+        <v>435</v>
       </c>
       <c r="B39" t="s">
-        <v>117</v>
+        <v>114</v>
       </c>
       <c r="D39" t="s">
-        <v>121</v>
+        <v>118</v>
       </c>
     </row>
     <row r="40" spans="1:4" ht="12.75" customHeight="1">
       <c r="A40" t="s">
-        <v>439</v>
+        <v>435</v>
       </c>
       <c r="B40" t="s">
-        <v>118</v>
+        <v>115</v>
       </c>
       <c r="D40" t="s">
-        <v>122</v>
+        <v>119</v>
       </c>
     </row>
     <row r="41" spans="1:4" ht="12.75" customHeight="1">
       <c r="A41" t="s">
-        <v>439</v>
+        <v>435</v>
       </c>
       <c r="B41" t="s">
-        <v>119</v>
+        <v>116</v>
       </c>
       <c r="D41" t="s">
-        <v>123</v>
+        <v>120</v>
       </c>
     </row>
     <row r="43" spans="1:4" ht="12.75" customHeight="1">
       <c r="A43" t="s">
-        <v>443</v>
+        <v>439</v>
       </c>
       <c r="B43" t="s">
-        <v>485</v>
+        <v>481</v>
       </c>
       <c r="D43" t="s">
-        <v>135</v>
+        <v>132</v>
       </c>
     </row>
     <row r="44" spans="1:4" s="2" customFormat="1" ht="12.75" customHeight="1">
       <c r="A44" t="s">
-        <v>443</v>
+        <v>439</v>
       </c>
       <c r="B44" t="s">
-        <v>484</v>
+        <v>480</v>
       </c>
       <c r="D44" t="s">
-        <v>130</v>
+        <v>127</v>
       </c>
     </row>
     <row r="45" spans="1:4" ht="12.75" customHeight="1">
       <c r="A45" t="s">
-        <v>443</v>
+        <v>439</v>
       </c>
       <c r="B45" t="s">
-        <v>483</v>
+        <v>479</v>
       </c>
       <c r="D45" t="s">
-        <v>131</v>
+        <v>128</v>
       </c>
     </row>
     <row r="46" spans="1:4" ht="12.75" customHeight="1">
       <c r="A46" t="s">
-        <v>443</v>
+        <v>439</v>
       </c>
       <c r="B46" t="s">
-        <v>482</v>
+        <v>478</v>
       </c>
       <c r="D46" t="s">
-        <v>132</v>
+        <v>129</v>
       </c>
     </row>
     <row r="47" spans="1:4" ht="12.75" customHeight="1">
       <c r="A47" t="s">
-        <v>443</v>
+        <v>439</v>
       </c>
       <c r="B47" t="s">
-        <v>481</v>
+        <v>477</v>
       </c>
       <c r="D47" t="s">
-        <v>133</v>
+        <v>130</v>
       </c>
     </row>
     <row r="48" spans="1:4" ht="12.75" customHeight="1">
       <c r="A48" t="s">
-        <v>443</v>
+        <v>439</v>
       </c>
       <c r="B48" t="s">
-        <v>480</v>
+        <v>476</v>
       </c>
       <c r="D48" t="s">
-        <v>134</v>
+        <v>131</v>
       </c>
     </row>
     <row r="50" spans="1:4" ht="12.75" customHeight="1">
       <c r="A50" t="s">
-        <v>446</v>
+        <v>442</v>
       </c>
       <c r="B50" t="s">
-        <v>479</v>
+        <v>475</v>
       </c>
       <c r="C50" s="2"/>
       <c r="D50" t="s">
-        <v>136</v>
+        <v>133</v>
       </c>
     </row>
     <row r="51" spans="1:4" ht="12.75" customHeight="1">
       <c r="A51" t="s">
-        <v>446</v>
+        <v>442</v>
       </c>
       <c r="B51" t="s">
-        <v>478</v>
+        <v>474</v>
       </c>
       <c r="D51" t="s">
-        <v>137</v>
+        <v>134</v>
       </c>
     </row>
     <row r="52" spans="1:4" ht="12.75" customHeight="1">
       <c r="A52" t="s">
-        <v>446</v>
+        <v>442</v>
       </c>
       <c r="B52" t="s">
-        <v>477</v>
+        <v>473</v>
       </c>
       <c r="D52" t="s">
-        <v>138</v>
+        <v>135</v>
       </c>
     </row>
     <row r="53" spans="1:4" ht="12.75" customHeight="1">
       <c r="A53" t="s">
-        <v>446</v>
+        <v>442</v>
       </c>
       <c r="B53" t="s">
-        <v>476</v>
+        <v>472</v>
       </c>
       <c r="D53" t="s">
-        <v>139</v>
+        <v>136</v>
       </c>
     </row>
     <row r="54" spans="1:4" ht="12.75" customHeight="1">
       <c r="A54" t="s">
-        <v>446</v>
+        <v>442</v>
       </c>
       <c r="B54" t="s">
-        <v>475</v>
+        <v>471</v>
       </c>
       <c r="D54" t="s">
-        <v>140</v>
+        <v>137</v>
       </c>
     </row>
     <row r="56" spans="1:4" ht="12.75" customHeight="1">
       <c r="A56" t="s">
-        <v>449</v>
+        <v>445</v>
       </c>
       <c r="B56" t="s">
-        <v>175</v>
+        <v>172</v>
       </c>
       <c r="D56" t="s">
-        <v>168</v>
+        <v>165</v>
       </c>
     </row>
     <row r="57" spans="1:4" ht="12.75" customHeight="1">
       <c r="A57" t="s">
-        <v>449</v>
+        <v>445</v>
       </c>
       <c r="B57" t="s">
-        <v>176</v>
+        <v>173</v>
       </c>
       <c r="C57" s="2"/>
       <c r="D57" t="s">
-        <v>169</v>
+        <v>166</v>
       </c>
     </row>
     <row r="58" spans="1:4" ht="12.75" customHeight="1">
       <c r="A58" t="s">
-        <v>449</v>
+        <v>445</v>
       </c>
       <c r="B58" t="s">
-        <v>177</v>
+        <v>174</v>
       </c>
       <c r="D58" t="s">
-        <v>170</v>
+        <v>167</v>
       </c>
     </row>
     <row r="59" spans="1:4" ht="12.75" customHeight="1">
       <c r="A59" t="s">
-        <v>449</v>
+        <v>445</v>
       </c>
       <c r="B59" t="s">
-        <v>178</v>
+        <v>175</v>
       </c>
       <c r="D59" t="s">
-        <v>171</v>
+        <v>168</v>
       </c>
     </row>
     <row r="60" spans="1:4" ht="12.75" customHeight="1">
       <c r="A60" t="s">
-        <v>449</v>
+        <v>445</v>
       </c>
       <c r="B60" t="s">
-        <v>179</v>
+        <v>176</v>
       </c>
       <c r="D60" t="s">
-        <v>172</v>
+        <v>169</v>
       </c>
     </row>
     <row r="61" spans="1:4" ht="12.75" customHeight="1">
       <c r="A61" t="s">
-        <v>449</v>
+        <v>445</v>
       </c>
       <c r="B61" t="s">
-        <v>180</v>
+        <v>177</v>
       </c>
       <c r="D61" t="s">
-        <v>173</v>
+        <v>170</v>
       </c>
     </row>
     <row r="62" spans="1:4" ht="12.75" customHeight="1">
       <c r="A62" t="s">
-        <v>449</v>
+        <v>445</v>
       </c>
       <c r="B62" t="s">
-        <v>181</v>
+        <v>178</v>
       </c>
       <c r="D62" t="s">
-        <v>174</v>
+        <v>171</v>
       </c>
     </row>
     <row r="64" spans="1:4" ht="12.75" customHeight="1">
       <c r="A64" t="s">
-        <v>452</v>
+        <v>448</v>
       </c>
       <c r="B64" t="s">
-        <v>474</v>
+        <v>470</v>
       </c>
       <c r="D64" t="s">
-        <v>141</v>
+        <v>138</v>
       </c>
     </row>
     <row r="65" spans="1:4" ht="12.75" customHeight="1">
       <c r="A65" t="s">
-        <v>452</v>
+        <v>448</v>
       </c>
       <c r="B65" t="s">
-        <v>473</v>
+        <v>469</v>
       </c>
       <c r="C65" s="2"/>
       <c r="D65" t="s">
-        <v>142</v>
+        <v>139</v>
       </c>
     </row>
     <row r="66" spans="1:4" ht="12.75" customHeight="1">
       <c r="A66" t="s">
-        <v>452</v>
+        <v>448</v>
       </c>
       <c r="B66" t="s">
-        <v>472</v>
+        <v>468</v>
       </c>
       <c r="D66" t="s">
-        <v>143</v>
+        <v>140</v>
       </c>
     </row>
     <row r="67" spans="1:4" ht="12.75" customHeight="1">
       <c r="A67" t="s">
-        <v>452</v>
+        <v>448</v>
       </c>
       <c r="B67" t="s">
-        <v>471</v>
+        <v>467</v>
       </c>
       <c r="D67" t="s">
-        <v>144</v>
+        <v>141</v>
       </c>
     </row>
     <row r="68" spans="1:4" ht="12.75" customHeight="1">
       <c r="A68" t="s">
-        <v>452</v>
+        <v>448</v>
       </c>
       <c r="B68" t="s">
-        <v>470</v>
+        <v>466</v>
       </c>
       <c r="D68" t="s">
-        <v>145</v>
+        <v>142</v>
       </c>
     </row>
     <row r="69" spans="1:4" ht="12.75" customHeight="1">
       <c r="A69" t="s">
-        <v>452</v>
+        <v>448</v>
       </c>
       <c r="B69" t="s">
-        <v>469</v>
+        <v>465</v>
       </c>
       <c r="D69" t="s">
-        <v>146</v>
+        <v>143</v>
       </c>
     </row>
     <row r="71" spans="1:4" ht="12.75" customHeight="1">
       <c r="A71" t="s">
-        <v>455</v>
+        <v>451</v>
       </c>
       <c r="B71" t="s">
-        <v>468</v>
+        <v>464</v>
       </c>
       <c r="D71" t="s">
-        <v>147</v>
+        <v>144</v>
       </c>
     </row>
     <row r="72" spans="1:4" ht="12.75" customHeight="1">
       <c r="A72" t="s">
-        <v>455</v>
+        <v>451</v>
       </c>
       <c r="B72" t="s">
-        <v>467</v>
+        <v>463</v>
       </c>
       <c r="C72" s="2"/>
       <c r="D72" t="s">
-        <v>148</v>
+        <v>145</v>
       </c>
     </row>
     <row r="73" spans="1:4" ht="12.75" customHeight="1">
       <c r="A73" t="s">
-        <v>455</v>
+        <v>451</v>
       </c>
       <c r="B73" t="s">
-        <v>466</v>
+        <v>462</v>
       </c>
       <c r="D73" t="s">
-        <v>149</v>
+        <v>146</v>
       </c>
     </row>
     <row r="74" spans="1:4" ht="12.75" customHeight="1">
       <c r="A74" t="s">
-        <v>455</v>
+        <v>451</v>
       </c>
       <c r="B74" t="s">
-        <v>465</v>
+        <v>461</v>
       </c>
       <c r="D74" t="s">
-        <v>150</v>
+        <v>147</v>
       </c>
     </row>
     <row r="75" spans="1:4" ht="12.75" customHeight="1">
       <c r="A75" t="s">
-        <v>455</v>
+        <v>451</v>
       </c>
       <c r="B75" t="s">
-        <v>464</v>
+        <v>460</v>
       </c>
       <c r="D75" t="s">
-        <v>151</v>
+        <v>148</v>
       </c>
     </row>
     <row r="76" spans="1:4" ht="12.75" customHeight="1">
       <c r="A76" t="s">
-        <v>455</v>
+        <v>451</v>
       </c>
       <c r="B76" t="s">
-        <v>463</v>
+        <v>459</v>
       </c>
       <c r="D76" t="s">
-        <v>152</v>
+        <v>149</v>
       </c>
     </row>
     <row r="78" spans="1:4" ht="12.75" customHeight="1">
       <c r="A78" t="s">
-        <v>192</v>
+        <v>189</v>
       </c>
       <c r="B78" t="s">
-        <v>198</v>
+        <v>195</v>
       </c>
       <c r="C78" t="s">
-        <v>205</v>
+        <v>202</v>
       </c>
     </row>
     <row r="79" spans="1:4" ht="12.75" customHeight="1">
       <c r="A79" t="s">
-        <v>192</v>
+        <v>189</v>
       </c>
       <c r="B79" t="s">
-        <v>199</v>
+        <v>196</v>
       </c>
       <c r="C79" t="s">
-        <v>206</v>
+        <v>203</v>
       </c>
     </row>
     <row r="80" spans="1:4" ht="12.75" customHeight="1">
       <c r="A80" t="s">
-        <v>192</v>
+        <v>189</v>
       </c>
       <c r="B80" t="s">
-        <v>200</v>
+        <v>197</v>
       </c>
       <c r="C80" t="s">
-        <v>207</v>
+        <v>204</v>
       </c>
     </row>
     <row r="81" spans="1:3" ht="12.75" customHeight="1">
       <c r="A81" t="s">
-        <v>192</v>
+        <v>189</v>
       </c>
       <c r="B81" t="s">
-        <v>201</v>
+        <v>198</v>
       </c>
       <c r="C81" t="s">
-        <v>208</v>
+        <v>205</v>
       </c>
     </row>
     <row r="82" spans="1:3" ht="12.75" customHeight="1">
       <c r="A82" t="s">
-        <v>192</v>
+        <v>189</v>
       </c>
       <c r="B82" t="s">
-        <v>202</v>
+        <v>199</v>
       </c>
       <c r="C82" t="s">
-        <v>209</v>
+        <v>206</v>
       </c>
     </row>
     <row r="83" spans="1:3" ht="12.75" customHeight="1">
       <c r="A83" t="s">
-        <v>192</v>
+        <v>189</v>
       </c>
       <c r="B83" t="s">
-        <v>203</v>
+        <v>200</v>
       </c>
       <c r="C83" t="s">
-        <v>210</v>
+        <v>207</v>
       </c>
     </row>
     <row r="84" spans="1:3" ht="12.75" customHeight="1">
       <c r="A84" t="s">
-        <v>192</v>
+        <v>189</v>
       </c>
       <c r="B84" t="s">
-        <v>204</v>
+        <v>201</v>
       </c>
       <c r="C84" t="s">
-        <v>211</v>
+        <v>208</v>
       </c>
     </row>
     <row r="86" spans="1:3" ht="12.75" customHeight="1">
       <c r="A86" t="s">
-        <v>193</v>
+        <v>190</v>
       </c>
       <c r="B86" t="s">
-        <v>218</v>
+        <v>215</v>
       </c>
       <c r="C86" t="s">
-        <v>224</v>
+        <v>221</v>
       </c>
     </row>
     <row r="87" spans="1:3" ht="12.75" customHeight="1">
       <c r="A87" t="s">
-        <v>193</v>
+        <v>190</v>
       </c>
       <c r="B87" t="s">
-        <v>219</v>
+        <v>216</v>
       </c>
       <c r="C87" t="s">
-        <v>225</v>
+        <v>222</v>
       </c>
     </row>
     <row r="88" spans="1:3" ht="12.75" customHeight="1">
       <c r="A88" t="s">
-        <v>193</v>
+        <v>190</v>
       </c>
       <c r="B88" t="s">
-        <v>220</v>
+        <v>217</v>
       </c>
       <c r="C88" t="s">
-        <v>226</v>
+        <v>223</v>
       </c>
     </row>
     <row r="89" spans="1:3" ht="12.75" customHeight="1">
       <c r="A89" t="s">
-        <v>193</v>
+        <v>190</v>
       </c>
       <c r="B89" t="s">
-        <v>221</v>
+        <v>218</v>
       </c>
       <c r="C89" t="s">
-        <v>227</v>
+        <v>224</v>
       </c>
     </row>
     <row r="90" spans="1:3" ht="12.75" customHeight="1">
       <c r="A90" t="s">
-        <v>193</v>
+        <v>190</v>
       </c>
       <c r="B90" t="s">
-        <v>222</v>
+        <v>219</v>
       </c>
       <c r="C90" t="s">
-        <v>228</v>
+        <v>225</v>
       </c>
     </row>
     <row r="91" spans="1:3" ht="12.75" customHeight="1">
       <c r="A91" t="s">
-        <v>193</v>
+        <v>190</v>
       </c>
       <c r="B91" t="s">
-        <v>223</v>
+        <v>220</v>
       </c>
       <c r="C91" t="s">
-        <v>229</v>
+        <v>226</v>
       </c>
     </row>
     <row r="93" spans="1:3" ht="12.75" customHeight="1">
       <c r="A93" t="s">
-        <v>194</v>
+        <v>191</v>
       </c>
       <c r="B93" t="s">
-        <v>236</v>
+        <v>233</v>
       </c>
       <c r="C93" t="s">
-        <v>237</v>
+        <v>234</v>
       </c>
     </row>
     <row r="94" spans="1:3" ht="12.75" customHeight="1">
       <c r="A94" t="s">
-        <v>194</v>
+        <v>191</v>
       </c>
       <c r="B94" t="s">
-        <v>230</v>
+        <v>227</v>
       </c>
       <c r="C94" t="s">
-        <v>238</v>
+        <v>235</v>
       </c>
     </row>
     <row r="95" spans="1:3" ht="12.75" customHeight="1">
       <c r="A95" t="s">
-        <v>194</v>
+        <v>191</v>
       </c>
       <c r="B95" t="s">
-        <v>231</v>
+        <v>228</v>
       </c>
       <c r="C95" t="s">
-        <v>239</v>
+        <v>236</v>
       </c>
     </row>
     <row r="96" spans="1:3" ht="12.75" customHeight="1">
       <c r="A96" t="s">
-        <v>194</v>
+        <v>191</v>
       </c>
       <c r="B96" t="s">
-        <v>232</v>
+        <v>229</v>
       </c>
       <c r="C96" t="s">
-        <v>240</v>
+        <v>237</v>
       </c>
     </row>
     <row r="97" spans="1:3" ht="12.75" customHeight="1">
       <c r="A97" t="s">
-        <v>194</v>
+        <v>191</v>
       </c>
       <c r="B97" t="s">
-        <v>233</v>
+        <v>230</v>
       </c>
       <c r="C97" t="s">
-        <v>241</v>
+        <v>238</v>
       </c>
     </row>
     <row r="98" spans="1:3" ht="12.75" customHeight="1">
       <c r="A98" t="s">
-        <v>194</v>
+        <v>191</v>
       </c>
       <c r="B98" t="s">
-        <v>234</v>
+        <v>231</v>
       </c>
       <c r="C98" t="s">
-        <v>242</v>
+        <v>239</v>
       </c>
     </row>
     <row r="99" spans="1:3" ht="12.75" customHeight="1">
       <c r="A99" t="s">
-        <v>194</v>
+        <v>191</v>
       </c>
       <c r="B99" t="s">
-        <v>235</v>
+        <v>232</v>
       </c>
       <c r="C99" t="s">
-        <v>243</v>
+        <v>240</v>
       </c>
     </row>
     <row r="101" spans="1:3" ht="12.75" customHeight="1">
       <c r="A101" t="s">
-        <v>195</v>
+        <v>192</v>
       </c>
       <c r="B101" t="s">
-        <v>244</v>
+        <v>241</v>
       </c>
       <c r="C101" t="s">
-        <v>250</v>
+        <v>247</v>
       </c>
     </row>
     <row r="102" spans="1:3" ht="12.75" customHeight="1">
       <c r="A102" t="s">
-        <v>195</v>
+        <v>192</v>
       </c>
       <c r="B102" t="s">
-        <v>245</v>
+        <v>242</v>
       </c>
       <c r="C102" t="s">
-        <v>251</v>
+        <v>248</v>
       </c>
     </row>
     <row r="103" spans="1:3" ht="12.75" customHeight="1">
       <c r="A103" t="s">
-        <v>195</v>
+        <v>192</v>
       </c>
       <c r="B103" t="s">
-        <v>246</v>
+        <v>243</v>
       </c>
       <c r="C103" t="s">
-        <v>252</v>
+        <v>249</v>
       </c>
     </row>
     <row r="104" spans="1:3" ht="12.75" customHeight="1">
       <c r="A104" t="s">
-        <v>195</v>
+        <v>192</v>
       </c>
       <c r="B104" t="s">
-        <v>247</v>
+        <v>244</v>
       </c>
       <c r="C104" t="s">
-        <v>253</v>
+        <v>250</v>
       </c>
     </row>
     <row r="105" spans="1:3" ht="12.75" customHeight="1">
       <c r="A105" t="s">
-        <v>195</v>
+        <v>192</v>
       </c>
       <c r="B105" t="s">
-        <v>248</v>
+        <v>245</v>
       </c>
       <c r="C105" t="s">
-        <v>254</v>
+        <v>251</v>
       </c>
     </row>
     <row r="106" spans="1:3" ht="12.75" customHeight="1">
       <c r="A106" t="s">
-        <v>195</v>
+        <v>192</v>
       </c>
       <c r="B106" t="s">
-        <v>249</v>
+        <v>246</v>
       </c>
       <c r="C106" t="s">
-        <v>255</v>
+        <v>252</v>
       </c>
     </row>
     <row r="108" spans="1:3" ht="12.75" customHeight="1">
       <c r="A108" t="s">
-        <v>196</v>
+        <v>193</v>
       </c>
       <c r="B108" t="s">
-        <v>262</v>
+        <v>259</v>
       </c>
       <c r="C108" t="s">
-        <v>263</v>
+        <v>260</v>
       </c>
     </row>
     <row r="109" spans="1:3" ht="12.75" customHeight="1">
       <c r="A109" t="s">
-        <v>196</v>
+        <v>193</v>
       </c>
       <c r="B109" t="s">
-        <v>256</v>
+        <v>253</v>
       </c>
       <c r="C109" t="s">
-        <v>264</v>
+        <v>261</v>
       </c>
     </row>
     <row r="110" spans="1:3" ht="12.75" customHeight="1">
       <c r="A110" t="s">
-        <v>196</v>
+        <v>193</v>
       </c>
       <c r="B110" t="s">
-        <v>257</v>
+        <v>254</v>
       </c>
       <c r="C110" t="s">
-        <v>265</v>
+        <v>262</v>
       </c>
     </row>
     <row r="111" spans="1:3" ht="12.75" customHeight="1">
       <c r="A111" t="s">
-        <v>196</v>
+        <v>193</v>
       </c>
       <c r="B111" t="s">
-        <v>259</v>
+        <v>256</v>
       </c>
       <c r="C111" t="s">
-        <v>266</v>
+        <v>263</v>
       </c>
     </row>
     <row r="112" spans="1:3" ht="12.75" customHeight="1">
       <c r="A112" t="s">
-        <v>196</v>
+        <v>193</v>
       </c>
       <c r="B112" t="s">
-        <v>258</v>
+        <v>255</v>
       </c>
       <c r="C112" t="s">
-        <v>267</v>
+        <v>264</v>
       </c>
     </row>
     <row r="113" spans="1:4" ht="12.75" customHeight="1">
       <c r="A113" t="s">
-        <v>196</v>
+        <v>193</v>
       </c>
       <c r="B113" t="s">
-        <v>260</v>
+        <v>257</v>
       </c>
       <c r="C113" t="s">
-        <v>268</v>
+        <v>265</v>
       </c>
     </row>
     <row r="114" spans="1:4" ht="12.75" customHeight="1">
       <c r="A114" t="s">
-        <v>196</v>
+        <v>193</v>
       </c>
       <c r="B114" t="s">
-        <v>261</v>
+        <v>258</v>
       </c>
       <c r="C114" t="s">
-        <v>269</v>
+        <v>266</v>
       </c>
     </row>
     <row r="116" spans="1:4" ht="12.75" customHeight="1">
       <c r="A116" t="s">
-        <v>197</v>
+        <v>194</v>
       </c>
       <c r="B116" t="s">
-        <v>270</v>
+        <v>267</v>
       </c>
       <c r="C116" t="s">
-        <v>276</v>
+        <v>273</v>
       </c>
     </row>
     <row r="117" spans="1:4" ht="12.75" customHeight="1">
       <c r="A117" t="s">
-        <v>197</v>
+        <v>194</v>
       </c>
       <c r="B117" t="s">
-        <v>271</v>
+        <v>268</v>
       </c>
       <c r="C117" t="s">
-        <v>277</v>
+        <v>274</v>
       </c>
     </row>
     <row r="118" spans="1:4" ht="12.75" customHeight="1">
       <c r="A118" t="s">
-        <v>197</v>
+        <v>194</v>
       </c>
       <c r="B118" t="s">
-        <v>272</v>
+        <v>269</v>
       </c>
       <c r="C118" t="s">
-        <v>278</v>
+        <v>275</v>
       </c>
     </row>
     <row r="119" spans="1:4" ht="12.75" customHeight="1">
       <c r="A119" t="s">
-        <v>197</v>
+        <v>194</v>
       </c>
       <c r="B119" t="s">
-        <v>273</v>
+        <v>270</v>
       </c>
       <c r="C119" t="s">
-        <v>279</v>
+        <v>276</v>
       </c>
     </row>
     <row r="120" spans="1:4" ht="12.75" customHeight="1">
       <c r="A120" t="s">
-        <v>197</v>
+        <v>194</v>
       </c>
       <c r="B120" t="s">
-        <v>274</v>
+        <v>271</v>
       </c>
       <c r="C120" t="s">
-        <v>280</v>
+        <v>277</v>
       </c>
     </row>
     <row r="121" spans="1:4" ht="12.75" customHeight="1">
       <c r="A121" t="s">
-        <v>197</v>
+        <v>194</v>
       </c>
       <c r="B121" t="s">
-        <v>275</v>
+        <v>272</v>
       </c>
       <c r="C121" t="s">
-        <v>281</v>
+        <v>278</v>
       </c>
     </row>
     <row r="123" spans="1:4" ht="12.75" customHeight="1">
       <c r="A123" t="s">
-        <v>335</v>
+        <v>332</v>
       </c>
       <c r="B123" t="s">
-        <v>330</v>
+        <v>327</v>
       </c>
       <c r="C123" t="s">
-        <v>324</v>
+        <v>321</v>
       </c>
     </row>
     <row r="124" spans="1:4" ht="12.75" customHeight="1">
       <c r="A124" t="s">
-        <v>335</v>
+        <v>332</v>
       </c>
       <c r="B124" t="s">
-        <v>331</v>
+        <v>328</v>
       </c>
       <c r="C124" t="s">
-        <v>332</v>
+        <v>329</v>
       </c>
     </row>
     <row r="126" spans="1:4" ht="12.75" customHeight="1">
       <c r="A126" s="2" t="s">
-        <v>428</v>
+        <v>424</v>
       </c>
       <c r="D126" t="s">
-        <v>429</v>
+        <v>425</v>
       </c>
     </row>
     <row r="127" spans="1:4" ht="12.75" customHeight="1">
       <c r="A127" t="s">
-        <v>428</v>
+        <v>424</v>
       </c>
       <c r="D127" t="s">
-        <v>430</v>
+        <v>426</v>
       </c>
     </row>
     <row r="128" spans="1:4" ht="12.75" customHeight="1">
       <c r="A128" s="2" t="s">
-        <v>428</v>
+        <v>424</v>
       </c>
       <c r="D128" t="s">
-        <v>431</v>
+        <v>427</v>
       </c>
     </row>
     <row r="129" spans="1:4" ht="12.75" customHeight="1">
       <c r="A129" s="2" t="s">
+        <v>424</v>
+      </c>
+      <c r="D129" t="s">
         <v>428</v>
-      </c>
-      <c r="D129" t="s">
-        <v>432</v>
       </c>
     </row>
     <row r="130" spans="1:4" ht="12.75" customHeight="1">
       <c r="A130" s="2" t="s">
-        <v>428</v>
+        <v>424</v>
       </c>
       <c r="D130" t="s">
-        <v>433</v>
+        <v>429</v>
       </c>
     </row>
     <row r="132" spans="1:4" ht="12.75" customHeight="1">
       <c r="A132" t="s">
-        <v>487</v>
+        <v>483</v>
       </c>
       <c r="D132" t="s">
-        <v>488</v>
+        <v>484</v>
       </c>
     </row>
     <row r="133" spans="1:4" ht="12.75" customHeight="1">
       <c r="A133" t="s">
-        <v>487</v>
+        <v>483</v>
       </c>
       <c r="D133" t="s">
-        <v>489</v>
+        <v>485</v>
       </c>
     </row>
     <row r="134" spans="1:4" ht="12.75" customHeight="1">
       <c r="A134" t="s">
-        <v>487</v>
+        <v>483</v>
       </c>
       <c r="D134" t="s">
-        <v>490</v>
+        <v>486</v>
       </c>
     </row>
     <row r="135" spans="1:4" ht="12.75" customHeight="1">
       <c r="A135" t="s">
+        <v>483</v>
+      </c>
+      <c r="D135" t="s">
         <v>487</v>
-      </c>
-      <c r="D135" t="s">
-        <v>491</v>
       </c>
     </row>
     <row r="136" spans="1:4" ht="12.75" customHeight="1">
       <c r="A136" t="s">
-        <v>487</v>
+        <v>483</v>
       </c>
       <c r="D136" t="s">
-        <v>492</v>
+        <v>488</v>
       </c>
     </row>
   </sheetData>
@@ -6647,26 +6620,26 @@
   <sheetData>
     <row r="1" spans="1:2" ht="12.75" customHeight="1">
       <c r="A1" t="s">
+        <v>47</v>
+      </c>
+      <c r="B1" t="s">
         <v>48</v>
-      </c>
-      <c r="B1" t="s">
-        <v>49</v>
       </c>
     </row>
     <row r="2" spans="1:2" ht="12.75" customHeight="1">
       <c r="A2" t="s">
+        <v>49</v>
+      </c>
+      <c r="B2" t="s">
         <v>50</v>
-      </c>
-      <c r="B2" t="s">
-        <v>51</v>
       </c>
     </row>
     <row r="3" spans="1:2" ht="12.75" customHeight="1">
       <c r="A3" t="s">
+        <v>51</v>
+      </c>
+      <c r="B3" t="s">
         <v>52</v>
-      </c>
-      <c r="B3" t="s">
-        <v>53</v>
       </c>
     </row>
   </sheetData>
@@ -6694,15 +6667,15 @@
         <v>1</v>
       </c>
       <c r="B1" t="s">
-        <v>124</v>
+        <v>121</v>
       </c>
     </row>
     <row r="2" spans="1:2">
       <c r="A2" t="s">
-        <v>125</v>
+        <v>122</v>
       </c>
       <c r="B2" t="s">
-        <v>126</v>
+        <v>123</v>
       </c>
     </row>
     <row r="3" spans="1:2">
@@ -6710,15 +6683,15 @@
         <v>4</v>
       </c>
       <c r="B3" t="s">
-        <v>126</v>
+        <v>123</v>
       </c>
     </row>
     <row r="4" spans="1:2">
       <c r="A4" t="s">
-        <v>435</v>
+        <v>431</v>
       </c>
       <c r="B4" t="s">
-        <v>126</v>
+        <v>123</v>
       </c>
     </row>
   </sheetData>

</xml_diff>

<commit_message>
try to push to heroku
</commit_message>
<xml_diff>
--- a/opendatakit.collect2/form-files/neonatal/neonatal.xlsx
+++ b/opendatakit.collect2/form-files/neonatal/neonatal.xlsx
@@ -4,7 +4,7 @@
   <fileVersion appName="xl" lastEdited="5" lowestEdited="5" rupBuild="22905"/>
   <workbookPr autoCompressPictures="0"/>
   <bookViews>
-    <workbookView xWindow="0" yWindow="0" windowWidth="21640" windowHeight="15560" tabRatio="500" activeTab="2"/>
+    <workbookView xWindow="3200" yWindow="140" windowWidth="21640" windowHeight="15560" tabRatio="500" activeTab="2"/>
   </bookViews>
   <sheets>
     <sheet name="survey" sheetId="1" r:id="rId1"/>
@@ -5359,7 +5359,7 @@
   <dimension ref="A1:D136"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="C17" sqref="C17"/>
+      <selection activeCell="C2" sqref="C2"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultColWidth="17.1640625" defaultRowHeight="12.75" customHeight="1" x14ac:dyDescent="0"/>

</xml_diff>

<commit_message>
display in two columns, add abdominal and chest xray, add umbilical ref
</commit_message>
<xml_diff>
--- a/opendatakit.collect2/form-files/neonatal/neonatal.xlsx
+++ b/opendatakit.collect2/form-files/neonatal/neonatal.xlsx
@@ -1,10 +1,10 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
-  <fileVersion appName="xl" lastEdited="5" lowestEdited="5" rupBuild="21721"/>
+  <fileVersion appName="xl" lastEdited="5" lowestEdited="5" rupBuild="22905"/>
   <workbookPr autoCompressPictures="0"/>
   <bookViews>
-    <workbookView xWindow="10860" yWindow="0" windowWidth="14380" windowHeight="15300" tabRatio="500"/>
+    <workbookView xWindow="1800" yWindow="0" windowWidth="18360" windowHeight="15280" tabRatio="500" activeTab="1"/>
   </bookViews>
   <sheets>
     <sheet name="survey" sheetId="1" r:id="rId1"/>
@@ -23,7 +23,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="869" uniqueCount="535">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="870" uniqueCount="536">
   <si>
     <t>type</t>
   </si>
@@ -497,9 +497,6 @@
   </si>
   <si>
     <t>xray</t>
-  </si>
-  <si>
-    <t>img/diagnostic_icons/chest.jpg</t>
   </si>
   <si>
     <t>ballardExam</t>
@@ -1489,9 +1486,6 @@
     <t>&lt;h1&gt;Lumbar&lt;/h1&gt;</t>
   </si>
   <si>
-    <t>&lt;h1&gt;Umbilical Venous &amp; Arterial Catheters&lt;/h1&gt;</t>
-  </si>
-  <si>
     <t>&lt;h2&gt;Intubation Video&lt;/h2&gt;</t>
   </si>
   <si>
@@ -1835,6 +1829,15 @@
   </si>
   <si>
     <t>selected(data('newborn_menu'),'ballardExam')</t>
+  </si>
+  <si>
+    <t>templates/umbilical.handlebars</t>
+  </si>
+  <si>
+    <t>templates/chest_abdomen.handlebars</t>
+  </si>
+  <si>
+    <t>Chest and Abdominal XRAY</t>
   </si>
 </sst>
 </file>
@@ -3275,8 +3278,9 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:J194"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A64" workbookViewId="0">
-      <selection activeCell="A97" sqref="A97"/>
+    <sheetView topLeftCell="C1" workbookViewId="0">
+      <pane ySplit="1" topLeftCell="A29" activePane="bottomLeft" state="frozen"/>
+      <selection pane="bottomLeft" activeCell="D34" sqref="D34"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultColWidth="11.5" defaultRowHeight="12.75" customHeight="1" x14ac:dyDescent="0"/>
@@ -3345,12 +3349,12 @@
     <row r="4" spans="1:10" s="35" customFormat="1" ht="15">
       <c r="A4" s="12"/>
       <c r="B4" s="33" t="s">
-        <v>374</v>
+        <v>373</v>
       </c>
       <c r="C4" s="33"/>
       <c r="D4" s="33"/>
       <c r="E4" s="33" t="s">
-        <v>375</v>
+        <v>374</v>
       </c>
       <c r="F4" s="33"/>
       <c r="G4" s="33"/>
@@ -3361,12 +3365,12 @@
     <row r="5" spans="1:10" ht="12">
       <c r="A5" s="12"/>
       <c r="B5" s="22" t="s">
-        <v>376</v>
+        <v>375</v>
       </c>
       <c r="C5" s="22"/>
       <c r="D5" s="22"/>
       <c r="E5" s="23" t="s">
-        <v>377</v>
+        <v>376</v>
       </c>
       <c r="F5" s="22"/>
       <c r="G5" s="22"/>
@@ -3374,10 +3378,10 @@
     </row>
     <row r="6" spans="1:10" ht="15">
       <c r="A6" s="7" t="s">
-        <v>503</v>
+        <v>501</v>
       </c>
       <c r="B6" s="8" t="s">
-        <v>378</v>
+        <v>377</v>
       </c>
       <c r="C6" s="8"/>
       <c r="D6" s="8"/>
@@ -3389,13 +3393,13 @@
     <row r="7" spans="1:10" ht="12">
       <c r="A7" s="7"/>
       <c r="B7" s="3" t="s">
-        <v>379</v>
+        <v>378</v>
       </c>
       <c r="C7" s="3" t="s">
         <v>147</v>
       </c>
       <c r="D7" s="3" t="s">
-        <v>380</v>
+        <v>379</v>
       </c>
       <c r="E7" s="3"/>
       <c r="F7" s="3" t="s">
@@ -3412,7 +3416,7 @@
       <c r="C8" s="25"/>
       <c r="D8" s="25"/>
       <c r="E8" s="4" t="s">
-        <v>381</v>
+        <v>380</v>
       </c>
       <c r="F8" s="25"/>
       <c r="G8" s="12"/>
@@ -3430,7 +3434,7 @@
       <c r="G9" s="12"/>
       <c r="H9" s="12"/>
       <c r="I9" t="s">
-        <v>382</v>
+        <v>381</v>
       </c>
     </row>
     <row r="10" spans="1:10" ht="12.75" customHeight="1">
@@ -3439,7 +3443,7 @@
         <v>4</v>
       </c>
       <c r="D10" t="s">
-        <v>420</v>
+        <v>418</v>
       </c>
       <c r="E10" s="14"/>
     </row>
@@ -3449,7 +3453,7 @@
         <v>4</v>
       </c>
       <c r="H11" t="s">
-        <v>383</v>
+        <v>382</v>
       </c>
     </row>
     <row r="12" spans="1:10" ht="12">
@@ -3459,7 +3463,7 @@
       </c>
       <c r="C12" s="3"/>
       <c r="D12" s="27" t="s">
-        <v>421</v>
+        <v>419</v>
       </c>
       <c r="E12" s="3"/>
       <c r="F12" s="3"/>
@@ -3473,7 +3477,7 @@
       </c>
       <c r="C13" s="9"/>
       <c r="D13" s="29" t="s">
-        <v>422</v>
+        <v>420</v>
       </c>
       <c r="E13" s="29"/>
       <c r="F13" s="9"/>
@@ -3498,7 +3502,7 @@
       <c r="C15" s="25"/>
       <c r="D15" s="25"/>
       <c r="E15" s="4" t="s">
-        <v>387</v>
+        <v>386</v>
       </c>
     </row>
     <row r="16" spans="1:10" s="12" customFormat="1" ht="12">
@@ -3507,7 +3511,7 @@
         <v>4</v>
       </c>
       <c r="D16" s="12" t="s">
-        <v>418</v>
+        <v>417</v>
       </c>
     </row>
     <row r="17" spans="1:10" s="12" customFormat="1" ht="12">
@@ -3524,7 +3528,7 @@
       <c r="C18" s="25"/>
       <c r="D18" s="25"/>
       <c r="E18" s="4" t="s">
-        <v>398</v>
+        <v>397</v>
       </c>
     </row>
     <row r="19" spans="1:10" s="12" customFormat="1" ht="13" customHeight="1">
@@ -3532,8 +3536,9 @@
       <c r="B19" s="12" t="s">
         <v>4</v>
       </c>
-      <c r="D19" t="s">
-        <v>419</v>
+      <c r="D19"/>
+      <c r="I19" s="12" t="s">
+        <v>533</v>
       </c>
     </row>
     <row r="20" spans="1:10" s="12" customFormat="1" ht="12">
@@ -3545,7 +3550,7 @@
     <row r="21" spans="1:10" ht="15">
       <c r="A21" s="16"/>
       <c r="B21" s="8" t="s">
-        <v>384</v>
+        <v>383</v>
       </c>
       <c r="C21" s="30"/>
       <c r="D21" s="31"/>
@@ -3555,22 +3560,22 @@
     <row r="23" spans="1:10" s="15" customFormat="1" ht="12.75" customHeight="1">
       <c r="A23" s="37"/>
       <c r="B23" s="14" t="s">
-        <v>433</v>
+        <v>431</v>
       </c>
       <c r="E23" s="15" t="s">
-        <v>438</v>
+        <v>436</v>
       </c>
       <c r="I23" s="3"/>
       <c r="J23" s="3"/>
     </row>
     <row r="24" spans="1:10" ht="15">
       <c r="B24" s="14" t="s">
-        <v>434</v>
+        <v>432</v>
       </c>
       <c r="C24" s="15"/>
       <c r="D24" s="15"/>
       <c r="E24" s="15" t="s">
-        <v>437</v>
+        <v>435</v>
       </c>
       <c r="F24" s="15"/>
       <c r="G24" s="15"/>
@@ -3578,10 +3583,10 @@
     </row>
     <row r="25" spans="1:10" ht="15">
       <c r="A25" s="7" t="s">
-        <v>504</v>
+        <v>502</v>
       </c>
       <c r="B25" s="8" t="s">
-        <v>435</v>
+        <v>433</v>
       </c>
       <c r="C25" s="13"/>
       <c r="D25" s="13"/>
@@ -3593,13 +3598,13 @@
     <row r="26" spans="1:10" ht="12">
       <c r="A26" s="12"/>
       <c r="B26" s="3" t="s">
-        <v>439</v>
+        <v>437</v>
       </c>
       <c r="C26" s="3" t="s">
-        <v>440</v>
+        <v>438</v>
       </c>
       <c r="D26" s="3" t="s">
-        <v>394</v>
+        <v>393</v>
       </c>
       <c r="E26" s="3"/>
       <c r="F26" s="3" t="s">
@@ -3610,15 +3615,15 @@
     </row>
     <row r="27" spans="1:10" ht="12.75" customHeight="1">
       <c r="A27" s="7" t="s">
-        <v>443</v>
+        <v>441</v>
       </c>
       <c r="B27" s="40" t="s">
-        <v>446</v>
+        <v>444</v>
       </c>
       <c r="C27" s="40"/>
       <c r="D27" s="40"/>
       <c r="E27" s="40" t="s">
-        <v>498</v>
+        <v>496</v>
       </c>
       <c r="F27" s="40"/>
       <c r="G27" s="40"/>
@@ -3627,12 +3632,12 @@
     <row r="28" spans="1:10" ht="12.75" customHeight="1">
       <c r="A28" s="7"/>
       <c r="B28" s="40" t="s">
-        <v>447</v>
+        <v>445</v>
       </c>
       <c r="C28" s="40"/>
       <c r="D28" s="40"/>
       <c r="E28" s="40" t="s">
-        <v>499</v>
+        <v>497</v>
       </c>
       <c r="F28" s="40"/>
       <c r="G28" s="40"/>
@@ -3641,7 +3646,7 @@
     <row r="29" spans="1:10" s="3" customFormat="1" ht="18" customHeight="1">
       <c r="A29" s="41"/>
       <c r="B29" s="13" t="s">
-        <v>448</v>
+        <v>446</v>
       </c>
       <c r="C29" s="13"/>
       <c r="D29" s="13"/>
@@ -3653,13 +3658,13 @@
     <row r="30" spans="1:10" s="3" customFormat="1" ht="18" customHeight="1">
       <c r="A30" s="41"/>
       <c r="B30" t="s">
-        <v>449</v>
+        <v>447</v>
       </c>
       <c r="C30" t="s">
         <v>152</v>
       </c>
       <c r="D30" t="s">
-        <v>443</v>
+        <v>441</v>
       </c>
       <c r="E30"/>
       <c r="F30" t="s">
@@ -3669,20 +3674,20 @@
     <row r="31" spans="1:10" ht="24">
       <c r="A31" s="7"/>
       <c r="B31" s="2" t="s">
-        <v>450</v>
+        <v>448</v>
       </c>
       <c r="C31" s="2" t="s">
-        <v>327</v>
+        <v>326</v>
       </c>
       <c r="D31" s="2" t="s">
-        <v>161</v>
+        <v>160</v>
       </c>
       <c r="E31" s="2" t="s">
-        <v>451</v>
+        <v>449</v>
       </c>
       <c r="F31" s="2"/>
       <c r="G31" t="s">
-        <v>452</v>
+        <v>450</v>
       </c>
     </row>
     <row r="32" spans="1:10" ht="18" customHeight="1">
@@ -3693,45 +3698,48 @@
       <c r="C32" s="2"/>
       <c r="D32" s="2"/>
       <c r="E32" s="2" t="s">
-        <v>453</v>
+        <v>451</v>
       </c>
       <c r="F32" s="2"/>
       <c r="I32" t="s">
-        <v>500</v>
+        <v>498</v>
       </c>
     </row>
     <row r="33" spans="1:9" ht="18" customHeight="1">
       <c r="A33" s="7"/>
       <c r="B33" s="2" t="s">
-        <v>454</v>
+        <v>452</v>
       </c>
       <c r="C33" s="19"/>
       <c r="D33" s="2" t="s">
-        <v>455</v>
+        <v>453</v>
       </c>
       <c r="E33" s="2" t="s">
-        <v>456</v>
+        <v>454</v>
       </c>
       <c r="F33" s="2"/>
     </row>
     <row r="34" spans="1:9" ht="18" customHeight="1">
       <c r="A34" s="7"/>
       <c r="B34" s="2" t="s">
-        <v>454</v>
+        <v>452</v>
       </c>
       <c r="C34" s="19"/>
       <c r="D34" s="2" t="s">
-        <v>457</v>
+        <v>455</v>
       </c>
       <c r="E34" s="2" t="s">
-        <v>458</v>
+        <v>456</v>
       </c>
       <c r="F34" s="2"/>
+      <c r="I34" t="s">
+        <v>534</v>
+      </c>
     </row>
     <row r="35" spans="1:9" ht="15">
       <c r="A35" s="7"/>
       <c r="B35" s="8" t="s">
-        <v>497</v>
+        <v>495</v>
       </c>
       <c r="C35" s="8"/>
       <c r="D35" s="8"/>
@@ -3756,7 +3764,7 @@
       <c r="C37" s="15"/>
       <c r="D37" s="15"/>
       <c r="E37" s="15" t="s">
-        <v>501</v>
+        <v>499</v>
       </c>
       <c r="F37" s="15"/>
       <c r="G37" s="15"/>
@@ -3769,7 +3777,7 @@
       <c r="C38" s="15"/>
       <c r="D38" s="15"/>
       <c r="E38" s="15" t="s">
-        <v>502</v>
+        <v>500</v>
       </c>
       <c r="F38" s="15"/>
       <c r="G38" s="15"/>
@@ -3855,7 +3863,7 @@
         <v>24</v>
       </c>
       <c r="D45" t="s">
-        <v>423</v>
+        <v>421</v>
       </c>
     </row>
     <row r="46" spans="1:9" ht="12.75" customHeight="1">
@@ -3864,7 +3872,7 @@
         <v>4</v>
       </c>
       <c r="D46" t="s">
-        <v>411</v>
+        <v>410</v>
       </c>
       <c r="E46" t="s">
         <v>25</v>
@@ -3895,7 +3903,7 @@
         <v>27</v>
       </c>
       <c r="D49" t="s">
-        <v>424</v>
+        <v>422</v>
       </c>
     </row>
     <row r="50" spans="1:5" ht="12.75" customHeight="1">
@@ -3904,7 +3912,7 @@
         <v>4</v>
       </c>
       <c r="D50" t="s">
-        <v>412</v>
+        <v>411</v>
       </c>
       <c r="E50" t="s">
         <v>32</v>
@@ -3949,7 +3957,7 @@
         <v>63</v>
       </c>
       <c r="D55" t="s">
-        <v>425</v>
+        <v>423</v>
       </c>
     </row>
     <row r="56" spans="1:5" ht="12.75" customHeight="1">
@@ -3961,7 +3969,7 @@
         <v>64</v>
       </c>
       <c r="D56" t="s">
-        <v>426</v>
+        <v>424</v>
       </c>
     </row>
     <row r="57" spans="1:5" ht="12.75" customHeight="1">
@@ -3970,7 +3978,7 @@
         <v>4</v>
       </c>
       <c r="D57" t="s">
-        <v>413</v>
+        <v>412</v>
       </c>
       <c r="E57" t="s">
         <v>65</v>
@@ -4009,7 +4017,7 @@
         <v>68</v>
       </c>
       <c r="D61" t="s">
-        <v>427</v>
+        <v>425</v>
       </c>
     </row>
     <row r="62" spans="1:5" ht="12.75" customHeight="1">
@@ -4021,7 +4029,7 @@
         <v>69</v>
       </c>
       <c r="D62" t="s">
-        <v>428</v>
+        <v>426</v>
       </c>
     </row>
     <row r="63" spans="1:5" ht="12.75" customHeight="1">
@@ -4030,7 +4038,7 @@
         <v>4</v>
       </c>
       <c r="D63" t="s">
-        <v>414</v>
+        <v>413</v>
       </c>
       <c r="E63" t="s">
         <v>70</v>
@@ -4065,12 +4073,12 @@
     </row>
     <row r="67" spans="1:8" ht="12.75" customHeight="1">
       <c r="B67" s="14" t="s">
-        <v>507</v>
+        <v>505</v>
       </c>
       <c r="C67" s="15"/>
       <c r="D67" s="15"/>
       <c r="E67" s="15" t="s">
-        <v>511</v>
+        <v>509</v>
       </c>
       <c r="F67" s="15"/>
       <c r="G67" s="15"/>
@@ -4078,12 +4086,12 @@
     </row>
     <row r="68" spans="1:8" ht="12.75" customHeight="1">
       <c r="B68" s="14" t="s">
-        <v>508</v>
+        <v>506</v>
       </c>
       <c r="C68" s="15"/>
       <c r="D68" s="15"/>
       <c r="E68" s="15" t="s">
-        <v>512</v>
+        <v>510</v>
       </c>
       <c r="F68" s="15"/>
       <c r="G68" s="15"/>
@@ -4091,10 +4099,10 @@
     </row>
     <row r="69" spans="1:8" ht="12.75" customHeight="1">
       <c r="A69" s="7" t="s">
-        <v>513</v>
+        <v>511</v>
       </c>
       <c r="B69" s="8" t="s">
-        <v>509</v>
+        <v>507</v>
       </c>
       <c r="C69" s="13"/>
       <c r="D69" s="13"/>
@@ -4106,13 +4114,13 @@
     <row r="70" spans="1:8" ht="12.75" customHeight="1">
       <c r="A70" s="16"/>
       <c r="B70" t="s">
-        <v>514</v>
+        <v>512</v>
       </c>
       <c r="C70" t="s">
-        <v>515</v>
+        <v>513</v>
       </c>
       <c r="D70" t="s">
-        <v>513</v>
+        <v>511</v>
       </c>
       <c r="E70" s="42"/>
       <c r="F70" t="s">
@@ -4129,7 +4137,7 @@
       <c r="C71" s="32"/>
       <c r="D71" s="32"/>
       <c r="E71" t="s">
-        <v>521</v>
+        <v>519</v>
       </c>
       <c r="F71" s="32"/>
       <c r="G71" s="32"/>
@@ -4142,7 +4150,7 @@
       </c>
       <c r="C72" s="32"/>
       <c r="D72" s="43" t="s">
-        <v>518</v>
+        <v>516</v>
       </c>
       <c r="E72" s="32"/>
       <c r="F72" s="32"/>
@@ -4163,7 +4171,7 @@
       <c r="C74" s="32"/>
       <c r="D74" s="32"/>
       <c r="E74" t="s">
-        <v>520</v>
+        <v>518</v>
       </c>
       <c r="F74" s="32"/>
       <c r="G74" s="32"/>
@@ -4176,7 +4184,7 @@
       </c>
       <c r="C75" s="32"/>
       <c r="D75" s="43" t="s">
-        <v>519</v>
+        <v>517</v>
       </c>
       <c r="E75" s="32"/>
       <c r="F75" s="32"/>
@@ -4192,7 +4200,7 @@
     <row r="77" spans="1:8" ht="12.75" customHeight="1">
       <c r="A77" s="7"/>
       <c r="B77" s="8" t="s">
-        <v>510</v>
+        <v>508</v>
       </c>
       <c r="C77" s="13"/>
       <c r="D77" s="13"/>
@@ -4212,12 +4220,12 @@
     </row>
     <row r="79" spans="1:8" ht="12.75" customHeight="1">
       <c r="B79" s="14" t="s">
-        <v>523</v>
+        <v>521</v>
       </c>
       <c r="C79" s="15"/>
       <c r="D79" s="15"/>
       <c r="E79" s="15" t="s">
-        <v>528</v>
+        <v>526</v>
       </c>
       <c r="F79" s="15"/>
       <c r="G79" s="15"/>
@@ -4225,12 +4233,12 @@
     </row>
     <row r="80" spans="1:8" ht="12.75" customHeight="1">
       <c r="B80" s="14" t="s">
-        <v>524</v>
+        <v>522</v>
       </c>
       <c r="C80" s="15"/>
       <c r="D80" s="15"/>
       <c r="E80" s="15" t="s">
-        <v>529</v>
+        <v>527</v>
       </c>
       <c r="F80" s="15"/>
       <c r="G80" s="15"/>
@@ -4238,10 +4246,10 @@
     </row>
     <row r="81" spans="1:8" ht="12.75" customHeight="1">
       <c r="A81" s="7" t="s">
-        <v>522</v>
+        <v>520</v>
       </c>
       <c r="B81" s="8" t="s">
-        <v>525</v>
+        <v>523</v>
       </c>
       <c r="C81" s="13"/>
       <c r="D81" s="13"/>
@@ -4253,13 +4261,13 @@
     <row r="82" spans="1:8" ht="12.75" customHeight="1">
       <c r="A82" s="16"/>
       <c r="B82" t="s">
-        <v>526</v>
+        <v>524</v>
       </c>
       <c r="C82" t="s">
-        <v>530</v>
+        <v>528</v>
       </c>
       <c r="D82" t="s">
-        <v>445</v>
+        <v>443</v>
       </c>
       <c r="E82" s="42"/>
       <c r="F82" t="s">
@@ -4271,211 +4279,211 @@
     <row r="83" spans="1:8" ht="12">
       <c r="A83" s="7"/>
       <c r="B83" s="45" t="s">
-        <v>393</v>
+        <v>392</v>
       </c>
       <c r="C83" s="45" t="s">
-        <v>459</v>
+        <v>457</v>
       </c>
       <c r="E83" s="2" t="s">
-        <v>534</v>
+        <v>532</v>
       </c>
     </row>
     <row r="84" spans="1:8" ht="11" customHeight="1">
       <c r="A84" s="7"/>
       <c r="B84" t="s">
+        <v>458</v>
+      </c>
+      <c r="C84" t="s">
+        <v>161</v>
+      </c>
+      <c r="D84" t="s">
+        <v>459</v>
+      </c>
+      <c r="E84" s="2" t="s">
         <v>460</v>
       </c>
-      <c r="C84" t="s">
-        <v>162</v>
-      </c>
-      <c r="D84" t="s">
+      <c r="F84" t="s">
         <v>461</v>
-      </c>
-      <c r="E84" s="2" t="s">
-        <v>462</v>
-      </c>
-      <c r="F84" t="s">
-        <v>463</v>
       </c>
     </row>
     <row r="85" spans="1:8" ht="11" customHeight="1">
       <c r="A85" s="7"/>
       <c r="B85" t="s">
+        <v>462</v>
+      </c>
+      <c r="C85" t="s">
+        <v>172</v>
+      </c>
+      <c r="D85" t="s">
+        <v>463</v>
+      </c>
+      <c r="E85" s="2" t="s">
         <v>464</v>
       </c>
-      <c r="C85" t="s">
-        <v>173</v>
-      </c>
-      <c r="D85" t="s">
-        <v>465</v>
-      </c>
-      <c r="E85" s="2" t="s">
-        <v>466</v>
-      </c>
       <c r="F85" t="s">
-        <v>463</v>
+        <v>461</v>
       </c>
     </row>
     <row r="86" spans="1:8" ht="11" customHeight="1">
       <c r="A86" s="7"/>
       <c r="B86" t="s">
+        <v>465</v>
+      </c>
+      <c r="C86" t="s">
+        <v>185</v>
+      </c>
+      <c r="D86" t="s">
+        <v>466</v>
+      </c>
+      <c r="E86" s="2" t="s">
         <v>467</v>
       </c>
-      <c r="C86" t="s">
-        <v>186</v>
-      </c>
-      <c r="D86" t="s">
-        <v>468</v>
-      </c>
-      <c r="E86" s="2" t="s">
-        <v>469</v>
-      </c>
       <c r="F86" t="s">
-        <v>463</v>
+        <v>461</v>
       </c>
     </row>
     <row r="87" spans="1:8" ht="11" customHeight="1">
       <c r="A87" s="7"/>
       <c r="B87" t="s">
+        <v>468</v>
+      </c>
+      <c r="C87" t="s">
+        <v>196</v>
+      </c>
+      <c r="D87" t="s">
+        <v>469</v>
+      </c>
+      <c r="E87" s="2" t="s">
         <v>470</v>
       </c>
-      <c r="C87" t="s">
-        <v>197</v>
-      </c>
-      <c r="D87" t="s">
-        <v>471</v>
-      </c>
-      <c r="E87" s="2" t="s">
-        <v>472</v>
-      </c>
       <c r="F87" t="s">
-        <v>463</v>
+        <v>461</v>
       </c>
     </row>
     <row r="88" spans="1:8" ht="11" customHeight="1">
       <c r="A88" s="7"/>
       <c r="B88" t="s">
+        <v>471</v>
+      </c>
+      <c r="C88" t="s">
+        <v>211</v>
+      </c>
+      <c r="D88" t="s">
+        <v>472</v>
+      </c>
+      <c r="E88" s="2" t="s">
         <v>473</v>
       </c>
-      <c r="C88" t="s">
-        <v>212</v>
-      </c>
-      <c r="D88" t="s">
-        <v>474</v>
-      </c>
-      <c r="E88" s="2" t="s">
-        <v>475</v>
-      </c>
       <c r="F88" t="s">
-        <v>463</v>
+        <v>461</v>
       </c>
     </row>
     <row r="89" spans="1:8" ht="11" customHeight="1">
       <c r="A89" s="7"/>
       <c r="B89" t="s">
+        <v>474</v>
+      </c>
+      <c r="C89" t="s">
+        <v>224</v>
+      </c>
+      <c r="D89" t="s">
+        <v>475</v>
+      </c>
+      <c r="E89" s="2" t="s">
         <v>476</v>
       </c>
-      <c r="C89" t="s">
-        <v>225</v>
-      </c>
-      <c r="D89" t="s">
-        <v>477</v>
-      </c>
-      <c r="E89" s="2" t="s">
-        <v>478</v>
-      </c>
       <c r="F89" t="s">
-        <v>463</v>
+        <v>461</v>
       </c>
     </row>
     <row r="90" spans="1:8" ht="11" customHeight="1">
       <c r="A90" s="7"/>
       <c r="B90" t="s">
+        <v>477</v>
+      </c>
+      <c r="C90" t="s">
+        <v>237</v>
+      </c>
+      <c r="D90" t="s">
+        <v>478</v>
+      </c>
+      <c r="E90" s="2" t="s">
         <v>479</v>
-      </c>
-      <c r="C90" t="s">
-        <v>238</v>
-      </c>
-      <c r="D90" t="s">
-        <v>480</v>
-      </c>
-      <c r="E90" s="2" t="s">
-        <v>481</v>
       </c>
     </row>
     <row r="91" spans="1:8" ht="11" customHeight="1">
       <c r="A91" s="7"/>
       <c r="B91" t="s">
+        <v>480</v>
+      </c>
+      <c r="C91" t="s">
+        <v>252</v>
+      </c>
+      <c r="D91" t="s">
+        <v>481</v>
+      </c>
+      <c r="E91" s="2" t="s">
         <v>482</v>
-      </c>
-      <c r="C91" t="s">
-        <v>253</v>
-      </c>
-      <c r="D91" t="s">
-        <v>483</v>
-      </c>
-      <c r="E91" s="2" t="s">
-        <v>484</v>
       </c>
     </row>
     <row r="92" spans="1:8" ht="11" customHeight="1">
       <c r="A92" s="7"/>
       <c r="B92" t="s">
+        <v>483</v>
+      </c>
+      <c r="C92" t="s">
+        <v>265</v>
+      </c>
+      <c r="D92" t="s">
+        <v>484</v>
+      </c>
+      <c r="E92" s="2" t="s">
         <v>485</v>
-      </c>
-      <c r="C92" t="s">
-        <v>266</v>
-      </c>
-      <c r="D92" t="s">
-        <v>486</v>
-      </c>
-      <c r="E92" s="2" t="s">
-        <v>487</v>
       </c>
     </row>
     <row r="93" spans="1:8" ht="11" customHeight="1">
       <c r="A93" s="7"/>
       <c r="B93" t="s">
+        <v>486</v>
+      </c>
+      <c r="C93" t="s">
+        <v>280</v>
+      </c>
+      <c r="D93" t="s">
+        <v>487</v>
+      </c>
+      <c r="E93" s="2" t="s">
         <v>488</v>
-      </c>
-      <c r="C93" t="s">
-        <v>281</v>
-      </c>
-      <c r="D93" t="s">
-        <v>489</v>
-      </c>
-      <c r="E93" s="2" t="s">
-        <v>490</v>
       </c>
     </row>
     <row r="94" spans="1:8" ht="11" customHeight="1">
       <c r="A94" s="7"/>
       <c r="B94" t="s">
+        <v>489</v>
+      </c>
+      <c r="C94" t="s">
+        <v>293</v>
+      </c>
+      <c r="D94" t="s">
+        <v>490</v>
+      </c>
+      <c r="E94" s="2" t="s">
         <v>491</v>
-      </c>
-      <c r="C94" t="s">
-        <v>294</v>
-      </c>
-      <c r="D94" t="s">
-        <v>492</v>
-      </c>
-      <c r="E94" s="2" t="s">
-        <v>493</v>
       </c>
     </row>
     <row r="95" spans="1:8" ht="12" customHeight="1">
       <c r="A95" s="7"/>
       <c r="B95" t="s">
+        <v>492</v>
+      </c>
+      <c r="C95" t="s">
+        <v>308</v>
+      </c>
+      <c r="D95" t="s">
+        <v>493</v>
+      </c>
+      <c r="E95" s="2" t="s">
         <v>494</v>
-      </c>
-      <c r="C95" t="s">
-        <v>309</v>
-      </c>
-      <c r="D95" t="s">
-        <v>495</v>
-      </c>
-      <c r="E95" s="2" t="s">
-        <v>496</v>
       </c>
     </row>
     <row r="96" spans="1:8" ht="12.75" customHeight="1">
@@ -4520,7 +4528,7 @@
         <v>14</v>
       </c>
       <c r="E102" t="s">
-        <v>532</v>
+        <v>530</v>
       </c>
     </row>
     <row r="103" spans="1:9" ht="24">
@@ -4562,7 +4570,7 @@
         <v>24</v>
       </c>
       <c r="D106" t="s">
-        <v>423</v>
+        <v>421</v>
       </c>
     </row>
     <row r="107" spans="1:9" ht="12.75" customHeight="1">
@@ -4571,7 +4579,7 @@
         <v>4</v>
       </c>
       <c r="D107" t="s">
-        <v>411</v>
+        <v>410</v>
       </c>
       <c r="E107" t="s">
         <v>25</v>
@@ -4602,7 +4610,7 @@
         <v>27</v>
       </c>
       <c r="D110" t="s">
-        <v>424</v>
+        <v>422</v>
       </c>
     </row>
     <row r="111" spans="1:9" ht="12.75" customHeight="1">
@@ -4611,7 +4619,7 @@
         <v>4</v>
       </c>
       <c r="D111" t="s">
-        <v>412</v>
+        <v>411</v>
       </c>
       <c r="E111" t="s">
         <v>32</v>
@@ -4635,7 +4643,7 @@
         <v>14</v>
       </c>
       <c r="E114" t="s">
-        <v>533</v>
+        <v>531</v>
       </c>
     </row>
     <row r="115" spans="1:10" ht="12.75" customHeight="1">
@@ -4656,7 +4664,7 @@
         <v>48</v>
       </c>
       <c r="D116" t="s">
-        <v>429</v>
+        <v>427</v>
       </c>
     </row>
     <row r="117" spans="1:10" ht="12.75" customHeight="1">
@@ -4665,7 +4673,7 @@
         <v>4</v>
       </c>
       <c r="D117" t="s">
-        <v>430</v>
+        <v>428</v>
       </c>
     </row>
     <row r="118" spans="1:10" ht="12.75" customHeight="1">
@@ -4677,7 +4685,7 @@
         <v>43</v>
       </c>
       <c r="D118" t="s">
-        <v>431</v>
+        <v>429</v>
       </c>
     </row>
     <row r="119" spans="1:10" ht="12.75" customHeight="1">
@@ -4689,7 +4697,7 @@
         <v>44</v>
       </c>
       <c r="D119" t="s">
-        <v>432</v>
+        <v>430</v>
       </c>
     </row>
     <row r="120" spans="1:10" ht="12.75" customHeight="1">
@@ -4698,7 +4706,7 @@
         <v>4</v>
       </c>
       <c r="D120" t="s">
-        <v>415</v>
+        <v>414</v>
       </c>
       <c r="E120" t="s">
         <v>73</v>
@@ -4710,7 +4718,7 @@
         <v>4</v>
       </c>
       <c r="D121" t="s">
-        <v>416</v>
+        <v>415</v>
       </c>
       <c r="E121" t="s">
         <v>45</v>
@@ -4725,7 +4733,7 @@
     <row r="123" spans="1:10" ht="20" customHeight="1">
       <c r="A123" s="7"/>
       <c r="B123" s="8" t="s">
-        <v>527</v>
+        <v>525</v>
       </c>
       <c r="C123" s="13"/>
       <c r="D123" s="13"/>
@@ -4737,7 +4745,7 @@
     <row r="124" spans="1:10" ht="15">
       <c r="A124" s="16"/>
       <c r="B124" s="8" t="s">
-        <v>436</v>
+        <v>434</v>
       </c>
       <c r="C124" s="30"/>
       <c r="D124" s="31"/>
@@ -4747,22 +4755,22 @@
     <row r="126" spans="1:10" s="15" customFormat="1" ht="12.75" customHeight="1">
       <c r="A126" s="37"/>
       <c r="B126" s="14" t="s">
+        <v>398</v>
+      </c>
+      <c r="E126" s="15" t="s">
         <v>399</v>
-      </c>
-      <c r="E126" s="15" t="s">
-        <v>400</v>
       </c>
       <c r="I126" s="3"/>
       <c r="J126" s="3"/>
     </row>
     <row r="127" spans="1:10" ht="12.75" customHeight="1">
       <c r="B127" s="14" t="s">
-        <v>401</v>
+        <v>400</v>
       </c>
       <c r="C127" s="15"/>
       <c r="D127" s="15"/>
       <c r="E127" s="15" t="s">
-        <v>402</v>
+        <v>401</v>
       </c>
       <c r="F127" s="15"/>
       <c r="G127" s="15"/>
@@ -4770,7 +4778,7 @@
     </row>
     <row r="128" spans="1:10" ht="15">
       <c r="A128" s="7" t="s">
-        <v>505</v>
+        <v>503</v>
       </c>
       <c r="B128" s="8" t="s">
         <v>75</v>
@@ -4837,7 +4845,7 @@
         <v>116</v>
       </c>
       <c r="D134" t="s">
-        <v>423</v>
+        <v>421</v>
       </c>
     </row>
     <row r="135" spans="1:9" ht="61" customHeight="1">
@@ -4846,7 +4854,7 @@
         <v>4</v>
       </c>
       <c r="D135" t="s">
-        <v>403</v>
+        <v>402</v>
       </c>
       <c r="E135" t="s">
         <v>117</v>
@@ -4906,7 +4914,7 @@
         <v>118</v>
       </c>
       <c r="D141" t="s">
-        <v>423</v>
+        <v>421</v>
       </c>
     </row>
     <row r="142" spans="1:9" ht="75" customHeight="1">
@@ -4915,7 +4923,7 @@
         <v>4</v>
       </c>
       <c r="D142" t="s">
-        <v>404</v>
+        <v>403</v>
       </c>
       <c r="E142" t="s">
         <v>119</v>
@@ -4927,7 +4935,7 @@
         <v>4</v>
       </c>
       <c r="D143" t="s">
-        <v>405</v>
+        <v>404</v>
       </c>
       <c r="E143" t="s">
         <v>119</v>
@@ -4939,7 +4947,7 @@
         <v>4</v>
       </c>
       <c r="D144" t="s">
-        <v>406</v>
+        <v>405</v>
       </c>
       <c r="E144" t="s">
         <v>119</v>
@@ -4996,7 +5004,7 @@
         <v>4</v>
       </c>
       <c r="D150" t="s">
-        <v>417</v>
+        <v>416</v>
       </c>
     </row>
     <row r="151" spans="1:9" ht="12.75" customHeight="1">
@@ -5020,30 +5028,30 @@
     <row r="154" spans="1:9" s="14" customFormat="1" ht="15">
       <c r="A154" s="28"/>
       <c r="B154" s="14" t="s">
-        <v>407</v>
+        <v>406</v>
       </c>
       <c r="C154" s="38"/>
       <c r="D154" s="39"/>
       <c r="E154" s="15" t="s">
-        <v>408</v>
+        <v>407</v>
       </c>
       <c r="F154" s="38"/>
     </row>
     <row r="155" spans="1:9" s="14" customFormat="1" ht="15">
       <c r="A155" s="28"/>
       <c r="B155" s="14" t="s">
-        <v>409</v>
+        <v>408</v>
       </c>
       <c r="C155" s="38"/>
       <c r="D155" s="39"/>
       <c r="E155" s="15" t="s">
-        <v>410</v>
+        <v>409</v>
       </c>
       <c r="F155" s="38"/>
     </row>
     <row r="156" spans="1:9" ht="15">
       <c r="A156" s="7" t="s">
-        <v>506</v>
+        <v>504</v>
       </c>
       <c r="B156" s="8" t="s">
         <v>54</v>
@@ -5121,7 +5129,7 @@
         <v>24</v>
       </c>
       <c r="D162" t="s">
-        <v>423</v>
+        <v>421</v>
       </c>
     </row>
     <row r="163" spans="1:9" ht="12.75" customHeight="1">
@@ -5130,7 +5138,7 @@
         <v>4</v>
       </c>
       <c r="D163" t="s">
-        <v>411</v>
+        <v>410</v>
       </c>
       <c r="E163" t="s">
         <v>25</v>
@@ -5161,7 +5169,7 @@
         <v>27</v>
       </c>
       <c r="D166" t="s">
-        <v>424</v>
+        <v>422</v>
       </c>
     </row>
     <row r="167" spans="1:9" ht="12.75" customHeight="1">
@@ -5170,7 +5178,7 @@
         <v>4</v>
       </c>
       <c r="D167" t="s">
-        <v>412</v>
+        <v>411</v>
       </c>
       <c r="E167" t="s">
         <v>32</v>
@@ -5215,7 +5223,7 @@
         <v>63</v>
       </c>
       <c r="D172" t="s">
-        <v>425</v>
+        <v>423</v>
       </c>
     </row>
     <row r="173" spans="1:9" ht="12.75" customHeight="1">
@@ -5227,7 +5235,7 @@
         <v>64</v>
       </c>
       <c r="D173" t="s">
-        <v>426</v>
+        <v>424</v>
       </c>
     </row>
     <row r="174" spans="1:9" ht="12.75" customHeight="1">
@@ -5236,7 +5244,7 @@
         <v>4</v>
       </c>
       <c r="D174" t="s">
-        <v>413</v>
+        <v>412</v>
       </c>
       <c r="E174" t="s">
         <v>65</v>
@@ -5275,7 +5283,7 @@
         <v>68</v>
       </c>
       <c r="D178" t="s">
-        <v>427</v>
+        <v>425</v>
       </c>
     </row>
     <row r="179" spans="1:8" ht="12.75" customHeight="1">
@@ -5287,7 +5295,7 @@
         <v>69</v>
       </c>
       <c r="D179" t="s">
-        <v>428</v>
+        <v>426</v>
       </c>
     </row>
     <row r="180" spans="1:8" ht="12.75" customHeight="1">
@@ -5296,7 +5304,7 @@
         <v>4</v>
       </c>
       <c r="D180" t="s">
-        <v>414</v>
+        <v>413</v>
       </c>
       <c r="E180" t="s">
         <v>70</v>
@@ -5335,7 +5343,7 @@
         <v>48</v>
       </c>
       <c r="D184" t="s">
-        <v>429</v>
+        <v>427</v>
       </c>
     </row>
     <row r="185" spans="1:8" ht="12.75" customHeight="1">
@@ -5344,7 +5352,7 @@
         <v>4</v>
       </c>
       <c r="D185" t="s">
-        <v>430</v>
+        <v>428</v>
       </c>
     </row>
     <row r="186" spans="1:8" ht="12.75" customHeight="1">
@@ -5356,7 +5364,7 @@
         <v>43</v>
       </c>
       <c r="D186" t="s">
-        <v>431</v>
+        <v>429</v>
       </c>
     </row>
     <row r="187" spans="1:8" ht="12.75" customHeight="1">
@@ -5368,7 +5376,7 @@
         <v>44</v>
       </c>
       <c r="D187" t="s">
-        <v>432</v>
+        <v>430</v>
       </c>
     </row>
     <row r="188" spans="1:8" ht="12.75" customHeight="1">
@@ -5377,7 +5385,7 @@
         <v>4</v>
       </c>
       <c r="D188" t="s">
-        <v>415</v>
+        <v>414</v>
       </c>
       <c r="E188" t="s">
         <v>73</v>
@@ -5389,7 +5397,7 @@
         <v>4</v>
       </c>
       <c r="D189" t="s">
-        <v>416</v>
+        <v>415</v>
       </c>
       <c r="E189" t="s">
         <v>45</v>
@@ -5415,7 +5423,7 @@
     </row>
     <row r="194" spans="2:2" ht="12.75" customHeight="1">
       <c r="B194" s="36" t="s">
-        <v>386</v>
+        <v>385</v>
       </c>
     </row>
   </sheetData>
@@ -5433,8 +5441,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:D139"/>
   <sheetViews>
-    <sheetView topLeftCell="A130" zoomScale="150" zoomScaleNormal="150" zoomScalePageLayoutView="150" workbookViewId="0">
-      <selection activeCell="A147" sqref="A147"/>
+    <sheetView tabSelected="1" zoomScale="150" zoomScaleNormal="150" zoomScalePageLayoutView="150" workbookViewId="0">
+      <selection activeCell="D18" sqref="D18"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultColWidth="17.1640625" defaultRowHeight="12.75" customHeight="1" x14ac:dyDescent="0"/>
@@ -5469,13 +5477,13 @@
         <v>137</v>
       </c>
       <c r="B3" t="s">
-        <v>385</v>
+        <v>384</v>
       </c>
       <c r="C3" t="s">
+        <v>393</v>
+      </c>
+      <c r="D3" t="s">
         <v>394</v>
-      </c>
-      <c r="D3" t="s">
-        <v>395</v>
       </c>
     </row>
     <row r="4" spans="1:4" ht="12.75" customHeight="1">
@@ -5527,26 +5535,26 @@
         <v>147</v>
       </c>
       <c r="B9" t="s">
+        <v>395</v>
+      </c>
+      <c r="C9" t="s">
         <v>396</v>
-      </c>
-      <c r="C9" t="s">
-        <v>397</v>
       </c>
     </row>
     <row r="11" spans="1:4" ht="12.75" customHeight="1">
       <c r="A11" t="s">
-        <v>440</v>
+        <v>438</v>
       </c>
       <c r="B11" t="s">
         <v>139</v>
       </c>
       <c r="C11" t="s">
-        <v>443</v>
+        <v>441</v>
       </c>
     </row>
     <row r="12" spans="1:4" ht="12.75" customHeight="1">
       <c r="A12" t="s">
-        <v>440</v>
+        <v>438</v>
       </c>
       <c r="B12" t="s">
         <v>144</v>
@@ -5557,24 +5565,24 @@
     </row>
     <row r="13" spans="1:4" ht="12.75" customHeight="1">
       <c r="A13" t="s">
-        <v>440</v>
+        <v>438</v>
       </c>
       <c r="B13" t="s">
-        <v>441</v>
+        <v>439</v>
       </c>
       <c r="C13" t="s">
-        <v>444</v>
+        <v>442</v>
       </c>
     </row>
     <row r="14" spans="1:4" ht="12.75" customHeight="1">
       <c r="A14" t="s">
+        <v>438</v>
+      </c>
+      <c r="B14" t="s">
         <v>440</v>
       </c>
-      <c r="B14" t="s">
-        <v>442</v>
-      </c>
       <c r="C14" t="s">
-        <v>445</v>
+        <v>443</v>
       </c>
     </row>
     <row r="16" spans="1:4" ht="12.75" customHeight="1">
@@ -5606,8 +5614,8 @@
       <c r="B18" t="s">
         <v>157</v>
       </c>
-      <c r="D18" t="s">
-        <v>158</v>
+      <c r="C18" t="s">
+        <v>535</v>
       </c>
     </row>
     <row r="19" spans="1:4" ht="12.75" customHeight="1">
@@ -5615,10 +5623,10 @@
         <v>152</v>
       </c>
       <c r="B19" t="s">
+        <v>159</v>
+      </c>
+      <c r="C19" t="s">
         <v>160</v>
-      </c>
-      <c r="C19" t="s">
-        <v>161</v>
       </c>
     </row>
     <row r="21" spans="1:4" ht="12.75" customHeight="1">
@@ -5777,40 +5785,40 @@
     </row>
     <row r="39" spans="1:4" ht="12.75" customHeight="1">
       <c r="A39" t="s">
-        <v>515</v>
+        <v>513</v>
       </c>
       <c r="B39" t="s">
+        <v>514</v>
+      </c>
+      <c r="C39" t="s">
         <v>516</v>
-      </c>
-      <c r="C39" t="s">
-        <v>518</v>
       </c>
     </row>
     <row r="40" spans="1:4" ht="12.75" customHeight="1">
       <c r="A40" t="s">
+        <v>513</v>
+      </c>
+      <c r="B40" t="s">
         <v>515</v>
       </c>
-      <c r="B40" t="s">
+      <c r="C40" t="s">
         <v>517</v>
-      </c>
-      <c r="C40" t="s">
-        <v>519</v>
       </c>
     </row>
     <row r="42" spans="1:4" ht="12.75" customHeight="1">
       <c r="A42" t="s">
-        <v>530</v>
+        <v>528</v>
       </c>
       <c r="B42" t="s">
-        <v>159</v>
+        <v>158</v>
       </c>
       <c r="C42" t="s">
-        <v>531</v>
+        <v>529</v>
       </c>
     </row>
     <row r="43" spans="1:4" ht="12.75" customHeight="1">
       <c r="A43" t="s">
-        <v>530</v>
+        <v>528</v>
       </c>
       <c r="B43" t="s">
         <v>91</v>
@@ -5821,7 +5829,7 @@
     </row>
     <row r="44" spans="1:4" ht="12.75" customHeight="1">
       <c r="A44" t="s">
-        <v>530</v>
+        <v>528</v>
       </c>
       <c r="B44" t="s">
         <v>97</v>
@@ -5832,882 +5840,882 @@
     </row>
     <row r="46" spans="1:4" ht="12.75" customHeight="1">
       <c r="A46" t="s">
+        <v>161</v>
+      </c>
+      <c r="B46" t="s">
         <v>162</v>
       </c>
-      <c r="B46" t="s">
+      <c r="D46" t="s">
         <v>163</v>
-      </c>
-      <c r="D46" t="s">
-        <v>164</v>
       </c>
     </row>
     <row r="47" spans="1:4" ht="12.75" customHeight="1">
       <c r="A47" t="s">
-        <v>162</v>
+        <v>161</v>
       </c>
       <c r="B47" t="s">
+        <v>164</v>
+      </c>
+      <c r="D47" t="s">
         <v>165</v>
-      </c>
-      <c r="D47" t="s">
-        <v>166</v>
       </c>
     </row>
     <row r="48" spans="1:4" ht="12.75" customHeight="1">
       <c r="A48" t="s">
-        <v>162</v>
+        <v>161</v>
       </c>
       <c r="B48" t="s">
+        <v>166</v>
+      </c>
+      <c r="D48" t="s">
         <v>167</v>
-      </c>
-      <c r="D48" t="s">
-        <v>168</v>
       </c>
     </row>
     <row r="49" spans="1:4" ht="12.75" customHeight="1">
       <c r="A49" t="s">
-        <v>162</v>
+        <v>161</v>
       </c>
       <c r="B49" t="s">
+        <v>168</v>
+      </c>
+      <c r="D49" t="s">
         <v>169</v>
-      </c>
-      <c r="D49" t="s">
-        <v>170</v>
       </c>
     </row>
     <row r="50" spans="1:4" ht="12.75" customHeight="1">
       <c r="A50" t="s">
-        <v>162</v>
+        <v>161</v>
       </c>
       <c r="B50" t="s">
+        <v>170</v>
+      </c>
+      <c r="D50" t="s">
         <v>171</v>
-      </c>
-      <c r="D50" t="s">
-        <v>172</v>
       </c>
     </row>
     <row r="52" spans="1:4" ht="12.75" customHeight="1">
       <c r="A52" t="s">
+        <v>172</v>
+      </c>
+      <c r="B52" t="s">
         <v>173</v>
       </c>
-      <c r="B52" t="s">
+      <c r="D52" t="s">
         <v>174</v>
-      </c>
-      <c r="D52" t="s">
-        <v>175</v>
       </c>
     </row>
     <row r="53" spans="1:4" s="2" customFormat="1" ht="12.75" customHeight="1">
       <c r="A53" t="s">
-        <v>173</v>
+        <v>172</v>
       </c>
       <c r="B53" t="s">
+        <v>175</v>
+      </c>
+      <c r="D53" t="s">
         <v>176</v>
-      </c>
-      <c r="D53" t="s">
-        <v>177</v>
       </c>
     </row>
     <row r="54" spans="1:4" ht="12.75" customHeight="1">
       <c r="A54" t="s">
-        <v>173</v>
+        <v>172</v>
       </c>
       <c r="B54" t="s">
+        <v>177</v>
+      </c>
+      <c r="D54" t="s">
         <v>178</v>
-      </c>
-      <c r="D54" t="s">
-        <v>179</v>
       </c>
     </row>
     <row r="55" spans="1:4" ht="12.75" customHeight="1">
       <c r="A55" t="s">
-        <v>173</v>
+        <v>172</v>
       </c>
       <c r="B55" t="s">
+        <v>179</v>
+      </c>
+      <c r="D55" t="s">
         <v>180</v>
-      </c>
-      <c r="D55" t="s">
-        <v>181</v>
       </c>
     </row>
     <row r="56" spans="1:4" ht="12.75" customHeight="1">
       <c r="A56" t="s">
-        <v>173</v>
+        <v>172</v>
       </c>
       <c r="B56" t="s">
+        <v>181</v>
+      </c>
+      <c r="D56" t="s">
         <v>182</v>
-      </c>
-      <c r="D56" t="s">
-        <v>183</v>
       </c>
     </row>
     <row r="57" spans="1:4" ht="12.75" customHeight="1">
       <c r="A57" t="s">
-        <v>173</v>
+        <v>172</v>
       </c>
       <c r="B57" t="s">
+        <v>183</v>
+      </c>
+      <c r="D57" t="s">
         <v>184</v>
-      </c>
-      <c r="D57" t="s">
-        <v>185</v>
       </c>
     </row>
     <row r="59" spans="1:4" ht="12.75" customHeight="1">
       <c r="A59" t="s">
+        <v>185</v>
+      </c>
+      <c r="B59" t="s">
         <v>186</v>
-      </c>
-      <c r="B59" t="s">
-        <v>187</v>
       </c>
       <c r="C59" s="2"/>
       <c r="D59" t="s">
-        <v>188</v>
+        <v>187</v>
       </c>
     </row>
     <row r="60" spans="1:4" ht="12.75" customHeight="1">
       <c r="A60" t="s">
-        <v>186</v>
+        <v>185</v>
       </c>
       <c r="B60" t="s">
+        <v>188</v>
+      </c>
+      <c r="D60" t="s">
         <v>189</v>
-      </c>
-      <c r="D60" t="s">
-        <v>190</v>
       </c>
     </row>
     <row r="61" spans="1:4" ht="12.75" customHeight="1">
       <c r="A61" t="s">
-        <v>186</v>
+        <v>185</v>
       </c>
       <c r="B61" t="s">
+        <v>190</v>
+      </c>
+      <c r="D61" t="s">
         <v>191</v>
-      </c>
-      <c r="D61" t="s">
-        <v>192</v>
       </c>
     </row>
     <row r="62" spans="1:4" ht="12.75" customHeight="1">
       <c r="A62" t="s">
-        <v>186</v>
+        <v>185</v>
       </c>
       <c r="B62" t="s">
+        <v>192</v>
+      </c>
+      <c r="D62" t="s">
         <v>193</v>
-      </c>
-      <c r="D62" t="s">
-        <v>194</v>
       </c>
     </row>
     <row r="63" spans="1:4" ht="12.75" customHeight="1">
       <c r="A63" t="s">
-        <v>186</v>
+        <v>185</v>
       </c>
       <c r="B63" t="s">
+        <v>194</v>
+      </c>
+      <c r="D63" t="s">
         <v>195</v>
-      </c>
-      <c r="D63" t="s">
-        <v>196</v>
       </c>
     </row>
     <row r="65" spans="1:4" ht="12.75" customHeight="1">
       <c r="A65" t="s">
+        <v>196</v>
+      </c>
+      <c r="B65" t="s">
         <v>197</v>
       </c>
-      <c r="B65" t="s">
+      <c r="D65" t="s">
         <v>198</v>
-      </c>
-      <c r="D65" t="s">
-        <v>199</v>
       </c>
     </row>
     <row r="66" spans="1:4" ht="12.75" customHeight="1">
       <c r="A66" t="s">
-        <v>197</v>
+        <v>196</v>
       </c>
       <c r="B66" t="s">
-        <v>200</v>
+        <v>199</v>
       </c>
       <c r="C66" s="2"/>
       <c r="D66" t="s">
-        <v>201</v>
+        <v>200</v>
       </c>
     </row>
     <row r="67" spans="1:4" ht="12.75" customHeight="1">
       <c r="A67" t="s">
-        <v>197</v>
+        <v>196</v>
       </c>
       <c r="B67" t="s">
+        <v>201</v>
+      </c>
+      <c r="D67" t="s">
         <v>202</v>
-      </c>
-      <c r="D67" t="s">
-        <v>203</v>
       </c>
     </row>
     <row r="68" spans="1:4" ht="12.75" customHeight="1">
       <c r="A68" t="s">
-        <v>197</v>
+        <v>196</v>
       </c>
       <c r="B68" t="s">
+        <v>203</v>
+      </c>
+      <c r="D68" t="s">
         <v>204</v>
-      </c>
-      <c r="D68" t="s">
-        <v>205</v>
       </c>
     </row>
     <row r="69" spans="1:4" ht="12.75" customHeight="1">
       <c r="A69" t="s">
-        <v>197</v>
+        <v>196</v>
       </c>
       <c r="B69" t="s">
+        <v>205</v>
+      </c>
+      <c r="D69" t="s">
         <v>206</v>
-      </c>
-      <c r="D69" t="s">
-        <v>207</v>
       </c>
     </row>
     <row r="70" spans="1:4" ht="12.75" customHeight="1">
       <c r="A70" t="s">
-        <v>197</v>
+        <v>196</v>
       </c>
       <c r="B70" t="s">
+        <v>207</v>
+      </c>
+      <c r="D70" t="s">
         <v>208</v>
-      </c>
-      <c r="D70" t="s">
-        <v>209</v>
       </c>
     </row>
     <row r="71" spans="1:4" ht="12.75" customHeight="1">
       <c r="A71" t="s">
-        <v>197</v>
+        <v>196</v>
       </c>
       <c r="B71" t="s">
+        <v>209</v>
+      </c>
+      <c r="D71" t="s">
         <v>210</v>
-      </c>
-      <c r="D71" t="s">
-        <v>211</v>
       </c>
     </row>
     <row r="73" spans="1:4" ht="12.75" customHeight="1">
       <c r="A73" t="s">
+        <v>211</v>
+      </c>
+      <c r="B73" t="s">
         <v>212</v>
       </c>
-      <c r="B73" t="s">
+      <c r="D73" t="s">
         <v>213</v>
-      </c>
-      <c r="D73" t="s">
-        <v>214</v>
       </c>
     </row>
     <row r="74" spans="1:4" ht="12.75" customHeight="1">
       <c r="A74" t="s">
-        <v>212</v>
+        <v>211</v>
       </c>
       <c r="B74" t="s">
-        <v>215</v>
+        <v>214</v>
       </c>
       <c r="C74" s="2"/>
       <c r="D74" t="s">
-        <v>216</v>
+        <v>215</v>
       </c>
     </row>
     <row r="75" spans="1:4" ht="12.75" customHeight="1">
       <c r="A75" t="s">
-        <v>212</v>
+        <v>211</v>
       </c>
       <c r="B75" t="s">
+        <v>216</v>
+      </c>
+      <c r="D75" t="s">
         <v>217</v>
-      </c>
-      <c r="D75" t="s">
-        <v>218</v>
       </c>
     </row>
     <row r="76" spans="1:4" ht="12.75" customHeight="1">
       <c r="A76" t="s">
-        <v>212</v>
+        <v>211</v>
       </c>
       <c r="B76" t="s">
+        <v>218</v>
+      </c>
+      <c r="D76" t="s">
         <v>219</v>
-      </c>
-      <c r="D76" t="s">
-        <v>220</v>
       </c>
     </row>
     <row r="77" spans="1:4" ht="12.75" customHeight="1">
       <c r="A77" t="s">
-        <v>212</v>
+        <v>211</v>
       </c>
       <c r="B77" t="s">
+        <v>220</v>
+      </c>
+      <c r="D77" t="s">
         <v>221</v>
-      </c>
-      <c r="D77" t="s">
-        <v>222</v>
       </c>
     </row>
     <row r="78" spans="1:4" ht="12.75" customHeight="1">
       <c r="A78" t="s">
-        <v>212</v>
+        <v>211</v>
       </c>
       <c r="B78" t="s">
+        <v>222</v>
+      </c>
+      <c r="D78" t="s">
         <v>223</v>
-      </c>
-      <c r="D78" t="s">
-        <v>224</v>
       </c>
     </row>
     <row r="80" spans="1:4" ht="12.75" customHeight="1">
       <c r="A80" t="s">
+        <v>224</v>
+      </c>
+      <c r="B80" t="s">
         <v>225</v>
       </c>
-      <c r="B80" t="s">
+      <c r="D80" t="s">
         <v>226</v>
-      </c>
-      <c r="D80" t="s">
-        <v>227</v>
       </c>
     </row>
     <row r="81" spans="1:4" ht="12.75" customHeight="1">
       <c r="A81" t="s">
-        <v>225</v>
+        <v>224</v>
       </c>
       <c r="B81" t="s">
-        <v>228</v>
+        <v>227</v>
       </c>
       <c r="C81" s="2"/>
       <c r="D81" t="s">
-        <v>229</v>
+        <v>228</v>
       </c>
     </row>
     <row r="82" spans="1:4" ht="12.75" customHeight="1">
       <c r="A82" t="s">
-        <v>225</v>
+        <v>224</v>
       </c>
       <c r="B82" t="s">
+        <v>229</v>
+      </c>
+      <c r="D82" t="s">
         <v>230</v>
-      </c>
-      <c r="D82" t="s">
-        <v>231</v>
       </c>
     </row>
     <row r="83" spans="1:4" ht="12.75" customHeight="1">
       <c r="A83" t="s">
-        <v>225</v>
+        <v>224</v>
       </c>
       <c r="B83" t="s">
+        <v>231</v>
+      </c>
+      <c r="D83" t="s">
         <v>232</v>
-      </c>
-      <c r="D83" t="s">
-        <v>233</v>
       </c>
     </row>
     <row r="84" spans="1:4" ht="12.75" customHeight="1">
       <c r="A84" t="s">
-        <v>225</v>
+        <v>224</v>
       </c>
       <c r="B84" t="s">
+        <v>233</v>
+      </c>
+      <c r="D84" t="s">
         <v>234</v>
-      </c>
-      <c r="D84" t="s">
-        <v>235</v>
       </c>
     </row>
     <row r="85" spans="1:4" ht="12.75" customHeight="1">
       <c r="A85" t="s">
-        <v>225</v>
+        <v>224</v>
       </c>
       <c r="B85" t="s">
+        <v>235</v>
+      </c>
+      <c r="D85" t="s">
         <v>236</v>
-      </c>
-      <c r="D85" t="s">
-        <v>237</v>
       </c>
     </row>
     <row r="87" spans="1:4" ht="12.75" customHeight="1">
       <c r="A87" t="s">
+        <v>237</v>
+      </c>
+      <c r="B87" t="s">
         <v>238</v>
       </c>
-      <c r="B87" t="s">
+      <c r="C87" t="s">
         <v>239</v>
-      </c>
-      <c r="C87" t="s">
-        <v>240</v>
       </c>
     </row>
     <row r="88" spans="1:4" ht="12.75" customHeight="1">
       <c r="A88" t="s">
-        <v>238</v>
+        <v>237</v>
       </c>
       <c r="B88" t="s">
+        <v>240</v>
+      </c>
+      <c r="C88" t="s">
         <v>241</v>
-      </c>
-      <c r="C88" t="s">
-        <v>242</v>
       </c>
     </row>
     <row r="89" spans="1:4" ht="12.75" customHeight="1">
       <c r="A89" t="s">
-        <v>238</v>
+        <v>237</v>
       </c>
       <c r="B89" t="s">
+        <v>242</v>
+      </c>
+      <c r="C89" t="s">
         <v>243</v>
-      </c>
-      <c r="C89" t="s">
-        <v>244</v>
       </c>
     </row>
     <row r="90" spans="1:4" ht="12.75" customHeight="1">
       <c r="A90" t="s">
-        <v>238</v>
+        <v>237</v>
       </c>
       <c r="B90" t="s">
+        <v>244</v>
+      </c>
+      <c r="C90" t="s">
         <v>245</v>
-      </c>
-      <c r="C90" t="s">
-        <v>246</v>
       </c>
     </row>
     <row r="91" spans="1:4" ht="12.75" customHeight="1">
       <c r="A91" t="s">
-        <v>238</v>
+        <v>237</v>
       </c>
       <c r="B91" t="s">
+        <v>246</v>
+      </c>
+      <c r="C91" t="s">
         <v>247</v>
-      </c>
-      <c r="C91" t="s">
-        <v>248</v>
       </c>
     </row>
     <row r="92" spans="1:4" ht="12.75" customHeight="1">
       <c r="A92" t="s">
-        <v>238</v>
+        <v>237</v>
       </c>
       <c r="B92" t="s">
+        <v>248</v>
+      </c>
+      <c r="C92" t="s">
         <v>249</v>
-      </c>
-      <c r="C92" t="s">
-        <v>250</v>
       </c>
     </row>
     <row r="93" spans="1:4" ht="12.75" customHeight="1">
       <c r="A93" t="s">
-        <v>238</v>
+        <v>237</v>
       </c>
       <c r="B93" t="s">
+        <v>250</v>
+      </c>
+      <c r="C93" t="s">
         <v>251</v>
-      </c>
-      <c r="C93" t="s">
-        <v>252</v>
       </c>
     </row>
     <row r="95" spans="1:4" ht="12.75" customHeight="1">
       <c r="A95" t="s">
+        <v>252</v>
+      </c>
+      <c r="B95" t="s">
         <v>253</v>
       </c>
-      <c r="B95" t="s">
+      <c r="C95" t="s">
         <v>254</v>
-      </c>
-      <c r="C95" t="s">
-        <v>255</v>
       </c>
     </row>
     <row r="96" spans="1:4" ht="12.75" customHeight="1">
       <c r="A96" t="s">
-        <v>253</v>
+        <v>252</v>
       </c>
       <c r="B96" t="s">
+        <v>255</v>
+      </c>
+      <c r="C96" t="s">
         <v>256</v>
-      </c>
-      <c r="C96" t="s">
-        <v>257</v>
       </c>
     </row>
     <row r="97" spans="1:3" ht="12.75" customHeight="1">
       <c r="A97" t="s">
-        <v>253</v>
+        <v>252</v>
       </c>
       <c r="B97" t="s">
+        <v>257</v>
+      </c>
+      <c r="C97" t="s">
         <v>258</v>
-      </c>
-      <c r="C97" t="s">
-        <v>259</v>
       </c>
     </row>
     <row r="98" spans="1:3" ht="12.75" customHeight="1">
       <c r="A98" t="s">
-        <v>253</v>
+        <v>252</v>
       </c>
       <c r="B98" t="s">
+        <v>259</v>
+      </c>
+      <c r="C98" t="s">
         <v>260</v>
-      </c>
-      <c r="C98" t="s">
-        <v>261</v>
       </c>
     </row>
     <row r="99" spans="1:3" ht="12.75" customHeight="1">
       <c r="A99" t="s">
-        <v>253</v>
+        <v>252</v>
       </c>
       <c r="B99" t="s">
+        <v>261</v>
+      </c>
+      <c r="C99" t="s">
         <v>262</v>
-      </c>
-      <c r="C99" t="s">
-        <v>263</v>
       </c>
     </row>
     <row r="100" spans="1:3" ht="12.75" customHeight="1">
       <c r="A100" t="s">
-        <v>253</v>
+        <v>252</v>
       </c>
       <c r="B100" t="s">
+        <v>263</v>
+      </c>
+      <c r="C100" t="s">
         <v>264</v>
-      </c>
-      <c r="C100" t="s">
-        <v>265</v>
       </c>
     </row>
     <row r="102" spans="1:3" ht="12.75" customHeight="1">
       <c r="A102" t="s">
+        <v>265</v>
+      </c>
+      <c r="B102" t="s">
         <v>266</v>
       </c>
-      <c r="B102" t="s">
+      <c r="C102" t="s">
         <v>267</v>
-      </c>
-      <c r="C102" t="s">
-        <v>268</v>
       </c>
     </row>
     <row r="103" spans="1:3" ht="12.75" customHeight="1">
       <c r="A103" t="s">
-        <v>266</v>
+        <v>265</v>
       </c>
       <c r="B103" t="s">
+        <v>268</v>
+      </c>
+      <c r="C103" t="s">
         <v>269</v>
-      </c>
-      <c r="C103" t="s">
-        <v>270</v>
       </c>
     </row>
     <row r="104" spans="1:3" ht="12.75" customHeight="1">
       <c r="A104" t="s">
-        <v>266</v>
+        <v>265</v>
       </c>
       <c r="B104" t="s">
+        <v>270</v>
+      </c>
+      <c r="C104" t="s">
         <v>271</v>
-      </c>
-      <c r="C104" t="s">
-        <v>272</v>
       </c>
     </row>
     <row r="105" spans="1:3" ht="12.75" customHeight="1">
       <c r="A105" t="s">
-        <v>266</v>
+        <v>265</v>
       </c>
       <c r="B105" t="s">
+        <v>272</v>
+      </c>
+      <c r="C105" t="s">
         <v>273</v>
-      </c>
-      <c r="C105" t="s">
-        <v>274</v>
       </c>
     </row>
     <row r="106" spans="1:3" ht="12.75" customHeight="1">
       <c r="A106" t="s">
-        <v>266</v>
+        <v>265</v>
       </c>
       <c r="B106" t="s">
+        <v>274</v>
+      </c>
+      <c r="C106" t="s">
         <v>275</v>
-      </c>
-      <c r="C106" t="s">
-        <v>276</v>
       </c>
     </row>
     <row r="107" spans="1:3" ht="12.75" customHeight="1">
       <c r="A107" t="s">
-        <v>266</v>
+        <v>265</v>
       </c>
       <c r="B107" t="s">
+        <v>276</v>
+      </c>
+      <c r="C107" t="s">
         <v>277</v>
-      </c>
-      <c r="C107" t="s">
-        <v>278</v>
       </c>
     </row>
     <row r="108" spans="1:3" ht="12.75" customHeight="1">
       <c r="A108" t="s">
-        <v>266</v>
+        <v>265</v>
       </c>
       <c r="B108" t="s">
+        <v>278</v>
+      </c>
+      <c r="C108" t="s">
         <v>279</v>
-      </c>
-      <c r="C108" t="s">
-        <v>280</v>
       </c>
     </row>
     <row r="110" spans="1:3" ht="12.75" customHeight="1">
       <c r="A110" t="s">
+        <v>280</v>
+      </c>
+      <c r="B110" t="s">
         <v>281</v>
       </c>
-      <c r="B110" t="s">
+      <c r="C110" t="s">
         <v>282</v>
-      </c>
-      <c r="C110" t="s">
-        <v>283</v>
       </c>
     </row>
     <row r="111" spans="1:3" ht="12.75" customHeight="1">
       <c r="A111" t="s">
-        <v>281</v>
+        <v>280</v>
       </c>
       <c r="B111" t="s">
+        <v>283</v>
+      </c>
+      <c r="C111" t="s">
         <v>284</v>
-      </c>
-      <c r="C111" t="s">
-        <v>285</v>
       </c>
     </row>
     <row r="112" spans="1:3" ht="12.75" customHeight="1">
       <c r="A112" t="s">
-        <v>281</v>
+        <v>280</v>
       </c>
       <c r="B112" t="s">
+        <v>285</v>
+      </c>
+      <c r="C112" t="s">
         <v>286</v>
-      </c>
-      <c r="C112" t="s">
-        <v>287</v>
       </c>
     </row>
     <row r="113" spans="1:3" ht="12.75" customHeight="1">
       <c r="A113" t="s">
-        <v>281</v>
+        <v>280</v>
       </c>
       <c r="B113" t="s">
+        <v>287</v>
+      </c>
+      <c r="C113" t="s">
         <v>288</v>
-      </c>
-      <c r="C113" t="s">
-        <v>289</v>
       </c>
     </row>
     <row r="114" spans="1:3" ht="12.75" customHeight="1">
       <c r="A114" t="s">
-        <v>281</v>
+        <v>280</v>
       </c>
       <c r="B114" t="s">
+        <v>289</v>
+      </c>
+      <c r="C114" t="s">
         <v>290</v>
-      </c>
-      <c r="C114" t="s">
-        <v>291</v>
       </c>
     </row>
     <row r="115" spans="1:3" ht="12.75" customHeight="1">
       <c r="A115" t="s">
-        <v>281</v>
+        <v>280</v>
       </c>
       <c r="B115" t="s">
+        <v>291</v>
+      </c>
+      <c r="C115" t="s">
         <v>292</v>
-      </c>
-      <c r="C115" t="s">
-        <v>293</v>
       </c>
     </row>
     <row r="117" spans="1:3" ht="12.75" customHeight="1">
       <c r="A117" t="s">
+        <v>293</v>
+      </c>
+      <c r="B117" t="s">
         <v>294</v>
       </c>
-      <c r="B117" t="s">
+      <c r="C117" t="s">
         <v>295</v>
-      </c>
-      <c r="C117" t="s">
-        <v>296</v>
       </c>
     </row>
     <row r="118" spans="1:3" ht="12.75" customHeight="1">
       <c r="A118" t="s">
-        <v>294</v>
+        <v>293</v>
       </c>
       <c r="B118" t="s">
+        <v>296</v>
+      </c>
+      <c r="C118" t="s">
         <v>297</v>
-      </c>
-      <c r="C118" t="s">
-        <v>298</v>
       </c>
     </row>
     <row r="119" spans="1:3" ht="12.75" customHeight="1">
       <c r="A119" t="s">
-        <v>294</v>
+        <v>293</v>
       </c>
       <c r="B119" t="s">
+        <v>298</v>
+      </c>
+      <c r="C119" t="s">
         <v>299</v>
-      </c>
-      <c r="C119" t="s">
-        <v>300</v>
       </c>
     </row>
     <row r="120" spans="1:3" ht="12.75" customHeight="1">
       <c r="A120" t="s">
-        <v>294</v>
+        <v>293</v>
       </c>
       <c r="B120" t="s">
+        <v>300</v>
+      </c>
+      <c r="C120" t="s">
         <v>301</v>
-      </c>
-      <c r="C120" t="s">
-        <v>302</v>
       </c>
     </row>
     <row r="121" spans="1:3" ht="12.75" customHeight="1">
       <c r="A121" t="s">
-        <v>294</v>
+        <v>293</v>
       </c>
       <c r="B121" t="s">
+        <v>302</v>
+      </c>
+      <c r="C121" t="s">
         <v>303</v>
-      </c>
-      <c r="C121" t="s">
-        <v>304</v>
       </c>
     </row>
     <row r="122" spans="1:3" ht="12.75" customHeight="1">
       <c r="A122" t="s">
-        <v>294</v>
+        <v>293</v>
       </c>
       <c r="B122" t="s">
+        <v>304</v>
+      </c>
+      <c r="C122" t="s">
         <v>305</v>
-      </c>
-      <c r="C122" t="s">
-        <v>306</v>
       </c>
     </row>
     <row r="123" spans="1:3" ht="12.75" customHeight="1">
       <c r="A123" t="s">
-        <v>294</v>
+        <v>293</v>
       </c>
       <c r="B123" t="s">
+        <v>306</v>
+      </c>
+      <c r="C123" t="s">
         <v>307</v>
-      </c>
-      <c r="C123" t="s">
-        <v>308</v>
       </c>
     </row>
     <row r="125" spans="1:3" ht="12.75" customHeight="1">
       <c r="A125" t="s">
+        <v>308</v>
+      </c>
+      <c r="B125" t="s">
         <v>309</v>
       </c>
-      <c r="B125" t="s">
+      <c r="C125" t="s">
         <v>310</v>
-      </c>
-      <c r="C125" t="s">
-        <v>311</v>
       </c>
     </row>
     <row r="126" spans="1:3" ht="12.75" customHeight="1">
       <c r="A126" t="s">
-        <v>309</v>
+        <v>308</v>
       </c>
       <c r="B126" t="s">
+        <v>311</v>
+      </c>
+      <c r="C126" t="s">
         <v>312</v>
-      </c>
-      <c r="C126" t="s">
-        <v>313</v>
       </c>
     </row>
     <row r="127" spans="1:3" ht="12.75" customHeight="1">
       <c r="A127" t="s">
-        <v>309</v>
+        <v>308</v>
       </c>
       <c r="B127" t="s">
+        <v>313</v>
+      </c>
+      <c r="C127" t="s">
         <v>314</v>
-      </c>
-      <c r="C127" t="s">
-        <v>315</v>
       </c>
     </row>
     <row r="128" spans="1:3" ht="12.75" customHeight="1">
       <c r="A128" t="s">
-        <v>309</v>
+        <v>308</v>
       </c>
       <c r="B128" t="s">
+        <v>315</v>
+      </c>
+      <c r="C128" t="s">
         <v>316</v>
-      </c>
-      <c r="C128" t="s">
-        <v>317</v>
       </c>
     </row>
     <row r="129" spans="1:4" ht="12.75" customHeight="1">
       <c r="A129" t="s">
-        <v>309</v>
+        <v>308</v>
       </c>
       <c r="B129" t="s">
+        <v>317</v>
+      </c>
+      <c r="C129" t="s">
         <v>318</v>
-      </c>
-      <c r="C129" t="s">
-        <v>319</v>
       </c>
     </row>
     <row r="130" spans="1:4" ht="12.75" customHeight="1">
       <c r="A130" t="s">
-        <v>309</v>
+        <v>308</v>
       </c>
       <c r="B130" t="s">
+        <v>319</v>
+      </c>
+      <c r="C130" t="s">
         <v>320</v>
-      </c>
-      <c r="C130" t="s">
-        <v>321</v>
       </c>
     </row>
     <row r="132" spans="1:4" ht="12.75" customHeight="1">
       <c r="A132" t="s">
+        <v>321</v>
+      </c>
+      <c r="B132" t="s">
         <v>322</v>
       </c>
-      <c r="B132" t="s">
+      <c r="C132" t="s">
         <v>323</v>
-      </c>
-      <c r="C132" t="s">
-        <v>324</v>
       </c>
     </row>
     <row r="133" spans="1:4" ht="12.75" customHeight="1">
       <c r="A133" t="s">
-        <v>322</v>
+        <v>321</v>
       </c>
       <c r="B133" t="s">
+        <v>324</v>
+      </c>
+      <c r="C133" t="s">
         <v>325</v>
-      </c>
-      <c r="C133" t="s">
-        <v>326</v>
       </c>
     </row>
     <row r="135" spans="1:4" ht="12.75" customHeight="1">
       <c r="A135" s="2" t="s">
+        <v>326</v>
+      </c>
+      <c r="D135" t="s">
         <v>327</v>
-      </c>
-      <c r="D135" t="s">
-        <v>328</v>
       </c>
     </row>
     <row r="136" spans="1:4" ht="12.75" customHeight="1">
       <c r="A136" t="s">
-        <v>327</v>
+        <v>326</v>
       </c>
       <c r="D136" t="s">
-        <v>329</v>
+        <v>328</v>
       </c>
     </row>
     <row r="137" spans="1:4" ht="12.75" customHeight="1">
       <c r="A137" s="2" t="s">
-        <v>327</v>
+        <v>326</v>
       </c>
       <c r="D137" t="s">
-        <v>330</v>
+        <v>329</v>
       </c>
     </row>
     <row r="138" spans="1:4" ht="12.75" customHeight="1">
       <c r="A138" s="2" t="s">
-        <v>327</v>
+        <v>326</v>
       </c>
       <c r="D138" t="s">
-        <v>331</v>
+        <v>330</v>
       </c>
     </row>
     <row r="139" spans="1:4" ht="12.75" customHeight="1">
       <c r="A139" s="2" t="s">
-        <v>327</v>
+        <v>326</v>
       </c>
       <c r="D139" t="s">
-        <v>332</v>
+        <v>331</v>
       </c>
     </row>
   </sheetData>
@@ -6760,151 +6768,151 @@
     </row>
     <row r="4" spans="1:2" ht="12.75" customHeight="1">
       <c r="A4" t="s">
+        <v>332</v>
+      </c>
+      <c r="B4" t="s">
         <v>333</v>
-      </c>
-      <c r="B4" t="s">
-        <v>334</v>
       </c>
     </row>
     <row r="5" spans="1:2" ht="12.75" customHeight="1">
       <c r="A5" t="s">
+        <v>334</v>
+      </c>
+      <c r="B5" t="s">
         <v>335</v>
-      </c>
-      <c r="B5" t="s">
-        <v>336</v>
       </c>
     </row>
     <row r="6" spans="1:2" ht="12.75" customHeight="1">
       <c r="A6" t="s">
+        <v>336</v>
+      </c>
+      <c r="B6" t="s">
         <v>337</v>
-      </c>
-      <c r="B6" t="s">
-        <v>338</v>
       </c>
     </row>
     <row r="8" spans="1:2" ht="12" customHeight="1">
       <c r="A8" t="s">
+        <v>338</v>
+      </c>
+      <c r="B8" t="s">
         <v>339</v>
-      </c>
-      <c r="B8" t="s">
-        <v>340</v>
       </c>
     </row>
     <row r="9" spans="1:2" ht="12" customHeight="1">
       <c r="A9" t="s">
+        <v>340</v>
+      </c>
+      <c r="B9" t="s">
         <v>341</v>
-      </c>
-      <c r="B9" t="s">
-        <v>342</v>
       </c>
     </row>
     <row r="10" spans="1:2" ht="12" customHeight="1">
       <c r="A10" t="s">
+        <v>342</v>
+      </c>
+      <c r="B10" t="s">
         <v>343</v>
-      </c>
-      <c r="B10" t="s">
-        <v>344</v>
       </c>
     </row>
     <row r="11" spans="1:2" ht="12" customHeight="1">
       <c r="A11" t="s">
+        <v>344</v>
+      </c>
+      <c r="B11" t="s">
         <v>345</v>
-      </c>
-      <c r="B11" t="s">
-        <v>346</v>
       </c>
     </row>
     <row r="12" spans="1:2" ht="12" customHeight="1">
       <c r="A12" t="s">
+        <v>346</v>
+      </c>
+      <c r="B12" t="s">
         <v>347</v>
-      </c>
-      <c r="B12" t="s">
-        <v>348</v>
       </c>
     </row>
     <row r="13" spans="1:2" ht="12" customHeight="1">
       <c r="A13" t="s">
+        <v>348</v>
+      </c>
+      <c r="B13" t="s">
         <v>349</v>
-      </c>
-      <c r="B13" t="s">
-        <v>350</v>
       </c>
     </row>
     <row r="14" spans="1:2" ht="42" customHeight="1">
       <c r="A14" t="s">
+        <v>350</v>
+      </c>
+      <c r="B14" t="s">
         <v>351</v>
-      </c>
-      <c r="B14" t="s">
-        <v>352</v>
       </c>
     </row>
     <row r="15" spans="1:2" ht="12.75" customHeight="1">
       <c r="A15" t="s">
+        <v>352</v>
+      </c>
+      <c r="B15" t="s">
         <v>353</v>
-      </c>
-      <c r="B15" t="s">
-        <v>354</v>
       </c>
     </row>
     <row r="16" spans="1:2" ht="12.75" customHeight="1">
       <c r="A16" t="s">
+        <v>354</v>
+      </c>
+      <c r="B16" t="s">
         <v>355</v>
-      </c>
-      <c r="B16" t="s">
-        <v>356</v>
       </c>
     </row>
     <row r="17" spans="1:2" ht="12.75" customHeight="1">
       <c r="A17" t="s">
+        <v>356</v>
+      </c>
+      <c r="B17" t="s">
         <v>357</v>
-      </c>
-      <c r="B17" t="s">
-        <v>358</v>
       </c>
     </row>
     <row r="18" spans="1:2" ht="12.75" customHeight="1">
       <c r="A18" t="s">
+        <v>358</v>
+      </c>
+      <c r="B18" t="s">
         <v>359</v>
-      </c>
-      <c r="B18" t="s">
-        <v>360</v>
       </c>
     </row>
     <row r="19" spans="1:2" ht="12.75" customHeight="1">
       <c r="A19" t="s">
+        <v>360</v>
+      </c>
+      <c r="B19" t="s">
         <v>361</v>
-      </c>
-      <c r="B19" t="s">
-        <v>362</v>
       </c>
     </row>
     <row r="20" spans="1:2" ht="12.75" customHeight="1">
       <c r="A20" t="s">
+        <v>362</v>
+      </c>
+      <c r="B20" t="s">
         <v>363</v>
-      </c>
-      <c r="B20" t="s">
-        <v>364</v>
       </c>
     </row>
     <row r="21" spans="1:2" ht="12.75" customHeight="1">
       <c r="A21" t="s">
+        <v>364</v>
+      </c>
+      <c r="B21" t="s">
         <v>365</v>
-      </c>
-      <c r="B21" t="s">
-        <v>366</v>
       </c>
     </row>
     <row r="22" spans="1:2" ht="12.75" customHeight="1">
       <c r="A22" t="s">
+        <v>366</v>
+      </c>
+      <c r="B22" t="s">
         <v>367</v>
-      </c>
-      <c r="B22" t="s">
-        <v>368</v>
       </c>
     </row>
     <row r="24" spans="1:2" ht="12.75" customHeight="1">
       <c r="A24" t="s">
-        <v>369</v>
+        <v>368</v>
       </c>
       <c r="B24" t="s">
         <v>51</v>
@@ -6912,10 +6920,10 @@
     </row>
     <row r="25" spans="1:2" ht="12.75" customHeight="1">
       <c r="A25" t="s">
+        <v>369</v>
+      </c>
+      <c r="B25" t="s">
         <v>370</v>
-      </c>
-      <c r="B25" t="s">
-        <v>371</v>
       </c>
     </row>
     <row r="26" spans="1:2" ht="12.75" customHeight="1">
@@ -6923,7 +6931,7 @@
         <v>39</v>
       </c>
       <c r="B26" t="s">
-        <v>372</v>
+        <v>371</v>
       </c>
     </row>
     <row r="27" spans="1:2" ht="12.75" customHeight="1">
@@ -6931,7 +6939,7 @@
         <v>38</v>
       </c>
       <c r="B27" t="s">
-        <v>373</v>
+        <v>372</v>
       </c>
     </row>
     <row r="28" spans="1:2" ht="12.75" customHeight="1">
@@ -7072,7 +7080,7 @@
         <v>9</v>
       </c>
       <c r="B2" t="s">
-        <v>388</v>
+        <v>387</v>
       </c>
     </row>
     <row r="3" spans="1:2" ht="12.75" customHeight="1">
@@ -7080,7 +7088,7 @@
         <v>10</v>
       </c>
       <c r="B3" t="s">
-        <v>389</v>
+        <v>388</v>
       </c>
     </row>
     <row r="4" spans="1:2" ht="12.75" customHeight="1">
@@ -7088,7 +7096,7 @@
         <v>11</v>
       </c>
       <c r="B4" t="s">
-        <v>388</v>
+        <v>387</v>
       </c>
     </row>
   </sheetData>
@@ -7116,15 +7124,15 @@
         <v>1</v>
       </c>
       <c r="B1" t="s">
-        <v>390</v>
+        <v>389</v>
       </c>
     </row>
     <row r="2" spans="1:2">
       <c r="A2" t="s">
+        <v>390</v>
+      </c>
+      <c r="B2" t="s">
         <v>391</v>
-      </c>
-      <c r="B2" t="s">
-        <v>392</v>
       </c>
     </row>
     <row r="3" spans="1:2">
@@ -7132,15 +7140,15 @@
         <v>137</v>
       </c>
       <c r="B3" t="s">
-        <v>392</v>
+        <v>391</v>
       </c>
     </row>
     <row r="4" spans="1:2">
       <c r="A4" t="s">
-        <v>393</v>
+        <v>392</v>
       </c>
       <c r="B4" t="s">
-        <v>392</v>
+        <v>391</v>
       </c>
     </row>
   </sheetData>

</xml_diff>

<commit_message>
add images to chest xray
</commit_message>
<xml_diff>
--- a/opendatakit.collect2/form-files/neonatal/neonatal.xlsx
+++ b/opendatakit.collect2/form-files/neonatal/neonatal.xlsx
@@ -4,7 +4,7 @@
   <fileVersion appName="xl" lastEdited="5" lowestEdited="5" rupBuild="22905"/>
   <workbookPr autoCompressPictures="0"/>
   <bookViews>
-    <workbookView xWindow="1800" yWindow="0" windowWidth="18360" windowHeight="15280" tabRatio="500" activeTab="1"/>
+    <workbookView xWindow="1800" yWindow="0" windowWidth="18360" windowHeight="15280" tabRatio="500"/>
   </bookViews>
   <sheets>
     <sheet name="survey" sheetId="1" r:id="rId1"/>
@@ -2005,7 +2005,7 @@
       <diagonal/>
     </border>
   </borders>
-  <cellStyleXfs count="418">
+  <cellStyleXfs count="422">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
     <xf numFmtId="0" fontId="3" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
     <xf numFmtId="0" fontId="4" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
@@ -2350,6 +2350,10 @@
     <xf numFmtId="0" fontId="3" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
     <xf numFmtId="0" fontId="4" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
     <xf numFmtId="0" fontId="1" fillId="12" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="4" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="4" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
     <xf numFmtId="0" fontId="3" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
     <xf numFmtId="0" fontId="4" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
     <xf numFmtId="0" fontId="3" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
@@ -2529,7 +2533,7 @@
       <alignment wrapText="1"/>
     </xf>
   </cellXfs>
-  <cellStyles count="418">
+  <cellStyles count="422">
     <cellStyle name="20% - Accent4" xfId="343" builtinId="42"/>
     <cellStyle name="Followed Hyperlink" xfId="2" builtinId="9" hidden="1"/>
     <cellStyle name="Followed Hyperlink" xfId="4" builtinId="9" hidden="1"/>
@@ -2738,6 +2742,8 @@
     <cellStyle name="Followed Hyperlink" xfId="413" builtinId="9" hidden="1"/>
     <cellStyle name="Followed Hyperlink" xfId="415" builtinId="9" hidden="1"/>
     <cellStyle name="Followed Hyperlink" xfId="417" builtinId="9" hidden="1"/>
+    <cellStyle name="Followed Hyperlink" xfId="419" builtinId="9" hidden="1"/>
+    <cellStyle name="Followed Hyperlink" xfId="421" builtinId="9" hidden="1"/>
     <cellStyle name="Good" xfId="243" builtinId="26"/>
     <cellStyle name="Hyperlink" xfId="1" builtinId="8" hidden="1"/>
     <cellStyle name="Hyperlink" xfId="3" builtinId="8" hidden="1"/>
@@ -2946,6 +2952,8 @@
     <cellStyle name="Hyperlink" xfId="412" builtinId="8" hidden="1"/>
     <cellStyle name="Hyperlink" xfId="414" builtinId="8" hidden="1"/>
     <cellStyle name="Hyperlink" xfId="416" builtinId="8" hidden="1"/>
+    <cellStyle name="Hyperlink" xfId="418" builtinId="8" hidden="1"/>
+    <cellStyle name="Hyperlink" xfId="420" builtinId="8" hidden="1"/>
     <cellStyle name="Neutral" xfId="244" builtinId="28"/>
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
   </cellStyles>
@@ -3278,9 +3286,9 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:J194"/>
   <sheetViews>
-    <sheetView topLeftCell="C1" workbookViewId="0">
-      <pane ySplit="1" topLeftCell="A29" activePane="bottomLeft" state="frozen"/>
-      <selection pane="bottomLeft" activeCell="D34" sqref="D34"/>
+    <sheetView tabSelected="1" topLeftCell="C1" workbookViewId="0">
+      <pane ySplit="1" topLeftCell="A22" activePane="bottomLeft" state="frozen"/>
+      <selection pane="bottomLeft" activeCell="H43" sqref="H43"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultColWidth="11.5" defaultRowHeight="12.75" customHeight="1" x14ac:dyDescent="0"/>
@@ -5441,7 +5449,7 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:D139"/>
   <sheetViews>
-    <sheetView tabSelected="1" zoomScale="150" zoomScaleNormal="150" zoomScalePageLayoutView="150" workbookViewId="0">
+    <sheetView zoomScale="150" zoomScaleNormal="150" zoomScalePageLayoutView="150" workbookViewId="0">
       <selection activeCell="D18" sqref="D18"/>
     </sheetView>
   </sheetViews>

</xml_diff>

<commit_message>
add images to abdominal XRAY
</commit_message>
<xml_diff>
--- a/opendatakit.collect2/form-files/neonatal/neonatal.xlsx
+++ b/opendatakit.collect2/form-files/neonatal/neonatal.xlsx
@@ -23,7 +23,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="870" uniqueCount="536">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="869" uniqueCount="535">
   <si>
     <t>type</t>
   </si>
@@ -1595,9 +1595,6 @@
   </si>
   <si>
     <t>selected(data('diagnostic_menu'),'placement')</t>
-  </si>
-  <si>
-    <t>Chest &amp; Abdominal Xray</t>
   </si>
   <si>
     <t>selected(data('diagnostic_menu'),'xray')</t>
@@ -3286,9 +3283,9 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:J194"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="C1" workbookViewId="0">
-      <pane ySplit="1" topLeftCell="A22" activePane="bottomLeft" state="frozen"/>
-      <selection pane="bottomLeft" activeCell="H43" sqref="H43"/>
+    <sheetView tabSelected="1" workbookViewId="0">
+      <pane ySplit="1" topLeftCell="A21" activePane="bottomLeft" state="frozen"/>
+      <selection pane="bottomLeft" activeCell="D34" sqref="D34"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultColWidth="11.5" defaultRowHeight="12.75" customHeight="1" x14ac:dyDescent="0"/>
@@ -3386,7 +3383,7 @@
     </row>
     <row r="6" spans="1:10" ht="15">
       <c r="A6" s="7" t="s">
-        <v>501</v>
+        <v>500</v>
       </c>
       <c r="B6" s="8" t="s">
         <v>377</v>
@@ -3546,7 +3543,7 @@
       </c>
       <c r="D19"/>
       <c r="I19" s="12" t="s">
-        <v>533</v>
+        <v>532</v>
       </c>
     </row>
     <row r="20" spans="1:10" s="12" customFormat="1" ht="12">
@@ -3591,7 +3588,7 @@
     </row>
     <row r="25" spans="1:10" ht="15">
       <c r="A25" s="7" t="s">
-        <v>502</v>
+        <v>501</v>
       </c>
       <c r="B25" s="8" t="s">
         <v>433</v>
@@ -3631,7 +3628,7 @@
       <c r="C27" s="40"/>
       <c r="D27" s="40"/>
       <c r="E27" s="40" t="s">
-        <v>496</v>
+        <v>495</v>
       </c>
       <c r="F27" s="40"/>
       <c r="G27" s="40"/>
@@ -3645,7 +3642,7 @@
       <c r="C28" s="40"/>
       <c r="D28" s="40"/>
       <c r="E28" s="40" t="s">
-        <v>497</v>
+        <v>496</v>
       </c>
       <c r="F28" s="40"/>
       <c r="G28" s="40"/>
@@ -3710,7 +3707,7 @@
       </c>
       <c r="F32" s="2"/>
       <c r="I32" t="s">
-        <v>498</v>
+        <v>497</v>
       </c>
     </row>
     <row r="33" spans="1:9" ht="18" customHeight="1">
@@ -3733,21 +3730,19 @@
         <v>452</v>
       </c>
       <c r="C34" s="19"/>
-      <c r="D34" s="2" t="s">
+      <c r="D34" s="2"/>
+      <c r="E34" s="2" t="s">
         <v>455</v>
-      </c>
-      <c r="E34" s="2" t="s">
-        <v>456</v>
       </c>
       <c r="F34" s="2"/>
       <c r="I34" t="s">
-        <v>534</v>
+        <v>533</v>
       </c>
     </row>
     <row r="35" spans="1:9" ht="15">
       <c r="A35" s="7"/>
       <c r="B35" s="8" t="s">
-        <v>495</v>
+        <v>494</v>
       </c>
       <c r="C35" s="8"/>
       <c r="D35" s="8"/>
@@ -3772,7 +3767,7 @@
       <c r="C37" s="15"/>
       <c r="D37" s="15"/>
       <c r="E37" s="15" t="s">
-        <v>499</v>
+        <v>498</v>
       </c>
       <c r="F37" s="15"/>
       <c r="G37" s="15"/>
@@ -3785,7 +3780,7 @@
       <c r="C38" s="15"/>
       <c r="D38" s="15"/>
       <c r="E38" s="15" t="s">
-        <v>500</v>
+        <v>499</v>
       </c>
       <c r="F38" s="15"/>
       <c r="G38" s="15"/>
@@ -4081,12 +4076,12 @@
     </row>
     <row r="67" spans="1:8" ht="12.75" customHeight="1">
       <c r="B67" s="14" t="s">
-        <v>505</v>
+        <v>504</v>
       </c>
       <c r="C67" s="15"/>
       <c r="D67" s="15"/>
       <c r="E67" s="15" t="s">
-        <v>509</v>
+        <v>508</v>
       </c>
       <c r="F67" s="15"/>
       <c r="G67" s="15"/>
@@ -4094,12 +4089,12 @@
     </row>
     <row r="68" spans="1:8" ht="12.75" customHeight="1">
       <c r="B68" s="14" t="s">
-        <v>506</v>
+        <v>505</v>
       </c>
       <c r="C68" s="15"/>
       <c r="D68" s="15"/>
       <c r="E68" s="15" t="s">
-        <v>510</v>
+        <v>509</v>
       </c>
       <c r="F68" s="15"/>
       <c r="G68" s="15"/>
@@ -4107,10 +4102,10 @@
     </row>
     <row r="69" spans="1:8" ht="12.75" customHeight="1">
       <c r="A69" s="7" t="s">
-        <v>511</v>
+        <v>510</v>
       </c>
       <c r="B69" s="8" t="s">
-        <v>507</v>
+        <v>506</v>
       </c>
       <c r="C69" s="13"/>
       <c r="D69" s="13"/>
@@ -4122,13 +4117,13 @@
     <row r="70" spans="1:8" ht="12.75" customHeight="1">
       <c r="A70" s="16"/>
       <c r="B70" t="s">
+        <v>511</v>
+      </c>
+      <c r="C70" t="s">
         <v>512</v>
       </c>
-      <c r="C70" t="s">
-        <v>513</v>
-      </c>
       <c r="D70" t="s">
-        <v>511</v>
+        <v>510</v>
       </c>
       <c r="E70" s="42"/>
       <c r="F70" t="s">
@@ -4145,7 +4140,7 @@
       <c r="C71" s="32"/>
       <c r="D71" s="32"/>
       <c r="E71" t="s">
-        <v>519</v>
+        <v>518</v>
       </c>
       <c r="F71" s="32"/>
       <c r="G71" s="32"/>
@@ -4158,7 +4153,7 @@
       </c>
       <c r="C72" s="32"/>
       <c r="D72" s="43" t="s">
-        <v>516</v>
+        <v>515</v>
       </c>
       <c r="E72" s="32"/>
       <c r="F72" s="32"/>
@@ -4179,7 +4174,7 @@
       <c r="C74" s="32"/>
       <c r="D74" s="32"/>
       <c r="E74" t="s">
-        <v>518</v>
+        <v>517</v>
       </c>
       <c r="F74" s="32"/>
       <c r="G74" s="32"/>
@@ -4192,7 +4187,7 @@
       </c>
       <c r="C75" s="32"/>
       <c r="D75" s="43" t="s">
-        <v>517</v>
+        <v>516</v>
       </c>
       <c r="E75" s="32"/>
       <c r="F75" s="32"/>
@@ -4208,7 +4203,7 @@
     <row r="77" spans="1:8" ht="12.75" customHeight="1">
       <c r="A77" s="7"/>
       <c r="B77" s="8" t="s">
-        <v>508</v>
+        <v>507</v>
       </c>
       <c r="C77" s="13"/>
       <c r="D77" s="13"/>
@@ -4228,12 +4223,12 @@
     </row>
     <row r="79" spans="1:8" ht="12.75" customHeight="1">
       <c r="B79" s="14" t="s">
-        <v>521</v>
+        <v>520</v>
       </c>
       <c r="C79" s="15"/>
       <c r="D79" s="15"/>
       <c r="E79" s="15" t="s">
-        <v>526</v>
+        <v>525</v>
       </c>
       <c r="F79" s="15"/>
       <c r="G79" s="15"/>
@@ -4241,12 +4236,12 @@
     </row>
     <row r="80" spans="1:8" ht="12.75" customHeight="1">
       <c r="B80" s="14" t="s">
-        <v>522</v>
+        <v>521</v>
       </c>
       <c r="C80" s="15"/>
       <c r="D80" s="15"/>
       <c r="E80" s="15" t="s">
-        <v>527</v>
+        <v>526</v>
       </c>
       <c r="F80" s="15"/>
       <c r="G80" s="15"/>
@@ -4254,10 +4249,10 @@
     </row>
     <row r="81" spans="1:8" ht="12.75" customHeight="1">
       <c r="A81" s="7" t="s">
-        <v>520</v>
+        <v>519</v>
       </c>
       <c r="B81" s="8" t="s">
-        <v>523</v>
+        <v>522</v>
       </c>
       <c r="C81" s="13"/>
       <c r="D81" s="13"/>
@@ -4269,10 +4264,10 @@
     <row r="82" spans="1:8" ht="12.75" customHeight="1">
       <c r="A82" s="16"/>
       <c r="B82" t="s">
-        <v>524</v>
+        <v>523</v>
       </c>
       <c r="C82" t="s">
-        <v>528</v>
+        <v>527</v>
       </c>
       <c r="D82" t="s">
         <v>443</v>
@@ -4290,208 +4285,208 @@
         <v>392</v>
       </c>
       <c r="C83" s="45" t="s">
-        <v>457</v>
+        <v>456</v>
       </c>
       <c r="E83" s="2" t="s">
-        <v>532</v>
+        <v>531</v>
       </c>
     </row>
     <row r="84" spans="1:8" ht="11" customHeight="1">
       <c r="A84" s="7"/>
       <c r="B84" t="s">
-        <v>458</v>
+        <v>457</v>
       </c>
       <c r="C84" t="s">
         <v>161</v>
       </c>
       <c r="D84" t="s">
+        <v>458</v>
+      </c>
+      <c r="E84" s="2" t="s">
         <v>459</v>
       </c>
-      <c r="E84" s="2" t="s">
+      <c r="F84" t="s">
         <v>460</v>
-      </c>
-      <c r="F84" t="s">
-        <v>461</v>
       </c>
     </row>
     <row r="85" spans="1:8" ht="11" customHeight="1">
       <c r="A85" s="7"/>
       <c r="B85" t="s">
-        <v>462</v>
+        <v>461</v>
       </c>
       <c r="C85" t="s">
         <v>172</v>
       </c>
       <c r="D85" t="s">
+        <v>462</v>
+      </c>
+      <c r="E85" s="2" t="s">
         <v>463</v>
       </c>
-      <c r="E85" s="2" t="s">
-        <v>464</v>
-      </c>
       <c r="F85" t="s">
-        <v>461</v>
+        <v>460</v>
       </c>
     </row>
     <row r="86" spans="1:8" ht="11" customHeight="1">
       <c r="A86" s="7"/>
       <c r="B86" t="s">
-        <v>465</v>
+        <v>464</v>
       </c>
       <c r="C86" t="s">
         <v>185</v>
       </c>
       <c r="D86" t="s">
+        <v>465</v>
+      </c>
+      <c r="E86" s="2" t="s">
         <v>466</v>
       </c>
-      <c r="E86" s="2" t="s">
-        <v>467</v>
-      </c>
       <c r="F86" t="s">
-        <v>461</v>
+        <v>460</v>
       </c>
     </row>
     <row r="87" spans="1:8" ht="11" customHeight="1">
       <c r="A87" s="7"/>
       <c r="B87" t="s">
-        <v>468</v>
+        <v>467</v>
       </c>
       <c r="C87" t="s">
         <v>196</v>
       </c>
       <c r="D87" t="s">
+        <v>468</v>
+      </c>
+      <c r="E87" s="2" t="s">
         <v>469</v>
       </c>
-      <c r="E87" s="2" t="s">
-        <v>470</v>
-      </c>
       <c r="F87" t="s">
-        <v>461</v>
+        <v>460</v>
       </c>
     </row>
     <row r="88" spans="1:8" ht="11" customHeight="1">
       <c r="A88" s="7"/>
       <c r="B88" t="s">
-        <v>471</v>
+        <v>470</v>
       </c>
       <c r="C88" t="s">
         <v>211</v>
       </c>
       <c r="D88" t="s">
+        <v>471</v>
+      </c>
+      <c r="E88" s="2" t="s">
         <v>472</v>
       </c>
-      <c r="E88" s="2" t="s">
-        <v>473</v>
-      </c>
       <c r="F88" t="s">
-        <v>461</v>
+        <v>460</v>
       </c>
     </row>
     <row r="89" spans="1:8" ht="11" customHeight="1">
       <c r="A89" s="7"/>
       <c r="B89" t="s">
-        <v>474</v>
+        <v>473</v>
       </c>
       <c r="C89" t="s">
         <v>224</v>
       </c>
       <c r="D89" t="s">
+        <v>474</v>
+      </c>
+      <c r="E89" s="2" t="s">
         <v>475</v>
       </c>
-      <c r="E89" s="2" t="s">
-        <v>476</v>
-      </c>
       <c r="F89" t="s">
-        <v>461</v>
+        <v>460</v>
       </c>
     </row>
     <row r="90" spans="1:8" ht="11" customHeight="1">
       <c r="A90" s="7"/>
       <c r="B90" t="s">
-        <v>477</v>
+        <v>476</v>
       </c>
       <c r="C90" t="s">
         <v>237</v>
       </c>
       <c r="D90" t="s">
+        <v>477</v>
+      </c>
+      <c r="E90" s="2" t="s">
         <v>478</v>
-      </c>
-      <c r="E90" s="2" t="s">
-        <v>479</v>
       </c>
     </row>
     <row r="91" spans="1:8" ht="11" customHeight="1">
       <c r="A91" s="7"/>
       <c r="B91" t="s">
-        <v>480</v>
+        <v>479</v>
       </c>
       <c r="C91" t="s">
         <v>252</v>
       </c>
       <c r="D91" t="s">
+        <v>480</v>
+      </c>
+      <c r="E91" s="2" t="s">
         <v>481</v>
-      </c>
-      <c r="E91" s="2" t="s">
-        <v>482</v>
       </c>
     </row>
     <row r="92" spans="1:8" ht="11" customHeight="1">
       <c r="A92" s="7"/>
       <c r="B92" t="s">
-        <v>483</v>
+        <v>482</v>
       </c>
       <c r="C92" t="s">
         <v>265</v>
       </c>
       <c r="D92" t="s">
+        <v>483</v>
+      </c>
+      <c r="E92" s="2" t="s">
         <v>484</v>
-      </c>
-      <c r="E92" s="2" t="s">
-        <v>485</v>
       </c>
     </row>
     <row r="93" spans="1:8" ht="11" customHeight="1">
       <c r="A93" s="7"/>
       <c r="B93" t="s">
-        <v>486</v>
+        <v>485</v>
       </c>
       <c r="C93" t="s">
         <v>280</v>
       </c>
       <c r="D93" t="s">
+        <v>486</v>
+      </c>
+      <c r="E93" s="2" t="s">
         <v>487</v>
-      </c>
-      <c r="E93" s="2" t="s">
-        <v>488</v>
       </c>
     </row>
     <row r="94" spans="1:8" ht="11" customHeight="1">
       <c r="A94" s="7"/>
       <c r="B94" t="s">
-        <v>489</v>
+        <v>488</v>
       </c>
       <c r="C94" t="s">
         <v>293</v>
       </c>
       <c r="D94" t="s">
+        <v>489</v>
+      </c>
+      <c r="E94" s="2" t="s">
         <v>490</v>
-      </c>
-      <c r="E94" s="2" t="s">
-        <v>491</v>
       </c>
     </row>
     <row r="95" spans="1:8" ht="12" customHeight="1">
       <c r="A95" s="7"/>
       <c r="B95" t="s">
-        <v>492</v>
+        <v>491</v>
       </c>
       <c r="C95" t="s">
         <v>308</v>
       </c>
       <c r="D95" t="s">
+        <v>492</v>
+      </c>
+      <c r="E95" s="2" t="s">
         <v>493</v>
-      </c>
-      <c r="E95" s="2" t="s">
-        <v>494</v>
       </c>
     </row>
     <row r="96" spans="1:8" ht="12.75" customHeight="1">
@@ -4536,7 +4531,7 @@
         <v>14</v>
       </c>
       <c r="E102" t="s">
-        <v>530</v>
+        <v>529</v>
       </c>
     </row>
     <row r="103" spans="1:9" ht="24">
@@ -4651,7 +4646,7 @@
         <v>14</v>
       </c>
       <c r="E114" t="s">
-        <v>531</v>
+        <v>530</v>
       </c>
     </row>
     <row r="115" spans="1:10" ht="12.75" customHeight="1">
@@ -4741,7 +4736,7 @@
     <row r="123" spans="1:10" ht="20" customHeight="1">
       <c r="A123" s="7"/>
       <c r="B123" s="8" t="s">
-        <v>525</v>
+        <v>524</v>
       </c>
       <c r="C123" s="13"/>
       <c r="D123" s="13"/>
@@ -4786,7 +4781,7 @@
     </row>
     <row r="128" spans="1:10" ht="15">
       <c r="A128" s="7" t="s">
-        <v>503</v>
+        <v>502</v>
       </c>
       <c r="B128" s="8" t="s">
         <v>75</v>
@@ -5059,7 +5054,7 @@
     </row>
     <row r="156" spans="1:9" ht="15">
       <c r="A156" s="7" t="s">
-        <v>504</v>
+        <v>503</v>
       </c>
       <c r="B156" s="8" t="s">
         <v>54</v>
@@ -5623,7 +5618,7 @@
         <v>157</v>
       </c>
       <c r="C18" t="s">
-        <v>535</v>
+        <v>534</v>
       </c>
     </row>
     <row r="19" spans="1:4" ht="12.75" customHeight="1">
@@ -5793,40 +5788,40 @@
     </row>
     <row r="39" spans="1:4" ht="12.75" customHeight="1">
       <c r="A39" t="s">
+        <v>512</v>
+      </c>
+      <c r="B39" t="s">
         <v>513</v>
       </c>
-      <c r="B39" t="s">
-        <v>514</v>
-      </c>
       <c r="C39" t="s">
-        <v>516</v>
+        <v>515</v>
       </c>
     </row>
     <row r="40" spans="1:4" ht="12.75" customHeight="1">
       <c r="A40" t="s">
-        <v>513</v>
+        <v>512</v>
       </c>
       <c r="B40" t="s">
-        <v>515</v>
+        <v>514</v>
       </c>
       <c r="C40" t="s">
-        <v>517</v>
+        <v>516</v>
       </c>
     </row>
     <row r="42" spans="1:4" ht="12.75" customHeight="1">
       <c r="A42" t="s">
-        <v>528</v>
+        <v>527</v>
       </c>
       <c r="B42" t="s">
         <v>158</v>
       </c>
       <c r="C42" t="s">
-        <v>529</v>
+        <v>528</v>
       </c>
     </row>
     <row r="43" spans="1:4" ht="12.75" customHeight="1">
       <c r="A43" t="s">
-        <v>528</v>
+        <v>527</v>
       </c>
       <c r="B43" t="s">
         <v>91</v>
@@ -5837,7 +5832,7 @@
     </row>
     <row r="44" spans="1:4" ht="12.75" customHeight="1">
       <c r="A44" t="s">
-        <v>528</v>
+        <v>527</v>
       </c>
       <c r="B44" t="s">
         <v>97</v>

</xml_diff>

<commit_message>
update powerpoint with new layout
</commit_message>
<xml_diff>
--- a/opendatakit.collect2/form-files/neonatal/neonatal.xlsx
+++ b/opendatakit.collect2/form-files/neonatal/neonatal.xlsx
@@ -4,7 +4,7 @@
   <fileVersion appName="xl" lastEdited="5" lowestEdited="5" rupBuild="22905"/>
   <workbookPr autoCompressPictures="0"/>
   <bookViews>
-    <workbookView xWindow="1800" yWindow="0" windowWidth="18360" windowHeight="15280" tabRatio="500"/>
+    <workbookView xWindow="1800" yWindow="0" windowWidth="18360" windowHeight="15280" tabRatio="500" activeTab="1"/>
   </bookViews>
   <sheets>
     <sheet name="survey" sheetId="1" r:id="rId1"/>
@@ -23,7 +23,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="869" uniqueCount="535">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="869" uniqueCount="534">
   <si>
     <t>type</t>
   </si>
@@ -487,13 +487,7 @@
     <t>head</t>
   </si>
   <si>
-    <t>img/diagnostic_icons/sagittal.jpg</t>
-  </si>
-  <si>
     <t>placement</t>
-  </si>
-  <si>
-    <t>img/diagnostic_icons/line.jpg</t>
   </si>
   <si>
     <t>xray</t>
@@ -1835,6 +1829,9 @@
   </si>
   <si>
     <t>Chest and Abdominal XRAY</t>
+  </si>
+  <si>
+    <t>Head Sagital</t>
   </si>
 </sst>
 </file>
@@ -3283,7 +3280,7 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:J194"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
+    <sheetView workbookViewId="0">
       <pane ySplit="1" topLeftCell="A21" activePane="bottomLeft" state="frozen"/>
       <selection pane="bottomLeft" activeCell="D34" sqref="D34"/>
     </sheetView>
@@ -3354,12 +3351,12 @@
     <row r="4" spans="1:10" s="35" customFormat="1" ht="15">
       <c r="A4" s="12"/>
       <c r="B4" s="33" t="s">
-        <v>373</v>
+        <v>371</v>
       </c>
       <c r="C4" s="33"/>
       <c r="D4" s="33"/>
       <c r="E4" s="33" t="s">
-        <v>374</v>
+        <v>372</v>
       </c>
       <c r="F4" s="33"/>
       <c r="G4" s="33"/>
@@ -3370,12 +3367,12 @@
     <row r="5" spans="1:10" ht="12">
       <c r="A5" s="12"/>
       <c r="B5" s="22" t="s">
-        <v>375</v>
+        <v>373</v>
       </c>
       <c r="C5" s="22"/>
       <c r="D5" s="22"/>
       <c r="E5" s="23" t="s">
-        <v>376</v>
+        <v>374</v>
       </c>
       <c r="F5" s="22"/>
       <c r="G5" s="22"/>
@@ -3383,10 +3380,10 @@
     </row>
     <row r="6" spans="1:10" ht="15">
       <c r="A6" s="7" t="s">
-        <v>500</v>
+        <v>498</v>
       </c>
       <c r="B6" s="8" t="s">
-        <v>377</v>
+        <v>375</v>
       </c>
       <c r="C6" s="8"/>
       <c r="D6" s="8"/>
@@ -3398,13 +3395,13 @@
     <row r="7" spans="1:10" ht="12">
       <c r="A7" s="7"/>
       <c r="B7" s="3" t="s">
-        <v>378</v>
+        <v>376</v>
       </c>
       <c r="C7" s="3" t="s">
         <v>147</v>
       </c>
       <c r="D7" s="3" t="s">
-        <v>379</v>
+        <v>377</v>
       </c>
       <c r="E7" s="3"/>
       <c r="F7" s="3" t="s">
@@ -3421,7 +3418,7 @@
       <c r="C8" s="25"/>
       <c r="D8" s="25"/>
       <c r="E8" s="4" t="s">
-        <v>380</v>
+        <v>378</v>
       </c>
       <c r="F8" s="25"/>
       <c r="G8" s="12"/>
@@ -3439,7 +3436,7 @@
       <c r="G9" s="12"/>
       <c r="H9" s="12"/>
       <c r="I9" t="s">
-        <v>381</v>
+        <v>379</v>
       </c>
     </row>
     <row r="10" spans="1:10" ht="12.75" customHeight="1">
@@ -3448,7 +3445,7 @@
         <v>4</v>
       </c>
       <c r="D10" t="s">
-        <v>418</v>
+        <v>416</v>
       </c>
       <c r="E10" s="14"/>
     </row>
@@ -3458,7 +3455,7 @@
         <v>4</v>
       </c>
       <c r="H11" t="s">
-        <v>382</v>
+        <v>380</v>
       </c>
     </row>
     <row r="12" spans="1:10" ht="12">
@@ -3468,7 +3465,7 @@
       </c>
       <c r="C12" s="3"/>
       <c r="D12" s="27" t="s">
-        <v>419</v>
+        <v>417</v>
       </c>
       <c r="E12" s="3"/>
       <c r="F12" s="3"/>
@@ -3482,7 +3479,7 @@
       </c>
       <c r="C13" s="9"/>
       <c r="D13" s="29" t="s">
-        <v>420</v>
+        <v>418</v>
       </c>
       <c r="E13" s="29"/>
       <c r="F13" s="9"/>
@@ -3507,7 +3504,7 @@
       <c r="C15" s="25"/>
       <c r="D15" s="25"/>
       <c r="E15" s="4" t="s">
-        <v>386</v>
+        <v>384</v>
       </c>
     </row>
     <row r="16" spans="1:10" s="12" customFormat="1" ht="12">
@@ -3516,7 +3513,7 @@
         <v>4</v>
       </c>
       <c r="D16" s="12" t="s">
-        <v>417</v>
+        <v>415</v>
       </c>
     </row>
     <row r="17" spans="1:10" s="12" customFormat="1" ht="12">
@@ -3533,7 +3530,7 @@
       <c r="C18" s="25"/>
       <c r="D18" s="25"/>
       <c r="E18" s="4" t="s">
-        <v>397</v>
+        <v>395</v>
       </c>
     </row>
     <row r="19" spans="1:10" s="12" customFormat="1" ht="13" customHeight="1">
@@ -3543,7 +3540,7 @@
       </c>
       <c r="D19"/>
       <c r="I19" s="12" t="s">
-        <v>532</v>
+        <v>530</v>
       </c>
     </row>
     <row r="20" spans="1:10" s="12" customFormat="1" ht="12">
@@ -3555,7 +3552,7 @@
     <row r="21" spans="1:10" ht="15">
       <c r="A21" s="16"/>
       <c r="B21" s="8" t="s">
-        <v>383</v>
+        <v>381</v>
       </c>
       <c r="C21" s="30"/>
       <c r="D21" s="31"/>
@@ -3565,22 +3562,22 @@
     <row r="23" spans="1:10" s="15" customFormat="1" ht="12.75" customHeight="1">
       <c r="A23" s="37"/>
       <c r="B23" s="14" t="s">
-        <v>431</v>
+        <v>429</v>
       </c>
       <c r="E23" s="15" t="s">
-        <v>436</v>
+        <v>434</v>
       </c>
       <c r="I23" s="3"/>
       <c r="J23" s="3"/>
     </row>
     <row r="24" spans="1:10" ht="15">
       <c r="B24" s="14" t="s">
-        <v>432</v>
+        <v>430</v>
       </c>
       <c r="C24" s="15"/>
       <c r="D24" s="15"/>
       <c r="E24" s="15" t="s">
-        <v>435</v>
+        <v>433</v>
       </c>
       <c r="F24" s="15"/>
       <c r="G24" s="15"/>
@@ -3588,10 +3585,10 @@
     </row>
     <row r="25" spans="1:10" ht="15">
       <c r="A25" s="7" t="s">
-        <v>501</v>
+        <v>499</v>
       </c>
       <c r="B25" s="8" t="s">
-        <v>433</v>
+        <v>431</v>
       </c>
       <c r="C25" s="13"/>
       <c r="D25" s="13"/>
@@ -3603,13 +3600,13 @@
     <row r="26" spans="1:10" ht="12">
       <c r="A26" s="12"/>
       <c r="B26" s="3" t="s">
-        <v>437</v>
+        <v>435</v>
       </c>
       <c r="C26" s="3" t="s">
-        <v>438</v>
+        <v>436</v>
       </c>
       <c r="D26" s="3" t="s">
-        <v>393</v>
+        <v>391</v>
       </c>
       <c r="E26" s="3"/>
       <c r="F26" s="3" t="s">
@@ -3620,15 +3617,15 @@
     </row>
     <row r="27" spans="1:10" ht="12.75" customHeight="1">
       <c r="A27" s="7" t="s">
-        <v>441</v>
+        <v>439</v>
       </c>
       <c r="B27" s="40" t="s">
-        <v>444</v>
+        <v>442</v>
       </c>
       <c r="C27" s="40"/>
       <c r="D27" s="40"/>
       <c r="E27" s="40" t="s">
-        <v>495</v>
+        <v>493</v>
       </c>
       <c r="F27" s="40"/>
       <c r="G27" s="40"/>
@@ -3637,12 +3634,12 @@
     <row r="28" spans="1:10" ht="12.75" customHeight="1">
       <c r="A28" s="7"/>
       <c r="B28" s="40" t="s">
-        <v>445</v>
+        <v>443</v>
       </c>
       <c r="C28" s="40"/>
       <c r="D28" s="40"/>
       <c r="E28" s="40" t="s">
-        <v>496</v>
+        <v>494</v>
       </c>
       <c r="F28" s="40"/>
       <c r="G28" s="40"/>
@@ -3651,7 +3648,7 @@
     <row r="29" spans="1:10" s="3" customFormat="1" ht="18" customHeight="1">
       <c r="A29" s="41"/>
       <c r="B29" s="13" t="s">
-        <v>446</v>
+        <v>444</v>
       </c>
       <c r="C29" s="13"/>
       <c r="D29" s="13"/>
@@ -3663,13 +3660,13 @@
     <row r="30" spans="1:10" s="3" customFormat="1" ht="18" customHeight="1">
       <c r="A30" s="41"/>
       <c r="B30" t="s">
-        <v>447</v>
+        <v>445</v>
       </c>
       <c r="C30" t="s">
         <v>152</v>
       </c>
       <c r="D30" t="s">
-        <v>441</v>
+        <v>439</v>
       </c>
       <c r="E30"/>
       <c r="F30" t="s">
@@ -3679,20 +3676,20 @@
     <row r="31" spans="1:10" ht="24">
       <c r="A31" s="7"/>
       <c r="B31" s="2" t="s">
-        <v>448</v>
+        <v>446</v>
       </c>
       <c r="C31" s="2" t="s">
-        <v>326</v>
+        <v>324</v>
       </c>
       <c r="D31" s="2" t="s">
-        <v>160</v>
+        <v>158</v>
       </c>
       <c r="E31" s="2" t="s">
-        <v>449</v>
+        <v>447</v>
       </c>
       <c r="F31" s="2"/>
       <c r="G31" t="s">
-        <v>450</v>
+        <v>448</v>
       </c>
     </row>
     <row r="32" spans="1:10" ht="18" customHeight="1">
@@ -3703,46 +3700,46 @@
       <c r="C32" s="2"/>
       <c r="D32" s="2"/>
       <c r="E32" s="2" t="s">
-        <v>451</v>
+        <v>449</v>
       </c>
       <c r="F32" s="2"/>
       <c r="I32" t="s">
-        <v>497</v>
+        <v>495</v>
       </c>
     </row>
     <row r="33" spans="1:9" ht="18" customHeight="1">
       <c r="A33" s="7"/>
       <c r="B33" s="2" t="s">
-        <v>452</v>
+        <v>450</v>
       </c>
       <c r="C33" s="19"/>
       <c r="D33" s="2" t="s">
-        <v>453</v>
+        <v>451</v>
       </c>
       <c r="E33" s="2" t="s">
-        <v>454</v>
+        <v>452</v>
       </c>
       <c r="F33" s="2"/>
     </row>
     <row r="34" spans="1:9" ht="18" customHeight="1">
       <c r="A34" s="7"/>
       <c r="B34" s="2" t="s">
-        <v>452</v>
+        <v>450</v>
       </c>
       <c r="C34" s="19"/>
       <c r="D34" s="2"/>
       <c r="E34" s="2" t="s">
-        <v>455</v>
+        <v>453</v>
       </c>
       <c r="F34" s="2"/>
       <c r="I34" t="s">
-        <v>533</v>
+        <v>531</v>
       </c>
     </row>
     <row r="35" spans="1:9" ht="15">
       <c r="A35" s="7"/>
       <c r="B35" s="8" t="s">
-        <v>494</v>
+        <v>492</v>
       </c>
       <c r="C35" s="8"/>
       <c r="D35" s="8"/>
@@ -3767,7 +3764,7 @@
       <c r="C37" s="15"/>
       <c r="D37" s="15"/>
       <c r="E37" s="15" t="s">
-        <v>498</v>
+        <v>496</v>
       </c>
       <c r="F37" s="15"/>
       <c r="G37" s="15"/>
@@ -3780,7 +3777,7 @@
       <c r="C38" s="15"/>
       <c r="D38" s="15"/>
       <c r="E38" s="15" t="s">
-        <v>499</v>
+        <v>497</v>
       </c>
       <c r="F38" s="15"/>
       <c r="G38" s="15"/>
@@ -3866,7 +3863,7 @@
         <v>24</v>
       </c>
       <c r="D45" t="s">
-        <v>421</v>
+        <v>419</v>
       </c>
     </row>
     <row r="46" spans="1:9" ht="12.75" customHeight="1">
@@ -3875,7 +3872,7 @@
         <v>4</v>
       </c>
       <c r="D46" t="s">
-        <v>410</v>
+        <v>408</v>
       </c>
       <c r="E46" t="s">
         <v>25</v>
@@ -3906,7 +3903,7 @@
         <v>27</v>
       </c>
       <c r="D49" t="s">
-        <v>422</v>
+        <v>420</v>
       </c>
     </row>
     <row r="50" spans="1:5" ht="12.75" customHeight="1">
@@ -3915,7 +3912,7 @@
         <v>4</v>
       </c>
       <c r="D50" t="s">
-        <v>411</v>
+        <v>409</v>
       </c>
       <c r="E50" t="s">
         <v>32</v>
@@ -3960,7 +3957,7 @@
         <v>63</v>
       </c>
       <c r="D55" t="s">
-        <v>423</v>
+        <v>421</v>
       </c>
     </row>
     <row r="56" spans="1:5" ht="12.75" customHeight="1">
@@ -3972,7 +3969,7 @@
         <v>64</v>
       </c>
       <c r="D56" t="s">
-        <v>424</v>
+        <v>422</v>
       </c>
     </row>
     <row r="57" spans="1:5" ht="12.75" customHeight="1">
@@ -3981,7 +3978,7 @@
         <v>4</v>
       </c>
       <c r="D57" t="s">
-        <v>412</v>
+        <v>410</v>
       </c>
       <c r="E57" t="s">
         <v>65</v>
@@ -4020,7 +4017,7 @@
         <v>68</v>
       </c>
       <c r="D61" t="s">
-        <v>425</v>
+        <v>423</v>
       </c>
     </row>
     <row r="62" spans="1:5" ht="12.75" customHeight="1">
@@ -4032,7 +4029,7 @@
         <v>69</v>
       </c>
       <c r="D62" t="s">
-        <v>426</v>
+        <v>424</v>
       </c>
     </row>
     <row r="63" spans="1:5" ht="12.75" customHeight="1">
@@ -4041,7 +4038,7 @@
         <v>4</v>
       </c>
       <c r="D63" t="s">
-        <v>413</v>
+        <v>411</v>
       </c>
       <c r="E63" t="s">
         <v>70</v>
@@ -4076,12 +4073,12 @@
     </row>
     <row r="67" spans="1:8" ht="12.75" customHeight="1">
       <c r="B67" s="14" t="s">
-        <v>504</v>
+        <v>502</v>
       </c>
       <c r="C67" s="15"/>
       <c r="D67" s="15"/>
       <c r="E67" s="15" t="s">
-        <v>508</v>
+        <v>506</v>
       </c>
       <c r="F67" s="15"/>
       <c r="G67" s="15"/>
@@ -4089,12 +4086,12 @@
     </row>
     <row r="68" spans="1:8" ht="12.75" customHeight="1">
       <c r="B68" s="14" t="s">
-        <v>505</v>
+        <v>503</v>
       </c>
       <c r="C68" s="15"/>
       <c r="D68" s="15"/>
       <c r="E68" s="15" t="s">
-        <v>509</v>
+        <v>507</v>
       </c>
       <c r="F68" s="15"/>
       <c r="G68" s="15"/>
@@ -4102,10 +4099,10 @@
     </row>
     <row r="69" spans="1:8" ht="12.75" customHeight="1">
       <c r="A69" s="7" t="s">
-        <v>510</v>
+        <v>508</v>
       </c>
       <c r="B69" s="8" t="s">
-        <v>506</v>
+        <v>504</v>
       </c>
       <c r="C69" s="13"/>
       <c r="D69" s="13"/>
@@ -4117,13 +4114,13 @@
     <row r="70" spans="1:8" ht="12.75" customHeight="1">
       <c r="A70" s="16"/>
       <c r="B70" t="s">
-        <v>511</v>
+        <v>509</v>
       </c>
       <c r="C70" t="s">
-        <v>512</v>
+        <v>510</v>
       </c>
       <c r="D70" t="s">
-        <v>510</v>
+        <v>508</v>
       </c>
       <c r="E70" s="42"/>
       <c r="F70" t="s">
@@ -4140,7 +4137,7 @@
       <c r="C71" s="32"/>
       <c r="D71" s="32"/>
       <c r="E71" t="s">
-        <v>518</v>
+        <v>516</v>
       </c>
       <c r="F71" s="32"/>
       <c r="G71" s="32"/>
@@ -4153,7 +4150,7 @@
       </c>
       <c r="C72" s="32"/>
       <c r="D72" s="43" t="s">
-        <v>515</v>
+        <v>513</v>
       </c>
       <c r="E72" s="32"/>
       <c r="F72" s="32"/>
@@ -4174,7 +4171,7 @@
       <c r="C74" s="32"/>
       <c r="D74" s="32"/>
       <c r="E74" t="s">
-        <v>517</v>
+        <v>515</v>
       </c>
       <c r="F74" s="32"/>
       <c r="G74" s="32"/>
@@ -4187,7 +4184,7 @@
       </c>
       <c r="C75" s="32"/>
       <c r="D75" s="43" t="s">
-        <v>516</v>
+        <v>514</v>
       </c>
       <c r="E75" s="32"/>
       <c r="F75" s="32"/>
@@ -4203,7 +4200,7 @@
     <row r="77" spans="1:8" ht="12.75" customHeight="1">
       <c r="A77" s="7"/>
       <c r="B77" s="8" t="s">
-        <v>507</v>
+        <v>505</v>
       </c>
       <c r="C77" s="13"/>
       <c r="D77" s="13"/>
@@ -4223,12 +4220,12 @@
     </row>
     <row r="79" spans="1:8" ht="12.75" customHeight="1">
       <c r="B79" s="14" t="s">
-        <v>520</v>
+        <v>518</v>
       </c>
       <c r="C79" s="15"/>
       <c r="D79" s="15"/>
       <c r="E79" s="15" t="s">
-        <v>525</v>
+        <v>523</v>
       </c>
       <c r="F79" s="15"/>
       <c r="G79" s="15"/>
@@ -4236,12 +4233,12 @@
     </row>
     <row r="80" spans="1:8" ht="12.75" customHeight="1">
       <c r="B80" s="14" t="s">
-        <v>521</v>
+        <v>519</v>
       </c>
       <c r="C80" s="15"/>
       <c r="D80" s="15"/>
       <c r="E80" s="15" t="s">
-        <v>526</v>
+        <v>524</v>
       </c>
       <c r="F80" s="15"/>
       <c r="G80" s="15"/>
@@ -4249,10 +4246,10 @@
     </row>
     <row r="81" spans="1:8" ht="12.75" customHeight="1">
       <c r="A81" s="7" t="s">
-        <v>519</v>
+        <v>517</v>
       </c>
       <c r="B81" s="8" t="s">
-        <v>522</v>
+        <v>520</v>
       </c>
       <c r="C81" s="13"/>
       <c r="D81" s="13"/>
@@ -4264,13 +4261,13 @@
     <row r="82" spans="1:8" ht="12.75" customHeight="1">
       <c r="A82" s="16"/>
       <c r="B82" t="s">
-        <v>523</v>
+        <v>521</v>
       </c>
       <c r="C82" t="s">
-        <v>527</v>
+        <v>525</v>
       </c>
       <c r="D82" t="s">
-        <v>443</v>
+        <v>441</v>
       </c>
       <c r="E82" s="42"/>
       <c r="F82" t="s">
@@ -4282,211 +4279,211 @@
     <row r="83" spans="1:8" ht="12">
       <c r="A83" s="7"/>
       <c r="B83" s="45" t="s">
-        <v>392</v>
+        <v>390</v>
       </c>
       <c r="C83" s="45" t="s">
-        <v>456</v>
+        <v>454</v>
       </c>
       <c r="E83" s="2" t="s">
-        <v>531</v>
+        <v>529</v>
       </c>
     </row>
     <row r="84" spans="1:8" ht="11" customHeight="1">
       <c r="A84" s="7"/>
       <c r="B84" t="s">
+        <v>455</v>
+      </c>
+      <c r="C84" t="s">
+        <v>159</v>
+      </c>
+      <c r="D84" t="s">
+        <v>456</v>
+      </c>
+      <c r="E84" s="2" t="s">
         <v>457</v>
       </c>
-      <c r="C84" t="s">
-        <v>161</v>
-      </c>
-      <c r="D84" t="s">
+      <c r="F84" t="s">
         <v>458</v>
-      </c>
-      <c r="E84" s="2" t="s">
-        <v>459</v>
-      </c>
-      <c r="F84" t="s">
-        <v>460</v>
       </c>
     </row>
     <row r="85" spans="1:8" ht="11" customHeight="1">
       <c r="A85" s="7"/>
       <c r="B85" t="s">
+        <v>459</v>
+      </c>
+      <c r="C85" t="s">
+        <v>170</v>
+      </c>
+      <c r="D85" t="s">
+        <v>460</v>
+      </c>
+      <c r="E85" s="2" t="s">
         <v>461</v>
       </c>
-      <c r="C85" t="s">
-        <v>172</v>
-      </c>
-      <c r="D85" t="s">
-        <v>462</v>
-      </c>
-      <c r="E85" s="2" t="s">
-        <v>463</v>
-      </c>
       <c r="F85" t="s">
-        <v>460</v>
+        <v>458</v>
       </c>
     </row>
     <row r="86" spans="1:8" ht="11" customHeight="1">
       <c r="A86" s="7"/>
       <c r="B86" t="s">
+        <v>462</v>
+      </c>
+      <c r="C86" t="s">
+        <v>183</v>
+      </c>
+      <c r="D86" t="s">
+        <v>463</v>
+      </c>
+      <c r="E86" s="2" t="s">
         <v>464</v>
       </c>
-      <c r="C86" t="s">
-        <v>185</v>
-      </c>
-      <c r="D86" t="s">
-        <v>465</v>
-      </c>
-      <c r="E86" s="2" t="s">
-        <v>466</v>
-      </c>
       <c r="F86" t="s">
-        <v>460</v>
+        <v>458</v>
       </c>
     </row>
     <row r="87" spans="1:8" ht="11" customHeight="1">
       <c r="A87" s="7"/>
       <c r="B87" t="s">
+        <v>465</v>
+      </c>
+      <c r="C87" t="s">
+        <v>194</v>
+      </c>
+      <c r="D87" t="s">
+        <v>466</v>
+      </c>
+      <c r="E87" s="2" t="s">
         <v>467</v>
       </c>
-      <c r="C87" t="s">
-        <v>196</v>
-      </c>
-      <c r="D87" t="s">
-        <v>468</v>
-      </c>
-      <c r="E87" s="2" t="s">
-        <v>469</v>
-      </c>
       <c r="F87" t="s">
-        <v>460</v>
+        <v>458</v>
       </c>
     </row>
     <row r="88" spans="1:8" ht="11" customHeight="1">
       <c r="A88" s="7"/>
       <c r="B88" t="s">
+        <v>468</v>
+      </c>
+      <c r="C88" t="s">
+        <v>209</v>
+      </c>
+      <c r="D88" t="s">
+        <v>469</v>
+      </c>
+      <c r="E88" s="2" t="s">
         <v>470</v>
       </c>
-      <c r="C88" t="s">
-        <v>211</v>
-      </c>
-      <c r="D88" t="s">
-        <v>471</v>
-      </c>
-      <c r="E88" s="2" t="s">
-        <v>472</v>
-      </c>
       <c r="F88" t="s">
-        <v>460</v>
+        <v>458</v>
       </c>
     </row>
     <row r="89" spans="1:8" ht="11" customHeight="1">
       <c r="A89" s="7"/>
       <c r="B89" t="s">
+        <v>471</v>
+      </c>
+      <c r="C89" t="s">
+        <v>222</v>
+      </c>
+      <c r="D89" t="s">
+        <v>472</v>
+      </c>
+      <c r="E89" s="2" t="s">
         <v>473</v>
       </c>
-      <c r="C89" t="s">
-        <v>224</v>
-      </c>
-      <c r="D89" t="s">
-        <v>474</v>
-      </c>
-      <c r="E89" s="2" t="s">
-        <v>475</v>
-      </c>
       <c r="F89" t="s">
-        <v>460</v>
+        <v>458</v>
       </c>
     </row>
     <row r="90" spans="1:8" ht="11" customHeight="1">
       <c r="A90" s="7"/>
       <c r="B90" t="s">
+        <v>474</v>
+      </c>
+      <c r="C90" t="s">
+        <v>235</v>
+      </c>
+      <c r="D90" t="s">
+        <v>475</v>
+      </c>
+      <c r="E90" s="2" t="s">
         <v>476</v>
-      </c>
-      <c r="C90" t="s">
-        <v>237</v>
-      </c>
-      <c r="D90" t="s">
-        <v>477</v>
-      </c>
-      <c r="E90" s="2" t="s">
-        <v>478</v>
       </c>
     </row>
     <row r="91" spans="1:8" ht="11" customHeight="1">
       <c r="A91" s="7"/>
       <c r="B91" t="s">
+        <v>477</v>
+      </c>
+      <c r="C91" t="s">
+        <v>250</v>
+      </c>
+      <c r="D91" t="s">
+        <v>478</v>
+      </c>
+      <c r="E91" s="2" t="s">
         <v>479</v>
-      </c>
-      <c r="C91" t="s">
-        <v>252</v>
-      </c>
-      <c r="D91" t="s">
-        <v>480</v>
-      </c>
-      <c r="E91" s="2" t="s">
-        <v>481</v>
       </c>
     </row>
     <row r="92" spans="1:8" ht="11" customHeight="1">
       <c r="A92" s="7"/>
       <c r="B92" t="s">
+        <v>480</v>
+      </c>
+      <c r="C92" t="s">
+        <v>263</v>
+      </c>
+      <c r="D92" t="s">
+        <v>481</v>
+      </c>
+      <c r="E92" s="2" t="s">
         <v>482</v>
-      </c>
-      <c r="C92" t="s">
-        <v>265</v>
-      </c>
-      <c r="D92" t="s">
-        <v>483</v>
-      </c>
-      <c r="E92" s="2" t="s">
-        <v>484</v>
       </c>
     </row>
     <row r="93" spans="1:8" ht="11" customHeight="1">
       <c r="A93" s="7"/>
       <c r="B93" t="s">
+        <v>483</v>
+      </c>
+      <c r="C93" t="s">
+        <v>278</v>
+      </c>
+      <c r="D93" t="s">
+        <v>484</v>
+      </c>
+      <c r="E93" s="2" t="s">
         <v>485</v>
-      </c>
-      <c r="C93" t="s">
-        <v>280</v>
-      </c>
-      <c r="D93" t="s">
-        <v>486</v>
-      </c>
-      <c r="E93" s="2" t="s">
-        <v>487</v>
       </c>
     </row>
     <row r="94" spans="1:8" ht="11" customHeight="1">
       <c r="A94" s="7"/>
       <c r="B94" t="s">
+        <v>486</v>
+      </c>
+      <c r="C94" t="s">
+        <v>291</v>
+      </c>
+      <c r="D94" t="s">
+        <v>487</v>
+      </c>
+      <c r="E94" s="2" t="s">
         <v>488</v>
-      </c>
-      <c r="C94" t="s">
-        <v>293</v>
-      </c>
-      <c r="D94" t="s">
-        <v>489</v>
-      </c>
-      <c r="E94" s="2" t="s">
-        <v>490</v>
       </c>
     </row>
     <row r="95" spans="1:8" ht="12" customHeight="1">
       <c r="A95" s="7"/>
       <c r="B95" t="s">
+        <v>489</v>
+      </c>
+      <c r="C95" t="s">
+        <v>306</v>
+      </c>
+      <c r="D95" t="s">
+        <v>490</v>
+      </c>
+      <c r="E95" s="2" t="s">
         <v>491</v>
-      </c>
-      <c r="C95" t="s">
-        <v>308</v>
-      </c>
-      <c r="D95" t="s">
-        <v>492</v>
-      </c>
-      <c r="E95" s="2" t="s">
-        <v>493</v>
       </c>
     </row>
     <row r="96" spans="1:8" ht="12.75" customHeight="1">
@@ -4531,7 +4528,7 @@
         <v>14</v>
       </c>
       <c r="E102" t="s">
-        <v>529</v>
+        <v>527</v>
       </c>
     </row>
     <row r="103" spans="1:9" ht="24">
@@ -4573,7 +4570,7 @@
         <v>24</v>
       </c>
       <c r="D106" t="s">
-        <v>421</v>
+        <v>419</v>
       </c>
     </row>
     <row r="107" spans="1:9" ht="12.75" customHeight="1">
@@ -4582,7 +4579,7 @@
         <v>4</v>
       </c>
       <c r="D107" t="s">
-        <v>410</v>
+        <v>408</v>
       </c>
       <c r="E107" t="s">
         <v>25</v>
@@ -4613,7 +4610,7 @@
         <v>27</v>
       </c>
       <c r="D110" t="s">
-        <v>422</v>
+        <v>420</v>
       </c>
     </row>
     <row r="111" spans="1:9" ht="12.75" customHeight="1">
@@ -4622,7 +4619,7 @@
         <v>4</v>
       </c>
       <c r="D111" t="s">
-        <v>411</v>
+        <v>409</v>
       </c>
       <c r="E111" t="s">
         <v>32</v>
@@ -4646,7 +4643,7 @@
         <v>14</v>
       </c>
       <c r="E114" t="s">
-        <v>530</v>
+        <v>528</v>
       </c>
     </row>
     <row r="115" spans="1:10" ht="12.75" customHeight="1">
@@ -4667,7 +4664,7 @@
         <v>48</v>
       </c>
       <c r="D116" t="s">
-        <v>427</v>
+        <v>425</v>
       </c>
     </row>
     <row r="117" spans="1:10" ht="12.75" customHeight="1">
@@ -4676,7 +4673,7 @@
         <v>4</v>
       </c>
       <c r="D117" t="s">
-        <v>428</v>
+        <v>426</v>
       </c>
     </row>
     <row r="118" spans="1:10" ht="12.75" customHeight="1">
@@ -4688,7 +4685,7 @@
         <v>43</v>
       </c>
       <c r="D118" t="s">
-        <v>429</v>
+        <v>427</v>
       </c>
     </row>
     <row r="119" spans="1:10" ht="12.75" customHeight="1">
@@ -4700,7 +4697,7 @@
         <v>44</v>
       </c>
       <c r="D119" t="s">
-        <v>430</v>
+        <v>428</v>
       </c>
     </row>
     <row r="120" spans="1:10" ht="12.75" customHeight="1">
@@ -4709,7 +4706,7 @@
         <v>4</v>
       </c>
       <c r="D120" t="s">
-        <v>414</v>
+        <v>412</v>
       </c>
       <c r="E120" t="s">
         <v>73</v>
@@ -4721,7 +4718,7 @@
         <v>4</v>
       </c>
       <c r="D121" t="s">
-        <v>415</v>
+        <v>413</v>
       </c>
       <c r="E121" t="s">
         <v>45</v>
@@ -4736,7 +4733,7 @@
     <row r="123" spans="1:10" ht="20" customHeight="1">
       <c r="A123" s="7"/>
       <c r="B123" s="8" t="s">
-        <v>524</v>
+        <v>522</v>
       </c>
       <c r="C123" s="13"/>
       <c r="D123" s="13"/>
@@ -4748,7 +4745,7 @@
     <row r="124" spans="1:10" ht="15">
       <c r="A124" s="16"/>
       <c r="B124" s="8" t="s">
-        <v>434</v>
+        <v>432</v>
       </c>
       <c r="C124" s="30"/>
       <c r="D124" s="31"/>
@@ -4758,22 +4755,22 @@
     <row r="126" spans="1:10" s="15" customFormat="1" ht="12.75" customHeight="1">
       <c r="A126" s="37"/>
       <c r="B126" s="14" t="s">
-        <v>398</v>
+        <v>396</v>
       </c>
       <c r="E126" s="15" t="s">
-        <v>399</v>
+        <v>397</v>
       </c>
       <c r="I126" s="3"/>
       <c r="J126" s="3"/>
     </row>
     <row r="127" spans="1:10" ht="12.75" customHeight="1">
       <c r="B127" s="14" t="s">
-        <v>400</v>
+        <v>398</v>
       </c>
       <c r="C127" s="15"/>
       <c r="D127" s="15"/>
       <c r="E127" s="15" t="s">
-        <v>401</v>
+        <v>399</v>
       </c>
       <c r="F127" s="15"/>
       <c r="G127" s="15"/>
@@ -4781,7 +4778,7 @@
     </row>
     <row r="128" spans="1:10" ht="15">
       <c r="A128" s="7" t="s">
-        <v>502</v>
+        <v>500</v>
       </c>
       <c r="B128" s="8" t="s">
         <v>75</v>
@@ -4848,7 +4845,7 @@
         <v>116</v>
       </c>
       <c r="D134" t="s">
-        <v>421</v>
+        <v>419</v>
       </c>
     </row>
     <row r="135" spans="1:9" ht="61" customHeight="1">
@@ -4857,7 +4854,7 @@
         <v>4</v>
       </c>
       <c r="D135" t="s">
-        <v>402</v>
+        <v>400</v>
       </c>
       <c r="E135" t="s">
         <v>117</v>
@@ -4917,7 +4914,7 @@
         <v>118</v>
       </c>
       <c r="D141" t="s">
-        <v>421</v>
+        <v>419</v>
       </c>
     </row>
     <row r="142" spans="1:9" ht="75" customHeight="1">
@@ -4926,7 +4923,7 @@
         <v>4</v>
       </c>
       <c r="D142" t="s">
-        <v>403</v>
+        <v>401</v>
       </c>
       <c r="E142" t="s">
         <v>119</v>
@@ -4938,7 +4935,7 @@
         <v>4</v>
       </c>
       <c r="D143" t="s">
-        <v>404</v>
+        <v>402</v>
       </c>
       <c r="E143" t="s">
         <v>119</v>
@@ -4950,7 +4947,7 @@
         <v>4</v>
       </c>
       <c r="D144" t="s">
-        <v>405</v>
+        <v>403</v>
       </c>
       <c r="E144" t="s">
         <v>119</v>
@@ -5007,7 +5004,7 @@
         <v>4</v>
       </c>
       <c r="D150" t="s">
-        <v>416</v>
+        <v>414</v>
       </c>
     </row>
     <row r="151" spans="1:9" ht="12.75" customHeight="1">
@@ -5031,30 +5028,30 @@
     <row r="154" spans="1:9" s="14" customFormat="1" ht="15">
       <c r="A154" s="28"/>
       <c r="B154" s="14" t="s">
-        <v>406</v>
+        <v>404</v>
       </c>
       <c r="C154" s="38"/>
       <c r="D154" s="39"/>
       <c r="E154" s="15" t="s">
-        <v>407</v>
+        <v>405</v>
       </c>
       <c r="F154" s="38"/>
     </row>
     <row r="155" spans="1:9" s="14" customFormat="1" ht="15">
       <c r="A155" s="28"/>
       <c r="B155" s="14" t="s">
-        <v>408</v>
+        <v>406</v>
       </c>
       <c r="C155" s="38"/>
       <c r="D155" s="39"/>
       <c r="E155" s="15" t="s">
-        <v>409</v>
+        <v>407</v>
       </c>
       <c r="F155" s="38"/>
     </row>
     <row r="156" spans="1:9" ht="15">
       <c r="A156" s="7" t="s">
-        <v>503</v>
+        <v>501</v>
       </c>
       <c r="B156" s="8" t="s">
         <v>54</v>
@@ -5132,7 +5129,7 @@
         <v>24</v>
       </c>
       <c r="D162" t="s">
-        <v>421</v>
+        <v>419</v>
       </c>
     </row>
     <row r="163" spans="1:9" ht="12.75" customHeight="1">
@@ -5141,7 +5138,7 @@
         <v>4</v>
       </c>
       <c r="D163" t="s">
-        <v>410</v>
+        <v>408</v>
       </c>
       <c r="E163" t="s">
         <v>25</v>
@@ -5172,7 +5169,7 @@
         <v>27</v>
       </c>
       <c r="D166" t="s">
-        <v>422</v>
+        <v>420</v>
       </c>
     </row>
     <row r="167" spans="1:9" ht="12.75" customHeight="1">
@@ -5181,7 +5178,7 @@
         <v>4</v>
       </c>
       <c r="D167" t="s">
-        <v>411</v>
+        <v>409</v>
       </c>
       <c r="E167" t="s">
         <v>32</v>
@@ -5226,7 +5223,7 @@
         <v>63</v>
       </c>
       <c r="D172" t="s">
-        <v>423</v>
+        <v>421</v>
       </c>
     </row>
     <row r="173" spans="1:9" ht="12.75" customHeight="1">
@@ -5238,7 +5235,7 @@
         <v>64</v>
       </c>
       <c r="D173" t="s">
-        <v>424</v>
+        <v>422</v>
       </c>
     </row>
     <row r="174" spans="1:9" ht="12.75" customHeight="1">
@@ -5247,7 +5244,7 @@
         <v>4</v>
       </c>
       <c r="D174" t="s">
-        <v>412</v>
+        <v>410</v>
       </c>
       <c r="E174" t="s">
         <v>65</v>
@@ -5286,7 +5283,7 @@
         <v>68</v>
       </c>
       <c r="D178" t="s">
-        <v>425</v>
+        <v>423</v>
       </c>
     </row>
     <row r="179" spans="1:8" ht="12.75" customHeight="1">
@@ -5298,7 +5295,7 @@
         <v>69</v>
       </c>
       <c r="D179" t="s">
-        <v>426</v>
+        <v>424</v>
       </c>
     </row>
     <row r="180" spans="1:8" ht="12.75" customHeight="1">
@@ -5307,7 +5304,7 @@
         <v>4</v>
       </c>
       <c r="D180" t="s">
-        <v>413</v>
+        <v>411</v>
       </c>
       <c r="E180" t="s">
         <v>70</v>
@@ -5346,7 +5343,7 @@
         <v>48</v>
       </c>
       <c r="D184" t="s">
-        <v>427</v>
+        <v>425</v>
       </c>
     </row>
     <row r="185" spans="1:8" ht="12.75" customHeight="1">
@@ -5355,7 +5352,7 @@
         <v>4</v>
       </c>
       <c r="D185" t="s">
-        <v>428</v>
+        <v>426</v>
       </c>
     </row>
     <row r="186" spans="1:8" ht="12.75" customHeight="1">
@@ -5367,7 +5364,7 @@
         <v>43</v>
       </c>
       <c r="D186" t="s">
-        <v>429</v>
+        <v>427</v>
       </c>
     </row>
     <row r="187" spans="1:8" ht="12.75" customHeight="1">
@@ -5379,7 +5376,7 @@
         <v>44</v>
       </c>
       <c r="D187" t="s">
-        <v>430</v>
+        <v>428</v>
       </c>
     </row>
     <row r="188" spans="1:8" ht="12.75" customHeight="1">
@@ -5388,7 +5385,7 @@
         <v>4</v>
       </c>
       <c r="D188" t="s">
-        <v>414</v>
+        <v>412</v>
       </c>
       <c r="E188" t="s">
         <v>73</v>
@@ -5400,7 +5397,7 @@
         <v>4</v>
       </c>
       <c r="D189" t="s">
-        <v>415</v>
+        <v>413</v>
       </c>
       <c r="E189" t="s">
         <v>45</v>
@@ -5426,7 +5423,7 @@
     </row>
     <row r="194" spans="2:2" ht="12.75" customHeight="1">
       <c r="B194" s="36" t="s">
-        <v>385</v>
+        <v>383</v>
       </c>
     </row>
   </sheetData>
@@ -5444,8 +5441,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:D139"/>
   <sheetViews>
-    <sheetView zoomScale="150" zoomScaleNormal="150" zoomScalePageLayoutView="150" workbookViewId="0">
-      <selection activeCell="D18" sqref="D18"/>
+    <sheetView tabSelected="1" zoomScale="150" zoomScaleNormal="150" zoomScalePageLayoutView="150" workbookViewId="0">
+      <selection activeCell="D16" sqref="D16"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultColWidth="17.1640625" defaultRowHeight="12.75" customHeight="1" x14ac:dyDescent="0"/>
@@ -5480,13 +5477,13 @@
         <v>137</v>
       </c>
       <c r="B3" t="s">
-        <v>384</v>
+        <v>382</v>
       </c>
       <c r="C3" t="s">
-        <v>393</v>
+        <v>391</v>
       </c>
       <c r="D3" t="s">
-        <v>394</v>
+        <v>392</v>
       </c>
     </row>
     <row r="4" spans="1:4" ht="12.75" customHeight="1">
@@ -5538,26 +5535,26 @@
         <v>147</v>
       </c>
       <c r="B9" t="s">
-        <v>395</v>
+        <v>393</v>
       </c>
       <c r="C9" t="s">
-        <v>396</v>
+        <v>394</v>
       </c>
     </row>
     <row r="11" spans="1:4" ht="12.75" customHeight="1">
       <c r="A11" t="s">
-        <v>438</v>
+        <v>436</v>
       </c>
       <c r="B11" t="s">
         <v>139</v>
       </c>
       <c r="C11" t="s">
-        <v>441</v>
+        <v>439</v>
       </c>
     </row>
     <row r="12" spans="1:4" ht="12.75" customHeight="1">
       <c r="A12" t="s">
-        <v>438</v>
+        <v>436</v>
       </c>
       <c r="B12" t="s">
         <v>144</v>
@@ -5568,24 +5565,24 @@
     </row>
     <row r="13" spans="1:4" ht="12.75" customHeight="1">
       <c r="A13" t="s">
-        <v>438</v>
+        <v>436</v>
       </c>
       <c r="B13" t="s">
-        <v>439</v>
+        <v>437</v>
       </c>
       <c r="C13" t="s">
-        <v>442</v>
+        <v>440</v>
       </c>
     </row>
     <row r="14" spans="1:4" ht="12.75" customHeight="1">
       <c r="A14" t="s">
+        <v>436</v>
+      </c>
+      <c r="B14" t="s">
         <v>438</v>
       </c>
-      <c r="B14" t="s">
-        <v>440</v>
-      </c>
       <c r="C14" t="s">
-        <v>443</v>
+        <v>441</v>
       </c>
     </row>
     <row r="16" spans="1:4" ht="12.75" customHeight="1">
@@ -5595,44 +5592,44 @@
       <c r="B16" t="s">
         <v>153</v>
       </c>
-      <c r="D16" t="s">
-        <v>154</v>
-      </c>
-    </row>
-    <row r="17" spans="1:4" ht="12.75" customHeight="1">
+      <c r="C16" t="s">
+        <v>533</v>
+      </c>
+    </row>
+    <row r="17" spans="1:3" ht="12.75" customHeight="1">
       <c r="A17" t="s">
         <v>152</v>
       </c>
       <c r="B17" t="s">
-        <v>155</v>
-      </c>
-      <c r="D17" t="s">
-        <v>156</v>
-      </c>
-    </row>
-    <row r="18" spans="1:4" ht="12.75" customHeight="1">
+        <v>154</v>
+      </c>
+      <c r="C17" t="s">
+        <v>451</v>
+      </c>
+    </row>
+    <row r="18" spans="1:3" ht="12.75" customHeight="1">
       <c r="A18" t="s">
         <v>152</v>
       </c>
       <c r="B18" t="s">
-        <v>157</v>
+        <v>155</v>
       </c>
       <c r="C18" t="s">
-        <v>534</v>
-      </c>
-    </row>
-    <row r="19" spans="1:4" ht="12.75" customHeight="1">
+        <v>532</v>
+      </c>
+    </row>
+    <row r="19" spans="1:3" ht="12.75" customHeight="1">
       <c r="A19" t="s">
         <v>152</v>
       </c>
       <c r="B19" t="s">
-        <v>159</v>
+        <v>157</v>
       </c>
       <c r="C19" t="s">
-        <v>160</v>
-      </c>
-    </row>
-    <row r="21" spans="1:4" ht="12.75" customHeight="1">
+        <v>158</v>
+      </c>
+    </row>
+    <row r="21" spans="1:3" ht="12.75" customHeight="1">
       <c r="A21" t="s">
         <v>56</v>
       </c>
@@ -5643,7 +5640,7 @@
         <v>92</v>
       </c>
     </row>
-    <row r="22" spans="1:4" ht="12.75" customHeight="1">
+    <row r="22" spans="1:3" ht="12.75" customHeight="1">
       <c r="A22" t="s">
         <v>56</v>
       </c>
@@ -5654,7 +5651,7 @@
         <v>94</v>
       </c>
     </row>
-    <row r="23" spans="1:4" ht="12.75" customHeight="1">
+    <row r="23" spans="1:3" ht="12.75" customHeight="1">
       <c r="A23" t="s">
         <v>56</v>
       </c>
@@ -5665,7 +5662,7 @@
         <v>96</v>
       </c>
     </row>
-    <row r="24" spans="1:4" ht="12.75" customHeight="1">
+    <row r="24" spans="1:3" ht="12.75" customHeight="1">
       <c r="A24" t="s">
         <v>56</v>
       </c>
@@ -5676,7 +5673,7 @@
         <v>98</v>
       </c>
     </row>
-    <row r="26" spans="1:4" ht="12.75" customHeight="1">
+    <row r="26" spans="1:3" ht="12.75" customHeight="1">
       <c r="A26" t="s">
         <v>16</v>
       </c>
@@ -5687,7 +5684,7 @@
         <v>50</v>
       </c>
     </row>
-    <row r="27" spans="1:4" ht="12.75" customHeight="1">
+    <row r="27" spans="1:3" ht="12.75" customHeight="1">
       <c r="A27" t="s">
         <v>16</v>
       </c>
@@ -5698,7 +5695,7 @@
         <v>19</v>
       </c>
     </row>
-    <row r="28" spans="1:4" ht="12.75" customHeight="1">
+    <row r="28" spans="1:3" ht="12.75" customHeight="1">
       <c r="A28" t="s">
         <v>16</v>
       </c>
@@ -5709,7 +5706,7 @@
         <v>20</v>
       </c>
     </row>
-    <row r="30" spans="1:4" ht="12.75" customHeight="1">
+    <row r="30" spans="1:3" ht="12.75" customHeight="1">
       <c r="A30" t="s">
         <v>77</v>
       </c>
@@ -5720,7 +5717,7 @@
         <v>47</v>
       </c>
     </row>
-    <row r="31" spans="1:4" ht="12.75" customHeight="1">
+    <row r="31" spans="1:3" ht="12.75" customHeight="1">
       <c r="A31" t="s">
         <v>77</v>
       </c>
@@ -5731,7 +5728,7 @@
         <v>33</v>
       </c>
     </row>
-    <row r="32" spans="1:4" ht="12.75" customHeight="1">
+    <row r="32" spans="1:3" ht="12.75" customHeight="1">
       <c r="A32" t="s">
         <v>77</v>
       </c>
@@ -5788,40 +5785,40 @@
     </row>
     <row r="39" spans="1:4" ht="12.75" customHeight="1">
       <c r="A39" t="s">
-        <v>512</v>
+        <v>510</v>
       </c>
       <c r="B39" t="s">
+        <v>511</v>
+      </c>
+      <c r="C39" t="s">
         <v>513</v>
-      </c>
-      <c r="C39" t="s">
-        <v>515</v>
       </c>
     </row>
     <row r="40" spans="1:4" ht="12.75" customHeight="1">
       <c r="A40" t="s">
+        <v>510</v>
+      </c>
+      <c r="B40" t="s">
         <v>512</v>
       </c>
-      <c r="B40" t="s">
+      <c r="C40" t="s">
         <v>514</v>
-      </c>
-      <c r="C40" t="s">
-        <v>516</v>
       </c>
     </row>
     <row r="42" spans="1:4" ht="12.75" customHeight="1">
       <c r="A42" t="s">
-        <v>527</v>
+        <v>525</v>
       </c>
       <c r="B42" t="s">
-        <v>158</v>
+        <v>156</v>
       </c>
       <c r="C42" t="s">
-        <v>528</v>
+        <v>526</v>
       </c>
     </row>
     <row r="43" spans="1:4" ht="12.75" customHeight="1">
       <c r="A43" t="s">
-        <v>527</v>
+        <v>525</v>
       </c>
       <c r="B43" t="s">
         <v>91</v>
@@ -5832,7 +5829,7 @@
     </row>
     <row r="44" spans="1:4" ht="12.75" customHeight="1">
       <c r="A44" t="s">
-        <v>527</v>
+        <v>525</v>
       </c>
       <c r="B44" t="s">
         <v>97</v>
@@ -5843,882 +5840,882 @@
     </row>
     <row r="46" spans="1:4" ht="12.75" customHeight="1">
       <c r="A46" t="s">
+        <v>159</v>
+      </c>
+      <c r="B46" t="s">
+        <v>160</v>
+      </c>
+      <c r="D46" t="s">
         <v>161</v>
-      </c>
-      <c r="B46" t="s">
-        <v>162</v>
-      </c>
-      <c r="D46" t="s">
-        <v>163</v>
       </c>
     </row>
     <row r="47" spans="1:4" ht="12.75" customHeight="1">
       <c r="A47" t="s">
-        <v>161</v>
+        <v>159</v>
       </c>
       <c r="B47" t="s">
-        <v>164</v>
+        <v>162</v>
       </c>
       <c r="D47" t="s">
-        <v>165</v>
+        <v>163</v>
       </c>
     </row>
     <row r="48" spans="1:4" ht="12.75" customHeight="1">
       <c r="A48" t="s">
-        <v>161</v>
+        <v>159</v>
       </c>
       <c r="B48" t="s">
-        <v>166</v>
+        <v>164</v>
       </c>
       <c r="D48" t="s">
-        <v>167</v>
+        <v>165</v>
       </c>
     </row>
     <row r="49" spans="1:4" ht="12.75" customHeight="1">
       <c r="A49" t="s">
-        <v>161</v>
+        <v>159</v>
       </c>
       <c r="B49" t="s">
-        <v>168</v>
+        <v>166</v>
       </c>
       <c r="D49" t="s">
-        <v>169</v>
+        <v>167</v>
       </c>
     </row>
     <row r="50" spans="1:4" ht="12.75" customHeight="1">
       <c r="A50" t="s">
-        <v>161</v>
+        <v>159</v>
       </c>
       <c r="B50" t="s">
-        <v>170</v>
+        <v>168</v>
       </c>
       <c r="D50" t="s">
-        <v>171</v>
+        <v>169</v>
       </c>
     </row>
     <row r="52" spans="1:4" ht="12.75" customHeight="1">
       <c r="A52" t="s">
+        <v>170</v>
+      </c>
+      <c r="B52" t="s">
+        <v>171</v>
+      </c>
+      <c r="D52" t="s">
         <v>172</v>
-      </c>
-      <c r="B52" t="s">
-        <v>173</v>
-      </c>
-      <c r="D52" t="s">
-        <v>174</v>
       </c>
     </row>
     <row r="53" spans="1:4" s="2" customFormat="1" ht="12.75" customHeight="1">
       <c r="A53" t="s">
-        <v>172</v>
+        <v>170</v>
       </c>
       <c r="B53" t="s">
-        <v>175</v>
+        <v>173</v>
       </c>
       <c r="D53" t="s">
-        <v>176</v>
+        <v>174</v>
       </c>
     </row>
     <row r="54" spans="1:4" ht="12.75" customHeight="1">
       <c r="A54" t="s">
-        <v>172</v>
+        <v>170</v>
       </c>
       <c r="B54" t="s">
-        <v>177</v>
+        <v>175</v>
       </c>
       <c r="D54" t="s">
-        <v>178</v>
+        <v>176</v>
       </c>
     </row>
     <row r="55" spans="1:4" ht="12.75" customHeight="1">
       <c r="A55" t="s">
-        <v>172</v>
+        <v>170</v>
       </c>
       <c r="B55" t="s">
-        <v>179</v>
+        <v>177</v>
       </c>
       <c r="D55" t="s">
-        <v>180</v>
+        <v>178</v>
       </c>
     </row>
     <row r="56" spans="1:4" ht="12.75" customHeight="1">
       <c r="A56" t="s">
-        <v>172</v>
+        <v>170</v>
       </c>
       <c r="B56" t="s">
-        <v>181</v>
+        <v>179</v>
       </c>
       <c r="D56" t="s">
-        <v>182</v>
+        <v>180</v>
       </c>
     </row>
     <row r="57" spans="1:4" ht="12.75" customHeight="1">
       <c r="A57" t="s">
-        <v>172</v>
+        <v>170</v>
       </c>
       <c r="B57" t="s">
-        <v>183</v>
+        <v>181</v>
       </c>
       <c r="D57" t="s">
-        <v>184</v>
+        <v>182</v>
       </c>
     </row>
     <row r="59" spans="1:4" ht="12.75" customHeight="1">
       <c r="A59" t="s">
-        <v>185</v>
+        <v>183</v>
       </c>
       <c r="B59" t="s">
-        <v>186</v>
+        <v>184</v>
       </c>
       <c r="C59" s="2"/>
       <c r="D59" t="s">
-        <v>187</v>
+        <v>185</v>
       </c>
     </row>
     <row r="60" spans="1:4" ht="12.75" customHeight="1">
       <c r="A60" t="s">
-        <v>185</v>
+        <v>183</v>
       </c>
       <c r="B60" t="s">
-        <v>188</v>
+        <v>186</v>
       </c>
       <c r="D60" t="s">
-        <v>189</v>
+        <v>187</v>
       </c>
     </row>
     <row r="61" spans="1:4" ht="12.75" customHeight="1">
       <c r="A61" t="s">
-        <v>185</v>
+        <v>183</v>
       </c>
       <c r="B61" t="s">
-        <v>190</v>
+        <v>188</v>
       </c>
       <c r="D61" t="s">
-        <v>191</v>
+        <v>189</v>
       </c>
     </row>
     <row r="62" spans="1:4" ht="12.75" customHeight="1">
       <c r="A62" t="s">
-        <v>185</v>
+        <v>183</v>
       </c>
       <c r="B62" t="s">
-        <v>192</v>
+        <v>190</v>
       </c>
       <c r="D62" t="s">
-        <v>193</v>
+        <v>191</v>
       </c>
     </row>
     <row r="63" spans="1:4" ht="12.75" customHeight="1">
       <c r="A63" t="s">
-        <v>185</v>
+        <v>183</v>
       </c>
       <c r="B63" t="s">
-        <v>194</v>
+        <v>192</v>
       </c>
       <c r="D63" t="s">
-        <v>195</v>
+        <v>193</v>
       </c>
     </row>
     <row r="65" spans="1:4" ht="12.75" customHeight="1">
       <c r="A65" t="s">
+        <v>194</v>
+      </c>
+      <c r="B65" t="s">
+        <v>195</v>
+      </c>
+      <c r="D65" t="s">
         <v>196</v>
-      </c>
-      <c r="B65" t="s">
-        <v>197</v>
-      </c>
-      <c r="D65" t="s">
-        <v>198</v>
       </c>
     </row>
     <row r="66" spans="1:4" ht="12.75" customHeight="1">
       <c r="A66" t="s">
-        <v>196</v>
+        <v>194</v>
       </c>
       <c r="B66" t="s">
-        <v>199</v>
+        <v>197</v>
       </c>
       <c r="C66" s="2"/>
       <c r="D66" t="s">
-        <v>200</v>
+        <v>198</v>
       </c>
     </row>
     <row r="67" spans="1:4" ht="12.75" customHeight="1">
       <c r="A67" t="s">
-        <v>196</v>
+        <v>194</v>
       </c>
       <c r="B67" t="s">
-        <v>201</v>
+        <v>199</v>
       </c>
       <c r="D67" t="s">
-        <v>202</v>
+        <v>200</v>
       </c>
     </row>
     <row r="68" spans="1:4" ht="12.75" customHeight="1">
       <c r="A68" t="s">
-        <v>196</v>
+        <v>194</v>
       </c>
       <c r="B68" t="s">
-        <v>203</v>
+        <v>201</v>
       </c>
       <c r="D68" t="s">
-        <v>204</v>
+        <v>202</v>
       </c>
     </row>
     <row r="69" spans="1:4" ht="12.75" customHeight="1">
       <c r="A69" t="s">
-        <v>196</v>
+        <v>194</v>
       </c>
       <c r="B69" t="s">
-        <v>205</v>
+        <v>203</v>
       </c>
       <c r="D69" t="s">
-        <v>206</v>
+        <v>204</v>
       </c>
     </row>
     <row r="70" spans="1:4" ht="12.75" customHeight="1">
       <c r="A70" t="s">
-        <v>196</v>
+        <v>194</v>
       </c>
       <c r="B70" t="s">
-        <v>207</v>
+        <v>205</v>
       </c>
       <c r="D70" t="s">
-        <v>208</v>
+        <v>206</v>
       </c>
     </row>
     <row r="71" spans="1:4" ht="12.75" customHeight="1">
       <c r="A71" t="s">
-        <v>196</v>
+        <v>194</v>
       </c>
       <c r="B71" t="s">
-        <v>209</v>
+        <v>207</v>
       </c>
       <c r="D71" t="s">
-        <v>210</v>
+        <v>208</v>
       </c>
     </row>
     <row r="73" spans="1:4" ht="12.75" customHeight="1">
       <c r="A73" t="s">
+        <v>209</v>
+      </c>
+      <c r="B73" t="s">
+        <v>210</v>
+      </c>
+      <c r="D73" t="s">
         <v>211</v>
-      </c>
-      <c r="B73" t="s">
-        <v>212</v>
-      </c>
-      <c r="D73" t="s">
-        <v>213</v>
       </c>
     </row>
     <row r="74" spans="1:4" ht="12.75" customHeight="1">
       <c r="A74" t="s">
-        <v>211</v>
+        <v>209</v>
       </c>
       <c r="B74" t="s">
-        <v>214</v>
+        <v>212</v>
       </c>
       <c r="C74" s="2"/>
       <c r="D74" t="s">
-        <v>215</v>
+        <v>213</v>
       </c>
     </row>
     <row r="75" spans="1:4" ht="12.75" customHeight="1">
       <c r="A75" t="s">
-        <v>211</v>
+        <v>209</v>
       </c>
       <c r="B75" t="s">
-        <v>216</v>
+        <v>214</v>
       </c>
       <c r="D75" t="s">
-        <v>217</v>
+        <v>215</v>
       </c>
     </row>
     <row r="76" spans="1:4" ht="12.75" customHeight="1">
       <c r="A76" t="s">
-        <v>211</v>
+        <v>209</v>
       </c>
       <c r="B76" t="s">
-        <v>218</v>
+        <v>216</v>
       </c>
       <c r="D76" t="s">
-        <v>219</v>
+        <v>217</v>
       </c>
     </row>
     <row r="77" spans="1:4" ht="12.75" customHeight="1">
       <c r="A77" t="s">
-        <v>211</v>
+        <v>209</v>
       </c>
       <c r="B77" t="s">
-        <v>220</v>
+        <v>218</v>
       </c>
       <c r="D77" t="s">
-        <v>221</v>
+        <v>219</v>
       </c>
     </row>
     <row r="78" spans="1:4" ht="12.75" customHeight="1">
       <c r="A78" t="s">
-        <v>211</v>
+        <v>209</v>
       </c>
       <c r="B78" t="s">
-        <v>222</v>
+        <v>220</v>
       </c>
       <c r="D78" t="s">
-        <v>223</v>
+        <v>221</v>
       </c>
     </row>
     <row r="80" spans="1:4" ht="12.75" customHeight="1">
       <c r="A80" t="s">
+        <v>222</v>
+      </c>
+      <c r="B80" t="s">
+        <v>223</v>
+      </c>
+      <c r="D80" t="s">
         <v>224</v>
-      </c>
-      <c r="B80" t="s">
-        <v>225</v>
-      </c>
-      <c r="D80" t="s">
-        <v>226</v>
       </c>
     </row>
     <row r="81" spans="1:4" ht="12.75" customHeight="1">
       <c r="A81" t="s">
-        <v>224</v>
+        <v>222</v>
       </c>
       <c r="B81" t="s">
-        <v>227</v>
+        <v>225</v>
       </c>
       <c r="C81" s="2"/>
       <c r="D81" t="s">
-        <v>228</v>
+        <v>226</v>
       </c>
     </row>
     <row r="82" spans="1:4" ht="12.75" customHeight="1">
       <c r="A82" t="s">
-        <v>224</v>
+        <v>222</v>
       </c>
       <c r="B82" t="s">
-        <v>229</v>
+        <v>227</v>
       </c>
       <c r="D82" t="s">
-        <v>230</v>
+        <v>228</v>
       </c>
     </row>
     <row r="83" spans="1:4" ht="12.75" customHeight="1">
       <c r="A83" t="s">
-        <v>224</v>
+        <v>222</v>
       </c>
       <c r="B83" t="s">
-        <v>231</v>
+        <v>229</v>
       </c>
       <c r="D83" t="s">
-        <v>232</v>
+        <v>230</v>
       </c>
     </row>
     <row r="84" spans="1:4" ht="12.75" customHeight="1">
       <c r="A84" t="s">
-        <v>224</v>
+        <v>222</v>
       </c>
       <c r="B84" t="s">
-        <v>233</v>
+        <v>231</v>
       </c>
       <c r="D84" t="s">
-        <v>234</v>
+        <v>232</v>
       </c>
     </row>
     <row r="85" spans="1:4" ht="12.75" customHeight="1">
       <c r="A85" t="s">
-        <v>224</v>
+        <v>222</v>
       </c>
       <c r="B85" t="s">
-        <v>235</v>
+        <v>233</v>
       </c>
       <c r="D85" t="s">
-        <v>236</v>
+        <v>234</v>
       </c>
     </row>
     <row r="87" spans="1:4" ht="12.75" customHeight="1">
       <c r="A87" t="s">
+        <v>235</v>
+      </c>
+      <c r="B87" t="s">
+        <v>236</v>
+      </c>
+      <c r="C87" t="s">
         <v>237</v>
-      </c>
-      <c r="B87" t="s">
-        <v>238</v>
-      </c>
-      <c r="C87" t="s">
-        <v>239</v>
       </c>
     </row>
     <row r="88" spans="1:4" ht="12.75" customHeight="1">
       <c r="A88" t="s">
-        <v>237</v>
+        <v>235</v>
       </c>
       <c r="B88" t="s">
-        <v>240</v>
+        <v>238</v>
       </c>
       <c r="C88" t="s">
-        <v>241</v>
+        <v>239</v>
       </c>
     </row>
     <row r="89" spans="1:4" ht="12.75" customHeight="1">
       <c r="A89" t="s">
-        <v>237</v>
+        <v>235</v>
       </c>
       <c r="B89" t="s">
-        <v>242</v>
+        <v>240</v>
       </c>
       <c r="C89" t="s">
-        <v>243</v>
+        <v>241</v>
       </c>
     </row>
     <row r="90" spans="1:4" ht="12.75" customHeight="1">
       <c r="A90" t="s">
-        <v>237</v>
+        <v>235</v>
       </c>
       <c r="B90" t="s">
-        <v>244</v>
+        <v>242</v>
       </c>
       <c r="C90" t="s">
-        <v>245</v>
+        <v>243</v>
       </c>
     </row>
     <row r="91" spans="1:4" ht="12.75" customHeight="1">
       <c r="A91" t="s">
-        <v>237</v>
+        <v>235</v>
       </c>
       <c r="B91" t="s">
-        <v>246</v>
+        <v>244</v>
       </c>
       <c r="C91" t="s">
-        <v>247</v>
+        <v>245</v>
       </c>
     </row>
     <row r="92" spans="1:4" ht="12.75" customHeight="1">
       <c r="A92" t="s">
-        <v>237</v>
+        <v>235</v>
       </c>
       <c r="B92" t="s">
-        <v>248</v>
+        <v>246</v>
       </c>
       <c r="C92" t="s">
-        <v>249</v>
+        <v>247</v>
       </c>
     </row>
     <row r="93" spans="1:4" ht="12.75" customHeight="1">
       <c r="A93" t="s">
-        <v>237</v>
+        <v>235</v>
       </c>
       <c r="B93" t="s">
-        <v>250</v>
+        <v>248</v>
       </c>
       <c r="C93" t="s">
-        <v>251</v>
+        <v>249</v>
       </c>
     </row>
     <row r="95" spans="1:4" ht="12.75" customHeight="1">
       <c r="A95" t="s">
+        <v>250</v>
+      </c>
+      <c r="B95" t="s">
+        <v>251</v>
+      </c>
+      <c r="C95" t="s">
         <v>252</v>
-      </c>
-      <c r="B95" t="s">
-        <v>253</v>
-      </c>
-      <c r="C95" t="s">
-        <v>254</v>
       </c>
     </row>
     <row r="96" spans="1:4" ht="12.75" customHeight="1">
       <c r="A96" t="s">
-        <v>252</v>
+        <v>250</v>
       </c>
       <c r="B96" t="s">
-        <v>255</v>
+        <v>253</v>
       </c>
       <c r="C96" t="s">
-        <v>256</v>
+        <v>254</v>
       </c>
     </row>
     <row r="97" spans="1:3" ht="12.75" customHeight="1">
       <c r="A97" t="s">
-        <v>252</v>
+        <v>250</v>
       </c>
       <c r="B97" t="s">
-        <v>257</v>
+        <v>255</v>
       </c>
       <c r="C97" t="s">
-        <v>258</v>
+        <v>256</v>
       </c>
     </row>
     <row r="98" spans="1:3" ht="12.75" customHeight="1">
       <c r="A98" t="s">
-        <v>252</v>
+        <v>250</v>
       </c>
       <c r="B98" t="s">
-        <v>259</v>
+        <v>257</v>
       </c>
       <c r="C98" t="s">
-        <v>260</v>
+        <v>258</v>
       </c>
     </row>
     <row r="99" spans="1:3" ht="12.75" customHeight="1">
       <c r="A99" t="s">
-        <v>252</v>
+        <v>250</v>
       </c>
       <c r="B99" t="s">
-        <v>261</v>
+        <v>259</v>
       </c>
       <c r="C99" t="s">
-        <v>262</v>
+        <v>260</v>
       </c>
     </row>
     <row r="100" spans="1:3" ht="12.75" customHeight="1">
       <c r="A100" t="s">
-        <v>252</v>
+        <v>250</v>
       </c>
       <c r="B100" t="s">
-        <v>263</v>
+        <v>261</v>
       </c>
       <c r="C100" t="s">
-        <v>264</v>
+        <v>262</v>
       </c>
     </row>
     <row r="102" spans="1:3" ht="12.75" customHeight="1">
       <c r="A102" t="s">
+        <v>263</v>
+      </c>
+      <c r="B102" t="s">
+        <v>264</v>
+      </c>
+      <c r="C102" t="s">
         <v>265</v>
-      </c>
-      <c r="B102" t="s">
-        <v>266</v>
-      </c>
-      <c r="C102" t="s">
-        <v>267</v>
       </c>
     </row>
     <row r="103" spans="1:3" ht="12.75" customHeight="1">
       <c r="A103" t="s">
-        <v>265</v>
+        <v>263</v>
       </c>
       <c r="B103" t="s">
-        <v>268</v>
+        <v>266</v>
       </c>
       <c r="C103" t="s">
-        <v>269</v>
+        <v>267</v>
       </c>
     </row>
     <row r="104" spans="1:3" ht="12.75" customHeight="1">
       <c r="A104" t="s">
-        <v>265</v>
+        <v>263</v>
       </c>
       <c r="B104" t="s">
-        <v>270</v>
+        <v>268</v>
       </c>
       <c r="C104" t="s">
-        <v>271</v>
+        <v>269</v>
       </c>
     </row>
     <row r="105" spans="1:3" ht="12.75" customHeight="1">
       <c r="A105" t="s">
-        <v>265</v>
+        <v>263</v>
       </c>
       <c r="B105" t="s">
-        <v>272</v>
+        <v>270</v>
       </c>
       <c r="C105" t="s">
-        <v>273</v>
+        <v>271</v>
       </c>
     </row>
     <row r="106" spans="1:3" ht="12.75" customHeight="1">
       <c r="A106" t="s">
-        <v>265</v>
+        <v>263</v>
       </c>
       <c r="B106" t="s">
-        <v>274</v>
+        <v>272</v>
       </c>
       <c r="C106" t="s">
-        <v>275</v>
+        <v>273</v>
       </c>
     </row>
     <row r="107" spans="1:3" ht="12.75" customHeight="1">
       <c r="A107" t="s">
-        <v>265</v>
+        <v>263</v>
       </c>
       <c r="B107" t="s">
-        <v>276</v>
+        <v>274</v>
       </c>
       <c r="C107" t="s">
-        <v>277</v>
+        <v>275</v>
       </c>
     </row>
     <row r="108" spans="1:3" ht="12.75" customHeight="1">
       <c r="A108" t="s">
-        <v>265</v>
+        <v>263</v>
       </c>
       <c r="B108" t="s">
-        <v>278</v>
+        <v>276</v>
       </c>
       <c r="C108" t="s">
-        <v>279</v>
+        <v>277</v>
       </c>
     </row>
     <row r="110" spans="1:3" ht="12.75" customHeight="1">
       <c r="A110" t="s">
+        <v>278</v>
+      </c>
+      <c r="B110" t="s">
+        <v>279</v>
+      </c>
+      <c r="C110" t="s">
         <v>280</v>
-      </c>
-      <c r="B110" t="s">
-        <v>281</v>
-      </c>
-      <c r="C110" t="s">
-        <v>282</v>
       </c>
     </row>
     <row r="111" spans="1:3" ht="12.75" customHeight="1">
       <c r="A111" t="s">
-        <v>280</v>
+        <v>278</v>
       </c>
       <c r="B111" t="s">
-        <v>283</v>
+        <v>281</v>
       </c>
       <c r="C111" t="s">
-        <v>284</v>
+        <v>282</v>
       </c>
     </row>
     <row r="112" spans="1:3" ht="12.75" customHeight="1">
       <c r="A112" t="s">
-        <v>280</v>
+        <v>278</v>
       </c>
       <c r="B112" t="s">
-        <v>285</v>
+        <v>283</v>
       </c>
       <c r="C112" t="s">
-        <v>286</v>
+        <v>284</v>
       </c>
     </row>
     <row r="113" spans="1:3" ht="12.75" customHeight="1">
       <c r="A113" t="s">
-        <v>280</v>
+        <v>278</v>
       </c>
       <c r="B113" t="s">
-        <v>287</v>
+        <v>285</v>
       </c>
       <c r="C113" t="s">
-        <v>288</v>
+        <v>286</v>
       </c>
     </row>
     <row r="114" spans="1:3" ht="12.75" customHeight="1">
       <c r="A114" t="s">
-        <v>280</v>
+        <v>278</v>
       </c>
       <c r="B114" t="s">
-        <v>289</v>
+        <v>287</v>
       </c>
       <c r="C114" t="s">
-        <v>290</v>
+        <v>288</v>
       </c>
     </row>
     <row r="115" spans="1:3" ht="12.75" customHeight="1">
       <c r="A115" t="s">
-        <v>280</v>
+        <v>278</v>
       </c>
       <c r="B115" t="s">
-        <v>291</v>
+        <v>289</v>
       </c>
       <c r="C115" t="s">
-        <v>292</v>
+        <v>290</v>
       </c>
     </row>
     <row r="117" spans="1:3" ht="12.75" customHeight="1">
       <c r="A117" t="s">
+        <v>291</v>
+      </c>
+      <c r="B117" t="s">
+        <v>292</v>
+      </c>
+      <c r="C117" t="s">
         <v>293</v>
-      </c>
-      <c r="B117" t="s">
-        <v>294</v>
-      </c>
-      <c r="C117" t="s">
-        <v>295</v>
       </c>
     </row>
     <row r="118" spans="1:3" ht="12.75" customHeight="1">
       <c r="A118" t="s">
-        <v>293</v>
+        <v>291</v>
       </c>
       <c r="B118" t="s">
-        <v>296</v>
+        <v>294</v>
       </c>
       <c r="C118" t="s">
-        <v>297</v>
+        <v>295</v>
       </c>
     </row>
     <row r="119" spans="1:3" ht="12.75" customHeight="1">
       <c r="A119" t="s">
-        <v>293</v>
+        <v>291</v>
       </c>
       <c r="B119" t="s">
-        <v>298</v>
+        <v>296</v>
       </c>
       <c r="C119" t="s">
-        <v>299</v>
+        <v>297</v>
       </c>
     </row>
     <row r="120" spans="1:3" ht="12.75" customHeight="1">
       <c r="A120" t="s">
-        <v>293</v>
+        <v>291</v>
       </c>
       <c r="B120" t="s">
-        <v>300</v>
+        <v>298</v>
       </c>
       <c r="C120" t="s">
-        <v>301</v>
+        <v>299</v>
       </c>
     </row>
     <row r="121" spans="1:3" ht="12.75" customHeight="1">
       <c r="A121" t="s">
-        <v>293</v>
+        <v>291</v>
       </c>
       <c r="B121" t="s">
-        <v>302</v>
+        <v>300</v>
       </c>
       <c r="C121" t="s">
-        <v>303</v>
+        <v>301</v>
       </c>
     </row>
     <row r="122" spans="1:3" ht="12.75" customHeight="1">
       <c r="A122" t="s">
-        <v>293</v>
+        <v>291</v>
       </c>
       <c r="B122" t="s">
-        <v>304</v>
+        <v>302</v>
       </c>
       <c r="C122" t="s">
-        <v>305</v>
+        <v>303</v>
       </c>
     </row>
     <row r="123" spans="1:3" ht="12.75" customHeight="1">
       <c r="A123" t="s">
-        <v>293</v>
+        <v>291</v>
       </c>
       <c r="B123" t="s">
-        <v>306</v>
+        <v>304</v>
       </c>
       <c r="C123" t="s">
-        <v>307</v>
+        <v>305</v>
       </c>
     </row>
     <row r="125" spans="1:3" ht="12.75" customHeight="1">
       <c r="A125" t="s">
+        <v>306</v>
+      </c>
+      <c r="B125" t="s">
+        <v>307</v>
+      </c>
+      <c r="C125" t="s">
         <v>308</v>
-      </c>
-      <c r="B125" t="s">
-        <v>309</v>
-      </c>
-      <c r="C125" t="s">
-        <v>310</v>
       </c>
     </row>
     <row r="126" spans="1:3" ht="12.75" customHeight="1">
       <c r="A126" t="s">
-        <v>308</v>
+        <v>306</v>
       </c>
       <c r="B126" t="s">
-        <v>311</v>
+        <v>309</v>
       </c>
       <c r="C126" t="s">
-        <v>312</v>
+        <v>310</v>
       </c>
     </row>
     <row r="127" spans="1:3" ht="12.75" customHeight="1">
       <c r="A127" t="s">
-        <v>308</v>
+        <v>306</v>
       </c>
       <c r="B127" t="s">
-        <v>313</v>
+        <v>311</v>
       </c>
       <c r="C127" t="s">
-        <v>314</v>
+        <v>312</v>
       </c>
     </row>
     <row r="128" spans="1:3" ht="12.75" customHeight="1">
       <c r="A128" t="s">
-        <v>308</v>
+        <v>306</v>
       </c>
       <c r="B128" t="s">
-        <v>315</v>
+        <v>313</v>
       </c>
       <c r="C128" t="s">
-        <v>316</v>
+        <v>314</v>
       </c>
     </row>
     <row r="129" spans="1:4" ht="12.75" customHeight="1">
       <c r="A129" t="s">
-        <v>308</v>
+        <v>306</v>
       </c>
       <c r="B129" t="s">
-        <v>317</v>
+        <v>315</v>
       </c>
       <c r="C129" t="s">
-        <v>318</v>
+        <v>316</v>
       </c>
     </row>
     <row r="130" spans="1:4" ht="12.75" customHeight="1">
       <c r="A130" t="s">
-        <v>308</v>
+        <v>306</v>
       </c>
       <c r="B130" t="s">
-        <v>319</v>
+        <v>317</v>
       </c>
       <c r="C130" t="s">
-        <v>320</v>
+        <v>318</v>
       </c>
     </row>
     <row r="132" spans="1:4" ht="12.75" customHeight="1">
       <c r="A132" t="s">
+        <v>319</v>
+      </c>
+      <c r="B132" t="s">
+        <v>320</v>
+      </c>
+      <c r="C132" t="s">
         <v>321</v>
-      </c>
-      <c r="B132" t="s">
-        <v>322</v>
-      </c>
-      <c r="C132" t="s">
-        <v>323</v>
       </c>
     </row>
     <row r="133" spans="1:4" ht="12.75" customHeight="1">
       <c r="A133" t="s">
-        <v>321</v>
+        <v>319</v>
       </c>
       <c r="B133" t="s">
-        <v>324</v>
+        <v>322</v>
       </c>
       <c r="C133" t="s">
-        <v>325</v>
+        <v>323</v>
       </c>
     </row>
     <row r="135" spans="1:4" ht="12.75" customHeight="1">
       <c r="A135" s="2" t="s">
-        <v>326</v>
+        <v>324</v>
       </c>
       <c r="D135" t="s">
-        <v>327</v>
+        <v>325</v>
       </c>
     </row>
     <row r="136" spans="1:4" ht="12.75" customHeight="1">
       <c r="A136" t="s">
+        <v>324</v>
+      </c>
+      <c r="D136" t="s">
         <v>326</v>
-      </c>
-      <c r="D136" t="s">
-        <v>328</v>
       </c>
     </row>
     <row r="137" spans="1:4" ht="12.75" customHeight="1">
       <c r="A137" s="2" t="s">
-        <v>326</v>
+        <v>324</v>
       </c>
       <c r="D137" t="s">
-        <v>329</v>
+        <v>327</v>
       </c>
     </row>
     <row r="138" spans="1:4" ht="12.75" customHeight="1">
       <c r="A138" s="2" t="s">
-        <v>326</v>
+        <v>324</v>
       </c>
       <c r="D138" t="s">
-        <v>330</v>
+        <v>328</v>
       </c>
     </row>
     <row r="139" spans="1:4" ht="12.75" customHeight="1">
       <c r="A139" s="2" t="s">
-        <v>326</v>
+        <v>324</v>
       </c>
       <c r="D139" t="s">
-        <v>331</v>
+        <v>329</v>
       </c>
     </row>
   </sheetData>
@@ -6771,151 +6768,151 @@
     </row>
     <row r="4" spans="1:2" ht="12.75" customHeight="1">
       <c r="A4" t="s">
-        <v>332</v>
+        <v>330</v>
       </c>
       <c r="B4" t="s">
-        <v>333</v>
+        <v>331</v>
       </c>
     </row>
     <row r="5" spans="1:2" ht="12.75" customHeight="1">
       <c r="A5" t="s">
-        <v>334</v>
+        <v>332</v>
       </c>
       <c r="B5" t="s">
-        <v>335</v>
+        <v>333</v>
       </c>
     </row>
     <row r="6" spans="1:2" ht="12.75" customHeight="1">
       <c r="A6" t="s">
-        <v>336</v>
+        <v>334</v>
       </c>
       <c r="B6" t="s">
-        <v>337</v>
+        <v>335</v>
       </c>
     </row>
     <row r="8" spans="1:2" ht="12" customHeight="1">
       <c r="A8" t="s">
-        <v>338</v>
+        <v>336</v>
       </c>
       <c r="B8" t="s">
-        <v>339</v>
+        <v>337</v>
       </c>
     </row>
     <row r="9" spans="1:2" ht="12" customHeight="1">
       <c r="A9" t="s">
-        <v>340</v>
+        <v>338</v>
       </c>
       <c r="B9" t="s">
-        <v>341</v>
+        <v>339</v>
       </c>
     </row>
     <row r="10" spans="1:2" ht="12" customHeight="1">
       <c r="A10" t="s">
-        <v>342</v>
+        <v>340</v>
       </c>
       <c r="B10" t="s">
-        <v>343</v>
+        <v>341</v>
       </c>
     </row>
     <row r="11" spans="1:2" ht="12" customHeight="1">
       <c r="A11" t="s">
-        <v>344</v>
+        <v>342</v>
       </c>
       <c r="B11" t="s">
-        <v>345</v>
+        <v>343</v>
       </c>
     </row>
     <row r="12" spans="1:2" ht="12" customHeight="1">
       <c r="A12" t="s">
-        <v>346</v>
+        <v>344</v>
       </c>
       <c r="B12" t="s">
-        <v>347</v>
+        <v>345</v>
       </c>
     </row>
     <row r="13" spans="1:2" ht="12" customHeight="1">
       <c r="A13" t="s">
-        <v>348</v>
+        <v>346</v>
       </c>
       <c r="B13" t="s">
-        <v>349</v>
+        <v>347</v>
       </c>
     </row>
     <row r="14" spans="1:2" ht="42" customHeight="1">
       <c r="A14" t="s">
-        <v>350</v>
+        <v>348</v>
       </c>
       <c r="B14" t="s">
-        <v>351</v>
+        <v>349</v>
       </c>
     </row>
     <row r="15" spans="1:2" ht="12.75" customHeight="1">
       <c r="A15" t="s">
-        <v>352</v>
+        <v>350</v>
       </c>
       <c r="B15" t="s">
-        <v>353</v>
+        <v>351</v>
       </c>
     </row>
     <row r="16" spans="1:2" ht="12.75" customHeight="1">
       <c r="A16" t="s">
-        <v>354</v>
+        <v>352</v>
       </c>
       <c r="B16" t="s">
-        <v>355</v>
+        <v>353</v>
       </c>
     </row>
     <row r="17" spans="1:2" ht="12.75" customHeight="1">
       <c r="A17" t="s">
-        <v>356</v>
+        <v>354</v>
       </c>
       <c r="B17" t="s">
-        <v>357</v>
+        <v>355</v>
       </c>
     </row>
     <row r="18" spans="1:2" ht="12.75" customHeight="1">
       <c r="A18" t="s">
-        <v>358</v>
+        <v>356</v>
       </c>
       <c r="B18" t="s">
-        <v>359</v>
+        <v>357</v>
       </c>
     </row>
     <row r="19" spans="1:2" ht="12.75" customHeight="1">
       <c r="A19" t="s">
-        <v>360</v>
+        <v>358</v>
       </c>
       <c r="B19" t="s">
-        <v>361</v>
+        <v>359</v>
       </c>
     </row>
     <row r="20" spans="1:2" ht="12.75" customHeight="1">
       <c r="A20" t="s">
-        <v>362</v>
+        <v>360</v>
       </c>
       <c r="B20" t="s">
-        <v>363</v>
+        <v>361</v>
       </c>
     </row>
     <row r="21" spans="1:2" ht="12.75" customHeight="1">
       <c r="A21" t="s">
-        <v>364</v>
+        <v>362</v>
       </c>
       <c r="B21" t="s">
-        <v>365</v>
+        <v>363</v>
       </c>
     </row>
     <row r="22" spans="1:2" ht="12.75" customHeight="1">
       <c r="A22" t="s">
-        <v>366</v>
+        <v>364</v>
       </c>
       <c r="B22" t="s">
-        <v>367</v>
+        <v>365</v>
       </c>
     </row>
     <row r="24" spans="1:2" ht="12.75" customHeight="1">
       <c r="A24" t="s">
-        <v>368</v>
+        <v>366</v>
       </c>
       <c r="B24" t="s">
         <v>51</v>
@@ -6923,10 +6920,10 @@
     </row>
     <row r="25" spans="1:2" ht="12.75" customHeight="1">
       <c r="A25" t="s">
-        <v>369</v>
+        <v>367</v>
       </c>
       <c r="B25" t="s">
-        <v>370</v>
+        <v>368</v>
       </c>
     </row>
     <row r="26" spans="1:2" ht="12.75" customHeight="1">
@@ -6934,7 +6931,7 @@
         <v>39</v>
       </c>
       <c r="B26" t="s">
-        <v>371</v>
+        <v>369</v>
       </c>
     </row>
     <row r="27" spans="1:2" ht="12.75" customHeight="1">
@@ -6942,7 +6939,7 @@
         <v>38</v>
       </c>
       <c r="B27" t="s">
-        <v>372</v>
+        <v>370</v>
       </c>
     </row>
     <row r="28" spans="1:2" ht="12.75" customHeight="1">
@@ -7083,7 +7080,7 @@
         <v>9</v>
       </c>
       <c r="B2" t="s">
-        <v>387</v>
+        <v>385</v>
       </c>
     </row>
     <row r="3" spans="1:2" ht="12.75" customHeight="1">
@@ -7091,7 +7088,7 @@
         <v>10</v>
       </c>
       <c r="B3" t="s">
-        <v>388</v>
+        <v>386</v>
       </c>
     </row>
     <row r="4" spans="1:2" ht="12.75" customHeight="1">
@@ -7099,7 +7096,7 @@
         <v>11</v>
       </c>
       <c r="B4" t="s">
-        <v>387</v>
+        <v>385</v>
       </c>
     </row>
   </sheetData>
@@ -7127,15 +7124,15 @@
         <v>1</v>
       </c>
       <c r="B1" t="s">
-        <v>389</v>
+        <v>387</v>
       </c>
     </row>
     <row r="2" spans="1:2">
       <c r="A2" t="s">
-        <v>390</v>
+        <v>388</v>
       </c>
       <c r="B2" t="s">
-        <v>391</v>
+        <v>389</v>
       </c>
     </row>
     <row r="3" spans="1:2">
@@ -7143,15 +7140,15 @@
         <v>137</v>
       </c>
       <c r="B3" t="s">
-        <v>391</v>
+        <v>389</v>
       </c>
     </row>
     <row r="4" spans="1:2">
       <c r="A4" t="s">
-        <v>392</v>
+        <v>390</v>
       </c>
       <c r="B4" t="s">
-        <v>391</v>
+        <v>389</v>
       </c>
     </row>
   </sheetData>

</xml_diff>

<commit_message>
change UI-- background image, page-header, make the button more looks like button etc
</commit_message>
<xml_diff>
--- a/opendatakit.collect2/form-files/neonatal/neonatal.xlsx
+++ b/opendatakit.collect2/form-files/neonatal/neonatal.xlsx
@@ -1,10 +1,10 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
-  <fileVersion appName="xl" lastEdited="5" lowestEdited="5" rupBuild="22905"/>
+  <fileVersion appName="xl" lastEdited="5" lowestEdited="5" rupBuild="23416"/>
   <workbookPr autoCompressPictures="0"/>
   <bookViews>
-    <workbookView xWindow="1800" yWindow="0" windowWidth="18360" windowHeight="15280" tabRatio="500" activeTab="1"/>
+    <workbookView xWindow="1260" yWindow="760" windowWidth="23760" windowHeight="15560" tabRatio="500" activeTab="1"/>
   </bookViews>
   <sheets>
     <sheet name="survey" sheetId="1" r:id="rId1"/>
@@ -23,7 +23,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="869" uniqueCount="534">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="868" uniqueCount="534">
   <si>
     <t>type</t>
   </si>
@@ -448,22 +448,13 @@
     <t>procedures</t>
   </si>
   <si>
-    <t>img/procedure_icon.jpg</t>
-  </si>
-  <si>
     <t>calculators</t>
   </si>
   <si>
-    <t>img/calulators.jpg</t>
-  </si>
-  <si>
     <t>nutritions</t>
   </si>
   <si>
     <t>medications</t>
-  </si>
-  <si>
-    <t>img/med_icon.jpg</t>
   </si>
   <si>
     <t>procedures_menu</t>
@@ -1403,9 +1394,6 @@
     <t>Tools</t>
   </si>
   <si>
-    <t>img/tool_icon.jpg</t>
-  </si>
-  <si>
     <t>umbilicalV</t>
   </si>
   <si>
@@ -1832,6 +1820,18 @@
   </si>
   <si>
     <t>Head Sagital</t>
+  </si>
+  <si>
+    <t>img/PROCEDURES_ICON.png</t>
+  </si>
+  <si>
+    <t>img/TOOLS_ICON.png</t>
+  </si>
+  <si>
+    <t>img/MEDICINES_ICON.png</t>
+  </si>
+  <si>
+    <t>img/CALCULATORS_ICON.png</t>
   </si>
 </sst>
 </file>
@@ -3351,12 +3351,12 @@
     <row r="4" spans="1:10" s="35" customFormat="1" ht="15">
       <c r="A4" s="12"/>
       <c r="B4" s="33" t="s">
-        <v>371</v>
+        <v>368</v>
       </c>
       <c r="C4" s="33"/>
       <c r="D4" s="33"/>
       <c r="E4" s="33" t="s">
-        <v>372</v>
+        <v>369</v>
       </c>
       <c r="F4" s="33"/>
       <c r="G4" s="33"/>
@@ -3367,12 +3367,12 @@
     <row r="5" spans="1:10" ht="12">
       <c r="A5" s="12"/>
       <c r="B5" s="22" t="s">
-        <v>373</v>
+        <v>370</v>
       </c>
       <c r="C5" s="22"/>
       <c r="D5" s="22"/>
       <c r="E5" s="23" t="s">
-        <v>374</v>
+        <v>371</v>
       </c>
       <c r="F5" s="22"/>
       <c r="G5" s="22"/>
@@ -3380,10 +3380,10 @@
     </row>
     <row r="6" spans="1:10" ht="15">
       <c r="A6" s="7" t="s">
-        <v>498</v>
+        <v>494</v>
       </c>
       <c r="B6" s="8" t="s">
-        <v>375</v>
+        <v>372</v>
       </c>
       <c r="C6" s="8"/>
       <c r="D6" s="8"/>
@@ -3395,13 +3395,13 @@
     <row r="7" spans="1:10" ht="12">
       <c r="A7" s="7"/>
       <c r="B7" s="3" t="s">
-        <v>376</v>
+        <v>373</v>
       </c>
       <c r="C7" s="3" t="s">
-        <v>147</v>
+        <v>144</v>
       </c>
       <c r="D7" s="3" t="s">
-        <v>377</v>
+        <v>374</v>
       </c>
       <c r="E7" s="3"/>
       <c r="F7" s="3" t="s">
@@ -3418,7 +3418,7 @@
       <c r="C8" s="25"/>
       <c r="D8" s="25"/>
       <c r="E8" s="4" t="s">
-        <v>378</v>
+        <v>375</v>
       </c>
       <c r="F8" s="25"/>
       <c r="G8" s="12"/>
@@ -3436,7 +3436,7 @@
       <c r="G9" s="12"/>
       <c r="H9" s="12"/>
       <c r="I9" t="s">
-        <v>379</v>
+        <v>376</v>
       </c>
     </row>
     <row r="10" spans="1:10" ht="12.75" customHeight="1">
@@ -3445,7 +3445,7 @@
         <v>4</v>
       </c>
       <c r="D10" t="s">
-        <v>416</v>
+        <v>412</v>
       </c>
       <c r="E10" s="14"/>
     </row>
@@ -3455,7 +3455,7 @@
         <v>4</v>
       </c>
       <c r="H11" t="s">
-        <v>380</v>
+        <v>377</v>
       </c>
     </row>
     <row r="12" spans="1:10" ht="12">
@@ -3465,7 +3465,7 @@
       </c>
       <c r="C12" s="3"/>
       <c r="D12" s="27" t="s">
-        <v>417</v>
+        <v>413</v>
       </c>
       <c r="E12" s="3"/>
       <c r="F12" s="3"/>
@@ -3479,7 +3479,7 @@
       </c>
       <c r="C13" s="9"/>
       <c r="D13" s="29" t="s">
-        <v>418</v>
+        <v>414</v>
       </c>
       <c r="E13" s="29"/>
       <c r="F13" s="9"/>
@@ -3504,7 +3504,7 @@
       <c r="C15" s="25"/>
       <c r="D15" s="25"/>
       <c r="E15" s="4" t="s">
-        <v>384</v>
+        <v>381</v>
       </c>
     </row>
     <row r="16" spans="1:10" s="12" customFormat="1" ht="12">
@@ -3513,7 +3513,7 @@
         <v>4</v>
       </c>
       <c r="D16" s="12" t="s">
-        <v>415</v>
+        <v>411</v>
       </c>
     </row>
     <row r="17" spans="1:10" s="12" customFormat="1" ht="12">
@@ -3530,7 +3530,7 @@
       <c r="C18" s="25"/>
       <c r="D18" s="25"/>
       <c r="E18" s="4" t="s">
-        <v>395</v>
+        <v>391</v>
       </c>
     </row>
     <row r="19" spans="1:10" s="12" customFormat="1" ht="13" customHeight="1">
@@ -3540,7 +3540,7 @@
       </c>
       <c r="D19"/>
       <c r="I19" s="12" t="s">
-        <v>530</v>
+        <v>526</v>
       </c>
     </row>
     <row r="20" spans="1:10" s="12" customFormat="1" ht="12">
@@ -3552,7 +3552,7 @@
     <row r="21" spans="1:10" ht="15">
       <c r="A21" s="16"/>
       <c r="B21" s="8" t="s">
-        <v>381</v>
+        <v>378</v>
       </c>
       <c r="C21" s="30"/>
       <c r="D21" s="31"/>
@@ -3562,22 +3562,22 @@
     <row r="23" spans="1:10" s="15" customFormat="1" ht="12.75" customHeight="1">
       <c r="A23" s="37"/>
       <c r="B23" s="14" t="s">
-        <v>429</v>
+        <v>425</v>
       </c>
       <c r="E23" s="15" t="s">
-        <v>434</v>
+        <v>430</v>
       </c>
       <c r="I23" s="3"/>
       <c r="J23" s="3"/>
     </row>
     <row r="24" spans="1:10" ht="15">
       <c r="B24" s="14" t="s">
-        <v>430</v>
+        <v>426</v>
       </c>
       <c r="C24" s="15"/>
       <c r="D24" s="15"/>
       <c r="E24" s="15" t="s">
-        <v>433</v>
+        <v>429</v>
       </c>
       <c r="F24" s="15"/>
       <c r="G24" s="15"/>
@@ -3585,10 +3585,10 @@
     </row>
     <row r="25" spans="1:10" ht="15">
       <c r="A25" s="7" t="s">
-        <v>499</v>
+        <v>495</v>
       </c>
       <c r="B25" s="8" t="s">
-        <v>431</v>
+        <v>427</v>
       </c>
       <c r="C25" s="13"/>
       <c r="D25" s="13"/>
@@ -3600,13 +3600,13 @@
     <row r="26" spans="1:10" ht="12">
       <c r="A26" s="12"/>
       <c r="B26" s="3" t="s">
-        <v>435</v>
+        <v>431</v>
       </c>
       <c r="C26" s="3" t="s">
-        <v>436</v>
+        <v>432</v>
       </c>
       <c r="D26" s="3" t="s">
-        <v>391</v>
+        <v>388</v>
       </c>
       <c r="E26" s="3"/>
       <c r="F26" s="3" t="s">
@@ -3617,15 +3617,15 @@
     </row>
     <row r="27" spans="1:10" ht="12.75" customHeight="1">
       <c r="A27" s="7" t="s">
-        <v>439</v>
+        <v>435</v>
       </c>
       <c r="B27" s="40" t="s">
-        <v>442</v>
+        <v>438</v>
       </c>
       <c r="C27" s="40"/>
       <c r="D27" s="40"/>
       <c r="E27" s="40" t="s">
-        <v>493</v>
+        <v>489</v>
       </c>
       <c r="F27" s="40"/>
       <c r="G27" s="40"/>
@@ -3634,12 +3634,12 @@
     <row r="28" spans="1:10" ht="12.75" customHeight="1">
       <c r="A28" s="7"/>
       <c r="B28" s="40" t="s">
-        <v>443</v>
+        <v>439</v>
       </c>
       <c r="C28" s="40"/>
       <c r="D28" s="40"/>
       <c r="E28" s="40" t="s">
-        <v>494</v>
+        <v>490</v>
       </c>
       <c r="F28" s="40"/>
       <c r="G28" s="40"/>
@@ -3648,7 +3648,7 @@
     <row r="29" spans="1:10" s="3" customFormat="1" ht="18" customHeight="1">
       <c r="A29" s="41"/>
       <c r="B29" s="13" t="s">
-        <v>444</v>
+        <v>440</v>
       </c>
       <c r="C29" s="13"/>
       <c r="D29" s="13"/>
@@ -3660,13 +3660,13 @@
     <row r="30" spans="1:10" s="3" customFormat="1" ht="18" customHeight="1">
       <c r="A30" s="41"/>
       <c r="B30" t="s">
-        <v>445</v>
+        <v>441</v>
       </c>
       <c r="C30" t="s">
-        <v>152</v>
+        <v>149</v>
       </c>
       <c r="D30" t="s">
-        <v>439</v>
+        <v>435</v>
       </c>
       <c r="E30"/>
       <c r="F30" t="s">
@@ -3676,20 +3676,20 @@
     <row r="31" spans="1:10" ht="24">
       <c r="A31" s="7"/>
       <c r="B31" s="2" t="s">
-        <v>446</v>
+        <v>442</v>
       </c>
       <c r="C31" s="2" t="s">
-        <v>324</v>
+        <v>321</v>
       </c>
       <c r="D31" s="2" t="s">
-        <v>158</v>
+        <v>155</v>
       </c>
       <c r="E31" s="2" t="s">
-        <v>447</v>
+        <v>443</v>
       </c>
       <c r="F31" s="2"/>
       <c r="G31" t="s">
-        <v>448</v>
+        <v>444</v>
       </c>
     </row>
     <row r="32" spans="1:10" ht="18" customHeight="1">
@@ -3700,46 +3700,46 @@
       <c r="C32" s="2"/>
       <c r="D32" s="2"/>
       <c r="E32" s="2" t="s">
-        <v>449</v>
+        <v>445</v>
       </c>
       <c r="F32" s="2"/>
       <c r="I32" t="s">
-        <v>495</v>
+        <v>491</v>
       </c>
     </row>
     <row r="33" spans="1:9" ht="18" customHeight="1">
       <c r="A33" s="7"/>
       <c r="B33" s="2" t="s">
-        <v>450</v>
+        <v>446</v>
       </c>
       <c r="C33" s="19"/>
       <c r="D33" s="2" t="s">
-        <v>451</v>
+        <v>447</v>
       </c>
       <c r="E33" s="2" t="s">
-        <v>452</v>
+        <v>448</v>
       </c>
       <c r="F33" s="2"/>
     </row>
     <row r="34" spans="1:9" ht="18" customHeight="1">
       <c r="A34" s="7"/>
       <c r="B34" s="2" t="s">
-        <v>450</v>
+        <v>446</v>
       </c>
       <c r="C34" s="19"/>
       <c r="D34" s="2"/>
       <c r="E34" s="2" t="s">
-        <v>453</v>
+        <v>449</v>
       </c>
       <c r="F34" s="2"/>
       <c r="I34" t="s">
-        <v>531</v>
+        <v>527</v>
       </c>
     </row>
     <row r="35" spans="1:9" ht="15">
       <c r="A35" s="7"/>
       <c r="B35" s="8" t="s">
-        <v>492</v>
+        <v>488</v>
       </c>
       <c r="C35" s="8"/>
       <c r="D35" s="8"/>
@@ -3764,7 +3764,7 @@
       <c r="C37" s="15"/>
       <c r="D37" s="15"/>
       <c r="E37" s="15" t="s">
-        <v>496</v>
+        <v>492</v>
       </c>
       <c r="F37" s="15"/>
       <c r="G37" s="15"/>
@@ -3777,7 +3777,7 @@
       <c r="C38" s="15"/>
       <c r="D38" s="15"/>
       <c r="E38" s="15" t="s">
-        <v>497</v>
+        <v>493</v>
       </c>
       <c r="F38" s="15"/>
       <c r="G38" s="15"/>
@@ -3863,7 +3863,7 @@
         <v>24</v>
       </c>
       <c r="D45" t="s">
-        <v>419</v>
+        <v>415</v>
       </c>
     </row>
     <row r="46" spans="1:9" ht="12.75" customHeight="1">
@@ -3872,7 +3872,7 @@
         <v>4</v>
       </c>
       <c r="D46" t="s">
-        <v>408</v>
+        <v>404</v>
       </c>
       <c r="E46" t="s">
         <v>25</v>
@@ -3903,7 +3903,7 @@
         <v>27</v>
       </c>
       <c r="D49" t="s">
-        <v>420</v>
+        <v>416</v>
       </c>
     </row>
     <row r="50" spans="1:5" ht="12.75" customHeight="1">
@@ -3912,7 +3912,7 @@
         <v>4</v>
       </c>
       <c r="D50" t="s">
-        <v>409</v>
+        <v>405</v>
       </c>
       <c r="E50" t="s">
         <v>32</v>
@@ -3957,7 +3957,7 @@
         <v>63</v>
       </c>
       <c r="D55" t="s">
-        <v>421</v>
+        <v>417</v>
       </c>
     </row>
     <row r="56" spans="1:5" ht="12.75" customHeight="1">
@@ -3969,7 +3969,7 @@
         <v>64</v>
       </c>
       <c r="D56" t="s">
-        <v>422</v>
+        <v>418</v>
       </c>
     </row>
     <row r="57" spans="1:5" ht="12.75" customHeight="1">
@@ -3978,7 +3978,7 @@
         <v>4</v>
       </c>
       <c r="D57" t="s">
-        <v>410</v>
+        <v>406</v>
       </c>
       <c r="E57" t="s">
         <v>65</v>
@@ -4017,7 +4017,7 @@
         <v>68</v>
       </c>
       <c r="D61" t="s">
-        <v>423</v>
+        <v>419</v>
       </c>
     </row>
     <row r="62" spans="1:5" ht="12.75" customHeight="1">
@@ -4029,7 +4029,7 @@
         <v>69</v>
       </c>
       <c r="D62" t="s">
-        <v>424</v>
+        <v>420</v>
       </c>
     </row>
     <row r="63" spans="1:5" ht="12.75" customHeight="1">
@@ -4038,7 +4038,7 @@
         <v>4</v>
       </c>
       <c r="D63" t="s">
-        <v>411</v>
+        <v>407</v>
       </c>
       <c r="E63" t="s">
         <v>70</v>
@@ -4073,12 +4073,12 @@
     </row>
     <row r="67" spans="1:8" ht="12.75" customHeight="1">
       <c r="B67" s="14" t="s">
-        <v>502</v>
+        <v>498</v>
       </c>
       <c r="C67" s="15"/>
       <c r="D67" s="15"/>
       <c r="E67" s="15" t="s">
-        <v>506</v>
+        <v>502</v>
       </c>
       <c r="F67" s="15"/>
       <c r="G67" s="15"/>
@@ -4086,12 +4086,12 @@
     </row>
     <row r="68" spans="1:8" ht="12.75" customHeight="1">
       <c r="B68" s="14" t="s">
-        <v>503</v>
+        <v>499</v>
       </c>
       <c r="C68" s="15"/>
       <c r="D68" s="15"/>
       <c r="E68" s="15" t="s">
-        <v>507</v>
+        <v>503</v>
       </c>
       <c r="F68" s="15"/>
       <c r="G68" s="15"/>
@@ -4099,10 +4099,10 @@
     </row>
     <row r="69" spans="1:8" ht="12.75" customHeight="1">
       <c r="A69" s="7" t="s">
-        <v>508</v>
+        <v>504</v>
       </c>
       <c r="B69" s="8" t="s">
-        <v>504</v>
+        <v>500</v>
       </c>
       <c r="C69" s="13"/>
       <c r="D69" s="13"/>
@@ -4114,13 +4114,13 @@
     <row r="70" spans="1:8" ht="12.75" customHeight="1">
       <c r="A70" s="16"/>
       <c r="B70" t="s">
-        <v>509</v>
+        <v>505</v>
       </c>
       <c r="C70" t="s">
-        <v>510</v>
+        <v>506</v>
       </c>
       <c r="D70" t="s">
-        <v>508</v>
+        <v>504</v>
       </c>
       <c r="E70" s="42"/>
       <c r="F70" t="s">
@@ -4137,7 +4137,7 @@
       <c r="C71" s="32"/>
       <c r="D71" s="32"/>
       <c r="E71" t="s">
-        <v>516</v>
+        <v>512</v>
       </c>
       <c r="F71" s="32"/>
       <c r="G71" s="32"/>
@@ -4150,7 +4150,7 @@
       </c>
       <c r="C72" s="32"/>
       <c r="D72" s="43" t="s">
-        <v>513</v>
+        <v>509</v>
       </c>
       <c r="E72" s="32"/>
       <c r="F72" s="32"/>
@@ -4171,7 +4171,7 @@
       <c r="C74" s="32"/>
       <c r="D74" s="32"/>
       <c r="E74" t="s">
-        <v>515</v>
+        <v>511</v>
       </c>
       <c r="F74" s="32"/>
       <c r="G74" s="32"/>
@@ -4184,7 +4184,7 @@
       </c>
       <c r="C75" s="32"/>
       <c r="D75" s="43" t="s">
-        <v>514</v>
+        <v>510</v>
       </c>
       <c r="E75" s="32"/>
       <c r="F75" s="32"/>
@@ -4200,7 +4200,7 @@
     <row r="77" spans="1:8" ht="12.75" customHeight="1">
       <c r="A77" s="7"/>
       <c r="B77" s="8" t="s">
-        <v>505</v>
+        <v>501</v>
       </c>
       <c r="C77" s="13"/>
       <c r="D77" s="13"/>
@@ -4220,12 +4220,12 @@
     </row>
     <row r="79" spans="1:8" ht="12.75" customHeight="1">
       <c r="B79" s="14" t="s">
-        <v>518</v>
+        <v>514</v>
       </c>
       <c r="C79" s="15"/>
       <c r="D79" s="15"/>
       <c r="E79" s="15" t="s">
-        <v>523</v>
+        <v>519</v>
       </c>
       <c r="F79" s="15"/>
       <c r="G79" s="15"/>
@@ -4233,12 +4233,12 @@
     </row>
     <row r="80" spans="1:8" ht="12.75" customHeight="1">
       <c r="B80" s="14" t="s">
-        <v>519</v>
+        <v>515</v>
       </c>
       <c r="C80" s="15"/>
       <c r="D80" s="15"/>
       <c r="E80" s="15" t="s">
-        <v>524</v>
+        <v>520</v>
       </c>
       <c r="F80" s="15"/>
       <c r="G80" s="15"/>
@@ -4246,10 +4246,10 @@
     </row>
     <row r="81" spans="1:8" ht="12.75" customHeight="1">
       <c r="A81" s="7" t="s">
-        <v>517</v>
+        <v>513</v>
       </c>
       <c r="B81" s="8" t="s">
-        <v>520</v>
+        <v>516</v>
       </c>
       <c r="C81" s="13"/>
       <c r="D81" s="13"/>
@@ -4261,13 +4261,13 @@
     <row r="82" spans="1:8" ht="12.75" customHeight="1">
       <c r="A82" s="16"/>
       <c r="B82" t="s">
+        <v>517</v>
+      </c>
+      <c r="C82" t="s">
         <v>521</v>
       </c>
-      <c r="C82" t="s">
-        <v>525</v>
-      </c>
       <c r="D82" t="s">
-        <v>441</v>
+        <v>437</v>
       </c>
       <c r="E82" s="42"/>
       <c r="F82" t="s">
@@ -4279,211 +4279,211 @@
     <row r="83" spans="1:8" ht="12">
       <c r="A83" s="7"/>
       <c r="B83" s="45" t="s">
-        <v>390</v>
+        <v>387</v>
       </c>
       <c r="C83" s="45" t="s">
-        <v>454</v>
+        <v>450</v>
       </c>
       <c r="E83" s="2" t="s">
-        <v>529</v>
+        <v>525</v>
       </c>
     </row>
     <row r="84" spans="1:8" ht="11" customHeight="1">
       <c r="A84" s="7"/>
       <c r="B84" t="s">
-        <v>455</v>
+        <v>451</v>
       </c>
       <c r="C84" t="s">
-        <v>159</v>
+        <v>156</v>
       </c>
       <c r="D84" t="s">
-        <v>456</v>
+        <v>452</v>
       </c>
       <c r="E84" s="2" t="s">
-        <v>457</v>
+        <v>453</v>
       </c>
       <c r="F84" t="s">
-        <v>458</v>
+        <v>454</v>
       </c>
     </row>
     <row r="85" spans="1:8" ht="11" customHeight="1">
       <c r="A85" s="7"/>
       <c r="B85" t="s">
-        <v>459</v>
+        <v>455</v>
       </c>
       <c r="C85" t="s">
-        <v>170</v>
+        <v>167</v>
       </c>
       <c r="D85" t="s">
-        <v>460</v>
+        <v>456</v>
       </c>
       <c r="E85" s="2" t="s">
-        <v>461</v>
+        <v>457</v>
       </c>
       <c r="F85" t="s">
-        <v>458</v>
+        <v>454</v>
       </c>
     </row>
     <row r="86" spans="1:8" ht="11" customHeight="1">
       <c r="A86" s="7"/>
       <c r="B86" t="s">
-        <v>462</v>
+        <v>458</v>
       </c>
       <c r="C86" t="s">
-        <v>183</v>
+        <v>180</v>
       </c>
       <c r="D86" t="s">
-        <v>463</v>
+        <v>459</v>
       </c>
       <c r="E86" s="2" t="s">
-        <v>464</v>
+        <v>460</v>
       </c>
       <c r="F86" t="s">
-        <v>458</v>
+        <v>454</v>
       </c>
     </row>
     <row r="87" spans="1:8" ht="11" customHeight="1">
       <c r="A87" s="7"/>
       <c r="B87" t="s">
-        <v>465</v>
+        <v>461</v>
       </c>
       <c r="C87" t="s">
-        <v>194</v>
+        <v>191</v>
       </c>
       <c r="D87" t="s">
-        <v>466</v>
+        <v>462</v>
       </c>
       <c r="E87" s="2" t="s">
-        <v>467</v>
+        <v>463</v>
       </c>
       <c r="F87" t="s">
-        <v>458</v>
+        <v>454</v>
       </c>
     </row>
     <row r="88" spans="1:8" ht="11" customHeight="1">
       <c r="A88" s="7"/>
       <c r="B88" t="s">
-        <v>468</v>
+        <v>464</v>
       </c>
       <c r="C88" t="s">
-        <v>209</v>
+        <v>206</v>
       </c>
       <c r="D88" t="s">
-        <v>469</v>
+        <v>465</v>
       </c>
       <c r="E88" s="2" t="s">
-        <v>470</v>
+        <v>466</v>
       </c>
       <c r="F88" t="s">
-        <v>458</v>
+        <v>454</v>
       </c>
     </row>
     <row r="89" spans="1:8" ht="11" customHeight="1">
       <c r="A89" s="7"/>
       <c r="B89" t="s">
-        <v>471</v>
+        <v>467</v>
       </c>
       <c r="C89" t="s">
-        <v>222</v>
+        <v>219</v>
       </c>
       <c r="D89" t="s">
-        <v>472</v>
+        <v>468</v>
       </c>
       <c r="E89" s="2" t="s">
-        <v>473</v>
+        <v>469</v>
       </c>
       <c r="F89" t="s">
-        <v>458</v>
+        <v>454</v>
       </c>
     </row>
     <row r="90" spans="1:8" ht="11" customHeight="1">
       <c r="A90" s="7"/>
       <c r="B90" t="s">
-        <v>474</v>
+        <v>470</v>
       </c>
       <c r="C90" t="s">
-        <v>235</v>
+        <v>232</v>
       </c>
       <c r="D90" t="s">
-        <v>475</v>
+        <v>471</v>
       </c>
       <c r="E90" s="2" t="s">
-        <v>476</v>
+        <v>472</v>
       </c>
     </row>
     <row r="91" spans="1:8" ht="11" customHeight="1">
       <c r="A91" s="7"/>
       <c r="B91" t="s">
-        <v>477</v>
+        <v>473</v>
       </c>
       <c r="C91" t="s">
-        <v>250</v>
+        <v>247</v>
       </c>
       <c r="D91" t="s">
-        <v>478</v>
+        <v>474</v>
       </c>
       <c r="E91" s="2" t="s">
-        <v>479</v>
+        <v>475</v>
       </c>
     </row>
     <row r="92" spans="1:8" ht="11" customHeight="1">
       <c r="A92" s="7"/>
       <c r="B92" t="s">
-        <v>480</v>
+        <v>476</v>
       </c>
       <c r="C92" t="s">
-        <v>263</v>
+        <v>260</v>
       </c>
       <c r="D92" t="s">
-        <v>481</v>
+        <v>477</v>
       </c>
       <c r="E92" s="2" t="s">
-        <v>482</v>
+        <v>478</v>
       </c>
     </row>
     <row r="93" spans="1:8" ht="11" customHeight="1">
       <c r="A93" s="7"/>
       <c r="B93" t="s">
-        <v>483</v>
+        <v>479</v>
       </c>
       <c r="C93" t="s">
-        <v>278</v>
+        <v>275</v>
       </c>
       <c r="D93" t="s">
-        <v>484</v>
+        <v>480</v>
       </c>
       <c r="E93" s="2" t="s">
-        <v>485</v>
+        <v>481</v>
       </c>
     </row>
     <row r="94" spans="1:8" ht="11" customHeight="1">
       <c r="A94" s="7"/>
       <c r="B94" t="s">
-        <v>486</v>
+        <v>482</v>
       </c>
       <c r="C94" t="s">
-        <v>291</v>
+        <v>288</v>
       </c>
       <c r="D94" t="s">
-        <v>487</v>
+        <v>483</v>
       </c>
       <c r="E94" s="2" t="s">
-        <v>488</v>
+        <v>484</v>
       </c>
     </row>
     <row r="95" spans="1:8" ht="12" customHeight="1">
       <c r="A95" s="7"/>
       <c r="B95" t="s">
-        <v>489</v>
+        <v>485</v>
       </c>
       <c r="C95" t="s">
-        <v>306</v>
+        <v>303</v>
       </c>
       <c r="D95" t="s">
-        <v>490</v>
+        <v>486</v>
       </c>
       <c r="E95" s="2" t="s">
-        <v>491</v>
+        <v>487</v>
       </c>
     </row>
     <row r="96" spans="1:8" ht="12.75" customHeight="1">
@@ -4528,7 +4528,7 @@
         <v>14</v>
       </c>
       <c r="E102" t="s">
-        <v>527</v>
+        <v>523</v>
       </c>
     </row>
     <row r="103" spans="1:9" ht="24">
@@ -4570,7 +4570,7 @@
         <v>24</v>
       </c>
       <c r="D106" t="s">
-        <v>419</v>
+        <v>415</v>
       </c>
     </row>
     <row r="107" spans="1:9" ht="12.75" customHeight="1">
@@ -4579,7 +4579,7 @@
         <v>4</v>
       </c>
       <c r="D107" t="s">
-        <v>408</v>
+        <v>404</v>
       </c>
       <c r="E107" t="s">
         <v>25</v>
@@ -4610,7 +4610,7 @@
         <v>27</v>
       </c>
       <c r="D110" t="s">
-        <v>420</v>
+        <v>416</v>
       </c>
     </row>
     <row r="111" spans="1:9" ht="12.75" customHeight="1">
@@ -4619,7 +4619,7 @@
         <v>4</v>
       </c>
       <c r="D111" t="s">
-        <v>409</v>
+        <v>405</v>
       </c>
       <c r="E111" t="s">
         <v>32</v>
@@ -4643,7 +4643,7 @@
         <v>14</v>
       </c>
       <c r="E114" t="s">
-        <v>528</v>
+        <v>524</v>
       </c>
     </row>
     <row r="115" spans="1:10" ht="12.75" customHeight="1">
@@ -4664,7 +4664,7 @@
         <v>48</v>
       </c>
       <c r="D116" t="s">
-        <v>425</v>
+        <v>421</v>
       </c>
     </row>
     <row r="117" spans="1:10" ht="12.75" customHeight="1">
@@ -4673,7 +4673,7 @@
         <v>4</v>
       </c>
       <c r="D117" t="s">
-        <v>426</v>
+        <v>422</v>
       </c>
     </row>
     <row r="118" spans="1:10" ht="12.75" customHeight="1">
@@ -4685,7 +4685,7 @@
         <v>43</v>
       </c>
       <c r="D118" t="s">
-        <v>427</v>
+        <v>423</v>
       </c>
     </row>
     <row r="119" spans="1:10" ht="12.75" customHeight="1">
@@ -4697,7 +4697,7 @@
         <v>44</v>
       </c>
       <c r="D119" t="s">
-        <v>428</v>
+        <v>424</v>
       </c>
     </row>
     <row r="120" spans="1:10" ht="12.75" customHeight="1">
@@ -4706,7 +4706,7 @@
         <v>4</v>
       </c>
       <c r="D120" t="s">
-        <v>412</v>
+        <v>408</v>
       </c>
       <c r="E120" t="s">
         <v>73</v>
@@ -4718,7 +4718,7 @@
         <v>4</v>
       </c>
       <c r="D121" t="s">
-        <v>413</v>
+        <v>409</v>
       </c>
       <c r="E121" t="s">
         <v>45</v>
@@ -4733,7 +4733,7 @@
     <row r="123" spans="1:10" ht="20" customHeight="1">
       <c r="A123" s="7"/>
       <c r="B123" s="8" t="s">
-        <v>522</v>
+        <v>518</v>
       </c>
       <c r="C123" s="13"/>
       <c r="D123" s="13"/>
@@ -4745,7 +4745,7 @@
     <row r="124" spans="1:10" ht="15">
       <c r="A124" s="16"/>
       <c r="B124" s="8" t="s">
-        <v>432</v>
+        <v>428</v>
       </c>
       <c r="C124" s="30"/>
       <c r="D124" s="31"/>
@@ -4755,22 +4755,22 @@
     <row r="126" spans="1:10" s="15" customFormat="1" ht="12.75" customHeight="1">
       <c r="A126" s="37"/>
       <c r="B126" s="14" t="s">
-        <v>396</v>
+        <v>392</v>
       </c>
       <c r="E126" s="15" t="s">
-        <v>397</v>
+        <v>393</v>
       </c>
       <c r="I126" s="3"/>
       <c r="J126" s="3"/>
     </row>
     <row r="127" spans="1:10" ht="12.75" customHeight="1">
       <c r="B127" s="14" t="s">
-        <v>398</v>
+        <v>394</v>
       </c>
       <c r="C127" s="15"/>
       <c r="D127" s="15"/>
       <c r="E127" s="15" t="s">
-        <v>399</v>
+        <v>395</v>
       </c>
       <c r="F127" s="15"/>
       <c r="G127" s="15"/>
@@ -4778,7 +4778,7 @@
     </row>
     <row r="128" spans="1:10" ht="15">
       <c r="A128" s="7" t="s">
-        <v>500</v>
+        <v>496</v>
       </c>
       <c r="B128" s="8" t="s">
         <v>75</v>
@@ -4845,7 +4845,7 @@
         <v>116</v>
       </c>
       <c r="D134" t="s">
-        <v>419</v>
+        <v>415</v>
       </c>
     </row>
     <row r="135" spans="1:9" ht="61" customHeight="1">
@@ -4854,7 +4854,7 @@
         <v>4</v>
       </c>
       <c r="D135" t="s">
-        <v>400</v>
+        <v>396</v>
       </c>
       <c r="E135" t="s">
         <v>117</v>
@@ -4914,7 +4914,7 @@
         <v>118</v>
       </c>
       <c r="D141" t="s">
-        <v>419</v>
+        <v>415</v>
       </c>
     </row>
     <row r="142" spans="1:9" ht="75" customHeight="1">
@@ -4923,7 +4923,7 @@
         <v>4</v>
       </c>
       <c r="D142" t="s">
-        <v>401</v>
+        <v>397</v>
       </c>
       <c r="E142" t="s">
         <v>119</v>
@@ -4935,7 +4935,7 @@
         <v>4</v>
       </c>
       <c r="D143" t="s">
-        <v>402</v>
+        <v>398</v>
       </c>
       <c r="E143" t="s">
         <v>119</v>
@@ -4947,7 +4947,7 @@
         <v>4</v>
       </c>
       <c r="D144" t="s">
-        <v>403</v>
+        <v>399</v>
       </c>
       <c r="E144" t="s">
         <v>119</v>
@@ -5004,7 +5004,7 @@
         <v>4</v>
       </c>
       <c r="D150" t="s">
-        <v>414</v>
+        <v>410</v>
       </c>
     </row>
     <row r="151" spans="1:9" ht="12.75" customHeight="1">
@@ -5028,30 +5028,30 @@
     <row r="154" spans="1:9" s="14" customFormat="1" ht="15">
       <c r="A154" s="28"/>
       <c r="B154" s="14" t="s">
-        <v>404</v>
+        <v>400</v>
       </c>
       <c r="C154" s="38"/>
       <c r="D154" s="39"/>
       <c r="E154" s="15" t="s">
-        <v>405</v>
+        <v>401</v>
       </c>
       <c r="F154" s="38"/>
     </row>
     <row r="155" spans="1:9" s="14" customFormat="1" ht="15">
       <c r="A155" s="28"/>
       <c r="B155" s="14" t="s">
-        <v>406</v>
+        <v>402</v>
       </c>
       <c r="C155" s="38"/>
       <c r="D155" s="39"/>
       <c r="E155" s="15" t="s">
-        <v>407</v>
+        <v>403</v>
       </c>
       <c r="F155" s="38"/>
     </row>
     <row r="156" spans="1:9" ht="15">
       <c r="A156" s="7" t="s">
-        <v>501</v>
+        <v>497</v>
       </c>
       <c r="B156" s="8" t="s">
         <v>54</v>
@@ -5129,7 +5129,7 @@
         <v>24</v>
       </c>
       <c r="D162" t="s">
-        <v>419</v>
+        <v>415</v>
       </c>
     </row>
     <row r="163" spans="1:9" ht="12.75" customHeight="1">
@@ -5138,7 +5138,7 @@
         <v>4</v>
       </c>
       <c r="D163" t="s">
-        <v>408</v>
+        <v>404</v>
       </c>
       <c r="E163" t="s">
         <v>25</v>
@@ -5169,7 +5169,7 @@
         <v>27</v>
       </c>
       <c r="D166" t="s">
-        <v>420</v>
+        <v>416</v>
       </c>
     </row>
     <row r="167" spans="1:9" ht="12.75" customHeight="1">
@@ -5178,7 +5178,7 @@
         <v>4</v>
       </c>
       <c r="D167" t="s">
-        <v>409</v>
+        <v>405</v>
       </c>
       <c r="E167" t="s">
         <v>32</v>
@@ -5223,7 +5223,7 @@
         <v>63</v>
       </c>
       <c r="D172" t="s">
-        <v>421</v>
+        <v>417</v>
       </c>
     </row>
     <row r="173" spans="1:9" ht="12.75" customHeight="1">
@@ -5235,7 +5235,7 @@
         <v>64</v>
       </c>
       <c r="D173" t="s">
-        <v>422</v>
+        <v>418</v>
       </c>
     </row>
     <row r="174" spans="1:9" ht="12.75" customHeight="1">
@@ -5244,7 +5244,7 @@
         <v>4</v>
       </c>
       <c r="D174" t="s">
-        <v>410</v>
+        <v>406</v>
       </c>
       <c r="E174" t="s">
         <v>65</v>
@@ -5283,7 +5283,7 @@
         <v>68</v>
       </c>
       <c r="D178" t="s">
-        <v>423</v>
+        <v>419</v>
       </c>
     </row>
     <row r="179" spans="1:8" ht="12.75" customHeight="1">
@@ -5295,7 +5295,7 @@
         <v>69</v>
       </c>
       <c r="D179" t="s">
-        <v>424</v>
+        <v>420</v>
       </c>
     </row>
     <row r="180" spans="1:8" ht="12.75" customHeight="1">
@@ -5304,7 +5304,7 @@
         <v>4</v>
       </c>
       <c r="D180" t="s">
-        <v>411</v>
+        <v>407</v>
       </c>
       <c r="E180" t="s">
         <v>70</v>
@@ -5343,7 +5343,7 @@
         <v>48</v>
       </c>
       <c r="D184" t="s">
-        <v>425</v>
+        <v>421</v>
       </c>
     </row>
     <row r="185" spans="1:8" ht="12.75" customHeight="1">
@@ -5352,7 +5352,7 @@
         <v>4</v>
       </c>
       <c r="D185" t="s">
-        <v>426</v>
+        <v>422</v>
       </c>
     </row>
     <row r="186" spans="1:8" ht="12.75" customHeight="1">
@@ -5364,7 +5364,7 @@
         <v>43</v>
       </c>
       <c r="D186" t="s">
-        <v>427</v>
+        <v>423</v>
       </c>
     </row>
     <row r="187" spans="1:8" ht="12.75" customHeight="1">
@@ -5376,7 +5376,7 @@
         <v>44</v>
       </c>
       <c r="D187" t="s">
-        <v>428</v>
+        <v>424</v>
       </c>
     </row>
     <row r="188" spans="1:8" ht="12.75" customHeight="1">
@@ -5385,7 +5385,7 @@
         <v>4</v>
       </c>
       <c r="D188" t="s">
-        <v>412</v>
+        <v>408</v>
       </c>
       <c r="E188" t="s">
         <v>73</v>
@@ -5397,7 +5397,7 @@
         <v>4</v>
       </c>
       <c r="D189" t="s">
-        <v>413</v>
+        <v>409</v>
       </c>
       <c r="E189" t="s">
         <v>45</v>
@@ -5423,7 +5423,7 @@
     </row>
     <row r="194" spans="2:2" ht="12.75" customHeight="1">
       <c r="B194" s="36" t="s">
-        <v>383</v>
+        <v>380</v>
       </c>
     </row>
   </sheetData>
@@ -5442,7 +5442,7 @@
   <dimension ref="A1:D139"/>
   <sheetViews>
     <sheetView tabSelected="1" zoomScale="150" zoomScaleNormal="150" zoomScalePageLayoutView="150" workbookViewId="0">
-      <selection activeCell="D16" sqref="D16"/>
+      <selection activeCell="C3" sqref="C3"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultColWidth="17.1640625" defaultRowHeight="12.75" customHeight="1" x14ac:dyDescent="0"/>
@@ -5469,7 +5469,7 @@
         <v>140</v>
       </c>
       <c r="D2" t="s">
-        <v>141</v>
+        <v>530</v>
       </c>
     </row>
     <row r="3" spans="1:4" ht="12.75" customHeight="1">
@@ -5477,13 +5477,10 @@
         <v>137</v>
       </c>
       <c r="B3" t="s">
-        <v>382</v>
-      </c>
-      <c r="C3" t="s">
-        <v>391</v>
+        <v>379</v>
       </c>
       <c r="D3" t="s">
-        <v>392</v>
+        <v>531</v>
       </c>
     </row>
     <row r="4" spans="1:4" ht="12.75" customHeight="1">
@@ -5491,10 +5488,10 @@
         <v>137</v>
       </c>
       <c r="B4" t="s">
-        <v>145</v>
+        <v>143</v>
       </c>
       <c r="D4" t="s">
-        <v>146</v>
+        <v>532</v>
       </c>
     </row>
     <row r="5" spans="1:4" ht="12.75" customHeight="1">
@@ -5502,62 +5499,62 @@
         <v>137</v>
       </c>
       <c r="B5" t="s">
-        <v>142</v>
+        <v>141</v>
       </c>
       <c r="D5" t="s">
-        <v>143</v>
+        <v>533</v>
       </c>
     </row>
     <row r="7" spans="1:4" ht="12.75" customHeight="1">
       <c r="A7" t="s">
-        <v>147</v>
+        <v>144</v>
       </c>
       <c r="B7" t="s">
-        <v>148</v>
+        <v>145</v>
       </c>
       <c r="C7" t="s">
-        <v>149</v>
+        <v>146</v>
       </c>
     </row>
     <row r="8" spans="1:4" ht="12.75" customHeight="1">
       <c r="A8" t="s">
+        <v>144</v>
+      </c>
+      <c r="B8" t="s">
         <v>147</v>
       </c>
-      <c r="B8" t="s">
-        <v>150</v>
-      </c>
       <c r="C8" t="s">
-        <v>151</v>
+        <v>148</v>
       </c>
     </row>
     <row r="9" spans="1:4" ht="12.75" customHeight="1">
       <c r="A9" t="s">
-        <v>147</v>
+        <v>144</v>
       </c>
       <c r="B9" t="s">
-        <v>393</v>
+        <v>389</v>
       </c>
       <c r="C9" t="s">
-        <v>394</v>
+        <v>390</v>
       </c>
     </row>
     <row r="11" spans="1:4" ht="12.75" customHeight="1">
       <c r="A11" t="s">
-        <v>436</v>
+        <v>432</v>
       </c>
       <c r="B11" t="s">
         <v>139</v>
       </c>
       <c r="C11" t="s">
-        <v>439</v>
+        <v>435</v>
       </c>
     </row>
     <row r="12" spans="1:4" ht="12.75" customHeight="1">
       <c r="A12" t="s">
-        <v>436</v>
+        <v>432</v>
       </c>
       <c r="B12" t="s">
-        <v>144</v>
+        <v>142</v>
       </c>
       <c r="C12" t="s">
         <v>82</v>
@@ -5565,68 +5562,68 @@
     </row>
     <row r="13" spans="1:4" ht="12.75" customHeight="1">
       <c r="A13" t="s">
+        <v>432</v>
+      </c>
+      <c r="B13" t="s">
+        <v>433</v>
+      </c>
+      <c r="C13" t="s">
         <v>436</v>
-      </c>
-      <c r="B13" t="s">
-        <v>437</v>
-      </c>
-      <c r="C13" t="s">
-        <v>440</v>
       </c>
     </row>
     <row r="14" spans="1:4" ht="12.75" customHeight="1">
       <c r="A14" t="s">
-        <v>436</v>
+        <v>432</v>
       </c>
       <c r="B14" t="s">
-        <v>438</v>
+        <v>434</v>
       </c>
       <c r="C14" t="s">
-        <v>441</v>
+        <v>437</v>
       </c>
     </row>
     <row r="16" spans="1:4" ht="12.75" customHeight="1">
       <c r="A16" t="s">
-        <v>152</v>
+        <v>149</v>
       </c>
       <c r="B16" t="s">
-        <v>153</v>
+        <v>150</v>
       </c>
       <c r="C16" t="s">
-        <v>533</v>
+        <v>529</v>
       </c>
     </row>
     <row r="17" spans="1:3" ht="12.75" customHeight="1">
       <c r="A17" t="s">
-        <v>152</v>
+        <v>149</v>
       </c>
       <c r="B17" t="s">
-        <v>154</v>
+        <v>151</v>
       </c>
       <c r="C17" t="s">
-        <v>451</v>
+        <v>447</v>
       </c>
     </row>
     <row r="18" spans="1:3" ht="12.75" customHeight="1">
       <c r="A18" t="s">
+        <v>149</v>
+      </c>
+      <c r="B18" t="s">
         <v>152</v>
       </c>
-      <c r="B18" t="s">
-        <v>155</v>
-      </c>
       <c r="C18" t="s">
-        <v>532</v>
+        <v>528</v>
       </c>
     </row>
     <row r="19" spans="1:3" ht="12.75" customHeight="1">
       <c r="A19" t="s">
-        <v>152</v>
+        <v>149</v>
       </c>
       <c r="B19" t="s">
-        <v>157</v>
+        <v>154</v>
       </c>
       <c r="C19" t="s">
-        <v>158</v>
+        <v>155</v>
       </c>
     </row>
     <row r="21" spans="1:3" ht="12.75" customHeight="1">
@@ -5785,40 +5782,40 @@
     </row>
     <row r="39" spans="1:4" ht="12.75" customHeight="1">
       <c r="A39" t="s">
-        <v>510</v>
+        <v>506</v>
       </c>
       <c r="B39" t="s">
-        <v>511</v>
+        <v>507</v>
       </c>
       <c r="C39" t="s">
-        <v>513</v>
+        <v>509</v>
       </c>
     </row>
     <row r="40" spans="1:4" ht="12.75" customHeight="1">
       <c r="A40" t="s">
+        <v>506</v>
+      </c>
+      <c r="B40" t="s">
+        <v>508</v>
+      </c>
+      <c r="C40" t="s">
         <v>510</v>
-      </c>
-      <c r="B40" t="s">
-        <v>512</v>
-      </c>
-      <c r="C40" t="s">
-        <v>514</v>
       </c>
     </row>
     <row r="42" spans="1:4" ht="12.75" customHeight="1">
       <c r="A42" t="s">
-        <v>525</v>
+        <v>521</v>
       </c>
       <c r="B42" t="s">
-        <v>156</v>
+        <v>153</v>
       </c>
       <c r="C42" t="s">
-        <v>526</v>
+        <v>522</v>
       </c>
     </row>
     <row r="43" spans="1:4" ht="12.75" customHeight="1">
       <c r="A43" t="s">
-        <v>525</v>
+        <v>521</v>
       </c>
       <c r="B43" t="s">
         <v>91</v>
@@ -5829,7 +5826,7 @@
     </row>
     <row r="44" spans="1:4" ht="12.75" customHeight="1">
       <c r="A44" t="s">
-        <v>525</v>
+        <v>521</v>
       </c>
       <c r="B44" t="s">
         <v>97</v>
@@ -5840,882 +5837,882 @@
     </row>
     <row r="46" spans="1:4" ht="12.75" customHeight="1">
       <c r="A46" t="s">
-        <v>159</v>
+        <v>156</v>
       </c>
       <c r="B46" t="s">
-        <v>160</v>
+        <v>157</v>
       </c>
       <c r="D46" t="s">
-        <v>161</v>
+        <v>158</v>
       </c>
     </row>
     <row r="47" spans="1:4" ht="12.75" customHeight="1">
       <c r="A47" t="s">
+        <v>156</v>
+      </c>
+      <c r="B47" t="s">
         <v>159</v>
       </c>
-      <c r="B47" t="s">
-        <v>162</v>
-      </c>
       <c r="D47" t="s">
-        <v>163</v>
+        <v>160</v>
       </c>
     </row>
     <row r="48" spans="1:4" ht="12.75" customHeight="1">
       <c r="A48" t="s">
-        <v>159</v>
+        <v>156</v>
       </c>
       <c r="B48" t="s">
-        <v>164</v>
+        <v>161</v>
       </c>
       <c r="D48" t="s">
-        <v>165</v>
+        <v>162</v>
       </c>
     </row>
     <row r="49" spans="1:4" ht="12.75" customHeight="1">
       <c r="A49" t="s">
-        <v>159</v>
+        <v>156</v>
       </c>
       <c r="B49" t="s">
-        <v>166</v>
+        <v>163</v>
       </c>
       <c r="D49" t="s">
-        <v>167</v>
+        <v>164</v>
       </c>
     </row>
     <row r="50" spans="1:4" ht="12.75" customHeight="1">
       <c r="A50" t="s">
-        <v>159</v>
+        <v>156</v>
       </c>
       <c r="B50" t="s">
-        <v>168</v>
+        <v>165</v>
       </c>
       <c r="D50" t="s">
-        <v>169</v>
+        <v>166</v>
       </c>
     </row>
     <row r="52" spans="1:4" ht="12.75" customHeight="1">
       <c r="A52" t="s">
-        <v>170</v>
+        <v>167</v>
       </c>
       <c r="B52" t="s">
-        <v>171</v>
+        <v>168</v>
       </c>
       <c r="D52" t="s">
-        <v>172</v>
+        <v>169</v>
       </c>
     </row>
     <row r="53" spans="1:4" s="2" customFormat="1" ht="12.75" customHeight="1">
       <c r="A53" t="s">
+        <v>167</v>
+      </c>
+      <c r="B53" t="s">
         <v>170</v>
       </c>
-      <c r="B53" t="s">
-        <v>173</v>
-      </c>
       <c r="D53" t="s">
-        <v>174</v>
+        <v>171</v>
       </c>
     </row>
     <row r="54" spans="1:4" ht="12.75" customHeight="1">
       <c r="A54" t="s">
-        <v>170</v>
+        <v>167</v>
       </c>
       <c r="B54" t="s">
-        <v>175</v>
+        <v>172</v>
       </c>
       <c r="D54" t="s">
-        <v>176</v>
+        <v>173</v>
       </c>
     </row>
     <row r="55" spans="1:4" ht="12.75" customHeight="1">
       <c r="A55" t="s">
-        <v>170</v>
+        <v>167</v>
       </c>
       <c r="B55" t="s">
-        <v>177</v>
+        <v>174</v>
       </c>
       <c r="D55" t="s">
-        <v>178</v>
+        <v>175</v>
       </c>
     </row>
     <row r="56" spans="1:4" ht="12.75" customHeight="1">
       <c r="A56" t="s">
-        <v>170</v>
+        <v>167</v>
       </c>
       <c r="B56" t="s">
-        <v>179</v>
+        <v>176</v>
       </c>
       <c r="D56" t="s">
-        <v>180</v>
+        <v>177</v>
       </c>
     </row>
     <row r="57" spans="1:4" ht="12.75" customHeight="1">
       <c r="A57" t="s">
-        <v>170</v>
+        <v>167</v>
       </c>
       <c r="B57" t="s">
-        <v>181</v>
+        <v>178</v>
       </c>
       <c r="D57" t="s">
-        <v>182</v>
+        <v>179</v>
       </c>
     </row>
     <row r="59" spans="1:4" ht="12.75" customHeight="1">
       <c r="A59" t="s">
-        <v>183</v>
+        <v>180</v>
       </c>
       <c r="B59" t="s">
-        <v>184</v>
+        <v>181</v>
       </c>
       <c r="C59" s="2"/>
       <c r="D59" t="s">
-        <v>185</v>
+        <v>182</v>
       </c>
     </row>
     <row r="60" spans="1:4" ht="12.75" customHeight="1">
       <c r="A60" t="s">
+        <v>180</v>
+      </c>
+      <c r="B60" t="s">
         <v>183</v>
       </c>
-      <c r="B60" t="s">
-        <v>186</v>
-      </c>
       <c r="D60" t="s">
-        <v>187</v>
+        <v>184</v>
       </c>
     </row>
     <row r="61" spans="1:4" ht="12.75" customHeight="1">
       <c r="A61" t="s">
-        <v>183</v>
+        <v>180</v>
       </c>
       <c r="B61" t="s">
-        <v>188</v>
+        <v>185</v>
       </c>
       <c r="D61" t="s">
-        <v>189</v>
+        <v>186</v>
       </c>
     </row>
     <row r="62" spans="1:4" ht="12.75" customHeight="1">
       <c r="A62" t="s">
-        <v>183</v>
+        <v>180</v>
       </c>
       <c r="B62" t="s">
-        <v>190</v>
+        <v>187</v>
       </c>
       <c r="D62" t="s">
-        <v>191</v>
+        <v>188</v>
       </c>
     </row>
     <row r="63" spans="1:4" ht="12.75" customHeight="1">
       <c r="A63" t="s">
-        <v>183</v>
+        <v>180</v>
       </c>
       <c r="B63" t="s">
-        <v>192</v>
+        <v>189</v>
       </c>
       <c r="D63" t="s">
-        <v>193</v>
+        <v>190</v>
       </c>
     </row>
     <row r="65" spans="1:4" ht="12.75" customHeight="1">
       <c r="A65" t="s">
-        <v>194</v>
+        <v>191</v>
       </c>
       <c r="B65" t="s">
-        <v>195</v>
+        <v>192</v>
       </c>
       <c r="D65" t="s">
-        <v>196</v>
+        <v>193</v>
       </c>
     </row>
     <row r="66" spans="1:4" ht="12.75" customHeight="1">
       <c r="A66" t="s">
+        <v>191</v>
+      </c>
+      <c r="B66" t="s">
         <v>194</v>
-      </c>
-      <c r="B66" t="s">
-        <v>197</v>
       </c>
       <c r="C66" s="2"/>
       <c r="D66" t="s">
-        <v>198</v>
+        <v>195</v>
       </c>
     </row>
     <row r="67" spans="1:4" ht="12.75" customHeight="1">
       <c r="A67" t="s">
-        <v>194</v>
+        <v>191</v>
       </c>
       <c r="B67" t="s">
-        <v>199</v>
+        <v>196</v>
       </c>
       <c r="D67" t="s">
-        <v>200</v>
+        <v>197</v>
       </c>
     </row>
     <row r="68" spans="1:4" ht="12.75" customHeight="1">
       <c r="A68" t="s">
-        <v>194</v>
+        <v>191</v>
       </c>
       <c r="B68" t="s">
-        <v>201</v>
+        <v>198</v>
       </c>
       <c r="D68" t="s">
-        <v>202</v>
+        <v>199</v>
       </c>
     </row>
     <row r="69" spans="1:4" ht="12.75" customHeight="1">
       <c r="A69" t="s">
-        <v>194</v>
+        <v>191</v>
       </c>
       <c r="B69" t="s">
-        <v>203</v>
+        <v>200</v>
       </c>
       <c r="D69" t="s">
-        <v>204</v>
+        <v>201</v>
       </c>
     </row>
     <row r="70" spans="1:4" ht="12.75" customHeight="1">
       <c r="A70" t="s">
-        <v>194</v>
+        <v>191</v>
       </c>
       <c r="B70" t="s">
-        <v>205</v>
+        <v>202</v>
       </c>
       <c r="D70" t="s">
-        <v>206</v>
+        <v>203</v>
       </c>
     </row>
     <row r="71" spans="1:4" ht="12.75" customHeight="1">
       <c r="A71" t="s">
-        <v>194</v>
+        <v>191</v>
       </c>
       <c r="B71" t="s">
-        <v>207</v>
+        <v>204</v>
       </c>
       <c r="D71" t="s">
-        <v>208</v>
+        <v>205</v>
       </c>
     </row>
     <row r="73" spans="1:4" ht="12.75" customHeight="1">
       <c r="A73" t="s">
-        <v>209</v>
+        <v>206</v>
       </c>
       <c r="B73" t="s">
-        <v>210</v>
+        <v>207</v>
       </c>
       <c r="D73" t="s">
-        <v>211</v>
+        <v>208</v>
       </c>
     </row>
     <row r="74" spans="1:4" ht="12.75" customHeight="1">
       <c r="A74" t="s">
+        <v>206</v>
+      </c>
+      <c r="B74" t="s">
         <v>209</v>
-      </c>
-      <c r="B74" t="s">
-        <v>212</v>
       </c>
       <c r="C74" s="2"/>
       <c r="D74" t="s">
-        <v>213</v>
+        <v>210</v>
       </c>
     </row>
     <row r="75" spans="1:4" ht="12.75" customHeight="1">
       <c r="A75" t="s">
-        <v>209</v>
+        <v>206</v>
       </c>
       <c r="B75" t="s">
-        <v>214</v>
+        <v>211</v>
       </c>
       <c r="D75" t="s">
-        <v>215</v>
+        <v>212</v>
       </c>
     </row>
     <row r="76" spans="1:4" ht="12.75" customHeight="1">
       <c r="A76" t="s">
-        <v>209</v>
+        <v>206</v>
       </c>
       <c r="B76" t="s">
-        <v>216</v>
+        <v>213</v>
       </c>
       <c r="D76" t="s">
-        <v>217</v>
+        <v>214</v>
       </c>
     </row>
     <row r="77" spans="1:4" ht="12.75" customHeight="1">
       <c r="A77" t="s">
-        <v>209</v>
+        <v>206</v>
       </c>
       <c r="B77" t="s">
-        <v>218</v>
+        <v>215</v>
       </c>
       <c r="D77" t="s">
-        <v>219</v>
+        <v>216</v>
       </c>
     </row>
     <row r="78" spans="1:4" ht="12.75" customHeight="1">
       <c r="A78" t="s">
-        <v>209</v>
+        <v>206</v>
       </c>
       <c r="B78" t="s">
-        <v>220</v>
+        <v>217</v>
       </c>
       <c r="D78" t="s">
-        <v>221</v>
+        <v>218</v>
       </c>
     </row>
     <row r="80" spans="1:4" ht="12.75" customHeight="1">
       <c r="A80" t="s">
-        <v>222</v>
+        <v>219</v>
       </c>
       <c r="B80" t="s">
-        <v>223</v>
+        <v>220</v>
       </c>
       <c r="D80" t="s">
-        <v>224</v>
+        <v>221</v>
       </c>
     </row>
     <row r="81" spans="1:4" ht="12.75" customHeight="1">
       <c r="A81" t="s">
+        <v>219</v>
+      </c>
+      <c r="B81" t="s">
         <v>222</v>
-      </c>
-      <c r="B81" t="s">
-        <v>225</v>
       </c>
       <c r="C81" s="2"/>
       <c r="D81" t="s">
-        <v>226</v>
+        <v>223</v>
       </c>
     </row>
     <row r="82" spans="1:4" ht="12.75" customHeight="1">
       <c r="A82" t="s">
-        <v>222</v>
+        <v>219</v>
       </c>
       <c r="B82" t="s">
-        <v>227</v>
+        <v>224</v>
       </c>
       <c r="D82" t="s">
-        <v>228</v>
+        <v>225</v>
       </c>
     </row>
     <row r="83" spans="1:4" ht="12.75" customHeight="1">
       <c r="A83" t="s">
-        <v>222</v>
+        <v>219</v>
       </c>
       <c r="B83" t="s">
-        <v>229</v>
+        <v>226</v>
       </c>
       <c r="D83" t="s">
-        <v>230</v>
+        <v>227</v>
       </c>
     </row>
     <row r="84" spans="1:4" ht="12.75" customHeight="1">
       <c r="A84" t="s">
-        <v>222</v>
+        <v>219</v>
       </c>
       <c r="B84" t="s">
-        <v>231</v>
+        <v>228</v>
       </c>
       <c r="D84" t="s">
-        <v>232</v>
+        <v>229</v>
       </c>
     </row>
     <row r="85" spans="1:4" ht="12.75" customHeight="1">
       <c r="A85" t="s">
-        <v>222</v>
+        <v>219</v>
       </c>
       <c r="B85" t="s">
-        <v>233</v>
+        <v>230</v>
       </c>
       <c r="D85" t="s">
-        <v>234</v>
+        <v>231</v>
       </c>
     </row>
     <row r="87" spans="1:4" ht="12.75" customHeight="1">
       <c r="A87" t="s">
-        <v>235</v>
+        <v>232</v>
       </c>
       <c r="B87" t="s">
-        <v>236</v>
+        <v>233</v>
       </c>
       <c r="C87" t="s">
-        <v>237</v>
+        <v>234</v>
       </c>
     </row>
     <row r="88" spans="1:4" ht="12.75" customHeight="1">
       <c r="A88" t="s">
+        <v>232</v>
+      </c>
+      <c r="B88" t="s">
         <v>235</v>
       </c>
-      <c r="B88" t="s">
-        <v>238</v>
-      </c>
       <c r="C88" t="s">
-        <v>239</v>
+        <v>236</v>
       </c>
     </row>
     <row r="89" spans="1:4" ht="12.75" customHeight="1">
       <c r="A89" t="s">
-        <v>235</v>
+        <v>232</v>
       </c>
       <c r="B89" t="s">
-        <v>240</v>
+        <v>237</v>
       </c>
       <c r="C89" t="s">
-        <v>241</v>
+        <v>238</v>
       </c>
     </row>
     <row r="90" spans="1:4" ht="12.75" customHeight="1">
       <c r="A90" t="s">
-        <v>235</v>
+        <v>232</v>
       </c>
       <c r="B90" t="s">
-        <v>242</v>
+        <v>239</v>
       </c>
       <c r="C90" t="s">
-        <v>243</v>
+        <v>240</v>
       </c>
     </row>
     <row r="91" spans="1:4" ht="12.75" customHeight="1">
       <c r="A91" t="s">
-        <v>235</v>
+        <v>232</v>
       </c>
       <c r="B91" t="s">
-        <v>244</v>
+        <v>241</v>
       </c>
       <c r="C91" t="s">
-        <v>245</v>
+        <v>242</v>
       </c>
     </row>
     <row r="92" spans="1:4" ht="12.75" customHeight="1">
       <c r="A92" t="s">
-        <v>235</v>
+        <v>232</v>
       </c>
       <c r="B92" t="s">
-        <v>246</v>
+        <v>243</v>
       </c>
       <c r="C92" t="s">
-        <v>247</v>
+        <v>244</v>
       </c>
     </row>
     <row r="93" spans="1:4" ht="12.75" customHeight="1">
       <c r="A93" t="s">
-        <v>235</v>
+        <v>232</v>
       </c>
       <c r="B93" t="s">
-        <v>248</v>
+        <v>245</v>
       </c>
       <c r="C93" t="s">
-        <v>249</v>
+        <v>246</v>
       </c>
     </row>
     <row r="95" spans="1:4" ht="12.75" customHeight="1">
       <c r="A95" t="s">
-        <v>250</v>
+        <v>247</v>
       </c>
       <c r="B95" t="s">
-        <v>251</v>
+        <v>248</v>
       </c>
       <c r="C95" t="s">
-        <v>252</v>
+        <v>249</v>
       </c>
     </row>
     <row r="96" spans="1:4" ht="12.75" customHeight="1">
       <c r="A96" t="s">
+        <v>247</v>
+      </c>
+      <c r="B96" t="s">
         <v>250</v>
       </c>
-      <c r="B96" t="s">
-        <v>253</v>
-      </c>
       <c r="C96" t="s">
-        <v>254</v>
+        <v>251</v>
       </c>
     </row>
     <row r="97" spans="1:3" ht="12.75" customHeight="1">
       <c r="A97" t="s">
-        <v>250</v>
+        <v>247</v>
       </c>
       <c r="B97" t="s">
-        <v>255</v>
+        <v>252</v>
       </c>
       <c r="C97" t="s">
-        <v>256</v>
+        <v>253</v>
       </c>
     </row>
     <row r="98" spans="1:3" ht="12.75" customHeight="1">
       <c r="A98" t="s">
-        <v>250</v>
+        <v>247</v>
       </c>
       <c r="B98" t="s">
-        <v>257</v>
+        <v>254</v>
       </c>
       <c r="C98" t="s">
-        <v>258</v>
+        <v>255</v>
       </c>
     </row>
     <row r="99" spans="1:3" ht="12.75" customHeight="1">
       <c r="A99" t="s">
-        <v>250</v>
+        <v>247</v>
       </c>
       <c r="B99" t="s">
-        <v>259</v>
+        <v>256</v>
       </c>
       <c r="C99" t="s">
-        <v>260</v>
+        <v>257</v>
       </c>
     </row>
     <row r="100" spans="1:3" ht="12.75" customHeight="1">
       <c r="A100" t="s">
-        <v>250</v>
+        <v>247</v>
       </c>
       <c r="B100" t="s">
-        <v>261</v>
+        <v>258</v>
       </c>
       <c r="C100" t="s">
-        <v>262</v>
+        <v>259</v>
       </c>
     </row>
     <row r="102" spans="1:3" ht="12.75" customHeight="1">
       <c r="A102" t="s">
-        <v>263</v>
+        <v>260</v>
       </c>
       <c r="B102" t="s">
-        <v>264</v>
+        <v>261</v>
       </c>
       <c r="C102" t="s">
-        <v>265</v>
+        <v>262</v>
       </c>
     </row>
     <row r="103" spans="1:3" ht="12.75" customHeight="1">
       <c r="A103" t="s">
+        <v>260</v>
+      </c>
+      <c r="B103" t="s">
         <v>263</v>
       </c>
-      <c r="B103" t="s">
-        <v>266</v>
-      </c>
       <c r="C103" t="s">
-        <v>267</v>
+        <v>264</v>
       </c>
     </row>
     <row r="104" spans="1:3" ht="12.75" customHeight="1">
       <c r="A104" t="s">
-        <v>263</v>
+        <v>260</v>
       </c>
       <c r="B104" t="s">
-        <v>268</v>
+        <v>265</v>
       </c>
       <c r="C104" t="s">
-        <v>269</v>
+        <v>266</v>
       </c>
     </row>
     <row r="105" spans="1:3" ht="12.75" customHeight="1">
       <c r="A105" t="s">
-        <v>263</v>
+        <v>260</v>
       </c>
       <c r="B105" t="s">
-        <v>270</v>
+        <v>267</v>
       </c>
       <c r="C105" t="s">
-        <v>271</v>
+        <v>268</v>
       </c>
     </row>
     <row r="106" spans="1:3" ht="12.75" customHeight="1">
       <c r="A106" t="s">
-        <v>263</v>
+        <v>260</v>
       </c>
       <c r="B106" t="s">
-        <v>272</v>
+        <v>269</v>
       </c>
       <c r="C106" t="s">
-        <v>273</v>
+        <v>270</v>
       </c>
     </row>
     <row r="107" spans="1:3" ht="12.75" customHeight="1">
       <c r="A107" t="s">
-        <v>263</v>
+        <v>260</v>
       </c>
       <c r="B107" t="s">
-        <v>274</v>
+        <v>271</v>
       </c>
       <c r="C107" t="s">
-        <v>275</v>
+        <v>272</v>
       </c>
     </row>
     <row r="108" spans="1:3" ht="12.75" customHeight="1">
       <c r="A108" t="s">
-        <v>263</v>
+        <v>260</v>
       </c>
       <c r="B108" t="s">
-        <v>276</v>
+        <v>273</v>
       </c>
       <c r="C108" t="s">
-        <v>277</v>
+        <v>274</v>
       </c>
     </row>
     <row r="110" spans="1:3" ht="12.75" customHeight="1">
       <c r="A110" t="s">
-        <v>278</v>
+        <v>275</v>
       </c>
       <c r="B110" t="s">
-        <v>279</v>
+        <v>276</v>
       </c>
       <c r="C110" t="s">
-        <v>280</v>
+        <v>277</v>
       </c>
     </row>
     <row r="111" spans="1:3" ht="12.75" customHeight="1">
       <c r="A111" t="s">
+        <v>275</v>
+      </c>
+      <c r="B111" t="s">
         <v>278</v>
       </c>
-      <c r="B111" t="s">
-        <v>281</v>
-      </c>
       <c r="C111" t="s">
-        <v>282</v>
+        <v>279</v>
       </c>
     </row>
     <row r="112" spans="1:3" ht="12.75" customHeight="1">
       <c r="A112" t="s">
-        <v>278</v>
+        <v>275</v>
       </c>
       <c r="B112" t="s">
-        <v>283</v>
+        <v>280</v>
       </c>
       <c r="C112" t="s">
-        <v>284</v>
+        <v>281</v>
       </c>
     </row>
     <row r="113" spans="1:3" ht="12.75" customHeight="1">
       <c r="A113" t="s">
-        <v>278</v>
+        <v>275</v>
       </c>
       <c r="B113" t="s">
-        <v>285</v>
+        <v>282</v>
       </c>
       <c r="C113" t="s">
-        <v>286</v>
+        <v>283</v>
       </c>
     </row>
     <row r="114" spans="1:3" ht="12.75" customHeight="1">
       <c r="A114" t="s">
-        <v>278</v>
+        <v>275</v>
       </c>
       <c r="B114" t="s">
-        <v>287</v>
+        <v>284</v>
       </c>
       <c r="C114" t="s">
-        <v>288</v>
+        <v>285</v>
       </c>
     </row>
     <row r="115" spans="1:3" ht="12.75" customHeight="1">
       <c r="A115" t="s">
-        <v>278</v>
+        <v>275</v>
       </c>
       <c r="B115" t="s">
-        <v>289</v>
+        <v>286</v>
       </c>
       <c r="C115" t="s">
-        <v>290</v>
+        <v>287</v>
       </c>
     </row>
     <row r="117" spans="1:3" ht="12.75" customHeight="1">
       <c r="A117" t="s">
-        <v>291</v>
+        <v>288</v>
       </c>
       <c r="B117" t="s">
-        <v>292</v>
+        <v>289</v>
       </c>
       <c r="C117" t="s">
-        <v>293</v>
+        <v>290</v>
       </c>
     </row>
     <row r="118" spans="1:3" ht="12.75" customHeight="1">
       <c r="A118" t="s">
+        <v>288</v>
+      </c>
+      <c r="B118" t="s">
         <v>291</v>
       </c>
-      <c r="B118" t="s">
-        <v>294</v>
-      </c>
       <c r="C118" t="s">
-        <v>295</v>
+        <v>292</v>
       </c>
     </row>
     <row r="119" spans="1:3" ht="12.75" customHeight="1">
       <c r="A119" t="s">
-        <v>291</v>
+        <v>288</v>
       </c>
       <c r="B119" t="s">
-        <v>296</v>
+        <v>293</v>
       </c>
       <c r="C119" t="s">
-        <v>297</v>
+        <v>294</v>
       </c>
     </row>
     <row r="120" spans="1:3" ht="12.75" customHeight="1">
       <c r="A120" t="s">
-        <v>291</v>
+        <v>288</v>
       </c>
       <c r="B120" t="s">
-        <v>298</v>
+        <v>295</v>
       </c>
       <c r="C120" t="s">
-        <v>299</v>
+        <v>296</v>
       </c>
     </row>
     <row r="121" spans="1:3" ht="12.75" customHeight="1">
       <c r="A121" t="s">
-        <v>291</v>
+        <v>288</v>
       </c>
       <c r="B121" t="s">
-        <v>300</v>
+        <v>297</v>
       </c>
       <c r="C121" t="s">
-        <v>301</v>
+        <v>298</v>
       </c>
     </row>
     <row r="122" spans="1:3" ht="12.75" customHeight="1">
       <c r="A122" t="s">
-        <v>291</v>
+        <v>288</v>
       </c>
       <c r="B122" t="s">
-        <v>302</v>
+        <v>299</v>
       </c>
       <c r="C122" t="s">
-        <v>303</v>
+        <v>300</v>
       </c>
     </row>
     <row r="123" spans="1:3" ht="12.75" customHeight="1">
       <c r="A123" t="s">
-        <v>291</v>
+        <v>288</v>
       </c>
       <c r="B123" t="s">
-        <v>304</v>
+        <v>301</v>
       </c>
       <c r="C123" t="s">
-        <v>305</v>
+        <v>302</v>
       </c>
     </row>
     <row r="125" spans="1:3" ht="12.75" customHeight="1">
       <c r="A125" t="s">
-        <v>306</v>
+        <v>303</v>
       </c>
       <c r="B125" t="s">
-        <v>307</v>
+        <v>304</v>
       </c>
       <c r="C125" t="s">
-        <v>308</v>
+        <v>305</v>
       </c>
     </row>
     <row r="126" spans="1:3" ht="12.75" customHeight="1">
       <c r="A126" t="s">
+        <v>303</v>
+      </c>
+      <c r="B126" t="s">
         <v>306</v>
       </c>
-      <c r="B126" t="s">
-        <v>309</v>
-      </c>
       <c r="C126" t="s">
-        <v>310</v>
+        <v>307</v>
       </c>
     </row>
     <row r="127" spans="1:3" ht="12.75" customHeight="1">
       <c r="A127" t="s">
-        <v>306</v>
+        <v>303</v>
       </c>
       <c r="B127" t="s">
-        <v>311</v>
+        <v>308</v>
       </c>
       <c r="C127" t="s">
-        <v>312</v>
+        <v>309</v>
       </c>
     </row>
     <row r="128" spans="1:3" ht="12.75" customHeight="1">
       <c r="A128" t="s">
-        <v>306</v>
+        <v>303</v>
       </c>
       <c r="B128" t="s">
-        <v>313</v>
+        <v>310</v>
       </c>
       <c r="C128" t="s">
-        <v>314</v>
+        <v>311</v>
       </c>
     </row>
     <row r="129" spans="1:4" ht="12.75" customHeight="1">
       <c r="A129" t="s">
-        <v>306</v>
+        <v>303</v>
       </c>
       <c r="B129" t="s">
-        <v>315</v>
+        <v>312</v>
       </c>
       <c r="C129" t="s">
-        <v>316</v>
+        <v>313</v>
       </c>
     </row>
     <row r="130" spans="1:4" ht="12.75" customHeight="1">
       <c r="A130" t="s">
-        <v>306</v>
+        <v>303</v>
       </c>
       <c r="B130" t="s">
-        <v>317</v>
+        <v>314</v>
       </c>
       <c r="C130" t="s">
-        <v>318</v>
+        <v>315</v>
       </c>
     </row>
     <row r="132" spans="1:4" ht="12.75" customHeight="1">
       <c r="A132" t="s">
-        <v>319</v>
+        <v>316</v>
       </c>
       <c r="B132" t="s">
-        <v>320</v>
+        <v>317</v>
       </c>
       <c r="C132" t="s">
-        <v>321</v>
+        <v>318</v>
       </c>
     </row>
     <row r="133" spans="1:4" ht="12.75" customHeight="1">
       <c r="A133" t="s">
+        <v>316</v>
+      </c>
+      <c r="B133" t="s">
         <v>319</v>
       </c>
-      <c r="B133" t="s">
-        <v>322</v>
-      </c>
       <c r="C133" t="s">
-        <v>323</v>
+        <v>320</v>
       </c>
     </row>
     <row r="135" spans="1:4" ht="12.75" customHeight="1">
       <c r="A135" s="2" t="s">
-        <v>324</v>
+        <v>321</v>
       </c>
       <c r="D135" t="s">
-        <v>325</v>
+        <v>322</v>
       </c>
     </row>
     <row r="136" spans="1:4" ht="12.75" customHeight="1">
       <c r="A136" t="s">
-        <v>324</v>
+        <v>321</v>
       </c>
       <c r="D136" t="s">
-        <v>326</v>
+        <v>323</v>
       </c>
     </row>
     <row r="137" spans="1:4" ht="12.75" customHeight="1">
       <c r="A137" s="2" t="s">
+        <v>321</v>
+      </c>
+      <c r="D137" t="s">
         <v>324</v>
-      </c>
-      <c r="D137" t="s">
-        <v>327</v>
       </c>
     </row>
     <row r="138" spans="1:4" ht="12.75" customHeight="1">
       <c r="A138" s="2" t="s">
-        <v>324</v>
+        <v>321</v>
       </c>
       <c r="D138" t="s">
-        <v>328</v>
+        <v>325</v>
       </c>
     </row>
     <row r="139" spans="1:4" ht="12.75" customHeight="1">
       <c r="A139" s="2" t="s">
-        <v>324</v>
+        <v>321</v>
       </c>
       <c r="D139" t="s">
-        <v>329</v>
+        <v>326</v>
       </c>
     </row>
   </sheetData>
@@ -6768,151 +6765,151 @@
     </row>
     <row r="4" spans="1:2" ht="12.75" customHeight="1">
       <c r="A4" t="s">
-        <v>330</v>
+        <v>327</v>
       </c>
       <c r="B4" t="s">
-        <v>331</v>
+        <v>328</v>
       </c>
     </row>
     <row r="5" spans="1:2" ht="12.75" customHeight="1">
       <c r="A5" t="s">
-        <v>332</v>
+        <v>329</v>
       </c>
       <c r="B5" t="s">
-        <v>333</v>
+        <v>330</v>
       </c>
     </row>
     <row r="6" spans="1:2" ht="12.75" customHeight="1">
       <c r="A6" t="s">
-        <v>334</v>
+        <v>331</v>
       </c>
       <c r="B6" t="s">
-        <v>335</v>
+        <v>332</v>
       </c>
     </row>
     <row r="8" spans="1:2" ht="12" customHeight="1">
       <c r="A8" t="s">
-        <v>336</v>
+        <v>333</v>
       </c>
       <c r="B8" t="s">
-        <v>337</v>
+        <v>334</v>
       </c>
     </row>
     <row r="9" spans="1:2" ht="12" customHeight="1">
       <c r="A9" t="s">
-        <v>338</v>
+        <v>335</v>
       </c>
       <c r="B9" t="s">
-        <v>339</v>
+        <v>336</v>
       </c>
     </row>
     <row r="10" spans="1:2" ht="12" customHeight="1">
       <c r="A10" t="s">
-        <v>340</v>
+        <v>337</v>
       </c>
       <c r="B10" t="s">
-        <v>341</v>
+        <v>338</v>
       </c>
     </row>
     <row r="11" spans="1:2" ht="12" customHeight="1">
       <c r="A11" t="s">
-        <v>342</v>
+        <v>339</v>
       </c>
       <c r="B11" t="s">
-        <v>343</v>
+        <v>340</v>
       </c>
     </row>
     <row r="12" spans="1:2" ht="12" customHeight="1">
       <c r="A12" t="s">
-        <v>344</v>
+        <v>341</v>
       </c>
       <c r="B12" t="s">
-        <v>345</v>
+        <v>342</v>
       </c>
     </row>
     <row r="13" spans="1:2" ht="12" customHeight="1">
       <c r="A13" t="s">
-        <v>346</v>
+        <v>343</v>
       </c>
       <c r="B13" t="s">
-        <v>347</v>
+        <v>344</v>
       </c>
     </row>
     <row r="14" spans="1:2" ht="42" customHeight="1">
       <c r="A14" t="s">
-        <v>348</v>
+        <v>345</v>
       </c>
       <c r="B14" t="s">
-        <v>349</v>
+        <v>346</v>
       </c>
     </row>
     <row r="15" spans="1:2" ht="12.75" customHeight="1">
       <c r="A15" t="s">
-        <v>350</v>
+        <v>347</v>
       </c>
       <c r="B15" t="s">
-        <v>351</v>
+        <v>348</v>
       </c>
     </row>
     <row r="16" spans="1:2" ht="12.75" customHeight="1">
       <c r="A16" t="s">
-        <v>352</v>
+        <v>349</v>
       </c>
       <c r="B16" t="s">
-        <v>353</v>
+        <v>350</v>
       </c>
     </row>
     <row r="17" spans="1:2" ht="12.75" customHeight="1">
       <c r="A17" t="s">
-        <v>354</v>
+        <v>351</v>
       </c>
       <c r="B17" t="s">
-        <v>355</v>
+        <v>352</v>
       </c>
     </row>
     <row r="18" spans="1:2" ht="12.75" customHeight="1">
       <c r="A18" t="s">
-        <v>356</v>
+        <v>353</v>
       </c>
       <c r="B18" t="s">
-        <v>357</v>
+        <v>354</v>
       </c>
     </row>
     <row r="19" spans="1:2" ht="12.75" customHeight="1">
       <c r="A19" t="s">
-        <v>358</v>
+        <v>355</v>
       </c>
       <c r="B19" t="s">
-        <v>359</v>
+        <v>356</v>
       </c>
     </row>
     <row r="20" spans="1:2" ht="12.75" customHeight="1">
       <c r="A20" t="s">
-        <v>360</v>
+        <v>357</v>
       </c>
       <c r="B20" t="s">
-        <v>361</v>
+        <v>358</v>
       </c>
     </row>
     <row r="21" spans="1:2" ht="12.75" customHeight="1">
       <c r="A21" t="s">
-        <v>362</v>
+        <v>359</v>
       </c>
       <c r="B21" t="s">
-        <v>363</v>
+        <v>360</v>
       </c>
     </row>
     <row r="22" spans="1:2" ht="12.75" customHeight="1">
       <c r="A22" t="s">
-        <v>364</v>
+        <v>361</v>
       </c>
       <c r="B22" t="s">
-        <v>365</v>
+        <v>362</v>
       </c>
     </row>
     <row r="24" spans="1:2" ht="12.75" customHeight="1">
       <c r="A24" t="s">
-        <v>366</v>
+        <v>363</v>
       </c>
       <c r="B24" t="s">
         <v>51</v>
@@ -6920,10 +6917,10 @@
     </row>
     <row r="25" spans="1:2" ht="12.75" customHeight="1">
       <c r="A25" t="s">
-        <v>367</v>
+        <v>364</v>
       </c>
       <c r="B25" t="s">
-        <v>368</v>
+        <v>365</v>
       </c>
     </row>
     <row r="26" spans="1:2" ht="12.75" customHeight="1">
@@ -6931,7 +6928,7 @@
         <v>39</v>
       </c>
       <c r="B26" t="s">
-        <v>369</v>
+        <v>366</v>
       </c>
     </row>
     <row r="27" spans="1:2" ht="12.75" customHeight="1">
@@ -6939,7 +6936,7 @@
         <v>38</v>
       </c>
       <c r="B27" t="s">
-        <v>370</v>
+        <v>367</v>
       </c>
     </row>
     <row r="28" spans="1:2" ht="12.75" customHeight="1">
@@ -7080,7 +7077,7 @@
         <v>9</v>
       </c>
       <c r="B2" t="s">
-        <v>385</v>
+        <v>382</v>
       </c>
     </row>
     <row r="3" spans="1:2" ht="12.75" customHeight="1">
@@ -7088,7 +7085,7 @@
         <v>10</v>
       </c>
       <c r="B3" t="s">
-        <v>386</v>
+        <v>383</v>
       </c>
     </row>
     <row r="4" spans="1:2" ht="12.75" customHeight="1">
@@ -7096,7 +7093,7 @@
         <v>11</v>
       </c>
       <c r="B4" t="s">
-        <v>385</v>
+        <v>382</v>
       </c>
     </row>
   </sheetData>
@@ -7124,15 +7121,15 @@
         <v>1</v>
       </c>
       <c r="B1" t="s">
-        <v>387</v>
+        <v>384</v>
       </c>
     </row>
     <row r="2" spans="1:2">
       <c r="A2" t="s">
-        <v>388</v>
+        <v>385</v>
       </c>
       <c r="B2" t="s">
-        <v>389</v>
+        <v>386</v>
       </c>
     </row>
     <row r="3" spans="1:2">
@@ -7140,15 +7137,15 @@
         <v>137</v>
       </c>
       <c r="B3" t="s">
-        <v>389</v>
+        <v>386</v>
       </c>
     </row>
     <row r="4" spans="1:2">
       <c r="A4" t="s">
-        <v>390</v>
+        <v>387</v>
       </c>
       <c r="B4" t="s">
-        <v>389</v>
+        <v>386</v>
       </c>
     </row>
   </sheetData>

</xml_diff>